<commit_message>
eerste 5 bioscoop data af
</commit_message>
<xml_diff>
--- a/documentatie_And_sql/documentatie/BioscoopData.xlsx
+++ b/documentatie_And_sql/documentatie/BioscoopData.xlsx
@@ -9,12 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7350" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7350" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="almere" sheetId="1" r:id="rId1"/>
     <sheet name="breda" sheetId="2" r:id="rId2"/>
     <sheet name="schagen" sheetId="3" r:id="rId3"/>
+    <sheet name="Hoofddorp" sheetId="4" r:id="rId4"/>
+    <sheet name="den bossh" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="131">
   <si>
     <t>tarieven</t>
   </si>
@@ -110,9 +112,6 @@
   </si>
   <si>
     <t>U kunt ons met de trein en bus zeer makkelijk bereiken. Vanaf station Almere Centrum loopt u in circa 5 minuten in zuidelijke richting richting naar Almere Citymall. Kinepolis Almere is tevens goed bereikbaar per bus via haltes Passage (buslijn M1 &amp; M4) en Flevoziekenhuis (buslijn M5 en M7). Voor actuele bustijden kijkt u op 9292.nl.</t>
-  </si>
-  <si>
-    <t>utrecht</t>
   </si>
   <si>
     <t>provincie</t>
@@ -333,12 +332,127 @@
     <t>Dolby 7.1
 3D</t>
   </si>
+  <si>
+    <t>Avondvoorstelling (aanvang na 18:00 uur)</t>
+  </si>
+  <si>
+    <t>Middagvoorstelling (aanvang na 12:00 uur en voor 18:00 </t>
+  </si>
+  <si>
+    <t>Vroege Vogel Voorstellingen (aanvang voor 12:00 uur)</t>
+  </si>
+  <si>
+    <t>Love-/VIP-seats</t>
+  </si>
+  <si>
+    <t>Kinepolis CineMeerse Hoofddorp</t>
+  </si>
+  <si>
+    <t>Raadhuisplein 12</t>
+  </si>
+  <si>
+    <t>Hoofddorp</t>
+  </si>
+  <si>
+    <t>2132TZ</t>
+  </si>
+  <si>
+    <t>023-3031030</t>
+  </si>
+  <si>
+    <t>CineMeerse heeft 8 zalen met in totaal liefst 1115 luxe stoelen. Vier zalen zijn gesitueerd aan de voorzijde van het pand en de andere 4 zalen zijn achterin het pand gesitueerd. Beide gedeeltes beschikken over een eigen bar/lounge om voor de film en in de pauze jezelf te voorzien van een versnapering. CineMeerse vertoont naast alle topfilms ook Live opera, ballet en diverse live-concerten van de grootste artiesten. Ook worden er regelmatig LadiesNights, MannenAvonden en andere events georganiseerd. De zalen zijn ruim opgezet en beschikken allemaal over een wall-to-wall scherm, digitaal beeld en een 7.1 Dolby geluidssysteem. Naast alle techniek voor de films is het zitcomfort ook niet onbelangrijk en daarom hebben alle zalen extra ruime stoelen en veel beenruimte om zo optimaal van de film te kunnen genieten. Naast de normale stoelen beschikken alle zalen ook over een zo geheten twin seats rij.</t>
+  </si>
+  <si>
+    <t>Met de auto bereikt u CineMeerse door de borden richting 'Centrum' te volgen. Rondom CineMeerse is volop parkeergelegenheid. U kunt uw auto bij Q-Park Polderplein in Hoofddorp parkeren en aan de kassa van CineMeerse een waardekaart kopen. Met deze waardekaart kunt u 3 uur parkeren voor maar € 1,50*!</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>CineMeerse is goed bereikbaar per fiets. Voor de bioscoop zijn fietsenrekken aanwezig.</t>
+  </si>
+  <si>
+    <t>Onze bioscoop is rolstoelvriendelijk. Ons gebouw beschikt over meerdere liften waarmee u gemakkelijk de zalen en de foyers kunt bereiken. Op de twee etages waar de zalen zich bevinden zijn invalidentoiletten aanwezig. Zowel de foyers als de zalen zijn gelijkvloers en beschikken over speciale plaatsen voor rolstoelgebruikers. Mocht u deze zogeheten invalideplaatsen willen reserveren of als u nog vragen heeft dan kan dat via telefoonnummer: 023-3031030.</t>
+  </si>
+  <si>
+    <t>3.90m x 9.90m</t>
+  </si>
+  <si>
+    <t>HFR</t>
+  </si>
+  <si>
+    <t>3D</t>
+  </si>
+  <si>
+    <t>4.10m x 10.00m</t>
+  </si>
+  <si>
+    <t>4.40m x 10.00m</t>
+  </si>
+  <si>
+    <t>4.70m x 10.00m</t>
+  </si>
+  <si>
+    <t>4.50m x 11.00m</t>
+  </si>
+  <si>
+    <t>4.40m x 11.00m</t>
+  </si>
+  <si>
+    <t>Kinderen t/m 11 jaar</t>
+  </si>
+  <si>
+    <t>Jeugd 12 t/m 17 jaar</t>
+  </si>
+  <si>
+    <t>Studenten, CJP, 65+</t>
+  </si>
+  <si>
+    <t>Laser ULTRA</t>
+  </si>
+  <si>
+    <t>Kinepolis Den Bosch</t>
+  </si>
+  <si>
+    <t>Bordeslaan 510</t>
+  </si>
+  <si>
+    <t>5223MX</t>
+  </si>
+  <si>
+    <t>Den Bosch</t>
+  </si>
+  <si>
+    <t>073-200 4600</t>
+  </si>
+  <si>
+    <t>Noord-brabant</t>
+  </si>
+  <si>
+    <t>flevoland</t>
+  </si>
+  <si>
+    <t>Op 25 juni 2018 opent Kinepolis in het Paleiskwartier van Den Bosch een gloednieuwe bioscoop met 7 zalen en zo'n 1000 stoelen. Het leukste uitje in het donker is uitstekend te bereiken met het OV en de auto, want we bieden sterk gereduceerde tarieven voor de Paleisgarage. Kinepolis Den Bosch is een volledige laserprojectie bioscoop wat resulteert in haarscherp beeld. De grootste zaal is uitgerust met Laser ULTRA, een exclusieve combinatie van spectaculair laserbeeld (4K projectie) en het ruimtelijke geluid van Dolby Atmos (uit maar liefst 64 speakers!). De rest van de zalen hebben Dolby 7.1 Geluid. 3D ontbreekt natuurlijk ook niet!  </t>
+  </si>
+  <si>
+    <t>De bioscoop ligt op 5 minuten loopafstand van het centraal station. Met de bus kunt u ook in- en uitstappen bij de halte aan de onderwijsboulevard. Hier vindt u buslijnen: 8-9-121-135-136-203-207-239- 300-301-600-621-628-639-643. U kunt dus ook makkelijk vanaf de omliggende steden en dorpen met openbaar vervoer naar de bioscoop.</t>
+  </si>
+  <si>
+    <t>Voor de bioscoop is er plaats voor bijna 400 fietsen. Wij vragen u vriendelijk om uw fiets in de rekken te plaatsen zodat er genoeg loop- en fietsruimte is voor iedereen. Dank u voor uw medewerking. </t>
+  </si>
+  <si>
+    <t>Kinepolis Den Bosch heeft mindervaliden plaatsen in elke zaal. Een lift en mindervaliden toilet zijn tevens aanwezig.</t>
+  </si>
+  <si>
+    <t>Met de auto kunt u de bioscoop makkelijk bereiken. Let op: stel uw navigatie in op Spiegeltuin 1, Den Bosch. Hiermee komt u uit bij de Paleisgarage. In deze garage krijgt u tot 50% korting op het reguliere tarief tot maximaal 4 uur. U betaalt dan overdag tot 18.00 uur nog maar € 1,15 per uur en na 18.00 uur nog maar € 0.50 per uur. Aan de kassa’s in de bioscoop kunt u deze korting verkrijgen. Na het parkeren neemt u de uitgang “Belvedere” U zult ons vinden naast de Happy Italy. De parkeergarage is voorzien van parkeren voor minder validen en een lift. Er zijn tevens plaatsen om uw elektrische auto weer op te laden.
+Via de randweg/vlijmenseweg en magistratenlaan komt u makkelijk in het Paleiskwartier uit. Volg de borden naar JBZ ziekenhuis vanaf de A2, A76, A59 en neem de afslag naar het JB ziekenhuis via de randweg.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -383,8 +497,12 @@
       <sz val="10"/>
       <name val="Montserrat"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Montserrat"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -397,8 +515,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE8EDED"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEEEEEE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -432,11 +562,91 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF064460"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF064460"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF064460"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF064460"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF064460"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF064460"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF064460"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF064460"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF064460"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF064460"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF064460"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF064460"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -472,6 +682,83 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -755,7 +1042,7 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView topLeftCell="B9" workbookViewId="0">
-      <selection activeCell="E24" sqref="A1:XFD1048576"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -886,16 +1173,16 @@
         <v>18</v>
       </c>
       <c r="E18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F18" t="s">
         <v>21</v>
       </c>
       <c r="G18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I18" t="s">
         <v>23</v>
@@ -907,7 +1194,7 @@
         <v>25</v>
       </c>
       <c r="L18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -924,16 +1211,16 @@
         <v>14</v>
       </c>
       <c r="E19" t="s">
-        <v>28</v>
+        <v>125</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>22</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>26</v>
@@ -942,15 +1229,15 @@
         <v>27</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="23.25">
       <c r="A22" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -960,25 +1247,25 @@
     </row>
     <row r="23" spans="1:12">
       <c r="A23" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B23" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="D23" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="E23" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="F23" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="F23" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" ht="75">
+    </row>
+    <row r="24" spans="1:12" ht="30">
       <c r="A24" s="4">
         <v>1</v>
       </c>
@@ -989,16 +1276,16 @@
         <v>2</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="75">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="30">
       <c r="A25" s="4">
         <v>2</v>
       </c>
@@ -1009,13 +1296,13 @@
         <v>2</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -1029,13 +1316,13 @@
         <v>2</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K26" s="2"/>
     </row>
@@ -1050,13 +1337,13 @@
         <v>2</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E27" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="F27" s="7" t="s">
         <v>56</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:12">
@@ -1070,13 +1357,13 @@
         <v>2</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E28" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="F28" s="7" t="s">
         <v>56</v>
-      </c>
-      <c r="F28" s="7" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:12">
@@ -1090,13 +1377,13 @@
         <v>2</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="28.5">
@@ -1110,13 +1397,13 @@
         <v>2</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="28.5">
@@ -1130,13 +1417,13 @@
         <v>2</v>
       </c>
       <c r="D31" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E31" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="E31" s="8" t="s">
-        <v>55</v>
-      </c>
       <c r="F31" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1285,16 +1572,16 @@
         <v>18</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F18" s="13" t="s">
         <v>21</v>
       </c>
       <c r="G18" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H18" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I18" s="13" t="s">
         <v>23</v>
@@ -1306,50 +1593,50 @@
         <v>25</v>
       </c>
       <c r="L18" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="D19" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="E19" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="F19" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="G19" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="H19" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="I19" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="J19" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="K19" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="H19" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="I19" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="J19" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="K19" s="18" t="s">
+      <c r="L19" s="18" t="s">
         <v>65</v>
-      </c>
-      <c r="L19" s="18" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="23.25">
       <c r="A22" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B22" s="12"/>
       <c r="C22" s="12"/>
@@ -1359,22 +1646,22 @@
     </row>
     <row r="23" spans="1:12">
       <c r="A23" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B23" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="D23" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D23" s="12" t="s">
+      <c r="E23" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="E23" s="12" t="s">
+      <c r="F23" s="12" t="s">
         <v>41</v>
-      </c>
-      <c r="F23" s="12" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="28.5">
@@ -1388,16 +1675,16 @@
         <v>4</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="28.5">
@@ -1411,13 +1698,13 @@
         <v>4</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="28.5">
@@ -1431,13 +1718,13 @@
         <v>4</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K26" s="3"/>
     </row>
@@ -1452,13 +1739,13 @@
         <v>4</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="42.75">
@@ -1472,13 +1759,13 @@
         <v>4</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="28.5">
@@ -1492,13 +1779,13 @@
         <v>4</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="57.75" thickBot="1">
@@ -1512,13 +1799,13 @@
         <v>8</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="42.75">
@@ -1532,13 +1819,13 @@
         <v>4</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H31" s="14"/>
     </row>
@@ -1553,13 +1840,13 @@
         <v>4</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H32" s="15"/>
     </row>
@@ -1574,13 +1861,13 @@
         <v>4</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F33" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1592,8 +1879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H31" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1728,16 +2015,16 @@
         <v>18</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F18" s="13" t="s">
         <v>21</v>
       </c>
       <c r="G18" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H18" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I18" s="13" t="s">
         <v>23</v>
@@ -1749,50 +2036,50 @@
         <v>25</v>
       </c>
       <c r="L18" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="E19" s="13" t="s">
         <v>80</v>
-      </c>
-      <c r="E19" s="13" t="s">
-        <v>81</v>
       </c>
       <c r="F19" s="1">
         <v>31224224060</v>
       </c>
       <c r="G19" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H19" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="I19" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="H19" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="I19" s="1" t="s">
+      <c r="J19" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="J19" s="1" t="s">
+      <c r="K19" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="K19" s="1" t="s">
+      <c r="L19" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="L19" s="1" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="23.25">
       <c r="A22" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B22" s="12"/>
       <c r="C22" s="12"/>
@@ -1802,22 +2089,22 @@
     </row>
     <row r="23" spans="1:12">
       <c r="A23" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B23" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="D23" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D23" s="12" t="s">
+      <c r="E23" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="E23" s="12" t="s">
+      <c r="F23" s="12" t="s">
         <v>41</v>
-      </c>
-      <c r="F23" s="12" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="28.5">
@@ -1831,17 +2118,17 @@
         <v>4</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E24" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F24" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="F24" s="6" t="s">
-        <v>93</v>
-      </c>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="1:12" ht="28.5">
+    <row r="25" spans="1:12">
       <c r="A25" s="12">
         <v>2</v>
       </c>
@@ -1852,16 +2139,16 @@
         <v>4</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" ht="28.5">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
       <c r="A26" s="12">
         <v>3</v>
       </c>
@@ -1872,17 +2159,17 @@
         <v>2</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K26" s="3"/>
     </row>
-    <row r="27" spans="1:12" ht="28.5">
+    <row r="27" spans="1:12">
       <c r="A27" s="12">
         <v>4</v>
       </c>
@@ -1893,16 +2180,16 @@
         <v>2</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" ht="28.5">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
       <c r="A28" s="12">
         <v>5</v>
       </c>
@@ -1913,13 +2200,13 @@
         <v>2</v>
       </c>
       <c r="D28" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E28" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="F28" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:12">
@@ -1965,4 +2252,1076 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L45"/>
+  <sheetViews>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="16.42578125" style="13" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="13"/>
+    <col min="3" max="3" width="12" style="13" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" style="13" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="13" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="13" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="13"/>
+    <col min="8" max="8" width="16.85546875" style="13" customWidth="1"/>
+    <col min="9" max="10" width="9.140625" style="13"/>
+    <col min="11" max="11" width="22.7109375" style="13" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="23.25">
+      <c r="A1" s="17" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" s="13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" s="13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B5" s="13">
+        <v>9.9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="23.25">
+      <c r="A8" s="17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B12" s="13">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="23.25">
+      <c r="A17" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="H18" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="I18" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="J18" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="K18" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="L18" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="15.75">
+      <c r="A19" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H19" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="I19" s="44" t="s">
+        <v>103</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="K19" s="44" t="s">
+        <v>105</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="23.25">
+      <c r="A22" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="41.25" customHeight="1">
+      <c r="A24" s="20"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="23"/>
+    </row>
+    <row r="25" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A25" s="24"/>
+      <c r="B25" s="25"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="27"/>
+      <c r="K25" s="3"/>
+    </row>
+    <row r="26" spans="1:12" ht="26.25" customHeight="1">
+      <c r="A26" s="28"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="31"/>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" s="32"/>
+      <c r="B27" s="33"/>
+      <c r="C27" s="33"/>
+      <c r="D27" s="33"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="34"/>
+    </row>
+    <row r="28" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A28" s="35"/>
+      <c r="B28" s="36"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="38"/>
+    </row>
+    <row r="29" spans="1:12" ht="26.25" customHeight="1" thickBot="1">
+      <c r="A29" s="39"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="41"/>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30" s="20"/>
+      <c r="B30" s="21"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="23"/>
+      <c r="H30" s="14"/>
+    </row>
+    <row r="31" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A31" s="24"/>
+      <c r="B31" s="25"/>
+      <c r="C31" s="25"/>
+      <c r="D31" s="25"/>
+      <c r="E31" s="25"/>
+      <c r="F31" s="26"/>
+      <c r="G31" s="27"/>
+      <c r="H31" s="15"/>
+    </row>
+    <row r="32" spans="1:12" ht="41.25" customHeight="1">
+      <c r="A32" s="28"/>
+      <c r="B32" s="29"/>
+      <c r="C32" s="29"/>
+      <c r="D32" s="29"/>
+      <c r="E32" s="29"/>
+      <c r="F32" s="30"/>
+      <c r="G32" s="31"/>
+    </row>
+    <row r="33" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A33" s="35"/>
+      <c r="B33" s="36"/>
+      <c r="C33" s="36"/>
+      <c r="D33" s="36"/>
+      <c r="E33" s="36"/>
+      <c r="F33" s="37"/>
+      <c r="G33" s="38"/>
+    </row>
+    <row r="34" spans="1:7" ht="26.25" customHeight="1">
+      <c r="A34" s="39"/>
+      <c r="B34" s="40"/>
+      <c r="C34" s="40"/>
+      <c r="D34" s="40"/>
+      <c r="E34" s="40"/>
+      <c r="F34" s="22"/>
+      <c r="G34" s="41"/>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="20"/>
+      <c r="B35" s="21"/>
+      <c r="C35" s="21"/>
+      <c r="D35" s="21"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="23"/>
+    </row>
+    <row r="36" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A36" s="24"/>
+      <c r="B36" s="25"/>
+      <c r="C36" s="25"/>
+      <c r="D36" s="25"/>
+      <c r="E36" s="25"/>
+      <c r="F36" s="26"/>
+      <c r="G36" s="27"/>
+    </row>
+    <row r="37" spans="1:7" ht="26.25" customHeight="1">
+      <c r="A37" s="28"/>
+      <c r="B37" s="29"/>
+      <c r="C37" s="29"/>
+      <c r="D37" s="29"/>
+      <c r="E37" s="29"/>
+      <c r="F37" s="30"/>
+      <c r="G37" s="31"/>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="32"/>
+      <c r="B38" s="33"/>
+      <c r="C38" s="33"/>
+      <c r="D38" s="33"/>
+      <c r="E38" s="33"/>
+      <c r="F38" s="30"/>
+      <c r="G38" s="34"/>
+    </row>
+    <row r="39" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A39" s="35"/>
+      <c r="B39" s="36"/>
+      <c r="C39" s="36"/>
+      <c r="D39" s="36"/>
+      <c r="E39" s="36"/>
+      <c r="F39" s="37"/>
+      <c r="G39" s="38"/>
+    </row>
+    <row r="40" spans="1:7" ht="26.25" customHeight="1">
+      <c r="A40" s="39"/>
+      <c r="B40" s="40"/>
+      <c r="C40" s="40"/>
+      <c r="D40" s="40"/>
+      <c r="E40" s="40"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="41"/>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="20"/>
+      <c r="B41" s="21"/>
+      <c r="C41" s="21"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="21"/>
+      <c r="F41" s="22"/>
+      <c r="G41" s="23"/>
+    </row>
+    <row r="42" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A42" s="24"/>
+      <c r="B42" s="25"/>
+      <c r="C42" s="25"/>
+      <c r="D42" s="25"/>
+      <c r="E42" s="25"/>
+      <c r="F42" s="26"/>
+      <c r="G42" s="27"/>
+    </row>
+    <row r="43" spans="1:7" ht="26.25" customHeight="1">
+      <c r="A43" s="28"/>
+      <c r="B43" s="29"/>
+      <c r="C43" s="29"/>
+      <c r="D43" s="29"/>
+      <c r="E43" s="29"/>
+      <c r="F43" s="30"/>
+      <c r="G43" s="42"/>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" s="32"/>
+      <c r="B44" s="33"/>
+      <c r="C44" s="33"/>
+      <c r="D44" s="33"/>
+      <c r="E44" s="33"/>
+      <c r="F44" s="30"/>
+      <c r="G44" s="42"/>
+    </row>
+    <row r="45" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A45" s="35"/>
+      <c r="B45" s="36"/>
+      <c r="C45" s="36"/>
+      <c r="D45" s="36"/>
+      <c r="E45" s="36"/>
+      <c r="F45" s="37"/>
+      <c r="G45" s="43"/>
+    </row>
+  </sheetData>
+  <mergeCells count="47">
+    <mergeCell ref="A43:A45"/>
+    <mergeCell ref="B43:B45"/>
+    <mergeCell ref="C43:C45"/>
+    <mergeCell ref="D43:D45"/>
+    <mergeCell ref="E43:E45"/>
+    <mergeCell ref="A40:A42"/>
+    <mergeCell ref="B40:B42"/>
+    <mergeCell ref="C40:C42"/>
+    <mergeCell ref="D40:D42"/>
+    <mergeCell ref="E40:E42"/>
+    <mergeCell ref="G40:G42"/>
+    <mergeCell ref="A37:A39"/>
+    <mergeCell ref="B37:B39"/>
+    <mergeCell ref="C37:C39"/>
+    <mergeCell ref="D37:D39"/>
+    <mergeCell ref="E37:E39"/>
+    <mergeCell ref="G37:G39"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="B34:B36"/>
+    <mergeCell ref="C34:C36"/>
+    <mergeCell ref="D34:D36"/>
+    <mergeCell ref="E34:E36"/>
+    <mergeCell ref="G34:G36"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="D29:D31"/>
+    <mergeCell ref="E29:E31"/>
+    <mergeCell ref="G29:G31"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="D26:D28"/>
+    <mergeCell ref="E26:E28"/>
+    <mergeCell ref="G26:G28"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="G24:G25"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="16.42578125" style="13" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="13"/>
+    <col min="3" max="3" width="12" style="13" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" style="13" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="13" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="13" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="13"/>
+    <col min="8" max="8" width="16.85546875" style="13" customWidth="1"/>
+    <col min="9" max="10" width="9.140625" style="13"/>
+    <col min="11" max="11" width="22.7109375" style="13" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="23.25">
+      <c r="A1" s="17" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="13">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="B4" s="13">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="B5" s="13">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="B6" s="13">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="23.25">
+      <c r="A8" s="17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="13">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="13">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="B12" s="13">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="23.25">
+      <c r="A17" s="46" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="47"/>
+      <c r="C17" s="47"/>
+      <c r="D17" s="47"/>
+      <c r="E17" s="47"/>
+      <c r="F17" s="47"/>
+      <c r="G17" s="47"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
+      <c r="K17" s="47"/>
+      <c r="L17" s="47"/>
+    </row>
+    <row r="18" spans="1:12" ht="14.25" customHeight="1">
+      <c r="A18" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="47" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="47" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="47" t="s">
+        <v>28</v>
+      </c>
+      <c r="F18" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="H18" s="47" t="s">
+        <v>32</v>
+      </c>
+      <c r="I18" s="47" t="s">
+        <v>23</v>
+      </c>
+      <c r="J18" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="K18" s="47" t="s">
+        <v>25</v>
+      </c>
+      <c r="L18" s="47" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" s="48" t="s">
+        <v>119</v>
+      </c>
+      <c r="B19" s="48" t="s">
+        <v>120</v>
+      </c>
+      <c r="C19" s="48" t="s">
+        <v>121</v>
+      </c>
+      <c r="D19" s="48" t="s">
+        <v>122</v>
+      </c>
+      <c r="E19" s="47" t="s">
+        <v>124</v>
+      </c>
+      <c r="F19" s="48" t="s">
+        <v>123</v>
+      </c>
+      <c r="G19" s="48" t="s">
+        <v>126</v>
+      </c>
+      <c r="H19" s="47" t="s">
+        <v>33</v>
+      </c>
+      <c r="I19" s="45" t="s">
+        <v>130</v>
+      </c>
+      <c r="J19" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="K19" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="L19" s="19" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="14.25" customHeight="1">
+      <c r="I20" s="49"/>
+    </row>
+    <row r="21" spans="1:12" ht="23.25">
+      <c r="A21" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="41.25" customHeight="1">
+      <c r="A23" s="20">
+        <v>1</v>
+      </c>
+      <c r="B23" s="21">
+        <v>126</v>
+      </c>
+      <c r="C23" s="21">
+        <v>4</v>
+      </c>
+      <c r="D23" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="E23" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="F23" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="G23" s="23"/>
+    </row>
+    <row r="24" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A24" s="24"/>
+      <c r="B24" s="25"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="G24" s="27"/>
+      <c r="K24" s="3"/>
+    </row>
+    <row r="25" spans="1:12" ht="26.25" customHeight="1">
+      <c r="A25" s="28">
+        <v>2</v>
+      </c>
+      <c r="B25" s="29">
+        <v>132</v>
+      </c>
+      <c r="C25" s="29">
+        <v>4</v>
+      </c>
+      <c r="D25" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="E25" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="F25" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="G25" s="31"/>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" s="32"/>
+      <c r="B26" s="33"/>
+      <c r="C26" s="33"/>
+      <c r="D26" s="33"/>
+      <c r="E26" s="33"/>
+      <c r="F26" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="G26" s="34"/>
+    </row>
+    <row r="27" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A27" s="35"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="G27" s="38"/>
+    </row>
+    <row r="28" spans="1:12" ht="26.25" customHeight="1" thickBot="1">
+      <c r="A28" s="39">
+        <v>3</v>
+      </c>
+      <c r="B28" s="40">
+        <v>143</v>
+      </c>
+      <c r="C28" s="40">
+        <v>4</v>
+      </c>
+      <c r="D28" s="40" t="s">
+        <v>110</v>
+      </c>
+      <c r="E28" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="F28" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="G28" s="41"/>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" s="20"/>
+      <c r="B29" s="21"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="G29" s="23"/>
+      <c r="H29" s="14"/>
+    </row>
+    <row r="30" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A30" s="24"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="25"/>
+      <c r="F30" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="G30" s="27"/>
+      <c r="H30" s="15"/>
+    </row>
+    <row r="31" spans="1:12" ht="41.25" customHeight="1">
+      <c r="A31" s="28">
+        <v>4</v>
+      </c>
+      <c r="B31" s="29">
+        <v>147</v>
+      </c>
+      <c r="C31" s="29">
+        <v>4</v>
+      </c>
+      <c r="D31" s="29" t="s">
+        <v>110</v>
+      </c>
+      <c r="E31" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="F31" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="G31" s="31"/>
+    </row>
+    <row r="32" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A32" s="35"/>
+      <c r="B32" s="36"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="36"/>
+      <c r="E32" s="36"/>
+      <c r="F32" s="37" t="s">
+        <v>44</v>
+      </c>
+      <c r="G32" s="38"/>
+    </row>
+    <row r="33" spans="1:7" ht="26.25" customHeight="1">
+      <c r="A33" s="39">
+        <v>5</v>
+      </c>
+      <c r="B33" s="40">
+        <v>120</v>
+      </c>
+      <c r="C33" s="40">
+        <v>4</v>
+      </c>
+      <c r="D33" s="40" t="s">
+        <v>111</v>
+      </c>
+      <c r="E33" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="F33" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="G33" s="41"/>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="20"/>
+      <c r="B34" s="21"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="G34" s="23"/>
+    </row>
+    <row r="35" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A35" s="24"/>
+      <c r="B35" s="25"/>
+      <c r="C35" s="25"/>
+      <c r="D35" s="25"/>
+      <c r="E35" s="25"/>
+      <c r="F35" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="G35" s="27"/>
+    </row>
+    <row r="36" spans="1:7" ht="26.25" customHeight="1">
+      <c r="A36" s="28">
+        <v>6</v>
+      </c>
+      <c r="B36" s="29">
+        <v>120</v>
+      </c>
+      <c r="C36" s="29">
+        <v>4</v>
+      </c>
+      <c r="D36" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="E36" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="F36" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="G36" s="31"/>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="32"/>
+      <c r="B37" s="33"/>
+      <c r="C37" s="33"/>
+      <c r="D37" s="33"/>
+      <c r="E37" s="33"/>
+      <c r="F37" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="G37" s="34"/>
+    </row>
+    <row r="38" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A38" s="35"/>
+      <c r="B38" s="36"/>
+      <c r="C38" s="36"/>
+      <c r="D38" s="36"/>
+      <c r="E38" s="36"/>
+      <c r="F38" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="G38" s="38"/>
+    </row>
+    <row r="39" spans="1:7" ht="26.25" customHeight="1">
+      <c r="A39" s="39">
+        <v>7</v>
+      </c>
+      <c r="B39" s="40">
+        <v>148</v>
+      </c>
+      <c r="C39" s="40">
+        <v>4</v>
+      </c>
+      <c r="D39" s="40" t="s">
+        <v>113</v>
+      </c>
+      <c r="E39" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="F39" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="G39" s="41"/>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="20"/>
+      <c r="B40" s="21"/>
+      <c r="C40" s="21"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="21"/>
+      <c r="F40" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="G40" s="23"/>
+    </row>
+    <row r="41" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A41" s="24"/>
+      <c r="B41" s="25"/>
+      <c r="C41" s="25"/>
+      <c r="D41" s="25"/>
+      <c r="E41" s="25"/>
+      <c r="F41" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="G41" s="27"/>
+    </row>
+    <row r="42" spans="1:7" ht="26.25" customHeight="1">
+      <c r="A42" s="28">
+        <v>8</v>
+      </c>
+      <c r="B42" s="29">
+        <v>147</v>
+      </c>
+      <c r="C42" s="29">
+        <v>4</v>
+      </c>
+      <c r="D42" s="29" t="s">
+        <v>114</v>
+      </c>
+      <c r="E42" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="F42" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="G42" s="42"/>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" s="32"/>
+      <c r="B43" s="33"/>
+      <c r="C43" s="33"/>
+      <c r="D43" s="33"/>
+      <c r="E43" s="33"/>
+      <c r="F43" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="G43" s="42"/>
+    </row>
+    <row r="44" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A44" s="35"/>
+      <c r="B44" s="36"/>
+      <c r="C44" s="36"/>
+      <c r="D44" s="36"/>
+      <c r="E44" s="36"/>
+      <c r="F44" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="G44" s="43"/>
+    </row>
+  </sheetData>
+  <mergeCells count="47">
+    <mergeCell ref="A42:A44"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="C42:C44"/>
+    <mergeCell ref="D42:D44"/>
+    <mergeCell ref="E42:E44"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="C39:C41"/>
+    <mergeCell ref="D39:D41"/>
+    <mergeCell ref="E39:E41"/>
+    <mergeCell ref="G39:G41"/>
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="C36:C38"/>
+    <mergeCell ref="D36:D38"/>
+    <mergeCell ref="E36:E38"/>
+    <mergeCell ref="G36:G38"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="C33:C35"/>
+    <mergeCell ref="D33:D35"/>
+    <mergeCell ref="E33:E35"/>
+    <mergeCell ref="G33:G35"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="G31:G32"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="C28:C30"/>
+    <mergeCell ref="D28:D30"/>
+    <mergeCell ref="E28:E30"/>
+    <mergeCell ref="G28:G30"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="C25:C27"/>
+    <mergeCell ref="D25:D27"/>
+    <mergeCell ref="E25:E27"/>
+    <mergeCell ref="G25:G27"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="G23:G24"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
eerste 8 bioscoop data af
</commit_message>
<xml_diff>
--- a/documentatie_And_sql/documentatie/BioscoopData.xlsx
+++ b/documentatie_And_sql/documentatie/BioscoopData.xlsx
@@ -9,14 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7350" firstSheet="3" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7350" firstSheet="5" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="almere" sheetId="1" r:id="rId1"/>
     <sheet name="breda" sheetId="2" r:id="rId2"/>
     <sheet name="schagen" sheetId="3" r:id="rId3"/>
     <sheet name="Hoofddorp" sheetId="4" r:id="rId4"/>
-    <sheet name="den bossh" sheetId="5" r:id="rId5"/>
+    <sheet name="Den Bosch" sheetId="5" r:id="rId5"/>
+    <sheet name="Den Helder" sheetId="6" r:id="rId6"/>
+    <sheet name="Dordrecht" sheetId="7" r:id="rId7"/>
+    <sheet name="Blad5" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="179">
   <si>
     <t>tarieven</t>
   </si>
@@ -375,22 +378,10 @@
     <t>Onze bioscoop is rolstoelvriendelijk. Ons gebouw beschikt over meerdere liften waarmee u gemakkelijk de zalen en de foyers kunt bereiken. Op de twee etages waar de zalen zich bevinden zijn invalidentoiletten aanwezig. Zowel de foyers als de zalen zijn gelijkvloers en beschikken over speciale plaatsen voor rolstoelgebruikers. Mocht u deze zogeheten invalideplaatsen willen reserveren of als u nog vragen heeft dan kan dat via telefoonnummer: 023-3031030.</t>
   </si>
   <si>
-    <t>3.90m x 9.90m</t>
-  </si>
-  <si>
     <t>HFR</t>
   </si>
   <si>
     <t>3D</t>
-  </si>
-  <si>
-    <t>4.10m x 10.00m</t>
-  </si>
-  <si>
-    <t>4.40m x 10.00m</t>
-  </si>
-  <si>
-    <t>4.70m x 10.00m</t>
   </si>
   <si>
     <t>4.50m x 11.00m</t>
@@ -446,13 +437,169 @@
   <si>
     <t>Met de auto kunt u de bioscoop makkelijk bereiken. Let op: stel uw navigatie in op Spiegeltuin 1, Den Bosch. Hiermee komt u uit bij de Paleisgarage. In deze garage krijgt u tot 50% korting op het reguliere tarief tot maximaal 4 uur. U betaalt dan overdag tot 18.00 uur nog maar € 1,15 per uur en na 18.00 uur nog maar € 0.50 per uur. Aan de kassa’s in de bioscoop kunt u deze korting verkrijgen. Na het parkeren neemt u de uitgang “Belvedere” U zult ons vinden naast de Happy Italy. De parkeergarage is voorzien van parkeren voor minder validen en een lift. Er zijn tevens plaatsen om uw elektrische auto weer op te laden.
 Via de randweg/vlijmenseweg en magistratenlaan komt u makkelijk in het Paleiskwartier uit. Volg de borden naar JBZ ziekenhuis vanaf de A2, A76, A59 en neem de afslag naar het JB ziekenhuis via de randweg.</t>
+  </si>
+  <si>
+    <t>5.30m x 12.60m</t>
+  </si>
+  <si>
+    <t>Laser</t>
+  </si>
+  <si>
+    <t>5.15m x 12.30m</t>
+  </si>
+  <si>
+    <t>5.30m x 12.70m</t>
+  </si>
+  <si>
+    <t>5.00m x 12.00m</t>
+  </si>
+  <si>
+    <t>7.30m x 17.50m</t>
+  </si>
+  <si>
+    <t>Laser Ultra</t>
+  </si>
+  <si>
+    <t>Kinepolis Den Helder</t>
+  </si>
+  <si>
+    <t>Willemsoord 51</t>
+  </si>
+  <si>
+    <t>1781AS</t>
+  </si>
+  <si>
+    <t>Den Helder</t>
+  </si>
+  <si>
+    <t>Noord-Holland</t>
+  </si>
+  <si>
+    <t>0223-677899</t>
+  </si>
+  <si>
+    <t>Kinepolis Den Helder opende in 2003 haar deuren in gebouw 51 op Willemsoord, de voormalige scheeps- en onderhoudswerf voor de Koninklijke Marine. Verschillende details van de Oude Rijkswerf zijn intact gelaten; twee van de zalen zijn nieuw tegen de Scheepswerkerplaats aangebouwd. De bioscoop in de kop van Noord-Holland heeft in totaal 6 moderne bioscoopzalen en 776 stoelen.</t>
+  </si>
+  <si>
+    <t>In Den Helder volgt u de ANWB borden richting Willemsoord, de bioscoop bevindt zich op dit terrein. De ingang van Willemsoord zit aan de route voor de veerboot naar Texel. Parkeren kan gratis op het Willemsoord terrein.</t>
+  </si>
+  <si>
+    <t>Kinepolis Den Helder is vanaf het trein- en busstation van CS Den Helder op 10-15 minuten loopafstand. Volg hiervoor de borden 'Willemsoord'. </t>
+  </si>
+  <si>
+    <t>Willemsoord is goed bereikbaar per fiets. Volg hiervoor de borden 'Willemsoord'. Voor de bioscoop zijn fietsenrekken aanwezig.</t>
+  </si>
+  <si>
+    <t>Kinepolis Den Helder is grotendeels rolstoeltoegankelijk, neem contact op met de bioscoop voor meer informatie. Er is een lift en mindervalidentoilet aanwezig.</t>
+  </si>
+  <si>
+    <t>15.70m x 6.80m</t>
+  </si>
+  <si>
+    <t>11.00m x 4.90m</t>
+  </si>
+  <si>
+    <t>10.10m x 4.50m</t>
+  </si>
+  <si>
+    <t>Dolby Atmos</t>
+  </si>
+  <si>
+    <t>Kinepolis Dordrecht aan het Wantij is dé bioscoop voor de Drechtsteden. Met 6 moderne zalen kunt u optimaal genieten van perfect beeld en geluid. Eén van de zalen is zelfs voorzien van het nieuwe geluidssysteem Dolby Atmos, wat de filmbeleving nog intenser maakt. Voor een hapje of drankje kunt u terecht in ons Cafe+ met geweldig uitzicht over het water. Kinepolis Dordrecht is makkelijk bereikbaar met openbaar vervoer, fiets en met de auto. Er is een parkeergarage naast de bioscoop. Vraagt u bij de kassa gerust naar gereduceerde parkeertarieven bij uw filmkaartje. Ook voor uw evenementen kunt u bij ons terecht, neem daarvoor contact met ons op via bovenstaand telefoonnummer en/of het contactformulier.</t>
+  </si>
+  <si>
+    <t>Kinepolis Dordrecht</t>
+  </si>
+  <si>
+    <t>Lijnbaan 200</t>
+  </si>
+  <si>
+    <t>3311 RL</t>
+  </si>
+  <si>
+    <t>Dordrecht</t>
+  </si>
+  <si>
+    <t>078 - 782 0000</t>
+  </si>
+  <si>
+    <t>South-Holland</t>
+  </si>
+  <si>
+    <t>Met de auto kunt u ons bereiken via de Noordendijk. U volgt de borden voor parkeergarage “Energiehuis” De parkeergarage staat naast de bioscoop. Parkeren in Garage Energiehuis: €3,- voor 4 uur. Afwaarderen aan onze kassa's.</t>
+  </si>
+  <si>
+    <t>U kunt Kinepolis Dordrecht bereiken met buslijn 10, halte Energiehuis. Voor actuele bustijden kijkt u op www.arriva.nl</t>
+  </si>
+  <si>
+    <t>De parkeergarage heeft ook een zeer grote fietsenstalling.</t>
+  </si>
+  <si>
+    <t>Kinepolis Dordrecht heeft rolstoelplaatsen in elke zaal. Wilt u deze boeken? Bel of mail dan met de bioscoop. Lift en minder validentoilet zijn aanwezig. </t>
+  </si>
+  <si>
+    <t>11.37m x 4.75m</t>
+  </si>
+  <si>
+    <t>15.20m x 6.36m</t>
+  </si>
+  <si>
+    <t>13.34m x 5.58m</t>
+  </si>
+  <si>
+    <t>Atmos</t>
+  </si>
+  <si>
+    <t>65+, Studenten, CJP &amp; BankGiro Loterij VIP-KAART</t>
+  </si>
+  <si>
+    <t>Kinepolis Emmen</t>
+  </si>
+  <si>
+    <t>Westeind 70</t>
+  </si>
+  <si>
+    <t>7811 ME</t>
+  </si>
+  <si>
+    <t>Emmen</t>
+  </si>
+  <si>
+    <t>0591-668250</t>
+  </si>
+  <si>
+    <t>Kinepolis Emmen is een ware blikvanger als u Emmen via de Frieslandroute (N381) filevrij binnenrijdt. Vanaf de weg valt met name de schuin aflopende onderzijde van het gebouw op die bijna over de weg zweeft. Met meer dan voldoende parkeerplaatsen en op loopafstand van Emmen-centrum een uitstekende locatie. De moderne bioscoop met 7 zalen heeft plaats voor 1249 bezoekers in comfortabele bioscoopstoelen.</t>
+  </si>
+  <si>
+    <t>De bioscoop is makkelijk te bereiken met de auto via de afrit van de N381. Volg de borden 'P Wildlands' of 'Centrum Noord'. Voor de bioscoop is er parkeergelegenheid voor € 1,70 per 58 minuten. Na 18:00u en op donderdag na 21:00 is parkeren gratis.</t>
+  </si>
+  <si>
+    <t>Kinepolis Emmen is per trein en bus bereikbaar. Vanaf station Emmen is de bioscoop op 10 minuten loopfastand. Met de bus is de bioscoop zeer makkelijk bereiken via halte 'Centrum Emmen' of 'Frieslandweg'. Vanaf hier loopt u in enkele minuten naar de bioscoop.</t>
+  </si>
+  <si>
+    <t>De bioscoop is per fiets bereikbaar. De fietsenstalling staat tegenover de bioscoop.</t>
+  </si>
+  <si>
+    <t>Kinepolis Emmen is rolstoeltoegankelijk, elke zaal heeft 2 rolstoelplaatsen. Tevens is er een lift en een mindervalidentoilet aanwezig.</t>
+  </si>
+  <si>
+    <t>16.60m x 7.10m</t>
+  </si>
+  <si>
+    <t>12.25m x 5.40m</t>
+  </si>
+  <si>
+    <t>14.25m x 6.25m</t>
+  </si>
+  <si>
+    <t>11.25m x 4.95m</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -499,6 +646,16 @@
     </font>
     <font>
       <sz val="12"/>
+      <color rgb="FF6E7474"/>
+      <name val="Montserrat"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Montserrat"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF6E7474"/>
       <name val="Montserrat"/>
     </font>
   </fonts>
@@ -646,7 +803,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -683,6 +840,55 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -751,14 +957,77 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -1211,7 +1480,7 @@
         <v>14</v>
       </c>
       <c r="E19" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>22</v>
@@ -2419,13 +2688,13 @@
       <c r="H19" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="I19" s="44" t="s">
+      <c r="I19" s="61" t="s">
         <v>103</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="K19" s="44" t="s">
+      <c r="K19" s="61" t="s">
         <v>105</v>
       </c>
       <c r="L19" s="1" t="s">
@@ -2463,205 +2732,205 @@
       </c>
     </row>
     <row r="24" spans="1:12" ht="41.25" customHeight="1">
-      <c r="A24" s="20"/>
-      <c r="B24" s="21"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="22"/>
-      <c r="G24" s="23"/>
+      <c r="A24" s="37"/>
+      <c r="B24" s="38"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="39"/>
+      <c r="G24" s="40"/>
     </row>
     <row r="25" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A25" s="24"/>
-      <c r="B25" s="25"/>
-      <c r="C25" s="25"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="27"/>
+      <c r="A25" s="41"/>
+      <c r="B25" s="42"/>
+      <c r="C25" s="42"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="42"/>
+      <c r="F25" s="43"/>
+      <c r="G25" s="44"/>
       <c r="K25" s="3"/>
     </row>
     <row r="26" spans="1:12" ht="26.25" customHeight="1">
-      <c r="A26" s="28"/>
-      <c r="B26" s="29"/>
-      <c r="C26" s="29"/>
-      <c r="D26" s="29"/>
-      <c r="E26" s="29"/>
-      <c r="F26" s="30"/>
-      <c r="G26" s="31"/>
+      <c r="A26" s="45"/>
+      <c r="B26" s="46"/>
+      <c r="C26" s="46"/>
+      <c r="D26" s="46"/>
+      <c r="E26" s="46"/>
+      <c r="F26" s="47"/>
+      <c r="G26" s="48"/>
     </row>
     <row r="27" spans="1:12">
-      <c r="A27" s="32"/>
-      <c r="B27" s="33"/>
-      <c r="C27" s="33"/>
-      <c r="D27" s="33"/>
-      <c r="E27" s="33"/>
-      <c r="F27" s="30"/>
-      <c r="G27" s="34"/>
+      <c r="A27" s="49"/>
+      <c r="B27" s="50"/>
+      <c r="C27" s="50"/>
+      <c r="D27" s="50"/>
+      <c r="E27" s="50"/>
+      <c r="F27" s="47"/>
+      <c r="G27" s="51"/>
     </row>
     <row r="28" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A28" s="35"/>
-      <c r="B28" s="36"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="36"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="38"/>
+      <c r="A28" s="52"/>
+      <c r="B28" s="53"/>
+      <c r="C28" s="53"/>
+      <c r="D28" s="53"/>
+      <c r="E28" s="53"/>
+      <c r="F28" s="54"/>
+      <c r="G28" s="55"/>
     </row>
     <row r="29" spans="1:12" ht="26.25" customHeight="1" thickBot="1">
-      <c r="A29" s="39"/>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="22"/>
-      <c r="G29" s="41"/>
+      <c r="A29" s="56"/>
+      <c r="B29" s="57"/>
+      <c r="C29" s="57"/>
+      <c r="D29" s="57"/>
+      <c r="E29" s="57"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="58"/>
     </row>
     <row r="30" spans="1:12">
-      <c r="A30" s="20"/>
-      <c r="B30" s="21"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="22"/>
-      <c r="G30" s="23"/>
+      <c r="A30" s="37"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="39"/>
+      <c r="G30" s="40"/>
       <c r="H30" s="14"/>
     </row>
     <row r="31" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A31" s="24"/>
-      <c r="B31" s="25"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="26"/>
-      <c r="G31" s="27"/>
+      <c r="A31" s="41"/>
+      <c r="B31" s="42"/>
+      <c r="C31" s="42"/>
+      <c r="D31" s="42"/>
+      <c r="E31" s="42"/>
+      <c r="F31" s="43"/>
+      <c r="G31" s="44"/>
       <c r="H31" s="15"/>
     </row>
     <row r="32" spans="1:12" ht="41.25" customHeight="1">
-      <c r="A32" s="28"/>
-      <c r="B32" s="29"/>
-      <c r="C32" s="29"/>
-      <c r="D32" s="29"/>
-      <c r="E32" s="29"/>
-      <c r="F32" s="30"/>
-      <c r="G32" s="31"/>
+      <c r="A32" s="45"/>
+      <c r="B32" s="46"/>
+      <c r="C32" s="46"/>
+      <c r="D32" s="46"/>
+      <c r="E32" s="46"/>
+      <c r="F32" s="47"/>
+      <c r="G32" s="48"/>
     </row>
     <row r="33" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A33" s="35"/>
-      <c r="B33" s="36"/>
-      <c r="C33" s="36"/>
-      <c r="D33" s="36"/>
-      <c r="E33" s="36"/>
-      <c r="F33" s="37"/>
-      <c r="G33" s="38"/>
+      <c r="A33" s="52"/>
+      <c r="B33" s="53"/>
+      <c r="C33" s="53"/>
+      <c r="D33" s="53"/>
+      <c r="E33" s="53"/>
+      <c r="F33" s="54"/>
+      <c r="G33" s="55"/>
     </row>
     <row r="34" spans="1:7" ht="26.25" customHeight="1">
-      <c r="A34" s="39"/>
-      <c r="B34" s="40"/>
-      <c r="C34" s="40"/>
-      <c r="D34" s="40"/>
-      <c r="E34" s="40"/>
-      <c r="F34" s="22"/>
-      <c r="G34" s="41"/>
+      <c r="A34" s="56"/>
+      <c r="B34" s="57"/>
+      <c r="C34" s="57"/>
+      <c r="D34" s="57"/>
+      <c r="E34" s="57"/>
+      <c r="F34" s="39"/>
+      <c r="G34" s="58"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="20"/>
-      <c r="B35" s="21"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
-      <c r="E35" s="21"/>
-      <c r="F35" s="22"/>
-      <c r="G35" s="23"/>
+      <c r="A35" s="37"/>
+      <c r="B35" s="38"/>
+      <c r="C35" s="38"/>
+      <c r="D35" s="38"/>
+      <c r="E35" s="38"/>
+      <c r="F35" s="39"/>
+      <c r="G35" s="40"/>
     </row>
     <row r="36" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A36" s="24"/>
-      <c r="B36" s="25"/>
-      <c r="C36" s="25"/>
-      <c r="D36" s="25"/>
-      <c r="E36" s="25"/>
-      <c r="F36" s="26"/>
-      <c r="G36" s="27"/>
+      <c r="A36" s="41"/>
+      <c r="B36" s="42"/>
+      <c r="C36" s="42"/>
+      <c r="D36" s="42"/>
+      <c r="E36" s="42"/>
+      <c r="F36" s="43"/>
+      <c r="G36" s="44"/>
     </row>
     <row r="37" spans="1:7" ht="26.25" customHeight="1">
-      <c r="A37" s="28"/>
-      <c r="B37" s="29"/>
-      <c r="C37" s="29"/>
-      <c r="D37" s="29"/>
-      <c r="E37" s="29"/>
-      <c r="F37" s="30"/>
-      <c r="G37" s="31"/>
+      <c r="A37" s="45"/>
+      <c r="B37" s="46"/>
+      <c r="C37" s="46"/>
+      <c r="D37" s="46"/>
+      <c r="E37" s="46"/>
+      <c r="F37" s="47"/>
+      <c r="G37" s="48"/>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="32"/>
-      <c r="B38" s="33"/>
-      <c r="C38" s="33"/>
-      <c r="D38" s="33"/>
-      <c r="E38" s="33"/>
-      <c r="F38" s="30"/>
-      <c r="G38" s="34"/>
+      <c r="A38" s="49"/>
+      <c r="B38" s="50"/>
+      <c r="C38" s="50"/>
+      <c r="D38" s="50"/>
+      <c r="E38" s="50"/>
+      <c r="F38" s="47"/>
+      <c r="G38" s="51"/>
     </row>
     <row r="39" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A39" s="35"/>
-      <c r="B39" s="36"/>
-      <c r="C39" s="36"/>
-      <c r="D39" s="36"/>
-      <c r="E39" s="36"/>
-      <c r="F39" s="37"/>
-      <c r="G39" s="38"/>
+      <c r="A39" s="52"/>
+      <c r="B39" s="53"/>
+      <c r="C39" s="53"/>
+      <c r="D39" s="53"/>
+      <c r="E39" s="53"/>
+      <c r="F39" s="54"/>
+      <c r="G39" s="55"/>
     </row>
     <row r="40" spans="1:7" ht="26.25" customHeight="1">
-      <c r="A40" s="39"/>
-      <c r="B40" s="40"/>
-      <c r="C40" s="40"/>
-      <c r="D40" s="40"/>
-      <c r="E40" s="40"/>
-      <c r="F40" s="22"/>
-      <c r="G40" s="41"/>
+      <c r="A40" s="56"/>
+      <c r="B40" s="57"/>
+      <c r="C40" s="57"/>
+      <c r="D40" s="57"/>
+      <c r="E40" s="57"/>
+      <c r="F40" s="39"/>
+      <c r="G40" s="58"/>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" s="20"/>
-      <c r="B41" s="21"/>
-      <c r="C41" s="21"/>
-      <c r="D41" s="21"/>
-      <c r="E41" s="21"/>
-      <c r="F41" s="22"/>
-      <c r="G41" s="23"/>
+      <c r="A41" s="37"/>
+      <c r="B41" s="38"/>
+      <c r="C41" s="38"/>
+      <c r="D41" s="38"/>
+      <c r="E41" s="38"/>
+      <c r="F41" s="39"/>
+      <c r="G41" s="40"/>
     </row>
     <row r="42" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A42" s="24"/>
-      <c r="B42" s="25"/>
-      <c r="C42" s="25"/>
-      <c r="D42" s="25"/>
-      <c r="E42" s="25"/>
-      <c r="F42" s="26"/>
-      <c r="G42" s="27"/>
+      <c r="A42" s="41"/>
+      <c r="B42" s="42"/>
+      <c r="C42" s="42"/>
+      <c r="D42" s="42"/>
+      <c r="E42" s="42"/>
+      <c r="F42" s="43"/>
+      <c r="G42" s="44"/>
     </row>
     <row r="43" spans="1:7" ht="26.25" customHeight="1">
-      <c r="A43" s="28"/>
-      <c r="B43" s="29"/>
-      <c r="C43" s="29"/>
-      <c r="D43" s="29"/>
-      <c r="E43" s="29"/>
-      <c r="F43" s="30"/>
-      <c r="G43" s="42"/>
+      <c r="A43" s="45"/>
+      <c r="B43" s="46"/>
+      <c r="C43" s="46"/>
+      <c r="D43" s="46"/>
+      <c r="E43" s="46"/>
+      <c r="F43" s="47"/>
+      <c r="G43" s="59"/>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="32"/>
-      <c r="B44" s="33"/>
-      <c r="C44" s="33"/>
-      <c r="D44" s="33"/>
-      <c r="E44" s="33"/>
-      <c r="F44" s="30"/>
-      <c r="G44" s="42"/>
+      <c r="A44" s="49"/>
+      <c r="B44" s="50"/>
+      <c r="C44" s="50"/>
+      <c r="D44" s="50"/>
+      <c r="E44" s="50"/>
+      <c r="F44" s="47"/>
+      <c r="G44" s="59"/>
     </row>
     <row r="45" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A45" s="35"/>
-      <c r="B45" s="36"/>
-      <c r="C45" s="36"/>
-      <c r="D45" s="36"/>
-      <c r="E45" s="36"/>
-      <c r="F45" s="37"/>
-      <c r="G45" s="43"/>
+      <c r="A45" s="52"/>
+      <c r="B45" s="53"/>
+      <c r="C45" s="53"/>
+      <c r="D45" s="53"/>
+      <c r="E45" s="53"/>
+      <c r="F45" s="54"/>
+      <c r="G45" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="47">
@@ -2719,213 +2988,208 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L44"/>
+  <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="H41" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" style="13" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="13"/>
-    <col min="3" max="3" width="12" style="13" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" style="13" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" style="13" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" style="13" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="13"/>
-    <col min="8" max="8" width="16.85546875" style="13" customWidth="1"/>
-    <col min="9" max="10" width="9.140625" style="13"/>
-    <col min="11" max="11" width="22.7109375" style="13" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="13"/>
+    <col min="1" max="1" width="16.42578125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="12"/>
+    <col min="3" max="3" width="12" style="12" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" style="12" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="12" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="12" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="12"/>
+    <col min="8" max="8" width="16.85546875" style="12" customWidth="1"/>
+    <col min="9" max="10" width="9.140625" style="12"/>
+    <col min="11" max="11" width="22.7109375" style="12" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="23.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="13">
+      <c r="B3" s="12">
         <v>10.5</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B4" s="12">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="B5" s="12">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B6" s="12">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="23.25">
+      <c r="A8" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="12">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="12">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B12" s="12">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="23.25">
+      <c r="A17" s="64" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="65"/>
+      <c r="C17" s="65"/>
+      <c r="D17" s="65"/>
+      <c r="E17" s="65"/>
+      <c r="F17" s="65"/>
+      <c r="G17" s="65"/>
+      <c r="H17" s="65"/>
+      <c r="I17" s="65"/>
+      <c r="J17" s="65"/>
+      <c r="K17" s="65"/>
+      <c r="L17" s="65"/>
+    </row>
+    <row r="18" spans="1:12" ht="14.25" customHeight="1">
+      <c r="A18" s="65" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="65" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="65" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="65" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="F18" s="65" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" s="65" t="s">
+        <v>34</v>
+      </c>
+      <c r="H18" s="65" t="s">
+        <v>32</v>
+      </c>
+      <c r="I18" s="65" t="s">
+        <v>23</v>
+      </c>
+      <c r="J18" s="65" t="s">
+        <v>24</v>
+      </c>
+      <c r="K18" s="65" t="s">
+        <v>25</v>
+      </c>
+      <c r="L18" s="65" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" s="66" t="s">
         <v>115</v>
       </c>
-      <c r="B4" s="13">
-        <v>6.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="19" t="s">
+      <c r="B19" s="66" t="s">
         <v>116</v>
       </c>
-      <c r="B5" s="13">
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="19" t="s">
+      <c r="C19" s="66" t="s">
         <v>117</v>
       </c>
-      <c r="B6" s="13">
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="23.25">
-      <c r="A8" s="17" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="13">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="13">
-        <v>2.6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="19" t="s">
+      <c r="D19" s="66" t="s">
         <v>118</v>
       </c>
-      <c r="B12" s="13">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="23.25">
-      <c r="A17" s="46" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="47"/>
-      <c r="C17" s="47"/>
-      <c r="D17" s="47"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="47"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="47"/>
-      <c r="K17" s="47"/>
-      <c r="L17" s="47"/>
-    </row>
-    <row r="18" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A18" s="47" t="s">
-        <v>3</v>
-      </c>
-      <c r="B18" s="47" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" s="47" t="s">
-        <v>17</v>
-      </c>
-      <c r="D18" s="47" t="s">
-        <v>18</v>
-      </c>
-      <c r="E18" s="47" t="s">
-        <v>28</v>
-      </c>
-      <c r="F18" s="47" t="s">
-        <v>21</v>
-      </c>
-      <c r="G18" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="H18" s="47" t="s">
-        <v>32</v>
-      </c>
-      <c r="I18" s="47" t="s">
-        <v>23</v>
-      </c>
-      <c r="J18" s="47" t="s">
-        <v>24</v>
-      </c>
-      <c r="K18" s="47" t="s">
-        <v>25</v>
-      </c>
-      <c r="L18" s="47" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12">
-      <c r="A19" s="48" t="s">
+      <c r="E19" s="65" t="s">
+        <v>120</v>
+      </c>
+      <c r="F19" s="66" t="s">
         <v>119</v>
       </c>
-      <c r="B19" s="48" t="s">
-        <v>120</v>
-      </c>
-      <c r="C19" s="48" t="s">
-        <v>121</v>
-      </c>
-      <c r="D19" s="48" t="s">
+      <c r="G19" s="66" t="s">
         <v>122</v>
       </c>
-      <c r="E19" s="47" t="s">
+      <c r="H19" s="65" t="s">
+        <v>33</v>
+      </c>
+      <c r="I19" s="67" t="s">
+        <v>126</v>
+      </c>
+      <c r="J19" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="K19" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="F19" s="48" t="s">
-        <v>123</v>
-      </c>
-      <c r="G19" s="48" t="s">
-        <v>126</v>
-      </c>
-      <c r="H19" s="47" t="s">
-        <v>33</v>
-      </c>
-      <c r="I19" s="45" t="s">
-        <v>130</v>
-      </c>
-      <c r="J19" s="19" t="s">
-        <v>127</v>
-      </c>
-      <c r="K19" s="19" t="s">
-        <v>128</v>
-      </c>
-      <c r="L19" s="19" t="s">
-        <v>129</v>
+      <c r="L19" s="8" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="14.25" customHeight="1">
-      <c r="I20" s="49"/>
+      <c r="I20" s="65"/>
     </row>
     <row r="21" spans="1:12" ht="23.25">
       <c r="A21" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
     </row>
     <row r="22" spans="1:12">
       <c r="A22" s="12" t="s">
@@ -2947,374 +3211,771 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="41.25" customHeight="1">
-      <c r="A23" s="20">
+    <row r="23" spans="1:12" ht="16.5" customHeight="1">
+      <c r="A23" s="68">
         <v>1</v>
       </c>
-      <c r="B23" s="21">
-        <v>126</v>
-      </c>
-      <c r="C23" s="21">
+      <c r="B23" s="69">
+        <v>136</v>
+      </c>
+      <c r="C23" s="69">
+        <v>2</v>
+      </c>
+      <c r="D23" s="69" t="s">
+        <v>127</v>
+      </c>
+      <c r="E23" s="69" t="s">
+        <v>54</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="G23" s="70"/>
+      <c r="K23" s="6"/>
+    </row>
+    <row r="24" spans="1:12" ht="26.25" customHeight="1" thickBot="1">
+      <c r="A24" s="71"/>
+      <c r="B24" s="72"/>
+      <c r="C24" s="72"/>
+      <c r="D24" s="72"/>
+      <c r="E24" s="72"/>
+      <c r="F24" s="73" t="s">
+        <v>44</v>
+      </c>
+      <c r="G24" s="74"/>
+    </row>
+    <row r="25" spans="1:12" ht="27" customHeight="1">
+      <c r="A25" s="75">
+        <v>2</v>
+      </c>
+      <c r="B25" s="76">
+        <v>120</v>
+      </c>
+      <c r="C25" s="76">
+        <v>2</v>
+      </c>
+      <c r="D25" s="76" t="s">
+        <v>129</v>
+      </c>
+      <c r="E25" s="76" t="s">
+        <v>54</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="G25" s="77"/>
+    </row>
+    <row r="26" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A26" s="71"/>
+      <c r="B26" s="72"/>
+      <c r="C26" s="72"/>
+      <c r="D26" s="72"/>
+      <c r="E26" s="72"/>
+      <c r="F26" s="73" t="s">
+        <v>44</v>
+      </c>
+      <c r="G26" s="74"/>
+    </row>
+    <row r="27" spans="1:12" ht="27" customHeight="1">
+      <c r="A27" s="75">
+        <v>3</v>
+      </c>
+      <c r="B27" s="76">
+        <v>120</v>
+      </c>
+      <c r="C27" s="76">
+        <v>2</v>
+      </c>
+      <c r="D27" s="76" t="s">
+        <v>130</v>
+      </c>
+      <c r="E27" s="76" t="s">
+        <v>54</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="G27" s="77"/>
+    </row>
+    <row r="28" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A28" s="71"/>
+      <c r="B28" s="72"/>
+      <c r="C28" s="72"/>
+      <c r="D28" s="72"/>
+      <c r="E28" s="72"/>
+      <c r="F28" s="73" t="s">
+        <v>44</v>
+      </c>
+      <c r="G28" s="74"/>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" s="75">
         <v>4</v>
       </c>
-      <c r="D23" s="21" t="s">
+      <c r="B29" s="76">
+        <v>136</v>
+      </c>
+      <c r="C29" s="76">
+        <v>2</v>
+      </c>
+      <c r="D29" s="76" t="s">
+        <v>130</v>
+      </c>
+      <c r="E29" s="76" t="s">
+        <v>54</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="G29" s="77"/>
+    </row>
+    <row r="30" spans="1:12" ht="41.25" customHeight="1">
+      <c r="A30" s="68"/>
+      <c r="B30" s="69"/>
+      <c r="C30" s="69"/>
+      <c r="D30" s="69"/>
+      <c r="E30" s="69"/>
+      <c r="F30" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G30" s="70"/>
+    </row>
+    <row r="31" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A31" s="71"/>
+      <c r="B31" s="72"/>
+      <c r="C31" s="72"/>
+      <c r="D31" s="72"/>
+      <c r="E31" s="72"/>
+      <c r="F31" s="73" t="s">
+        <v>108</v>
+      </c>
+      <c r="G31" s="74"/>
+    </row>
+    <row r="32" spans="1:12" ht="27" customHeight="1">
+      <c r="A32" s="75">
+        <v>5</v>
+      </c>
+      <c r="B32" s="76">
+        <v>116</v>
+      </c>
+      <c r="C32" s="76">
+        <v>2</v>
+      </c>
+      <c r="D32" s="76" t="s">
+        <v>129</v>
+      </c>
+      <c r="E32" s="76" t="s">
+        <v>54</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="G32" s="77"/>
+    </row>
+    <row r="33" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A33" s="71"/>
+      <c r="B33" s="72"/>
+      <c r="C33" s="72"/>
+      <c r="D33" s="72"/>
+      <c r="E33" s="72"/>
+      <c r="F33" s="73" t="s">
+        <v>44</v>
+      </c>
+      <c r="G33" s="74"/>
+    </row>
+    <row r="34" spans="1:7" ht="16.5" customHeight="1">
+      <c r="A34" s="75">
+        <v>6</v>
+      </c>
+      <c r="B34" s="76">
+        <v>116</v>
+      </c>
+      <c r="C34" s="76">
+        <v>2</v>
+      </c>
+      <c r="D34" s="76" t="s">
+        <v>131</v>
+      </c>
+      <c r="E34" s="76" t="s">
+        <v>54</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="G34" s="77"/>
+    </row>
+    <row r="35" spans="1:7" ht="26.25" customHeight="1" thickBot="1">
+      <c r="A35" s="71"/>
+      <c r="B35" s="72"/>
+      <c r="C35" s="72"/>
+      <c r="D35" s="72"/>
+      <c r="E35" s="72"/>
+      <c r="F35" s="73" t="s">
+        <v>44</v>
+      </c>
+      <c r="G35" s="74"/>
+    </row>
+    <row r="36" spans="1:7" ht="27" customHeight="1">
+      <c r="A36" s="75">
+        <v>7</v>
+      </c>
+      <c r="B36" s="76">
+        <v>268</v>
+      </c>
+      <c r="C36" s="76">
+        <v>3</v>
+      </c>
+      <c r="D36" s="76" t="s">
+        <v>132</v>
+      </c>
+      <c r="E36" s="76" t="s">
+        <v>54</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="G36" s="78"/>
+    </row>
+    <row r="37" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A37" s="71"/>
+      <c r="B37" s="72"/>
+      <c r="C37" s="72"/>
+      <c r="D37" s="72"/>
+      <c r="E37" s="72"/>
+      <c r="F37" s="73" t="s">
+        <v>108</v>
+      </c>
+      <c r="G37" s="79"/>
+    </row>
+    <row r="38" spans="1:7" ht="26.25" customHeight="1">
+      <c r="A38" s="75">
+        <v>7</v>
+      </c>
+      <c r="B38" s="76">
+        <v>148</v>
+      </c>
+      <c r="C38" s="76">
+        <v>4</v>
+      </c>
+      <c r="D38" s="76" t="s">
+        <v>109</v>
+      </c>
+      <c r="E38" s="76" t="s">
+        <v>91</v>
+      </c>
+      <c r="F38" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="E23" s="21" t="s">
+      <c r="G38" s="77"/>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="68"/>
+      <c r="B39" s="69"/>
+      <c r="C39" s="69"/>
+      <c r="D39" s="69"/>
+      <c r="E39" s="69"/>
+      <c r="F39" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G39" s="70"/>
+    </row>
+    <row r="40" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A40" s="71"/>
+      <c r="B40" s="72"/>
+      <c r="C40" s="72"/>
+      <c r="D40" s="72"/>
+      <c r="E40" s="72"/>
+      <c r="F40" s="73" t="s">
+        <v>108</v>
+      </c>
+      <c r="G40" s="74"/>
+    </row>
+    <row r="41" spans="1:7" ht="26.25" customHeight="1">
+      <c r="A41" s="75">
+        <v>8</v>
+      </c>
+      <c r="B41" s="76">
+        <v>147</v>
+      </c>
+      <c r="C41" s="76">
+        <v>4</v>
+      </c>
+      <c r="D41" s="76" t="s">
+        <v>110</v>
+      </c>
+      <c r="E41" s="76" t="s">
         <v>91</v>
       </c>
-      <c r="F23" s="22" t="s">
+      <c r="F41" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="G41" s="78"/>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" s="68"/>
+      <c r="B42" s="69"/>
+      <c r="C42" s="69"/>
+      <c r="D42" s="69"/>
+      <c r="E42" s="69"/>
+      <c r="F42" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G42" s="78"/>
+    </row>
+    <row r="43" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A43" s="71"/>
+      <c r="B43" s="72"/>
+      <c r="C43" s="72"/>
+      <c r="D43" s="72"/>
+      <c r="E43" s="72"/>
+      <c r="F43" s="73" t="s">
         <v>108</v>
       </c>
-      <c r="G23" s="23"/>
-    </row>
-    <row r="24" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A24" s="24"/>
-      <c r="B24" s="25"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="G24" s="27"/>
-      <c r="K24" s="3"/>
-    </row>
-    <row r="25" spans="1:12" ht="26.25" customHeight="1">
-      <c r="A25" s="28">
-        <v>2</v>
-      </c>
-      <c r="B25" s="29">
-        <v>132</v>
-      </c>
-      <c r="C25" s="29">
+      <c r="G43" s="79"/>
+    </row>
+  </sheetData>
+  <mergeCells count="52">
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="G34:G35"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="G25:G26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="C41:C43"/>
+    <mergeCell ref="D41:D43"/>
+    <mergeCell ref="E41:E43"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="D38:D40"/>
+    <mergeCell ref="E38:E40"/>
+    <mergeCell ref="G38:G40"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="D29:D31"/>
+    <mergeCell ref="E29:E31"/>
+    <mergeCell ref="G29:G31"/>
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L31"/>
+  <sheetViews>
+    <sheetView topLeftCell="I16" workbookViewId="0">
+      <selection activeCell="K26" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="16.42578125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="12"/>
+    <col min="3" max="3" width="12" style="12" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" style="12" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="12" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="12" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="12"/>
+    <col min="8" max="8" width="16.85546875" style="12" customWidth="1"/>
+    <col min="9" max="10" width="9.140625" style="12"/>
+    <col min="11" max="11" width="22.7109375" style="12" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="23.25">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="12">
+        <v>9.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B4" s="12">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B5" s="12">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="23.25">
+      <c r="A8" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="12">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="12">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="8"/>
+    </row>
+    <row r="17" spans="1:12" ht="23.25">
+      <c r="A17" s="64" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="65"/>
+      <c r="C17" s="65"/>
+      <c r="D17" s="65"/>
+      <c r="E17" s="65"/>
+      <c r="F17" s="65"/>
+      <c r="G17" s="65"/>
+      <c r="H17" s="65"/>
+      <c r="I17" s="65"/>
+      <c r="J17" s="65"/>
+      <c r="K17" s="65"/>
+      <c r="L17" s="65"/>
+    </row>
+    <row r="18" spans="1:12" ht="14.25" customHeight="1">
+      <c r="A18" s="65" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="65" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="65" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="65" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="F18" s="65" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" s="65" t="s">
+        <v>34</v>
+      </c>
+      <c r="H18" s="65" t="s">
+        <v>32</v>
+      </c>
+      <c r="I18" s="65" t="s">
+        <v>23</v>
+      </c>
+      <c r="J18" s="65" t="s">
+        <v>24</v>
+      </c>
+      <c r="K18" s="65" t="s">
+        <v>25</v>
+      </c>
+      <c r="L18" s="65" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="15.75">
+      <c r="A19" s="66" t="s">
+        <v>134</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="E19" s="65" t="s">
+        <v>138</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="H19" s="65" t="s">
+        <v>33</v>
+      </c>
+      <c r="I19" s="88" t="s">
+        <v>141</v>
+      </c>
+      <c r="J19" s="88" t="s">
+        <v>142</v>
+      </c>
+      <c r="K19" s="88" t="s">
+        <v>143</v>
+      </c>
+      <c r="L19" s="89" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="14.25" customHeight="1">
+      <c r="I20" s="65"/>
+    </row>
+    <row r="21" spans="1:12" ht="23.25">
+      <c r="A21" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A22" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="16.5" customHeight="1">
+      <c r="A23" s="75">
+        <v>1</v>
+      </c>
+      <c r="B23" s="76">
+        <v>291</v>
+      </c>
+      <c r="C23" s="76">
+        <v>0</v>
+      </c>
+      <c r="D23" s="76" t="s">
+        <v>145</v>
+      </c>
+      <c r="E23" s="76" t="s">
+        <v>54</v>
+      </c>
+      <c r="F23" s="85" t="s">
+        <v>56</v>
+      </c>
+      <c r="G23" s="77"/>
+      <c r="K23" s="6"/>
+    </row>
+    <row r="24" spans="1:12" ht="26.25" customHeight="1" thickBot="1">
+      <c r="A24" s="71"/>
+      <c r="B24" s="72"/>
+      <c r="C24" s="72"/>
+      <c r="D24" s="72"/>
+      <c r="E24" s="72"/>
+      <c r="F24" s="73" t="s">
+        <v>108</v>
+      </c>
+      <c r="G24" s="74"/>
+    </row>
+    <row r="25" spans="1:12" ht="27" customHeight="1">
+      <c r="A25" s="75">
+        <v>2</v>
+      </c>
+      <c r="B25" s="76">
+        <v>121</v>
+      </c>
+      <c r="C25" s="76">
+        <v>0</v>
+      </c>
+      <c r="D25" s="76" t="s">
+        <v>146</v>
+      </c>
+      <c r="E25" s="76"/>
+      <c r="F25" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G25" s="77"/>
+    </row>
+    <row r="26" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A26" s="71"/>
+      <c r="B26" s="72"/>
+      <c r="C26" s="72"/>
+      <c r="D26" s="72"/>
+      <c r="E26" s="72"/>
+      <c r="F26" s="73" t="s">
+        <v>108</v>
+      </c>
+      <c r="G26" s="74"/>
+    </row>
+    <row r="27" spans="1:12" ht="27" customHeight="1">
+      <c r="A27" s="75">
+        <v>3</v>
+      </c>
+      <c r="B27" s="76">
+        <v>89</v>
+      </c>
+      <c r="C27" s="76">
+        <v>2</v>
+      </c>
+      <c r="D27" s="76" t="s">
+        <v>147</v>
+      </c>
+      <c r="E27" s="76" t="s">
+        <v>54</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G27" s="77"/>
+    </row>
+    <row r="28" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A28" s="71"/>
+      <c r="B28" s="72"/>
+      <c r="C28" s="72"/>
+      <c r="D28" s="72"/>
+      <c r="E28" s="72"/>
+      <c r="F28" s="73" t="s">
+        <v>108</v>
+      </c>
+      <c r="G28" s="74"/>
+    </row>
+    <row r="29" spans="1:12" ht="43.5" thickBot="1">
+      <c r="A29" s="81">
         <v>4</v>
       </c>
-      <c r="D25" s="29" t="s">
-        <v>107</v>
-      </c>
-      <c r="E25" s="29" t="s">
-        <v>91</v>
-      </c>
-      <c r="F25" s="30" t="s">
-        <v>108</v>
-      </c>
-      <c r="G25" s="31"/>
-    </row>
-    <row r="26" spans="1:12">
-      <c r="A26" s="32"/>
-      <c r="B26" s="33"/>
-      <c r="C26" s="33"/>
-      <c r="D26" s="33"/>
-      <c r="E26" s="33"/>
-      <c r="F26" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="G26" s="34"/>
-    </row>
-    <row r="27" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A27" s="35"/>
-      <c r="B27" s="36"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="37" t="s">
-        <v>109</v>
-      </c>
-      <c r="G27" s="38"/>
-    </row>
-    <row r="28" spans="1:12" ht="26.25" customHeight="1" thickBot="1">
-      <c r="A28" s="39">
-        <v>3</v>
-      </c>
-      <c r="B28" s="40">
-        <v>143</v>
-      </c>
-      <c r="C28" s="40">
-        <v>4</v>
-      </c>
-      <c r="D28" s="40" t="s">
-        <v>110</v>
-      </c>
-      <c r="E28" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="F28" s="22" t="s">
-        <v>108</v>
-      </c>
-      <c r="G28" s="41"/>
-    </row>
-    <row r="29" spans="1:12">
-      <c r="A29" s="20"/>
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="G29" s="23"/>
-      <c r="H29" s="14"/>
-    </row>
-    <row r="30" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A30" s="24"/>
-      <c r="B30" s="25"/>
-      <c r="C30" s="25"/>
-      <c r="D30" s="25"/>
-      <c r="E30" s="25"/>
-      <c r="F30" s="26" t="s">
-        <v>109</v>
-      </c>
-      <c r="G30" s="27"/>
-      <c r="H30" s="15"/>
-    </row>
-    <row r="31" spans="1:12" ht="41.25" customHeight="1">
-      <c r="A31" s="28">
-        <v>4</v>
-      </c>
-      <c r="B31" s="29">
+      <c r="B29" s="73">
+        <v>89</v>
+      </c>
+      <c r="C29" s="73">
+        <v>2</v>
+      </c>
+      <c r="D29" s="73" t="s">
         <v>147</v>
       </c>
-      <c r="C31" s="29">
-        <v>4</v>
-      </c>
-      <c r="D31" s="29" t="s">
-        <v>110</v>
-      </c>
-      <c r="E31" s="29" t="s">
-        <v>91</v>
-      </c>
-      <c r="F31" s="30" t="s">
-        <v>108</v>
-      </c>
-      <c r="G31" s="31"/>
-    </row>
-    <row r="32" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A32" s="35"/>
-      <c r="B32" s="36"/>
-      <c r="C32" s="36"/>
-      <c r="D32" s="36"/>
-      <c r="E32" s="36"/>
-      <c r="F32" s="37" t="s">
-        <v>44</v>
-      </c>
-      <c r="G32" s="38"/>
-    </row>
-    <row r="33" spans="1:7" ht="26.25" customHeight="1">
-      <c r="A33" s="39">
+      <c r="E29" s="73" t="s">
+        <v>54</v>
+      </c>
+      <c r="F29" s="73" t="s">
+        <v>56</v>
+      </c>
+      <c r="G29" s="82"/>
+    </row>
+    <row r="30" spans="1:12" ht="41.25" customHeight="1" thickBot="1">
+      <c r="A30" s="81">
         <v>5</v>
       </c>
-      <c r="B33" s="40">
-        <v>120</v>
-      </c>
-      <c r="C33" s="40">
-        <v>4</v>
-      </c>
-      <c r="D33" s="40" t="s">
-        <v>111</v>
-      </c>
-      <c r="E33" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="F33" s="22" t="s">
-        <v>108</v>
-      </c>
-      <c r="G33" s="41"/>
-    </row>
-    <row r="34" spans="1:7">
-      <c r="A34" s="20"/>
-      <c r="B34" s="21"/>
-      <c r="C34" s="21"/>
-      <c r="D34" s="21"/>
-      <c r="E34" s="21"/>
-      <c r="F34" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="G34" s="23"/>
-    </row>
-    <row r="35" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A35" s="24"/>
-      <c r="B35" s="25"/>
-      <c r="C35" s="25"/>
-      <c r="D35" s="25"/>
-      <c r="E35" s="25"/>
-      <c r="F35" s="26" t="s">
-        <v>109</v>
-      </c>
-      <c r="G35" s="27"/>
-    </row>
-    <row r="36" spans="1:7" ht="26.25" customHeight="1">
-      <c r="A36" s="28">
+      <c r="B30" s="73">
+        <v>89</v>
+      </c>
+      <c r="C30" s="73">
+        <v>2</v>
+      </c>
+      <c r="D30" s="73" t="s">
+        <v>147</v>
+      </c>
+      <c r="E30" s="73" t="s">
+        <v>54</v>
+      </c>
+      <c r="F30" s="73" t="s">
+        <v>56</v>
+      </c>
+      <c r="G30" s="82"/>
+    </row>
+    <row r="31" spans="1:12" ht="43.5" thickBot="1">
+      <c r="A31" s="81">
         <v>6</v>
       </c>
-      <c r="B36" s="29">
-        <v>120</v>
-      </c>
-      <c r="C36" s="29">
-        <v>4</v>
-      </c>
-      <c r="D36" s="29" t="s">
-        <v>112</v>
-      </c>
-      <c r="E36" s="29" t="s">
-        <v>91</v>
-      </c>
-      <c r="F36" s="30" t="s">
-        <v>108</v>
-      </c>
-      <c r="G36" s="31"/>
-    </row>
-    <row r="37" spans="1:7">
-      <c r="A37" s="32"/>
-      <c r="B37" s="33"/>
-      <c r="C37" s="33"/>
-      <c r="D37" s="33"/>
-      <c r="E37" s="33"/>
-      <c r="F37" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="G37" s="34"/>
-    </row>
-    <row r="38" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A38" s="35"/>
-      <c r="B38" s="36"/>
-      <c r="C38" s="36"/>
-      <c r="D38" s="36"/>
-      <c r="E38" s="36"/>
-      <c r="F38" s="37" t="s">
-        <v>109</v>
-      </c>
-      <c r="G38" s="38"/>
-    </row>
-    <row r="39" spans="1:7" ht="26.25" customHeight="1">
-      <c r="A39" s="39">
-        <v>7</v>
-      </c>
-      <c r="B39" s="40">
-        <v>148</v>
-      </c>
-      <c r="C39" s="40">
-        <v>4</v>
-      </c>
-      <c r="D39" s="40" t="s">
-        <v>113</v>
-      </c>
-      <c r="E39" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="F39" s="22" t="s">
-        <v>108</v>
-      </c>
-      <c r="G39" s="41"/>
-    </row>
-    <row r="40" spans="1:7">
-      <c r="A40" s="20"/>
-      <c r="B40" s="21"/>
-      <c r="C40" s="21"/>
-      <c r="D40" s="21"/>
-      <c r="E40" s="21"/>
-      <c r="F40" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="G40" s="23"/>
-    </row>
-    <row r="41" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A41" s="24"/>
-      <c r="B41" s="25"/>
-      <c r="C41" s="25"/>
-      <c r="D41" s="25"/>
-      <c r="E41" s="25"/>
-      <c r="F41" s="26" t="s">
-        <v>109</v>
-      </c>
-      <c r="G41" s="27"/>
-    </row>
-    <row r="42" spans="1:7" ht="26.25" customHeight="1">
-      <c r="A42" s="28">
-        <v>8</v>
-      </c>
-      <c r="B42" s="29">
+      <c r="B31" s="73">
+        <v>89</v>
+      </c>
+      <c r="C31" s="73">
+        <v>2</v>
+      </c>
+      <c r="D31" s="73" t="s">
         <v>147</v>
       </c>
-      <c r="C42" s="29">
-        <v>4</v>
-      </c>
-      <c r="D42" s="29" t="s">
-        <v>114</v>
-      </c>
-      <c r="E42" s="29" t="s">
-        <v>91</v>
-      </c>
-      <c r="F42" s="30" t="s">
-        <v>108</v>
-      </c>
-      <c r="G42" s="42"/>
-    </row>
-    <row r="43" spans="1:7">
-      <c r="A43" s="32"/>
-      <c r="B43" s="33"/>
-      <c r="C43" s="33"/>
-      <c r="D43" s="33"/>
-      <c r="E43" s="33"/>
-      <c r="F43" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="G43" s="42"/>
-    </row>
-    <row r="44" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A44" s="35"/>
-      <c r="B44" s="36"/>
-      <c r="C44" s="36"/>
-      <c r="D44" s="36"/>
-      <c r="E44" s="36"/>
-      <c r="F44" s="37" t="s">
-        <v>109</v>
-      </c>
-      <c r="G44" s="43"/>
+      <c r="E31" s="73" t="s">
+        <v>54</v>
+      </c>
+      <c r="F31" s="73" t="s">
+        <v>56</v>
+      </c>
+      <c r="G31" s="79"/>
     </row>
   </sheetData>
-  <mergeCells count="47">
-    <mergeCell ref="A42:A44"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="C42:C44"/>
-    <mergeCell ref="D42:D44"/>
-    <mergeCell ref="E42:E44"/>
-    <mergeCell ref="A39:A41"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="C39:C41"/>
-    <mergeCell ref="D39:D41"/>
-    <mergeCell ref="E39:E41"/>
-    <mergeCell ref="G39:G41"/>
-    <mergeCell ref="A36:A38"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="C36:C38"/>
-    <mergeCell ref="D36:D38"/>
-    <mergeCell ref="E36:E38"/>
-    <mergeCell ref="G36:G38"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="B33:B35"/>
-    <mergeCell ref="C33:C35"/>
-    <mergeCell ref="D33:D35"/>
-    <mergeCell ref="E33:E35"/>
-    <mergeCell ref="G33:G35"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="G31:G32"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="C28:C30"/>
-    <mergeCell ref="D28:D30"/>
-    <mergeCell ref="E28:E30"/>
-    <mergeCell ref="G28:G30"/>
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="B25:B27"/>
-    <mergeCell ref="C25:C27"/>
-    <mergeCell ref="D25:D27"/>
-    <mergeCell ref="E25:E27"/>
-    <mergeCell ref="G25:G27"/>
+  <mergeCells count="18">
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="G25:G26"/>
     <mergeCell ref="A23:A24"/>
     <mergeCell ref="B23:B24"/>
     <mergeCell ref="C23:C24"/>
@@ -3324,4 +3985,816 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L31"/>
+  <sheetViews>
+    <sheetView topLeftCell="E15" workbookViewId="0">
+      <selection activeCell="H26" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="16.42578125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="12"/>
+    <col min="3" max="3" width="12" style="12" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" style="12" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="12" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="12" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="12"/>
+    <col min="8" max="8" width="16.85546875" style="12" customWidth="1"/>
+    <col min="9" max="10" width="9.140625" style="12"/>
+    <col min="11" max="11" width="22.7109375" style="12" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="23.25">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="12">
+        <v>10.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B4" s="12">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B5" s="12">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="23.25">
+      <c r="A8" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="12">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="12">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B12" s="12">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="23.25">
+      <c r="A17" s="64" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="65"/>
+      <c r="C17" s="65"/>
+      <c r="D17" s="65"/>
+      <c r="E17" s="65"/>
+      <c r="F17" s="65"/>
+      <c r="G17" s="65"/>
+      <c r="H17" s="65"/>
+      <c r="I17" s="65"/>
+      <c r="J17" s="65"/>
+      <c r="K17" s="65"/>
+      <c r="L17" s="65"/>
+    </row>
+    <row r="18" spans="1:12" ht="14.25" customHeight="1">
+      <c r="A18" s="65" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="65" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="65" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="65" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="F18" s="65" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" s="65" t="s">
+        <v>34</v>
+      </c>
+      <c r="H18" s="65" t="s">
+        <v>32</v>
+      </c>
+      <c r="I18" s="65" t="s">
+        <v>23</v>
+      </c>
+      <c r="J18" s="65" t="s">
+        <v>24</v>
+      </c>
+      <c r="K18" s="65" t="s">
+        <v>25</v>
+      </c>
+      <c r="L18" s="65" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E19" s="65" t="s">
+        <v>155</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H19" s="65" t="s">
+        <v>33</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="J19" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="14.25" customHeight="1">
+      <c r="I20" s="65"/>
+    </row>
+    <row r="21" spans="1:12" ht="23.25">
+      <c r="A21" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A22" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="16.5" customHeight="1">
+      <c r="A23" s="90"/>
+      <c r="B23" s="91"/>
+      <c r="C23" s="91"/>
+      <c r="D23" s="91"/>
+      <c r="E23" s="91"/>
+      <c r="F23" s="91"/>
+      <c r="J23" s="6"/>
+    </row>
+    <row r="24" spans="1:12" ht="30" customHeight="1">
+      <c r="A24" s="37">
+        <v>1</v>
+      </c>
+      <c r="B24" s="38">
+        <v>105</v>
+      </c>
+      <c r="C24" s="38">
+        <v>2</v>
+      </c>
+      <c r="D24" s="38" t="s">
+        <v>160</v>
+      </c>
+      <c r="E24" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="F24" s="39" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="27" customHeight="1" thickBot="1">
+      <c r="A25" s="41"/>
+      <c r="B25" s="42"/>
+      <c r="C25" s="42"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="42"/>
+      <c r="F25" s="43" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="57.75" thickBot="1">
+      <c r="A26" s="63">
+        <v>2</v>
+      </c>
+      <c r="B26" s="54">
+        <v>105</v>
+      </c>
+      <c r="C26" s="54">
+        <v>2</v>
+      </c>
+      <c r="D26" s="54" t="s">
+        <v>160</v>
+      </c>
+      <c r="E26" s="54" t="s">
+        <v>55</v>
+      </c>
+      <c r="F26" s="54" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="41.25" customHeight="1">
+      <c r="A27" s="56">
+        <v>3</v>
+      </c>
+      <c r="B27" s="57">
+        <v>262</v>
+      </c>
+      <c r="C27" s="57">
+        <v>2</v>
+      </c>
+      <c r="D27" s="57" t="s">
+        <v>161</v>
+      </c>
+      <c r="E27" s="57" t="s">
+        <v>55</v>
+      </c>
+      <c r="F27" s="39" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A28" s="41"/>
+      <c r="B28" s="42"/>
+      <c r="C28" s="42"/>
+      <c r="D28" s="42"/>
+      <c r="E28" s="42"/>
+      <c r="F28" s="43" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A29" s="45">
+        <v>4</v>
+      </c>
+      <c r="B29" s="46">
+        <v>262</v>
+      </c>
+      <c r="C29" s="46">
+        <v>2</v>
+      </c>
+      <c r="D29" s="46" t="s">
+        <v>161</v>
+      </c>
+      <c r="E29" s="46" t="s">
+        <v>55</v>
+      </c>
+      <c r="F29" s="47" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="41.25" customHeight="1" thickBot="1">
+      <c r="A30" s="52"/>
+      <c r="B30" s="53"/>
+      <c r="C30" s="53"/>
+      <c r="D30" s="53"/>
+      <c r="E30" s="53"/>
+      <c r="F30" s="54" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="57.75" thickBot="1">
+      <c r="A31" s="62">
+        <v>5</v>
+      </c>
+      <c r="B31" s="43">
+        <v>178</v>
+      </c>
+      <c r="C31" s="43">
+        <v>2</v>
+      </c>
+      <c r="D31" s="43" t="s">
+        <v>162</v>
+      </c>
+      <c r="E31" s="43" t="s">
+        <v>55</v>
+      </c>
+      <c r="F31" s="43" t="s">
+        <v>163</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F23" sqref="A23:XFD23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="16.42578125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="12"/>
+    <col min="3" max="3" width="12" style="12" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" style="12" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="12" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="12" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="12"/>
+    <col min="8" max="8" width="16.85546875" style="12" customWidth="1"/>
+    <col min="9" max="10" width="9.140625" style="12"/>
+    <col min="11" max="11" width="22.7109375" style="12" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="23.25">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B4" s="12">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="B5" s="12">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="23.25">
+      <c r="A8" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="12">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="12">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="1"/>
+    </row>
+    <row r="17" spans="1:12" ht="23.25">
+      <c r="A17" s="64" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="65"/>
+      <c r="C17" s="65"/>
+      <c r="D17" s="65"/>
+      <c r="E17" s="65"/>
+      <c r="F17" s="65"/>
+      <c r="G17" s="65"/>
+      <c r="H17" s="65"/>
+      <c r="I17" s="65"/>
+      <c r="J17" s="65"/>
+      <c r="K17" s="65"/>
+      <c r="L17" s="65"/>
+    </row>
+    <row r="18" spans="1:12" ht="14.25" customHeight="1">
+      <c r="A18" s="65" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="65" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="65" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="65" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="F18" s="65" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" s="65" t="s">
+        <v>34</v>
+      </c>
+      <c r="H18" s="65" t="s">
+        <v>32</v>
+      </c>
+      <c r="I18" s="65" t="s">
+        <v>23</v>
+      </c>
+      <c r="J18" s="65" t="s">
+        <v>24</v>
+      </c>
+      <c r="K18" s="65" t="s">
+        <v>25</v>
+      </c>
+      <c r="L18" s="65" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="15.75">
+      <c r="A19" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="E19" s="65" t="s">
+        <v>155</v>
+      </c>
+      <c r="F19" s="19" t="s">
+        <v>169</v>
+      </c>
+      <c r="G19" s="19" t="s">
+        <v>170</v>
+      </c>
+      <c r="H19" s="65" t="s">
+        <v>33</v>
+      </c>
+      <c r="I19" s="80" t="s">
+        <v>171</v>
+      </c>
+      <c r="J19" s="80" t="s">
+        <v>172</v>
+      </c>
+      <c r="K19" s="80" t="s">
+        <v>173</v>
+      </c>
+      <c r="L19" s="20" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="14.25" customHeight="1">
+      <c r="I20" s="65"/>
+    </row>
+    <row r="21" spans="1:12" ht="23.25">
+      <c r="A21" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A22" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="30" customHeight="1">
+      <c r="A23" s="34">
+        <v>1</v>
+      </c>
+      <c r="B23" s="35">
+        <v>301</v>
+      </c>
+      <c r="C23" s="35">
+        <v>2</v>
+      </c>
+      <c r="D23" s="35" t="s">
+        <v>175</v>
+      </c>
+      <c r="E23" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="F23" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="G23" s="36"/>
+    </row>
+    <row r="24" spans="1:12" ht="27" customHeight="1" thickBot="1">
+      <c r="A24" s="25"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="G24" s="27"/>
+    </row>
+    <row r="25" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A25" s="28">
+        <v>2</v>
+      </c>
+      <c r="B25" s="30">
+        <v>193</v>
+      </c>
+      <c r="C25" s="30">
+        <v>2</v>
+      </c>
+      <c r="D25" s="30" t="s">
+        <v>176</v>
+      </c>
+      <c r="E25" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="F25" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="G25" s="32"/>
+    </row>
+    <row r="26" spans="1:12" ht="41.25" customHeight="1" thickBot="1">
+      <c r="A26" s="29"/>
+      <c r="B26" s="31"/>
+      <c r="C26" s="31"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="G26" s="33"/>
+    </row>
+    <row r="27" spans="1:12" ht="57.75" thickBot="1">
+      <c r="A27" s="83">
+        <v>3</v>
+      </c>
+      <c r="B27" s="22">
+        <v>193</v>
+      </c>
+      <c r="C27" s="22">
+        <v>2</v>
+      </c>
+      <c r="D27" s="22" t="s">
+        <v>177</v>
+      </c>
+      <c r="E27" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="F27" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="G27" s="84"/>
+    </row>
+    <row r="28" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A28" s="28">
+        <v>4</v>
+      </c>
+      <c r="B28" s="30">
+        <v>114</v>
+      </c>
+      <c r="C28" s="30">
+        <v>2</v>
+      </c>
+      <c r="D28" s="30" t="s">
+        <v>178</v>
+      </c>
+      <c r="E28" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="F28" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="G28" s="32"/>
+    </row>
+    <row r="29" spans="1:12" ht="41.25" customHeight="1" thickBot="1">
+      <c r="A29" s="29"/>
+      <c r="B29" s="31"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="G29" s="33"/>
+    </row>
+    <row r="30" spans="1:12" ht="41.25" customHeight="1">
+      <c r="A30" s="34">
+        <v>5</v>
+      </c>
+      <c r="B30" s="35">
+        <v>114</v>
+      </c>
+      <c r="C30" s="35">
+        <v>2</v>
+      </c>
+      <c r="D30" s="35" t="s">
+        <v>178</v>
+      </c>
+      <c r="E30" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="F30" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="G30" s="36"/>
+    </row>
+    <row r="31" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A31" s="25"/>
+      <c r="B31" s="26"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="26"/>
+      <c r="F31" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="G31" s="27"/>
+    </row>
+    <row r="32" spans="1:12" ht="57.75" thickBot="1">
+      <c r="A32" s="86">
+        <v>6</v>
+      </c>
+      <c r="B32" s="24">
+        <v>114</v>
+      </c>
+      <c r="C32" s="24">
+        <v>2</v>
+      </c>
+      <c r="D32" s="24" t="s">
+        <v>178</v>
+      </c>
+      <c r="E32" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="F32" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="G32" s="87"/>
+    </row>
+    <row r="33" spans="1:7" ht="57.75" thickBot="1">
+      <c r="A33" s="83">
+        <v>7</v>
+      </c>
+      <c r="B33" s="22">
+        <v>114</v>
+      </c>
+      <c r="C33" s="22">
+        <v>2</v>
+      </c>
+      <c r="D33" s="22" t="s">
+        <v>178</v>
+      </c>
+      <c r="E33" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="F33" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="G33" s="84"/>
+    </row>
+  </sheetData>
+  <mergeCells count="24">
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="G25:G26"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="G30:G31"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "Merge branch 'Sprint-1' of https://github.com/Armaniimus/gameparty_project_met_georgi into Sprint-1"
This reverts commit 69f38d9475ad131ad5cde378fa1c4ef48e48118c, reversing
changes made to 360b0d5fa052a20134dc7690c38314b8451b7fa8.
</commit_message>
<xml_diff>
--- a/documentatie_And_sql/documentatie/BioscoopData.xlsx
+++ b/documentatie_And_sql/documentatie/BioscoopData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7350" firstSheet="6" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7350" firstSheet="5" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="almere" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Den Bosch" sheetId="5" r:id="rId5"/>
     <sheet name="Den Helder" sheetId="6" r:id="rId6"/>
     <sheet name="Dordrecht" sheetId="7" r:id="rId7"/>
-    <sheet name="Emmen" sheetId="8" r:id="rId8"/>
+    <sheet name="Blad5" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -803,7 +803,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -859,6 +859,9 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -871,10 +874,19 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1000,10 +1012,16 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2670,13 +2688,13 @@
       <c r="H19" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="I19" s="57" t="s">
+      <c r="I19" s="61" t="s">
         <v>103</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="K19" s="57" t="s">
+      <c r="K19" s="61" t="s">
         <v>105</v>
       </c>
       <c r="L19" s="1" t="s">
@@ -2714,205 +2732,205 @@
       </c>
     </row>
     <row r="24" spans="1:12" ht="41.25" customHeight="1">
-      <c r="A24" s="33"/>
-      <c r="B24" s="34"/>
-      <c r="C24" s="34"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="35"/>
-      <c r="G24" s="36"/>
+      <c r="A24" s="37"/>
+      <c r="B24" s="38"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="39"/>
+      <c r="G24" s="40"/>
     </row>
     <row r="25" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A25" s="37"/>
-      <c r="B25" s="38"/>
-      <c r="C25" s="38"/>
-      <c r="D25" s="38"/>
-      <c r="E25" s="38"/>
-      <c r="F25" s="39"/>
-      <c r="G25" s="40"/>
+      <c r="A25" s="41"/>
+      <c r="B25" s="42"/>
+      <c r="C25" s="42"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="42"/>
+      <c r="F25" s="43"/>
+      <c r="G25" s="44"/>
       <c r="K25" s="3"/>
     </row>
     <row r="26" spans="1:12" ht="26.25" customHeight="1">
-      <c r="A26" s="41"/>
-      <c r="B26" s="42"/>
-      <c r="C26" s="42"/>
-      <c r="D26" s="42"/>
-      <c r="E26" s="42"/>
-      <c r="F26" s="43"/>
-      <c r="G26" s="44"/>
+      <c r="A26" s="45"/>
+      <c r="B26" s="46"/>
+      <c r="C26" s="46"/>
+      <c r="D26" s="46"/>
+      <c r="E26" s="46"/>
+      <c r="F26" s="47"/>
+      <c r="G26" s="48"/>
     </row>
     <row r="27" spans="1:12">
-      <c r="A27" s="45"/>
-      <c r="B27" s="46"/>
-      <c r="C27" s="46"/>
-      <c r="D27" s="46"/>
-      <c r="E27" s="46"/>
-      <c r="F27" s="43"/>
-      <c r="G27" s="47"/>
+      <c r="A27" s="49"/>
+      <c r="B27" s="50"/>
+      <c r="C27" s="50"/>
+      <c r="D27" s="50"/>
+      <c r="E27" s="50"/>
+      <c r="F27" s="47"/>
+      <c r="G27" s="51"/>
     </row>
     <row r="28" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A28" s="48"/>
-      <c r="B28" s="49"/>
-      <c r="C28" s="49"/>
-      <c r="D28" s="49"/>
-      <c r="E28" s="49"/>
-      <c r="F28" s="50"/>
-      <c r="G28" s="51"/>
+      <c r="A28" s="52"/>
+      <c r="B28" s="53"/>
+      <c r="C28" s="53"/>
+      <c r="D28" s="53"/>
+      <c r="E28" s="53"/>
+      <c r="F28" s="54"/>
+      <c r="G28" s="55"/>
     </row>
     <row r="29" spans="1:12" ht="26.25" customHeight="1" thickBot="1">
-      <c r="A29" s="52"/>
-      <c r="B29" s="53"/>
-      <c r="C29" s="53"/>
-      <c r="D29" s="53"/>
-      <c r="E29" s="53"/>
-      <c r="F29" s="35"/>
-      <c r="G29" s="54"/>
+      <c r="A29" s="56"/>
+      <c r="B29" s="57"/>
+      <c r="C29" s="57"/>
+      <c r="D29" s="57"/>
+      <c r="E29" s="57"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="58"/>
     </row>
     <row r="30" spans="1:12">
-      <c r="A30" s="33"/>
-      <c r="B30" s="34"/>
-      <c r="C30" s="34"/>
-      <c r="D30" s="34"/>
-      <c r="E30" s="34"/>
-      <c r="F30" s="35"/>
-      <c r="G30" s="36"/>
+      <c r="A30" s="37"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="39"/>
+      <c r="G30" s="40"/>
       <c r="H30" s="14"/>
     </row>
     <row r="31" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A31" s="37"/>
-      <c r="B31" s="38"/>
-      <c r="C31" s="38"/>
-      <c r="D31" s="38"/>
-      <c r="E31" s="38"/>
-      <c r="F31" s="39"/>
-      <c r="G31" s="40"/>
+      <c r="A31" s="41"/>
+      <c r="B31" s="42"/>
+      <c r="C31" s="42"/>
+      <c r="D31" s="42"/>
+      <c r="E31" s="42"/>
+      <c r="F31" s="43"/>
+      <c r="G31" s="44"/>
       <c r="H31" s="15"/>
     </row>
     <row r="32" spans="1:12" ht="41.25" customHeight="1">
-      <c r="A32" s="41"/>
-      <c r="B32" s="42"/>
-      <c r="C32" s="42"/>
-      <c r="D32" s="42"/>
-      <c r="E32" s="42"/>
-      <c r="F32" s="43"/>
-      <c r="G32" s="44"/>
+      <c r="A32" s="45"/>
+      <c r="B32" s="46"/>
+      <c r="C32" s="46"/>
+      <c r="D32" s="46"/>
+      <c r="E32" s="46"/>
+      <c r="F32" s="47"/>
+      <c r="G32" s="48"/>
     </row>
     <row r="33" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A33" s="48"/>
-      <c r="B33" s="49"/>
-      <c r="C33" s="49"/>
-      <c r="D33" s="49"/>
-      <c r="E33" s="49"/>
-      <c r="F33" s="50"/>
-      <c r="G33" s="51"/>
+      <c r="A33" s="52"/>
+      <c r="B33" s="53"/>
+      <c r="C33" s="53"/>
+      <c r="D33" s="53"/>
+      <c r="E33" s="53"/>
+      <c r="F33" s="54"/>
+      <c r="G33" s="55"/>
     </row>
     <row r="34" spans="1:7" ht="26.25" customHeight="1">
-      <c r="A34" s="52"/>
-      <c r="B34" s="53"/>
-      <c r="C34" s="53"/>
-      <c r="D34" s="53"/>
-      <c r="E34" s="53"/>
-      <c r="F34" s="35"/>
-      <c r="G34" s="54"/>
+      <c r="A34" s="56"/>
+      <c r="B34" s="57"/>
+      <c r="C34" s="57"/>
+      <c r="D34" s="57"/>
+      <c r="E34" s="57"/>
+      <c r="F34" s="39"/>
+      <c r="G34" s="58"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="33"/>
-      <c r="B35" s="34"/>
-      <c r="C35" s="34"/>
-      <c r="D35" s="34"/>
-      <c r="E35" s="34"/>
-      <c r="F35" s="35"/>
-      <c r="G35" s="36"/>
+      <c r="A35" s="37"/>
+      <c r="B35" s="38"/>
+      <c r="C35" s="38"/>
+      <c r="D35" s="38"/>
+      <c r="E35" s="38"/>
+      <c r="F35" s="39"/>
+      <c r="G35" s="40"/>
     </row>
     <row r="36" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A36" s="37"/>
-      <c r="B36" s="38"/>
-      <c r="C36" s="38"/>
-      <c r="D36" s="38"/>
-      <c r="E36" s="38"/>
-      <c r="F36" s="39"/>
-      <c r="G36" s="40"/>
+      <c r="A36" s="41"/>
+      <c r="B36" s="42"/>
+      <c r="C36" s="42"/>
+      <c r="D36" s="42"/>
+      <c r="E36" s="42"/>
+      <c r="F36" s="43"/>
+      <c r="G36" s="44"/>
     </row>
     <row r="37" spans="1:7" ht="26.25" customHeight="1">
-      <c r="A37" s="41"/>
-      <c r="B37" s="42"/>
-      <c r="C37" s="42"/>
-      <c r="D37" s="42"/>
-      <c r="E37" s="42"/>
-      <c r="F37" s="43"/>
-      <c r="G37" s="44"/>
+      <c r="A37" s="45"/>
+      <c r="B37" s="46"/>
+      <c r="C37" s="46"/>
+      <c r="D37" s="46"/>
+      <c r="E37" s="46"/>
+      <c r="F37" s="47"/>
+      <c r="G37" s="48"/>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="45"/>
-      <c r="B38" s="46"/>
-      <c r="C38" s="46"/>
-      <c r="D38" s="46"/>
-      <c r="E38" s="46"/>
-      <c r="F38" s="43"/>
-      <c r="G38" s="47"/>
+      <c r="A38" s="49"/>
+      <c r="B38" s="50"/>
+      <c r="C38" s="50"/>
+      <c r="D38" s="50"/>
+      <c r="E38" s="50"/>
+      <c r="F38" s="47"/>
+      <c r="G38" s="51"/>
     </row>
     <row r="39" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A39" s="48"/>
-      <c r="B39" s="49"/>
-      <c r="C39" s="49"/>
-      <c r="D39" s="49"/>
-      <c r="E39" s="49"/>
-      <c r="F39" s="50"/>
-      <c r="G39" s="51"/>
+      <c r="A39" s="52"/>
+      <c r="B39" s="53"/>
+      <c r="C39" s="53"/>
+      <c r="D39" s="53"/>
+      <c r="E39" s="53"/>
+      <c r="F39" s="54"/>
+      <c r="G39" s="55"/>
     </row>
     <row r="40" spans="1:7" ht="26.25" customHeight="1">
-      <c r="A40" s="52"/>
-      <c r="B40" s="53"/>
-      <c r="C40" s="53"/>
-      <c r="D40" s="53"/>
-      <c r="E40" s="53"/>
-      <c r="F40" s="35"/>
-      <c r="G40" s="54"/>
+      <c r="A40" s="56"/>
+      <c r="B40" s="57"/>
+      <c r="C40" s="57"/>
+      <c r="D40" s="57"/>
+      <c r="E40" s="57"/>
+      <c r="F40" s="39"/>
+      <c r="G40" s="58"/>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" s="33"/>
-      <c r="B41" s="34"/>
-      <c r="C41" s="34"/>
-      <c r="D41" s="34"/>
-      <c r="E41" s="34"/>
-      <c r="F41" s="35"/>
-      <c r="G41" s="36"/>
+      <c r="A41" s="37"/>
+      <c r="B41" s="38"/>
+      <c r="C41" s="38"/>
+      <c r="D41" s="38"/>
+      <c r="E41" s="38"/>
+      <c r="F41" s="39"/>
+      <c r="G41" s="40"/>
     </row>
     <row r="42" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A42" s="37"/>
-      <c r="B42" s="38"/>
-      <c r="C42" s="38"/>
-      <c r="D42" s="38"/>
-      <c r="E42" s="38"/>
-      <c r="F42" s="39"/>
-      <c r="G42" s="40"/>
+      <c r="A42" s="41"/>
+      <c r="B42" s="42"/>
+      <c r="C42" s="42"/>
+      <c r="D42" s="42"/>
+      <c r="E42" s="42"/>
+      <c r="F42" s="43"/>
+      <c r="G42" s="44"/>
     </row>
     <row r="43" spans="1:7" ht="26.25" customHeight="1">
-      <c r="A43" s="41"/>
-      <c r="B43" s="42"/>
-      <c r="C43" s="42"/>
-      <c r="D43" s="42"/>
-      <c r="E43" s="42"/>
-      <c r="F43" s="43"/>
-      <c r="G43" s="55"/>
+      <c r="A43" s="45"/>
+      <c r="B43" s="46"/>
+      <c r="C43" s="46"/>
+      <c r="D43" s="46"/>
+      <c r="E43" s="46"/>
+      <c r="F43" s="47"/>
+      <c r="G43" s="59"/>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="45"/>
-      <c r="B44" s="46"/>
-      <c r="C44" s="46"/>
-      <c r="D44" s="46"/>
-      <c r="E44" s="46"/>
-      <c r="F44" s="43"/>
-      <c r="G44" s="55"/>
+      <c r="A44" s="49"/>
+      <c r="B44" s="50"/>
+      <c r="C44" s="50"/>
+      <c r="D44" s="50"/>
+      <c r="E44" s="50"/>
+      <c r="F44" s="47"/>
+      <c r="G44" s="59"/>
     </row>
     <row r="45" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A45" s="48"/>
-      <c r="B45" s="49"/>
-      <c r="C45" s="49"/>
-      <c r="D45" s="49"/>
-      <c r="E45" s="49"/>
-      <c r="F45" s="50"/>
-      <c r="G45" s="56"/>
+      <c r="A45" s="52"/>
+      <c r="B45" s="53"/>
+      <c r="C45" s="53"/>
+      <c r="D45" s="53"/>
+      <c r="E45" s="53"/>
+      <c r="F45" s="54"/>
+      <c r="G45" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="47">
@@ -3074,85 +3092,85 @@
       </c>
     </row>
     <row r="17" spans="1:12" ht="23.25">
-      <c r="A17" s="60" t="s">
+      <c r="A17" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="61"/>
-      <c r="C17" s="61"/>
-      <c r="D17" s="61"/>
-      <c r="E17" s="61"/>
-      <c r="F17" s="61"/>
-      <c r="G17" s="61"/>
-      <c r="H17" s="61"/>
-      <c r="I17" s="61"/>
-      <c r="J17" s="61"/>
-      <c r="K17" s="61"/>
-      <c r="L17" s="61"/>
+      <c r="B17" s="65"/>
+      <c r="C17" s="65"/>
+      <c r="D17" s="65"/>
+      <c r="E17" s="65"/>
+      <c r="F17" s="65"/>
+      <c r="G17" s="65"/>
+      <c r="H17" s="65"/>
+      <c r="I17" s="65"/>
+      <c r="J17" s="65"/>
+      <c r="K17" s="65"/>
+      <c r="L17" s="65"/>
     </row>
     <row r="18" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A18" s="61" t="s">
+      <c r="A18" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="61" t="s">
+      <c r="B18" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="61" t="s">
+      <c r="C18" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="61" t="s">
+      <c r="D18" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="E18" s="61" t="s">
+      <c r="E18" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="F18" s="61" t="s">
+      <c r="F18" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="G18" s="61" t="s">
+      <c r="G18" s="65" t="s">
         <v>34</v>
       </c>
-      <c r="H18" s="61" t="s">
+      <c r="H18" s="65" t="s">
         <v>32</v>
       </c>
-      <c r="I18" s="61" t="s">
+      <c r="I18" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="J18" s="61" t="s">
+      <c r="J18" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="K18" s="61" t="s">
+      <c r="K18" s="65" t="s">
         <v>25</v>
       </c>
-      <c r="L18" s="61" t="s">
+      <c r="L18" s="65" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:12">
-      <c r="A19" s="62" t="s">
+      <c r="A19" s="66" t="s">
         <v>115</v>
       </c>
-      <c r="B19" s="62" t="s">
+      <c r="B19" s="66" t="s">
         <v>116</v>
       </c>
-      <c r="C19" s="62" t="s">
+      <c r="C19" s="66" t="s">
         <v>117</v>
       </c>
-      <c r="D19" s="62" t="s">
+      <c r="D19" s="66" t="s">
         <v>118</v>
       </c>
-      <c r="E19" s="61" t="s">
+      <c r="E19" s="65" t="s">
         <v>120</v>
       </c>
-      <c r="F19" s="62" t="s">
+      <c r="F19" s="66" t="s">
         <v>119</v>
       </c>
-      <c r="G19" s="62" t="s">
+      <c r="G19" s="66" t="s">
         <v>122</v>
       </c>
-      <c r="H19" s="61" t="s">
+      <c r="H19" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="I19" s="63" t="s">
+      <c r="I19" s="67" t="s">
         <v>126</v>
       </c>
       <c r="J19" s="8" t="s">
@@ -3166,7 +3184,7 @@
       </c>
     </row>
     <row r="20" spans="1:12" ht="14.25" customHeight="1">
-      <c r="I20" s="61"/>
+      <c r="I20" s="65"/>
     </row>
     <row r="21" spans="1:12" ht="23.25">
       <c r="A21" s="11" t="s">
@@ -3194,326 +3212,326 @@
       </c>
     </row>
     <row r="23" spans="1:12" ht="16.5" customHeight="1">
-      <c r="A23" s="64">
+      <c r="A23" s="68">
         <v>1</v>
       </c>
-      <c r="B23" s="65">
+      <c r="B23" s="69">
         <v>136</v>
       </c>
-      <c r="C23" s="65">
-        <v>2</v>
-      </c>
-      <c r="D23" s="65" t="s">
+      <c r="C23" s="69">
+        <v>2</v>
+      </c>
+      <c r="D23" s="69" t="s">
         <v>127</v>
       </c>
-      <c r="E23" s="65" t="s">
+      <c r="E23" s="69" t="s">
         <v>54</v>
       </c>
       <c r="F23" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="G23" s="66"/>
+      <c r="G23" s="70"/>
       <c r="K23" s="6"/>
     </row>
     <row r="24" spans="1:12" ht="26.25" customHeight="1" thickBot="1">
-      <c r="A24" s="67"/>
-      <c r="B24" s="68"/>
-      <c r="C24" s="68"/>
-      <c r="D24" s="68"/>
-      <c r="E24" s="68"/>
-      <c r="F24" s="69" t="s">
+      <c r="A24" s="71"/>
+      <c r="B24" s="72"/>
+      <c r="C24" s="72"/>
+      <c r="D24" s="72"/>
+      <c r="E24" s="72"/>
+      <c r="F24" s="73" t="s">
         <v>44</v>
       </c>
-      <c r="G24" s="70"/>
+      <c r="G24" s="74"/>
     </row>
     <row r="25" spans="1:12" ht="27" customHeight="1">
-      <c r="A25" s="71">
-        <v>2</v>
-      </c>
-      <c r="B25" s="72">
+      <c r="A25" s="75">
+        <v>2</v>
+      </c>
+      <c r="B25" s="76">
         <v>120</v>
       </c>
-      <c r="C25" s="72">
-        <v>2</v>
-      </c>
-      <c r="D25" s="72" t="s">
+      <c r="C25" s="76">
+        <v>2</v>
+      </c>
+      <c r="D25" s="76" t="s">
         <v>129</v>
       </c>
-      <c r="E25" s="72" t="s">
+      <c r="E25" s="76" t="s">
         <v>54</v>
       </c>
       <c r="F25" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="G25" s="73"/>
+      <c r="G25" s="77"/>
     </row>
     <row r="26" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A26" s="67"/>
-      <c r="B26" s="68"/>
-      <c r="C26" s="68"/>
-      <c r="D26" s="68"/>
-      <c r="E26" s="68"/>
-      <c r="F26" s="69" t="s">
+      <c r="A26" s="71"/>
+      <c r="B26" s="72"/>
+      <c r="C26" s="72"/>
+      <c r="D26" s="72"/>
+      <c r="E26" s="72"/>
+      <c r="F26" s="73" t="s">
         <v>44</v>
       </c>
-      <c r="G26" s="70"/>
+      <c r="G26" s="74"/>
     </row>
     <row r="27" spans="1:12" ht="27" customHeight="1">
-      <c r="A27" s="71">
+      <c r="A27" s="75">
         <v>3</v>
       </c>
-      <c r="B27" s="72">
+      <c r="B27" s="76">
         <v>120</v>
       </c>
-      <c r="C27" s="72">
-        <v>2</v>
-      </c>
-      <c r="D27" s="72" t="s">
+      <c r="C27" s="76">
+        <v>2</v>
+      </c>
+      <c r="D27" s="76" t="s">
         <v>130</v>
       </c>
-      <c r="E27" s="72" t="s">
+      <c r="E27" s="76" t="s">
         <v>54</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="G27" s="73"/>
+      <c r="G27" s="77"/>
     </row>
     <row r="28" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A28" s="67"/>
-      <c r="B28" s="68"/>
-      <c r="C28" s="68"/>
-      <c r="D28" s="68"/>
-      <c r="E28" s="68"/>
-      <c r="F28" s="69" t="s">
+      <c r="A28" s="71"/>
+      <c r="B28" s="72"/>
+      <c r="C28" s="72"/>
+      <c r="D28" s="72"/>
+      <c r="E28" s="72"/>
+      <c r="F28" s="73" t="s">
         <v>44</v>
       </c>
-      <c r="G28" s="70"/>
+      <c r="G28" s="74"/>
     </row>
     <row r="29" spans="1:12">
-      <c r="A29" s="71">
+      <c r="A29" s="75">
         <v>4</v>
       </c>
-      <c r="B29" s="72">
+      <c r="B29" s="76">
         <v>136</v>
       </c>
-      <c r="C29" s="72">
-        <v>2</v>
-      </c>
-      <c r="D29" s="72" t="s">
+      <c r="C29" s="76">
+        <v>2</v>
+      </c>
+      <c r="D29" s="76" t="s">
         <v>130</v>
       </c>
-      <c r="E29" s="72" t="s">
+      <c r="E29" s="76" t="s">
         <v>54</v>
       </c>
       <c r="F29" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="G29" s="73"/>
+      <c r="G29" s="77"/>
     </row>
     <row r="30" spans="1:12" ht="41.25" customHeight="1">
-      <c r="A30" s="64"/>
-      <c r="B30" s="65"/>
-      <c r="C30" s="65"/>
-      <c r="D30" s="65"/>
-      <c r="E30" s="65"/>
+      <c r="A30" s="68"/>
+      <c r="B30" s="69"/>
+      <c r="C30" s="69"/>
+      <c r="D30" s="69"/>
+      <c r="E30" s="69"/>
       <c r="F30" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="G30" s="66"/>
+      <c r="G30" s="70"/>
     </row>
     <row r="31" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A31" s="67"/>
-      <c r="B31" s="68"/>
-      <c r="C31" s="68"/>
-      <c r="D31" s="68"/>
-      <c r="E31" s="68"/>
-      <c r="F31" s="69" t="s">
+      <c r="A31" s="71"/>
+      <c r="B31" s="72"/>
+      <c r="C31" s="72"/>
+      <c r="D31" s="72"/>
+      <c r="E31" s="72"/>
+      <c r="F31" s="73" t="s">
         <v>108</v>
       </c>
-      <c r="G31" s="70"/>
+      <c r="G31" s="74"/>
     </row>
     <row r="32" spans="1:12" ht="27" customHeight="1">
-      <c r="A32" s="71">
+      <c r="A32" s="75">
         <v>5</v>
       </c>
-      <c r="B32" s="72">
+      <c r="B32" s="76">
         <v>116</v>
       </c>
-      <c r="C32" s="72">
-        <v>2</v>
-      </c>
-      <c r="D32" s="72" t="s">
+      <c r="C32" s="76">
+        <v>2</v>
+      </c>
+      <c r="D32" s="76" t="s">
         <v>129</v>
       </c>
-      <c r="E32" s="72" t="s">
+      <c r="E32" s="76" t="s">
         <v>54</v>
       </c>
       <c r="F32" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="G32" s="73"/>
+      <c r="G32" s="77"/>
     </row>
     <row r="33" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A33" s="67"/>
-      <c r="B33" s="68"/>
-      <c r="C33" s="68"/>
-      <c r="D33" s="68"/>
-      <c r="E33" s="68"/>
-      <c r="F33" s="69" t="s">
+      <c r="A33" s="71"/>
+      <c r="B33" s="72"/>
+      <c r="C33" s="72"/>
+      <c r="D33" s="72"/>
+      <c r="E33" s="72"/>
+      <c r="F33" s="73" t="s">
         <v>44</v>
       </c>
-      <c r="G33" s="70"/>
+      <c r="G33" s="74"/>
     </row>
     <row r="34" spans="1:7" ht="16.5" customHeight="1">
-      <c r="A34" s="71">
+      <c r="A34" s="75">
         <v>6</v>
       </c>
-      <c r="B34" s="72">
+      <c r="B34" s="76">
         <v>116</v>
       </c>
-      <c r="C34" s="72">
-        <v>2</v>
-      </c>
-      <c r="D34" s="72" t="s">
+      <c r="C34" s="76">
+        <v>2</v>
+      </c>
+      <c r="D34" s="76" t="s">
         <v>131</v>
       </c>
-      <c r="E34" s="72" t="s">
+      <c r="E34" s="76" t="s">
         <v>54</v>
       </c>
       <c r="F34" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="G34" s="73"/>
+      <c r="G34" s="77"/>
     </row>
     <row r="35" spans="1:7" ht="26.25" customHeight="1" thickBot="1">
-      <c r="A35" s="67"/>
-      <c r="B35" s="68"/>
-      <c r="C35" s="68"/>
-      <c r="D35" s="68"/>
-      <c r="E35" s="68"/>
-      <c r="F35" s="69" t="s">
+      <c r="A35" s="71"/>
+      <c r="B35" s="72"/>
+      <c r="C35" s="72"/>
+      <c r="D35" s="72"/>
+      <c r="E35" s="72"/>
+      <c r="F35" s="73" t="s">
         <v>44</v>
       </c>
-      <c r="G35" s="70"/>
+      <c r="G35" s="74"/>
     </row>
     <row r="36" spans="1:7" ht="27" customHeight="1">
-      <c r="A36" s="71">
+      <c r="A36" s="75">
         <v>7</v>
       </c>
-      <c r="B36" s="72">
+      <c r="B36" s="76">
         <v>268</v>
       </c>
-      <c r="C36" s="72">
+      <c r="C36" s="76">
         <v>3</v>
       </c>
-      <c r="D36" s="72" t="s">
+      <c r="D36" s="76" t="s">
         <v>132</v>
       </c>
-      <c r="E36" s="72" t="s">
+      <c r="E36" s="76" t="s">
         <v>54</v>
       </c>
       <c r="F36" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="G36" s="74"/>
+      <c r="G36" s="78"/>
     </row>
     <row r="37" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A37" s="67"/>
-      <c r="B37" s="68"/>
-      <c r="C37" s="68"/>
-      <c r="D37" s="68"/>
-      <c r="E37" s="68"/>
-      <c r="F37" s="69" t="s">
+      <c r="A37" s="71"/>
+      <c r="B37" s="72"/>
+      <c r="C37" s="72"/>
+      <c r="D37" s="72"/>
+      <c r="E37" s="72"/>
+      <c r="F37" s="73" t="s">
         <v>108</v>
       </c>
-      <c r="G37" s="75"/>
+      <c r="G37" s="79"/>
     </row>
     <row r="38" spans="1:7" ht="26.25" customHeight="1">
-      <c r="A38" s="71">
+      <c r="A38" s="75">
         <v>7</v>
       </c>
-      <c r="B38" s="72">
+      <c r="B38" s="76">
         <v>148</v>
       </c>
-      <c r="C38" s="72">
+      <c r="C38" s="76">
         <v>4</v>
       </c>
-      <c r="D38" s="72" t="s">
+      <c r="D38" s="76" t="s">
         <v>109</v>
       </c>
-      <c r="E38" s="72" t="s">
+      <c r="E38" s="76" t="s">
         <v>91</v>
       </c>
       <c r="F38" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="G38" s="73"/>
+      <c r="G38" s="77"/>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39" s="64"/>
-      <c r="B39" s="65"/>
-      <c r="C39" s="65"/>
-      <c r="D39" s="65"/>
-      <c r="E39" s="65"/>
+      <c r="A39" s="68"/>
+      <c r="B39" s="69"/>
+      <c r="C39" s="69"/>
+      <c r="D39" s="69"/>
+      <c r="E39" s="69"/>
       <c r="F39" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="G39" s="66"/>
+      <c r="G39" s="70"/>
     </row>
     <row r="40" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A40" s="67"/>
-      <c r="B40" s="68"/>
-      <c r="C40" s="68"/>
-      <c r="D40" s="68"/>
-      <c r="E40" s="68"/>
-      <c r="F40" s="69" t="s">
+      <c r="A40" s="71"/>
+      <c r="B40" s="72"/>
+      <c r="C40" s="72"/>
+      <c r="D40" s="72"/>
+      <c r="E40" s="72"/>
+      <c r="F40" s="73" t="s">
         <v>108</v>
       </c>
-      <c r="G40" s="70"/>
+      <c r="G40" s="74"/>
     </row>
     <row r="41" spans="1:7" ht="26.25" customHeight="1">
-      <c r="A41" s="71">
+      <c r="A41" s="75">
         <v>8</v>
       </c>
-      <c r="B41" s="72">
+      <c r="B41" s="76">
         <v>147</v>
       </c>
-      <c r="C41" s="72">
+      <c r="C41" s="76">
         <v>4</v>
       </c>
-      <c r="D41" s="72" t="s">
+      <c r="D41" s="76" t="s">
         <v>110</v>
       </c>
-      <c r="E41" s="72" t="s">
+      <c r="E41" s="76" t="s">
         <v>91</v>
       </c>
       <c r="F41" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="G41" s="74"/>
+      <c r="G41" s="78"/>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="64"/>
-      <c r="B42" s="65"/>
-      <c r="C42" s="65"/>
-      <c r="D42" s="65"/>
-      <c r="E42" s="65"/>
+      <c r="A42" s="68"/>
+      <c r="B42" s="69"/>
+      <c r="C42" s="69"/>
+      <c r="D42" s="69"/>
+      <c r="E42" s="69"/>
       <c r="F42" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="G42" s="74"/>
+      <c r="G42" s="78"/>
     </row>
     <row r="43" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A43" s="67"/>
-      <c r="B43" s="68"/>
-      <c r="C43" s="68"/>
-      <c r="D43" s="68"/>
-      <c r="E43" s="68"/>
-      <c r="F43" s="69" t="s">
+      <c r="A43" s="71"/>
+      <c r="B43" s="72"/>
+      <c r="C43" s="72"/>
+      <c r="D43" s="72"/>
+      <c r="E43" s="72"/>
+      <c r="F43" s="73" t="s">
         <v>108</v>
       </c>
-      <c r="G43" s="75"/>
+      <c r="G43" s="79"/>
     </row>
   </sheetData>
   <mergeCells count="52">
@@ -3667,61 +3685,61 @@
       <c r="A12" s="8"/>
     </row>
     <row r="17" spans="1:12" ht="23.25">
-      <c r="A17" s="60" t="s">
+      <c r="A17" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="61"/>
-      <c r="C17" s="61"/>
-      <c r="D17" s="61"/>
-      <c r="E17" s="61"/>
-      <c r="F17" s="61"/>
-      <c r="G17" s="61"/>
-      <c r="H17" s="61"/>
-      <c r="I17" s="61"/>
-      <c r="J17" s="61"/>
-      <c r="K17" s="61"/>
-      <c r="L17" s="61"/>
+      <c r="B17" s="65"/>
+      <c r="C17" s="65"/>
+      <c r="D17" s="65"/>
+      <c r="E17" s="65"/>
+      <c r="F17" s="65"/>
+      <c r="G17" s="65"/>
+      <c r="H17" s="65"/>
+      <c r="I17" s="65"/>
+      <c r="J17" s="65"/>
+      <c r="K17" s="65"/>
+      <c r="L17" s="65"/>
     </row>
     <row r="18" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A18" s="61" t="s">
+      <c r="A18" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="61" t="s">
+      <c r="B18" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="61" t="s">
+      <c r="C18" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="61" t="s">
+      <c r="D18" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="E18" s="61" t="s">
+      <c r="E18" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="F18" s="61" t="s">
+      <c r="F18" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="G18" s="61" t="s">
+      <c r="G18" s="65" t="s">
         <v>34</v>
       </c>
-      <c r="H18" s="61" t="s">
+      <c r="H18" s="65" t="s">
         <v>32</v>
       </c>
-      <c r="I18" s="61" t="s">
+      <c r="I18" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="J18" s="61" t="s">
+      <c r="J18" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="K18" s="61" t="s">
+      <c r="K18" s="65" t="s">
         <v>25</v>
       </c>
-      <c r="L18" s="61" t="s">
+      <c r="L18" s="65" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="15.75">
-      <c r="A19" s="62" t="s">
+      <c r="A19" s="66" t="s">
         <v>134</v>
       </c>
       <c r="B19" s="8" t="s">
@@ -3733,7 +3751,7 @@
       <c r="D19" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="E19" s="61" t="s">
+      <c r="E19" s="65" t="s">
         <v>138</v>
       </c>
       <c r="F19" s="8" t="s">
@@ -3742,24 +3760,24 @@
       <c r="G19" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="H19" s="61" t="s">
+      <c r="H19" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="I19" s="82" t="s">
+      <c r="I19" s="88" t="s">
         <v>141</v>
       </c>
-      <c r="J19" s="82" t="s">
+      <c r="J19" s="88" t="s">
         <v>142</v>
       </c>
-      <c r="K19" s="82" t="s">
+      <c r="K19" s="88" t="s">
         <v>143</v>
       </c>
-      <c r="L19" s="83" t="s">
+      <c r="L19" s="89" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="14.25" customHeight="1">
-      <c r="I20" s="61"/>
+      <c r="I20" s="65"/>
     </row>
     <row r="21" spans="1:12" ht="23.25">
       <c r="A21" s="11" t="s">
@@ -3787,162 +3805,162 @@
       </c>
     </row>
     <row r="23" spans="1:12" ht="16.5" customHeight="1">
-      <c r="A23" s="71">
+      <c r="A23" s="75">
         <v>1</v>
       </c>
-      <c r="B23" s="72">
+      <c r="B23" s="76">
         <v>291</v>
       </c>
-      <c r="C23" s="72">
+      <c r="C23" s="76">
         <v>0</v>
       </c>
-      <c r="D23" s="72" t="s">
+      <c r="D23" s="76" t="s">
         <v>145</v>
       </c>
-      <c r="E23" s="72" t="s">
+      <c r="E23" s="76" t="s">
         <v>54</v>
       </c>
-      <c r="F23" s="80" t="s">
+      <c r="F23" s="85" t="s">
         <v>56</v>
       </c>
-      <c r="G23" s="73"/>
+      <c r="G23" s="77"/>
       <c r="K23" s="6"/>
     </row>
     <row r="24" spans="1:12" ht="26.25" customHeight="1" thickBot="1">
-      <c r="A24" s="67"/>
-      <c r="B24" s="68"/>
-      <c r="C24" s="68"/>
-      <c r="D24" s="68"/>
-      <c r="E24" s="68"/>
-      <c r="F24" s="69" t="s">
+      <c r="A24" s="71"/>
+      <c r="B24" s="72"/>
+      <c r="C24" s="72"/>
+      <c r="D24" s="72"/>
+      <c r="E24" s="72"/>
+      <c r="F24" s="73" t="s">
         <v>108</v>
       </c>
-      <c r="G24" s="70"/>
+      <c r="G24" s="74"/>
     </row>
     <row r="25" spans="1:12" ht="27" customHeight="1">
-      <c r="A25" s="71">
-        <v>2</v>
-      </c>
-      <c r="B25" s="72">
+      <c r="A25" s="75">
+        <v>2</v>
+      </c>
+      <c r="B25" s="76">
         <v>121</v>
       </c>
-      <c r="C25" s="72">
+      <c r="C25" s="76">
         <v>0</v>
       </c>
-      <c r="D25" s="72" t="s">
+      <c r="D25" s="76" t="s">
         <v>146</v>
       </c>
-      <c r="E25" s="72"/>
+      <c r="E25" s="76"/>
       <c r="F25" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="G25" s="73"/>
+      <c r="G25" s="77"/>
     </row>
     <row r="26" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A26" s="67"/>
-      <c r="B26" s="68"/>
-      <c r="C26" s="68"/>
-      <c r="D26" s="68"/>
-      <c r="E26" s="68"/>
-      <c r="F26" s="69" t="s">
+      <c r="A26" s="71"/>
+      <c r="B26" s="72"/>
+      <c r="C26" s="72"/>
+      <c r="D26" s="72"/>
+      <c r="E26" s="72"/>
+      <c r="F26" s="73" t="s">
         <v>108</v>
       </c>
-      <c r="G26" s="70"/>
+      <c r="G26" s="74"/>
     </row>
     <row r="27" spans="1:12" ht="27" customHeight="1">
-      <c r="A27" s="71">
+      <c r="A27" s="75">
         <v>3</v>
       </c>
-      <c r="B27" s="72">
+      <c r="B27" s="76">
         <v>89</v>
       </c>
-      <c r="C27" s="72">
-        <v>2</v>
-      </c>
-      <c r="D27" s="72" t="s">
+      <c r="C27" s="76">
+        <v>2</v>
+      </c>
+      <c r="D27" s="76" t="s">
         <v>147</v>
       </c>
-      <c r="E27" s="72" t="s">
+      <c r="E27" s="76" t="s">
         <v>54</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="G27" s="73"/>
+      <c r="G27" s="77"/>
     </row>
     <row r="28" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A28" s="67"/>
-      <c r="B28" s="68"/>
-      <c r="C28" s="68"/>
-      <c r="D28" s="68"/>
-      <c r="E28" s="68"/>
-      <c r="F28" s="69" t="s">
+      <c r="A28" s="71"/>
+      <c r="B28" s="72"/>
+      <c r="C28" s="72"/>
+      <c r="D28" s="72"/>
+      <c r="E28" s="72"/>
+      <c r="F28" s="73" t="s">
         <v>108</v>
       </c>
-      <c r="G28" s="70"/>
+      <c r="G28" s="74"/>
     </row>
     <row r="29" spans="1:12" ht="43.5" thickBot="1">
-      <c r="A29" s="77">
+      <c r="A29" s="81">
         <v>4</v>
       </c>
-      <c r="B29" s="69">
+      <c r="B29" s="73">
         <v>89</v>
       </c>
-      <c r="C29" s="69">
-        <v>2</v>
-      </c>
-      <c r="D29" s="69" t="s">
+      <c r="C29" s="73">
+        <v>2</v>
+      </c>
+      <c r="D29" s="73" t="s">
         <v>147</v>
       </c>
-      <c r="E29" s="69" t="s">
+      <c r="E29" s="73" t="s">
         <v>54</v>
       </c>
-      <c r="F29" s="69" t="s">
+      <c r="F29" s="73" t="s">
         <v>56</v>
       </c>
-      <c r="G29" s="78"/>
+      <c r="G29" s="82"/>
     </row>
     <row r="30" spans="1:12" ht="41.25" customHeight="1" thickBot="1">
-      <c r="A30" s="77">
+      <c r="A30" s="81">
         <v>5</v>
       </c>
-      <c r="B30" s="69">
+      <c r="B30" s="73">
         <v>89</v>
       </c>
-      <c r="C30" s="69">
-        <v>2</v>
-      </c>
-      <c r="D30" s="69" t="s">
+      <c r="C30" s="73">
+        <v>2</v>
+      </c>
+      <c r="D30" s="73" t="s">
         <v>147</v>
       </c>
-      <c r="E30" s="69" t="s">
+      <c r="E30" s="73" t="s">
         <v>54</v>
       </c>
-      <c r="F30" s="69" t="s">
+      <c r="F30" s="73" t="s">
         <v>56</v>
       </c>
-      <c r="G30" s="78"/>
+      <c r="G30" s="82"/>
     </row>
     <row r="31" spans="1:12" ht="43.5" thickBot="1">
-      <c r="A31" s="77">
+      <c r="A31" s="81">
         <v>6</v>
       </c>
-      <c r="B31" s="69">
+      <c r="B31" s="73">
         <v>89</v>
       </c>
-      <c r="C31" s="69">
-        <v>2</v>
-      </c>
-      <c r="D31" s="69" t="s">
+      <c r="C31" s="73">
+        <v>2</v>
+      </c>
+      <c r="D31" s="73" t="s">
         <v>147</v>
       </c>
-      <c r="E31" s="69" t="s">
+      <c r="E31" s="73" t="s">
         <v>54</v>
       </c>
-      <c r="F31" s="69" t="s">
+      <c r="F31" s="73" t="s">
         <v>56</v>
       </c>
-      <c r="G31" s="75"/>
+      <c r="G31" s="79"/>
     </row>
   </sheetData>
   <mergeCells count="18">
@@ -4067,56 +4085,56 @@
       </c>
     </row>
     <row r="17" spans="1:12" ht="23.25">
-      <c r="A17" s="60" t="s">
+      <c r="A17" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="61"/>
-      <c r="C17" s="61"/>
-      <c r="D17" s="61"/>
-      <c r="E17" s="61"/>
-      <c r="F17" s="61"/>
-      <c r="G17" s="61"/>
-      <c r="H17" s="61"/>
-      <c r="I17" s="61"/>
-      <c r="J17" s="61"/>
-      <c r="K17" s="61"/>
-      <c r="L17" s="61"/>
+      <c r="B17" s="65"/>
+      <c r="C17" s="65"/>
+      <c r="D17" s="65"/>
+      <c r="E17" s="65"/>
+      <c r="F17" s="65"/>
+      <c r="G17" s="65"/>
+      <c r="H17" s="65"/>
+      <c r="I17" s="65"/>
+      <c r="J17" s="65"/>
+      <c r="K17" s="65"/>
+      <c r="L17" s="65"/>
     </row>
     <row r="18" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A18" s="61" t="s">
+      <c r="A18" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="61" t="s">
+      <c r="B18" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="61" t="s">
+      <c r="C18" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="61" t="s">
+      <c r="D18" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="E18" s="61" t="s">
+      <c r="E18" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="F18" s="61" t="s">
+      <c r="F18" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="G18" s="61" t="s">
+      <c r="G18" s="65" t="s">
         <v>34</v>
       </c>
-      <c r="H18" s="61" t="s">
+      <c r="H18" s="65" t="s">
         <v>32</v>
       </c>
-      <c r="I18" s="61" t="s">
+      <c r="I18" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="J18" s="61" t="s">
+      <c r="J18" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="K18" s="61" t="s">
+      <c r="K18" s="65" t="s">
         <v>25</v>
       </c>
-      <c r="L18" s="61" t="s">
+      <c r="L18" s="65" t="s">
         <v>29</v>
       </c>
     </row>
@@ -4133,7 +4151,7 @@
       <c r="D19" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="E19" s="61" t="s">
+      <c r="E19" s="65" t="s">
         <v>155</v>
       </c>
       <c r="F19" s="1" t="s">
@@ -4142,7 +4160,7 @@
       <c r="G19" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="H19" s="61" t="s">
+      <c r="H19" s="65" t="s">
         <v>33</v>
       </c>
       <c r="I19" s="1" t="s">
@@ -4159,7 +4177,7 @@
       </c>
     </row>
     <row r="20" spans="1:12" ht="14.25" customHeight="1">
-      <c r="I20" s="61"/>
+      <c r="I20" s="65"/>
     </row>
     <row r="21" spans="1:12" ht="23.25">
       <c r="A21" s="11" t="s">
@@ -4187,141 +4205,141 @@
       </c>
     </row>
     <row r="23" spans="1:12" ht="16.5" customHeight="1">
-      <c r="A23" s="84"/>
-      <c r="B23" s="85"/>
-      <c r="C23" s="85"/>
-      <c r="D23" s="85"/>
-      <c r="E23" s="85"/>
-      <c r="F23" s="85"/>
+      <c r="A23" s="90"/>
+      <c r="B23" s="91"/>
+      <c r="C23" s="91"/>
+      <c r="D23" s="91"/>
+      <c r="E23" s="91"/>
+      <c r="F23" s="91"/>
       <c r="J23" s="6"/>
     </row>
     <row r="24" spans="1:12" ht="30" customHeight="1">
-      <c r="A24" s="33">
+      <c r="A24" s="37">
         <v>1</v>
       </c>
-      <c r="B24" s="34">
+      <c r="B24" s="38">
         <v>105</v>
       </c>
-      <c r="C24" s="34">
-        <v>2</v>
-      </c>
-      <c r="D24" s="34" t="s">
+      <c r="C24" s="38">
+        <v>2</v>
+      </c>
+      <c r="D24" s="38" t="s">
         <v>160</v>
       </c>
-      <c r="E24" s="34" t="s">
+      <c r="E24" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="F24" s="35" t="s">
+      <c r="F24" s="39" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="27" customHeight="1" thickBot="1">
-      <c r="A25" s="37"/>
-      <c r="B25" s="38"/>
-      <c r="C25" s="38"/>
-      <c r="D25" s="38"/>
-      <c r="E25" s="38"/>
-      <c r="F25" s="39" t="s">
+      <c r="A25" s="41"/>
+      <c r="B25" s="42"/>
+      <c r="C25" s="42"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="42"/>
+      <c r="F25" s="43" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="57.75" thickBot="1">
-      <c r="A26" s="59">
-        <v>2</v>
-      </c>
-      <c r="B26" s="50">
+      <c r="A26" s="63">
+        <v>2</v>
+      </c>
+      <c r="B26" s="54">
         <v>105</v>
       </c>
-      <c r="C26" s="50">
-        <v>2</v>
-      </c>
-      <c r="D26" s="50" t="s">
+      <c r="C26" s="54">
+        <v>2</v>
+      </c>
+      <c r="D26" s="54" t="s">
         <v>160</v>
       </c>
-      <c r="E26" s="50" t="s">
+      <c r="E26" s="54" t="s">
         <v>55</v>
       </c>
-      <c r="F26" s="50" t="s">
+      <c r="F26" s="54" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="41.25" customHeight="1">
-      <c r="A27" s="52">
+      <c r="A27" s="56">
         <v>3</v>
       </c>
-      <c r="B27" s="53">
+      <c r="B27" s="57">
         <v>262</v>
       </c>
-      <c r="C27" s="53">
-        <v>2</v>
-      </c>
-      <c r="D27" s="53" t="s">
+      <c r="C27" s="57">
+        <v>2</v>
+      </c>
+      <c r="D27" s="57" t="s">
         <v>161</v>
       </c>
-      <c r="E27" s="53" t="s">
+      <c r="E27" s="57" t="s">
         <v>55</v>
       </c>
-      <c r="F27" s="35" t="s">
+      <c r="F27" s="39" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A28" s="37"/>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="39" t="s">
+      <c r="A28" s="41"/>
+      <c r="B28" s="42"/>
+      <c r="C28" s="42"/>
+      <c r="D28" s="42"/>
+      <c r="E28" s="42"/>
+      <c r="F28" s="43" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A29" s="41">
+      <c r="A29" s="45">
         <v>4</v>
       </c>
-      <c r="B29" s="42">
+      <c r="B29" s="46">
         <v>262</v>
       </c>
-      <c r="C29" s="42">
-        <v>2</v>
-      </c>
-      <c r="D29" s="42" t="s">
+      <c r="C29" s="46">
+        <v>2</v>
+      </c>
+      <c r="D29" s="46" t="s">
         <v>161</v>
       </c>
-      <c r="E29" s="42" t="s">
+      <c r="E29" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="F29" s="43" t="s">
+      <c r="F29" s="47" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="41.25" customHeight="1" thickBot="1">
-      <c r="A30" s="48"/>
-      <c r="B30" s="49"/>
-      <c r="C30" s="49"/>
-      <c r="D30" s="49"/>
-      <c r="E30" s="49"/>
-      <c r="F30" s="50" t="s">
+      <c r="A30" s="52"/>
+      <c r="B30" s="53"/>
+      <c r="C30" s="53"/>
+      <c r="D30" s="53"/>
+      <c r="E30" s="53"/>
+      <c r="F30" s="54" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="57.75" thickBot="1">
-      <c r="A31" s="58">
+      <c r="A31" s="62">
         <v>5</v>
       </c>
-      <c r="B31" s="39">
+      <c r="B31" s="43">
         <v>178</v>
       </c>
-      <c r="C31" s="39">
-        <v>2</v>
-      </c>
-      <c r="D31" s="39" t="s">
+      <c r="C31" s="43">
+        <v>2</v>
+      </c>
+      <c r="D31" s="43" t="s">
         <v>162</v>
       </c>
-      <c r="E31" s="39" t="s">
+      <c r="E31" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="F31" s="39" t="s">
+      <c r="F31" s="43" t="s">
         <v>163</v>
       </c>
     </row>
@@ -4351,8 +4369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B35" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F23" sqref="A23:XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4440,56 +4458,56 @@
       <c r="A12" s="1"/>
     </row>
     <row r="17" spans="1:12" ht="23.25">
-      <c r="A17" s="60" t="s">
+      <c r="A17" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="61"/>
-      <c r="C17" s="61"/>
-      <c r="D17" s="61"/>
-      <c r="E17" s="61"/>
-      <c r="F17" s="61"/>
-      <c r="G17" s="61"/>
-      <c r="H17" s="61"/>
-      <c r="I17" s="61"/>
-      <c r="J17" s="61"/>
-      <c r="K17" s="61"/>
-      <c r="L17" s="61"/>
+      <c r="B17" s="65"/>
+      <c r="C17" s="65"/>
+      <c r="D17" s="65"/>
+      <c r="E17" s="65"/>
+      <c r="F17" s="65"/>
+      <c r="G17" s="65"/>
+      <c r="H17" s="65"/>
+      <c r="I17" s="65"/>
+      <c r="J17" s="65"/>
+      <c r="K17" s="65"/>
+      <c r="L17" s="65"/>
     </row>
     <row r="18" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A18" s="61" t="s">
+      <c r="A18" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="61" t="s">
+      <c r="B18" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="61" t="s">
+      <c r="C18" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="61" t="s">
+      <c r="D18" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="E18" s="61" t="s">
+      <c r="E18" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="F18" s="61" t="s">
+      <c r="F18" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="G18" s="61" t="s">
+      <c r="G18" s="65" t="s">
         <v>34</v>
       </c>
-      <c r="H18" s="61" t="s">
+      <c r="H18" s="65" t="s">
         <v>32</v>
       </c>
-      <c r="I18" s="61" t="s">
+      <c r="I18" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="J18" s="61" t="s">
+      <c r="J18" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="K18" s="61" t="s">
+      <c r="K18" s="65" t="s">
         <v>25</v>
       </c>
-      <c r="L18" s="61" t="s">
+      <c r="L18" s="65" t="s">
         <v>29</v>
       </c>
     </row>
@@ -4506,7 +4524,7 @@
       <c r="D19" s="19" t="s">
         <v>168</v>
       </c>
-      <c r="E19" s="61" t="s">
+      <c r="E19" s="65" t="s">
         <v>155</v>
       </c>
       <c r="F19" s="19" t="s">
@@ -4515,16 +4533,16 @@
       <c r="G19" s="19" t="s">
         <v>170</v>
       </c>
-      <c r="H19" s="61" t="s">
+      <c r="H19" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="I19" s="76" t="s">
+      <c r="I19" s="80" t="s">
         <v>171</v>
       </c>
-      <c r="J19" s="76" t="s">
+      <c r="J19" s="80" t="s">
         <v>172</v>
       </c>
-      <c r="K19" s="76" t="s">
+      <c r="K19" s="80" t="s">
         <v>173</v>
       </c>
       <c r="L19" s="20" t="s">
@@ -4532,7 +4550,7 @@
       </c>
     </row>
     <row r="20" spans="1:12" ht="14.25" customHeight="1">
-      <c r="I20" s="61"/>
+      <c r="I20" s="65"/>
     </row>
     <row r="21" spans="1:12" ht="23.25">
       <c r="A21" s="11" t="s">
@@ -4560,24 +4578,25 @@
       </c>
     </row>
     <row r="23" spans="1:12" ht="30" customHeight="1">
-      <c r="A23" s="31">
+      <c r="A23" s="34">
         <v>1</v>
       </c>
-      <c r="B23" s="32">
+      <c r="B23" s="35">
         <v>301</v>
       </c>
-      <c r="C23" s="32">
-        <v>2</v>
-      </c>
-      <c r="D23" s="32" t="s">
+      <c r="C23" s="35">
+        <v>2</v>
+      </c>
+      <c r="D23" s="35" t="s">
         <v>175</v>
       </c>
-      <c r="E23" s="32" t="s">
+      <c r="E23" s="35" t="s">
         <v>55</v>
       </c>
       <c r="F23" s="21" t="s">
         <v>44</v>
       </c>
+      <c r="G23" s="36"/>
     </row>
     <row r="24" spans="1:12" ht="27" customHeight="1" thickBot="1">
       <c r="A24" s="25"/>
@@ -4588,39 +4607,42 @@
       <c r="F24" s="22" t="s">
         <v>108</v>
       </c>
+      <c r="G24" s="27"/>
     </row>
     <row r="25" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A25" s="27">
-        <v>2</v>
-      </c>
-      <c r="B25" s="29">
+      <c r="A25" s="28">
+        <v>2</v>
+      </c>
+      <c r="B25" s="30">
         <v>193</v>
       </c>
-      <c r="C25" s="29">
-        <v>2</v>
-      </c>
-      <c r="D25" s="29" t="s">
+      <c r="C25" s="30">
+        <v>2</v>
+      </c>
+      <c r="D25" s="30" t="s">
         <v>176</v>
       </c>
-      <c r="E25" s="29" t="s">
+      <c r="E25" s="30" t="s">
         <v>55</v>
       </c>
       <c r="F25" s="23" t="s">
         <v>56</v>
       </c>
+      <c r="G25" s="32"/>
     </row>
     <row r="26" spans="1:12" ht="41.25" customHeight="1" thickBot="1">
-      <c r="A26" s="28"/>
-      <c r="B26" s="30"/>
-      <c r="C26" s="30"/>
-      <c r="D26" s="30"/>
-      <c r="E26" s="30"/>
+      <c r="A26" s="29"/>
+      <c r="B26" s="31"/>
+      <c r="C26" s="31"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="31"/>
       <c r="F26" s="24" t="s">
         <v>108</v>
       </c>
+      <c r="G26" s="33"/>
     </row>
     <row r="27" spans="1:12" ht="57.75" thickBot="1">
-      <c r="A27" s="79">
+      <c r="A27" s="83">
         <v>3</v>
       </c>
       <c r="B27" s="22">
@@ -4638,56 +4660,60 @@
       <c r="F27" s="22" t="s">
         <v>56</v>
       </c>
+      <c r="G27" s="84"/>
     </row>
     <row r="28" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A28" s="27">
+      <c r="A28" s="28">
         <v>4</v>
       </c>
-      <c r="B28" s="29">
+      <c r="B28" s="30">
         <v>114</v>
       </c>
-      <c r="C28" s="29">
-        <v>2</v>
-      </c>
-      <c r="D28" s="29" t="s">
+      <c r="C28" s="30">
+        <v>2</v>
+      </c>
+      <c r="D28" s="30" t="s">
         <v>178</v>
       </c>
-      <c r="E28" s="29" t="s">
+      <c r="E28" s="30" t="s">
         <v>55</v>
       </c>
       <c r="F28" s="23" t="s">
         <v>56</v>
       </c>
+      <c r="G28" s="32"/>
     </row>
     <row r="29" spans="1:12" ht="41.25" customHeight="1" thickBot="1">
-      <c r="A29" s="28"/>
-      <c r="B29" s="30"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="30"/>
+      <c r="A29" s="29"/>
+      <c r="B29" s="31"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="31"/>
       <c r="F29" s="24" t="s">
         <v>108</v>
       </c>
+      <c r="G29" s="33"/>
     </row>
     <row r="30" spans="1:12" ht="41.25" customHeight="1">
-      <c r="A30" s="31">
+      <c r="A30" s="34">
         <v>5</v>
       </c>
-      <c r="B30" s="32">
+      <c r="B30" s="35">
         <v>114</v>
       </c>
-      <c r="C30" s="32">
-        <v>2</v>
-      </c>
-      <c r="D30" s="32" t="s">
+      <c r="C30" s="35">
+        <v>2</v>
+      </c>
+      <c r="D30" s="35" t="s">
         <v>178</v>
       </c>
-      <c r="E30" s="32" t="s">
+      <c r="E30" s="35" t="s">
         <v>55</v>
       </c>
       <c r="F30" s="21" t="s">
         <v>56</v>
       </c>
+      <c r="G30" s="36"/>
     </row>
     <row r="31" spans="1:12" ht="15.75" thickBot="1">
       <c r="A31" s="25"/>
@@ -4698,9 +4724,10 @@
       <c r="F31" s="22" t="s">
         <v>108</v>
       </c>
+      <c r="G31" s="27"/>
     </row>
     <row r="32" spans="1:12" ht="57.75" thickBot="1">
-      <c r="A32" s="81">
+      <c r="A32" s="86">
         <v>6</v>
       </c>
       <c r="B32" s="24">
@@ -4718,9 +4745,10 @@
       <c r="F32" s="24" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" ht="57.75" thickBot="1">
-      <c r="A33" s="79">
+      <c r="G32" s="87"/>
+    </row>
+    <row r="33" spans="1:7" ht="57.75" thickBot="1">
+      <c r="A33" s="83">
         <v>7</v>
       </c>
       <c r="B33" s="22">
@@ -4738,20 +4766,25 @@
       <c r="F33" s="22" t="s">
         <v>56</v>
       </c>
+      <c r="G33" s="84"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="24">
     <mergeCell ref="E25:E26"/>
+    <mergeCell ref="G25:G26"/>
+    <mergeCell ref="G28:G29"/>
     <mergeCell ref="A30:A31"/>
     <mergeCell ref="B30:B31"/>
     <mergeCell ref="C30:C31"/>
     <mergeCell ref="D30:D31"/>
     <mergeCell ref="E30:E31"/>
+    <mergeCell ref="G30:G31"/>
     <mergeCell ref="A28:A29"/>
     <mergeCell ref="B28:B29"/>
     <mergeCell ref="C28:C29"/>
     <mergeCell ref="D28:D29"/>
     <mergeCell ref="E28:E29"/>
+    <mergeCell ref="G23:G24"/>
     <mergeCell ref="A25:A26"/>
     <mergeCell ref="B25:B26"/>
     <mergeCell ref="C25:C26"/>

</xml_diff>

<commit_message>
paar schoolheids fouten uit de exel gehaalt
</commit_message>
<xml_diff>
--- a/documentatie_And_sql/documentatie/BioscoopData.xlsx
+++ b/documentatie_And_sql/documentatie/BioscoopData.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\PHP\gameparty_project_met_georgi\documentatie_And_sql\documentatie\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\php\gameparty_project_met_georgi\documentatie_And_sql\documentatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{CB70D5C9-12C7-4171-B647-E04388C665D4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7350" firstSheet="5" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20405" windowHeight="7349" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="almere" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
     <sheet name="Den Bosch" sheetId="5" r:id="rId5"/>
     <sheet name="Den Helder" sheetId="6" r:id="rId6"/>
     <sheet name="Dordrecht" sheetId="7" r:id="rId7"/>
-    <sheet name="Blad5" sheetId="8" r:id="rId8"/>
+    <sheet name="emmen" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -290,9 +291,6 @@
     <t>Grotewallerweg 2</t>
   </si>
   <si>
-    <t>1742NM</t>
-  </si>
-  <si>
     <t>Schagen</t>
   </si>
   <si>
@@ -357,9 +355,6 @@
     <t>Hoofddorp</t>
   </si>
   <si>
-    <t>2132TZ</t>
-  </si>
-  <si>
     <t>023-3031030</t>
   </si>
   <si>
@@ -406,9 +401,6 @@
   </si>
   <si>
     <t>Bordeslaan 510</t>
-  </si>
-  <si>
-    <t>5223MX</t>
   </si>
   <si>
     <t>Den Bosch</t>
@@ -593,13 +585,22 @@
   </si>
   <si>
     <t>11.25m x 4.95m</t>
+  </si>
+  <si>
+    <t>1742 NM</t>
+  </si>
+  <si>
+    <t>2132 TZ</t>
+  </si>
+  <si>
+    <t>5223 MX</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -646,16 +647,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF6E7474"/>
-      <name val="Montserrat"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Montserrat"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF6E7474"/>
       <name val="Montserrat"/>
     </font>
   </fonts>
@@ -803,7 +794,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -839,125 +830,30 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -970,6 +866,96 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -979,55 +965,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -1307,25 +1244,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView topLeftCell="B9" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView topLeftCell="F13" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.3"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="16.375" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" customWidth="1"/>
-    <col min="5" max="5" width="42.28515625" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" customWidth="1"/>
-    <col min="11" max="11" width="22.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.625" customWidth="1"/>
+    <col min="5" max="5" width="42.25" customWidth="1"/>
+    <col min="6" max="6" width="13.125" customWidth="1"/>
+    <col min="8" max="8" width="16.875" customWidth="1"/>
+    <col min="11" max="11" width="22.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="23.25">
+    <row r="1" spans="1:2" ht="23.8">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -1370,7 +1307,7 @@
         <v>8.6999999999999993</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="23.25">
+    <row r="8" spans="1:2" ht="23.8">
       <c r="A8" s="10" t="s">
         <v>7</v>
       </c>
@@ -1423,7 +1360,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="23.25">
+    <row r="17" spans="1:12" ht="23.8">
       <c r="A17" s="10" t="s">
         <v>13</v>
       </c>
@@ -1480,7 +1417,7 @@
         <v>14</v>
       </c>
       <c r="E19" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>22</v>
@@ -1504,7 +1441,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="23.25">
+    <row r="22" spans="1:12" ht="23.8">
       <c r="A22" s="9" t="s">
         <v>36</v>
       </c>
@@ -1534,7 +1471,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="30">
+    <row r="24" spans="1:12" ht="28.55">
       <c r="A24" s="4">
         <v>1</v>
       </c>
@@ -1554,7 +1491,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="30">
+    <row r="25" spans="1:12" ht="28.55">
       <c r="A25" s="4">
         <v>2</v>
       </c>
@@ -1655,7 +1592,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="28.5">
+    <row r="30" spans="1:12">
       <c r="A30" s="4">
         <v>7</v>
       </c>
@@ -1675,7 +1612,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="28.5">
+    <row r="31" spans="1:12">
       <c r="A31" s="4">
         <v>8</v>
       </c>
@@ -1702,29 +1639,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="E13" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.3"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" style="13" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="13"/>
+    <col min="1" max="1" width="16.375" style="13" customWidth="1"/>
+    <col min="2" max="2" width="9.125" style="13"/>
     <col min="3" max="3" width="12" style="13" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" style="13" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" style="13" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" style="13" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="13"/>
-    <col min="8" max="8" width="16.85546875" style="13" customWidth="1"/>
-    <col min="9" max="10" width="9.140625" style="13"/>
-    <col min="11" max="11" width="22.7109375" style="13" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="13"/>
+    <col min="4" max="4" width="17.625" style="13" customWidth="1"/>
+    <col min="5" max="5" width="15.25" style="13" customWidth="1"/>
+    <col min="6" max="6" width="13.125" style="13" customWidth="1"/>
+    <col min="7" max="7" width="9.125" style="13"/>
+    <col min="8" max="8" width="16.875" style="13" customWidth="1"/>
+    <col min="9" max="10" width="9.125" style="13"/>
+    <col min="11" max="11" width="22.75" style="13" customWidth="1"/>
+    <col min="12" max="16384" width="9.125" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="23.25">
+    <row r="1" spans="1:2" ht="23.8">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -1769,7 +1706,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="23.25">
+    <row r="8" spans="1:2" ht="23.8">
       <c r="A8" s="17" t="s">
         <v>7</v>
       </c>
@@ -1822,7 +1759,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="23.25">
+    <row r="17" spans="1:12" ht="23.8">
       <c r="A17" s="17" t="s">
         <v>13</v>
       </c>
@@ -1903,7 +1840,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="23.25">
+    <row r="22" spans="1:12" ht="23.8">
       <c r="A22" s="11" t="s">
         <v>36</v>
       </c>
@@ -1933,7 +1870,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="28.5">
+    <row r="24" spans="1:12" ht="27.2">
       <c r="A24" s="12">
         <v>1</v>
       </c>
@@ -1956,7 +1893,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="28.5">
+    <row r="25" spans="1:12" ht="27.2">
       <c r="A25" s="12">
         <v>2</v>
       </c>
@@ -1976,7 +1913,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="28.5">
+    <row r="26" spans="1:12" ht="27.2">
       <c r="A26" s="12">
         <v>3</v>
       </c>
@@ -1997,7 +1934,7 @@
       </c>
       <c r="K26" s="3"/>
     </row>
-    <row r="27" spans="1:12" ht="42.75">
+    <row r="27" spans="1:12" ht="27.2">
       <c r="A27" s="12">
         <v>4</v>
       </c>
@@ -2017,7 +1954,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="42.75">
+    <row r="28" spans="1:12" ht="27.2">
       <c r="A28" s="12">
         <v>5</v>
       </c>
@@ -2037,7 +1974,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="28.5">
+    <row r="29" spans="1:12" ht="27.2">
       <c r="A29" s="12">
         <v>6</v>
       </c>
@@ -2057,7 +1994,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="57.75" thickBot="1">
+    <row r="30" spans="1:12" ht="55.05" thickBot="1">
       <c r="A30" s="12">
         <v>7</v>
       </c>
@@ -2077,7 +2014,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="42.75">
+    <row r="31" spans="1:12" ht="27.2">
       <c r="A31" s="12">
         <v>8</v>
       </c>
@@ -2098,7 +2035,7 @@
       </c>
       <c r="H31" s="14"/>
     </row>
-    <row r="32" spans="1:12" ht="15.75" thickBot="1">
+    <row r="32" spans="1:12" ht="14.95" thickBot="1">
       <c r="A32" s="12">
         <v>9</v>
       </c>
@@ -2119,7 +2056,7 @@
       </c>
       <c r="H32" s="15"/>
     </row>
-    <row r="33" spans="1:6" ht="30">
+    <row r="33" spans="1:6" ht="28.55">
       <c r="A33" s="12">
         <v>10</v>
       </c>
@@ -2145,29 +2082,29 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H31" sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.3"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" style="13" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="13"/>
+    <col min="1" max="1" width="16.375" style="13" customWidth="1"/>
+    <col min="2" max="2" width="9.125" style="13"/>
     <col min="3" max="3" width="12" style="13" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" style="13" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" style="13" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" style="13" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="13"/>
-    <col min="8" max="8" width="16.85546875" style="13" customWidth="1"/>
-    <col min="9" max="10" width="9.140625" style="13"/>
-    <col min="11" max="11" width="22.7109375" style="13" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="13"/>
+    <col min="4" max="4" width="17.625" style="13" customWidth="1"/>
+    <col min="5" max="5" width="15.25" style="13" customWidth="1"/>
+    <col min="6" max="6" width="15.75" style="13" customWidth="1"/>
+    <col min="7" max="7" width="9.125" style="13"/>
+    <col min="8" max="8" width="16.875" style="13" customWidth="1"/>
+    <col min="9" max="10" width="9.125" style="13"/>
+    <col min="11" max="11" width="22.75" style="13" customWidth="1"/>
+    <col min="12" max="16384" width="9.125" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="23.25">
+    <row r="1" spans="1:2" ht="23.8">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -2212,7 +2149,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="23.25">
+    <row r="8" spans="1:2" ht="23.8">
       <c r="A8" s="17" t="s">
         <v>7</v>
       </c>
@@ -2265,7 +2202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="23.25">
+    <row r="17" spans="1:12" ht="23.8">
       <c r="A17" s="17" t="s">
         <v>13</v>
       </c>
@@ -2316,37 +2253,37 @@
         <v>77</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="E19" s="13" t="s">
         <v>79</v>
-      </c>
-      <c r="E19" s="13" t="s">
-        <v>80</v>
       </c>
       <c r="F19" s="1">
         <v>31224224060</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H19" s="13" t="s">
         <v>33</v>
       </c>
       <c r="I19" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J19" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="J19" s="1" t="s">
+      <c r="K19" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="K19" s="1" t="s">
+      <c r="L19" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="L19" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="23.25">
+    </row>
+    <row r="22" spans="1:12" ht="23.8">
       <c r="A22" s="11" t="s">
         <v>36</v>
       </c>
@@ -2376,7 +2313,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="28.5">
+    <row r="24" spans="1:12" ht="27.2">
       <c r="A24" s="12">
         <v>1</v>
       </c>
@@ -2387,13 +2324,13 @@
         <v>4</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E24" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F24" s="6" t="s">
         <v>91</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>92</v>
       </c>
       <c r="H24" s="1"/>
     </row>
@@ -2408,10 +2345,10 @@
         <v>4</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F25" s="7" t="s">
         <v>45</v>
@@ -2428,10 +2365,10 @@
         <v>2</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>48</v>
@@ -2449,10 +2386,10 @@
         <v>2</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F27" s="3" t="s">
         <v>48</v>
@@ -2469,10 +2406,10 @@
         <v>2</v>
       </c>
       <c r="D28" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>48</v>
@@ -2486,7 +2423,7 @@
       <c r="E29" s="1"/>
       <c r="F29" s="3"/>
     </row>
-    <row r="30" spans="1:12" ht="15.75" thickBot="1">
+    <row r="30" spans="1:12" ht="14.95" thickBot="1">
       <c r="A30" s="12"/>
       <c r="B30" s="12"/>
       <c r="C30" s="12"/>
@@ -2503,7 +2440,7 @@
       <c r="F31" s="7"/>
       <c r="H31" s="14"/>
     </row>
-    <row r="32" spans="1:12" ht="15.75" thickBot="1">
+    <row r="32" spans="1:12" ht="14.95" thickBot="1">
       <c r="A32" s="12"/>
       <c r="B32" s="12"/>
       <c r="D32" s="1"/>
@@ -2524,29 +2461,29 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L45"/>
   <sheetViews>
     <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.3"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" style="13" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="13"/>
+    <col min="1" max="1" width="16.375" style="13" customWidth="1"/>
+    <col min="2" max="2" width="9.125" style="13"/>
     <col min="3" max="3" width="12" style="13" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" style="13" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" style="13" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" style="13" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="13"/>
-    <col min="8" max="8" width="16.85546875" style="13" customWidth="1"/>
-    <col min="9" max="10" width="9.140625" style="13"/>
-    <col min="11" max="11" width="22.7109375" style="13" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="13"/>
+    <col min="4" max="4" width="17.625" style="13" customWidth="1"/>
+    <col min="5" max="5" width="15.25" style="13" customWidth="1"/>
+    <col min="6" max="6" width="15.75" style="13" customWidth="1"/>
+    <col min="7" max="7" width="9.125" style="13"/>
+    <col min="8" max="8" width="16.875" style="13" customWidth="1"/>
+    <col min="9" max="10" width="9.125" style="13"/>
+    <col min="11" max="11" width="22.75" style="13" customWidth="1"/>
+    <col min="12" max="16384" width="9.125" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="23.25">
+    <row r="1" spans="1:2" ht="23.8">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -2561,7 +2498,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B3" s="13">
         <v>7</v>
@@ -2569,7 +2506,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B4" s="13">
         <v>8</v>
@@ -2577,13 +2514,13 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B5" s="13">
         <v>9.9</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="23.25">
+    <row r="8" spans="1:2" ht="23.8">
       <c r="A8" s="17" t="s">
         <v>7</v>
       </c>
@@ -2614,13 +2551,13 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B12" s="13">
         <v>1.5</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="23.25">
+    <row r="17" spans="1:12" ht="23.8">
       <c r="A17" s="17" t="s">
         <v>13</v>
       </c>
@@ -2663,45 +2600,45 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="15.75">
+    <row r="19" spans="1:12" ht="15.65">
       <c r="A19" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="C19" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="E19" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E19" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>102</v>
       </c>
       <c r="H19" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="I19" s="61" t="s">
+      <c r="I19" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="K19" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="J19" s="1" t="s">
+      <c r="L19" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="K19" s="61" t="s">
-        <v>105</v>
-      </c>
-      <c r="L19" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="23.25">
+    </row>
+    <row r="22" spans="1:12" ht="23.8">
       <c r="A22" s="11" t="s">
         <v>36</v>
       </c>
@@ -2731,219 +2668,239 @@
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="41.25" customHeight="1">
-      <c r="A24" s="37"/>
-      <c r="B24" s="38"/>
-      <c r="C24" s="38"/>
-      <c r="D24" s="38"/>
-      <c r="E24" s="38"/>
-      <c r="F24" s="39"/>
-      <c r="G24" s="40"/>
-    </row>
-    <row r="25" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A25" s="41"/>
-      <c r="B25" s="42"/>
-      <c r="C25" s="42"/>
-      <c r="D25" s="42"/>
-      <c r="E25" s="42"/>
-      <c r="F25" s="43"/>
-      <c r="G25" s="44"/>
+    <row r="24" spans="1:12" ht="41.3" customHeight="1">
+      <c r="A24" s="52"/>
+      <c r="B24" s="55"/>
+      <c r="C24" s="55"/>
+      <c r="D24" s="55"/>
+      <c r="E24" s="55"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="58"/>
+    </row>
+    <row r="25" spans="1:12" ht="14.95" thickBot="1">
+      <c r="A25" s="53"/>
+      <c r="B25" s="56"/>
+      <c r="C25" s="56"/>
+      <c r="D25" s="56"/>
+      <c r="E25" s="56"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="59"/>
       <c r="K25" s="3"/>
     </row>
-    <row r="26" spans="1:12" ht="26.25" customHeight="1">
+    <row r="26" spans="1:12" ht="26.35" customHeight="1">
       <c r="A26" s="45"/>
-      <c r="B26" s="46"/>
-      <c r="C26" s="46"/>
-      <c r="D26" s="46"/>
-      <c r="E26" s="46"/>
-      <c r="F26" s="47"/>
-      <c r="G26" s="48"/>
+      <c r="B26" s="48"/>
+      <c r="C26" s="48"/>
+      <c r="D26" s="48"/>
+      <c r="E26" s="48"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="60"/>
     </row>
     <row r="27" spans="1:12">
-      <c r="A27" s="49"/>
-      <c r="B27" s="50"/>
-      <c r="C27" s="50"/>
-      <c r="D27" s="50"/>
-      <c r="E27" s="50"/>
-      <c r="F27" s="47"/>
-      <c r="G27" s="51"/>
-    </row>
-    <row r="28" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A28" s="52"/>
-      <c r="B28" s="53"/>
-      <c r="C28" s="53"/>
-      <c r="D28" s="53"/>
-      <c r="E28" s="53"/>
-      <c r="F28" s="54"/>
-      <c r="G28" s="55"/>
-    </row>
-    <row r="29" spans="1:12" ht="26.25" customHeight="1" thickBot="1">
-      <c r="A29" s="56"/>
-      <c r="B29" s="57"/>
-      <c r="C29" s="57"/>
-      <c r="D29" s="57"/>
-      <c r="E29" s="57"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="58"/>
+      <c r="A27" s="46"/>
+      <c r="B27" s="49"/>
+      <c r="C27" s="49"/>
+      <c r="D27" s="49"/>
+      <c r="E27" s="49"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="61"/>
+    </row>
+    <row r="28" spans="1:12" ht="14.95" thickBot="1">
+      <c r="A28" s="47"/>
+      <c r="B28" s="50"/>
+      <c r="C28" s="50"/>
+      <c r="D28" s="50"/>
+      <c r="E28" s="50"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="62"/>
+    </row>
+    <row r="29" spans="1:12" ht="26.35" customHeight="1" thickBot="1">
+      <c r="A29" s="51"/>
+      <c r="B29" s="54"/>
+      <c r="C29" s="54"/>
+      <c r="D29" s="54"/>
+      <c r="E29" s="54"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="57"/>
     </row>
     <row r="30" spans="1:12">
-      <c r="A30" s="37"/>
-      <c r="B30" s="38"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="39"/>
-      <c r="G30" s="40"/>
+      <c r="A30" s="52"/>
+      <c r="B30" s="55"/>
+      <c r="C30" s="55"/>
+      <c r="D30" s="55"/>
+      <c r="E30" s="55"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="58"/>
       <c r="H30" s="14"/>
     </row>
-    <row r="31" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A31" s="41"/>
-      <c r="B31" s="42"/>
-      <c r="C31" s="42"/>
-      <c r="D31" s="42"/>
-      <c r="E31" s="42"/>
-      <c r="F31" s="43"/>
-      <c r="G31" s="44"/>
+    <row r="31" spans="1:12" ht="14.95" thickBot="1">
+      <c r="A31" s="53"/>
+      <c r="B31" s="56"/>
+      <c r="C31" s="56"/>
+      <c r="D31" s="56"/>
+      <c r="E31" s="56"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="59"/>
       <c r="H31" s="15"/>
     </row>
-    <row r="32" spans="1:12" ht="41.25" customHeight="1">
+    <row r="32" spans="1:12" ht="41.3" customHeight="1">
       <c r="A32" s="45"/>
-      <c r="B32" s="46"/>
-      <c r="C32" s="46"/>
-      <c r="D32" s="46"/>
-      <c r="E32" s="46"/>
-      <c r="F32" s="47"/>
-      <c r="G32" s="48"/>
-    </row>
-    <row r="33" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A33" s="52"/>
-      <c r="B33" s="53"/>
-      <c r="C33" s="53"/>
-      <c r="D33" s="53"/>
-      <c r="E33" s="53"/>
-      <c r="F33" s="54"/>
-      <c r="G33" s="55"/>
-    </row>
-    <row r="34" spans="1:7" ht="26.25" customHeight="1">
-      <c r="A34" s="56"/>
-      <c r="B34" s="57"/>
-      <c r="C34" s="57"/>
-      <c r="D34" s="57"/>
-      <c r="E34" s="57"/>
-      <c r="F34" s="39"/>
-      <c r="G34" s="58"/>
+      <c r="B32" s="48"/>
+      <c r="C32" s="48"/>
+      <c r="D32" s="48"/>
+      <c r="E32" s="48"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="60"/>
+    </row>
+    <row r="33" spans="1:7" ht="14.95" thickBot="1">
+      <c r="A33" s="47"/>
+      <c r="B33" s="50"/>
+      <c r="C33" s="50"/>
+      <c r="D33" s="50"/>
+      <c r="E33" s="50"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="62"/>
+    </row>
+    <row r="34" spans="1:7" ht="26.35" customHeight="1">
+      <c r="A34" s="51"/>
+      <c r="B34" s="54"/>
+      <c r="C34" s="54"/>
+      <c r="D34" s="54"/>
+      <c r="E34" s="54"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="57"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="37"/>
-      <c r="B35" s="38"/>
-      <c r="C35" s="38"/>
-      <c r="D35" s="38"/>
-      <c r="E35" s="38"/>
-      <c r="F35" s="39"/>
-      <c r="G35" s="40"/>
-    </row>
-    <row r="36" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A36" s="41"/>
-      <c r="B36" s="42"/>
-      <c r="C36" s="42"/>
-      <c r="D36" s="42"/>
-      <c r="E36" s="42"/>
-      <c r="F36" s="43"/>
-      <c r="G36" s="44"/>
-    </row>
-    <row r="37" spans="1:7" ht="26.25" customHeight="1">
+      <c r="A35" s="52"/>
+      <c r="B35" s="55"/>
+      <c r="C35" s="55"/>
+      <c r="D35" s="55"/>
+      <c r="E35" s="55"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="58"/>
+    </row>
+    <row r="36" spans="1:7" ht="14.95" thickBot="1">
+      <c r="A36" s="53"/>
+      <c r="B36" s="56"/>
+      <c r="C36" s="56"/>
+      <c r="D36" s="56"/>
+      <c r="E36" s="56"/>
+      <c r="F36" s="20"/>
+      <c r="G36" s="59"/>
+    </row>
+    <row r="37" spans="1:7" ht="26.35" customHeight="1">
       <c r="A37" s="45"/>
-      <c r="B37" s="46"/>
-      <c r="C37" s="46"/>
-      <c r="D37" s="46"/>
-      <c r="E37" s="46"/>
-      <c r="F37" s="47"/>
-      <c r="G37" s="48"/>
+      <c r="B37" s="48"/>
+      <c r="C37" s="48"/>
+      <c r="D37" s="48"/>
+      <c r="E37" s="48"/>
+      <c r="F37" s="22"/>
+      <c r="G37" s="60"/>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="49"/>
-      <c r="B38" s="50"/>
-      <c r="C38" s="50"/>
-      <c r="D38" s="50"/>
-      <c r="E38" s="50"/>
-      <c r="F38" s="47"/>
-      <c r="G38" s="51"/>
-    </row>
-    <row r="39" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A39" s="52"/>
-      <c r="B39" s="53"/>
-      <c r="C39" s="53"/>
-      <c r="D39" s="53"/>
-      <c r="E39" s="53"/>
-      <c r="F39" s="54"/>
-      <c r="G39" s="55"/>
-    </row>
-    <row r="40" spans="1:7" ht="26.25" customHeight="1">
-      <c r="A40" s="56"/>
-      <c r="B40" s="57"/>
-      <c r="C40" s="57"/>
-      <c r="D40" s="57"/>
-      <c r="E40" s="57"/>
-      <c r="F40" s="39"/>
-      <c r="G40" s="58"/>
+      <c r="A38" s="46"/>
+      <c r="B38" s="49"/>
+      <c r="C38" s="49"/>
+      <c r="D38" s="49"/>
+      <c r="E38" s="49"/>
+      <c r="F38" s="22"/>
+      <c r="G38" s="61"/>
+    </row>
+    <row r="39" spans="1:7" ht="14.95" thickBot="1">
+      <c r="A39" s="47"/>
+      <c r="B39" s="50"/>
+      <c r="C39" s="50"/>
+      <c r="D39" s="50"/>
+      <c r="E39" s="50"/>
+      <c r="F39" s="24"/>
+      <c r="G39" s="62"/>
+    </row>
+    <row r="40" spans="1:7" ht="26.35" customHeight="1">
+      <c r="A40" s="51"/>
+      <c r="B40" s="54"/>
+      <c r="C40" s="54"/>
+      <c r="D40" s="54"/>
+      <c r="E40" s="54"/>
+      <c r="F40" s="19"/>
+      <c r="G40" s="57"/>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" s="37"/>
-      <c r="B41" s="38"/>
-      <c r="C41" s="38"/>
-      <c r="D41" s="38"/>
-      <c r="E41" s="38"/>
-      <c r="F41" s="39"/>
-      <c r="G41" s="40"/>
-    </row>
-    <row r="42" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A42" s="41"/>
-      <c r="B42" s="42"/>
-      <c r="C42" s="42"/>
-      <c r="D42" s="42"/>
-      <c r="E42" s="42"/>
-      <c r="F42" s="43"/>
-      <c r="G42" s="44"/>
-    </row>
-    <row r="43" spans="1:7" ht="26.25" customHeight="1">
+      <c r="A41" s="52"/>
+      <c r="B41" s="55"/>
+      <c r="C41" s="55"/>
+      <c r="D41" s="55"/>
+      <c r="E41" s="55"/>
+      <c r="F41" s="19"/>
+      <c r="G41" s="58"/>
+    </row>
+    <row r="42" spans="1:7" ht="14.95" thickBot="1">
+      <c r="A42" s="53"/>
+      <c r="B42" s="56"/>
+      <c r="C42" s="56"/>
+      <c r="D42" s="56"/>
+      <c r="E42" s="56"/>
+      <c r="F42" s="20"/>
+      <c r="G42" s="59"/>
+    </row>
+    <row r="43" spans="1:7" ht="26.35" customHeight="1">
       <c r="A43" s="45"/>
-      <c r="B43" s="46"/>
-      <c r="C43" s="46"/>
-      <c r="D43" s="46"/>
-      <c r="E43" s="46"/>
-      <c r="F43" s="47"/>
-      <c r="G43" s="59"/>
+      <c r="B43" s="48"/>
+      <c r="C43" s="48"/>
+      <c r="D43" s="48"/>
+      <c r="E43" s="48"/>
+      <c r="F43" s="22"/>
+      <c r="G43" s="26"/>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="49"/>
-      <c r="B44" s="50"/>
-      <c r="C44" s="50"/>
-      <c r="D44" s="50"/>
-      <c r="E44" s="50"/>
-      <c r="F44" s="47"/>
-      <c r="G44" s="59"/>
-    </row>
-    <row r="45" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A45" s="52"/>
-      <c r="B45" s="53"/>
-      <c r="C45" s="53"/>
-      <c r="D45" s="53"/>
-      <c r="E45" s="53"/>
-      <c r="F45" s="54"/>
-      <c r="G45" s="60"/>
+      <c r="A44" s="46"/>
+      <c r="B44" s="49"/>
+      <c r="C44" s="49"/>
+      <c r="D44" s="49"/>
+      <c r="E44" s="49"/>
+      <c r="F44" s="22"/>
+      <c r="G44" s="26"/>
+    </row>
+    <row r="45" spans="1:7" ht="14.95" thickBot="1">
+      <c r="A45" s="47"/>
+      <c r="B45" s="50"/>
+      <c r="C45" s="50"/>
+      <c r="D45" s="50"/>
+      <c r="E45" s="50"/>
+      <c r="F45" s="24"/>
+      <c r="G45" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="A43:A45"/>
-    <mergeCell ref="B43:B45"/>
-    <mergeCell ref="C43:C45"/>
-    <mergeCell ref="D43:D45"/>
-    <mergeCell ref="E43:E45"/>
-    <mergeCell ref="A40:A42"/>
-    <mergeCell ref="B40:B42"/>
-    <mergeCell ref="C40:C42"/>
-    <mergeCell ref="D40:D42"/>
-    <mergeCell ref="E40:E42"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="G29:G31"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="D26:D28"/>
+    <mergeCell ref="E26:E28"/>
+    <mergeCell ref="G26:G28"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="D29:D31"/>
+    <mergeCell ref="E29:E31"/>
+    <mergeCell ref="G34:G36"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="B34:B36"/>
+    <mergeCell ref="C34:C36"/>
+    <mergeCell ref="D34:D36"/>
+    <mergeCell ref="E34:E36"/>
     <mergeCell ref="G40:G42"/>
     <mergeCell ref="A37:A39"/>
     <mergeCell ref="B37:B39"/>
@@ -2951,65 +2908,45 @@
     <mergeCell ref="D37:D39"/>
     <mergeCell ref="E37:E39"/>
     <mergeCell ref="G37:G39"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="B34:B36"/>
-    <mergeCell ref="C34:C36"/>
-    <mergeCell ref="D34:D36"/>
-    <mergeCell ref="E34:E36"/>
-    <mergeCell ref="G34:G36"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="G32:G33"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="D29:D31"/>
-    <mergeCell ref="E29:E31"/>
-    <mergeCell ref="G29:G31"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="D26:D28"/>
-    <mergeCell ref="E26:E28"/>
-    <mergeCell ref="G26:G28"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="A40:A42"/>
+    <mergeCell ref="B40:B42"/>
+    <mergeCell ref="C40:C42"/>
+    <mergeCell ref="D40:D42"/>
+    <mergeCell ref="E40:E42"/>
+    <mergeCell ref="A43:A45"/>
+    <mergeCell ref="B43:B45"/>
+    <mergeCell ref="C43:C45"/>
+    <mergeCell ref="D43:D45"/>
+    <mergeCell ref="E43:E45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="H41" sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.3"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" style="12" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="12"/>
+    <col min="1" max="1" width="16.375" style="12" customWidth="1"/>
+    <col min="2" max="2" width="9.125" style="12"/>
     <col min="3" max="3" width="12" style="12" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" style="12" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" style="12" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" style="12" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="12"/>
-    <col min="8" max="8" width="16.85546875" style="12" customWidth="1"/>
-    <col min="9" max="10" width="9.140625" style="12"/>
-    <col min="11" max="11" width="22.7109375" style="12" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="12"/>
+    <col min="4" max="4" width="17.625" style="12" customWidth="1"/>
+    <col min="5" max="5" width="15.25" style="12" customWidth="1"/>
+    <col min="6" max="6" width="15.75" style="12" customWidth="1"/>
+    <col min="7" max="7" width="9.125" style="12"/>
+    <col min="8" max="8" width="16.875" style="12" customWidth="1"/>
+    <col min="9" max="10" width="9.125" style="12"/>
+    <col min="11" max="11" width="22.75" style="12" customWidth="1"/>
+    <col min="12" max="16384" width="9.125" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="23.25">
+    <row r="1" spans="1:2" ht="23.8">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -3032,7 +2969,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B4" s="12">
         <v>6.5</v>
@@ -3040,7 +2977,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B5" s="12">
         <v>8.5</v>
@@ -3048,13 +2985,13 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B6" s="12">
         <v>8.5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="23.25">
+    <row r="8" spans="1:2" ht="23.8">
       <c r="A8" s="11" t="s">
         <v>7</v>
       </c>
@@ -3085,108 +3022,108 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B12" s="12">
         <v>2.5</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="23.25">
-      <c r="A17" s="64" t="s">
+    <row r="17" spans="1:12" ht="23.8">
+      <c r="A17" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="65"/>
-      <c r="C17" s="65"/>
-      <c r="D17" s="65"/>
-      <c r="E17" s="65"/>
-      <c r="F17" s="65"/>
-      <c r="G17" s="65"/>
-      <c r="H17" s="65"/>
-      <c r="I17" s="65"/>
-      <c r="J17" s="65"/>
-      <c r="K17" s="65"/>
-      <c r="L17" s="65"/>
-    </row>
-    <row r="18" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A18" s="65" t="s">
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="32"/>
+      <c r="K17" s="32"/>
+      <c r="L17" s="32"/>
+    </row>
+    <row r="18" spans="1:12" ht="14.3" customHeight="1">
+      <c r="A18" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="65" t="s">
+      <c r="B18" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="65" t="s">
+      <c r="C18" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="65" t="s">
+      <c r="D18" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="E18" s="65" t="s">
+      <c r="E18" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="F18" s="65" t="s">
+      <c r="F18" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="G18" s="65" t="s">
+      <c r="G18" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="H18" s="65" t="s">
+      <c r="H18" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="I18" s="65" t="s">
+      <c r="I18" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="J18" s="65" t="s">
+      <c r="J18" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="K18" s="65" t="s">
+      <c r="K18" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="L18" s="65" t="s">
+      <c r="L18" s="32" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:12">
-      <c r="A19" s="66" t="s">
+      <c r="A19" s="33" t="s">
+        <v>113</v>
+      </c>
+      <c r="B19" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="C19" s="33" t="s">
+        <v>178</v>
+      </c>
+      <c r="D19" s="33" t="s">
         <v>115</v>
       </c>
-      <c r="B19" s="66" t="s">
+      <c r="E19" s="32" t="s">
+        <v>117</v>
+      </c>
+      <c r="F19" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="C19" s="66" t="s">
-        <v>117</v>
-      </c>
-      <c r="D19" s="66" t="s">
-        <v>118</v>
-      </c>
-      <c r="E19" s="65" t="s">
+      <c r="G19" s="33" t="s">
+        <v>119</v>
+      </c>
+      <c r="H19" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="I19" s="34" t="s">
+        <v>123</v>
+      </c>
+      <c r="J19" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="F19" s="66" t="s">
-        <v>119</v>
-      </c>
-      <c r="G19" s="66" t="s">
+      <c r="K19" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="L19" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="H19" s="65" t="s">
-        <v>33</v>
-      </c>
-      <c r="I19" s="67" t="s">
-        <v>126</v>
-      </c>
-      <c r="J19" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="K19" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="L19" s="8" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="14.25" customHeight="1">
-      <c r="I20" s="65"/>
-    </row>
-    <row r="21" spans="1:12" ht="23.25">
+    </row>
+    <row r="20" spans="1:12" ht="14.3" customHeight="1">
+      <c r="I20" s="32"/>
+    </row>
+    <row r="21" spans="1:12" ht="23.8">
       <c r="A21" s="11" t="s">
         <v>36</v>
       </c>
@@ -3212,329 +3149,368 @@
       </c>
     </row>
     <row r="23" spans="1:12" ht="16.5" customHeight="1">
-      <c r="A23" s="68">
+      <c r="A23" s="69">
         <v>1</v>
       </c>
-      <c r="B23" s="69">
+      <c r="B23" s="70">
         <v>136</v>
       </c>
-      <c r="C23" s="69">
-        <v>2</v>
-      </c>
-      <c r="D23" s="69" t="s">
+      <c r="C23" s="70">
+        <v>2</v>
+      </c>
+      <c r="D23" s="70" t="s">
+        <v>124</v>
+      </c>
+      <c r="E23" s="70" t="s">
+        <v>54</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="G23" s="71"/>
+      <c r="K23" s="6"/>
+    </row>
+    <row r="24" spans="1:12" ht="26.35" customHeight="1" thickBot="1">
+      <c r="A24" s="68"/>
+      <c r="B24" s="64"/>
+      <c r="C24" s="64"/>
+      <c r="D24" s="64"/>
+      <c r="E24" s="64"/>
+      <c r="F24" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="G24" s="66"/>
+    </row>
+    <row r="25" spans="1:12" ht="27" customHeight="1">
+      <c r="A25" s="67">
+        <v>2</v>
+      </c>
+      <c r="B25" s="63">
+        <v>120</v>
+      </c>
+      <c r="C25" s="63">
+        <v>2</v>
+      </c>
+      <c r="D25" s="63" t="s">
+        <v>126</v>
+      </c>
+      <c r="E25" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="G25" s="65"/>
+    </row>
+    <row r="26" spans="1:12" ht="14.95" thickBot="1">
+      <c r="A26" s="68"/>
+      <c r="B26" s="64"/>
+      <c r="C26" s="64"/>
+      <c r="D26" s="64"/>
+      <c r="E26" s="64"/>
+      <c r="F26" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="G26" s="66"/>
+    </row>
+    <row r="27" spans="1:12" ht="27" customHeight="1">
+      <c r="A27" s="67">
+        <v>3</v>
+      </c>
+      <c r="B27" s="63">
+        <v>120</v>
+      </c>
+      <c r="C27" s="63">
+        <v>2</v>
+      </c>
+      <c r="D27" s="63" t="s">
         <v>127</v>
       </c>
-      <c r="E23" s="69" t="s">
+      <c r="E27" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="F23" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="G23" s="70"/>
-      <c r="K23" s="6"/>
-    </row>
-    <row r="24" spans="1:12" ht="26.25" customHeight="1" thickBot="1">
-      <c r="A24" s="71"/>
-      <c r="B24" s="72"/>
-      <c r="C24" s="72"/>
-      <c r="D24" s="72"/>
-      <c r="E24" s="72"/>
-      <c r="F24" s="73" t="s">
+      <c r="F27" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="G27" s="65"/>
+    </row>
+    <row r="28" spans="1:12" ht="14.95" thickBot="1">
+      <c r="A28" s="68"/>
+      <c r="B28" s="64"/>
+      <c r="C28" s="64"/>
+      <c r="D28" s="64"/>
+      <c r="E28" s="64"/>
+      <c r="F28" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="G24" s="74"/>
-    </row>
-    <row r="25" spans="1:12" ht="27" customHeight="1">
-      <c r="A25" s="75">
-        <v>2</v>
-      </c>
-      <c r="B25" s="76">
-        <v>120</v>
-      </c>
-      <c r="C25" s="76">
-        <v>2</v>
-      </c>
-      <c r="D25" s="76" t="s">
-        <v>129</v>
-      </c>
-      <c r="E25" s="76" t="s">
+      <c r="G28" s="66"/>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" s="67">
+        <v>4</v>
+      </c>
+      <c r="B29" s="63">
+        <v>136</v>
+      </c>
+      <c r="C29" s="63">
+        <v>2</v>
+      </c>
+      <c r="D29" s="63" t="s">
+        <v>127</v>
+      </c>
+      <c r="E29" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="F25" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="G25" s="77"/>
-    </row>
-    <row r="26" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A26" s="71"/>
-      <c r="B26" s="72"/>
-      <c r="C26" s="72"/>
-      <c r="D26" s="72"/>
-      <c r="E26" s="72"/>
-      <c r="F26" s="73" t="s">
-        <v>44</v>
-      </c>
-      <c r="G26" s="74"/>
-    </row>
-    <row r="27" spans="1:12" ht="27" customHeight="1">
-      <c r="A27" s="75">
-        <v>3</v>
-      </c>
-      <c r="B27" s="76">
-        <v>120</v>
-      </c>
-      <c r="C27" s="76">
-        <v>2</v>
-      </c>
-      <c r="D27" s="76" t="s">
-        <v>130</v>
-      </c>
-      <c r="E27" s="76" t="s">
-        <v>54</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="G27" s="77"/>
-    </row>
-    <row r="28" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A28" s="71"/>
-      <c r="B28" s="72"/>
-      <c r="C28" s="72"/>
-      <c r="D28" s="72"/>
-      <c r="E28" s="72"/>
-      <c r="F28" s="73" t="s">
-        <v>44</v>
-      </c>
-      <c r="G28" s="74"/>
-    </row>
-    <row r="29" spans="1:12">
-      <c r="A29" s="75">
-        <v>4</v>
-      </c>
-      <c r="B29" s="76">
-        <v>136</v>
-      </c>
-      <c r="C29" s="76">
-        <v>2</v>
-      </c>
-      <c r="D29" s="76" t="s">
-        <v>130</v>
-      </c>
-      <c r="E29" s="76" t="s">
-        <v>54</v>
-      </c>
       <c r="F29" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="G29" s="77"/>
-    </row>
-    <row r="30" spans="1:12" ht="41.25" customHeight="1">
-      <c r="A30" s="68"/>
-      <c r="B30" s="69"/>
-      <c r="C30" s="69"/>
-      <c r="D30" s="69"/>
-      <c r="E30" s="69"/>
+        <v>125</v>
+      </c>
+      <c r="G29" s="65"/>
+    </row>
+    <row r="30" spans="1:12" ht="41.3" customHeight="1">
+      <c r="A30" s="69"/>
+      <c r="B30" s="70"/>
+      <c r="C30" s="70"/>
+      <c r="D30" s="70"/>
+      <c r="E30" s="70"/>
       <c r="F30" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="G30" s="70"/>
-    </row>
-    <row r="31" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A31" s="71"/>
-      <c r="B31" s="72"/>
-      <c r="C31" s="72"/>
-      <c r="D31" s="72"/>
-      <c r="E31" s="72"/>
-      <c r="F31" s="73" t="s">
-        <v>108</v>
-      </c>
-      <c r="G31" s="74"/>
+      <c r="G30" s="71"/>
+    </row>
+    <row r="31" spans="1:12" ht="14.95" thickBot="1">
+      <c r="A31" s="68"/>
+      <c r="B31" s="64"/>
+      <c r="C31" s="64"/>
+      <c r="D31" s="64"/>
+      <c r="E31" s="64"/>
+      <c r="F31" s="35" t="s">
+        <v>106</v>
+      </c>
+      <c r="G31" s="66"/>
     </row>
     <row r="32" spans="1:12" ht="27" customHeight="1">
-      <c r="A32" s="75">
+      <c r="A32" s="67">
         <v>5</v>
       </c>
-      <c r="B32" s="76">
+      <c r="B32" s="63">
         <v>116</v>
       </c>
-      <c r="C32" s="76">
-        <v>2</v>
-      </c>
-      <c r="D32" s="76" t="s">
+      <c r="C32" s="63">
+        <v>2</v>
+      </c>
+      <c r="D32" s="63" t="s">
+        <v>126</v>
+      </c>
+      <c r="E32" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="G32" s="65"/>
+    </row>
+    <row r="33" spans="1:7" ht="14.95" thickBot="1">
+      <c r="A33" s="68"/>
+      <c r="B33" s="64"/>
+      <c r="C33" s="64"/>
+      <c r="D33" s="64"/>
+      <c r="E33" s="64"/>
+      <c r="F33" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="G33" s="66"/>
+    </row>
+    <row r="34" spans="1:7" ht="16.5" customHeight="1">
+      <c r="A34" s="67">
+        <v>6</v>
+      </c>
+      <c r="B34" s="63">
+        <v>116</v>
+      </c>
+      <c r="C34" s="63">
+        <v>2</v>
+      </c>
+      <c r="D34" s="63" t="s">
+        <v>128</v>
+      </c>
+      <c r="E34" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="G34" s="65"/>
+    </row>
+    <row r="35" spans="1:7" ht="26.35" customHeight="1" thickBot="1">
+      <c r="A35" s="68"/>
+      <c r="B35" s="64"/>
+      <c r="C35" s="64"/>
+      <c r="D35" s="64"/>
+      <c r="E35" s="64"/>
+      <c r="F35" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="G35" s="66"/>
+    </row>
+    <row r="36" spans="1:7" ht="27" customHeight="1">
+      <c r="A36" s="67">
+        <v>7</v>
+      </c>
+      <c r="B36" s="63">
+        <v>268</v>
+      </c>
+      <c r="C36" s="63">
+        <v>3</v>
+      </c>
+      <c r="D36" s="63" t="s">
         <v>129</v>
       </c>
-      <c r="E32" s="76" t="s">
+      <c r="E36" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="F32" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="G32" s="77"/>
-    </row>
-    <row r="33" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A33" s="71"/>
-      <c r="B33" s="72"/>
-      <c r="C33" s="72"/>
-      <c r="D33" s="72"/>
-      <c r="E33" s="72"/>
-      <c r="F33" s="73" t="s">
-        <v>44</v>
-      </c>
-      <c r="G33" s="74"/>
-    </row>
-    <row r="34" spans="1:7" ht="16.5" customHeight="1">
-      <c r="A34" s="75">
-        <v>6</v>
-      </c>
-      <c r="B34" s="76">
-        <v>116</v>
-      </c>
-      <c r="C34" s="76">
-        <v>2</v>
-      </c>
-      <c r="D34" s="76" t="s">
-        <v>131</v>
-      </c>
-      <c r="E34" s="76" t="s">
-        <v>54</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="G34" s="77"/>
-    </row>
-    <row r="35" spans="1:7" ht="26.25" customHeight="1" thickBot="1">
-      <c r="A35" s="71"/>
-      <c r="B35" s="72"/>
-      <c r="C35" s="72"/>
-      <c r="D35" s="72"/>
-      <c r="E35" s="72"/>
-      <c r="F35" s="73" t="s">
-        <v>44</v>
-      </c>
-      <c r="G35" s="74"/>
-    </row>
-    <row r="36" spans="1:7" ht="27" customHeight="1">
-      <c r="A36" s="75">
+      <c r="F36" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="G36" s="36"/>
+    </row>
+    <row r="37" spans="1:7" ht="14.95" thickBot="1">
+      <c r="A37" s="68"/>
+      <c r="B37" s="64"/>
+      <c r="C37" s="64"/>
+      <c r="D37" s="64"/>
+      <c r="E37" s="64"/>
+      <c r="F37" s="35" t="s">
+        <v>106</v>
+      </c>
+      <c r="G37" s="37"/>
+    </row>
+    <row r="38" spans="1:7" ht="26.35" customHeight="1">
+      <c r="A38" s="67">
         <v>7</v>
       </c>
-      <c r="B36" s="76">
-        <v>268</v>
-      </c>
-      <c r="C36" s="76">
-        <v>3</v>
-      </c>
-      <c r="D36" s="76" t="s">
-        <v>132</v>
-      </c>
-      <c r="E36" s="76" t="s">
-        <v>54</v>
-      </c>
-      <c r="F36" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="G36" s="78"/>
-    </row>
-    <row r="37" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A37" s="71"/>
-      <c r="B37" s="72"/>
-      <c r="C37" s="72"/>
-      <c r="D37" s="72"/>
-      <c r="E37" s="72"/>
-      <c r="F37" s="73" t="s">
-        <v>108</v>
-      </c>
-      <c r="G37" s="79"/>
-    </row>
-    <row r="38" spans="1:7" ht="26.25" customHeight="1">
-      <c r="A38" s="75">
-        <v>7</v>
-      </c>
-      <c r="B38" s="76">
+      <c r="B38" s="63">
         <v>148</v>
       </c>
-      <c r="C38" s="76">
+      <c r="C38" s="63">
         <v>4</v>
       </c>
-      <c r="D38" s="76" t="s">
-        <v>109</v>
-      </c>
-      <c r="E38" s="76" t="s">
-        <v>91</v>
+      <c r="D38" s="63" t="s">
+        <v>107</v>
+      </c>
+      <c r="E38" s="63" t="s">
+        <v>90</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="G38" s="77"/>
+        <v>105</v>
+      </c>
+      <c r="G38" s="65"/>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39" s="68"/>
-      <c r="B39" s="69"/>
-      <c r="C39" s="69"/>
-      <c r="D39" s="69"/>
-      <c r="E39" s="69"/>
+      <c r="A39" s="69"/>
+      <c r="B39" s="70"/>
+      <c r="C39" s="70"/>
+      <c r="D39" s="70"/>
+      <c r="E39" s="70"/>
       <c r="F39" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="G39" s="70"/>
-    </row>
-    <row r="40" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A40" s="71"/>
-      <c r="B40" s="72"/>
-      <c r="C40" s="72"/>
-      <c r="D40" s="72"/>
-      <c r="E40" s="72"/>
-      <c r="F40" s="73" t="s">
+      <c r="G39" s="71"/>
+    </row>
+    <row r="40" spans="1:7" ht="14.95" thickBot="1">
+      <c r="A40" s="68"/>
+      <c r="B40" s="64"/>
+      <c r="C40" s="64"/>
+      <c r="D40" s="64"/>
+      <c r="E40" s="64"/>
+      <c r="F40" s="35" t="s">
+        <v>106</v>
+      </c>
+      <c r="G40" s="66"/>
+    </row>
+    <row r="41" spans="1:7" ht="26.35" customHeight="1">
+      <c r="A41" s="67">
+        <v>8</v>
+      </c>
+      <c r="B41" s="63">
+        <v>147</v>
+      </c>
+      <c r="C41" s="63">
+        <v>4</v>
+      </c>
+      <c r="D41" s="63" t="s">
         <v>108</v>
       </c>
-      <c r="G40" s="74"/>
-    </row>
-    <row r="41" spans="1:7" ht="26.25" customHeight="1">
-      <c r="A41" s="75">
-        <v>8</v>
-      </c>
-      <c r="B41" s="76">
-        <v>147</v>
-      </c>
-      <c r="C41" s="76">
-        <v>4</v>
-      </c>
-      <c r="D41" s="76" t="s">
-        <v>110</v>
-      </c>
-      <c r="E41" s="76" t="s">
-        <v>91</v>
+      <c r="E41" s="63" t="s">
+        <v>90</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="G41" s="78"/>
+        <v>105</v>
+      </c>
+      <c r="G41" s="36"/>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="68"/>
-      <c r="B42" s="69"/>
-      <c r="C42" s="69"/>
-      <c r="D42" s="69"/>
-      <c r="E42" s="69"/>
+      <c r="A42" s="69"/>
+      <c r="B42" s="70"/>
+      <c r="C42" s="70"/>
+      <c r="D42" s="70"/>
+      <c r="E42" s="70"/>
       <c r="F42" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="G42" s="78"/>
-    </row>
-    <row r="43" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A43" s="71"/>
-      <c r="B43" s="72"/>
-      <c r="C43" s="72"/>
-      <c r="D43" s="72"/>
-      <c r="E43" s="72"/>
-      <c r="F43" s="73" t="s">
-        <v>108</v>
-      </c>
-      <c r="G43" s="79"/>
+      <c r="G42" s="36"/>
+    </row>
+    <row r="43" spans="1:7" ht="14.95" thickBot="1">
+      <c r="A43" s="68"/>
+      <c r="B43" s="64"/>
+      <c r="C43" s="64"/>
+      <c r="D43" s="64"/>
+      <c r="E43" s="64"/>
+      <c r="F43" s="35" t="s">
+        <v>106</v>
+      </c>
+      <c r="G43" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="52">
+    <mergeCell ref="G29:G31"/>
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="D29:D31"/>
+    <mergeCell ref="E29:E31"/>
+    <mergeCell ref="G38:G40"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="D38:D40"/>
+    <mergeCell ref="E38:E40"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="C41:C43"/>
+    <mergeCell ref="D41:D43"/>
+    <mergeCell ref="E41:E43"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="G25:G26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="G27:G28"/>
     <mergeCell ref="E36:E37"/>
     <mergeCell ref="E32:E33"/>
     <mergeCell ref="G32:G33"/>
@@ -3544,6 +3520,397 @@
     <mergeCell ref="D34:D35"/>
     <mergeCell ref="E34:E35"/>
     <mergeCell ref="G34:G35"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="D32:D33"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:L31"/>
+  <sheetViews>
+    <sheetView topLeftCell="E16" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.3"/>
+  <cols>
+    <col min="1" max="1" width="16.375" style="12" customWidth="1"/>
+    <col min="2" max="2" width="9.125" style="12"/>
+    <col min="3" max="3" width="12" style="12" customWidth="1"/>
+    <col min="4" max="4" width="17.625" style="12" customWidth="1"/>
+    <col min="5" max="5" width="15.25" style="12" customWidth="1"/>
+    <col min="6" max="6" width="15.75" style="12" customWidth="1"/>
+    <col min="7" max="7" width="9.125" style="12"/>
+    <col min="8" max="8" width="16.875" style="12" customWidth="1"/>
+    <col min="9" max="10" width="9.125" style="12"/>
+    <col min="11" max="11" width="22.75" style="12" customWidth="1"/>
+    <col min="12" max="16384" width="9.125" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="23.8">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="12">
+        <v>9.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="B4" s="12">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B5" s="12">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="23.8">
+      <c r="A8" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="12">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="12">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="8"/>
+    </row>
+    <row r="17" spans="1:12" ht="23.8">
+      <c r="A17" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="32"/>
+      <c r="K17" s="32"/>
+      <c r="L17" s="32"/>
+    </row>
+    <row r="18" spans="1:12" ht="14.3" customHeight="1">
+      <c r="A18" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="F18" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="H18" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="I18" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="J18" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="K18" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="L18" s="32" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="15.65">
+      <c r="A19" s="33" t="s">
+        <v>131</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="E19" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="H19" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="I19" s="41" t="s">
+        <v>138</v>
+      </c>
+      <c r="J19" s="41" t="s">
+        <v>139</v>
+      </c>
+      <c r="K19" s="41" t="s">
+        <v>140</v>
+      </c>
+      <c r="L19" s="42" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="14.3" customHeight="1">
+      <c r="I20" s="32"/>
+    </row>
+    <row r="21" spans="1:12" ht="23.8">
+      <c r="A21" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="14.95" thickBot="1">
+      <c r="A22" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="16.5" customHeight="1">
+      <c r="A23" s="67">
+        <v>1</v>
+      </c>
+      <c r="B23" s="63">
+        <v>291</v>
+      </c>
+      <c r="C23" s="63">
+        <v>0</v>
+      </c>
+      <c r="D23" s="63" t="s">
+        <v>142</v>
+      </c>
+      <c r="E23" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="F23" s="40" t="s">
+        <v>56</v>
+      </c>
+      <c r="G23" s="65"/>
+      <c r="K23" s="6"/>
+    </row>
+    <row r="24" spans="1:12" ht="26.35" customHeight="1" thickBot="1">
+      <c r="A24" s="68"/>
+      <c r="B24" s="64"/>
+      <c r="C24" s="64"/>
+      <c r="D24" s="64"/>
+      <c r="E24" s="64"/>
+      <c r="F24" s="35" t="s">
+        <v>106</v>
+      </c>
+      <c r="G24" s="66"/>
+    </row>
+    <row r="25" spans="1:12" ht="27" customHeight="1">
+      <c r="A25" s="67">
+        <v>2</v>
+      </c>
+      <c r="B25" s="63">
+        <v>121</v>
+      </c>
+      <c r="C25" s="63">
+        <v>0</v>
+      </c>
+      <c r="D25" s="63" t="s">
+        <v>143</v>
+      </c>
+      <c r="E25" s="63"/>
+      <c r="F25" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G25" s="65"/>
+    </row>
+    <row r="26" spans="1:12" ht="14.95" thickBot="1">
+      <c r="A26" s="68"/>
+      <c r="B26" s="64"/>
+      <c r="C26" s="64"/>
+      <c r="D26" s="64"/>
+      <c r="E26" s="64"/>
+      <c r="F26" s="35" t="s">
+        <v>106</v>
+      </c>
+      <c r="G26" s="66"/>
+    </row>
+    <row r="27" spans="1:12" ht="27" customHeight="1">
+      <c r="A27" s="67">
+        <v>3</v>
+      </c>
+      <c r="B27" s="63">
+        <v>89</v>
+      </c>
+      <c r="C27" s="63">
+        <v>2</v>
+      </c>
+      <c r="D27" s="63" t="s">
+        <v>144</v>
+      </c>
+      <c r="E27" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G27" s="65"/>
+    </row>
+    <row r="28" spans="1:12" ht="14.95" thickBot="1">
+      <c r="A28" s="68"/>
+      <c r="B28" s="64"/>
+      <c r="C28" s="64"/>
+      <c r="D28" s="64"/>
+      <c r="E28" s="64"/>
+      <c r="F28" s="35" t="s">
+        <v>106</v>
+      </c>
+      <c r="G28" s="66"/>
+    </row>
+    <row r="29" spans="1:12" ht="41.45" thickBot="1">
+      <c r="A29" s="38">
+        <v>4</v>
+      </c>
+      <c r="B29" s="35">
+        <v>89</v>
+      </c>
+      <c r="C29" s="35">
+        <v>2</v>
+      </c>
+      <c r="D29" s="35" t="s">
+        <v>144</v>
+      </c>
+      <c r="E29" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="F29" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="G29" s="39"/>
+    </row>
+    <row r="30" spans="1:12" ht="41.3" customHeight="1" thickBot="1">
+      <c r="A30" s="38">
+        <v>5</v>
+      </c>
+      <c r="B30" s="35">
+        <v>89</v>
+      </c>
+      <c r="C30" s="35">
+        <v>2</v>
+      </c>
+      <c r="D30" s="35" t="s">
+        <v>144</v>
+      </c>
+      <c r="E30" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="F30" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="G30" s="39"/>
+    </row>
+    <row r="31" spans="1:12" ht="41.45" thickBot="1">
+      <c r="A31" s="38">
+        <v>6</v>
+      </c>
+      <c r="B31" s="35">
+        <v>89</v>
+      </c>
+      <c r="C31" s="35">
+        <v>2</v>
+      </c>
+      <c r="D31" s="35" t="s">
+        <v>144</v>
+      </c>
+      <c r="E31" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="F31" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="G31" s="37"/>
+    </row>
+  </sheetData>
+  <mergeCells count="18">
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
     <mergeCell ref="D25:D26"/>
     <mergeCell ref="E25:E26"/>
     <mergeCell ref="G25:G26"/>
@@ -3552,465 +3919,35 @@
     <mergeCell ref="C27:C28"/>
     <mergeCell ref="D27:D28"/>
     <mergeCell ref="E27:E28"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="C41:C43"/>
-    <mergeCell ref="D41:D43"/>
-    <mergeCell ref="E41:E43"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="A38:A40"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="C38:C40"/>
-    <mergeCell ref="D38:D40"/>
-    <mergeCell ref="E38:E40"/>
-    <mergeCell ref="G38:G40"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="D29:D31"/>
-    <mergeCell ref="E29:E31"/>
-    <mergeCell ref="G29:G31"/>
-    <mergeCell ref="G23:G24"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:C26"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L31"/>
-  <sheetViews>
-    <sheetView topLeftCell="I16" workbookViewId="0">
-      <selection activeCell="K26" sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="16.42578125" style="12" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="12"/>
-    <col min="3" max="3" width="12" style="12" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" style="12" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" style="12" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" style="12" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="12"/>
-    <col min="8" max="8" width="16.85546875" style="12" customWidth="1"/>
-    <col min="9" max="10" width="9.140625" style="12"/>
-    <col min="11" max="11" width="22.7109375" style="12" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="12"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="23.25">
-      <c r="A1" s="11" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="12">
-        <v>9.9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="B4" s="12">
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="B5" s="12">
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="23.25">
-      <c r="A8" s="11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="12">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="12">
-        <v>2.6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="8"/>
-    </row>
-    <row r="17" spans="1:12" ht="23.25">
-      <c r="A17" s="64" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="65"/>
-      <c r="C17" s="65"/>
-      <c r="D17" s="65"/>
-      <c r="E17" s="65"/>
-      <c r="F17" s="65"/>
-      <c r="G17" s="65"/>
-      <c r="H17" s="65"/>
-      <c r="I17" s="65"/>
-      <c r="J17" s="65"/>
-      <c r="K17" s="65"/>
-      <c r="L17" s="65"/>
-    </row>
-    <row r="18" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A18" s="65" t="s">
-        <v>3</v>
-      </c>
-      <c r="B18" s="65" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" s="65" t="s">
-        <v>17</v>
-      </c>
-      <c r="D18" s="65" t="s">
-        <v>18</v>
-      </c>
-      <c r="E18" s="65" t="s">
-        <v>28</v>
-      </c>
-      <c r="F18" s="65" t="s">
-        <v>21</v>
-      </c>
-      <c r="G18" s="65" t="s">
-        <v>34</v>
-      </c>
-      <c r="H18" s="65" t="s">
-        <v>32</v>
-      </c>
-      <c r="I18" s="65" t="s">
-        <v>23</v>
-      </c>
-      <c r="J18" s="65" t="s">
-        <v>24</v>
-      </c>
-      <c r="K18" s="65" t="s">
-        <v>25</v>
-      </c>
-      <c r="L18" s="65" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="15.75">
-      <c r="A19" s="66" t="s">
-        <v>134</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="E19" s="65" t="s">
-        <v>138</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="G19" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="H19" s="65" t="s">
-        <v>33</v>
-      </c>
-      <c r="I19" s="88" t="s">
-        <v>141</v>
-      </c>
-      <c r="J19" s="88" t="s">
-        <v>142</v>
-      </c>
-      <c r="K19" s="88" t="s">
-        <v>143</v>
-      </c>
-      <c r="L19" s="89" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="14.25" customHeight="1">
-      <c r="I20" s="65"/>
-    </row>
-    <row r="21" spans="1:12" ht="23.25">
-      <c r="A21" s="11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A22" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="E22" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="F22" s="12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="16.5" customHeight="1">
-      <c r="A23" s="75">
-        <v>1</v>
-      </c>
-      <c r="B23" s="76">
-        <v>291</v>
-      </c>
-      <c r="C23" s="76">
-        <v>0</v>
-      </c>
-      <c r="D23" s="76" t="s">
-        <v>145</v>
-      </c>
-      <c r="E23" s="76" t="s">
-        <v>54</v>
-      </c>
-      <c r="F23" s="85" t="s">
-        <v>56</v>
-      </c>
-      <c r="G23" s="77"/>
-      <c r="K23" s="6"/>
-    </row>
-    <row r="24" spans="1:12" ht="26.25" customHeight="1" thickBot="1">
-      <c r="A24" s="71"/>
-      <c r="B24" s="72"/>
-      <c r="C24" s="72"/>
-      <c r="D24" s="72"/>
-      <c r="E24" s="72"/>
-      <c r="F24" s="73" t="s">
-        <v>108</v>
-      </c>
-      <c r="G24" s="74"/>
-    </row>
-    <row r="25" spans="1:12" ht="27" customHeight="1">
-      <c r="A25" s="75">
-        <v>2</v>
-      </c>
-      <c r="B25" s="76">
-        <v>121</v>
-      </c>
-      <c r="C25" s="76">
-        <v>0</v>
-      </c>
-      <c r="D25" s="76" t="s">
-        <v>146</v>
-      </c>
-      <c r="E25" s="76"/>
-      <c r="F25" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="G25" s="77"/>
-    </row>
-    <row r="26" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A26" s="71"/>
-      <c r="B26" s="72"/>
-      <c r="C26" s="72"/>
-      <c r="D26" s="72"/>
-      <c r="E26" s="72"/>
-      <c r="F26" s="73" t="s">
-        <v>108</v>
-      </c>
-      <c r="G26" s="74"/>
-    </row>
-    <row r="27" spans="1:12" ht="27" customHeight="1">
-      <c r="A27" s="75">
-        <v>3</v>
-      </c>
-      <c r="B27" s="76">
-        <v>89</v>
-      </c>
-      <c r="C27" s="76">
-        <v>2</v>
-      </c>
-      <c r="D27" s="76" t="s">
-        <v>147</v>
-      </c>
-      <c r="E27" s="76" t="s">
-        <v>54</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="G27" s="77"/>
-    </row>
-    <row r="28" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A28" s="71"/>
-      <c r="B28" s="72"/>
-      <c r="C28" s="72"/>
-      <c r="D28" s="72"/>
-      <c r="E28" s="72"/>
-      <c r="F28" s="73" t="s">
-        <v>108</v>
-      </c>
-      <c r="G28" s="74"/>
-    </row>
-    <row r="29" spans="1:12" ht="43.5" thickBot="1">
-      <c r="A29" s="81">
-        <v>4</v>
-      </c>
-      <c r="B29" s="73">
-        <v>89</v>
-      </c>
-      <c r="C29" s="73">
-        <v>2</v>
-      </c>
-      <c r="D29" s="73" t="s">
-        <v>147</v>
-      </c>
-      <c r="E29" s="73" t="s">
-        <v>54</v>
-      </c>
-      <c r="F29" s="73" t="s">
-        <v>56</v>
-      </c>
-      <c r="G29" s="82"/>
-    </row>
-    <row r="30" spans="1:12" ht="41.25" customHeight="1" thickBot="1">
-      <c r="A30" s="81">
-        <v>5</v>
-      </c>
-      <c r="B30" s="73">
-        <v>89</v>
-      </c>
-      <c r="C30" s="73">
-        <v>2</v>
-      </c>
-      <c r="D30" s="73" t="s">
-        <v>147</v>
-      </c>
-      <c r="E30" s="73" t="s">
-        <v>54</v>
-      </c>
-      <c r="F30" s="73" t="s">
-        <v>56</v>
-      </c>
-      <c r="G30" s="82"/>
-    </row>
-    <row r="31" spans="1:12" ht="43.5" thickBot="1">
-      <c r="A31" s="81">
-        <v>6</v>
-      </c>
-      <c r="B31" s="73">
-        <v>89</v>
-      </c>
-      <c r="C31" s="73">
-        <v>2</v>
-      </c>
-      <c r="D31" s="73" t="s">
-        <v>147</v>
-      </c>
-      <c r="E31" s="73" t="s">
-        <v>54</v>
-      </c>
-      <c r="F31" s="73" t="s">
-        <v>56</v>
-      </c>
-      <c r="G31" s="79"/>
-    </row>
-  </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="G25:G26"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="G23:G24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView topLeftCell="E15" workbookViewId="0">
-      <selection activeCell="H26" sqref="A1:XFD1048576"/>
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.3"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" style="12" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="12"/>
+    <col min="1" max="1" width="16.375" style="12" customWidth="1"/>
+    <col min="2" max="2" width="9.125" style="12"/>
     <col min="3" max="3" width="12" style="12" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" style="12" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" style="12" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" style="12" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="12"/>
-    <col min="8" max="8" width="16.85546875" style="12" customWidth="1"/>
-    <col min="9" max="10" width="9.140625" style="12"/>
-    <col min="11" max="11" width="22.7109375" style="12" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="12"/>
+    <col min="4" max="4" width="17.625" style="12" customWidth="1"/>
+    <col min="5" max="5" width="15.25" style="12" customWidth="1"/>
+    <col min="6" max="6" width="15.75" style="12" customWidth="1"/>
+    <col min="7" max="7" width="9.125" style="12"/>
+    <col min="8" max="8" width="16.875" style="12" customWidth="1"/>
+    <col min="9" max="10" width="9.125" style="12"/>
+    <col min="11" max="11" width="22.75" style="12" customWidth="1"/>
+    <col min="12" max="16384" width="9.125" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="23.25">
+    <row r="1" spans="1:2" ht="23.8">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -4033,7 +3970,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B4" s="12">
         <v>6.5</v>
@@ -4041,13 +3978,13 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B5" s="12">
         <v>8.5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="23.25">
+    <row r="8" spans="1:2" ht="23.8">
       <c r="A8" s="11" t="s">
         <v>7</v>
       </c>
@@ -4078,113 +4015,113 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B12" s="12">
         <v>1.5</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="23.25">
-      <c r="A17" s="64" t="s">
+    <row r="17" spans="1:12" ht="23.8">
+      <c r="A17" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="65"/>
-      <c r="C17" s="65"/>
-      <c r="D17" s="65"/>
-      <c r="E17" s="65"/>
-      <c r="F17" s="65"/>
-      <c r="G17" s="65"/>
-      <c r="H17" s="65"/>
-      <c r="I17" s="65"/>
-      <c r="J17" s="65"/>
-      <c r="K17" s="65"/>
-      <c r="L17" s="65"/>
-    </row>
-    <row r="18" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A18" s="65" t="s">
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="32"/>
+      <c r="K17" s="32"/>
+      <c r="L17" s="32"/>
+    </row>
+    <row r="18" spans="1:12" ht="14.3" customHeight="1">
+      <c r="A18" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="65" t="s">
+      <c r="B18" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="65" t="s">
+      <c r="C18" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="65" t="s">
+      <c r="D18" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="E18" s="65" t="s">
+      <c r="E18" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="F18" s="65" t="s">
+      <c r="F18" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="G18" s="65" t="s">
+      <c r="G18" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="H18" s="65" t="s">
+      <c r="H18" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="I18" s="65" t="s">
+      <c r="I18" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="J18" s="65" t="s">
+      <c r="J18" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="K18" s="65" t="s">
+      <c r="K18" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="L18" s="65" t="s">
+      <c r="L18" s="32" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="E19" s="32" t="s">
+        <v>152</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="D19" s="1" t="s">
+      <c r="G19" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="H19" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="I19" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="E19" s="65" t="s">
+      <c r="J19" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="K19" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="F19" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="H19" s="65" t="s">
-        <v>33</v>
-      </c>
-      <c r="I19" s="1" t="s">
+      <c r="L19" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="J19" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="L19" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="14.25" customHeight="1">
-      <c r="I20" s="65"/>
-    </row>
-    <row r="21" spans="1:12" ht="23.25">
+    </row>
+    <row r="20" spans="1:12" ht="14.3" customHeight="1">
+      <c r="I20" s="32"/>
+    </row>
+    <row r="21" spans="1:12" ht="23.8">
       <c r="A21" s="11" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="15.75" thickBot="1">
+    <row r="22" spans="1:12" ht="14.95" thickBot="1">
       <c r="A22" s="12" t="s">
         <v>42</v>
       </c>
@@ -4205,190 +4142,190 @@
       </c>
     </row>
     <row r="23" spans="1:12" ht="16.5" customHeight="1">
-      <c r="A23" s="90"/>
-      <c r="B23" s="91"/>
-      <c r="C23" s="91"/>
-      <c r="D23" s="91"/>
-      <c r="E23" s="91"/>
-      <c r="F23" s="91"/>
+      <c r="A23" s="43"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="44"/>
+      <c r="F23" s="44"/>
       <c r="J23" s="6"/>
     </row>
-    <row r="24" spans="1:12" ht="30" customHeight="1">
-      <c r="A24" s="37">
+    <row r="24" spans="1:12" ht="30.1" customHeight="1">
+      <c r="A24" s="52">
         <v>1</v>
       </c>
-      <c r="B24" s="38">
+      <c r="B24" s="55">
         <v>105</v>
       </c>
-      <c r="C24" s="38">
-        <v>2</v>
-      </c>
-      <c r="D24" s="38" t="s">
-        <v>160</v>
-      </c>
-      <c r="E24" s="38" t="s">
+      <c r="C24" s="55">
+        <v>2</v>
+      </c>
+      <c r="D24" s="55" t="s">
+        <v>157</v>
+      </c>
+      <c r="E24" s="55" t="s">
         <v>55</v>
       </c>
-      <c r="F24" s="39" t="s">
+      <c r="F24" s="19" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="27" customHeight="1" thickBot="1">
-      <c r="A25" s="41"/>
-      <c r="B25" s="42"/>
-      <c r="C25" s="42"/>
-      <c r="D25" s="42"/>
-      <c r="E25" s="42"/>
-      <c r="F25" s="43" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" ht="57.75" thickBot="1">
-      <c r="A26" s="63">
-        <v>2</v>
-      </c>
-      <c r="B26" s="54">
+      <c r="A25" s="53"/>
+      <c r="B25" s="56"/>
+      <c r="C25" s="56"/>
+      <c r="D25" s="56"/>
+      <c r="E25" s="56"/>
+      <c r="F25" s="20" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="55.05" thickBot="1">
+      <c r="A26" s="30">
+        <v>2</v>
+      </c>
+      <c r="B26" s="24">
         <v>105</v>
       </c>
-      <c r="C26" s="54">
-        <v>2</v>
-      </c>
-      <c r="D26" s="54" t="s">
-        <v>160</v>
-      </c>
-      <c r="E26" s="54" t="s">
+      <c r="C26" s="24">
+        <v>2</v>
+      </c>
+      <c r="D26" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="E26" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="F26" s="54" t="s">
+      <c r="F26" s="24" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="41.25" customHeight="1">
-      <c r="A27" s="56">
+    <row r="27" spans="1:12" ht="41.3" customHeight="1">
+      <c r="A27" s="51">
         <v>3</v>
       </c>
-      <c r="B27" s="57">
+      <c r="B27" s="54">
         <v>262</v>
       </c>
-      <c r="C27" s="57">
-        <v>2</v>
-      </c>
-      <c r="D27" s="57" t="s">
-        <v>161</v>
-      </c>
-      <c r="E27" s="57" t="s">
+      <c r="C27" s="54">
+        <v>2</v>
+      </c>
+      <c r="D27" s="54" t="s">
+        <v>158</v>
+      </c>
+      <c r="E27" s="54" t="s">
         <v>55</v>
       </c>
-      <c r="F27" s="39" t="s">
+      <c r="F27" s="19" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A28" s="41"/>
-      <c r="B28" s="42"/>
-      <c r="C28" s="42"/>
-      <c r="D28" s="42"/>
-      <c r="E28" s="42"/>
-      <c r="F28" s="43" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" ht="15.75" customHeight="1">
+    <row r="28" spans="1:12" ht="14.95" thickBot="1">
+      <c r="A28" s="53"/>
+      <c r="B28" s="56"/>
+      <c r="C28" s="56"/>
+      <c r="D28" s="56"/>
+      <c r="E28" s="56"/>
+      <c r="F28" s="20" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="15.8" customHeight="1">
       <c r="A29" s="45">
         <v>4</v>
       </c>
-      <c r="B29" s="46">
+      <c r="B29" s="48">
         <v>262</v>
       </c>
-      <c r="C29" s="46">
-        <v>2</v>
-      </c>
-      <c r="D29" s="46" t="s">
-        <v>161</v>
-      </c>
-      <c r="E29" s="46" t="s">
+      <c r="C29" s="48">
+        <v>2</v>
+      </c>
+      <c r="D29" s="48" t="s">
+        <v>158</v>
+      </c>
+      <c r="E29" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="F29" s="47" t="s">
+      <c r="F29" s="22" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="41.25" customHeight="1" thickBot="1">
-      <c r="A30" s="52"/>
-      <c r="B30" s="53"/>
-      <c r="C30" s="53"/>
-      <c r="D30" s="53"/>
-      <c r="E30" s="53"/>
-      <c r="F30" s="54" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" ht="57.75" thickBot="1">
-      <c r="A31" s="62">
+    <row r="30" spans="1:12" ht="41.3" customHeight="1" thickBot="1">
+      <c r="A30" s="47"/>
+      <c r="B30" s="50"/>
+      <c r="C30" s="50"/>
+      <c r="D30" s="50"/>
+      <c r="E30" s="50"/>
+      <c r="F30" s="24" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="55.05" thickBot="1">
+      <c r="A31" s="29">
         <v>5</v>
       </c>
-      <c r="B31" s="43">
+      <c r="B31" s="20">
         <v>178</v>
       </c>
-      <c r="C31" s="43">
-        <v>2</v>
-      </c>
-      <c r="D31" s="43" t="s">
-        <v>162</v>
-      </c>
-      <c r="E31" s="43" t="s">
+      <c r="C31" s="20">
+        <v>2</v>
+      </c>
+      <c r="D31" s="20" t="s">
+        <v>159</v>
+      </c>
+      <c r="E31" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="F31" s="43" t="s">
-        <v>163</v>
+      <c r="F31" s="20" t="s">
+        <v>160</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
     <mergeCell ref="A29:A30"/>
     <mergeCell ref="B29:B30"/>
     <mergeCell ref="C29:C30"/>
     <mergeCell ref="D29:D30"/>
     <mergeCell ref="E29:E30"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="F23" sqref="A23:XFD23"/>
+    <sheetView tabSelected="1" topLeftCell="E14" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.3"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" style="12" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="12"/>
+    <col min="1" max="1" width="16.375" style="12" customWidth="1"/>
+    <col min="2" max="2" width="9.125" style="12"/>
     <col min="3" max="3" width="12" style="12" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" style="12" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" style="12" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" style="12" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="12"/>
-    <col min="8" max="8" width="16.85546875" style="12" customWidth="1"/>
-    <col min="9" max="10" width="9.140625" style="12"/>
-    <col min="11" max="11" width="22.7109375" style="12" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="12"/>
+    <col min="4" max="4" width="17.625" style="12" customWidth="1"/>
+    <col min="5" max="5" width="15.25" style="12" customWidth="1"/>
+    <col min="6" max="6" width="15.75" style="12" customWidth="1"/>
+    <col min="7" max="7" width="9.125" style="12"/>
+    <col min="8" max="8" width="16.875" style="12" customWidth="1"/>
+    <col min="9" max="10" width="9.125" style="12"/>
+    <col min="11" max="11" width="22.75" style="12" customWidth="1"/>
+    <col min="12" max="16384" width="9.125" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="23.25">
+    <row r="1" spans="1:2" ht="23.8">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -4411,7 +4348,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B4" s="12">
         <v>7.5</v>
@@ -4419,13 +4356,13 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="8" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B5" s="12">
         <v>8.5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="23.25">
+    <row r="8" spans="1:2" ht="23.8">
       <c r="A8" s="11" t="s">
         <v>7</v>
       </c>
@@ -4457,107 +4394,107 @@
     <row r="12" spans="1:2">
       <c r="A12" s="1"/>
     </row>
-    <row r="17" spans="1:12" ht="23.25">
-      <c r="A17" s="64" t="s">
+    <row r="17" spans="1:12" ht="23.8">
+      <c r="A17" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="65"/>
-      <c r="C17" s="65"/>
-      <c r="D17" s="65"/>
-      <c r="E17" s="65"/>
-      <c r="F17" s="65"/>
-      <c r="G17" s="65"/>
-      <c r="H17" s="65"/>
-      <c r="I17" s="65"/>
-      <c r="J17" s="65"/>
-      <c r="K17" s="65"/>
-      <c r="L17" s="65"/>
-    </row>
-    <row r="18" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A18" s="65" t="s">
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="32"/>
+      <c r="K17" s="32"/>
+      <c r="L17" s="32"/>
+    </row>
+    <row r="18" spans="1:12" ht="14.3" customHeight="1">
+      <c r="A18" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="65" t="s">
+      <c r="B18" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="65" t="s">
+      <c r="C18" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="65" t="s">
+      <c r="D18" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="E18" s="65" t="s">
+      <c r="E18" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="F18" s="65" t="s">
+      <c r="F18" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="G18" s="65" t="s">
+      <c r="G18" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="H18" s="65" t="s">
+      <c r="H18" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="I18" s="65" t="s">
+      <c r="I18" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="J18" s="65" t="s">
+      <c r="J18" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="K18" s="65" t="s">
+      <c r="K18" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="L18" s="65" t="s">
+      <c r="L18" s="32" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="15.75">
+    <row r="19" spans="1:12" ht="15.65">
       <c r="A19" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B19" s="19" t="s">
+      <c r="E19" s="32" t="s">
+        <v>152</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="C19" s="19" t="s">
+      <c r="G19" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="D19" s="19" t="s">
+      <c r="H19" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="I19" s="18" t="s">
         <v>168</v>
       </c>
-      <c r="E19" s="65" t="s">
-        <v>155</v>
-      </c>
-      <c r="F19" s="19" t="s">
+      <c r="J19" s="18" t="s">
         <v>169</v>
       </c>
-      <c r="G19" s="19" t="s">
+      <c r="K19" s="18" t="s">
         <v>170</v>
       </c>
-      <c r="H19" s="65" t="s">
-        <v>33</v>
-      </c>
-      <c r="I19" s="80" t="s">
+      <c r="L19" s="28" t="s">
         <v>171</v>
       </c>
-      <c r="J19" s="80" t="s">
-        <v>172</v>
-      </c>
-      <c r="K19" s="80" t="s">
-        <v>173</v>
-      </c>
-      <c r="L19" s="20" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="14.25" customHeight="1">
-      <c r="I20" s="65"/>
-    </row>
-    <row r="21" spans="1:12" ht="23.25">
+    </row>
+    <row r="20" spans="1:12" ht="14.3" customHeight="1">
+      <c r="I20" s="32"/>
+    </row>
+    <row r="21" spans="1:12" ht="23.8">
       <c r="A21" s="11" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="15.75" thickBot="1">
+    <row r="22" spans="1:12" ht="14.95" thickBot="1">
       <c r="A22" s="12" t="s">
         <v>42</v>
       </c>
@@ -4577,157 +4514,157 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="30" customHeight="1">
-      <c r="A23" s="34">
+    <row r="23" spans="1:12" ht="30.1" customHeight="1">
+      <c r="A23" s="51">
         <v>1</v>
       </c>
-      <c r="B23" s="35">
+      <c r="B23" s="54">
         <v>301</v>
       </c>
-      <c r="C23" s="35">
-        <v>2</v>
-      </c>
-      <c r="D23" s="35" t="s">
-        <v>175</v>
-      </c>
-      <c r="E23" s="35" t="s">
+      <c r="C23" s="54">
+        <v>2</v>
+      </c>
+      <c r="D23" s="54" t="s">
+        <v>172</v>
+      </c>
+      <c r="E23" s="54" t="s">
         <v>55</v>
       </c>
-      <c r="F23" s="21" t="s">
+      <c r="F23" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="G23" s="36"/>
+      <c r="G23" s="57"/>
     </row>
     <row r="24" spans="1:12" ht="27" customHeight="1" thickBot="1">
-      <c r="A24" s="25"/>
-      <c r="B24" s="26"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="22" t="s">
-        <v>108</v>
-      </c>
-      <c r="G24" s="27"/>
-    </row>
-    <row r="25" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A25" s="28">
-        <v>2</v>
-      </c>
-      <c r="B25" s="30">
+      <c r="A24" s="53"/>
+      <c r="B24" s="56"/>
+      <c r="C24" s="56"/>
+      <c r="D24" s="56"/>
+      <c r="E24" s="56"/>
+      <c r="F24" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="G24" s="59"/>
+    </row>
+    <row r="25" spans="1:12" ht="15.8" customHeight="1">
+      <c r="A25" s="45">
+        <v>2</v>
+      </c>
+      <c r="B25" s="48">
         <v>193</v>
       </c>
-      <c r="C25" s="30">
-        <v>2</v>
-      </c>
-      <c r="D25" s="30" t="s">
-        <v>176</v>
-      </c>
-      <c r="E25" s="30" t="s">
+      <c r="C25" s="48">
+        <v>2</v>
+      </c>
+      <c r="D25" s="48" t="s">
+        <v>173</v>
+      </c>
+      <c r="E25" s="48" t="s">
         <v>55</v>
       </c>
       <c r="F25" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="G25" s="32"/>
-    </row>
-    <row r="26" spans="1:12" ht="41.25" customHeight="1" thickBot="1">
-      <c r="A26" s="29"/>
-      <c r="B26" s="31"/>
-      <c r="C26" s="31"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="31"/>
+      <c r="G25" s="60"/>
+    </row>
+    <row r="26" spans="1:12" ht="41.3" customHeight="1" thickBot="1">
+      <c r="A26" s="47"/>
+      <c r="B26" s="50"/>
+      <c r="C26" s="50"/>
+      <c r="D26" s="50"/>
+      <c r="E26" s="50"/>
       <c r="F26" s="24" t="s">
-        <v>108</v>
-      </c>
-      <c r="G26" s="33"/>
-    </row>
-    <row r="27" spans="1:12" ht="57.75" thickBot="1">
-      <c r="A27" s="83">
+        <v>106</v>
+      </c>
+      <c r="G26" s="62"/>
+    </row>
+    <row r="27" spans="1:12" ht="55.05" thickBot="1">
+      <c r="A27" s="29">
         <v>3</v>
       </c>
-      <c r="B27" s="22">
+      <c r="B27" s="20">
         <v>193</v>
       </c>
-      <c r="C27" s="22">
-        <v>2</v>
-      </c>
-      <c r="D27" s="22" t="s">
-        <v>177</v>
-      </c>
-      <c r="E27" s="22" t="s">
+      <c r="C27" s="20">
+        <v>2</v>
+      </c>
+      <c r="D27" s="20" t="s">
+        <v>174</v>
+      </c>
+      <c r="E27" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="F27" s="22" t="s">
+      <c r="F27" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="G27" s="84"/>
-    </row>
-    <row r="28" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A28" s="28">
+      <c r="G27" s="21"/>
+    </row>
+    <row r="28" spans="1:12" ht="15.8" customHeight="1">
+      <c r="A28" s="45">
         <v>4</v>
       </c>
-      <c r="B28" s="30">
+      <c r="B28" s="48">
         <v>114</v>
       </c>
-      <c r="C28" s="30">
-        <v>2</v>
-      </c>
-      <c r="D28" s="30" t="s">
-        <v>178</v>
-      </c>
-      <c r="E28" s="30" t="s">
+      <c r="C28" s="48">
+        <v>2</v>
+      </c>
+      <c r="D28" s="48" t="s">
+        <v>175</v>
+      </c>
+      <c r="E28" s="48" t="s">
         <v>55</v>
       </c>
       <c r="F28" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="G28" s="32"/>
-    </row>
-    <row r="29" spans="1:12" ht="41.25" customHeight="1" thickBot="1">
-      <c r="A29" s="29"/>
-      <c r="B29" s="31"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="31"/>
+      <c r="G28" s="60"/>
+    </row>
+    <row r="29" spans="1:12" ht="41.3" customHeight="1" thickBot="1">
+      <c r="A29" s="47"/>
+      <c r="B29" s="50"/>
+      <c r="C29" s="50"/>
+      <c r="D29" s="50"/>
+      <c r="E29" s="50"/>
       <c r="F29" s="24" t="s">
-        <v>108</v>
-      </c>
-      <c r="G29" s="33"/>
-    </row>
-    <row r="30" spans="1:12" ht="41.25" customHeight="1">
-      <c r="A30" s="34">
+        <v>106</v>
+      </c>
+      <c r="G29" s="62"/>
+    </row>
+    <row r="30" spans="1:12" ht="41.3" customHeight="1">
+      <c r="A30" s="51">
         <v>5</v>
       </c>
-      <c r="B30" s="35">
+      <c r="B30" s="54">
         <v>114</v>
       </c>
-      <c r="C30" s="35">
-        <v>2</v>
-      </c>
-      <c r="D30" s="35" t="s">
-        <v>178</v>
-      </c>
-      <c r="E30" s="35" t="s">
+      <c r="C30" s="54">
+        <v>2</v>
+      </c>
+      <c r="D30" s="54" t="s">
+        <v>175</v>
+      </c>
+      <c r="E30" s="54" t="s">
         <v>55</v>
       </c>
-      <c r="F30" s="21" t="s">
+      <c r="F30" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="G30" s="36"/>
-    </row>
-    <row r="31" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A31" s="25"/>
-      <c r="B31" s="26"/>
-      <c r="C31" s="26"/>
-      <c r="D31" s="26"/>
-      <c r="E31" s="26"/>
-      <c r="F31" s="22" t="s">
-        <v>108</v>
-      </c>
-      <c r="G31" s="27"/>
-    </row>
-    <row r="32" spans="1:12" ht="57.75" thickBot="1">
-      <c r="A32" s="86">
+      <c r="G30" s="57"/>
+    </row>
+    <row r="31" spans="1:12" ht="14.95" thickBot="1">
+      <c r="A31" s="53"/>
+      <c r="B31" s="56"/>
+      <c r="C31" s="56"/>
+      <c r="D31" s="56"/>
+      <c r="E31" s="56"/>
+      <c r="F31" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="G31" s="59"/>
+    </row>
+    <row r="32" spans="1:12" ht="55.05" thickBot="1">
+      <c r="A32" s="30">
         <v>6</v>
       </c>
       <c r="B32" s="24">
@@ -4737,7 +4674,7 @@
         <v>2</v>
       </c>
       <c r="D32" s="24" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E32" s="24" t="s">
         <v>55</v>
@@ -4745,31 +4682,41 @@
       <c r="F32" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="G32" s="87"/>
-    </row>
-    <row r="33" spans="1:7" ht="57.75" thickBot="1">
-      <c r="A33" s="83">
+      <c r="G32" s="25"/>
+    </row>
+    <row r="33" spans="1:7" ht="55.05" thickBot="1">
+      <c r="A33" s="29">
         <v>7</v>
       </c>
-      <c r="B33" s="22">
+      <c r="B33" s="20">
         <v>114</v>
       </c>
-      <c r="C33" s="22">
-        <v>2</v>
-      </c>
-      <c r="D33" s="22" t="s">
-        <v>178</v>
-      </c>
-      <c r="E33" s="22" t="s">
+      <c r="C33" s="20">
+        <v>2</v>
+      </c>
+      <c r="D33" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="E33" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="F33" s="22" t="s">
+      <c r="F33" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="G33" s="84"/>
+      <c r="G33" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
     <mergeCell ref="E25:E26"/>
     <mergeCell ref="G25:G26"/>
     <mergeCell ref="G28:G29"/>
@@ -4784,16 +4731,6 @@
     <mergeCell ref="C28:C29"/>
     <mergeCell ref="D28:D29"/>
     <mergeCell ref="E28:E29"/>
-    <mergeCell ref="G23:G24"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
id nummers van bioscopen toegekend aan de werkbladen in exel
</commit_message>
<xml_diff>
--- a/documentatie_And_sql/documentatie/BioscoopData.xlsx
+++ b/documentatie_And_sql/documentatie/BioscoopData.xlsx
@@ -1,26 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\php\gameparty_project_met_georgi\documentatie_And_sql\documentatie\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\PHP\gameparty_project_met_georgi\documentatie_And_sql\documentatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{CB70D5C9-12C7-4171-B647-E04388C665D4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20405" windowHeight="7349" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7350" firstSheet="6" activeTab="7"/>
   </bookViews>
   <sheets>
-    <sheet name="almere" sheetId="1" r:id="rId1"/>
-    <sheet name="breda" sheetId="2" r:id="rId2"/>
-    <sheet name="schagen" sheetId="3" r:id="rId3"/>
-    <sheet name="Hoofddorp" sheetId="4" r:id="rId4"/>
-    <sheet name="Den Bosch" sheetId="5" r:id="rId5"/>
-    <sheet name="Den Helder" sheetId="6" r:id="rId6"/>
-    <sheet name="Dordrecht" sheetId="7" r:id="rId7"/>
-    <sheet name="emmen" sheetId="8" r:id="rId8"/>
+    <sheet name="almere id(1)" sheetId="1" r:id="rId1"/>
+    <sheet name="breda id(2)" sheetId="2" r:id="rId2"/>
+    <sheet name="schagen id(3)" sheetId="3" r:id="rId3"/>
+    <sheet name="Hoofddorp id(4)" sheetId="4" r:id="rId4"/>
+    <sheet name="Den Bosch id(5)" sheetId="5" r:id="rId5"/>
+    <sheet name="Den Helder id(6)" sheetId="6" r:id="rId6"/>
+    <sheet name="Dordrecht id(7)" sheetId="7" r:id="rId7"/>
+    <sheet name="emmen id(8)" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -599,7 +598,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="9">
     <font>
       <sz val="11"/>
@@ -884,6 +883,27 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -902,40 +922,34 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -944,25 +958,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1244,25 +1243,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView topLeftCell="F13" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.375" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="11.625" customWidth="1"/>
-    <col min="5" max="5" width="42.25" customWidth="1"/>
-    <col min="6" max="6" width="13.125" customWidth="1"/>
-    <col min="8" max="8" width="16.875" customWidth="1"/>
-    <col min="11" max="11" width="22.75" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" customWidth="1"/>
+    <col min="5" max="5" width="42.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" customWidth="1"/>
+    <col min="11" max="11" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="23.8">
+    <row r="1" spans="1:2" ht="23.25">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -1307,7 +1306,7 @@
         <v>8.6999999999999993</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="23.8">
+    <row r="8" spans="1:2" ht="23.25">
       <c r="A8" s="10" t="s">
         <v>7</v>
       </c>
@@ -1360,7 +1359,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="23.8">
+    <row r="17" spans="1:12" ht="23.25">
       <c r="A17" s="10" t="s">
         <v>13</v>
       </c>
@@ -1441,7 +1440,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="23.8">
+    <row r="22" spans="1:12" ht="23.25">
       <c r="A22" s="9" t="s">
         <v>36</v>
       </c>
@@ -1471,7 +1470,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="28.55">
+    <row r="24" spans="1:12" ht="30">
       <c r="A24" s="4">
         <v>1</v>
       </c>
@@ -1491,7 +1490,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="28.55">
+    <row r="25" spans="1:12" ht="30">
       <c r="A25" s="4">
         <v>2</v>
       </c>
@@ -1592,7 +1591,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" ht="28.5">
       <c r="A30" s="4">
         <v>7</v>
       </c>
@@ -1612,7 +1611,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" ht="28.5">
       <c r="A31" s="4">
         <v>8</v>
       </c>
@@ -1639,29 +1638,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView topLeftCell="E13" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.375" style="13" customWidth="1"/>
-    <col min="2" max="2" width="9.125" style="13"/>
+    <col min="1" max="1" width="16.42578125" style="13" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="13"/>
     <col min="3" max="3" width="12" style="13" customWidth="1"/>
-    <col min="4" max="4" width="17.625" style="13" customWidth="1"/>
-    <col min="5" max="5" width="15.25" style="13" customWidth="1"/>
-    <col min="6" max="6" width="13.125" style="13" customWidth="1"/>
-    <col min="7" max="7" width="9.125" style="13"/>
-    <col min="8" max="8" width="16.875" style="13" customWidth="1"/>
-    <col min="9" max="10" width="9.125" style="13"/>
-    <col min="11" max="11" width="22.75" style="13" customWidth="1"/>
-    <col min="12" max="16384" width="9.125" style="13"/>
+    <col min="4" max="4" width="17.5703125" style="13" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="13" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" style="13" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="13"/>
+    <col min="8" max="8" width="16.85546875" style="13" customWidth="1"/>
+    <col min="9" max="10" width="9.140625" style="13"/>
+    <col min="11" max="11" width="22.7109375" style="13" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="23.8">
+    <row r="1" spans="1:2" ht="23.25">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -1706,7 +1705,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="23.8">
+    <row r="8" spans="1:2" ht="23.25">
       <c r="A8" s="17" t="s">
         <v>7</v>
       </c>
@@ -1759,7 +1758,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="23.8">
+    <row r="17" spans="1:12" ht="23.25">
       <c r="A17" s="17" t="s">
         <v>13</v>
       </c>
@@ -1840,7 +1839,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="23.8">
+    <row r="22" spans="1:12" ht="23.25">
       <c r="A22" s="11" t="s">
         <v>36</v>
       </c>
@@ -1870,7 +1869,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="27.2">
+    <row r="24" spans="1:12" ht="28.5">
       <c r="A24" s="12">
         <v>1</v>
       </c>
@@ -1893,7 +1892,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="27.2">
+    <row r="25" spans="1:12" ht="28.5">
       <c r="A25" s="12">
         <v>2</v>
       </c>
@@ -1913,7 +1912,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="27.2">
+    <row r="26" spans="1:12" ht="28.5">
       <c r="A26" s="12">
         <v>3</v>
       </c>
@@ -1934,7 +1933,7 @@
       </c>
       <c r="K26" s="3"/>
     </row>
-    <row r="27" spans="1:12" ht="27.2">
+    <row r="27" spans="1:12" ht="42.75">
       <c r="A27" s="12">
         <v>4</v>
       </c>
@@ -1954,7 +1953,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="27.2">
+    <row r="28" spans="1:12" ht="42.75">
       <c r="A28" s="12">
         <v>5</v>
       </c>
@@ -1974,7 +1973,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="27.2">
+    <row r="29" spans="1:12" ht="28.5">
       <c r="A29" s="12">
         <v>6</v>
       </c>
@@ -1994,7 +1993,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="55.05" thickBot="1">
+    <row r="30" spans="1:12" ht="57.75" thickBot="1">
       <c r="A30" s="12">
         <v>7</v>
       </c>
@@ -2014,7 +2013,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="27.2">
+    <row r="31" spans="1:12" ht="42.75">
       <c r="A31" s="12">
         <v>8</v>
       </c>
@@ -2035,7 +2034,7 @@
       </c>
       <c r="H31" s="14"/>
     </row>
-    <row r="32" spans="1:12" ht="14.95" thickBot="1">
+    <row r="32" spans="1:12" ht="15.75" thickBot="1">
       <c r="A32" s="12">
         <v>9</v>
       </c>
@@ -2056,7 +2055,7 @@
       </c>
       <c r="H32" s="15"/>
     </row>
-    <row r="33" spans="1:6" ht="28.55">
+    <row r="33" spans="1:6" ht="30">
       <c r="A33" s="12">
         <v>10</v>
       </c>
@@ -2082,29 +2081,29 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.375" style="13" customWidth="1"/>
-    <col min="2" max="2" width="9.125" style="13"/>
+    <col min="1" max="1" width="16.42578125" style="13" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="13"/>
     <col min="3" max="3" width="12" style="13" customWidth="1"/>
-    <col min="4" max="4" width="17.625" style="13" customWidth="1"/>
-    <col min="5" max="5" width="15.25" style="13" customWidth="1"/>
-    <col min="6" max="6" width="15.75" style="13" customWidth="1"/>
-    <col min="7" max="7" width="9.125" style="13"/>
-    <col min="8" max="8" width="16.875" style="13" customWidth="1"/>
-    <col min="9" max="10" width="9.125" style="13"/>
-    <col min="11" max="11" width="22.75" style="13" customWidth="1"/>
-    <col min="12" max="16384" width="9.125" style="13"/>
+    <col min="4" max="4" width="17.5703125" style="13" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="13" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="13" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="13"/>
+    <col min="8" max="8" width="16.85546875" style="13" customWidth="1"/>
+    <col min="9" max="10" width="9.140625" style="13"/>
+    <col min="11" max="11" width="22.7109375" style="13" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="23.8">
+    <row r="1" spans="1:2" ht="23.25">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -2149,7 +2148,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="23.8">
+    <row r="8" spans="1:2" ht="23.25">
       <c r="A8" s="17" t="s">
         <v>7</v>
       </c>
@@ -2202,7 +2201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="23.8">
+    <row r="17" spans="1:12" ht="23.25">
       <c r="A17" s="17" t="s">
         <v>13</v>
       </c>
@@ -2283,7 +2282,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="23.8">
+    <row r="22" spans="1:12" ht="23.25">
       <c r="A22" s="11" t="s">
         <v>36</v>
       </c>
@@ -2313,7 +2312,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="27.2">
+    <row r="24" spans="1:12" ht="28.5">
       <c r="A24" s="12">
         <v>1</v>
       </c>
@@ -2423,7 +2422,7 @@
       <c r="E29" s="1"/>
       <c r="F29" s="3"/>
     </row>
-    <row r="30" spans="1:12" ht="14.95" thickBot="1">
+    <row r="30" spans="1:12" ht="15.75" thickBot="1">
       <c r="A30" s="12"/>
       <c r="B30" s="12"/>
       <c r="C30" s="12"/>
@@ -2440,7 +2439,7 @@
       <c r="F31" s="7"/>
       <c r="H31" s="14"/>
     </row>
-    <row r="32" spans="1:12" ht="14.95" thickBot="1">
+    <row r="32" spans="1:12" ht="15.75" thickBot="1">
       <c r="A32" s="12"/>
       <c r="B32" s="12"/>
       <c r="D32" s="1"/>
@@ -2461,29 +2460,29 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L45"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B24" sqref="B24:B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.375" style="13" customWidth="1"/>
-    <col min="2" max="2" width="9.125" style="13"/>
+    <col min="1" max="1" width="16.42578125" style="13" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="13"/>
     <col min="3" max="3" width="12" style="13" customWidth="1"/>
-    <col min="4" max="4" width="17.625" style="13" customWidth="1"/>
-    <col min="5" max="5" width="15.25" style="13" customWidth="1"/>
-    <col min="6" max="6" width="15.75" style="13" customWidth="1"/>
-    <col min="7" max="7" width="9.125" style="13"/>
-    <col min="8" max="8" width="16.875" style="13" customWidth="1"/>
-    <col min="9" max="10" width="9.125" style="13"/>
-    <col min="11" max="11" width="22.75" style="13" customWidth="1"/>
-    <col min="12" max="16384" width="9.125" style="13"/>
+    <col min="4" max="4" width="17.5703125" style="13" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="13" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="13" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="13"/>
+    <col min="8" max="8" width="16.85546875" style="13" customWidth="1"/>
+    <col min="9" max="10" width="9.140625" style="13"/>
+    <col min="11" max="11" width="22.7109375" style="13" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="23.8">
+    <row r="1" spans="1:2" ht="23.25">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -2520,7 +2519,7 @@
         <v>9.9</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="23.8">
+    <row r="8" spans="1:2" ht="23.25">
       <c r="A8" s="17" t="s">
         <v>7</v>
       </c>
@@ -2557,7 +2556,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="23.8">
+    <row r="17" spans="1:12" ht="23.25">
       <c r="A17" s="17" t="s">
         <v>13</v>
       </c>
@@ -2600,7 +2599,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="15.65">
+    <row r="19" spans="1:12" ht="15.75">
       <c r="A19" s="1" t="s">
         <v>96</v>
       </c>
@@ -2638,7 +2637,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="23.8">
+    <row r="22" spans="1:12" ht="23.25">
       <c r="A22" s="11" t="s">
         <v>36</v>
       </c>
@@ -2668,215 +2667,238 @@
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="41.3" customHeight="1">
-      <c r="A24" s="52"/>
-      <c r="B24" s="55"/>
-      <c r="C24" s="55"/>
-      <c r="D24" s="55"/>
-      <c r="E24" s="55"/>
+    <row r="24" spans="1:12" ht="41.25" customHeight="1">
+      <c r="A24" s="47"/>
+      <c r="B24" s="49"/>
+      <c r="C24" s="49"/>
+      <c r="D24" s="49"/>
+      <c r="E24" s="49"/>
       <c r="F24" s="19"/>
-      <c r="G24" s="58"/>
-    </row>
-    <row r="25" spans="1:12" ht="14.95" thickBot="1">
-      <c r="A25" s="53"/>
-      <c r="B25" s="56"/>
-      <c r="C25" s="56"/>
-      <c r="D25" s="56"/>
-      <c r="E25" s="56"/>
+      <c r="G24" s="45"/>
+    </row>
+    <row r="25" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A25" s="48"/>
+      <c r="B25" s="50"/>
+      <c r="C25" s="50"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="50"/>
       <c r="F25" s="20"/>
-      <c r="G25" s="59"/>
+      <c r="G25" s="46"/>
       <c r="K25" s="3"/>
     </row>
-    <row r="26" spans="1:12" ht="26.35" customHeight="1">
-      <c r="A26" s="45"/>
-      <c r="B26" s="48"/>
-      <c r="C26" s="48"/>
-      <c r="D26" s="48"/>
-      <c r="E26" s="48"/>
+    <row r="26" spans="1:12" ht="26.45" customHeight="1">
+      <c r="A26" s="52"/>
+      <c r="B26" s="55"/>
+      <c r="C26" s="55"/>
+      <c r="D26" s="55"/>
+      <c r="E26" s="55"/>
       <c r="F26" s="22"/>
-      <c r="G26" s="60"/>
+      <c r="G26" s="58"/>
     </row>
     <row r="27" spans="1:12">
-      <c r="A27" s="46"/>
-      <c r="B27" s="49"/>
-      <c r="C27" s="49"/>
-      <c r="D27" s="49"/>
-      <c r="E27" s="49"/>
+      <c r="A27" s="53"/>
+      <c r="B27" s="56"/>
+      <c r="C27" s="56"/>
+      <c r="D27" s="56"/>
+      <c r="E27" s="56"/>
       <c r="F27" s="22"/>
-      <c r="G27" s="61"/>
-    </row>
-    <row r="28" spans="1:12" ht="14.95" thickBot="1">
-      <c r="A28" s="47"/>
-      <c r="B28" s="50"/>
-      <c r="C28" s="50"/>
-      <c r="D28" s="50"/>
-      <c r="E28" s="50"/>
+      <c r="G27" s="59"/>
+    </row>
+    <row r="28" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A28" s="54"/>
+      <c r="B28" s="57"/>
+      <c r="C28" s="57"/>
+      <c r="D28" s="57"/>
+      <c r="E28" s="57"/>
       <c r="F28" s="24"/>
-      <c r="G28" s="62"/>
-    </row>
-    <row r="29" spans="1:12" ht="26.35" customHeight="1" thickBot="1">
-      <c r="A29" s="51"/>
-      <c r="B29" s="54"/>
-      <c r="C29" s="54"/>
-      <c r="D29" s="54"/>
-      <c r="E29" s="54"/>
+      <c r="G28" s="60"/>
+    </row>
+    <row r="29" spans="1:12" ht="26.45" customHeight="1" thickBot="1">
+      <c r="A29" s="61"/>
+      <c r="B29" s="62"/>
+      <c r="C29" s="62"/>
+      <c r="D29" s="62"/>
+      <c r="E29" s="62"/>
       <c r="F29" s="19"/>
-      <c r="G29" s="57"/>
+      <c r="G29" s="51"/>
     </row>
     <row r="30" spans="1:12">
-      <c r="A30" s="52"/>
-      <c r="B30" s="55"/>
-      <c r="C30" s="55"/>
-      <c r="D30" s="55"/>
-      <c r="E30" s="55"/>
+      <c r="A30" s="47"/>
+      <c r="B30" s="49"/>
+      <c r="C30" s="49"/>
+      <c r="D30" s="49"/>
+      <c r="E30" s="49"/>
       <c r="F30" s="19"/>
-      <c r="G30" s="58"/>
+      <c r="G30" s="45"/>
       <c r="H30" s="14"/>
     </row>
-    <row r="31" spans="1:12" ht="14.95" thickBot="1">
-      <c r="A31" s="53"/>
-      <c r="B31" s="56"/>
-      <c r="C31" s="56"/>
-      <c r="D31" s="56"/>
-      <c r="E31" s="56"/>
+    <row r="31" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A31" s="48"/>
+      <c r="B31" s="50"/>
+      <c r="C31" s="50"/>
+      <c r="D31" s="50"/>
+      <c r="E31" s="50"/>
       <c r="F31" s="20"/>
-      <c r="G31" s="59"/>
+      <c r="G31" s="46"/>
       <c r="H31" s="15"/>
     </row>
-    <row r="32" spans="1:12" ht="41.3" customHeight="1">
-      <c r="A32" s="45"/>
-      <c r="B32" s="48"/>
-      <c r="C32" s="48"/>
-      <c r="D32" s="48"/>
-      <c r="E32" s="48"/>
+    <row r="32" spans="1:12" ht="41.25" customHeight="1">
+      <c r="A32" s="52"/>
+      <c r="B32" s="55"/>
+      <c r="C32" s="55"/>
+      <c r="D32" s="55"/>
+      <c r="E32" s="55"/>
       <c r="F32" s="22"/>
-      <c r="G32" s="60"/>
-    </row>
-    <row r="33" spans="1:7" ht="14.95" thickBot="1">
-      <c r="A33" s="47"/>
-      <c r="B33" s="50"/>
-      <c r="C33" s="50"/>
-      <c r="D33" s="50"/>
-      <c r="E33" s="50"/>
+      <c r="G32" s="58"/>
+    </row>
+    <row r="33" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A33" s="54"/>
+      <c r="B33" s="57"/>
+      <c r="C33" s="57"/>
+      <c r="D33" s="57"/>
+      <c r="E33" s="57"/>
       <c r="F33" s="24"/>
-      <c r="G33" s="62"/>
-    </row>
-    <row r="34" spans="1:7" ht="26.35" customHeight="1">
-      <c r="A34" s="51"/>
-      <c r="B34" s="54"/>
-      <c r="C34" s="54"/>
-      <c r="D34" s="54"/>
-      <c r="E34" s="54"/>
+      <c r="G33" s="60"/>
+    </row>
+    <row r="34" spans="1:7" ht="26.45" customHeight="1">
+      <c r="A34" s="61"/>
+      <c r="B34" s="62"/>
+      <c r="C34" s="62"/>
+      <c r="D34" s="62"/>
+      <c r="E34" s="62"/>
       <c r="F34" s="19"/>
-      <c r="G34" s="57"/>
+      <c r="G34" s="51"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="52"/>
-      <c r="B35" s="55"/>
-      <c r="C35" s="55"/>
-      <c r="D35" s="55"/>
-      <c r="E35" s="55"/>
+      <c r="A35" s="47"/>
+      <c r="B35" s="49"/>
+      <c r="C35" s="49"/>
+      <c r="D35" s="49"/>
+      <c r="E35" s="49"/>
       <c r="F35" s="19"/>
-      <c r="G35" s="58"/>
-    </row>
-    <row r="36" spans="1:7" ht="14.95" thickBot="1">
-      <c r="A36" s="53"/>
-      <c r="B36" s="56"/>
-      <c r="C36" s="56"/>
-      <c r="D36" s="56"/>
-      <c r="E36" s="56"/>
+      <c r="G35" s="45"/>
+    </row>
+    <row r="36" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A36" s="48"/>
+      <c r="B36" s="50"/>
+      <c r="C36" s="50"/>
+      <c r="D36" s="50"/>
+      <c r="E36" s="50"/>
       <c r="F36" s="20"/>
-      <c r="G36" s="59"/>
-    </row>
-    <row r="37" spans="1:7" ht="26.35" customHeight="1">
-      <c r="A37" s="45"/>
-      <c r="B37" s="48"/>
-      <c r="C37" s="48"/>
-      <c r="D37" s="48"/>
-      <c r="E37" s="48"/>
+      <c r="G36" s="46"/>
+    </row>
+    <row r="37" spans="1:7" ht="26.45" customHeight="1">
+      <c r="A37" s="52"/>
+      <c r="B37" s="55"/>
+      <c r="C37" s="55"/>
+      <c r="D37" s="55"/>
+      <c r="E37" s="55"/>
       <c r="F37" s="22"/>
-      <c r="G37" s="60"/>
+      <c r="G37" s="58"/>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="46"/>
-      <c r="B38" s="49"/>
-      <c r="C38" s="49"/>
-      <c r="D38" s="49"/>
-      <c r="E38" s="49"/>
+      <c r="A38" s="53"/>
+      <c r="B38" s="56"/>
+      <c r="C38" s="56"/>
+      <c r="D38" s="56"/>
+      <c r="E38" s="56"/>
       <c r="F38" s="22"/>
-      <c r="G38" s="61"/>
-    </row>
-    <row r="39" spans="1:7" ht="14.95" thickBot="1">
-      <c r="A39" s="47"/>
-      <c r="B39" s="50"/>
-      <c r="C39" s="50"/>
-      <c r="D39" s="50"/>
-      <c r="E39" s="50"/>
+      <c r="G38" s="59"/>
+    </row>
+    <row r="39" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A39" s="54"/>
+      <c r="B39" s="57"/>
+      <c r="C39" s="57"/>
+      <c r="D39" s="57"/>
+      <c r="E39" s="57"/>
       <c r="F39" s="24"/>
-      <c r="G39" s="62"/>
-    </row>
-    <row r="40" spans="1:7" ht="26.35" customHeight="1">
-      <c r="A40" s="51"/>
-      <c r="B40" s="54"/>
-      <c r="C40" s="54"/>
-      <c r="D40" s="54"/>
-      <c r="E40" s="54"/>
+      <c r="G39" s="60"/>
+    </row>
+    <row r="40" spans="1:7" ht="26.45" customHeight="1">
+      <c r="A40" s="61"/>
+      <c r="B40" s="62"/>
+      <c r="C40" s="62"/>
+      <c r="D40" s="62"/>
+      <c r="E40" s="62"/>
       <c r="F40" s="19"/>
-      <c r="G40" s="57"/>
+      <c r="G40" s="51"/>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" s="52"/>
-      <c r="B41" s="55"/>
-      <c r="C41" s="55"/>
-      <c r="D41" s="55"/>
-      <c r="E41" s="55"/>
+      <c r="A41" s="47"/>
+      <c r="B41" s="49"/>
+      <c r="C41" s="49"/>
+      <c r="D41" s="49"/>
+      <c r="E41" s="49"/>
       <c r="F41" s="19"/>
-      <c r="G41" s="58"/>
-    </row>
-    <row r="42" spans="1:7" ht="14.95" thickBot="1">
-      <c r="A42" s="53"/>
-      <c r="B42" s="56"/>
-      <c r="C42" s="56"/>
-      <c r="D42" s="56"/>
-      <c r="E42" s="56"/>
+      <c r="G41" s="45"/>
+    </row>
+    <row r="42" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A42" s="48"/>
+      <c r="B42" s="50"/>
+      <c r="C42" s="50"/>
+      <c r="D42" s="50"/>
+      <c r="E42" s="50"/>
       <c r="F42" s="20"/>
-      <c r="G42" s="59"/>
-    </row>
-    <row r="43" spans="1:7" ht="26.35" customHeight="1">
-      <c r="A43" s="45"/>
-      <c r="B43" s="48"/>
-      <c r="C43" s="48"/>
-      <c r="D43" s="48"/>
-      <c r="E43" s="48"/>
+      <c r="G42" s="46"/>
+    </row>
+    <row r="43" spans="1:7" ht="26.45" customHeight="1">
+      <c r="A43" s="52"/>
+      <c r="B43" s="55"/>
+      <c r="C43" s="55"/>
+      <c r="D43" s="55"/>
+      <c r="E43" s="55"/>
       <c r="F43" s="22"/>
       <c r="G43" s="26"/>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="46"/>
-      <c r="B44" s="49"/>
-      <c r="C44" s="49"/>
-      <c r="D44" s="49"/>
-      <c r="E44" s="49"/>
+      <c r="A44" s="53"/>
+      <c r="B44" s="56"/>
+      <c r="C44" s="56"/>
+      <c r="D44" s="56"/>
+      <c r="E44" s="56"/>
       <c r="F44" s="22"/>
       <c r="G44" s="26"/>
     </row>
-    <row r="45" spans="1:7" ht="14.95" thickBot="1">
-      <c r="A45" s="47"/>
-      <c r="B45" s="50"/>
-      <c r="C45" s="50"/>
-      <c r="D45" s="50"/>
-      <c r="E45" s="50"/>
+    <row r="45" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A45" s="54"/>
+      <c r="B45" s="57"/>
+      <c r="C45" s="57"/>
+      <c r="D45" s="57"/>
+      <c r="E45" s="57"/>
       <c r="F45" s="24"/>
       <c r="G45" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="A43:A45"/>
+    <mergeCell ref="B43:B45"/>
+    <mergeCell ref="C43:C45"/>
+    <mergeCell ref="D43:D45"/>
+    <mergeCell ref="E43:E45"/>
+    <mergeCell ref="G40:G42"/>
+    <mergeCell ref="A37:A39"/>
+    <mergeCell ref="B37:B39"/>
+    <mergeCell ref="C37:C39"/>
+    <mergeCell ref="D37:D39"/>
+    <mergeCell ref="E37:E39"/>
+    <mergeCell ref="G37:G39"/>
+    <mergeCell ref="A40:A42"/>
+    <mergeCell ref="B40:B42"/>
+    <mergeCell ref="C40:C42"/>
+    <mergeCell ref="D40:D42"/>
+    <mergeCell ref="E40:E42"/>
+    <mergeCell ref="G34:G36"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="B34:B36"/>
+    <mergeCell ref="C34:C36"/>
+    <mergeCell ref="D34:D36"/>
+    <mergeCell ref="E34:E36"/>
     <mergeCell ref="G29:G31"/>
     <mergeCell ref="A26:A28"/>
     <mergeCell ref="B26:B28"/>
@@ -2889,64 +2911,41 @@
     <mergeCell ref="C29:C31"/>
     <mergeCell ref="D29:D31"/>
     <mergeCell ref="E29:E31"/>
-    <mergeCell ref="G34:G36"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="G32:G33"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="B34:B36"/>
-    <mergeCell ref="C34:C36"/>
-    <mergeCell ref="D34:D36"/>
-    <mergeCell ref="E34:E36"/>
-    <mergeCell ref="G40:G42"/>
-    <mergeCell ref="A37:A39"/>
-    <mergeCell ref="B37:B39"/>
-    <mergeCell ref="C37:C39"/>
-    <mergeCell ref="D37:D39"/>
-    <mergeCell ref="E37:E39"/>
-    <mergeCell ref="G37:G39"/>
-    <mergeCell ref="A40:A42"/>
-    <mergeCell ref="B40:B42"/>
-    <mergeCell ref="C40:C42"/>
-    <mergeCell ref="D40:D42"/>
-    <mergeCell ref="E40:E42"/>
-    <mergeCell ref="A43:A45"/>
-    <mergeCell ref="B43:B45"/>
-    <mergeCell ref="C43:C45"/>
-    <mergeCell ref="D43:D45"/>
-    <mergeCell ref="E43:E45"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.375" style="12" customWidth="1"/>
-    <col min="2" max="2" width="9.125" style="12"/>
+    <col min="1" max="1" width="16.42578125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="12"/>
     <col min="3" max="3" width="12" style="12" customWidth="1"/>
-    <col min="4" max="4" width="17.625" style="12" customWidth="1"/>
-    <col min="5" max="5" width="15.25" style="12" customWidth="1"/>
-    <col min="6" max="6" width="15.75" style="12" customWidth="1"/>
-    <col min="7" max="7" width="9.125" style="12"/>
-    <col min="8" max="8" width="16.875" style="12" customWidth="1"/>
-    <col min="9" max="10" width="9.125" style="12"/>
-    <col min="11" max="11" width="22.75" style="12" customWidth="1"/>
-    <col min="12" max="16384" width="9.125" style="12"/>
+    <col min="4" max="4" width="17.5703125" style="12" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="12" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="12" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="12"/>
+    <col min="8" max="8" width="16.85546875" style="12" customWidth="1"/>
+    <col min="9" max="10" width="9.140625" style="12"/>
+    <col min="11" max="11" width="22.7109375" style="12" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="23.8">
+    <row r="1" spans="1:2" ht="23.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -2991,7 +2990,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="23.8">
+    <row r="8" spans="1:2" ht="23.25">
       <c r="A8" s="11" t="s">
         <v>7</v>
       </c>
@@ -3028,7 +3027,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="23.8">
+    <row r="17" spans="1:12" ht="23.25">
       <c r="A17" s="31" t="s">
         <v>13</v>
       </c>
@@ -3044,7 +3043,7 @@
       <c r="K17" s="32"/>
       <c r="L17" s="32"/>
     </row>
-    <row r="18" spans="1:12" ht="14.3" customHeight="1">
+    <row r="18" spans="1:12" ht="14.25" customHeight="1">
       <c r="A18" s="32" t="s">
         <v>3</v>
       </c>
@@ -3120,10 +3119,10 @@
         <v>122</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="14.3" customHeight="1">
+    <row r="20" spans="1:12" ht="14.25" customHeight="1">
       <c r="I20" s="32"/>
     </row>
-    <row r="21" spans="1:12" ht="23.8">
+    <row r="21" spans="1:12" ht="23.25">
       <c r="A21" s="11" t="s">
         <v>36</v>
       </c>
@@ -3149,223 +3148,223 @@
       </c>
     </row>
     <row r="23" spans="1:12" ht="16.5" customHeight="1">
-      <c r="A23" s="69">
+      <c r="A23" s="70">
         <v>1</v>
       </c>
-      <c r="B23" s="70">
+      <c r="B23" s="71">
         <v>136</v>
       </c>
-      <c r="C23" s="70">
-        <v>2</v>
-      </c>
-      <c r="D23" s="70" t="s">
+      <c r="C23" s="71">
+        <v>2</v>
+      </c>
+      <c r="D23" s="71" t="s">
         <v>124</v>
       </c>
-      <c r="E23" s="70" t="s">
+      <c r="E23" s="71" t="s">
         <v>54</v>
       </c>
       <c r="F23" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="G23" s="71"/>
+      <c r="G23" s="64"/>
       <c r="K23" s="6"/>
     </row>
-    <row r="24" spans="1:12" ht="26.35" customHeight="1" thickBot="1">
-      <c r="A24" s="68"/>
-      <c r="B24" s="64"/>
-      <c r="C24" s="64"/>
-      <c r="D24" s="64"/>
-      <c r="E24" s="64"/>
+    <row r="24" spans="1:12" ht="26.45" customHeight="1" thickBot="1">
+      <c r="A24" s="67"/>
+      <c r="B24" s="69"/>
+      <c r="C24" s="69"/>
+      <c r="D24" s="69"/>
+      <c r="E24" s="69"/>
       <c r="F24" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="G24" s="66"/>
+      <c r="G24" s="65"/>
     </row>
     <row r="25" spans="1:12" ht="27" customHeight="1">
-      <c r="A25" s="67">
-        <v>2</v>
-      </c>
-      <c r="B25" s="63">
+      <c r="A25" s="66">
+        <v>2</v>
+      </c>
+      <c r="B25" s="68">
         <v>120</v>
       </c>
-      <c r="C25" s="63">
-        <v>2</v>
-      </c>
-      <c r="D25" s="63" t="s">
+      <c r="C25" s="68">
+        <v>2</v>
+      </c>
+      <c r="D25" s="68" t="s">
         <v>126</v>
       </c>
-      <c r="E25" s="63" t="s">
+      <c r="E25" s="68" t="s">
         <v>54</v>
       </c>
       <c r="F25" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="G25" s="65"/>
-    </row>
-    <row r="26" spans="1:12" ht="14.95" thickBot="1">
-      <c r="A26" s="68"/>
-      <c r="B26" s="64"/>
-      <c r="C26" s="64"/>
-      <c r="D26" s="64"/>
-      <c r="E26" s="64"/>
+      <c r="G25" s="63"/>
+    </row>
+    <row r="26" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A26" s="67"/>
+      <c r="B26" s="69"/>
+      <c r="C26" s="69"/>
+      <c r="D26" s="69"/>
+      <c r="E26" s="69"/>
       <c r="F26" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="G26" s="66"/>
+      <c r="G26" s="65"/>
     </row>
     <row r="27" spans="1:12" ht="27" customHeight="1">
-      <c r="A27" s="67">
+      <c r="A27" s="66">
         <v>3</v>
       </c>
-      <c r="B27" s="63">
+      <c r="B27" s="68">
         <v>120</v>
       </c>
-      <c r="C27" s="63">
-        <v>2</v>
-      </c>
-      <c r="D27" s="63" t="s">
+      <c r="C27" s="68">
+        <v>2</v>
+      </c>
+      <c r="D27" s="68" t="s">
         <v>127</v>
       </c>
-      <c r="E27" s="63" t="s">
+      <c r="E27" s="68" t="s">
         <v>54</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="G27" s="65"/>
-    </row>
-    <row r="28" spans="1:12" ht="14.95" thickBot="1">
-      <c r="A28" s="68"/>
-      <c r="B28" s="64"/>
-      <c r="C28" s="64"/>
-      <c r="D28" s="64"/>
-      <c r="E28" s="64"/>
+      <c r="G27" s="63"/>
+    </row>
+    <row r="28" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A28" s="67"/>
+      <c r="B28" s="69"/>
+      <c r="C28" s="69"/>
+      <c r="D28" s="69"/>
+      <c r="E28" s="69"/>
       <c r="F28" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="G28" s="66"/>
+      <c r="G28" s="65"/>
     </row>
     <row r="29" spans="1:12">
-      <c r="A29" s="67">
+      <c r="A29" s="66">
         <v>4</v>
       </c>
-      <c r="B29" s="63">
+      <c r="B29" s="68">
         <v>136</v>
       </c>
-      <c r="C29" s="63">
-        <v>2</v>
-      </c>
-      <c r="D29" s="63" t="s">
+      <c r="C29" s="68">
+        <v>2</v>
+      </c>
+      <c r="D29" s="68" t="s">
         <v>127</v>
       </c>
-      <c r="E29" s="63" t="s">
+      <c r="E29" s="68" t="s">
         <v>54</v>
       </c>
       <c r="F29" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="G29" s="65"/>
-    </row>
-    <row r="30" spans="1:12" ht="41.3" customHeight="1">
-      <c r="A30" s="69"/>
-      <c r="B30" s="70"/>
-      <c r="C30" s="70"/>
-      <c r="D30" s="70"/>
-      <c r="E30" s="70"/>
+      <c r="G29" s="63"/>
+    </row>
+    <row r="30" spans="1:12" ht="41.25" customHeight="1">
+      <c r="A30" s="70"/>
+      <c r="B30" s="71"/>
+      <c r="C30" s="71"/>
+      <c r="D30" s="71"/>
+      <c r="E30" s="71"/>
       <c r="F30" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="G30" s="71"/>
-    </row>
-    <row r="31" spans="1:12" ht="14.95" thickBot="1">
-      <c r="A31" s="68"/>
-      <c r="B31" s="64"/>
-      <c r="C31" s="64"/>
-      <c r="D31" s="64"/>
-      <c r="E31" s="64"/>
+      <c r="G30" s="64"/>
+    </row>
+    <row r="31" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A31" s="67"/>
+      <c r="B31" s="69"/>
+      <c r="C31" s="69"/>
+      <c r="D31" s="69"/>
+      <c r="E31" s="69"/>
       <c r="F31" s="35" t="s">
         <v>106</v>
       </c>
-      <c r="G31" s="66"/>
+      <c r="G31" s="65"/>
     </row>
     <row r="32" spans="1:12" ht="27" customHeight="1">
-      <c r="A32" s="67">
+      <c r="A32" s="66">
         <v>5</v>
       </c>
-      <c r="B32" s="63">
+      <c r="B32" s="68">
         <v>116</v>
       </c>
-      <c r="C32" s="63">
-        <v>2</v>
-      </c>
-      <c r="D32" s="63" t="s">
+      <c r="C32" s="68">
+        <v>2</v>
+      </c>
+      <c r="D32" s="68" t="s">
         <v>126</v>
       </c>
-      <c r="E32" s="63" t="s">
+      <c r="E32" s="68" t="s">
         <v>54</v>
       </c>
       <c r="F32" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="G32" s="65"/>
-    </row>
-    <row r="33" spans="1:7" ht="14.95" thickBot="1">
-      <c r="A33" s="68"/>
-      <c r="B33" s="64"/>
-      <c r="C33" s="64"/>
-      <c r="D33" s="64"/>
-      <c r="E33" s="64"/>
+      <c r="G32" s="63"/>
+    </row>
+    <row r="33" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A33" s="67"/>
+      <c r="B33" s="69"/>
+      <c r="C33" s="69"/>
+      <c r="D33" s="69"/>
+      <c r="E33" s="69"/>
       <c r="F33" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="G33" s="66"/>
+      <c r="G33" s="65"/>
     </row>
     <row r="34" spans="1:7" ht="16.5" customHeight="1">
-      <c r="A34" s="67">
+      <c r="A34" s="66">
         <v>6</v>
       </c>
-      <c r="B34" s="63">
+      <c r="B34" s="68">
         <v>116</v>
       </c>
-      <c r="C34" s="63">
-        <v>2</v>
-      </c>
-      <c r="D34" s="63" t="s">
+      <c r="C34" s="68">
+        <v>2</v>
+      </c>
+      <c r="D34" s="68" t="s">
         <v>128</v>
       </c>
-      <c r="E34" s="63" t="s">
+      <c r="E34" s="68" t="s">
         <v>54</v>
       </c>
       <c r="F34" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="G34" s="65"/>
-    </row>
-    <row r="35" spans="1:7" ht="26.35" customHeight="1" thickBot="1">
-      <c r="A35" s="68"/>
-      <c r="B35" s="64"/>
-      <c r="C35" s="64"/>
-      <c r="D35" s="64"/>
-      <c r="E35" s="64"/>
+      <c r="G34" s="63"/>
+    </row>
+    <row r="35" spans="1:7" ht="26.45" customHeight="1" thickBot="1">
+      <c r="A35" s="67"/>
+      <c r="B35" s="69"/>
+      <c r="C35" s="69"/>
+      <c r="D35" s="69"/>
+      <c r="E35" s="69"/>
       <c r="F35" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="G35" s="66"/>
+      <c r="G35" s="65"/>
     </row>
     <row r="36" spans="1:7" ht="27" customHeight="1">
-      <c r="A36" s="67">
+      <c r="A36" s="66">
         <v>7</v>
       </c>
-      <c r="B36" s="63">
+      <c r="B36" s="68">
         <v>268</v>
       </c>
-      <c r="C36" s="63">
+      <c r="C36" s="68">
         <v>3</v>
       </c>
-      <c r="D36" s="63" t="s">
+      <c r="D36" s="68" t="s">
         <v>129</v>
       </c>
-      <c r="E36" s="63" t="s">
+      <c r="E36" s="68" t="s">
         <v>54</v>
       </c>
       <c r="F36" s="6" t="s">
@@ -3373,74 +3372,74 @@
       </c>
       <c r="G36" s="36"/>
     </row>
-    <row r="37" spans="1:7" ht="14.95" thickBot="1">
-      <c r="A37" s="68"/>
-      <c r="B37" s="64"/>
-      <c r="C37" s="64"/>
-      <c r="D37" s="64"/>
-      <c r="E37" s="64"/>
+    <row r="37" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A37" s="67"/>
+      <c r="B37" s="69"/>
+      <c r="C37" s="69"/>
+      <c r="D37" s="69"/>
+      <c r="E37" s="69"/>
       <c r="F37" s="35" t="s">
         <v>106</v>
       </c>
       <c r="G37" s="37"/>
     </row>
-    <row r="38" spans="1:7" ht="26.35" customHeight="1">
-      <c r="A38" s="67">
+    <row r="38" spans="1:7" ht="26.45" customHeight="1">
+      <c r="A38" s="66">
         <v>7</v>
       </c>
-      <c r="B38" s="63">
+      <c r="B38" s="68">
         <v>148</v>
       </c>
-      <c r="C38" s="63">
+      <c r="C38" s="68">
         <v>4</v>
       </c>
-      <c r="D38" s="63" t="s">
+      <c r="D38" s="68" t="s">
         <v>107</v>
       </c>
-      <c r="E38" s="63" t="s">
+      <c r="E38" s="68" t="s">
         <v>90</v>
       </c>
       <c r="F38" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="G38" s="65"/>
+      <c r="G38" s="63"/>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39" s="69"/>
-      <c r="B39" s="70"/>
-      <c r="C39" s="70"/>
-      <c r="D39" s="70"/>
-      <c r="E39" s="70"/>
+      <c r="A39" s="70"/>
+      <c r="B39" s="71"/>
+      <c r="C39" s="71"/>
+      <c r="D39" s="71"/>
+      <c r="E39" s="71"/>
       <c r="F39" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="G39" s="71"/>
-    </row>
-    <row r="40" spans="1:7" ht="14.95" thickBot="1">
-      <c r="A40" s="68"/>
-      <c r="B40" s="64"/>
-      <c r="C40" s="64"/>
-      <c r="D40" s="64"/>
-      <c r="E40" s="64"/>
+      <c r="G39" s="64"/>
+    </row>
+    <row r="40" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A40" s="67"/>
+      <c r="B40" s="69"/>
+      <c r="C40" s="69"/>
+      <c r="D40" s="69"/>
+      <c r="E40" s="69"/>
       <c r="F40" s="35" t="s">
         <v>106</v>
       </c>
-      <c r="G40" s="66"/>
-    </row>
-    <row r="41" spans="1:7" ht="26.35" customHeight="1">
-      <c r="A41" s="67">
+      <c r="G40" s="65"/>
+    </row>
+    <row r="41" spans="1:7" ht="26.45" customHeight="1">
+      <c r="A41" s="66">
         <v>8</v>
       </c>
-      <c r="B41" s="63">
+      <c r="B41" s="68">
         <v>147</v>
       </c>
-      <c r="C41" s="63">
+      <c r="C41" s="68">
         <v>4</v>
       </c>
-      <c r="D41" s="63" t="s">
+      <c r="D41" s="68" t="s">
         <v>108</v>
       </c>
-      <c r="E41" s="63" t="s">
+      <c r="E41" s="68" t="s">
         <v>90</v>
       </c>
       <c r="F41" s="6" t="s">
@@ -3449,22 +3448,22 @@
       <c r="G41" s="36"/>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="69"/>
-      <c r="B42" s="70"/>
-      <c r="C42" s="70"/>
-      <c r="D42" s="70"/>
-      <c r="E42" s="70"/>
+      <c r="A42" s="70"/>
+      <c r="B42" s="71"/>
+      <c r="C42" s="71"/>
+      <c r="D42" s="71"/>
+      <c r="E42" s="71"/>
       <c r="F42" s="6" t="s">
         <v>44</v>
       </c>
       <c r="G42" s="36"/>
     </row>
-    <row r="43" spans="1:7" ht="14.95" thickBot="1">
-      <c r="A43" s="68"/>
-      <c r="B43" s="64"/>
-      <c r="C43" s="64"/>
-      <c r="D43" s="64"/>
-      <c r="E43" s="64"/>
+    <row r="43" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A43" s="67"/>
+      <c r="B43" s="69"/>
+      <c r="C43" s="69"/>
+      <c r="D43" s="69"/>
+      <c r="E43" s="69"/>
       <c r="F43" s="35" t="s">
         <v>106</v>
       </c>
@@ -3472,46 +3471,6 @@
     </row>
   </sheetData>
   <mergeCells count="52">
-    <mergeCell ref="G29:G31"/>
-    <mergeCell ref="G23:G24"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="D29:D31"/>
-    <mergeCell ref="E29:E31"/>
-    <mergeCell ref="G38:G40"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="A38:A40"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="C38:C40"/>
-    <mergeCell ref="D38:D40"/>
-    <mergeCell ref="E38:E40"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="C41:C43"/>
-    <mergeCell ref="D41:D43"/>
-    <mergeCell ref="E41:E43"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="G25:G26"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="E36:E37"/>
     <mergeCell ref="E32:E33"/>
     <mergeCell ref="G32:G33"/>
     <mergeCell ref="A34:A35"/>
@@ -3524,35 +3483,75 @@
     <mergeCell ref="B32:B33"/>
     <mergeCell ref="C32:C33"/>
     <mergeCell ref="D32:D33"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="G25:G26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="C41:C43"/>
+    <mergeCell ref="D41:D43"/>
+    <mergeCell ref="E41:E43"/>
+    <mergeCell ref="G38:G40"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="D38:D40"/>
+    <mergeCell ref="E38:E40"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="G29:G31"/>
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="D29:D31"/>
+    <mergeCell ref="E29:E31"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="D25:D26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView topLeftCell="E16" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.375" style="12" customWidth="1"/>
-    <col min="2" max="2" width="9.125" style="12"/>
+    <col min="1" max="1" width="16.42578125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="12"/>
     <col min="3" max="3" width="12" style="12" customWidth="1"/>
-    <col min="4" max="4" width="17.625" style="12" customWidth="1"/>
-    <col min="5" max="5" width="15.25" style="12" customWidth="1"/>
-    <col min="6" max="6" width="15.75" style="12" customWidth="1"/>
-    <col min="7" max="7" width="9.125" style="12"/>
-    <col min="8" max="8" width="16.875" style="12" customWidth="1"/>
-    <col min="9" max="10" width="9.125" style="12"/>
-    <col min="11" max="11" width="22.75" style="12" customWidth="1"/>
-    <col min="12" max="16384" width="9.125" style="12"/>
+    <col min="4" max="4" width="17.5703125" style="12" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="12" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="12" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="12"/>
+    <col min="8" max="8" width="16.85546875" style="12" customWidth="1"/>
+    <col min="9" max="10" width="9.140625" style="12"/>
+    <col min="11" max="11" width="22.7109375" style="12" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="23.8">
+    <row r="1" spans="1:2" ht="23.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -3589,7 +3588,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="23.8">
+    <row r="8" spans="1:2" ht="23.25">
       <c r="A8" s="11" t="s">
         <v>7</v>
       </c>
@@ -3621,7 +3620,7 @@
     <row r="12" spans="1:2">
       <c r="A12" s="8"/>
     </row>
-    <row r="17" spans="1:12" ht="23.8">
+    <row r="17" spans="1:12" ht="23.25">
       <c r="A17" s="31" t="s">
         <v>13</v>
       </c>
@@ -3637,7 +3636,7 @@
       <c r="K17" s="32"/>
       <c r="L17" s="32"/>
     </row>
-    <row r="18" spans="1:12" ht="14.3" customHeight="1">
+    <row r="18" spans="1:12" ht="14.25" customHeight="1">
       <c r="A18" s="32" t="s">
         <v>3</v>
       </c>
@@ -3675,7 +3674,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="15.65">
+    <row r="19" spans="1:12" ht="15.75">
       <c r="A19" s="33" t="s">
         <v>131</v>
       </c>
@@ -3713,15 +3712,15 @@
         <v>141</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="14.3" customHeight="1">
+    <row r="20" spans="1:12" ht="14.25" customHeight="1">
       <c r="I20" s="32"/>
     </row>
-    <row r="21" spans="1:12" ht="23.8">
+    <row r="21" spans="1:12" ht="23.25">
       <c r="A21" s="11" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="14.95" thickBot="1">
+    <row r="22" spans="1:12" ht="15.75" thickBot="1">
       <c r="A22" s="12" t="s">
         <v>42</v>
       </c>
@@ -3742,101 +3741,101 @@
       </c>
     </row>
     <row r="23" spans="1:12" ht="16.5" customHeight="1">
-      <c r="A23" s="67">
+      <c r="A23" s="66">
         <v>1</v>
       </c>
-      <c r="B23" s="63">
+      <c r="B23" s="68">
         <v>291</v>
       </c>
-      <c r="C23" s="63">
+      <c r="C23" s="68">
         <v>0</v>
       </c>
-      <c r="D23" s="63" t="s">
+      <c r="D23" s="68" t="s">
         <v>142</v>
       </c>
-      <c r="E23" s="63" t="s">
+      <c r="E23" s="68" t="s">
         <v>54</v>
       </c>
       <c r="F23" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="G23" s="65"/>
+      <c r="G23" s="63"/>
       <c r="K23" s="6"/>
     </row>
-    <row r="24" spans="1:12" ht="26.35" customHeight="1" thickBot="1">
-      <c r="A24" s="68"/>
-      <c r="B24" s="64"/>
-      <c r="C24" s="64"/>
-      <c r="D24" s="64"/>
-      <c r="E24" s="64"/>
+    <row r="24" spans="1:12" ht="26.45" customHeight="1" thickBot="1">
+      <c r="A24" s="67"/>
+      <c r="B24" s="69"/>
+      <c r="C24" s="69"/>
+      <c r="D24" s="69"/>
+      <c r="E24" s="69"/>
       <c r="F24" s="35" t="s">
         <v>106</v>
       </c>
-      <c r="G24" s="66"/>
+      <c r="G24" s="65"/>
     </row>
     <row r="25" spans="1:12" ht="27" customHeight="1">
-      <c r="A25" s="67">
-        <v>2</v>
-      </c>
-      <c r="B25" s="63">
+      <c r="A25" s="66">
+        <v>2</v>
+      </c>
+      <c r="B25" s="68">
         <v>121</v>
       </c>
-      <c r="C25" s="63">
+      <c r="C25" s="68">
         <v>0</v>
       </c>
-      <c r="D25" s="63" t="s">
+      <c r="D25" s="68" t="s">
         <v>143</v>
       </c>
-      <c r="E25" s="63"/>
+      <c r="E25" s="68"/>
       <c r="F25" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="G25" s="65"/>
-    </row>
-    <row r="26" spans="1:12" ht="14.95" thickBot="1">
-      <c r="A26" s="68"/>
-      <c r="B26" s="64"/>
-      <c r="C26" s="64"/>
-      <c r="D26" s="64"/>
-      <c r="E26" s="64"/>
+      <c r="G25" s="63"/>
+    </row>
+    <row r="26" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A26" s="67"/>
+      <c r="B26" s="69"/>
+      <c r="C26" s="69"/>
+      <c r="D26" s="69"/>
+      <c r="E26" s="69"/>
       <c r="F26" s="35" t="s">
         <v>106</v>
       </c>
-      <c r="G26" s="66"/>
+      <c r="G26" s="65"/>
     </row>
     <row r="27" spans="1:12" ht="27" customHeight="1">
-      <c r="A27" s="67">
+      <c r="A27" s="66">
         <v>3</v>
       </c>
-      <c r="B27" s="63">
+      <c r="B27" s="68">
         <v>89</v>
       </c>
-      <c r="C27" s="63">
-        <v>2</v>
-      </c>
-      <c r="D27" s="63" t="s">
+      <c r="C27" s="68">
+        <v>2</v>
+      </c>
+      <c r="D27" s="68" t="s">
         <v>144</v>
       </c>
-      <c r="E27" s="63" t="s">
+      <c r="E27" s="68" t="s">
         <v>54</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="G27" s="65"/>
-    </row>
-    <row r="28" spans="1:12" ht="14.95" thickBot="1">
-      <c r="A28" s="68"/>
-      <c r="B28" s="64"/>
-      <c r="C28" s="64"/>
-      <c r="D28" s="64"/>
-      <c r="E28" s="64"/>
+      <c r="G27" s="63"/>
+    </row>
+    <row r="28" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A28" s="67"/>
+      <c r="B28" s="69"/>
+      <c r="C28" s="69"/>
+      <c r="D28" s="69"/>
+      <c r="E28" s="69"/>
       <c r="F28" s="35" t="s">
         <v>106</v>
       </c>
-      <c r="G28" s="66"/>
-    </row>
-    <row r="29" spans="1:12" ht="41.45" thickBot="1">
+      <c r="G28" s="65"/>
+    </row>
+    <row r="29" spans="1:12" ht="43.5" thickBot="1">
       <c r="A29" s="38">
         <v>4</v>
       </c>
@@ -3857,7 +3856,7 @@
       </c>
       <c r="G29" s="39"/>
     </row>
-    <row r="30" spans="1:12" ht="41.3" customHeight="1" thickBot="1">
+    <row r="30" spans="1:12" ht="41.25" customHeight="1" thickBot="1">
       <c r="A30" s="38">
         <v>5</v>
       </c>
@@ -3878,7 +3877,7 @@
       </c>
       <c r="G30" s="39"/>
     </row>
-    <row r="31" spans="1:12" ht="41.45" thickBot="1">
+    <row r="31" spans="1:12" ht="43.5" thickBot="1">
       <c r="A31" s="38">
         <v>6</v>
       </c>
@@ -3901,12 +3900,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="G23:G24"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
     <mergeCell ref="G27:G28"/>
     <mergeCell ref="A25:A26"/>
     <mergeCell ref="B25:B26"/>
@@ -3919,35 +3912,41 @@
     <mergeCell ref="C27:C28"/>
     <mergeCell ref="D27:D28"/>
     <mergeCell ref="E27:E28"/>
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView topLeftCell="E15" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.375" style="12" customWidth="1"/>
-    <col min="2" max="2" width="9.125" style="12"/>
+    <col min="1" max="1" width="16.42578125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="12"/>
     <col min="3" max="3" width="12" style="12" customWidth="1"/>
-    <col min="4" max="4" width="17.625" style="12" customWidth="1"/>
-    <col min="5" max="5" width="15.25" style="12" customWidth="1"/>
-    <col min="6" max="6" width="15.75" style="12" customWidth="1"/>
-    <col min="7" max="7" width="9.125" style="12"/>
-    <col min="8" max="8" width="16.875" style="12" customWidth="1"/>
-    <col min="9" max="10" width="9.125" style="12"/>
-    <col min="11" max="11" width="22.75" style="12" customWidth="1"/>
-    <col min="12" max="16384" width="9.125" style="12"/>
+    <col min="4" max="4" width="17.5703125" style="12" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="12" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="12" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="12"/>
+    <col min="8" max="8" width="16.85546875" style="12" customWidth="1"/>
+    <col min="9" max="10" width="9.140625" style="12"/>
+    <col min="11" max="11" width="22.7109375" style="12" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="23.8">
+    <row r="1" spans="1:2" ht="23.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -3984,7 +3983,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="23.8">
+    <row r="8" spans="1:2" ht="23.25">
       <c r="A8" s="11" t="s">
         <v>7</v>
       </c>
@@ -4021,7 +4020,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="23.8">
+    <row r="17" spans="1:12" ht="23.25">
       <c r="A17" s="31" t="s">
         <v>13</v>
       </c>
@@ -4037,7 +4036,7 @@
       <c r="K17" s="32"/>
       <c r="L17" s="32"/>
     </row>
-    <row r="18" spans="1:12" ht="14.3" customHeight="1">
+    <row r="18" spans="1:12" ht="14.25" customHeight="1">
       <c r="A18" s="32" t="s">
         <v>3</v>
       </c>
@@ -4113,15 +4112,15 @@
         <v>156</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="14.3" customHeight="1">
+    <row r="20" spans="1:12" ht="14.25" customHeight="1">
       <c r="I20" s="32"/>
     </row>
-    <row r="21" spans="1:12" ht="23.8">
+    <row r="21" spans="1:12" ht="23.25">
       <c r="A21" s="11" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="14.95" thickBot="1">
+    <row r="22" spans="1:12" ht="15.75" thickBot="1">
       <c r="A22" s="12" t="s">
         <v>42</v>
       </c>
@@ -4150,20 +4149,20 @@
       <c r="F23" s="44"/>
       <c r="J23" s="6"/>
     </row>
-    <row r="24" spans="1:12" ht="30.1" customHeight="1">
-      <c r="A24" s="52">
+    <row r="24" spans="1:12" ht="30.2" customHeight="1">
+      <c r="A24" s="47">
         <v>1</v>
       </c>
-      <c r="B24" s="55">
+      <c r="B24" s="49">
         <v>105</v>
       </c>
-      <c r="C24" s="55">
-        <v>2</v>
-      </c>
-      <c r="D24" s="55" t="s">
+      <c r="C24" s="49">
+        <v>2</v>
+      </c>
+      <c r="D24" s="49" t="s">
         <v>157</v>
       </c>
-      <c r="E24" s="55" t="s">
+      <c r="E24" s="49" t="s">
         <v>55</v>
       </c>
       <c r="F24" s="19" t="s">
@@ -4171,16 +4170,16 @@
       </c>
     </row>
     <row r="25" spans="1:12" ht="27" customHeight="1" thickBot="1">
-      <c r="A25" s="53"/>
-      <c r="B25" s="56"/>
-      <c r="C25" s="56"/>
-      <c r="D25" s="56"/>
-      <c r="E25" s="56"/>
+      <c r="A25" s="48"/>
+      <c r="B25" s="50"/>
+      <c r="C25" s="50"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="50"/>
       <c r="F25" s="20" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="55.05" thickBot="1">
+    <row r="26" spans="1:12" ht="57.75" thickBot="1">
       <c r="A26" s="30">
         <v>2</v>
       </c>
@@ -4200,67 +4199,67 @@
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="41.3" customHeight="1">
-      <c r="A27" s="51">
+    <row r="27" spans="1:12" ht="41.25" customHeight="1">
+      <c r="A27" s="61">
         <v>3</v>
       </c>
-      <c r="B27" s="54">
+      <c r="B27" s="62">
         <v>262</v>
       </c>
-      <c r="C27" s="54">
-        <v>2</v>
-      </c>
-      <c r="D27" s="54" t="s">
+      <c r="C27" s="62">
+        <v>2</v>
+      </c>
+      <c r="D27" s="62" t="s">
         <v>158</v>
       </c>
-      <c r="E27" s="54" t="s">
+      <c r="E27" s="62" t="s">
         <v>55</v>
       </c>
       <c r="F27" s="19" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="14.95" thickBot="1">
-      <c r="A28" s="53"/>
-      <c r="B28" s="56"/>
-      <c r="C28" s="56"/>
-      <c r="D28" s="56"/>
-      <c r="E28" s="56"/>
+    <row r="28" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A28" s="48"/>
+      <c r="B28" s="50"/>
+      <c r="C28" s="50"/>
+      <c r="D28" s="50"/>
+      <c r="E28" s="50"/>
       <c r="F28" s="20" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="15.8" customHeight="1">
-      <c r="A29" s="45">
+    <row r="29" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A29" s="52">
         <v>4</v>
       </c>
-      <c r="B29" s="48">
+      <c r="B29" s="55">
         <v>262</v>
       </c>
-      <c r="C29" s="48">
-        <v>2</v>
-      </c>
-      <c r="D29" s="48" t="s">
+      <c r="C29" s="55">
+        <v>2</v>
+      </c>
+      <c r="D29" s="55" t="s">
         <v>158</v>
       </c>
-      <c r="E29" s="48" t="s">
+      <c r="E29" s="55" t="s">
         <v>55</v>
       </c>
       <c r="F29" s="22" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="41.3" customHeight="1" thickBot="1">
-      <c r="A30" s="47"/>
-      <c r="B30" s="50"/>
-      <c r="C30" s="50"/>
-      <c r="D30" s="50"/>
-      <c r="E30" s="50"/>
+    <row r="30" spans="1:12" ht="41.25" customHeight="1" thickBot="1">
+      <c r="A30" s="54"/>
+      <c r="B30" s="57"/>
+      <c r="C30" s="57"/>
+      <c r="D30" s="57"/>
+      <c r="E30" s="57"/>
       <c r="F30" s="24" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="55.05" thickBot="1">
+    <row r="31" spans="1:12" ht="57.75" thickBot="1">
       <c r="A31" s="29">
         <v>5</v>
       </c>
@@ -4282,50 +4281,50 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
     <mergeCell ref="A24:A25"/>
     <mergeCell ref="B24:B25"/>
     <mergeCell ref="C24:C25"/>
     <mergeCell ref="D24:D25"/>
     <mergeCell ref="E24:E25"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E14" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.375" style="12" customWidth="1"/>
-    <col min="2" max="2" width="9.125" style="12"/>
+    <col min="1" max="1" width="16.42578125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="12"/>
     <col min="3" max="3" width="12" style="12" customWidth="1"/>
-    <col min="4" max="4" width="17.625" style="12" customWidth="1"/>
-    <col min="5" max="5" width="15.25" style="12" customWidth="1"/>
-    <col min="6" max="6" width="15.75" style="12" customWidth="1"/>
-    <col min="7" max="7" width="9.125" style="12"/>
-    <col min="8" max="8" width="16.875" style="12" customWidth="1"/>
-    <col min="9" max="10" width="9.125" style="12"/>
-    <col min="11" max="11" width="22.75" style="12" customWidth="1"/>
-    <col min="12" max="16384" width="9.125" style="12"/>
+    <col min="4" max="4" width="17.5703125" style="12" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="12" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="12" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="12"/>
+    <col min="8" max="8" width="16.85546875" style="12" customWidth="1"/>
+    <col min="9" max="10" width="9.140625" style="12"/>
+    <col min="11" max="11" width="22.7109375" style="12" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="23.8">
+    <row r="1" spans="1:2" ht="23.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -4362,7 +4361,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="23.8">
+    <row r="8" spans="1:2" ht="23.25">
       <c r="A8" s="11" t="s">
         <v>7</v>
       </c>
@@ -4394,7 +4393,7 @@
     <row r="12" spans="1:2">
       <c r="A12" s="1"/>
     </row>
-    <row r="17" spans="1:12" ht="23.8">
+    <row r="17" spans="1:12" ht="23.25">
       <c r="A17" s="31" t="s">
         <v>13</v>
       </c>
@@ -4410,7 +4409,7 @@
       <c r="K17" s="32"/>
       <c r="L17" s="32"/>
     </row>
-    <row r="18" spans="1:12" ht="14.3" customHeight="1">
+    <row r="18" spans="1:12" ht="14.25" customHeight="1">
       <c r="A18" s="32" t="s">
         <v>3</v>
       </c>
@@ -4448,7 +4447,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="15.65">
+    <row r="19" spans="1:12" ht="15.75">
       <c r="A19" s="1" t="s">
         <v>162</v>
       </c>
@@ -4486,15 +4485,15 @@
         <v>171</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="14.3" customHeight="1">
+    <row r="20" spans="1:12" ht="14.25" customHeight="1">
       <c r="I20" s="32"/>
     </row>
-    <row r="21" spans="1:12" ht="23.8">
+    <row r="21" spans="1:12" ht="23.25">
       <c r="A21" s="11" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="14.95" thickBot="1">
+    <row r="22" spans="1:12" ht="15.75" thickBot="1">
       <c r="A22" s="12" t="s">
         <v>42</v>
       </c>
@@ -4514,71 +4513,71 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="30.1" customHeight="1">
-      <c r="A23" s="51">
+    <row r="23" spans="1:12" ht="30.2" customHeight="1">
+      <c r="A23" s="61">
         <v>1</v>
       </c>
-      <c r="B23" s="54">
+      <c r="B23" s="62">
         <v>301</v>
       </c>
-      <c r="C23" s="54">
-        <v>2</v>
-      </c>
-      <c r="D23" s="54" t="s">
+      <c r="C23" s="62">
+        <v>2</v>
+      </c>
+      <c r="D23" s="62" t="s">
         <v>172</v>
       </c>
-      <c r="E23" s="54" t="s">
+      <c r="E23" s="62" t="s">
         <v>55</v>
       </c>
       <c r="F23" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="G23" s="57"/>
+      <c r="G23" s="51"/>
     </row>
     <row r="24" spans="1:12" ht="27" customHeight="1" thickBot="1">
-      <c r="A24" s="53"/>
-      <c r="B24" s="56"/>
-      <c r="C24" s="56"/>
-      <c r="D24" s="56"/>
-      <c r="E24" s="56"/>
+      <c r="A24" s="48"/>
+      <c r="B24" s="50"/>
+      <c r="C24" s="50"/>
+      <c r="D24" s="50"/>
+      <c r="E24" s="50"/>
       <c r="F24" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="G24" s="59"/>
-    </row>
-    <row r="25" spans="1:12" ht="15.8" customHeight="1">
-      <c r="A25" s="45">
-        <v>2</v>
-      </c>
-      <c r="B25" s="48">
+      <c r="G24" s="46"/>
+    </row>
+    <row r="25" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A25" s="52">
+        <v>2</v>
+      </c>
+      <c r="B25" s="55">
         <v>193</v>
       </c>
-      <c r="C25" s="48">
-        <v>2</v>
-      </c>
-      <c r="D25" s="48" t="s">
+      <c r="C25" s="55">
+        <v>2</v>
+      </c>
+      <c r="D25" s="55" t="s">
         <v>173</v>
       </c>
-      <c r="E25" s="48" t="s">
+      <c r="E25" s="55" t="s">
         <v>55</v>
       </c>
       <c r="F25" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="G25" s="60"/>
-    </row>
-    <row r="26" spans="1:12" ht="41.3" customHeight="1" thickBot="1">
-      <c r="A26" s="47"/>
-      <c r="B26" s="50"/>
-      <c r="C26" s="50"/>
-      <c r="D26" s="50"/>
-      <c r="E26" s="50"/>
+      <c r="G25" s="58"/>
+    </row>
+    <row r="26" spans="1:12" ht="41.25" customHeight="1" thickBot="1">
+      <c r="A26" s="54"/>
+      <c r="B26" s="57"/>
+      <c r="C26" s="57"/>
+      <c r="D26" s="57"/>
+      <c r="E26" s="57"/>
       <c r="F26" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="G26" s="62"/>
-    </row>
-    <row r="27" spans="1:12" ht="55.05" thickBot="1">
+      <c r="G26" s="60"/>
+    </row>
+    <row r="27" spans="1:12" ht="57.75" thickBot="1">
       <c r="A27" s="29">
         <v>3</v>
       </c>
@@ -4599,71 +4598,71 @@
       </c>
       <c r="G27" s="21"/>
     </row>
-    <row r="28" spans="1:12" ht="15.8" customHeight="1">
-      <c r="A28" s="45">
+    <row r="28" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A28" s="52">
         <v>4</v>
       </c>
-      <c r="B28" s="48">
+      <c r="B28" s="55">
         <v>114</v>
       </c>
-      <c r="C28" s="48">
-        <v>2</v>
-      </c>
-      <c r="D28" s="48" t="s">
+      <c r="C28" s="55">
+        <v>2</v>
+      </c>
+      <c r="D28" s="55" t="s">
         <v>175</v>
       </c>
-      <c r="E28" s="48" t="s">
+      <c r="E28" s="55" t="s">
         <v>55</v>
       </c>
       <c r="F28" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="G28" s="60"/>
-    </row>
-    <row r="29" spans="1:12" ht="41.3" customHeight="1" thickBot="1">
-      <c r="A29" s="47"/>
-      <c r="B29" s="50"/>
-      <c r="C29" s="50"/>
-      <c r="D29" s="50"/>
-      <c r="E29" s="50"/>
+      <c r="G28" s="58"/>
+    </row>
+    <row r="29" spans="1:12" ht="41.25" customHeight="1" thickBot="1">
+      <c r="A29" s="54"/>
+      <c r="B29" s="57"/>
+      <c r="C29" s="57"/>
+      <c r="D29" s="57"/>
+      <c r="E29" s="57"/>
       <c r="F29" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="G29" s="62"/>
-    </row>
-    <row r="30" spans="1:12" ht="41.3" customHeight="1">
-      <c r="A30" s="51">
+      <c r="G29" s="60"/>
+    </row>
+    <row r="30" spans="1:12" ht="41.25" customHeight="1">
+      <c r="A30" s="61">
         <v>5</v>
       </c>
-      <c r="B30" s="54">
+      <c r="B30" s="62">
         <v>114</v>
       </c>
-      <c r="C30" s="54">
-        <v>2</v>
-      </c>
-      <c r="D30" s="54" t="s">
+      <c r="C30" s="62">
+        <v>2</v>
+      </c>
+      <c r="D30" s="62" t="s">
         <v>175</v>
       </c>
-      <c r="E30" s="54" t="s">
+      <c r="E30" s="62" t="s">
         <v>55</v>
       </c>
       <c r="F30" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="G30" s="57"/>
-    </row>
-    <row r="31" spans="1:12" ht="14.95" thickBot="1">
-      <c r="A31" s="53"/>
-      <c r="B31" s="56"/>
-      <c r="C31" s="56"/>
-      <c r="D31" s="56"/>
-      <c r="E31" s="56"/>
+      <c r="G30" s="51"/>
+    </row>
+    <row r="31" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A31" s="48"/>
+      <c r="B31" s="50"/>
+      <c r="C31" s="50"/>
+      <c r="D31" s="50"/>
+      <c r="E31" s="50"/>
       <c r="F31" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="G31" s="59"/>
-    </row>
-    <row r="32" spans="1:12" ht="55.05" thickBot="1">
+      <c r="G31" s="46"/>
+    </row>
+    <row r="32" spans="1:12" ht="57.75" thickBot="1">
       <c r="A32" s="30">
         <v>6</v>
       </c>
@@ -4684,7 +4683,7 @@
       </c>
       <c r="G32" s="25"/>
     </row>
-    <row r="33" spans="1:7" ht="55.05" thickBot="1">
+    <row r="33" spans="1:7" ht="57.75" thickBot="1">
       <c r="A33" s="29">
         <v>7</v>
       </c>
@@ -4707,6 +4706,18 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="G30:G31"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:E29"/>
     <mergeCell ref="G23:G24"/>
     <mergeCell ref="A25:A26"/>
     <mergeCell ref="B25:B26"/>
@@ -4719,18 +4730,6 @@
     <mergeCell ref="E23:E24"/>
     <mergeCell ref="E25:E26"/>
     <mergeCell ref="G25:G26"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="G30:G31"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="E28:E29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
hoofddorp zalen aangevult in exel
</commit_message>
<xml_diff>
--- a/documentatie_And_sql/documentatie/BioscoopData.xlsx
+++ b/documentatie_And_sql/documentatie/BioscoopData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7350" firstSheet="6" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7350" firstSheet="3" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="almere id(1)" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="183">
   <si>
     <t>tarieven</t>
   </si>
@@ -594,12 +594,24 @@
   <si>
     <t>5223 MX</t>
   </si>
+  <si>
+    <t>3.90m x 9.90m</t>
+  </si>
+  <si>
+    <t>4.10m x 10.00m</t>
+  </si>
+  <si>
+    <t>4.40m x 10.00m</t>
+  </si>
+  <si>
+    <t>4.70m x 10.00m</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -646,6 +658,11 @@
     </font>
     <font>
       <sz val="12"/>
+      <name val="Montserrat"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Montserrat"/>
     </font>
   </fonts>
@@ -793,7 +810,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -850,8 +867,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -883,85 +898,139 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -979,6 +1048,319 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>304800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4097" name="AutoShape 1" descr="data:image/jpg;base64,/9j/4AAQSkZJRgABAgEASABIAAD/7QAsUGhvdG9zaG9wIDMuMAA4QklNA+0AAAAAABAASAAAAAEAAQBIAAAAAQAB/+IMWElDQ19QUk9GSUxFAAEBAAAMSExpbm8CEAAAbW50clJHQiBYWVogB84AAgAJAAYAMQAAYWNzcE1TRlQAAAAASUVDIHNSR0IAAAAAAAAAAAAAAAAAAPbWAAEAAAAA0y1IUCAgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAARY3BydAAAAVAAAAAzZGVzYwAAAYQAAABsd3RwdAAAAfAAAAAUYmtwdAAAAgQAAAAUclhZWgAAAhgAAAAUZ1hZWgAAAiwAAAAUYlhZWgAAAkAAAAAUZG1uZAAAAlQAAABwZG1kZAAAAsQAAACIdnVlZAAAA0wAAACGdmlldwAAA9QAAAAkbHVtaQAAA/gAAAAUbWVhcwAABAwAAAAkdGVjaAAABDAAAAAMclRSQwAABDwAAAgMZ1RSQwAABDwAAAgMYlRSQwAABDwAAAgMdGV4dAAAAABDb3B5cmlnaHQgKGMpIDE5OTggSGV3bGV0dC1QYWNrYXJkIENvbXBhbnkAAGRlc2MAAAAAAAAAEnNSR0IgSUVDNjE5NjYtMi4xAAAAAAAAAAAAAAASc1JHQiBJRUM2MTk2Ni0yLjEAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFhZWiAAAAAAAADzUQABAAAAARbMWFlaIAAAAAAAAAAAAAAAAAAAAABYWVogAAAAAAAAb6IAADj1AAADkFhZWiAAAAAAAABimQAAt4UAABjaWFlaIAAAAAAAACSgAAAPhAAAts9kZXNjAAAAAAAAABZJRUMgaHR0cDovL3d3dy5pZWMuY2gAAAAAAAAAAAAAABZJRUMgaHR0cDovL3d3dy5pZWMuY2gAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZGVzYwAAAAAAAAAuSUVDIDYxOTY2LTIuMSBEZWZhdWx0IFJHQiBjb2xvdXIgc3BhY2UgLSBzUkdCAAAAAAAAAAAAAAAuSUVDIDYxOTY2LTIuMSBEZWZhdWx0IFJHQiBjb2xvdXIgc3BhY2UgLSBzUkdCAAAAAAAAAAAAAAAAAAAAAAAAAAAAAGRlc2MAAAAAAAAALFJlZmVyZW5jZSBWaWV3aW5nIENvbmRpdGlvbiBpbiBJRUM2MTk2Ni0yLjEAAAAAAAAAAAAAACxSZWZlcmVuY2UgVmlld2luZyBDb25kaXRpb24gaW4gSUVDNjE5NjYtMi4xAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAB2aWV3AAAAAAATpP4AFF8uABDPFAAD7cwABBMLAANcngAAAAFYWVogAAAAAABMCVYAUAAAAFcf521lYXMAAAAAAAAAAQAAAAAAAAAAAAAAAAAAAAAAAAKPAAAAAnNpZyAAAAAAQ1JUIGN1cnYAAAAAAAAEAAAAAAUACgAPABQAGQAeACMAKAAtADIANwA7AEAARQBKAE8AVABZAF4AYwBoAG0AcgB3AHwAgQCGAIsAkACVAJoAnwCkAKkArgCyALcAvADBAMYAywDQANUA2wDgAOUA6wDwAPYA+wEBAQcBDQETARkBHwElASsBMgE4AT4BRQFMAVIBWQFgAWcBbgF1AXwBgwGLAZIBmgGhAakBsQG5AcEByQHRAdkB4QHpAfIB+gIDAgwCFAIdAiYCLwI4AkECSwJUAl0CZwJxAnoChAKOApgCogKsArYCwQLLAtUC4ALrAvUDAAMLAxYDIQMtAzgDQwNPA1oDZgNyA34DigOWA6IDrgO6A8cD0wPgA+wD+QQGBBMEIAQtBDsESARVBGMEcQR+BIwEmgSoBLYExATTBOEE8AT+BQ0FHAUrBToFSQVYBWcFdwWGBZYFpgW1BcUF1QXlBfYGBgYWBicGNwZIBlkGagZ7BowGnQavBsAG0QbjBvUHBwcZBysHPQdPB2EHdAeGB5kHrAe/B9IH5Qf4CAsIHwgyCEYIWghuCIIIlgiqCL4I0gjnCPsJEAklCToJTwlkCXkJjwmkCboJzwnlCfsKEQonCj0KVApqCoEKmAquCsUK3ArzCwsLIgs5C1ELaQuAC5gLsAvIC+EL+QwSDCoMQwxcDHUMjgynDMAM2QzzDQ0NJg1ADVoNdA2ODakNww3eDfgOEw4uDkkOZA5/DpsOtg7SDu4PCQ8lD0EPXg96D5YPsw/PD+wQCRAmEEMQYRB+EJsQuRDXEPURExExEU8RbRGMEaoRyRHoEgcSJhJFEmQShBKjEsMS4xMDEyMTQxNjE4MTpBPFE+UUBhQnFEkUahSLFK0UzhTwFRIVNBVWFXgVmxW9FeAWAxYmFkkWbBaPFrIW1hb6Fx0XQRdlF4kXrhfSF/cYGxhAGGUYihivGNUY+hkgGUUZaxmRGbcZ3RoEGioaURp3Gp4axRrsGxQbOxtjG4obshvaHAIcKhxSHHscoxzMHPUdHh1HHXAdmR3DHeweFh5AHmoelB6+HukfEx8+H2kflB+/H+ogFSBBIGwgmCDEIPAhHCFIIXUhoSHOIfsiJyJVIoIiryLdIwojOCNmI5QjwiPwJB8kTSR8JKsk2iUJJTglaCWXJccl9yYnJlcmhya3JugnGCdJJ3onqyfcKA0oPyhxKKIo1CkGKTgpaymdKdAqAio1KmgqmyrPKwIrNitpK50r0SwFLDksbiyiLNctDC1BLXYtqy3hLhYuTC6CLrcu7i8kL1ovkS/HL/4wNTBsMKQw2zESMUoxgjG6MfIyKjJjMpsy1DMNM0YzfzO4M/E0KzRlNJ402DUTNU01hzXCNf02NzZyNq426TckN2A3nDfXOBQ4UDiMOMg5BTlCOX85vDn5OjY6dDqyOu87LTtrO6o76DwnPGU8pDzjPSI9YT2hPeA+ID5gPqA+4D8hP2E/oj/iQCNAZECmQOdBKUFqQaxB7kIwQnJCtUL3QzpDfUPARANER0SKRM5FEkVVRZpF3kYiRmdGq0bwRzVHe0fASAVIS0iRSNdJHUljSalJ8Eo3Sn1KxEsMS1NLmkviTCpMcky6TQJNSk2TTdxOJU5uTrdPAE9JT5NP3VAnUHFQu1EGUVBRm1HmUjFSfFLHUxNTX1OqU/ZUQlSPVNtVKFV1VcJWD1ZcVqlW91dEV5JX4FgvWH1Yy1kaWWlZuFoHWlZaplr1W0VblVvlXDVchlzWXSddeF3JXhpebF69Xw9fYV+zYAVgV2CqYPxhT2GiYfViSWKcYvBjQ2OXY+tkQGSUZOllPWWSZedmPWaSZuhnPWeTZ+loP2iWaOxpQ2maafFqSGqfavdrT2una/9sV2yvbQhtYG25bhJua27Ebx5veG/RcCtwhnDgcTpxlXHwcktypnMBc11zuHQUdHB0zHUodYV14XY+dpt2+HdWd7N4EXhueMx5KnmJeed6RnqlewR7Y3vCfCF8gXzhfUF9oX4BfmJ+wn8jf4R/5YBHgKiBCoFrgc2CMIKSgvSDV4O6hB2EgITjhUeFq4YOhnKG14c7h5+IBIhpiM6JM4mZif6KZIrKizCLlov8jGOMyo0xjZiN/45mjs6PNo+ekAaQbpDWkT+RqJIRknqS45NNk7aUIJSKlPSVX5XJljSWn5cKl3WX4JhMmLiZJJmQmfyaaJrVm0Kbr5wcnImc951kndKeQJ6unx2fi5/6oGmg2KFHobaiJqKWowajdqPmpFakx6U4pammGqaLpv2nbqfgqFKoxKk3qamqHKqPqwKrdavprFys0K1ErbiuLa6hrxavi7AAsHWw6rFgsdayS7LCszizrrQltJy1E7WKtgG2ebbwt2i34LhZuNG5SrnCuju6tbsuu6e8IbybvRW9j74KvoS+/796v/XAcMDswWfB48JfwtvDWMPUxFHEzsVLxcjGRsbDx0HHv8g9yLzJOsm5yjjKt8s2y7bMNcy1zTXNtc42zrbPN8+40DnQutE80b7SP9LB00TTxtRJ1MvVTtXR1lXW2Ndc1+DYZNjo2WzZ8dp22vvbgNwF3IrdEN2W3hzeot8p36/gNuC94UThzOJT4tvjY+Pr5HPk/OWE5g3mlucf56noMui86Ubp0Opb6uXrcOv77IbtEe2c7ijutO9A78zwWPDl8XLx//KM8xnzp/Q09ML1UPXe9m32+/eK+Bn4qPk4+cf6V/rn+3f8B/yY/Sn9uv5L/tz/bf///+4AE0Fkb2JlAGQAAAAAAQUAAklE/9sAhAABAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAgICAgICAgICAgIDAwMDAwMDAwMDAQEBAQEBAQEBAQECAgECAgMCAgICAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwMEBAQEBAQEBAQEBAQEBAQEBAQEBAT/wAARCAEEAcsDAREAAhEBAxEB/8QBogAAAAYCAwEAAAAAAAAAAAAABwgGBQQJAwoCAQALAQAABgMBAQEAAAAAAAAAAAAGBQQDBwIIAQkACgsQAAIBAwQBAwMCAwMDAgYJdQECAwQRBRIGIQcTIgAIMRRBMiMVCVFCFmEkMxdScYEYYpElQ6Gx8CY0cgoZwdE1J+FTNoLxkqJEVHNFRjdHYyhVVlcassLS4vJkg3SThGWjs8PT4yk4ZvN1Kjk6SElKWFlaZ2hpanZ3eHl6hYaHiImKlJWWl5iZmqSlpqeoqaq0tba3uLm6xMXGx8jJytTV1tfY2drk5ebn6Onq9PX29/j5+hEAAgEDAgQEAwUEBAQGBgVtAQIDEQQhEgUxBgAiE0FRBzJhFHEIQoEjkRVSoWIWMwmxJMHRQ3LwF+GCNCWSUxhjRPGisiY1GVQ2RWQnCnODk0Z0wtLi8lVldVY3hIWjs8PT4/MpGpSktMTU5PSVpbXF1eX1KEdXZjh2hpamtsbW5vZnd4eXp7fH1+f3SFhoeIiYqLjI2Oj4OUlZaXmJmam5ydnp+So6SlpqeoqaqrrK2ur6/9oADAMBAAIRAxEAPwDS/wByVO195bslzzZ3C7Iqd75zfe5dx0k20YNsdf7KyWSzW4M7t/bGysLsoZRk2/VYv7elpaWmoKSmxU8q0qJ9pB9x7LZLnc4I72WTa1mCNEIEtZAXkDBBKzCURJGI3ZiBrYtGoPxnR0YLFau1ui3hTUHMjTKdKkaigBTUX1KBU6QAxp8I1dDF1ns7J/IPsLpj42/Hzb299xZ7sjZ2L2LU7f7fr8Dvak2X2rmMhDvHursXpKkwlDhaXrnZK47acVaGdanO/wANpq6OqnqXliKk3Nl9s3K207nzheI6JZL9VMbaiSXTRo8cNu5x4odpAsauaBypxTq+2xXN9cQbcHUCVvDVpalYgSC8nnp0gVYjNAekTTdX5mHAbp37X5LZm+ekdldin4+P2NNnslkMXtzKbvlz8+B7A2jsGgyuL7BnxVPj8PXZ/HRfZCCpZGWSCVy6qXPzHZS32z7HFb3dhzhf7f8Av82AhQPIkHgpNb3NwUkthJqkSF+/UBQowFD0u+inSC7vHkiudpt5jYrMXYqpfWySRJqWTThnXtpX4gcjpzpN47a7U7JpMn392BTb3r4t8TxZbeW4qjduG3/31R7z3DkY8x2D2Z29Ww7hzWNp9iU0FJXo2SpXr1xUjUMKvNG9lm8jmGGy3C62VZl3O5tzKTIUuEtZIkUiOO3LoJGm7lJVtOujkgU6Y21trW7tV3JPEsY3oyRkxtKrE5MlG06cHIrTAz0FPY2fwGSyFdRbHiqtr9Y5ncmX3ftvqibdeY3jSbArsmq4c4mp3HmsZhJd153+CYymSTJfaxvPT+NGHot7N9ps5VZrrcLdX3mOJLSS/wDDRGnjQa9QVWcxx+I7EIThqnzr0nu3CwwQ290WtXJn8CrEROSUKtqADPoVasMEU+zpb5OtWu/0Z5eHc+Qw/d+Ix1dv/I9n7z3blqTA7g2ztLbuMzvVxxee3vPFLR752Su1Ztt46hoKWTFZF6Ohhp6maa8aE1uoT9/W8lkj8tNKLNbKCOMukkkrR3BdINQMM3irMzOwkUM7OijPT8wKCycTE3pQTeKxYAqFBQAyAd6aSnaCpIAUnrJsftCvw1DufB4Cn6+3zvP5G7ez2wuycn3HsnAhdh1u7d0xrjs7svfO5t0w7Y27uGrgEeRfdFXSY6TAzVNSgk8IlmZzcNmE01vdXEl1bbbtTJNax2ErHxljQErJBHD4rBSCgiVnEigdtSAKRXNIngSOJ55ydbyrQoTUABy+gA11EkDSRWuOg8q8RgNqwVG1ex9r9h47eVPic3mMaaLcGFpMRNBubbe3sn1Zkv4Fkdv1skm16yWomyNfkKOtds1i66i+yNOY2mnMlnu75hfbNe2jWLSJG+qNi48KSRblS6yD9QUCKjKPCdX16q6VYIVFEFwkusAso1DT3KpQgEHB4kg9wIpTiVBt7dfRG1dmYw1O0ezd87y3Bsjt3bHZ+HyW+aPY3W+K3TkJKT/QJvfZE+0KWu3RuyPYFVGMtm8HuBUocjkYIY4HjhLOp7TNPPpCQR9g6S21xQ7gw1PtjE9a7dyOfnirsXkexsxubcuMocO269y7PpNr7pzE8m4MVsDZNHtKannxy1+StiZYM3NLXBpYKWWEhvvEtLlr243qVLWoaOzjjjZn8KOZpIkAjeeZpRR9CfqAxAJgsGWRASR+HHaqXFQ0pJAGoqFY5CIFOKnHdnNKCnDubsSbr6h6L3Fvefe3x02VmMznIKfbVXh8LsTYPdnYuzMrm6HGVfZe7di1S0WXqM5sKRaqlp55KXcFPiq2LD1TwzfeeyeS02xt0Tf7az+m5olGlRPraSW1ilRJHFtFOupTHIulmGqJnjMyBl0dK45rhLeWxMofbyBrKhQA9CyjxGQkEMDwPcAwUkGvUfYHWmahocPuPJ7B3P2DF2VsiTaoyWY2VuqjwvT2Z31mMjt3ZO7Xyu66LFbQ37mMtsDa+Vrdpw0+YoqVK0RslUZsfJTOl3zf7OOS5sk3a3s5rSc3aRCePxL2O3RJJ0CRF54Yo7iWNLhvCchSQVpKrdPbdt0s5ic28kkMtIXkEZIhaQkIatoR3KKxRda1Iwe0joAqDDFaWjzeWg3JRbHyORrsNFuijxFQaLI5Ghpo61cVTVVS1Ni63JL56WSppBUGaCKUOR+kkXT3il5bK0kt33lI0mNs8gDKjsV1sBV1U6XCtpoxUj16L7eCPWkt40ybazMhmjStSBUAAkKTUrUVqAa9Gd7I3nTbgx2Y7y6n6yXrTxY7afW+7Mp0/wBU5nbnx7wGU7T2Z2JJvzr7O1+7c3vhsVvaup4lo8EYaxTlMTRVtVF4pqdD7C+x8ubpbxS2G93s99tgu5LhJL6YSTq0UkLWmhoY4U8IhHdkerKxC9y1ov3DcrWf6WSys4re4S3WF/AUhXwwkd9bP3nUFqKAjODTpZ7k373V8qup4evcb3LlN67X+PuK2Vjep+k97w1FZ3FvvLb+pZqreuJ6t2rsyj3FNurFbL3Dha2ZdUgkpME1PNMIGecIGtHLnt9zHBuW4cvtby7ubl77d4X/AN11lHbEGE3UtxJGtq10siiirpkuNQzQMTBf3jzBt8lvBerJ9L4Sw2pX/GJmkrq8NY1JkEWk8TVUpwyOkbvuh2L8ft3dC0p3Dtb5VfHHM4fZvyRj61l3Ydl1tZk944TH7Y39sHtGv6vz8+9eq94UeV2a1GaWDK/cjGwUlWBFJUyKBTyfeX28/vLdeYeWht/McVxLtkyB3kjkggmke3khkZIvEjljlDk6FIdnTIUMSfdI4LZorawvzNYsizIxUKwdkUOGFTRlYU4kUAPGvTr8p/kd3F8n4OiOzvkbQ7r3LgMb1JmOp9jZmh2Njurtu1P+jw5TB4vCbN3fS43KYjsSj2NPksTUZuYxJXl5pKKXwM0VQU/Lmy22yyb7teyXtut5HPbErJJ9Q62wSIKssK+C0DNGkkcRJeoCys0h1J0ovr0Xa2VxdxSGIxyk6V8MGVmcko58TWAxVmwvEoAoo3Sf7V+SQ7ym2PNjutKPFd3ZDrjanTnZnb+7N6T9i5DtbHYbZWK6zxdT/At54k7Z65kptq4XHUVHNjI46rFQ0ERpqlXLu2rXYeYLLceYN45q53m3HY/qDeWFjHbJa/RpGQyReJbt4t0ECkESYkqdanA6UfWbde2m2bTtWwRwbszCKS6aZn8XWApGiT9OPUx1ahleCkDph6j+P9R2T2fsBfkHvrdPRfRu9Owtx9Z7m+VOX2BubtPZm29x7K2vNl8pjaeTH1+OTeGTxdNFQwz00GREtFR1KTsPFFp9m1zv+3WO3t+54oprtYo7hbGMiOQRTSKvieEFLgDUWICEsQQAWIqhXar+43J7KY/rh3iZ2YFdUasSviV08FoDWnzp0KOwuot+9Wb17FbdGz/jzv3sb4103W+ZwnTO/slTbny/aW2s/PU7wqqvZnWO1BXYruqhGwK05XPw11ZHWYLF6ZpNE1O8axlvnNuw81bXsFvtG68w2nL/ADG97bybztsbwR2csA+nH1F3Ppk25zcp4duUQrNLVRqVwSKLPb9xsLi8F9Y7dJuG2RROlpclC0kZrMSsSdtyfCYl9R1KtOBWgRvzaznw43Z2/t3K/Bvau/NmdXZDqfYlRuja3YUqTZDFdwyUNVJ2DQ7erJa6qnyW0oKsQ/a1MqwAytMscawJEWk/lC15ktbCeDmi6E92soEUmpGYxiKIMXMccS904lKDTURlA5L6j0Ddzls55xJt8IjiplRqp8TUpqLGujSDmhatABQdGZwtJ1/Fjuwovhj0ZTd6Yah/l/8AXdZ8kd97/wBm7wqc70D2FDWbUk+QHcmwKPJbueDC/wAN3JUwYdK6OKfG/Y1cvgphCZGYKQWe6n6f/XH5olt3bmmV9nht2jiWaAsfobSUwr+ooAP9oQzEjXSQppNV3JbV2k5dslDHbRFdM/6ncVInkAkB0lhmiii07SQDUB9sYHr+i2tsPMYjd+TrezandG503BtLPbdgwuxdtYHApgazZOdg3nLlat91NumU5CnyGONJSGkWFB5nMtlkXx+YbneN8sLzaoYuWFtYDa3sM5e4mlk8YXMTW4jXwPBAjMcmt9eo9o09Bpo7FLaymjuS24GR/EiddKKq0KNr4OH4EYI+VM2K7epe2+3u3Mlubb/SnU/xbb5/RbrbrHKYCbKdV9E7W6so3z+I7l29sDA5rK5bDDY+5anEyUskczmopK6iEONaHy6SBOar7la0sUur3eZ7yx5QeGe+sI1aaV7siI2EjzyM0/iRMS39oyt4h8aoWgOdpj3FpJI7eySObdVeKGUsO2IV8dRGoCkOtOIVsApStSFVNtXrbD92RLsrtnBxbW2Ht0brzedy+363aMGVrtoxNJuLYmxqCpO75d1Z3OU1Oq4mtrRTR5OSRpnSAqB7E1rNve9clXH762Uw7ldoyxW8kxkNZQDGZXiRPBozEMoFEApq6ZlgtrffDHY3CmCE1Z1UKNMddekOx1kqK1qS1agV6hJ1ZX0Gb6HFL2Fhetusu+d0UW5dj703ZuLEz7U2RBQbtrtgbg3Xvej2nlN17v23T7DzVDPA65TG09bWY+P7qKGSCaN3NrkzxbXue47lsYu91hspYXjtqNNOlNXhJhAPGpXSDg0GcdIYLhobm0jsb8xWwuUuI/EpoSRcByDWpTA7hQjj59PHUHX2X3X3TNhMfjtr9s43YWX3D2l2FUZybcGO67yvXHWM1dubs3eGXTASbf37lev6zZGOkyEsWI+33BLQOVoKdqtkjLl+lzPyxMm3LdWV1JYNFbxwiH6mKRoqRIhnLW6zxP2jxNUWsd50gnqscwk3R5btkmJuPFlkbVoarkuxCDUUetcCtOA8ujF7G3pR/LjcG0uod3bFz8uz+iPi73Pg+jOtumN3ZDEUVNvnC4jc/ZB3xkartau3hpo9x7kebKbhpI5aFJoaYR0iQMqU7BDm28tPb3bI+aLc29tPeblt8G73tyjM0iMy2wdliqDKSygCNQvcaBQdYOdmspeYr2bbF1N4VtcS20KGgBUeJpBah06QaFyaUFSTggnvufdfbvQ1FujbzHG9KfGXJbG2lUde5Tdm16/I4Dd3dGKZtybr25JXUm3N4Z/Ddibn67rqiKkFNm225SxQU1VV6PBLUHHL3L55f5i366kthNu27Vnud0A8MOIXkW0t3gErLrggcK0kaxrKRrKhmoKbnfw7psu3SNeqkdlIttDtwUlwjqHllE2jKtJXSrlitaDAyCmQk7JkwmX7YoXqcntHelZWdI09dvCt292Dur7ODC4uen2tSxZ6nyWbxk2PwlBSwUOQoYKSeljQQ0skYYhnLZuWotws+TZ9EW9WcQ3x47KOW0gLNK4ecmMrEweZ2Z43ZwxOpwePTV9bblPaXHM1rHJ+5Jrg7dGbmSOeYUQMsRqNY0xgBWCrTAWnUPZ/eHbHXW+dobzwe7qrC7p6+2fuHq3bVZX7f2/n/wC6mxNy4Hde0N3beotr7px1fhC82D3zmQ/lp1qIq2tkqUeKrtOomsNq2uyjv32+2UJeXDXs7KSfFlkCgyFqkmqooFDQKqhRpAHRJdXt3dPai5fugiW3j7VXSiVxQAVI1GpPcSTU16mdsbdrOvdwP1pXbu+QuH+POTiy/ZPTsu+thZTY+S33srduBrU697Vo+nsvvePadNjOzYqCkp6nJUeVraZsf5ZIqms8Aje92swgknsbG2l3EyRlllbQp0sAxaRI5W1xxlig0mrUWqg6gwpQuqTTyLbhWAKipoQSAFLKNLNxz6nJ6d/5gvWvwx6hg696m+M+79ydkdp9Xbi7W2h8hOzKmsxWQ2l2jKlZtfMdfbv2RPtbeW9uuKbE4Z8pmMCqYHJ1dPkqTE0+RklE1WY4465In907ne+apeftusrbZZEtZNqjtJlmEZpKtzEzCOOVj2xya3FKyFFFEPQg3GLlyG221dquppLoGVbnWhRjShjbJKUNSKKa0FTQkdSex+jtldO9SSYL40989ffOLqT5obk211vtLo+amyfT3yt2j8gMRBlKbpvtDPdAYbObh3fWYvG1W5svQbfaLLVO3s7UZWJa2naU0oEbQbvuvNnNB3Xmvli95W33lWSV33UmK72+7250t5b63jumVYoxIUi8UmNZ4vBbwnA8SgjaJNo2z6K2uY7623OFH+nBMckc2qRYJNKnW5RdRANEOsalPaSSnsjN4XdvbvU/UffHWGyfiNjugtu4P439xVfT3UuTj7Cqsr13nM9S727P7f2vmt3vWb+77yWeq54MvOKqgpxHTxQQU8UUCp7le8ubyPYN13zk63XctxuYReWNvc3TpBK7RpoVZmWbwIpAA3aukMSQo1HoMW8cUl1BbblJ4MCNokdVBI+0LTVQ4rk09aZYetYd+/7L98r5NrdF7d7R6xxsPUw3z3Tn9u5OXOfHufJb/ei2HuHbeVoc/SUW28r2jWUsuGniqosgJINcaaAJWdndE21+Z+T5Lze5rXeStyLeyik/TugI1aZXXT+oIBRlOKE1pUrRVDd3UW17nZwxo9gzxvI7KNSspIQg/ENVTUA/yrVh+TP+y9wd971f4yVGervj8aza8uxn3Hj8th899tUbVwFRunHVNHuLL5vLI9DuxslT08lTVyGeGNJAVRgq25Lj5rj5V2yPnOdJOagsguZECBWbxH8NgIgqCseioUD9temt1fb5NxuH2uIx7aWBjQliQKCoq3cc14/4Ojr/ACJi+K3aNLvp/hv15snrP469LddpuLCdlfICtyWy+4+ze5Mhi9l1m6tq4PN08uZoN+bmpFxdU+F2XPIKOngmq6tH8ckKJHdtNvnLm/7Q/MO6b1fb3u89vZy2FiI7m1tYI4pVe6ljVIvo7eS4kJe4AL0EETairMRKq224bZePaWVjBaWavIJ5i0cjyuwZI0YljO4jj7Yz2gl2xUDoA93fEjdb7Q6hyuIzdX2B8nu9tz5Wsp/it1n1/PufceG65r9m4zfOyOwqPPbJyOZwWSl3ti6qqlGBpaRKvGUtK0lQVYSxxjLZueuW7lN0W2ujHsW2vJaT314ZIkWWCUQPGWuFQuRLqTXUgleJDoWLN12Td18K/vLdBLdESpHFoOoOnighIiQq6CDSg40pVWoCu29yVO0I9u1vY218Z2X1tumoxdfX7RyeZjpcxlaHYUeawWIxNJvHHxVG9diUOJbNzj7GjqKakqgkS1EMn28IiMNxsV3VdzteX9yk27frdWRbpIiyI1wUldzA9ILhn0DuYFlqSrDU2rdof3Wdtvt529LzargErCZdLMI6oO9CZI9BOFwDQAggYEzf/cVf8gO/aDfWyuvt8Ue+spu3q3bPUeycXuTJ9u1u2dhbE2zidibD6rwONrdvwbr7AzOIosLjafFyyTCaSmphTPFK7iZWbbbt5sOWo7PnHmqDcY4ttki3G+nhSzaeTzncxyeDbx+HqDKqnJDBgBpKV7mymvvF2zbXt5DcI0MaOZQq0yoVl1O5ejA1/o08wI3ya+aXZ3yL7pxnaW6aOgxfyR29vzcONru+KqBdj5vcW0Ysdgdi9f7X3Z1VPU1nWHXkmwaPFV0lXVU0Bq5ZcpOlbNKKSBl3s3LO1WfKx224tvFt7hBPdKsjTB3KISEdUjLoNACFUUsADpqT1S9v55dyM0UhXw2KRFl0kLqahZSz6WOqpBY0OK0A6cqbqPO/GruLe28ekvkFtCm/2XfADO4XuHKCSl2F2h3JsPFbWym/Oquid34cbg2l2Vk8Nlc4ooo3qqaqyGPAnelSIuygy55pTmPZ9u2Lmzk64e93W9+mk26wlWWe0sZ5J0tNxvVrFLaxOkNWdAyxydqOzAdHFttr2VxPuG2bmi29tCZVuJ1ZElmQIZLeKoZZHGv4TSq1qKZIW7h7L338h9+b/qsxV90dxUufw1T3Pu+kpdq4zcG7sjv7YPXGbr8nuXc4w71tRiOptq5nM5VK+uhqoTTbZb7qeNapAIxrtnLI2fb7KHarG2gvLfXbRlHlZUtHnVnYFgS9w0UauS6keKCNWkkknuNxa7uJJbqV3jcrIVIUapApAGKUTUSuD8PlXpN9w57anbG/KSm6d2PgMayUeO2tt7bHUHXe5NtUO9MPi6GbLybpyW2sjujem4snvp8hWT09ZIhSCajoIahYo+R7b5dhveW9mDczbs7woplmu9yuIndHZ9OkyLFDEItNCvmGYrnpVuclnut1NLtdkI7mWWiWlrG3hiMKCCoLO5fVWo9Bq+Qh7E2qm4et8piqfYuU3HVbn3JT5GfsLGYCsylZ05ietvtaje2cno9u0+f3LunYlRsvebVObpWpcbT0dVS0VRHUzyRmA23jdlsN8hkn3eC3SGFY0tZZVQXkl2WWCIGUxxRz+PBphIaRnDSKUUEN0zbWRnsA0NtJI7sxd1SvhCIKWaq6mZND1eqqFopqeAVuwMx2v0LvbObw6grt+47v3qvd+eGL3Nj8ZTPuHbXX+x9sZTI7n3Vkuq967OyG9dr08OJpKapGWrHpaXE4qOqo6qD1F0ruUWzcw2Nhbb4LccvXUSMYWcqHuZZFESLcxTLDISzMPDAYvIVdDUZpbyXVk1ybQsbrKMdIJ8MCrHQ6FlwB3YotVOCekeuHpNpzVG4szt/YXfe3czksFuSu3Hg917ypp8fRYncuKq920OYpMLXbZ3PsWn3vk8nJt+asz2Lp2qSJKjCOwMFXIta5e/CWNveXW1Xqo8KQyxQ0dmjfw2RnWSOYxKvihYpDpwswFGQMrGI9UrQpcQkhiylsAEVrQgoGJ01YCv4fI9Ret92dQ0VDVbU7F2fvh6PcvZ/WlfuzfvXO+Hx+7dt9H4jI5OTs7r7bnX+ap22JvLc25Vq8fW4rI52oWLG1+IhDRulRI6ChRRV1GvAE/wCH9vSA1JJXHy6ZMTW9S47KZutymN7IyuEh3ZQTbSGK3Rtja+UbY0dRnVr4NzZOTb24oaTek9LJiXp6jHxmhhqI6xXiljlp2iLdwh3WYrHt89tHEYpA/wBTG8vedHhkKskYKAB9YJBNVKkUNVEDRRUkkD6wykGNguBWuSCQa0oR86+VBR25mt49M7O3V11vnZfXtFgO/V2bBuvL7q2dhN19xbB25tirpNxwZ7Z1HFuTD7267j3Hht3U+SWCpkoaTd2PWms81Jqf2R3cNjzFdWu47VuNybjbDI0K28jRWszvVDHI5jkhm0PE0bFQ7QNqwr06VwySWOpLm2iKzLRhINTKKV1BQ6sp7gy1oGoOK1qncRWYCpqNr13Ye7MhvDpbrvf822abZ9HksPiuzsntPPS5fdtXXYHZMmapKjD4Pds2KjiyuQXISJi62uEccskxi1qLhLtRew7TYpBzLeWnjNcFWa3WRAkQDzaCHeINVFKguqZAFaNI0ZMRuJS9lHJoCVAcqasaLXAanca4J9emnP57dW3uxpMim58xidzYKWjw2FyMeY3VJldo4WhwsGHxm0sfX7phpN3R0GxtsTLhUhnijkjpqUxqugqS9Y2e27psCxS7bFLYzgyyROkJSZjIXMrCItCTPIPFqCQSwJNa9PSvcWW4Ex3jJPGQqyIZAUGkDSNYWQaFOkgjyI4dCvlpfj7Q7J6+ye3KPb+2t/bMXMvmZ8zubdfZ23e79x7Jy2ClwNDnOuKva2BpOsMD2vBlZjDC1fUY+Ohw1VDK6tUppJIf63z7puMd40rbLdRxIkSJHBLZ+MsniutyJX8doNIBAQNqdSvwmq24/csNnHDBRtxhnkJuAzNFOilfDXwWRTHqqTUngCCM4fcFhOzfkpNhtvbez2P7L7DwXXO691UlDujc2c2mfjl090TJvHdcnWmwc5vrctBsODrxcBlZs3QYygMoxCRpTRPDKKjVbf8AmSw5QS2v+ZLi8h2IXFts8GlPqheT3zQwwtJHDFJcKyTEx1OlG1szBgVozYWM25Ga32+CJr3S90zV8MxJCHZwpZljIK93mRpFCKHp7/0Vdo9e9A7D+VOGye3tx7Y7y3zm9mU3ZNHS5Gq390t3j1Fuyh34cDQ7zqWpMptTsvcOEp6XNnJ4x54q3CVbRfceUyBPWu6bXu/Nm9ci3m03Vo+0RRtHBJ4Ys9ws7m38JmSJCyy20Ds0JSQLplWunTprSaKaKytd3S9jmlumYyMCxmhkR9Q1sch5ANQYHIrnqBvHH9QZPe+czXWOX33het8pvtKPbe0u18liN5d9Umz5cbQ5HN703dntp7f2p1xuXIyZiSuSNaP7OWWQR+WJR5JyNWkuUlltLTayY47XxIpiyJAZASiW5oWlQ0CksIyiocEt29FSLEYo5Z7tRI02l4wCZAlKtKK0RhxAGqpPGgz0Lv8AHusP7l/3WtVfd/3c/wBFf8Z/0Nde/wAU/wBH/wDp+/0xf6Vf7wfx/wDjn+mn+Cf7gfLr+9/g/wDuF/iX8I/b9l/jc5/UV/d21/SfTeJ/uRNr8fwKeB/YafC+p/0b/fP+g+Jnp/Rsnh/7mXnjeNp/s00+Fr/tfjrr8L/Q/wDfn49PSJ627s6n2VTfJzcHXEef6DzW+/jhQ9W9X4tKRO+W3PWbnpcHtfvPZ+X3HumGgxOztv8AbuINZkBl3oJ63ACOODGzxOGM4Mn5Z5kuk5TteY9yi3lrbdZL25mWNbFVVZJJbJhFGzs72alY6BqTEapF7qqYtfWHiXz2FsbVHgWNE1tKa6QJO5gMSkE5HaDQYFCEbUvXG6cx1Hjpeuc70HtbZXXm3KDuvfeCrd6b+zu+axsjkp27wi2xn8hgqjb53fSZKgxkWOw9UMakUf3UburOhO5bjc7K03hod2g3Pcrm6lG228vhwJGVUf4o0kayajEUZmZxr/CQDQ9NwWguWVxaSRWsESyXUi1YhWIUS6TSgYsAKGma1pjoznzo7C+KO/didDbe+MO6spuPGdN1G7OtcY/Ze158N3tJ1ecNtfce3DuzN7fxNH1zmuvcFvbLZ3G7fgSpqNw0rpVy1f7NREQF/bjk/eeXdy5133dpxG+9XUd3JYRliiTqgSW5ILyIktwAuoRsEKolVDAjoy5h3Wz3C22extUdmtIjD4zaaFNRZI1oiuQlTl6mtaYJJBGffm/utviEOscPtrEUnVPys3Pg957r3hmabadRvbLb9+OW6tw0Cbf2lkdv52Xc+L6vpKHdWNmlotx0CPNmVqKigZImlMwm27c4Nx5u5k22LeZfrtsWBbmxjWQQmG5i8S2eRpYQhnDiY1t5KaCizAkKFKrmye32zb7t7YeBca/ClJXVqjYLIFCtqCUKf2i5NSnnXP1L3P0vs/ofvfZO4uvIsb2puzprPdc7I3dtl8rWV/ZOZ3r2rsLcs+W7Lk3JXZ/be18d05s/bNTTYdMDjsXUZYZGSOrqHmEE1Ol5t2Lcd73r2+ltbZDYbduj7hdTmZ0ePRbSxxBYloJxI8hUhm0phyGppZza71LO03xfHpNcW6wJGUVgwLqzdxr4ZXSDUZIqKitQcf47bI+W+z+kepu29sZDpLZfVm25NndpY+jrt09Mbq7N77xI37unrrE02H2v2jJujbc27uq33Pk/t8JXrQUmKWtirqqm1LEyxnzSOQZOaeZLi9a6ueYEgkt+7x0hsRNHE0lI7cxzSJdtBG0roskhRDRhGSSJrGXe7jZttsLeGKKx1glwBruCrMVrI9UUwh2CiqqCwBGqg6KnsfAbq3p8Pdzbuodz9G7E2F0f2fU5+t2hu7bWZ2Ru/wCW1TW1W2dwQ7Ur9+UmN/uP3tuzp6OvjbD7NaopMnhcJmslUwAQTjySFve+2qc6bNylJsc824TbdNINzs2heSxErCLU8Zc3UMUxjOmfQY9cYQksDpDlpayJt0u7+OPAW5VfAlVvDlMYD6S1NDMNXwVrpJOKrqDSg3nhe8WxnT248t1D8adiVu8+2e26nea7PzFTt5exM7tqU7WwObr8LSZ3eO19mCiwlLtvHw41JcZRSVQraiilmaSb3qbZpeUFm5os4N033eY7K02wW/jr4r28co8R0SRo7eS4JdpnZyrsBoWQKFXp+W//AHvL9FILWys5LmS5JRKRo7igFQDIsSgBQq1A46ST0KmA7N+SR7W+MXeWw9rdDfFHfmC6h3jXdNdmba2V1h0psrsLFbBTsmj3dvvc1PuBMrsLc3ZWWllye3Y5J6CA5CpipKOmp/KInJXeWvJseyc58ubhfbpvtku4QRblZM9ze3Fu9z9MYYlEdJ0gRWSZqMdCl3ZtIbrUX7ya52u9jigtZGidoJaJGjhNYZjWq6iQVyAK0+3oHarsHKVs1LUda7/7K7E7Z+RWwt24f5Q47fGFw8O3tz7g3HuGoy1Ft3D01XW1T7uqcFS4akzi5fIiM02fip56GOGSm5PYNjiZim+bFY2uy7NeRybC9s7NJGkcQRpSQq+DrDvEY0rWIurllbpG9y1a2t3JJcXMZF0HFAzE100NdRBAIY1zQihqAMuy9yZXdXSnyc+SOM+QuRh+SGU2bN1l2B09t3Ye0cFia34z7s/uRsLeG8t2bs3XPisDkcZuJcrTYijxG0KSv3bBWRmrmSGi81TCVC6uOSeYuS+TNo2GOLku6aeI3s0s0sv1DRz3C28KIkpUkxs7yXDxRaO1HMmlGMLqVuYot53rcrppN3RY3pGiImkFI9T5UU0mg0AtqpUEElXHZO7e9N9di7a6iy3yHwPU22sF8Vo9k7qX5Edh7x3X1j15szrTY256pNnbg2rvPD5Wu2/u1c7XTw4DbWMxlacDkM3FDjT4HIUo3Xa+Uf3ad+uOVJby/XfTLYS7dbpFcyyzzxt4kM1swrA6qDLNJJGsqxlp8ipWbdfbzYzyW9juUaRPYlbhJmDxqgQoQ8cop4qV7VUMyVGivQR7S+TMG1viZ/oMx/V+Kye68f2b2bnl3/uzEY/fG2sb133n0/F1jurbn91t1UeWxG1uzsVlsJS5PbO58bHQ5TFTxzvBL5ixIzi5cuLb3Fu+b4ri0Fpd7Ku2zRGIfUNJDcGaJ1mqKwqkkgKEEhmDA0AAJGv1k2GPam8fXHdmdO79IBk0tVKV8QlVzWlBSlemj479nbyxuzO6uipOwNsbf6K7O23D2N3B11vPeE2wcP3BmekcXns31ftjH7txu3twZ9d3UG6cwtficXT/AG9PmK+ljhqpAio6Nc6L4H9X9zt7DcJ91jv4rW1exjNwLY3TrFLdTW7SxRGJISyvMQzwxu5QdzA72iMTm8gknt44BC8r+O2jX4alljRwrNrZqaVFAzAAnpu+K3d0HQ+U7n3HFkNy0G894/HjsDqrreXbW1cTnKyfe3YmR2rh2irctUZrDZ/rumXawycseb2+82airI4aOJPBV1DKo515K2Xnnb9t27fmb6G03C33PQKFJHtWLrHMjfpyQk/ErhlqA2nUoI9sm9XOx3Nzc2kKvNLbyWwJLKU8UULoyEMHXyoc5Bwem7pCau2r2z0puPqbqrbHcm/f43Bsybpju3bW3+zdt9gdr56PNYJKAdYoMNPktrS0eaoRQR18jVMWcp3d5bKkat8yzQSbHzNDzDvku3bQkJvDuVg8lu0FrGFcsbk6gsoKOX00BiIxkk7s7aRXsLqzgjllaXwPp5irFpSD/oWD4dGABP4gc46lQd1YzBdGdd9S7kwe795b36j+Q2U37Q7f7OzkO4uktvbASjpXz3Wm2djTR02e2XVb+3zHUT7yGOrqSkztPS0XmDT0sUkdbrlx9x3jdt1sr5LWx3DaTatc2A8O6aV8R3Jlo0cjW8VPp2dXMZZqAKzBm4b0WqW8U1uJZoLgSeHPmPSpq0ZFQQrt8YBFfWtKIvesG5sltzfWSyWwNjbApaTt6vzOW25j9pz7d3dtHJbvo5JqLY+PGVSo3DjOtcNTQf7jsVVTt4pVaW7sWYv7O1hZ3myWMO83l9OdrWKO5llEkc6wEK07lNMb3UhILuqitaUAoOlNzZXV1tu5bx9NBDbJeBXhQFWRpQWVVU1IiUAhQT5eZB6ROI/vfu3bdRshN4TU2zNstnN70u2c9uqqo9p0OcrcdSUeVyuD2/U1RxS7rzePxEEEk8EKVFRFTRpLJoRADi9k2/bbqLcW28vfzslsZYYtUhXUSodwNQiRnJyaAkkCp6RWFncbis9vHdRxxQxvORNIEXtGQoPGRgKAAVNOjW99fOzeHeuS6RZ9mYjZ22Oisfus4vbmG3Bk4andu6ewMfg8Pvrf+88vgKXasJ3fvDbu0cPjshJj6KgpaqjxUKSQteYyBnl7kZth5auuWDvk81k8rSW4dQyWwaQylLdZjMwjEhLAO76Se0ig6Wzb+LjeYt6uduilkXT4scmBLpQIPEKaM6QMgCtM16y9b9sbF330xt74k4fqbsXbmV3fWZTPZir6fr8Vv/cPyU+V0OZ3Xh/idPldrb1xTVvW2zNh4Xs3I7aqsVtKuDZ8VMNTPDNWRwtHfd05z2ee83ix5i26TZPrLWa4h3WMwpZbdDHTcGing7prmQKZYzNSNDVSQo6YtG2i6Hg3NnOtyYpRE1qQ3iXDtWAOr4WJfhbTViKHj0htx7Uy+xewux8NUdadj7Dx2z9w5jr7d+wN25bIT7l2RnInr8cNkdjbjoNubZp3ytPuXb87mmqMdSfdmidEiLRFgKNuul3Ha9oJ3uzuL+aNbqC5hjASVAVLSwQtLIwHhyBah20FwSaGhQaYra7mkmsJjaCqPF4hVqsp0hpAlKagG+HuAoPXozeXy20+q6bN9dZDpSsyW0+0NjdJ5/bG5u15scvd+wsdQmg3HvLL9UZ/aE9Ps3DUnZeejr6FXyuKyc64EQJJGKlXlcg2A7nzTDHvVvzXbjetuvdwtLiPbVk+glkq0cCXcUxE8rW0RjZvDkRTNrKtoIAW7raxbJcQ2V9s8wsrm3t7mM3DILgIwDO0TpVFErhgupSQtNQrXpb4vYPW256HpvN4fsLeO3+uqDB4DAd2bv7BpYMriesOzclW7yy+R2zsXAbZlbN5PaO4sfhop6N4YGjWavtV1CN5PGYtv+6bbe7/ALbcbPazcwSPJc7Xa21VN3aReAglnkceGskTSaWBYMQp8NCKEoI7CKe3tLyO5kXb00xXMzkUikbW2hADqKsFwQCBXJ40bcrk9u73p07Qqtv7b2NnKvtPERZyDGYfDY7rGmw1dFLPBTbR6nw+MNRLh9uU+LDZSBXqNflVCzvVBQZXlxu67vuW1iUT2Em2ySQQ24eO4WRSFOu6MgSMyl6QkBSKFsaCx1ClgNrs70W7pepeKsksul4GSlQqw6SWK0q4JIIx+KgF/AdT4zNVXU+S2tT9O4qt7FbsjY+Ype3uwqDaeE3HSYylyecpu76xt74TZm2+g9rbx25lVxOyWkr6yonzOFrXpykqJGyCwW/3K33KCfmRjIlykkMdoVEtk0Udvqsp3WWX61llq87HSGWQRsKEE3uTBDJaSptWnWh1mWuidXZ6TxqVTwFK9qAVoVLA9MUeL20Dm/kZF0vt9vj5nd+7q63211jN3NTVW4tpbsrNpNuLDYyaCoyx7XzWJ23iq+KojztTjTi6qQfamqFUjQoqbZ+aG5a2/Y/66v8A1niWE3G7/SQj6jQymVvpgTFF4wBBVTReIBHTlvf7LFu1xuEnL6ybTIJBHYmaQeGWUhP1aa28OtQTxHHPWel73rN0ba2nszvDBVHb2z+qemewuq+iMFTZnH9df6LMvvGvzO5cFvGfKba2xNlN/Um09852oykmLy0kv8SVzStVQwhQp1Y7Dte1Xu77jttt4N5fTLcXj6nbxGVdINGYqnaKdoA+XRTLdTzxW8U7644lKRigGmtPQAnh516hdP4g5Wkz6b0qNiU/V7be7SWgqu2c32Bg9gUvbEPWOUqMDVYRuuWfKN2jFTLC2ChqkOIqq1YIq7XBrQhDnW8hs7uwfZ4r1+bBLZ+Im1RWkl21gbxVkWT6qiiyLkiZkPiIpLJQ56O9ot7meznW6kjXZCZKG5d1hFwIsFdH+jBPhBGRgVag6DPId359ct0nujZm09g9S766MpsLPt/fvVu3p9q7q3Fu3be5hujbnYW8ZGyNfjKvfGDrIKaOGppaajiZKVGkieQu7HdnyhbQf1vh3Dedw3HbN4kYyWe4TCWG3ieLwpLe2AVXSCQVJDMxqTQjosut3kuItpVLG2gmtF0rLBEqPIQQweUj43BAoSPXyoA67474qt9bGzGNyWFzDdq9h9p7r7V797ard85qvi73y2YyZ3BtePdOwJqcbfwmT2TuHLZuojyOOeGSuXMSrNECqFUm28nzbfzGm5PuUT8vWlhFY7PtotkV7DSvhztHd6jJKtxGsQKSKdHhgqxqa3k3CKXbmtltnF7LOZrm4MnbKOKJ4IUBNDFjqBzWlB11vGu6c7T7Y2/4tx9r7a2LmNiYulraebauH3DlNn9oNsioq26x6u21V9iywQ9F0fbM64XbctdmRkKHbcoqqmF6pHhcw3Nt62DlottEcV9uVssKlr+YwiSJXjWeeeaOF/1lgDynTFR3AUBQ1QxbJaXm4KLxmgtpC39iurSxBKIiFh2FqKKtgGvz6KtL1fvGr39Wdcf3Rzmc3hgNwZTDbh2Ltpfutwl9rVFaN5UWPqqOmyuOilxUeMqEao/fiVrSKJV+u9y5k2i35fXmJt3t7faZoElgvrrthHjBfAZwzRuQ5de3tJGCVPT+27Tf3u5rtdvYST3yuQ9tACZCI6mXSQGUaQpzn1AI6DjY/V24u0uwslj+scNl4Y9v0W5+ycg8ebwtPufaPWuw1k3LuXcIy9bNtunyu4Nn7cpGqNNJHHV1dXCPt6cuRGCfmfmPbuVtksbjmi+iElzNb7YjCKUxTXl0ywQxhFEzRxzzMFGslUB73oCelu3bbcbte3CbVA5jjSS5ILrrSGIF2YsdAZkQVwAWI7VrjpX9k9i/H3ZnZPyQxPRGzMt3psLsWo37sjrrtD5O3y3ZOMwGXz21sltjt3b1HtWHaZwfcMmQxOTMlfXrUx1VDlIkloKeZKlZibatr5mvtt5bn5ivo7C7tkgnns9rGiPxEWUSwSM7zK9uUaMCNfgZGIlcFCjs09kklylnC8jOzqJJiGqp06GUaUYOCGJYnuBXtWjBg97d2HFsjdu4+udobJ7dwVfgNv7Ry2+8TvbJ4jLZiimpNmYTLbyny1BsajGBGzqLdtXNXYurndnosbJClU33AaQ35V3tt72qx3++3fbZ7WeaeOzls0kSNlNxIkGlp28TxjAFSRQKNIHKdhA6W73to2m6uNoO23MO4ReG0wndWKjwlZwVjXTp8QllbVhCoOanoYestxYn41YrafcOd6q7oxE3amz6Dbu3cNnn20vVXyM6QzM26evvlniE3nk9pU26NmUm+8JKmEw1Xt+nqcnt55p6lMgaj7WVG7i65o3DdLnbNl33axZpFdx3kwRzd2ssiJ9B4cReSCXwz4pmMhUOQqqq0cdJ402yG08e7tbn6otEYUqoikUEmfW1A6lhp0aQaAkkmo6CTbnf1d112VtDsPqDbadaJ1p3me7uusHR7s3Pmv7sy47cNLmtp7Zq8nX1sb5j+7OMoIMd/FpYVyNVTx6pGBJBO7XaLyINNcbxJJuT2SWrXCxxIwdVIadBpIUs5L6MoD5dMTX9vJbQ20W2xIEneUvqcsytSkbGoqqgUB+LpZdwd4bn7i7IrvkfsOhxHQtftTH7X23gdr9bbwmwVZs+lxmLqsdRDriTH02D3FQ4CkxbGEB6mrrVQuJKqoLtYg2Ll+w5es25V3HxdxW9nuLyae5jaRZHlk8R/qGkaRTIztXgq8KKtBUwuZLzc4W3qOeKIWqxWyxh1WQKqFVMaqFJVVXPmPU9An1bS5R91PXYfHbOyk+F2/ufM1NFv3FUuZ2rLj6fCVtNWzZHG1sM9JUz0cVZ56V3AEFZHHMGDRg+xDzDNbRbekd1NcxpLcQwq1oxSXW0i6QrKQQCRRqcVJHn0j2awudwu5UtvB1RQSTv4/waEQlq4IrThXFaHoe+l+59udWdgdCZvsrqfKbd2315trelRLunp8f6Oe+98rvak3HU7J7NxXYW7INwYyh3jsXcdXSSbfz+Ooad6SloCKd/OqyqGd35YutytubDtHMr3F1e3FuRbXziaytjb+GstusMXhuIp0UmaJ3bUzmoCmnTsW4xIu2R3G2xxxwxODJEumWXxCxV2ZiQWQmisAKAYznpHZWq7IzXS/X+H3T11smiwW/O1+0uwcB8iM/t+Kg7K7L3Bj8VgMXv/aeZ7bydfJU5/ae2Kx4apKCeFTHmcm8rSSGYKDGG42S35g3j6Ddp5L2xs7a3uNpgbXFbpK0ht5BbIvZJKFI1A/2aUAABrqOzvbiCzV4I0iuJJGiuZjo1lB3gyMaUUnh5sQM46WuG7k2lg/jj8kOioKnsig2n2Hv7rLsTovDZ3bO3d1Us1bsnc2Vx2f8A7z7pqMnhqTYeUh2XlX82Q2ti5JczXwrQ1oWlWMwtLyfZXvNGw87bjKg5rsLCSwlNoNEcgn0Mwc18Vo0ZdUUchdVLFlAarHf74kh2m92WGCu3zTrOjSMxZNFR2oCItTCgZtIYUpWhI6b+neyN3dUdK91bh6z33tfYe6d7Y6u6J7Hx8u7Jv799pdG9u4GWn3LsnB9dVe367D1e1sXk9uJWZPPxV1Lk6KWeCnjUxuxPt3U3fN2wbdd2V/LY+C97DNBGVtre4tnUDx7lJUcPOkulICjRyKrluHVLaNV2q9u0ngWVXWJo3asjpIGzHGVIIQrVn1AqSAOPTx8OPkfS/GvsfG7rzPWGJ7O2vhMrUb+qsPFiqWi3jHuLbPW/ZW0tlLRdjUKUu89ndeU+f7BjrtyUWOr6KHLRUNOs7FoYSHPcHl2Xm/lDdeV4rm3hF68EbvcxiVPDW4iklUIcM7RowQEEaiCRQdU2W+O2blb7gpkDxBmUwnSwJUgGtRQVOT5D14Fp2dP2DtP4rb93psnuzZe26fI9x4DZG9uqsJkanF99VuPq9nV+TxfYMNWmPpKvJdOZDIwviamkhykpOWjjappljZZCj3bb9g3LnrY7feOXZ7i8isJJ7K7lQyWSMsqBk0ktGl2oIdHKBtBYIxoR0ustw3a22DcreyvUjspJ4/qEUqJWqrBaNiQxHIZQdNaah0abaMOU7s3l8tcN8g/kPu/pXo7f2F657f7N7Xqvv+9sPuveO16qfZ3Te8c/V7tmwvfXZ2xM9nd25Wihqdo0lfLTTZKNqil/hlH54Q7ec0bny7snJdhytskN/ut3fPA+3SgWsgRI5riZVMKS2lvdQrRitxJErgMNZlYKzybVb3VzvMt7dFIIIVZZozrQlnSNT3FZXjOQCisQaCgXIKMndvZWbwMGJ37nMzR9Tb2qutuvOwKjZeL21hdzZ/YvUEsGWi2XRTJFQQ5YYajz8WV+zrw2PrMxT4+oqNUlLEUFa8nbDY3L3m0bdE2/W7XV7aG6aSRI7m8BVpslzGX0lNSUZY2kVaB2qkud73O/WJL+4P0hjit28NVUmOD4UoAobSGrniaE8OhM3hvHtre3W21epdndup3B8cOsfko+1/jt1lvWHZGJ7Pyuc3TjRHtzM1HWYep3xDszcODx8ONrInyVRgaXI1TU6eKacsSfbotk2vdbvd945efbebLrZfrd3vLbxns41jYCWP6vSsBmR2LjtErIuuhVerPHdXFtFFb3iTWaXQgt4mKiVmYdp8M0fwzwqe0MaYJ6fN69jZrAdp5f5J5zGfHbqbvHYveOQ60q/hnsDo6l2rtfD4HDYPOU/YeZy+3IsbkNj4ja332Tm20JJa/Ibkmr5JJ4JKf7GnqPaey2uy3zZYuTrdt3vuU77ao9xTmOe8Zmd5JEa3jikEi3BlognICJAE0q2rxGTp5p7jb7xtxYW8O5wXDW5sxEMaQRIWUhkpnRUksWyCNNQpPibQ7j7I3zHubryX48dY1Xx+2DksrL1pufbu6N75T5XYqbPZPc1P0nVdOYOmz+6fkbBnBjYqDPUL+KnpNtwyVldL4omtbmrcLbkeFNy3K0vt4ju9ztpNV1JbpbbeVMUJuDNO0UNrGmoyKtdUkh0Rip6vbGTeja2NvDDatDbvFW3RjLPXW/eq1aRsUJHwqK0PDoUPiBB8ie1esmwvSWT6fxmM2ln+2tzbi677CTpzb+K7ZHbFV1nsjMdM9fSTYp+w8pSZ3F5WkpqvG1tXHSUkCxT46ZTBKVJvciHlA7lepzSk6lYrW8hu7Z543tGtnmeK6LGRYWeGSrRpGHfSJDIhTUelvLUm62y29xtqxurM8LwzBXWYME1w6QC4V1IDMdIrpCtWnQfbQ7D2J0fuT5ydb/ACV68oN07/3DujYsOK2RjNwPubrDL9hdRfILD7p3l1LufeG18y26m2BvbakdfjI87g9xUtXAsICSPJIjRHkmwTbjeez2/wCwgXG17WZDI0ztAxt7ixaHx9CKscragv6ZQCr61I00ZA25MF5qtrgrE94QWRV1gOkusRqWqygE8dXAEGpx0HXxO7W7M2J3FujA9K7K2Jm8/wDJ7ZG9vi+2w930mNzG102h3tmMNR1WJxLb6z+NwCZjbzY+l/gtbn62Shp6qninrfKFa4s5vvLTa+XN23rct6uLHaLCF768mtlZmMECtJIjLHFNOUYDuEK+NQfpkNnoq221kvL6zs7e2Sa7mkWGFHIA1uQFNWZUrn8R0/xY6k/HrC9T7U+YPXVP2jXbawXSmyu8JRumq73xGf3rtmk2hs3M5Vqaj7XwfT1JuTK7r+6lxdPS5CDBR1lHVVcl0L0ZZ/be4We482ci3VrY7y1jum5bWFjvrTWhieeEHxYdaiZB3HSSFlUEHtcYct5LfbN4ikurYzW1vcd8JKVKoxBBqHjLVHmGQniCvRlfmVm/jL252PSd6/HreHdXYeU3iMb2F8lNs9x4DB4AYrfGbkx9VvKoxO5tlVGN27Ht2vzczYKnSjxVNWU1PTrUmRtSqoV9s9p3vk7Yds5G3XbbSw2+2tY9v2h4H1FjFEdSJG7TSPGmkyo8spdwaOiNjo25gdN7u9z36zaWZ9Zub0twRXk0qzMFQBiSEYItAfhJGelRh+2+uqfYHzg67pdvZz49dfdvV/W3YHS/xMj27mOyMLSdkbYzUlJtefcXdW66nCdo7dTqrZO48jkcaatJMZuKTJmOqpZEhg1nH7g3O53L273dL+HdL+y8eC/3xHjiLQMv6kcdsniQMtxIgRyh8SIxijAklSAzxRx7vbNE8CSBWhtmDGj4ozMQrAqACKgKwY4OAUF/e/45/wAd+8/2XTcH8B/uZ/d3+7/+n/cf3H+kP/R1/Av74/xX+7nm8H+kr/fz/wAI0aPtf9x2rxfu+3/6ue5/0Hgf66Ft+8PrPqPqP3PBT6T6zxvp/D8alfov8W8Xjq/W+LHSj94cteNr/q2/heH4ej6uT+08PTrrStfE/U01p+GmnHRW67bW8uztg95fISpwe2N0wZDsvaGAyNdk96YjF9mYrefY2Sy25aJtpdZ4mq29LvekzuOx0uPyVYmGegoQfLFFBLq8asy2mxX3LXLy38sCW9nI7IkVbeWOGNYyZJpBI0IjY61AlBrRXZgRWyhr8X00VkJJJ5VWLuJkRmaoVFXSJCw7TVc5KgGtJXyX637C2T25uvrTc/bm2fktX9PbE2Fg8p2h1Ju3cvaHW+K2VQbV22cTtvD7zyOPoZ49rdZSbhg247eKDG0eQpzT07EaCzuwzctQbdZ3uzW0FlabncPcxxNGts8tzPqllJiZUZriQq7vgu1GarLnqt/HujTzW92kjTWkYikpqbQkZCgsakBQWAHADAoD0CW55dwZiipuwdw1OElgys7bYjlxx2piq1DsTbu3aBDW7M22lDW4mjjwdRRLHkpqCGLMVCVDrNU1UdWymtmtpaySbXapKGjHjnX4rL+vJI2JpKqx1hqoGJjXSNKqUHSZ2kkVbiQrntxpHwgDKilMUzTOck16X29PjZ251ziN153sXbGP2Gdqbe6k3PkMNuLd+x6Hd+V2/wB60OQyXVea21tFty/3h3bhczQ4uWWvnxkFW2BRojkUpzNGGrt272O8273G1XSz28czQORqXS6MVcAMoJKkYxpYUINCD1WaBoHCTqVYrqFKHjw4Gg/bg+VekTsqPdGZo8jsDDz7WxG3uwd09cYLcW7954vDUu2tnZVs9WUW0Mxnux8rjqibrDb0VZl6p8pVRVNLHV42KYTiaKAou54LF9x22eeci/jWX6eMTMmtWCiWsQYLMFAU1ZW8M0IoTnyGdYJ/DStuSut9NdJqdPdQlamvmNXzp0K+4ertopvntHLdfbSznZHSvVG6s/T7j65w/bcW9N2xbfwuDpMPuTuOTsPYewxtibpSXfSQNS7whxsFNXxS0FE6XnFQAo+7X+1QbXs/MW+2FvzZeMLeHco4PCtZ5vFkaG2ginuGke4aAMRD4jGgkkXA09GZt4bp7i422xuH2uIeI0DvrkRdADyOyRhQgelW0gfCp9eklVZXcvdO+pt7drZPd+3+tN8d14+u7Q3jsDYNfnNo7K3Hv6sjbcGZ2r17R5LDbQqd9vtymqJ8dhVrqGqyMVMKdJki9SnG2WvLmwttmxwXECbhDYBIVlkRrprSAgFiWPjSRRu41Me0M2SGPSWdr+7jnumjc25mqxUERiVxUDA0B2AwONB6Dpu7Eze2MXtfGdOUvTWI2pvnrDfe/aHdvbmTG78P2t2BTx5zI0WL27v7Y2UztdtjZNTtqmRI5aKmhapp6iARvJqEpkY2rbb879uvMq843F7y9fQQGx23Tb/S24CCs0MqIJpfH+OrOR3GlRppeeeH6S2sv3akV5CzCaara3OpsMpNFoCBQD8IoAS2p12v0ns3M/HzsjvTdvyC6x2Tl9sbjo9k9bdESfxPc/cfbO7nGDzOSlj23iLDrrrXHbayVVUJurJl8bU5WjOORRUOGDl7v1/b8ybZy/Y8uXU8MsRuLrcMR20EfeijxGxNOXVQYV7gja+AoWFto2tJrqS6VSG0JHxdjg8K1VaH4qEVFOkD1x2xn+ql302CwHXm4V39sPO9f5mLsTr7bvYUFBiM4Imnyu14c/R1cu2d2UckCtTZOhMdXFyASDb3fmLliz5mXaEu7+/tzZXsV9E1hczWxZ4jUJMYmXxYG4PG1VYYPWrK/ksTP4cMT+IjRkSoHoGFKivBhxB9aenSm7B6gDrvXOdZ7M3LLsPpfbHUeP7hzmZ7D687NosR2FvbG0eFyOZw+6dhrQ4Su2ZvLfEdUMLTUgyFXjqa1PW1DzRvIbNzbsCX/Lu2TXzQ7nuwnbb7eeOWKSb6ZBJcUR41KeGh1EPpqCNNerLtd+9tf3ccGq1tSnjyIysqeIdKZDGuoimK/OnT/vJN1dl7SpflD2h/dnICr3FLtmmlgnas3B8gN/7a3Pidw78qOwjjt1zZ7Z+cTaO9oxJnjQ4/HZClo4aWjVatJJWD+3XO27Tu1z7e8vyXC3Edqt240kR2FvMkkNv9Ozw+DMvjWzfpa3dGYtJ2FR0rmjnntot6vY1MRk8MZzM6kM4ejalOlstQAigGcmN2tHt6LMdnQ9abonynxtyW5Nq70pcN1xFvLD7B212luzr/ACeY2lsZdu9wV0O+81TdT5HK5nar52sSqqauloKmqppXSrhMh7a20G3z7HZXV6t7zSll4RvrmJY5p4Y2gF1J+igjjMkmhzGulNdKDSuEhEk0N3cRxNHt3igmNWqFdg/hg1ILUAI1U4V4Vp0huuuqaXsmDGUtJ2d1bszdGX7R6+6zxe2+xtyZLaz5GHsKTLQv2NNnp9vS7P251t17PjIo9w1+QycU8Jr4Ggp5lEug4vrr6Cxv9weJ5Y4Iml8KBS8raVLFUUHvdqUUYzT7ekkaCV4ogdLMaFmPbk+eMU/PqJQdfbqxOe7NrMPuTHUdV0JLU5fJb52nXZ/OYD+NYHeuM2rgJdnb62Visvi6Wp3BuKpjn2/laqox2PrBErQ1SzyU8chbcbrYT2+zwXNmzJulIltpxGj6HiaR/FhmdGYIgIlRQ7rXKaQxDyW8qvcukgBg7i61IqGCjSyggEn4SSAfWtOmXA4ls3uDbG69/bnyOB2nursiDBbv7Hi8G7914dqitxOT3ruwbZfM0e4twZXE4jOHIo0slPHkqsGJKnzeQoujmsI5W2eKMgw26SeCkZCCIl0RUNFiP9mRoDVAAqApBOglyiJuFRRpGQOSCdYALVBq3BgdRFK8DUdDT2X0xs7ZWN+RWAwfenWG5sH1P2RtM9YTZzZWd2h258jtnbnrc7gcdvTYeLqcXmqnau38VtuGHM5zB5XJxrTPOhBmmRLh2x3tdy3DY7612y+MV1FPBKwcGC2MRDfroJNBldhoV1DEVKg6dRBlfbddbYl1t98IknQxzBaAyMHXGlwCdOk1K1pipoadIbeFNNQV2w+yN25DCdlYLtPapz2dxeC3LvugFBubGJmdp/3d37n87C+Xl3/iKjGUudq3gnyNLPHXRos4EksUNNtm+qi3rYtuSewv9uuRFFLPFbMWhfw5/Et44zo+ndXaBdQRwUYlaqGZ65hmt1sNzu4Fk227QkLG0iozxgoQ5NW8RG724gk4NDhP53ak+B6k2lvCTam2v4P2jl8jjdu7pqt54bPb3oc51QyU+/Up9o4Dc0WR2NtzcEu+MXpXcOFY5FqLXi6spBWKRLHbX31a3E9+fAXxAsMYVUZW8PR4lQ0jPHpbSysikOQyMQCCmeWyMMaW1syy6VEjOdRLjVqZKaQqNUdpDEEVDAY6WGK7ehz8HXO1KraXRex6DrKsg3Pt3eWc2Nns9WVtVtGgze5BtDeaY9dwRb3xHZ25TDS1FPksTUwfcNTJJPSUArHYLScqmzfmC/Xdd4u5dyXwZ7eO4SNUEpSLxbapiNu1tFVg0citQMQHl0AG9xvgvV2m3G3WVvDZisTCMsWIq5ExOoy+I/EMCBWmFr0qN19Z5uLrHr35Z4zceFq07j7V7UxW6NvdfbA3lszAdEdh7YzOO3Jg9pVG5YdtYbrHHZXdeCzBzuBwu3MhPU4jDU8byRwjQVO9i8aN77lubabv91WFvb28F9eyCb61TFRzrZ3lkeOgWVpe52Yk1BqSS8dHdb0TR+PM7yPFEugRHXgBRQKp4qFwBQDhQKHaNPv3umrzWOh3XFHmoNu5reu9MrvztKbFU/Ztds5chkMDSIN1ZKKh3J2NSUORnpcHjozUZPI1FRK8Z80rlmbyTZeTFs7uXbJHtJLqOztIrGy8Q2guSqSuxhQtFaF1DzytpjjAAY6QOl5e+5hpGLlRdxW7PJLcTkeMIQTGiiQhTKqdsaLVm4jNehBrcHl+sd4bj2B2/tXeu0d77Y29mNjbuwGexqT7twO5qTVLiMfNjd0TMmEpqeE00MqxCOWmguYFDE3MNqu9v5n2fbeYOUt0s7vY7m4S+tLi3ekMsTYdtcNPEJbU2ahmw/DoruPF2+4mtNxt5VulgMEiv3Op4rpDEgKUpSnAfD05bdpMnWT57HUG3sZv7OZ7bU2VkqKCmqMhX7WgxscmbzWZo6ai8UUE2Mx9JK9TrQRxwqS1l1AmN7JbRJt1zPuUu32NtdCEI7Kizl/0o42L1LK7sAlDUtTzp1uISK93EttDe3Vxb+JrSrND+NmAWgDqAdVcAfs6Wu+8PS5THjdOycmdxbVElTPnI8Vtip24+25pKySlxmZ3vhaCryW28HnN0hpTFFRTGmjgpwiEqtyn2qeOx3G72i7hljkVljs57uRHa4TTqZIGLGZ0hAGrxKsWYkknq25qs9pZXttcRMJFZ7i3t1ZRE4NNci0CBpKkjSAAooMdRdk5LrJsNvOj7G23vPcOarOv5sR1dX7Y3dSY+l252JSbgxVRQZ7eeJyOIzc+W2RR7cNbD/DaRaWV5ZA8ci2JCu/t95F1YybReW8VsLsSXqTRE64GQhkicFR4rPQ6ifSuBpZHFJavCVuIXaXwisbK1aODgsprRADgAetB5hzxe2tm1vXmc3Cu8qah3ptzPUlC2164SiTeeBzE9PFR5DZyR0YkppcA1PUz5MV0hRo5YfCFZX1MT7pvdvzRYbYdmaXYLq3ZxeRf8RpYgxdbjU1CswZBFoFQQ+qooQvisdtn2O8vv3mse6QSqv0z8ZkcgK0NBgx0YyajShWlPNe4ug2m1LJ21mdlxybFoeytqYOXrXbW7KqijnoIYqfO7j29X5rKy5rd2EodzYGmlgx+WBmeKueUBWEQAK7qfeUdOUbLff8Ad5JttxMNyuoEZg5rHDMkUYit5TBKymSIhQU05BY1eiXb5Fl3afbWFmtzEi20LsE0/FIjyOXkXxFBCMCSGJxQDpG47dHW2M7XO8cv1Udy9WLunMZRenq3fWfxkk206yrrpcPs6q7Gw1PTbkEmGp54EbIxRRz1T092VRIwBlfbVzLc8prs9nzX9NzT9LHE28LaxOPHUL4s4tHJhAlIY+GSQgbB7R0jhutsj3Y3ku0+JtXis4szK4/TJOmMzKA/YCO6lWpnieouzdnbFbbO917DoO0Zd9Z7rYbs+PcfX67Mrtr5PL4vdLJufIdtjK1/8bxmzqPZ2AzJhTHImS+/ihd1+3Prb3Pe7v661O03diu2W1+tnu5vBMsimRIzElsVUI0rPPHlqpRtIOqtKW+2uyFZrWZria2a4tREUIKpr1tIKkhVEbYw2CfSqfl3V1xNs3amD/0VRw7qwuG33S7g37Q75z8dTvTNbhyMNXsfO5Hb1VS1uFxcHXNAj0qUVGsSZWOXXUSI6j3b90c0pve7X68312iee0e32+S0iItooUK3USTKyySG8Yhy8mowkURSD1dbzaWsbSBtl/xxIplkuRM4MruwMUjIQVAgGAq0D1qxHTlBj9o7EwOyd31EG3u58DvzApS9hYCbb3YW25ep9yYnsSStqNhUG9qqkxG363f+4dibYpqwV2NfLUMGF3C8LotWjmnf3qOXc9e17dzCbDfY43uYfDMTsQ0csCSTW7gtJbpK4anaDIijVgqW7B4rOSG+vds+q2wyKkqnWgNGV2jWVcLIyAiuSFJNM16DbF7D7T7Cz3ae9vj51t2ScL1rgt19nblHXlPubcb9PdTUf3LZLK7s3NiYFq6Ha2EwrtFWVtS0SPTpIW9CsQgvrzY9s2zl/YeeN4sbi9vDFaL9YsSC9ul0CscDVUu0ukhVBCsyAZK1cWS6k3Dcd05ftp7W1jd5EELuTBE2qiGUUY9gINcsA2KA9NHa9NsX+4W6uzus+pKncewOx8B1/tLsDeW4us8rs7Y/xu+SGXq9z7sy/WHSWao+xN80+4MPk9m7Z+7x1fl56OvraU1SGhSOl8s5ElnHb7vyny3N7gXT77YQTXrWkkkH1G4Wq6bfxbtBGpeOKSVAXRUBkIqASADz95wvbb5eLytapa3nhwxuviFbWRdLv9OWeoMgBJVi2lTQGnEhE8QjkcMfoxDcXH5NrHj6+xi2Dg9BwksaDh0YCXqTuLY2zf8ATBusy7ZwO5MRsusgwWe30dr797j6x7HbcsUWV2ngf4hFunenWtdDsespMtXUyTUtEREJlvpAAMfNfKu9bu3K20OLm9t5biKSe3g8a2sLy0EJMVxKFMNvdj6lHjjcqzjUV86iA7ff2sS7jfKVjdY5PDkcpJPDJXK/iaMhaEjgM0NDRq6725vP5Mdw9cdXPuLcgp8/nU23hZ6yk3v2VTdZbHWeszWfylJt3b1FndzVO19kYCGrymRWgpQTTUs9VMFAlkUR/Spsm23k227WJr0RtK0Vuio9xKFrwAprkI+dK0FcDpDc3cu43YkurlgpIUNIxbQgoFWp8lWg8uGenSPfVJs2HbktH/oJ33L07nd5bH2fRT9dZqKs31jM5X7kzVL3JuDKU2J27FvaDBZWeL+CR5+ukraWNqSB6CaiikQEj7IdxfdI3fd7ZNzjiubh1uV0wNGscZtYVLyG3MiKTIYUCsdbeIJCD0rhvzZtZSpHayPaSERq0dfEqxfxHwBIAfhDk0FBQivTJt2XIdxdwHG4br7riTdfcFdJtDA7frsqNj7Lwm9t5mHGUO4sVmMru/am3dnz0mYm+4gny1f/AAKgaQtUxSQpp9nFns01jtm27XDvF2y27pSaRo2kkjQ4jmd42DKVwzAK7AVDqTXpq+3GO+v7q/NhDF4qktFEGCK5HcyLq7SWyBUqteBAp0nhR0OVyJ2XtXbtXjtw5TelViabJvuipy9RFg5Y4sW+2a6HEUyYfI0NNkYpKyTIwK7TRqVCtGFJ1KbmwSTct2v0ezgtdUkaxKq+KpLGZGZiykrRQhNBxrU9PIsV9cCx2axkWeecrEDIWfQwAETUCqwrktTPClB0LdNteiyPZHbOJzXc/StLTdI9Wb8pNoZ7csG8891/2zJsPHrtbE7E6jx+f2/lMnTbt3v/ABKoyOBWvpcXRUtakk6/aMEAI4bln2LYrmLY9yR9yu4J54lMUdzbGZhMWumgcKY4dIjlCs5ZOxjICa7n1Q7heI7Wwa3jaHgWjbQvhnQHr3NlgcUarKBjpq3901t3b9B0Xt7ZPZcvYHZXYuy6vdHYmwa7bJ2RiOndx1WWyEWD2bT723NnY8RvWryu1sbFk6yvgSiooZJkgVpZASDq23+wm2/cN3kikjtreWSJ3Cl9YjcqHRYtcjA14FQymopQVNbvaNxtbq22uZFE8iLKillFNahhViQBj50xXj0HuJxW6967Lz1Wu4q/JYbqDDU2Xo9p1X97swcRtrdW6IaLOZfAU1FicptzamBpNy5ammys9bU4uCaryEIQz1MwT2/PPYbZuVqv0aJcbhIY2uF8FNckcZZFkLOskrmNCECq5Co1dKivSBVluIJD4hKQioQ6jQM1CQKEKNRFakZI4k9L/F9GJLsnZPYW4e4+j9sYTf2zu5N24HB1u+p8rviOv6bqBRt1/uraO08BufM9f717Xr2EOzjmIKfH5RW+4knhp1Zxe13Rbzcd52pLS4imsxHqmmiZYZDKhdfBkNBNopR9Pwt2kjqjQiOO3mZ1ZHr2qe4aTQ6sdtfLjjPSE2NU7npBn6zYldurG7yi2zub7s4TJUWGpn60qtqZ+j7Px+ZrZa2jq548hgahKWSjjEsNZRTVUcis3jRq7sbDTZru0UL2LXEIQSqXP1PjR/TFRpYAiXIY00sFNRkh60SdzN9Jr8dY3ZtJA/TCN4lSSK9vl5io+XQ5Hq3ZHae89gdU9JZfZGZ3bRdWbQSh3NjaLe+08b3N2zuGoxu5t07Z3dN29nMVh+tsx19jM7XYKoydO9Nt3MnbCyUSlshE/si3zeDyRY7zzFvu63F1sBnE8p8IM1hB4IXTFHbwtPdL46g5VpAZSalE6VWVm28XFrY2cCpfFdCgtQSvqrVmdgsfZ86EigoSAA/zM3bHyOye691Y7CRZqk6h68r8vNisC0cW2OpOntsZpoqTC4CDKZWryMex9oV+51pqSH7nI1/hmGqSfl/byz8s8jQbVZXd8IZt0v1topJgTJd30sZNXKIF8aVYSzEhEqDheHWlg3HeGupoIdaWsBlcLwihVgMVNdKlwBxOfPpa743/AITZOC391f1NsvA4zqbuTD9S7xhqeyT1R3D3ltw4jA4yuyFDQ9vbRwmOfYcWX3pDXVMmGpqegydHjJ4aHIKZfuGndl2Xbt55i2vmcXm5Jc7Z49rHbiW4gtpGcaXeW3OiO5058NyGT8SliqkUjuJreymsTFAUm0yF9Ks4HkA1SV4ZHEZGKsDB+PXSWzu9cvvXbOe+QHV3Qm7cTs2s3D1ue4jkcHsXsvP4mQ5HMbIr+y4g2C6yyA2zRVdTj6rJrJBk8ktPQRhZZxIjnMu/X3L8Nld23Lt1uFk0wjuvo6PNCrUVZFg+Kca2AYLQqmpzXTQ1tbeO5d42uUik01TxMKx4kF+CYGDmpoPmA36z3Vt7Zu99rbu3X13t/tfbeIrTW5jrfeVfnsVgN2Us1HUU/wBhl8jtqvx+cpDTTVC1MbQzW+4gQSLJEXjZZzDtt/u+ybjtm175Ptm4TR6Ib+2WJ5IWqDqRJVeNqgaSCPhJoQaEVtJooLiGaa2WaEGrROSA1QRxGaitRxFRkEVBE7LbPKw7A3r1RS9qYzsPftJ232LkOutubB3RicP1n1pi9wZah2vmuquyaHcWX3N2Zs2bbOOzMGZyL0ePjwoxU1PUTVN53RM1xslvtMdjv29WlykDwWF1NetAokuiIhGsqmkS3E7ujrGACWddC5Xp1VvJb2Saxs5IywknjSHWSkfcWKnLlEUEFiTgGp49PFCu7u7Nm7dbH7ap8HL0DtWj29lu8VyFdtnrzZ3WkEWeyXX23N+1WF29UUmF3hubfVXkKbF7gqq/z5rI11JjEhiCLMxRcybPyru01td7kjvvc7SW+0vpe5uLgBBcvbrJKDJDDbhGkiRKRIrykmtA/FHebhbePBbsFs1USXS1CRoSfDEhUUVneoVie4kKOsudwWO2ZtPYG6+oUwlZiu3egMxjuwtsV249kdwdh7Dr9u59dpdvZvdu28ZtSjr/AI5UG6txYUVu1kqteYi2rVCc5Foa5gxxHbXbqh5p3K2aUbo8th9IZbVdGpxaQShp2+pmEeXGI5HAKxDQOkmqJiy7fby0FuBOZAHzQeI60X9NK4BOVHFs9ITYHXGZ7Dj3y+GqNsQDr7r3cXaO4Yt1bx2js2Ko2btGSgjz67fbducw7bv3asmUp/sdv4tKzMZMeU00DiCSwjTUHUgdvrWhB8qYz51zjHGvSFmXJYn5CmKedT/q/LoWNzdBdr9edpUnRnY2zW687OrKXadQdr7z3BtbbUFDj997boN2bUr8vuauzsO1cDj8vtrKU9Us9XXwJAkgWYxyAqCuz5l2a+2aTmPb7xrjaFMn6sEcsjMYnKPoiVDLIQ4IAVTq4rUZ6fe0njuBZyIEnx2sygCoqKsTpGPU4ODnrhJLubesOT3RkMdU5inweA2xj85XYja9HicZi8JjqLG7P2rFm4MDjMZh8dLWrRU1ItTVpHUZOvbXNLNVyu7GVuu3bS9rt0dwkU08sr28cspaSRyWmm8LxHZ301Zyq1EaYAVAAGpDcXEc9yIneJFXxGVaKq4RNekBV1GgBahZvMno/e6Oge0tz9j5KfcHaXT3yR3Z2B8WMV8ik7YPeFdLR7f23hNn4XJ1u2arc29KzbU+X716t21g127UbMrFrWiUosSNpieMGW258rbDY2e08vJJt207fvC2EllZWahXkn1yMpiEVYreaaUyNcRhNUqtpZgx1G91Bu1zPLuG623izXtqZ4J5ncAKhVQyMWPiNGihQjFgqEE0pgCP9JO4P4J/BfvKvx/6H/8ARV5ftcb4/wC4X+kD+/38I+3/AIB5fH91+zbz/wAV8n7/AN74/wDJPYr/AKu231n1WlNP70/eWnvr430v09dXi8dXfXT4en9Pwq/qdFX1y+B4Xht4n0vga6/h8bxK6dH8HZprWvfqr29F7wf+gnbmxabdVc2+d8duZzb2/sVhsNhZW69w3SO7KTK7Yn6r7Oh3ikWcftXGZTF/xP8AiO30hxZpZ/CWnYrYhTdoOe9236bbIIrCx5SgntJZLmYC8fcrd0mF/ZG3/S+hZH8Lw59UuoV7Ojeym2iytoL1ZZ5N2ZJAiRkxfTSKVMEyyDV4o4kpQU4V8+g62PsPsntjc+U23sCgyW6N2Vm2937rzdBHnMdiZsjtnZ+Iq95bxyGQq83lMVj66nx2LxMlY9M8ryVDwqIo3lCL7NOYN75a5Q2u13Lf7iO02mO5t7OFzE8gSa4kW2t0RYkdlLySBAwACgkswFT0ns7bdd6vJ47MPNevHJNJVwCyxqZJGZnZQ1FXUQTU0wCaDoQOncPuDd+6qHozZ2F2137T9l7fzeV2lsjJdg5Hq7ZWE7Yy3V2SlpOwTmt05zrvBp2B1DiIaqNI8pUjDZGopjSg1Ucsayt3m13e6yWt/bvNtW7wXQjeXw7aWWa1huNT25LeKq294q1qpWVVIPa+A2JobQPDIVubZ4tQCs6qkjphuCkvETQggqc0JFD0H/WWBz8mA3/23hNo7r3nS9R7f27X1G4T1lj+yer9rU2/MmNjw1HcVVuQVGN2XhMhiKqoTb0r01SXzlNTxokHiE8T28zW8lztezyXkMIvJH7BcNb3LCIeL/iwjo0hD6fFGpR4bGpNdJbtwVWa4WNmMYAqUDpVqjvrw7a6ccR5cekrtfB1GYz2A2LVb1w+yNu7z3DsvD7i3XuTMZaTrvblLlK+GloN39izbYpM9UyYrZVNk566s0UVbkaOGOpENO04aNjfw7eaaG4eFPqI9axu60dQaCTQSNQVqCunDADiKdNl5UidFkbwmprUHDUrpqAaEippXhnhnoyPUNZgOrtnbk39mtx7T7DwXWnd2Ehbopdp70wm3/lb1800eJ3rWVfeOKxeIrZOm8RkcDg5JtqZDyiq/iCTtRwSyuJAHzVZHd94tdogj8O9ltm8Hci6y/RTJqaJo7RzRZ5I2lAnXw5AooHNO032wzxWV1dqGa0jI8aNe3WjkL3OMlA+nsoyk8R6pDbIp+3dqfKEL2BQ9OUmOY/IbaHx8xOVfbvSW6q6i3PUUOd25gaXce6dMG5+udm7m8G0qNYsnlq+ljenWQaGYs75K3LG/e3FwnKx3N7h22G63vw/Fv7VJIvEidzFAT9NcXEI+pctHFGdLkGoAe2+Ndy2/f0bdPpzEovYrMsFhlKtpcDU4HipG/6YAZmyBTosLHyerUzufWzOzPI5e7FpGcl2dzySxJJ+vuSKUxTHl0QjqP6CSdI1W8bHT6rXvoJte1ze3veevUHp1EnKQEMzrGjOqIWYL62uVQEkXY6Tb/W966ZYaTjoYK3YVFjfjziN/wCa2Hvymrd/9m5DA9d9mpm8VD1fmdtbLwF+w9of3eWifOVm8qDOZ/GVEVd54qSKnLoEkfkA6HfZLzn672Cy36we2sdrWfcNt8NzexzXMv8Aik/jaxEtu8UMqlNJctpbUBgmz2kcWyRXktrKJZZysU2pfDKIveummrWHIoTgioGQeh4z/aWQ+R+wu49/bnlzGN79291Z1Z1zjNv9F7O6+6/62390h1MyZPsfdfyPx2KrMNkshlsDR4fbRoKugpJ46ysx9MksCiliaMpj2uLlbdtlsISsmwTXs13r3F5JZILmdPBt4rBipVNdZS4buIkkcuWdtT5eS/sbm7LKt0irAY4SFLopMjvKvEqO0AjAKqoWgFC1br2Lt6CcZnrjP7m3z13i8T1fTby7FzXXuQ2fjtl7837t77/ObOyVHSZTdkstDhNw4vL0WMrklE24KXEyVUFJGSYFH017bQzw2ZnX62WN5IYCyh5BHp8QopIqELqCeA1LUivRIsUjI0uk+CpCs+aDVWlftoaD5HpU5bZm9twfHXF9uZfFZDObK2V2lT9A7f31XdmbbmpMDT1O2c72TTdY4fp2qVd90uMmq8pXZoZ9AuJWWplo2QVLsQRW93t9tzTc7PbzRx3lxafvGa2W3cM7B0gNw1yD4LEKix+Hl6BWrpoOlTpLJYJO6MyJJ4KyFxQChbQE4jJLV4ZIpWvUXeDwY/aPx82flt09S1u1ana+Q3hlsx07gaWu7O2zjt6dgZKDM7N72rZcZtSq3Z2Ps2Paq5DD4aprqujx2Lr6VIayMzyLCoG0NY3u/wC9WU89xuV1Ghjtrq4k+mR4Y2RBChEi2olr+s0aEue5lYinVvq1nh2+yuESO2iZg0kUa+KVdgWLmqmUrTsDMKcAQDXpAbs2RDt3A7L3PSbu2VuOl33RbhrqPCYPOQV29NpUeC3DVYOCj7N27Ekg2dms3HTiuo6Q1FUJqOQSB7e97Xvcm47hvW1ybReW8tg8UbzzxFbe4MsKylrOU08eOMtodtK6XBWnXruxW2t7K6S8hkScMQiMDJGEcqBMmfDZqagKmqmtelTt7e/V1TsNtk9gdZu+SwmO7Iy22Ox9i15xW/s3vjceIwVBsLE9kVeffM4XLdV7HrcVNOaLH0dFkpTVFVqdIIYq3DZuZo96G8bDzABBNLaRXVhfLrto7aJ5WuWtFi8KSO9uFkA8SR3jGkVQ4o/b3m3tbNb7hZsWSOQxSwkK5lYAR+KWDaoUplVofQjNWDfnVXY3XW2eqNxb1xox+2u39k1HY3WE0e4MPl4cvtP+8OV2vX5VcZjMpX1e25TuLb9TA9PXQ0lTJ4g+hkIb2ebdu+1bnd7xBYSaruznFtdjQylXCK6qWKgP2OCCCQAekc8NzDDa+MT4LqXiFaihPcQPLIz6nrBsfcnXGD252jjt6dWHf+5t27Qo8N1lutd8Zvaf+iPd1PuHE5Go3xJg8TS1FD2ItXt2jqsWMXkXipYhV+dW8iKPe9wtN0ubraZbDd/prWGYvdQ+Ekn1EehlEWpiDDRyH1LntpwJ6bikhSOZZINbstEapGg1rWgw1eFDjpS7d3H0ZF19X4HdHUm76/sePAb2iwvYuC7QOOxk+6s1ldmy7Drc7sSu2vX0YwGxcRi81DUQ0tYk+XlysTu0X2oDk19tvOb77a3m2c0Wkewm4tzPYz2et/ARLgXCxXCzoRLcSPCysyFYhEwCt4hovguNnWyeG42yVr3w5AkyS0GslPDLRlCNMYDggGr6hwoOmPHZjMpgKfapzWZfaseZm3FFto5SvG3o9w1OPixc+4Uwf3BxUeenxcCUz1oi+6amRYi5jAUDlBj506JDSpNOjsfHbuCfE9Rd1fHGn6oy/c25+8qja1J0xhROczg+vuzJZZcFnd+4vrak27k8xvftjKbGq5MLtmpp62jODmqpqgR1DSWSNedOT9uueZuV/ca85hTaLfZUkbcrwP4DzWaETLazXTSJHFt4nUS3KMp8UIq6lC5Pdo3a9j27ceXLey+rN6wFvAU8QLMQU8RIwpc3Og6YmUjTUmhr0islt7sHbcmJ3Vumm3HBUboOYqsTuXKtWzVG4qvDVRwu5Pt8pkAZsjW4XJ66CtJZvBVI8DHVGwWQNqv+Xdxjudp2qW2aO1WMS20WkCJZB4kJMa4RJEGuPhqWjDBHRFeW25WDxXdxrDy6ikpNSxXtkGo8WQnS1eBx5dCfmN1T0uHxvXSZPYGV25gUwGT/ALy7H2vFjs9lpKnFvPWYmfdFVhcduCsraGHcFTR1aVSpRy1NKbNKixO7UfL9vBut5v0Ut49/OrJ4VxcSvbpUoQy27N4aUaNaFRqFTQ5PTv7zZ7W226VIRZRupZoY1WVgK1HiUqSQx4mhoK8OsnXNPPl83l9o4HaO5uwMzvjHTbV2HsLAQbir8xuHduYyFNSbcKYraVTFWZnNYyGWSWkpft62KoqrR+GzBg/vKKlrZ7jebtFZR2ci3NzdOsWgRqD4qF5wRFHJ5uCrAAZ49N2UsKzX0MVg1wJ0aKCMlwwZj2PSPDuoHwkFTU4wOhu7a+IXbPRXVHS3yAyFbh851Z3NhcemK3vtuqqKePbfY0p3JBvHpnN4zMwYnN1O/eu027NFn2oqaoxdDVTLSvUrUkxAs5a5u23m6fmixt7R459svjZyxzUrIuhJYLlAK/oXCtqiY/Eo1iqkE2vttudrXbpWmBFxCJVZPwkkq8Z/poRRh5HBoQR0gOutvY3cGE7MjTrnsTfOQ2z11Xblx+Y2HJN9h19U0G59txVu/ezaSHbe4GbrWhwVVLRyhpcZ4sjXU8j1ZVfDKu3q6vLW65faHerK0gmvVinjvBVrhGilpBanxY6XLSBWBo9UVgErnqlpHC8d2GtpZGWIsjRfgNR3SYb9MDjwyePpCpd6brp9hZjr6LeefpNkZLc+D3ZW9fRV+R/uxntz4zG5bF0m66zHxTLjFzGBx1Y1PDLKhkaKqYIQFb29Lsu1Sb9ab8+0QNvUdtJapflU8aOFnRzCr01+HI41EA0quePVku7lbKSyF04szIJTBU6WelNZHAEAD7cenUDZ26sXtDP7fzeS2tTblXD7rwGdqqaTMZPCz5PA4yd2zuz1raBmNBT7ponaCStSNqmlB1xcj3vetqm3e1u7RdxMUEttJBo0I6iR6eHMQw1EwkVC1CtkN0p2zdRtTR3EFop3BJ0ljuNTBlVQweMDKUkqKsQSKY6z7/3x1NnqPsmm2X0Li+u6jdfbdXvfYWRi7C3nuqq6s60kXNrSdK00eZmWk3nj6Vq+kds7kI/4rI1EASA7Al+37NzPbbps15f86SXO3wbZ9JdWf00Ea3N3qQ/XGRR4kLaVZRCh8Oj14jpqS62x7K7totmVLt7kSx3HiOzRxaSPB0YRwSQdZGrFBjrn1t2B1RsfvPAdh7i6Noe0encTuOpr8l0JvnfOf8O4Nq1dHV0LbdyPYe1aba+Y/jOPFUKujyKUiQLkKeEz0k1OJIJH77aN53Dlw7Q/Mz229OiK+6WcKIwZXVmeOCRpVUOoKldRNGNGBoQzHcW0V6LkWIa1BYi3kYsKEEAFwATpOQacQKjqD2RvTG/wXI9e9Wb47P8A9Ald2bvPsvbXUG/MotW+za+SvyO19l5jc1VhUxu0N39k1XV9PRQ5LMY/G0EPkaSFIVW3utrs1nJzNuHMd1y5ax76lsm2w7quhria07bh4i2gSRQpdM1IyxDMNYpWgdlu5RtdttsW6SvZNK1zJaEMI45hWNW46ZHaIDuAFASvGp6w7N7M692x8c/kTsKqO+dpdx72m2HU7G3xsrO7ugxe+tnUmcix3YXQ3aWAx2+dvbQGwcpia7+8kORrcVm6lsthoKFIEiqnqadvcuWv3pzHsm9Xc8EtjYo5htJraCQpcNgXUVw4M0MipVCE+IHJFCC1DeG3sbuziDq8xXU6uwDKv4HQdriuQW4VwDxBU9ndgZ7rHI5jcOAbaNVM+39w4M7e3ztCg3xt3IQbtwGU2jlcrS4HN4zJbcoty7fweYnmoslP9vU0bgNSyGUBfbXNHLtjzLbWtlffVoizxT+PZTvbSqYJUnVGlidJTDI8YDxiquMMKZ6UbbuE1i7yQmNgVI0SrrU6gVrpIK1UHifsyCQS/wCN2xm91bh2/tPauKr9wbj3RlsRtzbOExkLVmUzuczVXBjcLisbTxDXW5HK1tTHDAiAtLLIqqLkD2q3O9s9ssb3dNyuY4NvtonnuJpSFSOONS7u7HCqigkk8AK9btreW5mgtraIvcSuI40XizMaKoHqSaDo2PTPbO+vi7sDt+XeHRm7UyncWzNy9V9Ld0ZWjymx91dR7+2XknwPYeO2buTO7aylNnNtDbe78lgt5bTjWEyNX05klpZoUYxbzJy5yv7i75skUPNMMy7VLFf7hs8MySwXEdxomtJru3jcN4iyWqy2c5IoUcgSKWXoQWO4bpsNlcn93lBdAxQ3UkdHUx6lkSGR1IC/qESqM8BVSOid4PNZrbOQpsztjNZbbuZokqY6LMYHKV2HytJHW0c+OrEpcnjp6etp0q8fVSwShJB5IZXRrqzAyv8Abx6DfQidYZ/pvbyZiftXrLdHZVWuW2PWbbx2A7BHX2IXEYvcBqt/4PP1FNt3OZKU7s20BR0FVTGN8ZUXm0Sg6QF+Y7Dm2+ezTlrmK12+DwrlLlprX6mQu8Wm1kirNEi+BN3urBhKvbVOPRrttxtECzHc9uluJNcbRhJfDXSrVlV6IzHxEwpBGk5zw6g7Z3J1pjNp9sYbc/VEm7t0bvxWGo+qd4HfubwI6aydFuilyuZy8+3sfRSY7sv+O7YikxH2+RaCKmMn3SXkGn2Y3dnu015s81rvAhtIWY3kPgq31IKFVXWx1QaHo9VqTTScdI0kt1S4VrbU7U8NtRGjNTgYaoxn7ekhtzFZjO7gwOC24jSbgzOaxOFwEUVdT4t5M3lK6nx+JgTJVdTR0mOaWuqY0E8s0UUN9TuqAsF15LbwWlzPdgfSJGzy1UsNCglu0AlsDgASeAHTcHi+NH4DETahpINCDXFDUUNfPy6MLj6Tbfxt7A37tnu/qgb67v6k7UxGG/uLuLcWLzfS9Udr1m4Md2jtTsqDbFYuZ3S9bWNRnG1eGzMMEc1O7SGVG0sCtzh3jnLb9sblnmMWHKt9t8xlurZGW/VpBEbSWzeQNDEEGvxFkickMoXSRXo1gltdve5N7ambcY5V8NHoYTSviCUHuYnGmmK/F6EAcJijuvc2HwhyGDwI3HnsXhkyu4sg2L2vgEy2Rp6GKtzeVqfvGxW2cIs4eedxL9tSRFiG0+xhfXX7r228vvpp5/p4HmMVumuaXQhYrGg065pKUVRTUxp59F0MRvLmGAyoniOqa5DRFqQoLMa6UXzOaAdCDD9h1fv3b74bcG0t6bj2b2JVU24I8nicduzpDNjaG8aH+A1n3lRUVdF2d1nuj+HGrrYavHQU0tCFHjmWQ6SaL6jmjZ7hLuzubDb76xQwMJHgv4vqIT4gdVUNZ3Nvr0qUkZlepqpXKqVYdtuo/CnSe5hmYSCgeBvDcaSrVPixyUqaqopTjXoS9r9LZ7e3yd3r1dtSn2B3PmsVl+3srHkOm+yNt9a9Y7pi2Jgt0bkl3n1hv3e2HwOIp9iYV8auUxlNJQUs9djqUUUMUDyq8d96urbl3YUabcjFbxGC3+onjluiwLpHR1U+JI8oOnUTXU2sg00lq2WS9vCwg1O+p9CERgYJxiiqpzSnAUxx6BOopd5dk1+f3Ur5vsTdlfT7r7H31VpSZXJ5qngo5my+5N77qrpqVoBT1MlZJWVdYJphBrZqho2IBMlk27ZoLOypFaWS+FaWqkoiEkaY4Y1rxFAqrQV4LXpplmuXllBaSU6pJDkn1LN+2pP7ejC7U2f1IG7/AMfQdo91ZvpWPp7AQYreW29pYDr6j3L3plcPh927A2J3PtLce98mtD1bQ9k4HNUMeQpKmurqmTFUlbDTU7VHjiJuZbqW2vOWxYWlpPuX1YelwrmRbanh3clroVj4yJKoyVUoWqfLpbtdsLlbtJZzFD4R7tQVC4q0ayFqdrFTTidVB8+pdDvvMfMH5IUOY7H62k3buPsHbi7B2Z1n8ccPs7qGkTO4PY0u3uqcTt7DRYmXb1Ntvb1fjaSWuglHnqqWnZBMpCaSTeYF9u+RZ5du5ihtLXb3jubvct78W5HgCZWu5JSjI7TSxltLj/RG1MCSSVNkP31uqJLZM7zApHBbUTu0nQBqqAi08zgDzAp0VCWOSjq58ZVhYMnSVNVR1tGbJNDX0btHXwSQk6klglRg4PIt7kRJI5o0mhcNCyhkYGoKnIIPzB6KCCjFGFHBoR51HHrNoXSVIDA2uCAQbEEXB44IuPduvfb1IiQN62/T9Rf6H/G/9B79Ty69UUr5dGN6X2+0OzO9u1o+58l1PkettgU2C2xjdrbipqLffZu4O0ck+1H69osQu4sHnpeu8pttsmdx1lGtVBSU5jSeB1qLGPudNw8TeuROVW5Mj3a33LcDPcy3ULPa2UVkgnF00ngyxLdpMIvpkfQztVkcFK9HW0W6mz3rcv3sbVreALGqMBJM8raPDC61Yx6dRciukUqDXoa+kN6bc3vsvbXWOOx/XnQm4uoOv+29zZXs7H7B3n21U/LTP1lYld070z2v09Cme2nn900+683JjNs52Wgkp8SrQO0CSQRSMi5n2t7LeP33ePLuFteXEEEFu8iW7bdRT9XdW14CssSNAgMsSsuujAsQ5A3tpnntbmG2TR4MZmndRqWRQyrGskRoHIkfDHURigFMlml2mu2Nj7G3ZhezNsZXLdiYvfWO3j1ttDIbx/0hdZ4na2apMGuJ7ihn29itvy4zsak/3I4uKgyOWp6igpy1atPKEiMlywWtwYvHjjcLIskZcBqOK6XSoOlxXtI7hU0PRDFLKhkWNmSqlX0kiq+atQ1KmmQcevQlbP2Xn917E7LwtNsrO7ox3VWKg7iyG4eveu9v73TactXVbX2k+V7U7LoJRldn9R0uGyE3j0TVdLDuQxxmnjllqJoiq7ngtd02i7+sSOS5b6IxXU8kQZR4jj6e3I0SXJl0ipCkxHDGiqX1BeGeIoSE/UBRVJBwDqfiEC1NBWjDhxPQl7Mx+8djdI13buL2dSQf3p7XrOr9o98UnZZpexNsZTAdY103Z3U+O67o92jK1W1d/bD7GofvM5lcMaAxwfYUNaXWsp1fv9ibdNz26W43E/uGOJxPtbQwtDPL4sMtvcu5Qyo9q8RKKjBWLFmBIUhpLxYIplSD/Gyw0T6mDKukhkA+E6weJ4Co+xwXqbdmM2PnewcBPS7k6ixO7No9cZvfW3cj9lt+o3xuPbTb2w2059u5eXFbqyE2MpqKpVqhsdJQQ1lE5jn9UTuxa817Jdcwbfyxfo9rzlLZz7nBYXMeqVbWGf6WS4E0Ykt0EhZaKJRIyOKphgHp9qvIrG53K3cTbMk0drJcRNRDK6eKsZjYrI2nOShUMDQ8OhV6sl6jy9G+y+7W3xRUFduDYtPs/s7btc2boej9uR56eq7NyzdS/aA9nZDcGGliix9MlfjzQVCNMGcegouZbPmuwn/f3Ikdi90lvdPe7XOixNuk/hKtihvyf8TWBwzOxR/EBCmnEKbK8sru2j2zfprkwI8a2k4dmSzTUWnKwUPieJgAD4SCQDw6YvsNqeO/948v5P71/YeP+7T6f7i/c6f736/4hb+Pfa/ufwf9er0eW/sQfUb3qp+6INP0Pi1+o/4l0r9L/Z/2WrHj8PPR0XeHY0r9W9fH0/2Z/sK08X4vjpnw+Pz6JPNEg/yZI9CRx6VVIysaKoX0pZVS8YdSVBuAy3sGF1xqe4nj/q/ydNinCn2dM89FjDjq16p67+LLVUIxlNHT08mLmoyKj+Iy1tTJKKmCqhtH4FRGWQM2oi3tK7Xi3cHhJH9GUbxWLEOG7dAVaaSpzqJIIoKV6VILM21w0jyC9DIIlUAoVOrWWYmoYY0gAg5rTpRbRn6cOPy2P7V2nv7KeWPPZDHbi693FhabLQ1UOy89BtPbVXtbdOIr9u12BqexZcZX5XICUZNMZTTUtJGJJRMhNvUHMzNBNy5eWKnVEskN/HIYyhniM8gkidZBKLYSLEtNHiFWclQQXLRtu713GKYrpYq0JXVq0NoFGBXSZNJY8dIIGes298PuPqiv3BsTD9qYvd21944HatTuDNdT7l3Z/ox7Do/Bj9zU+Ir48hR7dG7RsfckzU88VZSTQUWXpJTESyhyk2Hc7Tmmztt5ueXLix3C3nmjS23SOIXduys8WukbyiIXEYDoQ9WidSQK06e3GyuNqlNuLxJraVFdZoC/hSjBOksq6/DftbFA4I6669n2nXbV7K2TuXdW7ttZTdMG0clsVKfcWLwXUVVuzauSydTUZDumOup6ytrKXHbWyWQg29JQwvUw5auKMUimdvbPMH77ttz5d3Xa9us7jb4HmTcQ8ckl94MqKEXb9JVAzTqhn8Q6TEpIBZQOnduWynhvra7uJIrl1U27alWDWpJYz1BamgkJpzrIBweuHWWXw+Oye2s/vQ7N35tHYp3juv8A0Hdn5/sHDba3G/8AD8THUYDGttOJhj9yb8q54ZIEpKikapnwh+9mjjSHye5ms7+8s9027Z5bzb9zu1hgXetvjtZJYu5zr0z1DJAoIYujALMPDBOrTqwkghe2urpYbiBGdjZzGRQe0ea0ALk4oa1TuoKVBWpEUiylz4UvJKHS96W4ciSF5DK4anVjoZiz8XJJv7Fi1wFJrSn2/wCTP7OieorXy6OP2hujbmazA2h3v8ctofFmuocD2J2pt7/Ze+sa7b25tz5vtjbeD3H03tncuM37vnMQU/SWOFLE2Pkgkeuo6KunkDSyObAH6+93ZpuY+QN6tdzgnv4LO5huZ2+kt4bWUw35tvBjZhdijHSx0vKO4hQB0dpDBbUtN3t5ImSF3jMSjWzuNUYkLGnh1waZAFKA1PQF4fsLbzZzrSu331JsXd22uvdp1W1MntLb0uY6zqOyVlO5auh3Hv8A3ltSpG4ctvHG5bcEMhyKeKSqo8ZTUcieEN7NbzYNxFlzBFsvNN7bbjfXS3MdzPouxa0EKtFbwzKY0gZIj2ZCvI7g6j1SG+g8ewe82yGS3hiMTRpqi8X4yGkdDqLhm+LzChTjpe9P9j5XBDZWwui9v4rbfcfaW3t+dDdp767Cr9i7n2dv/b3bu5NvQbZp8Hhuw9tVGA6Wrts0mPSnqM/BV/d63M6TwLrVyjfdukgk5h5j5t3VrjlTb2t9326ys4ZkntXsopHnLvbyGS/8Z+5YTHpAGgq9cP20kc6bbt222nh7pNrtp5pZFKSiVlEdFdQsGgYLas8ajoJO4Ny793b2n2Tn+zstjcz2Bl9/buyW+K/A0u2Mbtqu3nPmaiHc2SwGJ2NR4zYuPx1dkaQmL+DUtPQSQpGYUEej2NLG8t9ys7TdbZWEN1DHOhdGjco6h0DowV0IDZRgCpJBANeiqaCS2kltZSNUTsjUYMtVNDQgkEY4jj9nThvHdOC33tnYVVnsjjcfubZOxqjr7Hbd2d1fg9t0X8O2hW0NVsbObt3RQ5Wl/vnubdi5/LfxPKS0f8QpP4bTK7VIqB4CHatpu9kvt5jso5ZrG9v/AK+Wa8vJZmVplKzx28bq/gQxeHH4cIYRnW5GnT3Lrm6hv47b6krHLBb+BGsEKKG0GqGVgV1MwZtTkFu1RmtQ0ZDK9fUnWOK2zjdvHKdiZLcNNuvM9iHL7jxp29ho6LLYaTqX+5s7PtjPoalKbNDcMZWoVqg0aoFRyXoLXmCXma63K43LwuXI7Y2kO3eHE/iylo5BffUD9aM6S8PgGq9viVqQOmpZduTbIbaK317g0nivcanGhaMvgeGexsgP4nHOnyPSX2ft+j3LurBYfIV0mIxtdkKaLOZ2noIspWYLbkcyz5/NUuLkrMecvPhsQk9VHRLPG9W8QiQhnHsx3i/m23a769t7dZrtIyYIGYosspFIo2cK/hiSTSpfSQgOoig6Z22zN/ewWuoqjGrsKEqgGp2ALKGKqCQtQWpQZPQg703N1jj8TW7D692XhM1Dj5dxYGbu7Njc0O7OxMbRdjV+4Nm79w+zcjl58X1HlazZi0mHyGOpzWw1VFrMumqZp/ZHsthzJcTQ71zBuckMkqwzjaIvCaK0c2qR3Fs1wiK14gn1SLIwQhqaezt6UX0+2ops9vtw6IXQ3bag0w8QmOTwySIT4dFKgkEcc56CKKbGJj6+Cehnly01RQPj8ild4aaipYfuP4hBUY8QP99LWhovHJ5E8Og8Nq4E7rcm4gdJ1FqFYSRlalmNNJDV7QuaihrUZFOkKPbC2njkgY3ZZTHIGoqqK6wVodRaooailPOvTttvY29N7Q7rqtmbQ3Pu2n2Ftit3tvqo21gslm4dm7LxtRRUmR3bumXG01QmB23j6rI08c1bUmOnjeZAzC49tXW4WFibVb29ihaeUQQCV1XxJGBKxpqI1OwBooyadNpFLLr8ONm0qWagrQDiT6AdQtsbbzm5MlVU23MK+brMXhs9vHJ0UaxaBt3ZuJq9y7myVcrzUxmx+MwmPnmqFV/K0KsEBYj3u+vLWyhR7y48KOSSO3RvPxJnEcajB7mdgB5VpXHW4Y5JHPhpqKguR8lBYk/ICtenLsHd9NvvfG5d6U2ydl9f024q6Wug2P13jq/D7I2wGgjhWh21jchkstXUlAhi8uiSplvK7G9jYIeX9nl2HZdt2aTery/kt4xG17uDpJczUJOqZ0SNWY1pUKMAefSm+vY729ub36GGFZCSIIAyxpig0AsxABzQk1Py6aZMYlJUUypkcflVmx1FkGfFyzSpTyVcInfGVDVENNoydA3onQXRX4DMOfZrayGcSM1vJHpdkAkABOk0DihPY3FTxpxA4dMXECwNGq3EcoaNXJjJIXUKlGqBR14MMivAnpZR0K007Qx1dJXJG8arUUZqDTS+SGKW8Qq6WjqdEZk8TFol/cRgLqFZl0Ll1BMbKfRqVGSPIkfPjwP5dJHGkkVBHyr/AJehRwWey2NyWBy+MqDhsrtyKkTD5XAPPgctSVFBJJLRZZMpi5qauGcglk1fdq6ymw5491fa7O5tL+xu4vHs7osZobikqMrABo9EgZPCYCmilMnGerPuE/jWc0YWOWBAkbwjw2qtSrlkoxkBPx1qaCvQnZHee8t30+Dpd07ly+fpNtUf8O29R5KoMlJhaFxT/d0+Lpo1ijoVyctOJqto7SVNUz1MpeeSSR3tv2zbdpjnh26zSFJZXnfQPidzUsxNSaYCg4VAqKAihQjurm5vJEku5zI6osalvJVAAGKeXE8Sakkkk9DBvzJ5Hser2tk9pbH2ttPbGUyWb2v1j1nsiaLcGXwx/idNX1eFqGC1XYW5pslnM4XoarMPV1MwkNNTOYIEiQu2y6j2u3u7Hd91kmurKBZ7y/uoxBGyN4jBy9FgGhUOsKewAFqV6UzwSXLQXFraosc7tHBBE2tgw0gjSKv3E9tRk1pw6wVrxYrshst0Y/ZW2kwGVbMbSGQy6DtvZzbagpqmty+Qzu1Mdtqlostja+Kolhmoo4Hp441V7SAkmF29hdWEsW5xwSbfMqofG0tBMJcKtG1B1aoFCKGuK9MRxzRzRG3d1uFJJCVEiaeJPCh48D5Zp01efI73fA4fDY7N5bOU9Jn5qydsvkM5WbhrJqzK7jyedioqwvHhZkxSlqtYWdahqd6iVjIx9p0WDYxuN9uF5BFYPJCIx4aRLCumOFIi60MoMvwFgCNYRRQDp+j7i1pbWdvI9yqyaiGLmQ1dy4U4QhPiAJB0ljnoweb+Sm+N1bU6s672Ti9l9GYvavUNf0VuzK9QQ13XNZ3jt3dG5qbPbhy3f2fosia7fn94Z8djTX02QlmxYfHpLHTxXKgPWnJW2bVuPM3MO53N3uk1zepuUMN6TcLZtBEyxrYxNVYXXW+lo1VyGCsWKhiYfvCa/i2ja7dYrZUUwNICIw/isoZpnoD4dFWoYsAdTCgbSAEenaOapp9UUzU1S9K0tNMk0DvG0ih4WQ6pYJhEzRyABXSx/PsbJIJFhl0soZQwVgQQDTBHkwrkeR6KZUMLzQ6lbQ5QshBUkVyp81NKg+Y6Mv8AHTsr44bBw/Z+G7/6p3J2ZT9jy9bbQpMptiPZgz3XPXlHuqp3P2vunrrK7qpp5dsd11gweEoMDkI9dAMZUZanroZBUQNGG+aNl3fdLe1uNh3iS13a0cz26F2W2ncjT4d4iAtJBpZjQZV9LUOmnSixuLeF5Eu7cSW8g0uQAXUZNYySArVp9oqKivQaU/VVBtjCYvunsDY/YO6fjjuqbf2z9t7m2FnsfiajH9qJsrMZXY+xNybxy+08lgI917RranEZfceLiow9ZhjIlNPTyTrJC7tvMVvf393sMjeDzDbrqkhlXR4qDQrXEC6nLWzO2lWJrUEEDBPrvbzbRwXgdXspRUGNqlCdVI5MALKFUlhw+fl0W5FYqhcqx0i5X9LG31UEA6D9RwOPYkIB8ui6pIoDk9Ypfob/ANfx/sb/AIufexjHVvIdPtR1RufLdeY3taiwe5KTrJd80PWG7u1cthKtetNr9h5qlrM5h9tPn8ZFkKietfadDJkZoRC1QIkOhG4BDs++x2257js8xik3NLY3lrZQODczQqArMVk0IpM1UTuANKkihoYmzt5rbbZoJ3RXfwbqadaQxOWOnSya3ZBGQznTUE0APQS7GwO5sx2lsDDbHrdo0u8ajfm3Y9o5Le9btPG7Fg3HS5qlqMHX7prewlXZMG2Vr6eOSpGaX+HPT3SpQxs6m++bta7Hsu477fwXDWdrbtczR28Uk8xVF1MqQwq8kslMBUDEnhXpuytXubmKzhdPEd9CsxCrXOSzUop9TTpk+SfbWI7g7Axm/sJ1Zs7qHeNPgaSm7SreuMpkP4R2j3ZBuDPZrffecGFglg2p1vkt85nKo8e39pU2M2thYKSCPFUtPAFQFW0bdf20O6HdN5lv4rq6kubdZoY4vp7eQLotAqIpdIgCNUgMjVIcmnSmaSLVEsMAjdECNpYtqZa1evz+WPToFt4djb939NSyb23dndzChqaitoqbK10s+OpMjX0uMpMtlabFqUxsOY3BHh6Z8nWLEKrKTxearkmmZpC3tfL+ybIZ22na4beSVQkkkagOyKztGjOauY4jI4iQnTEp0xhVoOlF1uN9feF9ZdNIENVU/CCQoJCiigsFGo0qxFWqc9JfI10mTr6vIywUVLLWTtO9PjaOHH0ELMAPHSUVOqwU0IA4VRYezK3gW2gigR3ZUGkNIxZj82Y5Y/M9M3Vw11PNcvGiu7aisahFH+lUYUfIdYKiJacxhKmnqw9NT1BNL9xpheeFZXo5vuKenb7ukZvHLoDxawdDutmN0YuCShWhIzTyNK4JweI8/UA9NEU8wcVx/g6k5Kjjx9XUUCV2Pyoj+3Zcnipp5aKUS0yTMlO88NO7GJptEmpBpkjIFxyWraV7iJJmhkiJqDHIAGFDQE0JGaVGeBHSi5ijtpJbdZY5SCpEsRJWhWpAqFrk0NRgigx0IG6KrKb02tgd2UnXW09p7X2Bhtn9S5jObNxtRjqfc25qin3RmMXuHey12WyM2S39urHY2saqqoI4aWSKgUeOMj1Em02sOz3242E2/Xd3e31xNuUUV46v4MdYUaG30ogS2hZl0q2pgXPcfJXcz/VxW0qWEMMUMSW7NCCNbDUQ8lWasritSKCg4DpO4jYu8c3tbeG9cFs/cuX2T10Nvf3+3bisFkq/bGxhu7IzYnag3Zm6Wmlxu3f7zZaCSmoPupIvuqhCkephb2bz7jYW93ZWFxfRR39zr+nhd1Dy+GNUnhqTqfQpq1AdIyekghkaKWWOFjFHTWwBIXUaCp4Cp4dNGPmxsX3RyNFPXxzY6qioRT1v2f22QmjAochKwhn+7paZ/U8Hp8qm2oe3Z1uHEX006oRIpcsurUgPcoyNJI4NmnoetW72yeN9TCzgxsI9LadLkdrnB1KvmuK+vSm2NuPEbXyz1mf2Vt/fuGrYaChyeCz0uUon/hkG4MJmcg+3szh6ykrttbhyNBiJMamRRahqWkr6gxxGUxuiLd7G63C1MdlustneLqaOaIK1HMbopdHBWREZw+g0DMi1NKg7tZ44JVea2WWKo1IxIqAwJAINVJApXNATTPSt7HwHXlRhsDvrrzIVf2m68puqbdXXNTia5aDpnIyblzE+z9hYnd2azFflezKQbJjp6hsu8EDK/wC3NqmJJJ+X77f1vdw2LmC1TVaxwC13BZFLbgghj8e5eCONEtG+oLKItTVA1LRaAGN/Z2xs4d1sW/RkldZIaGkDEsyRBmYtL+nnVT0BNemLrbcGzttbtp8rv7Y47G2wcXuHH1e1X3VndmJNX5fBZDGYTOSZ3bgbLFNq5mqgyZo1/ayH2v28vokPsw5isd43LapLXYd8/d26eLFIl14MdxRUlR5YxHL2frRK0eo5TXrXKjpJttxZ210Jb+z+ottLAxa2jqSrBW1J3djENTg1NJweueIw2wP70TUOX3rmKfb1FufHUeL3lRbFXMpV7bGYaHLbmrdoV2cxVcksWIiSqhxPmLVUjmnlliA1lyW53prC3nh2qL6t7ZnmtnuCpSXwwUiSVY2VgZCVaTGkDUobh1YQ2CyzobqQosgEUgjqGXV3MylgV7RULmpwSOPWTfW+cz2BvrcnYOSo9vYHN7mzM2ZqKPYuBoNk7cxtU4jjRdu7ewKU1Bt6lRIVZYqcKEcs17kn37Ytktdg2Pbtgt57ieztoRAr3sr3MzqPOWWUs8rGuS32deu7qS8uprx0RJXbVpiUIo8u0Dhw+3zPRnB2521t/qXpvA9ujaG9/jPv+LamITr7a1N0/t/sXM9ffHHsjdWRj2vV7029tSq7H67y8m4Ow8v4ctkmfIZilqYw8lRSUsMcYb3KS05m3XmDb9iu5bXnbZbU28F7Pbzm3gkv4PEikVCYoL9V0guoZtJGlirUosggk2+3267vI0l2m7kLtCki63WFwrKaanhJPAkCoyMV6AHIbj2JNhHoMB1lBis1B2fl93Y7duV3dnNwVZ68mpaOLbvUeY21KlHtjJUmEq6ZqmpzSwxZDImZ4ZAsOkKd2u2b4t4k+4cxmWzO3R2sttFBHEpugWMt6kgLSoZAQqxaikekMKtUliW5svCZYNv0SfUNKsjOzkREDTCy4RgpFS1AzVI4dCbt3svrCg3Jne79z7B2tmezqHuHbW99tdCt1/jqb4l5/Y8rZnI732zuzA47cOO3HhMNRVwoYcXiKBmpXpmk8knoC+yqXZeZI02fliw3Bm5XG2SW13uk1zI27fUL4S27xuYzHIXTWZZGIfVpKjj1dryxlN5fywhdwacSRwRootwpqWXRxUA00gYAFKGuGTvGm3XSbyweH310ftDoLc23NgbPon2ftPaeb2e+ZxOXoZt1bf7C3LQZ/O5+qr91712/uKmknyEUkEFXRQ0toEZHLH+w75s/MG1Q3+wbzFf7aGe1+qgdZFeS2cwTamWimRZY2D0A7waADpFc2lxZ3EkN3btFcfHoYU0hu4AA8BQ4/Yc16cdqZTB1Ow8DS4qTYnV3YWwOzaPcsXcC7i7Hou2txYzc9OlLiaDA4vbsVdhKTAdRZLb5yM9dSfZZeKTKQtEag6whPfWW4x7/ALjeSy3247Hd7Z9ONmEdobSOSFmaRzJJolaW8SURhHZoqRmumoqtge2kt7e3rDbXCThzdsZNeluHagbtjIqSBqyKDjV762fau3Nldn7kzm7974nd249pZzrzYeF683HjcdX1+UzU+Bn3O/cmMyEK5DJdIbo2nU1tFJ9jOairy8SxSxGJS3t3fk3u83zljbds2uxk2mC5jvdxn3GKR1WJVlEYsHQ6F3CKdY3pIuhYiWDaqDrdn9DHY7jc3N1KLpkaG2jgZQddULNOrCpt2QsKqalxQinTDtzMbnwlNncbt3O7kxdJvLEx7Z3Th9u5jK42HeuCOSospT7X3FjcdVU1PujEy5mgpqiOgrEnpzVwxSBPIisBTPaWNw9tPe28DNbuZopZlU+CwUqZEZgTGwQsCwoQpOadFSPNVooS5MlEKJWr1IotB8VWpQeZp0Ziq2T011jBV4vc9ZL3F2RUUmByFFXdZbxXDdV4Pb26+tM7U1W2N3V+U2hT7+XuDq7s/IYuWtx9Opws8OPq6KWQNULUIENn3jm3mmaO+sLD9z8tK00LJucGq+llgvIwk8AjuHtjt15aLJ4bt+rV0kUUUqTK+stu2sSWt25uN2DKf0HAhRGjbVHJVBKLiKXTqX4aAq1CcIrb2PxuuR8rLWRlMbVmjnx9NTyyy5URr9hBVRzuogx1RIW8zoxeNbab3PseXT3ipEtjHG1ZlEglZgBFX9RlKg6pFFNIOCeJHRRapZM0xvpJFpCxjaJVJMtOwNqIpGTXURkDgOlXSxCNLsHJFvSiNIxJIGlI4w0jsb/QAn29xOMD9n+x01SlCR+X+bqfrjt/nI/8z5/1p/mb2831/wAzb+1+n/H3qh/hPGnDz9Pt+XV9Q9f+K6y7V7+yWx+rcR1nuzFbU7v2Jh6js3cfXPUO+sdQZjrLrrdPdWy63ZG/Oya5sQ2C3rH3Lt+fE4nIbejlra3EUEkUk6xxTuHMf3/LbbnzFcbraeNt8tI4Lu7jLpPcfTSRywJCCWhNo6tIsrUR3IVW1ICOjvxYrSwgjaaOd5B4sca6WWINrV1m7Q6zggFVqQFYkEMQeiaT0umFI3lklaNETzSkGWVgAuuQgKrPI3J4FyfY441NKfIdE/AfLpNTxmNnQWBsdNwSBe9rjgkX/wBuPdBQEqeHp17pTYbbOc7H3hs3YPXOA3LuHce6cjt3ZmztnxTyZ3M5nd+fqqfG0+G25SwxRAtuLcVWFo6OJNbSzKl3c3JfBHLBHO92YzO0jMzwxlarWkYYDUzuq0BbNfKg6W3UkVzJbx2gkWFY1UJM+qjUrIVJ0qqM9SF8q5JOevUkfVZ6x3Kco/ZSd4rvXbI2XDQwbaHUJ60/hmV/vsd3yVTDesfYAzZohilpF+wFKJvP6yNLEn76G7W4i+k/cIgfx9Wv6nxtS+H4dP0vC06tde6tKUAzRTAYW+P6jUNNKaNNM189VeH+zj3XHU3ZvcOV3Hg+rdlZve+V2fsLePaW66XDLRqm3OuuvsWcxvLeOaq8jVUNDQ4XBUOnWzyh5ZpY4YVkmkSNlUtzbQS2cE9zGk9xIYrdHYKZZBG8pSMEgu4ijd9IqdKMaUB60EkZJZEjZkjXW5UEhVLKgLeg1MoqcVIHn0FheNohOn7sLxiVSqFtcbLrGmMrqbWp4Frn6e3+mdAOa46HyHZEW094bN3H3bS5/tTqqXbfXG5d5ZTprsHEbmrsXt3f20HyWyNiZPsIwbj2/wBfdi4uGKKnq9v5MJW400ktJ4ldfSGd+N5b7bc7PyluG2WPNlxE8+3peIGiLB1aaVreJ4pJVGs62U1DsC59TOx8OWdLvc4LmbbI2VJmiNGA0kIutgVU9uAeIBA6AMsNTgAhQzlNR1MI9R8YdlRAzhLaiAoJ5AA49iYVoK8aZ+3z/KvSD19Oh+xuxqLuGj2nuGg2ltbovqbYEfVXUvePdL1G7907Uxu5d55fNU8HcPYOCSfPbuevz9LDK1Vjdu0E9PHFjgIolZwGB2330Gw76eXd75wku963e6ur/a7a4jjRobWFYddtEYY1DxWuoEPKTK2s5amDS4ge9svr7HaVitLSKKC5kRiQ0jF6SMHYkNJSlF7RTy6LzVwU9PV1tHS1lPkaWjrKmkpshSRzw0tfS008kNLkKWCrip6unpa+nRZokmjSVI3AdQwI9jH5nz6KlNR8+hG3T1DuDafVXU3cFXn9gZbbPcNTvygwuH23vXEZvfW0sn15nv4Fl8Z2ZsunZczsesyqSRZDFfcK8eQxlRFOjjWq+0abhZybhcbUktb+KFLiVNLdqSM6oSxXQSxjbAJNMkdOeDMIUuGiIgZiisaZKgE088VFfTHqOm/Abi64x3WvZu3Nw9X1G5uyty1exJusu0It+ZnBU/VdHg8tkarftHU7BpKCowvYB7BxFRT0cctbPTviGp/NAJGcgJru03WXdNpurTdxDtcIlF3aeCrm4LqoiIlLBofBYE0UHXWhpTrwaFYZ0a31TNp0PqI0UPd28G1D14eXQeQSQUVZjqqpp6LMU8clNWVGNmepWlqUinLPj614WgqI/MkdnMbBlVwQ1/ovlV5oZ4o5HikIKLIAKqSMOtag08qjiMjpuJkgmglkiSWMMGaNidLAHKsQQRXzofPj1DnkSWeeWOFKeOWaWWOnjLtFTxySM6U8TSs8rRQKQilmLFQLkn3dFKIiM5ZgACx4mg4mmKnpuRg8juqBVJJCjgAfIVzQcOsDLq/1x+f9f/e/+I936p0YPGfIPeNV1ht/pjL56TbO1Nqbd3Zs/bW4to0sO2MtSbM37u07+7D2r2E+0KHF5vunb28Nw0NGsdJuKtrabEpApp4wusEI3nLMC7xJzBaQrNcvIk09vN3rJLFH4MEkTSlltXhRnOqNQ0laMcDo5sryJ4fobuUxREFVnQElFNWdSi0MquwUUJovEDj0ArYysjxmPzlRSucRX1k8FLVGSIRVNRjftpa6CJ/3Hjlp46pLuyWUvcarEexOLmBriezjlBuo0V2TzUNUISMAglTivlmnRcbW4S2gvXiItJHZEfFCyAFgPOoDDy8+hC7epcDF2Bma7aXWG7+ntlZ6nxG49j7C3zlMnn8/jtp5nE0dTi687jy2GwFTuXGZw+Sso65aZYJqeZRGzquoknKq7pFsVlbb5zDb7rvcOqG8vrWJYI5JVdgwEKySiIphWXWSCCTStOlG6NavezSWNi9tZtRooZGLsqkD8ZVSwJyDTgaeXWPYGV2rg4d5DdWwaXfcmd2PmcBs+aq3PuDbX+j/AHrW1uJqMT2RTpgJI13PV4CjoqqmXE5ANjapa4vKNcUftfulju16doO1b61isF6k92Fhim+pt1Vw9qfFB8ISMyt4iUkXRRTRj01azWsK3YubETF4WSIl2Tw5CRplGn4yoBGlu01zwHSnoMQcjU5Os2th9xZXB4bFxZbKTVWNfIPhsdGaDG12Yzs2Jiko8ZhYM1kYokqZmjhRp4VkbW4BObUXJhUXjRi5qamGummo6aas1001fOtMdJ7w2njt9EJPpaCnjU1V0jVXTimqun5Ur0d7sXrvbMXQGwNw4v4xdjdJdj7AGxcb3LvnePY+rA9tY7t7CZnfHVHYO3emd4YXBb22lDvXa6RT0VVhzXbanxVPFUJLqq1JBG27pvm3+411se783W13tO5Wct5tO3pYypPB9NJFHchr2MtbSRIJU7ZNMzO5pVVPS6Sztbjlz942u1yx3VvcJFdXBmQxsJVYx0gakodipNVqgUUOT0A1OaZsfRUi0ApquKSrlqsmKipeXJU9Qaf7KB6SVjSU8eP8UgV4lDTiZvITpW0kxxyC4nma5LQMqqkWlaIV1aiGA1MXqKgkhdI08TUhcxtDEn0+mUFmaSpq4NNI0ntUJQ0I+KprwHQv57sdtwZau3Fjtk7I2HuifduP3Zj891rQZjZn92v4ZiY8bTYDauJoMzJiMJilrqZciZ4ojXLkAWWdVJT2hs9ngttqXZ7q4mvbPwmhk+vYTtKrklhMWFJAQxWhFCtAerSXUjXP1MSrDPrDqYAU0kUA0UytCK1B49IhaydqxquaeqmnkmMtdIKuaKsrFqXMlWs9YGao15BHYSSNqLayxDH6mJhQQiGNFVAulBpBVafDReFFoKDHCmOmS3eXYksWqxqamvGp458z0Z/avanWGy8nnewOqtiby2t3JTdkQP07g83VbH7W6r251Pmdr7q23uDau78NunZIyu/Ow2qsvSDHZD7eOAhXcwrOImWO9y5T3nfNotuWub94gvOXHsh+9LmHx7G6muopY5UliaCfTbQfp1ZA/qtSpPR/a7xb2G4tumy2hhvllP0sThJ40jZGQowdP1XoxoStSaHBHQcZrYGV21s7rzeFZVbZfG9h0u6GxGOxW6sRmtz447Pz8m38qd7bZo6uXMbJqamsUNRRV0MBrab96IFOSKtt5gtdz3nmPZYYboXG3NAJZZYHjgf6iISp9NMQI7gKuJChOhu1s9ILnbpbWx2y8dovCuRJoRHDSL4b6G8RPijqfhBA1DI6EHaY7C7ng6g+Nmx9nbZzu4qzsDIYzr2nwW2dr4Tf+7t39n1uDxUGB3Bv2cY6szOLjrKCFcfDkqtKTG+SRlZAzEoriy2nlu/5j52vt0u1jktIxdJLNNJbRR2wch4bYaljdg51lF1SEDFeN1muL63sNpjt4ux28NlVVdi+SHkJAIHlWlBxNAKSe6utava2d682dj87s3fe+shsqj/vbtXrTbO5aTc/X++abL5fbmW6i3/jqrC41c32LtJ9u6qmfGRVNNKtQXWedWD+03Lm72z2O9btci4tdnFy8kU+4TKYpIWCyLcxOzVjglElVVjRQAKKaqFO6JPc3NlCsUT3ggSIx2selgyDTodUHfKKdzUqxqTXB6BPa29cptHPbOyclDid34LZW98TvuHrnfNPV7g6z3Bl8ZXYuqraHdO0FrqOjyeK3LS4eHH5ZEeCesx5aBpVBBAi3Ha7fcLfcIg7293cWzWpvLYiO5RGDAGOXSSrRli6cQr91OimKd42hNFeJJBIIpKlCwI+JagEECjeZGOou5900m7ew9y77rdn7TwVDurfGZ3lV9ebHoanaew8JQ5zP1Gbqdj7LxkFXWVm1tnY+nqWoMfCk80tDRqgV2ZATq326az2SDabbc52uYrVbaO9uSs05ZIwizylgFllJGtqgB2rUAHrfio921xJAnhtL4jQpVEoWqUWlSiUwKZA4dNm/wDLbX3JvLdWa2XsqHrjaGYzWRr9t7Bpc/lt0QbOw1TM70W36fc2dJzebjx0R0LVVX7zj6/T23sFpuu2bLtVjvm9nct5hhSO53BoY4DcSAd0pgi/Ti1HOlcDq+4z2lzeXU9jYi1s3cmK3DtJ4anggdu5qepz0md27s3FuBMjDW14pcblK/G5et29g6aDb+0pcxiMT/A8fl02nh0pNvxZanxZaL7lafzsZZWL3le99u2bb9sjgWCJmliR41nnd5p9DyGRkM8peVk1muktQAAAUUdaurue7kklnKDWVZkiVY46qoUERoAgOkcQKnJOSekBtXcOD2huaPO7k672r2thocRurGz7G3tW7sx228hWbh2vmNv4rNVNZsrP7Y3HHkdm5XJQ5nHiOsWnfIUEK1Uc9MZYJFzg0wc+X+qvSdTT7PTpOdkdmQdg5brGvy/VfUm3KDrTrXr/AKxrMF1jtOTrej7LoNgw1FNLvTsqqwuRqMjne198JUls9uGOSGprnSNgiFBcI2ewTbba75Ba79fST3tzPdpPdyC4a2aalI7dZF0rbwkfpxEFVyM16OFvYnnsprixiaKJURokrGJAvHWyEHU/4mBB6avjlsPBb17Zp23nsXPdjdbbF23vPtHs7Zm1exNpdX7hyXXuwsHWZ3Npit6b2ZsdRCj0QtURwR1GTqKNZVpI2qCpAc9xN8u9g5cH7s3q3sN9vbu223b7q6tZ7uEXNzMkSB4baj99SFYlY0cq0h0AgmexWCbhfSiW0ea0hgmuJkjkjibRHGzFg0hAIU0JUdzKCFoxB6Zu7NnZWl7N7TyGE+P+/OgdoY/L0O6KXqXdKb3z1f01sfsFKHN9a4fc+6t44XEbirMfmMBnaF8VlcrT0r5qnqYZodYlQkVbXbX1nt9labpuBu9wjjVJ7kxrF4rgUZ/DUlU1HOkYHRTM8ckryQxBIiaqgJIUelTkj5nPSSp831/RbW3fhF2HU53cefp9kttbfWY3Lk8dkOvK3D1NVU73ioNt4Z029ujH70jnjpY2yKtNj4oFkhtKzkoJLLfZty2q8/fSw2EDXAubOKJWW5Vwoty0sg8SJoKFj4eHLEHtA6XNNtaQXEMFk7yusWiaVqNGwzLpVOxlcmg1ZAFePSCNgrXKqR/aa2leL6iSQLD/ABIHs96L6AAg8a9C1v7CY+fcmzNo7X6r3f1xu3HbI2pgd57e3jla2sze5ew5KSXIZfeFHj83h8BVbRw266CtpJ6PFOJI6eFRIkzrKD7DGyz3trZbzuO88yW19YPeTT2k1vEI0gtKhY7dmWSUTvCVYNL2liaFBp6NZ4Y7262+z2vbJIrsxJE8bvrMk2SzrqVfDVxSiZApxNenLqjtrM9PS1mb23m8pJl/43t3KptA1lZDtD+9fX2fxW7+u96b223UR1+zuzaTae46KYwYLNUNTRO0rs9gxBvveyjfZLaGSGNbZVbVcFVaRo5UeKeCNu2SAyIVJlRg2AB1W1ngtLaaRpXa7ZingjUoUrpZJSw7X0tUaCPnXoPN1bky29d1bo3tuBqF87vHcec3ZnXxmLx2Cxj5rceUqszlXxuDw1LQ4fCY5q+tkMFHSQQ01NGVjiRUVR7O7KzhsLOzsLYMLeCJIY9bM7aUUKup3JZjQZZiSTkknotlkaaSSV6a2YsaAAVJqaAUAFTwGOmT2p6b6cKirpZqDG0kWLpaerojW/dZOJ6hqzLCqnWWnSrSWZqaJceimOLxKmpWu9zY+2I4ZEnuJWuXaN9OmJgulNIodJA1HWTU1J+XSiSaJ4LaFbVFlTVqlXVqk1EEagSVGjgKAVHHpfdf5vrvbf8ApHp+weuZOznznXG5Nsdd1lDvrM7Jh667MrqzEybc7UdcXjqs75o9u0dLVxHA1gp6St+7DySoY1BQ7jbbpdja22zdPoxHdJNdK0SymaABtdvlh4RclT4i1K6aAGvV4TDEZ1lh8QFCqEMVCtijj+KnoePWDrLr/Ndrdh7I6x21Wbdxuf39ufE7VxGQ3bnqDau1cdW5eqSnTIbi3Hk3ShwuFoVZpqmofUUiQ6Ud9KMp3C/tNrs7jcL+Xw7KIapJKMwUVA1EKCdIJqx4KKsaAHrcEEtxKkFumqZsKooKmhNBXiTTA4k4FSemfceCfa+49x7bmymCzc228/m9vzZvbGVhzm18xJg8lVYuXL7azlOqU+a27k3pDPQ1iBUqqR45QAGt7W/YajyI8/Q/n0yDUBiKfI9Cbt3pqv3htTGbl67zmH7G3PS7e7N3/wBqdYYKhzuP3J1L1z1TNt3/AH929M1m6LD7azWH3tj83NNQx4Ktr66kgo5RPHFI0IYl3zmDZ+XotsbedzS2+tvYtttC4Y6rq4JEMYorDU7A0rRajuIHSuysrzcHuls7UyeDC1xKBTEcdC7HIwAfLPp0mN+7h27uzee5dzbR2JhusNs5vJyV+E6827lM5m8FtCgkihRMRi8tuWrrs9X0qPG0muqleTVIRwoAFtg2/cdp2Xbdt3bfJtz3OCIJNuFwkUUk7AmrvHCqxIc0ooAoPWvTN7PDcXMsttaiGBjVYlJYKKU4nJrSp4ZOAB0902N2tnOvaKh2vsrsnNduYXL7y3RvnL4x4c/sodSY3CYmbHPR7UxmHlzmHyW3K+KuqMvlaqpOP+1mhU+OxPtHLdbnt2/T3W67zt0PKU0NvbWMUgMdyb95JA4MzyCKRZUKLFEi+IXDHPT8cMM1mq21rO+4IXklKjUghVRmgBYaTlmNAB5muJ/a+xt0dd9hZnZG8N17P3xuPCUW1vvNz7B7LwXb+zq6ky+0MDuDDUuF7E2zk8xhM2mEwmWp6GpghnY4uuppqB1SWmdAfw20FqggtoI4otTNojVVXU5LMdKgCrMSWNKliSc9JPGeb9SRmMnCrEk4FAKnNAAAPQYHT/t/pjs/MdS7v73w2xs3lOnuvd7bV66312DRpRTYTam9d8UFfkto4TNQCs/i9KdwUuMlEFV9s1CJikDTrPLHG1pLq0tXs4bi6jjmuZDDbo7ANK6xvKUjBNXYRRu5ArRVZuAPXkWSQTeHGzCNdcjAGigsqBmPkCzKBXzIHn0/9UUvUTZ3M/6bH7Qi2udib4O2T1HFtSXcbdqDA1H+jBM+u8nTFp1y26vD/eBoL5EY8MKW0pBCbdRvpgtxy+LP6v6iLxvrfE0fT6x4+jwu7xvDr4de3V8VRg7ia31N9T4hTSdPh0B1fhrUEaa8fOmARx6bcXRVSQU9QSkU+sIk1PIf262JI5mlhUOKtI4nYGOSynjhtQ4OB4TM8TLqQipBGCpqKHGk14EftFD0mJlVVlR9Lg9rA5DChBFDqFOIPr546EiRaCryM1RjYMjBSzeGTTl64ZLIyVjQxmvqaiuCIZzVVpkkXUCyqwDMTc+2bCG5gtIobt4mlSorAnhxhKnw1VKmmlKD0JGAAenb+W2uLuWa0SVYWoaTv4kheg8Rmeg1anqwrmhya9KygpwoU/Q2uoJ/3n/WAPtUc8Okop0a/oLv6v6NFPX7P2/hdtdo4PftB2V118h8HiKDI9wdebiw20s9tnEbRxc+55q7ZbdU5yuzpq8/S1OMq55QhaMMyx6AbzVyy/MApJdNLtjwi2u9tmd1t5ojMkskg8HTL9WFSkLBgAwUVUFtRrt11FbyEMmmapMU6BS6uU0qG1gr4NTV8HBOCaUC3+Ez/wCY/v1svx/3z8Wr+8Mvh/jNv4l/fzX/AA2/91vuvR979fuPR4bc+zH94x01/wBW9yr+7fGp4Aroro+kp4n+5VM+H/DnXXpb+6Fro/rDttPrvpa+MaVpq+qr4f8AuLXHifxY09Aju+l3h2/vDO7q291jhKCryuIye46vZnSWyZaHau3du9e7ex1LurcFBsjBT5ut2pt/GY7HjJZWrqtFO1RNUVevQz6Edmdn5O2ew23dOaZXiSZLVL3e7lTNNNdSsYIWuJRGs0zu/hxItWoEjAqBVJJ9Zu95cT2+2KHKGRoLKIhESJAHcRrqKIoGpmOKktWh6D6nl2BQdf5mtE+5qrtms3JHh8ZiqnAbbyXWB6sy22q9M7nny1VVNuGh7Lotx/bLjfBAaeKlZ5Q4kA92vIOYrjmOzgMdqvJ0dt40sqTTR3318c6mKLw1HgvZNDq8UM2ovRaFerW8thBt80ne27u/hqrojQeAyEO9Sdazh6aCBgZBr0iMFWbMxybtG8tm5bd0uT2VmsPsmbFbxfaA2Z2BWT0D7f31l4lweaXeWFwkEFTHNgnNElc1QjGpj8VmWbta7xcnazs+7RWgivI5bsSweP49socSW6HxI/AeQlSJu/RpI0HVUMWstpELr6u1aUtCyRaX0aJDTTIe1taqAezFa8RTN4n8gb4idh5752dS/ITdGwNr1W1+neqdyfJzprFdndkYjqvZfdHZ0e76Hov45bKpt/HHbtfaeW3d8mN44ajxpqMZPUzV1KqRUtSzxwzJ9u5j2Per/f8AbNq3JJtw2q4Wz3GJQ1YJniWZY3qACTE4aqlhmla46vcbdeWcFldXNuyW91GZLdzQh0DFCwoSQAVPGh+XRQv53Hw/b4R/zL/kt1Dj8NBgti7i3WO4uqqKi+/fEQdedsxf3xx2GwVVk0jrchjNj5nIV23fuHBMk2IkJN7+zc+tMdJgRWvmc/6vz6rvx/U/blVi+r8nt3bWbraP5D5vc/XPVlLtfM4/IZjsvObbz2C27ubZn91sFlptyRL/AHhzdBTpTZSkp6fJu4an86Rs6F+6z7VY2Fxuu9vBHtlkrXkk9xp0QCJWZptTYQxpqOoUIFaHp2AzyTfT2xfxpP0tKkjVqNNJoRUE8QcevUWjq9o9edg1lPujrR99UOBwub2puTY+8t11OOSDsI4CswGUzNPndiLj5xRbU3kzVuPo2MhYU6wVbyHW3sluIt25i5fhk2rmT6GeeeO6t760gVybUTLIsZiudY1T2/6cj4oWLxhcDoyItts3KWG6sPGWJWhlikkx4ukqzK8VKqsmVGcCjEnPTT1zvmLZ9ZQ4Xd1HuTe/T1fufBbl7J6hxO+MvsDDdlS7eWtXHNkshh4q1Mdl6JshK1NXfbTz02twltRIe5i2A7tDPebRLbWPNyW0tvt27y2sd1JZ+Np16EcrrRtC6k1KGoK8OmtvvhaOkV0kk21NIr3FosjRLLorSpWtCKmhoSPLp5xMXQ8PWu6MnuCfsnK9u5Wr3Bi9l7OwyYvDbG2NTJNgq7bO9NxbvrVyeR35HUQNkMdU4WKjx0iFYqr7kn9v2jvG56k5j2212+PbouU4kilvLyYvJc3LESrNbxW6lEtqHw5FmLyDJTQOPW4htQs55Jmma/YssUS0CoOKuzmurONNMivDB6Q27l2Csm2h1/NveWJtmbcfe43rHg6cp2QIqn+9cG1kwErx1Gxaedo/4XJW/wC5Aq0nmsbezjZ/6wU3T+sC2Qb62b6H6IyH/E6jwDP4oBFyRXxQn6daaembv6Ctt9AZ6eCnj+NpH62dejScx1+Gvd69Tspv/wDjGL6ww2Z2ZseTC9XUtdjzHgcENq57f2Mye5JtyZCPsTdGFkTM7hyd52oqauBSpo6G0cfKghNb8vmzuuZr603m9+s3Nlf9eUzRWrpCIVNpBJWOJO0OyZV3qW49Xe+Ese3RTWcJhtqg6F0NKC+oiV17mPkDxA4Z6UVd0pV0u6ty4LJb96Y2z/D+qa7ujF5av7DpKvbu6dv/AN1ot44Dr7auaw9Nm5qztrcOPqkocdt+vWkrDkEeCqendSSp2Ld4t7sPqYYLqMxzS20iXcTQyCWF2jkOlgAysykq6VRwQUJHTW4230F00PixSIQHSSE6lKsKihNGGPJgDj8+gP8AImpF1APIutEYgOy2JJ0gn6AG9r2sfZvQ+n29Jag0zx6Vuxdj1HYW6KfbFFuPZW1Z6rH53IjNdg7nodn7WhXA4TIZ2alqc/kA1LBkMlDjmgooSC1VVyRxLy4sTb/vUfL+1y7pLt15dIskUfgWELTzHxZUiDCJO4ohfU5/CgZjgdKLKy/eF0tslzDESrNrncIg0qWoWOAWpRR5kgdN9duqjrdlbc2imztqY6swWb3DnJ980dHlYt9blg3BT4eGm29uermy9Vhp8Ftj+Es+Njp6KmmikrJ/LLMCgR+HbpYd1vt0bdLl454YoRZuUNvEYjITJEojEgkl1gSFnYEIlFWhqy84a2itvAQFGLeIB3tqphjXIWmBTGenTE7r22Ni7o2vufbWZ3HmzBjj1XnafdkmHxHW1fUZ+lyO96yu2ymKq03em78RSLSrG9TSiimUTguRo9obva9ybfdr3TbNyht7EFxukDQCSS7URMlsqzeIvgeBIxckK+sduOPSqK+g/d1xZXUDySCn0rCTSsJLAykppIfxFFOIoc565NsnfG0cF172lUQQbfwm7pdx5zrjcVRXY2r/AI1kOtM1S0eZjpsZSNk66ir8fnTDHAmSpaenqm5DtFdvfl3rZN4v+YOWIZTPf2SwxbjbhXXw1u4y0dXYKrh46k+GzFfOhp1U2V7ZwbfubpogmLtbyVU6jEwDYBJBVqfEAD9nTDvHdm4uwt27p33vPJvnd272z+X3RurMTU1FSyZfPZ6tmyOXyEtHjqajx1M1ZWVDuY4IYoVvZUVQB7Mdp2uw2Pa9t2XarcQ7ZaQJbW0QLNojjUIi6mLMdKgCpJJ8yek13dT311cXl1JruZXaSRqAamYksaAACpPkAOnLe3Ym/uya3C5bsbe2597122tpbe2LgchurMV2bqcFsjZ9EcftjauNmrJJpKTAYChvHS06eiMM1hcm9rDbLDbVni26yihWWZp5BEoXXI5q7tTizUFSfQenTck0spQzSFtKhQWPADgPs6Ve6+u989X7jqNldj7O3BsXdtFQ4bJVm2t04uoxGYpsfuHE0edwddJRVSrJ9plcPkYKqnkF1kikUg/UBvYOYNi5o2uLeeW93tr7aHeSNLm0kWSMvFI0Uqh1JBMcqMrDyII6fvrC9225ez3C1khulAJjkUqwDAMpoc0INR0ttnZre+zMdnpMLmt97T252XtzJbH3IdvZTN7cwnZW1aXM4TN5bZefmpZKbF7z2vSbjxGNq6vHTfdU8VdS0sksYljiIOllSR3hhliNzHpLrUEpqrpJUGo1AGlaVoadF7gChdW8M10kYrTjQ+dPPpa4/c+Wz2Zpqve+Tqt4SvtzF7Dp81varzm66/aW2cfQ4/b+Dn281Rmaeqg/uFgaKOLEUfm+ypYIRCkITSFvPZeKsIguZbcJMtwwt9C+LpyY5NSNVJODUox8mHTUU2guXhjlLRmIGXUdGqnehDCjLxFaj1B6ELsDb+19tb33Zt7Ze7cj2BtTb+7M5gdob7q8TDgYt37Pxs0K7czv8BiyGXmwOTydHMJ6mhNXUpRmVYhLIyM5csJnniSYwiMOgkZCCrhiWDFgeANBTz418uvXFQxQyFwnYpJBGkAUAI9K/Z6Zr1Kz+8NwbtptrUWdnpXptk7Xotnbcp6PG0WNSiwlBPUVSJUCihhNdXz1VVJJPUzF5pXbk8e0+1bHt2zSbvPYRuJb66a9uWd3ctK4VSRrJ0qFUBVWigDA6vc3lxdJaRzsCsEQhiAAFFBr5cSSaknz6yZHdWUym1NsbOrEwyYrZtfuLIYRqXAYylzVVUbrnx82XXL7hpaZMnl6ambGRmliqpXjplZ1iA1n3u22e0s943Xe4WnN5fRwxzh5ZGiAtw4j8OJmKRk+IdRQAsaFuHW5b6WaxtLGTw/AgZ2j0oocmQqW1OAGYDSKAk08umOnLo4eMssiuHjdHaN1kQ6kZHWzI6MAQwsQeRz7NiAwIYVU4IPSAVDGnEcOlMiQRTSGmkedG0M8s8QillfR69aBnuEdiASSSOfz7omsoNahTkUBrj7encA4NfmepccjKVdXZJEZXR0YxyRujB0kjdSrI8bAFWBBUi45HurrqqGFQRkHh8x9nTwIp6UOP8nTntvdO6tjbgw+8Nkblz2z92bdrUyWB3VtjLV2D3FhMjGrJHX4nM46enr6CuVHYeWORXsx559o902zbd62652redugu9snTRNbXKLJFItQaPG4KstQDQjyHVoLm4tLiO6s7h4rpDVJIyVZTwwwNQaGnWPauW2fjot34/eG16POLuTbMuKwG5JqncH8T663BHl8bmI93YTFYjL4uh3Fka2lx02Llp8mKijSmyEs4jM0cbKh3y03ub903Gybi0L29ystxbARBLqIo0bQPI8cjRKpcSho6MWjCVCsele1ttYkuIt1RhDJGyrOoZ2icDUrBAyh9TDSQTgMWzShQb18pxSY37DGaoq2XIisWnC5SWWSlWn/AIfNkPJ+5i0K60i0jTIS2r8ezb6ZFvWvPqJSWjEXhFv0wAxbWEpiQ1oT5igpjpIbpvoFsvpoQRKZfFC/qklQugvXMYpULT4s16WHZ2J6xw2cxdN1NvTdG+tu1GzNnZDNZjd2z6fZOSx++shgqSq3vtmixdPms4K7B7dzryU9JkDJGa2Ma9AABKLZ5t4uLed982+K2uhPIsaQyeKrRBqRuWoKMw4j7CQpOkUnS2R1+mmZ4yoJLrpIbzFPl/sVNK9BRPBTyxVhnrFpGho5ZaRDSz1P39Ys0CR45WhuKNpopHk88v7SCLS3Lr7MJXkQxiOLWGejmoGkUJ1Z+IAgCgya/I9N4oSzUoMYrU14Y4V9eGOg2yMNi4/NiR/r/k/7H349VTjqP+odB5UJSCui/if3/wDDvKfvP4V9p/EjCUYj7I1/+Ribyhb+X06L/wBq3tDcCXw38Ar41O3XXTX50z+zpZHor3g6POnH+fWXeVJsDBbQ2pR7Uz9N2Bnd7bWw25OxpM915k9p5TpjfGG3RvTGzdc7Kzrbvy2L39gM9tgYvKV+YahphLJUR0kUMRpJJqkuuLV5L20vFvZkjiSRGgUr4chk0UaQFS5aPR2aWUDW+oNiimOYLbzwNbxkuykSGupdNcLkKA+ruqD8IoRmrU3Zvc+5Tunbq9jdp7jbtuLZW3d84H++G7c1L2lDsmoxi9b4DdmL/iNVLvmLZ9Vi6IYKkq0qhj5KaEUqIY0teSWOGN5ppFWJVLMzEAAAVJJOAAOJ6oqFiqotW4ADjn06DeSJqdpI51eGWB3SeOZWikhkiJWWKaKQB4pYnBVlYBlYEEAi3uwIYBlNQcgjz+zr2VOeI9elNvPYO9ev8lRYTfu087tHK5Tb+D3TQ4zceNqcVW1u2d0Y+LKbfzcNNUpFK+NzONnWaCS3rQ/j6eyvaN82bmC2mvNj3SC7tI55bWSS3dZFWaFzHLGSpIDxuCrDyPSm6tLuykSO8t3ilZBIFcFSVbKmnoepm/8AsTf3a+7srv8A7P3nuXsLfWdTGR5veG8MvWZ7ceXTDYmhwOJXIZavlmq6pcbhcZT0sIZj44IUUcD2o27bdv2iyh27arKK3sI6+HDCoRF1MWaiigFWJJ+Z6ZmmluJGlnkLytxZjUn7T0p6Sr7M7uq+qeto8nHufJ7djw/UXUO05ziMNURUW6t05vM0eCx+SelxuPkpP7052oknqsrWiSJqyMCQxAiImnTl3k635n5klh+mtJfE3XdLkeJICYYI0aQoC7VEMSgLGudJ7dRyvQ7hvMm2bcjeJKmm1tYzpXDuzBQTQfG5yxxXjTh1t2uwvW+X3/jt7bNzOT33hqStwWychiN6Jt//AEY9pbf3NQkbsr46HHZqj3rSYgYuqphQrNDBLJIsqzEKL63CG85jtNhudl3iGPZJnWe8SW3Mv1llLC48BdTxtbs5dG16WYBSpXOLWsqbXcXYubZjfx1WF0k0+DMjgh8Bg+kqRTgeNek5s3dMO1d54LeOT2rtjsGLDZqLN120N902TrtobsZJmnmxm6aTC5TB5WqxVdI5My09XTSk2IcezXddubc9qvdqt9xubJpoTCl1ZFFmhqKB4jIkiB18iysPl0jt7jwblLl4UlIbUUlFVb/TAEVHUttm1FRsWo7IGe2XBRHfQ2WdnruOkTfqVdRgpNyLm6XZkhfKNsanph9oMmXaNazTAbsdRY/fCLv6cufQ3hm+h+t+sMLfS0Egi8I3GE+pJ7/C4lKtw6eNkzWJ3Hx4dBn8HwtY8WpXXqEfxeH5auFccekqWSIKGZVBIRdRA1MfoPwCx9nNK8Ok+BQdLXH7OhyPX28t+zbw2JQf3Q3Bs/br9f5XNzwdlbuTd9LuSrfcGyNrLjp6fP7X2cNthM7UvV07UD5CjCxy+UlNitVI4ngeqM4BpSvS23bgKrp7d20dv12L67zG8tjVGB3fncjhdzUvZmz9xyZiLBbz23tjcSUFbW7Mr4Nv4yWOkyNLjpGSfzzU1U/nidUCe2XSc27Xu93Fc7hDtV6stpCksRtJ4ghkglmhLKtwplarRtIARpV0GlhU5u4RtVxYxabaW5iCzyMjeKjFtLrFIMxnQMMEqprQkkdIvdOfqd17o3LuufHYLCVe6c/mNwVeG2piodvbYxcmcyE2RqsTt3A0bfa4fb9K85jpaJSYYIVROVX2e7Tt8W07Ztm1JczzxWtvHbrPduZZ38JAiyTSt3SStSrucsxJ4notu7k3V3c3JjjRpZGkKRKERdRJ0oowqCuBwAoOh/21TfDut7B35hNx5H5D4LqvLS4KHqvssUWx8zvvYkNLGlXujI9h9YYs0uF3/Lm6iNsfQU+Oy2LFBFKKyR5XQwsANxf3jt+Xthv9vt+XbjmqEStuu2BrmO2uix0wpaXr6pLURA+I7SQS+IR4ahQdYPIk5Te/vone/j2xiotrhhG0kYAqxliWgkLHtXS66R3Gpx0gsR2JBtbZOLxewcZurYfZdS3YeC7F7QwHYudpI+x+rt8Y/D4+l6xq9l0cNJQ4XEY+Oiq/v5Fq6kZiOsEc8YWFSRLdctybpvlzd79c2l/y2v0k+3bXcWcTGzvbZ5Xa9W5Ys0kjl08MaF8Ex6lNXPSCLcPpbSOOyjlgvyJUuLmOVh4sMgUeCUFFCgA1ydVaHgOodDmNq0/WlZsyPrvCtvabe9HuWg7YbNbgiy+M2vT4KsxtV1vHtKmqY9rT4TI5mojyb17RnIJNEIkYRk+zH93bq3M0G8DmKUbAti1s+0CKExvcGVXW8M5XxxIkYMQjB8MhtRFR0yJ7Ybc9p+70N8ZxIt1qfUsYQqYtFdBUsQ2r4qigx0NGL6T7M3HmeqcR1tszfUO2fk/uDF7R6Upt07m25jMV2lvDD5rF7TyOFqt0SVG1uvWqNt7/AM14i2ReljwsVbC1TJGS8xTbNuu2bruO5bZcXthc83bQwS9S3Qq9sLoM8GlZS8sa3ECjuDaZCrUwAA9uNpdWNta3SRzR7Rep4sBd1bxPCOl9Xh0TVHJXtIDKCK5NSgJsRW4jKZHDZKFaXJ4bK5HB5OmE0FQtNlcTXVGMyNItVSyz0dWYK6lkjEkMkkMunVG7IQxFiqSRT0r+XRNqFKg46W23MJkMzlMThMRRyV+Zz2TxuEw2Ph8azZDLZeshx2LoInleOFZa2uqY40Mjois4LMq3IbvLy12+zvNxvpxFYW0L3E8rVokcal5HIAJoqKSaAnGATjrSRyTzQ20KFp5HWNFHFmYhVUVoMsaZx0N823aTrwdp9bdkdeZ2m7hwe5sTtvG5E7wgxlJ1bl9o5rJU/ZOC3LtOhxuWod+VO44GhpKaZMjSpiZaZ5UNR5LKSWV6/Mi8p80cs8xQvydcWr3Tx/TlzfR3ESNZyxTO8b2oiNXYGNjKG0kJp6VzwDbm3XbNz2913iORYlbxABA0bHxldAGWUuKKDqGihIrXpTdcTbBbIVmH7Qm3RjtlZDGZmubLbA2/t3M76pd24rb2Z/uHQ0U245qWCj2jk90VVPHnRHJ5Gov3EVpIltrmSDmP6e3vuUUtZN+ikSMQ7jNPHaNBJLF9U7rCCWuI4FYwEigckE0Y1c2+ayXxbXcw4sXGsvbojTCRVbwwrPwjZm/UA+IAcKVEbE7U3Vk9v1O4KLbuYqcDQZbC7YzO6KOhq12piN0bkhqJcHgMlumoSPBYbKZlKOZ6SKrqYZJo4ndQVRj7N5922i23GHa5dygXcpIpLmG0d18eSCIgSSpAD4siR1AdkUgEgHJ6TR213Javci2cwIyxSTKp8NXcdqF6aVZqdoJBPQjf6R6j77+If6Lukf8AmUX+hT7P/R5S/wAP8H93f7sf6UPtP4xb/Tvb/L/71X/4uf8AlPhvx7Jf6tr4Pg/1m3r/AJK/751fVHVXxfF+ir4f/JM/B9N/vvt1dK/r5Nev912X+4f0dPCxTTo8amr/AHJ8/F/izToL+q9hxZra/bm96T5QdZfHzcGyNiboFHtHdW5+xdrdgd5Yet21kZsv1v17PsnbWTxWVO8YoP4PLQ5WuoqarnqkjkR4fIyIeab2Ebly7st77f3W87fcXMU31aw201pYzRzIIp5hO4dJYifGR0QlQjEMGoDqw8Vbe7urfeUtrlVMXhh3SWZGQ61XTQMjU0MCckgFSM9FJrPBE0kDmOmeCCOaSmkKRtTROfEgkjB0xprXSP7Nxx7GDA1JJrn4vX16QqRQLwHp6dXp/wAoj+c7F8Dc3jOnvk30/s35EfE7KZdXkiy+xtobh7Y6beunX7/Mdd53O0Bnzu3QWM9RtquqVpjIpkoJqKWSp+6bI9DQ9OajQDUR6f6vTrdu+FO4usvlz3RlPkd0hsXa20Ogt/78qa7qvdu1/iisGz+7fjr8Qkqtr7SbdfZm7qChxvXPZOc+Znde5d3bdio8ZS7hmwOw4QI6YxVdXOjS3MU9zObiRjJp7GYFU0inYoApXixJJJ86AAXd/wBNFotQDkVqa5znNPLgPzr0ez51d0fC74n9Nbm+U3zHwnXp2lsqgpsFSZjcOwMHvfee4MlVtkavbvXeyaOuxtXkcpnM9XvUfaUglhpImeaoqJKenSoqI3gTQiuOmlLeRoOvl+fzWf5u+9P5iG/GxfXPVGxPjD8c9qZlazr/AK164wGE27unPVGPmnbG7x7c3jtmixtZubdTB4pKejp3jxOEEMYpInqhPkKqsiiUMkvfCVKsjAEMDxqDWopinA1z5dPKxVe0kPUENU1FPSn7fUU6vww38rHP/wAyv+XD/IP6n6q2k+z9qZas+RG6/kd3hBt3Dtmtp9WYTekNOclujO0FDTwZ3eeapmahwNNUSMJ6+W5C08VRJHZdXhqJGXWAKhAQOGaV4AcOvFgNfHSKUBPy/wAvVGf87j5x9I/ILuLavxb+GGx9odd/B/4b0J6q6nh2ngKPF1na+5drQDa24O1915r7WLcG6zL/AA16PDz5WaprDTfc10jLV5WtB8aioPXqmlCej4f8KG9nbR2t85v5V1Dtnau3NuUOZ+FPxXyuYo8Fg8ZiKXLZSu7f33DXZLJU+PpaeKur6yGFFlmlDySKoDEgD3bzH29bBJY1/i6N3/wp4/kvbZ2/lt3/AMw74ZbbwDYPD1+GwnzJ6X67pMdr683NksfiJtudu0G1MCzNh4N1YvMUH8foI6WCRJaimzASWOurZ4q8ft6orY7uPr69Ft/nbbD682x/Np/lJYFtq0u0MVlfhf8ABjIZLEbX2jg6AZXetZ8iO3qSE7pw8yYqnkhylVTRU+VqJVkrFp0sEkZQntPdNeDwfokiZ/GQP4rMoERYeIVKqxMgSpQGgJwSBnp+DwWkf6h3CUbToAJ1U7QakUUnieIHAHq4v+a18t/5o3w8+TXemH+J38ov4ldr/DfqjZ+3d8Y/vreXxC3zueJMRB1bgt69nZjO7x2b2zsja5xuz8+2Uilkix1P9tT0emUu6NK6k1bHGvHpOC/aVc1+3qqv/hON8o95fIv51fzTuz9+bA6bfF9pfFnsX5Tbh6VxnXGPqOnIe2tg9gbJ/uVLgNv7hqdw7nxG38BSbsyVLBQx5ghoass7vNHDLGiO3WMl/bbm1uPr4Ynt4pKmqxyFGdQK6e4xrmlRSgIBINxPMytGZDoZgW+ZAIqTx8+jwfFH5I9sfzDfg/8AzPO8flr/AC8/jr8Ne3/hr8ad/wC9+gvk31R0BU9H7zxG7c50b2jlpdr0tB3RFvvN19DVbdpadsgVrjjarG5qFGpVmlpKpUO4bfsfNu0myvVjvNnldXOiQ6WaGUMpDxMDVJIxWjcQQcVHTsUt3YzrIupLgAgahmjChwwxg/5R1V3/AC3sX0x/LL/ky7w/m+9i/H7r75HfI3sT5AT/AB7+GG2u6dsjcXV3WMdPJk1ze9P4b5KGvqqvKZnaW4pa6rgqBXlcFR4+hq8cKrITOax28MU09yiUnlC+IwrVguFHGgpXyA+deqvc3D29vbPKfAi1NGuO0uRqoaVyQDk/s6ND8XPlXt//AIUd/Gf5zfHL5vfH3pLF/M/or47bj+SXxz+VXVvX6bJ3nMmzZWxsGH3RkqipzGUkw0W4K7D4qopqWY4rL4SeTVSxZDHQVrvDh0wM0HlWlPt6J98LemNl47/hLx/NH7ardt1OR33ubtXqasxOa3P1mMVDgcPjO7uodmfc9YdkZKGdd34rKJQVsOTlxkscdFkYajHzL5Ynumt5rx57yK4t1S0QgQOG1GQFAWLLTso9VAzUDVXNBZtAjj0PVzXWPT0+3Gf5U9dUUpc8f7H/AFh7f6Z62v8A+eHsPp3E7I/4T7x7n2/itq9f7t+CPReQ7hyG08TjMHlctgcjh+ll3nnKyqoaONq/PPhp6lxU1AlkMhuSebukVc/InpwmukNw1H/J1dZ/OP8AmB87f5eCYTaPxl+E3xZ7I/lFZHpjaWM693g/UKd5bDqMhlth0GDp9zdjZqPO5jA4nJ4ysqqU4KrzVDU4vcdAkLST5GWWpjhYs7Kzs0MNlaxwxlmdkhVUGpjVjRQBVjknzPTk1zcTsJLmZ5HVQtXYkhRwUVJooHl5eXWiFUdj9j7o2H131fuXe+5c71z1NUbxrOr9kZTJzVW29gVXYeUpc5vubauOe8eLbdeZo4qqtCcSzrqsCWvey2ba7Lctz3a0sIo9yvfD+rnUUebwV0Raz5lE7R8qDyHSOe4lkiiheRjDHXw1PBdRq1PtOfz+fWLGwkG5B4ueATf8+n6ezpfQ9IuA6ECKgakmo0pp6WsqZoKKphfFu9UY6io/diovTEr/AMQpprLJEFbS5sL39sxzLPFO0sTxxKzo3igLULgtxPYwyDiozjpRJC0EsAimSSUqkimE6qFshOFfEU4I8j69CZW7Po6bbeS3Rl+wtptn3bFyU+yKI5TJbvra3M/eS1seXiWhpcdt18CKGRch5pWaGd4Y1V/JqUmtN5mlvbfbbLl+6FgrPG13JoSFUjUaXiOpmmWQsojoBUamqNJHSu4tQEnubvcYzdsA/hLVnLsTqWQUURstCWrWhoPPoP3WHxQsskhqGlnWWLxBY44VWnNPIk3kYyvO7yh00KIxGpu2shBEC+tgVHh0FDXJOailMAClDU1qcCmSgDtDA91SCP2U/bn/AFHqRCHCtpbQyqW1lPIEVeWZkAN1t9Tzb6+7YxXq9ME8D0ZvdeM6Tq8X23n6WLefUO86Tcmwf9EXR06f6RcLVbOzGPrpt7126u26uXBVdJXYQRUtVQq2PZqr7zxW0pqQDbBcc0Rxcu2s99b7vZtHcDcN3RBbMZUciIR2ql1AJqjUYjtLVU4YQbtaWsF1uCNZyWVwDGYbN2MulWVWOqUgVqp1CtDkCh8gQEThmV0kikU6WSWN45IzYGzxuFdH0kEAgGxB+hB9jTUjAMhBQ5qM1/2OiI6hggg+h6j1FtJC3AB/x5sD9fegc1PV9GP6XTBV2uT/AMFH+8m/t7prqLGoMiIXRNbpHre+iMO4UyyFVZhHGDdrAkKDYH6e2a6VZ6EkAkAcT8h5VPl1dRqdVLAVIFTwFfM/IcT1nyGLqKaXJmmZctjsVWQ0FRnsVDVz4NpqoTmhP37wRx0/8RFNJ9us3jebxtoB0n3S2uDcW8E8kDwu6BjDLQOp/hYAkVHnQkdPXUC21xcW6XEcyo5QTQ1Mb0/EpIB0nyqB0lapbRsxFvqf9cc/63FvbxFaEDHSbjx6HLrH4O/JLujIQ/wvrPsHaG2clsTcW/MDv/dPVPbtVsfcdJhts1G5cJiMFmdpbF3IMjk98pHHT4h0VqaomnT9yzLqjfmX3U5I5aSRJ+YbGe+juVtpbSG6tRNGxfQ5dJJkKiIg6wcjzoKkCCx5X36/0NFtVyIWTxElMMuhhSoowQg6vKnHyrwJZfkN8e+4vjhuaq292xsTc+3U/ieTxmC3RV7X3diNn71kxEVFNkarZGb3Xt7bbbko6RclCsrxQqY2lXUoDKWWcoc8cuc97VBuewX0bFo1kltmkiNxb6y2lbiOKSURMdBoCc0xwNPbtsW57FdPbbjbMAGKpIFcRyaaVMbMi6hkVxivRb89RrSVU1Eldjsl4REVrsVUmrx83mhjm0wVDRwF2h8vjcFRpkVh+L+z6CY3UCTeBJGST2SjSwoSMip40qM8CD0nuoPpZ3g+oil00/UhOpDUA4NBWlaH5g9d7K3hu3rfd+1+wNh7gye0t87Jz+L3TtLdGFqDS5fb+4cLVx12LyuOqLOI6ujqoldSQym1iCCQWLy0tr+1uLK8hElrKhjkQ8CpFCMZ/MZ9Om45HjdZENHBqD01ZDO5rMZ+v3RlsnWZTcmVzVVuPKZrISmsyORz9dkJMrXZeunn1mqrqzJyvPKzg65GJI5t79Ha28NqllFCq2ixiJY1FFCAaQoApQBcCnAdWE0omFxrPjBteo5Oqta/bXPWfcu5NwbuzNVuHdGYr87mq4QrUZHI1D1E7RUsSU9JSxayVp6Kipo1iggjCxQxqFRQot7a27bbDabOKw220SCzSumOMUFSSWPzZmJLE5JJJJPT+4bhebpeTX9/OZbuQ1d2pnAAwAAAAAABgdMirf8A1va3pH0Ofx52B1b2f2lgti9u9g746223uOSlxOJzPXPVNf3RuzK7tyeZxOLwe2MbsTFZrC5WtmzP3soiemNVP9xHHFHTyvKo9h/mS+5jsLGGbljYodw3AzKrwzXAtwsRVtUiuY5A7qwUBDpDVJ1rTpdYQ2MzzC/vGhjEZKFU16nqKKaEFVIJOrNKcM9I7J9bbxpJuyp8ZtHe9ftvqbMtit9Z+o2Zm8fFsaKq3JPtXbx7IiEFXT9d5PO5qJaGKiyc8Uv8T1Ual50K+zyFpXiieaMJMVBdQahWIyK0FQDitBXjTpG4UMwVqrU0J8x5fy6SVDU5DE5GmrKQzUOSx9VFU07ywBZ6SrpZRJG8lPVRMFkhlQXWRDyLEfj3qaGK5hlt501QyKUdcioOCMUOR6dO2809tPDcQNpnRg6N6EGoOajB9ehDk7Z7Dfquo6Tl3PKeq6ns5+56nabY3BLBJ2c+25NoSbsfM/wxdwJIdtytTGkFYuPAPk8Ak9fsuTY9rTeE35LSm7LaCwWXU+IA/iCPTq0fHnVTV5Vpjp97md4ngeWsLS+MRQfGRQtWleHlw+XSk2rvDuz465HdcOGXcfWGV7a6bzGwNy0e5dl0lPX7s6T7fxePq66OioN77fqpqfAb2w9PTz0OZx8cNQ8AElHVKGLFPd2HL/NMdk85iu4rG+W4iaKU0jurZiBUxOKtE9QyNUVwy9WjlurMyhNUbSRFG1L8UbgHGocGHAj8j0GsuTrKumxtHJHQNFicfPjKJkx1HDNHTVFW9a8s9TDFHPV1yTyHRUSs8qJ6AdIA9msdrFFLcTIz65XEj1diKhQoABJCrQZUUBOePWpbmWaK3hkCeHChjSiKDQsWJJABZqnDNUgY4U6cVTbn8Em8cWSx2fp5sPTUNFSRQVOAyVHoysm4szk62pq0yGNy71DUSUtJTQSUjJ5nZ0YAPX/HlvIwPDawZXaRmJEivVPCVFC6WQjXqZmDAhQAQTRmsAgerOLkMoUADSR3aiSTUMDpoAKcakUFcE2NyFJDj6qtx9fRUuWpZK7EVNZQ1VJTZihiq56CWuxFRURRw5Shhr6WWB5oGkiWaNoywdSAr6YUVJB64ol7H/bD/ivv3TtOPU+GDVa/1P8ATn/YfT3cDiBx8z145B6VW3qLH5PKYyirsxSYXF1OWpMbk8/UU1bkqTAUslXDT5DLVtBioarKVsWGp5Gnlp6aOSqkSMpGjOyg0upJoLS5mt7Vp7iONnjgVlVpWVSVjVnIRS5GkMxCgmrECp63EI5ZYo3mEcRYBpCCQoJALELViF4kAEnyz0qJoKJrY6CorMri6aGvpo1rZphjnrKmpnSoy2Dx7JEcfjMlTxU0/gnjFQ8gYVOuygegVyPHkiWK4cqzAAFtIApHIwrqZSWWoNAPgpXNHKgsgcvGNQGTSpxqUYpXBoRn8XQ5dZ9iQ9fZPceRpurent3x7l6m3V1Q+H7H2ZJvTB7eO7MGuEk7P2jRVeVpGwHbu3dIrMNl0eRMbWEyLA49PtDe7DJuFva28u/7jEYr9L8SWsoidgj6xayFU77RvgeOgLLgt59PSXqeJ4qbdbKPpxbmPSWWunSZqM1RMfi1A0B4DqFsytTD53DZiGlxOck2tnMJlpMRuKjTM4TKz4evp8nFiNzYtpIVyuFyjUfhrqZmQVNO8kepdRIO7u3+ptbi3Z5IhNG6eJCdDqGUrqjbOl11VU5oaHNOiyNwroy0YowNGyDQ1ow8waZHmK9C/vHekm/d2b/3ZJs/r3Zz9hb1ym9ptudd7Si2ttLZcuUyVXk22v1xhVra3+6Wx6R6wxQ44S1AWBEUyEi5LNu2hdug2i3G53s/0dt9KHuZdbTCir4tx2qJZ+3D0WlTQZ6XtemSK9h+jth40qyllTuj017ImLEpG1e5anVQZ9WVXgpo2aSVIvFGJJWZgvjiLaQ7D9SozG39L+zYVNKDjw6S6goGc8T8ujD9ZbIh3j1p21LlPkt1r0/hdqz7c3KnTPYm5t+0FR3xuCnxm5Ww9bsrau1cBntuZzcm2BRSUMVZlBTilmycaiaKNixB+/30O175y9dQ8h3W6bpLqtE3KyhgaSxhkeMSiSaVkkjgbDyKjdwQnS5BoaWUbz293bybwlvZ/wBqYJncJM6KShCLUNJ+FSVNCaVA4gn9zL/yrVP+Y+4/TD+u1vtf87/wIt+P0f7V7GWhf9+Lxp58P4uHD+fRd4jeh9fL9n+rHTv0DivkJme3MdtT4rY7deZ7o7E2h2d1xitu7KoMNktybl2dvLrjdGN7W21R0ufhlxv2WV6x/iwrJLxTw0iSPBLHKqH2Ub1vW08vbXd7xv8Aex220QaDLcS10LrdY0rQE1MjqooOJHl16KCW5lSK1jLTtUBQRU0BY8aDgCeg52b372fsHE9d4Tb2X2xuDZPVe+95do7D677D2BsjsrrSj372FtDD7D3huXJ7M3tgMrjty1GY2rt3H0/gyIqKanloIJ4oo50LsZOpQuGFGOD6/wCbqgCyAEHNMfOn8656BDaGzaneW6dubIxdPm63LbnyNFtjbmPwtCuZzOV3LmJosXtjEwUss0BqHy2ZqYKd3DF0EhZVY8e0d010kWqyijkuNS9srFF06hrNVDHUq1KilCaAkdLbNbN5dF9NIkGliGjUO2uh0ChZRpZqBjXAqQCR19C3LfzMPi1/J/6m3v8AEPYGd6a3H8tfjf8AHXB7Cx+1NzfJbftR0lu/F/G7r+gzj5PJxDa2T2x1d8kO5O0uzt2JB13gqY5nOy4xJsxk6BGoBEV7vujbWu3SLtV5di4vIrQizjEhiEpI8eYFl0W8VP1HFdNRgipG4oBcGQGeNAkZkHiHTqpTtHqxHAefULf/APMb+Jv/AAoK/lY/J/40bCaHrn5p1nUGX7C258XN3BMzv/Jdj9MfZ9rYJulMlBR0v+kig3LV7SkxZkxUa5qjpKqoFbQRU7qag2I06mJGgcWPAfMnyHTAXIA88U/1fPr5uVfQVmOra3GZKjqsdk8ZWVeOyWOr6eajr8dkaCokpK/HZCjqEjqaOuoauF4poZFWSKVGRgGBHtmOSOaOOWGRXidQyOpBVlIqGBGCCMgjBHWu5GKsCGGCDxFOIP8Aqx1vLbg/mmfIb+WD/I6/kmbn6Ag21K3Yu7N5VvZdNn8dDXPurr7q7sfN57K9aU9TUQ1BwOP7A/jogrclSquRpoYAKeRPJJd0/P5dOUBZifl/g6rV/wCFBfxM617cx3VP87D4br/Gvi185KDbrdrYqho8fSVXUHyAx+Bi25X0O4cTikWnxMu6n2lU0uWKmpSPd+MyLy1LfxGi8mqdaGKjz/w/PoT/APhRsAfnf/KdB/7wa+Jn/v49/wDu3mP9N1deJ/05/wAnR1f5g/8ANS3P/LB/4UXd0bg3FT5PevxW7l6r+PGxPlD1HGsWRo9x7JqOr8RR0+9cPgMgxxGR3tsBMlUT0kM4jTJUM1ZjHmgjrmqIdeQH+rj1QCqKP9XHos//AAoU7A6+7X/nV/yrey+qN1Yje/Wu9fjn8Kdx7I3bg698nis9tnJ/MHvSpxWRpK2VmqJhLSuusTWnRwyyhZFYDQ+IV9etxihp8+rPv5xf8r3+ej8t/mV35uj4k/KTd20vh12dtHZO1MX043zF7S632PWYk9SbZ2d2XhMv1Hh6o7QXEbrz8GTaugaB4clHVSPOrGZwfYoM56quigqRXqtD/hPD8cvkF/L0/mT/AMyLp/uLDY3aPdHTf8u7trPwNicthN44GSah7K6rym1dw47I4+StxtdjsnLjPPFBVJFUBEKVFPG2pAhsNysNyF19FcCQQzvbSYZSJIjpkWjBSdJ/EKqaggkEdONA8WjWva2lgfka04cK5xxx1Tb85v51fz6+b/xv2V133H82Mru/E77ze6x3L8bNj9Jbc6Z2vtrHbUyuEm68rNxdi7Ux2Ok7kxe9XR8kcRJKaTD1lDG00TSiF1at7vcpdz3O1uNpEO2RLEba7Eqv45cEyr4QGqLwiAKkkPWo6syRLFDIktZWJDpQjRTh3HB1D04cD87UP5deB2h/Nx/kb7z/AJRWyeztv7N+bXxm7yyfyP8Aj71/2RuwYzB9t7XqajdO4MhitoS1M0stFHEN9bqp62lp6ZqXHZGeiyFSywVdVPTmEazAzNI6mMt+nQUKrRcMa9x1AmuMECmM1cxUi0oQwSkhJrVtR7gKCi6aCmc1NcgdGZ+Mvx97R/kC/FT5W/LL+ZP3dspPkvvv4i5r4VfBf4zYXsmk35veg2jX7gzW6aXHUpxbmmpdl43sGqpMozY6SppcRQCskqKhayqgpfboJwCcDpqig1XhWtf8nSd/lC/CX5DfKv8AkAfzA/ix1rvTrvd++PkHunovd/S+3qjtuHK7Z2FgBv7ae981tXda0gytJ1ZumeXZuWyNZhxAJPuq2OWb92ocqV7bukW5PuMcdtPGbW4a2YzxlA7KqsWjr8cZ1UDcDQkYoS7LCYVgZnU6119prQHyPofX9nGvVC3z5/kS/O/+Wv0nie/vktRdR02wM32HgusKF9i9ijdmZbdG4sLubP46OTGjB4/x0Bx20qwyTGSyOEWx1ezMD59MECmGB/b/AJurMf8AhQPgqncnR/8AITwOP+3ORy/8t3qHC0Qqaylx9KKzJbQ6go6UVNfXTU1DRU5nlGuWaSOKJbszKoJDqCpI89XW24fOp/ydXifyifg3/MX/AJU+7+5NofOjuDorfv8AKYm6S3c+585nO96Lc/QuBjzEFDkaDObP2B2Hs5M/DTbup8xU4bNYh6fB4TJfe1ExkykkdAlUluEuZZrJra4VI0djOjRlmkUoQqqwdfDKvRq0eoBWgJDC8bII5xIhMhA8Mg00kEEkih1ArUUqKHPy60Pd60W0Ml2rvWm6wVoNhZXsXcVJ1yMvMmPaHaWR3RV0+0Fy1VXyRw0Hiw89N9xJMyrDZmcgA+zQyCCGWdwSqKXOkFjRQSaKASTjAAqei96NIEU8WoK4GTQZ8uPSp3113m+qewN59ZboqduV249hbiyO183WbQ3Jid37XqcjjZfFPNgNz4OepxOdxshIMdRA7I/0+oPtjaN0tt62ux3a0SVbe4jEqLMhjcA/xKcg/tB4g0p16eB7eaWCQjxEbSSpqPyPU7ZWNGU3Jh8ed0YXZjSVTzx7q3DPV02Hws9FTTV1PVVc9BSV1VG809OsUWiJ7zSIDYEn3XfLr6Par65/dM9+oTSbS2VWklDsEZVDsikAMS1WHaDTOOndvQy3tsq3qWzatSzyEhUKgsCSATWooMcSOnjcuOjpczmhW7wxO6MhLT0OVGbwBrMrjs5kstFR1tbSPX1MGOlpazHCqkWod4mTzwsiixDCuz3LS2FgLfZJrO2Vmh+nuAsbxJGWRWCKXBV9IKgNXSwY+nVtwj/xi7e43FJ7hqSGWOrLIz0ZgWIWhFcmlKinSdoYaaSshSuqXo6VmKzVUVMa2SnQIzB1pVkiaYmQKtgwtqv+PZrM0qxO0EQeUfChOkHP8VDTHy6QoiFkV3KpXLAVp+WK9SKWWWMs0bvCzxPBJoYrrhkFpYn0kBo5B+ocg+3KDAIr1sE8QfLpX4Dbe4dztlI9vbdzu5Dg8Hk9zZ+LB4vI5eTEbWwkH3Gc3HlxjoaiTG7ew1KQ9ZWzaKalQgyOoI96YgAdwHkOHH0+3r3r0ue0u0dzdvbqTfm98tX5/elZtnaG3dxZ/IxYWlOSi2HtnF7H2stFQ7fxOGxtBQYjZW3sdQIPC08v2xlmkkld3ZBbR3EX1CTSRtD4hMCopXTGQO1iWbU+rUSRQUIFMdLZzautq0EMiyiICcyMG1Sam7lAVdKaaAKakUrXPSEy2FzWHjxsmYw2WxEecxkWcwkmUx1Zj4s1hKmWop6bM4eSrhiTJ4ioqKWSOOpgMkLvGwDEg+/Wl/YXpuxZXsM7QSmCcROrmOVQC0UgUnRIoYEq1CARUZ6pPDPAIjNC6CRRJHrUjUhqA61pqU0NCMdccTuaPBYTe2Hk2ls/cL70wVFgoc3uTG11bntivRbixO4DuHYFXSZOhp8RuKvjxLY+omqYayJ8dVTII1dlkVi/2pr++2e9G7XduLOZpjBbuqxXOqJ4vDuVZGMkS69ahSpEiqakCnXre5EEN5CbSGTxkCa5FJeOjBtURBAVzp0kkHtJHXDcmc2ZlNtde4vb+wl2ruXbWFzNDv8A3Z/enMZw9m5mu3Hkclic8cDkAMds7+B7fnp8b9tQ3iqDAZn/AHGJLG2bdvdruvMd5ufMH1e13M0T7fZ+BHF9FGkKpJH4qd9z4soaTVJla6RgdPXVxYS2u2xWm3eDdxIwuZvEZvHYuSraD2x6EotFweJ6a6Dem8sXtLcuwsZuzceO2JvTK7bzu8Nl0OZr6Xa26s5sxcwm0MxuLBQzpjsvktrLuCvGPmnjeSk+9nEZXyNc7YBmB091MH/V69F9MHOK1p8+m3LYraC7Dx2ag3dkp9/1W683i8rsB9pSU+JxOzqLFYerwe8oN+HMyQZbIZzL1lZRy4gY+F6KOkSczyibQhSl3vB3yezfaIxsC2kcse4eOC7ztI6yW5tvD1IsaKr+KZCGLaQo016UmO1+jSYXZN6ZSpt9BoEABEniVoSxNNNKila06s+/lg/zbdyfCWsq+re6MlnN2fGisf7rFbfosZLm9z7Ez2XzNHHk8ls+rlr6WKg25DS1FTX5DFS6oqqZWek8VVJKKrHb379iIvcU2u+8sWcUPN1SlxO8gjjliSJinjLpYvLrVY0cUKqaPqRV0SLyFz1+4BPYbrO7bTQNCgUsysWGrSajSmklmU1qR20YnVtd/IDpD42fzK/i1UbRy+Vw+/uq+y8RTbk6/wCyNoVVFW5DbOdh838D3ts3KtHKcdnsJVmSGop5FXyRmpoK2IxSVEB59bBzHzh7Pc7fXwQSWm+2Uhhu7OcMokQ0LwzLjVG4owProkQ1Ct1P9/t+0c2bOYJWWawmUPHLGQSp/C6NmjLn+asCCR18675g/D7t34S937i6T7gx9q3Ht/ENp7soKWrj2z2DtOpkcYvde2aqqjjaeiqApiqIrtLRVkctPJZ4zfqzyDz7sPuNy3Z8x7DNWB6xzQsR4kEq/FFKATpYVBB/EpVx2sD1i7zBsF9y5uUu3XyZHdHIAdLoeDLXy8j6EEeXQMdi9Vbk6zx/WGT3BX7RrqftvrbGdqbXTau8tv7tqqHbOWzObwdJQ7wpcFWVcuz92R1eBlafFVoSrgjZC6gsVU827drXdH3NLaOZTaXLWknixslXQKSU1Aa07sMMHiMEElUsLwiEuR3oHFDXB9fn/wAVxB6Z8Hmtj4vZ3YmI3BsGs3LvLcFJthOvN6027q/DRdb1WLzn3+6Kmo2pT0U9Dvn+9eDBoI4qqanFC/76FmNvabcLHfLjeOXrzb9+W22e3eY7hYm3SQ3ivEUhVZy4a28CX9QlVbxPgNBnpTbz2MdnuENxYGS8kCfTziQqISrVclACJNa9uSNPEV65dhbHi2HnaHBQ746+7DWt2jsjdpz3Wecrtw7coH3rtbFbok2jkMhkMPg54N67KbKHF56jWF4qLK000Mc06KsrHhxgHpB0hwAPp7917p527LloNxbfnwOVkwOehzuHlwWehyz4CXBZpMjTNis1Hn456aTAtia8R1Arlkjak8flDKUv7blkEUUkrKxVVLEKCSQBWgAyT6Dz6si62VQQCTSp4fn8uhF7Fp+xOrOwO1utcp2Mmfya7tlxnYmZ2H2FV7s2R2Rm9u505ykz1TuLHVa0PYVNT7gP8QpqysSWRK4tNZZ9Te0223ybnYWm4RwyxxzIHEcy6HWvky5oR8iQeIJB6vLEYpniLKzKaVXh+X+r7ek3u3e+5OwN657sXszcOa3ruzd+4J9yb43Pm8iZtwboyuRqlmy2RyGVnSTVk8izH95lYByDY/T2rkErrIImAnIOlmGoBqGhIwSAckefTkYjR4zIpMQYFwpoStcgHNCRwPl06bFwWwd19k7Z2/vrelV1N1juDddJjNy9gS7YyXY1X17tKurDHU7hqNoYJqHL70mwlEwMlLSGOapIJQf2SX30+5WW0z3FpZC93aOHUsCMsImkC/CrPVYw7cNRoPM+fTpEEly4UmK1aQ6dfeUQntDUA1EDBIArxp112Du3cm7s/U1u49+7t7Og2tjabZ+2d17sq83kMkOutmh8NsykpaXNVuTr9ubfocHFCKTFmUxY5JBAORzfbrW2s7ZFg2+G0eZvGlhiCgeM41SVKhQ7k1q1KtSvVJGZmYmRnCigY1+EYHGtB8vKvTz2h1N2H0dvrLdY9r7Zm2fv3CUG2srltu1GSw2XlpMfu/bmL3dtqqNft/I5bEyrlNuZqlqQsc7SRCXRIEkVlDWzb1tfMO3Q7ts134+3SM6JIFZamN2jcaXVWGl0YcM0qKjPVp7ea1laC5j0zAAlag4YBhkVGQekIq3P+H5/4p7NOmCtSPTz6VGZ3fu3cmL2jgtxbp3Hn8J1/hKvbOwcNms3kspitj7br81kdy123toY6tqZqTbeDrNx5eryEtLRpDBJWVMszKZHZjupNPl1sALUgdNUaBbf1Nv8Pr/xPu6igLHrfTrTwByVK+lgQ/JB0nghSpBBN/xz72q0p69UNAOhW3dvrdfY9ft3I7snxFVWbW2FsjrLCPhtr7Y2nDDs7rrBU+29pUldSbTxGEpM1m6XEUyLWZitSfL5We89bU1ExLlzJ6b0gDFanrFQ09tLFefwP8B9fdlFc9VPDoUjsvduJ27tnd+X2ruXFbO3pPnabZm78ngMrj9rbxqtq1lNj900u1Nw1VJFiNxVO2MhWQwZFKSWZqKeVEmCMwBbhvrG4urywt72GS/twhuIEdWkiEgJjMkYJeMSKCU1AagCRWnVHjkVIpniYQuSEYg6W0mjBTwNCaGnDz6MrV1++O0eiMJlN3dt9Wxbd+K8O3+peq+oMxLiNvdvZja3a259y7wzOQ2HiMJtqGs7C2ztPcKTVGbyeXyEtTjVqooo20MqOQwQbZsvMlxFY7Fe/WbyXvLy+jDvarJbosaid2crDJIlFjRFGqnDGHy01xZo0l1H4VsBFFExAkKuanQBllByxPDP5hjSQY9cfJM9RVrmPvo46ahWlibGvijTapq2auZ1lir0rbIkIRkaI6tQtb2flrv6tEWGP93+ES0hY+IJdWECUoUKZLVqDinn1tVtBaNI00g3DxQFi0jw/C05cvWocPgLSlM1r0N3XXevaHVMWyJuuMxhNl57rfsTLdqbL39htk7NbszEbxzW2aHaFYj77yWDr85lNqw4Sh/yXCVbz4ukq56ipihWeeRy/RTUEVqKEeVMHy+Y6T6NRLE0UGoI/Z9nTnR0/eWK+ONRNTUe4qH4ub67vx1NV1y0mHfZud79612Llhi6Nq545dyQ7l2119vKuKRB4sfLTVMhYSTRgog/eu2tuz7J9Wh3uO2F0YM6xAz6A/DSVLkAgHUKjABHTwgmKfU+Gfpi/h68U1AVp61oD8sHNR0Enot+bfp/P9b6v9fV7Xd3qOt0j/L4fy9emXGYDC1eB39mq7smn2HubamBxmT2Dt9cRuOtzPZ+byObpsRktubfz2C0UWz6vBYKqmyM1VkZEp6mnjaBfWxBJtyv9xg3Ll2wteV2v9ru55ItwuvFhRLCNIjJHNLFL33CyygRhYxqViGOKdXhghMF9NJuQhuI0DW8WlmM7E0ZFZSBGVXJLYIwPOgX7oXF1VY1RhMEm2sZ9njKdMPFlq/NrDV0mNpaXIVwyGSC1f8AuYyMMtZ4LeKkM/gi/ajT2vsobuGDwr6/Nzda3YzGNYqqzsyLoTt/TQhK8W06m7mPVJnheTxLa28KGgGgMz0IUBjqbPcatTgtaDAHSg6eqN7QZrdEXV3VGe7H7XkwWNyPXW6dlv2GOwujtybd3NiMxH2tsOn68qYqifP0vhSjEldHJTUnnWRNM2hgGOaZYrGTl7d73nf9zbTaXhku45DbLDfK0TotrNJcAmNQ58QGJlclaVp0bbTaXW4/W2thscl9etFVBCsjPFQgGULGDUZANRStM0JBSGS+Lvyrqppp5fjX8hquaeWSaaaTpvsieSWd3Z3mklbbju8zuxJYksSbn6+0p9yPbwH/AJXzZf8Asutv+tvS4cn83k93Ku5f9k0/8+zpT9Y/G/5fbWzuQ3tt/r/5UdN7365xY7B6r3HtLovvaPdOV7NweSxkGBwW1t1bO2/S5Hr3cDUddVVcGbnljpKYUjRsdcqD2S7r7nckwS7WbPmHZb1JrlYLpv3lZRi3gKszXDLJL+sEkRF8NO8lgwwp6VW3JvNDpcifY9xh0xmSNfpLg63BChKhO0lWOTjFDxHQbZT4ufMzO5PI5vLfGT5PZfMZnI1uWzGWyPTHa1fkstlspVS12SymSrqjbMtTXZLJV08k880rPLNK7OxJJPsyj9wvbmNEhh542RY0UKqJeWoCqMAACSgAGABgcOkJ5T5sZiz8s7jqJqSbebifXs49B9lOjO/MJuPD7PzHRvcmM3fuGpmo9v7TresN802589WQUNRk56TC7fnwSZfLVMGNpJql46eGR0p4nkICIzAR7bvOz71F4+z7rbXcP8dtKkq/tRmHRde7ZuO2FRuNhPbk8PGR0/48B0EyV3kiL05jnYoWiu37cjWOgF0NtDEWv7MxSo1Ht86dI6mmM+lehTyOJ68m7U25het4uxe09jV+W2HSLiarC0u1eyN31uRhwo3btHBY3CyblipMlW5yerx2HnjSomlHhlMJdihDFpcczScs3txvq7ftvMYS50tE7XFrDpaQW0zs4hZ1EYR5VqoB1KGpnoyaOxO5wQ2Cz3NkWjGkgJK9dOtFC6gCWqqnPkaHoTt0/Dj5XVu49w1e0fhj8ssNtOqz2WqdqYXL9K9p53L4XbdRXTy4PE5bNw7JoYczksdjXihnqlhiWolQuEW9vZVtvPfKsO27dDuvPuyz7ukEa3U0NxBHHJMEAlkjjMzmNHcEqmo6QaVNOl9zy7vb3E723Lt+lqXYxI8UjFUqdKltA1EDiaCvWHcPwc+dmGp9uTZr4m/I+ogzW3aXM4P7LqffO42pcLUV2RpaelyUGExWUm2pklq6SZ2xWSWiyMMbpM9Msc8TyKpPcHkSFDJNzvs6oOLNeW4A8hUmTppOW+Y3OleX74n08CX/AKA6Ty/DD5qyK8kfxC+T7qmgMF6E7VDEyMVXQh2prk5HOkHSOTYe0h90PbYMqn3B2OrVpS+tvL1Pi0H5/l1c8r8zAE/1dvqD/hEv/QPUPffxr7k6x62oNw72+Pnyi2Bnoc3npt4ZLfvT26tq9X0mzYaXDDbFXis1lsNRZH+PJlZK0ZBasJRQQ/beElmez2z85bPvu+XNttfM+yXm2iCP6dbK6Sa68YmQzB0Rigi0aNBU6idWoUp03d7LfWVkktztd9DPrbxTLEyxBKLoIJAOqta1wBSnRbEqwT+q9/6/639R7GoNeiShGQcfPoQF7DzEfX9B17S43a9Jj8Zvuq7DptzUm2sZTdiDMVWCptvti5d+wxpn5dp09LSieHGGT7aKsZp1Gsn2TrskC8xS8zC9u/q3slsDb+PJ9KEWVpRILavhC4LNpMtNRQBa0HSr6yQ2H7v8CLwxP43iaF8SunTp8T4tFM6eFc9CZ1z8dvld3JR0fY/WXxy757y27RZpKRtw7W6e7I7O2jX5HCS01XVbeymUwGDydBWRpHLGlXRmdX8E1m0hwfabeuZOWduMu27xzRaWN3JEaLLcxQzKrgqJE1sGBBB0tQjUPOnTlrZbhJ4dzb7fLNGr+UbMhIzpNBQj1HQrVnwI+WdZsuvyw+E3zgo+1sh2FWVJwGM+K3ZtL1fTde1eJapE1FUjbD7gpty0u5JDTw0fiaijxqqfIZBb2GYOedni3uG1HOGwvyom3qPHe/ja9a7EgWjLXwjAYRqL6tZkqNNM9LZdqnks3l/dd4u6NcE+GsJEIiK1wfiDh8AU06fOvSQpfgN88xIrSfCP5eKAfz8bO5rH6/X/AH5Z/PsRLztyYSP+RdthH/PVB/1s6Lv3Tuv/AEbLj/nG/wDm6V1B8FPnVT+Uv8HvllUGWmngUVHxv7r/AMmklULHXQfb7TgJrKUi8YfyRXJ1ow9qP648ovo0c27dhge25tzWnkascHzpQ+hHWv3XuYrXbZ+FMxv/AJulPTfCX5+S00GPqfh78w3oIGVqegl+PndTUdOyq6hoaWTaJgibTKwBVRYMR+fapecOUyB/yKNu/wCymH/oPpltr3Qn/knXFP8Amm/+boFK7E5vbOazO1t1YbLbc3JtzK5Hb+49u5/HVmIzuBzmIrJcdmMLmsRkYqbIYvLYuvp5IKmmnjSWGZGR1DAgCa3nhuIYri3lV4HUOjodSspFQVYVBBGQQaEZ6KpEZGdHQq4JDKcEEHII8ujWY74Y/M+aho63G/EL5PVmOq6WCrx9ZQdA9rVWPq6SqjWopaqiqqbaT01TS1MUgdHjYo6tcGxv7JH5x5SiLeNzTtykHOu5hBBGKEF8EcKHpb+590HaNsn/ACjYj+Q6Xmb+Hfyvek25Q7d+EvyzpazGYqeDcufquju5qpd2ZapyVVW09dBhanZEMO2ocVjJo6LwwyTLUGHzswZioI9t512GObc7jdOe9oaCWUNa26z2y/TxqiqVMolJm8RwXqwBXVoGBXpdd7RcAW0dns91VE/VlKSfqMTUHQVomkHTQVBpU9Axv/q7uDp6rxdB3B1N2b1TW52CoqsHSdk7C3XsWbM01G8UdZUYmLdGJxT5OCklnRZXg1rE7qGIJHsWbbvuyb347bNvNpdiKnifSyxy6dVdOrQzadVDSvGhpw6KLizvLTR9XayxVrp8RWWtONNQFaVHDpt2ltzcu+dwYramzNvZvdu69wVkeOwO2ttYurzWfzeQlVmioMTicdDPW5CslVGIjiRnIU2HHtVuW57ZsthdbrvG4QWm2QLrmubl1jijXhqd3IVVqaVJA61bW1ze3EVrZ27zXUh0pFGCzMfRVGSemvyiM2+hBIsQQQVYqwINiCpBBB5BFva0sB59J+jUbW+OnzkxFFU5jYXx4+WePoN57UrMJWZfZ3UncNJR7s2NuuhjGSwtVX4TARQ57aG58dIn3FK7zUVdDp1q629hCbnvkaGR4bjnDaUmRirI93bgqwNCCDJVWBxTiOjVNl3dwHG13JUioIjfIP8AteB6Ue1/jt8ttl792JvjFfA/vzcFPsrK7N3DWbH7O+P3bG9ti73zG2pqGuzOO3hho9n7fbI7H3dkKRxU4gSAx0Uxg+4kt5CST848m3u2bnt977l7Yj3HjIlzZXdvBLDHIWEfht40lJoUIHi/iYawq/CFx2rc1mgmt9hudKBCySxvIrOo7iRoXtds6c0GKniQ7+QFN8h6LcGJyXyC687O6zFdTZii622jv7ae+9nbb2ps+nzlXmm2J1Phd8xibD9e7Rr9yNHSY6kkkhoo50Um7Ak15ObkyO1vYeT7+wuWMizX89m8Ekk07IqG4u3g/tLmZYu6RgGcgny6S7oN4d4G3aK4RVTRAkwcKkYJbw4g/wAMalsKMCo6C3ZnXXaHa1fX4nqvrff3ZeVxtEMjksZ1/s7cW8shj6AzJTLX11FtzHZOppKM1MqRiWRVTWwW9yB7EG6b5suxRJcb3u9rZ27NoR7qWOJWahOlWkZQTQVoM+fSO2sry9YpZWkszgVYRIzEDhkKDQV6WjfEn5gq5v8AFD5LAD636K7SA+p/7NawA9kJ9xuQP+m42en/AD223/Wzpb/V7fif+SLef84ZP+gegk3ftXenXmcqNq9hbO3VsLdFJDTVFXtree3cvtXP0sFbAtTRT1GHzlJQZGGGrp3DxM0YEiEFbg+xHt267bvFrHf7TuEF1ZMSEmtpEkjJBoQHQspoRQ5446L7m1ubOQwXds8UwFSsilWyPQgHPTptDp3ubtOhr8l1j1D2h2RjcXVJQ5Ov2DsDde8KPHVssIqIqOuqtvYnIw0lVJTkOI5GV2Q3At7Lt35q5Z2CWKHfeY7GymkGtEvLiKFmUGhKiR1JFcVHT9ptW57gjSWG2zzRqaM0UbuAfQlVIB6iZ34ifLqZHCfFP5Kym1lWHontKVyb20oke1Xdjf8AAB9kje5Xtyoq3P8AsgHqb61H/WXpZ/VnmOn/ACr99/zgl/6B6N78K+9v5tXwH/jWG6k+Mnf+5+tty19Pk831dv3499v5bbMeTFRQ/fZ7bT0mDoa/ae56/GUjUkk8TSUsqsr1VJUvBB44Y90+XvYf3Ujhm3nnraYN7hRkgv7W+tBJpIbSkoMhWaJXbWFNGBqEdA76hpytf8+crF47XYLuSydgz28tvMVrUVK0AKMQKeh/EpIFJPzl+SP8zb577WpNm9v/AMvLcmNxe3NzVWe2BuXb3xc75i7L2XQ1MzCXCU+8qp5KLIUmTx6QwZNf4ZDS18kEc4p4ZYofETe2PKvs57U3j7jsvu7BLdTW6w3kUu42Itp2A/tPAHchVqmP9RmQMU1MGbUZcy7pznzTbra3vJzrGkmuF0trjxEB/CHOCCKBu2jUBoCBSrOT4afMUFiPiR8l4y7MzEdC9ppqZv1Ox/uoLu3Fyfc0t7me3JOfcDZP+y61/wCtvQK/qvzMeHLt9/2Ty/8AQHQD7r2vu3Ym4MltLfO2dx7M3XhZIYsxtjduEyW3NxYqSppYK6njyWFzNNR5KhkqKKpjmQSxqXikVxdWBIp2/cdv3azg3Da76G5sJQTHPbuskbgEglXQlWAIIweII6Kbm1ubOeS2vLd4rlfijlUqwqKiqsARUGvQv4L4wfJ7ce3KLO7b+Mne258DuOkxuZwG6cL092XlcdXYqeGWemrcFlMXhJMRkcZmIKlJPMBOsixxtE6gvrDN77gchbfeS2e4c97Rb3cLNHNbzXlsjK4NCHV5A6spFKYpU1HChvBy1zFcQRz2/L97JBIA6SJBKwKngVIWhB9es3+yf/MBmCr8VPkozE+lV6N7PJJ/wH91rn20nuX7cSNoj9wNkZ6E0W+tSaAVJoJfIZ+zpxuVObKFjyzuAAz/ALjTf9AdLHY3wz+RE+5aWLsz4ufMXHbO+xzRrqrZHx833kdyJkFw1c2AipaTN4Cixr0U+eFMlYzyB46RpGjBcKCWb57kctptsrctc68uSbvrj0Le38SQlPEXxSWjdn1CLUUoKF6A4r0oseVt5a5Ubly/ugtNLVMFvIXrpOmgZQKaqV+VadJrM/GP5X0G38SuY+J3dm3KHbVNXxVOdHQ3ZOHmyCZDIyV/m3Llqnbwirpce0329I7ePw0yrGNVrk12/nHkafcLkWXPe33FzcMpWAXsEgXSgWkMYeqhqamArVqnpqbl/mMW8Sy8tXUaRA1cW8q1BJNXbTmlaD0GOgr2DvrM9W75oN1UeE2xk85tt8zR/wAA7D2ljd37eM9fi8jga2HNbT3BBLRVdVQx1zvCJow1LVxpKtnjFjrf9lt+ZNnutmur26gtpyhM1hPJbzjRIsg0TREOoYoA1D3KSpweiyxvJdsvI7qOGJ5o9Q0TosidylTqRwQSK4qMGh4jpMRSIERRqsoCrzquPoOQBf2eE1JPSLVpoCMdDt0B1DufuXf9HgcN1p3v2ZtzGCPJdiY/46dfV/Y3Y+J2lJJ9s1fjcPDR1WKjMmTeCMNkDFTNqI1a9HsJc68xQcs7DcX771tFjfMfDs5d7nFvatMQWCvJUN8AY0SrY4Ur0a7NYS7lepCLK6mgA1TLZIZJQnAkLw4kccfy6WUfwb+cKhtPw0+Vaxxq8rmX499tqSisgsDJtJfJMVZRoUsxA4GkcFT+7ftYpQN7lbBUmgpuFoc/lLgY48Olg5U5o8uW7/8A5wS/9AZ6jv8ADj5lwskcvxJ+TcDO6xoJ+hu06ddbMEUM8+1Y4411EXZiFX6sQAT7eX3S9sm+H3F2I/Zf2n/W3rR5V5o8+XNw/wCyeX/oDpx3D8LfmVtHP5nbWb+LXfTZbA5GqxVe+D6w3duzCvV0khhmfE7p2ljM5tbcVAzj9qrx1bVUky+qOVxz7cHuZ7bnh7g7GfsvrX/rb15eVeaX4ctbh9n081f+OdP2c+MHfVVtzYdLtb4b/KfD7uxmGzUHZGazXXPY2Wwu8M/Pnq2q2/kds4aLYlFNs/HY3bUkFHU08k1W1RUxtOHAbT7Ktu9w+Vodz3+bdvdHlybaJZo22yCG4t45LeIRKsqTSm5YXDPMGdWCppU6aGlelc3KXMb29osHKG6LchWEzGCYq5LVUqvh9tBg5z/Mpjt3rP8A0UbtxG2v4D25t9a7ZG0twVNJ3V11V9Y7qbO5GheDdSYvAVkkklfs7H7noqukxuRuDVpTvqAdGHsR8kcxzcz7TeX9xc7VK6X1xAjbPdi8h8JHrAZJQBouHgZGkj/AWFDQjoq3va5NmuobaS1u4maFJNN5EYXqahiFbJTUCFbzoR5dY6TZO7ItoUHYM20tzQ7Bym5clszGb9m2/l4tkZPemFxmOzma2bjt2vSLt+v3bh8HmKOtq8ZDUPW01HVwzyRrFKjsMwMHPRGWFaau7pyx1HJO1oonkKRvIVjjaQrHEpeWRlS5CRICzN9FUXJA9uFlQAswAqBk0ycAZ8ycD14dV7mNFBJ449Bkn9gqeh7xOYr831nXYbdPdG4qOh6o0S9LdLZhN47k23lJey87p7Zm2MUnn2X1XPTU1HBlsxJPFA2fcIiFp01eyKe3Nrv9g238pxSpuGr967rG0MUkP0qarPxlIE934jkxxhSfByW7TTpTE4ezuDLubI8IAt7Yh2EnisRNoauiLSvc1fj4DPSdpI10q9g91/bZSCCrD6qwuNJA/B5HsQGoJBrXzr0jFBQnPp0JO2M3gcXgd94rL7A2/uvJ7pwuLxu193ZXJ7gocv1Xk6DOU2Trtx7Wo8RXU2IzeRz2MgbGzw5SKenjp3LxqJDcEm5bduV3uXL17ZcxXFnZWc8kt3ZxRxPHfo8RRIZmkUyRJE58RWiIYtg4p0tt5YkgvYprJJJJFVY5mYgwkEksgFQxYGlDwoPKoLKuuQ6IzoJFlIUER2BGrS1w1vrz9fp7OhQUJFR5g/6sdJ8tQKaenQl0lHtLcWN3tVtumj6xTa+08Ll9m9fVp3nvSPtTfAmxGA3BjsLlQHx+0M5kqMTZearyCLSQ06fZwsY4kHsNTT75tl1sNsu0vuwu7ySG+3FDb230FtR5YnkjPdcRo1IgsZ1k/qN3N0YhbG4W+dbgWojhVobc+JL48uFYK5oI2ahYk4FQo7RUJHwNa3/Nv+v9vVqt/tvYhr/R8/5dItA9c/5f+K6Q9QikFWH+APIsb/nji/ux4VHTQNKo3STyMOhZL2K2N72AI/r/AE4974gHz6qao2Rg9WdfyRYyPmxuGxOheiN9OOLhv9/Z17HpPIsRrv8AT8e8K/v5uV9iJAPxbzaKf2TH/COp9+7rjnm/oO07ZKB/zmt+tukfUf64/wB798VOs1+nzGfWP/Eg/wC2P/Ffb8fD8j0iuOJ+zpfY0W0H88/7yx/4j2shP6hHz/ydFUvn9vSv/hOMzNHLjcxjqLK4+pstTQZGjgr6OdfVZZqWpjmhlBP4ZT7Ntu3G/wBruor7bL2W2vY8pNA7RuppxV1IYH7D0T3Ucc0bxSxq0bChVgCCDxBBwR1qwfzgf5GvX2B623f8rPhRtNdn12xsfVbm7T6J29DK+2MrtShjlqc3u7rbGK0p27lNuUiNUVeGpwMfUUMbvSR080Phq+lX3Y/vX7zvO8bb7e+6F6J5rlhBt27SUWQykgR29zQBX8T4Ulw+uivr161x19xvbOzit7je+WrYRNEC89qnwlQKl4x+EqOKjtIHaARRtZf4U1Xl+ZfxDAax/wBmh+P5Fv7RXtjaTAMP7SkixB+ouPed/uAK8h87L5HZ7wH87aQY+fUKctj/AJEWwev1sH/V1OvrNUXCp/wRP95sffBiPiv5/wCXrLqT4W+3/J00dh08lTsXPRxRtKy0tPUFVVmIjpK+kqppCFBOmGKFnJ+gCkni/tcixskolA0+E5FfUIxX89VKfPp2wcJuFuxNO6n7RT/L0WrE/T/Yp/vTeyFeK/aehRP8LfZ0JOLF1UHkHgg/nn2oh+M/b/m6JLj4E/1enVT/APMR/kc/F750bM3Lunr7am2OiPk7BQ1OR2z2ZszDU2CwO8s0kNTLDh+29u4eKnxu4qLM1TpHLmVgOdowsbLNPBE1FNlV7KfeR5x5AvILHf8AcbndOUTIsclrcP4kkKEUL20jkupjCjTEW8JhqFEZg4izm3krbN5SSa3hSDcskSoKBjXhIBhga5amoYyRg/Ov7K6+3x0z2JvjqXszb9XtXsHrjdOb2ZvHbteYnqMRuHb1fPjMnSeemknpauFKmnJinhkkp54iskTvG6sesW1bpY71tm37xtdys23XUKXEEq1o8cihkYVAIqpGCARwND1jlcW01ncTWtwhWeNijKfIg0P2j/UMdfRn/wCEpMnk/lfT/wC0/JPtxf8A1kbCf/ov3zq+9l/09Sx/6VFv/wBXrnqVOUTXYl/5qv1s5U/0H+uP97PuA7P4V6NpuP59Okf0X/X/AOJ9i6x+FPsHRdL5/b1PT9I/2P8AvZ9jLbfjX7ekU3Dqav1X/WP+9t7GFt8PSF+PXyCP5kNQU/mPfzB/1XX5w/LMXJBW3+nrfukAfUEAG/8AsPfQPk0t/VPljOP3bbU/5wpXqMr9Qb279fGfP+2NOvrN9A+roLpMn6nqHrZvp/TZmFP+w94Hb+mttxFeDsf2MT1J9aXEn/NQ/wCHoTT9R/wYf9DP7AEvH/anpX1rk/8ACmH4q7f7k+DafIVsLn8pvL4o5eu3Fj223VY+krBtLsRMZtHPNk1rqGuat2/hdzLg8tXxxBKhcdj6rxvGWZxNH3eeaG2Tng7NK4FnukPgnVQASxapIjWlaka0AxVnHp0S8z2f1W1tKv8Aawt4i8Tg4YfLFGJ9F6+fvg8m2LlxORwudqBkUpKXIffY0ZDEV2EybtKklBBWB4ah6mkRVP3NOwikEmlTw3vO6aKC8hmtbu2SS2cFXjkAZWX+krAgj5EdRojvE6yRSMsgyGUlSD8iDUEeo6Oh/Lw+MrfMn5r9BfHp455cHuve1Bl99rBBO6p1ptES7o7EaarhZBizUbVw1VTU00jKr108MQPkkRWBfuXzS3J3Je+77GaXMcJjgNRiaTshIU/HR2DEfwhjwB6MtksV3Dcre3f+yrrcUOVXLAkcKgUr6kdfVCFNT0UEdHR08FJSUkENNS0tNFHBT01PBH4oKengiVYoYIYlCoigKqgAC3vljISaknP+yOpsUklSTnpmrf1v/r/9G+054n/S9LYvL7etLT/hVlVmn3z8JFU28m2e+/8Ak3LdTW/22r3mL90r4efh87L/ALW+gF7hfDs5+c3/AFi6A/8A4TCVTTfKj5Eox/7l/pn/ANt2LtZR/vDez771/wDyqXLX/SxP/Vl+mvbY/wC7DcR/wpf+Pdbo2Q/Sf9j/AL2feCP4Pz6mdOPWg5/PkbZGf/mHfISTcW7aDYO5uvumukV2Ft/F7Kz2dqO7s9laLDVGUoNx7jpsoMXszJbd29m5ZYa+ogFNPRY6KlCee7v0J+7zcblbe23KsVnthubSe8uhczGVEFsodtLBGBaUOwppXIJrw6g33AWJ+Yb0vNokSGPQuknxCeIqMKR6n/Y6s3/4TVTeX47fJE3vp7nwQ+t7f78bHm3uCfvf55u5XP8A0jD/ANX5Oh97T42bcBT/AIl/9Y062Lqj6Sf8FH/Qre8N7jiepdj8+k7P9W/339r2UT8G/wBXl0uXj/q9ek7Vf2f+Wf8AxX2VXHBv9N/m6Xx8V6TFd+r/AGH/AEV7I5/x/b/k6XQ8D9v+br50X86lyv8AM8+VQH0/jnXX+89M9cn/AIn32C+7H/04vkD/AJo3H/aZcdYje6H/ACvW+/bF/wBWIut0L4BG/wAEPh0f/Aa+mP8A3gsF75S++H/T3Pc//peXn/V9+suOSP8AlUOVv+lfB/1aTo2mEbTuDEG1/wDclTr/AMlSRrf/AGF/cb7fKYZrpwK1s7lf96t5l/lXoYTjVbyD5A/sNeh8l/P/AAb/AIr7DI4Dot/6B6ZW/Wv+w/3v21Pg/wC1H+XpVF5fb0Vz5T/y8/ir839o1+B7u6vw1VuaXHy023+1tvUtLguzto1DpaCsxO7KSn+7rKemljVzQV4rMbMVHkp349jH26+8D7m+zd/b3HK3MUr7Mr6ptoumaW0lWvcvhMf0Wb/fkRR/IsRUEq5h5G5b5vtGh3awX6orSO5jAWVD5FX/ABAHOlqr6jr5+fz3+EfZH8v35Ebg6P35UNnsPJAu5OtN/wANBJj8d2BsGuqqmmxedhpHmqUx+Wp5aWSlydEJpvs62F0WSWExTSdvfZb3c5f96+Qts532BfCZyYL6zZw72t0gUywOwC6qagyPpUvGyPpXVpGE/OXKW4cmb5Ps96daDvgmAoJYySFcCpocEMtTRgRUihN7f/CWLd+4Zu+fkpsL+Is204+o6XeKYj7ShIXclRu/amFnyYrhTrkiZMZSRxeEzGAadQTUS3vCj+852rbl9peUN/8Ap/8Adt/WCCzM2pv7EWe5SBNNdGHYmunVmlaUHUo+wt7crvW7beJT9H9MZtFB8fiRJq1U1fDilafn1up1kd4ySLgMOSdQ4U/2hpANv688/i9/fD9nHhKvnXgMevlx/wBXyp1ldbt3DP8Aq+zpBZZCL/knUByTc8j6ksABb63/AD7eRs0PkB5fb8h6+nQis2GD5dBfnUYpKVHGkgqf6A31rz/t/wCn+9CHbmXxo9Zpwz+fA/tx/qqeCpjBpw6BLJLac/ixFx/jpN/95PuRrUgxg+Xl0hfGr8+tQT+fTrPzT61tfSPjJsvi39r/AEqd0XP+2Hvsz/d5f9OY5ozj+tFz/wBoG29YRfeR/wCV32n/AKVMX/aRddVWYzJ52fA0m13zWZl2zR5ar3FR7aly2QfbdFuGvo6TG5DcVHgXnOJpM9kMbQwU09bHCtVNTwxxO7RoqjPdRQfPrHhqVqR+fQp7D673lv1t0xbK2/VbhfYmxs/2ZvFaSox9N/Adg7V+1G5Nz1P8RrKMT0eK++h1wwGWpfyDRG1jYo3rmLY+XBszb9uKWy7juEO1WRdXbxby41eDANCtpaTQ1GaiCncwx0ps7C+3E3gsLZpTb273U9Co0Qx01udRFQtRgVJ8h1O25VNi8niczHQYvKnC5HHZwYrOUQyWCygxNZT5L+HZ3GySRDI4OvFN4qyn1KJqZ3juNV/Zhf2wvLK9sHuZoPHie38a3bRNH4ilNcUgB0SpqqjUOlwD5dM27GOaKcRpJ4bLLokGpG0ENpdcVQ0ow81qOlRuLOtujc25t2T4nbW2P7x5zL7jn2/tHGLgNm7d/ilXLWviNr4QSzphdvY7y+OmphI4hiUC59s7Rt37p2ra9njvbq7+mt47Zbm9fxrmbw1C+JPLQeLM9Ku1BU+XV7q4N7d3V40MUIkdpGjhXREmo10xr+FF8h5dcYbtoCj0/Vf8bi4b/XP9fa/5Hj02e7C8PLpzjAT0g3Yj1H/Hj0j+vvXHy623aNC5Pmf8nU+BQnqIu31H9R/vfHvxqcdW/s1Bp3enU7RJb6/2df5/Vqtb/fc+9VX5de7/AJ/xfn/n+XSOqYvIGt9RfgfW3P8AtwR79w+zrWHU1w/SYr4fJE6twQDbj/D6X4P1974Go6ouexvi8urL/wCSRGY/mzuUEEAdDb4Fj/4d/XRB55v7wq+/tQ+xANf+W1af8dn6nn7ulRz1fL5fuyU/9VYOtuAfUf64/wB798Ves2uqKf5nv82vuT4F/IHZnUPXfV/Wu9sPuLpzbvZNVk94y7oTKU+TzG+Ow9sTY+BcJmMfS/YRUuz4JFLIZPJK92tpAzw+69913kj3s5B3fmvmXfN1tr+33ebbkjsXt1jMaW9pMGIlt5W1lp2BIYCgGK1Jx+91vdPeOR+YLXadv262mgks0uC02vUGaSVCBpdRSkY8uJPRBqD/AIUrfJ2jnppKn469GVNJHLE9VBBkd/UtRPTCUNNFT1cmeq4qaeSK4SRoZlRrMUYDSckW/u/fawK/hc3cwiQg6S0lmQDSgJAs1JHyqPtHUYD7wHMLMuvZLIrUFgplGPOhLkA/kfs62fv5bPz16+/mG9Dv25s/b2R2RuPbW45dmdj7AyVdDlpNrbsp8dQ5YLjs5FSY9dwbfyePyUUtJWGmpXciSN4Y5InX3gD77eyu8+x3OEOwX9+l7tN3B9TYXyqY/EjBKOrxkt4csbDuAZgVZGB7iomvlHm+z5z2f9520LRTI/hTwsa6HABw1BqUg4NB5ggEdWSQUsFRFLT1MMVRTVMDQVEE0aSwzwyeiSKeKQNHJHJGxVlIIZTYgj3FdnNJE8csMjJKjBkZSQQQaggjIIPA+R6OLrgf9Xl180zMdL4746fzo8B0nhKSLH7b2D/MK64xm0aCGXyx0WyqzvDbWZ2VRajPUuXpdq5KjjbU5cMpDWa4Hduy5jn5u9ghzNdGt3fcqvcTkCg8VrJvFoKDHiaqeVOHWHLbeu0+4cO3ogWKPdYhGoPBGmVkAyThCOvp+0f6Yj/zbQf7Y/8AG/fE+L4v2/5esnpPhb7f8nVUH86r+YL2N/Lf+Jmze6Os9kbJ37md9d4bf6YyeI32c6uLpMDujrbtbdVZlKI7fyeLqxl4KvY9PFF5HeHxzSakZtJGQ33dfbDZPdfne+2Dfb26gtbbbHv0a0MYYyRz20YVvEjkUoRMSQADUDIFagrnPmS65XsLbcrSCOSU3KR6ZK0ppd69pBrVB1qv0f8Awpx+UUCXT46dCtcBhqrewuRa6/Tcg+oPvLUfcW9thT/kV75/vVr/ANs3QJb3u3+QZ2ezyP8Ahn/QfV5P8pL+dPtr+YVu7PdJb960h6j7y2/teo3hjYMLnJ8/sjf23sZU46iz1ThZchRUWU27m8TVZWF2xc71/kpNU8dU3jljjxq9+fuy3XtDY2/NGyb09/ytJcC3kEyBZ7dnBMesp2SI2kjWBHRiq6TWvQ05Q9woua3k2+6sxBuUaawFbUjqNIJFQCpBPw5xmvGmxpt+3jvbnVHc/wBRxYf7A+8bbHR4K0X9TxDU+ooKCnyNf2/LoUXddfHFP8vWgl/wqh6Iw3W/zw667i2/jqLGwfIPpDE5LdLU2lajK9g9cZvI7PyeYqokI0ebY525ThiP3HpXa5a9up/3POYrndvbG82e6mLPtm4PDBX8MMqJMq18/wBVpfsFBwp1j37j2awbxb3iqAs8PdTiXQkEn/aaR+XWxz/wk/JP8r2sv9R8mO3P/dH16f8AifcG/ez/AOnqWH/Snt/+r1z0bcnf8kEf81X/AMnWz3T/AEH+uP8Aez7gKz+Fejmbj+fXz9N2f8K/fmrt7ee7dtUfxf8Ai9PSbe3Pn8JSzVDdrmomp8TlauhglqGi37HEZpIoFL6VVSxNgBwOhNj92Tk/6e3f9+7lrMase6ACtAcfo/5eo5n5qnWWWP6RKKxAyfI06e9of8K4fntvWursXgfix8SGrMbt7cW6apcpnuwcDCMNtbFVGbzMkFXnOy8fS1VemPpXNPRxO9VWS6YoI5JGClVd+xHJOww291eb5ugikuIrZNCLKfEmcRxgiKBiql2FXICqMsQM9Nx8w3d2zpFZpqVGc1emFFTxpmnXDH/8K/vmxVeNm+LnxeVWAK2btlWIbkcNvskGx/P0/PsUR+wfL0YoN5vfz8L/AKA6QHmWQmptF/Jj/m61te9u0833/wB3939+bjxeLwe4u8+2uyu39w4XCfdHC4jMdmbzzO9MrisQ1fNVV/8ADMfX5l4oDNK8xhRdbM1yZr2zbo9q2zbtticulrBHArNxIjQICaYqQPs6Dc0zTTTTFaB2LU+016+wn8fRfoPpFfx/og61H/rmYUe8At2UPcXyHgXcY+bHqUXNJpT/AEz/AIehLP1H/Bh/0M/uOZeP+1PS3pBdqdcbU7h627C6l31jo8vsrs7ZW6NgbtxkgBSv25u/B1uAzVL6gQrTY+vkVW+qsQRyPaSzvrnbL+y3Kyk0XlvKk8Tj8LowZT+TAHp9lR1ZJFrGwKsPUHBH5jr5EPeHTu6vjH333F8e98h13R052Nu3r7J1DQyU0eUXbuXqaCgz9HFISxxm4sbFDX0j3YSUtTGwJDA++pXLm923MWxbTv1n/YXduk6ioOksAWQkY1I1Vb0II6hu8tHs7y4tXqSjlakUqPI09GFCPketxv8A4Sq9H5WTq7vj5F7j23tlMNJvyp666q3DPs/Exb2nqp8HtfJ9rSrvWfH/AMdr9nAY/b1Lj6aCp+zgrYsoCpkZgmIH3ot1gfmHYtot7qb6hLPxbqLxCYR3uID4daLMAZCxIqUaPy6H3JsDJYXMzKul5aIad1ABqz5qTSnoVP5bbVR+qT/Yf703vFN+H+r5dDdPw/l0wVv63/1/+jfac8T/AKXpdF5fb1pSf8Kvx/v/AH4O8n/j1+//APWv/FupLX95i/dL+Hn77bL/ALW+gD7iVKbMBxrN/wBYugQ/4S+X/wBmv+RI5/7J6g+v/iR9o+z7713/ACqPLf8A0sT/ANWZOm/bYUv9wH/Cl/48Ot1XIfpP+x/3s+8Efwfn1M6cevnffz//APt6P3D/AOGT05/j/wA01wHvo7927/p1Wzf817j/AKvN1BPuF/yslz/zTT/jvVxf/CaH/snX5Kfn/jNOB/8AeFx/vHX739P628r/APStP/V9+pC9p/8Akj7h/wA9f/PidbHFR9JP+Cj/AKFb3hvccT1Lsfn1pxfJf/hRT8m+mPkj8helcB0V0VlcJ1D3f2z1dg8vl33/APxXKYrr/fmf2pjMjlFo9101IchW0mJSWcQpHH5GOhVWwGcHKP3TuS+ZuUuV+YLvmLdEub/bra8lSMwaVaaFJGVdUJOkFqCpJpxr1DG7e627bbu26bfFttsyQXEkKs2upCOVBNGAqaZp0DWc/wCFNnyVnkpXw/xr6Qx8CYyggq4cnnN+ZiafLRU6pla6mno8nhVpsdWVl3p6V45ZaaMhHqJ2Bcmzfcu5EIYSc07uTqqNJtxjFBmE5+f8umF9595qKbTa8PMyf9BdJOb/AIUxfKWQ/ufHnoT+noquw1/JP0bdDn6+0T/cm9vmrXmjefn3W32f8o/Slfere14bRaftk/6C6oq+WvyI3L8tfkJ2P8iN34DB7X3H2RW4KryWC241e+Fx74HauC2nTJRPk6irris1HgI5XMkjHyO1rLYDJrkHkzb/AG95R2bk7arqaawsldY5bgqZG1yvKdRRUXDSECgGKeeeox5h3ufmLeLzebmJI55iupI66RpRUFKkngv7et/34A/9kIfDr/xWvpn/AN4LBe+Lnvh/09z3P/6Xl5/1ffrN3kj/AJVDlb/pXwf9Wk6XHyO7azHQvQ/c/d23sZjM1nuo+r9/dj4bEZr7v+EZPKbM2xkNwUNDk/sailrfsKqpoFSXxSxyaCdLA8+yP2y5bs+cPcDlTlTcJ5YrDcbtLKaSAqJFSaqOULK6htLGlVIrxB6OuZdxl2nlze90hRWmt7WSZVatCUVmANM0NM061j0/4U9fK6Uer48fHwm9/TJ2Ov8Atr7vf30Q/wCAM9qQP+Vo5h/5y2f/AGxdYwD315iP/LHsuFP9F/6D6N18LP8AhRdW9v8Ad+yOovkn0rtfYuK7I3Ph9obe7E64zWalodu7gz9dSYnAwbp21uJsjNPha7LVapUZGnr4zQowdqaVA7pF/ux9xzb9m5V3TmD275lvLjcLK2e4ksdxEbmdYwXYQywxxaJNAOlWRg7UXUla9C3lH3tbcd3s9s33a44o55VjSeBmorMQqh0ap0knLBsehz1tqYZGEQ/KL+kG1mPqIB+gtxz+PfKndGDLgd3+DrJuD4QPL1611/8AhTn0jht3fDPrDvKKgjO7umO48ZhP4raMTJsbs/D5HG57Hs2pXlE+7MHgZU/V4/HJZRrZhnf/AHcPON/Y+5/OnJBlH7n3HZjuGg1xcWc8MaFBwGqG6l1Y7tKZ7R1Afv8A7XFc8ubbu6p/jNtdCPV/wuVW1D596JT0z69V3f8ACVIeX5TfJo2uF+P2MB4/r2JgD9L/AI0/j/kc5/3nhI9jeTyTn+tMNP8Asg3HqNvYlx/WXdc/8QT/ANXout4mti9B4/xHB1W0gggqbi4/I598LC/6S1/2PP1/4r8+ssrZ+7jj/V69aof80j+eZ3z8IPmHvf44bD6c6j3jtza+3NiZunz27Zt4rnaio3ZtfH56riqFw2foqDxUs9WY49KatAGokn31e+7L9xX2r95vZbk/3K5l5l5gt963A3YlhsJbRIFFve3FsmhZbKZ6lYQWq5qxNABjqEue/erf+Tuadw2Lb9rs5beFYiHmEparxpIa6ZFH4vTqu+b/AIUtfKDIJeb49dDpe/EdZ2CvBADfq3I/1tzf3kHF/do+ykLBk5y5pJH8U9geBqP+WeOB6DS/eb5uVAv7h239k3/W3poX/hQ38i6+QPN0F0yt/qY8hvgfgf6vNN7PYv7u32jRdC83cyafnLZf9sI6bb7yvNJ47Dt/7Jv+tvVeXy7+Wm7/AJu9sbe7Z3rtLbezstgOv8T17BjNrz5OooJ6DE7j3XuSKvlfLT1FQKuWo3XLGwDaAkS8XvfKL2U9mOXvY7lfcOU+WdyvbqwudwfcXkvmiaQSSQwQlQYool0BbdSO0mpbNKARJz7zxf8AP272277jZwwTxWy2oSHVpKq8j1Oosa1kI9KAdBDiYAirYXNvwCefwL8e5lHDoCt5DNelhQxxSqkoKyIbgGNwVdS2lkJU2dGK8qbgkc/T3c1U0Iz8/wDVxHVAAwrXHy/wfy6UkEYcgWHFm5+gtax5+gX3XhXqwBY46XO0M5LtPc23dzUuLwmcm29labKxYXctAuV29lpqYOoo83jXaMVtA+vVo1CzhW+q2JXvO1x73tO5bPLeXNtHdQmE3Fo/hzxg07opKHS+KVoagkefRjtt+217hY38NvDM8EokEVwuuJyKijp+Jc1p6gHy66nmMtXXVjxU9PNka6syEtNRxCnoaM11VLWPSUFMpYU1FTmbRDECfHGqrc2uVtvEIILa3EjusUSRCSQ6nfQoXU7fidqVY+ZJPTEzs8s8uhVeR2k0oKKpcltKj8KrWgHkOs0ICgO3+uP6nj/Wv9fbx9OqKumjMM+nTpToWszfnk/0/wAP+ND3o1yBx62q17m4dOdl/wBSf02+n4v9fp+q/wDyL3qmfz/ydW8Ucaef8ukdUpazA/7b/D6/X6cH6e91456bYcZI+k7Xx6o5HX+h4/p9f94/x974UHl1UgOAV+IdWV/yUQD81NyE/qHRG9wP6kf3u67+v+294U/f2BHsUKcDvVp/x2fqePu6NXnq9rx/dkv/AFdg620h9R/rj/e/fFbrNrrWq/nI/wAvP5hfLP5Udf8AY3x96ePYOzMN0BtbZOUzH9/+rtq/bblxvY3auercZ/Dt77221lZjBityUUvnjgenbzaVkLo6r0m+517+e0vtZ7Zb7y/z5zZ9BvE2+z3kcX0t5PWF7SyjV9VvbyoKvE40lg2KkUIJxg96eQOb+aearLctg2n6iyTb44HfxYUo4mnYrSSRG+F1NaUzxqD1V1T/AMj7+Z5k5KelT41xUUVTLDTvX1Hc/QQp6JJ3EbVU4pO0KqtMNOp1t4oZZLKdKM1lOWB++R93EA09w6sB8IsNzzitM2QGfmeoe/1nPcZWWvL4Va/EZ7ag+2kxOPkOtyT+VX8HNwfCvoufDdiwdVQ9ub2i2em+Y+m9tvtzZ1PR7E23HtrbENXVVCQ1+8N51MJqa7N5qWKmWtyFbIscIjiWWbmH95L3r2/3e5utDy99aeVdv8f6OTcW1TyPcOrzOFHbDb/pokMWWCrqchnKJkXyDydNyftEtvetE24zMHm8AHSAo0quogFiMkmgySAKCptbpIh6SBxYcH6/qv8Aj3BFo9SK/wCrPQpuB3NTh8/s6+bV212Xi+3/AOe3Jv8AwRilweS/mM9dYjD1cDB4Mji9nd07V2XQ5aB1lmV4cvS7fWqU3F1lBsv6R3X5d2a45e+7hY7Neoy3sPKLCZG4rI1kzOh/0rsV/LrD68vFv/cwXKU0fvaNARwISVUBB+YWvX0z6P8Azcf/AAVP95/5F74vRfGPz6yXk4H/AFeXVNX89j4x/LX5R/Fvo7b3wt2S29+6OtPlnsHt+ClXc3Wm12weC231b3Tt+bcQqO18/t/amS+zzu7MfCaNnqJpRUahC0aSsmS33aOcOSeTec9+u+ftx+m2G72Sax1eHcSapHubSQJS2R5FqkTHVgCnxAkVj/3A2rdN22q1g2m38S6S6WUjUi0URyKT3kKcsBTPHh1pdZD+Rl/NgqMtl3yvxdaXMyZXIS5d27u+Nup8rNWTyZB28Hbq013rC5Pj/b59Ppt7z1X71P3frdEto+fNKxjQqiy3LAXAFfpPLqKx7Y89OizfuSqsNdfGt81zX+18+r+v5IH8mXuv4i9w1vyp+UE+2tu70g2Tltp9e9U7fzNFurK7fq90PTwbh3HvHceGkqdsQ11Lh6WSipKTGVeTimWullkniMSRy4s/eV+8pytz/wAuJyFyGZ7jb5LiOe9v5UaJHWIh0iijkCymslGZnVNOgBQ+olZE5D9v9y2G8bet5KJP4RSKBSGKliNTMw7a0wAC1akkilDtv4D/ADCcW5W/+Pq+v+294ZWunwbfStDmvzNWz+yg/LqQbr+0bP8Aqx1ok/8ACsbtLCbk+Yfx56oxrx1GS6u6CqM/uKeF0cUeQ7K3plnosJUASl4q2mw2z6atKlFHgyMTBmuQnTz7mG0XFp7eb9u0yMsd5uZENeDJDFGpceoMjMv2oeoC9y7pX3KwtV+KKEuT83YgD9i1/PrYA/4Sgf8Abr2r/wDFl+2//dH177hz72X/AE9Wx/6VFv8A9Xrnox5PNdhX/mq/+TrZ6p/oP9cf72fcB2fwr0cTcetXfM/8JFf5bm4NwZvctZ3b834q7cOZyebrYqXsnoZKSOqytdPXVEdNHL8a55kp0lnIQPI7BbXYnn3lvY/eZ588KKP907RpCgf2Vx5Cn/KV0Cp+V9vZ5JDNNVmJOV88/wAHXNP+Eg/8tbSoPdvzhaxDDV2R0G1mUkhgD8aLBgfofx7E1l94vneZl1bXtQ8sR3H/AG09I5eWLAVpNN+1f+gOnqn/AOEi/wDLdgZSndvzfJ+vr7I6GP5P9PjWD+PYgh9+eb3FTtu2/lHN/wBtHSR+W7HUP1Zf2r/0D1oXd0bRxfXXb/bvXOBnyFXhdg9mb+2TiKrLS08+UqcXtbdeWwWPnyU9HS0NHNXy0tCjTNFBDG0hJVEWyjKvaruS+2rbbyYKJp7eOVgvAF0DECpJAqcVJ+3oIXkK295dwISY45WQE8TpYgVp59fYT+Pv/MhOkP8AxEPWv/vGYX3gJuP+5l1/zUb/AI8epOk/tZv9Of8AD0Dvze+S+N+HPxr358kc7TR1W1+r871fXbzV4p55INh53t3ZG0t919FBTAzT5TGbPz9bU0iANrqoowQQSCF9i2CTmLmCDYbZqXEyzLDkCrpFI8aknADOoBPkCT0oknS3hM839mACxzgGlTQcaA1p59GhpqykyNNTZDH1VNXUFdTQVlFW0c8VTSVlJUxJNTVVLUws8NRTVELq6OjFXUggkH2CJQVcqwIYYIPS4imDx60Ff+FU/wAQclsD5adNfKrYu3aqsxXyh21Tddbqp8JjZqusrO6+uFosPhjLHQweSoyW9Ovq/FUlBABLPUSYKpIJ9KjM37tfNsdxyzu3LV7cBX2+Q3MRdgAIJSS9K8FjlDMxOB4g6AvNdixubW8ijJ8T9JqAmrD4a+pZcAei9bi/8vb4t0fww+F3x5+OUcNImb2B19jDvupotLwZPszcZk3R2RkoZxFFJU0lRvTMVopWkBdaNYkJsg94l888ySc3837/AMwuT4dxOxhDChWFRohUgEjUsSqD6mp8+hxY2q2VnbWi07EAJFaFuLEV8mYk/n1A+QPypxXUvyf+Dnxopmpand/yz7F7oopqKVrTUPXHS3xz7P7N3JnoLRS2qY980W16FEJi8kNbOwY+JkZPtPLcu6cv84b+ai12u3gYkUzLcXUMKIRxoYzK1R5qB59PyXawXG321KyTuwHHgqFiR9hAH59Gorf1v/r/APRvsHnif9L0cxeX29aUv/Cr7/j/AD4Pf+Gx39/7tupPeYf3S+HPn22X+C76AfuF8Gz/AGzf9YugU/4S/Qzr8qfkJUtBOtNN8ffFBUvBKtNPLT9kbNNTFT1DIIZ5KbzJ5FRiY9a6rXHs9+9bJGeVOXYw6mRdwqygioBhkoSOIBoaV40x037bg/X7gaHSYxQ+XxCufl1uoZD9J/2P+9n3gp+D8+plTj188D+f7/29I7i/8Mjp3/32u3/6e+jn3b/+nVbN/wA17j/q83UE+4X/ACstyP8Ahaf4Orjf+E0gt8dvkoP+/wBWC/8AeFx31/x947fe/wD+Vu5X/wClaf8Aq/J1IftP/wAkW+/56j/xxOtjSo+kn/BR/wBCt7w3uOJ6lyPz61++4f8AhPL8Lu5O3O1O5tz9n/KGg3R252PvjtDclBgd6dUUuBos/v7dGU3VmKPCUuR6UymQpsPTZDLSpTRz1VTMkAUPLIwLnITZfvXe4nLWxbPsFjs2yvZ2FpDZwtLDclykMaxqXK3aqWIUFiAATwA4dAK+9q+X9yvry/nvb1ZppXmcI8QUM7FiADCTQE4qT9p6Ciq/4TVfBcWH+lj5Z2KXt/frp7/Hj/mRH09qJvvm+6C1psOwYNP7C7+X/L98+tx+zfLFR/j1/wD73F/1o6TtX/wmw+DMbcdr/LE8f2t9dP8A9bW46JHHsrl++t7qLqpsHL/p/YXnp/z3dKk9mOV2439//vcP/WjrUV+Z3T21vj98oO9uk9l12dye1er+yNxbOwOQ3PU4+s3BWY7D1Qgp58xV4rF4XHVFc45doaSnjJ+iD30K9veYb3m7kXlHmjcooo9w3Db4LuZIAyxh5Y1dggdnYLU4BZjTiT1j/wAx7bBs+/bttds7tbwTtEhkILEKaCpAUV+wDrfi+AQt8EPh0D/3jX0x/wC8FgvfF33x/wCnue5//S7vP+r79Zucj/8AKn8rf9K+D/q0nT78s+t959w/GL5GdVdc4b+8W/exOje2tnbOwP8AEcViP4xuPcGw83jcRjv4pna7GYbH/d1tQieaqqIII73d1UEgq9p9/wBp5W9zOSOYt9u/A2ay3KC4uZtLvojR6s2iNXdqDyVST5Doy5vs7nceVOYLCzj13c1pJFGlQKsykAVYgCpPEkDrTBg/kUfzVIivk+K50hhrA7x+OIZl1Auqt/pbkVGZQQCVYAm9jax6rN97j7vTDHuD/wBmG5/9sY6w9HtR7gD/AJYHlX+3tv8Ard1YH8Yf5DPfu5vllt3sLs/rOL41fGvZXYG194QbA3x2psTursrceJ20+Ly0u1qbI9c1GV25U024s1RSwz1OQlpHoqKchYqt4lEsT+4P3yeQNn5Cv7PlXfX3rnm4tpYIZbe1uLSCF5AypNIblImpEpBCxhi7rT9NW1KMuVPZ3mGffbK73q1S02mGZJHjeRJXkCkMVURl1oxFDqIoDwamd3rEL+0CfwvpF7cMAzEcG5P0/wBc++L+5GtABjz/AG46zCiB0D06oK/4Uwdm4jaP8vrAbAnmppM9213tsjE4ygLgVYxO0MduHeWbzUMRkjLUmPqsXQUkrAPpfIxjT6tS5t/3c/L97f8AvTzNzAtu/wC7Nv2CWKSYfCs1zcWwhjY5zJHFMw/5pnOMwV79X8dvyjbWRI8a4vEop46Y1ZmYfYdI/wBt1V7/AMJR4S3yi+T7ECy9A4hef9r7Bwp44PPo/HvIr+8+b/mBvJpU/wDO1Q/92/ceon9japzJuv8AzxH/AKuxdbyGQitH9ABe3+x0/wBDfn6f4/7b3wpZqxp3VPr+3049ZXWr9/VJHzs/k3/Hb529pf6U+5O1fkThq2BIBjNq7A3H1PhdpYedcJgdvVdZRJnem9zbomqctQ7bpWmWqydRCsqMYEiDsDmZ7MffZ9z/AGU5M2zkjlLlflyfb7VZALm/hv5J3ElxNcnxDFuMMPa87AaY1OkKG1EV6CnMPs/y5zpusu8bruV+lw6qNEDwqg0qFxqgds6amrHJNKDHRC67/hNn8GqC4i7W+WDqoA/d3x1AQARp5KdFoLAkf7f3NMH95h77ysinlLlHPpbbh/3tPt/Z0ji+7TyI6hjuu7V+Utv/ANsvSFrP+E+Xw1xkojh7N+TkgA+su8uqj+D/AKjpdP7PsY2n94p71zIGblflb8ra/wD+9l0y33a+RlJA3Xdv+ctv6/8APL1Rp/MA+LvXvw/+RkfUHWuY3jnNtnYO190tXb5yGEyec+/zNXmqepg+5wG3ts0P2ca41DGv2usEtqduLdKPu2e6HMHvD7XbdzvzNZ2cG6zXVxA0dikqRBYpCikLLNM9SBmrkV4AdYze6nKO2cj80/uXap55LX6aObVcFGar6qiqJGtMYxX59FioKRamnaNndEkXSXQ2cA/S3BuCPqPze3uf0bQytQEjyPUZEBwQcD16HftDsKo7e7E3F2LU7I6y64qdynDmTZXTmzabYHW2E/g+38Vt9DtzaNLVVkGJOSjxK1laVkb7jITzzmxkIBRse0psO0Wm0JuN5dpDrpc7hKZ7h9TtJ+pKQC2nVpXGECr5dKbq4a8uJJzDHGWI7IV0IKADC1NK0qfnU9JqFAgCD6n9Z/rb6DgfpHs0456b+EEA/b9vTzAgjAJHrI4B/sj8n/gx9+4/Z1vCAH8XU+GO/wC4x4vwD9WP1+t/qfeifwjraig1tx8vt6nwxtKwP4B4/A45/wBsPfqhcdXWrdzY6d4VDWAuFFh/tRJ/Nufr/T3qhAqet/GcHt6c/CLfRf8AN2+o/wBV+n6/W3umr5njXq9V/wAnSLmQgEf2W/1/Sw/P+v7c40px6bK+Gaj4eoWXxlJTYbEZKLNYytq8q2cTIbepoq9crtdcVWU1Lj5c1LUUsONmi3TBUNU0IpJp2SKBxOImKBk0c8sl1eW0lnIkUQjMc7FdE2tSWEYDFgYSNL6gKkjTUVp50CLFKkoJaupBxWhABPl3DIpXhmnVi/8AJXjC/NPcji3q6J3ve30ud29dH/ff194Zff1r/rFU8v31af8AHJ+p2+7tQ89XzDj+7Zf+rtv1tlL+oe+K/WbHSjxK+pW/pcf7ybe7A0B9aH/J0knyWH2dCrhIuI+P9QRa31Nv6n86vdC9HYH1/wAnRdKCAehTxsN0UgA2ZeVQyfX/AA40rb8fW3vSSd3Hy9aeX+HoqmHzPVDf85X+cJ158TOrd6/H7oPeGM3V8sN74es2vK+3auPIUnROJzNJLTZPdu4a+kd6al35T0cx/g+KZjPBVOlXVIII0iqs7/ur/dn37nje9p57512p7bkO1dbmCO4XS9/IrBo0RGFTa1FZJCNMi/px6tTNHCfuTz/Z7FaXW1bZcK++SLoOjIhVhQsxGNdD2j17iKYOkt8JaTxfMv4h+kWHyf6BJ/wI7W2mQbD6e+qvP4/5AnOp8/3Tef8AaPJ1jXy0R/WLYBTH1sH/AFdXr60NIDojH9FW/wDsP+Re+C0Xxj7D1l5LgH/V5DpQ0v8AZ/4KfZhHxj+0dJJfxdFZ3JTzU28NzRzI0btmquoVWBBMNXNJVU7gH+zLBMrA/kH2k3Yg7gxU1GiMY/5pJX9h6FNkwfbbYrw0U/YSD/MdP2K/Sn++/PtJD8Z+3/N0juPgT/V6dFZ+d38zH41fy5up6zePbe56DMdj5DFSTdZ9F4LK0r9i9jZZhUpQmHHqtXUbb2alZTMK/P1kIoKNEZE+4rHp6Oonj2n9nua/dXdbS02OxeDY0ZReblKpMEICqXoe0SzGtViU6iWBYqgZ1j3mfmLb+X4ZJruUNcEHw4VPe5rjHELjLHA+ZoD8y/5J/IDsj5a999q/I/tuuhr9/ds7qqtzZlaNZkxuJpRDT4zb+2MLHUzVNVDt7aG2sfR4rHRzSyyx0NHEryO4Lt2D5T5Y2rkzlzZ+V9kiKbXZQiGIGmpqZZ3IABkkcs7kAVZiaZ6xn3C/uNzvbncLth40rampwHkAPOigADzoOvoV/wDCUdNH8r+rH/gS3bh/9Y3X4/2N7e+ff3sv+nq2P/Sot/8Aq9c9Sbyh/wAkIf8ANV+tnSn+g/1x/vZ9wHZ/CvRvNx6JnN/M2/lt0NVUUFb/ADB/g/R11DUzUlbR1Xyw6Gp6ujq6aV4ailqqebfyTU9RTyoyujgMjAggEe5bsuQOe9EZ/qTu9CAQfo7j/rX0RS7jt4JBvoag5Gtf8/UtP5nv8tUgAfzDPg2f9b5Z9Bn/AB/57/8Ap7F+38i87Iy6+Tt1GfO0uB5/80+kUu4WGf8AHof97X/P05R/zNv5bcjLo/mD/B9+D+j5YdDN/X+m/j7FVvybzeFzyruQ+22n/wCgOkb31iTi8i/3tf8AP18on5G1+OznyJ+QedwuSoMzhM13d2xlsNmMVWU+RxeVxWS35nqzH5LG19HLNSV+PrqOZJYZoneOWN1ZWKkH3nZsMcsOxbPFLGyyraRK6sCCCI1BBByCCOB4dR/uDrJuN+6MChncgrkEFiQa8KH+fX1/Pj7/AMyE6R/8RD1r/wC8ZhfeBm4/7m3X/NVv+PHqSZP7Wb/Tn/D1WX/P5iEn8ob5vRfh9g7Q/wB57Z2C3+2v7U+2SiP3V5cA4ePIf2xSH/L0n3Qk7Rd/80yOg7/4T2fLyT5Z/wAs3pxNwZVsn2P8evP8dd/SVE0stbOOvqOgPX+VqZKl5KurkyfV+Sw33FVIzfcZCGqN7qwBZ718s/1a5/3VYY9Nle0v4P8Am6T4gwABSYOAPJdPSjY7s3m2W0jGsifpP9q0A48SV0kn1J6tA+QXxm6k+TVF1PQ9t7dj3BF0t3h1v8htgeQqBiuyerslVVu3Mi6sjCelaCvqaeeE+iaCoZWupIMcbRv257D9e22XHh/V2ctjPgHVDMAHXPrQEHiCAejKSKKXw/Fj1aHEifJl+FhTzH+cdDnL9f8AYt/vfsP/AIj+fSscB1pSx/LU/K3/AIVcdH47BZVsj1x8ZqTvz49bMEE8zY+bMbR+M3flT2hl46cxxU4rZ+ycnkcealPIKuixdIwkaNYwuV7crHlv7su93E8Wm+3Fra/lOK6Hu7YQLUZp4IV6HgzsKVr0Efrhdc42USt+nCGiAz8QRy5oeB1dvz0jrckrf1v/AK//AEb7xDPE/wCl6kWLy+3rTQ/4VFbp/ub2z8Ic3/djZu79fXXypwX8F37gv7ybdT+9NB1ztv8Aja4sVdDbcG2/4p9/ianyf5HkqeGfS+jScw/umCqc+ipGbLK4P/EvoBe4fwbPgHM2D/za6BX/AITHb73nle+e3+usnubLZHY2x+jM5lto7aq5YpMdgMlu/svYc256yhtCtQJc1UYuCSYM7IHQlFXU2pf96jbNvh2HZ92itFXcbm/VZpRWrCOBwgIrQUGMAE0Fa0FPe3Espury3aQmJIwVBpir1Pz4/wCx1uSZD9J/2P8AvZ94Rfg/PqYk49fPD/n9j/saR3Fx/wAwR07z/wCU2wHvo593D/p1WzZ/0e5/6vP1BPuF/wArJc/804/8HVxf/CaX/snb5Kf+Jpwf/vDY73jp977/AJW7lf8A6Vp/6vv1IntQKbNf/wDPWf8AjidbGdR9JP8Ago/6Fb3hzccT1Lcfn0Tzc3zf+Fm1dwZ3am5/l78Xtt7o2zmMlt7cm2893/1Rh8/t/P4aunx2Ywecw+Q3ZT5HE5jE5CmkgqaaeOOaCaNkdVZSAex+2/uHf2sF7Y8hb1NZzRrLDLDY3Lo6OupXRliKsrKQQQSCMjpI/MXL8EskM++2aTIxV0eaMFWBoQQWqCCMg8OkXU/Pn4KnTb5p/Ew2j5t8jenjb6/W28faOf2q90CGp7b7/wAf+jfd/L/hPSqPmrlft/5Elh/2URf9B9Jus+evwZdvR8z/AInvxb0/IvqBv7X+G8T7Jpvab3UOuntnzB/3Lrz0/wCaPSyLmzlYf87Lt/8A2UQ/L+n18/b+Ylndub3+cHyo3js7cWD3dtPcXc28ctgNzbZy2Pz+3s5jKrINJS5DD5nF1FXjcnQVCcpLBK8bj6E++vHtDt99tntZ7f7fuVnLb38O0Wsc0E6MkiOsShkdHAZGU4IIBHn1ibzhcQXXNW/XNtMklu907I6EMrCvEMKgg+o63ofgKLfBL4eA/UfGzpkf7bYWCHvjh75f9Pd9zv8Apd3n/V9+s0OR/wDlT+V/+eCD/q0nRxtm/wDHz0X/AASv/wDcKT3F6f7h7v8A884/6vRdC65/sD9o/wAJ6GeX8/8ABv8AivsgHAdIP+gemuIfvx/46h/yaf8AivtPd/4FB/melcPFft6Yu3fkJ0r8Zeucj2h312VtXq/ZOLik8mY3PXrTy100EX3P8MwGIgE+a3NnahYv2cfjqaqrqg8RROePZbyz7fc6e5O9w8u8i8uXO5boxqyW69kYYlQ80rUigjrjXIypXFa9O7rvu07Bt7bhvW4RW9moPdIck+iqKs7U4KoJPkOvno/zXP5i+b/mQ/IuDd+KoMptnozrCiyW1ekdn5cx/wAUgxOQqqWfcW9txRwSTUtNuvflZjqaSoghd4aKio6Ok1zvTvU1HdH7tPsJYewfIK7FJPFdc2Xri63i+iWiyShdKQxFgJDb2ykqmqhZjJLojMpjXB73E54n543w3aIybVADHaRNxCmmp38tchAJpgAKtTpqbc/+EpVOF+TfylIFivQ+31AF/o2/qC9rfXlR9feMP96FQexvJ2P+doh8v+XDcOhN7KtTmLcif+UI/wDV2LreFr47RNx+fqf+C82PH0I/4374RuQYUFRWv+frKW0fU6nokfbvy5+J/UW6a7Yvavyf+PPWO9aGCkrK3Z3YPdXWmzN0UdJkYEqsfU1e3tx7kxmYpqevpHEkLvCFljIZSwIJlPlr2e93Oa9rtd/5Y9rOY9y2OYN4N7YbZe3EEmh3jfRNFC8b6HUq2k4YFTQg0OP61csbZObTdOY7C3u1ALRXFxFG4BFRVXcEVBBGOHRf8t89fgrOHEPzR+JkupAP2/kb0855Zfwm8Wu1zf8A2HsZW3sF78pIjH2U5uADDjs+4f8AbP8Al+fRvBz9yGIwDzttANfO8t/+tnQPZf5sfDKaobwfLv4w1A1NYw9+9UygizAWKbsb+vuQ7D2O96xD3ezvNSmg47TfjP8A2T9My8/cinI502muf+Jlv/1s61W/5t+/Nhdq/MiHdHWe+dndh7YHVGycadxbF3PhN24P+I0lfuR6qgOWwNdX0H3lMlRG0kXk1oHUkC4v2f8AuZ8u7/yv7HbPtPM2x3m3bql9eO1tfQyW8oVpiVYxyqjgMMg0oRkdYU++u57bu/PLXW07jBdWv0cS+LbyJIlQXqNSFlqK5Fa8OiK4uK0aAA/jj83sB/Qc3HHvK0YyeoXPoOHSrhUohCBTIwPLX0gi9lJUatN/rb37jSvDq57AQPi8z6dDh2d/oIv1i/RNP2/An+hzY3+mcdw1OzKp5vkLbJf6TKnq0bNRBT9MSMKP+BRZT/cwoE33H9n3XvNa044p6eX59WWiAEju9Pn0HsAv6m5Xi5v/ALDi/wDre98MDj14CupnOOPThEGkawA0/Tg/jj6H+vv3D7er1Ln0HSgxFNT1uTxePqMlQ4Oir8njsfW57JJVvi8FR1tbBTVWdysePp6zIyYvCwTNVVC00MtQ0MTCNHfSpT3EjwW9xPFA80yRs6wx01SFVJWNCxCh3ICrqIFSKkDqwHiOkesKhIBY8ACQCT50HE0z05rCsM80EckdQsU9RDHUwhhDUxQzPFHWQiRRIIKpF8iBwHCMAwBuPe1cyRo7IVJUEqeKkipU0xVeBpiox1ZhpJRDXPH/AC/n1N8S2/6daf8AY6vr/r+9169oH8ukS/1Kn6H9J+tx/Rj+WH+8+3KUyB+XVAcaSKjyr0y1qaYpFPKkG35te9wf6+/caEceqGqVqO3y+XVkn8l1NHzR3F9Rfore9x/S27uvP9v7wr+/qa+xA/6XVp/x2fqefu7LTny/I+H92S/9XbfrbCT6n/W/4n3xW6zY61t/5xHz/wDmT8VPlHsHrv48dwnr7ZmY6D2tvXJ4UdfdW7sNVufJdi9p4Osyf8R3vsjcuVh82K25RReGOdKdfDqWMO7s/Sb7nPsB7S+63tlvvMPPvKf1+7Q77PZRzfVXkFIUtbKRU029xEho8rnUVLGtCaAAYv8AvX7gc38qc02O3cv7v4Fm+3xzsnhQPVzNOpNZY3bKoBQGmOGT1WNSfzov5p8SD7f5RPGwHp/4wl8dWH9NJ8nUbA+8sD9zL7t1a/63Nc/9HDdP+27qHx7xe40mDzHny/xe1/60dBN2r/NE/mQ9z4er2/vv5bdorhq8FK6g2RJgOqYayMrpkpav/RXgtmSVVHMp0yQSM0MgJDqbn2NOVvu5eyPJs0Fzy/7a7Yl1EQ0U1yjXcqEZBWW7ad1YeRBBHkeifcfcbnbdUaG95hn8M8RFpi/6tKlR8uHVekeH8bM8mp5HZneR2JZ2YlmZma5LMW5JJPPuaAooKdAup1cc9GG+HdMIvmX8Ryo4Pye6C/8AfrbTN+Pr7CHP/wDyonOv/SovP+0eTo65aAHMXL5HnewD/qqnX1gKYWAH+A/3o/8AE++CcBqy/YesvZfxfs/kOqQP+FBXzK+Snwd+F/V/bHxZ7I/0X9g7h+TuzOu8xn/7n7C3t93s7LdU91bkyGH/AIV2Jtbd2Fg+4zW0sfP9xFTJVL9voWURySq+Uf3WuQeUvcXn/dtl5y2n6zbItmlu44vFmipKtzaRq+qCSJzRJWFCSuakVAIjv3F3jctk2e3utrufCna6WNm0q1VMcjEUdWHFR5Vx1UJ/JT/nE/Ij5VfI7ePQ3zP7QpOxN29hbbiz3TO6JNmdd7Eljz2yaKrqd0bJah652jtPHZKXN7UDZKmlqIS8Iws6a2M6KJX+9L93flXlLk+w519vdlNrBYzeFucQlnl1QzFUimrPLIR4UtEIXiJQThOkHtfz5uO5X9xsW+XfiNJGXtWKotGWrOnYq11L3CvDSR59baGK/Sn++/PvAGH4z9v+bqZbj4E/1enWmF/wpo/l+y9fdp7W+fHXmKkOze45sNsHu2npopHjwPaWFwYo9o7rlVC0dLjt87Rwa0cxCRxR5PFeSR3nyKj31H+597mx7vy/e+2t/N/j+2ap9uLHL2jv3JXNWglf1+B1AFEJ6xx90NhMF8m/QJ+nMRHPTycCit9jKKfIj1brVsiRRCCoFiDz9fx/vR95rdRMfMHr6Rf/AAlOGn+WFUj/AMCU7b+n/an2D75s/ey/6erZf9Ki3/6u3PUtcoCmwr/zUfrZup/oP9cf72fcB2fwr0bzcevjYdhfEj5SVHaPY9VF8Z/kBNTzb93hPBNF0z2NJDPDNuHIvFNDIm22jkikRgVYEqym4499grDmTl0WtpXfrL+yX/R4v4R/S6h2523cTcTkbfOQXahCN6n5dYqP4kfJ8KNfxm+QIvY/8yY7G5/qD/v2/wCvsyTmTl2tP37ZV/5rx/8AQXSNtr3M5/d89P8ASP8A5ulTjfiZ8nVdC3xq79H0tfpvsRRyefrtsWNvbw5j5fr/AMl6z/5zR/8AQXTZ2vcv+jdP/wA43/zdIPMYnI4KryeDzWNr8Nm8NW1mKzGHytHUY/K4rJ46olo8hjclj6uOGsocjQVcLxTQyokkUiFWAYEezmOSOeOOaKQPC6h1ZTUEEVBUjBBGQRx6ROrRsyOhV1Okg4IPmCPIg9fY++Pv/MhOkP8AxEPWv/vGYX3z53H/AHNuv+arf8ePUpSf2s3+nP8Ah6rY/n2oG/lJfNZfw2wdn/X/AMStsL/intd7cLp91eWDX4pGP/VKQf5Ok+4mu03nyQ9alH/CWr5YnpD5ubo+N24Mj9tsv5Y7JbHYmCQOYYe3eroMturZ8pmbVDRxZLaFXuOhYWVqqsmokLEoimc/vG8sfvTlC05hhStzts3f/wA0JyqPj8REgjI9F1H16D3Kl34d5LZMcSrqX/TJU/YAVqT6kAdfRFP0H+t/xJ94Kn4V6H/RI/5inyox/wAK/hf8hPkjUy0wy/X2wcmNjUdUUMWV7L3LJBtbrfFSRMwealq965qh+50BnjpFlk0kIfYj5H5bk5v5v2Pl1K6Lm4CykGhWJavMwJqKrErEepoPPql7drY2VxeMKiNNQB4FuCg08mYgfn189z/hPw+QyX84v4p5zL1tVksvlaz5D5PKZKunkqa3IZHIfGfu+prq6sqZmaWoqqupnaSR2JZ3JJNz7zr9+Ikh9oeaIYYwkKC0VVXAAF5bAAAYAHl1HPLJZ9/spHYlyXJJ8yUfPX0va39b/wCv/wBG++bh4n/S9TPF5fb1pT/8KvP+P9+D3/hsd/8A/u16l95h/dL4c+/bZf4LvoBe4fwbP9s3/WLoE/8AhL+LfK35E8/X4+QH/wBiPtP/AHr2e/esNeUOWsf8tE/9WX6p7cf8lDcD/wAKX/j3W6fkP0n/AGP+9n3gp+D8+plTj188T+f0f+xpHcQ/H9yOnbn+g/0bYA/7fn30a+7j/wBOq2b/AJr3P/V5+oK9wf8AlZbj/mnH/g6uL/4TT8fHb5J2/wCf0YL/AN4XHe8d/vff8rbyt/0rD/1fk6kL2nr+59w/56z/AMcTrYyqPpJ/wUf9Ct7w4uOJ6lyPz6+af83vjt3tmvm/8ys1iuju3sriMv8AKz5EZTF5bHdab0r8bk8bkO394VdFkcfXUuFkpq2hraWVZIZomeOSNgykgg++tPtrzZytbe3PIFvccy7fHcR7JYo6PcQqystrECrKXBDAihByDjrFjmTZt4l5h36WLabl42vJ2VlicggysQQQuQR0WaT4yfIPSf8AjAPdN+P+aV764/8AWFwPY2POfJ3/AE1m2fZ9VD/0H0SLsO++Wy3f/OGT/oHprf4y/IQOLdA90gEkEf6K98j8gqP+LDb2y3OfJ3/TWbZX/nqg/wCtnTy7BvpP/JFu/wDnDJ/0D0Fu59uZvamQrtv7mwWX27n8cUjr8JnsZW4fL0Ek0EdRFHWY3IQ09ZSPJTzJIokjUlGVgLEH2c2t3a39tHd2NzHNauKpLCwdGGRVWUkHIpjz6STQT20rwXELxzLhkcFWHnkGhGOvoX/AkW+C3w/B4I+N/TYt/wCSHg/fC73y/wCnu+5//S7vP+r79Z4cj/8AKn8r/wDPBB/1aTpQfK3sbefUHxf+SvanXWZ/u7v7rvoftjeOzc9/DsVl/wCDbkwGzcnkMRkv4XnaHJ4bIfaVkKv4aqnngktZ0ZSR7t7K8u7PzXz/ALTy9v8AZ/UbRdzW0E8Op01I97aow1xsjrVWIqrA5welvOd7dbbyvvN/ZS6LqG2kkjegNGWN2U0YFTQgGhBHWqX8O/59fzYxfyS6mf5U94Q7/wCgMpuinwHZeJm6w6e2scXgtwRy4gbvizOyOvtuZ6I7LrayLKSQxzlamClkhKN5AR0M9w/uee1F3yVzFDyFyp9FzgLYybfN9XeSAyxkOsRW4unipPp8IsynRr1DIHWL3LXu5zRHvm3fv/dfG2dn8OdfChSit269SRq36ZIalcgEefW9TRyxVBgngkjmhmiWaGaJ1kilikVGjlikQlJI5EYFSCQQbj3x5v0eKSWKVCsqgKysKEEEggg5BB8usvrchtJBqKggj8uqVP5+3wQf5T/Er/TfsXESV3cXxapsxvGjp6KINXbn6orFpZuy8BoDx/c1OCo8dFnaMHySWx9TT06GWsscovuRe868ge5R5B3q508tcyOlvGWJ0w7gKrbMBmguamBqCpdoSxCoeoz96eTzzByym8WcVd024GWg4tCcyr/tQNY/0rAZbrQwxiII1sB/j9L3AFvfaccM8esMSBUenDra4/4SmRA/Jr5UcAD/AEFbdHJsCDv2jvzYj6e+av8Aeikj2N5Mpx/rTFw/54Nw6mD2aYLzDuYHH6M/9XYut4LJRaYTxYX4+gsNP+sDbj3wer+mpOc1r+3rJuyesnH/AFV6+eZ/P+6F7s3v/Mz7L3Ns7pvtTd+26vYPUsNLuHbHXm7twYOqno9lY+mqoqfLYrD1dBNLTTxlJVWQlHBBsff0XfcI37ZLX7qntrBdbzaRzpJuIdJJY1ZSd0vWAYFgQSpBFRkEHz6xe93Nu3G6583Wa22+aSNo4KMkbMD+igNCBQ0II/LqoOi+MfyEjjBl6A7pQ2HEnVe+VP8AtmwIIt7zFHNPK4FDzHYA+dbiH/oPqOBy/vzfDsl4fshk/wCgelDQ/G3vsSLfonuNbH+11hvcW/174P6+7f1r5V/6aXb/APsoh/6D6seWuYyMbBe/84Jf+genWr2RurY2Qp8PvLam49n5WopIshBjd0YLKbfyE9BLNPTRV0VHlqWkqZKKappJY1lVSjPEwBupAObDcdv3OJrjbb6G4gVtBeB1kUMACVJQkBqEGnGhHr0VXtlfbdIsF9ZywTFdQWZGRiCSAQGAOmoOfUHpYY+MJGCANbAcf6kfT6/hv96Htbx+zpN8A/p/4OlBTR/R2+gI0i36je/+PA/2Pvx9PPryr+JvyHTzChc3Jstxf62AH9PfifLz6uAX7nOOnBReyqLKPp/X+lz/AIn36nqetV1tQHt6coVt6V+o/UbfQ8Ajj3oZBrw6sSaiNPz6eKdNIW3LEcD/AHnUb3/P091Y1rX16cwoKqO7p7gT8gE8j/Yn/E/0590yR174ATxY9OOlrf2f03+n+P0/4Lb3qg6tRuPnx/2OkJILrYj+l/8AD+hH9Qf6+3ODV6bAU9rYbpqq01xSKw9Wk2/xFjZh/iPz71WmQcV69imluPVkf8mJGX5mbhJ+n+gzeyg/+TZ19x/sLe8LPv6UPsQD/wBJq0r/ALxP1O33dqjnu+U8P3ZLT/nNB1tdR/k/77/fc++K/WbHWox/PypPN80+sJLXt8X9kqPr/wA/W7qbn/D1e+xX93pn2Y5nH/h0XP8A2g7d1hV946o552pvL91Rf9pFz1TkmNj8QcL+LkEXIPN+Lc8+87yKYPHqBcMAy/n01VdFHyQo1Ac8AXH9QB9SfeuHVx319ek9U0yEEgAf8Qf9cn6H3o+o68mRpP5f6vToW/iFGR8y/iULC4+TvQl/yT/xlXaf+H09gz3ANeRedT/0ibz/ALR5Ojnlo05j2EHH+Owf9XV6+rjALHj6f8aP/FffBC3+Ja+h/wAvWYE/BvtP+Ada1f8Awqwj8n8vHpZf/A0evDb8cdH/ACLt9Pean3Jf+np79/4r0/8A2mWHUT+62eX7Kv8AymJ/1am60TOr9+bu6c7D2J2x1/k3wu9+uN14Lem1skoMi02a27kYMnQ/cwakWroZpacJUQOfHUQO8TgqxB6Z71s+3cw7PuexbtbiXa7y3ktriM1GqOVSjioyCVJoRkcR1BNlez7deW17avpuYZFkjPoVNRjzGMjzHX1G/h/8htofLD49dS/IDY7JFhOzNrUWXnxvnWpm25uGGSXGbs2pWzhY1lrtqbnoqvHzOFCyPTF1ujKTwu555G3DkDn3feSdzf8AWtLrwkmIAEkT6WhmpUgCSJlele2pU5B6zJ27d7fe9msN2tv7KWPVp46WGGQ/NWBH5dDf8jvjn1/8tvjz2t8cuz6QVGze19oVm2qypWnhqqzAZMmKu21u7ERVN4P49s3ctHSZWgZ7otZRxlgVBBMuRubdz5F5q2LmvaG/x2yuBKEJoJEoVkiY57ZYyyN5gMSM06It6sIN0s7vb7kfoyoVJ8wa4YV81NCPmOvlSfIDofsP4u94dpfHntXHjG786n3bkdqZ2OLWaKvWn0VOJz2KklSOSowW5sJU02RoJWVTNRVUTlRqt77a8scx7Xzdy/tPMuyzeJtl5As8TGlQGGVYAmjo1VYeTAjy6xX3Cwn229ubG5Wk8bFT8/QjzowoR8qdfQr/AOEqK6P5YdQL3/5yT7bJ/wBjh9gn/iffPf72X/T1bL/pUW//AFduepO5Q/5IKV/34/WzVT/j/XH+9n3Aln8C9Gs3xdOkf0X/AF/+J9i2x+FPsHRfL5/b1PT9I/2P+9n2M9t+JPt/y9IZfPqav1X/AFj/AL2fYvtvh6RPx6+Qx/Mllkb+Yz/MES/C/Nz5XAf4Ad779tf6++gPJ5/5CXK//Sutv+rKdRrfD/Hbz/mq/wDx49fWO+Pv/MhOkP8AxEPWv/vGYX3g3uP+5t1/zVb/AI8epJk/tZv9Of8AD1XD/PmTX/KX+aA/1WwNpD/kntTYhPHP49mnt4pHujyg34TI4/Ykn+fpLuB/3VX/APpCf5dfMb6j3/uvpbsrrjuHYtWcdvTqzfG1Ow9q1p1lKfP7PzdDuDEtMI2Vpac1tAglS9njJU8E+86N12213na9x2i8BNpcwSW8oGDpkUo1D5Ghweo5tpntriG6SheNg4rwqDXPy6+vR8fe6dp/I3ozqPvnYs6z7T7d692tv7DL5FkmooNyYmmyM2JrdP8AmsnhaqaSjq4jZoamCRGAZSPfK3fNputh3bcdlvlpd2s8lvJTgSjFaj1VqVB8wQepjjkSaOOaI1idQ6k+jCo/Oh61Fv8AhWF8sTKfjz8HtsZZrzy1HyF7ao6OolU+CI5bZnU+Gr2p2EcsM853BkKijmuVeDH1Gj/NP7yd+7Byr4k+/wDOVxH2p/iFqTQ5OmScgHIIHhqGHkzj16CvN97ohtbFTlv1X4jAwueBBNceqjqmn/hP/R+D+bj8RWAsFHfQ+n9fjH3QP+J9zJ7/AH/TpebP+oX/ALTLfoi5X/5Ltj9r/wDVtuvpPVv63/1/+jffNY8T/pepoi8vt60qv+FXKF9+/B+342x39/vOW6lt7zD+6Xw59+2y/wC1voBe4XwbP6Vm/wCsXQKf8Jgo2X5WfIkkf9y+U4/2P+kban/FPZ7963/lUeWh/wBJE/8AVl+qe3H/ACUNw/5pL/x7rdLyH6T/ALH/AHs+8FPwfn1Mqcevnk/z+YmP80XuJ/w2yOnLf+i3wK/7H6e+jn3cP+nVbN/zXuf+rz9QT7hf8rLcf800/wAHVxH/AAmoUr8dvklcHnujBW4t9NjY73jp976n9buWKf8ARtP/AFffqQ/ajGzX4/5ev+fE62MKj6Sf8FH/AEK3vDm44nqXI/PpOz/Vv99/a9lE/Bv9Xl0uXj/q9ek7Vf2f+Wf/ABX2VXHBv9N/m6Xx8V6TFd+r/Yf9FeyOf8f2/wCTpdDwP2/5uvnr/wA5XUf5lnyjH1UZrry3P/fnuvD/AL2f8ffYj7sH/TieQP8Amjcf9plz1iN7n/8AK9779sX/AFYi63FvgaNPwZ+IQ/p8cOnP/eEwfvlB75f9Pd90P+l5ef8AV9+suOSP+VQ5X/6V8H/VpOmf56c/CH5jr+W+Mfdygf1J2BmOP9sPZ193V1X3Z5VVjQteWgX5n661P+AHq/uACeS+YqeVnN/1ak6+dBBjy0QJU/S/A4Bt+b8++3HWBNAKA8fPrfg/kTfMc/Jn4lYzrXdmW+97X+NX8K65z/3M/kyGZ2C9NL/oy3PJrd5Zf9w1BLiJpGLSSVOIeaQ3nW/G376PtYeRvciTmrbrfTy9zAr3a6R2x3akfVx8T8bOswJpUyMqiidZk+znNH7+5cSwuJK7lYaYXrxaP/Qm/wB5BU/Nanj1fvQwRPTvTzxpPBJGI5opFDxzRzqQ6SIwKPGVFipBBHB94A3cssbrLC5SZTqRwSCpUihBGQa+YyOpspWIKQCCCCDwpwp185r+cN8D5Pgj8w9yYbamFkx3RPcK1vZXSc0EEyYzGYmtq1XdXXsErAwJU9e5+cwJAJJZExFTjpZCGqLe+/v3VveuL3u9qdr3i+uVbnHb6bfvUeAxnRRpuNIC0S6jpICFCCTxI1r4Z6wO9zeUm5R5lube3iK7VcVntCOAVvijrwrG2PM6dJPxdWw/8JRFL/Jz5S2vpHRW3fpyf+P9orn/ABsB/ifeMv8AekkD2L5MrT/laYeP/PBuHRr7PNTfdzJP/ESn/VWPreJy8ZFOSBaxH0B49JFrjSOPp/sPfBmv6ERJwa/5f8PHrJfb5Ky0J8ugV3Ao1PYW4Y349X9nm5H1vb/Y/wCHsytT5E8FA/w/6v8Ai+pH2w9iV9eghzliJfTYaHNh9b34H4+jH2f2mJYG1Z1KM/lXoW2mIzU/Z/q/LoDtxW85IFtWs/7dCf8AeL+5M2iph0k8Mdanyftr1qR/zw5mj+YvXSg/X44bOIH4v/pO7gufp/gPfbD+7wqfZfmkDh/Wm5/7QNt6wa+8oQOetqb8X7pjoP8AqIuuqvcOmuMO99IFyebsSfp/sT9feepNKAceselFasxx0p4ULkcWA5/wAB+n+HHvfWx+o5qMdOa2/Qv0A5PPP9T/AMFHvQ9Tx6vlqKo7enCMaVAHLH6/1Fx/jY3P+8D3oZJPXmoKKp7unSmQKP6kkcWsCbn+n4/3v36tTTqwonD4unmBbEseSLX/ANj+B/j7bpU46sO3LHPT1AtrG4H5tfhRb6f6/wDX3X5DqwxVj1O0/wCv9LfTm173/wBe/wCP6e90NePXqn06QUim5+gNuP8AW+tj/h7vw48Om2B7WrnqJNH5I2AuDY6eeQf6XH4P+8+6mox5da+LJ9ehk+K/yYzvxD7Yr+18BtHGb0rqzZ2X2fJhstkavFUqU+WyWEyT1qVVHT1Mplikwiqq6NJEh54HuJven2j2r3p5NHJu77tcWdl9XFeeNbBC+qIOAtHBWh1588dDbkDnafkPep95gsFuJWt2tzG7FRRmRtVQDmqenn1YNL/Pn7UgfSPjfsdvVwTvrPi9v8P4Fx7xLP8Ad28gEH/kf7xT/mnbf9AdTF/wSu5k0/qpBX/ms3/QHVYfzR+VW4Pmx23t3tfcuxsTsKt2/wBc4nryLEYfLVmZpailxG5d3blTJSVVbSUcsc8su7XiMYUqqwqQbsbZUexnsrs/sZyluPKeybzc3trcbjJuLS3SoHDyQwQlAIwBpAtwR51J6h33B55uOfd7tt4udvS2aO1W2CIxcELJI+qpAyfEoR8uiqtSeJSCDb+n9fxz/j+fczkVB9egOKowPl0x1dMqepfzyD9CD9bf7z7b6cIpRl6TlTCCSwH1uT/xUfT6e9ZB+XVqBwT+Lpw623rVdTds9Ydr4/F0+Yr+sOxdk9h0WIq5pKakytVsrcuM3LTYyqqoVklp6aumxqxPIqsyKxIBI9lO+7VHvmy7xs00rJBeWstq7pTUolRoywrgkBqivSvbrw2N/Y3wQM8EySqpNA2hg1CfnSletj6T/hVX3nTvYfEHqxrE/XsndoP9P+dD/T3hSn3FeS46U523QkVHwQf9A9Sy3vDcPg7Cgqf9+n/rX1Xp/Mr/AJ13ZX8yvoraHRW8ehdldXYzaXbuB7agz+293Z3cFdWV+C2bv3Z8WHlo8njKKnipKiDfks5lVy4enVQtmJEte0P3ctg9oOZL3mTauYby7uJ7F7Ex3CxqoV5YZSwKAHUDCB6UJ6C3NPPU3MthDYPtqwhZlm1hy1aK60ppXjq4/KnVKn2YMdiBqt+m3B4H1/ofeRfQCrXjT7Ordv5cf84zuD+XN19vfqvD9aYDuHY+592U+9MFidybnyu25NmZ2fHpjdxnG1NDjct9xQbihoKF3pysSQVFM8qXaol948e8X3dOWveDetn5gvd2nsN1tYTbPJboj+NGH1xq4cgAxsz0IyQ9DgLQfcqc+3vK9nc7etqs9rI/iKrMV0MRRqUBqGoMeRFRxPVmVN/wq/7ppSFHw160axUDV2run+yf6/3TA9xQv3IuVVp/yN9w41/soej6T3XuXNTs0df+ah/6A6pd/mV/P2P+ZJ2/tLvHKdBbT6U37htmx7J3VkNp7qy24U37jsZXS1e2K3MRZDF4uGHK7fgraqlFSqvNUUjQQyP46WBVyN9p/bNfarl+45ateYrm/wBtaczwi5VVMJYDWqaa9jEaqcAxYjLHoDcxb8vMF1DdmwWGVUKMVYtqFagnA4VI+f5Do+X8tH+fp2h/LT+ODfHTaHxz2J2li27B3T2Ady7i3vuDb9eKndFLg6WbGmgxmGrafw0gwqlZPJqbyEECw9hH3N+77s/udzNFzLfcw3NrOlqlr4USIy0RpGDVbNT4n8ulez80ttViLEWQkAYtq16ePy0nqwUf8LCPkFEbL8JuojzwT2nvPkXPNv7uqfz7BEX3R+X4gAObrw/bFF/n6WPzpqydt/6qf9CdT4f+FhPyGaw/2Sbp9SDcA9pb0J/r/wA88Pz7NIPus7JEBTmu7p84o/8AP0mfm4N/yzv+qn/XPp0h/wCFgfyIfSv+yUdP83+naG9f9fkHAX9m9v8Adt2qAqU5nuD9sSf9BdJ35qRtVdvP/OT/AK59PtN/wr2+Q8pUt8Len1H+HZu9OL3+t8F/j7NY/u/2EYIHMs3/ADhX/oPphuZ4jk7e3/OQf9a+tYfvfsjI/IXvrvTv3LYWj25le8e4ezu4clt3H1M9bQYLIdmb1ze9KzC0VZUxxVFXR4upzTQRSyKryIgYgE29zxtG3jatr2zbFkLpbW8cAcihYRoqVoK0JpWnl0F7iQTzzzBaB3ZqE1pUk0rQVp9nWztsr/hVl33sTZOz9lUnxB6nyNPs/a23trU9dP2LvCCath2/iKPEx1csMeGdIpamOkDsqkhSbAn3C9z7EWk88so5jlAZi1PBXFTWn9oK/s/LoTHmeMlmbb21E1NJABU+n6eB+fQDfMz/AIUb9z/NT4x9tfGTc3xg622NhO2cJjsJX7pwm+d0ZXKYePG7kwu4456TH1+Jgpal5JsMsZDuoCuSOQParl/2TtNk5i2fmFd/kke0ZnEZiVQ2pStNWs0pWvDpq55iWa1uLdbIqXXTqMlafloFf29a7MWO/ZCstvT9Lf4f48m9/wDY+50UD06CzY88dX5/y/8A+f5358Bvjbt/4zUPS2yO4NsbN3DufJ7Ozm6N2bjwWTwOB3Rkf49UbVWnx1JX09RRUe5K3IVcMmpCFrfFotGGaBefvYbaud+Y7jmJd7ltJ5o0WaNI1cM6Lo1gl1pVFUEU4itc9CjauZWsbNLSWz8QITpYPpwTWh7WrQk5rwoPLqrD5i/Jvfnzj+UHZ3yf7Hx1HhNwdj12INPtjGVtdkMPtPA7ewOM25gdu4ebIHzGkocbiUZ20xiapklmKBpG9yhyVynZ8k8tbby5YytJFAGLSuAGkd3Z3Ygf0moBU0UAVNOibcr99xu5rp101oFWtQAAABX8qnAqa+vSp+E/yaznwh+TvWHyh21tDE77zfWA3r9jtXN5GrxOLyv99Ou929eVIqshQwT1UH2NJuySoQoh1SQqpspJFOeuVIueOVd05XmvWt4rrwqzKocr4c0c2FJUGvh04jjXre1Xx22/t74xa9GrtrStVK8aGlK+nV8VX/wqp74MjD/ZQ+qTdvqOxd3/AOH4/gp/p7x0/wCBR2viecrjh/yjp/1t6Gq8+leG1f8AVT/rn1Uz/Mm/mY73/mZZrp3Nb16o2t1bJ1Bjd7Y7HwbZz+Vz65hd7VW2Kmplq5MrR0hpmoTtmMIEDavK1zwPct+1ntRae2Cb4LbeZLv64w1MkYTSIfFpSjNXV4prX0HRBzBzAd++jraCIRavxaq6tP8ARWlNPSV/l3/Pzdv8ubsff3Zez+tdvdmV2+9jxbIqcZuPN5LB01BTR57G5410E+MpKuWaYy45Y9DAKFYm9x7Xe6Ptrbe5m1bdtdzur2i29x9QHjQSaqoyaaFlpxrXrXLu/ty/PPOtoJdaBaFtNKGta6W6tSqv+FP3eMjFD8TOsAObEdhbs55Nv+XL9fcIf8CZttKf1zuOP/KOn/W3oYD3NkGRsy/85T/1r6o4+a3ynzvzh+Re5/kVufZmI2FmN0YbamHqNt4PJVmXx1JHtXBUeCgnira+CmqXeriow7BksrGwvb3kL7eckw8gcr2fLMF+9zFDJI/iuoQnxHL00gsBStOPz6A2/wC8Nvu5y7i1uIiyqukHVSgpxoP8HRp/gF/NP3x/L22F2DsXafUG1uyKbf8Au6j3bVV2e3LlsHNjp6PDQYdaOnix1BWRzxSRwByzFWBNrewD7s+xth7qbptm63XME1nJbW5twkcSyBgXLg5ZSDVqefQg5W52l5YtLi1Tb1mV5fF1FytO0CnwtXh0diq/4Uq90jVb4q9bWI/PYO6AbWt/zo/8fcRSfc32V+PPF1+VvH/1s6FQ937gcNiTjT+1P/QHTDN/wpU7mJIPxV63uf8Av4e5/wCt/wDnQX9ppPuW7Ewzzzd/9k8f/Wzp1fea5rjYY/8AnKf+gOmap/4Un9xGw/2VXrskDTx2JuUcf152/wDX2mf7kvL8lQee73jXFvH/ANB9KF967taH9wRY/wCGt/0B0zy/8KRO4ZrM/wAV+vV/HHYm5P63/O3/AGjf7jXLbg/8j2+z/wAIi/6D6dT3xvV/516Kn/NVv+gOqJ/ll3plvlh8huyfkFnNsY/aGV7HrcHWVW3MXXVOSoMX/Atq4LasMcFfVwU9RUienwSSsWRbPIQBYD3ld7d8kW3txyXsXJlnfSXNtYpIizygKz+JLJKSVXAoZCB8h1FnMW+Scyb3f73LbrE85WsaksBpREGSBWoWvDq1npr+er2N0f0v1X05QfHjZu4aLq3YG1dhUebqt85ygqstS7Uw1HhqfIVNJDgqqGmnq4qMO6LIyqxIBI94w85/cw5b5y5q5j5puOdr6CbcbyW8eFIYmVGlcuVUlgSATQV6lfZfey+2fads2pdgikW2gSAOZWBYIoUEjSaEgevTD3d/Pa7H7q6d7W6grvjpszAUXanXm7+vavOU2/M3X1OIpd34SrwdTkqeik2/TRVU9JDVl40aRVZgLm3t/kT7nPLnIvNW0c02/OV9cT2c8c6RPFEqs0ciSAEgk0JSh+R8j1bfPe+/3zZ9x2h9ghjS4heEuJGJGsFagaRwr1Q/DTKqAH8fS3P+8H6295jkevUIH59HI+C3zR7F+AveP+mfr3E4/dcOR2zmNo7t2Pma+ux2F3ThMl4auiSoqaJZZaSrw2doaWsp5hG7jxPFwkz+4s93/abl/wB5OT5uUOYJZYYxPHcwXUGnxYZYyRrTUCp1Rs8bAg9rk8QCBZyZzZfcl7wN1solkBjaKWFiQrqcjIrQhgCD8qcCersYf+FQ/d0BKj4ldYMCEGr/AEibsvZNJH0wZF+PeHMv93H7czUDc/73ivBbXzr/AMK+fUut94fdsAcuW1B6yP8A9A9Em/mEfzjMz/MY6XwvVXYnxi6/2XmNpbuot47K7DwW8c7k9wbZqxBNj85j4aatw9MlVh9yYmoMNVTNKsTTQ01QVaSmi0zX7C/dR2D2A5i3jf8Aljnfd7qG/tBa3Vjd+D4D6XV4pSscaHxYu4IxJoskg/EegLzt7mz88bdDY3mxwRSRSiWKZGYuuKMBUfCw4jzIU+Q6CL+Vt/Mpz/8ALG7J7N7GwHUWH7fk7J2NQ7LqcRlt31mzRio6DO0+bjyFPW0e39xmqaQwmJomiT9WrVxYjL7wv3euWfvG8o7TyfzXvN/Zbfabgu4pJt5iEjSLDNAFYzRSro0zsaBa6guaVBCfLHMlzytd3F5bWqSSSR+HSQmgGoN+HNaqOrp63/hWB2PWxaF+D+zYzf0t/p0zbi4FrBR1ept/Xn/ifeHq/wB1b7MBFRvcDmg0JPx2NT/2ZfPoe2/vJvFu2tdqtifmX/z9B/k/+FP/AG/lHY0/xA6/pEb6LP2ruOrYccAsmz6NSVP+0jn26P7rP2gQnwvcLmSnAajZH5+VoOhFbfeH322AA5ftGp/SkH+XpO1P/CkfuGuv5Pip15GX+oXsXchP1uV9W3h7eT+699rUZSvuNzBQcKrZ8f8AnB0bRfed32EAf1XtDT/hkn+bpPy/8KCO0Mm2uo+MeyYibhRF2Jnebra/q203Hs+tv7t327t+2L3B3r56ktv+tY6u33n94YBn5Utq+VJn/wCgOq3fl78qMz81O29v9sZ3ZON2DVbf69xOwRiMXmanOU9RTYrcm69xJkWrKqgx8sc00m62iMYQqFhDXOogZcexnsttHsTyluPKOybxc31tc7lJuRlulRXDyQ28JQCMAaQtuD61J+XULe4XPNx7h73a71c7elq0VqtroRi4IWSWTVUgUJMtKfLoF8fpCLGDYWCj/YC9z9Pc0cBU9AUnWwAwo6UCSxLZFcE/k3+v9Ob/AE/xPvw9T1YkU0L1PSaJF/WrMQAPp/Xi4/J/p71xofLq2IwAPi6cYJIQCWcEm5+v5P0F/wDe/fiTUAHPXgPDXURnp5pnjtcsP+jRYD/evdW8wPPq6inc5z09U2lrEEfU6R/r8XNuCT/j9Peq0p5nqwGo6m/IdPEY4v8Aj8f42/P+Puvn1sZz5dStX+H9nV9Pz/xS/vXW6jpGyx6gD+Rc8c/QH/eePdx5j8h1TzJ8uoToOGFr25+ov/X/AGP9D79QZBHn1TiQRw/ydNVVSRygm4Dc2JH15+jDkW/r735kUx59eYK1CMEdJioxUT6jpA5/xGk2/wB6PvWQf9WetYYfMdNU1Aig8AMP8B/sT9ObX/331924UI4dUB1drcemiaGylCP6kG3HJ+h/oOP9h78RjUOrK1DpYYPr0mauEqWVgStzbkjn/egQfbeT59ODsND8PScqItJta35HP++sfesHHWz2moOOk5WwKwYj6H8WN1P/ABA964YPXiK9w/MdJGqo1cn0pqBt+bkn6Acfi/tsih4Y62BrFad3+HqGKZALW/2H/G/qPeu30Neq1rg9cDAENja3+9/7f3sVOF/Pr1DwX8+ostIjXYf7EH/e/wDX9+0/Pr1KCtc9R/sk/ov+vY3/ANe/9fe9Hz68PQcfs6kU1GA1/wAD+n5H9OB78FBz5daJHl04miQ8gA2+tx+D+Tx/vHu9B6dbBFK065R49HYXC2+nCi/5+l+Tx73+fViBmp6eKbGRgcrySLMQPpx+fze/vYFcdN+VPLpQUmLS4ICW/wB8P6+3lFAOmmpx8+lRR42McWW3+tf/AF7n/Ee3KDB6b6UtNQxoBcCxuAf6Hn62t9PdhWtfKnWsAHpzWgjZQbD6f8Vvb/XJ9368acTw65LRRpbgfS9h9OPweOffuvfPy6kpEo4tdTzbj8gcH8+94oPXqlKnIxw67WlRrkgfX/ff1+nvXXgQx4/6v2dT6elCq5jCF9LFA9wpbSbBrc6SbXt+PexSq14edOvEGhpT5Dy/4roTTtHbu89/bC2H1VkM3Vy71m2TtcVG+oaPFmn37uatpsTkKdXxK1SrtmlylbH4p9Dy+LUbOQLhq23HeNv2fed05rt7ZGtnuJkWxLuDaxgtGzeJQ+MyA6hgVpw6OLq222a+srXYpp3ikjiRzdBVInbDhdFR4YJFDx+3q6Kq/wCEzn8xJXYjc/xjuPpfsre/H0/p1URc+4QP3ovb3P8Aur3ev/NG3/7auhAvIu6twu7b/epP+tXRd/kx/I0+dfxP6Y3h3xvem6p3nsvYFPBk93UfV+7Nx7l3Lh9vtOsNfuebD5TZO3lnwOCDiXITRSyPSUoeodBTxTSxn/Kn3geQ+bN8suXrVL22u7g6IXvUiSNn/DGGSaQh34ICAGaig6ioKe/5O3Xb7Sa8d4ZI0GpliLlgPNqFFwvnnAzwB6qHp6mGpjFmB1H/AF/xwLcfg+5zPr0E+sFVTRICTb8m9rcc+/U691b/ANRfyKPmt3d1R133HsjP9C020+z9mYDfO24M9vrdlDmYcPuTG0+Tx6ZSjpOvcjT01ctNUr5EjnlVW4DG1/ePe/8A3leQ+Xd43bZLzbd1e6s7mS1laKKAoXicoxUtcqxXUpoSB9nQ8svbzer60tbyK6tRHLGsqhmkqA6hhWkZFaHOT0nO9v5IXzM+PXUXYHdW/wDPdFVOz+ttuVu6Nwwbc3vurIZuTG0BQVC46irdgYulqaq0gsrzxKefV71y595XkLmjmDauXdv27dUvryZYImmigCBm4aity7AfYp63f+3W+bfZXV/Lc2rQwoZHCtJqIAqaViAr+Y6qd2DszJ9nb82R1zt2Sgj3B2Bu/bWycFJkppKbGx5jdeZosDi5MjUQQVU9PRJW16GZ0ikZIwSEYgAzlvW62uxbPuu+Xwc2dlbS3UwjALFIkaRwoJALFVNBUAnzHQJsbSW/vLSxt9InmlSJNRwGdgoqRUgVOcdXC1P/AAnr+dHOjc3x1H+vv/eg/wAPx1kfeMT/AHxPa5cttW94P++Lf/tr6kwe0HMvleWP+9y/9aeiSfMr+Wb8gfg1tTZ+8+58t1dksRvjcVRtjELsPceezdbFkqbGT5V3rocxtPbsUNK1LAwVkkkYvwVA59yN7Z++fJvutuO5bXy3aX8V1awieQ3kcaAqWC9pjmlqQT5gfKvQe5l5E3jlW0t7zcprd4pZPDXwWYmuktnUiYweq+mpomXgAn/W/wBe/wDvXuZD59A3pmrHhpVP0uV/PNyOAD9OOfbb/Pp5RQU6P10d/Ke+b/yFoKLcGH6uj652jlIDPj919wZFtjUdVC72hnp9vNR5PfdRSVcf7kNQmIallis6SMrIWx755+837PchTXFlfcy/XbrEdL2m1r9Q4I4qZAVt1ZTgq0oYHBGDSRth9rOct+SOaLbRb2rCqy3Z8MH/AGtGlIPEHRQjz6PZtL/hOj3Zn1pKTOfI3q3C5yeJnnpMVtXdm4MTDJDTJNMsWVq5Nt1lQiy61RmooyyqrFVLFVhWb79vI2u9e05K3Z7KGPxNcjW6OayKgHhrI6j4gfj9R8yO09gd4SBZLrf7ZZaiqxo7Af7Y6CeHoPXpFdp/8J0fmns2mqsj1xvjpjt+CnhleHD0mezWx9010qBilPTUe6sPHtVGmUABp83EoY2Nh6vZzy99+X2f3aaODebPdtrqO6W4gWWIfnbSSzH/AJxdFO4eyPNFsrvY3trcqFqFDNG7fIBl0A/a/VK/bfS3bnQO8qnr/uzrjdXWm7qVDKcNurEz4962k1vEuQw9YRJjc7iZZEYR1lFLUUshU6ZGsfeVvLfNPLnN+1w73ytvVtf7W5oJ7V1kWtASraalHUHuVgGXzAPUV7ptG5bJdNZbrYyW90M6JFpUVIqp4MtQe4Eg+R6D1aeFk1XsebDjix4J4Hs/+Z49Fhr5nPVhfwJ/lj/IH+Ys/asfQ+f6rwjdOnYv96R2ZuLcuAWo/wBIJ3j/AAP+Df3c2Zu01Zg/uRWfc+YQeMPFo8mptEB++H3jvbv7vq8rnn5NwP72+p+k+hhWWn0vgeLr1Sxaf9yE08a54UyMuUuSN35yXcDtctugttGvx2Zf7TXp06UevwGtflx6szx3/CXL+YbXMCOzfiHD6b2k7F7a1fm/MfRMiA/j6+8epP7yv7uELMJYuYQBxP0UZ8gfK5r59CG49o+ZbfMl3ZEfJ5f+tPVJffXQm7fjR3n2d8fuwqzb2R3r1Lu2v2buSu2nW1+R23V5LHePyz4WuymLwmRqsfIsgKNPSU0hv6kU8e83uSubdp595Q5Z522Lxf3Lu1jDuFp4y6JPCnjWSPWoLaW0sKipoeo33Cxl2y+urCdlM0TlGKVK1HpUA/y6RdLjIQoOlSR9TpAt+eP8PYpAr0j4D59Dv8dvjtvD5NdxbP6Q67nwFJvHe394jh590V1XjMGh2ztbO7wyH31dQ43LVUOrFbfnEemnkLTFFOkEsAJ7ne4vLntJyPvXP/Npn/cFh4IuDbJ4kn+MXEVtHpSq6v1ZlrnAqfLo+5W5a3Lm/frHl7avD+uuNfhmViq/pxvK1WAJHah8vTqyqp/kWfMqhlCT7l6DQixsu9t4sAtiR+nrgj6D+vvFq3/vB/u/3CaoF30j/njQf4bjqWm+7f7hFqvPto8v7aT/ACQ9Et+T3xQ7P+HO59q7Q7SyOzMjk92YGfcWLk2ZlcrlaJKGnyEuNkWslyuBwEsVT9xCSFWN1K86r8e8jPaH3l5P96tj3LmLk5bsWFrdmyl+sjWJvEEccp0qrvVdMi5qM1FOo2535E3rkO+s9t3mS3aaaLxk+nZmGnUVyWRCDUHo3eyP5VHyb3z1zsXs3Cbm6bpdvdhbS2xvDCRZPdG7ocnFi924Kk3BjIMjTUmwq2CCuShq1EypLLGkgIV2HqMMcxffa9m+WuaOYOUtwt96fd9svbixuBDbRlPEtpWhkKM1wmpNamhoCRQ06H+z/d/543nadt3Wyu9uW1u7aO5j8SWUNolRXXUBAwDaWzQmnr0oIf5RHysY2G8ujAxNhfdW+bD6AXt1o3A9ln/B3ezBz+7t+0/880H/AG19Gf8AwNXuAik/X7Xq/wCa03/bP080/wDJ6+WkjKRvPog3Fxbdu+gbf656y4P/ABX20338vZUCn7t3+n/PNB/219VH3befUBY322Fv+a03/bP0o6X+TV8v5iNO8ehbXCgNvDfPB9R/59lzwvtM/wB/72QTB27fx5/7iwf9tfTR+7lz6pZmvNsqP+Gy/wDWjpV0P8lj5iTMp/vj0Bb8A7z35cn/ABP+jHi3+HtM/wDeC+xarU7fzB/2SQf9tnTT/d656DDXe7bQeksv/WjomXyF+PnYPxS7Li6p7NyG1cluOTbeK3SlTs/JZLKYh8Zl6ivpaVBUZbDYKsFSkuMlDq1OFHFiQfeT3tV7o8te8HKFtzrypFdJtEs8sCLeIscgaJtLEqkki0rw7uHp1GPNXKu48o7u+zbo8LXQjWUmFiy0atMsqmuM46DimkLoGFv9j+f9ube5G6D3H7PPqTqP+83/AD/tv9b3rrdB6dJeVeLj+vNv8QRfn/E+7jGoU6oTQ/Lptlvzbngcf7H/AHv3YUpnqi8QeobiwLAX/qP94uP8R/vPutASRX7OvMPNRx4jrHHQ4yoos5VVmfTF1+Oo8fNgsM2EyeRfeFVU5KKlr6CHMUbDGbYbC452rmlr/RVKhghvMQCxNNcxz2UUViZIJGYTzCRF8ABSUYo3dN4jdlEyvxN29e0IVd/GAkAGlaE66mhGoYXSM1PHgM9JWeMMLqOR9P8AD+oPtSMY8uqEBhVcMOmOpjuCbWP1It9Dz/vB/wB79+yp6rh8U7uk7VQh9QYc/i/1+lxc/gj8f4e6sKZHDp1WJqj8R13jsNtrKY6tgr90Rbc3HHWSz0S56glh2fUYCjxVVVVRl3Hj3yWYh3fV5WOKloMcuKelqVkLyVsDKsblG43l/ZywywbTJdWRCowtiDcCRpAoPhOY4zbohLSSeJqWlBG2SFlnBDOzwy3scDgFg09RGQqk01KrtrY4VdNCeLDoLatQFuwMQbTcSWUqWA9LWJUNc2Nief6+zQitVrX5jpKKr3eX+rj0nKmmANxewN/zcX+v1ueDc/7D3QZw3HrZxRl+Hz6bpIeOLah9efx/UcfX3UimD+3rxo4r+LqOULLY2Nvofz79pYZ60K/n1HMbA2t/vXP+8+3PLh1aoAz10aZyb8W4J5+g/J4HvRBNOm2NTjj1KiiXgENxfSV+tyb3F+SPdqdbpj59TVjtxyP8eTf/AGP09+61wNadS4YQDdbf7H/G9/8AYf63v3XiSePTxDoLrCHTzCLz+IMPIIi/j8pS+rxmQ6dX0vx9fd1B4ngDT8+qmlSpIr6dP1JHb8W+lv6H+h/2/t0eXr00/pXpS0yfQ/T+v+P1/wB5Ht0Gpr5dU6UVMq25N/8AY/7yP9bj3qvAHr2KdOdJTrN5xJV0tIKejnqlerkkRaloFDiip/HFLrrqonTEraVY/Vh7v6fbTrR4HqOWBFxfkEA8f4X/AD7tn8+q/wCTryn8W/rz+Tb8f7C/vXVus0d9R/p/h9T+Lf64t79/h6qAK/LpwjNmIuL/AFA/NgB+P6c+9+VerDiR0J3x/lKfJD4+c/q7x6mH+335gLj2G+cf+VR5p/6V1z/1Zfow2ip3XbD/AMvEf/Hx19X+t/W/+v8A9G++S54n/S9TvF5fb0jM1j8fl8fX4nLUNHk8Xk6Oqx+SxuQpoa3H5DH1sMtNWUNdR1KS09XR1dPK0csUiskiMVYEEj22jvFJHJG5WRWDKymhBGQQRkEHpYADUEY/2evnRfzjv5cGR/l9/ID+8vX+Mr5fi/3Lka/KdZZAiaqg2LuBtddm+pspXu0j+XDKWqMPJOfLWYkhdc09JVye+jnsj7orz/sRsd0nT+tVkoW5XgZo8BbhV4Z4SBcK+aKroOoa5s5fOz3QuLZD+7pT2f0G4lCf5rXiMZKk9VF1mQV6csp+q8/48D+ov7nImgJ6CXX0kv5cja/gB8NG/wBV8beoD/t9lYf3yX90P+V/59/6XF5/2kSdZP8AL3/JD2b/AJ44P+ra9Bj/ADXnMf8ALr+Xrj6r0xugj/b0vtr2hz7pcjf9LKH/AA9Pczf8q3vv/PLJ/wAdPXz/AD4d1Z/2a/4s88v8jOj15/oezNsX/Hvpp7kmvt1z76fuS+/7RpesdeWf+Vj5f/57oP8Aq6vX0rp/q3++/te+K8/Bv9Xl1mOvH/V69a0X/Ck+Yw/H344kEjV3RlV4+v8Ax42XPvMH7lv/ACuXOf8A0rU/6vJ1FXvN/wAkHaR/y9f9Y361JMPR5XP5HE7fwONrszn89kaHC4XD4umlrsnl8vlKmKhxuLx1HTo9RV1tfWTpFFFGrPJI4UAkge+iV1dW1ja3F7e3CRWcMbSyyyEKiIoLMzMSAqqASSTQDJ6x3ghluJooIIy87sERVBJLE0AAGSScAdbkP8uT+U3sH4ubfwPaveGDwe/PkjXRwZaI18UGZ271CzrHPS4jakMyy0NXu6hYXq82FMiTXiomSFWmqeTn3gvvNb17h3l7yzybeTWXIaaomZCUlvuIZ5Thkt2GFhxqXulBJCR5be3vtrY8uww7lu8KTb+3dmjLB6KnEFx5v64WgqWt3rf0j/ffn3hxPwfqaU/z/wCTrNsz/j5qP/lnX/8AuG/vcf8AuFvX/PMv/V+Hp66/sR9o/wAvQzyfn/XP+8An2HR8I/LpD/0D0WT5MfFLpH5g9aZDqnvHZ9HuXB1Cy1WEy8QjpN07MzhQxwbk2dnljerwmYpxYMU1Q1UWqCpjmp3kiYb8g+6POPtNzJBzJyfuZhnoguLd6tBcxgn9KeOoDrk0OHQnUjK1D0Xb5y3tHNO3Ntm8WweBjVWGHjbgHRuKsP2EYIIJHXz/AD5v/Dfsb4K/IDcvSm/w+VxYiTcXXG+Iqd4Mbv7YGSnnTD5+mRrilyNO9NJR5KluftcjTTIjSw+KaXt77Oe6/LvvNyNt3OewdmsmC8tGYM9rcxgeLA5HGgKujUGuNkei6tIwn5x5Uv8Ak7e59ovhqSniW8o4SREkKw9Dghh5EEZFCdjD/hKZJes+eFvpp+L3H+x+RNjzyeD75x/3pq609jc+e8/94rqYfYRdUXOB8x9L/wBrPW6Nt0Agkj+xcEgflXNr/wCwB98ad1b+3HHBH8h1Km74Bz5/5evmEfzY5T/w6H821BsF743SLH/BKK/+w59/Ur92LH3dPY0f+Gntf/aHD1iDzXQcyb0T/wApDdE4oYw0YJ4A/Uw/qf6D+p9ztgDhn/Ueg8ATUk46sl/lAvf+ZL8cI72DDuFVH9AOhO0ebfk+8R/v3Y+6r7omudW1/wDd52/qWvYc/wDMWOVaDtH1X5f4ncdbpe5f8/8A7BP+hffA7Zf7M/af8vXQyb/L1qr/AM9WPDjvPpSpzOdFDTp1JmoY8bi6U5PctTWSbjzb42ohxtRLjccME2Rijhralq1ZqaNzJHBOyiNuzX93xPeL7Xc229nYM7NzDIxmkISBQtpYhlZxqfxSpJRQhDEULKM9YXfeTjhPMWxzSXKAix0iMVMhrLLQgUC6QRklgR5A9Xf/ABnLn4Z/FQyaQ56C6LLhSWUP/oqwWrSzBSy3+hIBPvnL7t0/1+veGnD+sm70/wC5hL1lL7e1/qLyZXj+57P/ALR4+hTp/wDOf8h/9FL7DQ+DoZv8J6WWP+sf/BB/vY9opOH5n/B0nf4T0ImLte351Aj/AGGoH/ob2Q3Px9JZf9EP+ry6EXGfRP8AkL/oUeyqYUC/PP8APoum+I/6vPrVV/nQF/8AZ28aFuV/0KbE/r/zvN5/639B77gfcM/8R42av/Ryvv8Aq91g777V/r7IP+XSGv8AxrqurHXMKn/Ae8zDx+fUO/Lpx966304dlbKfrbf+8+vZd3bD3/LsrcFXt6TfPVm4m3d1pu16RYnOb2LulqHGNn9u1Il0xVJp4SXR10+m5SbXf/vXbrLclsrm2WePxBb3kfhzx1JGmWOraHxWlTgg+fW5EMcrxF0YqaakNVOBlTQVGf2joO5lIJI/23A/x9rwRQCnl03QAgjh1Bbi/B5JJH+v9fr+PfqCtOqMPMcK/wCr8um+UG7f65Nv8frc/wCv+ffiK09eqmgqR8P+rPTTMv1sObeoH6MP6/64/wB59+qOB/b1o1GQM9M1SoPI/ULfTkf76x97/onh1ojV3rx6T9XGGF1/1iPyp5+o/wB696JKnPw9W7XWv4h/qp0m6uIuD6TcXuObEAf1P5t7b6upDDS3xDqRszddbsHcsO6KDAbI3NWU2L3JiI8R2NtDF772lJHujbmT21U19RtjNK2PqMxh6XKvV4uqYeTHZOGCqiIlhX2Wbvtce82D7fLeXUCNJHIZbKZoJv0pFlCiVO4I5TTIvB0LIcE9P285t5A5jRqAikihlyCKkHBIrUehoegzajEEaQ65HWNFi8krmSZ9AC65ZCAZJWAuW/JN/ZkaPU/nj/J00O004jz/ANXr0zz0+lvpcG9j/wAQbHg8e9Ag4Iz1Vhp7lOOopiBN1HP54/x+v+t78pwP5dXBBFR+fXHwlr3Fv9bkg3+n0/p735/LrRzg/l0K/VG8evNkQ9sRdhdIYDuubfHT+6dgddVO4N6bo2cekey87VYqXA98YGPa1v74bi2ZSUlRFT4bItHjqn7smVwFKPv16aoaih6DBKYqq3YvwAXKhSSBYsQo0qGP4HA9+63nPWUIp4/oDb8fnge/dbK0APUyFBwbfX/C/H+PvfVehEXfW6z15F1Ua7HnYcO/JezYsZ/d7boyqb1n21BtCbI/3uXFjdz41tvU6RDGNWnGLKDUCnFQxkJeNj20b2eYxE/74Nn9AZPEl0eAJDMF8HX4OrxCT4mjxCO0tpAHT3jy/TC01D6fxPFpQV16dNdVNVNOKVp50rnptpoxYc8i3/Fbf0/Hs4HEdJG6UFIDxySRe30/pxf6cH3b16r59C5Ubb2JTdYbU3dQdmplOzcxvTdmC3T02NkZ6gbZWzcPjsLVbU7BPY9RO22dzDe2Rrq2l/hFJElXjPsRJMzLKoBXFdbo28XljLs+jZ0gjkhv/GRvFlYkPD4AHiR+GADrJKtXAFOnCsYhjkE9ZixVotJ7VzRtfA19Bw/LpKY6vq8XWUeToJft67HVMNbRVHjjkMFVTuJYZfFMkkMmh1HpdWU/kezSaGO4ilt5l1ROpV1rSoOCKih4emem1ZkZXQ0cEEHqHPNJPNLUTtrnqZ5aiZ7KuuaokaaWTSoVV1yOTYAAX4Hu6KqIiIKIoCgfICg/l1XVUsW41qT9ueuBYIrSESMEVm0xoWkbTyQicFmP4H5926qTQE0xx6V+7Nsy7K3Tm9qT53ae55sHVpSPuDYm4aXdmz8qXpqerFRt/clCsdLlqNFqRG0iKAsyOn1S58DUBqEV8mwfzHXlNajHpjh+Xr02RTTCN4A1oJJEnaOyHVMkZjRtZXWNKOeAbc3tf37zr50p1sZBFcV6EPoNr/I749qFQN/p06mYOQwP/H+4ABDY28YPP0vf2Gucf+VU5oJJp+7rkH/nC/8APoy2k/7tNsFM/UR/8fHX1iK39b/6/wD0b75Mnif9L1O0Xl9vSYqfz/sf+ivbJ4j7eli8f9Xr0Uv5e/F3rH5k9Cb9+PvbNA8+2d640pRZikSI5vZ256IGo23vXbc8yslPndt5MJPEGvDURh6edZKeaaNxFyrzTuvJm+2HMWzS6by3epVvgkQ4eNx5o61B8xhlIYAjV5YW+6WU9jdLWGQUJHEHiGB9Qcjy9QRUdfM+776b7I+B3yX3r0x3VsHau7Nw9fT7gxlPit54/L1nX/YG2ty4LLYjavYmGXG5TDZCux01FkY8xinSqVqTKUqQ1cflp6mmHTTY992v3J5Qtd02Tdrm2t7nQzS2jKlxBJG6PJCSyuoNV0P2kNGxKnSysYD3Cwudi3KS1u4Ed0JoJBVHUghWGcjNRnDChyD19CP+W3/273+FvreT/nGbpz1udTv/AL8fC+t2/Lt9Sf6++aPuhnn/AJ9NP+Wxef8AaRJ1kTy6KbFsor/xDg/6tL0Gf82T/t3N8wf/ABCu6f8A419t+0H/AE9Pkb/pZQ/4en+Zv+Vb33/nlk/46evn3/Dg3+WPxV/w+RvR3N/69nbY/wB599Mvcin+t1z7n/li33/aNL1jry1/ysfL/wDz3Qf9XV6+mBP9W/339r3xYn4N/q8usx14/wCr161mP+FLTaPj38bz+f8ATTlrf6/9xcvb3mD9y3/lcuc/+lan/V5Oop95v+SFtH/PV/1jbquz+QJ8Zsb2x8g95/IHdmOjyGB+PmIxke0qerhkamk7O3wMlS4zLxkyimqn2ptvF5CQRvHIYKutpKhTHJFGxk7753P9zy7yNtnJ22ztHd71K/1LKc/SwBTIn8S+NI6CuNSLIhqCR0GvZjYI7/erveriOsVmoEQINPFkqA3odCA48iytggdbg2Q/Uf8AY/70ffKt+H+16ypi/D1r2fzdP5r+a+K2Ui+Ovx1lw1T3vkMPBlN67yyVJTZqj6lxOYpDNgqahw1Us2NyG/crSzR18SV8c9HRUJhklpqj7uPxZg/dp+7TZe5Fu3PHPSS/1RWQx2VnGxjN46NSR3kWjrbowKdhDu4bvQRkPFPuZ7mTcsuNj2Jk/fJXVNKwDCFWFVAU4MhHd3AgLSqtqFNWOu+Tvyhz+9KfsfcXe/ZO5940q5taPI7t3HWbsoKCHcWMq8PlYaHbu4nyW3KOnlx9dIsMcVIiUriOSERyRRsvSKy9u+SNs2qTZNq5Xs7PbHKF47KMWxbw2DoWkg8OQnUoJJbuyGqCQca7nmXf724F3e7vcyzgmhlkZwNWCAGJVRQ8AKDy4Do93wR/nBfJ/wCIG9tv4fsLfW7+9OgKitpaHdewt+Z2v3PuHb2GlkhhqMx1puPO1k+TwuWxEAMsWNkqDiKwGSN4oZZVrIIb95fux8ge6G13s9htdttfOdDJBuNpGsQkkoaLdoigTRsaamI8VaAq1AVYX8n+5+/cu3cMd9dy3mzntkhlYsyg07omYkgr5LXScigJ1C+b5bf8KEPjT1DjRhvjNi6j5G9gV2LgqYsrImV2l1htiSvpoqqnXNZbIUFPntxZKljqUaWgx1OkIYPDJXU86Mi4V+3P3GuduZLw3fuRfLsuyxvoNvA0c93MFNCUKl4IUbOl2Ltj+xKkHqaOY/evYdrjWLYIzfXxXUGNUiSoqNRIDMRiqgDzBYHHWrD8qPmj8iPnBvqj393/ALxhztThYK2i2htjD4+HCbO2Pi8hJSy1uN2vhYWmenjrJKGIz1FTNVVtSYo/NNJoW3SL2x9p+RfaLYm2DkfZFtbeRhJcTMxknuJACPEmlYlnbJoBREqQiqMdY48zc275zdepfb5c62QERRqNKRqTUhFHr5k1JoKk062TP+Ep6aa354/kn/ZYGvc+lbfIYeMLfRZWBa9tR1WJIC25s/3pZ7fY2vrvP/eK6mb2DP6PONf+XX/tZ63Rtujj88R2/wBurX/2xX3xn3Un/GMVr/mH+fqU94yD/pq/z6+Xh/Nqq1i/mkfOAFgLd+bpB/wslFxb+v59/Up92M/+A7ex3/iqbX/2hw9Yg81ivMm9enjtU9Ezps1EYlVSqgCy/wBTxyWPudgePQcY1IAGOFP8p6sr/k65CKb+Zb8bYla7N/pi1Nq/1PQPajEW44Fvz7xG+/aa/dV90c51bX/3edv6lz2IoPdflRVH/KVX/sjuOt2Lcv8An/8AYJ/0KPfBDZf7NvtP+E9dDJuP59aof896ATfILovV9B1Jkh+fr/fHKfgfU++1P93aD/rT85KP+mif/tCs+sJfvLADmnYD/wBI+n/VaXqszCd4fInG4bG4TCd9d14fCYbH0eLw+Hxfae+cfisVjMbTR0ePx+Nx9JnYaShoaCkiWKGKJEjijUKqhQB7zNvfbj27v7i4u77kPZp72WRpZZZrK2d3dyWZ2ZoizOzEkkkkkkk1J6hG25u5stoYorbmfcYreNRHHHHczKqqooqhQ4AVQKADFPl0LHx77y+R+R+SPx+xWX+QPeOVweU7w6ox2YxGS7X37XYvLYuu37gKXI43JY+qz81JXY+uo5XimhlR45Y2KspBI9x77me2ntzZe3HuBeWnt/skV3Fsl9LFJHY2qujLaysrKyxAqysAQQag5FOhVydzjzfdc38rwT817k9s+5WyOj3MzKymZAVZS5BVhgg4I49bmeP+sf8AwQf72PfBmTh+Z/wddHX+E9VNfzpuwey+vOi+n8j1j2HvrrnK5DuH7DI5PYe7c/tDIV2O/uZuWo+wrazb2Qx9TVUX3MKSeKRmj8iK1rgEZu/cO5Y5a5n5x5/t+ZOX7HcIIttgeJL6CKdUYzEEqJUYKSMEjiMdY5/eJ3Xddp2HYpdq3O4tpXvWV2t5HjJHhE0JQgkV8j1Qvt75F/K+RUJ+TvyKbgE37s7LP5AP13Mfx76d/wCtN7Vnj7Z8v/8Acus/+tPWJQ5x5uJA/rVuVf8AnpmP/P8A1IzGc3vvzMLuLsLeO7N+bh+0p6E57ee4sxujMiipTIaejOUzlZXV32lOZnKR+TQhY2AufYt2fY9l5esU23YNotbHblYstvZxRwxgsaswjjVVBJ4mmfPoqu7693Gc3O4Xss9zTT4kzs7UHAamJNB5dOsSrHGFBP0+g4H+x49mfSfHQ2/6FZ/4X/Ff9LfQ+n/Zb/8AZlP4f/pDP8T+z/vh/c3/AGX/AO1/hH/ZVHl/3Kf3Qvb+Ef5R95/Z9h/+sKeN4P7j3Ov71/dGrwO2vh+L9dXX/wAk38H1H8eNHSjwDpr48X+431FNR9aeFw/t/PR6efQFZbF5LB5LI4PN4nJYHN4WtqcXmMFmsdV4fNYXKUMrQVuKzGHyUFLkcTk6GdDHPTVEUc0Lgq6gi3s8trm2vbaC9s7qOa0mQSQzQsskciMKq8bqSrowyGUkEZB6Zkjkid4ZY2SZG0sjgqykYIZSAVI8wcjphlsbn/EW/wAfx+fb/wCXr02eI6UmPyuwqXr/AHxhMxsfLZXszLZ3ZVd152PS7zrMXhtibexM2R/v9t7M7BSimx29Kne1NU060tbNPFLiWpy8YJYh0EsG5vue3XEG4Im0xpKt1amNWaZ2A8J1mrqi8IipAwwNDWuN1j8KVWjJmJUxvqNFH4gV4NqHAnhxHzD9wQb2+p/33+3Hswyw6Y4Y6b54/rz6Tz/rfj63H1/3s+60r9vWqUz5dMlRFbU1r2N2H0/2I/4p7txH8uvU0mo4Hj0yVEX9pR9fqLH1D/jfvVQag/l14gg6k/Z0petev8f2d2LtLYOU7K666dx26q+qoKntHtzK5DB9a7MFNicjk4q/eGXxeNytdQUNbPQLQwulO4NZVQq5RGZ1K963GXZtrvdxj2q6vnhUMLSyUPPJVlUiNSQGKhtRFa6VNATjp+GNLiWNTMkVcF5DRRQE5PlWlB8yKkDPQM1UJbWwABV3Q2uUbRIyCWIsqOYJQupCVVtLC6gmwMj5fZ/s5+Y8+qjvGfiHTLUQlgRazci4tyP+R+6nHW1NQFbB8umaWmuSrAt+bAfQg/X+oPHvxFaHz60KDUp/n1GMYi4C2/1h9ebXN+b/AOv79gjrRBU4yOlzg9v9bVvXXZm4NydjZnbvaGAq9gxdT9ZUWwq3PYXs6kzOarKTserz/YMOVpKDrltg4CKGtpIp6WrbNTSmnj8ZUsCm6ut4i3XaLW12pJdplE31l00oRrcqgMOmHSTN4z1U0I0Aaj6F5I4GhnkaYiYafDShOok0arcF0jOePD7EGsCkA/0H14545HH9fZv0xxBPn17RzY8jkEH/AFv8fx791r59YvEyuD+L8Hm/+tb/AA9+6sWwQep0KXtz9AB/vP8AvHHuw/l1Tpzg+oFvr/vj/vA9u0GPTrRNM9PcA0m1v9t/tuf8R/vXvfTRyKjp9prnT9Lgfkf7Hj8e7/Z9n+HqvQkRbI3ZFsPH9nSYWdNg5TeeX66x+5TVY801TvfBYHF7my231oBWHMxz0WDzNNUmd6ZaRxKFSVpAyApXfNqbfpuWBeD9/R2abi9tpeotpJXhSXXp8MhpEZdIYuKVKgUPSwWV0LFNzMJ+gaZrdZKihlVQ7JSuqoVga0p869Jx1IJI+jAk/mx9XH4H49nK8Ps6SEU6wlSSOP6f7An6f7D3b5dVPHrKLDSP63/173Fv9v791vrPGoBFhZdP0Fv8fp9B+Pfs9V8sevU0cH/iP9h9Pfutg5I6EToEf85IfHtr/XvPqWw4/wCe/wBv3PsNc5f8qlzR6fu65/6sv0Y7T/yVds/56I/+Pjr6xVb+t/8AX/6N98mTxP8Apep2i8vt6IF8zvm/1j8Jch8cK/uN4sR17333lR9E5LfVTWR0eN66zG4Nn7r3DtndW4HmU067WfNbbjoMjPI8MePgrfvZJBDTSI4n5U5P3PnE77DtCl76xsGv1gUamlVJIkdEANdemQsoAJYroAqw6re7hb7cLV7ltMcsyw6yaBSyswJ+VVpXgK1OB0bCoYMFZSGVrMrKQQwKgggjggj2EW+E9HUXl9vVGH87b+WTS/PjoX++HWuLoovlF0tjcnk+sawNBQydgbeZjW57qTMV8miJky7RtU4SWoYRUOYAXyU9PW1shmb2U90H9vd++m3KZzyreuEu0ALeE3BLhVGapwkC5ZPwsyIAH+a+XBv1iWt0H7yiBaI1pqHmhPDu8q8G8wC3RpP5btHX4/8Al9fDCgylFV43J0Pxp6eo8jjq+mmo6+gr6XZOGgq6KtpKlI6ilq6WojZJI5FV0dSrAEH3H3uXJHLz1zxLFIrxPu12yspBBBnkIIIwQQcHoR7ArJsu0I6kOLSEEHBBEa1BHkegy/my/wDbuX5hf+IV3T/8a+/e0H/T0+Rv+llD/h6c5m/5Vvff+eV/+Onr59Pw3b/nLL4qAXt/sx3Rw/8AYnbX5/3n30x9yP8Ap3fPv/Slvv8AtGl6x15a/wCVj5f/AOe6D/q6nX0xp/q3++/te+LM/Bv9Xl1mOvH/AFevWsh/wpiJHx3+N/8A4mrLf48jYmYt7zA+5d/yuXOWf+Wcn/V5eoq95f8AkhbT6/Vf9Y26VP8Awnb28mN+FPY2fkhphVbl+Rm7WSpiZHnlxeH2B1jj6SCq0jXEafJfesiMTZJdQtr9g/77d283udsVrrbwodjiOk1oGe5uyxH2qFqflTy6N/ZSLRyteyECr3zkHzoI4Rn869XpZD9R/wBj/vR94VPw/wBr1NkX4evmq/JvfeS7a+UfyE7IzVVV1tZuzuPsHIU71usz0uHj3NkKPb+KVZv3YqbC4KlpqOGNuYoYFT+z77ye3WxW/LPIfJ+w20arHabbbwnRSjMIl1vjBLvVmPmxJ8+sFeZr6TcuYt7v5WJaS6kYauIXWQq/IKtAB5ADq1f+Tj8CehfnLle+MZ3eu8xD15F1i23m2duKHASqd1wdmSZUVrTYzJrVBjtOk8fpXQNf11cQF96L3s5w9m7flSflOCxka8hvHmF7G8grBJYImnRLEQKXL1zk6eFDWQfazknZecY+YG3czVtjbiLwmC/2nj6q9pr/AGYp6Z6vEqv+E8/8v2Y3eXvT6kcdkYzgf4X2ebfT3hsPv2e8hAJ2nYK/881z/wBtnUs/6yvJnk15wr/ar/0B01w/8J4v5fbOAZu9uB+OycX/AFH/AGZ3H19p5/v4+80Rou0cv0oDm2ufn/y+9Px+x/JbsNUl7k0/tV/619Vcfzjf5XPxe+Bvx66u7M6Pfsh9ybx7gpdj5f8Avpu2jz+PGFn2XvDPP9pS02AxTQ1n32EgtIXYCPUNPNxkT9037zXuD74c481bDzhYbVFZWW3C7iawhmjcuZo46MZLiYFdLHAANfPqO/dj235d5M2XbL/Z2uTcTXPhP4zhhp0M2AEXNQOjf/8ACUxz9z88HYcn/ZXQBc/Qn5E/4f8AI7e4F/vTkLL7GD/pdV/ZtXRh7CKSnN44f7i/9rHW6Bt9voQeCh/2BN73BsLgcf7H3xq3Qn/GFp5Ef8ZHUr7sMEEefTluByaO1wPrf+vI/wBha9v969hxjqjjPzrn5V/1enHpHtA/xitOi87msXZtQFixI+ptdSTxz7OrWrVRRWq4P7epb2mvhhQMHAPQOZtuJ0t9EZr/ANDqA/3pvZ9bJ+tDJXNVXoa2Qwh/L+R6AvchvVMv+pAH+xC+5N2UfoBvUk/4etz8afP/AAdatf8APXwkC9vdA7i/vDt+Wpqtj5rAHaEdXId20tNT5yuyf96amhERhj2xUSy/ZRzF1c1ilArAMU7Qf3dl03+tpztafSTBRvry/UEfpEm1s18INx8UDuI/hz1hR95dAeZuXn8Rf9wiNFc/2sprT08vt6qHw0KPAq8EaRqP1B/1v8PfQnC58/TrG2uo/LoW+gIEHyW+O4CgW726iJ4tYDsDb3H45J+nsA+61P8AWv8Acg+f7h3D/tEm6FHJJ/5GnKCgf8tO1/6vx9bp2P8ArH/wQf72PfzwycPzP+DrqA/wnqn/APngqG6G6WB/5/SAP6XOyN08n3nx/d5f8rx7ijy/dUH/AFf6xk+8z/yrvL//AD3N/wBWm6pJ6greucR/emTsTYeZ39T5HrzdOH2RT4Te9XsU7Q7OyUNImzewsvPSY3Jnde39pzpM9TgZBDDkvKqvIoSx6objBuc62I2vco7Zkuo5LkyRCXxbda+LAoJHhvJikgytMcesPIWhUv40JeqEJRitHxRjTiAK9vA+fDrnCgVFBszBQHYKFDMBy2m5Cgn8c29mJpU0GOvdZibc/wC+/r7117py/u/uT7T+I/3Y3J/D/wC7n9+f4j/d7Mfw/wDuT/Gv7rf37+++x+1/uV/ef/cV/Gdf8O/if+Seb7j9r2l/eFh4vgfvK38f6j6Lw/FTV9R4fjfTadVfqPB/U8H+08Pv06c9OfTzadf00mjw/G1aGp4erR4taU8PV26/h1dta46b9yTbiq9wZ2s3lNuOp3jW5evqt2VG8my8m8KncNRO02Vqd1S7hJ3BLuGeqcvVNXXq2lJMh1E+7WMdjBY2cG1xQJtccSpbJahFgWMCiLEsdIxGBhQnaBgdaleWWWWW4d2uGYtI0hYuWPEuW7ixPGufXpLzIQbAf0/33+B9qxStcgdN449N8l7m/wDT/W/1x735AA569XjTqHKTyLcfT/D8jj/be9Dyqfz6ZP8ALqDIDYjnngXHB/qT+Pp/X341rUHPWvt6apl5455/A+n4t/iRe/veStetVpQeXl00Tpp5t6ebfnST9f8AED37jT+Lr1dJr+Hpoq4KiHxvNS1VNHVQLUUzVVLUUq1lI7MkVdQtURRrWUMzxsI54tcTlWCsbGzaSRyl1jmRijFHCMraWFCUehOlwCKqaEVFRkdXZGj0uUYAjUNQIqOGoVpUfMYr0nqqHnWB9RzcfXm3+3HvfnnrdajWpz0wzxfkfg88/T/Xv9R/j711s0cVHHpsljBFwLOCb/7V/wAVPvXD7OvDvFDx8uoDRq3BuBe9+P8AeuOBb36ma+fXgR8D/D1HKBbhyCALvcenTa9+fe+PDrx/TNPLpU7o2LvDY0uBp96bVzu05t1bSwO/dsQZ7HTY2XP7G3TFLUbZ3biknCmrwGehp5GpZ19MiqT7K9o3zZd+TcZNk3W3u0s7yXb7s27hxDdQECa3kp8MsRYalPCo6fu7G7sWtxeW7xGWJLiLxAQXjcVSRfVWAND59Jdob8hTcD/H6fT/AIn2bDGTw6TfMfmOlJVYvaUezMFlaTdGQq981ufzdDn9ly7flpsbg9vUcFM+DztLuRpjDlKrL1DyJJTKgaALc2t6iaG63p9+3Cyn2eNOXo7aKS2vxMGklmYnxYmgpWNYxQhyaN/gXywbYu1WlzFuDtu7TOs1qYyFjjAGiQS1o5c1qoGPyyn44dIHNgx4J/I/1/6j/W9nGDQdF3ThAhJFvr9Lfj82t7eGAOqtwpTp5gS/1H0I+n0twb392HTZOQR090yFfxf+h/1hbj3atSOtcehOfrXfFH1/hu4arZ2Zp+ttybszXXWD7Blo1XAZbem2cbQZvPbRpK/V5XymKxWThqJI2VY9D+lmZWAQJutg25y7It6h3SOFbp7YE6hGx0rJwpQnGDUVFRQjq/gyCJbnwj4TN4YfGSKkr6+R+WD6dJjgqw/4N+b/APEnnn2Zj08+qHqM402H4+o+vN7fX/W9+rXqpxSvSw2J/o6bO1A7Sn33BtYbc3UaN+uafb1TuI7xGDrDseOpj3NNDjF2u+5xTjLsrGrShMhpwZQo9l26/vn6VP3Etqb7xo9X1hkEfhax4tPDBbxNFdH4dVNWOnofp9f+NGQRaTTwgpbVTt+LGmvHzpw6a3wW46LA4TcuTwOZotv7iqMrQ4DcVRiMjTbc3BkNvmkTcFFt/NVFOmPy9Tg5K2EVcUEkklMZkEoUsLq0u7SW5ubKK7ja8hCtNCrqZIw9ShdAdSBwDpJABoadNBJFSORo2EbVCtQ6SR8QUnBp504efUVCTcn6f7H6gf7f2/1rz+fQkdCRzw/JH46+eCopxUd29RVUBqKeaAVFLN2BgRDV0vmRPuKScowSVNUb6TpJsfYX5ueKXlTmvw5FbTYXKNoINGEL1VqVowrkHI8x0ZbUrLuu16lIrPERUEVBcUIrxB8iMdfWKrf1v/r/APRvvk4eJ/0vU6xeX29atf8Awqbj2lJ8PPj6u9KLcVfhv9mXbxQbXrMfQ5MZluku30wM0k2Thmp2xsGXaFqpABJJAGVCGI9z793Fd6fnLeBsM1rHffu2rNdq7J4f1dp4oAjIbWUrp8q8acQHOdDbDaYDdrIYfqFxHStfDlpxxSvH/LwKS/4T2fzQZ+/ussf8K+9txCo7v6f21EvU+4MnLap7O6mwVJFTphXqpX1ZDePW1HEkThrVFbhRFUWlkpa6b2afeH9rv6ublLznsVs37gvZa3SLkQXDGtaD4YpjkcQslVqoaNerckcw/X267ZeSD66IDQf40FBx82XgfMihydR62TMh+k/7H/ez7xj/AAfn1IycekvNHHECkUaRIGdgkaqigu+tyFUAXd2JP9Sb+0039j0qXi3Va/8ANl/7dy/ML/xCu6f/AI19jL2g/wCnp8jf9LKH/D0X8zf8q3vv/PK//HT18+j4bL/zln8VWP4+RvRth/X/AIydtcC/+F/fTH3I/wCnd8+/9KW+/wC0aXrHXlr/AJWPl/8A57oP+rqdfTHn+rf77+174sz8G/1eXWY68f8AV69ayX/CmAavjx8bwPz3Vlv9h/vxMwf+I95gfcur/XLnKn/RuT/q8nUVe8v/ACQtp/56v+sbdMv/AAnC33i6345/IDq6OWMZvandlFv+sgvaUYrsLYu3du46Wx4aP7zrGrHH6T9fqPZP9+PZriDnHk7mBv8Aca52trJf9PbTySt/xm7XpX7H3cT7HvFgP7aO7Ezf6WREVf5xHrYTyH6j/sf96PvBJ+H+16niL8PXz1/5lnx73D8afmt3bt7K0FVDtrfm8c52v13lZIiKLMbS7AylZuCOKgnLEzHbOWrKrEVGvTJ56FmsUdGftd937niy589quU9xt5g19a2se3XyVGpLi3RY2LAcPFULKo/hceeBhf7i7FcbDzbu0MiEW88rXMDeTJKxbH+kYlD81rwI6sv/AJCHyb6C+Omd+TFd3r2zsvq2l3PD06NvS7vy0eMGYOGpu3kywx6srNUnHtmqQS6QdH3CX+vuDfvk+3fO3uBbclQ8m8uXG4SQQX6zCDTRDJLtjIGLMoGoQuRn8J6H3svv+y7HFzQN33OG3MptvD8VtOrR9RqpXjTUK/aOtk/GfzNvgDn8zitvYX5Y9OZLOZ3KUOHw+LpNzLJWZHKZOqiosfQUsQgvJU1dXOkaKOSzAe+f9x92/wB8LO2nurn26vkgijaSRiYcKoJY4lJNAPLqc4ueeUJpY4YuYrVpXoiqHBJYmgA+ZPR26Y/vAf1t/vLD/inuBbwZJ/ojocW/Efb1r7/8KZrr8PPj+vIA+S1DcfkqOruxSv145v7zV/u6af65fP5/6QiH/s6j/wA3UL/eEH/IY2L0+tr/ANUn6CX/AISlcT/O5vrdfi8FX6gE/wCzFH8n6C3sx/vTBRPY7OP93RP5furoJ+wbfp84LWg/xU/9pPW55gnA+p58X4Btwpvcg2PBvb3xq3MU8Zhwzx+wfmOpd3Ra4+fWrt8yP+FKGS+NHyd7w+NUPwvp97J05v7LbITebfISXbrbiXGCG2TO3v8AQjnf4R5xLzCK6o02/wA4ffVP2r/uzuWvcX2x9vuebj3YvrafeNntN1eBLKJ1jN1AkxjDG4UsE8SgJArStBw6hG991W2HdL6yGxCUwytFqM2mukkVp4RpWnDP29FFyH/CnfcWVUyR/CDHU2oMBr+RFTUatRvzbpGm+gHuS4f7qblWI4949wOAB/iEI4f9RHRvbfeKurVBTlSM04VuD/1p6GX4cfzvty/MH5Rda/HrIfGnE9e0fYi74Em7KbtWs3NPif7qdd7t3xGEw8vX+CjrTXzbZWmJNTF4xMX9WnS0W+/33BuXPZP2j5q9yrD3Evr+72xrPRazWsUaP9RfW1qausjMNKzlhQZIA8+pE9uPfe95x5t2jliTluKCG5MtZlmZyvhwySiimNQalKcfPq5rcJvVOT+b8/j9I94L7QoWBVHkP8/WSNxSv5k/4OtVf+ehc/IPosD89TZEHi553lk7AW5JZrWH5PvtH/d2kD2p5zJ/6aKT/tCs+sJfvLgnmnYFH/KAf+r0nVVGKhqKZWpZ6eqpKqA+OopK2mqKOspZVHqjq6SpjhqaaZeLpIisL/T3n9FJFOiTxSo8DDUskbKyMPIqykqw+YJHWOJVoyYipWQYIYEEfaDkfYehZ6B9PyU+PIH1Pe3Un+xP+kHb9yf9v7Anutn2v9xvT9wbh/2iTdCfkig5z5QFD/yVLX/q+nW6Nj/rH/wQf72PfzxSfCT8z/g66fv8J6qC/nfW/wBBHSn/AImk/wDvEbmt/vPvPj+7y/5Xf3G/6VUH/V89Yy/eZ/5V3l//AJ7j/wBWn6oZ2x/wHT/lmv8AvY99X+sOlFOleCRf/H6/19+6310T/X/b+90690p/4lv/APhv2n3PYf8ABP8AR5/B/t77u/g/+hr+9n8a+x8VvsP9Df8ApA/yrTb+738d/c/4Gc+yz6bY/H8X6ex+q+u+o1Uh1/XeD4fiV+L676fs1f2/hdtdGOnvGutHh+LN4fg+FSr08HVr0+ng6+6nwas/F03by3duvsDdW4t9783Hl94b23hl6nPbs3ZuCq+9zu487WaRV5bLVmlPuKycRqCQqqFUKoCgALLO0tbC1t7Gxt1is4l0RRp8KrUmgqSeJJJJJJJJz00zM7tI7VkY1Ynz8vLHAdJGf/in+w+vtQMdUpSuMdNkn+25PH+9/wC292yQc9er68fXqFJzcG/1/PP5/px9fdRxH+r59UPGlcdQn44/HNjbn/YfU+7KeJP2dVI9RjrniMdTZfOYLC1WZxG2qTNZzEYeq3RuGSph27tikymQp6Gp3JuKakp6mshwOChnNTVvDFJItPExVSR7R7hdS7ft+438NhNdS29vJOlpbANNO0aM6wQhiFMspGhASAWIBPTlvEk9xbwSTpEkkio0smEQMQC7kVIRK1YgYA6bNyY2HEZvN4anzuJ3PS4XL5TDUW5tvS1FRt3ctDiq6ehpc/t6asgpaybBZmCFamjaWKORqeVSyqSR71t1y99t1huEm3zWktxBHcPaXICzQtIqu0MwUsoljJ0uASAwIBNOt3MYhnmtxcpMkbtGksZJR1UkBkJAJRhlccCOoe7N5bz3fBtCi3hujO7lpNg7QxuwdhwZ2paoj2nsLGVFXXYfaeBDRRmnwFFU5CaSBCXJMpOphayPatg2LZZN6n2Pabe1m3G9fcdwaAUNxdyBVkuJcmsrBFDcOHAdOXN5e3KWkV7cPIkEKwW4fPhxLUqi/wBEVxx+3pOf3V3RU7Xy296XbG46vY+Az2F2tn960uCylRs7b+6ty0eTyO2tsZzc8NK+ExG49yY7B11Rj6Conjqq2no6h4UdYnKm1Cc9Jq6Hwe0+XTTt7Ebbytbl491bvXZlHR7czGTxdacJXZ4ZncNFDG+I2yKegZJKQ5uYlPuX9EWnkcj2T7ze7tZw2T7Nshv5nuooZkEqQ+FCxpJPV8N4QzoGTX5dGm3Wu33Elz+8Nz+kiWB5I38NpNcijsiouV8Q/iOBTpBHWyq5j0MyqxS/k0OVBaPUvDFDxcfW1/Zw1AxCmorx/wAtOi4VcBwCG8wOPT9sbYe6ez99bN612PjqbLb17C3Tgtl7QxNXmsBtukym5dy5GnxOFoKrce6sphNr4CCqyFSiPWZGto6GnU65po0VmFQDXjg9eYqVLemek3VUU9DW5HG1kaxV2MyFdiq2NZIZ0hr8ZWTUFdAtVTSy0lTFFVU7qJYnkhkADxuyMrHfA160pDAKfyPWWsmyFQaX+JVNfVslBT0uPbIVdRXNT4imaWnoqKheomnajxlI0ciw0yaIobNoRQeWYIrWETi1hjSsrPKI1CAyNRmZqAanaoLMak4qTTq7tLVPHZmGkBdRJooqAFqTRRQ0HAenT9Hjdjv13Nnv755T/SV/femxVH19HtSSTbtX14+CqKqs3w2/1yfggzlLuREoBhvtGaSBjP5QBp9lz3e/DmVNv/ccX9V/oGmfcjOBMt54oVbX6TRUxtCTJ42ugYaNPn0o8KxG3G4F637z8cKtuE7DDpJMvi1pqD9uinDNeknoDEED6/Uf71bj6/09nBznpEacR1mVQxsRxz+P9hwfx7tlj8utdTIIwWAFyxI/2N/6f4/X251Qkip6eKbxyKJInSVLldUbq6alJDgMpK3UixH4PtzQynSwIPHpkEHIII+XT7Apta3+sbD624/1h/X/AA96p68K9WBp0oYqmsakix71lY2OhqZ62DHPV1L46nrqqOGCqr6fHmQ0cNfVQU0ccs6IJZI41VmKqAG/Dj8QzCNfHKhC9BqKgkhS3EqCagVoDnrecDUdNa0rivrThXriYyCeOOb8/jk3Iv7dBpQeXWuOeoUnI5B/tfj/AGH+te3twZ60enPK4n+DtjFOVweVOTweLzl8Hklya4w5SN5P4JmSIo/4fuPGaNNZSHUadyBqN7+0dle/Wi7P0dxD4NxJb/4wmjX4ZA8WLJ1wvXsf8QrgdXki8ExDxo31xrJ+m2rTqr2tw0yL+JfI+fUuo3JuXJYTA7UyO5M/W7U2xW5ev2xtmuzGRq9t7Yr9yyUkm5MjgMHLUSY7EVmdeggetkpo0kqjChcsVHtxLOziubq/hs4lv5lVZplRRJIIwRGsjganCVIUEkLXHVdchWOJpGMKklVJJVSeJA8ifP16xyqlHWTx0lalZHTykU9fTpNBHUqoFp4Y51WaJWvazC/+w9vRO8kccjxFHIqUJBKn0JGK/Z1VgA1A1QDSowD0MPU29d370+R/xSj3duPK7ij2T2P0hsLaCZWoE425srB9iYqbD7ZxdlQw4rHTV0zRIdTAyG7G/sEb1sOzbFynz82z7dFbG/ivdwvDEKeNcywESTPWve4Ra0oMcB0d2V7eXu6bELy5aQQNDbw6vwRI40ovDtFT8/n19Wmt/W/+v/0b75XHif8AS9TZF5fb1qu/8Kq1DfDX48Ai4/2afF/++m7T95I/da/5Xzev+lRJ/wBpFt0FefP+SLB/z1J/1bl60z+nexZemMl/pN2Y29MB3ts3P7I3T0f2RtjdWPxGJ2Bmtv5x67dE+6dpVu28wN/0e5cHpoYaRqujpIryiqjrKeZ6c5ybvtFhvm2Xmz7tapNtlzG0M8T17lYeRFGVlOQykMpoykMARFNtc3FlcwXdrKUuI2DIw8iPUHBBGCCCCKg4PX0Y/wCXh879kfzAfjbt/tzBJRYPf2I8e2O49gQVAkn2Vv6kh/ywU8byzVL7X3JGn3+HndmMlHKIpG+5gqEj5fe5XIO4e3fMl1sl1qexY+LZXB4Swn4SaAASJ8LjFGFR2lScjOXt5g3ywjvIsSU0yp/C44j7DxB8wRwNQDq1X1b/AF/+JHuN5v7HoRrxb7eq1P5sv/buX5hf+IV3V/8AG3sZe0H/AE9Pkb/pYw/4ei/mb/lW99/55n/46evn0/Dc3+WXxT/8WO6N/wDfnbXt/vHvpj7kf9O759/6Ut9/2jS9Y7ctf8rHy/8A89sH/V1evpjT/Vv99/a98WZ+Df6vLrMZeP8Aq9etZn/hSwuv4+fG9f6905b/AN4XMe8wPuW/8rlzl/0rk/6vJ1FPvL/yQto/56v+sbdUN/ytvmFT/C35SYDdu6J6iPqfsSgHXPafj8skeJweWyNFU4nen2kcqpNLs7NU8VRMwSWf+GSVkcKNLKoOUf3h/a6T3S9u73bNuQHmOzf67bqkDXIisrQFjwE0bFRlV8Tw2Y0XqMfbvmdeV+YYbi5am2zr4Fxx7VJBWSnmUYVPE6SwAqet8v8AiFDlqKjymLrKXI4zJUlPkMdkKGoiq6KvoayBaikrKOqgZ4KmlqqeRXjkRijowIJB98XLuCe1mmtrmFo7mMmOSNwVZWUkMrKaEMpFCDkHrNC3ZXWN0YMhFQQagg8CCMEHolfzJ+FvR3zV6/pdkdwYWqFdhJqmu2Vvvb0sGP3rsjJVcaQ1c+Dyc9NVwS0GRjhjWsoKqKeiqvFG7x+aGCWIde2Pu9zh7Qb3NvHK10pt5lCXllPVoLhVrp1qCpDpUlJFIdakVKM6sW8z8obNzhYrZbtCdSEtDNGQJIyaV0kgih81IKmgNKgEa5m6v+E7HyPqdzDE9Td7dKbnwUi1ckWQ7Fi311/lo0hs8UUmM21tfs2jmbxfqcVUYLDhADxntsX36ORLvbLy737k/d7a9tohNLHafT3KFTJHF2ySTWrE65AaFAKVzWgMCbn7Cb/bSD9373Zy2xNA0wkibzPwqko8v4vy6O18Qv8AhOhhesd/7M7U+Svdy70yuyc9gd14rr3qjG1mF24+4tv5Kny9Ec1vncCJnszhBV0qa6elxeIqHC3+4UEp7if3M+/S287TuGye3fKT263MLwtf7qUaRFkVlbRbRM8YkFaqzSuoPGNh0IuWPZWPbru0v983bxZYmWVYbcFV1KwYapG7mWo4BVPz62aab/PJ/rj/AHg/8b985LziR/RHWQ1vx/1fLqhP/hR1/cHKfG747bb3xveXZ1NWd65LNU82Lw6bpz04wfT/AGIlOaTbEeQx9bU4yo3FkcbQVdahMVCK+N3uWRWzH+4AvMVtzh7iblsGwi9mTbIIGWWTwIh4t7Hq1TlHVXWFZJEQ5fQQOB6h336+hk2Hl63vLvwgbt2BA1N2xPwSoJGogE8BUV6An/hKYCr/ADr8gUS6fi+k6pIJBHKn+zCmSHWhIJRzY/4exB/emii+x2TppvRUkUr/AMkmhofl/PoH+wQHh83jz/xX9v8AjP8Ag63MMRJYD/FCB9Ba6mx/w+l/ybe+Nu5A0uM4/wBgf5D1Me4pUn7f8vXzUf5sPXu48f8AzCvlRv3KUFNBtXfvyE7Vx+1simZwVXVZGs2PPtyk3PDV4KiyVRuDBJQVGepRFJkKSkirRIzUrTrHKU+pD7sgp93X2LGK/wBUtq4fOyh6ws5s0/1p3/VwW7lx/tz0SSjxEbwr6VA/FrcfXgX+pv8AW/udaaQQOPQe7pGNeA6sx/k/YLbw+f8A0Zlancq4/cmNyfZ1Nhdp/wALqpzn8XVfH3th8llxmEP2lCMTMiR+GQF5NVx+pfeGX38rnc4/u3e4FjDtBk2mWPb2uL7xFHgyLvW3BI/C+J/EBrqBoPyPU1ewcNi/uPsFzJuOjcEknWK10E+IhsrnU+v4V0HFDx/Mdbj24uJrfThwf+SPfCnaDWMnyr1n9PxFfn1qu/zzJXg+Q3Q08TtFPT9W1dVTzI2h6eppd719RT1Eb3GiSnnjV1b8Fb++z393iiS+0vO0Mi6on5glR1OQytY2YZSPMMCQfl1hR95VynNfLzqaOLGqn0InkIP5ceqyK/c+6d9biz+899Z7L7q3nurIPmN0bk3BJ5s1m8rPDFE9bkXMUAaokp4Y1FkUaFWwt9c8dl2naOX9o23Y+XrGG02S0i8K1trfEUSAk6UycaiTxJqT1jtcTXFxcT3N7Kz3bmsjOKMTQAVFABQAAYAAA6F7p3A0eL75+Iuah3ntXcdfvHuTr7JZXbWDqchPuPryXEdtYLD0mK37DV0NNR0eU3HTR/xChWllqUehYFmVhb3HvuNuU157f+8u3vsd3a29jst3FDdTqiwXgk2+WRpLQqzMyQk+HJqCkPinQs5QgWPmvkW5+villn3K3Z40JLw6blFCy1AoXHctK1Getxyg/sf8s/8Ainv5+JOFPmf8HXTVuHVQf87s/wDGB+lf6nuf/eP7kbov/vPvPj+7y/5Xj3F9P3VB/wBX+sZPvMV/q7y//wA97f8AVpuqF9sn9iMf7Qn+24/4ke+sHWHfSvJA/wB9/vj7tjy691hZ+OeB/vZ96J4+vXuhB/0yds/Y/wAM/wBJW8/4f/od/wBl2+z/AIs3i/2X/wDvD/e3/QrfR5P9HH95/wDLv4fq0+fjV4/R7Lf3LtGrX+7IdX1v7z4H/czTp+ppWnjacV4edNWera5f9+H+y8Hy/s/998K6f+KrTHSBrhS/cz/YvUyUYmcUr1kUMFW8H+62qoaeepginIHqVJHUH6MfZhHr0DxAol092mpFfOhIBp9oHWjSp0k08q8emioJF+fx/rfgf8V9uDgPTqi8Olu8+E3NgdlJW7Ii2Bt7YmLzW2N5dt7Q2vujdFTv/duafK7i2hJ2K0+RpdtUG6pBBHiaOCknoyuKV6vwTeFk9huO23La9w5guIt8k3G6v54riz2m8lhhjs4YwkU62hCGUwmpmcuGrJRNQLaulwktZ0sopbVbeKFHSW5iRnaVj3J4g7VDVAUUOAS1CAFAV3cqhkRY5Cis6K/kVHIGpBJpXWqnjVpFxzb2JGoCwU1WuDw/l5dFmcVFD5jp/wBwYfa9BtzYmVwm+Itybh3Hj9xVO99ortfMYaXrHIYzNLQbfxc24K+Z8XvVt14cnICfHqkdCF8M2qQg+yfb7zdrndeYbO/5fNrtdtJCu3331EcovkeLXM4hQCS1+nk/T0yEmSutaAdLLiG1S12+WC/8W5kRzPCI2TwCrAIpc9sviL3VWgXgc9IKSRQ7xFlMiIjsgYF1RyyxuV+qo5RgD9DY2+ns5INK6aLwB9fUfz6RfLz6Xv8AdndW7OsavMbY6WmbAdHMMr3J3Ztil3Nli2O7g3DS4zqum7XqZ6+s2ptKjx+VxdTi9umkgpJq56mZaryyIpUPpcW1jv8AMt5zQzy7mBHt21T+GqxtZo31ZtaIssplDrJPrZgulfDoCeljq0tnEibeFMFWmuEJJcSmsXiCpVdIUhNNCRXVnoGqm7k6mZ9Kql5Hd9MagLHGhYsVijHpVR6UHAAHs9AC5QAVJJoKZPEn1J8z59Jal8MSTSgr6fKvkPIeXUB8ll4MZW4GLL5eLA5GvoMtkcDDlK+HAZPL4qCrpcTl8lg46hcVX5jD02RqYqSqmieopoqmVInVZHDeJ8/9X/FdeWgI1elAepOza7Y+G3EK7sfZmY39tX+Cbko/7tYHd8uxcj/eDIYSso9rZ3+8cGNyrrRbbz8sFbUUfhtXwxNCXTVf2R8w2e/322fT8sb7Btu7ePC/1VxbC6TwUlVp4vBLxjVNEGRX1fpkhqGnSyyltLa4D39m1xaaWHho5jOoghW1Cp7Tkjgf5Fj27uOm23gd94XIbJ2Vu+s3ttah23Rbm3LRZJ891vW0edxmbn3h1w9BkqKjxe6MjDj2x8slVFVw/YVMiiMPZvbm67TLuW4bBfQb3fWcNhdPcva2roIrxWieIW94GRmkgQvrAUqdag16rBP9NDdxm2ikMyBBI4q0ZBrqj/hY+vpjhUFFVFPHNHJHJGk0MqMskciK8csbCzpIjAqyEfUEWPs3H8+kxUEagOuAjQKoRVCqqqEAAChQAAB+FAFgBwB791s0bIGehD6o6h3j352Ft3qHrqHAS723mczBhIt0b02v13gZP4Lt/KbkyX8R3rvTKYXbWEZMRhagwGpqUNRUeOCINLIiEs3re7DlrbLrfN0aQWFvpMnhRvM3c6otI4wzt3MK0GBVjgHq8MD3Ui20Y/WaoGaVxU58sDpPb83vk+yt05jfuao9p4vJbqkpshX4vY208HsPa+NkpKCmxEcOM2dtyix+C28rU2NSWWKmjCSyu05JeVj7rsezW/L212mx2c13La2wKJLfTyXMzhmL1eeVmkly5ALGoAC8FHT15eSX9zLdzrEry0ZlgRY0UgBcIoCrgVIHGtfPpHulQokRUKVCLIEjqYniKTL6Qk8ThJIisgswIDLz+fZuhRihJqhplacPl5cOkTBlqAO759L/ALAi61G7K1uoZOwJev8A+G7e/hz9oxbch3s2bGBx/wDe8V0e0i2CGJTdJqxjSlpmoBEZv3dRJJyz/Wk7Nb/10TbRzH4s3ijaTMbXw/Ff6fQbj9bxPA0eLXt8TVp7adLty/dn1b/uc3B2/Smk3QQSatI8Soj7dOuunz00rnp1652NkOzdw0PWe2Nr7r3l2V2FX4LZ/VO3dp1eKp5srvbOZqjpFxuSp8nAXr4cli3mhpEp6ijaKueOWWUwI6Mt3S/k2mKLdpLy3h2i11z7g86SM3hLG2kxaD2sJdJbUrgpVVUMQQkijinE0DRyNcSAJAIyoGrUNWvUKkaK0oVoaEmgPSj7R3TvLeG/ctX9g4XBbc3lgabD9e53Bbd2jhtjUGKqutMbT7H+xrNu4Gnp8dHuGlGDMeSqbNLW1qyTSMzMSUXKWybTy/sVvYbFd3E+1yyy30Ut1PJcu31cjXBIllJYxkydi8FWg8ur7ld3F9ePPdxolyAImWNQijwxoppGKimf2CgAATFOv0Yf4A/X+vH+H49iQilR0i9D0u9r7X3Jvauh25sraG5t4bo+03DnGxu1MXk9yZWbAbcwc+4s5XR7fw+Nq6+PH7UwOGrslka3U8MNCjyyrDFTvI7dCrlmkHh0AAIpnNTqrnVUACgpTia48CP4c8a/7Hy/y8MZThu8QnS7U0rBY6hPVBIzRhwI5VPjcmM3FjyOfdwyhtBP6gFSvnSvpxHW6HTqA7DwPl+3p727sjd29I90y7S2/XZ+LZG08nv7d70P26jb2zMLPR02W3HXfc1EAOPoZ8jAriPyTEyCyHmyW83Pb9sawW/uliN1cLaW4avfM4JSMUBozBTxoMcerJDLMJTDGWEaGR6U7VHFj8h+3pL08kcVRTTSQJVRRTwTy0spdIayKORJJaWZ4isqQ1SKUZkIcKxIINva2RWeOWNZCjlSA60JUkEBgCCCVORUUqM9NKyq6uy6lBBKngaZpjyIx1Mm8k5rcnT456ag+8k0xUyzzUVA1U8s1LjI6qcuxKRDRH5XMjqlySb+6RMsYgtZLkPc+GMsVDvpADOVFOJyaCgJ8urtUiSZYiItXlXStchan+Vc9Lre+GxmyM9uzr7H7i667OiwW6lSj7b69m3PWbf3JSUNBJTuNm124sftmuqNoZOarEzGtxFPWGpplsUQFXb8CRruK9+qmWMQtEbXt8MksrCRhp1+KoUqtGC6WNVJoRtZV8BoRChYyB/GzqoFI0DOnQa1OK1HEZBHnpnAdPZrsj4zbl2Tna/aG9tn9ofHvGdhbM37mpM3lO1d9Z/uCWPL7m6agwG2IMdgNj7T25S49q6lzNatYJJT4vJyTG/Nm5cyWlpzHtW4bS1ztV5Y7jJBfWiqsVlFDagxx3pkkDtNO7MsZjVhVSSQMKe7Rb2cs1jcx3Sx3UU9uGhkJLSs0gDNFQEBUGTWmPnx+pHW/rf/AF/+jffMY8T/AKXqZovL7etWn/hU9AZ/h18egBfR8o8Y5/wA6p7QF/8AefeSP3Wv+V93oef7ok/7SLXoLc9/8kWD/nqT/q3L1pK0dKDAqkfUWsB/yIe8+AMAdRF0dX+Xp85N5fy9Pkhhe1sYa/L9Z7nai2p3ZsWllj07s2PPV62rMbT1M0FH/fDaU0jV2IlaSEtMslK8qU1VU6oz90/bmz9yOWp9rKIm8QhprC4av6ctPhYgFhFKKK4ocUcKWRaCHlrmCTl7cUuCSbN6JPGPxL5EVxqXiOHmKgMevov7G7B2Z2xsfanZfXe4cfuvY2+cFjdzbW3Fi5Geiy2Gy1PFVUdVGJFjngkMcmmSGVEmglVo5ESRWUcu932692i5vdr3K3aG/t5GhmibirqSGBpUGhHEEg8QSOsj7aaK5iS4gcNC6h0YcCDkH8x0Q/8Ams0lTW/y7vl9TUlPUVU8nSu7GWClhknnZIo4JpXWKJXkZYoY2diB6VUn6D2IfaWaGD3Q5GknmVI/3lANTkKKswUCpoKliAPUkDpPzGjPy7viqhZvpZDQZOEJ8utBD4m1mNr/AJLfC2gotrYbC123+/Oo6fMbixtXmajI76qK/uXBZWiyufgyGQqsVQ1OEx86Y+nXHxU0MlNCryK0pLnpLz/Z3VvyT7pXM+6TTQT7RdNDbSKgS2CWToyRFVDsJGBdtZYhjQUGOseeXZY337ldEt1VkvIQ8ikkyVmUgsDgaRgU4jj19Jaf6t/vv7XvjTPwb/V5dZgLx/1evWtL/wAKS4TN8f8A44AXOjujKt/642XF/p+L+8wfuW/8rlzn/wBK5P8Aq8nUV+8n/JB2n/nq/wCsb9aoNJsbcb7UPYNRs7c9d13R7po9mV+7qfGZKl2l/e6qxc+4KfZMm8hjK3CY7dlft6jmrYaNjJVtRxPOsLRoT76LOGKOsbhZCDpJFaeh01FQD5VH29Y6Kw1UpU+Y4flXPVq/8vH+bpvf4f42h6c7pxec7Q6Bp5JBgZsZLFLv3rETOGkp9tJlKymx+c2k0pZziZ6inaleQvTTqoNPLiX79fdf2n3Pnn5n5WuItu50IAlMgP011QUHjaFLxzDFJVVqgaXRsMsvcg+6N1ywke17vG9zso+Ar/aRfJNRAZP6JIpWoONJ2lekflv8cfk5habMdJdt7R3rJJAJ6rb0GQGM3piBqkVkzmysutBunEENC+lp6RI5VXXGzoQx5ic+e1nuB7eXE9vzdyvdWsQOlbnTrt34U0XEeqFuIwG1DgwBx1lLsPNGwcxRLLs+6RTGlTGDSRf9NG1HXgeIzxFR0ZXZX/Hy0/8Aywrv/cf2DLL/AJJnNP8AzwJ/2mWvQhvP7KL/AE/+RuhXymQoMVRVWSyldR43HUUb1FZX19TDR0VJBGCXnqaqoeOCCFB9Wdgo/r7DVpa3V9PBaWVtJNdyELHFEpd2J4BVUEsT6AdImdUUu7AIFqScAfn1TD8wP53HxM+NtDlMD1fnqH5IduxJLTUO2eu8lHV7FxFcwlWOp3Z2VTxVe3lpaaaBllpcU+SyAlCpJFAr+ZMrPa/7m3uXz/d2t9zXavsHKxCmSW7Wl3IoJqsNqSHRjw1TeGoB1KJKaTG3Mvu9yzy7HJFt8y3+58FjgasYPq8oqtBTgupq4IHEafXyU+R/dfzD7Yyncfem45M1uPIwLR4PFU8U2P2vs3bCTTPj9ubOxDPJHjsDRu7kOGlmqZzJNUSzVDyyN1a9ufbflD2r5XtOUeTNtW32qEl5GrqlmmIGuaeTjJM9BWtAqhUVVRVUYr8x8y7vzRuUm67xcl7phRAMJGnkiL5KK/MniSSSetp3/hM1jt2ZHbvyv3/mMbs6k2zLB8c+ntr1W1aTbGEqsm/TeK7aOTyG4cDg1gy1blqmh35j5Jc/kYEmz0kkjCSR6eXTyz/vNoLCxuPaHb7Se6a6kk3rcp1uZJJNBu22whI2kJEcatEwWJDpipQcep69iJJpouapJFjCItpAhjUKGEf1GTSmpiDXUctxPW2FjZAFIvb0XJNyCSCb/j/e/fI2/B/VOfyx+EY/l1MV6lTw8/Lr5qX80OhDfzLvmdULGokqe8dxGWUIqvLoSk8QkcAM/jDELf6XNrc+/qL+7Lj7u3sb8uU9rp/2RQ9YS84L/wAirmIAYF5L/wAfboAtr7hocFtjf236nY2zNz1e+cBiMLjd17jpcnU7m6wnxmfo87Ubj64qaLIUdDj8/nKWkONrJKyGriagldVQOA3uWtw2ie/3Pl3c49/vrWLb55J5bO2ZFgvhJCYhFeKyMzxRE+IgRkIcAk06I4roRQX1sLOGRpkVRLIKvDRqlojwVm4MfQAcKg2BfykajaMXzl6Exk+1MvNv6TdfaWTo99LuloMHQ7Ij+N/alFW7Ql2SuPZKzMVefkSuXKtUqY6dDB4yCG94mffstt7b7u/uVepvEI5bW122J9vNuDK10d925kuRc66rGsVYzFpoW7616l72HezT3J5XgNoxvzNcuJw/aIhY3AMfh0oWL92uvDHDrb53A5apf+lyRf8Aoym/+9++Fm1oFgAHpnroBP5+uetW7+eRSGbvro+TSCv+irJxtcXFhu7INbng31fT32d/u7v+nU85gcf6xP8A9odn1hV95Yf8ijYDT/iAf+r0nVcvT+3Nz5XLV+7sV1XX9z7e6ixcPana+1p4Nw1W2V6z29kaKnzlV2RlduVdJuDA7Fq5KmGjrK6mqYJ4UmHjddJIzo3qW1j287Z+/Btl3fVsrG6j8MSJcSA6DbpIDG8ynuVWBUnjkjrHe31mU3D25nSMeJIjE0KLx1HJC04n08iAelN0dCW+T3RMzUkGNV+/+rqyPHU8jTUuMp6zsXBVlJjKSeWaeWWkoaWpSGJpJHlMaDyMZNXsK+5o/wCYT+4AWZpSOXr9DKwo0hWzlVnYAAAswJNABU9opToR8mgjnnlUsgSu7WraAahQbhCADmoAI8yfXNetymh/3X/in/EX9/PQ/A/aeunp4H8v8I6qP/nZU5n6I6bsP0dyX4/AOytzj/Ye89/7vI/8jj3FH/SKg/6v9Yy/eYzy5y//AM97f9Wm6o668x9OwxVfR4LIb8z+E3HS5zI9aLtfO5bB5/rzbdLDntxV+4czt6dslRYKeSkegysMcEf2uNlerNXFYKOpm5NcPHd2ZvBY2c9o8Me5LLGssN1KTFEIopBpaRA3ixsSQZFCaDk9YgWxiTwpinjTrMrNbFGKPEtGYsymoViNDClQpLaup+eylFnM9nc5jNv4baOMzWZyeXxu0tuS1k+3dqY/I1k1XR7a2/Pkp6rJTYTB08q01K1RLJM0Malmv9FG3Wk9ht232F1uM15dQQRwy3lyFE1w6KFaeUIAgllILPpAGomnVZ5Unnnnit0hid2dYY66IwxJCJXOlRgVzQdMjt9ebj8D6e1woPt6ZPUnVitP+dyWv+E67fa0mj+P+S32ur73V/AvBz9xb7nyenwafV7apcV+COniU4t8FOPD+0r+H4afir1bs9Wrp+Xxf5v5/LqNIb8D/H6/T/H/AB9u0ApXqp4dQZb8Xsfr9f8AC31PPvbeQ8uveRA6EGV+1MP8f8jkk3LX0nx83R2//DM3tKk3nhJMdmu4dibKo9w0mezHV1Llpt4vU4LZmdRaLOy4xcXKztSw1MlVC0MSdrCxk3CDc2s4zuaRGGO4I71iY9yBv4WY1I+Z8ia+MzKjxeIfCrrZBkVAwxHGtAP2D0HXLsDpLeXWC79p995brjBbo643jsrZWf68g7O2Zubf2Sq99bWr94Y7cmzMXs3Kbjw289h4HE0cUecy9BkJafD19fSUs488xSN+lQDnOQaY8+PofT16YrqJA6B95KL+H+H7OX+J/fmb+JfeSeAY37YIKA47x+Lz/dgyefVq0+i1ufbIW4+r8Xx1Fl4WnwtAr4mqvieJWtNONNOOa9Ki9r9GYvpm+tEurxtZp4emnh6KUrq7tVa0xTz6FvBUu9ey+ltx7Nwm3+naPbHxzXdXfW6d41se2dodw7gw+86vb2z6jbZ3Vk8jDmO1cThMgIJMVtuigaooTLJLqk/ZT2TXL2G1b/bbhcXV813unh7dDbqWktkaPU4cRhaQuw+OQkgip0gayNqJZ7VokjTRBqmZjhyD5VqdQHkKA8MntHQCpkMnSUWSxtHlctQY3NiiTOYqgymQosVnkxlSa3Fpn8ZS1MVBnY8VXMZ6QVccwpZyZItDnV7PJIYJJYZpIEaWKpidlUtGWFG0MRVCww1CNQwajpKGYAgOwB4gEgGnCoGDQ8K8DkdJ+ZVIP4PJv/Q/635B/wB5934Z8utUqBmh6dNp7Lye/MxXYPE5LaGJqaDa27t3zVe9t34PY+Hkxuydv125crjqHNbiqaTH126snQY+SHEYqNzWZfINHS06NLIo96pTz62SD2+deg+a0iBtLrdVYB0Mb6SARqjYBldPyDyPeqdXBr2N02zw8fTUQDpJ/I4Gn/ffT3759bHb2sMeXT1tzbuFzVBvWqzG+cBs2r2xtGXcW2sRm8XubI1nZ24I83hcUnXe1ajb+KyVBhdyz43KVOUWrzMtDihS42eNqgVEkEcnqV6qS0ZBC1WvSOZURygKlwofSpAIjZmCufzpZlIBP5Hu1MZH59bIoSV4cf8AV8uolTTQ1EbRTRxTwSEa4ZkWRG0sHGtHBVrOoI/xHvyMUIIPd15lVl10BHmOhD6w2rjt4bxjosn2lszps4XA7j3tjN879/jP8D/vFsXEz7n23tij/geLy1X/AHq3ZmMbDR4kSQmnNa6CW4IRyreLp7OxZ49pmvVkdYHt4KatEp0OxqR2Kp7j5DJKirByJRNIKzLG4GoM3Co4fn6f5cAxt+dn767i7E3R3B2vmajenZHYO4TvDfOezdFjKKo3HnqgU33b5THYCjxGHpY54KVIHho6emhWNbIq/X3bbtmsNm2q32LZ4zb7dBEYYBGzMUXPcrOXZmBOqrFiTxr1sXLyXAurlFkk1iRlcdrUp2sFoNJAoQKY4ddbMxe2N1dgbWwu893Y7qbZW5t44jHbs36+2tw7uw/WO2MvloIMzuxtm7ZWr3ZujGbRx0z1P8Nx6y5Crih8UIaRgPZlBGY4YYzK7sihS7nuegA1MQKam4k0Ar0zcyeJLPMsKxhmLCOMHStSTpUEk6V4DJNPPpVVGxqHE0nXebxXbHXdad7bp3NiAmJzW5cfujqqk2tufE4TE767Vx8m3qWq2Lgt20WR/jmIkoqjJVq4yjqZJY4poVjkeKrIro6BkIoVYVDAjK0OGHkR59JC5rXgwzUGlPn8vXpp3HhaPb27937ZoN27W39T7W3Vn9tpvnY+QyOW2ZvIYXJ1VAu6tqZPMY3C5nI7b3EsArKGetoqOrmppkeWCN2KBzS0egFKVAIHCg+Q4fLH2daBDVIavqeOesVP9Pz9LW/23+HHvxIqcefW+lHiMzmMBWDI4HM5fA5H7TIUAyOCylfhsiKHLUNRi8rQjIY2opaxaLK4usmpqqIP46immeKQNG7KdHjmn59bFPOv5Y6eMvncJW7O2Vtmg2NgNv5na8u55tw77xuQz8ud7GXOZCnqsHDubFV2QqNt4pNj0MT0VAcbTUzSwSsZ9bAeyey26/tt837dbjf57mwuxAtrt8iRCKy8JCspgkRRNJ9U5DyeIzUYALQdLJriB7KwtU2+OOeIyGS4VnLz62qgkUnQvhDtXSBUHPSKdiLFHZdV4zodl8iMR+0+kgSRsV5U3ViBwbD2eAV4rwznyPr8j0jOP9X8uuCxyTSpBTpJPK5ISONGeRjp1HSig3IVSTxwB707pGjSSMFQcSxoB+fXlieV1jjQtIcAKKk49OPDqekdauK+5+5UY2oyS0rUaVo8kuQp6ZZY6iXFhw5jSKo0x1DLbUxQG/tnxbY3vgtGfqkh1iQoaBGYggSUpUlalQa0oT074E/0S3Otfpmm8LQHGrWFDVMfGlDQNSlcDPS+OO2nSdYDIT7knfsut3z/AAhOvazZtTGuG65pdv0Oco+w8Zvxs1HTtNuPctdNi5cT/DWYw033AqdJ8at6FmvYZ4p5AiK2sRkeHIzdumQZJaMCooRSua16slw0dtc2sltEzOy6XcHxIwp1VjNRRZCaNUGoGKUPQcVELSxtH/ZYgspH1YXC8kXBFz+R7VlQSG8x0nBxQHHTJQYHCHN4mbcOPyOS2/FlcfLuDHYetp8Xl8hg46yF8vQ4jKVVHkKXG5Wsxyyx008sE0cEzK7I6qQUt9HdvZ3i7fNHHuJicQSTKXjSQqRG0iKysyK9CwBBIBAIPTkXhCWIzozQBhrVDRite4KSCAxFaEjB6W9BP1/iV7UoKDrUZSg3ci0vWOV3Ruevn3V1HSUm7YczQ5IT4OnxOE3juGp2vD/Ca81NNDRymSSeONSVQETbTzBcy8o3U3MpgmsiX3SC1gQQ37NbmNk/VLyW8SzHxU0szCgUnz6WC5so03SJNu1JNQWzyOdcAD1BwKOxTtbgCc8Kjp4682fg9x7u2jg9675xfUWzdy5X+H5TtTdO3d3bi2xtPHwrJ97mqvC7Jw2b3TuCmoZlSKWDGUtTUpJKpKWB9iITwvLNDHIrzx6S8asNS6srqGSuoAkVGQMdInhnSKKdomWCTUEkYEK2nDaTgNpNAaHBOemDbu7t17LrMzkto5WXA1+4dpbr2HmpkpcZXtXbO3vip8FurCSJkqOuggizOIqGjMsSxVcIN4pInF/ZdvOxbTvsNjBu9kJ4ba7hv4AWddFxbuJIZOxlJKOK0NVPBlI6etLy6snlktZijyRPA5oprHINLr3AgBh5ihHkR0EsuG+wqKbIUj/Zz4yenr6SqXQWo6mhlSppalfKJEvTzQq41AqdPqBFx7WzwR3kU9vPGHhlRo5ENe5XBVlxQ5BoaUPp0yrNA6SI2lkIZT6FTUHPoc56EvcHVneXT+RfP712d2/1FlN3Sblw02W3JtreHW1buU5TGYzJ7ywQnrqHBvkIMhhN2UU+RokBjko8lAzx+KaO4csrrknmGJNp2+72rc4bEQTC2jkguhb6Cy20pXVJoZWiYRSHOpGoag9L5U3myJvJkurdpzIplKvF4lQDKtaLUEMNSjFCMUp0iWwE6Y+KtFDPHjZKiTH09b4GSgesp4lmmooZggiaohgYM0am4Q39iMXEDXD231CG7CCVo9QLhGJAcrxClgQD5npGba4W3S6Nu4s2cxLLpOguoBKBuBYKQSONOkpWYBXZv1Wcr5EUlUkKMWjMsYYJKYmN01A6Cbix93IBoSoqOBIyPWh8q+fr01T06d9lx4fbO69tZ7ObSxO+8Hg8/istmNj5ysyuOwe8MZQVsNRXbZzGRwVVQ5uhxmZgjME0tJNFUIjkowb2XbxZXm5bRum37fu0thfz28kUF/AqPJbuykLPGkoaNnjbuAcFSRnp23ljhuIJpoFliVwzxMaBwOKkjgD/AKq8OnbJZmuqocviqGWtwW0Mpuar3XBsPH5nNVG0MTkZRV0+NlpsXXV08VbkMDhKs42myNSsmQNEvjaUqxX2ptIpbezs7e4u3uLiKJI5LiQKHlZVAaVwgVFaRgWYKAoJIAp1V2R55ZY4RGrOWCKSQoJJCgkkkKDQE5oOkRWUCSAgi/B/H+F7H/W9vkA8et8CBTPSYmweiRaqJ2glhYTxTRs0ckLwnyLOkikNG0RW4IIKkX9slKgqRWuKevy/Pq4NKMDQjNejQ7Z7F+RtPU9KYLbnzr3FtvEdrJQRVdVB8h+5cRtboKOq3rkdlMnd32EbRbMioqTGrnak4eDMoMDPDPd59dMgSufbrkSe5lurvkbaHvJMPJJZW5ds17mMWps+pPRzHzXzGkXhRcw3ywKMKs8oUfYA9OkD21kN17ywG0slvb5Mbq723XV7i35Rbl2juDJdm7ij2DTbUrMVhtn7rpt575kbAbxoO0sbVVdTjji7VGOo6HRWrG08Kk42zYdl2OMw7Ls9raQkfBaxRxDjX4Y1UcTX7ekV1uu6biQdwv556ZBmkZ/l+ImmOg1gw9MtPQRfw+hpZKOnmiepp45UqcmZZ2lWqyZeV45J6dT4o9CxgRixF+fa6OAxTXMhuZHWRgwRyCsdFppjoAQG4mpOTx6rLMHhtY/p40aNSNag6pKmuqSpILDgKAY8ujI7mr9ydndQ7R3h2B3ftjOZLpJdp/Hfq3pHJUc1N2Pjunko9xbwpdybelxe3aLA1/XW089Wz0E82QrajMfd1SIWMSwqxHYW1ptG9X1jtuwTRxX/AIm53d8DWA3JKxsjanZlldQG0qFSmQCSxHnZ5oI5ZrhSY6RJHQatAGDgCqitKmpxQngCBE2EgqpWmMMQlMQiaXQvkMKtqWIyWLGNWNwpNr+xHU6aVxWtOkpGpqgAeXUI7dgRixVFjFtUjlVAFxyWNgBc297CkkACpPADrRNRpBoo6GDaOy8BU7X3zmshvzbm2M3tOh25VbY2TlMXuqsz3atTm9xQYbM4vaGRwuEyG28JV7KxMrZivfOVeOgqKKMxUjzVRWE7UcCRgn9n/F9aZiCUUZ6kU8fiQfktyBzbj+o/A592rqrnHXvgWg+I9YaqhEytqAJPJNrgk3sOOP8AinvRqxoBgdbppUsfiPWePqqurdlZbsNa7aiYbD7wwmyqrDVG6sHT76qcpuDDZbOUeTxGwpakbmy+zaOkwssVdmYIHoKGtlgppZFlnjU6NMBeqgZJbj/g+zqPisClMQRH9Ofpz9eTb6X9+pQHq3zPDoTcRW5PGU9fT4/KZbG0+Zx7YjNU+MyddjoM9h5J6epmw2cgoamnizOEnqKaKR6OqWWmkkiRmQsqkUeCCVomlgR3jbxIi6hij0IDoSDpcAkBloRXB49WDMAQHIBFGAJFR6EDiPkajoZenMNvPDVm4++dqYHqTdeO+OKba3lurancEm2s1t7cNFvLKVeyMPQp1Xm8njsn2rCMnXtJVUePvLj9ENU7KREHJN/k2+6S05bvbm8hm3QvDBNZaldDCFlY+OFZYMAAFgQ41LSmohTapKpe7iWMrDRmWTIIbUo7agtn0IoaGtaVL0u3cbNkZKzJY41dLNNXVE1FRTfwtFmqvPLClI8Mb/aUdJUyrohVdIhQRiy8+zS4juGt/DtLkRXAChZHXxMKRq1AkamZQRWvE6uvWzW63Ae8tzLB3VjVimSDSjAGgVqGnmBTpZ9c9XtunJZHGx7j2NtaTEbR3bvCTI7+3NSbPw+TTZ2Cqs7NtjCZCsiniyW+90pSmjwOIS0uWyUkdNGys4PtQaZIBp6DJ/4r1PSc4C6vix0Z/rfrb5DbJ7M2ds3rfKPsfszuHqFs1t6ownbHXe2Y890/2hsXJ7oyGJz+9pt40209sUu6tlYeoGQwuYyFBlIpESlnpoq14YmS3m32O5QpDuFnHPAkqyqkq6gJE+FgP4lrj7TxBPTqSvEWeOQq9KEr6HiK04Gn+o9F3ppYJqWmkpAq0jwQvTKkTwIKdo1MIWGRI5IQIyLKyqV+hAPHtaxbU+o91TWua9aXTpUr8NMdc3P+2/w/P+H+t70tBU8T1snBp1G1n+g+v9f+N/8AGvfu758evUPUwkD/AA/1/dSanr1f29QaixJF7AgWIP8AtyPrb3seVR1oVoP8HQz9gb33DvXpPqEn499Ode7I2VuTce0cT351h1PLs/dPcm7KfbG2xmNqdn9lnLZKn7C3Bt2hoYsu9OkdOYKvIS1BUayoB2zWe1bVzXzJYLzvuF7zBcQJfzbPuF4J/oreSaTw5ba20I1vbs5MSElhpQLU8el91LLc2VlcfuqCG0jP04uIItHiuq5Ej1IeSgLNwqammCOi6+OGnRI4YooYowRHHDGkaIHYs4RECqoZiSQByefYxqWr69FgpkAY6U+0tqRby3Dsfbh3jtDaTb33vh9lSZndVVkoMTsqLMZHH41d6byOMxuQrafZ2PNf5p5KSOqqjHBIEhLAAlt9uf7vi3WZ9uuJYrS0N2TGFpNpDsYYizAGYBchtKioNela2niQ2sq3cRllnMPg1PiJwpIy0poYmi0JJIIoOkxu/AU23N2bn21/F8Fuxdm7t3Lt6l3Tt4Vs23dxPtvMV+DXdO1JMxRY7Krg8+lEaqhepp6aqNLOnljjcsgV2N4b6wsb5YZIVuLeObwpCutBKivok0MyFk1UOklag0JGek8sZjlkhajNG7JqHDtJFRUVoaYwDTiK9KTemwsHtSr2XTQdv9ab5g3f1XgOyq/I7Cl3HlabrzPZ2LJSzdLb7TIYXFT0nae22x6JkkpFqsdCauIrUN6h7Lbfdru6i3GReXb2KSC+azWOfw0M8alP8chOog2zBiVrRzpYAefSmG1t3mjjm3KKNGhMviUZwGoSIWC5EjEU9BUV6DinoXqaOvyy47O5HE4egoajKV+NxdS+IweUydZDS4Wi3blBT1NFjcLlK9ZKRHaWmmrpmCUr6wQV8lxGksFo1xDHdzO6wo7r4kqIpaR4EqGd0XvIAYRjLimek6xkqZlR3RQpchTpVmNAshyACe0Go1H4emvOTUeXyeTyNNhsXgaSuyVTkKXAYlauTD4SKapaopsXiv4nVZDIfw/FgiOAzzzzhEBaRmuxtaQyW1rb2811JPJHGqNPLp8SQgULvoVV1ucnSqipNABjr1xIs0ssyRLGrMSsaV0qCa6RUlqDgKknHTHLGG5NwQfrfkH/AB5H4/2/t/z6bHcvz6bZY7ahYccc/wC9j82PvVKAdXBDDSePTe8VyQRz9Re/I5PBFrH37r1fwt0vdh7X312llMJ1FsPZku/tx5ep3RlNp7awlDjaPcs2dG3Fr8plTnwcfXZHF7f29tiWrGOr6wYpNEriMSyt5A9v247Hyxa3vNu+7uLHb4VhhubiZ3MQjMumNPC7lV5JZgutE8Q1UElVFF9jbbhuMkW02FmZ5SXkSONRrroq5L4OhVStGbSMnicpYbSysOzaXsGv29vSk2Tn67L7W2ZvY7cqRsXdPYe3YMRltybNot1zw0+Klrtv7cz1FWVtLTyT5CjSrgeaJIpoyTuUXqywLHFEY/FpMWLBli08VFCHl10BFQunNa9JoTY6LhpZpRJ4VYVQKQ0modrkkFY9NSCATqFKU6cN94PrfCQ9fSdcdg57f0+c6123uDsuDObEn2MvXfa2QmyK7r6zwM02Yy6b825tmGnpnptwxiljyAqWAgQxkBFtlzutx+8huu2R2oju5IrUxzCXx7ddPh3DUVfCeSprEalacTx6bmSFRE8EpaqAvUadL+aj1APA+f8AIK2n6pw1R8c8p3pJnd7QZ3G974Pp/wDu1F1hkqnribCZbYdVvKo3JUdyLllxNDvqjqqbwRbWeiNTVUP+VpNpJVCt+Zo4+dYeSx9Gbp9ofdVU3Ki60pceB/uJp1/T6iAZwdIYlSMZVLt8sm2HdvDkFqLkWrSBCUDFA/x8Nemp0YJAGc4CupgolrqmDH1kmQooaiRKDIT0j4+auplA8c82Pkkmkonk/MZdiv8AX2JrV7iS3hluoFiumUGWJWDhG8wHAAYD1oK9JLlIBczw2lw01srERTMpQuvkShJKk+lTTp1wlPWz5fDU2MaNMtPm8NBh3nmpqaFMzLk6WPESTVNcy0FNCuSeIvJUH7dF5k9Ab3u8lgt7K9uLvV9HHBJJNpDMfDVGMlFQF2OgGgUajwXNOk0aySzRRR/2rSKqVIHcWAWpNAM0yceuOjK/K3tL5G9ud4btzHym3VQ707f2dkcn11uHOYbGdc0WCiq8Dla2vr8Vish1NhsPsPcFPT5DLSSrWUgnLxTRgSePxqAV7abTyJtfKdhde3dhJb8t7mqbpEk5uvEbxY0RZHjvGa4hJSNRoIUAqTprU9Gm/XW8XG4PDvs2u/tQbY0CAKFYsVBjVVbuYmuTmh4U6AKJQ1rfX+vHPHFz+fcgA8a/s/PomHl0J3V2wouyN4Um1aneOzdg0T4ncWcyO6d+Z+l23gqTGbXwtVna+jpK+sjkgrN0ZOnozBi6CwaurHWIEE+wxzfzFJytsVxvEGx325XQlit4bPboWmlaSeQRozKtCkCM1ZZPwJVqHh0cbFttvu26W1hebjFaWjBnmuJmACIgLNprhpCMKuNR6Q8SUj5GliTImlx8uUghXM1dHUKaPGPXpEmcqsbCs1YTS0f+VSU0YeaymNQXt7Py030xeS3BuBFVoVYEF9NTGHNBTVVQxx+Lh0XyLGkzrDNqgEhCSMpBKhqLIVORVe7TxHDj0+9h4nA7Y35vbb+zd/43tPa2LzuWxOB7MxGBy+3MV2BhBKBDuXH7d3NBDncDTZbkrBUqtRHa9wCPabaJrm82vbrncNqexvGjV5LN3WRoGH4C8fa5UeYx5EdauAqzTJHcCRAxAkAprBHGhrSp/wBjHSBWUxyKyyMkmqyMjtG+oryEZSrXK3vb8ezQqrKVZar5g5HTIZlYMrEN5EYP7R0MXW/c24Ons11pvfrLD7c2z2x1dvfL73wfaM+Oj3Rlcg+Qx+Ox+I2/mtpbtXNbBrsJtVqWqmpb40zTSZCXztIEiCBvduWYN/8A33Z73fT3HL19aR2r7bURxoUd2eVJYglwJJtShgX0gRjSBU1WQ3xtUs2toES/hleQXOSzBgAEKmqaUzSgqSxr5dBtNV1NbPJU1k81VUSs7vNM2pvW7ysqiwWKIO50xoFjQGygAAexHHFHCixxIFjGAB+z8z8zk+fSEuxJZ2qfM/n/AKv8nXan8W/1/wA/76449369TNepAKabBbH/AHv/AIr71+eOt9Y7KbkAEEkXFrXH1H55H+8e9kUOePXq1yOuNRWSSrT46SrldKdKiakopKmR4qZKh9VVLS0zOY4FnkjvIyKNbC7XI9tJbxJJNcJColfSJHVQC2kUUMwy2kHFeANB0488rpDbvMxiTUY4yxKrqNWKrWi6jk0AqePUSRQotcfkknn+gvb/AGHu9OqdQJY45UYOiOjoQysuoOjAgqwPBVh9fdfhPnUHrXxDPAjz6VG9ewuw+yMl/GOxuwN99h5dmjb+J773juPeGQEkOMxeFilSq3FkslNHImFwdFR6lKt9tRwRk6IkCle3bLsm0LImz7PaWaMAG+lhjiqAzsAfDVagO7MAeBZiMk9KJrq6uNP1N1LJQkjxHZgKgAkaiaEgAH7B6dI56nxxw0b1LiJppZoKR538JqBGBPNBSs+jz+EAO6rrKixNvZj4Sa2lES+KVCF6DUVrUAtxIrwFaefTfiPoWEyt4YYuE1HTqpQsF4aiBk8adQJFvc6Qf9vyT/rEWv72DU5PHqleHS033tTZW2sZ1tV7Q7RxHZGR3f17Q7q35hsVtbce3JuoN61WXy1FVdWZit3BHHTbuy2MxlHTVkmTxoFA61YjXlNTFW3Xm43c27Jf7M9pHBdGG2d5Ek+piCqRcKEzErMSAjVYU41qA5IkaLbmOcOzIGcAEaGP4CT8RHqKD5UoTin6+pD1JF2pR732fNVU2+4th57rurzVNR9h0lRXYmqzWJ3Ng9sMr1me2QaOjeGtyaskVJWtHCVJb2UpzJc/10m5Qn5evVt22/8AeFtuiRs1m4WRYpIJZ8LDdBmBjiyXQFqinRvLtdmvL9tvMG7xPeG4a3ubJqLLHgtG8Y4yxsoOphQKaDJr0FrR6jyOASf9gP6D6fn2KeiitBx66p1n+8pHoopZK6CrpqihSnp2qpvu6WeOopWipljmNTIk8SsI9Dq9rFSCQWZ1iaGVJqCFlKvU0GlhpYE1FME5qCPI9XTUpRl+MEEUzkGvDzz0ZL5QdjfIvuSv6g7N+Se7MLvTJ7m6hoh1ZmMRT9WY6aLqzHbs3OlFQ5nA9WYzD02AysW5KnISGDL0seWaGVGa8PjtHvt5Ych7Jbcy8r8g2E9tabXuP0t/FMLwgXXgRN+nLeFjOnhFBrjZo6giuqvR1vM283UlpuW8yq811D40Tr4YqhY5KxgBDqrggH+dCyQwRizMo5PpBHJF734/A9yDx4nPROKDub8h0YDofqLbncvZGJ2FWbr3xiKet6/7G3jk67YvU2Y7T3Jjc1sTZO4N3UuApNnYjL4+tyuFyT4WKKvzKyx0+KppnqJU0RkgJc180nlHZb3e9ygs4rWO9t7SJ7u7S3icXEscKO0rrpjcvJpWM1ZiBSpNCaWu3R39xZ29nPLLO8LSzKkRqjrUmNRU+IAoB1igzSgOegWx5FWlA8rCmhqPs2qXhX737SCdovuZ4UV4PvmpYWZ0jDR+cqF1Lq1AYyK0XiKMuKgA4qRwBOdNTitDT0PRQrGbSOC4+dAeJ+f+XoeMj1jgNydv7g6o+NuR7N+RKZTcFNguiqnB9S5bE7+7hlamiq6zzdVUFZn9zYatihhrDBSU/wB1UzJS+VkjRyqEu23G93NltNxum1wWt1IGa/txN4vgcdAidV0SsTp1VoFqQCxGVjCwCXsa3MhkUKLVggCyNUa/F1EMiha6aAkkZAB6bcHt7d219q4ruvFbRnm2VJvyp2NtfsHN4/EZ/bKb0xm3zmsztHI4CuFdhstlajbGbpqoitomp4gqtTv5dQCS6vtl3Xcrjky83VRvP0K31xYQPJFKbdpfDSdJVKyIgmjZex9R4ONPF+OC9s7dd6trNzZCfwEuJFV0Emmuh1NULFGBFVpX4c9I6ngjiRAtyECoLszsdIFgXYsxIH1JPsSsxdjX7eH+qnRYB4YzXpyiF+Wtf/Y8D37NQFHWqU73H+x1NSLnWRwbaQf9h6jYWv8An/D3onBHXqEnUa/LqVHBEZBIYkLhCgk0jWEJDFQ1gRGzKDb8ke914A8et8SPQcOlcIxmMaTi9p1SVO09swzZau2xQZKupKrHU2Xqmy2+OxXf+JjEmJcrRUCVsP8AD8XCscSzL5HBYvUiyuP8a3VTHd3JWFLlkUq5jGi2tQNGv4Hk0HXIasVNBQKXJuEXwrQ6oYu8xBjUBiWll+IL8QXV2oMVyeuUdLQ/aVNVDl6eWaHKUdBT4+SjrKaoqqOphV6jNl9M8VJQY2oJjmjfVOwUuisLKXFnufHhgewYRtC0jShkKqwagiphmZ17gQNI4Eg9XMFv9NLOt8plWVY1hKMGZStTJX4VVD2kE6jxAp0t+ydjYfYPYe4tl4zsLrvuOi2hXw0eN7S6uqclktgbqFZiMfX1OQ2dkc5jcVlpKOllrXoJ2eCO9TSyhS8YV2b2ncJ9x2u3v5dsurF51Ja0uwFmTS7KBIqkgFgNa+elhUA1HVZYUjmdBKkukikiZU1AJ0n5VINMVrQkdKbIda0uK2l1Bux+yOua49u02+Kqo2zRVmfG4uqE2RuL+7ixdofc4ODE0k+7mVqzFjGVGQBpVIn8T6QyD9+a7rmKzj2e7eTbTACUEZ+oM6eIBbjXqrGKa9YXiCtRwWW9gZW28SXkMMdwXAkmLBIwhpVyAcE4FK5wadICNUAtpFw355/T9CL/AOIuPz7PKGgp59IKnBpjoVejm3FQdv8AXVZsfp/bHfG6KDdIzeH6T3bsV+xtodnV9DRV2Qq8FunYFNNSS7txT0kEtZUQCRGvTCUt+37D/NdztNty1vU+/wDMbbPs4hCz7os4t2tlZ1VZFnYERMXKoDQ11afPpXt9vc3V9a29hYfVXbMdFsE1+IQCSCgy1ACfyr5dI/eG7Yt9bq3Du+n2vsPZKZ3IiqfZ/WG3/wC6fX+3JYqOmo5sdtjbJrsk2Fo2em88sBnkP3M0jkjXYGO07W2y7bY7S+5X140KEfV7lL49zKGdnDSzaU8QjVpU6R2Ko8st3Nwl3cS3C20MIcg+FbrojWgAoiVOmtKnPxEnz6S8jWF73PH+uOf6c39mJNKg9M1Oeo2t/wCh/V/X/D/e7fn37H5cf9X59ex6/PoQ8J1/ndybE7L7Gx+U2TSYHqf+5P8AefF5zemEwm98x/f/ADtRt3BHr3ZNdKmb7B/h9dTtJlv4ej/wqjKzzehh7Lrnc7e03HaNqlhnNxe+L4Txxs0S+AgkfxpR2w6gaJX42wKdWWORo5pRp0pTUCaHuNBpFDqzx4U6aNubTfcM7tktx7a2LiW2/vTN43dG+quvxe3M7lNl4lsm+x8LX0GOyslVvTclQI6HGUzRJDLWzIks0KXcJty3lLAaLaxuL68E9vDLa2KrJNCly+hbiVGZNNvGKvI1SQoJCselUVhNJHHcTOkFlIspinnqscjRU1xowBrJUgAeuK9I3J5nN5Kikp6jL5KWGSsrczBjqurqXwtNnslEkVZm1wENRHiKfK1iRpHUTwRRzSxIIy+gAAyisrCC6+oSyiE/hrA8yqolaJCSsRlI8QxqSSqklQx1AV6QvNM0fh+M2ipcISSgYihbRXSG9SACRitOnvfT7EranG5brrEZTbG35MRg8Rkdt7p3nS7v3c28sXhaU7x3a7UmLxiYvZO6cxM0mHgYO1OI5YCxMfsm5fHMMEd5Zcz3kV3uQmlniu7S2a3tvppJG+mtxqd9d1BGtJjiupW8+lV6lmwiuLFfDhNI2heTXKHUVeQj8MT1AQ1yVbC/CINHlMVtTHdf7x2NvHeuK7iwu68tm8mKbEUOIw2xDtvIYXI9Xbp2Ju+nyNTk8xueqrYqqoroZ6Omjxk1JT+J5hK1nbm0ud3m5h2Xfdns5eULi0S3jDyM8l0JkkS9huoCqrHCFKqhVmMis1dNB1WOcWn0F5Y3cqbpHIZCQABEUYNC8bZJaoqa8CB+aLy+Wyeey+Wz2cyVZmc/uDK5TcGfzOSl8+TzedzVdPk81mclUEKajIZTJVck872GqWQmwvb2ZWdpa7bY2e27faJBt1tDHbW8EQokUUSBIo0HkiIoVR5AdJpZpZ5pp55S9xK7SSO3FnYlmY+pZiSfmemlZmgmgqImaOenngqqeVeGhqaWVJ6edDzaSGeNXU82Ye1Br6+XWqE0zw6FzJdk9sbhy2+Oxu1N090ZTa/ySz2bbujd2IdcYne+4sNXHcNaKvJ5jFp11u7c22N41VLXVEZillxTSu8aU80iN7De62207vexLartc/OO0FbuzF0dclkbgaPEdYWFzAlzAGUfCJQBXUg6NLG4u9vhlLPdJs17G1vOYgAJlXiqs6mJmjelTkpU0Kk9BVJj9oQddHctXvrw9gxb0iwlR10dsZCLGDYz7e+/l7C/v5PVfwiORdzEYsYdo/uipFR5NHHtb9ZvJ5k/dibF/wAhj6E3A3U3CavqvG0CzNoF8Shh/V8euiv6dK56SmGzG3fVtfH95eP4ZthGaeFor43ik6ah+3RSv4q9POdxOb2DsfJbV3v0ymG3V2vget+0Oq+z95Q7hxe59v8AW1RJmZ6TO9e4iGsh27uLZnbUSmOWsrYZZAlCDAVOoeyqyurLmPmC13fYeeGl2jZ7i92nd9psvBeCa9URBoruQqZobnbzkJGwFZO+vT81vPYWTW95tGi6u44rm1uJahlhJJDxD4WSYAip8gcVpRX7i7K6L3Xu/rKjn+PCbB6Q2Tkco+5cF1rviql757DxGdo8bNlKbc/ce76HIUWUrsTuOgebCtLi0TG42qko/wByySew7t3KnuBs+y81Tx+5Z3Ln6/jQW1xulso2qzkhZxGYNtt2Vo1khcLPSVjLKiy4yOjC73PZb2fbo05fFrtEBbUkEha5kDgV8Wd6aysgqmF0oSteB6DjKdbV2z8jsHK77oa2t693bhNkdk5Or613Bt7eGdwPVe9NxVdBR0edyePNbt/YnaFZjcVVwUuNzgpZBkFi1xaWKAS2XMDb/t/NKctim+7bPc7XXcre4gt23CCJSGAYLJPYmV0PiREhk1BGJFekM1itpPtn7yP+KXCR3NLeRHkEDtkVyqThQe1gKNSop0xyjCVe4d3bb6425u/Mw7y3NT7X6lfK5SpHYNLhcnuo0eFwWWwW01XA7y3ZvvE1NJi6umCmnjrH10ilyAV9pabvc2vLsu93Fr+8oYVl3GG1i128t14Qq1u09ZoY4J9TxH42Wiv1Rrq2gfdEshMsEhMcEjyFZFhL5WUJRJDIlFcHtByOsPZez+zep907l6N7Sx25No7m6x3VlcfuTrLN5V56TZW9p6PHxZwnC0eRrtvUG4qqgp6WGtqKYfcSpBFDM58IRFW2bnZ7xYW+57e7taSlwpkjkhfVG7RSK8UyRyxukiMrK6qwIOOks9vJZ3EltcKolWldLK60ZQ6lWQsjBlYEFSRQ9B0iOzLEqs7u6osaKXkdywVI0RQzvI7EBVAJYmwHtcSACzMABkk4AHmSTgAdNAMrBaE1NAB6/IevUn7itjpHx8VZWJQyVK1xx7VNT/DDkY4Wpo8hLjRJ9m2RipnaEVBjMyxEoG0en3VYbYzi5a3Q3QQxCXSuvQTqKB6a9BYV010k5pXPXmaRVKLI3hE6tNTprSldNaFqYrStMdKnek+x8jvHP5DrXbu5dnde1eSR9r7Z3nuek3xurAYh4KaOSDObqx+E25S7irFrFmmEsVFTDxOkYW66ih2OHe7babKDmO/trzfljP1NzZwtbQyvViDHC0kpiBWi0LtkFq5p1a6NrJO8llE8VoWGlJG1sooK1ag1ZqfsoM0r0od45nbOYpNpYLbe1NrYqPZOAyO2MnvXA0246HKdzSy57I5Km37vXE7jyVemKzwxtZHQpTUsdPEtJCutC9z7Scv7fu1nJu+47ru13LJfzpdR2Fw0LpttIkRrS2khRfEi1qXLMSSxx51d3B7SVorazjjKwK0f1CKyG5FcSujZViPI1IrStAAOG1aDaVTi92w7k3blNrS4La1Tl+v8Ljdr1W48fvTfLZXC0UW0sjUQ5XHUmxKGvwUlVVy5qSKqVXx8UDRESK8ZjuVxu0VztL7ZtEd2s90Ib+WSdYWt7bRIxuFBR2uWWQKohBUnWWDClCkt47Ro7pbi6aLREWgVULiSSoAjJBAjBBJLmvClOl51z19g90dp4PrrfvZ2zelsDkKyvpM/2ruqnzG6Nk7OWkwFdmaWpyNPsymyOXycOXq6aHHQGlRlSrrI2kKxq5Ca83qWPYZN72jabm/lKq8VmgEM0lZAhAEunQUBLmuSqmgqR0pl257XcJNtvriKKRCVkkVhIgIXUKMho2rABBpU54HoPxSPMis0RX6MUZSeQ2pWYMqnUCARcA/4A+zzXpNA359IdFRnrM1JH4JWeSRahWiEEejVHKrNaTVJ9Y2jBBX8NyPbRd/ERVUGMg6jXI9KDzr59X0jSSW7hwHr0Ie3OuNq5qn2ocr23srb2R3dR7310OU/vBjqXrnKbVkiOAXs7MVO3p8bBiOw6Tyti3w7ZGdZVSOpFOzj23PJeK9sLKKNl8VRMZCwIjIOox6R3SK1MNRaV68qx0mM7ODoJTSBTVXAapwpHpnpLVlHuHZuOgpWhqcHV722lDVZRlyGIyNLmNi7mOPyGKoJ6WCOskw1X93jPJUAzJVBlRSsVmDs2G4w7hNfPbTiS2hma2KmN0ZZoiRL3NTxFyukqunBIZq4cuLZ4UtxLGVldBJXUCCjjtwK6TxrmvDA66xGwN27modz53AYSXN4zZe2od4b0q8MiSU20NuyZin27FkM4jeE0gbK1MCFIhK3+URt/aOnV1ve17dPt1nf3Yhuby4NraLLWs0ugy6UIBr2g5agqKelfRWN3cJczQQl4oY/FlK0oi101bh5+Qr69JtaSXVypIv+AT+B/wAT7MxIOHSUoRj/AAdC5uXpLsLaO1Nr71rsXSZXae6dnbe3xFntpZSj3fjdr4jduXzeF23juxKzAPXUvXu68xkNv1SwYnKyU9ZJpsis11BRab/t15d3djHIyXcU7weHMPDaRowpcwhqGVFDCrKOGTgglS9pPHGkpWsbKGquQA3DURhSfT8uNemvKbc27tbL7KqF3Dg+z8PkMDs/du6MVt47k2+uMqMky1m5ep8zk8piqKspdzYeCFqKtyOOSppI3nEtLJLo5bgvty3Oy3qI2U22XiTT2trNN4UuoJ2w3qIrlWickOsblWIUq4FenpLe3t5bMmdLmJkjllRNS0rl4GJFQwAoWWozVeHXe5srgt0bz3HnTt7J7f2xXVOYO1NqY3MplavamHElR/c3bVTuTKUNPU7lpdtULQ01TX1EKVuRWIyyWkc+2tt2+/2nZdu2+C+im3NPDa7upoyqzuSDdTLCjkQtM2pkjVjHGSFA0inS24vbbctyuLvcYZRbGNo4I4WXVGFXTbozso8RYxQOxGtwKk1PUuPsvsKl6jyXRMWWoF6uzHY+L7dyeA/u3t5shU9g4bbVXtHHZePd0mMfd0GPp9v1skRxqVq0DyEStEZLsX32fam32LmU27fvtLRrFJdb0EDSCUp4erwyxcV1adXlWlOi0S3AtWszIPpjJ4rKAMuAFBrxoAOH+c1C96aZWDqGVkdXR1uGWRGDxspBvqVlBB/qPZqWBBUgEEUIPTQQihrkdR6pKuonnqaiSWoqqmeWpqamYl5qioqJGmmnmdjqeaaRizMeSzE+6qURVjRQI1AUKMAAYAHyHl14qSxYt3cST5n16hGjl/tKeb/j+vuwcDzz1rQTknoRtqdibk25g90bCmqcivVnZP8Ao/o+2dmbYGCwVbv7G9aZmXP7NWXcdfgs3V4bOYvP1L1n30CoaiZ2+6WZLKEl0l0bS7TbbpI9xYO0M1wrTRxu2cxh0LRjgEDDHA9XiSATwtdRM9sCBJHGQjOo9HIbS1c6qfb0q8x8csts/M4nbnZ3aHUHWm4Ze58d1DvDbmU3PX7s3B1niMjgdr7mfu/dlDsDDbmx1f01j8ZulY5KzFVldk5a+hqqZaEOqa0uxb7tXMm0WW+7LLJLtVypeGR45IS2l2jYeHKqSKdaHBUYyKg9OX9jdbbez7feIFuozRwrK4FQGHcpKkUI4Hj0AuUxEdBksnQU1dS5enosjX0VLmKBKqOgzNJRVktNT5jHx10FJXx4/KwxLUQLPFFMsUiiREcFQbawKHy6TBW8+meTHux1+PnRpDW9WnVqKgnkLcX/AKe9FwF01xx62EPE9K/IbJ27SdXYXfcPZO2qzeWT37nNpZDpiHGZ5N57e21jMDQZfHdmV+ZkpDtip2zn8jVyY2Cmim+8jqYSzApqCFiX1027z7e21SrYLbrMt8WXw2kLlTAF+LWo7q8KV4YJeMSeAsgmXxdWkx0OoCmHrwoaU/Z8wGyj2/t2g27ujLZve2Q27vegxezs11ntzCYGXPUu9hms3LSbljzW8cbmaMdbVm0cBCa+ETQVMlfKftwIT+57Qzblf3O5bdabfsq3GztNcW+5XU8ngtbGKMNEY4HjJu0nlPhkqyhB393Dpe1nHbW8kt3d6LtoYp7WOICQSLIxDa3Vv0WjUatLAk8KDj0isQaPF5PHZKbD47L0dDlcbk6/B1/3EOM3DDj62CqqMLlGx0tJXLjstTwtS1DQyRzLBK2hg1j7Nb5JryzubSK9lgmkheKO4i0mSFnUqJYw4ZNcZIZdQK1AqCOkcHhxSxyvArxq4ZkaoV6EEo2mhowwaGtD0pt9ZLBbk3ZmNz7ZwuD2li90V+T3EmwNrUWdpts9ZHJ5Sukp9gbfqtx1+UyuaxG36AQiCreolLxuELFkY+yrl203HbNotNq3W8uLu7tI0tf3jdPE019ojQG8lWFUSKSV9WpNIoRXgw6VXptpZ/HtioSQGRoUUqsJJP6Sk/GFAB1DGaACnUnOZfaiT7Xm63xW9Nl1FFsbDYnelXlN7JmavcO/zT11Lvbc22KrDYfbdRtbZO56epjSmwcrVklLEsqS1M6y2G7Cy3J49yi5kubO9ie9kms0jttCxWwZGtoZlkkmE1xCwJaYaQx0lUUr1qaa31W37ujmhZYVSVmkqXloRI6lQpSNwaBM0FQSa9MkUfijj0xsiOGWIiIrEwj0h0iIXxnxAjUF/QCL2uPZ1qDMxLAsOIrUivCvnmnnxz0jYaQFUYPnTj60+z+XT9h8pldu5CjzmBzWX29msbN91i87t/KZDB5vGVKo8f3eLzGKqKTJ42pWJ2XywSxyaWZb2JB2CScDz68QqodQz/q9OhSzvXW/uqMBtut7I653Bg8F3r1dRdh9Q5HKZCsxGFz+Bqs0tJhe0dvphqmbGbsXES4ytxzY+ustNJVEzxxyxwgkkF1ab7LFd7TekfQX81rO7W5rJ4ReK5to3nRCIjKBWaDUpeIorHvouIl26Ka2u0JW5gSZYxLgFqNFM6IxDOqk0SQAgOCQMdQ8hQ7NyG39jnY2N7Iq94Um3szV90y5yHEVuzMflRuUUm3svsZ8JT/xDA7HpdvVVNHlKvPOgiyMgIkVGF7WB5kG4cytvLbf+4FljbZ/oxN9T4AhrcfW66o8xmr4QgFPDwRq6pOu2mDa/pPqBfFWF342jw9Zf9Mw6e4Jo+Iv+L5dCVncZgukd04DbWa2Phd2d2dQ9sZOq7OjzO9du9p/GvsbbeNiwmR2lsqgxO03ppMxQeVp485WRZZ6fIQTCKMRtG3sMbXd7hz9tO47rY79NZ8ib1tCJtbQW01jvVnM5kS4uWknDCN6AGBTFVCAxqDUrJUh2e7t4p7FJd2tbnVOkjCW1lQUZIyqlWIoQH4eYOcLyzHYXV9Vunce4MJ8etp4/Dbp6xl2hFszM723lmMNsntjMxwCv7n66mopMVX46ox2Tv8AwLbdUarGUEEnhZpjz7e2/lbm6DZ9r22/9zLyW8s92W9N9Fa20ctzt8VdO2XmrWsgdP8Aci6XTLIw1UXq8+57VJeXdxBy1CtvNamEQPJIyxXDfFcw0oQVP9nEaqoxU9Rsd1wm2e08j1V8gcnuPoDJ7bo80u813BsXJbk3btXO022Zs3tXCZXY2LqqTJx/3vyD0dN9wH8VJDWCdgyi3tdPzU268p2/Nvtxa23McFy0Rslt7uOCCeJpxFPKl1IrJS3UO2kirshQUPSaHbki3R9s364ksPDVvGZ4jI6N4euNTGhqfF7RUGgDVyOsOyMru04et2Z1/J2XHvXtaaPZu7NobJdshjexdjyRY3K43YC4LbdHNvLdeWm3fQy1FVQHz4urpYKYinM0Tv7W73ZbQL2DfN/Xbjsu0qbu1vLzte0uKskl14krC3hjEBAWTEiMX7wpHXrK5vPpJtssDP8AV3jrHNBEFYSoBVIwFUys+stVQdLLQUJr1k3Hvfe28aTZmI3luXM5+i6v2hB1jsLHZh4yNjbHxGdz2cg2RiYVp4JqPGYzcm48nUGGbXNHVVcwZvoqnoZHCuhBVwHVlNQwYVDAgkEMCCCMEZGOi3SULKQQwNCDihGCKeRB8vI9J+OykXsL8ckDkmwH+JN7e7gFhSvTwwBn5dCVh9zyborOr9mdsb933B0/serrsRQR4Ojpd1ZLrDZu58w2d3nN1vtPJVWMx9dkclmCKxqOaqhiqKj+2oAUh6faYtrHNO+8rbFYnm/cFSWZ5maFb2eCPwrcXcyhmVY46oGVageVST0rF1JcDb7O+vZTtsGpY1WjeCrnU/hqQfiYAmtfkMU6SsFI+QrGx9FksXizVVNdTY/M7jqUx2IpIFNS2Pr87UhZ48ckkEaGZV8qpM/jVmFmJ3LcfSWpup7Sabw1VpLe0UySse0OkS9pcgk04EqNRA4dMxwm4m8BLiOLUxVZZzoRRmjSNnSCB884+fSr3TnNqLu5s509i9/da7egocH/AAWhzu+pc1vvD5qHCUtJumvXeu3ocDMlLms393NSwwqj0tDUCmd5AG9k+0bdu7bGNv54utu3TcWkl+oeC1EdpLGZWaBDbTeICYo9AYmoZ11gA0PT081uLs3GzpcW1uADGGkJlU0ox8RSD3GvDyNMDAw0eAqNw7Xqc3Tbn2zPncNuPauwcF1iaioTsjcmOzdHmsnHuHamCpsZ/DsltDbNVTNTZGpnq4quKrroVSOVCWR653WHbdyjtJ9vuE2+S2mvp9zIH0cLRNGpinlL6knlUhkUKVKqxJBwd29pNegLbMr3hlSCK1XM0moEgxoB3KDgmuDj0672hsDPb6puxqnD5PZmL/0W7AznZW5IN5bxw2z6zJ4HbtdQ4/J4bZFPmZIm3pv16jIL9tgqQmsqVR9AuoVnb7dLbbztQnindby5S1hMEbSANIKq8hX+zhp8UhqAM8KkMCGRzOo0gxqzyBzpNFrqAFMvUU04zjjSofax/Rvpf9J/r9Pp+v8Aw+vsyz6+fTdft9eldt6XYyHcabx2luHdWWyG1Mrh+spdubkg28+1uzcrUY+n23uXNxS4+vl3VtumXzQVOGiaCSveeIB/Rb2VbvHv8p2k7HvFtaW0d7HNuguYTN49igcz28RDKIJm7SsxqECn16U27WC/VfW2skshgZLYxvo8OdqBJHFDrQZqn4qjppr4c5tLPVGLzeKqsdntp5uqx+U21uTHyq+Jz+Ir3pMnhszga8ximq6TJUrQVlNKEYSRsklivCrTZ7nYmS3uK2t1DVLi2ajNG61V45VFcqaowrSoI6rHLNZXEUjRhpIJNQhmXUmpTlWjY0IJFGHnTPQw96dIw9MnJ4HeG6tvbZ702lvyl6/7N+Ov8XpN67nwUs2w8Rvmo7ewm/tjw1nVVV1XnchnI8bjsXT5Kry9BMRHO0njl8Yd5Z3+bfEiubW3aflyaBrix3RUeJGVZjCltLFORObpVQs8lAj0LBVBXU5fwRRSMD+neBlE1uxU0Zl1s6Fe1YakBU+JRQEkggFqlbi3/G7/ANPYuXGa56L+GQeuWOjoZ8jR0+RGTelqJftzHhoYKjKTVM6mKggo6epZIppKiueNNN9RVjpBaw9pL6S5itLiW1MImVdVbgssYUGrs7LkBUBNfUZxXpVYx2015bxXYmMLnTS3CtIWIIQIrYJZ6CnGhxmnTNUfe06VFDNqpp45zHVUssRUwV9J5oCk0bqs6PSyO6Ml1N7gi4Fn1MErRXEZDxlao4Nao1GqCDQhhQg/ZTpllmj8S3lXQ6sQ6EUIdaqQa5BU1FP29KrsKs6yrshtluqtu752ziafr/Z9FvOn3/uPEblyGX7XpKSoXsHc22qjDUFBDiNg5uveJsTjpxJV0kaOJWGpVVDtqbtHHeDeLm3lmNzI1ubdGQLbkjwUkDHumUA62GDUcaVO3MBKm3R1AjAYOQSXzqYU4KcUHHjgcA11XYu/6nrvGdRVW9tz1PVGE3pkeyMH1tU5eqm2ZhuwsxiRt/L71xWClY0tBuHK4RftamaIKJYySyl2ZivEcaGVo4kV5GDysoALsEVAXIyxCIqgmpCqq8AB1VgX8OpJCjSoJqFBJYhfSpYnHEknzNZfUu6+w9idl7T3r1NijmuxdrVGVy22ceevsJ2tE7/wHK0OWqKrr3cu3t2be3LR0WArKuWVa3HVUFMqfc2R4UkRLe31ht1tLebpfwWtipVXnuZEijBZgqAySMqgu5CrmrMQoqT04lvLcyLDBBJLMakJGGZjQVJCqCSAAScYAr0laOfZEuws8uWrewavsymy+zqPrnwVeKyPW8HX1LT5IbvotyT5Spl3RR5ilkel/gVPjQMciNMZQt/ZdPDv8PMG2jb7fbY+U2huH3PUsiXrXZKfTvAEUQNGwDfUNL+qSF0k9KEawbb7nx5LltzDxrbUKmERCviBySXDDGgL28a9QNnZLbGH3htjMb32jLv/AGZi83R126tiQbjrtnzbxwcOr73Ax7rxUNRk9uvV6gfuoI2kTTa1mJDu+Wm7X+y7rZbDvQ23fJoGS03Awpci2lNNMpt5CEm0/wALGma+XVLOW1gvbWa8s/qLJHBmtw5j8RP4RIoJQn1GelJtSk7brOv+/I+szvDH9NJBsndfyC29gNzSUWz5tv0u+5k6hl7IxEmSx43+21d55TTip5aWtqKWuZqrRCzs/tm+5j2naL7lXYt73lF3zdC9ptyMrhrqa3g8a4EYQMkVI1MhVmVQDpUmlOrRbdcXcO5X9lZ6rW2CyzsCD4aSPpjqSQzdxC1AJ8yAOgmDSI6SRvJHNFIskM8LvFPBLGweOSGWIpLDPDIoZHQhkYBgQQPZ5w6SfGKgZ6bnqUrGlrPvGrJJ2krKqsnq5K6oqZqqWWeeuq62aSaorKisnLvJNI7vI5ZmYsSfd3EhasgOommfl1RSjLpBGB0ut37o2xuah65pttdZbd61rtmbBxm1d1ZrbWb3Jk6rtvdlBkslXT9r7lTPVtVFt/dWWpK2GnkpMZ4qCJaVWjAuFQqsLK7tH3Q3m6yXcc9w0sKSogEETAAW66R3xqQcsKkHOakvNIriJViEbqoBKk1Zh+OvEMfl+3gAnqaiWLCZHI1mPaphnyFHhsbkVyaQNjcqF/iFT58WC9RkYK3HHQrsqxRS2sxc6fbksrSbja2kF3odY3uJoTGW8SP4FpJhYyj5IBLMPKmelMUAj227u57TXE0qW8MwkC+HJmRqxDukV48VoFU+erHUJUKfTkH+n5FvoePZiDqAFOHRfTwzUHHT7gIMLJnMFFuStymN2tPm8PDufJ4KgpstncVtubJUybhyOExVXV0FJlM1QYhppqOmmnhiqKhEjd1Vi3tu5a5W1uTaRI98I3MKSsVRpAp0K7AEqjNQMQCQCT1QiMujMWEOoByoqQKitB5kDIHr0YLuHauwsFtvbG4uneytp7j6w3tu7sfD4bZE2UrYe/6ag6y3NNjtrdq/IrruWKswvW+Z7L21n6c4ilw+Rnx89LQPJ4o5fL7CnL0t/Pum4pv+2XI3u2iiIvHjRbQJcxq0lpYzIazpBJETIZAXVn062UL0aXVyfoIraxnVdulbXLArEu8kRYLPMrZRmRgAFopAB01Jom9jiHbOEym7MjszY+88LmsZu3r3F0O6Mk01Vt3ctTh8ZkU3tituYTO4rcFNlNt0lWrYvIVUT4lquaVP3pYXiC7mFprhY4Lbdbq1vIJYb12gFBLGrsvgSO6MhjlP9oikPpVeANehX7Ycv7fzLzjsmw7rFq229aS2YoQHjPhlxJHUMAy07SVIyfMdJmnnbSgKobAAkg3ayjk2IFz+bAe0jb3dDVSOP9jf9BdZkR/dS9u3FDvO9f8AOa2/7ZOldS5WihosdDBtrb8eRof47HW5ySPK1tfnafMxRw01PlKHI5as27ANuxq/2EtDQ0VQGlZp5J2EbIXT7rfSmUvOfCJRljXtCFDU6WWkhDn4gzMMUAArU5tPum+2ylGG6bwXAZSWltWqGFMhrQrVfwkAEHNT17D0+Po8hja2sxlHm6airKWpqMPlWrf4bl4aeRJZMdk2xlXjcn9lWqnjm+3qaeYox0yIeRabmG/ZHVBGjMCA6g1HzFSRUfMHpZF9zz2yamre99IHl41rn7f8S6FGh3ThKXeGL3fRdX9XUz4yqy877abbVTkNnZSLKY3+F09Hl9vZfLZGlrIMHExlo3BScVB8s0kzgEEg3Tc1s5rR9xndXApI7nxFoxY6XBDDVwNSRTAoOjdfube1ksiSfvTelI4hZbQKcUyDZEY/w9B/TbUxoDKstaqk6bLOgvGSrLDJaK88SMoYCTX6gCbkD2vfm7cu0mGAn1Ktx9R34J+VOlMX3JPal6f8iDmEV9J7T/th6c12fipDqD1kWnSNMckJBstjcy08r+o8mxHP0sOPaZ+dN1UmkFv+av8A9B9GUX3F/aSTB5h5iH2T2X/bB0sMRBlcVtzcuzsTuvdmL2hvSpwldvDamOzc1HtzdVdtupnr9uVm4sPAiUOZqsDXVMk1G9Qkhglcstjz7LZ+cL17i3u5Nus2uoQyxSsjFkDCjBWL1XUBQ04jo0i+4d7RGMr/AFl5lCNTUBcWVD55/wB1/r1Cj2JhnNjNX/7CSl/of+mP223uDvK0pbWv+8yf9bOl0X3AfZtyK8yczf8AZRZf967qcvX2AcQqrV8bqCssqVKM9QzOZFkkSaGWCJo0YIBCkSlVBYF7sUre4++ox/xe1IrgFHx+yQH9tejOL+729l3oTzLzP+VxY/8Aeu6favYW0azEYXHQ4dMbXYp8qa/cVDV5BszudchUxVFHHno6+rrsHGmBiQwUf8PoqBjE7fcGd7OC9fcnmOOa4mYW7xvp0xMh0R6QQdFHD95y2pmz8OkY6M1/u7fZGSNE/rHzOGFauLmxq1TitduIx5UA+demb/RTtwvqNXmLabBPPQaQRc6gf4br1H6Hm3+Hvbe6fMAoBZ2f+8Sf9bulkf8Adwex7lQeauaxX0udv/71nXE9Sbbf/lMzKE6gGWfHkrxwQJMY6kgn8gj/AA9sH3W5iBP+J2X+8S/9bul8f92t7FuCTzXzZ+Vzt/8A3q+p+Q6p2bWTmWko63DxGGhiWkx+SramBHpaNKeqqA+blzFY82WqVNTOHlaOKZytMsEGmEVb3Y5jFD9HZfZok/629Lov7sz2HYZ5s5u/7Ktu/wC9X1Fn6h2pMkUcUmXo7Uq000lNWxNJUzapC+QkNVS1Kw1cocArCIoF0DTGp1Fky+7nM0bNqtbJ+6oDRyYGO0aZRUD51bOScUMk/uwvYKTSP62c3rih03e35PrnazQn5UHy6X2+9sbD3pR7RpqLrvZnX1XtbCJg6/Ldd4+twVZvhaelxtJR5XedHW5HLYKpzlKuPdzVUFHj3qJaud6jzEx+IrsPdDmnbvqVaaO5EkhkH1XiSFNTMSqHxAwQVoFJIAAApmpq/wDde/d9umRv6z82R0ULSK521QaACpH7qOTSpPmSekniustnUD0aV+M/vFjoM3Q5msxOZkaGHLx0UbxPhK7KYEYTclNhK+OQieOirqSVjZlkRgG93ufdrmiR2kiitYpjEY1ZFkOmprrCPK8ZcUwWU4xToxt/7rL7vRiWF+a+b2jMiua3W21NBTTqG0hgprkAjOemKbpvabPIUnzMKSSSukMdVRtHAjuzJBE02PlnaOBWCqZHeQhQXZmuS6feXmhVA+isCQOJSWp4ZxMBU/IAegA6Vw/3UH3dpSwPOXOgHkBd7Zjj/wBIjqBnOuMHS7Lr9mbd2ttfK7t3lu/br4ffe8s9SYHMbRpcDiNx5XJ4XDZ7IZPAbRxmI3RT0pWt/iCu8skUSQuJGRCKOS+dt65m3yTcN2vWg22xtH12dlG7RztK6orypWWRnh4popSpritcHvv0fc/9svuxcu+3tx7f7nvN7e75d3UU8m9T2knhLbJA6iH6eztAuvxWD6ywIAoAc9Fp6v27Ubw7H2ZtCg3xs3q8b9zlDs6q7C7LzEu1uu9pY3dE0ePyGZ7C3AlDkKjb20oaaT/L6pad5IYjcaT6hL2/vBBtF7dXe2z3qWy/Ura2qeLM7w9yCGMEa5A2VWtCfI8Dzc2+e5trpXs7oQSSK0LyMQo0SDS4YngrrgniPUcenTt3GdPUdZtodTZjO1uUlpd0xdo4KTFLH1ztHdOP3lmMfgsZ0nuuqzGV3L2B1rkNp09NV02UzCwZCXyqXUMzRxJOXzzA1tJ+/tDUEf08zUWeVTGC7XUSKscU4c0ZYwFDagBRQzauzavOfo00JVqxrUolDgRs1WZKcCxJIoSamgCkRkDQpFvoSP7Vv9tYexARwJOOkxYHsXh0/YHHpXVFVjkxpyGUrcbWNiWfKR4qLG1NEn3s+QnaoKU1akdFDIi00jJ5HZQpLWBQbhO1pFBePeeFZxzIJh4ZkMisdAQBashLsDqANADWgqejHboBcyXFkln415JC5h/VEQjZBrMhLUVwEVgEJFSRTOOsePnjhnx9XUU8eSo6Wso62TFVctVFR5KliqqeprMXM9NJDVUdNl4IjBPLA0c6o+pWDqpCuWNisyJIUkZSviKAWBoQGzUMUJqAaj8iei9SFEbmpyCFNaeRI+VRxIz+fS037uTbe8N+703dtTYWA6k2pnM9W5nBdY7Zy2Zze2+u8NUBWpdt4fNbkllzmSoKFULLNVNrJcgBUCqqbbLS6tNvsLO8v3vL1Iwj3LqFaZvNiq1AOaUqcDJJqTaSSMySyiMRxk1CA1CilKVoP8A+QpTpigqXqYooBXVNVSY556SkpZK2espcUZKh6uroqCmlmlgxUctXUNNLDCsaNNK0jKXYkmDmQEeJWukUJ9PLjx6ZUK+orSleHz6FzreHuH+Bdz5Lqqs3lQ7axfU9bF3/AD7S3E2BoavpLObm29R5LC77pI8pjpN17Fy+7abFmoxXjrUmqaeCRoD4lZSXc+Ydk2O85e2/d9ySC+3W7+g2yNg5M9yI2l8JCqsqt4alquVXHxV6VwWN5uEN/Nb25kt7WLx7lgVASOoXUQSCRU0ooJ+VOmeet2e2yNo7exGyHwu9MLmd2Ve7d/x7nyFZSbzwOWegfaO3KbZElPHhtqNstYKkPWUzvLkjUgygFPd4LXfF3/edzvd/E+xTw26WW2mBFa2ljD/UTNdAmW4+pqtEcBYtNF49eeSyNhZW1vYaLyN5DNc6yRKrU8OMRU0x+FmrDLVz05bM/uCa/NDskb4GH/ubucbaGwI9vzZM9jGkj/uOu4F3IyUS7EORL/xdqc/frBb7car+672OZPA288r/ALv+t+tg+r/eRm0fRaj9UYTB3fV6KeCG/T1fHjrdl+7vEnG5+P4PgP4X02jV41B4WvXjwq/HTupTT0pajdvY+U6sxO1cvBW13XON7Kzu76bc1XtKlqaiq7P3BtPC4XNY+v7fqcO269wS/wB1sBSyQ4CtzFRS0SI1VDSRSSySutjn2qC6Gz2k9rFdJD4y2MbRJIsBfSJRbpQpD4nbrChC1RWpp00YrmSMXcscrRs3hmdg7KXpXSZDUF9OdJJamaU6ydc9jdgdR7ywfY3VO9tz9bdh7YOSfbO+dmZWfB7p2/JmsNkduZeTEZemIqKGXI4DMVdHKyWZqepkUEar+1LBXR0kRXiYFWRxVWBGQQcEEcQePn00RXzpnBHlT0Pr0kmEnhkFPIFqHaWQTVDPMz1E0jSyTzySGWWeeaVyzyPrZ3Ys2ok38ixp4aaKQKAoVcAKAAqgCgAAAAApQYFOvMSxZiSXJJJOSSTUknzJPE+fQq9kZPq2r39uOu6L232Bsrq2rjoIdrba7R3Phd7b8x1M2CxtPuGLcG5sHjcbicl/ENxpW1FKYYEaChmhiZi8bMSvabfeBtVlHzLdWtxvSEtNLZxvFCzB2MZSNiWXSmkEE5YE8D0plkjEkrWSyJAe1VkIZgCKMCcg1Nfy6TTUtPBiaConhy0GQyFXVy0jzU8UWGrcLTBaaSpoalj9zU1sGTDRSgDxIoAvq49qEmkkv7qKOSBrSFFEgViZklbuCuvwqjR0Zc6j6U6USQRx2NvNJFOt1LIxjLKBC8S4LI2GZxJVW/CPWvUdTZQOLf14Fzb8e1oyRT869IiMg+Xz6WXXe2Nr7z3vhNs707U2p0jtjKDLHK9p75w+59wbT2mKDBZPKULZbD7MocnuesGcydFDjIBSwSFKmtjeS0SuQg3W7vLDbrm7sNom3C7TTos7dkSSTU6q2lpKINCkua+SkDPTiBGZVknWKM8ZHFVGKioFOJx+fSg7g2HurrTIbIx2b2nLsrE71672n3N1tTVm6tmbu3hVdedl0X32Ayu7Ny7CqTRU+XqavG1Lw46phocji6YxxzwI5uxVy5e2m6xbpdDcRdXkV0+33+iOaO2We2OlkghnqQul1DsC6SNUhiMBffyNGtnBHbeDbKvjQMdPjlZaGsssdNRDKdAoCi0FM16R5oNu4nZeU/vr1/vKXeW74ts7m6S3uc1/A9pY3b2M3Bm8Nv3K1u3KrGzSb+gz8tBLjcfW09RFHjK+jn1amDAqZX3e53zbJNm36zTYbXx4N6sTF4k8sjxI1oscwYC1MJbxJFYHxUZRw4MILRbS5F5ZStfSeG9nMH0ogDESl0I/V1jtU17SD+aFv/j+f6/n/ivs67f4ekmr/D0sduU2xqs7pfee5d17aNHtDO1+whtrbFJudtxdiU32x2ntXdMk+Qxw2ztLLlpvvsvF5ZKMxoVjOv2UbrNzBCNnGx7XaXRe+hj3H6mdoBDZNq+ouIAFbxriOi+HCaB6mpx0st025mvfqbieKMQu1toRXLy48OOXICI2dTjhTA6gf3S3nUbOruyW2tuap6/od00WyMv2D/CcjUbQot9ZfGy5vHbQyO6HhOOTdOVxEMlXDSSSComgUyabEXXte2KX6bUt5Eu4mE3EdrqAkMKtpMixjPhq2KjAIp5HpIVk8IylG8PVpL5I1YNK+tD/AKqjpGeKOCJYoI44YkDCOONRHGlyTZVWygEn2qZi7amJJPmcnpqgFABQcf8AUOu8lLQyChfH46voo46CmpshUVMk1VSVubRZHrJaWq+3jpqX7iIq6UYdpY0Utypv7S24uUNyLm6ikcyM8SoArJCSAgZdRZtJqDJQAnHEdKLlrZhbG0tpI1ESpKzsWDyiutlOkBQ2KJkgdCThN69cdbJjsts/E1u/e0HjycFZN2xtjbFd1JR7P3X1tSYbO0mK2DDk6vcs3Z2w+xa6smwW6DkoaQ0MdLUfYU9WGjAW3jYt85nM23bnuP0HLP6ci/uqaWPcGuILsyJruSvg/Q3NqqrPb+GXLl08RkIPS6xv7TazHc2lv426gsv+NIrQCN4gpKxg6/qI5SSkmoADSQuroLMvtHd+2sNtHP7m27uvEYTf2Hq9wbF3LujE5OgouwcHj8lJhcluXbGZyFNT0u7MdT5uF6apraRpoVqwyMwY2IoivbK5uLy2tLiBp7ZxHPBAynwGIqsbopJi7fhU0NB8uit1kVUeTWS41B3qS/q1T8RJOT658+lXvv8AgW39g9Z7fx+ztzbZ3BufZ2P7J3zuben92K7+9D1+Q3Pj9k7j6irqChXPbV6xym2Nf3mNr6iV6zK0aVLqPEnsP7Gu8XfMPM+47hu1pcbVBdGx2y1sxOhhQJE1xHfh3MU94s47JI1GmJygPcejC5e0WwsreC3eO4dBPcSy6DqJ1KhgYVZYStSytxYA0qKnnuvEUdLtbeGM3dSbc6o7Q677Cp8RSdPp1jurDb13PRbmp6aDdsud3jka6opsDi+qajb8X2uFySfeGfK1RiY+W0bdhdX6btske2pc7ry1e2Dyzb3JeQPHA8LEwItsqK0z3okNZo6IqxpqBpl64jgkt724m8G1v45lSOxjhkXWrCkjCRmIVYivwtUksaHOJ3WOy+wMCmG7bTsGp+Ou3Mtge2oute68vLvXFYrfe6NkYenxu8+o9kZnr3F53cB3huGh3EccVqIKbGMszx1NTHG1/d9wuOT+ZrjfuSNxWx3O+s4ra73DaJ0WUoshM1m8sUimPveLVESTRlDHTg9NQtue2/RbpbPLbrIzxw3MbaSeKSAFTrpTUDihGoCtD1g3Jhvj1sPc2P67ev3D29jNm9xVKbz746a3THgtq9tdEmgwYgxXUOyd97bkfaG9aKr+/wDFlso1TSzSFFaJ4UDMjjfn7chuO829xZ2SXG1BbDadyt3eS13INJWe8uIZFea1dSlYkCuBUjS1etp+6Yhb280Ur6Jx41xAwAeAgVSNGqokB4McVBywIoFaU2xEw+c3FDm8udxYvsjBRbT6rze25a7Hbs6unbMZPKZndvYeJyVBR4rNYh6HH4uqxdNR68mlfUVNPPTrCqk6kffXubTbWtIxZTbdKbrdLeUK8F7+miJBayI7Oj6pJUkZqR+GiOrlj0n/AMUUPOJCWWceHbupOuKtSXkWgBwFYChNarjgJua/2WneO3d1b6qtwb46k7Rzdb2tnsR0T1x1dFuLpHbdRBUbcl6Y2NhN87i3/S7qodr7gWqywy2QqY8pVYY0NMI6SYzeT2xsFpvu2pDs253rX9jbWcMce7XTKby6mApNJcIipGjEeaAA+rajp1dSQSO9xBCI2eQloFxGi+Wg0zwGPU4AoKgzt3G7Tpt84LFdxQb9wWxoNwUlL2ZTbUxdDSdm4vbos2VG3MRvH7DGQ7mjgZGgjyPjhKtdvqt1G63W8XHL+4XfJUu3XO/Nbs21veSO1jJNwTxpLbW5hJqGMVTXA8+r28dtFfQLuwnjslcC6WJQJgnnpWSih/8ATYp0od87n7DOQoe0c7uamochN2BunN7Z3DVHYeK3tQ7gpqva+bpdw7m2xt9KOqw001PV4eehkq6SHE1M6zpjS6x1QVBtG38vvaXO0QWokheyht72JGne2ZQssTxRSSEqQG8VWCnxACpmzo6V38m6W0ls8zNDJHI09uXVElGvQ6u4AB7l0Mte3joxXrB2/kMBktw0G6MFtXaOxsXmOvdlZ7Jbf2XvbLdiUtHnjh2pN15vdmSyk9dlNu7+3Xn8fUZPK4CQqMTPVpFCgR0X3flCw3Lbtrm2zc96utwuor64SO5uraO1bwTIWghijiCpJBbxMsUcwqZQpZjUHpLuM0FzMLmC3SFWiV2RHMneal2ZiAQzNUladuBk1JFOHZfyI6E7Cbo6s2Zlqrcvf2zunKbcnS+2XxG+st3j1n2Nlds9jdc7Dx9VsA7q3BQ5Pfs8dCIYMFNT7hhnlWLQJdMRL57LlX3Ct9r3u0l8W82q9uW2u/0yq1nfrHJaSTLFJojmaIOw0yq8TenE9OwXV/s5u7RxpiuYkW6hOmk0GoSBCwBZAxXihDedego3ImC3NvSkwfX3XW4NnZvcG5MvhI+tP49kN4SUm7MtvfL0u39h7GjyuOpt4fb4DE1uNwS0uXmyOXqcnSTTzzhpxBEILI3uy7RPc8yb5DPBZ26yXG4SRrb/AKcMCme4uQreChaRJJWMYSNEIVV7alG5hu7tIbCyZGnk0R26sZO53OiOMnvYAFVGolick56Z9z4rL7cz1btTcW1Z9mbl2jNPtPdW3q6jrcdm6XcmCq6mjzS7lx9e7TUO44KxWhqogEWNogAo+pUbRc2e5WEW7bbu4vtsvaXlpcKyPGYZVVo/AdAA0JXuQmpIOT1q/wDEguFtJ9uW2uIEFvNGAwZpEJDPKGJpKThgKDAoOnXYGytxdjb82Z1vsylp8lvHsDdOA2XtLH1eTxmEpK3ce6MnDiMLR1uZzNVQ4fD0tRW1CrJVVc0NPCl2dwAfancL612vbb/db9yljawvPO4VmISNdTEKoLMQBwAJ6SxRSSzwRQCsrsFQepJoB8ul3LgE2bluwdqb0xVQdzbYO5dnNBhs3i56PC7725uWDF5Soq8jQfxLHbl2/TU+MydMgoqjxTzTwVMcrxJZybcrlr/aLO926cfSTeFcVkRgXhddSgKaNG5LIe4VADKaE9S77JrHH7rcrJOhLrcSJRSKBxHIK/0lweHqD0Nvwg692f258yviP1R2FiP7wbB7O+TfQvXu+MD/ABDKYn+N7P3p2ltTbe5sR/FMJW43NY3+JYXJTw/cUdTT1UOvXFIkgVgRQoslxEjiqs4BHyJ66Oc4bjebPyXzhu23TeHuFrtd3cQSUVtMkcDujaWDK2llBoQQeBBHW3v0R/Jv/l2dnfPD+bv8fNy9Pz7d6y+PO3vh1B0dWUva3bUFT05Udy/HbdO79/bqpspkuwJv70zndNHDlETcz5ehpmpxEsSUrSQsZDb7SSbcYmXSiKulqntqpJOTmhznHWKe+e9vuXs/IHszzHZ7yJd03KXcTfqbe3IuRbXkccMZVYf0x4ZKfpaGNa1LUPVeG8P5U3XPxw/lTfzH+wO9+sUrfl/8Wvl1t7qfYPbNNufsLG4qo62y+e+JQw+awOz49x0Oyszgd5bW7VydZS1GRxM9dFFlArPHNTxrAWNZRptt9JNH/jcUuitTjKeWKgg1BI4EHqYNq95N15o95vava+XN3K8j7xskl7c2RjgZvHVNy1K8uhpVeKS3RWCuFJTgQxra58uP5a3wQ+OHZWE2R1T/ACT++/lTt7K7Hxm6qzsPq35EfIek29hs1XZ/cuIqNmVkVZ2ZkZGzOOocFTV0jBwpgyMQ0ggk23O3trKZIoNhknQpqLK01AakU7UcVxXj58Oop5B93fcvmvaLjcd5+8Ttex3SXLQLa3tjYl3RUjcSiluvYzOVGOKHqq3b3xC+AfwW+JPQvyn+fPVPa/e/Yvy0rtxbh6h+OW198ZbrfAbW61oEoq2ky+4dx4XLYPdGQrKfAbkxFc08dc0UkmSpYVgeMTVDh+O3t7Oysr7cInmlmBMcQOhNIoNTMFLVNQygUwRjj1kA/P8A7r+53PvNHI3tVv1htW0bCkcW4bxPClw8lw1QUjjdXjUF45FoVqAjNqB0qAH/AJinwd+PnXPx8+Nfzv8Ahhkd9v8AGL5Lz5Tbcmz+xJ4sruLrLsXDnOJPtqTPUoljrYJ6naWbpTFNNUTRVOHmZKieKRfEg3KwSK3s9wtTIbKbUKSAakdTQqSAAQaHTjgCc9SN7Je6PN2884c6+1PuTDaDnfZVWcXFmCsdzbvopJ4Z4ECWJqgAESKCqkZh/wAnv4b9Y/MHtbvOh7H2Zne16rp/oDdPaXX3SuK3XW9e47uHsDGVlDQ7c2JuDsKhamqtsYzNVlUtOWgqqSp/eM6yiKmnBSbTYpuF5PC6F2jgknSIHT4joVCoT5K2rNKH0I6O/vHe52/+2fLfKEux7pDt0e57xFt97uskK3LWVuysZLiO3aolZFBNGVlxppV16Cf+ZH1P8a+mfkhHs34wZKKfaqdc7IyXYW28dvqn7S211v3LkKSsn331rtTsumkmG+MNtRDRq1bJI8q1ks8LkGIAEm6x2cVyEspNSaFZxqVwjlQWRXXEiqcavWozSpkP2A5k585p5HO6e4EBG4G+njsZ3tzaS3VirKLe6mtSB4Dzd/aABpCsOPVsP8mjpb+Wf8262h+OPafw4z+Y7v2F0/unszfXc9V3j27iMHvQ4vsXbO3qSjotmbR39gcfhZ4cZv2iiDRRpGwoHZlLy6vZ/wAo2ezbxM223+zhrhI3lNx40g1fqAKvhrpC0VwK1Pw18+sf/vVc3/eF9nreXn/lr3Xgh5Qvd1h26y2ldvspJINdrLKWaee2kaQFrZzkkjWADQde6D6S/lv/ADK6U/mZd0dUfEPOdP4/4z/EHC7k6zwWf7r7Z3ZWYLuBNp/KvdeU39FVvvsw5emr4NqbYhXG5JaygjbDsywAVNSJk23WWw71t/M97HsvgfS2gaJfGkko+mdi9SVrXSo0kEdvzPRxzpzn94T2i5x+7jyhzP7qw7rPzHzZJbbjNBt9jCstgZ9lgS1K/TVjKme5PiRlHImALdiaQ52Z8UPgh8MPhx8evlD88dh9n9+dk/Kunq9zdWdI7N3dX9e4DGbBpqXF5RM3mMxiMrt3P1Bk29uHG1slRHVMjSZOlgjg0iWpJGm2bVs21bdu++2s9xc3ZZre1VvCTw0IGqSQAvVgwZdPEECnFuhjufun76e8fu/z77Zexe+7ZsPL3K7C23PeryBLuV7os6eHHHJHNEP1YpEClQaRO5atE6Hz4LfED+VF8u/nZk9n9R4Tszs7o2q+I+e7TzfVvZeT33s2v6r7WpexencLTY2h3ts/dW3M7uoUWD3bX01TA89Zj4KnU0dVWhonp1/K2zcr71zHcW0MVxNtv0Zm8O4Ohkl8RAVDRMpYKGI4UzxbB6CXvf7wfes9ovYm23jmu923a+eE5ui2uDddtS1uFvrFrPcJGdra4gmig1S28bKwVJGWgMcVGDlK+Vnxa+MHwF+HewOtu4ti0vY/8xnvDGwb9yHk3jvvF4/407By3jjoaKuwO2N143ae4tyRyUEtNCtfS1aS5BqyQ66SlphUhzd9tsti2e2s7y318y3BE71LAWsRppQgEK0r0NQQdNTXghebfaL3T90vf/3l5g5l5N359t+7hscpsI6W9q77zdR5Zllnge4hhIcMxjdCI/CUUkkcpcx8n/5c3wg6G7Aw+0Otv5P3eHyVwWR2fj9y1W++tO/u7KPA4nLVma3Bi59pVcWU7WknbLUFHh4KyRlOgw18QAuD7GnMux7Lst/Fa2Ht5cX8LRCQzQzXdAxZl0HQsoqAoPEHIx5nDn2o+8r77c/cv3m88y/fM2Hle/ivXtUsN02nbGlkjWOGQXCmOwp4bNIyDz1Rt8uif/CHqD+VH8ivjd8oOw9z/A7dtJu/4PdIYLefbM2Q+QPcsNR2juTH7D7Hzm5pcFR4XsqixW2Zsnk+qa0iIxfbwtXRqihIyPZHynacq7zsG73t3ywGutuskldxcz/4w3hyMxoNIi1GOtAGA1cMZnH3z51+9/7ae53tNy1tH3hLJ9m5+36Wx2cR7RtpFhC93ZRQCVpbFpJwibhHmupvDYk1boBf5fPw++F38wT5LfLHf+0+md47Y6S6g6/2NujqX4e0Ha1em8N85/IbZmx2YxtR2fujcS5KPE1+8dpVJaWfMUUdLPuKjV6qCnhIBJy5se1c2bzus8FiYba3t/Hh2uKarysoC6PHlXEbOO4nSVMigEAHqVfvIe93vt92v2p9meXd455sbrn3e9zu7TeedpNvQ21pCk4eJ1sIIdBkS2uFoqwSF1tZSI3dwSVT+aN0h8c+mKrqmHqL4qfJv4n783Cm56jsHYXdeTqc9sKlpcfPQwYhett211XuqXfAmmmmaatp85LDBDHGklOs0hZQzzPb2FtdQJa7Jf7fcMjNNb3lCg7lC/TsVWWSMdwZ34mgXgSZ3+537ge6PPkfOUnO3vHylzny5am3XbNx2CMQ3jM6uZfrrZFtxaUAXTG1uGZixVyigGk7txsE3XWVp8hj8lU5mfcG3P7v11PXwU+LxpiTLS5g5fHy000uUWtxavDTrG0RhnZZCxClWHPsyLz+sN+8MyC0FsfGQqS7EsPD0N+HS2WrxGKdYu/3vXg/1N9klZGM53DcdDV7QBFaaqjzqKU6K9vbqvfG0NhdV9pZ/G46j2N3VFv+frbJ0+5NuZKvy0fWe5oNobzfM7exuUqtwbSNDnqlI6cZWmpDXxEzU3kiBYZEWO77dfbnvGzW0rtuW3mEXSGN1VfqIzJFocqEkqgJOgnScNQ464WzQTJFbzMo8GXVoNRU6CAxI4ihPnx8ugxPpsoFzcFv9qtY6T+bH825HszqTU/s6aHaNKnNc/5ulluHbWfwa7T3fuXY2V2dtHsyGfcOw7UNdisBuzbWLypwucm6/wAplVqhk6KjyVFPSmoBqFhq76ldRpJHtW6bbfHdtk23mGK/3namFvuPekk0E0ieLGLtI9PhuyMG00Wq8KHowv0kWSO/fbRa2t0S9uiBhEVFAwhLliVB8yTk14U6Fzcm9s7s7q9oevett2dN9Od0bc3fsneG7s7LnN3R/Jbb/X3ar7zoFqt07h29SbTg3J1E02GxGZXY0eNgarpElqoYJaowsTx8mruG+bZzDzVfLuW7bddC82ULGLaPbZZLNbW5EAifXcJcEyOPqjKYxJpBOkHq43b6eyvLLb0MFtcReFe1YSNOqymSPVqWkZQgA+HSpBJwadInt3qDsbpDd9f112fgf7q72pNr7V3XJjKHL7f3Z9vgd97Xx27tpZVMhtXKZrDTmvwOYpp/B9x5oZJBFMscnp9iHYd82fmKxh3XZ7nx9vaZ4Q5V46vFIY5FpIqsNLKRWnlUV6Q3Frc28rxXKFJQoamDQMKg1FRwz0IW8MxU7l7f2vsTr+g622VT7LqMHg9j7YwXZ2J3n1PQblNBhju/fdD2R2JkRt6o252Lu7GPlq6bI1IwlLVSvTxssKhfYU2HZ023lbdbzmS/vtxvL4Sy313Nam1vHgLyfT27W1mokWS0gcQoYx4rqodu49GtxfvNuVotikMEFswNvGJFliV8M7h5RpZJHGo66qOGckp/duUw2a2b1o9dkN/VPa2FoMptnctDm8PtDFdeYnqnHSQ5DqCk2DNg4KTcmSzEseYyL5SbKxuCjQCKaQCwNdlj3SLeuY2iTbf6nSGOWxkt5J5Lx706kv8A6sSEwLGrIgiERrUNrA6a3KKOKCyjuEuk3kVFwkyosQhNHt/CCgOSysS2rFCNPSn6n2z0bX19/kLv7uTqvFyZXYU+CPXfUVHveo3FsHNVmaXfm6fudwbm219k23qWgx8uDWmocxSZ2WeoUvTmkUyG19d3bbduMnLy2t3usRMSxSSr4YmUqHjldCTHIiMSVJVgaK2kNXpAkarLEl34kUDLq1aTUrQ0ZQR3KxAoQCKVIBp1ipq/rnd9VtjCZ6ixXS2F2X1zu/FS742TtLcG99w9vb2xX8ZzOxsv2Lt6r3QKfDbh3zWy0mGrq/HTR47C0i/cGnqCliTi05j2VN3vrS7n3q6vtyhmSyvZ4reLb7aTw4547SVYavFbqGlSOQGSVu3UtalR4lldG3hkRLSOKBlMsSM5mcZVpF8nkOCeC1z200yNn5XpKgm6qrd77D7U3bFj6/eE3em3MP2Dt3alDuzFzsq9c0HU2ep8BV5faNbiInd8/PlBVrXTRotKsMbMPdt6teebq35rt+Xt/wBrsppEt12K6ntJbhoHGbxr6EyiOdZKUgEWnQCTJqYDpy0l2aNtte9sLmYKZDexJIqBwf7EQsAGQrxk1HupRSAehfpeqsvuPr/r3YfWXyJ2z3LuPfuU613bgvifsiHssbspO3eyKHeGE3BgIcRmMBQ9dV/YXVGB2rSU24MkK2k+5p83SLRCeNZiia43Ll/aH5m575o2WHaBtsUljPvV6sWqTb4nWUSiWMPKtm8rakiJJDCtC3DSfXTx2Wz2d208cridbRGoqzFCDUMQniqgoz4wD5dBh11SYGm3lWybzzm29rLsvFboztPjN77DzPYm3d3752ew/hXUO4NqYSpo6kRbzysMtBNVTTLR0jRnzEhgQv5gvNx/dFk+wbXPfi9nt4We0uorR4LS4FZNwjmlDBhbxkOEUa3BGmlD1Wxgga6njvrpbcRRyOBLE0oeWPC25RCCDI1V1E0UjPHrLQVTbMzWzM7vfYiYvbmV2niK6vxU+Cip6jdXXObfIYfNb42226KfJYtt25bH0+QGJzkcRo6XL0iTQohgYe3rq1l3Lb96stk31pNzW5k+nmeQlYLpNMkNvKINDm1jcp4kNS7Qsyszah1uO4S3uLKa829FtxEqSxqtC8Zqsko8TUBOy1o9AocAgCh6c96bQlxna25uvtsbP3zhKiPfE+2tpdebtkpNx9n0MeVycdPs7am4JNvQCk3Bvaqpq6kgY0UWmrq5QI01Nb3bYtwnn5Z2rdd33KymuPo1mvbyzDRWjSIn68sIlOuOAMrEazVVGTTqt1FEt9c29rBKkIlKwxTENKFJ7FcrhnoQDTielZjM9RbDfK9N98de5ukwO3uw8xX71x+PwuK2h8j9o70wu1s5tag65xe6t9U1VTbL2rDvSWlq8/gqrGNLUPDOyslQYipVf7PdX92nN/KG+oN4lsEtbdZ5ZJNomie4jla6mtrfS0914AaOCZZBpBVSCobpZb38ccC7Vu1sXsFmMrGMKt0jeGyiKKSQlY4mkIZ009xqa1p0GmXhxlPknpNvZDMbmx6U+NMFfUbbbD5WurHxVFUZ2NduY/I7jelpcdmGq4YHFTM0tDTpUyiIu8UYpiklMIlvY4reQlqr4oZFXWVjrK6xgll0kigo7FBXBJWVCmkRaThkKQTgFqKCxoDWnHGT59QsjUUM1dVTYmmnocZJKHx9HUVf39RTU/jjGievVIxVyGQM2sKo0kC3Fz60S5jtoY76ZJbxV/VkRfDVmqchKnSKUFKn+dOn7p7aS5mksoGjsy1Y43bxGUU4F6DUa1NaDjTyr1P2hsrdm+Mw+2uvNm7h3luN8bnNyS7f2fg63O5k4XbuPlzG58++NxcE1UcZgcRTSVVdUldEECFmP0vW93CzsYPqdzvo4bUMsYkmYIupjRF1MaVY4A/yV6ZSNnbRFGWfLUUVPzPXDHDY9ZszdOSy26tz0+/KOt2nF1rtnGYCny2zt0YGvqK1971+5d2S5CKp2lUYCjEE2Lp6ennjyU08gZlsSEN5Lv8AFvuy21jtVo/Lkkdw26XUsxjuIJUVfpVggC0uBM+pZWZgYwAQPVyL6J7S6klupFvQU+niVdSOpP6hd/waVytPiOM1wl/JHp/3br8X9U0fceT9VravD4fx+rX+bcezSr18qV/OlP8ADX8qeVem/wBDT8L69HqtNerjwro0eXHV8sdCv2jjtmyZf++XUGw+3Nm9F540WD2bW9ty0+eyNfvLbe2dvS9oYqHf2CxlBs3cFTjtxZUVi0NGz1eLxmQoxVJGZUX2i2ld4Tb4E3+4tpt4DP4klmrJEVLnwtKP3qRHQNX8VaV4ncrwGVzbK629AVEhBYetSKg5GP50rQJF6zduO2jS0MuRzadc7l3ZTZaXbC7irKbbG490bUglppMjNt6GtNKm4aPC1VRRRZY0pq6anmdI5NPoLZk2y53W4ii8L+sFtakGbww0kMU/wjWV7oy4D+Fq0sQKjNelb2m4Q7ZbbhJE37ouJ9CnUNMkkWWUAHUpC1Gqn2E0HSp38epd2UFTvLpzA722vV/3m3fVb76wrnp9xbA6g2c1ZQ03W1Btbs2uyDbr35lMrF902VOQo6ZqOVUSLWg1EO7DJzZs1xDsfO+62F3Gba3j2/dVHgXW43Wl2vGmskXwLVI+wRCN211JOTQKbm1tdzivNx2HbbhIYWeS6twfEitYa0ipM1HkLZLE1pwoAtSk6Tfm+sNtPbu1cl91nepE3nnuxcH19vDF1tX1dn9/R7cfYOa3bSwRjHtm85gcZVQ0szUtaVo6mGBZUDjS5pccv7Bd71f71bKkHOBsYtsn3G0cLexWnjfVx25J1COOWQFxqSrqW0mmQjjv7+G0tbSWsm0eO1zHbzKTA8oQwtIPhLMikA0aikCor0pqld9ba6cpuoKDe+6sjW9hdjYHsjdnxww2zK3PCqoNsdYvX9Sd8NvLBRZih3FkcrtjfuZpEwtAY6rFUgmqq6PSV8LsG9Pc7nuANjHFy5DCpTdHnREa68eSGezNu4WSLwNKkTMdEhcImRlprRIra3YXDNuDOQbYRsSI9CskviLVX11I0AalAq2DhBZDdlbm9l7EroN1TV3+in7/AK7ocDuTspt51FCm5K/cm8Uqes+sMtST0OwetsfR1fgysdG81HJnqiOqcLNVIsbsVlDb7lusTWYH1xF28sNv4S1jWOIrc3KMGmuWYak1AMIgVyFJNfELxW7B6mL9PSz6jRqtVEI7UAwaY1Z4npO0ebqth7P3ntqt682jVJ27tvauVwe6t27LlyW+duYrC7lbPQ7v6Sz1TUUrYeq3w+EmxGWr4oq1Mvio5qS62ZwaxXcN48qw3UcjQym3lCsD4cigExSUPYyhgSpoVDA0yOmZLdohE8kbKHTxUqKalNQHXHcDQio9OjIdm7V2tubq+Teu58l150RkuouoerNm9Obb2hiOxuwthfNnN46qeXuzfm0O7ZcrmNmY3uLbtVumgn3fjUtjaesglp7wT09QTHHL25mLmO+2naw24Pd3s13u5llhhu9p1hUsIJ7BUE3000UUjW8jlSyCq6gyDo+vxcvttlNeyMkMKeBYijNDKoLPOY5iQutZGAdVDUY9xBBPQFdl7dyuAoOtdtVXUG+utdxYnqfGb13jLuDL7gzkXYmN3jXyZnb3d+M25V0q4/rbZ2e23WUNKq0xNHUPHHJJKJJEUm3Ku5W253HNe62/Odjuu2y7u9laC2iiiNk1soim2ySZWL3k8Mwd9T0dQxVRQE9J9wj8GPbLc7ZLbTrbCSYu7OJtbErcKh7YVZQFoMEjOcdBBa9rckm1h9fYx6LPlTHXTQy/b01YaepSkrVnbH1slNPFRZGOkqHpKx8ZWSRrS5GOiq42hmaB5BDMpjcq4K+9VXU8YYeItA6giq1FRqHFajIrSoyMdeAwCK6ScH1p6Hz6kY7bWc3M+QpNvY6vyVXisDm9114xrRJV4nA7VoHzWd3GJJpYhDFt2hp2q3dCZEEd0VmABanvLWyEMl5KixSSpbqJKlXeU6EiIoa+ITpocGtD15EeQusYJIUvVeIC51V+XHo2G7M9tntbvbqnuL5x5bLbd637c6pwu6N4bn+L8+0d99wbyp9nbcyGzMDuLdOH3LuTLUW3e3+zdzbagXcM2beCeKOcVi0qxW0RNydtcHK/KHNXJPtMsj7hs+6XFtbQb7FLDaW0k7i5+ntikcHjbbarNSHwSQBqXWzUDCHdrqW/3Hb9039I1iuLeIubQjXIsahNb116ZpAO4nFfIUNIG/8AsXvjpbtXp6vGW2dsnvv499WS9O0mC2D11sesz/X+zocRuCm243Y2cxeB3B1p3XvnefWXYNRVVmfgOSqKSCTTVPT1kI8Yp5A3HZd62i933lx55tg3C7e9hvJTIEnkY+HcmCCcLcW0MU8TIEkVa0DJqSh6Lt7tby0vDZbkoF5CixPFUMUUAGLU6FkdjGQSVNBwNDXorVHttsLV7Y29lsxTbP29unH7Mr6rN0tU+6aHEbJzdTBJj9zZjE7Xqspk8pPtyhR698O6HMpJAI/AlS6Aif66O5gv7mzt2uLm1kmhWJlMTNPEKNEjzKqgOaIJQTEQa6ioPSJ7Z4Dbq7hEkRJNQIcBG4MQpJqBkqe8cCAehTp+te12k3F21svqjfGydh9NUHVO8t0b9682zvTYNHtfaG4ctRbQ677tw2Q3ZkYtwYmv7iy+ElyOHydPUNSPmJJGg+3p4SkKQ7hBtrbbtV5uw/f18J3sorxlZ3kUGZoqwooaK21hCQK6AKFnNToxrciWaKD/ABWNlWUxClBWlaMa63Ckj5+QAw273mpNpz5zN9bZ3cSdUdqZLL5raNfu99v1/bUO3+v+wa2fCr2PmNvUU1NtTtTH5ajhylcuBrEkmhq6eaVmiqERku1Qz7zHYQ81WVu/NFhEsd4tr4osmmurYCY26TMDPaSIzRr46tQqwHcCelFxKlsLz92TSLts7aojLo8YJFJqTWyDslVgGPhkeXljpkl2NvzKbwzm2sjR1E+8sfDPuHc8mVzdJlZYYZaSlzdVls3uemrM1RTy11Nk4narkqJx9xUKszCXUofbmLl3b9j2/c4JlTZZGW1tFhiZASGMaxxQFY2AQoRpCr2qSo00PSi02XeN13O42vQDuSK00pmlWgAUOWaXUylmBwakknOa9C32ZPS7kq9j7A64+N2a6o2du3cU+9ul03Pgc3uPvnsjbHY1FgdqY7HZHs2PCYiXuLryPdG3a2XbrYzGNFTy1M0KTVDxn2HuVbC92eLd+Y+bPcMbrvMNmtpu4gkSHabaS0aWZpYbJnYWN08Uii4LydwVSVUHrd1cQ30tjte0bGLW1e48S1d1ZrqQTBIwsk4/tokcEppXtqckjpB12Bq9rVmb23WGkeqwE1ViatsdIZ6GKpo4mglpopfFCUalkUxPG6I8UkbIygqQBDLuMG7bFFucCusNxGk0ayjS+lmBBIqeINQQSCCCDQ9SN7RbfLtfvByxt0skbyQXbxs0J1ISIpPhagrTh5ZBHl0YD4QdhbP6j+ZXxH7X7Cy/939g9Y/JvoXsLfGe/h+Uy38E2fsvtLam5NzZf+F4SiyWayX8NwuNnm+3o6aoqptGiKN5CqkihdY7iJ3NFVwSfkD10Y5w2683jkvnDaduh8TcLra7u3gjqq6pJIHRF1MVVdTMBUkAcSQOtoXdH80/4M1vbf8AP+3dhe+Zf4b80/jZ0psX4s5WDrbuWkn7G3ts74cdkdW5vHQo/X8NdseXF9g56jolqs+mIp5DL54pXp0eZV0l5ak7sTJ2yxhUwc9hFOGMnz6xy2/2l5+G0/d0tJeXh4mxbrc3G7KZ7YiGKTcoJ1b+2pLqhRmpHrONJGogdIfvL+cx0z8tf5IXYvx47j35NQfOGvg6l2dWbam2pvnIP21D1t3L1HuRu0Jt6UO2KrZGPyOb2Pt2ebIQ5DK01S+SoKgRRaJqRJEcm4pNtEttO/8AjVQo4ksAVOonOaYNTkivmB0JOV/Ynf8Akz7we080bFtob29Q3M4lEkK/TGe1uY/pxEZBKyrNIApRCoVlqahiAl/nM/zasv3H8pNhbm/l9fNTvvE9MUPQe1sFuam6t3p350Zt5+zqbsTtHIZqes2lk4+vp8jmW2plMKsmRFFKk0CxQidjTmONNvG6NLcI9heSCHw6HSWUVq3ljNKdDP7vHsbbbFybudn7pe3m1yb+26SSQm9hsrx/pzBbqgEq+OFTxFkomoUNTp7qmBsv5g/A/wCdvw2+OXxb/mFdm9q/HztX4mJlNvdXfILauzcp2ht/P9f1tDjaBMBuLC4TGbh3RDXPhdtYmgdUpCnlxlNUipCvPApULi2vLW0sr6Z4nh1CKYDWmg0OlkBDVFAFpWgA+fRxde3/ALp+1/uHzdzx7SbJY7vse/aZb7aZ5ltpEnBZtcbu0cRUPJI+WrR2XTUK3QK/zFPnF8fOxvj58a/gh8MMdvtPjF8aJ8puSTeHYkEWK3F2b2LmDnHn3LJgaUxR0UEFTu3N1Rlmhp5panMTKlPBFGvlLdyv0lt7Pb7USCyh1GshGp3Y1LEAkACp054EjHUheyXtdzds3OHOvut7kzWh533pVgFvZktHbW6aKR+IeJIiiWgJAEaksxODW/yuv5gHx56M+KOP6W3F8i9z/DPuDZHyhpfkBVdj4npXcfc2zu+9jU+0jt6fpvsDBbJr8bnqzGZOGeaNo6qelgo5KejqqepEyuIrbVuMNraywG+e2uRci4EqoXV1VNIhYK6kgtU0PbniDkBL329m+dObfcCXmiy5Jt+aOWrvl87MtjJfRWU23zmXxBe28k6tGroQDVQxYGRGWhFWn+b58tPhP8nOrenT8NN37a2zj6PtDtTsPtLpGr6c3tsnflTv/f09NBP2dUbxlwdZsDI0GWpcMzS46kysc0Qq4JGjkfyQ0JZzFdbRdpZTbSgiQvK8sBQq4dytXLAshVggoFbtxjJCiX7rntt7r8gcycz/AOujtdxPM+32ljt27LewT24trcEi1EAkW4VkL4doyDpYAgUaQMv5F3yw6A+Hfy07D7M+Ru/v9HWyM78dd2bExWb/ALrb13d91uvJ9k9RbgocV/Ddibc3Pl4PPiNsV03nkp0pl8GhpA7xq9OT90sNo3a4udwn8OFoGQNpZu4vGQKKCeAPy6Gv3xPbHnj3X9rth5d5B2T6/eYd+gvZIfGt4KQpaXsTPruZYUNHmQaQxY1qBQEif/LM+V3QXx9+Jn803rPt7fv90d7/ACO+PFPsXpnCf3W3pnv75bqj61+Q+AfF/wAS2xtzNYjb1svvrFQ+fK1FDTf5Vq8miKZo0fLm7bft+0c0215caJ7m28OFdLHU2iYUqoIGWHGgz9vRp94f2v565890fuy8x8qbH9Xs3L2/m+3ibxreL6eD6zapdeiaWN5ey2lOmJXbtpSrKCL2zPlf8EPmf8OPj18Xvnjvzs/oPsn4qU9Xtnqzu7Zu0a/sLAZPYNTS4vFphMxh8RitxZ+nMe3tvY2ikp46VUWTGUs8c+ky0wRpue1bztW3bRvt1Pb3NoWW3ulXxU8NyDpkjBD1UKFXTwABrxXol3P2s99PZz3f599zfYvYts37l7mhhc7nst5OlpKl0Gd/EjkkkhiP6ssjhixNJXQrWj9Dz8FPmB/Kl+Ivzvy+8OpM12Z1f0VR/EfOdV5jtLszF763lkO1+16rsTp3Nw5ag2Xs7bO5c7tWOuwe1K6epmkpqGhmqldY6WjUQLUL+Vt55X2XmO4uYZp4dt+iMOu4Bdnl8RCW0xqxUMFrxpjgvDoJ++Hs/wDer93PYi12fmuy23dOeX5ui3WHa9te1t0sbFbTcIyjXNxNDFOVlnjVVDO6rQmSQ6iha/kL8xPjp/MI+DeAynyf7Jo9hfzDvj9U5XFbJ3K3Xu7KrHfIHYM80eTXb2YynX+zMjtzbdZOtVItKK5qSCly9KZlaKnyVW8RDue7WnMGxJNut1Tme0OiOQof8ZhJqEYoulXjJOktg+tZGKS57beznuT93n313C19ruWX3D7u3MKpLfW31dur7TdAaPGjS7uUmmUaRq8MOzwvpIZ4Iw1pPzA+b/wF+UHZmC39sf8AnH/KH4w4nEbGxmz6jYHSexflZt3auXyNBuDc2al3fkKLEbPwVNLuDIU24IaKWVoWdqbHwKXIVVUY8yb9s2830Vzt/uHcWMKxCMwxQ3RBYMx19rRipDAcK44+Qxk9lvYr7wntZyxfcv759yvlTmu7mv3vV3DfbrYZp40eKCIW6NJcysIUaEuBqA1SOaZJNSP8u75YfHvoL41fzY+t+0+zanEbt+SHRtRsjpGKs2tvnPVfYu4l2D8jMCkdVksBtvL0G3qmsye+sSHnzE1BDqrCxfTFM0YI5P3rbdq2Hm+z3C4EV1d2QigQKxDP4c6lQVVgtC6jJAzxwes0fvHez3uT7i+6P3O+Z+UuVEm2flfmBb/fzHPaQrZQ/WbNKSqTTxvMqpaTUWBZGolKVZAxff5bXY3xN6z3z2Bmvkb218i+ht3Vm2qDH9OdzfH6ryNJV9fZf+Iioz9buKDCS12Vz1LlaWKnp/sJMXX0MtL9yJAk7U0sQW2STaoryV90vL22fw6W1xYkBo5CfjbKvp0jSQh1EMwxhhLn3oOV/eXmzl7lmw9r+TOV+Y9kS7aTfNi5lVGW8j0aYVhMoSOFo2LN4gmjkD+HSqCRWOb/ADY/5gnRPyE+N3x9+MXVPam+PlBuTq3etdvXeHyb7F2K2ws7uBUxO5MPj8FQYuow22a5oa2n3Kgq3kx0DOmHo2kkqJ2mlJ7zhzLa7ltez7FBcyX0toXaTc7hNDyajhYwWZwlD3a+46ENSdR6iD7lX3aPcX2y91vcv3b5y5P2/lHat329NvseUtru/rIYayQSvM8iyzpVDAdAErUM8oVUQKvWtX3Hf+6EWkE23Dj2IAJsq4vOEsQLkKptc/QexL7KkDeN4rT/AHHUZ/046iz+98BPKfsYAK/4/udaf80bToA8PTZ3qLc/VvZ9ZsPZ2/cfmq07n23t7fm16/eHWXYM+Hqjg6/a25MQpxlJu6SgrqiGGtx1JVvNDUNBHIUfQhmXcvoOc9s5s5Xg3u/266iAtLm62+Zba+tg4EqTwS97Qh1BKSMlGXWVBFT1xJ8G55fm2PdJLa1uYZl+pihlBmheh0NHKnaGYGmpQ1R21IwOpfamzFxLpWY7qDffT9RsTF7a2F3LtTsPJ1k+5sd3ZTwTtu/My7VyW3tu5jrPa2fqZoExuBroTPQaPEJJixb2m5Z3eY3E22bpzVabnNezz32zz2cWiM7dVRBA0wkkS7uYwrtLMhAetaLTpy82o/u1d5s9uaC1iKWt2ksgL/U0LO6xEK8cLAgKp4U+fSbpU7EpK/FbJeor2m3ttjAbbwWGrqmi3PSJs/sPMY3PYinwKL/eE7OpMvlVhrJ0xq0eShYSeWNWeSNzbRy7cJdbxFBHW1u5LieaNWhZrm1R4nMp/S+oaOOqKZNcZFNJIAIQatxtyltK7aZYFREYhx4UpDroFW8MMQGIXS1a1pkEQ8t17n934KuwnUkPbPY+I+OXX27N2d+Vpy+H3H1V1rkU7CyGD3Z2P06cTXNR4/pjccQxE75GaBMlk67yVMyPAkbomst8u7Y6+aJrK1gv71I9khUTLO0MkEbrDeLKKLeiUuCqERhdC11k9Nz29s+j6FZmkjiJvGYpoDqzVaErkxaQCC3dWp+HpG71xn926iFJsMvWu52x1RhN/dQUmy+w9jZPYf8Ad6j29TY6bctNvZ5KvNZDtSnpk3HUU9O5hpKo+qCBXpIkOrOG6WW4tLuOWWONw9vd3DwuZTKXZgqxhTELbV4SllBZCCGbuYppJImVJISqqQQ8cYYBdNACSSdRemo04HiOA6UtRm974fAYzoDd25Mft7q/b/c2O7LzEEuGwe9NpbX3/ltuYHb+V3pXZvamLzmW3hS0GwaSBqrA0VdW01TTU8iRUZq3cn0F+l/th3LbYpZhLC5gjo0EshGpQg8YRtCzONKs4XSSHrpz1ue2aC6a2uNKOjASEEOqjBr2Fg4ANSATXI446Hr5I47b264E3rvqq3Lg/mH3h2Xit81GD2nt7q/anxa3D8cOztuU8XVPZmwk2xX/AMY6k3XPk6CFa3b2YiXwUlW9RVLRzQTKwC5G3mo3VdpeCfkDaEmsmLJcm/i3Kzctf20quqx3cYLHw3t10HSFjaQMKG+72cyPZxXYdd4ugkoJdDE0MoCwSKQWMXaBUO2oVJYLTpJ/IjL9v767A3Tm+xMNtymp+kYthfHBqLrTM0ue6g64pNm4DJUGz9jbAyVLns/RS4LMwbfyuUjegqJ6KepaqkUxhlT3f2v2zlDYOV9ttuWLq7kTepLrmJptzQx7heSXcoknubtTFE3jIZI4u9Q4RYwdWW6c5jvN03LcZJtwijU2scViscBPgwpElEjjBJIU0ZiP4i2F4dADGkkskcMMctRPNJHDDBTwyVFRUTzOscNPTU8KyTVFTPKwWOONWeR2CqCSB7knUqgs5AQAkkmgAHEkngABknAHHoPgfDgk/wCE9SYkIeSNkkilgmmpaiGaJ4J6eqppGhqqSqp5lSamq6SdGjlikVZIpFKsoYEe9A4UhgUIDKQagg5BBGCD5EYPl17gMHNc/IjFPlTp/wAZL9hU0+enpMpU4fbuTwmS3DLjZsjjRBjP4pCGoancuNieXak24khkoqSt1JMs8l4NcqhSnuYWu7e426KWNby5hlhg8VUkGsoQH8FyBOIiQ7Ie0gUaimvV4pBDJHO6sYY3V30kr2hhUa1yhYVUNxBNRkdGhg6Tost2x3VtrPU+6vi9vHbeOpt19D/GrO7P392/292JvDdVbjK3q3ovatXiFpMjUZvI4rKUldJn8kVJop1mWGQrIY4+subYf6j8s7xHvVhzFtDoYN45iSWCwsVihLRX166kPFGqFZB4IolUKawWQMIJ9umj3+8tU2+42+9WQSWdhRppw7d8ESmod2Pb3ZNGrQ0NIfaPZFOvZfcmUj6W6G2YO6tn4HHQ9fYZcz2LjPj9kMpHsvcOSPVOd3LnKjcGwO7qHLbYqqfOpVNPVYeozGYxr00Xk0xCjlKCK15c220g3K4vYIA8SXlwiRtcRq7GOUCMBHtzGVEMgqJIlRwzceirdJZ7ncbm5u4wt3I3iSKGLFXYd4YtkSa6lwQCGLCg6DPbuKzGE3HS7ZrZINh1eyc1U7tr6HcGXHWeYxOU2dTLmqvCY3cktC2Y2xvvI0+K+1wcKqZFzctO0UfnYMV11dWt5YPuNuTeQ3UQgjkgX6lHSY6FkMYbRLApbVKa08IMCdOOmxDLBN9NKvgyRtqZH/TZStCVrTUrn8I/iIxXoSOvuxtwDtjL9qN2rv8A6f2r2xWdsbO3n33lsNufu7K0mzu19uZ+n3ttrdWejoP4l2purc21sumOzUsUkGYqYqx8kVgS5VNctebJsRsth2mDcN7tLSIQbXBLDYiXSVjPhhy0drD8TJUFBpEQJYjq8At7y8R728eCzkkYvcsjzaBQsK6e6VjgGhrnWaDpLbZ3F2r05uXBU+zqSt657dxFStRidwbPWnyfZkVF2VsOixUOx6TI4mpzlFksJuTam5UlixsVM9b58iQxWU+JEm87Pypzhtl8m/FNw5RljCzWt2SlnW0uTKLllYRskkU0VDIXCaY+BXJUWV5uW2z27WQMG6q9UliAab9WPT4YI1AqytUKF1aj60AS+yMLgKvceNpd6HduE63wFfSN2jl9l4Wiy+8NmbMpqlqLNZPEbezdTQ0ldm8ZInjWlqXRVkBElipHtbzFul9b7dO+ytZTcz3SMNpgvpWjt7m4IDojyxhmWNwa6l44oc16rYbfJP48jW042u1Gq9lhUFoY8rqIYHIYUIoSMnSaU6fRu6irNwbSi6Exu5Ou83/dDKdd5Hc2F7BzNFuXtOqys2doc9uisqIchQR7FbfWz6iKhym3qCqkx3jjmg1SxysrF6WV3t23b1d8+7rBfWX1g3CKB7VPCsIgsfh2w0qxuxbzamS4kQSHUGIFBRRbId0vdu2/l2wdL14jbErL3XD9xaXu0rEZEGUU0FCATXoN8Rtzcu5cxQbN2VtzMbk3hlqz+Bbc2jtfA5Pcm4MtnC0tPTYbCbX27TVmZzVcZoGVaajhkmcIwRTa4FqMsmiZmLRNRtVeIIBrU+oNc+vRK4MRkRhSRSVI40K1BFBxoRwHQ8fxj4f/AMZ1/wCjj5M/3b/0Z/wzwf6Quvv4t/p0/uH9v/eDz/wjwf6N/wDSv/lP8O8n8Q/gn7Xi837PsK/T88+F/wAlLafH+qr/AGU1PpfE+Gv+/vB86U1Y1/j6V69tr/Yz00U+JPipx4/DX58PL8PSIrdx4ukw2yNn5Kp7WrtvYCqxW5sxtvIZaLb1HtrdGbr0Ttd+tdr1NRm9uJXbp2/hcZT0e4a6kpa6olo4lrqWSCliDrQN1uxez2l/ZG3fx0t1GqeNqootnmdSjKEepmijJBB7XDHCitpaqtveWFwt4rxMz18J0UMxlVUZSGZgQEd6UIypAzPom3kevuwuvYcpVYjrvKw4v5DU+1cimyGfcbbNnqNqYLMy7myU2OzyZbDbW3ZUI+MwM0kmWqru2NkWESQFj/umbmDZOYEtY5+YLdpNgnu0a4XwBMomljWFQ0bLJPEtHmA8NDiYEkMpeG+tdtuLG5lli2+dE3O2hpGwlAYojmStUKxsahMswoUpkDdsDv3v7d3avVo2hjdlfJXs7L/G2t+JOD6o3Z0nhqzDYzrei23urb+D2fS4TEzbSpN7b72VtKWbOYzd3n/iENV6Kh6oxyRSILnb+T+Vtt3/AHjfrGHbuXrTdH3l7u4uGlR5p1RHumB1tbq0zhFh4B1SRQuD162bdNwubKx2y9llvrmAWrRRqVIRWLCM0IEulAW1DyJXNKdEtw+Gqt1riNtU+WpzjJsZnpcLU7t3MuA2ylFS4qszeZaiy+dqqHDYyszqYwjTC0MuTyjwwAPVSxKRtczxbc11eNAfqQ8YnFvGJJixYJHrWMF3Eer8VQkepsID0TLE8qQxaz9MVYxFyVQihLFC1ANRGaUJagPd0pdu90dr7S7HHdWy+wty7K7ZeTIVkfYO0Fx+ztyUk2b29LtTLGjg2/jcXi8W2T2vUyUFTHBSRCSKVywMrs5Q3OwbLdbT/Vy92yKfYwAn0sxaVCFfxFqzszMBJ3CrHy8qDqy3Fyk/1aTst0Tq1rRTwpWgAAx8h+3pj3f2Duve9B19i92Vq19N1XsfFdXbIpThsNgjg+vdvZXMZrD7Wqo8NiMRXZWpoMruHIPJkcpJV5eYVAjlqCkEKoad5Z2EgKMtRShFTXuDAkMCCKeWMVr1WNVRAgShBzWvoMUPAj9vl5dLLCbkwmyafetDvmXHLsPu/pbIzU+O69Ow+xd5dfS0u4p9x9U7cGc7IXK5XpeGHee2aeTPpjqqn3PJtWq0Kx++eMkM8m8zWxh5chtzuUO4RQXMm5xSRxzRAobuWHwFBlmMZ0xPTwjKCr9q9LEWzMgfcHl+nMDtELdlLK1D4St4hoqBviX4gpqMnpufH7p7Iw278ZuHOptTcnS2y8hu+Dq/KY+l2DsHGbG2dt/GUnYVZgsJU1tGcT3JuDJJh5ZsdBiVn3TV1FZka+riqI/3kUbbRst3abht1ik9tu1wlvJuUJ8e4lld3+lEsqqfEs4kMgV2kIgUJHEhU4dkN1NHLa3UrI9sjOtu9URFAHi6UPwSMdJICjWasxr1EwM9dtmo371XvvZPYVL2d2DQdU7Cwmeyu5uw9tbl6s2lmN0be3Jl6PMdSx0f3fbu1uxNkPQrjsBkGpqSGKOmrsck0rQj2YLc7LcbNJvO0R2N3ZxGe8tmt2g8GS5h8RWKzrWKObxQ8ckxOpGLeIcMOmTDdC9itbx5opDojkWQPqWN9JFUNGKBSGVMAimkZHSR7X2btDavYe79h9d9jnunaGMyKYXb3ZOF2RuzrufegqqOmFQ1DsLdSS7w2/lKLKVMuP8At5g8stTTl4dSSR3pyxu277py7tW9cycu/uXeJYjNdbbLcw3QtiCcNdQUglUoA+paAKaNQg9bvre3hu57WzvPqrcHSkwRoy9QP9DarAgmlM1IxinQvd9dx/JL5B7U2b2J29SzJ1L05PH0NsGDbmxcP1z1B1ZuObbtHuTN7Bwe2sLSUFJgt67sxu2Bnc0s6vUVVRBJKxiVVgQr5c23k7l3dbrYNku0bmW+g/esySTNPdXFsJTElwXJOuCOSXw0K47vxEli9dfvG4tRf3MDCwil+nD6AsaSFdZj+TlV1EHyHkAAEztfdXSfX22urN94La2R7Q7vxG6d6T9lde99bQ2nuj4o5HZddhspiNkTYHF4LcOG7Dz+5aJcjHkahsjU0dJS5KCKSESJColMLRucxzZvKX8W1LyILWIbe0DXP7yN1UeOLpXH0qwDIjEdXwCxyQGZk2ttugETXH71L/q6tHg6M6dFO/VhTUmmWoBQEwNgdE1i1uzKnseHI7X21vTae9t67Mxs8kY7C7zr+tchQ4yu6m2zjsZSZjce0uzOzKtnocJX5fCvG07x1cdJV0rqSj3TnC18PdrfZ51nvrCeC1vZGBEFityhkS6lkfw4ZreBRrlWKXABQujinTsG1z1s2miYRXCO8CgAyTGMhWjVVq6yMcLqXPEAjoRcJB8i+gtqJ2/kes+9NobSj2pv3oz489prmN19d43pnN9oLU7rzuOgzOHwsdFuh95dcbxzcc2Byn2FFuKjz1XW07FISiJU3TaN332Gw5c5wsot+jni3HereFEmkvbdIntSne9YV1qg8aLW8QjWNh31LhtJrSzeXcNrkezdGhs3ZiixSalk1EKO/BNFcKraiQTpp0VHLYLB4FsRSbf3Ditx0FdtjbubrZcPisriI9u5zLUCzZvY+QpcxS00lVmNn16NR1NXTCWgrLLNTSNG4sL7a4urkTtd2bwukzworsr640akcylCaJKvcqmjLlWAI6LGRYiuiQMjKGNBTSx4rQ8SpwTwPl0sNxVvbW4Nr4DfG66zsnK7BlgpuntqblzmT3bX7Jah65pKfJ43qTb2TylbVYuXFdc0OUiqaPBJI8GHSoEkMURYn2ij3LZpN2k2BdxtpeYrW2S7ktWeNrqKCUtGk7R/2iRysrIHoocgrnq729wkAv1gdbKRzGHAIjZx3FQeBK8aEkjpO09SldhMrT5HfEVDT7Jpf4ptrZ+Un3FXx5Ku3Nl8ZT56i2lR0VNXYDa2Tmo4xlsjPWPj4a+nx5VZJqoQRMtKeHdweBteuS5YRz3EfhqVEaMYzMSVklWp8NAocqW4BNR6ZNDC7/UUWNaqhqa1I1afJTQVNaVA8zToZ+ts53X1Z158jqbr3eeH602/vXrvZnVneuz8hltk4vdvZfWO/d4UeaxG1drYPN01XuvM4o7hwtNXZyTbjU1TSYt/8sl+1neJyyfftpvL3YtveKa8ivpJpILiGGSWCOSxKSkzzhfDt2DqBFrI8SRdK1I6WzbRd20N+86fT3kAj8SCRlV2S4BA0oTqeoaraR2o2piOotLv/J53dWyc5V9r9lwUvSnVtDD1ll95dg5THbs2RV7BxVXncNsHpfO4Kkz42fjKPsKukqNsY+nWhTxl1nqKSZzMEk20yx7Tudj+4tue43O/ZbyK3txLbzRTyhHlvIpWj8VmtRpnYlgGIKo6jSdQ3Nqt5BOJ7kRW8GqNzII5VkSOoETqGCgS0KDBKChKnIwZCgyOCxseK3NjKeTdG5YaDep3JUZTMSZWChzNFkkqcLkcc8rY2efLZOo/iFRVSrNXJOgUS6HlVrLdWu9wXb7LOfobd2sRAEjCF4nQ60cUYKiDQqiiEZ01A6kLkO8h5E555T3XmhfDhUrfSSAOzqkkUgCsgGWLHUeJB86V6bztbL0mKoc5UwiLEZCeWlosgRM9NU1EMfklgjeOFz5Y05KkBh/T2UiCWW5ns41BukGp01LUA4BOeB9es3F+8R7ZQ28d3JuF0LZ2Kq/00tCRxHw8eu4YI1W5q6exN76asWAF7kGmDDj8Wv72dp3EggW2f9Mn/QXS2H7zntIlCd2uv+yaX/oHpYYHCHNRZlqTLYKKXA4uLL1FDkMrBjMpkaaepio4oNuYnIfb5LdGTeWUN9pjoqmp8QaTR41Zghudt3CERFrNyrMV1KVIB49zatKj5kgeXRtb/ek9nzrrvN0CBWhtZqn7AFJPTxtnDTbnqpaTAVNHk56bF1GcrhA1QI8ZhqKCWpyeWys8tPHBjcViIINVZUzslPS+SPyOpkS6afad0iRmexkoK1ppPAj0J41x659OjO2+9Z7NEqv76utRpxtpR6nzA4dKzHbK3JVbgp9rR4yqj3BV7Nl7EpsbV0tXj5Z9kQbbqd3/AN5Ypa+npqZ8bUbbo5KuAh9VSgAiV3IU0fl/dyFItP8Ajaf9BdLovvd+yaYO8XmOP+KTfZ6evSYXO4KFUL5imAmhiqYyKfJPqhmTXG3poDpZl/smzD8ge0jctb1JqKWWASD3p/0F0bQ/fE9j48tvN7nOLSb/ADdPeLymDr6k0sGdxSSLSVtYXrZZ8bTCHH0c9bUD7zI09LSGoaCBvFFr8s8lo41eRlUobjljfUTWdvYjUBRWRjVjQYDE0qePAcTjo2g++Z7FYX993oIFc2kwGAfMjp6yWQotvZKoxG4JK3A5ekWmerxObwW48VlKRayliraRqrHV+Hp6ynWqoqmOaIugEkTq63VgShi5V3u8hjuLO3jlt2rpkimhZTQ0NGWQqaEEHOCCOjIffW9h7d/Dn3jcEkHFWspwfUYK1yOsce79qqwJztOACL/5Dmf6Af8AOs/w9tScj8zMcbcP+ckX/QfRjF9+P7vy0rve4f8AZFN/m6ljfWzEYRHcVN5GUyLGKDNFygKoWC/wu5UMwBI4uR7RvyFzUR/yTR/zki/6D6Mo/v2/d5Tjvm4/9kU/+bpzqN0bYpcbhsvJuDHS0efhykuNFH93X1jriK58ZXCsxtDS1GRxUi1aERJVxQNUR/uwiSKz+0h5E5oeWWIbbRo6B9UkYA1CoyWAOPQmnA56MY/v7fd1QRsd83KhrSljMeH5dZMxujaWCqUpavdeEqmahosiJsPLV5ukEGQplqYYmrcTR1lLHWRRkeaBnEsDHS6qePaW35C5sulLptDKNZWkjxocGlaM4NPQ+fl0aN9/v7uFq2huYNweqhqx2UzDIrStOI8x07byyOH2DufKbP3TmsdRZ/DmkFdS0b1OcpV++oKXJU5p8tgabJ4iuU0tZHrME8gjkJjfTIrKE1lyVzLullDfWO267WSuli8antYqaqzhhkHiMjPRg/8AeBfdws5pIJ973MSLxAsZjxAPEY4dYZ83tyl2xi94S7kw38Fy2YyODovHNUzZVshioUqK0T4GGlfN0dKkci6aianSCQsArkke2hyFzZJezWS7SfHRFkarxhaNgUbXpJ+QNePp0Zp/eF/dqit4bpt93PwmcoALGbVUZNV4gfPrnDnNnVOO3blo9+bOSj2dDQVOQFVlnoavKQ5KvGOpztPH11LTV28JI521Tx4yOqkpof3ZVSP1e229vedDLaxjYJNUtQO+I6SM0ekh0/n0vj/vGPuvxpK7cybl2Hh9Bcd3zXFKfbTpOf6QNj3Uf3mpuf8Aq2bh4/xP+4a/N/xf3tvbPnQ5/dAp/wA1Yf8ArZ0si/vJ/uurprvm78f+jfN1Lxu7dq5yvpsXiM4lfkaqRoqeip8PuR55nWNpWWMfwTS9ooyxIJAA/r7S3XtzzfawyXFxtiJAo7naaCgyOP6nrjo4sf7yv7rs06wQbxvLzN8Krt01TSvz9Og27E3rtI44UKx0W6548hVQzYiaXcmHipamTC5rFU2ReupIcdUPPhclkIqqOBXeGokgEcytEXVpJ9teTuYdludwutwT6aKWKPw5UMUpYK4dl01YAOo06jQgGq565+f3gn3qvaL7wuye2O3e3F3e3F3tN1fPeR3lvJbgCeOBIyrE9xDRkkD0FagnoFN30G5MDt2o2xuLedWud6r3Zj6jZG1a3dedkxdPQ75ops7mtx9b7ZTGtjsW/wDeTB4+szWSirMdM8j0oSnqJVMsMl7Pdbful7FvG2bbF+7dytmW7nSBBMZLZ/Djjup9dXAid0iiKvTuOtVOluaW77fdbP4+07lI/wC8bWUNEDITFolQOWiQrgs4Vmeq8KaScgTMf3N3jurGfLfFbU7x3RPsfvPr3bO8vk5B3jvXZFTvTvmn6v3FtbPY2mqctuha/Jbv7BwfZNe1XhIMJVQ5+bDiYO7xrVxmkRteXIOWILzYohfyXLbXaDabWV4bZZ3eUE0Uta27RwJ40rUjEtBWjL0jEMd7LfyxXTraRw/UP9Q6B3MahacQHbWx0qO7RmhII6ALG46q2zNkMtPuU9cbh2tj8RvXbOo5/G7hzeSqMvi3oJ9qZnbtNLHt7N4+iqWzUdfW1NBCtPQuIp/vDBE5291b7jFFFDbC+sJnktJ2BjaOMIrBxKkhBkQsPCKKHNWFV0VIaltbmzlKXStbTrGk6KwIZg9CjKV4VU6gSRgevUnaW3t4b4zlJsvYmH3Tu/c+92lxVNtTaMOWy2Z3p5kbLz4hsNii9RuaGdaFquSnkSeNjB5mUlNQb3fc9l2Hbp955gvrWz2ezUSy3d4yRxQCojDmR6LFlwoNQe7SOPVbe0vNwuo7Hb4JJbqU6FiiBZnNCxAUZbAJI+VfLrvdW79273z2Z3lvHP7h3xvXMss2c3JuvO5XP7q3HkKGnShhqdxbi3DWV+VyGUjpKSGjElRKTFDTxR2UR29mkagfE58MnVU5ABAppoMrTI+05yOk7kCiIgDDFBjz4mv4vLy+zj0YzryPsDO0m6vih0lDvf5ASbi35sntvqSDq7J7727tnbnanX+BSs3p27SdR1uLSl3PkcZsiSt25Lmc4aClw9BSSZGKQwzIPYS3jdHt7Pb+ZeYt2TZ+XrdLhd2sbxIZvqElUw28ZuFYtCytSULCHaXV4LAFSejC0t0aWawsrT6ncJGjFrKjGPQysGc6DRX1fBVyApGocQOouW6k3Fm8Oa3dON3dtr5Cbu7WwWBO1+yFfD1PyEz3cebyldPuHZj5rD7cwm1X6210Em6aivyVZBXtuvH1KfYU6MZE8fM1hYzyLaXNvLyfZ7dJcPNZgv8Au6K0jWizqjySyC5AfwAkasPAdf1GOLHbLlxGrwyJuU1wI1WXt8d5GyULaVXw6jWSSO8HtHGPs99gbbzG2elPkVsCu2lsfana+4tx9i7/AOpNp7ck+UYxdTtiDabbC2vu7d+ZfrvPdWY7L4KLJY2j+1NJJWVNVWQ188csSKY7zuW/7nytdbn7ey7dcb9cQpLt7bsbgWbF2RibgQhblT4RbtoHD6Q4Gek9ta2tvuQg3hZktoyySrb6PEBUMAELBkK6wATQjTUiuOkt1zjd75ftrHUvx5h31muwtrbjye/OsJNtR0cXaWGpOuXr9+4be/22KqJqLGbm2jtrbgzNZJTu9NTy0krwmSJVDKN6vds23ll7vniezttomhjtL9pSxtC9zot3hVnAZopZpPCTUAxDKGoSaet4Zp75YdqEj3KuzQAafEopLKxAOkOFFTTFeFcdKLu7ursr5EdgV/d3acWHr9770w+JNfuHbeycb1/id+1GCpP4bU7ukpsRRUODze6s/XK82cysAJqsnI5kEVliS/L2x7Ty1YLy9tEzCytpCPClmM7wB6MIzUl0RVp4aNnSK1apYt3M890/1cyd8gwwXSrgfiH4Sa8SMA4wKAL7OUXVvVOz5Ysdu2s78xHevREM1VX4+HtDojbXR/c2B3jtrMS0efxWcpqjC/JV+rKelraNo5BDt9KzK/exSpNBCJEPLm57xvd/vY37k8bXc7bftBtztc293Jc28iUF4ngDVYide3wnPiMvxYBoov7a0s4bFrPdhcRzxF7gCN4ljZT/AGba8Taa11DAP5dNG39ibwxlDuvsvd24t69bz9dYvrncOOy1bVZfG9vZbMdrYzcMvR2e2NS7jymB3Dk9pZSt23CavcFHVscRhqmnq6OOsUxQmtxuWx3q2nLu2WFhf2V7JdW0tvGsT2KpbOgv4bgRJJCsqiRv0XXvlDJJoNW62Ir63d726muILiJY5UkYusxMoPgOhYq5U6fjBwtCtR06x9jJDs7tSPPYtsZ2P3HS9X4eKZutuu6frubqbFVFFlMnvijymXxL772l2Zn92bSoJ5tzbbaKHPU75h8nPNLUyhldnBeWl7Z2W0SWknKtvDcR3IeSWS9juw6tFbw6SYFt442KmKSkkY8KOMCMU6rKYXgmlu1nXdJHjeIhVWFomBDSNXvLswqHWqt3Mx1dIjc1JNt7dVVhcmcHkcptOunw2Xzm192ybuwm78pisnVyjdmM3d9zkqLN0WTjeL7aqpbUlVSRRSeMPJLqMLFxc2EVzamSKKZRJFHNCInhDKKRNDRSpQg6lbIYkVoB03KNMxScB2U0cq5bWanuD5rX1HEZ6WPYXfvdXa8W56TsTsbcGew+8+1cx3tuTbEdFits7Iynce4cQu3c12Zj9l7ZxOE2ris1kMHD9gWx1LBRxwo0ccasHPu37u20bk28R2UI3b6f6M3IzKIA4kEBauF10ahFeB4U6YDyrAIDK3havE0nClqFdQB+VRjHHzr0iauo3Nk8ThN0zZqhf+7Eu3usds02NyGEw28MTQ7fxVVmdsnGbfwEeN3JU4jExPIi7ieKaZ8lIkM1ZJVGMCipYQzXlgLVtM4kvrhpFd4HMjBJdbyaogz4JhqF0AsECV6uonKxSLJ+ohWGMIaONIqmkLRseTcdWK1p0I1PuvsvC/GnMbNl2Jtqi6c7Z+QFDWZjvCv2Ua/sWTsbrna9Gcr1hit/yZUV8W28RgtxR5/K4JaIyV9ZOGeqvK8PtA9xy9d8ww2CPBJzVt1iL2G2U0dbWcyQxvw0LDJIpRSCArKGpRVPSpV3CCzkfx5FsLmYwT5amtSGIcVBZgoLEEGtCK1qOn3c/dnb++O1++fktU9n0+b7EymPqNn5rsDG7C632k2/8L2ZjY+nPFRdV1lFQRbWi3H17iSryYTEVOSwkwSSaWlml+7YgXljl+DYOTuS7jlwJsqyrefRSXNzJ9NJaE3oP1KEicxXTDtlkWKVa0DqujpZFfXcd5uu52+5P9cFMEUyRKDMJSISNDd0WuKuVVnVqAkE6ugZo8tV9X5fCy4L+/e0ez9hyZ2Q53D73k2xUba3eGp5Nj53Y+f2pHFujb9XgcadOTdqyaWqnYGB4UDIRRa3F3u4G6WO5W52u4eGW3dIWaR4RqFwsgdghMj18Iqq6FrqDGh6YuLeLapZ9s3Pb5TewrLHLGZQqpMwUwspQMaItNaknUaUIFR0qv4P0759Onvv+H/6UfvfJ/ou2L95/oV/h3k/jXh/vx9t/pN/vN+1/B9f93/sP3f4p5/2/ZV9bvOn/cvaPG+h8Kn1k2n63Vwr4VfC8LPi/wBvrx4WnPVvpRx+hutHiePX6cV8DhXjSmrGn4KfjrjrFubrDuKXa3X/AG/uTA1mWwPeFZ2Qmxs7DmcFms5uWq6fy1DtrsU5Da+LyNTuXbEO2snWQwqcjRUUVWhL0vlQFvb1jvPKe3vuGwWV1FbDa1txPGVeOKMXamS30yuBHIZQCe1mIOGoerTW2/bxd/WTRTXV/dGRiR3SMYe2UlFyojpTIApw6bsJJ19uKbY9L2f2bvGg29j9s71SsG2Ou03DlevstjIsg/Xe3sQMhlqCh3Zit9ZCGkfIV0BifCU08iMsskWr3Tc49+2qDe7jk7liym3ie7t2K3d2YI7pHZBdSyMqM0UlvGX8NDiVgKUDU6bF4m4/uu33rdpjYW8LxxaEDmEDKIg/ErkAk+XAkUqBerOu+oa/qr4Z7xyVTT9TbW3lu/fPXHyY73wG68/2Pvel3XT7kgzVRXUXxxWtgz+JxnT/AFzUU0NPkcJIuO3bPkLKRU02iZHFuu+x71z7ZhfrZYI4rjZ9teOKJDEIwp1XeFY3UxJCzAGPQQDQkqy0dsbbapB+lqLJczAuTqqTQIBUBFFKrXVWtOFQW27tSu7LymF6u2vh8vuCLO9vba2DsXtOuyVXtLE7Z2/uLM5ijTCVFHuKsg6y2hlOwKNoc4n8cr4qqgqMYYI5Giapb2r3rdbLlfbt45r3K4S3Fvtct/f2kUfjySvDGp8SsStdTi3zF+khDK+qlQvV7ZbndJ9t2gGSSL6gQW7FiFjSR6sqBqRoZPjoxB1CmanpVfJafrHbvyv7KqOtsdhE6c2p2dgJdnJ01i9xbTwOZ2ns6n2zHV5zq6DsGfc2VpqjcWSw1ZVUeQqnyFBUZSV6qBZKJ44RrlzcN05p5I22/wB222Oy3ncdvcXFnOdawvMjqI5wr6gNDKZIyyyKCUbQ4NN38Frtu8XUdlLLJYwXCmJzpDsqFTUEDSaMCFZaqaagStKyvlZ15u7bPYezexewO3Nk9vZX5Vdfba+T9RvvZ25cXvWfE0HaO4tyYyXbnYlXt6gw1H/pY2WNryR7ioaXHY+OOtBip4QulnvyZY2ezcubby/tnLkm1bPtiDb7K1YEL4MIAEkSNJLKkDuW8MSu0mkBmwR01fzyXN7c3k92s1zMxlkcADuJ+E6QqEhQK6QF9BjoTN7bK6s6lyHwg378ROz6zcna1X2Z2tQZftCPbyV+O3HvPqPv/HY/o7vLC9GbnrN29h7Ih3VtCupKuba24Nv0azfYARU9WZJnISj3i63LdfezlzmxGn5YsILV7dZI3tUNrd2DvcWyXmmGOYK6NWVZneJnKuyUUA3WwK2/KF5ZmOO7upHQlW8VtccyqskkIZ2Q92F0KGUYDGpKO7v6k7Iods/Irsnsft7Y/Yydi9hdV9iLubb3anXM1Z3LXdr7o35lF7gy3UstLX74qKClZ8lI0FIMdLtiplcVlLNSlI498m80cvbtecsWWwcvXNk+1pdbVLBc2twn0L20cAa0iuKpEy4SsgEiSqBodX423zbb3bDuENzucdxBcmK5SWB0ZbhWZ9ExTLqcmiEqVzUFRh9+RFbuvszPYPrTe28Pjlt3H/HTqGpyHUO9upcTuzdVZ8s8FX5XFYfL9g7d7HydHN2329lNwf3PlyGMTcCUS4KgoZ6eioqOmdiLcv7XYcjfvFNpk3DeE3DeZYbyR2hjt9vJMkyxCJUht4beIz+HqRC8pZTIzMAOqyud8MlzdzwWTwWSyQo3iM9zTSnYSzsZWC6qE0FDQZJ6SG1tkQYPspfjRjex/it1/uah7b2r21hfnxursLK4nH7e27i9rYjL9f4zau+cFWZ+h2fQGXOQZ+rwsFJJn03JEaSuqIJMUQHZ76Letoh53utr3642yXb59qm5TFuKSNJM0VzJc2siK8xAjMSSk+GbdtcaOJh0woezml2yOa0W5jnS4TcA1GXQoKLFLUBRVgxXjrAqw016Qm18rgMbV9ldz5v5K5bG/JfrruCh331TRT9a5/tbbHfW5qTNZrO57s3I76yQn21g8xkd10kFRTybjxNTBlafIPJVJ43kSM4v9vW4sNr5Uh5Kjfkq8242F6qTpavZW7RrGtqsaFZSiRHTphcFCvYQyjUmiupY7mXczuTDdI5/HjZlMniyBtRkJIKambNXGa5BqaPGP66637awmZ7H3RvXP1G793Tdu7/7W2d0h1BJXbZ6lq81njj+sNqZPatBQYyDEHtrfNdVzQRYFqrDYXb09HCDT1KzrCX3G+b/AMv3cWw7dsUQ2y1+jstuut0u1VrxFiDXUschZmb6KEKreMFklmVz3JpJW2tltd9rudx3ORZJFmllS2hL+HJX9JWXAAnck1UkKtBg56Xu4Ox3787A+LO//lH8mtpb07By74za/Ze5cvgsvSUHW3T1NhMVVdc7r7g7w6Vqsf2F2B2Zja3IVlBlMVHSQ7h23T4ijhmrpoaxxF605X2nlnYudLXkrZr2Fri7kk+ikq6NKoSImygvDLbxWsqLVVRfCbudULaR0lfcLq8udsfcJYyI4xSRCFah1N+o8ehmlDHJJqPM0JJa/k3v7svffSm35t3/ADO3T8jM9SS7Mx9fsfA7hyEXVe1sFgdp7t2z0/Pktt5ubb2Rr+5dr4jD1VPURJiao7fxeQihmqYXmVZEHJBt15u3GJfbl9nsYxJBb3u4Lrup/Ca3E3gyKZkTa2VkWCsieIYzojKodJlvEMJ2S3uRzALrcWYGWCCgijV1dk1V0M11qDeIApC6gWNSCU/80M38SK/f1dWfGekrMFjcQ2zdupR7dOIqeksh19tzpTq7Gxbtw25chh9ndgZ/uTcPbY3M+7J8lhaSgkH2rwTVEzTN7NPa2Hmr+pW3Tc4wbhHzLPdXk9zBuTK88XiXc7RRjw5ZkSEQhTDGshCRlVAUCgL+YDYR7vPDt9xbyWCRxrHLbjSjhY11NQohLBiVZioLEVJJNSj+5MN1lsLr/pfZHX3b+P7sqt37A2N3p2FJi6zeFHiPjz2tvDCZfFb6+PdNiKjJp19uLPQRxYyty2cpsamYpp6aLHS1Lxq4kPbHb71t+3Leb2ytoJTF9HHJAIne5t1k8SCSaYxLco0PcvglzCDIXUE0IQNc/wCKxWaySNCH8TS5bSj6dLBVroIf+IAMQoBPl1YR8dt17Q2n8SerNh7g+Lmy+/8A5Jdi7k3xs/429W9r9f0GJy+5tvd9bwoctsLt7qCfFYihk+QmDp95bLrsXmKbdmWWmw0LfaUqrRVbq0O8zbrv/MXuJumzWe/vByFttmTd7ltTg/Q3sHhPd2t88UizW960LqbZCkyMjswUSICopsYNu23l2G6nsEbeZ5eyKc5nhk1iN4kdShhUjvYMjVFG7SNVXqYvrWLZ+9Nu70oOxdt/INO1sDhMFnWqsHQdRbC2Ek2XwvbVDv7CyUtVvin3dtzPrT/Yfw0S0tLQUsyOrPGqSzelxupurC525rWblk2bSyRjUbmaWge3MJxEySqe4sQSx4HVVQfIsYjm8bWLzxAurGhF4PqqdQK0wACAPSlCPnyW3B0Lku4+8H2ztTZWQ07M652d1jnPjOlP118aqXs7ZWH2rgd+dh7d2ZkKfKZ7c3Wm/qLE1dRAs08OUqMxWTVk9gQvsIcrWPPMO18og7wUskvbqfc494R7ncJrOUytbQiasawXMMjJUldAiUIBWvS+8k2qR9xb6Os5hjW3NsQkKSqB4jlAW1RsPmTqqfMMASzmMx2RgrNwbByG6NwYTA7WxOV3JS7zmphuna1QqrjK/FS1UKw4jN0E2Vgmq8b/AA0OlPi6iCKe9XHOCKIL9dulsdu3mO3t768upIrb6RW8KY/GHpQtG2ghXMlNUgYjsI6stjebpb39/aPJPBZQLJcNO41xoTpCip711AlQnwrjj0cXpH4+4GH5F7y2PvzIbP8Akt0j1Ftbce5d67t6H39kcl1Xuisi6tl7GxmG2X2fUZLr6i27uTLNRS4VchUajT5enmRKHJGHwmOOefcIbRyjs+82lrc7XzDuN5b2sMG425W5jjkvFtGkmhSO4Zo0LCQIPiQg601V6Oth5eudzub6Fp459rtkkZpIpQYzIIGmVY9Tx1ZgpUsOB41x0GfcextidQ5bPdgY3C5PcnR25+4qbM/G6bsGDf3WuU7i+OSZjIZan3FDgtwYqkzE+wsniqSLbtXnvvxk48hVwyRw65C0Yq2/fU33e7rlvZeZ4Lm+221kt94ltI4nEN9QIqvSR/AuA1Zfp2BGlWq1B0WPbxWOytuF/tciPc3CtYs8tKwgCRwUpqZWRlAkoK6lI45T/b/c3XcVTjqHrHa20qrYtRi9x7xpcDuXYU1JkupN2dq4yGmzHWOA38+6a/e3ZeB6NNDDBtXNZapWKqZ5KlsdHq8Ps2suWj4n1cu8X7bo6QQ3DrJoil+mJYuLejRxG4LHxSuXAAqDUkufcjEixm1h8Aa3So1MNeKFwQW0fhqMedcAMdNjt97L6zXdcOE2Nno8ntvctHWx7l3bishvPrHCYbc8O1txUOT62hz+OyGNwe88hu+lengyFHV1FXZ62CNYoWkWvhx7vvV7arfXtutq0byLbo0Udx4qq0Z8dlq7xGMqwjIABCPWp6ceY2VnGDaQu8taPIQ7R6aggKrUCuGBBYE1yOHST3hn9t47B9V0u0+p9xbEmNBV7gk7D7PyeWztT29R1OcMWB3BQY+px+N2nSbO2pNQz0MUuLinhnaI+R/NGSb7da7hJe7/AHO58xxXkVUiWxskRFs2VCZELBmmaWYMrFZCCvBRpPTEtzb+BZw21i0TgFjPMxJlBI0mmECpwqta+eR0IPb2ydsbUz3f9BvjT1Bv7rrHbEpth7A6xqsV3n1nv/c1ZNjBvaao7q25ubI7Yw2PTbFU2ZpKqkkyEFZV6qJdE0bj3TbBvVkeX9se6TcVmkm+su5ylvNChBaBVt11eIQxEbZBUDUcHDl/cWdzLe3NvafSIiJ4UKFpFYqKSN4jUpWlR5eQqeLxn+m949lfKYdG7S692H1jvDs2twrbB6t2DvVew9ibfrd2bLo9y7P2hi9753eGcjQZhpYY6mpzeajiw1XVOK+WCKB9Otm5t23f+XbfmnYIpZ9va4NuouA1m5MdybeZyLoRsFjIZlwTKoHhaiwq5cbVdWe4ybVfEJciPxD4YM4FY/EUUi1VrgE8ErVqAV6502UwfyF3n3bJi9gb9k3/AJnZmLzvV0G4O9KbcNPsMdcY/Ex9g1O/96b9x8OX7Npa7bmHnixNHHNTSUUk0ccLPDAvsP3st9yBtfKB3DfLIbDFePb7k8O3tG1wbpn+mW2t7YslsVkceIxqGALHuNOjawt15nu94js7Ob95tb+Pao86sqLCv6viyylS+ANIAJ/CAMMGjaFd0FtnF7Er87ujA9rVXbvWe88Dv/FZbZ3Z23JPh7vnIbup8TtPsCknwVbTt3vnMbsukly9JRUDRY0yV3gqlMsCMTrd4ua719wjsbeaw+gvYZrZ4pbaT96wohaW2YSClmkkhEbO1XAGpeJHRHa3FlGIGkZZVmiZZA6OPAY0CuNJrIVGQBQHgfI9Jymy9DkvjZuXH0mS6yxtdt7t3aVVu7Cbgy23pe7d7z7m25u6j2nlOq8bDs2HdmM6s2ThaGrTd8bZ96KbK5PFVC0quoIFKQ3a3k8rzIbQqpgVYyChWvia5C5D6jTSAq6QDXVWoQNLGUVQp8UEhzX4gaaaLTFBXVnPy6Tm/q3tncGN2n3bvvFZBMD2DJX7H2Vv6nwGE23gd0VHSuE2ltXM4bDw7XosVQPX7IxGXw9PkJ/t0llesjkmkmlld2bsNms9sshY2VuVsw7yaJHeTulZpX7pWdjqYlgtSAMKABTpya/luJ/HmestAupQFwo0jCgAUAAJoPmSeuewuvO2+7abKYvpzqLNb9qeqtpZndO+n64wFXk85Q7SWrrs3Wb133Tx1ksr4zB096VK6KCGnp6dIIJLzSRmQp3LeNi5cvIV33fxBLuUtLSO6aiFokVXjgIWi473VmJJLOKKrUVwwXl/btJaWQaK2ISV49IashZkLgtVj2kAqMAAHNKiXm995nA9I/FPBb2l6I7K6oq6Ltvcm19s7Fy2Mqu9dgYDc/ZmPp9/YHsbLUcX3fXW8srNgpa7Z6VkFdT09HXmraOYgJEgjsVvt75qawbcrPdopLcSTTJptJ2WFjGYgameAVAnFVbUoClQattLnwbayMiwS2zo+lRUyICw1V4BH/gORnNSMJfDbk232f2JL1F1LsrrPZux+yO8/uOvMj3TmcRHufYFHuGhqNn7Z212L8gZRQSU2w9t02RSvrFlj+xOUgSqcSOo1PX23Xm22I33dt1v3v7bbgk8VhmKXRIJneK0I0meTT4euoPhlh2g43abhG0rW0NjbPC8pKmcHUpZCgDSKdWhK6guRrAOekJhOwMt01vTIUuP291RvjefX2+VnpMluXG4/srbU+Q2ZLuPbddQYxjkH2Zuvr3d89f9xJLLSVSVq01DVU0kKgiVbf7VDzNtI8S7v7Xb7y20kW7G2lCy6JVJJUyxTx6acRTU6MGrhiC7exnOmKGS4ic/2g1qSNSngQCrVrUZwpBHQu5+foPe3Y+1eoekcP8AxWHF7K3Hgsf2luM7o633V8gex6+Co3Nt7P5/qxct2NT9c5+bKO208BgcXUVFFlatqR5JadJ1WnLN8fdNh2/ct9n3pjtcVxFNIphRxb2i0SYa9Sl1UHxZJWIKIjNQmtTPZTZ319Ft0m3mS7mieKFVlEZa4YVjJqKDI0heBJA9ABv7D6D2TgPiVhcxsHYHZkfyk6g3NRYn5Z5DPY3eO2sztLceQouzN2ZjZOP2HmM/jq/ZdD1LtDE4SlymahxFZi9xVOVp5I67HyQVEFSBovcLbrn3F2naU5msr7kvetnO47W1uuuIEXEFqqmdY3iuRNI7OhEqNGFdTG1A3RtZcv302w3t/DavFu9pceHKrOEYqIZJ2ZAXUqVjAwFOuoKtmnRNt7dV1+2ZcWcf2F1X2RiarrDr/tPcWf6t3ad3YnYlD2BTGpk2Vu3y4/E1kXZ2xTePcGGp0nko5/21kdzb3IMHM1nJIlvdbfe2l3Jez2FtDeQmNp3g/wBEjILL9PL/AKHIxAbjwz0S2+z3l1Be3ls0UtpbQJc3Do6kIjsVFRUEuv4lFSPtx0wZep6iI7MoI4O0t55Gt2lt/F9Vb2rdz4/BR4nf1JPixu/de6MPJiZ8rmNg5ekhrEwOOZoMrj4Jaf7tjPHJen03NvjcsyWVxtdnYR3ksm7WYgaRpbVlk8CK3dXVIrhJCjTPQo5DaRQ9NtNZTjcTdC6numjVbaZ5PhkGGZ9VWZCoogyVFAc5Biu4sl8Wst2Fszc2QpMHXdc574kbcp9ubL+KGJ291/u/rrvPbWzJtn7Kn+S2L3TSVG1q3sPLbqw0mV37UYKR2y1PVRT05WYuspLy7Fznb7Re2wd13ZN6kM8u7vJLFLaySeJILF1/U8FUZRbq+FypI/D65O3yXKsv+45gGlYAqsr0x4gqBqJrqIycGh/EaP4A712B1PtTYf8Aszvxp65ptjdo7rzW/Oifl1urZz5HeVRnvj7ubE5rfOwOrcLVY/cWE753VUbtix2CxW29x0C4orLNQF3iqJ1cCe60/MdvcbhvHt5u13dcyWL2kE+0xMGhtmuGLJdXKvJHBBamDU91IwlpHpkCKwDAQ8t/u92is97t4hZyLJIJZG0mXQNPhKyq8pcPiMLpJNV7uHVc4rNxdXd27kO/MDuDZW89v753zQbkxOQTc+xt39abgz8+cxk24JsZ1tkts7jw+4OuZM6MomHxU9PT1UtGuPVGpJjC0qTPt3OPKMF1t9xa7jtN7bQ3CPCILi1vEBSQxp46SQPDcFCgZ1OgHWNLKCA6rS7XuBAWWG4jkZR3MskdagNWMhtSK1e054ZB6V/YOx/jx1t8mdz9Zp3XuPuz41ba3RS0g7y6Mxu2v7+7+2PktsU9fTbn2Jt7dtdhtr0u4Tues+ylo6+pgipzTVEZmaeMOwjsPr2t7V9ztoY76n6scDNJEpB+FXdFLAJStV41oKU6LZSmlzA5Kn4S9AxqKVNMAlq0/wA/Q67i3D05VfI/YO5+kt75b4+bLqvi115N23uD45Z2ux1ftjflL0quE76wWGoclSdeu3968vRhNw7fov4imQNZVeEVzyuqxDti80w8ib3Zb/y9JuO7x8wXVvt0HMOmU3MDXuqzuHkjNxSIqxNvJJo8JVRWMaqpIwWHaJ98tWbclhsGs1luJbBQpiZYyXjVG0BnBVQ4XUWNWozVo+95Z7b/AGTv/qzcfyH+aG0u7d313cG58L2v3HsDa3ZfdWT2T1ZsHEbIwvXG4o+tt0SbL2B2htbPrhS9DR4qWkyFUizUWTnkhpo0jOOQ4fq7G8eLk7c9h2q7sIh9LuJjjulkk8VZg8sTvcRyxRsEWshCKEeNUJBYv3mRoLiMHc7e9mhmLCW3qYiAQylUICMGYVbt7iSGLDg1bhlyXyZ7A3T2Z8qe8N3bk3NtzeWwdkbv7C6m2dt7dHS+yfj9Tw4rEz7n2tu3AYyi2XhtsdR5veuMp4tuY6illWhqpViikneNwjtCeQ9l2rYOROV0O3fu+WS0tdzuZF3Ce9jDeFbyJPI00kt1Fbt+vI4GpVqwUEFQsVpurXV5u+6Om4fUojGCINbrbsQZJdaii+E7/AASRXiTXpAYHJ7H3xgn637h+QmO6+2Z8d9rdo0Px/quqOhc1uF+4d47jzObz09Zktx4ZNrbox+N7HzeNoFmzW7Zpaukw9ZS08dNAlNWAH5tLzb7v+sGycnPPu2+PavvK395GptY4Y1WNPCYyQs1qruAluAC6s5Z6x9FzSiSIWNzuYFramUWpijajl27mBADqsmkHv8AI0op1Hp62zlZ9ndV9R9v743z0D8iNsbboe2essT8Luwt67xzG+On8Hu+uycOR3LhtlY2mw0m16bLbmyL7pxGWwde8lJXJFVSwu0xjjbvtttty33f9j2nbd12bc7ma0v5+ZLCKOOO8ktlQxxzXBLCVVjH08kcg711JUAVasVxJb21tcTS29zCiSRpZzHUYxIaMyJTtJIDBxkYIzTTAoNgVXTlPtjtJe5ensxvTrrC9QdtYPZuRxi9h4Dce89y5n+NYXrF1aLJdcb33RgttU+PzW6sJOyxUyV746pjWammkD8fMqcw3U+yxcq7km23dxebfLckfTtHFAuh7kq2meOCWXXFbyAHWE8RSVcL06u1rb2U95JvVsLqCOKWOFtTGVpGI0IR2M6AB3GBQ0/pdGA7K29vTtLvztTcGX3N0dsDsXdnxe31v7dPX/XnatPsjZXUWUwggwG4fjhuk9u0lVQ47dGQx+ClrH2BtGsnpUiytDDh66mpoqiGIj2fb9o5S5L5PsoL263nbBusVwl7PbmW4kMsk0q3LLaJAPFhqAJ5FYkLWUSSMvSm6vLrcd13GXwVs5zamBoUkOgBUjQx6pS50vSpVSMntKqD1m3B1/vob9+DXxg+RPbWLznVO2N8f6PJ8RsyfZxofj/gN7dpbfzfc3X9J3FK+J2ju/LLTZiOtFZPn6mgwP3SwxyUqhY3Kds5z5eveWPdT3G5O2K5hu2sW3BZpYpjNf8Ag20q2t0NtIM8fdGwEZhV5ytTrqSDC/2C8sL3lraNxv4ZS7+E8cbDRbtrTxIGuB2P2kVZWIQEAUoAS9d67b6nwXZuSoOkdzLm9nZjcG7vsNoNQ5xKvqFk7P3ftna3VOT3nn6yrxvaWQx2zMXicjLufFVdRhqv+JiNZ3kgmkMm8tS7lc8s8t3O8XJn3eXb7aW6maMQGSZ4EaVzDpXwCzk1j0ro4UFKdBncFgTcNxitohHbpcSJGisXCqrEABySZAAMNU6hmp6Wfy72ruHqLsij+OO7u1dvdw574u4TIdRHsLYW78Juzp8bcbI/3y2/trrCsocBh8jiKfZsWfno9xU2VqMpUxbhjqUWp8EKL7KuT9rt7c8w7zbctna7jeb8395aSK31LXaqIJ5bhhLLFKZTGpheDRG0WkhdTEl/cruWVNvtZb3x0tYPBjkFNAiJ1oidqsugGjB6tqxWgA6VfdWyNq7cwnxg7P2Fs3bO4k378Y5aDee0+tG3ttjNdd9+9YYp8PvHeu/NtPlM32JQ772fVVuP3Rnqyrp6PZmbneP7bRQGZEJdj5ufmjdefuWNxiFg+1bnbwxvKiyQ31hcgtC0czk20ovVV4tMTmaLIKK4FTG+20bVa8ubtZPK73EDO3cFeG5iKliEj/VQREhv1FAJHEqa9IfpzrrYfY+/PjTisXnP9L3ZHY/a24Ye5+g9856b4/7GpNp7by1NnMZTR/JrL5OfBwVncmy6PJLUZCkpo67CViQ04Wad4Fc73rctw2nbeaS1qu37TaWUS7budui3cniSL4ebEBSFtJmWiu3hutXJC6iCyFVu7q2dpGnu5pWe4ikLIDksT4uatIoJJHdqNONKh3umk6NOe3bl9mb13fg56b5A5Ch69xEeyMjmdr7d+Pk2Tramj33/AHkzeVpt6ZfemzHWmpIcNPEKrM0tMah5llmBF7WbnJjZWG57HZzbRJseu9na5CTybnhTa+AiGFbaeMs7TA6Y3OkCgp1b/dbCrXVrfTJuKXw8BRHVFgHcJtZOsyowoEPxAV88M+3dhdgdydjYjbGyKKv37uXsvsqj682dmq9aDadHvPde4MkuK2suRrs/W0WE2nVbgpvBM0VdVRx0Ik8UkpZLsuk3PYuWdpKXcsNlb2VibuW2QmVoIEGqQqqBnlWNqjUoOqmoChxaaLd93mn3WaOa4M9x4TXTLRXlI7QxoFVmUA6fLA6VP+j3v77T7nw5D7P/AEi/7Kt5f747T0/36/jP8I/uDf8Ajnk/hH8d/Y/jn/Fp1cff6PZX9VyR4vh+HB43hf1g0+FL8Ph6/qaaKeJ4Xd4Xx07vDr0q+s5k8LxPrJ/B8H92atQp4PiaPBr/AL78Xt1cK41Ux0Gs/wDeD/SBvX+E/Zf33/vJvP8AvF/o++1+x+5/jOX/ALw/3f8A7v8A+S/3L8/n/h3g/wAk/h/i8Xo0ez6b91fuTb/3ho/cXhw+B9b8Pwp4OrxP9EpTj3VrXz6R2P73/eV1+7vH/e9ZfE+m1a+J8X4M6eNaYp+XQt4P/ZR/9BWE/j/+nb/ZnP7/AO1v47/Cv4L/AKEv9FP8cg/vp9pb/c7/AHi/uzr/AId4f8r+8vq9Oj2Etw/12/67Tfu79xf63H0dxo8XxP3j9V4X+K/8L0fUf2mr9PR869GMf9Uf3Nt9frv37rX6nh4OnxE16KZ0eDrp/omunl0w7L/2Xv8Avuf9I394/wDQr/p1pf7wf6Nf4F/s13+gnTnfs/7h/wB//wDfkfa/wj7Tzfx3j+PePyejV7Etn++PH2b6/wAb6n92L9X4en6L6msfi005+o16/D09ng6vOnRXP9H4V99L4Wj6s+Bqr9R4Pdo4/wCg6aaq93iU6WvVn+l3/ZSfmX9l/dD/AGW/X1P/AH//ANIX8T/h3+lz+9sf+jj/AES/b/7g/wDT/wD3T+88v3/+Tf3d+5/Pg9hLmv8AdX+uN7Saf3t/Wb6y68D916PC+n+mk1/vavd+7/E/s9Hd9RSmNXS3b/E/cnNWv6P6TwY9f1Xx6vEWn0vl49Kaq/gp0x9xf6YPuq7/AGZz+F/6Q/8AZdOi/wDRJ/e238e/0Tfx2l/0f/6O/wDRh/vxfJ/c773y/wAd/Z/hP3Hh/wAs+z915J/qX4Nx/ra+J+5f6xbl+9vA16P3jp/xzx/rP1/7fRTwceJp/Br6d3f97eNF/WCn1n0Fv9Lq018Cp8HT4XZXTWuvNK1zTpJUH+if/Rwft/8ARf8A3z8PTn8cv95/Ev4l/fzfn96v7w/3r/3Pf3l/hH8O/vb/AHL/ANwn92/4dq/yr7n2a3/9Zf3tJ4X1v7t/x3R4enVTwIPC8Hwv0tOrX9P9V+p4+v8ABp6rt37o8OH6jwvq/Ft/7X+w0+I3iePX9WmmnieFjRTzr0C+3/J/feL+Cf3U/jX8Wm+1/jP3f92fvPBkf4J/FP4d/ua/ht7fw/T+/wCXw6eb+xBu2r+rsv1f130304r9Pp+opVPE8PV+nrr/AGv4dOv5dJbTT++V+m+k8Txmp4urwPx6dVO/R/vvzrp+fS8qv7n/AN49vf6L9X+i3/Tfsb+D/wAa/ul/swX99P7obE/0h6/4V/xlP+738T+8/h3i/wBxH8Q+30/7ltXtIv7y+nuv35/yXf3ZNr8PxfoPB8ab6emr/FtenTqr36NX+hdMjwvET6X/AHG8daaqeNq0prrTv41p5Vp+LqbQf6RP77d8/wCy4/3v/gn998199/d/y/6Rv7v/AN8Nz/3L8/3H/GW/45/DfP8Axz+E/wC5D7P7r+Mf5H5faaX90fu3lb+uX0/1f0yafFp9P4nhR+PSn+K6NdPD8Ts1afB76dWHjeLffu/Xo8Q/D8dNTaa/6JWnxUzSurFeg5b/AET/AMP2z/df/SHb+91R/eX+Lf3I/h3+jz/frfb/AN2P7v8AH99/u/7wefz/AO47w/wzR+7957PIv3z9XP8AvP6bwPCTR4PjeJ4lZNerxceH4fhaPxavEr26Okx+m8JPpdVamurTp00FKafOta+VKUzXobe5P9lu/uNkv9Avl0f7M927/c3/AEg/3y/2Yn/ZbP7s7S/0S/6WP4f/AM4/+H+J/f8A/Fh/3P8A8W+6+6/yD7T2txX5Z/1Y/wBX8umu/UK1pTNKUr+eemHfP+jr+9O2P9lh/v3/AH8/vn3L4f7o/wCkv77+6/8AEYP9E/8Ao+/iX+//APN/o8/iv8Xt/uS8Gr77+17CW2/vf6G9/rr9L+6/p7T/AHI+m0+LpP1Xj6f0P7fR4f4K/B0YzeDri/d2vx9cnw6+FezRXurorXzpx6Cnbv8AEP7n7Z/g39xf7x/6UqP+AfwH7r/Th/Fv4Pjf7tfwn+H/AORf6J/v/B/DvB/lf97Nej0afZ3d+D+8b/6n6n6P6E+L4tPo9GpvE16s/VUrrr2/T0rmvSSLV4UWjRr8Uaaf2ladtKf6HWlPPX0Ke9v4f/onT+Jfef6ef9LXZX+zDfxHz/x7+B/3lx39zP8ASV/en/c5/pU/0pf3g1/wT/JP4R4v4r/l+v2HLKn9ZbXTT+rn7vi/cmivh6/BP1H0/hfp/TfSeDTxu7xNXgdlOjJvG/dt54f9r4o+trprTWfC1au/X4uqujGmniZ6Ej4L/wCjX/Tht3/S/wD6S/7r/dZH+4f+h/8Aul/fX/T1/A5/9G/8V/vL/lX+jL+G/wAT/jf2f7lvFo/dt7JPdL94/wBXd0/cP0/77+jbX9b4vgfS+Ini/D+n43iaNGrupWnbXo25Y0fUWX7yp/V/6+L6jRp8XXoamj/RtPh6q6ezVTVnoDpP4/8A6UsB/db/AER/wf8AuGf7h/d/6Kv7vf6P/wC7m5v4N/fv+J/78b/Sn/o8v9x/Hf8Afz/3n+383+5P7b2KovA/cE/7x/eH1f1I+r0/VeJ9Rrj1+Dp/W+l+o4eF+j4GrT+lq6IJv9zx9P4X0tG8Guj+z7tOuvb4nh0rq7tdK91OhQ6c/wBml/0ldW/6Ff8ASz/eb/Rv2D/svX+kDxeX/RD/AHW3N/ej/Rz/AH8/35f8V/u1999n/d//ACv+JeP+H/5T4fYL5w/1p/6r80/1w/df7r/e1n/WH91a/wDkqePB4H1f0X+NV8bw9fj48Ovjdmro32n+s/7y2z90/U/U/Szfu/6ulPpdD6/D8b9KmjVTR+L4c06SnUn+jb/Qb2N/FP4V/s0X+lr44f7L15v77av4N/H99/6U7/ff8Yh+2+4/u3/Ev76f5Vrv9j6Pv/crbx9J9Nuf1tf3Z9PN9TTVq8Pwzr0+F+pXTq0+F3cNGadBey+o8e0+n/3I8VPC4U1ahprr7aVpXVjjXFen3o7/AEaf6Vuu/wDTz/ok/wBH/wDsw/8AxmX+9X9/f7wf3T/h1R/ez7//AEVfv/6Iv4tr+3/g/wDlH8a1eP8AyLT7jjn/APrZ/U7mP/W6/e/9Zf6vj9zfTfS+D43iL4On67H13h/F4uPA/wCG9Hm1fu/94Qfvr6X6X66T6rXr8anhtqp4fZ9P4nw0x4nH9Ppm+RH+iD/TJvn/AEE/w7/Rx/GG/u5/db+8f9yP4TopvB/AP73f7+vx/d69f3n+TW8fh9V/Zz7ef1t/qltP9evE/rBoPi/U+D9RWp/tPA/Rrop8Pfx1dO84f1f/AH9c/wBVdH7q8NK+B4nha6DVo8Tu06v9pw0dKHaP+zLf7Kx3t/dL++/+yV/6VOmf9mV/gn92v7m/6Tr5X/Q7/eD+Jf7+H+If577f7b/cV5/tfv8A1/a+xBcfQ/vW106f6xeC30urxaUpJp16Oyv9ro1fqU8Xwvx9B4afDH1Pifu7WPG0aa8U1adWNVNPy+HVinRgPjl/GP7y/H7/AEOf3w/2dH7Cm/2WH/Sv/Av9lu/uh5+4f9LX99f9mI/4xt/Cv9H/ANv/AAr+7v8Av3vu76f9yPuJt4/ef715o8X91/62njy/1h+h0/vT6nwbP6Twfof1NXj+J431n6+n+hp6FB/dn7v22n1f9YvCX6Hx9f0/heJL4mvxe3+z0aPA/T1Up3V6QHwE/i/+zUdJ/wBy/wC6X+lT/TVi/wCBf3o/in8I/g391uxf7+fc/wAN/wB+5/AfttH3Gj/LLfb/AMN483s694fF/wBbvmzV9T+7P3UdP0/h+J4ni2/gafGzr4019vxeJmnSXlbwf35tXjaPE+rFfE16dOmTXXR+Gv8ADnhpx0Wff3+hz/R707/dT+/n+zD/AHXYn+zI/wB9fJ/AP4z/AH1f/Rd/dD7/AP3Jfd/3Jv8AxDy8fcf5z8+5Bsf6yfvvmP8Ae30/9WNMH7r8L+1p4I+p8WmKeL8PnTh0HW+h+ltfptf7x1N4+r4PiOilfPT+XrnpSb0/v5/eel/2Zn/ST5v9H1f/AKKP4p5/7u/Z/wASrP4N/cvx/wC4X/RR/HPvfL/d/wDyP7/z/wC7Nfsq5Y/q3+5h/Uf6f6HxP8Y8Kvja9P8Ao/ifq/U/D/b9+inl0v3P6394H98a/qKD46aKVzo0dvhU/gxWvQtdkf7L/wD7LT1f/dT/AE0f7MV/o/6Kv/eT++P+jz+6P96fkp/pk/uf/eL/AH7P93P4j/dL+C/w7/cT9z/GPtf8o+69l/JX70+u9w/6x/u/6f8ArBN+6fpPA1eB9Na0+p8Hv+p169Xi/radGvt0dX3j6PwOX/3X4/jfQJ9Z4munieLJXwtfb4enTTT2VrpzXoUPlF95/pC+QX2f+yu/6c/9M+3f4r/srn9+ftP7v/6GcP8A3h/up/e7/fnf6JfuPuv70+b/AH8P9+PH/wAolvYD5S+h/dXJn1X71/1vv3WfC/fn0/h+J9a/hV8D9b6v+z8D/QPpdVO+vQt/3a/vPd/3ZX+ufjtX6HV4mjwE8TV4nb4OnX4lP1PEpXFOiE1n8P8A7v7d8f8AAfJ5c59z9t5v49p+4g+2/j+v9n7f7fV9jo5+316/z7mm18f967tq+q0aYdHiafA+E1+np3VrTxK/jpp6Bs/gfuraqfS+Jqm1eHq8f4hp+or26aV8On4K6uoj/YXn8P8AFLeeP7L7z7DV9pqfy/xX7bj+IW0aPt/2b6r8afatfH/S8TwqaT4mnV8WKaK/h411Z4U8+i/9LS9PE1VGmumlPPVT8XpTHGvl0bbq37b7T4d/7Nz5/wDZIv8ASp2z/D/7mf6OP9In93v707G/2YjX/dL/AIyf915/4b/CP7zfsadf8H9H3nsq5i/fH7ovv6vf8lmkfh001+IV0eJ+nr8PVp1duqmvFen9u+j+rj+tp9N3V1aqVz8Wnu06qVpmladWOZ//AEl/6E/5if8Aot/uR/sk39xex/8AZYP7+f6LP9LX2n2/Qn95f4N/ov8A9/f/AHl/2Wn+B/xT+8n+4nyeb/l9fee8a7z+oX9aPab+sH1P9df33Fr1fWafE8e9+i8Wv+L+J9T4nwfp116f0vC6HUX7++j5s/dun91fQNr0eHTw9Efj6a9+jTp49/w6s6uiEbW/4cO/2SR/7gf6V/8AZDP9J+8v73f6Lv4D/Bf70eXr/wD0o/6Q/wC5X/GXP7rfZfwnyfxL/cH59Xg583uUN5/1mP8AXN2r9/fu3/Xc+mP7q+v1+L/ZS+H9L4v+LeLp1V09+j4vLoPwf1p/ct59H439W9afV/TadFNa/Ho/U+LjT8Va46QvZv8AsjH8C+Xn9wP9Iv8Af/8A037K/wBk4/uf/eD/AEP/AOgj7vL/AOkP/SN/pI/4yN9z/Avtf4D/ABD/AHNfcaPJ+15vYu5O/rx/Vbkv+tvh/wBZvAT99eN4PieL4Umrw/pP8V8Tx/D1eH+np16c06Ld5/c3713j90av3X4h+jpr06Kr8Xi/q00aqau6tK46TMmv/Sp8Wf8AZ0/4x/oN/uV019//AHF/uf8A3r/2Ub+P1un+Gf3O9f8AeT+DfxC/8T/3P2t5PX4vZRsf7j/dHuP/AK1mn9+/vm++s+o+o0fvnTH49PqsaPg0+F/i1fhxq6W7l+8PG2H+stfpf3fD4Hh+HX6Tv8Gvh/OurV+rSv4tPRku0/7v/wCyV7d/0f8A8P8A9lI/2eD54/7L7/fb+8P+kj+M/wCjjq3/AEW/3r/gfr/vD/o8+y+28n+4n+J/cfxP9vw+wrsP73/10tz/AHx4n9af6s7J9f8AT+B9P/uRdfV+HXv0eL8Vc6NPg519Kp/oP6v23039j9ddeFq16tOhfBrTt1Ur+fxeXQYdd/xT/Zadm/6bv4p/ssf+lPtz/QP/AKHv9Gn+l/8A2c/+7e0f4J/pF+0/4zJ/or/g+rR4fVrv/Dv3/B7PObf3x++bj+pH0X9Y62v76/fHi/S/ufv+p+m/0D6vTp0eJ+j8Wv8A0TpPs/7s0L+/vG+g0SfR/S08T6vUPD8T8XhV1V09/DT+HqD1b/s1v+mr5R/7KV/pe/v7/oc+R/8Asw32Wv8AvH/spn3dF/pQ/vp/pb/3+v8ABP4N/D/vP4v/AL+L737X7X/K9Hs52v8Ac/8AVPlT95/R/ujw7X6P6TT4Xj+C2vT9F/inh/HXwv0NGvX29Nbj/wAlW7+l+q+v8aTX4ldWjX+lTxv160pXxO+tKdEpp/sdFN/wN/hHih1/wb7f7v7Ow8f233/+QeTVp0fcft/8hW9jZvEo2nR9RXHi1pX507uFa6c/l0UmmjGrw/PR6Y/KnClcfn0ertz/AGVH/Rt8WP8AQn/oF/0kfwfsj/Zgf7w/6dLeb+7lN/c7/SJ/eH/fs/xH+J/d/wAK/g3+UfxX7f7n/JNPuAuUP9dv+tPuX/Xf9+/1YpZ/uL6b926tf1D/AFH03hfq6PC8PxPE7fC16f1OpF5j/qdTY/6s/Q18M/U+L9Ror4Tf2mvv8TxOFfxaNPbq6Brp7/R3/drcn+nr7D+7P+y0/Iv/AGW773+PfxP/AGYH7vE/3S+//wBFX+5/+L/3y+4+2/vn/v17X8/+R6Pc1wfu/wDe+/fS1/eOuD62ni6P7M+Do1/pU8Lj4Pn/AGnf0BJPrPodt1f7jUk8H4NXx/qaqd1dfDX/ALXt6asR/sxX+y+4/wCz/i/+gr/Zi4v7qfwP7D+M/wCnj+50v2f9xvt/+Mj/AH/90tH8S/gv+4z77wfc/wCVeL2ELr/W8/1xZvqdP9fv6tv4/jeL4P7p+pGvx9X+I0+o+Hxf1dGrT+nXo3t/37/V0eH/AMkP94jTp0a/qvDOnT/o/wAHHT2aqfi6Yezf9I393t1/3y/iH98P9Jtf/pO/0mfwf/Tj/pg/gFT/ABn+Ifdf8Zv/ALlf3Y8d/v8A/IP7w31f5Z4vZxyx/Vyu0/1e+m/q/wDQL+6v3Vq/d30OseH4fh/4h4vi1p4efC4durpJuX12q7+v8b94+Mfq/qv7bxqHVWv62nTT4s6/nTo4O8/7g/7LEv8AFP4n/syn+mbdX8E/0ff6KP8AZXP4b/c3a/8Apa8f93v9wH97f9E/90P4d/A/2f4t9/5v8t83sBWH1v8AXC+8bV/U76Kz8L6j6r94avHn8LxNX6/h/V+L8ePDpX9PT0J18L907f8Auvw/6w6rz6vVo8Hw/Djp4er9HX4P8Pdq4d1eiyfH/wDuV/pU2f8A6Tvu/wDQ/wDxLH/6Xftf4f5f9Hv8RoPvPuf4j/l/8H/jX2H8V/hn+53+E/dfw/8AyrR7HfOX1n7kuP3VT+ser/dXXXT6rQ+mnh9urw/E0eL+jr0eJ29Bratf1D6q/Q+F/jXw/wBjVdXx5+LTXT36a6c9ZcP/AHz/AI/1v/e7+4/91P4d2R/ou/01f3o/2Xn+638Q35/Gv7tfff7lf7n/AN9fvv4No/d/vV9p95+/9x7fn/d/0u8fu76r6/XbfXfu3w/r/F0waPE09vjeDp8Ty8DXo7dPTC+PqtvG8PwqP4fjV8HT3V01zp1fD569Nc16TvWvh+86+/0rf39/0Cf6XsJ/ev7b+P8A2f23+4H+/wB/CvsP9xH+l7/Rfby/Z/7mPtvt/wDdHh9r96r4e6/uP6X+tf7vfwK6K17/AANWrv8ApPqeGr9Our8WrpiHTW3+p8T6Hxhr4/LVSmPF8PjTup8qdD11T/svH+n/AKJ/vR/cj/Q7/C3/ANL/APpO/wBO39yP414+w9H99P8ARt/xlrR9t/ANX9zv8k+78en9v+Ie9bX+9PBv/wB708b6g+BTw/7LRHSnh4p4mumvvpxxp69c+B+j9NXTpGrj8VWr8Xyp8OPTz6QtR/sv/l6B/h/+m37P+4OP/wBmov8A3H/jf+k/+9G5f4r/ALL/APd/7hv7o/3J/gvg/j/738U+81/t+P2pvvrvpLz91+B+8dJ+n+q1+FqrjxfD/U0eunu9Om4NGuL6nV4NR4nh01U/o6sV9K46wbb/ANIf+j/eX+j/APvn/oq/u9Uf6V/4r/Af7jf3pvtT+/X8C+7/ANwv8f8Auv4R9n/Dv9/1/Bf89/kX3ftBd/ur97bb+9vpf394w+g0a/H8L9TwNdO/RTxNWv8AxXxPh79PTsP1H08303ifS6T4/DRq7ddPKtdNKfqaflXpS0P2H2Hxw/0f/wAF/jH91uzfu/8ASX/A/wDRf/e3+92/Puf7uf6Uv+Mb/b/3B+z/AOA37H94tHj/ANy2j2y/i+Lzj+9/F+k8e20fRa/qfC8KH+0+l/xiv1Gr4u7wq1/R6cHh6dr+n069ElfEp4ddT/Dr/Tpo9Mav6dOkjuT+5H9y9l/3G0f3I/u7gPv/AO8X3P8Aeb+/39xdv/6X/t/uf9xf+i3++33H8K0f5R/yt/uX9qrL96/1i3n96+L+9qnT4WnwPB+ol+k4fqfW+DTxK4000Y63L9N+57LwPB+k1fir4urw08ate36bV8NM6q16WOwP7ifwfO/3o/uf9v8A6J+x/stf8H/jn8Z/iW3f7u/w7+8P7P8AfnTf+B/wf/cn/Cv4h4/V7K94/f37yi/d31en942via9Xg6NEni6fC7vB/wB/+N+n4nh1x0Ywfuj932/1fg6/p7jT9PTxtepfC8bX28K+F4fdo1efTNuD/R75O9/4d/ox/u39lWf6OP4L/pP/ALufZ/37wPh/0Ofxj/c54v7tfc+P++v/AC5fufJ/uS+29mdj++Kcp1+s+r1D6vX9Nrr4L/7l6P0/7Sn+43+iaafp6uimb6XTuNPC8Kh8OmulNS/2dc8P4/w186dHfx3+zz/6U/nN/eD7D/Zpf9lTpv8ASr/E/wCFf6eP9BPk2j/ez/Q9/oz/ANw/8T/0Y/b/AMf/AIjz/drXb93x+4Psv9af+r3sV/VH94f62v8AWC5/d30Xjfu36rRcf8lX639b6b6rX4WnHj0r29DG7/rF9dzr++vpf6xfRReP43h/UaNUen6TwezxdGnVX8NPPolO3f8AQh/cDaur73/Sb9129/f7/Sd/dz/Zcv8AR5/c3Ef6Iv7jfwX/AH/X+lb+M/xjz/xL/cN/EP4L9t6fu/c7bz9Z9Ov031n1Hjw1+ip9R/apq+Pt8KlfG/F4OvT3U6B1j4HiP43geD4b0+o/svganDOv/fflr01xXpZdNf7KB/Gdm/7MV/p4/ur/AKNN9f34/wBE/wBl/eL/AEwf3ib/AEXeL+M/5L/cb+6Gn+Lfw39z7u351+whzZ/rs+BuP9Qv3J9Z+8rf6b9510fu/wAA/WU0Z+p+pp4Xi48OtPLo32r+qnibd++/q/A8FvqvArq8Xxl00/o/T6vgx4mnVivQF5rX9luH+Gfx/wD0X/3kq/4Z/HtP2visP4X/AHk+3/3Bf3j+xt5vF+39NPsXWWj6jbvrvpP62/SL4vgfFSv6ng6v1vA18K56SXfjfTXv0P1X9V/qv0/G+DVp7fE0/p+Np9PLpVf7n/8ARx/zSz+7X+hn/s1f79/6Ov8AZrP/AD6/37/0tf8AkQ/0cf8AVu93/wAT/ef/ABI+t+v/AKej6j6D9mj6T/a+L/S6Sf419L/y7eD8v7P6j/rf1//Z">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="7715250"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4098" name="AutoShape 2" descr="data:image/jpg;base64,/9j/4AAQSkZJRgABAgEASABIAAD/7QAsUGhvdG9zaG9wIDMuMAA4QklNA+0AAAAAABAASAAAAAEAAQBIAAAAAQAB/+IMWElDQ19QUk9GSUxFAAEBAAAMSExpbm8CEAAAbW50clJHQiBYWVogB84AAgAJAAYAMQAAYWNzcE1TRlQAAAAASUVDIHNSR0IAAAAAAAAAAAAAAAAAAPbWAAEAAAAA0y1IUCAgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAARY3BydAAAAVAAAAAzZGVzYwAAAYQAAABsd3RwdAAAAfAAAAAUYmtwdAAAAgQAAAAUclhZWgAAAhgAAAAUZ1hZWgAAAiwAAAAUYlhZWgAAAkAAAAAUZG1uZAAAAlQAAABwZG1kZAAAAsQAAACIdnVlZAAAA0wAAACGdmlldwAAA9QAAAAkbHVtaQAAA/gAAAAUbWVhcwAABAwAAAAkdGVjaAAABDAAAAAMclRSQwAABDwAAAgMZ1RSQwAABDwAAAgMYlRSQwAABDwAAAgMdGV4dAAAAABDb3B5cmlnaHQgKGMpIDE5OTggSGV3bGV0dC1QYWNrYXJkIENvbXBhbnkAAGRlc2MAAAAAAAAAEnNSR0IgSUVDNjE5NjYtMi4xAAAAAAAAAAAAAAASc1JHQiBJRUM2MTk2Ni0yLjEAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFhZWiAAAAAAAADzUQABAAAAARbMWFlaIAAAAAAAAAAAAAAAAAAAAABYWVogAAAAAAAAb6IAADj1AAADkFhZWiAAAAAAAABimQAAt4UAABjaWFlaIAAAAAAAACSgAAAPhAAAts9kZXNjAAAAAAAAABZJRUMgaHR0cDovL3d3dy5pZWMuY2gAAAAAAAAAAAAAABZJRUMgaHR0cDovL3d3dy5pZWMuY2gAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZGVzYwAAAAAAAAAuSUVDIDYxOTY2LTIuMSBEZWZhdWx0IFJHQiBjb2xvdXIgc3BhY2UgLSBzUkdCAAAAAAAAAAAAAAAuSUVDIDYxOTY2LTIuMSBEZWZhdWx0IFJHQiBjb2xvdXIgc3BhY2UgLSBzUkdCAAAAAAAAAAAAAAAAAAAAAAAAAAAAAGRlc2MAAAAAAAAALFJlZmVyZW5jZSBWaWV3aW5nIENvbmRpdGlvbiBpbiBJRUM2MTk2Ni0yLjEAAAAAAAAAAAAAACxSZWZlcmVuY2UgVmlld2luZyBDb25kaXRpb24gaW4gSUVDNjE5NjYtMi4xAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAB2aWV3AAAAAAATpP4AFF8uABDPFAAD7cwABBMLAANcngAAAAFYWVogAAAAAABMCVYAUAAAAFcf521lYXMAAAAAAAAAAQAAAAAAAAAAAAAAAAAAAAAAAAKPAAAAAnNpZyAAAAAAQ1JUIGN1cnYAAAAAAAAEAAAAAAUACgAPABQAGQAeACMAKAAtADIANwA7AEAARQBKAE8AVABZAF4AYwBoAG0AcgB3AHwAgQCGAIsAkACVAJoAnwCkAKkArgCyALcAvADBAMYAywDQANUA2wDgAOUA6wDwAPYA+wEBAQcBDQETARkBHwElASsBMgE4AT4BRQFMAVIBWQFgAWcBbgF1AXwBgwGLAZIBmgGhAakBsQG5AcEByQHRAdkB4QHpAfIB+gIDAgwCFAIdAiYCLwI4AkECSwJUAl0CZwJxAnoChAKOApgCogKsArYCwQLLAtUC4ALrAvUDAAMLAxYDIQMtAzgDQwNPA1oDZgNyA34DigOWA6IDrgO6A8cD0wPgA+wD+QQGBBMEIAQtBDsESARVBGMEcQR+BIwEmgSoBLYExATTBOEE8AT+BQ0FHAUrBToFSQVYBWcFdwWGBZYFpgW1BcUF1QXlBfYGBgYWBicGNwZIBlkGagZ7BowGnQavBsAG0QbjBvUHBwcZBysHPQdPB2EHdAeGB5kHrAe/B9IH5Qf4CAsIHwgyCEYIWghuCIIIlgiqCL4I0gjnCPsJEAklCToJTwlkCXkJjwmkCboJzwnlCfsKEQonCj0KVApqCoEKmAquCsUK3ArzCwsLIgs5C1ELaQuAC5gLsAvIC+EL+QwSDCoMQwxcDHUMjgynDMAM2QzzDQ0NJg1ADVoNdA2ODakNww3eDfgOEw4uDkkOZA5/DpsOtg7SDu4PCQ8lD0EPXg96D5YPsw/PD+wQCRAmEEMQYRB+EJsQuRDXEPURExExEU8RbRGMEaoRyRHoEgcSJhJFEmQShBKjEsMS4xMDEyMTQxNjE4MTpBPFE+UUBhQnFEkUahSLFK0UzhTwFRIVNBVWFXgVmxW9FeAWAxYmFkkWbBaPFrIW1hb6Fx0XQRdlF4kXrhfSF/cYGxhAGGUYihivGNUY+hkgGUUZaxmRGbcZ3RoEGioaURp3Gp4axRrsGxQbOxtjG4obshvaHAIcKhxSHHscoxzMHPUdHh1HHXAdmR3DHeweFh5AHmoelB6+HukfEx8+H2kflB+/H+ogFSBBIGwgmCDEIPAhHCFIIXUhoSHOIfsiJyJVIoIiryLdIwojOCNmI5QjwiPwJB8kTSR8JKsk2iUJJTglaCWXJccl9yYnJlcmhya3JugnGCdJJ3onqyfcKA0oPyhxKKIo1CkGKTgpaymdKdAqAio1KmgqmyrPKwIrNitpK50r0SwFLDksbiyiLNctDC1BLXYtqy3hLhYuTC6CLrcu7i8kL1ovkS/HL/4wNTBsMKQw2zESMUoxgjG6MfIyKjJjMpsy1DMNM0YzfzO4M/E0KzRlNJ402DUTNU01hzXCNf02NzZyNq426TckN2A3nDfXOBQ4UDiMOMg5BTlCOX85vDn5OjY6dDqyOu87LTtrO6o76DwnPGU8pDzjPSI9YT2hPeA+ID5gPqA+4D8hP2E/oj/iQCNAZECmQOdBKUFqQaxB7kIwQnJCtUL3QzpDfUPARANER0SKRM5FEkVVRZpF3kYiRmdGq0bwRzVHe0fASAVIS0iRSNdJHUljSalJ8Eo3Sn1KxEsMS1NLmkviTCpMcky6TQJNSk2TTdxOJU5uTrdPAE9JT5NP3VAnUHFQu1EGUVBRm1HmUjFSfFLHUxNTX1OqU/ZUQlSPVNtVKFV1VcJWD1ZcVqlW91dEV5JX4FgvWH1Yy1kaWWlZuFoHWlZaplr1W0VblVvlXDVchlzWXSddeF3JXhpebF69Xw9fYV+zYAVgV2CqYPxhT2GiYfViSWKcYvBjQ2OXY+tkQGSUZOllPWWSZedmPWaSZuhnPWeTZ+loP2iWaOxpQ2maafFqSGqfavdrT2una/9sV2yvbQhtYG25bhJua27Ebx5veG/RcCtwhnDgcTpxlXHwcktypnMBc11zuHQUdHB0zHUodYV14XY+dpt2+HdWd7N4EXhueMx5KnmJeed6RnqlewR7Y3vCfCF8gXzhfUF9oX4BfmJ+wn8jf4R/5YBHgKiBCoFrgc2CMIKSgvSDV4O6hB2EgITjhUeFq4YOhnKG14c7h5+IBIhpiM6JM4mZif6KZIrKizCLlov8jGOMyo0xjZiN/45mjs6PNo+ekAaQbpDWkT+RqJIRknqS45NNk7aUIJSKlPSVX5XJljSWn5cKl3WX4JhMmLiZJJmQmfyaaJrVm0Kbr5wcnImc951kndKeQJ6unx2fi5/6oGmg2KFHobaiJqKWowajdqPmpFakx6U4pammGqaLpv2nbqfgqFKoxKk3qamqHKqPqwKrdavprFys0K1ErbiuLa6hrxavi7AAsHWw6rFgsdayS7LCszizrrQltJy1E7WKtgG2ebbwt2i34LhZuNG5SrnCuju6tbsuu6e8IbybvRW9j74KvoS+/796v/XAcMDswWfB48JfwtvDWMPUxFHEzsVLxcjGRsbDx0HHv8g9yLzJOsm5yjjKt8s2y7bMNcy1zTXNtc42zrbPN8+40DnQutE80b7SP9LB00TTxtRJ1MvVTtXR1lXW2Ndc1+DYZNjo2WzZ8dp22vvbgNwF3IrdEN2W3hzeot8p36/gNuC94UThzOJT4tvjY+Pr5HPk/OWE5g3mlucf56noMui86Ubp0Opb6uXrcOv77IbtEe2c7ijutO9A78zwWPDl8XLx//KM8xnzp/Q09ML1UPXe9m32+/eK+Bn4qPk4+cf6V/rn+3f8B/yY/Sn9uv5L/tz/bf///+4AE0Fkb2JlAGQAAAAAAQUAAklE/9sAhAABAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAgICAgICAgICAgIDAwMDAwMDAwMDAQEBAQEBAQEBAQECAgECAgMCAgICAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwMEBAQEBAQEBAQEBAQEBAQEBAQEBAT/wAARCAEEAcsDAREAAhEBAxEB/8QBogAAAAYCAwEAAAAAAAAAAAAABwgGBQQJAwoCAQALAQAABgMBAQEAAAAAAAAAAAAGBQQDBwIIAQkACgsQAAIBAwQBAwMCAwMDAgYJdQECAwQRBRIGIQcTIgAIMRRBMiMVCVFCFmEkMxdScYEYYpElQ6Gx8CY0cgoZwdE1J+FTNoLxkqJEVHNFRjdHYyhVVlcassLS4vJkg3SThGWjs8PT4yk4ZvN1Kjk6SElKWFlaZ2hpanZ3eHl6hYaHiImKlJWWl5iZmqSlpqeoqaq0tba3uLm6xMXGx8jJytTV1tfY2drk5ebn6Onq9PX29/j5+hEAAgEDAgQEAwUEBAQGBgVtAQIDEQQhEgUxBgAiE0FRBzJhFHEIQoEjkRVSoWIWMwmxJMHRQ3LwF+GCNCWSUxhjRPGisiY1GVQ2RWQnCnODk0Z0wtLi8lVldVY3hIWjs8PT4/MpGpSktMTU5PSVpbXF1eX1KEdXZjh2hpamtsbW5vZnd4eXp7fH1+f3SFhoeIiYqLjI2Oj4OUlZaXmJmam5ydnp+So6SlpqeoqaqrrK2ur6/9oADAMBAAIRAxEAPwDSS6qg3TJvzOYKjoJsbGRT0u68NVVVTMw/h1U8VLDSVFMtMlPHjXIFMgkBESAK7LdgS3HhiCBmlDDJVgKCmK14kkn+da9D3Zkvn3S/tYrRo2ACzxFmZqqTpApQBUGFA4AChIz0MW7ekJo8EIKjI52sr67LZSsw1HuOtmm2/jaGrrHdYselN9tJTVcisWlj1BGI1WtbUiF0Q+tdIVFCkpg145GR6Z6EjctpJZi38SU3s0jyRrOR4fhkigQih1VBqPTP2jD1bsSg2vt6eDCwWSkxEeUmqshOqrVwNUSw/cyBRElS01bFIVGlLxgKyqAL3km8SSrV1saYB4/7A6TRWlvtMCR1Bj+FCCDUnUatp8zpJyBjiOHWDdWzUrcZV0tYs9f5I6gSIxjlip3q5JEkQ08WumlkbWSRplQCykc29+1EntNKcD5/b0/LaxG3Hi96SLX1AJxp8xXzoK/Pj1BwuzdvYxKTDVuKiNJBKk5amx9OIXqIw9QFVERIIppJVYeOJdMbMAAB73qr56mOSa+fz6bW3jhjC+AAq4AKgcPTyr9nDpX7zjx24Uo8DRYvHyuRQ/dT7iglpcYJ6ptVNQ5OsdYxDHUPTafyrDSgu3vTsAC5rgcBmv2DpiwtbwLLbzeFJ4kwZfEGlVUk0V24itPX5dBl2zU94Ybas8jbJ6tqevqUSy5LCUENXkqSeGhWZ1r711RQVmOpqCGlHjjopoZI5SGj1FYzEns7ezkkTxbub6nTQVIFAc0IAoT9tcfn0d7/ALvv0VvdRWmy7YNqV9U0MaOysVqAVd31qozQIy0ORkLpnYzuDZWQwuTzXX3Xu7T2FFhqai3P/cPEUk/W2PmlnrIcZVNvrI5OkyW3cfm8VSNUwJkMbPVwyM9JMXlhdygS0v7e48DcbmBrEt+m8rFZXAAJ/SCkMUY0NGAoAwwadDE73y3u+z3W68rcs7iOZIYVF+NvgWTboWZysJN48qtBHNGmtPFieQPWJiXTV0itt72yqpuXbi1VbLvPEypjdwUWeSWopsTkhWSY6sx2SyMccNDUvjM6HHkVjC9gYkC3j9rpoFJtpVoYCC8TDzGCCPMVB/n0GNt3a8gi5h2uVn/fSSCG7SarKjhyjI7fCxSUHNSDTApUFWU3W+7azHbn3Jiu092wVqS0WfrNr4HP5nBbUyRopFkqsPFR02aostUQnGXgFRC8KRvKjoyqfGrElxbLJawzWMTFgUV3VWYVGDUggZpg8eFMdGNry5vN1t+97nY8x3ayQaLuS1gkkigbSaMiqJEc0RiNS0AqCGANAEmwcllMT27urruom3ru6jydRntw7PgZ8Gm667J5ZcNumDL7nymZrMXVfc1ezKGSSvp4atw9ebxxTknWuuxENtt71UiippSX4tIAqlF0imHIAJAxxp5EvLjXrc47xy3cPuV88qTXlgAYhcPI4iufEnaV1c67RGaREdiZKaVkyGMhjNo126NyYqtyOJzlfQ7aleLBBsvlq2XHyNVY2WpWDBUkENO2FlphBHPL56iUVM2h0hGlHQGa1iWRJJEjeUUZyABWhAOonjxIBxQefkIZNu3i7n2u9it7i5ttukElvbCR3fQXRyFhQV8I4VmUk6yQwTgV9v8A7D2xIlJnc9t3dWLqtv1ORWvp6LE5Wqpoaf7arpqiuxtNg5qOQQSUjmfw1EsMdNImtyjpqBFb7HuNiGjEqtC6hopGIGr0BZtQORSufSlcdTpzT7v8h84tte9zbTdW252zSC8tII2eONdLK8lvFA0LqpVtXhsyIjDVqHHoseS/vwtTQ46TZO5RtPBxLT02NymUp4NyYeij+7SRYTVZKej3FPNNJ90ks9VOblxGiwiGP2eRLbjW6XKGZ2J1KO0nHpkDyoF/ynqDt0k5gea0srjYLxNltIwkcM7aZ446ueLMVnYltepnaudKhAidKSkyuZr0qTjZ63BSVCRBYJsfHkt3QVFM1Q8NPWYyqhkwn20UFAGl8cDMshtqkOolxFT8TAilajAzxzxzXH+TpHdXt7JVrRGiOtRodNc4K6iA6FfDKqEqaLg0rqNT0/01ZuqgpcNjtv8A3s2UihjGMocNI0lJvGoEaJBjjW5JJJcdLmmYQGasjcB5j42kUp7a/wAXVpZroqIRl2enYBkn7BSuP8PRoz71JYbZteyGb6thpgjtdRW5dhpC1YalaTVp7wQSx0kqR0ndydnbX3nk5KPPbS37FuLa9NTw5naOO2pj9z4ra1ZhoEgplyGQxtbR0oqctn5FjhcUccQqWi+4aNgSiu0h+nVTHLGbZyzRyFzVyxJIUNUkKvHPD4QR0F99vpd1luYdx2+8/ftikcV9axWieHbiBUiDTPCyqjyTECpSmsjxGDdBzXUfTO66mKiy2Jrtk5Lb+Or6utwu7dvSbMy9bjqiGX+K5HHS4qeujyb4KSGWpjjqD5zIrtHTyL519r2F5FGTC/a3BoyGGPh40Pd8hTyrw6DFt/Vy9ufB3G1ET2+oSQzoYZCrA+IQUqCYaagHNQchCNQ6k4vsbbO3dtLtN8NSYjYuXFZm9iZTbtdWbw3ruDKUFbjMM9Lu+jjymOp3qcvHDDLT07HGfZwU60cnkazIja0meZ5fFLXQCrKrBURQatVTStBnVx1cR6dCRN/2mHa49rawW32FvEn2+aB5Li6mkVooyLlQ6KWkAXwwfCEaqI21GjdO/Xm9thY6Klw7ZLc8l8q1FlMa+FyFXvigx0TTPHuCqxUFRLismKqKTzy/a1v7MY8fH7TunvIbor4scSV06kOrsLHOnVQsKU81/I5HRpytu/LlmBZz310wkmMdwixN9VHGtaTGIP4L69QY6JagVGO1iMmYBmy9BS0w0bYrpoaXH/xmop1mpqOirYhQVOQfbUVZUTeSNhHVvAaiKOO8aJJIGJ0j3AtVeUg3ITUwj4FqZC66cTwrTyJoOrzW22Nv5t7RCm0STGKJrlgSqahpaU2yuxoPjKK9BVVVmB6yePBY6XEQbkrMLtGvyuOqpaPcWU3Htjbu28hJjYkpnwqyZZ8ZXxVy01U0zy+qmZWRXEdQ8QLF1JMPEMURkjXTqjRGeQVJ7qLWq8MUqMnIr0e8uWm01t13S9SwupUl8C+uJ4YLWURqB4VZVQiTSWYsWKtVVoJCvTTmE28Msdv0PYdDkcrRSQ5ArjMtJuqeFaeWCJqQbl219ztWXI0sGSi8uNSunlpEANTGjIWSlrJJLGJWsnCmqjWpjrxqdD6ZKVGGKgNxUkHLm7jZzOtrt/OCyMHWXtZ55BpYLpM0amAOFcExCRtAA8QAioXuL25TY17x1lBXz1FPMKto6sVlWGVFpoamWRaqplji8KftmNnDIFYABRdI9yZa/psoBBFRQHzpwH59Dnb+X4Nu0ul5b3EkkL+J4cgkcUqgYkO7AacqVJqKMKAZbqPEV0tdS4XRNkcdFHOKGNPuUWtqpIE8sTlUpJp5YqhlMrSuo8NuDJ9FqSRZnZtLmmqtMAH86VHCnn8ugVf2e5RrHtMUfjbfGjeDpDDxGK6mDGiFmRqFyxHaP4uh3632Fm90Z3G4ksk9XU42qpsTXV2qnpKOnxySiCCWGOSleE0koaESOrnWSwvckot13KDbbeScLpRZA0qqMnWQCRgg14/Z0H1S3bbbzcN0na5VbUwWbIxOlok1iPSGUigOkVBBJrQ1r0kcv17unHbxyG2/7vV2Ry2PjrWqcPhJI5oaY0UyfuZAyViz01GSyxu3k8zCTgCQgG6bhZfT294LxVtnIpK+K6gTjFCaZGKY9OllnfNvO2NdwWbnXD+nBEQukKVA8RXYMoDHSadxJphuovb9EucSDLbUwWY3JO8M8mL6r2VtTc2a3Tip2xTVW5Ew+OpKCd2x2LpUZ56ta0MsETSsqqCfabb5hah4r6YRorBTezSRBZKvojLNqWjuSAF08TpFTQdGe/C4t9vs7yW3NzctGztYW0M2uEmMGUoqx6VTTnUslKAntA6BbqbP4bDJNioeqNz4HJLt1s1mtyZvB4zE54ZjJT1VJiqJcDmag7gzmCr8XjfupstRT1QgknhiaFCRO5nfW807RmO7ja2D6AqMxFFy7MygqrBzpCGlaEkngC/lLdLDZIJkk5cuU3UwfUPNcRQpKHl1LDHHDI3jzQPChka4jLBCyKFU6XYWN01tHjavaclVDS4PC7cxVVgpKOjp6qqTdNHnMnPlhumrr5qT74xYSeR7w0tLTQU1Mx80kqu0jJoI3dbyQTtJcSyCQg6QIyiqgQAY7gKkksSxJFAAArmaKw3G1Fwoi2VIGhhVdR8RJmaVpS/hq5WJqkqqqAuGLAkkwGMxOKrcNtqnxuK3HDkK7KYrA1+VxeSpqrF5uorayaXDZXGzU9DBRUBSSmjC07z1k5mIESBY7kPTy3Md1eyNd2zQrG06xOul41VQJFYM9WrU9wCKB8RNcC2C9tbXbIV3fb5vpHf6aK7iqUelSjllQjAFQo8RzSirRcqjsfM7lyiSDH7th3pu46VyFNSYnASblo8bjqmGjzbZvBDGUeZ2vUTzIg+9Wmjq5is7a3DvIUGxWm3QMn1O2mysFHZrkcRlpATGEk1tHMACe3UVXtAAoB0zuO4XclndbdynuD7jfC6W41RR6nMaFld9BjSWGNwqUOlSakGlei9Vk6wUWWoaz+FSQrk56iJ6p8vakqmVDURwUK1FJVimpqZkWN4CiSPcsxuoAuS2bxYpomk1aNNBoNQCaEmjCpOSDmnkM9IDzBFcW19t19Da+G0v1GuQToI2YUeIIDG4WNaAaKKSKkmq0j1tPUZGTB43KFczj58hQBc7i8bkIa+SKetmpZIWeWvVMas9O7xWjaIMq+QxkXDsBRDHfz2jBLzQ/wCnKyhNQWoJotWzSpNTkivoaGeW+ueWNt5lt3m5dW5gb6mxSSS4W3MojlA1S0irEHATUimgcihqwe1MZAz9di6HJztDm6qkoKinx4lyMEOiEVOKq4slDR0rxmnuFZ4wVpGVxLNZX9mcUb0txNOvwDWK0qeGoUz8X8/ToIXG42arvH0G33AuzcSfTSBS7JEQCY5NQCkCPzoCENdT0BHKspsigpaqeOsx/jpEp6qmqpZxTUtfUSpMJKW0lTT04qaeGNPNL+7I3DODHEVuJI5JHQaWFcFaZA9fUgk4H+U9aWx3CzsoL0mSGZlOuOckKjswYaalgoeMKAz5J4nCHoYdk7Jxcu1Mjk81BW1C1eRrKiQorrV1VPFSxwq0MMsKPHU/doDE0IVv2U8TWZtcecw77eQ7/Btu3yosyxKRXKhi1TqI8tHkcZyDimX3tF7W7BuPs/uvPPN9lcybM+5TKxgIEzRC30xmJXA7/qaElAHpGBGygtrLnuDCVj7jl2kzVFqOrqq2ip6unT7eeLKU0a0uQpqaeFoViydJGkscSK6sG1It2v7kC3mhe0S/ZKSOih6ZI08VJ/okkGv59Yg7jtd+3Mt1ynbXni2tvczG31hdD+JRRLGhBAE6KrKoBrgqKnpE1s+fpc/t3a2EgTGYbdlBLt+oio5MNjNu7fyVRE0b1mMw9TRLTV258wIxTos0jxysqwy6mYNFd/pooJbqVhrQ6u6pLAGtCwyAOPl6jpiFt8uN723l3b4vDsb2IWmmLw0ijkdQHaONqI9xLp0dxOo0RzWmmDuza+Y68rsTUir3zvTKZKno842QyFe9Fs3Z1YrLDj6vOUGPxQ25hInpA8lSzieoZQv23qkaX3W3uor9ZKxwxIjFP6bgcQpJ1MM4GAKZpiivmLlvceTJtucXO4391NFFetIzFba0dsQm4RI/AhYqKsTrYqV8OuosTE9Q5LNYzq+HCwU8s1ZvKt2zvTfrZLB0lBlTltsZDc0uBpqT+LAZHD4Kjrd71lQ/2ckM+akkgqMqkr0tIsKC5tUlu5biZAoRXt7cq1RokoHPb+NhGozUKB+nTU1b7O8UY5auhJNNvEZN5erMrRgSq3iKpikk8Mxxl2YNTxXLsZlAVB1n3RuDauHxE+6KKLO1c712Pr6Pb1dQtBQZSmqMrOrRy5mbK0OIw+IwdO5q6zKVdbTUFNSx/uPIAI/frWPcURLS7MZkCFHmiNSCEHdp0liXIoFCkknA8+jTmHceWbvcJN85as7qLb5boTQWN2NCMpmYlDN4qxJFbhgZJnlRFQVYkYDbtSm2/ubB/wB8jRx43ItTVWVqdyUeJp3r8rQSGS+OqGpa2JMwuEnVo6KqpaqbGy21xJKp8hOXeaJHtYkWQEgaGOnSQONSpPcOIIr8+HUaK23SX9pvW4XUtu8jMyTQxay5LNUUVwjCLOlkYx1AoDUnp4rqGmkhNRS1WRyOBE9HbLyY7KCkx75aGWWKlFPVUtH5KuVp3qRGYoneWMi/9EUUjkBZAqXdDSPUtW0kVbBOB8PnSvQuuo7RZPEtzNLtMjAvO0ch0LIGogDKgZiW8UCgqRTqBi6CrilqMpUZgVX3M0cq00NNUY1xErNQJkIKdXSmRnajBKlVZ5bFle5vaRy0ojFufm1Qw9Sp8/Pjw+zq9nbC32+e5feFYFW8OAh4yBlVlC1CCujgaMTQ0YV6G7+7W1cftdsrn6vcePoKXIUMWdrKPb0GVnqZnx0k0dMKGfKYmgrimSq4oZEpar7oRyCRYLB0JNNeXBuhBbxRPOwZokeXSAuoDVVUZlqoJGpdNQVL5B6tZi+jhlkuXH7qSNRPNDDqczESHQwd9DlSyKfDINCCEqG6LxVZCTclZS0CNmKabFSyV1Xg5qGOTJ46FqiJPKlHJS/7kKenikjheWRJI3c6dAB5PSIoIzQJ+phXrQGgPnXHmcft6LYpb/dLtXlacyWg1zQeGGdAXVSdBSjAVVSWBBNBShyEG9NzbgwG5qfrDIGn3vhuwaCfCYxs9l59ty7Ty24K+pp48vUHD4aoqxsOGDyVVZBTQGaCPWsVVTaED3WNHt3ukbRLCRIwVQ5cKMqKsoLnCrU0rSoPTUdxJa77By7eKLq13eM2cU1xM9qtq9w9EuJPDgmYWqDVJMscZcICFkjIFTCbI+N+OwexN3be7JpsNubH5ldo0yLHNX4atql2hh1SGryG8cVV4XKZ7CZKuVauhoJ0H8NDJFI84hiIBG681STbhtsu1M6OmscAwBdqafDIYK6ioLeeaUB6y75I+7pZ8rcg88WHuJaWd5bXktqIQZJIGYWsLOJ/r42gee1ndleO3IHhkxmUu0S9TMT1v0hgXNJS49Mdt+GalSu/hvnopXymxqoZzGY/M5DCIuVrsxhqyHz3dnqp3T94zgKoUzbjv00WvWpuqYrntk7Syqx0gGtPQeVMnov2rkX2S2rc1jmjlj5bR2EvhakYTWR8dLeeW2XxWmiYasfqOR3mWiqFdlKaKoOdyG4951ddtfb+HG4qjatLDRUEG0ZxDLUtnKTJQwisoXojGJXkrJAsDIZPS3lJSR9hhW1sVS8lcRCd8mShpQg8a+Wn7OFOhRfxLfJvM3MPOlxc8rbZa/vR9mtVEX0UjpXx45EBaMwkAlpiNBqxofE6TvWu/cdufbW3dqbbn3LU7LweBmV9271aZZM9SQ1j0cdemUqqTbhkonnxoan1UMVVK00iF/SxYwvYHsprq9uwjbjJLSOGAUodNdNKyd1D3HVpGkGgPCEuVk23me4sNv5Vlu4uXLexX6rdN0NQ6LMY/qPFKWbGNiihAYllYsyFjQlll2LRpkcx1vjNjbwyezMhJjH3P2TllotiZXAvT09XHS4uSirNzUGdFNurMY+eMU0lOojp3jbzpMzU4UttUu5rHeDfWCTQhjHaRr4wc4BZGWNoiY1cEkGuoHyANTCXcZdo512RbLmZ7C3a4juL3cWjsJI0hb9ISg3UF6kd4yuBFMn9kQGYFtGjPmt709S9fhMGxk3JlMdHKKZ0qNx0e3KqqqqegoG3VLBPXY3F4zcMtXEmMRV8NZJFPJEZNDlAvYbCYbizkv5SlpC7VLUgMoCkkRAaXMsWglzgqh0mgPWVfMnvQl5s/NVnypskNzzHukERijUybuu3S/UJEPrzKLi2Xbdw+tWO2jAaOa6jSdGd4+p+AWs2o+UlyTbZx1GJ0mlqGrIcdFQYxgyQeLHlTLHRPO0giimePxi4QE3ULt7NrusVslv9VIoXQqhSxaQU/wBEPaX4dwbJ+I0z0E/befmDkTctwu94Ow2Ds4lnnnmWBYLSZnWosowJvpmq9IWi1KmIoix0go5qNsdgZmLcGzexVg2zVbQyked2htzcO6qulT+G7proaFKfAvW4Td+06uQ1dMKGaRcfTPABTxRpSsw9jLbre7s7SSw3Db2a8S4FJJ0jXUrorE6wDFIoNdekuQfiq3WNHNt7y/zLu+377y1zRaw8q3+zSePtm1Xl3corWl5PAiG1lmTcLB2XQ1uJ1tkZGAiRLdsJbrTrSry9BH9h25ndhRYPcGX3DmJ4Nx5/A5vO5LLmA1G+HzGFwm9p87lZqKFMFjsJJFDG9RK1ZPkaWKqqVd3d757O+hSTYPrPqI0t4yiRsqItf06M8QiQE+I8gLEqoRI2YLQn9uOXJNw5L3Xctm9z5thfYro7ncWqXdxZ3V1NPPb2/wBdDLFBdi8mjhk+njsz4WgeNctcokkschjP4PP9t9z/AKJMJ4/7of3cv/Aan+E/3b/i/wDCftNH/AX+5n3Pp/hGn+G/xr1eX7j1+yT9zReLo/rJLX94fVU1DXr8PXorx8Wmdfx+D200Z6mj/Xn236fV/rL7F9V/U/8AqvSr/SU8fT9V9Nr8L6X6fP0X+437z/3Ya/qOindK4ja9Z2NVlJ2qtxTT4vKPh0oapq+nhkp6SeCeprKmOCmo8RTioiugkLLLIqFmIT3IM7TpbKQvZpYKTw4mtMHJ+zy6wk2iLaW3SeWe6CTArI6KKsDpGksWKhY1qK5xWmT0bzsDHQbunpNkYkS1G/c1MibLoy802MnjoKuinz2WyqUUTV9PR4Sh80hfT4zOtPrlQOWBSjvYxNNIyrajulZwQQSO0KeBJNMfaAOhJcXNnu0UUyvpuGQi3VGBoImLTSSIBqCqAxBrnsJIr0+Ltuk2pQ1NLHTSzGj+5xtRiqemilyOQqatytK01RU1VNR01NSyP5WZCxCgpYu9/Zik3igMSKmjKQcAedMVPp/PoDXU5vJLYbUjGyJLPJLRKUJp5sKlfIkfafNM5vMy5PF0WCrcL/Ac5DTYvF181IpjxLrTr4mr4Ks1Ek4mrXo1M6OpIdzosnA9bQvE0rGbxImYupPEajXTwpQcBTy45z0dXkyXC2UiRskqRBHRKaDpAGtTUmrcSD58MYAdPRSLk4HpqWCqnUrLEK2paKmLUhjZ6wBBFJoqJo7BVFiyrfn2ryaih9OmmdEAeQgihNDX/Bj+XS/G7MYKummmx0MsuWpaenEkcT1i1FUZnbwihilnWSZ4tAWNox6gdN7+2GRgrDVQD8vL1/y9ahtyZIY4ppKa6qFGotUAaNIqSfMDzOOg77h7f6mymDl2jNis3vHfiCKfbe1Ov6tMyuIjx0U9TMMnWKuQoMNX4daCqeWM01fVUxkvNSLEpJQ2u37lHL4njRpZNXxHmGk6q0BHDVWopkA0+I16EG77vyuVt9vSxuLzdFXVHBYOHOhV15akgiZQrlgyO6aiWjoD0FO2OqNpYjPbT2/s7P01dkN6bErcn2BiN0TzbppsriHzSVGOyOMpsbT4rBTRGpX7YTVMkso8azxwQyB5C5Fd3l8Jmu4QsUUw8Foxp00AqKmpJxXFBniwp0v3HZOXOTrbZzsO6eNf7htbNu1tev8AULJ4k58JkSNY4fDrpXU7O9V8RUjbPXHe/Vu3aHJpitvNR4eiYCvr3okjp8FXU+Kocr98JqCraSmgyVVTyBTI0YgUWGtQ3tV4rvollrr4UY1YVOOHp/qz0HZtltg0lpZBUFBKTGNMTiONi5oTTUw4Gmn5gHpSYLdVFJsLNCDAVfYWQpdnnG5rE7S2jnM7ABlI5qKPCbv3Dg8VkMZhc3WnHytepSLQIpGWEL41KSQiO9thPOsIZtSGSRVJpmqKxBZRqoafLoU2MkF1ydurWVpLfXyQDx47K0mlAV2CGK6niSSOKRvDLLr9CaDtHQHfHzdGzJt54Hbu8N5ZraeB3BuvHbao121gqvObj68GarstSxb02tmaQ1lVkavadFURJTumqvqWmEAUUys7K98trv6K5ls7JZphC0mh2CJMwA/TcGgTxDxrgcckU6BXI3Mlltl0Hk3KWK4M4itIbfUJrZmMpS4hu0jmZWtqKFkVGkOrTp8Op6OZgtt7I2ficxj9z9m1mP3hUNl2pqzdO6MZR5fOQrlEqaikx1AJ5wlNT0qosFDjR4XZ9YRi6kBu8u9xe5gMO2h7EEBwikhTpopJNOJOWbh1kvyfy3yBHyrvNzvfP5tObZ7d5rdrq5hRp08QSSRog1E6YwNEUQAcmoU1Wgd9m7pz3cmNpMVlTgafrWBMaNvUO0tjba2KmUoMPjKqXE4bPbgwdBhtzbmgknl/ik7ZOfKZOSoaKaWVlSAqe28ht2Egcm4oKh2ZtNcalU1RTTtqAoOfOvUE32zRbg24+B/yRLqYS6408ITmNOyMksJBG1BKY6sQSrkYUhB7Rrtxbb67noq7I0ccg8cW3ohlqrMR7aSaCHH4vH7Z/vDLuBGgrsjTQTFIKZUXIVDFgsChBS4jhlvBIiGp+PGnWeJL6aGoqQM/CMZz0abPu+8bbyi9rcXCkJQWYMhm+mUjSiWyzGVQjuqu2hB+qxLEJjrIl3oKCplylVVQJUQU5oaulr62WaVWfIZJXrp2d2et8rzLqlkDoQINIDBX0oCyqlDSoOOiO5MkiWdxNeNJHqEbRsHJ/jbuPEsSW+LIPbwIBisHsWnzmHyE2fXHybXyBbEZNK2KlyFfPWYyrxGaoBioKxJ/4NOs+IQtLA0VRAsoiLBag+w3e35juIYYC5u1/VUKWVdLBozrpQOO80U1BI1AVXGQnKfIMG7bbdbhvZjj5YbVayNIqSSvLEYp0SBX1eC/6S1ZSroHVCQJegKTF7U3/Xb7p8tjcNvCl/j8G38LMk+cqd05Kqw1JKkONnzGUqo6rH1uJkd9JppQJaWQtJGf3NZuJJ7JLRo2aKia2BoEFTk6QKFSAPz6jEW2zc033NEV3bQ7kHuha2rDxZLqZkUqieNK2tHirjScoaspo1YW/uuKmm25vzGZzZ8GH2/RZDZlVFUQ5Srx+6aXDbXrciNx9pbqp67DV2U3VSbgXNzY3BCrqEky0VNVVWLFVDR1chZsd2t5rm0+mvNcxLg9gKamXESOGCq0YBaQAEIWVZNLMgJBzjyhucN5zDs1xtKWW3bW0Iu4h4gmdULlr2Z5Iy0/il9MI1EzRgyW4kjR3IL9Yx4batJvvZPZEO+sxgdyYqkymAwGycJLlayqhq66fE/3uiizNNi6vARSiOBVeoghlqB4WlpXZKXSc373FyLK72/wVkjJV3mYKuBXSKFgxFKjNM/Fx6JOSU2HZBzRy/z0N0m2q7gWe0t9rg8SRyzmMT/riFrdHBAJKamohaFisVBg6X6+xG2tzYePc+8cjjd8U8ePxlLtTb+16HH4/NvNicfX4fb2492ZOhOVQ1mMWojzGDyQxeWUskscUVPRwzyBLmTfN0khb902ULbU1Xe7eRmZBqZXeOFe0kMQYpB4kdRRqs2kT97Ie2/trtN5LJ7j81btF7lQFbWx5XtLGKC3u5ZIklt4r7c5ZPFjh0o8d/YyJaXtJY3hZI4mlVd9gdh7N6yzVNQ4jr/fW8FxsAm3PWwQVeKwu3kaprYMh4KibH1lQ8mKeISxQP46SVJkcVBQjUZ7VHu26be0t5dwQln/AEAO5mSgI1ZAq/qBUDyr0B+ctw5D5C5tt7Tl7l7ddxWC207qZg0McFwXdZPBBjkk0W4pQOxV2zrKEAp/Gzbj7dzDZAYinmaro63B4TbjR4DdX90epXemrcZlqPYWdo83j5N27ikxbz5epq4o54YYo6qAU94tKmQW1hBoaYL3rJJJVk1TYoDIpHYCaIASD8BDCtQnZHcedNynlkti9v4Zt4Lf9KY21hqqGjtXBUzvoLTMVVlH6q6CVIEjD7q2ZEavaOG/h3X+9Itx4JNvQYHCZLLRb3poMPkKB67EGnjbD7foKGOlamkpa6uhSCGRTTtJZSzF2l686SXa+PaNC3iaiiiPSVoG4M5I4FVJ7c0rg02HcOXLEy7LsPibfzCL8NaXECvKbgEOulF1BYFqad0lAp7WJArN25Hl4KuuwtXhKbG1MlNUzfcY2WaeZ4pYYa6OaAVz1Uc05Ebx+NX1qgVBrW4WtyE0pcLKWjDAUbArwzQCg/4vHQl5cuLwz3exT7asNw9u7+JASz6CBICokLBmwRQHVTt7hjpy2HQS1O6dvR5Gen2tSHLUqirysktJRUinI08/lzEEUsNVJRRtIGZoDA8iIp1A8+3NwLRWF3PDC00giY+HHQsx0nCVBGo8BWozw6DO0XCXG62e3Xc4trfxVSOSQlVGqQEeKNSnTnJUoSADXoyu3sfvPJdp5Om2zvjFNkXp8vIYaWroabF5Vcz4KyspJKvHwIKGrSkUKPFqELoVjB0n2Hby82232CG4vtslFqgQvrVmdAhorBTVnz68Qc9KZNhaTejBNvETu0xit4oGQxvLJhlkesaRDSSNVWAoKDjpD/M57HDeFPkqXBVG36vAxQ4yuoqOVpKPI5+g1Y+ohOVoGlqZXqpo5LNO0c0pku3kQBQeQQzm3eKS48YSnWruACqMNQOk4GmowBQU4A1PQcgtdu/d6rR4BAZRWI6hITJ2oJFrnSSM6TkUJFAEn2L2njtj73wce7qOs6u2RXU9Vu+uymFqNx5vJ0WanP22Jp9wZvY+2qGuw9aFrKiOkhoqmikaQJLUKuqKT2kt7J762lWN/qrpVEAqqopXt16EldgwJFSx1UyFPEdLot3/AKrrbybmrnaXjeVlMkzDxRqSAXMttFqiAJoAjhzTWR8FUxgexuscvW02FodybYq6DF5Kjgm3TQvk3kqps8a1cSuVzFdTGbNZirNC6x0MKmrZyZHiYKxUyeO6t9U6QylylBA+kfDx0rUAcckkjFAetwXOzbpDNYPutp45m1LewGZ0R2DaQ8zRh5dRUhUCiQlg7pjCjzFdicvWyVtBQ0mWhrc9MKfD1+ZocrU4DE56lkkoolxTx08lTSRxRoxrW+3EayeIQACNlYhhmXwrd5GBWMFpEjKh3UgMS1SFqfwdxPHUcgm67hBBbzXVzaW1wxdlEcswkEMU0ZKlIiASuP7Q6NIOnQO0hcbdxuF2ztmevrMa1Bk8XkMPkNsZDbe06COnwtZRZCUZ3JVla3kq4arbNUlO1LSVMQpKqZCplH7qM1crPcXYtreRHtpInSZZpGq1QNCKoGnTKNWplOpRTtNQQE3niZLT6uxWKFGMlLWFQUUiniNwYtG1Oxu0kU11JHQr7yqMGMhualqcXls9V5FVi/jGWNQlZJkshPW1qUe5ZiGxFViauLKzu9PjKGOKYHxojo5kUq222na0s5VlijRV7oUpoCqFUmEfGGBRRWRiRxNCADVpbpbqHbI2Bh8RlSWrF5ITXQswPaBqZ6rGKHhVq4DTaVOjZGhpRkMHjKrDYWeqyWqkx1eKalxAhniix+PqQarOktVrBTQgupkdXdkAZiZXjOPFrbyuszhE0llFX4lmFPDAAqxwfIAkgdCOSeyh2Sydbu3+qtkIZOwy/pkaaKSTICXogBKn4jpoapzPieWXIvlqrCYLDPVVeSqqg5VIKGjoYYwYauurswYXxiVUdO7z1NU9oCrXRk0AvxpbwCMxl5ZlSi0WpJ40Crg0qAAvH1rXp6Lc973KyuBeW62tk0g+pkndYkRO0E621MGOhizNjI4giiIwm+6OoxlTJ15g8duTD0FVG2K7OydXvIbH/vIhakzmJfbMmFw1XuOuwMENPPDWQZKhxtW0pjeSZYiqq02/94XMf7z3EWalKPAUQyldVVKsrHQGBIIZSRTBQ5JF+/7nao7uLkm0/eNk8qtHezrKIhII6Sw6GVdZjoCHBCsOIYAU99vIj/xGU02SXIYGtWox1VHVVmIpWydHTvG0dLIErVyqMzF5pJJHVmXVYogjdeJWDLESoWYaSCFJCMeOKafkOI+01vb3k3jwtf1klNmzSwupkjDTRppKjVqL8CzE1Df6VaCDgqfH5jqys27lslmljmp66nhpoMxksLlZqFqhBj6OlyOOnoM89Fj5I1pgI5IhNTqY6gOryBo23uyni5zsb63s0eM6A8jRhwpBYvqqCillNQTUg0K5oes5/azmLadz+7BzRybu3Md5BOj3UsVgl41q00cvgx2wi0sLqbwZV0ssWgPCZBcExhgS8zbcwkFeY6GmqcZX11DFUU0+IyYfF1skEEaUAgy8Vc1RVU9LRhEMZBQRhkA0Lb3IkUkjRkmjIpowYUYZ81pgnrDK92na4b6AWyS291PEZIWt5A0DEL2BZvELMqrQEZp3LwFOmnBwU0lfTYoJWZPN5SDO4+q2lTYgZKrq6XKYavoMk/lambE09Pk6KWopwaxY5cgiSx0xVo3kjY3NEltyZgFt0KSiUMV0lHVlyCGBVgDg0GNXGhMuS5W23cYfoXlm3u4iu7B9uECTNKl3azW9xQOjw6ZYZHj7wryDUISjJrQT6jfuVhwU+S3nhEr5M3m5KFtszYBsLkaPDRY6GDEY/JUJyFfRZen+6KpU1hkihqNTFKcRRKWLINpiMscNjIyxRxCj6tQLFjqINKg04Dy82qepJ3r3NvodquN05w2yO4vby90SWD2/00i28cKiFHjDGOWMtTW50hzULHojHSXxWcbDwjH5Ev8AwKDMZmvpM6uVr59xUUeQqKjJigkqIaDHYpqXEJUyU0IjN3prA+Oyp7EUVs6PIWcEmNQUp2EqONDVhUipyadQHu2+LcwwiGBkgjupXS4Ls84jlYt4bMqxRP4aMVUhVqOOkUHQn7s2Ngt/7G2pUvgqmbb9PkMdm48HkEgnrn/iJjGTkykVBX1uPkyEDQxgxOamOmXyjVMNIAU27c5LfmO9ivpFW9kjEbEalVfDLGILqALAiRqsKajTtXqducuSU3v2W5Xu+WrOabluyvGvLdX8KWaSS7iiW9ecwMyxuj2kJWFgxgRmrJJWvQpH+GxYjclXD13LV1awxVyJQT0+PP8ACoYa2hOMWCuxaYlJpKytEomPkMTsgjMTO2r1vFeWz7dane/EUkq7OCSzCjBtQfV8KkAVAOa6sUCHN1/sm/Xe+80xcq2+2stsiWu1W/hgJLLMIwAGiQMRXu0qSAwYaKEFNU1VTVu1pK+LG1m3aXJVlLTvhs1JVV9bjcNHQzQY9DXhqDEVtWfDOryVEInAWOWmjWPUrmg8SO6ihZ1llRCxeMKoZiylu3udQKggBtPEMxNCApDbm9g+qn8W1s2REVJtTaAscgALllQgqlKsNXBkSmGRFJlWxVVNWbc3Bk8XSY5JqDDxQ33Pmtr4EysKSvxlOkKCKHGR1zTyTQxxxJKxn0pcD2ZptVxfQvaRbYbq5ZDPMEUqrlQNRemrHaB3V7QATSvRb++7CG8+t3DfvodnBWxgz9RJEhBCtEp0dq6iSVp3Etp1UHWffH8J2ctLUZSNa7DYfC4KXbUGM27ubMUnkkn8kCxYqGq3IuJyGYpas1c8JkjjMiO+ok39pbdpZ4VKqRcvIwnqyAgCoPdRC6oQFU0rSnTdu21Wt7uUsza9vjVGsisMzqz6lFPDDS+GzqSxBamoGh4dFr7O3h3FjNz5PKbOzubkzuQxlLtbMbdo9q4FoMVimlevV48pmaWtOMzFql5RWuk9ZEapbNHpQqYW1ptskEaOAYdQdGVn40pTsIqp/hFARxqMdBzmG75rg3W7eKW5G4KRHPB4aLpozOCTIGow1atTBmBbgDQhCYOu3zFn6ml3/XZPdH3ePSHEU9BvGi29Q7UpJDLDW1cmLl2/gINz7zhVqSnpWoWEwhMxEcyhFiemjtiIvp10V+MlSzMfIatbaUyxNfOmQeN9v3Xdbea+i3p3uagGFUuUt4oFoVkcx+BEJ7oKI0jKUoNfY4I0N2+d3dsdo5GHbO98zkdqmLF/ZZbFbbw+RrHnaek/jM9BWT/xmKbcOVyNIgjeimq4cfSyrBB4ldxLG3ZWNhtaPJaWwchiy6qAV4DSKHRSvGhY8a8R0Yc2c/c8+4d9b2PNe/TW8Zh8KcW6vI7IxEjLITKDcM2kARM6xKQihVoGVy64+T1dsimqeuHmr9tbOSaWipN21m1Xz28jWZOaeVM1u3b826qCaaeskd6h2oq2abHQrHDTeYgNInveXLe9kTcJVWS9C6vDV9MfbSoRgpAXNKEdxqW+Qj5T+8BzLyXtd1yPsly1rys8hT6ua1El4xlLUmuIzNUzH4lMcjNCFVIWrUsv4NybIzW8qHY2R2vJhZ8jlZ81Lu7c+84q6HfplwH8Klwc+281QVAjr91JWqkEbVjrDJHGAss2hIS5bTdYlurn62NrbSFjhjhIaE6hR/FD0KpSpGgE/wBEKdQjn5h5C3XcNg2KPlW7t958Z59w3PcNySaLdNUTDwVs5bUNby3IYKtbiUKwB73ZVik4eHP7S2Bgv7w9oYLadAprsTtOfcODwmOyUO39v0+PxeHzlXs7cVXPUZCqNWK2SOmaFqiaiVC4hkkMEaiK6i3C7voF22RpYwrvQmjO+ovGkigYUBakE9x4kUYlLbNuvJewcp7xcc7WttZXs1xb2qTxxGSO2tRDHDdy2c7OzGSR5/DVkBZIzhGLRII2IoMzjc80+6t/ZbN5LNz7ZwUeayZxWwcLhKX+LQ0JosHg8fj/AO7+y9s5Skq3SeKBqVKmWd3aRpCCdUgW0Pg24SOMNIUXVMzHSaamY65JAQOOo4AAHkxeJe2e6TPuW6XF7JdSRRePKkdkkarMtVhgQGK2t5EYjSpjUlq1x0KEkNTtnN5eufGVkOGqdxzY6kpKVqfBSV+3aF6NQ1HOKvJO2O/hsCxUFVWmOdVjAtEfqQRXNru1sII5FN5HGGZ3HiBZSGFTQKpOoksq4NSDUHqYZtl5g5Huzul3Z3FvtN3cNDBbI4tjLZo0LEVDySCJowqwSzUI0AqUZeu/7h4/cu88hVnL1O7cXhqrE0q7lhH8PrFys2PozNVU1H4WqlOInrpqFGmijWTxSVR0BwhR7jvr7PtdrbJZpbXsgkkWByGXQpbFQdNWWjGhNNQTPHo39uPbS+9z+b905k3ie8v9ktLi3sLrcIWAljnmKxxy0Ck9pDIgdVDaXmbSFZTn3RiMJvavp9v1+WpTRZOmbc1TuOoxFLT4jK4pTW42i2iI5KmGTNMMVVVM0gq5JvD+rQySiOMn2d7zYrSa/tNlYzDTD9PG1XBYBjIaAqo1LTtoDUVoc9Sdz9FsPu/zpacucze60TWU4l3GTmG/gpBJDCzwxWatI4uLphbSM/6xZ0CEIrqyxgL9t7GOCztTJg8xV7px9HjDjtqYCPbuIxmAjpa6uTcGRz1XU0k2Cx8tdjsViGx1BSTNTml8bNHL5GdwMLvcrpraylvoEtVNDdd7PIHICJEoCvUGRwzOKgjiNPUA7JyNsEHMXNG2cn73ccwRxPLFsRFpHa2c1pEXu7ncJWkntwsgtLVooLWTS4ZjofxVFQ6/099l/wAJ/h/8azP2P/Fp+x/2YTq37f8Ag/8Afb+8/wDdv7f+9P8AwG/vD/uR/gPi8n3X73k/5SPZp+5Nn+p8b93w+P4njeJ9M+rxPA8LxdXg/F4P6Xi1+Ds/odRD+/t4+l1fULo0+Jp/e+210fUafDp9Vq1a+/6bT4unvr4f6nU74yxz5fumHaElHhNp9l7poaqvSXFSVmUo920eDxFRkaOkwcNfV1dZQ5ppqGSGVQqIrU7SU6mLyLGr3qdLHbXu2LSWaOiPq7QgZwrMx+HQoNTnhxNaHoBxXdirbu27W8Vvf/Ry3J8Orifw4i6IoZiyu7CjcAKHQKVUC7kKzsjbUuB7V6tWKv7R6g35l8jtzBVdOlfiK/D56WkpN07V3fT1VVAlbhsxj6GSErHLT1STSE088EpL+97zt+17nBPtu4gjb7u3WNnRtLBh8LRkcGU0IORgVBpTop2t9wSCNNvLSbjb1nQfgeNtPiI4qMOMHIPoRU9Kqg727m7u3Pk8x2Z1f151HDtOKkipMBsna+bwmEr8plFrMhm8zWDc++995bOzxwfZ0cNVHViKOlg0JGHWYeyjbOXLHlq3lgttwu7oyEFZLqUSMqooURqVjjCLUFyKGruTXgAe2t7PzAjxy2FvawkJEyWyuqlz8UvdNMWelMrQYoFGem7cWWoMjRJSNgcnjczWwUktaJqqmqsbIqRBpZ6Gqhjp52MjyGQ0zQRmAIoLubFjyCOVS2uVGjBOmlQRnAIJPD1rn0HSdVcTqCziFF0itG1EkavIUpQU+016AXcO+IKKtqZJ5qWgFM1M0UrzxJR1H7NZK1IFnLsZ5Y6dmVYyOFuL2I9rTULSv59VDwxSEyHz1CvDNcdBpPX4jt2LaWClFbBhcia+ryVLhqSLJ0tflMRFDk4trZDI0FW8m2XrxOk33MzRmKOBtSFmKhm4nktInlQqs4AoGNCAxpqAIOqgBx/Poy2HbLfma/s9vu0mO3yNJXwE1iSSJNYt2dWHgayQS7HsFTQ8Oom+ej8NsWPZGbx2bzGxdw9hZevoKCDb0WepFp8Dmoq6gy+FyVZUV0kmKq58JKadKL1TZCSramWB4Vd1RWG6ybk91bPEk1vb6dZl0kaloysuKtQiurgKVrXoZ89e2EHIe08sb/8AvCaw3fezIba3sxMrLA7SRSwzMX/RbQVBiI1SeJpCFAWIp9d/HjD7JbM7g82bxOQw320GOyuM3EIsjP8AxGlSKqpsnROVx9QaaonWPQaaMa2ZmHoUBVcX080kcSkNqqcrgDjgjhgeprQdAjati2awQz3Jkjo1FeOWjkjtoyN2sVeg+FeJPADpZ4TYu692/wB6MpkcRXbmGInqdy5SmrEgFVU49PtKaJdv0JiQz1aSwRzyVTwrHE6Rg2VgPaGe6tbXwFeVUDkJGT8NckBj5V8hWpzToR20N08jW8sUkszPoMZUFmwAFhSmXogOsqACFHA0Jedx9TYLcu+ctnsNnK/F1VIYKqm3FDFWYasG4ocd5TKuJmpsRkDltuVkETSSxfaGeq9V5GJdl0N/KLcRTQAxtgxnSwILEHhUaXHrXB8uiu+5QsrveLq9sd0ZHi0ul13xOJBGGNEZY3MsDAaiNGpxUFq1I/bMg6xxkdP2Rl9z7mwPe+HiyMu6G2/1/tSjwPY3lMqUuU2pmMFNQZvZe/5sZVPFl4MgaTC5eWSWpmyELosExPPBeRyGx+hjn2QlfCSSVmMRyaOrhg0QNNJXU6YUIRkCWPdbe5uF5hkujHzU0TJezWVrBALmqaTKhhCsk8kZYXAYxRzMzSO5YmpbaPcuY7M7QyOVrJaLHYmgxcWxNuVtTSRtubFYynfLVcm3sBWY2f7SjyORyORnaqr4y9RFEzQUNQlIWPs8nWGG3bQKSPJ4zqp7SaKKtUZGlR28PNhXoG7FPcXu+KrGOK1W3+igmeOs6LWVzFCytRHkdyGlHeF7InEZNXuqkyFF9tiaBqdsdBAtBSy1E8E+SxcTiGKlp52rVqKPILWHUokmilYyFvIzBgfbSjDVAyammP2en+Tp66nmjmjjt5P0UQRoGIZlFMKxNQ1c5IJJJqT0tttZNpMfXY+ppK2mbEUrGHJZRFMFaySywOEgiVJJaeOGq1gQxRwlABzwPaSdCsqkGoJ8v8Pl6dDHYb9ZttubeaIq0MVVklyGNSpFOJAV60AAoM1x1Gym0d2bykqt2bVwtXuBdpNDSSYyXIJjqDC5jclDXU1DnxXrSCWvlp5okOSp4zHL9ih8DQvZh57yzs5ILae4EckoahoSWVSpYU8sHtrjURWvTUHLfMvNx3DeNl2iW7g27R4kAcKIXnR1jlLUq1HUGZVo3hqdJXBD5t/cUqZXcm0sbDjcim3Rg4c5kSuVxIk3TkKHyZ/Ibhwc8mbxEtXVZZPA6UtdVTyKpkl8LftRJXgBjhuHahk1FQNLEICdIVgFNKZyoocAniRRte73Mdzu2w29tG62ZhW5kYzRr9U6jxpLiBzNGztINDBJGYgaiE+FR92DsHIYPE4TL7goKWoqMdUpGcTtzHTHIQZ/K1tJipa4U2UrqpIKMRZIVM8lTIJKelj1sRH+mPeY+b7eOaaw2+RPFddXjTsfC0AMxAKAF27aChALGmTUdZs+xP3a98utp2vnbmzZLu62yyn8Fto2CKN9yW8nkit43liuZWW1hfxfGklmV3igiMjIIirBA9XY3GUe7e4N2YinpMTh812HlsVgq3cC/wATzddkqTDRrmstt+tRq1osdlcitTUxzfcGGSjLBViVQPYluJ55tt2WC8Oq6Fussiw1RACaqGVqGoBAIFSG9eoI5Y2/Zdu5292OY+WfBteXbjeriw2+bdGW7vGkjjPiy208SsNMjBn8XUqPETQIAB0wdt5LrXbD4feW+6/PTZKiFRn9r7aoIMn/AAbL7rwzKuBz+64MQaF62vx9RMVojXZCl1R+aH/NM2hdtq7jepJaWOiNWOiSU6SyqQdSx6gRkDNFPkePEK87X/I/L8tjzVzfPdXO4IjXdhtiCVYZ7qFqQXF94DRSOUZz4ZknjYgNGKI3aVaoqpew8lF2FLBRtubP47cGQ8lFQYLC0uAxBrM3hKKg+2wD4SXcuXhYzfcV2TUTVUAhjVRFFqc/gtTt6SbZGZPo0OfFkeVmY6TUGQtoUUGlV7Qanj1j9zLzLPz1uNvzhf21ku/XMDj/ABG0s7GKGJTLEqNHYx263E5q3iTzqZZF0AkqoLGF21hKfGYAmrq0nFTio4slUUuHpsfR5aVY1eopmoIaealWNPuEL0tGFWIqFDgFg+7gK7L4acGwCakcf9VT0YbLI9lbT/Uzf20BEjLGFWTIqpAUigJBKoBTAqBWrblOvqfdG2cTjavA00GVgn/yalrpTHT0zpUmOMTDHu4q8dX01JTVTRurKxWMTQh0Kh9JSjtJGeAIx9nz8xUj/AeiO72uOaxisp4dMmJAHNNJLEAkAmqsoVs+g1KDUdGU25Nn97dcxYXHYLDbWzG0Zn3FvKbFJQrkI6unUGOrwVZU6pmpJZpSIKmsmlZ3kSIKrtdiSc29leq9zPI4nXwY9Woqa5IK1IB86KOAJNfIQ2FruN4DudsIraWGSKtvDpVomUE+JCzEsddCdUhPcAooeguwvYVFktxbpoqHJZXfmJxMMtDUT7mmpsFTUVVPjlauoaGVNvUVTlY3qJCJiYXaSNiY6kR+LVeSyZLeBdAgmZgewa60Y0PxEDhjOPMV6F2380QXG87q9rNJum3wwurPessGlZIlEigiFGkOokN2klfhcChK7l6o3DndpZHOVe+q7bteDgqbb209s4ta3bsn8RlTKYLDyz09XUbgzVTnRdq1KkyxtTQ+JnTxhSnl3Pwb23tVtxIra2klkbSyiPtZ9JAQKppwoSWqBQ16JbXZRfWF7eybp9NEqobOC2jMkRaSsscLZMzmQV1l9VAtDhadDF1xubJmrTGPiN0bT+SeClmL4KgxCQ7aXF1GMaqHYGN3huuCLDU+HqMVU1ELYCaGnnep0qsbwuHUjvkMmpJTbz8pyoKzamZiQwXwfDi7i4cKfF1GgDVytS/Pd2t7by228WEkG925V5Y1UhdUjsRMryL4SQ0ZR4WCXIAXSahLbuyGGostSV2CppJ8mkxpq2empKOnySRQxrRtFmqOCKSlp8nWrTtIalVbUReNWa0sh7YGeSCVbxqD48klak1qjEglBWmny8yOArf7TDY3FpDtUYdFAhVYgNekplZloQr4NGzUCqg4JBbdNbvLdeXbObilq8njTtrLbcxMHZWfh3PhoqyGPHE1MW36eKvekxOGjqTBUCBa5qplUNFEERo6JBbxSzQWEKIxcSyC3TQxrXicCrEE1JH2nzP7K1u7DbLDddygVNra2uLW3/esyTweNqTU8duiswSEPR9KzF2pVUoCkfE9N47GZCXM7Kzu6qiDAYTKZCpXNzQYHq3FJXWfL1m38FT1mnFYanyWRklhiqZKUMJSWaWSa0Zj9SVQDcViRpHGnSdcrHOlWOkFmovlqpTFAtTHxt3trv6jZ57iWKFXiVCTFZxGUnU8MeqkUWpywVtA7qsWLGgg1uI3JQdSxw4Xc+Zhwm4aXBiGrix206Tc2ToslkvuTXJlaGhpc1DhciFnVWxVVBNHGbIyNKtkls9rc7qGkhrdQlsh5DGNOKFa+HrAIrqX7K6ejrmGzNpy3Fb2e9Stt86RlQ0UCzM0gEhDMn6ngmpK6W4UqAXwJ+NTbOC2JLtjC4fLzbizdZkZarKZeokj2xR/xGkWauSExVFNisduKsylbO9RHUQALZTJUKwbVqZJm3IXUs6LYxKCscajxCwY5OCzIABp0nOe04oEdth3iZHtbdQkktUMhbtZT8QNSERiTVifzI8xR3PRFcNlZ91ZnGzY3HYXBUeCyIopqjcEmMejp5Kaq25hzPkqOOmy9a4pqmUukgKLaXwhg5Ht06Ce1js7OVZ5ZZHmQEBA9aESPRSSgFVFKcajVSh5udlcB727t7yJ4rSPwkJJ/UCmtEWraVYSDI8/lU9ITr2Rt07jpZKmgy1TQ0Sx09LQ4mGifMz19OzVNHGxqaaahqFikp1m/apyiCIaE8agsab7cfuywk8KSJGarO0xbQBgNUqQwrWmWzXJr05smxRcy31wfEmUmSGOBRpLDxKgEBgENONAPIUoOgx3vnN+U+WzK7b3BsdJaCrydZkczU9a4jc8eTkrG8sevb+6smdt4qGN0Kjw0oc6jIBENVr2lrazW0Il+oiR1VRGsrKyhfISxFZD86sfTPmv3mz3giGC1uopjZFpWmKFg7PShlhlcw1FMUU1qWIAqQHFFgaZq18lFja6Hcf2NNHkM7SzGix80k1IwhxqUQqTTVUpTytJHpnpU8hKsADY98ZGy5BjPBTxoDk/YMU8+g8NsuLeR3WKWK/jw88ZouooSEABoSwqGGVoa8K9LWthkjxdIJFeXJIk7BGqInh8kbzyU0tJSvUVE0VLUiSOMiN2jULZQDdi0RGlUU0j88fLNTTj55z/AC6f26Tc9zup724iEkooIqk1Zc0IQkkKCQKLUUxjj1GxGPgyCx4GalljyO4pKeCqbGI8NfNXV8iXjpT9nLW5VHq5FVDpWWR3XQBwvsuvxJHS6RhojFe49ooPPIC4r8gBnqQuUJ7G5S62LcLZknvKIGgqshYtXt7HaUE0oPiLEaacOkNuATxY2PbOQSWJMAcrhYcUKSGDKwyxQNLTYuslRikDNVSGMHV5Ano1jRb2st47dWa7hk1NKokZgaqQcVX8h9nn59BrebzdZrOPl69tGis7GWS2hhdAs6sBrEclPV2oKnVQFa0UdJjBbZaSlylXkMk2JgXCVmMrK2OrrZ66R6ankZaSeUFqupqpoo2gNNA0cUzPoIGpyXZHiDJFHFqZiHAoKeWfy41yR88dFdvtt8ttd7ld3rwwRD6O4kVmLioIIOasStVKAgNlcVNXuOLP7lw1RnspksZkMdQ4vCT0VXkMUf705iLGUiYKkx8+Rqs/S0WOxWNw8KmCjoaCXytE7TzBoovIWLJFYbrZ2tvE6wS+JqVSPDV2JkZiojrrdjlmcAVoq9zHoXybde8y8ib1v25XlvJeWP00kc0yH6uaFQLVYRJJdqixQoAUigtnZjraaZRHGGfqXA0+LjopPTmpPMIGgCRzY5alolqRFJDXQo0lHCsf7rp+jUum5I9mUkrzFkdWjU5r+KlaVwaAnyB4+Y6C1jY2u2xR3VtNFeSxuE8On6WojUVIkUM6qAdTKKA6dJNelxj8bUwilxdZUZRsbmWiWSmpqvIVJrvvJqkL9hjZar7yJ1rIzBFIkqSPMl72DKUs1vbzOb0RRm4iwrsACtKV1NThTNKEAdP2/M17YWF1y6u4XSbbPSS4gjeRo2LfCViY01jgGDBj5kAkdOdDW12C28c5ujeu+87W1sK0fWm1dyb3y+UmqNyYCuR8tgaDbdXVTU+ZwoxFZUeVlfwUqqCJYdKxshltbJLxraxsraLJku2SNV7JFbS3iChV9YU5rUeRGQ3aX+8FNvuprzcrmWZym3q7mWssRBYeE7UeMqaEgNQ0+GnRkavDZjdXTWWyW6trY/Z9PW1VTkd4Yms299ztvaOZ3BUPlqTaO16uvNbkarGQ0McREuTrWrf4RAsYZvPChD9g+22e720UF6bq9FuqW7ibvnWMeHJLMqhUrqLCiKEMhLUGkkJN43Tfro39lvEMkFtNOBcQ+HWOB5G1KIslnSgHczAhBpGKAkRbsLbuyqiiSszeF2dl9swx7Zr4cfmKGDa2Rldkmq46elwkctHjIMri3p5I6RlSoo1QMViT0+5N2u93Pb5Hu9supo5JFZdSAq2hhpKmuSK1/wBk56CW6jb7hE2nePpAkAEJBZWjquQ1BqUM2D/EtMgdMXyE7Z27jtuUX+jbD5zclTDJDJHXYvE7xj68xLY7HVlTkcljdw1NBjaPcFHTrTzlHoGkpahFkqUrPBCPuiba4pp7lxdsqISfjMYlbuoFKKSVJGc0IwCtSQoi3iRNl5Vs7iwW4u9xZydVvDdC1iCiRmk+pdUjmKqp/stSMNTiUKn6iX2fXisxUGRORrsrmMgn3NI7x1Mf3mOraeJtVDBU01bNiqV4AGRvuvKsRT9bAuy941UlQtFFcehr58OB+XRdZXlxLE0sk7y3L6SGNalCvFQQxUFfMNUClK8elZmJdvNiNvVeNrY6g4+VI59oLXYxp8cJ66oShqTT/aVlZZfI0iiY05Z1U8KRZOhk8aRAlGAqXoaHAqM0z+3oyuEtfoYZ3nV7YSBYrQSprAJYhioVmArXjpqQDShHSPy2MoUrY9yVlSuKqKekp1P3LrHUK00fkaJKaojWehqUj02lNWyn0WBUAFSrDSTWvEVxTj0T3dskdytyf0nCIQpqCNQ1YDCopjNT5Ux0hx0tm8PJTZHdU+AXKUOSgz8u5K7M7jyOSTBtkXkjrq/A7gwVPswx4Onr3JqIllgptErtEwZT7Rwb5a3wMFojLTtYAKBwHbUMWqaedKig49Hd97Yb9sKfvXfLmBpqrcqXaZnMer+0MckCwMsevJUuFIc0oRUSuucTiKjK7Y3BuasxG8twY7JRJt+rzv3uQraiKspKs0+bw0uPpMhi6arRJI6uheSOYCTTPGqSxCWNncVmEE8EQeNCpLlKKMEHSasCVIqCK5FQTmhPeSJrM7ts+87tc295ucU6Lai68SSTTociWIpHLGjoSGjLK1GoygFdSr/PVGGrZaHKvTfxDxbgzONoK2toaapr8fW0k8c9O2Iy1LRy4+HJTinZfLTSieeHW2tUZwWbSCUqUwraFYqK0OKGqk6qfIigNOJHR7zHv+1y3InlQzoLqeJJZAhkiGtXXw5UUxB6qQXRtUi1OpVYjp9yM9ZWNizMKCrFBTOc1SVVPS5PHUiBHLVGQpZq12iqa2igRY7xC8NvIha19wQxItxXUoc0RuBPyUgDAYnzOa+XTO77nuVxNs4rDNLbo0l1CyrJGuCS8is7AM0aqB2iqU1AtxxYJKyjqJXqsZuWppM5vDA4nFYeippRQ7G2Niaaj23s+Wg2xWVdPhafExUmutq3oVWZHqnMlJKIiiF1xHbWVvcXEKxGURyEMxAMksjGSTVICWrqoM4+EalGehJtW5bzzHumz7dusm4R2kl7ZwvFDE7pZ7faRR2lkYrRtMPhrDWQtGNdTIxikPb0LNFSNR12SzVDFXrBJXNgsfjYZ6JWjEWQXHrkKilgMMQx+Np4U8byK1XHQxMwR5JCGDrzM1raWdwomuFQTSyMtAdVGKqx82JqQDp1GlcdS0LGO33ze+Y9neax2ma6awsLOOVWeMRO0azSRjSfCgRQEaRBKIULCMu56BzN9zbCmx1Rk5d/bZ2bWU+rbeVwWcStzU7bdyFLUV1FlcecNgNxVEU8lOkM1JEFSVZjqWOyswE8GyPbyUayechxPFLDRCXqAQwDoCONScFcMfLqDdy9yoN6SEpzJb7VG9p+7b62vzJcxrBVpFaIiC7lTAVkRF1LKCyJivSV3RvfHbD2ht/fqdiR0uL3dkcjT4/H7Jqtu7m3BvLGR5Cho6/EUsUsWQbFz4JgdUj1GNCLrDkT1MCyq5LS13S7kspbJmmtwkp8ZWWNWo2liTQMD6d3qPhJUj27mveeTNki5i27mVrXbb+e4sC1mYpLm5j1QmaKAMGdVUMO8NGtCyMwaQK5f/7y1v8Az7faHm/vb/GPsvu8N9t5rX/uv9z/AAzyf3w+w/3If3sv/Dfu/wDJ/t/Hx7Oqxaq/VPT4a0P8NNVK/BXGjj516j/xrrw9H7mttXi6tGqKldevwNWiv1Gnv+q/s69minS76vxG2MhHiNybTyFbBkY8lQ7pjzOBq67F5nEZ+GSralSfJ0OUlylDmcalRIkdOlU6xxVBBJjk0vqZe2a2njDREFGRwCrKRkFSKEHzrx4/PpFBZ2F3awXUTBhL+qdBNVNWFC1SQwFQFrgGh406PJhMnRDIVsixTDNqIJjVPK5/eZGM8lafMi1UpqgZG1hmRxybm5TXFqXghDqPB4afl5AelBjHQXW+3Cxubh7a80WZ1glQKkV4Anhj5/PrrO5GGogkJyVHFUU9DDLKk9ZQUdY1MssY0U9BK1JHV+CenZmFOJZA1rqFOopT+mxjMbGp0qQCRUiuSKkcfOg+fl0I+WbMlLG77Y4tTTOC1DpjbSWXURqJXgBUnjQHoBd/vXYDK4dMltzfmchrYq+nip+tsBDu3cJcUzVEXnxf8Xx0y4uWCaLXUCc21AqCT7fjuUMDsk8Q0kEtO3hpSoB7tJzxxT5GnQxGzT3d9bra7PuE5mjkWODaYDeT6l1FSYRKrCM6lDMG+YB4dE37azYGRnytFs3dj7S29UYis27uPLbUzGDpHzkRiiy+3d0UlRPRSPiJqnz4/wAqzw1KzU8njMi3VDOy0TrokljFw1dUaurUWuCCARXAanlUVp5grmSC526c3kWzXZ2eEp4dzcW80KmUYkilVipC6w8Vag1RtNaUHe2u2cJ1dV7yweZ2hLR1e5MVTS5iv2Du9ds5U5OhjeTB0sEe4tm9l0dJ9rVVDtXwSqq5GMs33Ca429pL7a7zcY7SS1uVV4pBpW4jMiaajWO2WEklcK2dJ/C1KdGuwc/w8n2/MO2rtXhz38Sie4spfClBQ6o1USwXQUA11rUeIDVmpTownXPdOzexKHB47N0+79n77zzUmMptyz52CrTKVuGytXlMTNsVsXhMRW7ZbbkLyMJJjVRVdbUBHcNGpdE+03NnJeBJIpLFh/ZqhWildLLKS7rJqanALpUUo1T0I5fcW25uj2594iuot4VI447hpQzF4pGkR7fTHGYFiVmoO8O7VZqhT0cLcn+lCmlpcb2Fk6PcO6aqgwcu5qnHdT0OxJ5YshjXqtvV+5RgZZMdQZTK0CpNMXWOWplmjm0kzeyrZP3bHGv7rkc2CySIha4aYVVtLrHrJOiNgVABotCuAoHRDe21k0Mq31wrboqia3dYWjZizs8hcBytTUEkgklhSgPU2uw+R2ltDPTUNZl6HMUu33lx9PU11djamrfK+R6/CUEWNydG1RDkZNTSRSyOrtGGKhRp9s+Kl3cQO8MckJkYFlVWA0fC7FlIBXyIpStAfPoXteReINrtjI0sYjmEMhIbxGBLRpocPlwCe7iK4Ap0ROggqqupqYqn7agyddUZCr+7ppKc1sc9ctLRJHGk/wB3JAJ6SliVnWJWaKJWBFwAKgoBOOHy/PoItLJIi6npK7M1Q2RqovA1pUKBwqQAese7cATHEKZkIgX7eaugMmmcfaTRTeOQywO7MEGvUfEIh41sSvv1RTJoxyQetXFrMwJRKxKpXxErQ0GaHFccfKmB5dBpjJsVRUcGPaQ+OgamhqYBRzyzz1lW7UkK1joZJKWnggfWqvCTqkLNpAb3QCjVHClM9J45bYWiQn8BDFdJqzElaE1qAoyMcSeGelxTxJPRTtVSCSnooqmogqIYhUVVNlYqeNqTwwwPEJnyMuqnln8Wik1IbNGWMdmqMqtcgfl/scen4AkiUml0gBnGNRDgdtACK6yNJNKLUHhWigxcUCNU+CTKUslVNTUKUVRjUx61NBBTmKtyGNjmpSlXh5vC4WVv85bWnlQa2SOasAyAqKmta0PkDnB/4roX2cCQxTNBcyrO5SPw2jCa0AIkdAVKtGQpFTk8RqAJKj2HkaaPcCvR4hoNrif7Xc7bvyaR7ZrY6CtodM+NrKqvlpqaTMU/hgjgkTztNNpgVmCsEe5L/iUgdyLn/QjGCWBYEDA4hTU+lB3efQj5BuFXmuyltLKP+rYcHc13GVVtZY4pFZgJJSVRpkCooy+tgIgW00HPMbXodnbxXKR1ODxlBV2qqWjy2UhhodcDT5Z63Hyy1MGRqaqsoaZkjgCyyLEjyKlwzkNJfm/2wwsZWkb9IsiEmpGnuGkqApNSTRfX06yO3XkqHkfn4brbttltYKPr44r27EcJSM/UCSF2ljnd5o00RRKGl06mRSe/pXYHtrY+6abckWw9xbX3HlVFbkKLB7er4KbP1ksGNp6yrrpaeujoIpSscqx+eH7yGm0qJ38gaIAubku6huttfdY5fp4iqMZQdAUEhEWhOCeNSoOdIFcZO7H96nZ7/Y/cqL2z3Db5N/3RLi5WPb3A3CaaSJJLy4mMyQICqh/CeFZTDVDczSOgUlE3bvSo+O9BtnbWK/j27OvcJm81umnp8nPQztQbmzSS4LL496/HYmjmrZYJJHqjWZF08lSI4oEMaSoZQtNsTfJLi7nRYtykjSIumNUaEumCSFGfhUcMk1yOcvMfNT+z8/L+zbQZ9x5Ssrm4vEjuSh8G6nDwTRiSOONpmjYa/FloDIFVUCKysGnYXZlV3rX7d2t1zi90YmjglrdzbqqN71SVWNq/u9EeMjXb8NbkqSoxlaumV2l8xmq6lREkKwvNUGu07S+1/UtdzQyNRUh8IEMNPxFmpxBpQUwBmtaKBvcr3GtvcKPZtu5ZtN0ghEk15fncpxIkjSU8Pw4Fdu1wC8jMzapJKIqCMvKMux9jPSYrFNQTRQ1+HyVTFpqMAtdj42ppwiUyDMxBZKWFn0QOnpiitHG6+kqqkZGqjHJyaGhzkn1/z9BO1t57aD6tFpHGDocxhkBXFBrFKDABHDgKGlFFNjslj8zRz5ejMwmrpKsxU1DT0sU7R1SfdHH0SVEUdOSapSUiuEGkE8XanYVdYnB7fM1PDFT+R49GkUs4ktGubfGvVhQAe4FtC1AGWGB8vzFnLY6lXH0NUY1W1U0uuGCeeSpMcaTOyLCDKyCJuABrRVAY2IAS28h1OKEEJpCmmBU+vnX9vl0q3CI+I8TXfixvMZmmVfxFVBChc0otaAYr0F+cxOdpcbn8ntvdzUVLuOmgxeaxzY7G1tTV4HGyVFZLFRwSmn/u/nKg1lpqyAtO6KqE3QON1WWaKO4iOuIgqQSFqwI/2y/I48+n7rbpVtJ73a78fTTo5aMhS/hxNxpjRIQ5qVqSMHhXpY1eG2zjuucXSYxsviZZmxmGig2pRUQoo6eDHvkMfXVUsMGdxWNqxVxzQVUEuuSekLRgwFhIiNPqJtwJKqYxVy8hOoNqAKgHSSpABBwA38Xma3V3a2WzybdFcvFHLbwwwx2qIFIRWdnkKmRVkBfS1SzaSV7Ae0QJ8YmPo8FVVtLOJoa+lyLZlKPHaKM1EEH8KOLiw1TSUmGhxoZVZIzHMCVJZigU1UiZpYxKrNpKCAkgmhOvUWBZy3qaj9tekcErxNM72bR7eZA43DQjBa0CFEXTHGAMdpB/YB1Pw+/8/Ud3y5qj2jt+aTJY6GPN4B961lbR56WhohLU1WE3BSikr9t11BiWVoZpZsiyL5g8BQaGK59ojTl02U26OkaN+jOIVDJUkBZIyNEgL4IAXVihBo3T7bldTbyJNs2hDcSQATxtMZVlZO7xY2GkxskZByXoAxIpUdBjvqqy+4+1sRTxbixnWTT4/OCpZ994na4yGemFRWTbPzf8cllqpKT+7tWMjBV1lfSpOWKiO6BvZoggtNl8aSJrqBWX4Y/ENAQNYSNcaWFCFU04/YXWYn/rTFt775+7HgtWZLl5/C1sYy3hGRtVS0bFl1OoNaYrQlxm2l19ubfFbVJ2TTb0yOJqxij19Nl8nk3w1HPTxZag3ntnN/a4/a8WLoUY0qJQVFTPSzECUa5UeU4t57nSoNiyROmvx6KoLFipjIDeJUAV7lAIIocEAP7tYbRLfyqnMIu5bZzELPxXkEaBVdZ4pNKw6TUqFjYlTxFSCxtdmbSx2YraDH56mly+PhoRR4f7ajo56k5JyppKuPD5SalgykM0lJ4Fk8j+ISNOFYjQUt204jYRMFPiVfUSBp8+9QSpANaUzSlRWvTF/ukdjEu4bdaJNfRwIYllFULIQCWQh1bOBx8zngFLQ7HzdPu07Iauym4FweUr48Ps1M1hqyLB5SpyUM9bDtDJ4mgSWnyENOjxilp2l8HkmSMBnMjMObKCF9xZkh8RO+dlIDKFopkDcVzxJzQVOKBiLc9x3SxjceI+p6pAy/2JYl28NQAUrpIAHwgmnHJjK/r6Om/i2Og22cJV1KD7qDLy10mXw80VHkchXUtV/GXoU3BkKAUyrDDFPI8LVJeenkMqSALLuUyyWiS3XiAYEiBQj1KqpGnUY1atSSBXTRXABHRpEYRZXm9XMtJoquNtOrxNBDVap0l9JAFKmhYVXNekh3McbX17QUmRhyGNjloHomoaI09Fk6w494nkyFbT0tLjKytSCFWAoyax2nJnlLBEQx5fha3tY5JYzHNpYSq5JZO6o06iWCknz7QANI4khra7+73CGOFEMt9PIJlUH/Q/gKlRjVUDIzUkEnAAUYnI9l7C3Em4OtO0dxbKmix2UxuQq9vDB5yhkg3BgajBZKnw0GexlWtJkajD1sypUuq1NE/imi8c8SuPbhtO17/Zmz33aYp4NayxrKCrVjkEql9J+EOoJAJVsg1ViDJ93uFslxa/ubeb23uXkiF3BGB4augCKIGYBmKGtC2RUeYyDOZH2NXNJSzGKhc00kMtZkQ9bJJRRyIxad0CSIGvp51a7kk39iC3j1IDMAW7gaCgyR5dV3m8MVy4sneNT4LAySanJUGvdpFc18619a9OW1RStPR7iaKk3BW0i1JnxuQqq0RSLQTipmp53oZsbXmhLwMk8kc0LSxH0yaWVixcCVllt01wxHtEiBagsKAjUGWuagEEVGR0siNm1vDuLXiT7kQWKSMSQY2DkY0sR2kM1RVTg0IJm7RiyWayeilSmSSaokydW88NSrU9HGoEsReGdJIlmnkjiNyoWIFtDM4B9vN5ZbbYmW8YlDSNFFKs5GAK/iwT9vT/ALccsc0c6c1iDluJILmNHurqdtZWC31DW7KCQIhrVSaYUk5rnNuGnr8RuXcNVSNDhTuB8k+Sw+2WzNJt2qw2bydLXU+JhnzGXzmZyNCldH6KWonnNP8AZqdROgkqsL1L/b7Q6GYRUAefSZA6qQWYKqop0nioAOqgAGOhluvJk3J/Mt9a3V+s93LGxpaeIkNxBKyU0szNJJqkDVQjsMePw9BDW1UtVJR0T0VTQ17VaQU9FDBVVk1XFNNNTxiaqgdxE9RHNchl8aQrfg8MdxjwVkkLBoitS2ABT/IKdAS+kO6XNpYtbywbkk4jWAB3aQMaZYEkMwbhSgUYzxgZLc1dFNlP4cDUTRTSUdDj5JpKOXDmMyCphoZoKbxLFAkh108EDP5Y7nQpJa0UCCOJ2IqKEn+L7eJ6SblvF0L7drWzjLqxeOKEkqYKE1CUULRamqqoyK0ArWLjMRu+BsFu6mxmPGNxE2bxFbh83jm3rgssa7GlmlrZ6Wgx2T2rX5CplvDJTVfkjihVZdWmWP21OYLhpbUT6LqqyIyNpYBX/DWoYUw2OB8sHr1pb7ztdvt+8ybdHPtgS4tJILiM3ERaSE97aBG8Dh2VkIeoKAOGUMhE/b00NVROa6esGSnqY540do6qgoDXSM9Zh8NUUtDF9vR4vV+tqeaQurMusqD7fYzKxCRDwjkmvcKDBIPxVIpxGOJ6LY4tve3F3eX8gv0WvhhR4TFmyiMoAjEQNSdDVb4RivTsWxtJ4ctWbm8a08IkoMxnMtj6avyKQLAlJSQJWSUFdUTBjFHS3RqiRiIgGCra5an6Zh7XNGRQSBX1IBUfPy8/PJekh0LdyX3+MW4SkkjIGZq0AUMQ7aV00+I408KUlYhcRUY3c01bRTJW5CnyM01Xg55MfurHYsqlO8+Jz8yscVGsM7zNPCPJDJFqVHkKgIb2Cf6rbnWWlsrqrxuex60OVAqzYoATSpqcDIt2LcdsXYubLaSyH78ltne2vIarNA1CAEZmCoh1eJIVXXRNKFWfUq/yFI28tpy0lFm8picecGK6fLV2Wr6im3tubEUnklz+58JWTeLKQVOpIqRikRqImLNKV1j2XBxZ3PifTrJJ43hxIiKPBic08ONwAQRTU4qc4A4dVi2o3cUbteNHqszPNJKzMZpYkDK8kTE6oiz0Q0GsEmtK9Ee33g8FS0NGd6UuLxGB+515avo9uZSlxLZSOLVj0z0+DqJ5pU+55TXTlZpNKtHdgxFquQaQljJxopzT5f6sdRdcWKsqPuKRQ2VdLTGNghbiNZSpJrwFDXFRnpsx3U+aw/Xmak3jm8hiMLk9xbbyW3eoshPsOh3bm9v7mrcJLisZTYnLb6xu4qquq8lDRSRYmjSoemp6GSonhiDuETSXm3yTK1nITdx6xJIqOYwFBDMZFUjUKkEmnyJOOj+z2LmOw2m2sN7SdNm3CZPprLVb/USB2jaOPwHnSUJI8cehKUqtdOelGRjps3U4OLa/Zm09w0ODkliwOS2pi6TbP2O3azGY+Sbbu4YN1Zl8gaSapihWalijo/tjblirFlJB4cc6TxSWzMBqDnVVqnuUotOHma9Hd5tFy25X+33ux7jZbxDbMy2zW4EJWFkjDRTfUy61QsBqQFNOK5r07nLRV1PLTU1FUtiPNUxUdPFjKtKylzkdRjnrhFNULFUSxq8LyVIaWMq0aJGJNLJ7dYDUrKe5viPCozT/AFf5eii2YGG6SS3YQIAkcek1EoZNdCRXyJbI8gKgU65ZSqxNVKmOqMDuelpc7iYY6HPNt/GU+y8dlaI2nh3DuKsy9Mm2kwVPFI5qaaKZ5V0pGUMpZGEMgSmpC6MWddR1aCDQgU7iT5EimTmmTXdfppLmGaKyuFsLuJI0maJVhSVQAyNIWpH4Qr3AGopTTqw31e4OzcptbLbVxGPNXSzZPdG3cXv3I4mDbGHSbcO3ozPQVowVJXVX96ftWk+xespaZqynp2lSomJ9SW327aLe/luZJ1W4kRXaEMWJER/CCcLU5oaVIwMdHV5z3z5uHLNnytaWfibfbzXMEF88CQ0a+hRZPFManVKY07GkUMVViGbPSw2bRUWD2xUYfYsufip1yOS68q5qOmWfbtdhhSUW4JMiq1ObiyORxcmZgn/iEtPSyQTuNCTJ5b+9XEryzRyX0SFAonjLV1LICy/w6RQMNOa8cUFevbZs9mbZ9u5WlnM0dw23XEkSq8MkGlZfEAMplKl45DKUTSRQBxroWztLN5bCYWGarw5Vc0MvWzZ4YKWuoTrx9DFii206XF0wocXFlaeQ5CpU1tWFMPiEBj9b22yQzyyxw3CMkWlGiDdytliXfUTlSKAgeddWrCHn+x3zZbaxvN42WWIblHJcwXrW5SKWIfpL4UHhIgRZ43WR11tUAAoUIIw0OV3FuDGbWxFVuGo3HT0UNZj9uzzU+Mgmm2/X102WSmaehpUmqo6XI5aadPuhJPT07+OKZIdColuEsNulv7pYgiHTPJQkguFAqASAKqoGME5IJrU35YsN75jtdos4rmSXdr6d7RHYipTsRF8xRNVcqCqnDgHDnuHKVe185W0r1mXy1LWbchGSfHtU4qGiyklQII8hS1ySV5oQHolESyuPM9SyJrYt5Cy1g/f2228klvHbutyWjU0eqU4MKJkg5FMUGcYHO/7nD7Wc47vtu371fbtZzbPFBcXCk2jLc1Us8TLJdUjjmjZY21DxUeoVS5ToLO1avubMdc7oPXfWfYG6RnMplYqfO7c2vX5qfbOEqBU/x+syGPxWK3ImIaXBSrSszVNPJTpXCQSu3qZdAvL1rfWdtf7jbRTRxrqSWRVMhWgSlSmoB6nC5IpQcOghvG4e5u8ct3t3tHLW4XUu7XssFktnA85hM+ozIiLHO4aSH9NV1K+lywLHPQa7E6H3dszD9pw0mycFv7b+P2ntTN7pymG7A6+3LiMVNiFqJqysnosTuLPZOOiC1klPVRNQ5Gp/iVTFRJj/ADSwwlYOZ9uu3sfGeaOSSR4ohJBcREnUAKF40qDxUggFQWBIBIBye3G88vfvW2hjs7iFYhJMba9sLtNVsJfGDpDNOyqoDE1jcsxRUjOtQcuF7t6wzVBhdqfKPb9bldkV2OyGWwVX1pX4h5qwxUmSoMPLisFl2oKjZiTxQ0dJTVuQgSaCnao8KRASgs3207lHNc7py3oG8KqwkXOoR6VIPcUJZ6VY6VJqaajw6Vx892c3KtnyRz2Fk5ZeWbcbF7R1YiWRTGzrCwTwDKERFkkjVkWojVQZKgb/AHs+Ivkt/dz5J2/jv3/3f9+tm/c/w77e/h8H8H8f8Rv/AJD59d/tf3f1/te1/wBHzfT+12qnh6aeHLStft+H8VPXz6Cv709lvE/sObNFdWvx7TVr0fFSlPi/T418Purq7Oj2dc7Rp8JNPXR0tTSSZ+ryO4nElDjKCuy1PNNCBLkEgoaSjkyCBgzOIEfUAZSzAMaPKklVV9UaARgkk0PoM1+X8vXo2vYprOzZpLfRfXEj3Eqqqq+hqFHlCAZPxV0io7mrg9SMMKio3FlfC09QshqZGMJQPIpkcyKqqokiM6HSNFnYrbnkES3AVLO3ahAoMHy/4r/N1DkDMLmVJpVPcSCfgySMeX/FfLrDv7FU1bjI8rFQ1MW88RRiGjmq66oo6doqJp5YTTsaeSKB6mQBhMY5FjVLDk29kzB1LFGHhMakDj+f+qvQy2OviSrJIjosZ+nKmlGNCQSCRwyMdBh0f2zL2B2jj8PTnLYeHa+0P4jltvZikesyuTzNOWopavG5XHFqVMdiaCalSnMkcUtU8uqzJYRkXM9m6bQdRQpJKAHUgAA5oQ1CSSDXOBWo6yB+77vdtf8AubZGyFzE9pZNNNbOrPLK0alQ0Txdi+GGXTqALMRkgkBHfKTHncW5MLltptTVOdqcXLt84N4P43Wbiw7z0+fg3E+MyUxwK4mhz9K1JPUS61FSUiIaWBAHuWg8MD28wYgPrLLRQhoV0VUaySpqB6Z4E9J/vDz7fu3MFnvWzPCs7W4tPBctNJdRki4+rKOTBoWcNGxJIDgRkFo6goOyto0W4t7VO3d31mQV6X7imy1XITVOamgaTHRTU2U8muClgYiNdZkidIw59NljFskrKkZhKqmaaSMD0K8K+dfLh8zi/aWkct3NDfl2lAoxeuSKqCr1rpHAA8QK/JTt9f8AWNVVY6piyO7Keo2Xi2qcFkKrPQ7Zjgw214Zqj7aWtqoqXFVUk+Rqo2iEksj/AHMwCIS7D2TXt5HFpGgGZjSONa9x4UHGgAyacBUnA6HuzbW48dZbhvoVQiV3VCFQVIzRKuzCgqascDj0aHpre3RnWWNG1u+T2rsfZ9Jh9zZzrjOdZY+LsL+8eTxuIqmw1DuugeslzO2q3c+Ro6SkxlaErqalX1VDQCR3jC3MC80O8b8qQbfNM0qQXQvS8fhR6l1NFpFJNIZiyEqTWqk00lU9js1sm0z71aXcVuKPC1t+oZIyzBiwqWiZioCmhBA7s8Bl3xhMTjdt0L5jd+D3vm6rGUebzEe0994vc1Xj8nkMfT5KGkyeapY8zHBWbfpJKinq9czQ00gjR41KkMVbJf3V4901vt0tnZrM8EX1Nu8KlEdkJWNjH2ysFZO0FhUhiCKD6+TZjvEFttsZmkhtw0zrIHklnWjMUm0vrWNa1cFkoAaYySmGefL5zMQY2jeqpMOsJWqp6DEU01S2TnpwZ8pUT0uPoa2OnghMcdXKwMiwmNY1b1SDOnhhWZ6SseBZvIfhFTT1oK/b0XeMbl5oUsy9pEgLOkMQNZSuZGKIGA00DtTCkBQSSQo7TzU+yH2nm81RirxuPysS5vFLWzQoITDVKj4eipECUFbUUqTRIar7inklnGpVAEyKIU+qLpC41OvY1PP+kfMD5UP+Don3W7PLku2zbtbs9vBOBdW3iUqtf9BVRSNmXUAW1KS2RSjdS6bcu2d5Yynq9p4HeOKhcZKGiym4dnY/FYzMxxVLU9eu3dz0eazmGrTha9oTVRtIW9dwHVW8adYrqCR1uJYi9AxWOQsy1yCyFUYahWmPL14iS+v+XN02yyutg27cIYC0kcc97ZxQxSkNpcW9zHcTxSeCzJrBNe4cV+GFunGY+Y4vHy56CrgahhMFDSy01b/E6mrp9JWJqenq0qZqSjYVRjGotE0bM9hp9uRTmRSdOKn5Y+dfLoi3vZrW1ntYReLITChCIQ5Z2wACoYFgtHpntIqfLqUJ1SnojSQJGuGaLHiJZJaWFzXUdPDHGTFjYqiogRUZxqdIkJkGmRwH9205NTxFf2H7erLKY0gaOIUgIixVQdaAAGkYJHE5IHxYY56ALd+48xtXcsdbiKjJYyrxcVRkaLHVFOtViZMhjnkp8JuWpofBUY+vyWGhyXjR8hSHwQIqeRmiUFRFFHcxlJYlZCQC2A2k8VBqCA1PI8R8+gpdbtf7HuUM9hdSQXEB8WKJxqj8WM0hneMq0TvCJCAZEOlcV7adKztHsXsLc3SeJG7MbDTNnquATZzcu5drVmV3NJQZCpqslVbK27icPhZNu4OKqjpEnp1R4V8Mb+WeSUNEm2uysbbdpzbOWRfhWJJFCAqoAkYs3iNgkNg91KAAki3nbnLnjf8A26s35mRCl5OGW4vJrV5ZdDOZTZwJHE1tb69OpEUR1VSS70IBHGdq7vw+0cTsjGtiaChpqg1mMy1LQNjs3VxVeSMlZjk3MJMdlqDG1NZLOKqSGaNZDCsesLEpU5l222lumvZQ5ehVlJqAKcdOVJwKClfWtSOo1sud9/seX7Xliya2jtFlEsM0cSpOxLHUi3VEuI43Ltro6q2lR/oaaVI8eOXbAyW5sFMu7a3MZOmTPRVqZWilimpjSQ4/Nw5CpOPGLxtNilanlNW8gXVJ67k+0lSZTHBMTbIAVU4NR5g0rUlvT08h0sfwG2kT7jtpG9STvruVfUpjKgeHIGJQIgjBVtVaFq6qjozmx9j11FjoJ6OSbMVGGyzY1cwKs5SX7+KGBK+hyWQp0MQTHOxRqd2107tpKqwIVO9xD4rIzAORqpwx5UHp6evQjsdk3EWS3kELy28cvgeN8dHAGpXcDSCvmpIIJoQKGh3duYlsVgTQnz/f19TjaWCrkNJVSxjzyVc7xJVIYZ5PsoFiWKThWJ0m+kArmlVmEjFdCAviorjSBUf0j5deuor6fc7fb7MzLAIpIJ43JqCSrhyhIKqIiGBIwFJBAHTDnHppN1Y5hQSR0y01HBTzSC9KXRpKdMpGajzpj2rJbGRWsrvExJJJc+WLTDIddWyzDz8jpxTVTy9K/l0ebVf3EtmhuFRpNRjjIpRclVINToLYrw1UrxNehNraDAyS4/IUOUqqZ6JIqLIffR00tNRVU0EFMwTxRLFBBXVKkwsVlYqqHU1tZJ0kvXW4ieBCGrIjISNSgkgZ4so4io4nArTo5SSx2maxkundz4q2xtiFMqP2B5NPxeG1RQkHK8SR0FGfwmOqMZXYqRkCUFfPkkqZEqayGepSXx11Pj6qhEitT07gOwqrIwdlQtYAGwdvHhuAranQKQKDyqpYHzPDt9M06S2UzS7ZebTcMotIZ3kiaUMXUaqMKgggAZIfBqaAngx7Pycj7cyW00liWnyckm4tu1lRiqVJHy1M60kuCrBQSVk5gpYqpiggkooquoCySAtGFDlxAxvLa8zqX9OUBmC6WzqAJVSagVJDFVqFpUkllrPbw2W6x6w7Ohe2LKhYUoGjZVLMtCxIoYxIwDNXSAFtVVuRxhpINxTZfarbFoExFB9pT0CvV7hSseZamtpHogWyBirBQKtTE7tOgGpE0KEMRjYyTWXhzNdyeJVyT+mVA7TU9lRqwQKHgTU9HtxtUd7Yiy3lLiPZbOFYphDQgy1XLAAUk0sE0kVLKcgdBltTZf8AePKVW2JcNhcZJDMM3Ft+VYoYI4PLJkWrYPMakQVdbW1Es9RMwdVeXU5Ae7HF5fJb2wvm1NHXTqQVFeGaUrSnAZxjPQWsdtWK5XYbiZBKpEix3GlG0tWRG+RkLVrQjuFcHpw3TgcZDjp6efDUNTRU7y0iU8eLopxJHBkpWdPL9nPi8pUCukkmiqJiHe4/dH6VpbzM9CrEFqP3E5JUGtCdS4AqAMHy8ypns7dEkS4jjl0gqUiVax6ZCtGKqyOWqSpY5AFGB4IjC08EWYmapqxUVPkWnxzRQS08MMdFdK2jyVVXYynMw+3VDTGMVRlJMUMmpdXt+QtpOmMgVqfX8gD6nNaU4kU61ZMhuVMt0j1iaNTSgULxWQun8I7aay2FRqioN3tnBR4+hoUq4MHmfuXoctlEycVTVVOOw9IFarpK+OeCswU1PUjILKdCSyGaNVZvGsqOUNcm5eZlMsYUNEmmgV2PmtCHqNJGaYJoMggH8xzxbS1tHMVM8kkcwValxrViiEDBVwQfOuOhSxux5KmPb2bOR27t+ixcmRmny+OocjlcpS42XFmTF0LRS1FZjJ8vQvTTCnpfNT2ip2lAjkKyewzf7qI7+7slinuLqVURIHYKhKsSzAYZUIYamCmpYKSQKdCTlxrjfOUbXXCkNlbSTStc+HSVy4SI6nABcIUJVGYKhDsAGYkjjV4jK7Y6/XK1dVSUNHl/s8zUU+LwldXVe1cO8X2O3Iczm6mtnr6fcEO0tJfxeFoKycpHEVj80xATDfbrH4VZGi1RVaUKJGBq+lAoUoZsZqCoyc6QH7ffxv73FwkQTcLdVtogIgaaRoDSUJx4QJXV+LIFTXoqPZ256+uyVdtmn2/i4NrUdJhanFZbNTtUbgepXDTREwK1b/C8fiklqFl/bhSRp01vJoHIs2OICBNwnu3a7kZw8cQpHl/Pt1M9FoKk0FQBXoUQcpJY30lpZ6I2giTU7SAPRSWpQNRU1SgnA8mJpToLKxkoqGX7ahqlwss8UDxxx0VXPUUqR0stMEVK6npoqyacIzedl0gspUJpubxGeZqF1+pRdVTqUVJOripJUDGPlmvQmuYdmsJoJZu+0mkKiNCkjUijAjOlZAFZy2rvpXPbQCoX7mosRDXZAzD+OVIaJFGKjnocTS1Uv2tRFGMw2qqqoWAlSf7emEPpQrLLESvtfatKY40jBjUiq+IauRUj4RgVwRUk5IKg9F+4PBcSzbjc2wlAakyRKYkRiAygSfEeOdKAAUoxXHWTEwyVuNkXwU1FHS08NRLSRwTua2fwxL+8z+OokMaytZAxjVdTaC1yr8rmGRWNWqaVqKKOP2DI+3gK9IYLeC8g8NDEknhq8SAEs7GgJOohjQHFCV4mnEjhtTcMeEzqy1GTSHGz0uQjlklIgpadFAkpoxHChSeWWCFEA5l1svpHJUv3+xF9YGJLcu4lVkUca1pUEnFKk/YD+Yy9rOZJuWeafr5d4jtbeSynguJXJCeHoLCNgqkuXKBVWhOorwyVSW+8k+bytfkKCprvty0CRLM8rLpx4gp2SCP9kUVPkZnvYC7BtJZGsS7tlmbGyhhlVQ+SSo9STnjqZRgn5V6S8678OZ+Yb7cLCadrYKirrYt/ZKqMUoF8KKVqlVAFAwUmuSnamWfI0tRHTMaXIHKU9QtbWTSRU2LSmhlMtK7vLE9RCsUZdktJUMTo1cqPb5Uppc1MWmhAyCTSlKD/ADDz6L2uGuVngiKxbiLgSo0rFTEiBqqxZgzDBOQz8FrwHUTDtUSR5SmkkqY696pEqKxaamo5J6EIklTXLNFHVVCSRVLMWY6XhXRZi5De25hVozgxgdorXPkKcM/z6MNqEgj3CNxIu4vL+s5RVPhmhaTVRmGlsk40ClDqNelfX1GQjpYxRR5VqDHVdGd0UdTka+TBrh5KWslo56XCRwNBQnFzV+qnSMNKdTj0OZC9LaOPxvEcx+K1RG1AHrgN3cW1aRXhwHEUpbmSW5+lENnbXTWkBC3atJI0CxspePTEFpCqGQlBUnJwG1FlTtmllpcjIseUzEtQMUZ548TSVlR93B5oZJkojUUWNwdRHC0aMwlqIHDKAjBg0Z3fXMawlmWMd4CmVgACRQVIJYE1NKA/ZTPSDlvZriW/treOO7mDQPNKttGzkopBagdEidQFBIZhkChBGk5cciR4ZtwyJLS7d3LPUT7f3JG1VXYKvo0gJkbBquHeJpKapqY/uTTTMjhyqHyNr9vSV8WOOoaeJRWOvdUnBbuGCAaVHzOMdFVrPHJHurW8iLZ3cjkzUDJp0igQeGxjcaxqKsKg0X16FDsfDZXb28q3EZTAb/wtRmKDDImX7jx1Nj947mxe4MdDV47etdiqLIZSm2/T7topadY8Z95ljSqAxrZXZiCPZZVutrilM1qwjdiItuYtFGVOYVYqpfwzXu0x6v8AfYHQjv0NhfiKOwkhNxbRW8kt+sZZtaBTMNJYR+Iw0aSXZaamcMWAyYGWpzclHgHz2TxVFR4ebFZGXb1Ft/B5JMNDO9LkJpslj6aKqerxNFWR0qNPUieWapjgMoFkjY3EwWdvLevbLIgfxkVzI4LtTSqqT+JxqwKKFLU8yINrs9y3a6tuXtv3Qw77eL+7kkfwoYlRPEkkd5oo5JEighFGpVjXTUgaAXbv/b4xdNvhqTHbkyvXWSyeLjvFumWt33DtOoaShqqWL+K0NRj8puKKlhFQPK7+Wzxa/WrA72a7a6t7GXxYxerGQw0FUMg0kkUJIj1Gn2Gp4dRxzJsW5bBHuOzcwWjyK0sMlw9pP4sghbWGEYkUBpSqllD6SaaaDVXosmR69/0a1rb12vX47svbh2pUZL7HMZ7D5muq9t5ungrDmdv5ulx1RT7Z3JS06RrUU6oMlAIqiBirv4fZws0N5CImQwHxNJKqyUdCQQwOkula0PwnDCoz0FLC3uNjvLrdbLw9ys1tZCYrpo3drdyP1IHKyfTzgAE6f1AodQckEPtmbsqM3vDb/ZnadF2BncDBkt2QYOj2Lk6KiyGa3fUbfNNsvr7FZbJYLcS7f24M6KMZOlqvuZJ8E1UtHD9zIXk1uEE0NpPYbHJax3lY2ke5RmRIvEVpnKI8ZeQx6/DIIAk0l+0UKSz3Ldd73Gx5n5ka/ltmllhtfpSCZbgxhILON2VhDDXQsiuzVhLmNGYkMNm26zce00rKvN4mt3JWUtTkttbkbA0dJmTUZiCGejQ4SkmbG0GPx0kmLeUT0glpcpAGKKJNBkTOYrkrpcrGQJY9WoHTxoRxBoaEHIODTyF0B3nl03YubJLq5SSXb7xofCnQyKGQGJgNGgmMsJIyyTKCyngSzb2p9p7iy9HLktt5Lbu2KqemrayhyWSbEU+Sy2QhopZKbJUOHyujG1FLl6iVCal3qJIxpp7ArIVVr4sUYCyq0lD+oFqaVND3DBpxx0GuYm2+63PxW22SDbmKyNbyMUUuyoWUrG+AJK0q2qlKHgehiz+dwGPpquhTsTDNkqujp3EmXyQxNVlpaOnilkylGaqOlhrKJKwGCmx0cctQpp1Mcba4gyCESaNUtiyqGNNIDaakjNK0JGS3DJqcHoc7teWhkk+i5rilumgXX4sjRNKVVGJXWEDIGqkcIBesYKr3LVXYqB9t1mbWTD023P43n8ZhchQ1FZSY05MPtnITybgSXx0lLBuHHVMi0ktMtM0kkDQGacPJHZLcBbkRGNvEEaa1cVNKOBppmobJrUZBoCB0Idgurjlq+vIb2x+kW9m+kuYZGWLUDA58ZXNFWWIsEK6CSrLqcM4PS1zmRpd+YbJUUVTSxHbG1I4Mfhq3KFqHNZKjqIKyXHbobIYGE5fHVX8DpzLAqT08wIElpBpUM2u3ycv3Inig1te3peZynwqwNNGlzpoXIqc0rinU3c3c7J7y7Iuzbnu3gpyvytHabXbG41LNLC6M6zma3UyqyW6HwowUZ9NWDkjpK4LIYt8QaKmwOP29kcTknyWXyL1z0eU3jW11YMlJlIqbJ5urooftpKpMfRUdBRU4MFOsn2shLTexE0UyXtxM93JLDL2xoyqY4RoC6QVQNRqFmLsckgMoovUKWd1tibBa2A2xLPc4blJ55fEMc9yxfUXRGfSuklUVI46kAOUPFWrb26aPsztmv2Fl9wrl8jtHb+a3f/AExO5Jds0+4sBPLTxbXzjbNXLV+8c/HBVpFSGagjo8fUTvFLJFM00kN7i1/dO2x3FnbEJJIkVUZA4VyNUi+MyqoB7mANSq1UNhSTx8zw8y847gnNN0LiSxt5LhI2jcwiSNgqx3DW4LzeGrYLLpU1ViGLHpSbF3jldl9p4XeGMwe092YKKppKze2yN2RPltq1lPU0lfSYmPcG2T2Xsyr3Tj9sV1ZS10WKojUTippkllEkEBimK9621dy2qbb2uJ4blw0cFzAdEyGnc0cvgyiFnXUNZAwaDuI6FW3Xd3+/oL7b7+OGybwbjcUiMbqo7vDUwS3kIuUiJQiGMO3E00oKp7I5LHbcpMjls6KWlqIp5q6nnxNLjcBSYipjjbKTy0WKgNBj6HD6jeKnC08MCosa+gAgztopJBFb27EwhNBEhZyy/CAzMSzNTiSSTxOeke8TbZsttcXu8Qhb/x1khktlSDwZQpkLJGAirESQQgCBaUFR0QPdO4di9lbmyi4faWR27U56rp8pjo9v1Gf3U8ORrqGjqdy1GbhyuRozWJFOlRJooKWlhpFhQIZ4kbyiGzt9xsLdGurhJClQzMFUkBm0hQqkVIIFSasSa0JFIT5m3flHmvebz+r/Lku3xXHhyQwW8k1zplMUf1DTGV0LDxBI4WNFWJdCgyKrFw4/gVb/xz29/x+/8AAv1VX/A3/jn+n/j3v8f87/h7MfEj/wB+Sf2GriOHr/p/nw6A/wBHP/Bb/wC5vg8D8Xpw/svlx+XV3OIws2iGkNRlJp48FXJTNO708ul6FVeoqoFmqTjzPSzlWpYqiZFUeMyuQH9hKF9NS8cejxFLUyK1yFNBqowqCQPWg4dS3zZdqbSykiu5GulBVi5NWWoWIN3NoYodLKCwXTpq1K9JbrKnmbI5LJ1VeFioYqqPkRtPUSSy+GKliRnVnYRSKoAIOngHVawj3eQfTW8SZXz+XnU/s6iy2kmosTWoadpQprwFatxoagdRu4M5t3FdT7p3G81XBEKvCbYxtTR6P4u9RlKqkjqKSioIqqNcpXVwM8qREBjFSsZCEBHsi/WkvLa3VwKK0jrjNK0NTwC486VPQv22Rtjtdyl3Gzk8S7bwoJYwzItHUMqkcZCpHYRlfz6Kj09trcPWMm49ybEehzu0934/GkU2Tgy8jVmGdlrcfW0Qhhx88dTSLUS6VnjZ5FkC6VkQh1G6RR7msEN02maJ9Q0kaq0oQeIz8uht7ebxvHt7LvW5bDDFPtO424hlS4EhRotYdHXSY2DDNNQJo3AHisZs9i8fis9uRzn9x7knw8OL2phaKZxJjqCTJ1KURq6czRpgsLT1UUsscMttTudKxa2lHooghC28SoNdZSRxNOOB3HgK+XzpTop3jdLq5K3l7dS3LvblLVA9fDjDtojCE0iiDaiqYGagDVq6C3eG2KbLbch3Ts6izjbp+6gr90ZTJ4SbD1GLyQSEVFNk6WqFRNLhqZm8MT0L1aqkd1lZY2f2tqKqsvAGgofL1HpStaevHoJSweLDNcW0b+OCGdmWlDQfEM9tar21wKg+fTj158ks7tLP7Jo+1cTsbbOF2NJBkMdJieucXlt05aknqnxtR5KtMgFrxTwzPKr1DhpvDZZP1EoNw2RLm33JbCe4eSdCpVpXWNWAxpwfDqRkr+wkjo75c5yO27xssvM9paxWNrIj/o26PMyBtLUo66yASRqYFiPiwejW1Pdvxs31SUGyNgbuzc++N17ozyVO9uwNjY/ZnXFPQS4NZMVh4Ny5jfc7R5iprqlaaNK7H0NLGsEdqkGRRKFrO05qs9yur3erGGPZYbaPwYrWdp52kDHxWaFbdDoVQCNDuzEsNGB0P9w555Q3Pb7bYOWq+POblrm+3CERKWZgYY0YyyKp0doLlQCFFRUllJvauqMPtjb/AFhjcRgMVtzBYZcXt+TbdHU0mKr55VgbKZmrgqxDVwTbmqZI4jFNqhWONmilm1CQmm32waa+3B3kN1M/iSCYglQtQqDTVaRipxkk0YA1HRLWBIdvt4FjEYDW0Qt+5QSBqrUggyOwUg8BUqzV6A7aNZQ7aq6enmpKaWoTcOZirMVFVVv2FU611V644a+vStyFBj6SQx18aVsEjyKPtYrN41MbkPKjIhIDICHWlRw4EggGuR2kDz6VbQLSyNJ11TJcSRm3JYIxq61oWDOiLUSDxFYmmhTUgAn2jRw7vpsjkGo0qsXTS01TRYXCvjKuFqyjDS11JQmR/wCLUkte7RxPIhaRqeHQSrMQVVqXtjHGshMgBBZq5BxU0xjjw4+XQf5mEW9i53BbWJbNmV0t4Sh0uACyqGJcVoBWtSooxB6SefpMrtza+G23mKrN0WNzL1UW3cPtbcFJRTxx5THvjRgMxn6jHx46gxWap6+slq2qJammjgaWMI8cYIvA0bzPIqrqTLvIK8CCTStSQ1KUoSQPn0n3GDcdt23bduu55ls7gMLeC0mVCBIrII2lKBEjlVnL6i6BSwIIHTf1bksnh3l23RbXpKXXXQVkuEr63c9FvamnoKOONc+cHXVpwFfjcxQSSLUGlp4JUlhRnZUgh+4du9MgEj3BJ4Fl0lDWvbqpqBU8AScfbhHy5Lc2h+ig2hFlD6lt5GnW5VkVf1jEzeC6SpUMVVSGWpICLrGveGFnpmWbD0ctNTVucSraGreoqqhaKkhNFK9Oa6FFNdJGIoElZY45mW6mHSFBdA5bBYFgMkYrX9v7PL58ehnzBYm2jjkgt3jjlm8QIxZyFQFWILAEnIUNQBiMaKaQg6uN48fkqnHY3OZjP1WP8dPjsbDR5eo01klLHj8Y0dVJDJk1qKoxQtBHCatlcvGkiqyMoC63jQsqrWhJrT+XD/V9vQckkht7O/uykr3PglqLoYKpK6QS7DVU0BUANSpFQCCWzET4Wu3kZ83g6zFYKmo6yOTGYXEUUuVNPRvUIlbLhqyfHUmamoa6IPVx3JRIWcoywvY4mSZLYBZqyV1F2agGMANkitePnmvGnUd2UtldbtrntDHZBdPhwxhn0g5cx1VZCtKsPKlaEKSBwzOK6zn2ljJMUstBDLkK3FiWr2hHJnswDk6uoko6LE1uSMMVZG1TPDRSCeldogsayUrCTSTpJfLO7FqvxwxKjAFSVGRgE4ORmvUjXdryjLtVmLVmSMOYmd7ceNINZYhY5JSoddbLGdSVXSA0Z1Hpf9eTZDa2NxkuK/ufunEZHGSbVWh3TgKXetZjq2vxuU27mNv7k2ploMriKXM0lDmdVNVwAnGuacixhWUJryFL53jmeeJtayloneInS6yKVdGVtBK0ZThhqDVViOjDbvqdq2iCW2NndWUsf0ypNGJ3RgHjeGaGQMiyaWFGSoUMo8q9DBsnDNtzaP8AdZZFnxGEWWnYFKWnlKiJaB6g09FFHSTNNkahlew1zyytNIzO7k3mYPOJyf8AGHOla8DnVT5YFfkBTpZtkctptUu00LbRbp4soXTqWgEJYgUUjxH04yxYs3Fujc7Qhw1HhIAYEZUwGNpsPHU46KIVVHjJZ1WJpjVERv8AcNKscCIskjupAPq0krySvcaa9glJfSxwTTypwpTuJIArw6LuY9vuYbO2bb2KySxtG70p+kUAjOqp7yOK0FK4rx6g7nqKXH5Cmq4BRLDDkpaespytNI6zU1Pqn0VaRx1H+VPVt4zGzK8gBVmCnVu3MlylwG1FyB4ZyMFu3tNRjTmoqBxGejmzs02qDYoZCBAIBJcM4FfEWMB6H4gzasAEitKHHWLF5td4tLG21qbcjyTzpiaSRKPa8GMz0Cw0dLk3pI8VlIsrLHRxl5opkhgnlkUzalJidqaKSzArfG3hShkPdKXjNSyV1KUyaKRVlUdtDkKGtbN4La92yAXm4zyNGTcKsSpJHShX49dRQtqAUk9wNaFs3LhKnGTVePoaGgwNLNMklVi0SlD0sNRNRLQGfJYXDYvEKmOE5epkSNJJJZAIIljWQxvWMyyxW8jzGVgpCv3CpANaK7u/dTtBJwO4k0rWV2t5J4oLVYY5CrSoAugVKU741VRoqSaAGpooABIQFJsih3vk2pdx0dXW0OGTJUOMxFJO9XiqjNR0FHW4TIZj+D0i5emy9GHH28nnaJHcsA0hVY1V1cPaQKIJAHqruWoGCaqPpDdp+zjT04ndlb2O7Xz3m72tbEt9JCAx8HxmUfTtO8YEgYVwc1byYmiwtw5reNLuHbWy4cBWR7boKWuy9PS4qkw4rs9FSv8AZS5re+48xX5CWT+C0xL4uCKugNR4WLLUyl2jftrKwNtc3rSObpwqIa1VK0qipQadVQTQVr8qAEM/MW9W+921hFRtpglYm1TSFLRgrqkl7tZT8JZiaiuTXpd7Jx9Bk8pDHkqWSHGnGZt2q5o8TWtFlIaXFwJU5qnkyE1U4p0nRbRNJGGCmzQxmwj5g3S3blLl60260RdzjnkWehKl1YhlOoAkMcgVAFBg1I6CVns4s+Z913Lcb2VrUQrcVAVzUlf09JYBlB7cE4AJx1HkzkOLwL0VTt6PctHTNkcn9/Jkcpj8xVUkkbCmojg8YBQ1aUD1PlhqzJGsqMImjjKGRgy1k73BmjvGjJVV0aUYAg5IZsjUBSnkc1PACaHeL7TClzaxPAhYvoZgzqQdIcKADQnH5A8K9JDF47KZHN4c1cklFlshWUc9PgIqGiSHKT08f7yUn8InyNdPPGvjlmlWSPT5VXSFAUvyzQRW8z+JWFFOp2OVB9dVBTjT7Ol8VpfyXltDcQ+HdSnUkSAFHogJzGSwfIJp6jgOjE46skngePNJBBTfZSssEAPjgp64oYa2kemipooDRtrYhQbSABiCb+yxleFmFqtWrxJ8xkhq1J1YA+XQbMO0SPY7rcyO80MyhomAXWFYoqppNaKtSaDiB6mg17QqOr6xNsUGOiyNXNk4IKbtDF7xiw1Bj81vRt5V742hxtPtqY1VRsKbblPj3kevokrZckrxo3hiiVgduEe8s1/cXEyoyAmzkgDExxeF3NWTH1GssBpYKENSKknoR8x3T7DtQtdn28TwgmdY1PdICIy6yKoULGGOpe1iSKVGnoz/AHDuDP57Z2IDYTLy0NHVjB5fL713djtwZmtmWarx+Dm29Dg8dkcdEHppqmhkK5REhgpkbxRapRJa02zl2w2yyfbSEepkPgx+GrswEjF1ZgwGNWQSTQZNOot2+a/vd8ubyCynjRnjMbS1Ck6Cjrq8gpJpSooB8x1XzuTHzZOl3NioY8ZiXeOmFLlMgtf4XFDGaZMPSQYuOvixkMjMiJ90RxqvOwtcRQXXgPbzFHkFa+GugEajUuS5UsR56fyXqTdu2RJ7Ta3XdAJvDljuZF1OjkhdCkKKqKp+ICnEnpAZM4iLB/3dmp6XHHE1Ms8xoamfIz5CoCpEIopl8VG1DA0ZEbrTh9Mis2tg2pXCblbr6/UzJKoFHAQKOPD4tRrkFqYIFPISi0s7nbZtsQIbmBwV8Ml9TcD3CgCgV4JUVFamvQV5aeirI3dEhljj8kYmmEjUhguiswkKPPH91BH+2CugarBfUR7NIUlVtJNKgUFRq8z9mOke4TWE8AniUu0btrNCYjkKSGNW7gKioAA4DNOnfbeQp6dA1DRq6VWNyFBPFEpqadKWWKSGVZ2mlkkp544yoEmrUki+oKOPbUqMzDxpOxXDjNGLA4wAARXy9OHV5Egu7NYdstWjvWj0tIBWKONTU0clyGAAFTwPGg6RNXXRz5JlmhEABWWKSaSKsarpY5PKvgXwxzYyqx0UZR4i8vmXgEJay0o6xhQwr8sZpmuc1Pyx9vRMlzbzX00zoyxnyNGJUGo01yhRRSlW1cMDqDuWeWtpZ418kVdWtH9u0DrH9tTsIpYqqmqJIJUSWKWM6QynmPm4PNVQdoqKDJ/y9Oz3LKJqaxNMNEdMaQCpBqRjI/l+fQY5jKFJ0M0U1XLPlvKjwLJTSJNUA0K5CapgpKkTVLawbSJ6Tota/DmkLWmEpw8vsp5fl0jF4xeMSBpbtp/7YYapoobVQlmJP4higI6i9h90bjg3Htre/Zc+9c9U7ibz5Xe1NJhqjdtdg8dLHtSl3PJHURNSKwEFRT0ENQKeGonpGX0KpLFO27RZWtjNtWwwW0UUFVS3ysas36umig4JYM1OGroR7zzluMG5bHvfNP17JP8AFfwCL6hoEP0yzAEaRSjrGDRXZCMUNZG1uxdz7qqxjuwtv7c2NWNhsVX7Xw+3arctNT7nofv8ph89l8pTVW4c/tur3Dh1VYXStejnp45mYQsoJQxhsbW3cvDcyT97a2l0VSoVgi0VGCGlRhuGT0XbpzTvW8R20W8bLabXK1vD9LBZNcBLlVaaKS5nDzzwvcRmiMWMZUNiMDgL6yT0dFJQrW4+oj/h/hmoabzxCXDfbQYyDHGBoBDUUU0EciSLTmaBwARoSyjZjhuHIlthpDBhqAIqO4N50INKVoek/i3m22gFnvDCRoHgkELurGNwImiIwGjddStpLKRjC46aJpKqAV2RgmqIYpagTJT0WWq5aajkjpEgfG0eI838HosZGYYQKSOn8MJUaFW3peKRlFSmBgah+Va8f5/PougkmtrqaUMdbDUfDbGVytMpTAqukgUAoKYedldlbb7iy+GpsHsrdHU+DpNv7X2nnsJvHdzdi4585R4+Km3hvGHLPh9t1+0v7zZtp8m2DTGzfY08saU7zm08pd4N5tkF4800d3PreaMwoIyQSTHFQEh2RaLrLDVgtTNHtrvIN/mTx1uLKGnhzpOwkRUqdT6jpaOvEpoPmVBqOj1dN9F1/YnYmWy+AahkwGMmqcS2RpdeEiq9urTVNCJaiPMztVw0GXgxOvXVzPPTRNGzeFmLACb3zVt+1WCWO4xab5kEpjlTxQJNStQaF0s6FhTSBVh21p0c8y/vflbZtp5t2+aRvqZWjhmtplt5Y7dEKu0lHaaMSYHeCrISCaMwITb2psvkf4Tj2wWElxNHuTItjMht6nzhxmNr5op5KQzDJyVT5GCio8Y/2nnrVqZIoTLENJLMbILOyhv7hb5laWMM0NxorxCnRpoU1O41YYajQ54DHlm83XnDmfYrabl5pN5hCRJd2bSupWFDKkksbVSQW8AbTo8E6FqK6RUr/cKYHa+1MvhtqYbEUMWaxKY7IYLK0UOB2dNS5nIUdPV1EGYnmxu1tt5OOGrqKhammWUS1xjiKvNKI3b297q4urX6ueUtE5dXjJZu1GIAWpZl4KQaUGcAV6HPOabJtG07zFy1tlqibhaC2mtLqNIoKSSojMZmEdtbzLUyq8XianKx5kfQSKT4vd/WWaq87tjNZiWvrsNV7fir1wmPlzFDhs1jymTjwWTq6bKS7fr4MbK1HHVUIpatlkdIZEEssIHzG3vYYbea3XwlkWQAlgpZfh1gFdY1UNGqOBoSoPWKgXdeWdyuNx2rcpvq2gaASiNPFRJVo/guRIYnCEoGj0uasAyh2XoSOup6dqOnwOCyFTSxsWGdxUuHlpsji6ynoVkpYoq+siM+IxtMkxnMskc0lVVO0QkKDWzU6sGMsw7+IINQQSa4GOP7KdHewzhoYts26U+G/bPG8el42RRpo7AsiBSDWlWYla0FStd14PE1X8NlGDiGUjqHgaSqxbLI9bDOZo448vTU3hpIchQsBGi6XRWZ2dlAU+hd6OKggjtp6fP8x1ffdvsq2zxwMLkMVlDrjWCco4GkBkIoOIySSOpmfh35ids5PO4DbFfX7i6wxlZmd+4iegmq6jaGIziNh9wLic9jqSOeaLBruGhWvq4R4aeKSQtKoK+2JJtsM9pBdXSKLmQR27E0DvQyKtCRViEYgcTTz6V2v9abDbtz3barB/qtrikN7GVrJDHKDBMY3QFiqCVfEYYVSSSARVa9OdpYHc/S2x9lV+Fm2/l8HvXc+7kqMjDk8nidz6sdisBgTtCjkpsnuCd8VUUklJXynIyrLMkPoR4/aK72p7ffdw3ITK0T2sVusUeGTS8jszsWCEEOpUaAV7u4hsL+WeZEu+W+XtrurLwzFeTXcUs6SOszlFjXwqB5GClAjEPllBI1DtUsEMmQoafMvT5x8HNha2tp6+m2Xlauk+8nzs9FhIYcTD/FcxQ10mYqFjcLTTlIjI7rojmMfr29itHgjcp47yBQjSKpKhQ0hzQEqgJp50AHEdCflfY7nfrfdru2iu3260sZLi4uoLOWeOF2mEVmHVPFeIS3csURcqQviVIPdRdVmJx1FtvZ+SzDYep3JlMOuXbHx1H22PxD1W6shhNu4mN6rFUtbuvc2S2/SQ5KVKbxx0y1sSsXkW5LxeSy3l/CiNHaJLo1fEWpErs9Q1Io1clMgklTSgPQi2rbnXbLO83yyge+VENkHcIH8SYxroQxCS7mdSHopGkGpB7CcezNldRzbf37TdjwDEYWhnzG7cVR7P29hcVuzI9rYTGT0mzsTHuunr9vZPBti8xlZsnPWwT1FfT0ULxyU8yOY5mdxm3Vr7aJNmCSTuUhked38NbVmDzP4YDiQsECKDpXU1Q4p0WvYbRa8scyWG57fELYbg089tHHHDKlxFG8UQWdVSQSWzTPIEU6ytVlGmodC73qcDsuTHTZqqqqarrJqWbHwV2ElzWUy0cZoosFU0NDRRwZGqyuQfJa6erNOoqIjJJA8gQvGbW8zXZlijCGlQSrUCmp1gk1AoVoVrUHBA80W42+07Rb7TfybhIfFqUDReK0vhFI4isaFZDIS5o7ItQGKMxBKhF2PveDe53FmMZvel6sptrwYPadZj85X0mTqt65TKV9bNVbgrNkzYioye3cuFoIYESeo+4pYaWSaRKJZZ09v7dbvZtFE9ubkSM8isi0ESqANAcNRxUk1AzUL3EA9Iect8j5og3bcLffodm+ijt7K4trqUu99NJJIzXP0phZ4JAsaJpZ9SBC5EQd16JRishkdr10dVUVtIks89XLUtS7hOSp82Q1GZcVulNv5epmbCzRPKG0JHNOZ5FEhA1Qie4hS5i0LHUCgFVAKjOU1AAMMeoxw9YA268uNmvBO86hiWLhZSyy/DWO48FyxiYFgaaWOpqN5q+/3MzGn7T+7tH959v/AAHyf3xoP+P28v8AG/utf3n2X8U/gX7X2evxf2df3X7XuniR8fENNdK6PwcNP+lrivr8s9Kf3fc6fD+jj8Xwaf7kr/uRq1+J8WnxfD/BXh/T7erbNg5rOZmphnzdCYNVFQY5qumCrjzFSUy09dkYYJat/taWWrRnCzVDtDAipI17n2GpU8FVCuCASxB45yOAyaeVM8R1JV/4F1tm4z/Slb0BPAAH6csgHctTUoC1SDViBQHNT0uc1iqLFxHLY9lakhpxX65YVnpqioaXTSQrJGauKT7tZvP5WKCMn0sfoF1tMZo2gf4yQPQ0pnBpw4U6jBLq+iukiuIAtx4hAKNXBVqk1pQAmgpWvRa+4xt7bu5Np9gYnB4zM7iqp32nt7FT18mPqWWppZJcjkaqum+6FDNQ0ME0stb4NViE0/ukm8cR0zwSOwU9zGgIxwFMVFTw8vywJdt3O7t/3Ve3Nqku6wk24IJjLaqsWD50FVBqwBNO3zNQux3am49q4fJ7Tk2TPtfZsn3NHvTdf8bye4shgMdl2gFPmNjnFUm3azH1OMmq53mKUtTSw08eunjWVI39sPtyTTQXCXBM8ZrGigLq41D6tQI4UoQa4JpUERpzRc2NnfbPNtHhbNP23MsjtKYVIXS9uUWJlYMST2lNNNKhgG6VvVWBlqptwbeirKmDYeJk29uLZtdT5DE5XMTwZEVjLE2Q8kmUpduU7TRyUUcyS1Zp6uMySlSFifmanhvopcElGBBAoBXFMV/ZwP5lcTNEstrHLr2uNEnt2DIz5JrVvjVBUlQ1WowqaGi4OwMHPDuXbceWgwv2a5OOGXFVU1dFnNw5PJGdaKeNaCibGZabGpTySUlBOFLuszCaMpHd1SDC7A+QpwoPXjw8s/5+kLstxf2jqEeBjppkMzNXTgCjUGQp+eRQdRNl7Bh39u3ddBQbHjrKjA42mxebr9zJLRVU0MMjVc/2VOIoIKXHywt4oy0k7VMiSswQJF7ST3kNtHE81xpR37VXPHA9c+eKYpno7g22O7uNzjj2yskMQjmluKoVIOptAFABTtoS1SGNBQUeV6+w+zsHnMFDtWGh27uPN1Uq0s2ZgzUElbTpQmpnjoExRqajGf5NCYwCEQehUGos1jcyzOrNICVUE9pGCTTJNAft8+lSbPtlnBPBFYlY5Zez9VXFQBqOhY6shIqKUAGPmRLoMxns1RUWO3BlpZUxFRDmIafMRYyhTMwMoQYHH1E6NJUwmkpHkhghcVSeNy105VG4t1d2iqJ5FKEoCaYJqQMDJyTjh+Zta29zam28eJfohOs4SXSnja3oQpYHUSFNFXuwa1HBNZTbg3dPCdvbhwWNqHytRlGx+6YXw9BiWioJoqOKtlgpo5MnL5fMabHwKtRVyQvCrJM4k90MzW0g8aB2XSqho+6tTQ0GSAMVY4FQTgYM7i1j3DaRJt19Ebpbl3a1nTwtJVCIwzAAPVtWiNcnS64Y1JeKtq+khn27TUc2QykCyMmRp56uhqWpagfws5Cj+4JhkmaUmopIqgQtHr0a7xepeTTJPbTh0CI4pnt/o47cvdqah1LBqHsxXBzkVAOaVx1l3LXYebFYsbuxf90MDk3zOxYd21tIu7U25S1MyUW45sZR09Ph/wCJbhrFxtOXljBqKKGRwqOqlnYX6gPI1p+rMlJjEDp1EA6anNFyR8/l5CS4n297Pb4d+tTYbXca9sG4PGLkQKWVbho0VYvEnOhCSDqjQkANglX7rwG1KrBYrau2etcdv58RsuorM92Gm3M7S5zeabHxtTXCDGVOVpfvNsV2VmemM5jiaqmRDF+6k11RWUt39RJc3V7JCskg0W+pAsWshQG0HvpQ07qCvqOhlzPZctvtlhy1ypyZa7obawdrzfVhuBNffRpJMTELmNTaFg0esLH4j6SKsr9Bzh8dsACh2vmMxXZOt3zX4vemCxtHUPmJsbmqqgkqKjNZOpqXeqStqKdVEsi5CY1MsShYCrsVOZDeFfEjQaUHhuT29tPhoMYPlTFeI6ijbv6us/7v3O8laS7kW6gWOsuiVstK5fv1MoBJDnUQBpNSQva2oy1PkMblRhvuKjGK2TbP1z4OupnmRqiGGuxVBQn+Nw1VQJnqGqjBDPSKxkMzaxSsnQhaqslMjtFfkaHyIr5V/Lz6ONySecCaeyEva3iSyeEyt8QLIq/qqzAli5QMvEudQTp83Xj9nbs3Bt/sbe2EqKjCV1FmFq9l5Ktkko6I5b9vI53GzLisFk6+tKCFoJBTG8JgKhJUjkbZkulsTDBeL9WKAuoIPbwqKmgPn8/2dNWVjsEXMFlfb1y7MvLThilvcsSNMgGpo30RtJIi0Kmnw6T8RDdFXNRurbdLTVW0J4twbMq6zdeO23jhglnhym1qOsyeTrIp8g9Dj9yVMuNSWrqaiSaGOnpooC7S6CIvZk6wyqfrI9EuhWdyeDUA4A0pwFBmpoB59AwXF/YzPFy/crc7brnighSMNqgDPIdTlFlOka3LMoCquosBRejVYzD9dnF42sp8bX4ncdQsNb/eSr3KKrbFJFMUiaWuxtJiZKmOAUDyOGglZ2m9V5C4QEqtdiWUjw2tx+FVPiGg4Bi4Ukn5Af4epClsOWxbWF1EbiHcXUEySTK1uCWALuqw+IqiOuFLHUKgmoToVsTiKDGYzC1EFVQxQ1GTXGVaVH3FJBXzz1UMGMosRDnKWmyc1TOZENNCsOtpFBKItydeOzySJJGdQo0YwaYNdRUkADgc/IVPRgdstbXb9vuob2FICksV6zsUDjWojEKSoruzVBVQvFdRAUE9G9kwlNSZbTHNFk9rxYGjnxEZQR1SS0VTkK2uydplo5o5YqWGSmeZvMqkm0kalbkFnPqgd51Md+JGWXNRVqBVqNQoSwYAU+w56CXN11uNybS12aZnsriRHt1k7WCBdGphg1Gg8ajtOfVM7m23kMxX46nxwgnXJNQJjfspg1ZLQwvNSUmueeoMCzyUzIvmCRtGjqXBa/tZDc21rDM8reGEJ1ah2g4YnAqRWuKmpBpjquzXV/eJpkD3E6wvJK2piXJopULUhCowKCoB4V6TmPipsBlK6knw75BR/EIo1rsv5WvOQ6fsJTK9VT0sf1YeAalU6lsPdw7zwx3BuwK6QdKU4A+dTQk/b+fQn3S0+o8LY9usGhlRhOCZC5Ku64FQoI0qQeBNAcGnTJnBlKaOajlyyrNAPJTGXN12QwuNpZxHK1HEtPUS63gKp5gsTBoyAg1AJ7vCYfFWQQ1LcaRhXc0NCcD8s1rxxnpbGr3e03c1sipbAupMkrlYlRwGCLWpOKt20KkacinWLbe5Ny7UyGGz+3M/ujZFdQVWWDrt5tn5H7qlykMElfJkKOv21LlJ3Zpp4187zTwwhXhKVDeT2n3Xa7bc4ri2vraO4VlTtkMiiqmoAIbSK0FdNAcg1GOq7NJZlIU+qurfZfEDMkAhfWVIcMwKB20vla6iAAR3NUOuQ3FXb1NfubdGWbObvp4MVFHmcqcfj2hpcTjY8XhKc4yjx+MhpqdKBSjsnlnqHMk9TI80jad2Vim1CK02+DwttDu3grqbLsXc6yzH4jgYCiiqAo6Tz22zz2k8M0mrdJ6yfVSNoIJJYjw9IprqampbizGporbtHFRrXVuTarqKSWFoKeknwxqMVVPmp/svs5/JqT7KjSoU6UvLDI9iyMgZvZpcsZIViKgqalg4DDSK1FPM0/YPn0D9wmFreW8cMau4YKclKAIKkVB4MK0PGv7cNBPRVAeKfKOuW8ORlo6unpJcrlUqoZ9c/wDF6qPL0clEMtHUyIkdTI0bAsY4QpAXV2Gi8PTHWHUNSkhVpTFKq1dJpwoeFT0s2RjcSvb2lvqvhRC7FsMDqP4lHcMUJoQaAV4Ytu4Wmp9wxzZuljws09LjXppa2sGXx8lTU0lPJJT0uQNLj6ahyemrgnipY5GlJCC8jgXYnkkSABHMoDNqCDSQK4qKsSMEE0pxOB0cm6t90W6nt7f6SR1EUckjeKviR1jkVWKIEJIBABJoBQtx6MDnIYqPa1dUz4KqhycBOOiyKVhqIaupgjWiNLF56Q1LWMRWZ4pXXyFUUJpdpCq0n8SZTHdobdv1CpWjKGqwJoaDyoCAaVOagABz2NyeZrXbWRjLDQGBTVGZHXgwNeFRj7egh6ywlHt2aTc+W7Ar+w87ubM0NXiuvsRt6k27tjrjYtIf4dnRvyryuOnzu6N+5ncsh/hbY3KCgxuHoZa+d3qsjFQ4hjeJdzvZprdbNLXbYkNLh2LyzzHuTwQraY4UjFH1oWkdwgAVC8swct262V/cRzbkL2OW3aGKBIUjW3D+H4gm1jVI4l1KpElFRPFGWCR2f7j2zk5OjMdvzHYEV205sVEsle2QapwWLSKqa9DUvXymakSvqIYkWF/JUVlbTIhQlYm9w7tG82UfN1zy81+yXpmecwsCJHZgKuukUNMkkUREaoIFR0GN8fmW8aLad/vg7WS2m12jwwxqiIlQEYKBqKR41Pqd2y5LUPVeW+9xphsFWxZIxUiVopcrT4/Elnq3SOpdcXUU9S0qUtDTTIkrJrV5Whdm1Kun3MdjEbq4hnQl5EJjZpKAZUagRSrEGlaUFQOJ6OUsrTYIr62hBi25rdaGElmMglfSQWNFGgedTQnh0j98V9NW01RlI0oZKEjG1UFTj6isjhp4qWljebC0lTC8iVYyVZKKiZXTzJJGiIyDyazKyRfFWBy4kAYFHC5JOHIpUaQNIpggkkHFEEFvuu17Ql8s+uEuqmZSe/NdNQTljRmGSDQCmahVm6Sjx6pHRMGqoIoa6oyVFPkUopKScwGSmoaiSjTIST+LUIBJBHYXPqFvay1lnuxJLKpVSfDVGCk1FckAlf2E/l0eb3abZsn7ssbIh7gRi8uJEMgXQ+miRsV8RqA9tVHr3VHTPgKSBauahly9JtbGZSto4KnMZypzVXjcDS1Ahiqcvk5MRiczmUxlL4jLUCnx1RUFFLotyR7cuZGijaVLdprmNSRHHoDOw/CniMiajwGp1Wpyeim3Tw4L4xyOm2zNUAln0qRxdlRmVQRk+HU0B7c9J87frs9ksdtfCPUZ3I5PLJi6L+G01flp5K/Iyok1TAcdRZDN11JSUsEclPDT07POLpBC0khX27NeRW0Fxe3A0Qomti5CgKorksQinjUkgDzIGeiqfbpfCtYbVvqJzUUiGpjI2TkAsVChSvrnSMnpEbc3NvXdWAojWZvJwbYqK7RPjdw7ewuFy6Cnq51pDLJQU1TmIqWT7CWR4qZjdbGWaR7e3GtLeG58VSPF0nKsSDw9SFPGgr+WOmoN93zcdoW0dnbbC9fDkhiWQZJGVUyhW0EkKaHixJ657nTEYajxs+UxWE3LizmZa+p27lpc+m3dx0FIkdRVR7iTAbi2tvBMPVQaVIp6mjqvFJwQUZjWRWuILiOK4kgnZComQJrjYg0ZdavGWU5yGWvEEY6Yv0az+iW5toZbYt4n07lzHIpAJ8QJJHNpIpT4SR9jVHrcmO2NlulKXt7rTqzJfGHBfxPPYfcnTzZ/tXe+Kqqbb1FSVzb62tmewtrS7gg2fuCKqEMGFmzG6K3H1+PrTJNBDPS00YHsL69h5kueXdyvRuEkcMU0V+wt42BcsrQyJFJUyoV1mTwoUdJECa2WQ9Thy1ydvlt7JX3OrWV3tNjFuEkEsTpMIruAoZFaIMjSssJjoVPiKCSBpIKgmz7s3Vt2ixW0t4Yinx9TR5GHIY6pfL0S0sm1d8Va5qlxuQpaGSkamydJQh5kkho/JGbJUNT+JkUc2i2sjS3dtIaNRHBU/FHVGOfIkUrWnmBmphnmS85i2u02rlbmCxjjktx9ZA6Sow+nvxHdRRusTeGsixvqICeIrHw5ShTQg/4yRJqakpsZlopFgx8NCKeSnernxtByKCixtXLLUU9FUUUN4IozTyokfKaSLqqaNQoagUaq4oKn5/af9XqSWtwfEMMMgkUREVIJK1Boq1qAVGBg08qcesddUzVcUwp8dioJ2pIKaCES11JItOJJKeTITvSQLLWS05eciGMx3V9Vna5LJQoGPiNQknyP5fL/AFcOjk3MdwIo1s4hIkaRsQWU1CgFm0ju0iuBSta0Y1q+7T2mu3shT5Kv3Lnq2jq5qjcOLiy+5amroqGlkmgo4YsLjcjD4Uiy1XBKkcTNNGgDNoRVB9sSzKwnMUI1ikbaV/FSp1Fc9oIr+QqT0/FtkqyWlrdbnI8EuueBZZW0eGW0Dww4ookZWAGQKV0gZ6NX1ZVS1fZORqaPJV3X+Mrqd6fP43C7mOHSp24Fhkr9u5GtgytGmeianj1ClIlSpfiw5f2GNzMS7RbrNAt5dxupheWLxP1fwSAaG8OjH4saePy6f5s2m9mtN0W1tUjgmtiujWo8KMrSh7tMhSmrSag1NKcegz74yT47c+4q+j2/SbYr5K6oKyV+ZmjzkEdQsEuPkioKL7mpNRUYidmjrvNOKySRQ0zgSH2Y7PEtxt1ujXQnhACnSoKEgkNkgCmsfDRdNMKMdIdrnveXIbKMnTua2KMLtnZJQ5QDs0ZDaeDVOqtCxFei6ZzMZbcVFQYmvlm3VS4+B6yGozCbRrsq9Xj3oAsEdSabC4/F5txLrFVrhVWhkdXHoT2rG12VuTcR24SQ1roLhaGoyKmo+VDjy6FUvNu978Ydpvtxe5so1Vla4W2eTUuk0VzHGI3OP1NSkFWIPl0ydh7cp6OlTceJhmpYoKdZZoaCGpzUtZJRz1j0U9Klb9xVVdQdRiYtEKmXS8moeg+3LSckmGR6tUCpoPIcfIf4Bw63zfy9HbRrvG2xaLbTUpFql1UZ9BUvV3ONPcupqMxxToNNs5/YuYyMFbRVmfytNuZaHb2Zym4aKPasVNSx5enocYlLjsZXilyMVVl6gyLUxSVtTE8aipMLyKrLJobmNWEqr4i1dUQ6icVNTQEUH2DOKip6Cm2X+xXclt9LcXEkN34drdz3KCAIviqq6ESQrIGkNdYZnGkawhIBGRtv5mtylBsODIz73fAbgh21if4aZaSq3HWU9RKlLTUMO0Zooc2j08qimGmphKNGZvLJJqKFbq3S2XcJh4EZi8aRpO3QukEl9dNNPxcOB4AdCa42q9N1Ly7FdjcBbXf0VuIseOwdgvhiBqS1GUPeoBGrUWqUxW5Who2y9ZPkc1s/JYvE53L0GfwlDNlaiirsFFJVRvPWQUVMuLq4Y6YhJC91kW6wT+PQFs6tMkcQhSVJGVJEc0BVsMKZqKeXnwqK16IdquV2y9ub7953W37hZRS3VndWylpI5rfvjbUujw3BXD1qrUIRtNOnabJbrl23tSuze4MnVZLdK5Te9HlqbCQ7Qi3xiN0ZGokpsi2BpaOOjpds0NXTVKQLSRUkU1QJUIJ9CMW0FhDLPDZsCIAlu0evxPDZFBozEs+sqyk6mJppJ453uW/8w7rYbZJutyxkuJZ9wWdYxB9QLmSpYRRhYkiR0fQERF1FwBwAGDcVPQ7Z6HqN4Vla1Bkj2NQbX/u9Pi8jJmd7bLmpDlpKzO5Spq0wW39u7aFIhmpqGSaryTVJSWMLGyyFMsgvN/hs5I/EhS2M4fUuiGQEp2gDxHeQMctRVC4+I9DCJ5OXeRtw3G1nmt5rm++gu4yjaru1bwp0SYs2mKONoQ7LGWMmA1KUYNOre+9oYjeOcGf2dUbm3FXVNdR4mHCpjKalxVPW4zIVWFkyNRmcltNBk3pU+4xEdJUvTxVDGjmpp2khRivnPlze932i2g2jePpIfGjaZsl3VXXUqnRL2vwkqAxTuV4yC3Utfdu96fbDkj3B3bdPcDkifdtxFtK21R2iWXgpOF8aJLlL4xRlJYo2jQREshlMccTymEq00/cO2MruLOT7eztHTUWer46yPD1+ZxWLxuRyVXJXJB93s+bK1NRNl8ZTHwfc1FJHJCJNKACSQoIYtqeGyso50Z5oYhGJgGLaQFrSWgJDEA8c0zXFYln59sdw5s5m3nZ7m3t7XcryS5Ni3gQ25eWSVgpsdbKphU6RWMCPAUAElUl3vv8A29j92TZ/d2P35X7r7AwGzodx4KozVVRZ6npNj7QxeztpY/H7ip2Botrx0eCp4aSnjilnhpGeGQuI4o4/bFtrQWZs7A26WkMs0iMqAITNM80jMnAyM7sXatGarYqaofcbmHZbffV3XedkvYt13S1tvrbCIrbuptraO3h8KWJFUQyeEr0CGTvcSM70IKRlsvuPMY+arr9p7ZwuPM8OB8q4Xb2IqkFHStVz0S1uVoaisoMnLjslG/3ZaBJW9TeWpdT7E8UMFuyJHdOxNWoCSCfWgOQCOAqfsAPUIX24bpuMMs91s9rDDVbfWIoomARcrqZSVco4rIaaj3NqkYHoaOiM3taHbuHqqfZG25N+bfqd00VDvapy1LSTYKuaKlzmys7lsTVUlQmRq587US4yjlYxxqwj80qRREMXbvBePcMEvWFq+gmKldVKhlVtQ0+TE8RQ0yR0OeRN05ct9jtZpOXLRuYrZrqNb6WTCFlSS1lkgKMJG8QvChJ0klNdEQ1H3/RjhfH4fvMt/Dvs/B9p/E855/v/ALn7/wDvp919hq/iH96P8t+nn+2/yf7bT6vZX9TNSmdeqlaLSlfgpq46cV4as18uh/8A1S23jrb6bwvgrLqrw+q1eD/v/vpTX4f6fhfi6hbA3fuGqbJ7eyOaauNDBgo6qvqMQwnqMPmlda+ten+4x9JVVckcNS5WOaNydMTf5sBjRogHMyIPENaCp4gY9SB+Rpk8eo2h3G4urRdrupvEt4WRwxXNCSScaQW4k5BOAcADo4uZ3FJn8KaKZIsXFQ5P+JHIRUUdPDXYujppXjdqGoWOmx2Omqa5InhiV/JULEEKqDqLreAW7RaZCQUKhSa5xXu4swAqCfKta9FL2Cwb1u+7pC0j1RZYlqAmtsHSa0HGvDyA8ugJqMmtbX47O7u2dQ0NLDT1W3scdsVlXnsrVRZCSKWklrMDVR0Rwq5aWlhjqPtnm+2PjDTsjMQolSRdSRzl3rqBcUA8j3AEGnHPH0x0Jtp8O3LyXm3/AOLuWRPCPiOddGUaG0lQzAAlSSMDUQT0lItj1uV23WYOp2/FUZOqiloKOgpGrnhggqZpIkx1VUSU9P8AtnGukUivBIVlBsTGADfxUV1nWcCIVPH5cQftz0o+inlsJ9tutnf64qqaqN2VbCtWgAKEKQQTXzpjph6U2JtvbW4clTVcHi3DgMTichXYzTVVWaxxp5mpKfKNWzQMGwtFWSJTxy3iddSIABpVH5biRtHdUSGgJppPmQBUVJHoPUnoKJtENvBcRQlVvI0XXEwJkoxIrUjCjhUkeQA9BC7crq+JNuVNJm67bk8smYym4ajK4+ngw392WenTCVmeyGTqoaimjq6uoY0ngSLx6ku/rAFKq0pVVVkUBUINTqzqAA+wDia5xjpva47mGzrHMYoQ9ZHNPD0pRO8n4QrYBFM8T0p+lPHHuyUbei2xunIVEQqc5UYuGfK7yydFBkmMmOSufNNhMfhctLBLoleiqLLHNIJFp1YuT7uYlh+omuXihAoNVFjDEHS5ooclfJQwqaClSOhvYWsl3HebdZJbS3Z1SPPHqkmZa6Gir4nhCN2NdWgnDHXoBqLG4tqw7f3vHLJt1JcRWZKgy+TXA0xyeRXbuYqaOrzUNSKFoHy0lNTUzUzVDiL7eUFylMmlfaC0u3utqMiXYF0A0a+N2KZFqqHNdAJIamajFWOejqaGO03Ce0s9tYio1yW9XcISpkBC/FRV01oNJJbSooOge7Xq+tMdvKvqcalBQZerlopsDDuKtxGGehr6CjyEVVXVO4M2aKgp6nH07BpaugmCmmLEEksyHGzz3yWLpfxq+qOheNTQ5WhRRVqHIo2a49KkG/7dt31O0vY7iE3WOessdw4U1rIWZ5ZNCBlXTVkNNORmtCzHG7SyORzeKar/AL0Qwbio8hkstlcxVY/buZqs3W46rj2ecjQZPC1+6amKhPk/h8Mc609AseuSmMc0kJi8rwxrIYtMjAgKBldIpqpQhcjiaZBpxFSiDbLHcbya3hvBPYJMhe4ZyqSNK4/RLVjaU6TXQuoqhGooFdl5zyVWViqMrt3K7AoI6/M57EYWPY1HVz1EVAsaSyZWfa+Y3FuGWq1V+haOMVs0FREvkks2onb6W0PLEQKVdSeBHEAgAjhn06pblop7i02a9jcrK0ME8KFmkRu7WY2kkDsDQBQxVhQnNT1h23sOjyudye6tx4iepoa/H1lBkNwZqeKbE7enhoKGGq3HuKkyVPBjsBLWLDFR5BXnKxwozLLZ9ISXF26RRwQygSAghFFGbiQq07jTJAA4mlOhLy9yzHeX15u267bK9i6SRS3kp1R2zgIDcTiQCOFWOiOXU3atSGzTp8pMPQ9h7XXDf3U3NjtqZGkpqyPIVm4UxuWyW762vp85VZqfGRnIQ5HbWRVzOHjqB4KmQIVTSjruMNbSmV7lTKM4WoCUoBWuGzTIyAaD0rfXEHMW1w7dZbRdx2DAKZJJ9Mkt3qDvKY6HXAdOoEMArEAngem/clPm9zY7ZWFwu4TtbEYfLSo2IopW3bTms2jNGMPX0ywL9hQ4LFSUBmWkZok1OYGdpVVvagMkOuRog0rVAI7fiJB9asRip8808uiIJdboLHb7bcGt9ujdWdD+vQ26gqwoFCxIVLBcYquokV6e6mueXH5yWSgwmK3PncNX5bdGSSvo1xO1c3Ni6Kgo85UrUNSVUOH+8haaGmyIqJoFd1kDCMMWliKlauzRxvpUUyy5ov2ngdPGmKdGU27LcmdIbSCK/vIGnuHLgxwyaVVpakgrEGBZVl1FQ1G1UqUBuPY+58bW7Ow24sh/Ad4bJ2vmEx+SranJZ3F7pptyQTPFuehzuY8VFC9JkMnZ6SojppYA8KkeNFkO7S/tphdz21Ht5JO4UCldGCtB/wAezXPngO828p8wbTccu7LzBqtd4srM+FI7SSRzpcAzJcJLJRcmTKEIVBQMKCpb6PIruzY+DwcmL/gGAxGPpZV2FTQfYfxGsirp8h/F69qmobMbixldVs1REzaca0rOBHJNEzRKSWhmZ/qNbGulya0xwHoaf7b504hWMRXu2JGLAW0GlNdqgK+IVaokckl5EJzikRP4Sy9qz23jUppdoywioMeGoqzH0dMspp50gydQtYaSKKnjaCsoop4/81oLKQh1qEbU35vIWwTVq/sJ49LI1Lpt1tHG50RtHEAaUq2oKFAIKhq49SM46F2bIYNoMfBnaikWixFNka1FkpcjnapJUCx1U6UVBj62uopY6UCmBgiM7C/jZGZQW5pJIFYwJUuQpI0ig+1iB+0/5ejbarCw3OeNd3u1RLZWnVXE0mploMpCjuBTBCrU0oKHT0ZjaW+OpYOvpMxg+xdjx0Na+KqsC2KxWay+VydTS7foaPdOHoNtYmhqN00mToZM5SgQ1OJqJGnbyIVMczEN13B9wihl226eiyLKGIAWslYyWPYwopPbIKKQCDqWhNzbNZTrBf7Y9t9E8kaQtaFih8OMO0gRgJUOohWVk1V4+dRNr5hWVWEqMlHHQVyDHqj1f3UMkMWQmWpelyv2VFK6ZBoi0FTKslSKjRyQwRy1oOm6RQQoBoBpIJUUBTU1NIwVFFpX0JHVNkI2iyjn2yQX9tcSF5dGoeGpWskZIAbuNQSpalKDgvSbanmx+5q45GGCGveOb76m0RST0FNUxzNKapXiqaWkMsrr4o3Yvd1LFLg+3CsclpEkMpaAiitmhI9KEE0AyR6EZ4dCi13qe5tzuY25hcQuskSrUEkEZJYEaDqwrVFcn16CbIZOCLN46gENC91ml8UqO9TS/aVksUckEVOaeKWohlVgfKzQiNm1ROWQhcsbiCdlZiwyGBwcDzNTQ/trShGehVrt7zc9kFyEiiddMsNDUMzHUNKaVLA+RNAK9hqvWamq56qkkrpqH7qrNS1PLpo0EFLMYjGlVPP5lad4I1DroVJNa39KI2q/ghGVTJ2tnLGpFRgCmATj0p8z0XvfyyGWK1hVBCAEVY17WFe4sTVyAKg0B+xVPWXICJ56n7VVjpYzHCTURu33EoijMrfcxxTRoviCtpUsCSSFVbgO2isiBHNWzWh4ZPlg+v8AnJ6Kd8nS9nS6EZSpEkTEHNVBHCq0pT148AMdKHaaUtNQ1BkOTrA1VUrN+0s2Kp6ekSeJ6mOPxPOuQl+9EVLFEv8AuxS0iAaQ1dTyAxmMICFBpWjGpwM40ihLE+hoD0U3Oxm+3KWK5dkVn0JKoOkuAsjEaeNQVCoMGoqQOkzuytWWsj8sWEqaxaakQCmweJpXegpJnjxf8RqaOmjTOSFpXEc1Us1QkY0tKRpUKbST9L4HWOpIJYk1bLAVNVp6Cg9B0pn2dI5yUuVluQqRyBcAGMhFaigKSR5kV4liSekfXUtFQ5HGZDbmFljnrclTJnc7QZqsxEuOpEjeSrzeRjkP3G683TJTww42GmrIyuseaUQxPEr0AuGD+NQk/gcAg4oAKfCvHVVT8h59Fu/ptyyJb7QKx+J3OjMpFDqJfjrYY0Ubgcn8IOdPR57O4GmgyVQ5rabCx1Vbj3rK9/uDU1rVmUq6qScTQmvkaf76sNUwZPIUFj6fYagigtzcSxw1t2m0hwoFKAKgFKHSKaE08aemegde7qIt/t7+1kAkSv6pOsDtNSS1a6uJqeJ6AjJibb8802ORYKhhAlVFBPFQ01RRJPBJOK2WljqtFPF4xKUKFWYKGdfqH0P1jlZjqUMSlQSQcgaa0zSo/wAnWQsawbfsVhc2aCOR4ENwWYAMW0E62o3aCValONBUdTt5ZqmyuHwyZJsdQ/axUFRhqvCUeI24KCm8onyU00dLCtZuPI1y1KtPX1VqioqrNGEhVB7TbdbzW812YFkIZnEiTM8uqoAUKWJWJV04Re1V49xPW77bdnEthPeblHLeHwpBcwhIdGkBnfTxkJDZY01yGqjTkhdu7OUVXQU61JnyYpWalFHVeRqJYUcQwrHHUVMTKscNm/aEMeqR2Bcm7HNpAyOTGoR3GosKV+daAitfWuABjyK9xuraOK7W5TxrGKfQkLA6KsuG4q1MY06RUsQW82OrqoYMfH9tTsubypjK0sAqlkkWGIO8s9I8vijaljo2vJoUgJZy4v7VqSZ+/wDsFFNRpk/I/OvD+Q6JJIYodvaS3JO6zSr+guqqqMmqk/h0caeVCWHSYqcs1TCspqaV4qzxUbiphaWWGNXNRVVcMNFLKtJHFpeKF6mYMZX1rH/RyOBEcRhiAG1Y4HyoSfM/L7CembzdbyaA3zW8cpkhETO4FVBILFVQ9qimlS54nUFrwVWz8njqCvjSjpFzXnxldEzV3kgD1NQsqx5FBTGaKempKmMyLFMJoJzH+9G9iPdb63WWBiX0MrK2paHgRVc8CwxUUIrgg56Z5e3HcIr+CKzc0fUpQ4qCDk0DBkDDVpIZTTuU9M4qcyaasp6HIfa0VVXRVVRT01eKJclUUBZKasejpXbxPjZHKxFSfE5Gn6j3qXwA0TS24MoUqrEVoG4ipH4qZ9aZ6UWVje3Ee4C33MJbOayIHCiXQcExqTTSTQfwkinHrjXZiqr8hlNw5aors/laqp/iO4a7JVk0lflKirMUmqpqppGyuXqah1DyP5FGlkcEtyWFt4YYIrWDTHGo0RKijSoUUFFA0qAOGPlw6NRf3DX8u5XUEsyUWS61uwZwwAVS9RLLwBNGAC6SMipArG73wdB2v1zld14n/fuYbddBl6GozkmNx+00zWLRqrDru96t3Wo28alQk6yyr96tMy+hQwN90tJ7zZ9ysoJnSR4WTVFXxaMCGMVMiQCukjgc0NOiTlLddmt/cDlXc+YLRX2qO9jf/GXWO2V0oYfqnYj/ABdWA8TuBdVI1KTXqa3YfXsmD37gd6ZWLe29KfduMymKk2fvLIYrrzddV/EZauszuVrcXlfHt6DFHIS6JMY1M1XUUiSOKq8STl/0F+lztstmiQbeYmWXx46zINICIgZaEkgatVaDhQklZDXnHkdNl542vm65k3XnKPc4bixO13bLtd45lc3E908UyGMRJIxia28MSOgLiRaeIl5sZnc5W7j37UQ1Wei31mcbuihlhyVSXro2irVxWMlkqpajKrisPjI44oqadp6cKyrHBEgSH2cwmOBILJF0iFNAXhw+IkAAVJ44z51NT1GO+neN9ut55vv9dwu5XK3RkLs5IIYRxhnZ5PDhiAVVJZVGkAKNK9DXQzRyNIq4jJ4+SGkbHSzFq2HI0NdkqNVpsf8A5LGKYzwlDUiGbSs6WLghSB6WsvhgTrXUGpilAcnOc4FfLy6Vbd4Nmt60u1yongvH4pMgZXlSka1Wi1Aq4VqBxk4GJMMGLaDHQVVbkXr87M9O2Fy9DBjccaaKSqqI5qbLy1ZqmkrMdjlk1RIukzSLCxJQnxZi0uB4SmisjFmrQVBULQUJPmeAJ+SRY6JbwTaluJhmOdBGmnJDLIzau5VFCB+JgpqRUXsPtl9wV1XDR4uKPE5GgyeVyQx2Fy1bRUNEHrKyGnebW1U9OktPGjB6tY9A0ySByo9lW53p22xjuGk1XCSRRDW6KX1MiMc0WoDFsLXGB0LuTtr27mXmOXY5pYLe3ntLy4X9OV6PDBPPDCugmU+NLGsQq+kaquwAJCj6+SjlyOKhoK9Mfk6KSbJ01VjcfAI6KrxtIKxKgRSvTtPWUEsEKB6cllhDFlYOEdrdJWgtpneDxLdgI2Rz8QY6aVAOGBPxYJxilQxt2zQ75c/u1Z1juaFvEhwgAUluwle5TRapUgZzUApzN5Rdz7oyed3Nmaqkg3DuDDV+d3BT46LMR09JUZKCHOZ6gwVRUUddW10FIfMtH9xCambTHqiRgiKEhNltSQbfbrqhiKQwM2j4VOiMuAwUVwWo1BnJySu3s4bXc44bq5L2YZSLimpdOpdUoQ0dqIKhKgk4IANAkquh25j8ZWPtjPZ7P7frKjcUEdfktrbdpJq3Hmtp1pNvQbfw1XViCuxJppoJZJTLRmLSgGqJnKGF76WQJewRR3C6TojkdgDRgWLsq1BxQABga1OepQWDZrPZY73aru5n2ydJlaWW2t+5S0ZFqkcTEl4irqZHHhspUBFKGgNZjJ7f2xSjd+Zq2go4Zp9skS08mXxOGzWRxkFXh5ZMVWGhos/VUdHSl1o6uRqJ4zLK5kBaP2YtHJca7SJ6TkawAaMyg0ahALKKkdwFRUDBoegeb6x2P6fma5t9e3ITaMzoZ4IJ3TXAGjkMcU7qiMRFKTE4DMwdaoZvVew+h93dgSdwZ7vHbe08DjeuqnLVewKmKt3h3VvHt5ttZo7S2xs/AzYSkxWK2dDUyUNTWZaWsxWJx2FopIgqVRpaFy/eNz5ktbGHa7Dl9ri+ku0jE5YR2sVv4ieNLI4YuZBHrCIqu7y0GI9UilX0XJE/NnL/ADZs3NCtbTWCz3ljMDJeR3scZJj0tFHEtrQo0LxkR6FVHSGhEavxFLlsNvJ8/sr7nLZbZmBOW3DnMZjn2xS7WlqKGPB025qaXNYkwQy/xivDFaJzMlTKsaOjPHKHrh7aWyjsd0RBFcSeFHFKdfi8XMdFbuBRCc40glgRUdCNrFxzFJuvK1y09xZ23i3dxDGLZIG8NYROPGjIDGRwSI+7WdKMGKuJuzemcB2dtrKUeSyXYJ3BV5bK7egj2dtyGfb9Nt6pxL1keTze5np6zF0VU9YhpUpZ6aqmqKJpURqWRxKEO8cwXWz3sZCWgsfCEhknmKyF/EAKJCKFgVzr1KFaho+R0Jfbv2hsvcq2nsriXehfeLLGs22WYntkgWMPquZ6aIiQHpUSMyjRpQvrCA3BLgYd9bu2P03uKh3Vs7ZuH2o9HkMjmsXX4qro6XA4tMrPSV+wcfuOKmqqd62eljikq5IUWkSCKSWVWaQz22+v323b7zerLwdwmZgyIrgAlnKikuhjVQtSVBqdRUDAjfeNgs4+aOYeWeUd5tb/AGixRGW6jlWSAosaanV7dZRUBimnUw1LoUkgkp7efV/dVLI9FsWrip4cbX4vJ1NKmF3JjqzIUu5MfT11Hi92TVcTYXftfjcfjaSKoeOhlsImEn2+jwl633bZ56Nc1BoyK2pTQoxUsue0Ek0z58DWvR1vntT7obHrtNhhLKn01xPEsE6sy3cK3EUFwroEunSNF16Y2AodZTTp6SU2I3puHK7l3Zk8DtjAdh7b3FksJt7YuP2bPW7GxEuZoaIpurBV0eWy1fUTY3J0rzKla1XjaEBC6eAmm9uJIkCW9ktzJLtjRI7XDv8ArMQxqj0RVAK6cijEk5BAboqm229vrrduYZ9ms7Xn20vprSPZobQtt8YeFQl3BILmaR5YpxIxjkDW0YWIkNGzQdA1U7W3Dhd7Y6n3FkqbZmYx/XmRyudzVGaWuqX/AI9HlKCoqt0ZiaurI6XN7prM99gcgr1clO1RTyIgIWOI9juI5raRreHxIzLpUGoHaa4FK6VArTAOR9sWX2z7jtO+QQ75eGzvY9vaeeSIJI/6ysKzOGIElw0ugyVdk1K1DQKH7rzaGNy1FCdldn0WC7VqYKyi2b19VU9XFBWTzUdDUZXBZfIbuiiwWGy2UfywUs0c0lJkpBGGWkN1Yvvr6W3krdbeZNsBrNcjJxUBlEYLMF4kEVXNNXkLeTOUdu3y0iTl7n2C19wJtUW17LKjIkjFVaSGe5vCltbyS1KQkM6TNQOIKrrUG++rc/ujszZ+3cvRy7XSnxG2MI2V3quTfA5GeJMdUVyVcW3qKOroAI5qp6qahkNO0oSnRoJmF9We6W8Fhc3MJErVZlSIgMcGgBY0b0AORlsjq/NPI+93vN+ybJuto+3Ugt7dpdyEnhEhYy5dYk1R1qxdk7a0jBVuL12d0Thuh+zM7HsXelJ2P1wuZGxMNukVVTicpveJ6LF5HPbiw215qTFnIbfxtRVw4+VTLVU0GSmjMVRUBYqj2X7HzHeb7s1nLu2zyWG7vEJprVtMng1JUI0ikrqYVYfCxUHUqmqhNzR7eQ8lb3PPtN/9Zy0Z/oYZndRJcsiRyTyRRpRZII3ZUJDMgdko74Ye/uTkP4T9x9lWaf4L9p/x8269P2n99v4Z/dvyW+6+68v/AClara/Ro+39Hsw+qHiaKpr1U+FeOjV6cNP8+kv7ku/o/qPo5vB8L/fs3wfVeB4Va11eL5/l8OOpnx+wD1GSxc+Imk/j1UlcN1Gqr8i+Qr5WtFU5PJU+ZqcbTUkOEnaeJZPDq8hKs8isWKu7nRCzSlRGMKKA8eAxWteiDZrWVoQ9skjTqjSzEeIXbSMsQ1D25AoKnhmvRuamSpizuOnyWWNZTUdLW0NPkKWlopStM6U8s1NnnpGkibE1CxpNBUGNG8sYPLchGEj0aUSmdWkk4Ofhr5+o9OjlJ7oF74h9Ug0SNpyRQf2hpmuKE5qPXoMpd21k0JqqaCrr6OlyVRVtHT0sk+YVaaQtFURRxymOrpXjitTyD1mNluQePbvhRipIFSCP9X29KP3jcvo8IO0SMrgKDq7RjANCBTB40pXpl3PveOo27jzLiMzvP+9lZBBntlUTzYSWmp51mZ8fuisXzY5qnGUSFpVkaSmEksVxaz+/W0aQvJSJRoBWNmqaEj4lpkZPy+eOvbzub7jbWjTyS3EkzariFCUOfwSkHS5RRU1qoqAPnh6t3s20cvV7j6wwm1cbV7vwNTs3O0GR20+7ZcdksfuaGoxD0WCwVfR0GQr4ZcbLTxLUskFbSuTGzJEB7pd2MN7HH9fcyRWsL+KZI204KMCpNMVDE4IIIBr0QyIbuS1s9h24T7ldlYPoxr1zSLINIAhKuaEYpTUOFRxTe9dyTDO4Ham46rI7wkapq8dhqbtLL7QMFBPXRRyDJYDFY/EV+YyGWplM1NRz51o46TTHTUk0iyXU0uLbbO+52p3+jZa6samP4tQBAVSeAHzrWh6T243Tb7xdg3i007mJSrRXRXw42zQxIykGTQSA7GlcKejY7JyNN1qnWdRR0ucmqM9uXA4ysxuLqPvszidn/fUsW491x1ckiCnyXhkgpaCJRPPUNJKUgjWIS+wxf2Uu5R30Sxo0cULvqkoEL6aIjj8Sg9zUpwGTUjoQXXMZ2m1babSCVZ5UjjEhLDQ7MS7qwNQxUKB5ZOK0PWTuLuTrDO7hr5NuHsXN53YHbVLTZ+abCY7RsGtyW5q4VBx2Rxs8OT3DpydFapmpKNJcWYoKeNZkSOQk2x7buENu8V3FafRS2gSPwmZvGAjFCUcERqAaAam8Spc01EdCkbxbrFtuua4k3Wyv43vJDGB4EjyAMAQdchDR95VaoQF8lq0969SbM7VzO5KHIbhgwu0eu9kv2VJNi8TXZrP7x3VT5LG7apdlbOw01BQ7pnxWVp8nPX10vnp1pqejqayQPKsMLOWe8bhtdrtzmyaS5uZ/pV1MqrFGVLmSZk1x6l06VA+JiiDB1dLv6nRc33c9nOsot7WOTc70woZZmKyaCkER0TvCVapCkaQHlOFwRDfeVwmNxIXAYY1GGainppM/vGXcO3Mlmcd5Jq96XDjcOOgaf7u6yzR4xlnkmVGlM5Kn2J7eKWVz40hMpIOiPS4B4Zow9cE/y6C3MVxtm3WaQ7Ptw/dgVlW7vRNbvMlddI1ljAzgssNCWA1F8HqNX7boev6bYWXytHXxbarTipdyLQw4LLZKkyFHiskuGmjyOJWiy2OygZ1hjomQY+smMjVDrLrkd+OUXkd1pA+oUll1VVTU1PHBHz4ig8ui+72peWpuXZdwJGzXIjMxg8GWZSiELTRSRHoRRDRXaus6hXp53TQ4/f8ANgX26dt5LM5CjE+05qvcOJXKYHy0UeVbFZfCUNTLSU+eBlkmlSSGVaaQu5uItXtOjNbJKH1BK/qkBqMAaVBwSvlileHn0abpbR8w3m3w7c1rJcyrqsBJNCJYQV1hJY1JSOUkksGUgNVsha9DPtXF0Wx9uYjEZTc0TVM6fwrJZWumrGo8zuDKCqrqqh25Hmx9tO3n1xwIIW8ojD/bI0jgXVTJrkEVFLBlXFVUUA1UrU0pXP2k9MSSRbctttw3DXKkDxST1bTLKxZn8ISUouokLQCukNoUkgNmXymWro6x9p1+3XrqWog2/KuSo5quSF6mfw11TS01DV4qGOtoqWWHwRSaw00PiKKCQl5Y4yy+JUR1J7SAccK1BxXj03tm5XSxXZsPBe6VVg/VRnBLkhioVkGpVIKgk1IApTg+YOgqk2tAtZU1dYHrBkc3gtw0uBr8VNVPSmGKfcmGKrt7JCRWijlNWXDLIT9wdEbApm75XXgSKLIhZW/2rDuHqKZxw6kjZLNLXa7PcCyyTxSiSe1u4reaHhgzwyL4Lox0q4lBVgTV8LSLvHdO1svFhq3Tvuv3ZkmzmG3XtqHEUuc29jaakipv4dSYGppczWy5uPL1CTmK2Nxk1Kkb6zOJg/t21i+nBhW1RYFCssus6nJrq1x6FCBRSh1vqqahaZC3MO/bnzBvFzebpPKTLqt1tYf1kQLTSiNqIozqdIVVNM1atS6bE23t7ESZepiwNHSHIY2Jo8ZWYyWhqql5aZWxdNO89HDVUxx9JJojisXogdDWs6kUbXHbyNJJfOfCWN2iqcM/kB65/n1G+9ExuLXa4gt1rR51UEMqoaqrYBWowAcgGnTbVS47I0OJqcVjc5FV4mD+GfwOCiky1RAHWGqjpamPbMWVqVkaKqb1jWGjYSF0QXBNDa3FbqRlrCDqLAE08s+Q4DoYbxv2ytY7KYtUFxBCsLJIVGMEfB3VLMwqak4yOHSfoNz0VVHszP17bj/heXrRmMK20atKatr56HJxwHH1lZSwZCrj2s2XxkkeYMZp6kmMlJxGhVmblZJVlt4mj8T4GEgrpqK1oSBrCmq1qOGDXpZyzum3bddbXvO5QX/0pJuIGsZDE0jI4Co0gV2+maWMrNo0PQHTIApBM/05urc2YKruKo2hh5s5X1Ry1RPQYvauGoshJU1ecyU9GJMjU46enrpx6aqrlg+4eYGdS5sC24tLewtg0cc5EQqoTW7EYQDHcacaAEgCoA4de5h3ndub5dw3LcGthuM7tJJHAiQIHd2kdljjYihZiS5oSW7iWNehth3DmNuZyllp6jG752nWVRyWXoKquirvs3GOq6HHVe1KvyS5OFmytJGZ6K6xVEJ8jgzrC3um5We1X+3QPF41tv6v4ZkpRDH2uQy00s3kGzpqaEDUCFuS/wB9Wi7lZfThdhmiaSVCNLISrIjVFNBJIqKrrpwqF6ytFV5HcGTjxWChzlZPPRZCOgLR46vmkaKCoaJ5atcgsQSEPJOJ2Cw6GZ0ULZS9p0itopZpjHGoZS1CyihI4DTXNAKDNQATXIrttujt9uWze+UTaUjBeRY9ayBVWRS5NB3VLVAWhP4cBDuPD0OKyrvBU1yZOhyeRw+XpKnGUcWLw9Sa15kocHkDkGmzdI0EkUyvJBDHFr8bksNIMrW4ea3ZvCHhPGskbhjqdSoqzrppGa1FATXiOjhBJLukXiS6IbaU2y6lUqCCaBCSDJijAt+Z6dKLDZWDES1D0LyyTYuTI0M+QiWSWipIZn89dNSU4D1NDHBDpuQVaQoQ1rEurcWwuljmkourRROBJGACfOuceVeivcba83HbxPtd8kbxS+HcySlNSCvwYpRiKChqSaAcR1HrdwmatlyUgimqDJJIs048dVUGQR6YDC8yrTfZyxh9bXlmmld2kYEAajti8ZiB0AcUFKACueFTq4egAAAHS4vZbPJbCMSXdvo0xTSVJEmBpYEnRo408ySeFAMWBzBXbuZmiqYkrKtdaU07LA06L40qFjnMngoo45ItXrRWlkhVUuCp92lhQ3VvWI+Eq0r6HNKilWOfWgBJPSG8nuLiybxLmP6tp9ajAYig1FMgLQppOATgCoAqj6HJ0mUoY61RUSMstYZdDFYaubymCKMLLa1NSSmxKs4dhdFWxsoaP9d1Y9unFOI/2T+X29PxTyR7Ray2gAl+p1SFuEgrQ8RUhcA5Oc0FOnpBkKeWmrfN9vJUqFBiaN7iEtNTSSU8APiqTKHPpCXJ9VwS3t9dIj8OmocDX+dCeg7di33C9uZJW0TRuCmmi92PiC0FD9lPX16N9QVVNQbWjq6anr6taeiT+GmoyeNTI1lTTxU+mpemMNZJTUFHKfEkUn26VKKxAJWzElymu2NuJkTW5LgVPE5GCDqIzXND1GdjBu82928+9mFp3OtFgA0Kok7QeK1KgEggUFfXou+TqswuZkoMvVUeOkirHgaeB6uZpKI/YrUUlRZTTS0cOmSKNQ0gqTVuZSU0gMQNZlBc2cZddIYKxFKjUQRXIY1BPoFFBWvWT1xtG+nbotn3i8IgfWiMqMGJZUHcVQAxr+AAkEtU4I6CfeFLTYmGFcZLJRxvNkTDDVGlkfU1UJ8pj/4rNDFQ5B4xOpimAVbEiNfr7N7a5ZyfFUMcElK0yMHTUla0OOPr0GZ9jC2kPgTeFMqsmiYqrEqR4g8Q6Vc1I0sPsWpr0EeS3FkaGRZ610CVlfC5LJBImSqqcQTUkUXmkkkcN6VlSy62TSSwuqqqxuewUOkjGKA/6sdFxW7tY0N9LVDOj0ajGRkoV4kkihoQePDPAKHPZKLJbdrMuxhmrDCwJplkgmUTwqJX00cMNLE9MgdtMRVhwAY7gjSJoeOOjaAPywfnnPV7m5intb+81xGZ2CUoFajKa4UBAVoa6cio+GvRX9xdzYja+HxuNpUr63PtXV9LnsJEsdElFhUpaCbF5Mbrq6avqq7MZeqbUYxS/bw08IJDSSqyLLaynnneR1AtwoKPUli1WDDTQAKBShqSSSKCmQlunNNjYbNaWVu7tubyOtzAqKqrFpjMbmc63eSRq1XSqqqA5LVBltiVdSv2IqZKeaRKOGP/AHE1dHW4qWGago53raOvhnWOeiEdcNVWplikBvE7IVumnOqAsVofRhmteFONajh0I9kjaHc4oWkDBR3NCyshUqKsJAwGghvjBIIypIIqucxjPssaK+f7Z0zjwVlEUnhnq8YkE5oVpsmhaWGFJ5E0slWiSo7K8kjK6D2gjuPFkCVbVFqV8EBiRqqpoK0HArUcQMjArurCK0tr6SKNFgu3ie0LMCyBSFKyAkrk1DCQBgdLM1CAUBUVTUUdbFEr/wASaOtpmqm8TPT4yKrVxSxRNi46bFSmYjT/AJS4kf1L4x6S5p1ujEjw8EAVy1ONa1bHy/b17xprO2u4ip/eAWSN5DpOmEOCFVfCCQnV/TNTkaRghZujbOPjxG23XD0s1Nm0rDQy4qipJcXlKtYKmtr4cjNOZ3nno5XZZo/XrayK30tdZazTDV3KwqCcjODjhWmD0QbntMMe2bLMlmPBuI28F4VBjlOks6OzVLNGWKsuf4QaU6BDqD+6FZX1eHzWLrMPuE4+aqwiVAq0w2bSnqg1RDXUktPVJDNQ0y1E0Dyft2hlTyebQs5jepOqpIsgkhLdxBBIqDw4edAaccYoMArlEbJdy3drfRPBuKQl7ZWBWKSjqGDjSwBCF3XVQdrDVq0hzHhspNJuLE1kOGwtBUzUowBx8WWgWooaOGGGSCtx8k9PjsbOoVXDQyqpDITEun9xHGiBInViXFdVaYrXgeJxj9uehje3F20+6WMsMMNrMV8BYhIqsqBRQxlgikijYx8PaPMymwOlt771wHZ2/Nv4mlTZvTezsTursXMHKthaLAYfJbsx+19t4mHG5rIUSZPd2dzmcSGKmooWepgEknpjiPskvOYrDbbvabC7Zjf305gtUVS+orG0jsxQHREirlmwCQDxHR9d8sTsY5bUFNt8OkukSr4ZUsVjKyFV8dkDHGlWUdpqQC6Qnq7atFPW7sz26KGtqctPiv7zY3r/ACOfzuC21TYOsmpHqtpy5fFZvO0uU3bVUdJWspllxWOiepiiqGApWem/eF1HHJaQRGiB/B8VQHcsK/qBSq6YwSOGpiAaAaumLa/t+X9y3S23SyeWzdRHFuUiTieIdysv07d7xnsqSrFADpA4dTsF2BsqDFT7afrXsLcedqMpgpcJvnZfYWFxHXs1TVuF/h+9uvNwUwy1TBtSCjkraerpqhUnevEUopPtg02rnbtzmu/qG3C3XbvDKmCSEtMldWto51cAeICARpNNFRq1UAeO9Wm2/Rz7dtEjbhDIrJehwY3KuCiSQyAt26dWqp1a6UXTlrrsfS5rL0seOrpocRRTUQlStaopKGnFc6RU9ZlKOsq4oZ6PFvMyeWUFAX1r+D7M4dEVuDcIDMAQCKamoM0IHFgK0HSa9l3OW/kmtq6ZGErQ1YxIC1ArasaY+ALY86+fUmvqMBFgTjdxb1weEzOOEtfQ0uZxU60ecqDJSl6J6/HVcWRx2Qy2NeN6GpMM1NVTIqsP0hi2dLyORpbSyZ4ZHCO6uupFHAhHGllDVDCoYA1FehTt+7bNdXW0xXu5Q6oYHesqyeFLKxOqMyQvrEhVRpahXXQFStQQr3Rv3DbYwUceVgjoXx1AKeKnp8fJLKs1RI9e9VUVlNSqaySGoT99/FH9vGrGVyAx9uW1m0skk/iEhnLGp40FKAE4FM8TXyHQi5i5mt9ls7faDbBJIrZIlRE+FtXiF3dVGt9WGIVSoBDsaHppy+36XLYKFYs/isrlqnJUtRFuXB5Sh3btejE1LWvHTPWUdU2EMMQ1+QQTszSftrLo8iD0V1+q0qRMkWkgJIhR8EAnSwD+np8xw6audhi3DaLW1l3KKbcGuhrvLaZbm2XUrlQXRvp6KKklWbOFfTqAjbj2nAKSCDauar8Sm4aDcGC25uXFbVnwdDX7pjnjhz0G28DW/fZJaSgzFWKWiqYZqecTCKXVTOPFDuC/QrKbpUBh0yTRs6kohqVMjCiiqirDIpUCoyUF3yxOs9lBsF7Mbq+aays7i2gdBJdawHS3gYNLQNIqRMNDaypBUiipvfGayOK21Pitw5DO7g3Xtehhh3FX5nKmr3DmRgMXhMuatqAzmoWecVLMVqJFeZIvumkllOp3LBIHVZrTwVsnNYxEAEXUT5jFB8uHDh01zfc3+3pNsW+/XvzLYIq3jXjt47mCONx+mchiGNQxGoASFmckl5g3n21XdeZjojaOKqpMTu/G7g7GWTE5anXK7IysFHTpXQVE+JjpvRvOgxVJanaaSqq2ePTHC0rSEku9s2GLe7fmu+fRuMKpYhmrplVnqgoaqTG7tRqYq1SQMD3lbefc+95P5i9puSdqkuLHerGXeZ1tpA09nHZo8soYxFSguYowXjr4ktY8AuKxOxuq98bKjbI9Z9P7Xw2b7D652dXbsx3Ve5t1SbG2xm9+bcir5NvJSb73Hk85JvvZtVXpNkkoHXBYaqqKug/cipllO9i3m33CFo903S5dLe8nhja/SFZpEhmZBLSBEQQShf0iwEjx6JDluiS+9t/cTYtquN25c9r5La63S0RLj6F51to3ukZhAsc8zSNc22pZG8MiCFWMcqkCpj0Wc7cyWWx9N27ufbO1Nv4jYO4M6ex0o0rsH/ezBQKaTGZEnKYbCZXNZgQx09PQhoaatq6kRwloyxVfNHt1rbyPtVjJNO9xHH9Mp0sEkYAtwZlWOpZiKkKpNK0HS6Peef8Ae9129fcvmWCx2S1224uf30sSzwm5gTsjb9WCCeaYqsaxllRy9F1LU9IfsrsvBwbufr7c/TFHhqjZmVxuVw24k39OanCwK9PlsflN5Y05hNuVmYqqMAfZGtoYw8wRI5JWRnd2i0uJrWPdIN+8aK4DUiMSgMNJWkLU16a92ohjTzAr0Ue5PNWzbbzBuHIe8+0KbZuWzzxhLn6+ZpoCrxyFtwiM7Wz3BUaWiDQKkjFQhbSAHdfvCj7k3fszbu3Os6aPP15q6PbWboMriqbJ1CfaPUPDmcZRVFHBjsRRwxEillr0WjoZZZE1MyEGohG2Wl7PNuDeDGKyIwbTxp2kirEkUqBk4x1H825N7mcxcr8vbJyXEN5uXMNnNA8SSSFl1UlQMkcUSLkKzqsUTM2cURfZux6zb8uXwVS9BVZraslPR5gwVNVTyY7M5D7nIZqngnqRT0tVtmejZ5KKVlppaiCT1vJojZ1G3XUUwhuItQglFVqOIoNJpkhtVa+hx6joLc78s3/Lu5bhsN8sbbjt8ngXWgkhJcmVVkqqyQFcow060Nat2sVLtOTM5PKba2XQbt3HjaWsNbLnqbITSJiMlS0IlqamsqKikhjkyO2IMWwlXGmSppZIqYoCJCQaSNEsbTGBC4AC4BIxQAVwGJHHHGtaEdObU25XF1Z7Pb7rPDaSsWn1MwjIFWdn0rV4EjyUqy0Q0Fajo1CPh9w1+VoMTQUm2cXsvH4vFYCmmkeoyc01XWrXUGcqsnVQ1lDLu7LwzSy1DyuYY1jjip4ViSPSRqlxAkZlmeaeVy8rCmle3KquCI1NAPPzYkkky/Y/u2/ud0tbaGGztbCJI7JJCTK7PMrpKZCHj+qkRiWLErRQsaBVXSurVP23i+5yn/Fo+x+3/gtB4f49/FfvPDfx3/hl/wDKtVvufuOPDb1e96IterQldXiatbV06dOr7adtPhp5+XSzxt48PwPqZfCp9L4f08dPE1+N4fw/78/Vr/a6vwefQU9F5je1Bl81l8LvLaO4trHz081NnNiY2rxnjrMhUw0UeJ3xFUxbppJlyVD4dUM9jqieUHXGwMdxtra48JJFmS5U1Gh2WuM1Q9jUGaMDitOog2mfczbzrBucLbQx0nVChIOqtFnUeMAWSmGArp1CtD0LG7N35nCPk4a7DtBnKAVC5bGU8dNTVjTxxmqTGV5q5lgkrI43Y2eRdIkQsVV+HbZYZkjeFg0ZyjVqKeoPoemLuJbQyK0khQjui9D5AitNQ9DwwfPpf9D/ABA+dPyW21j+3upPhX31u/rfIQ1uLwu8us9j7x7L2pl63G5SuoMxQ5PJbX22cZkpsTWQIftqObxxWZJtUp9C14GaoUFhxqFwMcAcn8zTos27dPBYPcSxwkqFAaVTVST/AGimlRgEAVHr1fj2h/J07Up/5VXw/wC7urOgM72J3vtbeG4u0e1tpbL2Jv3dvZG/sL8qcBiN3Gvxu3MftWofJbf2J1xtDr2jpocQ+YFNkq3NUtU9NVUlVTI3Payy2SCMMHbGpMkVFQfKoAA9ck8KdK7HebG25jvZLiSLw1VyPGoEJHa6gdxVmYtQEV0qoyDU0Bd3/A3u/p3Zy5v5F/H75K9LdZdsb/p8Htim7F6d3D17kNubkiSqyMc+Gfd2CxFT9p/CqWOWtqJ1np6SMtHqMkulkl7Ld2cVtJEF+qRSxV9QD4AamCDx4ChzXoQ8lWnK/Me87xs2+x3P7pu3jWC5sRHK9vWQlTkp4IBA1s5ZdAIAJNOjF79/kn96b623/L7m+L3Zbdy7l/mGY/fe8Itn7v2PNHnepsh05mqTY9Nnsj2bV1mayO5tlUuDqJampqcjT4xNuUkMz00UwmcLWyvE07eLmBvrJ9apHH2rTW2oFVYgcNRKihA7uFelXN2ySXF1zkdo3lTy3tUsLTXN+TNcSOINNvIkr28crIVAijilYmIt+mAGdVeuh/ib0Z25/NCwf8tXpP5X5DujA5Td2S62pflH/oHyI2icn19tTce4d5Nh9jUPbeRiymJoNw4JqOlr2zsFJUxyrWJJd41kWvaySyCJZikRqNQ0gmtAGAJNRx+39o6CUG+WNpa+PcWHjbjEyS+G4dkTwy2qN3AWj5U0IoK0rWlWD4c/y2e0Pl5sb5XZH46vM25/iXtGl3jt7riTAzS5Ht7a0W9c1iczPtSow2cigg3DDiMTVZajoUo6yqy9XI9NDItTLHqbEUswkRu6RVqwrnFARn0r+zHRl+9bHb57KW3XwLaSUxJrqVVa1V6pQHUQakKKMS1RWogwfH7N9g/B75H/ADR2/uf+D5P4p9m9GYbK9b4ra09RubsGm7Nrc64rYN7DcDxYCSjyG1ofJQ0+JyTv5GqDOjRKClSyik1C5esLaYlRqFKMG4inoCKniDSg81cu8320KLPafEF4wluJJ4q+P+kUfSGBICk6TRfhKhqk0oYTan8vH4B5z4mfH75r/Pf+ZK/QO5Pnfju1d5dUbUl+DvdPyAzO2oNh9nZ3H7jRt29Ubzzi5PJ0a0UcsuSmxe3quppptLCU05kV+Da1tYbKztLxbWCJAGhVO0qo8MKCGUKoxRcgeXTA5ytr5OYLre+UG3i+uAkVrfmbTJC5IuS7J4MplkKIwaRfDYrUsxIFAi+Ov8v7qL+Yh8n+0PjR198uE2l0t1fht9drddfMfAfGHcm1m3vsLq3bdDmTlqfoKTfm0t8Z6Gl25UtT0dbXZB8yXSeU/eyNqlQ7daQbduMim6eW3ZXeXxi0mkirEgPXw6mp0L2gABVUY6F3N2/bhzRyJBdScvQ2O4rfwLt72KR2tRINKRs0Z1XqQxhVinlIlq0heSQ9xSXyI/lx7G6p+KVf85/iF8yth/zDfjvtDuDB7Y7L7A230j2V8fezdobw3dj8pjsXUZHp7eNHl3qMXlcuI8TFl4ciJHnqVB8KRyMhu8ETzSRRThYAAhjJIK6sjUGodJoSPU4p1HtpvO4wWNpe3e2O+7zTveRXSqCswWsbmMxAq0oYhWoAQMlhTof+rvgX1FtTobqTvj+Yh89OqvhXJ8g9l1fYXxx2ljOkey/lFvDePX1NDj1bsjc+B6fmlPWvVefrKnz0GSyFRIa6KmqJhaKnmtS2hgCL3mPxKgBgwYkEj4SARWnafPyBx1bd923i8lkXwRc/THUz25QxxrpDuFkUsHCg6pKYX4malaFn7F/l19jdRfzAfhh8GOwN0bMrMH8tOyeoKrpz5Mdd1Kby603f133ZnMPS4LvvrCDG1G25N14qefd1W0CNWYqomrKKVWkWCaKd1DQF9SO4BoqkUrVXYAcaYx5+ny6R2+4xwpBNbW5ZNc0wZj4bJLbxGVqadVHzhgRStTUNToFfmv0PlPjb8i+4/i4+589vbMdNdt5/rqn3hRYRdtbl3Sdt7trcVjN9YvCxZLdNRiavOiIyU1P93XtHdGkmeRFPssWKFZLlVCsisUx8PbgrT5Uz6dDW/wB4vp9q2Sa4mljkkhjujQ1lFTrWYPQNU1Ok+ekM2QOnLPfEnI9W/BDr753707Fh23it5fL3sL4v0nWWe2vlarLVp2/19D2Fg+yMp2Dh9550xZDK08ktCcXHgaGOimgaeavYMkAXrakRE1LPShVQMYBOTStK/n5Dy6Bj72Eu7VUYR2hYyLNM0mqYNJIsbsF16HKrUUoASat59H0+S38sPqb4mdb762T3n/Mx2N1788Ov+oqLtWm+FR6U7E3VsnD0GZwVHvOm2LnfkHNiqnYUfae5MXkhekhWmSSeRIo52p5f4iavFoMeuUBh8UYDVyBTuGMD5EfPHTlre27/ALwNnt8pE2Y7tnh0AJVWZ4njaRyzDDLIjBQaKa16qUyG76na2Pw42VjNuY5Xlr6zPihhjxkOA8NGDh8lV12KK0Ula1dZyxMpaHxInjRXcKI725hheO2uSsMi6JF9Rxofs6ajsIrDcLzVYKJUkWQSO2oCqCjDSSoFfLNSPtPQM5PZ2c2XWBZZGxdHlUqKuSiWnpuJ5aSkycslJURNUfc0eTjUVLrpkdlc6GCMtkCssqqymoGK58qimfSlPlTpe8E+3vIpYKj1LKNNKkK2CKghviPGtfToy2x8MPDDuQmCmytDT4t6euSGdpspBRVb5OLDtSfblxi6GajaWSMsCfIdUhDW90uNLBoSupWBBAxSopWvqa46W28zwSQXQVkk1KDKAaFFYNQ8O0MASOJzmnRq5M4cvNj8rNQYuiqIdu4Cnw8NJLTJNHNkaOavzlLuSSoKTZrN5UDRBDHHTUccbhY0/ZHlD6QOiSQl2KmRy+oHAUhUMdKhFU5JJLmlSe6oJ7ayG0vfOl9JLBLM0hauqhlUyCInFUAFDigPr0zbfzsOxMluOomqKfD4yGox0cdZksJWXhqY6Olevmaihhlz81bJVTtHKsELgtJErROg1lrcLVr+O3AR3Y6mKxtxBqFFa+HTzBJHA0IOOhtt1zZfumSa9ijDpGgFFDUowJ0mocvUGtBwK4INepvZOPqq2Ggyr1VLBW09Pjca9NSPiZa7CRUkGTqJM3VSzSyVm4J4hrM0zRLDPUaVEaRrZnuXDZyzx2dzM6WckpMkuliCpKg6FwqgD4U1VA4kk4Ld+k3jY7ncZLK11zJH48PeCRIxKqrYPcCTU6aDJ0ih6RdJj9xVkeMiwlThI6iuw4q61IKKeqqZ5sdMZJxX1U+Zq4nx8324qpKRIBF5m0eNYY0jU1nWwtGvvqXkeCORljc0FQ2AVFF0mh0g1LUzUkkksj3S/wBzvNnsrCBLe4klgEkgViTL2nU1WbUA2pmFABxA0hVCercnNmMjX0lDR5sZCA1E9fV1NBTtt51kET1EuAn111TWfaRJIr64KdDUrFHEJVZnDRieFIhJGkdsyqqHUdZA8mGKZp5nFSadCXbtwtJW3BodxuLvcraeRpNUamIyOwBIqXJOjUTVRR9AUMKkIvJbMkO2s/m4N2vDWCafJNLidz4DHmi2xTxv/E8vOMHUR5Hb2Hwi0UkrVLFJqdAztIrKoHkv0FxHbNE2nCtrR/jNNKVYaWL14VycDp+XaWnhvLuG/AugTKrxSxKoiQVlc+EdUSxjur8QAJNCKdZ9s4LJf3U27T7TwdVkYKmCkXDXYwVFRh0VKldyx02moy5xsVAhlhqaipjmq20gpr1gWmu7eN5ZZJlRfhYngGOAhNdNT6AGnrkdJ7C3uJ4Lewt4GeIUli04Ji4mVBTWQtKrqZSwpitR070dHTV0z10E0NHjnRzUPEs3j+3QTCWKVhHI6IZYW1NFZ9b6UOr6P1kijjDFmkOBw4/6vX0z1We6sru9ujb2yIqM0mhK/qKKAqONPUnGSacB0Z/A76wibfjp8rjaiFM2Ytsy0cEJrIZ1pmp6lJYaQiuWqp6dKcSVBCmqjZY2WUKioQ1Ptd28+u3uNZi/xhWODmoIJFCCa0H4aVqpqT0FbyzkO6SzpahJpHMUkSZ0Emo+0D9tfOnRbK3NQ11ZWTUVBMdN6OgNLUwvRR0v3EcsjwVtSEkkhrJdIpkhidNYLvoax9mwtvDCxyMtW7pMZOKCoHmBxJPyHUs2u6zPGJ4mmdoUEVsWIC0GlmyxOHb+zVFYau40OegV3xvfFZfbqJIuROMiqMlS/Y4/Jw4ypxuamr48W+ep6fLVLB6SdaA+WJQ81QsAdJFZEV7wWj287MrLrIA8RlrqVa0UlQMgk0PAV4Z6pu2/7Xu2xpJNBIItUgaCCQRmK4cqvjqkzPVGCAMuXbRXWpVQwBLDT9spT0FS+Sp8viZ8bNmM1gcBUQYahxtGHp6nsDJzRR1MWJ2Ft6fGVSZCuggaVahVh0XcOV08qbdEJmK6GqEV3GpmOAiaiuqRqgqKgUzWg6Bu37fcc+XD2yJIL63CvczWtu/gxQx0D3tx4SsIbKAIwllVCdVFK1bV0K+Q21XbO2Ds+o3ZVYzJDPYqbNbVrMXX4rK4xqaogqPHNFV4uUTVMkEVeIzL9qUZX1D1OQXRJ/jEsDKVkRQxDAg0aunypkD1r0juNsk27ZrC6uZFkSZ3+nMZR0bRTUQysS1NYodNCDg1JHXP/R3t/sfYO28dS47DS9mYLcMdZHvihwOamy9HtZonqpKPLPPHDtHKUlFWU9I1JNkAUoaKSWNZZHZghJNdXW37pPO9242uSPQYHZdBlHAx0IlBZSQVBOogHSKVaUtr5W2TnTkPZ9rtLC1bn233BXj3CKGfx0s2Vy0dw7KLKRUkWJkeYjwYi6rI1WVAi6UGdwG6K7rveGLqoGwOfydPli/2ww9BJUCGqpqCOmepjp1jmrHlmSOnWkhp/Jqe7TBohDfSrLa/WWsmqN4wyfxfbwJOB51JNeI6iTlTb7jb+ZTyzzFZtDcW17JDdhgojXNdJBdVHfU0GhVBFT3VU8G16evr9y4vbdPkafB0m8KvF7Xnrc7UjGYGgGfrccI6rd2REMsMG3aSv8Us86VMlNTvSk/QX9hncJIotun3KS3eaS1R7gRwrrlYxq/bCtcyspKgUBOqnn1LVtc3O3bk+2Rgpa3YWEmQEIBKEb9bSjFkDgHsdgGSi8chdu3GV+yM3ufa276KfFZ3AZvK7VzMWch+1q1zVBUmlrkyDV06+emFeQiGHSr2AUEvp9qbK6tdzs7PcdvlD2U0aTxOnwlHAKlceYPn/k6Kp3Fh9XbbhqE5LW7NcDS7PSpaTW2V1EU0/YAS1OkVsfbGDwseUxGQwuQyuOM2RrsRXStkHw23MxW7YyMGDx8E9PS1RoTk5KK4UIIoUEpESxKyr7dpr144nsZFFzqTUtFqyCRPEbuIrRSa+ZqPOlV/t/tvLlnc7ntnMu3SzbaYLmS2nDS+HBcvY3Bs46xI5UyzIlMBFAYsojD6WzZ/8eyeVyFFXYikq6iGnbHtTxUFRSVlPUI5+5y9BJkJ1xX2yUdMrMuqWUq62ZkvqWzskaLJ4pCA1Hz9B/PoNcux7juO5Xm3PtEcs7RNEyqtHj05aVNZEeFTNamhHlWoiY/bmPoAKemjljjo56AUMj1dTNGktJVNVTeapkMs88U1VIQI3JVCQiqFVEDRuGEYU07gSw888KfYOjuHl23+saRAyrbyRLbkklQUIL6jQltTGgB4HtAAAHQp7M2/T5ufeNXunPYGmq6PHVVfgY54cqIdw7opKqmpaDD5apNVksotXPjMhNMainjFCaxI4XMEImKo5ZJ4YrT6O1Zk1hJNNAUiIJLoKBDRlUEEhtNWFW0gs7xNfDd2t7y4glE114jnU9TMoYL4pZmdiddWK9gc6aqAwEPPYRKCuxdNW1NP9qEFFlq9K6oO5Krczw0tduSPIbdyVQmaxFNiqjKrQRslGlFVyUbGKWofy+3bG4dvGCRtq+ONSo8MR1ZYysijQxcJrI1FlDAMFFOk26JbzNA9xNGIwSs0qOTPJOSGnDwu2tFjLlF0oEcpUFmLVXtHsfE11LRU0VQ1NBBLVOtRHTyNU5eKWeNqGLKszBnmp6WErrjhpNBLF1ZrEEd/zHebfLO4tvErpVl1gCOgo7rUUpU8KuTimOpc5M9ntj5xstrt5+YBZMBLcxOYJJTcsxDQWzGIs4kdFKmQpDHE1ddTQ9C7m9tUmwcP1n2TT7R6M7uhqunOxe495bA2f2XunP1Ue16LI5PDUey+2Nn7W3R15uXrDf2xZ8YmQx2Cx2VeTKtVRzzzTRa4oUU7Xl0L2xuN83DbvFu7e0s7kQwF1lJJLQvJFcxyicAqzSxgItNIUkMYnuty2yNr+Tb7CNzDbzePGgkCvEoVwAhdGQo9FVUZtTlyzdooVjKeWo27h82tBWLk6+tGQkotwVWImanhyNNFJjI28FfWlM1R0bmOemEjLRFGi1Oys3sZsrmeWFnAjK9ukMDUE6qgqAF9D+KtceZPs+4Wp22HcLaxJnt56OtxooC+F0qSSZAB8Iwo8249KLefV27do9XbU7T3DT5DEdc7/gei2lu7OY2k+zztfDWZnDZDG4plRBnPHmcJNRyxroplnUBo4xIjOG9t5g2q/wB93Tl+2u4n3myI+qtkclow6o6NIPwalkDCtSRwJoQJB5hgt7Ll+Dcm3KtrOkaeJIiF1dw58PtFZFbRTiqVyUUEMVH8SdkbK3BvGXMbq2Lu7d3VPVOwd5dtdq7O6qpkwVfJjdp4eSnxT0NTjtGMxeGqewM5hqaWUSLL4ZpUQpMRIEHPl1vFvsstvsV5b2+/XlxFZ2dzeAvGhlkAkZloSxWIOQDguFBwadMcntYeJt0kcbNHDC001laxkeJJGCwESRPGreWkBq9r1AALdPHzQzHxj2d3xtDO9BfICbfeKzfUPX2Zyea3Jt6s2s2wN65CPK7iyXXO5sjBS1uxc/v3B4qWIZirx8v2kuVq3o6moaqVkBX7dWvNd5yhfWPPPL0NvuAvJ4fBtZHljmiBCCSLxAkyRE18NSMRgMg0U6Oub/daCT3N2nnLZ7+Pb94s447eO6idiiy28pljudTI0ZklqQysFJNBMxZyOix9z0FHBsPpXsPN5rDyVHaO581urI0NFkIayrfam392R7ExtZl8BgcRWZKkSty6ZBUp5pKVsgtOrFTCqGUW7Hcr9dvux2dpKtpt0cMKs6uFMjxeM6pI5pLpjaOpGoKWpqLVChbn7eLPmL+r/OW87jHJzHum6T3O5lIkRDF4qRxMsMEKBVLPJUIEVqBQtE6UPXO76Gm3hubLbf6jyu2Rk8zXvl81LDj9tS0GXw8dNh6fCTUVRkqqsrMMmKZagPGxo4W1SRg1Ek4VnddsNzt1vaXO6iWPwgNJJckN3awVACvWuRngOAHUve2/uCuwc8bvzJy77Ztt9ydxefxlSO3SCWGka20kUzyGW18LSzK+qMHUwUu0gKC3v3z3T2ThsntTBnC9bdTbV7FzWCBq89DfdW/R9/DWxbqrpYkp9y0mQx+SEcFGXjgx6CNaabyaBLfbeVth2ncI9wmL3W/y2ygO4PZCtKLGoP6dCKsaEue5q0wCfcD3i9yPcG23WLarOHYfb623Gbb2UXJYXN2zySyrcyudNwsrSFliBWKEBEjNRHVAbj7Q3J2LJU7d3rsDr3L0sG79p7iosRj9obzpVwMuDo63BtjayvbM0WdqdvxrmqmTKY56mYtNpKMkqPETC32lLNVktt0u1kNtLC0mte4yMG8SgTQJF0AIwUUBIyMgCb/7ibzzhugi5g5T2ee1iv7W6j2+O1nWKL6dTF4UhEy3LQHxH8aJpWqWJUh6jpD7q3HuOTPZGpxmQxuIwuc2lQ0O9sRkNu7alwO48fsmrqq6mxe09oZLamU25iptn4SKmeGKFWamQiWmjCq0QeWws9EKPA8tzbS6rVllmV0aRQrNJN4od/EJIJNdWdRJavRdec+80wXW+T7buNvbbbvW2x2G+209nYy2tzDZzeLDDa2MllJbW30aQxGPwwGiIDQ6QNHUTqqg2DiOwupt4btwPYKbDwlU2VzmC2DuKlx+6txZuSOpq6eTEy7tx268LiZ6qnhomyUbQ1EFdQU0lMogl/e9q94bd5No3O02m5thu7r4cM11E0kSgEYZIngdlpq00YFWOruHb0Adk+kst65W3xLa4htbWQXDxxFnMswbVUpK5UF1VFlAbS6LpopyXHOxTbgoMNtDb2290bkgrtxml2PTZ7C0tb2HmMDHumonotmS4ugjropsiq5EGoP3U/gVYVIp7FGrEzWha5vJ4onWLVOysViVgg1PqalFWlfKueNehJvcse8W9ts+y7VeXVk140e2G6iQ3sluJ3aO2aOIMpkPid51PpogHh0IYYIMHS4fPZ7B0uH2Bkcmm39+dZ7vyG+cZJurGbXz+5KO+Dl2rksVVUtdtPObH8UJgycDTVb17MWjkj0JGjmRr+C1nF3cLEJYruEWzeGZFjIJSQMCJI5KkMpoNJ4givRrLtkEM95t8FnaLcKlxtt9NeDxkilkasYgdBqt2gCKviDVIzl8FSArzTY6lAk2uyVaVK0NNlIcpV1NQUlhx1G7zmkkqoWeBYFi4V1MhuzSE+r2sr3JcFh4erRpHqxAFfXJ6WJCPprjl5LdxfiJbtbmUkDRFGXfTUVUBVNKita6jxoMX8J39/cP777nEfYf7Lh/pev/AHk2Z/x5X+zI/wB3f4v/AAv+8H94P7jf3k4/hOj+9P8Ay8PH/Bf3fZNr2v8AeNPHj8f95eB8MlfH+hrSvw6/C/F/Z6e3+06b/fXMn7s8D6dvB/dP1Oqgp9P9f43i1pq+m8Xt4+Jqxq0dvRWsD2DgpqffVBianC10dXQx7Y3DXRY0qMxl80JqPEGbI4mAVW5sHi/HMnm8gFox43iptE8gqktmVoXkHDKhs0/KuDn/AFHqPV3iG4tNwtIHjJYiORkQDWxJ01dRWRQAQDU0xSi0JRm5sfi8VtnJ4DCVseAo6jGT5har76uyaVVDLHDPV1rCXIGWpqWkimKtEWsSDJcAe1EbB5MjUeNB8vIY/L/N0Q38a2lo0MT+HCVHAlq1/Ec8cf5+rNf5Kvy4+VnV3yc2L8cume+cngPj58m60dY/LDC7jrxRbQwPTO4dtZ2n7K+QFDncpFiv7jbr6H6yXKbkXcFLkMXLRDDRpWTTULVSMoGTKi9sjAgkZA9ajUMen+GleiWJnAgeWk0cTBlUmhOCV0toJzShHnjFaEfTz6S7g6no9ob4+MvRG+vj1R/Ljrfr7N70z3x3pct1rRSdZdh72jzG4MZgOwtn9LPhsf8Awnbu7a+LH5qrxca1EsSrUTS+esimmWoyhTHGy+KATTHH8qcDx6QTxStKl1cJIbNmC+JkkqKZBapFRkV/Lh18i/50/Mfvz52/IfffaPyR3XuPI9j0clJhaupymbWPH9b1eGr56c7H2btvbtRlMPt/aGLz9RE8cEElPAtVDPUzOamRipWSyaZpZNTNXBXBXzywAXGKUrw9ehTI1tK72NjbtbrEF7xIKpKMf6GX192k6iwFVJxQKNxTq359/Hb4p/y2P5Ofxz+Y+B3FBP8AOn41/LP4u9nfLCk3dU4jd3xx6K3xvbN7Jfce3YglXPlJK/dmU25VVuSdNNBhMLNJMtS08cDWgt7Lwo5YbZQKSDUv4Vd2ZqeQq2T+wV69ue4799Ze2u5btK8pktnkSVq+NNDCiRmTOtiEOlWNQK1LA5NWn8qT4u574Ef8KAPj78O+3Y/tt1bD7W3bUbOylLj9yPtrsvb2T6V7Kze3OwOvsvNjGiy2zsziKiGrjmqamLxvLJG0flhkWP0azfV65MkGjEEY4UqOORwx1q4ubJdiltLVtKuBJGjh6kdxfS2kqdBw1W48AQKgx38t/wCQG5vjp8bP5wfcnWe4qrrrf3VWw+rN8bSz2NWipMjtx6j5L0w/heUoBGtHLia1ZlpGjqGkoamhlqImT7curF8bytLeXUL0dlHDhUOoqvkMVqAPToR7hZwRXOw7fuCh7MEmRCApGuORzX557WJpQClAOhK+XHZ/x2+UP8nX5j/K74pY2h2x2T3l8nfiDUfKT4zQZenweG6a7i2ou6svvLc+Cq6nMT11D1F3FR7ofNYvz09OoqErYBLLJFNQUa5Y4hC0nwsxBZVHmAxwK17jwFTTh5dEVzLffvGGx8TxEgVo4ZZX0BkZ4xR2aigqtKmgLAg0qwquT3f8yetP5YX8num+LH8rrpD584bcXTPyDq9/7h7Z+BvbHzHl6frMX2/mXipNv5LqvcGDptnRbt1VEho6wCtzbU6NGomieE7SBJLWLxrFJmFaawDSrnHcCaf4KemenY923Db95uf3ZzTdbUj+H4ptZJIqhLcVakbpqIqQATqbUQvcdJI7/I56G3n1h83u3K7vzZG88pu3ZPwo+Uc3Y3UXZOK3h0hvLP0Nd1NTUOR6+ko6qmi3h1NlMriJaSmrHhoKWakDJPFG80IHsltL+KC/uLR7cJGqyFlU8NIZjqIGa5ocn14jqTubOVL685N2bmv9+teXN1PapFcOhUP4tEAiUsdHheEiyIFRKhQKlWoCXyi+cmzezfi1XfDv4zfA3Z/w86U3v2TtvsLuzqqk7e7R7r3/ALw3BtWOtpttV2e7o7AxeLkmweMZqXLUOMjooYXyNO5WsYySSOgn3S2nkJtWjisyA6yg6y7AUpQtXSuoilMVr8uhptvtfvG32kC81WF3uHNaFrW42iSN7ZbOFySJfEWMo0shVJVYsokCshYk6+jYfzVfi18qPllsP+XP8hvhP0x2r8genI/5d/R3TctR0jsvJ9uZHZnafTFPmtvbz6OzOP2Vi6nJ9YJhcrXQSSZqSkoMZXTvUx06SLBMWNTCb42dwA0kTRohIDAIymjlhmtK4B+0E8eo2g3N+VU5l2B5orHcLa8ubmrtEz3KSiMwRQvRPD1BKvKjGq0UoBgqD5CU0mF/ma/8J2/iBHlsFN2t8Ear4PbU+Wm39ibix25ZOnex9x9+7Xz+1+j6/dceWrKfdcOwMXVHHVww3lo4aSrMkmiN4YqZemiyktYriXxLg6YkdxxOsswoo0qVUin7ASa9BZoLrma35l3HZLD6PZITPf3FrbOCYYzB4dv3SETyxyOHWTSMKTI6qpWhTf5pvwB+W2X+b3zW73zvwm+VWQ2Bt/5b/IftPbfeNL172VurYh66ze4YazF72gqMVtebbmK6727iMauUXIGqjgoFgkqqqWOnjd5S25O4rfXxgd1tGXuXwWUDQ0jM3ilQCXBHqKAUyTQdctxcnzcscstvcMEm9R3NLeUbjDNIfHjtooozt6uZEWJ1LCugh6mTsXvb+wmzEH8gH48Y/b2Lkqc0f5p3ZmJx6T09fO89NP0Ttyty2VqKfN5GHM7yq6rGCosKOSZ/LL4FvHC5CiCWOOxnlnl4yMdTEYOhacMKBTzpjPE9B3c9vvbnmu027Z7Gji1hQRRq5Lr4z6jpdvEnaSpNE1dx0qNCkg+O2+ovkV86tlb46r/ms/y4uyuvaz4+fDTsHcnx9/mr1Wy92dX5vr+DqjrWk3hs/ZHb+7Uwx2R3VtLMQ01PjYaow/x+QvWJAr1FTU18C9AzWzCUHUFJrQrUL8NTTSwNPtGPXAVuWgi3WFtv0GCSUKIxJHKQ0hXxBGgPjRMpb4qKrkEUoKHWHiqKrLuBgc3gaSpyWIyFFQVWc+9xuFoXoKCKaSXKUONoJs/SNVwPIEjlpk81Q8Ynkp4nMil7yCBNfhO2RVUpXJH8RAxWpzUAYBNARcsUm5SGC3mj8YRMiPOxRBpUmraVLgUBoCBUkamUGozpgaPE4Kgwu38e2JpBkZ3oZ5KTEvJE1XVNl6/7SGpWenVnyUiftpF9rHTjxroHPtyWUyMJGfNPL5YFfy/n0msdvjtons4ICrM4A1BSQT3EKD56qcBTTjHQsbJpYKx6OizElO0UMKT1CVC1FLQtUNUwmnE1TFUIktRLUsrK+lllQEaW9Gotv7x7aBriCB5JDU6UoWoOJAI9Bw8j5jJ6F+xcsf1g3D9x32+Q7faoFj+pnUiINIVoHYEZDMDqGosqmisdKsLm0t0JS5nHVOQwjbuEddiYsXisfWyfxDNUceQU5qlwkmKvFjtyvTmSGjWqgjgXUCV8kal0u4wzSWlw1vcrb6o3ZpHAKxnT2mQNTVGDQtRq4pWjGgPfb43U7dbSP4ySmFAoqJg4I7G4+JX4QcEHNCMqDbm5ctXVe7qmtpspi6mTKxzR7a3ytA+QwtFW5WZaiioIMnNjclPHNFW6ZBjYGhMjNNpUsZA3u0G0yWWwttjl3Fu31E8GoK8irUMCgZQo0ims+VATwJlypaXmw7zu9jvVu8Mcl1bRx2sy0cuzaHDAlXFUr8AINQDTB6bK/LVFficEM3W1mVqMXSvBTZdclSSLFj6yV0pNT1C0k8GOx8UP2qQ+IvHLCqq0hcMqeK1WF53tIkjjkIZ49JywyeFQWYnUTXIOQKZP7e9hhvZrO8uHluVldElJGmMHtqGf4lUCgFK1GCaghT1LT7go6Fo6bGxQtFJSRuFp2hlngXzLQ5BY66m0OKaM6QjAh/V+47WCWCT6YTxPLIZQymlSTRjTUtVONXr5YwB0s3faLG33eHcraKM2BWaWWUoipG9vGOwhXGXRuIpQio1MT0EM9VTaY6h8lXT77xOcqNv1m34qKbF0U+z6rEvWjOf3hFQYqnKCqqnoRBIJWES63kLBRGJGM1yI45FUW6xjQ2D3BjjTQYFAa+uOHEJxz2O1O8toivZMdbhdUbCqjIYatZdXYVJqKVIYmqp/LbEwO7MJ5cthjR44lYvDT01NVU9djsNDNUYmnzePJGPybHOpHIVqXeIeJTpLEMNJJLBKuiTVJWprUdzEVKniAFrgDNfTrV5Nt9+1zZPaqIlWMoFIrpUE6XUdshJKtViQNPqahwwm/wDd22sdRY7bO1qTDZajo1xEVfmcjBuLCSJSyxrFPLtWpxEFTkKKqkAEdOcmI4OPQdKXLrvZ1vWuPrrrXZsS9EVkdSeFHVwAQOJCgn1GehDDv5jj2qHY9oNvvMKrEsjSiaNtFakxvEGOutAviaVHBTjqbLlY5aGmT7RI54lles+2rf4g9bV1Qmlr6p5TQ4uZ3iXUY19CaFBtcqCqjjnDEeJ2EjSCKaVHADLcfPz63KuzqGuZYD9WoOqVHLamcVLfDHUqRVeAoc1xURot3zR7apsHQ1tTT47LVEVfLhcbXyU9LajaoixrV6RTpJBUY4ZefRKZfLBcAKuoyMptrW2ja5d4mM2jQshPAYqKU7gdIxgVz5UABud03DXNAxcTPOJJpFOlXIyNIAzQniDwxxr0CYpRTSxVCRJLLRyLFRU3lNTHrIQOY6im0ikmp4NMrNKrIWB0lmNmtdqvgvRiNQozfLPkeNTj1+zoVcs3t1PudkktqJlheqxNqAD4FQy4FANVTjHAk0IKbiw77/we8odubmx2Gz+MqZ6Ojo6mSsx9Zk984bcOPx0uDxmVeOlrXrME9c+SaupFqYJHoVhVrGQxomuzZz7er2jSW7MNTClEj0M+thwoSoUKaHur9owl5dk5l27mY7Zvtta7tExKwyM6STXqXMUJtoHKhnli8UzGRNSUiKhqggEqpeq6DLmv2vgK7LV/YuDlyUmWoJMeybclocVlqzH18y1jRQ5Hb7UEccfm/i0VJeayRh/NCSKTuEiKlxLEotHA0kEFqkAgU4NXy01xnyPUEx8nRXcl3tG2zzycy2rSm5ieIrCEikZHYv8AHDpxq8ZY+7tFSyVHjdOKo9l9XLhur8ptvdWYSrrKvf8Au/bW26OioNgYwT/awx1ueyNNPuyfNRmuWnjqUnqKekildYGkqapHUitJpLnc3m3GKSKAHRbpK9WlahYlUUlAtAcUDEjIAXMrcwbdt3LvIVvt/JO52m67r3XW83lhZhYtuiLJCiyXc8Qu3mLuq6wxgiD0ieSWfUq56S3NNXbUipq37gZwZNYdztFPUx4ysearbK0uGlocKMdiRBHjZovvcczyJCwMcqxteBK7naKZ2pQxgao6gVXFNQJqa1rQjy9a16U+32/su0RxuHS6MwS9IdxFN3+KsLxQ+HGU8OniRMWAyGCnsAobU23T1GZrIMTP/AaunpcjX/xWoyNNRU8MlKk2RkLGqq6enSJaCKzeSSWaVmRER5GRDqaXwoI5J49cJZVKqpY93aMAE/EfQADJIAJ6SwW0L7huEO2XDW19GryrKzhACp1nJZQFCepZjgBSSB0vqlEylHEEnx8UlWKiGal+5Q0tNK0USyVssKhJYaZI5I5GeGN1CsQEa5BRAm1MmGZAO00yR5AE4JrihP2nobSInMptQktvFds1Z4w1UVtIDsVFGWPTRiyKQASAp4dYN77Y6t7E3VtLrzcfcGE6sNd1lk8xuDvfsbEZjeFTuffWyNuVVRjuvKGloanCY/HYXc246JKbG5SrklnGJk80zVD0/hIZW+37Ztsv9yg2B73/AB1YodusjHEI7eWYAzsZKkvHGxeRBgyKVQANq6MOa9k2Hfr/AJa5TXmDbbW/ksBLdcwblK58ZrXUjW6M3gwqgRWeFm1STRBVV5JAsZT/AFljdvZuetrcjumg2diV2dWUVVuv7evqDnKSLCLXYbaES0GQxlFDUb2zEENBHW1xjplikd5EYKVB3vNzc20MAtdtN1ObiMrFqUaAZAHmqwJIgQl9KgsSAFpWvSTlDabPc7766TdIrSxS3W3uL4kprgKJWJT4kUZknpoXxSiuuoEE1pm2ZgZ8xk687cxVLV5mbKsuTz65qgpafBYYtUzz1G4c/uibGYLB0lFGggYVFSi3QLASdKe730628IkunYW4XtQIzF2FKBEjDSOfOign1HW9uvNssJr24soEfd5LvS00MgaSOIl2cOZ9EaaQArAt+HsIAp00xZ7r7bfZVdt3f3bG0a/a2JeroqTIdYbhxGZos3lqOCSsMwz29pdm01PQJItPTyLYvC8joYpWMniqG3K72mO827aZEvZACYr0FGjUmh1LF4pLUqQAaHjqApUh2/mHbH3+K33jmC2j2pCAqwSx6ZHVgz6pbhrdUVV7eJ7jo0mrlVh1HW47cD5PfUz9b7oxe2KM5eDb8266bK0eUpKzLfw3E7cyOPp8xgKzL7omqcguRqsTBMtVDSQNKUnpY5B7U7hctCsFgi3Mcs7mDWkbDQRGXaQsUcJGFUqrkaS5VahiOkO3WdvuEk28XFxZXNrH/jEZimWckPLII7eRFdB4zE+I8bMHVFqFdaAq3G7XxOaxG+t05/snA4jL4bBbUi2xtrJUdZmsx2VkM1vzbm3I8JhMji4Idv7Sj2/iKqfLzVNU6U7UlAKaF3eQKrkd/It3Z2kW2TG3dn8SVaKsVELVcE63LntFBxqWpipZzDsw2a2tZ23K2kkm1V8KRZSaNUAaKKgrmoqNJFGNCAq8DS7sweYqMRLWbSgGDdPvUzWRTcONkx1dWUtGsmPptl02dze4KnHx1RqZUohVN4o3ZolVXX2kvtt27dlFwLWdpJPh8MNG9UqakSFFWtKd1Pt4Ho85a5+5x5a2m5j2jdoVs7ddTRypFISsrANHH2PK3GtVPaK4UFgTGZfYe6uu829D2btGl6K3b1nX9YYDeWF3HtHdlNunMyZCbE5ikfde3MzDksrR5zKbRzwlyMFTFS0/2cMdO9ENfidJeGCQLaW1y16Zo5XgRWRQmCMEFRRXXtOW1HUGxXoFWe4Tz7hJJFClrZurvJdIXkoS9QnAk6QwQ0IGlcjNOi596S47eW9O1N2bA23PiesajsbdGW2nDlqPbWJqqHZu5965Fdo4WTH4KKm2rTZODHVEEUtNi4IUpxFKsISCFgDSzb6aDbba8uC25eCqPQs3ekYMjE01U45bBJGKkdKLJXX6iF44lVpFeRdSmutwg01qoqaYA1AVzQN0kOycxv8A/uxsbC73pd2ZvaO1qPI0myMNm4GxdQMf56atranbMOTdXk29PlayeOk+3X+Hy1CTNDMWmkJK9ot9ihvd7udoW3j3S5kV754ADVwulfFK4MvhqtdXeF0BhQL1IG92e9Ja7Zcbvts1xs9uGhtVmPgySFViJdYjnwgW0owGl6EK58m/qPb3dG+927k6m+P2C7N3E3cdQuO3J1rtiKkVanZGHzNLnMJN2pHQZSmw2T27tbclJS5F2MU9LFk6akWGGaZYz7T808wcu8pbCOZ+dNxtLS0tELfVysQNRUl1iqC2p1U0zUipJFD0m5bsL7deZpNt2OGVopZa3EUscQitEcmGOe6k1aVjhaY6mRW4iNVkLaennNdRbbyP3mJxk2Roqqnp6WNpZMnNXVNev29P5KqeiGRE0i1VRKiyCQwU6OQwVYwo9h7budr+LbrO8vxG3jOxoF0KAWaihsgUXIyzHINT1l37g/db5Yn9xucuSuS3vUXaoUVmaZr2dzFbxPcStGEtndfqGZGcxQQIAJAfCo7FN7IxWy/DsvY9JuKFd1UWAzdRvObCUm5Mg23d1x0v96NtYGbTCDmcxtyXwwmOlqY8RE9WzvIxj9I/sLu8na8uZbRxaNKq2ysUGuOgV5BQmiNUkau/t4CoHWFnM+1cvWNty3y3HfaOZre2uf3u8SzSCK5DGe3g7SRJJEKKdBWIM9WJKk9TMD8hMXkNwda0XdVXhazEw1lbWwb+3HQZXcGfwlJWUuYgbcGUq8PkMud1UtJkq+Kkx9G+PymqjM88zsFjb2jn5fktbTc5djilEwUEWcJWNHK40ICFERYA1IdM6eBrUYbB722m6b7yVa+6strd7fbzP/u6vYpbm6iWQSN40rLLIt6IpZFWKKWGdTGX1kqFoUvH7rO1t99k70xFXiNw1FHjtwSYaet2lj6XblXW70jG25M1TbTy9RVUdPU4ynz8lXjop6epmjkgSodI5YSUFj2sV9Zbfbyo8dXQnTIdY8Jg+nxEIYqStGoaMCVNVYjrHV92fa+Y+aN2s7mC6VROY3a3WOBmuVMXirauSiFRLqjDKzKQrlQy4Oj1Jsgdm1VAtLmN3w9rYzam26PFbHqaFp8j2pPU02LgyW3qwpS09dW7o27hqqSroZZITLWvSyrpN7sFt73SPZYjcXEUK7MZXNxds4VbcAMyyNU08JnGlsjTqB4A0mjlDahzRfWax7jdLzZHYwItlMApvVCIJIixVS1xFCdcbMKyFGGa5LGOva7ce/K/b22cnUVOOqpMocpFj66OCDJ0KS1GQy9CYFrEjpY6Kp1M0aRKEWYAAhC4PpLqC0gW4uSilSulm4qcAeWScD7c06iy25d3Lf8AmCfZNn8SYuZWkSIgK6KWdzStECgFjSgA+S1A9V+Jp5MpLt7FVtJio6CmrKSn8+4qfH0lTWRUkFVSwSVmR0HEtVU1KFknWokp4I5CrSxXBCATEQ/UOrGtDRVJNPPAyaelK/LqRZtpik3NthsrmGFYleMGWdERpAoZQXkosRkCCrazGuqhdQahOQUGNxWIXcFJmMjjd4/w+hrcjhYphiKPaVFPDPkJa+PKJkVp6fcmWyNbJUP9vNL/AA3HRQeZ/I4iLwd5Hkge3U2+QH4lycEaafCAPPJJNBQVJAtrbwWv19vfSRbqERmhUhBApVmJ16gBM7tq7CwjjC6jqOgDFs/ZnZefE+E3V2htbcE2Ao8hBVdn0W4pNx7XG1ti4dnoaCLLSUgra6mlosdFQ0ivD9x5JY7RqHWUk7bht1rbRXNptU6GZ1KWnhqkuuZxqLLUKGqxZzWlAxqSOh3bcuc2XMM9runNVnPbW7N428W8xuLZYYMAawviMhJAAKlwWVtADBitsdsXO1+I3V2HQZTBNs/bI2tt/OVFZJBHV0c+XNa2JkpKOugEWYbMwPKqxxCWU09PLJMiqug7n3eygvtv2iWOT6+4WWaFFBIYR08Qsy/AE1KKmgqygEk9bh2fcbh903RN5tv3eqw2s0sigOkbKWjKo66ZBKKjBLEA6lHwkbP789mf6Ovsf7x7V+//ANk3/un9v/Ett2/uX/s0394v7sfYfwL+H+f+7X+Vfw/y/wAIv/lmr739j2k+m2z6yv0MtP3pq1d39r9NTxPirSvbXjX+jnoM/Vc00r+87bX+7vC/s7an0taeHqpppoxX4a9lNfVVmxd+Zodebqp6fEbRx8e2cPlafHZaEikilP2IZZIqKqjahrMgmTyEcz+dwZJapIxADqjcdyIiTQ5ch6FtXHjT/J5flWvUU2l7dS7ZdqIreJbdXVDHgcK1zgnU1TU5JppFKEMsX/eLa+BiWpmocjg5a3IVdHUU8ASop6yEQUWUonymapMccZRy5F6aOe7vpmS8cT65GKhhFNIjJqVqen+QZ4f5M+od1XVrZtHKVeJ3JBrUgj4ssMVPHPGuOhZ2T8lO9/jhvefsjoTIbn6O3w+z937Ept/YjMYyr3Ht3Db8xFZi9z0+z920mFxX918/mdt/eUSVVM/8Vhp5pBSTQu5ZnUiTVqMlTwoBTjjyzTPTMlwQrJBbaAR3M7BxUd2KhVr2mgNSeAzxW/xmz3bG0+4eqOx+od57qxfa2zsdkN/4zuDZO9UpNx7A3JlFqhR/x6qo6rL1FWqvWvFWUEopsjVxTH96KKOeNSbdrqOzhuJnlER1qqgggtQ50EFaEitGqRkgg1HUqe3HKd5zZvO3bba7bJfarSWaWaORCkBZaKbhCs4eNCwLR6UkbDK6BGotqrdmT7N7t+Q+++wc7t2l3t2R2Pm90brwsG39sbYTc++83C2a3lv6DZ2PkkTb+D3fuXLT5Cnx+PWPD0Iq2ipo44kiiTTyPJbW04DOWUktU8C5IWulRVBUcAaD06tb7baWe/b5tBkjtooZ1hSJwoZmihVWnZGkllCTtRwC7Iuo0JI6SW7DuvcybK6+3J2NuHfnX/T2JyuC6s2H2Bufee5tv9awbgyc+5M9i+tcBldyVu1dlUO6sjPFV1VPRY+GmqqiNZjCsjFvb/1LtGAWatfI0/bip8/Pz8+g/wDuW2iu5AiRMgAoJFYsW/oHUVAK0oNNKAUAr0YnCd7/ACy3M/XO5cd8h++KDfnT+2X696b7lx3bO88nvnqzYtDXVNBJ111PuJd2S7r2fRbVpK2uxkSUM1LRQUk7RU4TlVZOqBop2kqxIIDE4oDStThfQDzz59GsQjvrC+2lLZEEaMrzRomQ8is/wiskwYFfEatFAUEUFABx2+vkDQ7B7G63o/kJ2FW4rs16rFdq4SLfOZlw/ZOEObps/i03LJQV8p3hEmUgWrNPnzX0tPXAyQRxVEcdT7epCkhaCBUqAKLgYpQEA0oDWlKfPonkO4XFr4F9ub3MqyOxMpEjAMKalc1arLg6iQMgAcekltbs/L4jN75x0/YNdsaj3DImz98Q5CfKwbf3Nt7b9TRnbeLj2rQ5rH4Dc02LzLRVFK9fFJDjUqqiskkiHgZPTfVJEogi1kjUoTgD5ljSowCKDiRQAmvSnZxtN7uMx3nc0s0QtHJLcKWJUUCJDHrVHbWRQtQIrM7sqBSDC7J+e/zj6uOzOsfjF8+flZsXY+HwIx2P2pgvkp2fsLpnbFXVVIG4I+sNhVG/6PH1mBwtdNW1zVK09OtXWiocRygfutpPcR2zm8iaJEY0SNmLFclSxUDQXNBp7iMZFT09Js+3S7/Zwcubjb3s00SiS5vI4ktxJRUl8Bblv147ZQT4jBAxVqIQorH3r/Mg7e2R2Z2Pu/ZPZ3Z+4+z964zcm3d391Sdub/pN77r/jcUWG3Bid9ZqoKbi3pia/G4+Knq4zXQUlfAEQ3SMe0drslzdmK7u7l43NCyUyVINQGDVGqua6j68epB5i91OWuXody5X5e5as76yjZhbXTk6EmV10u1vJBpYxhaK0XggkgrTTkH+uN9TUeM/vh2FlM9t3bW7chm8ftx/wCKUeHrN2ZHzUeQrd17iw+Ox+2cJuV1llahevrKiRRRkUkahoFmdPfWiPMLexjjkuotJkWhZUFKaEY62TGaKANWT8VOlfJ3Mk9lYyb/AM431/a7Duj3EVpIkojlupao7XM8Si3huk1kxM8rt+mTEmYg3Qz03zt786E2d2JhvjH3V8multvbv3jXbd3KNq9kbu2PtWbE7cSfC49sthNlV+DotxUMsFdU09PT11FIYHqZ4qmSVyjO7ttjeRMgmmj8ZoleRISV1k1NDU8QDxJ4ZUAVHRdz/wA2cr38O4SbLst61tFfyWtpPuqQzrawRUVRHpjUaJGrRAg0kkSvK+l+gK+NPee6+uN6JmMDu7FwdpZLcWE3dsrsClzue27mdnb9/iVNkNvbkj3Rho6fK4Kvos5KkkjY3x19LVqksBE92933ezZzFcRiaKOKrEJQklRqNMipFKqSaYIrTgg9r+bINsm3LY7yDa7y53UJBHNeaxFEZj4Y8bSjEQsrlJo0TVQgqNXE7/yL+cf8w/M7cqtmdu/Nn5p1+U3+cntHe/ReF+YvaUHXtXsvd8GZ2/m9jbuk3du/cmE3DHmNvUeieGop6iklirJ1eGSLyMGNl3Q3tvI9veNLtxQFLicOzOaKQwVSOyrUIqK08ujz3V5Ct+WNz2+LfeX4LDniW6D3Gx7RJBDb2cbPKogM8onrPoiSRW7ggckhskAjk87nt19ZY/ovNbq7W2J1amYzHY1LtPOb73bTbbPZuU2q+yt07u21trJVK7Rq6ip2UiYnJ5XHYylpcjj2aCENA5MbEV1cxEt4qzaHB8NdJUZDCoH4q5FSWWgzUDo6uuXdi3Bba1uNtuNmeezkrf3LSpPM2iSGTw5HAWS2ER0SGJEhkBcIhVywTm6fkv8AK7dHx8b48bm+Q3dnZ3Reyd3Yyt2rs+fufeuT2Bsyux4qRR4bZ+C3LufI46Ct2zkKmsixbRUavIlaxZ0CmNDfxTLNE82pTpH6bEla8dWjgKgitOGacTWKJrVtv2jcbKwignCXX/JQtlQSqaU8Fbhv1XVHB0Z76gsexQqbpKvH7WwmAGNpKbA5DMmnx9Bt2rpchiqnNjFLEuSbM5LVlajP1NBFQViJko5KannKLHFrjaFy8aTVqinQSQVpQA0+z1HlUVz0ihLbMRDBO8Us6BWSTUDIw4qTV6hSrUZSFY8Kgio81MWGrsdBXiGvosPQY6epkTE42pzua+0kd6r7unxzy1CyVIoJEMUEEMrPoALEkv7LaXRmMMYMkjsBH5CtOGBXj5/PA8uhvCm1tt0e4k+CkUTPcKAXcUaodQxK4QigCmoGTmom4s0ufx6VdLkHUmiFphLLhWxCJTMS+RoatIJIEpaFWXwyKakBCvjHD+3zE9pJ4TQEU/CQSSSf2gk8a0HnXy6JZt2j3W2F225r4jSKQ6dgVVAAqgGdNaDiw4UoAehCwbyY2iOep8hVnJfcvg2jwmWo0WZo9vUmZr6qrwtX5KzH0dRQTo9NJTRxQAxsfOXjaP2xf3FnPDDtrWIV0/WeZw5BBcqqg/ASG4ipNKVWjA9M7LZ3E15LereliaJDApXV4ipqJ0mpC0yCMD+IUp17defyWTxu2IsFiKiMruB5RlZq2hpazGU6TrNnw9GuRkWrSmQXhp2TxSyOGQIysnsrt7VLaW6d7gMWjCtGAdJBBCGunifM8R5kih6GLXdxf/SQfuuRTDcCRZmZQ8fht4kzEFu4hcBTgngAe3pip6rD0kmGpqfHU8NRUZCN6iOWio4qmvRqeox89QTrFDTVOiGlnLrJqaMONN3CqvRJfDuGkkOExkkChBA9f4hw9M9E+6ss97t4tBpha4LECNAxcqV1EA6KEBcV8yaZ6FWEwYbFxxSYGpqZIUp8kJqOBJBjECQxoKqokeVopsoZYYopZl8Sk6kBVhYuhkeWYslylG1IobBY5OKeS0JIGfI0PSLmDbUu1IpPDHBRLoKxKhTQCtTQM2oANSh8qgAAKMnUVEGarXIkZ6eojSSomIdXqJpo1bHKJbwSGGuLKqL5GmVWILEX9mNu8Zt4wy0OTgnhkhsZ4fZT+XRtdWF1JczLFMrWjxRxgaVA1ABCi4oWDYAGotQkV49LCs3PjqXbZozRRrPWVlQ9ZHelQJH5XSqjpywknfyvpZCWUo91BUD1UMEzy+IsuAKpx/n/AKv9gMWdlDa72JrlCYYY/AlUtxfSQpGfIca+dMinQe3g/iNJaSSmdY5qkNI1dM8ZmUrDS1AqSkcWqKFZdUcjiV3F7AAe7l3dJWjTUB20xTGScVrxpkeXQ0hsrazl263vbkQyOfG1EPqowIVTXSEBC6qqSGJHCnWTJF8VhtyZmoWrrMdg8dX5DJpho6mpqxjKHHV2Zr0jp6UrEIVx1PNPISQHjRrSBVJ9tieASWqsQrORTWQBUkKMnNakAfM8M9OT2d3Bab9cMxaCEP4ngqWbQI3c9qjTpCguT5gGjAAnpt6s3JRbxp9nZipkym1YN5MF2tidy4jIUT7j28MxncXV7oochRx123Y8Ji81iJIKn7itSpkb/MRzKjBX769Fsb2KKEytCpMzRlToYKjCMiuvW6OCoC0/iIqKgrb9pl3dNrkcvbx3w12TXKFPECyPE0isKxiNJIyGJYHBoCRTrjRbgx02NyFBT1pWnR61aZWqYAaqlqZ6aGkqJ46iSnixstW0RjSV/IUDW0KLN7rdRkyI5XNQf5GoFAS1ONMfb5dCzliUR2051opaLw5FDCvxYclmUJrJ0AnVQZ0itegi3NW7U21ksdvOjp94V3ZSY7HbGqFpaWky0jxy18sVFksZRzU80+Uyk0ctOiUqpTvUTF3LBgoKdY7yQSwymIbUWMi5IOQKhsgABq5qQBinHoTXe58sbXJs+72H71l9xhCm3SgRxyJ8cgSaEENJLI0RjUR6UZ5NT6wQoIQ7Vretcz07vuirOwt5VCZPJY3cPa2GipanEV2Uy4yWQmwm64qbHVG4aTPw4+oqnSenlqJaHzGKpaGldFmC2eO+j3WykFhENCslrIxB0r2hkyFKagBQgVoCKmtOgxtEvJt77d8ypNzluD3E9xFcb/ZhGjeaQtI8N0hRrhLlYXJEiO4QuySaIyocNuL25nt1dcVXW+2NzYOWvq8nteuXH4fblNJLV4nGVFRQUW59x7pirc1noo6inWhZqelc0tC9A0aUjSyPMXHlt4dwF/NBIRpZSWc0GqlVVMIaZzTUagFgMdE1pb3+58ly8nbdvFmrvdQS+HFbRh2VCypcXF5WS5VSCh8JG8KMxkiEyMZCJfWHVW08FtGnjy2Srcr2GtbBhkr62gq9v4rYWKpa7N1ldiMPVw5+qh3fFm83kxVtUVNDQT49aNpYxMJIlVLdX24Tbkz6FXaljJVFOp5XOnuYFF8PQFIADMH1506cmvL3KeyWnLTW7SNNzS08SG6kVoo7SNGuPEggZZ2W4WaSRZGd443jERKhgwBGmsocdiMLWPR1uGienoYMfUyLLEUrq01StNUCrnWaKalNUsTP4DdwVBBKkG9vcSTyoksDhWJdSRSgpgUwQTwz09vmy2W0bbPf2W7W8joI4JFjYHU5c66MdSuoIUkrk1HoelrjcjRbiyuBjzUW3ttUWZlwGLyFVhsdkcrh6Gj+xpMVW7gajyWRrq3PZf8AzldM0oiWWoOlYYoWEAKLuK6t7W4W3MtxcoJJEV2VWZql1iDKqqicEGKhcklqt0NeVpdtaeK83aS3tbO5dUlkCtJEkZUK02mR2Msi1LVeg1AAgIShwZb44919m7nxfY+4MbHt/Z3ZuazG6qXvDsqLK47Fdi5va9bjtu1+4afEUuI3Vns5vCWsgpRVVG38ZV0sFa0c1SkRZpvaC55m2DlnbJbd5e+zWOB7O1o7Qa11LFjQqJpJK+Iy1UUHkvSLlT255395OfYdg9vttj3Pcbi4lukuJ5oLU3CwipuJPqJBEsywxB28Kq1UHSXNWMR0ztX/AEYHJVGd6q2N2rn4tk74wO0l7PXdeQ6p2xuTc+FyGMx2/wCXYOIo46rfO8sTkqunqIYsrJDh4qKnePwPVmnqqeNubObNo3yO3g2/m28sLc3VvNcPt6KtzLHE6u9uZpQPBgkUEMY/1SzV1BNSPl1tv3KPvFTWtpZXPLthA1pBN4RuL+wktmlkZ6t4KXUhlkkBjDM4iCxIVU+IFcl0x/SvYe+qKofN4/r7G5jaNdtrA4obUr90nD0c2I2/i6uTcMUe5qvIZE5fKUeZ80wimiiWpkliRYorGQW3/P8AsuxCyFxLezR3kbXg1JFUJKzaYzpMa0jppGCdIBYlqnoMe333O/c/3Jl5328XXLW3b3yvui8vmV7i/wBDXFn/AG88ei3unJbUDU+EpYkIAA3SV3B8Ht277mki3XvOmxuNpa4ZOlgweNhqarJyR0k8LUVdV1uSh+zlqNSJDVMlYlGDI4p5GlkDJF959gtTrtduuWkNE7wqgLUVOGNSPTFfUdCW7/ux/dvemMe8+5PLSWgczBbZr9nd9JCqzybeugeWukmgFiI2JIIj434tTbTpMdicJTYpdu4+thyskVNQfaZWsygoXpGYBX3LJPLCJGCzVU8hkjGmRgCqDcfu9y/eVFwlzHcspXW6goorUE6WDfkq/Z09d/3cnuzy8LaXY9z5c3HbopkmeytLiaC4chdLFGv7WK3JHl4k1T5gjAXu38VsPDdbbvzW4J8zgu2sbWzRUGMrqpcVt/dtClVt2XH7djWgxtXDJnWx8OXqaKrpKynVhU+SNZTF5FEqX+63O6bULKOG55dl0F5EOp07ZavUsD4Zfw1Io1KMDStOsMebtni2Tc9y2ne9quNt5ktvFSe3vIzCTIsgQ2zR0OibQHYMNPx+dK9Dd1Jk+mtldoUWN7P6bxL9b9r9bf6LMNS4uo35uoSVm+6qmo63sytm/jODrdy792nhdwKFGIamo6bNRU0iUbzQPFOokuby+t5Jds3cPc2l08tx4gjUhFDgRKoroUsKqXyyg1ajAgK75tk2zXdrbzWX0sd3bqIlUs4Mcg1a2JA8RtLKDpGGII7lILz83uwart7uPuR8Z3PuvIbdw2+8Bg5czvxsluXsjtzbfUey9u9cYj/SJvHIYXJ0+Wr1/urDU5WeSnx0tfVBpIIqSMxpG5tcS3N1tm8TbPS6lhMvaUCW7SVkICAqdTaiKgMAMHFekFxJd2FjJt7zCLR4haGNFDTl3JKlyjqEqQSMfD2kE16KT/fXomq2/Sddb43FSYrsWo3r1dhNnLiWyu6ty5DbcFdnJuxEnwozlLtrZ2UhxmbxkuNTKxxS5X1U9IU11Enu9wOYIt2W9sFEm0fT3LTxvojUSkRC3IcRmRwWSQNpPbXU1aKOlsdhsbQ7dtk18kG+XE8CR0/VdnGkymSME+FpWRdAeniZCihYgS97ddUdN0vtPvLbm+thN2Fv3uHsehx3TuJoqjde4OsvjZg9uUGPxWTy+2dybRotu4Dde5d+zZCSCdspk5aPHnHVFFSXE8iE8O6WMm9z8sSTy/TW0Vukl1IssXi3cjBlTxwFSWsYoVRiSwdZNI0hh/Y8s+6M8Vxzft/LkskMkNzfw+DDDIU263UtPcR2bEMscEmZJvBMUKlSGb8Ia9J7p2TsbtHqbd25Ur32ngO+uutwb9pqlqafEjbe1MnjKzIRYgJksFm5c7PT1VY+uWqFL5ZIliMbtqRbzrtl9u3LvMm12AjN9NtdxbW2sEfqSxuo1mjL4ZOgGg1U1VxToN8nbhdWm4rcreRQWMtxHI8jv/ZyRg6WqWVg6Fy6sQyB6AKTgKXvrdOLrN9/IzO9GJhNq9d4/dW7sz11h8nh93Rbuy+w6velZT4PF7TdavcstJkcPtWugqq6uyWRqm8epjUyyyRO4Z5c5YNpsnJNhzBJc325iBEu5S0Ph+KsNWadVWEENKulEjjADUGgKGpN+7e+PPobnfdNpTbbLc3tYI7m8hgdLuWZQkd3PYyRsUimuHLy3Ey0Q+KxjEaNGi18deYaj3DulcZuX/cXtzcuG3o+7Wxu2WhoYdEldkC9XksdJLXJXl4qaMZNErHjQmfRKsXj9yTuE9xBama2iMs6MgRWYD8QBpWgNKkhcBvhqK16x35L2+x3nmO323eb1bLaLqC5N5NHAxCALJL3GIPIDVVBnCyNGDr0OE0FP7g2tQbk3VNt+pwWEbcGNp8LUtnWx1ZQpk8bUySY6KmpcdTR0cdTjKLDQRUlDL4wDoDSwKNJRRBO8cCv4jCIkjRUYIoeOc6uP+HpBumxx7lu8mzixh/ekaxlboI6+KjdihY6LqjEelYzpFRQsgxQVPkP0Pl+tu0exutoeu4NvZGhyu16abb8c2Plp1wMFDhMy9VTZOrxWOx6RVTZIzxGWnpopBoSBJNDn2Q8p8x2nMXL2279abl41tcK7pMo06iGZSNOt6MGXS3cTjPR97g8l/u7nHfdk2fY0S3UwKscbhk8NUjZ2WRo41AZyzAFVAPYoJU9LOPIY+DzVO2MytJmhWfuGjcxnG0lBikgp0o54pw3mdpJF8QT0S2mWzMAhjHAZgUuog1tSvdmpJzVSKUApnz4Hhk13LdLSylM/L18U3h2CHwseEiRBQEdWrqY6qimCA60LAKm9k7akyWc3HWYWhSvrYqfE0WRIzL4EZOCd8FWbroaGbGU1XmKivkxhFJVCRNDTUYgMJp/PK5RzBcGsEU50xVYoQhcA0bQz1IUDUuDXGrB1UHRv7W7I11NvV3tyCa7WGJblWuRbNJEzxfU28GlWmkkMTlXUIx/TbUhhEjkyrYrY1NX7j3z2/tGkzew4Mdndm7B692bLiIG7V7ZjoqjObfg3TkanF5PE/6PuqJMljslnVkhppslLVUtGhDlz7Cqy7rJBt+0ctbkf3k7xXV7d3iu309rqEcnhJqR1mufDkSDLKlHkNQFVpH9yJTd8zbnuW77Dtlns8Z+jstu2mO2mjvpVle6jgupI2WKaO1jkQTylVbU0atG7oVJT225WUFPW1LmHI5vekGIjyAqIKGCAZChonhlpVmxlDQ1dTG0VQyGSWSaPSVKLpUIJKSQOTU0SMGnE4Jr86Z+XUEXm33NlAq+GJb7cDGJCQqhZFWhSqBWPaaVJK0pTAABhus9xYjZVFvuuO26fLVG5dgbh2VjqHI4nH11Phc7uSqjpKnPkVqvJkRicJVVhx7IwqvufCwZ1VyCLddul3V9qi+taIQXkd1IY2ZC6RAlY+2mGkCawe0rqBGadCzbdyGyW293VrtzG1urF7AxuobTJJJ3MSxq6qpbRnU1Ap1CpCpru3941XW1V0plsuuR63pd3ba35FtxMbOaqu3Ptfb1fgsPQU0CT09JS4ajpcrPJM0sPkSQvLGRLK4lrb8n7Ku8xc3w2YXfvpZbMTVr+lNKkrnNe4tGvA5ACnCrQk3vnvdJbtuXtxKT7VE0BUCFVI8GIKkKgadEZOX7dRar/GTXL/p/7h/g3k87/a/6AP4Z/FP7tUPm/up/fv7X+K/xLy+T+Gfxj/cN/E/Jb7f/ACDyaP2fZj+5dl8T+yjr9T4miop4nh+n8VO+nGvf8+gl++t18H+0b4PF1Zro8XhXV/Z/grwpivVSIq6CnydDh8xVbmr4Iq3ITUUdLiaOuz38Tr5I66Pc+PwNQ0NJCZ8hjIgaGWrV3p5TMCRNIsgoQMweSLSFoBVjj0CEmp4Hj648hSOJWjjkgtrtpX72ZfDQM9TkyKnanxKO0twOr8TAvGN2bufLUqfwBI85SZubM5bE7Uy2+MJRTVKU0dRkq7Lrt5soUrJaUYow1DRTio1R6bJKNUdDcxQR/wCMNpjBVdaq2a0UAmlRX5/5un7Tlvd98mEW0xLJMUlmEEk0SsRGryuyqzipCqcKak0HxHoY94dIS7V2Rha6bfORz2+cSkOeyeNzlRjc91zhcpVRUtdPTVGPyuPyNKtVPj5Y6dIaiGX76cIfQgMfsptt8e7uZleALYVKoy6llYA0qCCDxFagjH7epZ5j9qLDlPl7abuDfDcc3xxx3N3C4hmsYXdVlEb6kZdZR1Xw3Vtb+agFTD+NeVx6Y/O0m18NUZXdWeqKSLe0uQrn23h6Lb3nkqn/AIPLiKYUVJNPK7U1HTPNCJ5wXYxRqkXv3MEEjSW73Eum3jqYQo1ktw7q5NOJIrQeuT017O7jDFBu9rs22tPvF4Fi3FpZTbRLbatZEbRgKrOw0IrMFZ+OkaU6FDcNJtnZNfRYTIxLkt6bcmy1NR7r3LuDGZ7cy7byGWoIKPOZyvxVEU29iKWbJQ0FFT5GSjlWolaKmWRJizJ9vlmuT9Qh02rgVjVWVAwXIGo9zUBYsK44kHoRc9bbtfLsY2S7g8XmKyklCXs9zFcXTW7TII5J/AQ/TxLqSKOKZo2VyRGrK9Q7bXxDZvKGecNI7wzJrVVrq9a2SIwOpZ/LDULJ9qglkiRyos5uFIC+ZxEpZgNPrwx9v+D9nQA223k3KdQrkzUx+JtWc0PEGncQDQZOB0ps1tXK5KHL0dFvLM7OpKrG0kWSTaNFTUdbuAY+sFTAlXlJqdsxQ6kVkl+2nhjl1aZdQGkp1niBg1QhqMdJc/BUcQOB44qD6jo6v9hvbsbjov3jPhKJFtlP6+hq5JBbAGSpCk4PQN7Ww5w1TPjX3JhFxlWK6DFxRYfHYupwWmZ5JqeDJUM71NTSUVLMCfu4tRZAwkUkoxhLKNLMF7gD+f7fMn/iugVt9gI7hLZrtBC7aAaBdAJoasOKqP4h5cfLoA+ytp1m0dyb3qaH+PV3X2O7X3R1zS9h43ILkMBkNvCurspHt/HLD5cLWVGRxMv8WEcdTLGBKhIV7sWdo3GPcbOw8QLHuT2cd01oRR0YgAk10uNL1Q1C1IPS7nvlK45Y3rmmfbPqrrke25hudkg32M67aaJGd0iR0127tLABcKqu4ClePHoJsjW4I5jRHFUyYSBUioBAMM1amNlpJfJDVMmIpoZ6+aSVWErXkpWLXMko1A4iS48AsBS4J7tWqhIPH4jTA+w/Z1Ht3cbab8BVZtuUARhPD1BCpJVv01BaprXiuclqnoV9xYLaeOztRn9mR7c3Lhd1YLJ7ipcPu2g3Ltwdd/fVFGv8NrJ8pFtzA52rVMpFDQSUlXX0i+eKVmVgHJdb3F1MjwXSyxPC4iLRlG8bFdS6Wd0AodWoK2DginQ43vbOX7C+/eXL0lpfWF/byXiQXaXMLbeHYDwpWlW3hnk7wIyjyxUZGJBJ6yPKm9Zsfl61PuqfGxYGlpsUKDJHAYKgxuDpKiroMVjKekqMdBTZKrxcrMkbgTuRGZBqd3a1vAXjiOkksWatWYkkVJwaiv2jjT0alkXe5La8vAHihSKOOHQ3gxIkSMUjRaxhXZCTQ0YmhbiSpsZ2BKm581kevto7f2/snObuoKetxq0+QytPV02cSLGbjosJR5VpsRhoalaq/wDkdHS1ENOViVzBGY/dJLTVbQx31y73KRmhNFNVymogVYmnAk1OaVNejyHnIRb9ut7yvy9Z2Ox3t2BJAFaZBHMAlwkCy6o4VIY0aNFdE7A+gaelLuDpLZOJ3c1LPLXxw5Dc+Rr9rPWR4+got24OgrFaOkwtHRqaWsxc9E0UhlhiUkS6dQKsFatt1vJbUNpAYRgSgVJRjxqeIINeJ/LpfvnIHLe38x3NrFcyPZtfStYSuI0W7gjeieEidrRvHpaqjzpWoPSt7c2513V7KyNbks7uvfPZkm0cOaOeWLIVabZ/iWco6mhxNR/EdU8ufq8vU/ZTMJKqrmV6ltKqjmJHtdxfpeKiW8cG3LIaiqguACNWMBNIrQ0pj8xhz/tXJE/LFxd3O/7jvPuBLYwOGZZDHamaRJDC3i973Piv4bFWkLVkagAJRLdebZ3ZicVSU+aq6uCnxOBqjt/H7cw9PUyrFkqijydTDuZ81JT11PSZStryjxikeTyrJH5qVIuFl3LFNcaoUqWbvLn0FO0KKEigzq+efMG8v7buW27Wf3rcyILe1YWkdrErfGwdhcNKyuqOzkU8MkkMmqNVqM+zdibgy++K5du4ahpJYqmjfH0Um4abA0DrHLmMXNLV0yUzV2aos3PQffUtRUUyyGoiSKOZlhLS+v72CxsnubtiLdI2LsVLEKvcSNNSNI4geWaVNBvkrlLfOcOcLHl7lXb4pN6u7uC3soDPHAkk0z/TxRlpdCt48tCrPTS1AXCoSx0dn9N9t0eIk2xW4vG4raOTaSuyGBqZq+tjo9wQVjPQZmjFDRTQpVeCqqDNULepl8vqJuykCy+5HJKSrOm565QNNVjkrpx21ZRio4cK9ZZWX3FPvTS272tz7f2UULLwfdNpIV9VVcaL1jUVarfEa+eR0sMf0rk/4/lsO+O2hNWLisfXJk6+pyYqamXKJX09PAdONnqMbUx0WNmlDpFGiSRWfXK1/Zpa+63Le2bYu+vbTT2LTtbBFRdQkVQ1QWZe3IyCckY40At39xf3y5k9xj7Z277ZZcx2W2Jvt48t5WJ7SSf6dU1QpODKZ+0qFAKBjqIKlhQpun81StJTrmK2joqmijhylFiK56vE5yamp4Y8aMjQZGoxYnGLmaeWGWRXkDuOPTcg6595tiu7pr2azuHnr2l40DKD8VGEjHIoPLh1kBaf3aHu3JtVraHm3lm1mUkyarrcHDjGgMqbZpquc6jxHp1xyXTmVyTzzmqFRkIzJLT5nL16RVtlpJKekWlpoMbnYIK2mlIlFRI7MjcJx7aHu5y4dESQXMcJwV8NSozUk0lBIPCgHXv+TcfvRs1b0cw8u7hMqnw0s7q6jlDAUUq1zt8cYIOQxbBA6DHL0+S2ri0x2Ro6+mVspW+WWKhpqqOrWqZaZau2UbGw11NBURDy2n1RKjAxrJ5I1G9jutpvEUN/ts0csBUBclSCOIOCymnCq5weFCcYua/brffbfmrfuVufdsu7HmBNPjRqY5UaOUa45EIlEE0bawS6Smq/MFQk6N5ZcjE6U/jrEMNPH/EI5amjqlK09RLBUQVRWKWaEL5nRfGiAhfSAR7OqI8BDy8QW7DQjiMEZ+QOa/n1Hs9xLYXzSW9s2hdMLeKC6EdrUcOKFsamHaBgYoejYbc6923WYahrDJlB9xjYEp0ibHUsdI2mby1kUQxRnNZPNM8n78k/iDCMaggPuBt59z9923dtwsYLO2IhnePVJ4jFgrUAP6iilAOAFePn11L5G/u+/bHnfkblLmfeOc96H732uz3V4bQWsIRrm2jmKKXhmYqpeg1E8AaDI6Ru8etMBhKfFzw1eUb+J71x0M4kqryVEdRhtzV7QVD+WFSitikjQwJGyRuwA5LA15b9xd63r99i4tLVTbbbLcoUV/jjKAVq7dvdUjzIGeiD3a+5j7V+3W6+x9lse+8wvHv/ADlY7Bf/AFFzbEeBdsfEeER2kXhzACisfEAFaocnoRpesNqTUi0b4bGrEkaIjQy7mgmRo5GkjnVk3RoaeNpG061dF1fpsBYEn3R5p1OyXCLqNSNCN8sa1YgHrJkfcN+7m72kl1tO8zPCmhdV8Iww1FhrFvbw62BNAx7gMA0Aplm622xPUmslxGMacqqAxJmaGEKq6L/bYvPY+nDBfyFGq5Z9bhWVmH3M5qhJ/wAdDKeIZIzX8/Dr/PpVdfcU+7bc20NtHy1ukBjYskkW5XDOtSTgziYUqTxB8qUAA6K98mui8jk+od34/Z1FX5uV6SLLtiKWuSkq5K3E18NXSR0GvH5KuyNNDT62agklc1kqoVkhlSNmkTkr3St7jdLaLmFEgkLeHHMgPh0YUPiAvRTqA7xgAmoAqesT/vKfcK3ay5I33cPZS6vN2t44vq7jZbx423CRoDqBspYLVFu+xnJtWVJHZEETzzMiLUH0zulMRvvDY/MwmtxOaMG1/HPGauTCNW5eKux1fiYaqrgpaOoos42p3bVohqKkoolcOMh7yIPAzqRqXvr60HmaHy/wDrjby/dmHdba3uAxhciClCxQl6qVUsACHP7C1MmvR0EmSkNbU5ZcXi5qHIzJU1MldW1Lx0mLpoKiTI1b1a08FHDJTNeojidKRZkYa2kDFQ+2osQoY4wB88UHz/aepdtBFHCZLgwwkSEO7MSw8NQxdq0opHEVCVBFa8BQ250fU940azLVNi9qZKBZK3M4XxxS1lDkaSqg8eKmyNLkKGRZdQZpQkymCS8ZeZAYgTzTzrZ8mIqyL4u6NmK3Y+hHc9Mqvp5lsUpUjKn2I+7Bvn3mZ5bxL3918gQ6o77eY4y2uQxGltaJJ23E/crPQiOKJ1Z5FkeFWO/1T0fsHpzb8G39n0FRBHHPLV1GQnrayTIVtfVUVLj6+unnNQWjlydLQxCoii0Ux0WSNEsgx43/AJ45i5juHnv74hGXT4UXagUEkLQfEASaFqn59dgfab7tHsv7MbJbbLyfyZBK6SeO19uwS+unmKhGm8SaPw4HZVVT9NHAhCrVSRXpNy0ux4e9q6F6evO+KvYGFFBFHPT/AN3qfZ+P3bQrl1qMatIJEy1fl85TeGVpirwQzqEBDsV8bX7chBxIn0I3F9YIPiGQwdhDVpoCq+oUrUpQjgSiWbZovvm7MfFuV5pk9snWMq9IfpI91vS6soAPieMYWSpIKo1ApSpGfIbbwmUpXoq7H089I7azSPGklGJfG0P3AoJVkoGqBE5UO0TNY+wtYb3uu1yLLYX0kbg17Sc0zRv4h8jjqZOceROS/cGzksed+VbDdIWQx67uFWmVTxEdyAtzD9sciHJzk9BbtP489UU29dt5bf8AJV5zbGBy9FUU228jHlI8fkaSrq6qDObbym5sJT5bdOGoKzEVZGOkpqTJkVywGeWna8kEpw+6G9X+2y7faxxxb48TLHdIVqG00RhDJpieQOAWDMqspbSGYLG/Lf36+41bcpx33OvIU11fclW0zzXe03ixyXNrAY6vPBcofEuLOMuwdZI4poPDWVjNCHukBDfVRtzbOfzS9a1G4KfY8bwx7VzOb2BlsbnuwcJS5+sqKjOUubrM7u2GlpsdnselCGxlXRipixoqZHikBp45b2q6vb22txukEA3EoDcxRTK6wSFB2EaUY6kbV3A01UAIOo4F3NhtUwF7aX04tbb9GNVgnK3Ks5ZmMn9m1CqihEZ0jUGFAoi9AVM2S7E3NX1FFFNp2zQRRZdlqDV+WXd+03npGmnMsjU0bxu+hpCfLUM5BZizBz3RGnlIrrofHXGMjS/l+z9nWUn3C4Yh95bbXttvUW67Pfr4yoVo30Z7STXyU0BNck549Hn94wddw+gZ6x3DQ1E3ZURiqYDhd801BWMaWZ43Y7D2VUpVReN6qc0kiS6TK6xIZ0kRBpQEyRzjt19cx8p/TwPLXa4yNAJp3vg0FKj0zggnj1hx7C848p7Vzv8Aeki3vmDb9tdPcPcUJ3C5t7YOa11J48yllpiuBqDBRRehEpt27crJ1paTLU1RUujSLBCJZJDEjKjy6FjJEUbOAzH0rcXPsHycvb7EuuXaLhU9WjYDhX09OsjIfdT2ruH8O290uWZJK6dMe7bezVrSlFuCSa4pxrjp/jkjmQSRSJLG19MkbrIjaWKtpdCVNmUg2/I9lBUqSrAg+h6HdCKVHEAj7CKg/mDXoO9/47OU+Lq9zbP3JFs/cG29udi10WYnraukolxOU2Nl6fe9CIqagyqvkd0bSpajHwCOnE1VWy00RljUlhJXtrzA1hvCbPeIZdrvHjRosYkVwYmFaHD0ByBpyQaAdYM/f39qNu539nNx9xrSFF5y5XjWeG6VavJYSSLFdWzsOMcQlFyhYN4RjkEekTSE1d7j7l7M37lc1mztTL5jOYrD7U2hsY1OKlpVzdHhcIcXU5PPVMddJRx4TC0sMtXV1SJT45FiJqKvVKjpk1t9htuyQG3hZYrN5pZ3FeDyyFtI9WZmooBJyAq4zwzvNy3znG7uLtbCWfd0igt4Bn9QRx0kkkYvSOKNVaSR6LEgBLyCoodnZddBFtCGuio9q1Ap8Ji9vQ4rJSZRyrVFQWrc7t+UiSko6zFwwKRUTTI8lJOPFHJK7CNG0FJ9Fw0uly8pZdK0xhW4EgngKHINSBSvrvfltr9odtsw8mhLRRRpR2gUeKpY1LrQEHhwGSQ19M7N6r2f31treHYmwcl2Nsp9xYPO7521tGoptt7x3zgMRDKke3MbvSenx1fg6PcVZDTJX1lHVjx0LvLqDRm6LmG43e45f3Fdguo4N7EZjtnuDWNHcgFmVRJUqKlQyHvA7SD0abPaxwbpYSXcLKl05E1zBCruph4sju0IOkAlqTICAQzrnod927j60pNtbLyOwshiKPJbY2/mNudp/b7tz24KbMbzxO9N4Sbd7FR48fSbcxlG20dwUNBi6agrK+KU4iSqqbGqVZoT2Tl7m6WXfdu5qtbqW1ub6O9sGEdugjhaC2kmthpVZFR50ZpTKTKJJZBC6whFi6Z7r7ye31pv24+4PtX7oW9rELZdth27cS8aw20Nmuz2Swo7TSX9zbQ/VyxzTwqGt5YTca50VWLt2l15unpzuHK7A3GNrVFZsqDDL/F6WFtx7Jq4d/bOG7MfSw/wWiqJss+GizximjC1VPNVwSRgvBASZmsd2tuYOXbfcLYThZ8+HqCygxPoY6mYaaleNVIBrhj1gBtm2TbHzzuMbWUCQ20s6x3F5BI0ModZPCJt0RyaipWOjo1KMCinoHt45qOTG5R/AKzcGaq8pDHlarIzZCbIz1TmCjx7NNFAKemxtPGPG0cksEQYKwSOCNQY2Vu8MkShtNqiDTEo06aVJOCSSx41ofPNSenOZ7+xk27dIIbaJ9zmupGNzqD+KzthV7UCpEuQVLKCaEKEUAKKLMCh3lNhdwvnhuBNpCfB4CipsrHT5bGNTTxVuSTcEWFqcCm1KKno5W+6gNTE9RCY7uVI9r5gGg1QeH4PiUdmI7WIqF01Da6kYNDQ16B21XE372ki3Ga5bcUtAba2hV6SQrVZH8dYmiW3RFcl11gsuk1oaC3h9l7Jp6/CZDsnL5TbtLuTN0NLgamlGViqzTffyUFTnaivppo1qcRt6FJQxip1mmeMUkF59UkIfvb7cPDuY9otknmhQtIpYDu0aljAPB5cUqaKDrbFA0ubZsfKFu8F/wA27lNBLc3Cx2CQlw5IfSZZZlJAhgWtSI9bECKMF9TR5u3uzc7vTtPsHdO6t25Xfm4KrcdFRZHdmUgXD1dV/drH0GJ2/FUYmTI17L9tt6lpkghSd46SF44gswCA15V2Db9m5f2ja9q2qGy2+OIlbWDuRGlYySUbSuotI7MzEAuSWNCT0GuceZVtOaeZXe6M959UC8ixi2XVDRFHgB2BOkVw1BqJIevUTCbRyOOgp+wZYK6fF0tFXZbIYh4nbI1KGGpppawU1VJFDUwUUVSHhErxTyaH0ICACr3DcLVnbZVmC3LFUDcFqchCRkFqZABAqKnPSjlvlPflhj9yW2+WbZ44p7qSAgtKUUGN51ViFZIy9VZmVmKvpFVylNnZyk/0rbertuVc2YqN6UFb/G6XEz4jHbewtVFXZzJUeJ35k6CbL5qj3jQVGNmceSjQUy11OmpHqPJGh3m1A2fcBKjBoNIQuHJYEKGMSGishDU4mpU1BpQiD21vnf3L5Nfa72GVt4V5Z4oZIYYYJBLO0Ue4XMfiyw3SvCXJaNSiSRUdPEDoJGT3TkMpBuXC9j7a+0yElTiMpiqBjW1CYbJY9KCsqUweZXI0tHlMdS4upnpK6U0lV/EKiJiqQCRQW9v25LZNuk2q7YxoGSU0UeIrVoXUKSp10KgFAgxkCnQj5x5m3Ledz5ptfcHYBaXUlxFd29opkkSGSIR1WG4kmJnRIA0crkTNcyKXYhnr0DbplMnlYsj91JT0akPjqOuhVYHpqmsqZYnghSRGFW7xr5Vmd5FjSNYwurkTgxJGYwp10o9PIgD/AD/Zx6guSPcL/clvhdBLMuWtVlAyruxFBq+KoyCdQAUDBHQjwS5Kh29lYoU8VNX1f3WbeGljhgpqBanTSzwGVp5aCOSrrVUCFaeQlFDKQLsxHCktzDM2fDGlMniQK1pxwPOvRnue7y7XtF7tOpVlvpjJOgUKpCuxQxKxYqCzcIwjUUVFASZMEX8ZpJWioaus/u3SUtTk4qiRft8fR5io+0o5Z0lm8kseXZXIUiQBkkeyk6vZj9Rbx6V1qodiF+ZAqR+QH+ToDPs+7XFzcvLBI8sMSu6nOlH+EkE1OqtfPFT8+jH/AOzW9nfxL+JfwnqnV/C/4F/Dv9DPWn8A/wBG391P7p/6If7t/wB2v4D/AKGfF/uU/gX2/wBj/eX/AHO6f4x/lnsv/cm3/wC+2rr111tXxP8AfuqtfFp26q109nw46Y1R8fDbT9N4FNT00f77pq+HVn1rmvl1R9vz73a2Rx1HiFrdprtmpEW3QWqaHc2dpqHcW6q2g3tk8hjKChoarM43K1VXSRVOuOenpRTQweZIXnYVWhEplY0bVQscUDUUFQKkgFQppwrUnJoABvQuNte0SHXavCf0V7llkUSTMs7OqKrOkjSJqJDKoVF1BSxUvS218rvHcG48nWVkLJNhshj62tZRVbgrMnuDH1UlO236rwVEcO4JZKc/cVEhEgjlkV7vKfaPdbiOCGGJVJIcMVJoAoP4wclfQcMVGB0IuQtlvd93Hc7ueZQrwPFr06pZJZUJUQEKwE5NNTHIDEHL9Dn8c8Tk924XfOAze667bdFsiHG47HbllP8AGcfjJpsnkYMLQ1e1XrWjM0GaL1FLeMtUhTGbrEoAc5mvZ7AWFxt+1C6ubiSjQ6hHjQWZvEK5GlaEeRPGuOpp9hdg2HnJ+bdk589yJuXNk2nbhLbbgtq24a5VuooYbUWK3EQDtJcNKjswU6CGFMqbPaXxu2OOuNhQb3ysXYe3aCfJ7421jtq0uM2/FueorI8tk8P9zTQ0FUMnjavCSSVX2NO0QkMTa6holKvHO4e4u5Ju+6Wu37b4FwjrbTzzu7LF3Kjs3aQgVyF1knBBCVNBmx7f/cz5K3T205E3vnH3E/eG2T213vm07VtdhaCTc5VjeeGztGfcrWa/uJLclzaRQoVkV43m8Pw3mrs797U3XX7+37s6mkx+G27hN8yUEmPxGOipjnKzYFVX7dwOX3DWVK1GUy9VT0cRMcE8zUlOWIihj/MybJtlqlnZXjoXuXhrqY5VZaOyrSgArSpAqaZPXMn3J5+37d983/Zg8Vvs8d8oa3t00iV7IPbwSys2qWQoldKu5RNRCKtT0ZrpDc9JX4SOrzlNJK0+HMuJfHRGORKwtVpDE1Uk8cwFP4z5v2WQOw/cAZlKK+S8/TS3ZARIA+oVGkHNB6mmOj3ky92LTczbzDMwNs/03gHQRMyER6nqexSasKGpxUAkEaKnsbb42/8AwevopWrK6eKKOqijpZII4KmrgRqqOs85niK1GoDSjtbkkAsfZG+03LblDexz0twKspLAkgEAaaUOD9nywOpZT3B2m15Q3Lly523VuchCxTKkTqqu6OzrKW1o2pSMKSRxYBmBMvX9KdI4Hbz7gz+EwtDioYafLZOqzeRpafHQt4Ud5ZZszIaI2IUIkjgMQBcmw9wBZc98+7rertljuDSXTFhGqRRVNM+SCmAanrsVzt91T7nft1tu781c0e3O32XK1rIgu7m8v96McSmXww9I7yV3d3dFChaE0yM1If8AzBK2hwOH6s672lMcbtDFpuqsm2rTxijwVNWBtsyY3I4nHNTxYqGoWLIzASUCh1hnliJVTKiyz7Qy7luMu+7zvBWS9l8JUnouqgModHK0bBUUD4GCvGp5yf3iG3+3nJkXtj7ee2lhLtm12X10l9tBe8MK60sJ7G4gS6eWDSyXM1GhIlGqWOYLpoCBde4KTO5yOZFy9dWY2SlqMbicLjq2vyuYrqdJaqnoaOaPE5fHURpqXHyVDtVoIfBTv9FDOkwbhOttARVFRqgs7BQKkCvEEklqYzUjiT1zq5X2x903BXCXEs0RVo4LeN5JJWUEhFISRE0qhYlwF0q2QASDObG633Z8i6SPEbVyGQr6HFpmoaHJbq+wQ4ykqch5qWnq6VPvpD91OhnlNK0qKI1+ppzJGD963rb+UoXv90lCKCDojJrI1MKvAlqGlTQCucdT77W+1PPX3id6seUORI3uPDDg3V+VWCyt2lFZ7k/q+HFqoWCa2d9McSySlFNqPVfxf6462xOHpajHR7rzOKpY4xnNwvNmJlrFSBZK3FU+SaakwSxPB/kgo4YJqWFjGZZWvI2N3MXudzHvc8htrlrS0JqEgOlvOmp1oxOc5Cn+Hrtt7Pfce9jva3a9r/e2xrzLzRCoMl/vS+LDr8xBYM8ltHGKCnieO4ph1BK9NPyLY7fh6RTDrBRJV98bIxNSBBBNLLj6zbm//PTiSojllWMiNeVIKaVsRYWUchyy3ac7TXMrPN+5rhtTEnOqIZ+2vSL7z8EGx8zfc42vZLW3s9p/11NqUWlrFHFEBX8EMaqi0zlQKE/PoxtbtzA5GNYa3E0NRCravA9OngdrFbywqBFNZSQNYawJH0JvH1pue42LmSzvpYpDgsjEH9oNesuOZOWuXOcrWOz5v5esN1tU1eGm5W8Vz4ZYUZojMjmJiPxIVbAzgdFO3L8VdoYTc+W7F2RQVUW4ajzZB4azKVlRQx1dTS1OMrXoqWorRj6ELjMjVLCvhMVMGSKD7aIO/uXtg907yaCDbeYpEaHUFWWNdL0rUawoAZaheBripVyRTnt7o/cP5Utt+vuc/ZPa57XfzC9xJtt1O81oxMZhKWEk8ss0d06M5Ec4eMs48G5tQgicjO6stt/de5zJRYyu+42FuyrxGbyaUuSEtNPFjspja7F09BkquieknzlVEDUI8ASVopFayxrIJ2sPEiijLSVSaISooKkFSQymoqCADQGv+zya5zurDeNxvBaWDpPtt61pcz6ZgUdUkidNErKY2mZSzqUHcGGAoIVvSsFXU9n1mTxtTQ1uByW4qX7SoojCmbxGTwlPSUm6MLuPXTUNferVoJColqqaNUiRGPkVXS81SJ/VveFeNhL9FPWtaZjahWv5+nmehd92izuD94P2hurW4SSwbnDZwrIQJA0d/a+Kko7Tw0k5ZR2gE1ANwvvCfr6WugmSpcdt5hPLUSxU21tuVElLF5Z/Cvk3VE9T9nAZZSgaeNWkMelS4AIu1x9paX29tII4qync3IIHH9JcV/I4+XWJ9lfWG1/fI50vt13i2tbJvbm1iU3U0cKaxuwc5kdVrp4fnTz6EZ8vRRmISGqjM3+ZD4/IKZfU6ftBqUeT1xsOL8qR+D7Cq7Lu7J4i7dMU/iCmnCvH7M/Z1PcnuX7ZwzfTy+5fLi3FaeG26WAbiF+E3FeJA+0gefU6GaKojEkLh0PFxcFWsCUdSA0ci35VgGU8Eey10eNikikOOIPQxilhuIori3mSS3kQSRyRsGR1YVV0ZSVZGGQwJBGQekZ2BtmHc22sjRq0dPWqIqujrjDBL9pW0bB6StmEsMxkjorEsFHkaAyxKQsrhhPyjzBPy/vNtcBz9G58OePNGjbDUAI7hWqn+KlajHUL+/8A7QbZ71e2298sS2qHmSCKS62K5oPEgvkXxIlViCBFdOiwzqe1kbURrjjdCM7H3FA2RWoZqijq6WaeaOrgeQVDSTg0pR28Sqy00sikGNQdd9J/s+8rpV/QMWHqNOhuGM+vEgef59fOxeXE15eJONUFoZNUkq1JJyBkUXSCRkCleHp1YFtoxNgcWYP8yaVfH/neV1NY3mJmN/6udZ/PN/eIvM+r+se+6h3fVyn/AI2fTHX0f+xVf9ZD2b1MSf6qbRkmpP8Auvt+J9egf+Q26sfszau189lX8eOpeyds/eOGtIlOcBvdpZIYtcbVEkSKX0A3KqeDaxFXtvay317zBZQsBNNtc0Sk8Ks0QFSAaCpyadY//fO5t23kO29gOdd5ikk2jaefbHcrpIdJlaK1SSeQRKzxq8ulDpUsoJ4sBXoP6z5k9cUhhkOP3JPRymEtUUGPoKoxxygEOIKzM4maRh/qdKjlbMb+zIe0G/6SfrrPVmgLyDh8/BNP5/Z0DLn+8q9ho+215V5slI01L29hGO6tBjcZW8vToQOtfkXsHsrIthqCefEZnUq0+JzPip8jXXE5eSkhgkqaaSOAQHyKs7SoGDaTGsjxh/mHkDeuXrUXszRTWv43hLEJwA1alU5LYoCPnWgMx+zn3v8A2h97eZhyZy4m62HNTxvLBabtBDH44iSSWZYJLe5uQzRRxs5EgiqoOmrDT0PbAMCrKGVgQysAykHgqym4IYH6fT2BxjIOeso9TB1AB9dQ8iKU8619Ps48OquPkFtHGYvtLL1NXisW/wB62J3PQZOj2htk5ujqqetrIlrcxu+LEf3klq66uopZFZ6gGTSqIQI105Z+3W5Pe8rbc7yt4iqYGUu2g6MALGWKiiaa0GTUnJPXz3/fW5NseVPvH88QbfaRLZ3ktvvEPhwQiSN7mCO4nbxljEpQXbSiNSSVjCoGog6TtZ1ZuPcG99kbYrMLn8JX5iPHZDLU2Zhlgkp8FlMMMp/HgacyijlyGPlUY9amFQ81Ugk8ZkBB5u2/QbTs247vIyOkOoKFOC1dKqf9saEitBny6i/259p9192fdDkP272sTW1xucyrdTSqD4ECI813c01KD4NvHI6oxVmYacMw6tPwWBo9u47H4nGaocfjqKKjhpgq6CsMcUUUjO/kqCY4ogihpGstgSxF/eH+47ndbrc3N5fN4l5LJraQ1r/pRnSF+QGKACgx19HXLPKGycm7XsfL/K8DWXLW22QsLTbotPgqgYN4rEp4slwxqZJGf9R3kkcGRy3RdvkJ8mNu9MUU2OpWpcnu5qaCoXHSVMMCUNJWGugpchUeVlaeB62geHTEHYyjQ3jUSSxDfkn2+vOZil5da4tqJIVlFWkKkalXBpQGtSPsDcOsXPvOffC5X9hIbjl7ZoINy9ygscj2NyzR29nFKmuGe6IaN5hNgRwwuGIJeSSJQglrjrvkbv7DZ7M9mu+KffO6K47VhqZ48pPgtubYwy0W4qDaWLgmME2UImrY6meueoNRHM3jRQHJabY+TtiuLW22GOBv3PAguGiDAPJI5aNpnYGqntKhQACM8AAOVNz96r3k2zna+945eYom9y71ZNliunt4mtbOwUJcR2FtatEIGQeIzvIQSZHbBkZpGPN8WvkzuXtmav2tvzbcGI3FisTU5sZeglEOJyeMp8hR0TvS0eTrZMp5aYZGFpFVqtxGss8jRRJpES+4PIFjy+kW5bJdPJYyPoaKQVZGIZh3KunTRSM0pgVYnHRD7pv32rz3e3S39vPdrZ7XbefpqJtl/ZgxWe4Mqd0bxu7m3vJNOpNBEMzMYkjgkESXB15I0ljkikGqOWN4pFuy6o5FKOupSrAMjEcEH3EwJUhhxBqOuiHmDQGhrkAj9hqD0TPviakyvYkJ3RuKqxNFS7Ewn8Aw9BtQtS5DH4KfI40UOIWikp8HEKeCnXLTyRxUUdTU1yK7RM0lY+SXt/f3E3LsT21okl0Lp0uXaQKQzKrB2DVcliQpySKMwBwnXA372fJG2e2Xvhu2x7TMV5T3C2G57eka641IaRJrXXkAWVzHNEFNWRY4YndGDOGr4/ZVc1vXcNZSiqTFJjEpcDDkII4aqPblJuza8eMaWCkRqaDIVMkkk9Q/mmEjSkByQzM97mRtDymI5AvjGRGkKkkFyraqE5KjgMCgAwOHQ7+4buEm8feH27cCGSIWG4RQRsMCFLKUJhQFD1JLMSdRY5rUk8ZNgTzxzwCT/sAAST/re8Zuu2/VEffebqqXvneOGpdbSVOXwoWSlRquqjqJcZiIadKeOnMpeTzlQgUarvwCT7zG5dtzJyxtFwxwtqgCnAICAnJ+X5Y49fNd94Td1X7w/vPBBqVJ+atxk8QqwlTVeyaaowDowNO0gMpNCK46ct/dVbs6u3fm9j7rgpKbOUUsNfX09LXUWQloGyUAyFCgho6upkpa3I0tUlVHTVCxVUcEsP7QV7s/YXg3K2huUhljJGkxyKysCAKg1Arp4Eglag5x1FiCBhdyWc6y2TSaxNSndUghFqTVjkVzQrQZJ6sX+H2X3NW9aGi3AlX9tjcvkaDAy1rxvUDF0kWNlFLMyDV5sfUZB6bxuQaaKGOIAKgVYA907Kztt9hmtgollhDzBQRVizjVn+IAfaania9dtf7vbnDf+ZPZrfdl32eeWPZN4+ksZJ31lLWa3ilW2FPgWCUSEL+HxNFFCgdGH33T42r2duOiy9dTYzFVeHrqfI1tU+iClx7U0jV87gT0zOtPQpI5VZEZgpsR9QDeWjMvMGzSW8TPMtzGyqvEkMD6Gn2nA4nrI/7wd5Ybb7B+9lzuDqlmOUt2iqeGuWwnhiUeheWREX+kwAyR1Tfj6oVO78jQ42unz8UGQyeLxFIcFJVUm6VgkFFiWk2u8VXUos326tTQXCo01pUlVSBmUkjS2kTTQ6GZVLgNla5YBsVp64OMU6+ZfZpT44KS1fS3hxlPFWRivYrIK1+XFampVgOrJdoV/Ve+MHmdvbBj7ez9dhei905vK1lRsLDde0kGcwG3ptybpnjqNx7veKLZuFn29DVz5qkWryGYx8L0UMMMsrOjFtHuAWWfdI7ZIjPpULIXIWtIj8C1kapBTAUmo1dMwWlrY3J3C1vLiW+acSsJkaNV1EKFVjnQjlmBA00PEZIKVtvubGv21kYtp1Gyt7bpWll2NgtjZjC7sz2XFdkHejodx9Obg2xkMbj6DsjE5KoWanqXZoadItSFiskUjdzBJBZwvdeLHZf28s6lEVVRSx8cPnwiBQ8fnQZ6G94dp5i3iSPbt2tzuttMkEG1qsrtc630kWcsSmJpSzlmroXSKqxbtIwJ1fv+eq2/sTD4qo3hu/e+4tg4Sg2HtilyG5jkt+7vp2qMPtOpTH1VLOOxWiqo6NcTSwVFTDLUyxM8TxuhvY7tY3yS3SuY7eNJT4sgCEpGwUyIDXVCSKh8BgFIBBB6KN72y82pkiliXxyVPhglqNpLFXNRpkA/AAaAmpFOhS6qyeexe7u0t21mz8fkd3w9cdubei27kod97hn69pjsfNbA3Hu6upIJq3cEGZ2Ni66cU9dmakYulrUMtQTHHFEwO5mhtJdt2XbJNwddva/s5PGVoIvHdZ0nihBIRGSV0GqOMa3XtUZJEqctWj3c9xu7X8dnu0UUrJDEJZdEaIY5nkFJJFfJHiSMEB1MWppBKHmYKLIhYqOrooBj5YxGtLUyTywPWASy1EmKErpSUk06cNAF8qAtpIK2GsLOlSQSzCuflwFaZNPX/P0GNyt7W7dUiZY4YH0AodQBehZjGGOhC3moFeNDii4xexMvV9Vt3Bldyxij28mY6b2nt6oz2SbP5zbm3qyLe+awG3qR6TI/wzYmycnlaSvqPvKyixQq55UpVlnRyA6l9t0PMcmwW+1k3LoNzuJ1jQRI8gNvG8jkqXnnWNo10q7hFGsqhWp54V5Dy/Hvce4TqQsmzmCJ3BktYZBeNDUhqW1vMI5SrP4YcEKupQ3QYbcpqWanqdwZSBsnXT5Q1NPQQfxP76CmjykVKlbRZFDT/bM2PDRiSVZ6emacxRrKRr9iC78SqpGdCBaVNCK6Tih45zQUJA4jh0VcttYqs17eRPd3bXHiCNBKroomQGRJVYKhMdVDOJFUvpVWPcMeRk2dFnZ6dayfN4aabF01bkti0k29ftKvOzQz0xrIaDLUyVEFMZdNbLX1BRZll8azSIIPdLe5uHsw8cVJxUiOU+FULUHOk0rSq0GRThWvTe/7bskW9XscV2LnbgsYa528G7CvOVda6ZF1FdWiQu1A4bSH06enPfPcMWxcTmNq4vGNlMXiaODF/wANlkXJZqsTJ5CnoHo6WoqIKWurKBsrI3mimp4GVz40UxhQUNtsFvfXce53D/46zeJUEqlQCA2kFgCFwDU+vHoX7x7vbjypsd5yPslmr8vw230jRTIklyVmkRpIPGMccrxG4qzIyqQ1UXswQ/2zvesodp77fDbfp8LtmTBk5bsDalXFt/deD3bu6riqdvbdqZtnYebKPlMTUBIa13gydbQioWKckWje+6bXaX15tqXdw5kScSCCUaonWMFWxJ2lWDYAIDEavn1T2/5+5i5Y5T55l2PZbaDbJttNnNvm3MLe/tLi7ljntkWW1TxxNHJAEdysssccphZgjeGUDmd0038Dp9nZ7t3O4reO2cvJnsnNG+Y3U0tRjMccdlKCGr2+ssX3aRwVb1tRkIZZ5mlkNRCsCoyHEVqyTm8i29GgkURrhUoKllOcgZAABFKChqTWNtw30XG0DlvdueLuLfLO6e8mLNNch5BGsciAxal1gK5kkdWZyzeIoRQVGSjWlj3Dt7bR2zuM5aprxFDX4t46rbtVkcgDJjoMJXVKpt7MGWNox9tHUu/jQyFmjSW6TxHNvcXJuEFuqknX2kACp1Z1ClD5fz6EMsFlY7psmzrsl2N2acBZbdklt5JHYeGID/YSggqNIc1pUsVrUUM7k0aGbamMr8jFslsrLmAMitPVwJlmEVGcvWZPHwSjKNiqRGeJtU9LGpP26o9SbpduhkZI7u6SP96CLw2MWoArUtpVXNV1GleDVA1EhR0Zc5tstvus8WyNdty1JIZYDfhHkjZqDVJJECshjFTUak/gAZz0hKXbMGRyFLuGGtqps3t6KvWDIp91j4aimyv7FfTTxKYWraaohgS0U0JWItpjj8of2bPMsNIXjHhPSgFCcZ/LPnX59AiDap9zaXdIL5zuMAbW51IrKx0kVr3Ap+EqMHSATXoYvuet/vb/ANzt1+L+Ffw37T+/+L1/xn+A6P4n9x/cjT/dn7z/AC77Xw/xDR+z5NX+Ve0dN30/7lwateqvgt/Z6vhp439pp7a1017tP4elH02yV0+DPx0U8dfjpq1f2H9j5/x18vPqmHJV+T3RlajKZPJ5vc2araSorcpkMxVSVGSmmocdJLJLNkK2ryFRXQ0VLSA6pCrvFHpAXiwxjRLaJYo4kjhUhUVBihNKUAAFa/YOoKvbu83m9mvr69uLzcpVaSea4YtIxVKlmkdnZ9IXiaEgUx5DR1FtEzUpymeoqqbEnI0eeosU9HV0xy1XgqWvixdRFl6YyTwUay5iZnjEVp/ECGKq1incrkeJohf9QKULcQAxGoU9e0ZrjI6HPJe0AwG63K2Z7EypcxwlWUyNCriMiValUrK1RTuoKHGDNdBbPyFZvHIV+CzlIvXE1fS7n7Xw3Y6UuQ2zlaOnTI1k0s9JjlSDGVG36SuqKyJ6yoEcUqpNMAadQwF52v402Nla3l/ef9nZyWlFmWQqwXSTVjqppOgFtJIAoSRk992Hl17n3ThvYt6sV5DQx3vNFnzDV7C7sVureSaOZFU2g8BmW5jF86WxmhiMhMqxRSWV5VcHisHt2s23i8dLSrh4cVtuSg2tVVlCNqRQUbHA0E1HV4bE7dmnp4kNOalYKOL7cO0bCIlIFgfc7673drx5FYSs90DOseievZKygM8wjIJoilicA1NW65SQ+2/I22e1237S+3vbz2VnDsX+6eW7mvdllWV7vb7S5ujDa7SNzS6jiL3N9GkcZeWWkASGGgTsehWv7d7OTEJTtTQ773rUUkUNbHMho03NXpAaOoNW71yQxyK5kjeUiBHmYmNHYZf2jldpsWlrqMEeqop+EVqKY+zGcY6+cne4ll5s5gFuU8Nb64ZKNUEeMwXSwJLcQagnALZAPRgev97UmEqKTbzy4WH+JGGYPGtLU09ElRjzLM9X9+vgixVPJGwjZkZH8kY0oB6y1lNHfOj1yK/z4/n0Jttu40eO1YxiRiCa0IFRxOoU0A+ZFDjh5jJlZafGVWLSoixtXTmvigrJJMhSUwwtCC01ZkHkFFkG8CLTxmoRWhhMZa0kYB1MMNa6wxDUrSnz+0U6FTTR2sjW00EckesRa9Sgp25auh6ioGqhAIqAV87eMZGhxePVlDqaSkks/rGvxxygjXe2iTlR9FsLWsPeDMrt48jA0bURUY+Xl8uvqquLaKKS9tu54WklDCVmkJDs2pWLliykMRQkjT28MdVd/wAxqiolyXTvmjqhTx47fFEkdDIsc4aqbbEUehm8rSemPQyGN1dGIJHF8gPZK4nMXMx1gytJA7F/OglrX9ta1BqOuPf96LtlhDJ7EW8VsIdvhg3mKGC2Cxohc7YOxEAVRihULQg5wOiB7SlzD70TZ21s5uHB43dtfh6XM4PCZHI09Dna6iaX7WirMdTHHUWSEclbPTxpOrpAKl2UsWaMzfJ4Bskvb+KNniVis0gUlFYZIY5UYBJFK6c8AeuVO3DdP32+xcv3N3FFfPDFLZ2rShbiRWoiGNNKymrlArAgFzQksV6vz6e6twvWW1afH4unip6/Iz/xfO1UEcOrI5GpiRah2doEZaeUorKqrE4VED6nDM2HPOHM9xzJu9xcSZs0rHbI1RoUHDUBprNO6pbjjAWn0vfd/wDYvaPY3262XlexjSLmaUpfcwXcGljd3jKdcTu6mtta6vChCeGCqGUBXnn1yO2O3tsdR4VMpn2mlqazyR4vHU0bvNWTKNIOsqKeKKJjqYyPGCqsA2qw9s8rcpbjzVdtDaUS1jK+PM1KIDWmK1YmhoB58aCpCn33+8FyH937lhd85vlml3S5SUbTtluj+JfTReFriWbQ0NukfjI0skh7ENUjmk0RPTt3l8qd9dh5jb+VpZocBQbMz6Z/bVDS08VcqZSkkqVx2Sy09VGKPK11JSVcsIK01PDJG7ERi7XyY5X5C2PZbe+sYo2lN1EYbiSRqFkYUZV00KKSK4qRipNBThh7z/fG93fdbmflDm26ns9qXlvcU3fY7Pb4Q0VveRvG0dxJ9SZ2uZV8NRSUmKmoJGgdwxi/jz89M9uLc2K2Z2ri8THBWxrSw7uxDy00UNSCgSfP09bWVcUaVUsh8lVFLFTU/pDQRxeSoiBfOns9t8FnPuXLk7pKufpZakNjgjUqDQHDVqfxDgcs/u3f3kvMm6cw7fyZ78bZaz2dy4VeY9vjWF7etRqu7SEeDNBUqC1usUkS6nMc57RajFLHNGksLiSORQ8bgMoZWF1azhXW4/BAI/IB945spUlWFGGCOux37PyII/IgkEfMEg+XVXvzD6t27s/dg7gx246baUeYpo8Ru1INq4rcVfU1lRDNFQy4Y5KKSHB1tZiqOSlmniaOQxeILFIPMWyR9peZb++22TYbiFppITqtSzso0cGBp8SxsQQCSBqpVQB1xm/vDfZjlPlvnDbveTZr+Hbbfdkex5ijtraOdjfaQ8NwS70trjcrcSBmUK0ptpZv1Xkm6BnqDcFFXb721mtrYneNXQ7o3ZiZ6uWhp8NkNu7cDOMdkGyVNS09PlcB5KHG0FP4pJZqVPVLHNI0YgMh80SSDYN+iuXiEq2U60yGb9NqUr2tQknFDTy8+sPvu3Wls3vr7I3uxWt9Lt785bNIXURvFCDuMCsZdPfEWVY17qrWpDk9vV1fvCrr6Wuqk/mnPt7/AEu5pslmajHZrG9Z7Vrtr0MkM4o8xlF3PlKeqpQ328ivLHi55nW+mNmVTrsjA5G+2B3CPluwFtbB7R76UTuCCY18NSDSuKtQetKimR1wl/vGLiyk9/ogxcXI5ctEAdWQH9a9NV1AeJTy01U1we1qAZtdaTL06TIEqKyeJaqumqZkeoqHpY5YERZHlA+1YNZW0jw8cAi/uUH1ghVYhdWAox65p5/4esCYlkEcly0SkeEQSWqx1HSXoeAQf6hx6P58Sa3O4+bcO263yfwlWx1VjYJJxOlIaqmyVXWmGwjdUrJFiZAQYwqs6KplcvC/u1Y2slpYboo/xsSGJmApqBrQE/0dJ8/M14ddXv7tHm7mVOYfcH28ur0ycrHa13mCEuWWG6huLa2kaJakILmO7HiUA1GGI/h6Ork/+Lbkf+oGr/8AceT3B0X9rF/ph/h669WQAvLWgpWVSf8Aeh1UQNyu++NxQ4uOolSTdu4hTUvOlr5erejMGqRTqNOANJ/UGPNveZ1qgW1gaZgJFRdT/wC1oflx6+VSfehd7lu6RaW2yZpnhgrwOssoqT5L+2vVqvX0sk+yNrTym8s2EoJJTxzI8Ks5uvpPqJ+nHvE3msAczb+Bw+rlp/vZ6+lH2MJPsn7Okih/qrtNf+yC36KN/MBq/tOnNtvISKdu09rhxGEM7Om1uwJQiCbVTujxo4ZXUg3HNr3Hvs5GZd/3JU/tPoX4/DTxIRmmeJHWFH95vM0PtV7dmQj6Y8yAUHx6hZ3JxXtKlQagj86dV4bJof44cKs+OqchQvU0r1kdBZaiSleofypCtPDWyhNBCKAjsiqTpIAHvIKbxFSbw3AkoVUtWgOKVrT/AFefXGawgjeRRcg+CWErFACwUagQFBJKj+Q8qU6Ml15hqeh7po4Nu4ahRaHdGUoKb+C5zNVW3FpKOlq6LM5DD1NeKbI5uCroDK0EkpijlYgeIrIsSh/mEonKm7TXzkA2jV8UKH1MtEU0qqnWRwrnz8+p6+7Tt29Xn3i/ZK02OKSa7g5lsppxbaipihuY5rucUNfCitkkaQ00hFZjRRTq2KOWOZS0Th1DuhI+geNijj/XDD3iG8bxkK60NA35EAg/mD19IFrd295E81tKHiWSSEkeTxSNFIv2pIjKfmMY6qe+Tm/arO911m28eBkaXbONxtD/AAoRpPT1+Vc1+YjqEFM8FRVslJm4hGxkIgcPYWZr5N+3dibHlazkkLRyTlpNTY0jVQUrUAELXhkEeg64H/fl5isN4+81zm1k0Vzb7XbWe3yKDqVporSNpo2CkHXDPI0bCvY6MCOPRg/iVtvHzRZfdX8Kx8VY8SYzH5H7emmraRqVkqM3RidU1CmrZ6uhmdEMeqalR3DsqMoa929xkit9s2zxCYmkaWRQSK0ACH/jTDgfOnn1k5/dzcnWd9ce4nuBBFDFuVvZWu2Wsvgo5T6uSaW40tUMpAso1KqV1LIddcHo6eSrYsfQVtXLMkC0tM8zSyJLJHESGWN3SBJJXTyDkKpJ/p7g+0tZby5traGPVJI4RVqBUkjFSQPPrqLvO/7Ty3tm7b3vMrrtm32r314Y1Z2WCJXeRwqgk6UjY/IAk0Ar1rf787bruxN2bh3BS7dWizW76r/cgfvsjn67MT/dfb4WJocgaqNJ6GgdKaOKnSKN0jX0arH3nBtfLUW0WFnZvfFrG2H6a6VjWNdNWqyaSdTDUWOaknr5Yee/d7dvcTnDm/nK82pE5i3u5e4umDyTa2Z6QxRxymQRxwRkRxRqaLGqoKhVph3ZipcLNtPBybZzeC3RNt+hyWTpsnKpFUcpEKilihwcVxhoaSGFZ4Y7/cymoHljU6VG9vf6lNwuVvIprHx2SMxg1Gk6TVz/AGjM1VJ+EU7ScklG9yQWy7BZJtNza7p9KslwJj2sWHwrCKiBIiupc63DjWoNADKbBx+5afb22Nz0U1TTTSYuKro6pDGtQlfUaZbLWmmmeRaQQI7rxqc2kBCXCO7tLOd57WZFfNGUioK181OM1+fnTob8vbjzJtNrsm/bfcTQyBRLbTxMY5EnFHBSVQXDRFVbBU6gtfhBFqlRvneabG2TlMJtGu3Dms5SYWbLwUmQwmOkoaSuoJqiqyeNptwV9M+YpqaoiEdmkgRhctOratGMQ5a2WPf96sr7dkgtIHkESyhwWKOFVXdU0qHBrqXUaZCeXXdbcPfT3ZvPab265s5W9spd337e7ay+uutj+nu7a1a6tfqLiW2tzeRTPd2YBDWVwsKeKdBuDHHrmKt8qjU47E7WzWd3ilbn5quPDw7exq0dBjBhFjyk1dkKXHSyVWRqHStxlFFJKkslHCzoioT+9VSX7aSWyXm52m27bKu3j9T6mY6mZyFFNQVBSjEqKaiNRJFdK4G/fptN8m5b9teZ+fOatlj51Yzbf/VTZFMMVjbqzTNO8L3N5KtzLIVS4LOqoyxQormGRzw+K2VWu3rkyW8kk+1YxbSg8Ap94bRVgHjlZXWVyWtoVRcW5uAce6qgcqNQYEy/8dfoIf3eV49x94zaDI5LnatxqKelo+ag04+VPmDxHVi7lgrFV1sFJVLhdTAEhdR4XUeL/j3i4oBIBNBXJ67tzvJHDM8MXiTBSUSoXUQMLU4FTipwOqY9+dLb97C7m7D3LjdtNkdp0u6sRgMjUJnNs4yU10uGwsjUlFNuLL49DUzUFXG6oI3BknRL/wBk5a7Xv207ZsXL1jc3em+ezWWNNLsSqp8RWNWNAQc1GFPpUfOx7ze1fuZzx70/eH5n2Hll59hseb720v7xZIoraG4lvmURC4uZIkBkeRVUU1M0ka0BYKRxxPx6r8NXYnGZuWioosOJaStr8vX19VuLfmLB+6rq+jxzZDcFLJkcDQRfZUtHAtHT+GnVlEjtf2VRc77dNBcy2XizXDuoEUKDw4HbsQNKUhQJI41FmdmLMQMDqQbD7n/uLtk2wy85SbdtPL8tlLdpPul5E813bQW6XV01vY2Um4blNLaQGpjS00xINcpVeB8Ng7Kw3XG3aXbeNpoqaCmWsq6moEs8kc1XPVVFbW1DmaJI6UIZSIgWLinQRsXERdoF5k3685l3G43acCp0wrHRexAOxQQasSQSxpTUcUBCjrh7IeznLfspyrtHt3y7dTS2zyPvLXQ8WKW8u2EcVy80YLJHAqyW8cNuXeoQM2qRXdgg7l3Zit2rmOrcRW0M9WNuZnL7nnmzMmIpcLQU1AJcclXkaeiyJpajLVUiIsMkTxzY81EkgRDTtNIntbyvPDeJzPucLx2cdFt6rUSM9UPGvaAcGnxEUOCOsMP7w77xPL8PJe4+wfKW7wXXMV/PF/WE25WQ2cFvKkyWrZCm4muEjeRVfXCkJjkUmbSocfDnoem3VieueyKnH121sFj8/v8Arod05TcW2ZMWJdv7AyDvPuDMZmowdJjsVkd6YaKkQVePXHUkdXIKvJIrw65V3e+ntb+a1lUGObwYo0YEGrSUNAOJCtUkEHAopIr1x42ozRKG25m+sgjaRtPr8LEmooNFcZ9agV6bdib63b1/iczVSRwUtNuHpve/WtbS089L9hk9u76xUu3qmrqKeaKaVqYZirFTHMiJ5qmCNIyou3sYXlglzCkYmKsLlLjVXiY2DaaVGGUafsPDq9iAzSzzIJUVDWpoqlgVXFOAJxjj+XUL4r9c9f8AaHyS2Fit/wCTqdmdV1O5tvTb63XFuDaOz6vAbPxeTnGcmj3Nu2oxu2sNuDcg8FJiqvKPDQ0dbUQeSSNG9aLd5LqDa7p7bS934bBF0F6sRjsBBYDiQDUgHo82ZLW53lvCBgLLrgZ5AoUorHuYgZZgNJoKGlKdLDO7mwWL73G7IxujA9df6eI9x7VzO28Ia3B1e2Ntb2/gNDuvrbalPHgsDnBtbB7eiiWCCKghqpacxyCJXkCJH2+eHl6O3t49d29gY/8AGGOp2KZSSSruNbnubNCSaE8VMF1Be7hNcbokoha5DII1dYwTgtCg+JYlAGkaajHr0ItB3blNvRfIXIQ7wr8vvbuWg7M6x7i3TtGpxmWxna23+xe3tu713TvfNY6fFPtwbemx+LNFhsNjnSSsqpHrJKqjpoIoakM3eyzTvsSJAi7TamG6tbecFTE0NuyRwKwYuW8UiSSR6hVVUVHZiyjvl6Pb549G4TLNdGaSO7e3rK+h3QG6CErDJoidooYS36lZC7RqFrXdidr70oNx5/LZXceO3djGylNj63K7erpo2oJGhmp9tU24tmtStFsfcO48bFMZYVq3vHCbRNpNU41hu7Vkig8No5tBbTIBmlC5R8eIiEju00qfXACu67Fvdnf3d7LuUN/Z/UiJ5rV2XRXUkC3NtpItLidFaqGQmimikDxGMfU47A7i33trC5DD4imTc+Yw1NS7e2xSxYmjiosjQVKyYWhrK6LccMNFQZ2p0RxyfdI1VLLLLUOynyB4y3Nnt19dwysTDHIWknOvKmuplXQWqgrgqQoAAAOJeurPZb/ddg2LdLe3UXktsYobKMQgo8Ta4xIwnUCK4OkCjhpGkd5CVoyQlwdXtzcebppEq8nU7WjmxkGN2zTbb3DHhMi7h8rVT19JRRR1K42URUiVONjlBELVhYIbxqWvEvLSymqFt5gGBlDxllOV7W7l1DOl6UrpIr0VbLsE+xbtvhWKW4v7OIxrDYpb3IgkI/WZm08YsKJIVYjSZqgDCVamzayRRz/byY40UkUNYTDHQz1cUkrRLLh0yM8kcsctbCR5msRCxuxZSDHxIShAU+KDU8a/tp508ugw237wl2gkkVtseExo506CwJK6ohIxDIzqe/jQnOOgV3bLh87Qb1p83nqtqhEmxswpqTFxR0tZiq+hrKzGUeRPjoosbILeereZyEVk89iInVoXQ2zQR1FagZrkGhp6g+XrxHQMv3tbwcxR7xfEXugxsUSMrqSVdSK4OhYyoy9a6QQGNQGG3rmvw2d3bmI+tNvbqxPXOU2lseoy2P3NU4LEU2F3jTYuOgz2Wh21g8o+NpZdySwx1XhNWa40+iqnYmbR7Dcoure3DbrNC1+JpfDeAOQYi7GJNTLqJVKAnSF1VUYoepz5RurDfd9vLTknZ7625Mk26yN3FeyQRRxXaRpFNc/TRTLGGuGXWV8Uy6azMclOkDmps9ge2927z2v0risRuvGfxrLybmoPNubDTbXUV9Nmt9YLD0tfi6am3JWQUt6OMRBvNUSPVTK12c0iEMu1Wtncbs5tm0jS/a2risbk/hrSucjAFOgvul5vO2e5nMfM/L3tvZw7/ALmf6m0Vrm2FvR0m3C2iDIqy6amIle1iXkbWKlc7v3Z1XuhK6PqLr3tWGgwW29p03W2wN59xbVal2JtKv2pjps15anDbYyM2cze5tyFp8fXzT42qGLVdcnikpoKUq2ex5gs44Tvu52Ul27y/W3NtbSp4z+IfCZVec+EqRYdP1O8mhFCWL9+3rbeYrW2t+XNkvwllZRJte3XN3H4FrbPHGzBBSaRpZpNTCR5QzIVIZY/Dijd6SuCRy0Ve1ZRR09PSQwz0ZqMn5Gkgppo4dw/dVMklW6aG8QVqcCZbsRcsDsa1VXgAZSxJDYp5VUgY+fHHSOSS0lubi23qSaOaOGJIXi1SK5Kq+m4V3JfTnTQp3UrTJ6EuWo2s21sXjML19umfftZlXnznaGT39hv7my4ikoUrFw2F69XreSR85RLVBmqTumq4m0GnjDrKiWD6w3Jae9h+gXCwJGwlFTQFpPFypIP+hrWnHBqxu0ZivZI9tspWeW3jZpXdCviqA7OiiNlJCsVCa2K6iS2cPv9z67777b+5u8bffeDx/3Uyn3H8O/u5/Fv4to/znn1/ueH6fa+r/N+1n7xtdGv6+ClK18RaV1adPHhXtrx1Y49Bb90b9p0/umevw18N/4q6vs8vSnn1S3seopqXPUklVFO8cssdKXigEyqtQxEyN+5C8LSQK58il3VFYLGzEMgk3JSbdiHA095HrT9teP7SDXGYo5dlSLcIzJGxVuwkCoocmuRQ0Fa5NAQFJNQbGny2BOEWt3VS5TA5igSPHU0qSVC0lVQVNLTUmNx2Dlpq2KnSais0FRULTU4R2eJn1Fh7DISTXRDqQ9wFOGSTX8s8eplW7207ek26rLBfx/pqwrpZCqrGkZDgAqQVY6VySpJJp0rPjTuLcOV3BlNkbGye4sdVVNdjauuq8ptld17fnkpsTuWtfGZ/Js38VwUmWycNLD9tHLTx1EcVSutpxGWI+co7W22mPctyt1kiRx4ao/huC7CIulMMyo7MvHNCKYIlj7rlxzRzB7iXfInJXMX7umv7Gf62a9s476yljs4juq296soYRWtxd7fBHOxKoIvFEviR60exzrutyO5aHcuSyO28ztSWHee+DiGrWqsIm6MWDNUyZ/GbLzNZV/3VpcyKZ6qbECMVNEXnqC+qpR5IJ5oiWyuI0F1BPqtYPEXsZrdxgRGWII8hTUAJCNLfpoahTTrF92nfJN72fYQdn3fYIDzReQRJCdwist+t7g0bcWs9zW6s4PqDaSF7RZzKjLe3EEcTktJTFuDae0q/tDuqXeO4ocPRYjsHdtJTSwS43H1VRMNx5ozVFNhoIqiVljFOgWnp6coVkZY7FBbKCPcbtLDYhY2zO8tsjkFXYZRaAvhRk5JNeBODnglPy7tN1v/ADzPvW5RwWttuM0QYSRRsT4spYrDQu2EwqIQakDIwGexojSb8xDUNVLU4mDcNJSVGQjxjVE1bhZclFSVUlJhJC9ZXVlTjnaRaOEPVkA6BdSwNb+dVsHaVQtyYyyoThX0mmpuAUNgsaLwqcjoMcu2ZbmG1WKVm2sXKpLOqVLQ+IA5SI9zyGMFhGtZCAaDBIP1vTrmfIUFHW4arp6XEY+WJ9xQbthkwuThnNT5xMYsrj1xtZR1cix+JJi00tPIbFH0BgRZ7+kreBdRqHb4WTuB8vWop5+Vfz6yE5g9ulFr+8ti3FXtIQDdQ3f6UyEGte5VR1f8ArrYeQNAbd8Z/wAW3H/9QNJ/7jx+8Npv7WX/AEx/w9fT3ef7mXf/ADVb/jx6q5/mRZODG5XqFpaNauSXH74WAvO8SU8om2wqTsoDxyGJ3DC63BXhl5vkB7H20lzbcyhZiih4C1BUkUlxXiK09fyPXHj+9O3O322+9kDLZiWV4d3CEsVCnVttGIyDpJqKiopgjNS7fC3Y8G6e+MDk6sQk7ZxFfueelCx1lPkPOKfBpE7h1WLIY5tw09cGVXIaEuxuLgd+5W7tt3Ju5xRSlWmItkLAg8e6lfwsquufLA6xR+4hyFDzh96DkO7vbbVb7THcb9P4bgqHtoGe0ZyMVS9e3JpxbFTUHq9sEqEDtqduCQpGtwpZiFuxF9JNrn3iFTUWKLRRmnoK0+Xr19EayG3jto7mUNM3ZqVSAzBSxotW04UmlT6VJ6pL+YPYT7u7TzENPkamTEbQrY9vY2P9qOjNQ1FFUZmf7VppHFd/EdNFNIqorw0MBY6z7ys9vNpG1cu2EXhL9TcRfUyMCSe49maUAEdCBU5LY49fPp9973Gn9xfffm9p55V2Xl24/q3Y27AAJ9IXF01KK7PLfmZiWFVQohNEUAoc+AzuRoYo6Kgy0ryQmaeMYrINSUyiKCpx8smRgRaADJI/7LgsC4VWEYJJkqCW3ikaR3TQGoCGFTUkN2mrdvmMYqRXrC642zdLmDw4LOYuV1tqikCqKBoyZBRBrHwnIJoDp6GiT48772dlqHKYDLLna1cFW5GtbAZWLbdfQ1klFXOaGmnrqPIRV5qYEESxqivUPLpAVNUily75ZbhbSQ3Vroh8QKokBcEAjJoQRQ+fkOPUl3HtJzXytu1pebJvC3W4Cye5meylFu0bsjkxKZEIkZkFNIAMhNFxkWa/HPs7sir+PtBmNybZnzG5MZBuqhxtLBLHi63Ija081LFRV9PWY6BMdm2ePxmCOKruqLM7aqjxRY98+csbJHzqYLfcVgtZwkshkqVDSaqsrDBWq51MuWoMCo7GfdP97PdTcvurScwblyHNv3MXL08+2WtvYlVnltrT6Yww3kBZJ4ZPBlkht3t4plMdsPERJFAnT3yc/wB/d0XuHObunpNn46GWkylJicxHiqDN5LJY2qqHp8HWNTZPcVJkJMjQ0AWFqadpJKsRgFIY5o5TLkhLfa+brfbdl13NwyOjzxv4kMaFddUIRKdxXVWmnI7iQeo9+9EObOePu071zd7rXFny7Baz2W42uzXliljuu5XnjPYlL2OS6nMbW8H1L2qxIWuIP1mWJEKKC/TW346Su69zGNpag4PKV9fJQZ2czHF5Orx6/bZSkxeRm8wqqiiaoSNkAULdY7qxt7HW+bgku2cy2byr9XFaPrhBBdA8blGdeIDUNPsJ4dYnfd/2nb4fdz2Nn2pg1qeZtrkacnsZvr4VZEY1JbFACFrTSKNUdWve8UOvoBPVSHy9623/ANmd+tRbO21SZespuvNsTSA5WipK3G0y57N6ZRPkMhQYuOWvLGMq5e6htL+kn3kn7a7ttO0coRvf37RxG8lWpX9N2ZFoOBY6aVFKHhUdcR/vw+3/ALi+4/3iby05U5ON/eQcrWl28dsWlntraK4m1zSUIijXVII5CaoK9spwxV/U/wAcd50OLy2DqsRQY5a+CX7TIVmVxmSxsOUkdxTtT1uGm3FUQQVE8vqqGUw+MNpY+z+/575dguIyLx5LmLuaGOOTWVUVZSCqr2qMgkU/FTPUE8u/dI98dy5aXfpuV7ey5XuaLFuO5X1jBbFpnEMUkRNw00+uRgEWGOV5SyeCkhdAx6uq+sabrrGVFA8RSvkgoEr6GxkSgno6JY1jjlD+SKOA5KcB4xBr8oZkQssUMMe4HNtxzDuSxra+FbW5LKp0nVqNdTBSU4BQoGqnd3GuenX3SPu9cu+z/Ise+Rc1ruO580ILW43Ow+tthCkTkR2tj40EFyoeaGR55pkgLFIlWJRHrkTffPa9J1zs2ufHVdNNueqTwYim8sbywVIl0LXyxNHNHJFjpUMsiOpSXxGElWlQ+0HIvKtxv25xXE8JG1RMGlZhh/Pwx6lhg/wg1rwBG/3x/vFbH7Ie2W/bPabip9zd7sJbPZ7OMgyQrcKYpNwmoawxQRs5gJFZrgIqK6JO0VT2KxoospFkAz1KyBETGgwS0UdIp4WOkMahq3yBHSZnMwZTey6bZSWkqyW4h0MJtX9oa/s9Kfy8uvnWsLSWO4luG8NrSOP+zU9xJANeOP8AD+XV03XGn+4W0NBYr/d/G6S4s9vtk4can9Q+h5PP594gc2gjmjmAHiLyUf8AGz19R3sLIZfYz2XlK6S3Ke0GnpXb7fHRXfm7s4b42V1rtl8zLif7wd37Gw0dQYDVxUprdub/AI3qIqOMwiapjS7L5JFX0ldShjcc+0+5nar7mK9FqsngbVPMRXSW0vCdJbNAeGB518usTPv9cgf64tn7BcmtzDNZ/vznyw2dJSgmjtzcxzQmdIQYjI6+JqIaQatIUMgJ6aurfiY3WWRoMzRbu3PDltlZ7F5vb+agOIomGVxNRFl6fL46nigzErUNJI1mScRTXjktdCLiG+92Y7+EWkezxH6qMpIryMVQNVCr/px5IFaqSACM1qBD20f3bO0bNLvW6cwe6m5ttm2S6oRbbXCs96qRJKTbL+8p9HiSP9PGrgyPMj0QRtE8g87V2vtrbGQyu+KzbG2toPu2vOQSQ1lPh5I8nuvPvX0uJODxa0+1tr0qZPKQU1NjsNPNR64oI40bRE0oP5g5h3PfUg2yC8luUtQ4ljjjrFpjQKZVZmeWXAY65aEcRpqQMkfZL2O5B9mLXct9u+W4thv98bboNkv913F5N4+ovS7ttNy62tpb2U5lWKJ4rSNjNrmhkmnVFPSM+QHyMxvTuEbGmklbemSpLYyKejyEGAeokWEVdTHlZoqKPIUtDLUXljppPuySikQiYVEWuTeQpuZp/rTOF2VJKHuUykAmi6FLaGIA+KgFajVShd+8p98PZ/YLaE5dTaZL33cubENBB4U6bfbSsigXD3M8cYu4Y3JKRQBzJp8OZ7c8afKaTLZvcNbuLJVBydRlshU5TIVMaQxyVVdW17VVXNTRxrHTJNPLrKxhUiW/GkBR7yVWCGCGO3t4wiogRAMBVUUAp6AY64LT7tuu+7xfb7vd7LeX95dtdXs0za5Z5ppDJK7O1S0sjlmYnixqermOhqgDY+WnLx1ldDOvmywx8mLyOdrUxtJBWTZKmkmd3raLIQHHNURrE1alBHM3lld5pcdPcFJpN+2uJYSqGGgj1BkX9WQjSxGkBkIahqE1UNAAB21+5BJsdj7H87y3276I/wB/SvdyqpScxLYWagyRROLlxHJ4qp4REspQiMs7HU09i7q7EyfW/ceGqtgGkqaDbW6lweRqMrQ12JydGtJ48eqNAi19TkayCpEiwNSRxNGoV5gZQU1tWz8uWnMnK1xZcweKrXUQkjWM6w4bOK6QhcUrqJFagMBkU83e4/vfzH7Ie++282+xbWMqcsbm1ruDXsX0ctpLYSOshDB53uoLZnlKoml54/AkNpLUDX10RhSkqytI9TErzJHr0BgTKiLrVZJxfhbrc/ngH3l7qaoKEBQpopP7D8h186RSMRskiO0zSqGkUVAqMqM5fPDHQ6dZ4all3Fk8hj6eaWjpqGipaGStgBnkSuBp6qWOmeVQh8iWJVXREJJZRcEoklZooo5WBk1MWApg+WRX59CyxtE+tuZ7VG8FERE18SDUHsPDgOFQPXj0a7B5KuwmIpIKzJHLRUMEdJF9/LQvaoeoqy1NQ0kYpqCE1MklpdAM0kpLudOtgXyxRlqhKOTqJGPsqeJp5V/w9SFtl5dRWLxS3ge3RDHFHLpOliTXw1NFXUT3U7iTU4qerCOu9jYCrwm2d2T02SxWVye0cTRGtxWTzW361aOOlo46iiqZ8RUYx0hMsQYSwSBZoYo38jKEC45c3cy7om57ptttcxSWkN07/TzxQSgMWNCuoSajUlqGhUkjSKddlPu8eyftluft1yRzPzDyhd2nM9/s0EB5j23ct1spJYRDrkSdEaxjtUWMJaa0E8N1RHSUllYgT80KKuxe1MA9DisQMHW52lOUlnqJDllzsFG0WIlpsdBBDQKj4uKqimcPJrEiJGiLAxc89qr2O73DcGubqSTcFhbRVaJ4ZkVnoxNT3lSF0rpqxzqxDv8AeEct7jy3yRyhacu8q2G3+3km5WxuI1lDXAvks7iC1IgCkJrtIZY55VmuHuPp7UzGMxReIj/iK71e9MnVwvQJRJs6CCOOnpqOneQw7v2VCxK04YtMjJqme+p5XYv6m5EXue6ryvLHRtZuFapJPEOfPy9B+zHUQ/3flpK33g9gvI5ovo02fcYwqqisT9IwPw5JBoWJ8ya5NDZHNLURyIscKvG6MNZkCusxZBGPGwVWiVNTOdevgBVY+8bYYopEctNpcZoeBHnn+KtKClONSKddstz3G/sZ7SK22qSeGY+F4sXcYpGICNJHQUtwNTSSawUoqqjl+0uHTNSsNd3W0dTiHki7bgkpPuKuanMWQh2N181ZrmlhDRGmopF0+FWIlJW5UgmSOctIHJ1fHUnaVB8MAkq2sLQA51NUGpHb88dYY/d4s99ut/8AvgtHZ7TcInuTdSXAvRMbUPDMs1wXYxuFEKqkkLFTokUO1AFboeoP4bU1S1U82NqK77Gsx0aU9StSBj6urgraikSJ7ErL/DqUzBVCSPTIxBKK3sASyzRQG0g8RYC6yPUFauFoNQ1FToLNpODRjwrTrMjbdkuLrcIua932q3G6RxtBY3EaxTGGB2BeSC8NrDcxrfaYnlhMkkamOMKzULNkpaSnneoqaepqTHUVH3Syfc1jSwVQWhZGgSs1pBFCaOMxwoqwxSB2Ca5JGZTPc3Fg9nE0ESXdvwIRDqBJYFzkOe6lSCaUBNAAArtNlsvPW28x7nFuO43nJvMcKiSGa6uYBH4KNYyw2kUawXFlFMsRabRMviyFn0jW7OUTN/HSDaWO3nUY+r27RYvPVNYcRuzd1NTKNpJkZaKKfG0eRpqfI7nzMMWQq4SzVEiwUVNIqFJ2V5pp45f5h3LnHbbe6Mskc9gyPdpCNPjAElSvaVBYK2oLTgcKCtOFf3pPYjlv2D90rnl3li68fl7doTd7TDLIs09qdKiW1uTqjkCxM4eBytJYnjBd5UnoZTYOytq9OdKU/VNZUZrd27u/sL/czqmWsp+wKOtrN4b2bPVm3oKPrSTGmHa2KmqqHIrHkqmRHrZ5JI40mH3KQqId+vt/3eTdJ9u8Ha9vuQ0kzMhUxxZaQPU+JTVwFfM9QTb7ZZ7JtMtyLtkvTE9sIypfXNKrKyFlVhGXUnSGp8NAdVK129gdm5DrDbeVyVHmtp1uc3hgZNpQ7X3PhMRuai3SmYlwVTWT033mAytTgpqCbAUk1LlsdW4irgmp4YfulgkZWl5VF0yiQtpjcuKVGACKnIqKGlDX1pUDoMX8zbDbx3aSWzTSxBVt5lDiRpEA1UCtQAVIYMtGC5wD0Aexu74loIWlWPZe68PkKDP0W6JdzUSYLMvj1oIXgwMYxpSgze38nUVFVFMMtNL4pl8UUc9MrPW6szIJYnAmtHXQ0WgkjjXUSe5WWgpp41qSDgq2ffojJb3cZWz3eBhKly0oCN8IpGNFEkR6sD4hNDVQGQEiBgt5rt3buV3WcdWbhGKqfsKCChi80eRV6qL7bIU0sVQ9BPj/ABVpqJHMyRz0+ua5Vl90EZkZVD6SMtX0HEUoSOFOHEdGLXcFrZX000DTRkeFG0R/HjSysp0sudXGhU6vMdGR2dvfI4mhpsnV4ivze3d3Gmhz+Drqrc+zOuMxLjKdsvR0O4v7u5HEwZ2n23lJ4p6PGUtRClPUw07ghPGjBne7GK9Hgx3IgvYv1I5o1iluEDnSxiEqSCMyLVWYqaqWHHIlrkq4mWWwvntnntX0QyCZpYLQGNC36zKwE2itEjVlowUgjClKZ7Oyy4+gw+RekGExdRUw7fxYBoqTFUmWVGylTS0VBT0cC56urIIZaurqkeonSOJHmfwoUfsrVY5prmMHx5FrK5yWI+EEsSdAqdKiigkkAVPS7mm8tRElpLbxLa/Uj6WM1VYoiAJSiKqATMQpkeQFyAoLsVB6F7efV+zeh95fFqsps5srtjdm8djbK7k36a2uap65Tcm6sxksdgNhVUe0c9t3cEUux9uQYKHII9RBLU5H7rVqpo1Rgfs2+7nzTZ+4MVxY3W32Vpfz7balU03DRQxRl7hfFR0PjStJ4ZAKiMIfjJozb7NDt+6civfGMbncTrOs07AW8iFxDCVETxyBYiI6GnfRmNVUr0De2aPN4PDbkwNBR0OWqczuKuhym4rxzUuLIp6+qo8PVNV5r+ETYzK/bxTQrFHJWST6AoiPkYie9a3nubS6mmdVSPUkWBWpWslAviApWhyFAJLA4oJOV7ffdn2TmDbLC1gf6u7db6+YK0cVFd0t5Hkl+n8OXwxIlAZWYAKVoSUxuPGZTF4jOJX4ypjjwf2+S3hW0dJlIG2/Rx1VDST12WKw11ViqXG5GtpIagBQUmqhExEhKKY2zxXPhzQvVGWqEUIYHgQRQEMOB4EZGM9AnfTNtUEtvexAVlHjshdSpoGNSdbL4fbqVcipBoQQpJs/hcm2IqKCllx2Z21WbnzmZx9XnqrN4ylMOQp6RabdC0NcmFy+KENNTTK0zhIKuNFZ6Z9Ksh7DIqzoaMJCgU6NJPnioqrZ+014HGYUv7eZtvniV45bFriSVDMZFU1CgTBWCSRnSpFcBgMpw0nQ6y6s+SXWdNgtnV+3KIbQ69l+aNZvXIYfIbN3RsDOZn4i7Bl7W7OwWI7S6n7A3Dit8R0NJksTBT5HyfwiWXNY0U8mRpZ49SW+2ez3G5upzKwuJAqI4zpphqagyg09Pt49DHlD3W5t5I2nl/abeCGTYbN57me0ZDEs/iNqQzvbyQzzqHAosjEAqEZSgKkl+J39Rbr3B2H2NvbJbtpfuauirv7t7VzGbxVNmqmstjsXT5/cyiuioMVhYqSNVjjpxU1CyOITDHEAimaye0t7OxsY49QGnxHVSQBVjpU0qTU8TQfMnoktuabfmPeea+bua7++8WaUS/SWkssayvJREE9x3hIoQqgKF1OKhTGqggx+0Op+7lr919o7i2X2RX4SqqdtVOS3BR7Q3bkMBVUm4I46TaeTl3JVQ1CPg3pCkFOlZWV89eYPOJSQxcvnaFYLeGOIJGi0FcUya8ABU8agLStKcKH2y/vC43vc90vr+Se8nmUskZeQyFgAp1MzO6RrRdLNKzaQxYGtVFsuDJF4aTPNSPmZKrLV0IgoqhcbAlP9skMkUUytkliovsmBDSv4JnfyAo2lazuqRuwrooFIqPX8hmv5+XRrsNtcXd9bRzGP6wtJcowUsqhQKHzcqpjNM0Q11ChIAt7cocPip8DncxHHuGbIz1smX2NR1GbwuepsVQx08lHlclmYsTXUOLpNwGtqEgagkq5hHTTGb7YPDrTvNPKs8EH6SIFCzsFZCxrVVXUGLJQV1BRUimrNFsVpb2lxBeXyNPe3IMn0ieIkioDiR2CsqpLVqaNXbUkpgdK22Xv4/wCDz2+7t4v4Tm9Hj0/d/wAB0/cf8BvJ+/ovq186/wAe39Nr8X1A+CtdS/Z4nDj5V4fLoM13bT4Hhyadfg00v8WrxfD+zVnT1V7tHEmuzdPVZPr3F5WTIVFJS4ymkyk21sbgsbEZIMjvXL4asoY1k2dUyiZnrnaCkoWpZEnkQ+PUZXLrHbSFb9loCzEDWWPkgYVOoYwKk1qB0Htg2+e+3S1WTlqKZ5XWOBXl+mjhjqQ91KkgVVtiQxMrMkcehhI4xXh2ttuiWjxG5otzbeyOMfNDbe4BsTCO2EpM/SYylGUr8Vkpqqjp90SVkdKXMrtTCU2ZWkRzO9tqlIaS3Fu4cLqUzN3adWARQ6ePDP8AkFed9ohhhs9zG9Ws1sZ/pLn92RVgEyRgO8UutVuSwXL9mo1ILKdbHG+AWxqiR99Nkq40mL3PHiTtpBWV2MzOSpcHU5CaszdJS46X76PGxvVUsdRodtZkWF+HQtHHutu62dns1xDpE8V0PFLIJFUMjqVYGgbBYfmSM8MyvuC8gvzFzJ7obXuUMk21bhyvN9Jbw3gsJ7l7fcNtnjeGYpJ4bRypFKK9geMCcNCJI5D+UO1No7d29tbL74yEWT3DtLb1Nh6abP18M1Phsk2NxFNPkqWeOgxbTNkqlJFWvqEXIRwVMtKZEjLRGCN03W7vb/cbbZkZLK4nd30Bg8o1uaMpZjpUHCDsqA2nVnrqV7d+3+3cl7byFu/vPuMMe8bPtlnHt1/dS20m3WKpZW1tM1nMyRWw3KWWNGe5KyXn6QaOc2h1OFfTGF25m8fu/trI7dg21/fPdPZu6YcLlMFLhq7AbPfeEzz7f3JT0tZRQ1GRkfZsuSjmnSoenmyMkcN4ydQi5svdxtbyy5etdwkmENvbwtLDLqEkpU0ZDntXxhGQCuoRqW4CmO/3Y+T+RJuQ9497OZuXdptGueYd10WW87XFKLexiitZphMhie48WY2iTRzFJVs3mnEUbm7ZJDS/wzD4mio1ipPt6amp7MaOKsWWnpYaZV1xVlK8RxUFEqK6SNoip2UMpjIDrG8dxeXNzJJ4zNLqBBYrkhhTDV1k+mSeGeHWfe9bfytsnKNltd7tlhbbJJC1l4MNs0MQaW3mDES2scZsEZdfi3JRAkZbUyV6AHurbjx9e7lrcnUYyupHzOzcxgDJSUImxBjz+1Ymo6KuWnjpWlgq45Z4qyeLgSKGIHkLDbk6+jO+2UVvHJHMIpopqMwD9r0ZlJJWqmhANK+VKdYpfe92Xf5/ZTe935i5mtt0247vt11tUc1vC72KSMjyQ2m4gCS5jaVNSPNEjmLw/EkkKU6HSTN1mO27DVUmMlyc1LTUbPFCRSp9nDOiZCXz17UlMstHjwXUNIiTS8KwS7gHW23w3d54c12IYmJGo9xDFaoNKamIZ8GgJUZIrjrMDm7nC/5fh3a7g5dlv75JpXitkcWgkhhutFyxuLxY7WA29owuFM8sUVzQpDJQhxV3/MjeCpyvTVZTLIIa+h3lkEnZmnjnBO06cNFEk85i8AoQHQLGpJDgNqLmfvZBJYrXmaGbT4kbQx6RQMKGY9xoKkljQ1JwRilOuQH959fbfue7ey97tTXcm3z/AL0u1upPEe2lLw7OAbTUx0qscUbSIEQVkSWjeKW6wfAHH+De+662oaSNv7siihqRCKMjVNO9QaCYNHDKoCQJdBdXjFyLrd73fYScu2YSOv8AjyMQSWxokFGGTxqT9vRV/dmxtbe73P8AI0+iU8nXKQuUQEsNx21zo8T9JiqLWjDSApL9taWFN2Dvai3k+2IOua3J7Xen+2xG6cfmMLVUkr0hgp6ioyNNNVYqWigiesT9mAVctTHCZKYOJCsUOS8v7PLtQ3GXmCOHdw2ue1dCpAYFlCaQasdJ8lVdQV9BXu6V7T7ve4ye4cvK9j7Lbtu3ttP4cWz80WNw0sJdJI453vpb0+JHbxmTQZS8sjPb3E8P1sTgQUN9tZDJDsDsQVtIKCrbeW6mqqJZ/u4qKaXNVyvRioaGnWqjpy2lZNChwv6ebDLHYbe2O3bSYJvEhEEYSSlCwCijfKvH5V6+eD3Pv94HOvPzbxtIsd3bd71rqyGVt5muZBJCNXFYnJUE1rpoa9C9tTsHp/b74vdtdk8w+9c9tpnz9Nj6PKxYbGZajlOKhx9fTU1bQ0tU1dDD9yBFTywQQBCp87aQkbbt3k8axW2UbfBKBCzMpZ1Yaiy1BIoTTJqSDigHQl2nnD2/22S15huLy6bma8sSbuOJJBDHMh8JY5FV4lYOq6u1GVFoR3mgXVN3fgMzueulwOTra+ofbWQmhxFPgHpIMrlMFQZaulgxUNRUL9nNkhS64ZHaWfwssXjkmconv3RcxW6LLEAocCrNWgJAyRXhXPl546Nf9crbtw368udv3B2ZrN2EMcGhZJYY3fTGrsAmsr2sSz6SF0s7aQcH4/7Yx/Y20dv5nsLAxDKbczFTXUW4MPlNzYhqWWcYXK00w8sO3IpKfIZBFYxf7kob+P1HyvoiP3A3a+2jcZLbab8BLi3VWglSN1dQZQ1dWsDSvGqqGBOSVA66Dfc95E5Q9xOU7Dmfn3km5u922be3mg3bbL28tJ7WeWKyezIightLic3FxVovAupmhliUmKNJnaYVO7tjvS9O7ji2nFS1k0+2MxTZTN5rK1UuTfbdXDNl8tWUdfkoclW1VZQw+V6aIzxNFZPC7rGtNIDuUN6afmWBdyYxgTK8NvAmlElXUoQqulVUg0aoOqvdQksJ9+8/7d2+z+x++bj7f2y3iy2UtpvO+7vfpe3V5ZTm0lkuDczGee8n+otopoNEkKWzRSmCDS0aGoHpXL5vb/euy8Lj87U0dNUbxwmMqRhszVtjcvh5chTRmgqI6aolhmWZPXOsjcuHVxruDkRzPbwT8o7zdPAGf6OVu9AGV/DbuBoDTNBTyIpjrkN93Dct02f7zPs1tFrurxwyc4bPDJ9NO7RTw/vG2/TcBiDUqGYN+IEMK9bD1ZUS0sazR0/njRnaptKsbQ00cE0zyxqyt9xKXjVFjBUsXvcAe8KreFJ3MbShGNAlRgsSBQmo0ihJJ8qdfS/vW43u12qXdntMl4isTPHCSZViWN3LRRKrNPKWVUSJaFmcGoAPRZaVp1+VG765Y4YYU6j2LF/lj/bMZ5Mvvlo0acx/thgr3Um6HQCLsSsjMYR7a7ZF4j1/e0jEpkikaVIFfLyPn+XWJW02u9Xf32fchYtus5ZH9sYYRHIzNGytupMQciJi4YhRMighELMhkOkOP1C+KnWnWpXBxCCnekpKGlraepippmniWoaFhDTiT7gQFANIJikZXW7MPYOlnnthctaz3Blnr4sjhkYoRUhqMdQatTWowCOsjbDlncd9PLycwctbZFs+xzrPZW9mI7u1F1bq8EEkHi2kEllLtQDxx6FXS7MBp8JD0700VE0tRDTzQRjHzKWpoKOOOoSepp4v8l/iEapLFj0p5PuBTKdP3EhlJ1ED2jklmSyihlgWkp8VZTliAWSnHhUEZHljFammpd15qu9zsd2vpXtUbZdys2nkS0jZooL9LgW7R/q3wjmhjWdHAEEjRmrJRa+flJ1lUbcrqTe2JqGqsdV1DRZaLIVVRUTUtZPDIlBU+Vlmkjx7CnMHiHjjiIiWJCpZY519u+Z5N4tZdpvIws8IBjeNQqlB+HSoVQy4p6iuO0luPH3/AL7vux+3m9bZ7n8p3c72G9TPDuNhfXEt1NHeHvN1DNdSzXdxDcjWZtbSG3mC6pAlzbxoW3bsUk01LTypLIkU6yrDFFMaVBUM0itrWJVljBcIpcJ6QE+pUe5VQUDSxsKUpUkVqOP2H7PPPr1gJtFhaRvBbXFqRcuwYgKaMh+GuMipAoaYFPMdW67EVn2LtpIpjEzYSkEc8Xik0MYhplQSLLBIL8i4ZSP6j3iNzMwTmje2ZAwF3ISrVoe84NKH/Aevpb9n4Wn9kfay2iuGhd+U9sjWWLRqjJ2+BQ6aldNSVqtVZagVUjHRf/k1NQYHb3VWT3NlqWGlo+9tjS1WSq462OCnpaXEdhVVG8S09UzUlakKpHJOSVdfJqGh2X2LeQhLfXXMdvt9swkfapgsalMuxhUhiQAYy2QpwuMmlesbfvaT7Vymfu58wc472F2ix9wdumursi6rHaWzSzB0SKaVhepCCJLiJVkmOrRGimOGNuq/lT8eaGepnrt95pMMlbRTVcku3Ny5fGitmmyVqLSuAq6mBQ1OsrzReWKeORUEpfyIH4OROdJokig2q2+t0Mi6JI45Ao09wIkVGLAkZyKEkUIJQbz9737rdnv99uG4e4u+3XL4lSSeKa1vrnapZJVk0ottc2styiW7oJlVUghimEHgeIqNHGOeyuytn9sUtLldjZelz+3WpsiZMtSSU/lxuappMV9nSTUFXC1bQ5SOjrnnKSokkSPGXjtIvsIbny/uPLXjRbxbtDuSvHoibIeNhIXIZTRlqqg0PGorUdZIcpe7HLPu5Ds9/wC1+/2m78gX9pfw3252YkE1ldQvarBBPDOiNbPMsssiJcQ6pBEkiKYjqdL/ACJ2VtDsHq3dGJ3LU4ij+3pn+wzmRlo4o9u5tIWbG5F6uqnpoaOSikqQ5DTQ64ZHiLBJ3VzLkC93PbOZttlskcq9TJGAx8SL8YAGWqFNKV7gMYxH/wB73ZuQ+cfYLnzaubpYmit2U2Vyskamx3WgSzlaR6pCuqZVuA5StrJIAQxjPVE+1M8MVUyY/JiooMjjyaeuarT7dqGopJ2gqI61qgoaSZKpvELgEOdI9XHvL2a1JZnRawtlaeYORj7Ovm926+WBgspKXMZActgqwwak4B1Y+3h1aP8AGPciCDc+Hx8+32q9tJQnJZirra6LL4+ozdK1PjMRVYj+FTx1U0mSpZAnmlp43E7qJPMsYaKPcbbku4dre5Ny1m0jfowiMKSgLGQyuf01WPVWgYE0qAAT10b+5Zz7e8pblz7Y8ubbscnNZsoIlvd1a9ebw7iVYht0W22pie/uLvcDaFQJUljjSUxiUOyE2i1e5a1ocJkMNPk6YxVlLlMpHLFQQ0uZo6ak0Us2HnYeLDSSxSN5ZK2pnWWTwmJkH3Kw5Pa7ftErXkd0kO4RvHJHbGshZCxP9sMCVQRXSqrgFWqSvXSHl/e+a/dO0n2S8gn3D27v7a+2695igK7atvMYEt/EXaCy3F1tk0iy+GjzSSrrdLyFYVR317Owdt1+ws1l9mZeimosxt/ctYlbHJRzwNUlOcfUxRySxSCiq6OZKimZQuuGcMCQyk5cbReQ7rDDuFrMJLWWAaHr5edag5qCCDkEUPnT53OfOWt25E3rdeT+YNv+m37bdxkiuohR/wBRSQNDI+h4mw0boxR0YOhZWUlabInOJpq6TyrU68TRfbyxVBWSaaRII5U1N9xFTeZQ8cEZiUzBCXV2JA1M9ZHKpTJ409eHnn8/lwA6R2AEEbmR9Z8JaMDxNBWhyBUDApnJNST0O20tvVmcrabZ2GpKaCb+KUtLRCdsdTMlPVajkqzHUKVlPTUcMUDE/wCaEMjNdliR1LJL26hsYZ7u8mCwRqXdzXgOJODk/LJ8q9DLlfl7dea9w23lblXbnut5urmO3s7aIBpHdyRpiQMP8FPM6RxuX2jiqDC4LD47FySJjqTHRwUNI9V934qJJGakHmdRI0lNBIInI0odIAUAL7wy3y8nv7+7urmDTcvKzSNp0dzUwVGBkE+prUmvX0w+2mw7Xyny1svLeyb+t5sVrt1tbWCLc/Vp4dsngtPDcMTI8M/ZSOvgwaRHAqp8Vf8A88d9U/l2l1/R1NOKionXP5HWVEsD0i5HEYVqeTzKkkdRNla1HjaxMtPa3F/cx+zu1SJbbnu8iYZhDEfOgAaSopwPZQ/I+nXMr+899wLWbcfbD2ttZ63Nqk+93yqRRfqdFvZqRWolCwTPpIzHLEww/SS+E1ah3vlqJ4JoZxsqGZmmSbyS6967PA1mS6QCDxsEjWzBZCDwFJEfupGRyvI1c+MuP9q/+HqGP7uy88T7xGzW2ii/ujcWBNST/ir8anFADQU4E18urUZZY4YpJpWCRRRvLI7fpSONSzsf8FUE+8YURpHWNBV2IAHqTgdd2ru6t7G1ub27lCWsMbSyueCooLMx+QAr1Qp8gM1vHG9udp4DEbkz+Px+ZymOrKnb+Dy9ZT4vIU82FxVFWVGax4rqalqZZqElCNLlk4ay+8zOWVs32Dl24lt4y0dqqGWRe4HQGCowUmleNf8AY6+bH7yVxvMPvz79bfbbncJb3XN24zizgkYI6/WSozzxM6DVoqAAK0446Zdiby3ftrJ1ORxvY+5Waokjy+PymKmypxbV0MjzmgzGO3WcVUVQIgRjN9pV0U7t4m8hB0P7xZWu4WiWt3tsTx08OSKUgsARl1MYcAg8BqVhSoI6APt7zfzVyPzBDzJytznuG37rHJ9RbXtnqjFV1VikWdozIki4YNHJDKrNG6sCy9XjbC3M+5Nk7Z3JkkTCz5zbuBz9XTlqWnosa+SxWNzMiVlfqNLTF4siqzvNIoLJKwICMwxP33bWsd6v7KGswiuHhQsS0jirKnaaFqBcUWnAEZA6+iT2z5023mP2p5N5wlI2qz3DYYt8nighENpayROG3FFkjEiqjXResZkaUxE6Tq1sq1wvWFL39m9m9PZnBQ7o2Bvjf21N0ZuPBZiKDeslNtaSOpbFYWorkerjpcxh8vWmBqCKqSISSyOYVdDLIftpdSWu6Rbe1wI5wTHJbtCiFgc6mlChy0dCNLk6Rw4kdc8/v/2p33aeXueY9j3C52KSTXb75BuMl3s6oqyxeBBaIZra3lvBDbytLG1u8rQOklvK8Rn6c/i30y3eW+OxO75ctV/HinosTsh+m+z8XvnERY3rxDVnDdw7Tx9Purf20YMocPt7GZ6rqqfyuyOtMyQQQVkUdSOuZb6y2zbLbl6W0ivIhM/11mFBaaM90elcs1W0EaQ5YjRgnUOa20Szx3Eu53Nw3hGF0jmcsxRnUsQy00qfFIWraQGOpRVTSuXtHbKY3fW/MXn8btXda4/cOTyO6aeOSizGy9wUGOyYyOSq6Oux1VTvWberq2ACnqKCSGR4XTwuFIPuUYY7Z9nshA0sf6SLExqHWqgLXUCdY/pVyMjoI7deSm7juLm3inics8sE4BjdVNSGVWFBRadpBHBT1Wp2FkNkVm5N31mwKWqw2z9wZmqyWf2wKmKjgxki1tXmv7p4erqsBFt+loqE0cyYOZQK4QJNGYqhmSF19mt2sFuly2uVVAWT1GAHbuqSfxClK+YHRZzFccv3G67ldbDbSQbTPIZZrUso8NiWdoIm8IRBFIYQn4wvFXYAFW4Ptnc7bl3XuKCXM0O1qH+FyYyoqMXXQUWKotVDhtlYcw00uQwu1se+16Hw0dLLPJSJBSrDFK+hWZKbSOGBIg6tMxNUBFScmQ+TMdRyeOakZ6MxvW4Xu47pu4hlj2uMo6SNEyxxqSI7VKDXFAvgppjQsV0oERjpFTkYjc2D3T0Dt7c2Hy3adLuuXtCp2/Dj5KPFZPaOJ27U7eocnnMtFhdxYjNbexu4NyGKKixVdBWyqIoH1UDzU0MvsKzreJzHPA8Fv9B9GJPEIKyvIJCFXUrq7RxgkspQZYAOQWUS9sO5Wk/Ku23djc7iLlrtrWSJUjlhQOimSREmSaCOSWPsicVIK6vDLordF+osb8g9l5GlzG6saua2zPk6TEw5/bMcW455cUtfUU+Xq8JiNl1eMjyNZiKallqqimro6KuuYmm8aSEE6N/tV2JIraYLeIupopRoANKrq18Fc0AYal4gVIPQcl5T9xuW5bPc98255+XbiU20N/YkXVVDMs5hW1dBJLAgLyRyeFLmNpNCuKifj4pcvlcVW5A4nLbfxtduCesw89FvTbm4qXdVFkp6f+I7gxc1BEiY9qGSSnNPJDFPFIschjKpG/tuWQeFL4EhE0mkq4KMukjghBoaHNakZPrTpdtlorX+3vudlHPtNj46SRMt3DIZVc1e4jKErVewjSrCikjAPVgfwM2hkd/fJnrLaL9mYHqTeFZvXJY/q3M0WD3dl8zQ9xQYTLVvT2NxOx9tbe3RvLOUGd3dV0ONNTV7drqdQlRJO7vGWYE857Eu/wDLt3tAtYrq0vUFtdxXJkaOW3kZFuUJtkkl1vFqEYipWQoKqtSJR5S5xbYLrd13qxSluGeG3Qi1KFkkQMBdzW6OsUUjlvqEaqoxdi51HbL6v/4S9VW5OuDJ8r/lVgd2dzz7L3risdlOuOktuR4XaO9Oyd3f3q3hvbcG+a6q2tv75BbhommqafBV24ocb/Bo6tkhpjHBTqkjWvLlvZWVtYWYSC0gRIoYoloqJGNKqKEdoQAAYp8x1jRee5Vzc7nLuL28s00ju0rTS/HrAJomhkjIapxUEeQz1j6P/wCEi3xo2r2Ditx/In5M9gd/bE25mqbOYXrfbXXmK6VhyklJkKKtjxe+900e89/ZfO4aeKj8cy4lNv1hMjPFUxE29mEe2KshkeUkGlRSmR+Z/wBXn0SX3Oc13YQWSWCIY2Yq5NTRqcQFWpUioJqMnGT1sr7j+P8A8RtjdObq2xuXor4/bc6Hwe3d95reO06vqjYNJ1lRbYzdLksx2VW5jaybf/u9/Cc7STVdRmddOyViPK1QH1NdeyQIjM6KIwCTUCgHn/LoKxS31zPHFFLK9w7BFAJLMSaKBmpJJx1rVd5/zjf+EzfUfacXXNP8bOmO8t1da1MlHic50l8IuqN17QwU1PT0NQkm0t6biwu0NuVmOR5FjirsXPNQCWElJ9Gh2RS3FnHEZxbhogaVUJx88Egn/VSvR9aWG93N4u2vuTQ3TqG0StNwpVSSiOAKGlSaDgadBp8j/wDhWTiaypkwPw1+NmTqaWt22Z4ux/kPlKTE1OF3HNJXRtS/6LtgZXcCV9HSwxwvDNJuOF5pnZHpkRFaYhvuZmRXNpCABisnEn1ADUoPWv2jqYOVfYwX89oN93Y6WBkkS1BCqoGEeR01rI7ArQRGmCCSaDU/7Y/mi/Ivv7vfsfLdp7e6Gnnz9Vnavcm4dvfD74ewVuVfK/bVVdXp2PX9FZ7fqbno6yuin+7qMlka4yBneXhNO2kludvS4DRGdqEh0Fa/0lopNRjiOi6Kzt9n5vvdjWW9j2u21xpJDO5UKCCNDhnUFGIYqAwrUkefQEbU3Xia6SGVZ8ADi6ubBU1VBXUmRoayPxijpqahXcNMh/i8UgZpvEZlM15I0hBYBJJAQsjHXpejhMghq1NShyPL7MEt0IbTc4buWwsRdW4nhka1+pZ1ZGQghdHjqNLVqSQSCx1KqVPRif7mVH2P2H3cn3H8S/uf95/Fd0+D+Mf3i/vH/ez+H/wfxfwn+Gf5D/DdX3H3H+W+Lyej2WfvmH4/AOnwfGpRPh+Dwq6vi1Z1fDTtr59Cn+oD6vpv3pH4nj/R6vFl46fH+s06f7Pw+2nx/wCiUrjqpPrXsrZ3W+Fy/Y1ZSUm7N8ZqZ9mYXYa1uUxuO2LtmnV6qonaorqrLVGXxdXCKWmpI5FnJ8U4qZGZiZhRf2F3fzQ2MbGKyT9aSeikyMeAFANJBqSceWn5RlyTzhytyXte6c4XdnFuPNd0z7bZ7QWnjisbcAM0rszuZ43BWOKMmQHTL45yvij7uifq+o6bwWQG3K3BbHoBJncftXJVdRl6zH5TIVNY9KmOilrKqNqaumqpp29cvi8zJL441kUEMB3JNzlhM3iXL9njLRQQoFKnFSKU+dBx6kjmS65KvOQtoubXaZbLl2Gtwm3TSPOYpZC/9kGJHhuSzn4ipYhiFBHQufGLcWL3bQdobU2FuOtxZwlDjMFt6PH4nHYXGYmCUbqhyG68XXUtRVT1FRX11clTTfcU0a6IaiWpkjZkSQGe4kL2Fnsl7uSB0F0s0mruLFVLLEQ2nBClTkmpUBTmmR/3KtzuOZeZvdXkrkgSy3V7ypc8vWxhQwxWUV7e2kMm6BoEuJX8GaVJVUxrrAcvKhoCcCjxA2QmY3Dnd41GExef2/DLmMJvbeE9dBhamOqU0sVNW5ipx+DwqVU06/xKOnpoaObIQQGmWO0kk0MbhepvFyLbbrATTRzFY57WLQ0oILMWVQZJCCCULEvorrLHh0b5J5Tj9s7GDmX3Z5gituXbyytZdz2fmC/N9Z2F1ZXENnBPbTGX6WGP6C7WK5gipZm6lh+ljigSOFaosx8ue4euezewKPENh6ukxfZHYLrjt1U9dVVCYqr3JuJ12rPNS5nHVUWLxmUyjVcUNJJDMtREoMjU6mE5GD255Y3radte6ikVpLaE1tyFXWESstAhBd1WhZqihNAGNeuKvLv3svef2k5v5ml5O3K1SdL68jdtyhW5ka3M0nh2Z8d20Q28ja0SHQ2oAOzxqED6fnD3TXz0VZU1mPpsDXyQQZb7Tb1ZR4/FTwwzUtZ9lUS5vdU+QpJGrkPkbRLNJToqRgeRJChvavlOHxYYbcm8Qao1aUlnByNQ0xaGoPmADUnz6lH/AIPn7yW4TR3t3zdbx7bdRfR3TRbTYrHEF1B/DYxXZkVmkoHGl2YBVBpp6cY+4O1uysTXYreG6ZcpgiaH7jbsWAo8W1MaOuhraKrRTA+YWJ6ylgaSDyv+3GoZQwGspk2HYdjuo5Np25Y7piQJjIZa6hQrXK4qQGAySckcFW8e+nvF7wcvS7N7h87Pe8t2ipK23W9paWIBTMcrR28MLyaTSiyFzGtaBSW12rUeX8WRxO2Y8VlpsLmdsZDKVmSibJwwULSVf3ep8vVZSMIsy1dRTywRIssciBQkMUBRoMaFDBPftPCLuGdI4oiEYtp/iQJRvIhjgitSSw67PX2+b3DzLsXLlhZbvc8sbxYX2879vshuYYrT6iONIlsrq6uEuLF4JFeRLFA09tFLBLFpCSEVafOHamH23uPr5cfVQ1Az1Lu3JV1RKKemyFRUF8MsmXykpx+Pq5qkw0/2IeSoqESmoURWVkfXkB7X7pfbjY7y1yjBoGhSNFqYwoDKI41qwAB7qACrNwpw47ffo5D5T5M5o9vv6u7v9Qu6W+4X95Neya9xmlmnW4/eN/Mbe3ZnuYpFii1MzG3tlnYIZwGlfFjKUm1d94SGsXHyVVVg8uuOrq7L5DF0NXNFT0uYraiXMrj8xafC7bSrcQvSNHTxIrFXIiEiznGu57BfJFLKiiRRLHFEksjKT4YjVCy01uV7ga188noIfdWv7flL3f5bub7a9rur42tw+2XO77hPt1hb3UKC8W7ubuMNqS2hjfXA6iNoyVqrFHFlWP3junIRy09HiX3LVNkKWtrcTSSUe2a7FbTyT4+cwLVZSugXMZ7G4rJQ1MreLGR1KsyQ2l0IYRvth2azCyPcfTKCY45pj46ySprU1ESlY4TIhUGsjCncunPXUnl73p9zOY72a2TZot6ea1hu7zaeXVl2iWxtbuSzlR4pd0b6u93GO0uPFlRPprcpKphuxKoApU+X2yKvZXeG8VqKKpWh3FURbqw9dMkNPBX02TpqVMiI6OlNS1LU0e4BVRSGaVXmVFl0ASxu+SftxusW68p7Q0TqJIUFrKi5KtHgEk0qGTSwoMVpU0PXHT77fI+58j/eQ9zjuFs7WW87hLzFt9wwKxy2+4SNK3hihNYLky28hYqfEheqI2Oissxb66fqTcIq8kAfUKDbj6fT2PwAPX9vWIzOWrWnGuAB/gA/Z0q8rU0q1cbbbq1ggw0dGKCelaupK6pdqNqjIZN3aGmQVUFREInkAgdlEYVXALKjiQhD9UKs57gaEDu7QOOM4GafLo5uZUMwO0vpW3VTG6Fkc9lXc4XuBFCRpJxhuIvp+I/XFV1t1BtnHVslXT5GviTL56hraqqqWpclmKKmyoxkdNPPJBhZMWtf46ingVA06tJIPIzWxB9zN8i33mK9eBVkgQBLeVFC9iFgzVArIrMDRicAUHqfom+5P7X3/tV7N8l2u638u37xdyTXm87VdXDSE3V6sT2sTW0hQbbcx2iROYlR5J1lV3cArGif+cfY8WxOlMlRwS1MeY3VkMfgMc1LKInRKp5qjJrOWik/ySswVFWwsw5DMqm2sH2o9odjl3bmlbnhb20TyOSKipGhRxFDVqj7D6dI/wC8R9yrfkH7uu47KJFO7cybhbbXbxa9MnhQSpfXMyjJKILeOJ8U/wAYUcSOqkOkaUZLuLrPcRpqLH002+cJClLQtMNVZDXxNKWim1pEqrJGW0lVPkXTdtYGRvNT+ByxzBYF2dhZTHU1OHhsQBmpz/l8qdcY/u2W/wBf94v2H33wI4YX5y2cLHGSauNxtwxIIoMEcONR5162OfeDvX1DdVEfNXf24dnd1VabZzea2/V5nrXbcX8T29mK3DVk8Ueaz7mlqpsbLDU1VC4jYqpJQPz+QRkl7X7RFfcs2zXUSOkV7KWilUMuUSjANgNnjxpj5dcQPv7c83my++N5+4NwliN7yzZxpd2crRORHeXYdC8ZDPEXiOK6dShvQ9F36+3z2LHQPLjd+bso5IYp4qiSHdmRjZIsjUGOaKOCSsWeokq5ppS8aAj1u7Lp1t7kvcLWzuGaG4s4pIW4I8YYYHnggCnr9nE9YFcu7/v+1XFvuWz8w7hZbrDIJEuLW5kiZGDaldCjq/iBhUUyD3eVerg/jrvnJ7864oMpnkdtxwNLQZqpGPiopdVA0tPTTVsMCtT00slJFHKQNMKmYJEkcemJMYPcDYo9k35oLagsWjE0MZaulWY1Vamp79WBmmTU1J78fdF91t191vZnZuZeY7iReZhuNzsO53SQgyXt7Db2skN9NpR1SYWPhRO7gpI6VcgsidJr5EVUNb1/np6DF1u5oKehyWPrJ8dkoZKDHinoXycmRr45qtKSVsRkMLGXijhepBZjCQ/lUG/t6n0e926XzxW8jfqRpMgV21VjVUJGqj+JUUOdNCpFD1FH31W3HnL2d3K65Ns9137aLVPpL242S+aexg8Blu5b3cLaAtG72a2cySs8S+GlzbzfULVYWrk2zVJX4/J0tHkJcfUVuKqqGGuoppKeupHqI0jTJUMylZYaqkF/GzsWU2IANrZIqnfESO0MGZaCh41BHmD8uuLllOBb3qRzMsrRmKOYEhlJpRlOCClDQnhjHVs/RlBPiumursXVaPucdsTbNDUeNw6eelxNNBLoccOmtDY/ke8Puc21c28yMOBvZv8Aj56+lf7vkTQ+wnsjCxqy8o7Op+0bfb16Kd/MUyFbT9J4KWBZKQU/b+01ikZlJqymz+x5XZoLPG1IHCgCQnyEG6AAFpH9k7a3l5kv0kYOW26QsAPhrNABnjq48OGKGvDBb+8+3jdI/abkmSG1e2hg5sjSKR2BM5FjdszeGAR4IOkDUTrOqqBVUvTfSZaWfAVG1sdjqyXIZjN0lbLJSTyyCohpYKhIcXDi6en8lQJKidZTrklCtCmhQbn3k09oFv49wmnXwo4jGoYCoLEVYuTg0FMAcTWvXEqLc/G2WbYbOwkN5cXgnYxsSCqqwWNYlXUctXLNTSKCpqD1fy7szksd2pvjaVSxpIcltKbJTU2QgnIOf29m8djqCmqaY6JBJDLuGR5FJVleJfowBWKveiyjueXdtv4Yi7w3KgtHTUIZEfXpOcHSPl+XXQL+7W5wm5e93efOTt0vooLPeNhk8OHcW02x3KyureS0eaNyoaWJXnVciQGRlQhn6tq3HFW7lhyW3qOsbAS1GJkjXcMQosm+LytRGwglpsVkWSJqjHTpDPA89PJG8kbrIkZC+XHTblg20QbjNCbiPxc29GTXEp7z4qgijLqVgrYDKasKgdjebJ955tu9z5V2vcl2S9SyDwbwt3bzGHcri3b6KI7ZM6SrJHcCK7tpJresgtZlRIjIsra/HbO0sttff+6dtyPFnN10mby9fuTdE8NJQtkhl/Dl6bKLj5pjjtviamrDVN4TenVtQmCIbZj7BuUW57ZYX71js5oY/AgUlgvbRkLAAyaSNOcE1xnr5vPd/kO+9vvcPnbkMyLeb9tO731pfbkyrEZ/DmYJOIWdktllQeKApJUMP1CBXo1Hxb3lkOtcmtDl9o4+qq6vduOqajsujyU89fltt5bCVKJidHg8G5ttpmKE5WKuoVlqYJKWopJn/wAsgdQxznsA5ksrm3hvWVDbsY7UqoVJ1aqyastGzITGyk0KsGVQVbqZ/ux+6+4+xfuFy/zLue0xzbT9fHbbrdxNrku9tukAljjQtGl2sEkP1du61VLqFBMx1R1uKpshSyxUs9LJTyU9dEr0qJNCs5Yvb/NehWjDM12L8aAF1AqBiXcWVxFqjuImSWJmWSqmg00Bq2c1xSmDSvn19DW1czbRuU897te4Ld2t1FZz2yxzIzP9THNKvhwPoKI1tF9SrVYzxmWRQFiqxDvk/wDGvZ/asOX7Ai3bj9l7v2mgo83kamN6bE1iwrrxqZynfTPRVkhmWSGpRmnWjlXUlSv2wjmLkXnXc+XpbDYm2qW62y6j8SBAVeRa11aCCFMYKkMGoAwZqr3A86/vR/di5C96tj5193G9xNp2Hn3Yb9tu3TcGW4g2yb6ZISY75JVmu49xCXEfgyW31CSoYLWGKcmOYE2pfjWtDmKfELQ5+ozf938ZRsm3MFvbG1NFkMhkqOhPYs1duGnolzG06KqgqPvafHU8ElNE5RgGiM/uXxzdBd2Et+s0a2iuWLNJA4GldRiOh2USUIoWYjgfXrm7uH3d925b5si5Hutt3Gfm6ZEtIbO2sN1tZnlllVIb9Y72yhuZrJipJjjt0m0tpKVFTaP0n0Fh+tMRSVeWf+M70mx81NX50+emmhir51rp6KjQiGWiSmmWNQwAmaSBZHYkRLDjnzl7hX3Mcwt7VBDtUcmtEIDM5Xg0hypHnp+HNDqpU9oPu5fc55O9j9quL7fL398e4l5YyWF7uKF4obeKfUJ4Nu0MssYcHQ10Ss8iAaFt1eSNxZ3xvLb3XG0s3u/cdbBjMPhKKorqmomF1aT/AHVEEVo3nnqql0jjjQ+SaV1ijDSOiMD9q2zcOYt1tdus0L3czhR5AA8SaA0VRUnGBU8Osh+c+ceR/ZnkPd+buZrhbLlLabYSS6KGVwqhI4YQ7VmupiBHGGaruQXYKHca7PavbGZ7T3dnd45bHLBUZusqpooPuVrHoaCBYVx9FCn2sGPaioqSMa3FNeaVpZCVLjTmrsXLtrsW32W2W1wfCgRU4EAkk6iTqLBnYk01ADAp5dfMT7te7G/e7XPHNXuDzDYqu47rdSTaQ/ieFCioltBHqBUwW1uiRKxDMyrVmrno8vwao8fQ9o7nqVqGePcPXuGr8VeSd6qWro92bLps1FkGq3mkVaWRyViU6gXBJUJoMbe6sk8nKQUgVjuNL8KUo+nTSgqTxPoPz6zV/u8oNvtvvKbdJG7aLnY7yWDjUyCzdZhJqJIC+SihzXFCptqmVJGihmpxPFIzNdkWWOKWnMM0JkVgdJZiTG/0Dxm5BK6sYo9SrJKk2lxQUBoSGqDT1A4Eeh8xWncy9NrcXFrtt7tjT28oMokaNZIUeJkZA9SSkhPdGdOmqHvV9CtRD3BgsFn/AJE74jld66RczR+WgnqTTNFNR4TFPK7xRVsdRLSGRx4jGLuQAbEMPeYGyXd9a8qbIAmiM2sYEgFahlpSukgNjNeHXzoe+uz7HvX3m/epWkaa4Xm3dC1u7ldLx3crElRIGaMkjTpHcccQR1MqOuKvs5I6qPCJicttysnoTGuXpaOsnpJ0mTGZmFqE/b4uNZ2gmP3EY8KwkAMnJNra8Taxp8fXDKK/CSKgZQ1BLHjwrWvr0AL7lG95+/WttqS33SxfwWUyxxuVZj4c/aQkSDtJL0CAVHb1aL0Tidw7d6x2ztrcO4ZqzLUuDrKGsztNi8bSJi8nNlcnFiPFTMKiKSWnwjQxLMyfbS/bKJVE8oWXHjn1LefmO9vbW0jMZ0TeCzvqkjVAHBowqFaMmikOA1RVQSvZz7p43XZPZLkjlfmfmDdEvYri82eG9tbW1aCznkmjuIPDkNvMsU91+9PDRrmO5t5XhC1hkYRz3f8A8p3or/Tt258hatv4oM71b8Te8t99e0+3K2IPldw53b9P1xhcfLPJRmbH100G7Kuqx89Kwkpq6mpprsUlhZz2v2m3v+a4HW4kV7S0kuZFKZZ1ZY2Q9xqNE5ocEMB20GQL/eFc57ly/wCwg2yfa7Wbbd95mtrS1uEnMyLbR2slxFNCfCh8CXxLcLJFSePRI7JORKqxUS/C7tGgpeq+z+pJcH1gampx+Y3bm+1s7DWbx3LXUufpE2/tvrLau1MjV0WGfc24dyrEomFRF9s9YaqSTywe5n5r2ywv5dkuprOZ7mO6Qo0DMhUKwLs7Lnw1SpIAJbA8+uLvKO/3ey7g8kFyGjIPiW8wqklC1aCoq1D68K/aGn+ZX8Ke9/hd0Xszs3cGzd27D637m7e756x6nyPZmxt49Udv7s6z6qyuwptlb+311zvHPZGu6+yO/wDD7zmGIwsn+5WOmwldUTCSJIKuSRFjdpowyfpkk0p5D1x51A6Ct/eW5tL17IqjDSaBw1A5oEViwLsoHEDgNRAzSm/F7Uzm+spgaraW0c62QrKAV1LV4mlGRpGrKHN0OCnr9xZbEVGNg2vR41Qa2ryEsMMsU88bSRCCaKo9szXENlFOlxeoFDUoxoQNOqiBtWsngF8xXNajow2nl7duab7bm2PYLqS6eIyI1ugkTUsyRM9xLG0a20cddbzMAULIWXQyydbDH8qj+RP8g/5jT9r1+G3NFhOqv41R7D7Z7l7FfMz7Nxu6cV/DMvXYjYO18N9nku0uydvQVsRTTXYvG4qgq5oKmspZqinSoK4VvNzlsZLZEhtISXVgoq2ocKmpofiIHEhST1IV/Ny5yHtvOO1b/dz7tzRuWi0uLd5HEUDwvrM9E0rJKjDwY3LUSOS4RUrkXG9wf8IrN9VOwKum6o/mFbd3VuTAU1Y2weu+zfj/ALi2V1wKqsNzT5Peu1+6Owt3YfQ7EpWtic48UYEIpzHp0CBLQxs8oceO2GcAAn+TAD7AM56hy9343sVtZNEy7XCWMFszs6R6skjKOzVwC7tRe3gABqcfIDpr5OfDDt3dXS/flNUdRdh7D3rnNvb+kaTcVXkX3ju0VuZ2tXbZ3TRYusw2W2rurYctJW4bIY+SameiVZKgxOY6cEdxb27yS2sluGkWMNoIQqY1ABOkmtQ3rjOK8TJdjue/Da7PfbfeWhsJrySOa6Q3AkW8nLuieKsekCSBe3QSRoPihCFQWDfyz/gl8i/mrm+zNi9XfHne3YPYu2a/r3ccfb+YyGy9l9Hdc5Csrcjm6uXujHbpwm78d2x/fvbODq6XG4/HZ2KqgyChq6KSJZaWNPHAl5pksyShqihD8NONe0aaaaCoUHyJBFTm83W65TEm2cxWoSVlF1MZ49Mk+taIyOsrCSperFWlZch1jdGC8v5XK9r7D/nQ/EKk6/ynbeT27XfLmPZ2QynXcCdebh3B1o3YsEVU268NHSx11L1rNtGlqMhurGU7PSVmCiqoyftmEjLLaaF5EEEi+KJUpSp7a0emnFSMZ4faOgzve1b3bWUl5u9pN9DLaTFtYVCGKq8BPiqHoHIYaMvgjtYE/UF+bncW9Pjx8PPk73z1zQYfKb56Y6L7N7Q2vjtwY+tymBrMtsXaWU3LTQZrH43I4iuqMU/8NP3Aiqqdli1HyJbUD66laG3mlQVZVJH+r06jDZ7SG+3Xb7K4YiCWZY2IIBoxpgnAPpXHWoB/Jn/nu/zLv5jP81XrrpzsHJ9bL8cc1tHtzcvY3X3XXVWIx+D2nt/anX+46jau5sfu3K5HL9i4+WTsqowVBUS1eZyVLL94sC0aNOKinK7S8ubi6hEkhC0NUUChx5kgtjyoRxzWlOhLu22bVZ7df/R24ZllUJcSM5fTqpRQGWOrA1YlDhe0CpI2Gv59/wAo2+JP8qb5Wdg47P4jBbt3ltbEdJbNXJxU1VWZXIdy7hxmxN0Uu2sfWJNSZDdWJ60yudy1Ek0c1PG+NM00ckMUiMs3SSZLGf6dkFww0p4gJUk8QaEHIr544+XRTytBZz75ZHcUmO3xkyTGAqHUKO1l1Ky1DlcEUPDFa9fI029LVb82vltqVdZS1UBGKmmz8FFRQLg6aKqWaOlyFPrgqaCpenxxjeVUFMusoA4j9QQuZBtd/bXaxsp71WFmJ1mlKoaUZQWqBXVippXE37JFLzdy5u/L808MsX6Mj36Rov0yB6hZhVZImKxaWagjGrTRguRaz2e2VsbD0NfUbgkxdTJhzHgsRgaKtqJMzTU1FNDTrUQtPS0lBiFlkSNJh4Gmkvb0K1ktpDuF/cGNbbWmuskkjCimvlglm4mmaAdDHe77lDlbaYb9t+a3uza6LO1sI5WM6iMgeJqeNIrcEhQ4Cs7E40g0LJsaqq8nuubcOfyNZjKDJnP5eoanpJ8vBXNGgqshSLQFcnWmB5YYtc3inMcMLMQ4iNhderHFAltbIpdNK5wR6GtAvAn8z5cese9ikl3Hdpt03i6ljtpvFmZkBkDEAll0d79zKo1UagBJDAUJhtmS0mf3rsKqnqMnV0mBaLeOE23Ubfrf7n0MWOooKzNZiryGZ2zh6nIYgQtS/YNap+2me4KRzgBHc6obWaNKAv8ApM6sNdTwAoxCkmtf846FmxRW1/ve2POHaCBfrooHib6cIqh5XdnhR3j06Sho1GNfhbo1/wDpLxP2mr+82f8AuPH9z4f4nJ4v4p/GvH/enz/xvy+T+Gf5R/EPH5PN+z4fH+97L/oDq/sItNa8B8NP7P4fg1fh4UzWuOhH/WG08P8A3LuvE+m+lpVqfH/uTXxK+LozqpWvbpp3dVqY/rqn2vvLdW0ex8hicLl8VsjN1GIirshSvin3DX4qNcTS11Wpkakalp8jJWQBYzJNPBD41ZJkcn/1/wBVaWl5YRs8Mkq6qA105qafOgBr5E+nUcDlFNg5h5h5d5wnjtd0tLCYwpIymM3DIvho7gnSFV2kQgEsyoANLhuglhrK3DyZCGknC/eUktBLOkTqJ6GpaOQyU/3MMVRDHWQKLMURzDIQQAxHsyeOOcRs4rpbUB8xUUNPQ9AaK5uLBrlIXp4kZjLUOVahqtQCNQ4GlaE8K9Wa/wAubZkmRxXbu6Kp8NVYta3Zm2DgKuroRlc29ZTbprclJRUFfNS009FiqJUadnmjctMiQCWdkjaEverdja2+x2UJljuPFa4FwgbShVSqgsgLBmJNMUwSxCgkdMv7s3ldNz5r91Nxv9rh3HaLjZI9pl25kgnaVJNy26WeWS3uHjja0gjUeMxYsutdCO1F6tB3ZiqySiSqxKYameCejqcr93imqaipxmIp8lU0lFipabLYdMfllyclOtNUSGeCnjMoMMmtdOOW23cUcrRzPNQhhEUfSFd9KszjS5ZNGrUBQt29wz12h5r5b3zfl2Oa1sdquL0XUEm8W93bCf6+0tXa6jsoXkli0SG7CtE87vBCzSStEzUrQZvWm26e3O3qbcuLqBNVdob8jkqXCCahp6rclXFE80U7RpTGgmlaR2ikMshIj/pfMZDuP7u2U7ffKsSWsWPJiq54VJDAAUIoOPXzHyw8vLzHzjHzBtLvPLut1WTGqNHkIU0agUxsWYlW1NhcUHTztLD4HC7hzdDiNj1+Sysub/hkMNTnqymmxl8itXTUVNTRUU8lTRxRwwgpVF5p3YIzKVb23eRbjuVvai63FBEq6m0IKN2kFyScHJyKAcQOl+yXPLfLu67zFt/KEs15NOYoVluHVof1QyRqojJdBpAKyEs2NTVHSgg7DG2s3ms3ksTitw1MdXQ7U3DQ0NVm9vVWHyDTNRzUmYgy+LUSZaSqpahqaHGzya4aad5Zo2iBZDdcrQ3FpDb291JEFrPG5VXBFK9tGGKUrWlCRgg4Ee1+5lxtG6bvvW6bPbX0sy/uy7tkeW3aJ2Ph0m8SE1kJViqwsahJCzoyCt1OA27kKWjghgqRR0FbM9VUh6/L1+QelqaauWqanyk+QSrbLZmpqlrKqqm1ywySmNGcxQzLizuO52k7mURM9wsaoWYKo8QMpqyAMCigaFWoFBUgVK9fQdyb7X7ryxDf8uXO9iz2Ybne3FvttpPcXPhWMsU0UMVpezPb3NtdRXNw13cXCxM0zyiIyElpeq0P5i8spyfSxzFN/DjS0m+3ji8UNdTzQpktuS0cMsUM6xpLJTKv3KKWijmkKo0ifue5v9lYwLfmr6SYS6zbrUEoR2ygkEitAfhOCQKkKcdcxf7za9lutw9ixv2xy7bJF++ZW1rFNHOXk26QHVEygyMKG4WhWOaQoklwg8dii4vsqbY2b2rkMdPQ5n+6WdxG89s5qHJVtNLl6XHRJj6vFVi/5BkcbLk8lDUS1QqAJyWKxnxaGkkcbGu4294txA8X1Mb21zBpHYXJNVZSykLGQqlcCgJzUDAq358n5L33lvcNlvbS8m2m9tt42q/J1rJ9PoHhzQyiMjxLiNnlSdNTVK/2dNV8mwewdnb9w+O3HsrKU+Uw9cuTiSoemhxck1PiMg+Mqa77GNZoYZo56MLKIpnp1FlWSVTC7Ymb5sO6bNdX1hukLfUI6EMNT1LglRqNDRwSRUVJBwCGA+jD2093uRvc7l7kfmvkjcI4eXZrW5jNmZ0gjt1t0iFwghK/4x9BKiQgoVEUU6zkeFNEWB3vzpDaHyJjk2zl8mMHuTA0NFldtZamgaXJY05Za6KakqqSoIo6+gqJKRZpYYKiF6gxopaMxCX2JeTOa9z5JjS/trRp9snlaG4Q0CMyBSpRwC6uA1BqBFK0rXthn7x33feTfvNvecrcxbzbbNzvtm1xbxs12PE+straeWaGUX1o7i3msJLiBxJJE6zRSCIuUTQl3Sl2P0lu/reuxNPJ49zY3cn3q4HO7fxG45MRkzRVtTTyQUWRyuCx9FW1qiiaVhQzVSLCQ3kKOpbKjZeY7He47hlR4LiAr4sEzR+ImtQyl0jkdkBDYDhWqDVQR1wV90PZvf8A2u3La7OTdrLedqv1mFpu20R3rWEzwTyQTR291d2VpFdNG0WoyWrTwFHRkmYN1ZJ8UvhXjtt1GB7S7Dqv4vmI4cZmdt7f+xyGNp8BXSUsFaKnJ02VpKPITZ7GVMojQNHCKGogdgrzeKWngr3I9057j67lvZI/Dgq0NxPUMXAJBVCrFQjAZ4lgaYFdXVf7lv3Dtk2e05O98Pda4N7vUiw7psmx+E8cNuCokgub9Z40lluA9HihCrEoEcrvMH8NLLR9vj4JpXk8UK3aV2J0pHxHHCiIAqQxppjjjReeBYsSTAo8e6kiiRS0poqKoyT8h5knJ8yeurDxbVtcN/uE3gwQDXd3VzOwAGgNI8000rYWNQTqdtMUY0rojRVWgP5id0nujtCrXDVqVOy9iwVOL26WqqURV0lRV0sWZzFChcvMMhUxwRokLyrJTUq1KhVeQjMr205WXlTl+FLmOm63bCS4IFdJCkohYDgi1ycB2Kg8Ovm+++97/L7/AHu9czbDOD7f7BC23bNllFwDIPqb7w5CG13cunSAiv8ASxW+tAUdukN8Z0qK3uPYFGs8whodxU2UjgWUpE0n3FBFUsy6Dq1U8IuCyBtC8kqEc751Cry1v0mkams5Ur5j9KQin59R191J5ZfvE+xdsJWESc37TMFBwSdwtFNceg/Og9KHY6kZCoR1V45VKtcB42VgAFKgMZPLqsAARa5NlBIwYiRmLFZAroNQqaHHp8/P/Bnr6hdzuorZLaGfb5riG5nW0dYo/FCCQMC8y/hgFNLtQhdQ1DTUilv58JBTd/4V1TRDT7D2s8wSM+GlpYcxuXzSGEFIWjSEBQhIVywB4AByi9omeTk241NVmu5qEnLMVjoKnNSfPyp88cJP7xqGC0+8TtSRQiO1j5d29QqCiRxpNeCoQUXSqjSFwDgcAAQx2Vj8bW1D0TA1EiKhpVZPFOstbGr02PrJJKcPSNLLFoAkRizLcBSwUj9A4AKgVHxelPUdYZRLYyGaKZiyldUJAodTAURjTHCmRx4Ur1aV0BW4/G4fcWJpZKurhxeSp6yWumgX7yGbLmmxVBh1CTy0tfPQwbceRph5KdI52N9EUkghL3T2t5rnaLlYkW4ljkj+KinR34PkXMrUBozFRShND1O/u9+e4tn5f9y9j3DcL1tos7+w3EWsUPjgQT+JDPeXAjX6lIrP6W38SWFvDRZtUySqoMY85inV8NlcdUJBXYqooo1VJpglbVVCJU1GSoamaaEzwpPTwqyqzPeSVxpiCqDFNncaNw2+5WsN5HcBqBWKqAyhSvcxajVqKVxgtU06I79stxdcs877MsX7x2G95bu7Np4rmzg+oluLWcM1xHDaW1lal4HiVbwSeGUKB4lCeJLSlgnn27LlMbkYzBmsLl58VkFaSGRhLTlsfVUshaXUsy1MLhpElsUXgtct7y6hlWdLeaJw0LqHQg4oe4EHgQRnh183Js7naLnfNr3O3e33Gzna1nilUB1lWsUiOGIZXR1KtQ+RFTnq57rWoVes9lzQlSG29h1jDKkQHlhgji1o0kUaK2scByR9BdrA4mczwmXm3fQRUG7mYgGmFZi2c0wPMdfRt7P7rabd7Ee1DSztbonK2yQxTvDJIpkuLC1SEJHFV5j4siqUQ/F2llFWBPP5jSTSdDbcM/j8i9r7XklFOj6FB2l2Oto1kYuRGHHLEE2vx9Pch+yDIObdz8IHQbCQKGIr/awcSAB/LrCr+9Ignb2Q9txdyq1xHzGnjPEpVWYWNyrOiFmKBidQUu2kdutqajSsaPI09Aa9Unix1a/2RmVykVUUdak07LdGnSOamVjdSgkjB+oHvKYPGz6D/aLmlOHlX+f7D1wmKzRxs6EiF+0kHDAENQ8K0IByKVAPp0Yn4s79qsF8h9kZnN5KprDuHITbcyNVkp6mtmyFRm6KTH4WGsqJFqZ5I2zv2QZnIUItmeNLuoP582sXvJu82tuChjh8ZBGAD+mRIQtOFQpGPXgeByQ+6fzsnLf3kvbHe9/a3ubW93IbXdybmDNEF3BGsvHlDGrm3acSipGUFWX4he5kc7LtbGLVbjQU01IlRNPX7QxlZVwVYpRDiqejkwhjqq+SqysmTiNPjoXrJxOY4Y3kkSKWXEa3sxuMki7a3ixt2iK7dVZK6pXdZNQULGIzqlOhSCSygEqPoSvN3h5ct9sn52QbTutoYbqbceX7e5ntL2RGg2+ws57WO1kvJLi+a8rBtkYuJYxFWC7dkVxTh8zdoR4Pu1N6ZOPOVW3exsNS5eorsrjjT08OeoqefHw4AtT0GLr0ocbT0GONaEVK0xSTBGaQA+8mvbC+Fxysm1w+Ct7YSmEpG9TpY6jIRrcd5Z9BqUJAIAXA4lffs5Zew9+bj3FuvrZ+TebrOPcLO9ltxHEWhiWBLRWW2tSDaxx2v1MOn6qASGGeWadTPKivj3j5Iq7HVkdK5qQlRV3rkkmxUcP3AgjqGWo10iSO0TE07Rv5xHrKsqqANNwZS8wJJWmntoDkAfEKGtccaj5dYocoW8rz2mlQGX9QeJUoKHiVao+ZFCD6EU6Pxgu7a3Yhk25n8fk59t1VZNRzZalmlpc1hppGrRWvTGikgr1qKGSpaQGmYS0bvrjUvFEiRlzJyTbbzJHuu2ypFu6KKagGilAA061ZXDAUFCQdQGk4NRnZ7O/ej3X212m49uef9nk3b2qnundlrIl7Yu7lrgWUsNxaywmaneI5UMLnxYiCZorgxFB3b1vvWgr8RtKqw+6spj6TH7kbA5CSpoZ8hPSVAydLWUhyGOqGq6igr8UnkPjaWhmWISqhMa+4c/qZvu3XsVzufjWsEjmHx4Ar6A4KHUI2oilWzmhUkA166M3f3ovajnjl6bl/ka72HmK/sdrW/ba98aa2hkFkqzxwWz7lbiS8uvFTw4CI2mS5VbiQBCZAVvY256zeXyLxe46+syG11yXVNDvPE5P+K1uUyuW2RSbrw8+HSjTcFbuTA7S29uWhymRmkxtHSw1tPAJZppI6uqlEUm7zYwbRyPdbVt1oLoreGzlQR0WOVo+9j4SRSStGyoA7VDNppVQAcGfa7mHc/cr71eze4PO3M8OwG72NuZrS9muk/wAftYLnVaWpF9e3FlYRXgEiG1jaPwIg47HYlTMb8+WPSuwaHJM+8MTnMpjKCsnTEYKtpa6qq6jHz0VFVYmmSGoWgizNNUV6MaOolpZmiWRlOlL+4v2b2z5r3iWISbc9vbvIA01wrKQDXJUjXQgGjU01wSOs/vcz77H3d/a+xu3TnmDet9htqxbLsEkN0pYLUKb1P8SQglUcLPLJGDqFs9G6qk7Z+SWa763BTrn8rRbY2nRiolw2JoYp6uXD1sMf+TZnL1FbT46kylROkxpxGjKsAuYgJJJZJ8gdj5HteUNvpt1k1xuLaRNI5C+IPxKukuyAcR+WqtOuOPvV96Pmj7yHNQl5p3eLa+SbdpX2varYPJHZGgCTStIsQup5AdMjtQ1qIRHHpjAAVlGlDl8XT01JNvDTT0uTzGHkxD0Bkirp4JIYoKihcZN2qxWRsdK6UkZAwlUFQM7RjLbzSSUt6sY4nDluAIyD2ilDT18qHrG3dols9x2+3tg24jw1nubd4BHUO6sArIfEYPVScYbjqA6NL8Z95bX6p7Syu8d8ZaqxW3m2vm9n0Dy7Qr6mSObFbj2znAtU21YNxRVtBT4qgkH3ZqJ5WRAtzEFf2D+fNqv9/wCXDtW0wrJemaOU0lVa4YEgyFaNU1p5fbg5MfdF9w+T/aH3zs/cD3C3SW15Wi2zdNv1/RSTlWe3dYlaO2EniISwXVq4UqwTuFhFf80ehqCWrq6Dej7hqI4ceJqLD4jeNVDLJUU8kkVNSSV2GoMTRzTgAySaykUkZSQqSzLCS+0/NckKQ3FtDAgLFGkdAeIqW0Bnag4A0OajhQ9Ppv7wf7uG3bhPfbXu+/X9xMIBerBt7uG0RSiNYRPuUdvbFpHDMY0IoHEpZtDR1Qbu3dtjeHfG5N9YzIZCk27V5qCtocusP21TK9PSUsNPSfatIecnPSMEE1maIm8YINshbSxvbDljbdqmjRrmOBYnTJHaKM4JANB8h6VOadceefOc+W+effz3E9yNqnubfl/c9+vN1tZ3CLMqT3DzRQvGsjp4jhgDVmAoaV06jsS/yTvidhf5iXdm59g9VbZrchnNnbK3nkvkV2nmNybm271hUbEyOHwmB6U2Uhw3WuXrMFu+HtNMhnTEmcnTdWJoJqZIIIsdV1UyQcv3V2tvaXMTCEEyAM9FWowRQV1V9fLgFpkQS+7WzcvTbjzDy/fW7706Q25mS2ZpZHjY69XjEwiAxVoEqdR7mkGkoXb5uT9jfAT5Mb/+OW/KDZfamR2Jg9i4Hde4+ustisJt6Lsys2TtTJ7pxmLos3gdt5bJUuKqaynxL11SZZK2sxctTJH5KyQEK797fbfvclvH+8vAvLY6W1IzqyFahe1kPYST5cT8uskPaH76fOntNab7fnk9tw5a36l1B9JfRWtzBdxzSI04+rt7+MC4jZlZSjqNMOkqUIbZ/wD+Eigi35S/ObtTcOyKjA7t29mOm+r8NkZa2vlx2P2vU47eW5cptvA4nJ43G1uLSeopcZV1srxxmub7dhFGkSFxfyXsFvtH1lxb3gnjkVe8oniM5eRpXeRa6y5KgD8IQZJJPWL/AN5L3q3n3buthh3nluLarjb3a3is7Sa8+kgtIbWytbK0trO5kZbWK3WCSQsoDyy3MrOdAiRKx/8AhMH1N1V3F/My7rxPaWwMBuqt6L2TuHt7qjHZmXJZEdS7w2p3piKnFY2gxe7MNTV8ldsTce+5JY6xRBLT5ekp5xqsgQ2222d5dvNzLK0sCMCz6FMjCi+Iwj7O/LAACmrgKU6hLm2S3G57jebV9PHYXEhcQWhuGigEv6n0ym6Amb6cHwSzF6lCVkkBEjXdf8LEOnqPsP8Alg7C3uuOjmyvU3yj2HlRlAqGox+B3dsjsXaNdTRM7AJDk9z12EWUhWfTEAtr3B3eSGFI5hWoan5EH/V9vRDtECXclzbSHsMeocK6gygUr8ieGaE9fP0/l+fCXvX+Yh8p+ivgp1/u3c9BtXfe6KXc++KqFp8rtDqzYuEjlqOye2qna4zdFgK3Lbc2ulStAs01G+ayUkGPiqVkq4yyG2jspLxr9bKP94MDEJ9IL6OOnWQG0DiVBpWmM9He4T7tDtUOxyb1cHYoSLg2XiMIfEPaXEYLIJHOAxUk5JNBn60vaXbXxD/kvfBvZ9BWx1G2Oouo8JQ9e9XbGxpoKvfPZe86qHI5mTH0V1xlJmN8b1yy5DN5zJz+GJqmasrqhluQVN3d220Wgd1PhjtVVyST+z7T/wAUOmti2PfOf+YTaWsitfTVklmmYqiKManbJpwUAAkmgHWth/Ld/wCFNvc3yl/mV5Xr35Hbe2F1D8U9/U249h9Z7P2vNj8pF1fnqHHvvbb3Y/ZvaGbxtFuLdRq8PgK7E5OSmiw+FpBWxVhooI6GeSYuj3VmvrXXIRbyRtqSgAVq4NaEmgx8QGa0GABHdcnQRcvb8IYEbdLO9iCTh2JkiMbBlC61Qano6gIzDTo1GhZqV/8AhU18jfj/APMj57fG7sz489mYjfm3dudNYjpnJZ7B1mb2pmcHuTbPZm9t8zZLIYbfW0cBXQbbyuI7Eo6vbGdpDWYfckcVW9BUSima6iS+jninubeRHtDDUGjEtSvwgEEjPH51+wrsuX7uz3HaNqv4ZrfdxfBW/UjjEOrRQuzBlSQFCdLGuCCARn6Bv8sH4e9ZfAb4OdP9Q7OkaK20cZ2Z2tu7MyR0c+5+y927dxOT3zurJtPSYtcdjaMU0VDQxTRpLRYfHUsU7yzxzTyq9vhjgtEcLpZwJJK/xFRX7KAU/Lon5n3S73jeZlll8SKBmtbZVoaRLI5UCg7izMWJ82Yn0HWjZ/JZ3LUVP8+npk9G52lp+rdzZ35O4qapzsaZHJZrqem607U3Tt/GwUklPWLQbgrzt/GzS18NVTywiJo7PHJLHIFOXXUXCJRgzMdIYCtKEmp8jQU/y+XU/e8ENzPsVpPIYmEFnAk5jkJUuGWPsUalbvNSdQGmgCVz1t+f8KEPlTgfij/Kd+U+ZyVXiI8/3jtOT4ubIxmZkpI4M1mO+aWu2fumKn/iFVQ0M1bt/qmTcecSKWeFZhijGHDMvsX3zutrKI6+IQQoAJqacMBiKgcaGnGnWOuwxQy7tZ/UsBbK4aRmKAAVAqfEeNSASCQWWoxUV61JP+EbnU9fl/5g3yl7YqYKhaHrD4xVGyi61yijjy3ZvZmxazFrS48RtelnxXXOQYOJGZWVdR5A9lu0MJArClNFeFDUn8R41/ZTo95rtzZyT27ag4mC0rVKAHKgYAJAzUk+tMCzn/haP2w2H+MPwo6KbA0tRS9k/IHfHaU26ZMxWU9VhJel+vU2xDgoMHAkdNXwblTvJ5pa2SYPQnGJHHFIatnhUbvm3ChatWo/wcOB49IuVqJevMzUQaVb7CSa1FCPh8vXr5u6ZXIYDM19diMrXYysLVEcM+MdqUyxSVBWWnqDFOn+SyxpcqfIr8ah9bOJBFd2lvFPArxgKSHzQgVBFRxBPHFPLps7nf7Nu19fbZuU1vdPrVXtzoJVmIZH0sOxgMjIYUJHXLIbxzuVwi4LJVX38Iy4zUlfWa6vMVFVFiqPC0sNRk6p5qp6GhxlEkUMAKxoB9DZbPR2UEM/jxLpOjRpXCgFixoBQVLEknia9J7zmLdNw25dtvpzMgmE5lkq8rMsSQorSMWYxpFGqqlQqgCgx0KWxqzIzMadsLPS5jbzPPQTYSObFVVPW0CwfxCbMGOMUpqI42RXV3SRpm0OjBmX2WXUSiQNGxZSPxZwagUrkjHH7MmvR5tt3M0Xhyw6LmI1QxdhDKQWLgCgbOcg1rUcR0Mu3N0zZCryOX3hT1S0lHDNkcNRLTS40ZTJxLVxw7YrZsHTy1cWP3NmkpqYx0TRyQvUKHRlRIyheIpFpgrqqKkZoMVbu4lR3Z40pWhr0Ltv3Q39/JNvOYtDuiUKLJIAxjhIhXUqXEmmOiadOsGlFC9CV/e7s3777b/RX8aPL/ejx6v4D2N4vH/d7+L/AOjDy/3k0f3d+z9Hk1fxDzft/f6vR7QfS2Wmv73v/wCy0/FF/FTxv7L4/l8H9Dz6G31fM/1Phf1L5X1fUaK+Fd0r4HifRV+o+Gnbqr4urHi/h6rtzaVP8QeqrMtHnarKQUuZqsqk9bVPU1mXposhXJWVORgp6ufKUVdUSU9Y7BlarikKSSpplcawMhQqkZRUJTSQBQLgUAxQihHyIwOHWOm6JOLs3Fxfi6nuEW5ecM7FnlUO4dpFVzKkhZJCQQZFYqzrR2bIkWSWON5Y4EeREaeUSmKFWYK0sggjmmMcYNyER2sOATx7cclVZghYgVCilT8hUgVPzIHz6QxIskkaPKqKzAF2rRQT8R0hmoOJoCfQE46ut+Em5Nh4brXdW18Luag3fk9t7kdKenocfk8DVZ5Wp93VdDnFpMpj4nkxTrV6KKStanrP3mLQxpTzR+8e/dDbdx3Bdrv5bV7cyuvihirpCCqhtbxsQSgU6tPaBwY1Fesn3DubeWuWtw9xOV7He7HcBb7RcC0CW7Ld7pKl9bSW8G3wXKKfEunZTAskbTPpoYYiheMyL987C38u18J1Fm49wblqsBhM5vfHZ2kfF1O03haIb/xGR2zJmMNueBcWJZMdSTvG6y15SdoZKFkllitOT905dlvtw5kgMW3xyyQWrRFW8ckN4LJIUeOjCjtUdq1QHxAQM3+TPvBxfeO2Gz5M5O/dkXO+5XS39zYma6kOy7Ra7nbRmXdVQ2F21/cSKYEtrWqgzQzzyJaMzNSB2PkWyPafYsk1PU0VZk+xN91vgloqWTJJHUboykgoa6kVjS/xKjm0+QlzoZdHAVi2VdpFosbLSdUaQRKTU6a6FyDg6WFft4+g64I75dmff98EqmOeW/unAKrrC+M/a4BK+IppXNR8NMEkU9pyYzHR09Njs5RTHMAT1ktHTVsP8JraqPWtJNHXQUpo68zxOt0DQSylpElYsHbfisVJZDUHSAaZAwDgnBHrmmCB0usrSESpFFexlJQGLRhhoYjVpIYJRw2MVUmpDEdxd+sKnHLvP+G7pwlRo3/F9ttauqEqIt0w74wdZJXbWjx7YLLyJLNW5CRjTZKQxpNNOk804ge5S7grpb+JFKCkLB5AKaTG2kPUsOCj4hxwQBXoT8kT2f72n27d9sJl3OBobCVxJ9Qt7Fqe18MQSZaSTtR2opZ1d30E9XV42Nsfj8fHS07ZGpFJFCtVO8SVdZSwCKCCeepjpkhEj0ojfTKyylQQS7qxOG90y3VxdGS4Edt4hICKQgOT2oWqATUYFAT5Ajr6TbK3n5at9rt7XaZL3mk2yLdvfTpLfVpGZIZ71YhHM8FVBd2Txlj1xhz1U3/MpyuEyG6euKTHyU0mVxVJuumzXiEZnjaU7ZmoY6l4yzgrGXKJJpYKdQGh1ZsivYuzvrfa95muFYWkzxNDWtKgSByAcfw1IqPImoIHHv8AvTOaOU9+5z9sNt2i5hl5k221v4dxMfhsyxSSWr2qO6MzrR/qGWKQIwDeMqmKeOSQguOWjmzOOWopMhOs+KpaYU1LCkGQrI/4bTwShGqYcjTQfeU4eKmniiYozLIwupDS9I0gt5tLLiUnJqoOsmgpQkg8Qfy65r2qWx3GxEsUrI9ui6VGh2Xw1By2tU1LUIyg5NTwyP8A1F3xW/HrsbPUeLZcx11mUp/4zt2bw1FVRaMVHPRpS1lPT4eCbdWBeT+H1s6JDTZOaJ5DocU1TThfmblCDnHaLJrlmi3eE/pXCVHFgHwS36bgagMlRSmNStkP7G/eN3r7t/PfM6cvWltuXt3usSLuOyX6rLG4jiZ7XU3hQhruyeQxu4RY7g+IGUq6stqHWPyX6M3ZBgNu7b3ZT1G4NwtVx0+K3K+WiySmSoTI5OiqqvJpVvD9tWV5aCBHdJEQilEqQMUx833kDm+yubrcb2wIs4SGaa0EdMCgZI4wp4DLaRnL6Qeuwntp9737u/NPL20cl8pc4xne9xS5S12TmKS/BUhDGsF3e7rNdW4EoIIhF7Mgtw1tbeLKsUUpXO+aWXsvJddYeXaDbV2Pt7tzFdcGeDKVlVh8fRas7gDjIdsz0392aM0ONoqKsx2SqaJEmlzS0kYmWlqV9yJyi8PLW37vcpuAuN5udvO4qjqolc6RIGZxWQliWVowzUEZckax1hJ94kb576e4/ttyfu+xjZfbfZ+dByKbywL/ALpswl0LKcWtuRHZBYIBBOtw8cBdLqC1CGK1BJ3N09/9U9XYxId9di4tcxQK338EbUFVnshMJfAlTJgsHSmrnXISyK7S01GqAXkdYkDWiGz5I5l5gvZG2vYZUtJKNGZdaxxo2QA8pFdAxSpJHCvXSDmX7yfsT7Qcp7eOcveLbp95s1EVxFtslreX24XEKaJZpLPbzcLateOPGKyGBI2cRmRQrUqq+RfzS3L3DBV7X2dBW7P2BNT1FJXpNOgz24I5o5BKuQahqLY6gkhcU7U0ckyTqX8shjlNOmQPJHtfYcqvFuF/ItzveCrAdkfqE1DJ/pGhoBQDJPIr70v36uavfq23Hkjk60l2P2nMjiWN2H1u4KukxG+aOQrHEGUMttEWjDt+tLcFIihLvHUZefGUcFOJJhAYEOqKmaaGmDM7SVU3+ThYUiezliqItvovMnJptlupGeilq5qQCeGBnNR6dYJTeJuT7ZbRxBpFj0VwpYLxq57aChoamgx5ZNB8cMDj8Ruva+76rJtFjqTOisq5nx5kY46hovKQ1Myy1EEq108ZWSHysyAhTaSxC/NBuL/at3sooQbh7WWKNAw+NlKjuwM186AefDqffu5z7Lyn7r+1fOG8bl4Ww7fzJt+43twYmYpbWtzDNI/hqrSnQFqAiuzCoUEsAbfst8k+ksPlY6St339tkPsKmqp4BtvepoKqkFXTrUzwvHhlxrz0rko4aVJFLBiugqfeMsXtvzjPE5baV8MsCzNLAWBAag1aiwB40GCONSMdp92++993fl+SztIecZTdQxNHDHBt+4LCIi8QJ8KsUT6VUoDIdSMCYxGkkgkq/wDlV2FtDtXs2Dd+zc2MjQYra+JoWgEUlJWrkqDJZCsM7UWQFM9Tj4Eq4m8qgxmVdINwCZr5C2LceWtlO27hEvivMz+IhJUBlA06tIo9Qaj08+uW33wfd7kv3y90LXnfki7uv3Vb7Vb2fg3qRxTGWGad2kWNJZQ0OmRSGJB1AgqKAmb15LjuuYqqikShzWQyWzsWmMrqfb9DljjqzKnH5YtRT5SKOioMzVQkYwSVlVH9vJVGXSJAGAqmR7/wJNUkapMzMtSgbTqUBtOSte6gHdQDhg497LcWmzpcwB45pXijEb+CkpGrS7aDKAEc0EepmGmpNKmoHD/SluPpLem5K1NowZnDYA5M9k0aZrHUWQwlHRS0FHFV4jEZTLYqXOF8pkzTjSsqR000iLpkkWRCDf8AY9v5x2Sxs23Exyyuj2kulmBajHu04FUrxI7qHyockPZv3l5k+7R7ocwc22vKabhtdra3Fjv23pcw20ngkxGMwNKkjDwr5YZFKRP2oY6ASE9N25fnFFjKDAZ2n2LVZilrqearwVM+56THzR4/UmErDnUxceSoamrlECrHC8NUlFIq6j5BJGCGD2tVvqLMbwElJMcrNDqBWhZEjLNrjROJowLiuaUpJu+ff0mO5bZzT/rbSNbj6fc9vhtt2aFhuCzp9Zud9HBb/RXd9d/qxqDbeFaLIgWLVG4cm/Y/Z2N31vSDdO2cbhNh1G5MxM+T2bSz5atqMLWU8qUT1GXyM23MDjTUZtZGl0UIkQvGTUqJZH1SDsux3O07dHZ3d1JdGGMBbpgq66ksKKHc0QUU6uIyK9YX+6fuJsPP3Oe4c2cr8t2XLtvuNwJJNitnmlFtIsccc7GV4IEH1UoeZUjqsZYxkCgqebafyrz2NwGB21jNux/7h6DHbfGUyNU8MGRrKRKWmjrqeM0L1MFHPU3YBZqjWWuHNmHuPNz9s9mu7vcN0u724Bkkecqmig1VYgDSa44VyOs2uSfv9+5PL/LfKPJW0ch7BL9Bt1nsyXdz+8RJJHaxRW8TM0W4R6S3hgv4YCuSTpyQC0/Inv3fXZ2GOyMwm2kw2Lz8GfL4qky4rVr8bRZ2gxrTVFdWPE8VRS5eZmUQQtLLoY3IUk45M5T2bY7o7rZm4+oki8KkrJ8LMhYUVQBQqAKVoKjqGvvG/eZ9wvebZ7XkjmSx2ODY9uvjewDaobpSJRHPGGMt1cTTSiZZS7CTuLhSNNSCSOvopYEgrLE0tcXNNI8qSSM0UdO86yABGVo2qADdbXuATa/uWoJQ4ZD8aGjUFBxNKfs6wXvLdoyk9SYpMrqNW4AnV889QVaWnlSSOQxzROkkcsMnqjkQh0eOWJvS6MAQQbgj+vt7tkUgrVSKEEf4Qek3fDICrUkUghlINDxBBU8R8j0abJ/Jru7J4PbWQrt01qZmLOZF6PN02L2hHhstSTUWAxqUmXx9JiIsZT7m2tJt2JqaoqoJq/7LI31QweL7kGW/JfLNnJeQwbdGLV4QrRMZCw7nY6Szk+G/inUq0Wo8zWmQu8/eL9598j5f33dedNwfmO23J76DcYjCviS+HaQrJKIolH19v9FEUnkD3BVlJYKqF0Bl+19/9gYep2tuzJZPc0dVLQQYQVuXnoIcRkYayKryFVDjsa2Mw2Xkq4o3jvXRTfaRuPG6udTGkOz7Ttc4vLC1igkpWQxxrV1oVUMxBYAEilCKkegI6BG7e5nuBzlssXLHNvM247ptcBK7fb313cPFZu8qyzyW8HirAHl0EPqUgAkjv0sDkdU4Cgwm2IKqXxCClpJKOoWnlNLFS1SpJIiTVaqoMtZJOZNEIAkBJD8lvaCZ3mkEZJDEhqnNRXNBXy9Tw6Ptkgi22z+pSRWfS0elCR4f+mbz1eQX8j097324YKQzeKQLBHKY4GcQzs0FJLI8MzVVNUtLjaWBi5EaxGy/rIHN1kJHhk0YUz5GuP2np+6soiq31u3iW5Vu2uQQtSDUHUiD0A+2gr0SvKYibc0sNAjrQ1tKJHkxFUIDU/YPLBNS1tRBDBHPQUD00gbVPodkMTcl1BfjLWxMwjJDYDCtAaHA8if9n7eghLGdyEVkZAkiDuibTUrqBViKVVaEGpzwPnTqCdmJFGv2pTzxyMKufziQU+ldQeo1vTyBbFmjgVxJIQpAPv31ErGshqlOGPlkfP8A2ekv0McdfCcB6mrE19eNSDT0Wv8APpKbs+yipYkYpHlGYAxopWT7RVXxmcXEkZmSTWPINTg/4Cyvbkl11Knwh68K/L9nRVvEsKwsmulw3CnGmOPyIrx49PHV+xxuLdm3sbmqaYY/cGJyeQx6R1n21TkaSnnyeNmahWndqmcpU4yqRo7KbROxBQeq27XrQ2s7W7jxY3UMSKhcBhWuBxH/ABfA65G5XG7b9stpusD/AEV7bySQBX0tIqvLG3hhSWbuikUink1QRxNvPubZPTcT42fY24EFZSxvgqgx4PRlE2yK98zSy7prpqhJXxUo8ixRSSSJ91HZWd/EApHaXm5ssovYywJMg7seJTSdAp8XDh5eXHqf7nf+V/bqC5tJeUb0RTCMWMrC3Pim11C4Q3biSvhMajQxprFansCDyXdGxszurAfw/qvGbtoqGagrs3FubL5rbmRpoocVRwZaCi3ZsjL0FfgqWCuhSWOtp3WRm8iVaVIIkkMP3VfrZXQG6vA7giKSJUeh1kqfDmVlY6eIbHArp4CPNx9wOXtx3OwWDke1uvDKvcC6knhkFIY0dVuLSeNkCyKGV1AcsXE/ijuKH7UwW19mVtaMLh6mihr8hNVbbwtTTwRyUuNyBqWxtNLVu89fkV26jCleoqWasqXZyfCz3RRY/VXKxrd3WplSksgqAxFNRC/CuqlaDA+dOiDmyz2fZZ5ztO3PEkkmu1t3UAokmoxqzlmd/BroLOS7ZroJNOfx+2/VblzucqNvPTQ19PhKqrqoMrUU9VR0tcPGuMrZaSbHVE+SxVTlZCsiRyU1VRQguZ5LqHpzDKLeK0Sepi8QKmioJFMioICsB8irHFB0dezuzXG/7rvD7T4a3aWck8v1DI6I9QsTsjIxkhaVqNQpJGtW1tjV9VX/AITJ/GvaPx5/lG9BV2M2ftvAb87izHZvZPaGfw2qqyO8c0Ozt5bU2vkc1lZqiplnOM2Ht/HUlLTL4Y6GFPG0ZqTUzTiKwm+ptkuK111yeNASB6Dy9B9nUR8y7ZJsu8XWzyKBJbkI4U1GsqpYiueJ8ySAAKkAdajn/Cqz4d9j/H/5t7m+RG6p6LcHTHywlTdXXuSoaLF0023d4bZ27tjae+dmV8UsNHFHnKSN6auiqJJTDW0OQ1Dy1Rq0jJLi2kh3F9P+inWCK0xkg6amqmnl6GuDQfWW9Q7jyba2s7aksWEJhbQWUyV0uhfTiRaiheilXAXvFdgH/hHa+91+B/yGg3VjMXX4yX5NDIba7JpY8fT5Pd9MvUXXG3anb2Sp6a1dLT7Ii2zT/bVNSAZhknVb+JiVWxz2L/XW1lHoMUlZI6k6Wca6AkUzXVQVyfn0HOeLTeIZtlu94u1neezUwTKip4kMTGFWIX4iDGU1EaiEFa8SS/8A4Tn0Evbn84H+YF8isNuKspJtx5L5M9m76wU1Zj6+lfB98/IHEZjrPBUEU8c2RNTlVwtfm8rXidp4hQ4qlaOFJ38jW2NNcX887GkKrRT5uSasT8lNAKedekG/Wn0EENsWBoAdINQpatOBIqyoDQ5AIGKdGA/4Wb98ZbaXxZ+H/wAdqWgP8F7p7w3n2ZufM3do4sb0PtPE4ek27NTrIv3MeayvdkFaF0kiXEp6kFyV+6uRCiDiTX9n/F9J+XEU3EsrnsGlWqKjSSSfnXtFP8I6UX/CSj+XVS9TdE7r/mQ7pyOKqd1/KzbNV1j1btyhxdXBXbL6m647Gz2I3Zks9mauSAZHJ9nb62dRzQUcVO8FBjMDSTirmlyM1NQ62qFkhErvUmtBnGc/LiOlXNd9HPeLbQ24jCohc4yQp0kHjTS3mfPgPPXn/wCFOf8AMwre8f5m+7en9q7vi3x0H8S8avSuK23gK+FMMvbC02OzXdm6YMlVYyqnpd4YfetUNqV8UeqllXacIIsBJKm3Hb23KVwrBJY1Hhu2ojNajRqAoxGW448/I95Q5uPJsKCSH6jbrpybu2j8JH1IKRus5ikkVow5IQ1WpOoCuddvq/fHc++excZD1liKzI5/E0e7t417bfwW6shlMRsTauGzm6d/7n3dkOuqSLeK7Q2P1rjMhUZypx0UccW34KuWZDaQlttksYo3M3iMlACtaqaLnSh1CjGpNTUEYIHV29wOYdwuoTbfTxyCRnWTQBINUh0GWdBGxaJSqLoADKcqXJrfJ/K5/kl9ifzjd6Ybs3cvzU62kouk6/q7Bd19fb7bt/sXt7BdYUlDI2xMJs+g3IsGBz3XNft/Avg8XLT7qjpMWlJNAYIZKdaeRdZhtDxRsPC0gL5MBTSMLjFPl9vDoPb00Ynhu7pGN1rLvQakdixdgWdi5qW4moOcV1AfTG+bvT3Z/wAg/iH8jeiemN34DYHZfcPUm8uttr7y3OuWOB2/PvTFT4HI1+ROBimzMcYxFfUKr0yNMkjqy/S/tbcxtNBLElKsNOeFDx8jxHyPRJtV1HY7jZ3koJWJxIKCp1LlTTUtaNQkVFRio6pu/l0/8J1+r/gR8n9lfKmr+S2/O296deYDcFFtnBUew8H1ltup3FvHaOf2RuzO7ogptxbzrM3j6zC7hlko8fDLQikrFSWSepVRECTbeX12+4Wc3bSBa6FIpQEEAVJYkAGg/wAPl1JPOXuvd83bY+3HZILYy6TcSRsSZCCjlyoVEV3dAzEDT6KvRO/+FhOZqt1fDXono/C1fXeQzE3ccvfE2wsxmcxB21vOk6425k+v6GDqjaMW26jEb0xGJq+35K3dTQ5emzGIx1NBNDQVtDLkajHmG4TNGsaq4Uk5PmBwJHzz0BdjtPqGuHaIuAAFUiqs1QwVvMA6eNCKAjzA6K//AMItupJcTgv5gfcGUw09NWZbcPQPWOIr6uSSaamG28b2dujdWKp5bQo9OX3PhyVkiSRPCp0oXcMxtBVklKmqg0GKetceppnj9vRhzZFJBPbpKhWQipUnVgBdIDUBKipAwPsBr1WN/wAK+vk72P2T/MW2V8ecjsus23178UescRW7LyObyFdJjeyMh3Vg9ub03rv/AAsCU+NhocZFLR4/bBjjlqS9btqqd5W1LT0+r91eZoZNWkKANNOJoa56ps6PBbwXEIQuXLvrrSgqoGCCcivlgnB89O3Jo33866R5ZJNZji0uiyzt5DFCEC2jBey8A/4ezC2YGBG/CPM4wMVPRFfIRduoqZGoaDPcxrQUpjOMV/b1ARC97WHDtdmVVtGjSMAWIBaw4F7kkAXJHtSTT+X8zTpGqFhWnrnywKno8XUfVtTBs6jyWblxWMauycVVRPUzSJTrTz0yK/37U33M9RKiVWrTBHJNZFQhraCHrq4VpmZdRx9v2U4AV+fUobHsrrtiXEyRrVyyVNAaLVgTUliNQ4VNBT5dDPhtubSxeY2ruzsTaOM7M2PtvcdSua6tky1Xs3bm8sX4BV1cmUzMS5PP4LPw61DVVGsFRFJI62aKeVGKtxS+ubK+sNs3FrS+eP8ATu1UO0TE4IRuxxxw1Qfy6E1tY2cMdpvO6bdBcwBpIVsZarDJ+iT4r9xkEkbsrdpXNFNUdlJav717G/ifk/0ff7jP9J/8J+0/vRkPuP4B/dH7T/R/5f4rb/R//e//AC7T/wAq37fkv7Mvpbvw6fXnX9Nx0p8euvi8P7TTj0r5dE39ZuX/AKzX/U1fpf3lq8Px5tXhfS6Poq6/9wvqP1aU16O3xK93QUb6zGzOydzQt111jg+oZKxsvV5LBnsKSo2kskSVGUSLE5HsSpgrcBDSRCeCGnqctVtVKKaFNdSNVRrl/b912Pa7a23vmObdZoo0iF3JAiTSHCl5FtlEbM3aWKxoAdTUCmioudt35P533m0XkP27h5Zfwa3dvLuQlgkkht0MkiSXqwfTPLKk7+CsuhjJFBDEGjXxXTpXbmE3FmszU1MGPkqsPj8fU4fHZHKrHUTVzTxxTVtJRmOL+LvBImrxciMyrdGA1Ka3jTJGi6+011ECn2D5Y/bToK8vwWN1dTu0A1qE8GMtU6uBalBqyK8KAkdX1fyYMR8Ndp5rsPId7YA7e7Cbb9Zleuu5cNvzGz736k7S2LvLGVeQ67wPU2Zy+O2F26+45KfFTRwZehqoKCkgnmRnpp6qaMCc32MO92b2G43csUMTJPHKint0/DLqODqGtWUk1r5MFInb2v5k3/2v8bmblXaLC/h3O0vdk3va7srILmByj3Viywsl3AR4cLxTW7QyqaiOUq0g6JLv3deQ+K/Y9Z1vtc7Z7xoctuHc+Q3H2ZhsVUT7l3Rif41nafZuZ3nmcPLlNs5LPQTZdYpzFPXxpBFKsRLVUU5JbzlrbecDc7hNcX1rHCVS1jkIRQAEqYY3DOgYLU1A7mz8FBM/tx947m72C27b9h5d5Q2DdF3e2nbe7i4s5mvpoLgzgW+5XFvLbtKQ8kdO+qpCvhBPqZxMSX+DZTcGc3Ln6uP7iTcuTzWZr46aGekp45cnU1mVytLTwUQLwUsVTUuyRuyvaQItyLkbL2xwKoosaqnrXSAoJr50AH8+sVHWS4vb+djrluZJLhwO0DWWkcALSgDEkDjmg6WG19qYTF4ZauOrmOLNcUoaUmeo+4mevjjgyKwzQuweiDhlE37Y8bDUt2f267vK2thWQ5JxT/V/xfSvbbGzt4mInb6RWAjU6jqJagcAg/DWvdjBWo6ZuzabEZXBrFHRSGsw9NWCjnkrKmsE2Tp4ZmyNTJTTSQ01BFVyohEcwljjNxG7MyqaWYlt5HaWeqO9cCmlKjtqMn7RQ9X5mlsNwsoI7SwKTwRFdTSNJ4kwDB5NLUWMPUdp1KDWjHA6SWQ+VnyHlkqKFt+1FC8sFfjZ6bGYLbNFKI8hPSPLTtLSYZak1VI9DEtNJrM9HZhE0bSS600XIPJoCTHZ1dQQ6mZ5GAoGFQHcgBtRLYo5ozVIUgaXf3vfvLGW4htvdG8srmWJraVtqitbORlMiMitLaQRSM9uqLDbtqL2tvqtYGigeSJkH2V2j2j2tJt+p7EztduCOhfLR7cnqMNicUWWvrojlJYY8TQUEdXJPWU6I7OZCrR+MMAlgc7Nsmx7Clym0WUcBKp4ugk/Cp01ZiTgEn51LHJJMY+4Xud7ne6E21T+4XNF9uUcUszWIuQqohlMUcphiRUjSqwRRUUBVSGOFaJEirwSgqsJj1yFXP6qCkpRX0YqpaN5YPu6SnOMCQU7NK8cjfqDCO5kYt67tTULm4eKNRpZiVNK+tTkilfP7BQYHRRoaxtI552/UijVXWuk4KjRQDJU8PLiSck9Q9x7ho6/IJvNc1Nkt31Vb9vX4XNbWxNfi6WipcRT0EVS89f5sdW8AQwwNj9UQh8hcOELLrSCRYfpGiC2wFVdHIJJav4cj1rqzWlKdMbtulvPcrv67iZt/aTw5be4to3jCLEsasTJVGNO0IYqrp1Bq0oHUU0sDpLBI8MsUkc0UsTGOWKWI6o5I5FIeN0bkEEEHn8ezFlVgQwqCKEHgQeNR0EY5JInSSJysisGVlNCCMggjII8j1Kkrq6qrXyNVW1lRWtItTNXTVM8tY8sbIUlaqcyTeYOqhXJNmt7bEUMUQhiiVY/hVAABnjjApxr+fSlrq7ubp725upXuah3lZmLmlKEudRrUAAngadd1UFLFTUbw5AVdROZ5aimihmWKgUiEQxSVFQIXnrXbX5QkRhVFjKyyMzpFtCxZw0dKUFTTPH0rj0zXOQPP1xHCkMDx3et3LM0YBonw0BLaSXOdVF00C0diSEhgseLg2Vh6tPCgXsC/wBDYcAc3+nJ93IAzTz8v9jpNrY4JrimfT8+l717U4vEZyhzmabF/YU0lc7R10c2TlmjpKH/ACynpcPjxJUrkpo66NqKerNNQGWJw0w0PoQblHLNA0UVakjAoMlhSpOKYNQKnhjoUcpXFhYbnDfbj4P06iSokVpCQI21BY46t4h1KUZ9MdQasADQftpbMzeNpKfNVWbkq1kqDWZmlp8tNnqPH4XzvQyCXD4upqsuldLkaVWLVCU6SpJFIkTQ6POTPcwynwlQqUOmpWmo0rjABwfKuQQSSDQa2eybla253N7kSI360yRyiURx6zGfERGaSM61zrCagUZV0MhZb7uo6mDs2OgyUkFPjaXaGSrcZJNV0/8ADfDUV8CSyVZMjwY6opW9CIoFTIQ0koSGRS9IirWmsKQ2sBsUbA8sZB8/yz6Kd4hli5oeCWWNrf6dngJdWjCuagNlgrKSaD4q1JABr0gMBsfIUX3NRWwisyU2Qr5YJYGppZZcZVCOSF3nFNEkM9Rp1ltPjNgwW31vIRKwWOojAGDWlR6evRZBYy2MAkvBqumZgukivhsKg1A7dQoa8DxA6FXbezKJsnmhUz43Gy7d2xjsnS0eSXPUVfuKOu3HhduUGDwFft6gfF/dwioNdUxZKopqaampZLtIxjjkYnndGtUWCRxJIVZk00jCoz631MDpJXQNIZtTLgLqZV23bfGs83wBY4VbS5ILa3EahWTFQSCQxp61FesHZm5aLC1mUrt2Y+fKisrarNYvE47Hw5fA1GepZvusXDviizuVjlyuBlqQKurRpZyZFUMqxuUOoLbVDDFBLoAUoW1FGC0pRCgw2aCgH+DoQbzvgstz3K63i1ExaX6qCBUWeF5wwZBdpcSN4sBPfIHLkmlRpJHRV9x73bL19Wm4Nv0tNgK3F5ufCYOnpclCuDy+SjzGRocnjqyWpxmTrKZNz5aaYLVz1sCU87oInEcKKdWloEjVoJz9QGXXJVTrUaQQQNQFUUcApqOPE9Rvu/MP1t3cfvLa4htckM/01qizKtvK/iyI8TM8cjKlxKxAkeVQjEFGoihAUWHyUsGNr0pqlUrsocdipBSyGKuqqRY6iuWCWNS80mO+7pvKFV2RZ1vb0grZZ4g00NakJqfPCuAPSrZoKjh869Bm22+7aGyvjCwiefwYDpxIyANJQ8T4epNRoaBx6AE+u2sB99g8MKtp2FLS+OmdKXSqzUsECzTVk8MdPLUJI8hJTWY2k1sygaWAWmBXURSlc1P+Dj/qp1OezW0N7HaRyavEEdIyiUUFQKl2AUkVORUitSQMHoDe0KNqagyn8QMtFNT6Z4SKgTioq6nTCyr9s6K1PUksqvdjpF2+h9rrJUaWHQoI8uHD8/QZ6A3M/wBXbi9Fy2llJZgDUFjglSpyCeBB4cfPoKaDCfY1NDUJj33zJQYF8zlsNRxZB8bh8nlIpoMXi8r4oaaWWpx0aQ19atO0gm0tSuYzFUSovuJPFhkRZhbo76BLUBiq5ZlORn4VrTTXUK9oJFY2Qs7u1nksjuksVqZ5LVA5jjlkUiKOagUkxik0gQtrp4RKkSOq9rK3M7Q2zkqXcW1cDuDbW69k4rG7MytLtfa2Lkpa7H5Clr4KrcVRtpYcpR7lx2LORjqlrZpchNLpdpJIQs3tBa/TX03i2tzJHcR3DNOrPI6moK0jMnaUY6dOiiDhprUdC/d7jdNh2Y2u87NYXe0X2zwwbXPBbWUMieHKJQ919IBKt3GvjLJ9QzXD1DM7ReG/QIw1UctHj6XxRQy0OQkqUkMNZNDVJUrG1bPkH+8mEQokooAqU9MDJEzl21Iuo/aMapWLHuUKcgU40Ax5kniePUVLOXhtoFQAxyM4YBjXVTUW7jTSEHwqMVJz0ZXbe2cTAMdJNS5HNRz1FBOchha2nmTFVeTiRmz1ZR5KSsSbHyU1dII4YWjmLWfV5AUJHL4jtTUAAKFW4kDgMDjUDJHl0NbG2hjMRZGdWIpJEQdJYZejE9tCcKQfOta9WAbPp8TLi4qSJaZEVqtooJoaimXXLQRM6u1DQV9XTh6ezKTUPCXXkaiA5JcmeKTXpcx6VqVoadxp8TKDnBwDQ+nCV9tsNvuYVWGZI9xaZkRHqqshjDEEKrsKgsV7mq3lXBQO96ieSmi80lOMhVyS1czpLI6JDPPIqUc0tQxmOl47hJdUgU3Nv0+zOJAFAqTSgBNM44imP2dBq9nGto44ljBLHQgIABY9prkgEY1VNDn06I3tnbbY3ftG1LW1GempcrXZBYI6KCpzle70slJL95XqGq3etyJlVIn0xmMPM7qysoU3V9EICkhC6uytaLUGtAK0qBTP8hXoJbJtE/72imt1a4eKQyhFUNI9QR3NTUQzBqDzya4oFdlctRS09TTYx6OtrKOplhnp2cfc02er5p6akpqx4Xl8scMsViP03i1MdC8N6DpVmXsOQfUfKuD8vXrdxPE7SRxMvjhirKTlXrwaleFP28ei1UOLz+8twfY0yPX5uvirK0ibTTmWOgxtRlKiV3cRwU8EdBSM+t/HCka6mKICwPWlgtYPEY0hBA414tT/AAn/ACDoF2tjuG97j9JaxGW+ZXelKVEcbSOTwCqqISSaAKKtQVPTlWVWaoaTb8VBuESU2IgyslC2Pq41yGCr9ZOcp2bGVNbU09NVVUg+2qY5Ps6yCRJAySfcRxNhLcvPI8XdIyqdXBsDTQNQGg8uINR0sludyig22C33EmG2WR4vCbvhYk+KKxlmUM3wsDodSrYOoKpNyb2zu59m+PcW62zlYmRxi0gapIrxFFS1f3tFkKQmJ6qkQfayx1RVgJo2Q6mN0TWtrHb3X6NnoSh9KfIg+pzUV4GvRtvW/wC5bztAG7b611cq6aCzEvTSdSMCcqAVKtTipXjwRe066HGZiiykkThsRWUGWiraeoaGqoZaHI0csVRGh1pUpHIBqjCiQg3VgR7V3YcppVvjqmkgUNQfzB/Onr0H9olSG5ScpRoWWYSKSGUqykEDgQDxFK0rQ1oOjvbwweN3VSbZfbEebWv2zgc/NWblx+Ul8GTm3BPNLJWwI9BDJiY6vE1EMYgadpYaiNW0jyOgDVstxFJdGWWNoZGV449NCqqq4J1HWdQY1AAoaUNK9TJvc2239jsa7Za3KXtpDNHc3iSMVmkmkZi6jQpiUxMi6SxIZNWNTDpW/FyuSm33nOr9vYfH0dLNQukldJPgqdosYY4nzu4t1793jDtvG4LDYYUEdSXpmM/3dRHBBJ4bxki5v8KOxj3O7lkdo3DBY1ldiwqqokMGp5GYtShUilWIxUSf933eEt+Y9y5asNuEVk9vJqkQwq6xFVM81xe3IhWKC3VDKNB1mUoiGh0n69P8t7quk6O+BHxM67RaGnlxPR2xs1m3oqhJ6CbdO98XFvjd1bBVA6J48hurctZMHBYOZL6mvqI42RBHtG3DQygwq+lxQrqGrSRQUK1pSmOsbPci+O58/wDON4LhJg25Tqs0ZqsgSRkWRTVqhwoYGprWtT0RL/hRf8YMd8l/5UPyPqY9vS5/evx9xEHyO2GlNTrU1MFR1olRNvyPwiirZ6qlr+psjn4WhUAGZopGP7Q9ubnb/UWx0mjqwYGtKZzX5Uqf2dF3Km5/u3dlLprgmjeF46A6tQqgAIIqXCjhWhIGT0Vf+QT1TgPhB/IPqe86KkOFzPZuxvkB80N4xpVSVNPSV9LtOsxG35sZVutMRjJ+v+qcPWRIiRRwvUOE1czSUsfHjtJ5p7hpHYsy6lClVUaVXFT+GpJJOonyoBfeRZXG82dnZWMcEKiONxG7OHdzrkepoAKvpUKAAiqMmrGkH/hI7QV22/5hvyawmQrv462V+JWR3DSZnCVtDlNttSZPtPprN+CevhmM8uVpGz6wOGM0kNSlRDL4Xj8ftLtFwly8kio6/EtHUqe1tPA+RpUHgRQjB6U8wW7W1oI/EDoZUfUpx3Ix+2uc18+oH/CyzcmZy/y4+KmwK7OZl9nbY+Ntdvaj2/O8h2xjtybx7S3VhclmaWKmiDRZjPUPX+Pp62WeVYzSY6nVLHWS3vMkizwon8PCo+YJofl6dL+UYLaSxunnIH6lCxDUwFKAkYyxPEgUrnPW1P8AFuLd3xm/kH9VZnrrB5DI9hdcfyyIezdp7f2tQx47NVu/6j4+VfZNBj8bS0cMTfx+fdOQCtIkbVE9WWktJK5DG0IMVilD3COtR60r0GLwpcb7KCP0zcaKH0DaaenAfZ1rRf8ACfb+WX/Jx+c+xuys333gumPkR8nOs97Z/YtbtDbXbvdtDs/sPYWO2rseopfk7t/qnsrIbF7yaPeuZ3hXUORrMzj6LE0+YpHamxePkjpiqaxjiYykStqBppDEYHA0FD509Ol+83NwqwEWyaCAzSMgY6zWq1bUBjNOJPEmnW1B1T/JE/lP9Gbg6n3l1X8IenNo7z6N3tP2N1rveBd0ZDemF3lLW0GTpsvlt45rceS3LvBMLX42GbF02bqsjSYhwxooqfySajHwk7RmgNRk/aPPyp0Qi8uA0jqVDupUkKoNCCDSi4qCQaZI49VRfFD/AIULddfMj+cdtv4Q/GHonrXFdNVuV7e6u3X8nM5XSVu/e6cF0V1p2fvTr2Xqyl2vj8didvbBg3Xt/MVGKgzFbmhW4HJSVUMWJq5ZKVkouD9TDGsYCMD3YqQBUeeB/n8ujQ7ev7svZ5Z3M0JU6OCqzMFYZB1MR5gr8J+IdHl/nj/znsd/Jy6w6N3dR9OY3vXe/eW895bfwmxcp2FP1pBR7a2TteCu3FvFc/Bs7e5rmwW5Nzbfp5Md9pE1XBXyFaiFowxUSzCNkWhJatKCv/Fcei60szcpNJ4iqiadWo0414YPkD0VT+QP/PQ+RP8AOJ7G712/2H8der+otjfH7qfres3LurY25d1Zurz/AG7vrdW7qWljoqPO6qbCbPzG1ts1MlPj2krq2iqcbJI+Qqo6tIqSysxYAkEaanFD8sE+f+TpuRIRG5VWEgk0gFgwIoa5CgEg0yMUI6ol/wCFdn8yzs2r+VW0v5eHWu79kr1L1x17112X27jptg9f7k3lhu890Vu5M5iDQ783HiM3urrTI4bqOuwtRSSYKpwldNTbgq46qSekqI19or0lklBSsYWg9dR4EeeKiv8Al6N9npDJbyRylbgvqJGR4YwQ1cAmhI8xQHGOrNf+EZG/9u7i+F/y02lBPla/eWG+UVLvfcWVrIZWoa3Cb76w2phtueCvrKhslU5P+Lde5iarSaGMIk8Eis/mZY67YhjSaJlo4apGPMfLHW+YZjcy21wJdcbKQGOqpINSaMAwBqCK8eNKU61Gv58/dG6fkR/NS+bm7d+yRP8A6Me6N5dGbbwuLnONocfsfoTL13V+2HppcjX1n22Wya4N8rWzvKI5K6qqHiiiSRIFRTlnupSGGrVp9R6ZGa/s6NLdYIbK1V1YxrEHIqATqGrDcAatgngKdUhVe3q2vr5v4RQwsWBWGmFPJTB6JaKa2RiWpMlHJHURxMytFM7GRQVGpgPa2G4WONFmdq8a1qa1BofMfn8xw6KrixeWZvp4U1cKEEALpI1Cvaf9rWhAPEnpTbX2XV5OiqkoZ4qpoZGSop6mp/hrUubikRKKSnaWCRo5Eu5AdS0yKBoBIX2nnnZ5AxSi4ofVSMg5of24zmvS6w2xjCYopQ0hOVJ00kFKFaio/MGuMZoTtbN2Hkdt7YwSZTK0RhqoK3JGfISViJWT0FRJDlKRqySSZ6qCNkHgWT7aXQym5j0aS+WdHqYm1S6gjqtKrXgSBSg/LqStp2O5sljXc/07MxyTwyS+IqyFDR0D0OqlOFVNCKkCnSw3Fmq/C9eTYXduOxeIM80ec2rUY7yrkoYp6mGKnm3NDMQony8UUM0EL+WPxRqEspdfaCCJHvpbq2nJT+zlByvbw0+hUkg09TWtB0INz3CSDle22zfNvSKZP17CSIFXo5Go3APxiVQjJxUBQABVuiQ/xwebR/G8pb+KfcfZf5Zf+GfZfcf3i8Xh+1/vDr/3Iee/2Nv3NH3Hp9nGlNPwZp6+Wrh68Pz8606ij6qfXp+oamutKN/DXX6a692r4f8AbdA7kcxW7gWqLQ0UVHi6aaaipUp4oZKaCoyMCSzSSUNPTDM5mZaiNKivrhNVzwwLrlPiiCnAjSAxDWasQp9CQDTj8IxgLQVPDJ6Cs97c7istYo/DhQsihQCqlxqJ0geJIdQ1SSanKqKt2rRc9QY3flTV53I7E25hdyVVBRU9PW02Wp6SWSliyH3Xiq6GapqaF6eaMUj6tE66l4ZXH0bvTb0jW4dlUk5Bx+f/ABXS7luPdGmuX2qyinmChSkgqe6oGk1Whx6ivoeosHZfY2AyldSxVVTS11fV0MldjqzF46ctWxUi0cj0OOfGpR4+XJI3rkpoUnmXTqlc3ZqGztJo/EFKaTRlxg5z5mnoTT5DpyLmLfbCcwKzBmkRmjdVarKNJ0Lp0oX/AIlXUcVY8ehE6sx6Z/L2xTR7mztEkGTnlOPyhqlqZZIMbgNtYTN11Z9zElFKVeVGivLDGyQyMVDguvKwoPFjKRHAFVpgVLMAKVP5U8xToUcu2zbrculjKLm/UK5IWTXqZwsUELs+rtNDpoaiulq56NvmNoV0Wzp8lisbj0oJDkjUZD7ephdNdZUss8UsTVUcbUzqKeEanEShYyWIe5VFNF9S0LTkzY7Kg/hHAYr6n9vDob3+13S7XDcQ2MYtnEpWcoynSshWpywUq3auTQALWteglp8BUVVNi5Egjx1FA8piyOUrXp8YmOx81O8ldSUstJLNMfuikcl4Wl9DeJH4b2peQKTglhTtHHIwPTy+XRVb7XLeJAwdIbbuPjTOVQIjLVlFCxoxAIALGh0qSOgi3pvXD022cZW47EVVXLl2ygxFfkces+Llmgmejyc9fWvKfvs5S09VDPHECZqIzxeYKGCOYQWZmkKO4AWmsA9wqDSnHB9eB8iegtue8xWu329xBZMyyF1t5XT9NipAk1tjVIiuDQHUhZdVAQCXHJ5Kry9fVZOudJKyslM1Q8cMNOjyEAFlhp0ihjuB9FUC/s6iiSGNY0HaOH+HqPry7mvrmW7uCDM5q1AAOFOAwOHUmFMzlKSURvkq2j21jmq9Ciuq6bDY6fLU8MkiiJJoMVRyZbLqWdzFE1ROBqMsiq9G8CJwWVQ8raScAsdJpWtCxovDJp8hhTCu6X9vJ4Rnlt7GHxaL4jrBGZVBbAKxIZphUnSut+OtgCaCtx0MWI2/SVUFLWSCjiGQpVqYqlaeSSsqaeGeeCGN4xVQQ0juIpJD5HQWXUysAzExq2SKGg/Z1Jd/bJHBtivpMmjU4Vg1DrYDUF4MAtaE1ODTI6KrV0bQV81DA0lXpqDDTSLTVED1kbNammjpZ40qY/uo2VlRlDWYD2KUkDRiQkAUqcggeueGOopmgMdw8CVYhqL2kFq8O0ior6ddJTSeRadzBA80HmVp5IlUo8IqYAZHJWBpgq6SSps4uQp96aQBS4DEA0oAfWhwONK/Ph1pImZ1jJVWIqCxAHCoqSaCvzpx6iswYghFQaUXSpcglUVWc62c6pCNR5tcmwAsA4BTia/b/q8ummIJqFAwBQV9OOSePH/BQY68rFCSApJV19SI4s6MjEK6sAwDcH6qbEEEA+/EV68CVNRTgRkA8RTz/wBQ4jPUioSaTVXmk+3pauqqkhaKGVKITReGaekpZJC4Y0kdXFdNbMiSIW/UCdLQAJqqwA48ftP206ckDtWfwtMbsaEAhaihKiv8IYY8gR69CDsDAHMy5ui+waWqSjgmpcpHVU1M+KqYZpHpVVq4xwRrkMrFBStUBkMROkSKshPstv59Kw6W7TWqnzFPl8jWn8uhPy1twu5LyN4P1AEKyVA0HUaZbtGpwF1YpkAip6HjEVORg3VBh4a6COrONxxyePzk9UMjFRz0/wB3kaGljxVVDW5EinaMWaaeFlJu8gj/AHCpVUgnJStAQMavkTw9eFeheJLqG/8Ap/GEcxhHixysQ3hsKstEIL1BApUg+rUyLEs9PuF8pHkabIYutxeZyWFrEy1FRQ0GZippYnoMphvFFGs8Vdj1USxLGbA/qJszXZCNABBUio4/OoNenIZ47r6szRlXEpiJcKAQNJVkA41AINB6Zr0I2C23T0mFlrq+IxzVPgqKeE6DGHUN4RFACGlikQAqbqFsf639tA9/aMZFf8P2dGMsJS2QzBvFbQ2k4FCOwr/FqX/efPj03zUjPHHQvG0pV4zLJHLPHRu3haaSiqXMp8XijCiZtPoYgaXa5DjAKzvXiOH+XrcYa5gtrUQgOrGrliAeLFSTwoOOOPkT0D/YmUmx+38pnzjoI8SawUKTTUzRTSR1MkSmrVYpMpGs9fBNIkOu2jxxhwp1u240MhWBT+pQ/wCD8sf6qeXRXus5gjuty8ClgX8NWZSD3HjSsncVJAGaUFfM9FTy2cgl2BtfEhsVXVuL3lu6qp6yTzTZijxc2K2YaaglhmmSCTCVdas8qCelP+UxzeNgrTK5hb2jruF1dF5FjeCNDFjRqDSkuKVIehAw1KUrU0IDe6b9bT8lbDsa2Vm95bbre3IvqOboxSwWCrBJV/Da2V4mdNUWrxGl0tpLKcFPvKszu5MTXbzrp62gpWo6SKOlhpqCmw1FRo0dHTYSgx8VHQYPH0xb/NUkUSopZ41EwRwoa0jihcW6UbJOSS1cnUTUsT8/s4EjoofmC+3TcLe43m4MkahURQqokSqCEWKNAkcKLU9qKqipIGqh6OVs7fG2FxE+Qmps8MZQLJTU+KqUxGKyEmRip5p4KOeI1UsFG1NPOHjeeUwtSxxu3jbSoIbmCQ/poyfEO7JFPOnDyxjgfXqUuXt82q1U3V0lwYlidUioiMZdJ0A5YAK7BgWqCoB7TpAD7szBU+WxX3ZpK6sqqugmy1PPixT5eihf+Iw0OMpkpKaRq2tqZYJ5VQyPGuiLXplCsVct5mWYBMAHSfw18+JGB9nRfve2pLYieQNJPLGZlaPTIq9+lRpBLM2DQNTgCAw6AWs7d7Uaormqt87gNdW47bOCytcmR/3I5PCbL23jdobX29lcpAfvcpgMFtvD01HBQTyy0iRwLePUL+zSLatp8KMQ2EQhDvKihaAPK7SSSKKDS7u7MWADEsTXPQGj5x5v287hBb8wXUTXEcdvdmKQgzRQoiRwTOprNCixqPCctHVQStRXoTst2ttPe2z9646q6xhwme3Lno9x5LcOOz9QNi4HN5Kpgkq8xi9mHEmrwtfVTwS0tJBT5VMfT0tbMppnjhQKXw7Ve2V3ZPFuWqxhi8MRshMr0woaYsdQpkkoXZgDqqT0Mtz5/wCWt65Z36xuOSPC5mvrv6k3cV0RZQszIzyQ2Hga4paq6qFufAWOVl8DsQhH4rrEZzA5vdmP3dQTVeMyGPxuHx8uPyGRy+7d3V3hyTYumSj/AIlAqrj2dxPIGVqkGKRRCstXGsnv/BngtntyYnVmkYkKI0GBjixJxT8x5AhvZ+UjvGy7vva7vFHcQSxwWtvokkluriQhig0grGFjDNqNQW0qaLrkQx/WWc80yYSemw9TJgKz+HVdRRyQ5CjkqqDIssnjkxs01VVYapkicxVYAhqAwdbsTdC3eh06gCtQaUORUceBoeB4HHQj2oNa3UcE6QuYJvDejB0JR6NQpXXGSDRlwwyK16PXtWkwiPVy5OeOOnfFVAx2qrrVHng+xhg1QQqWFPT+LxOsskCilLEetgQGr17rTALYNqEoEoCimk6q5Pma1FKnVTy6mXb7e0je9+t8Hut3ezYykMGjChDoOVVSgXuKgRlsEnon3yW7BxeBky23MbkzPWUmOoaeKrpp1jqK4w5Cn/ZhmUzRJTA05chG8jwTSMjghdIh22N50jLx6Gbu0kHFfM8CD8jTOOoc5u3CPbmktYroSSKFV3RqgtUFkU1KlQQaEVqCSDwoQfIVNZu77WWiwldU5jGYevqdxVtCslatdSUNTV1zZqooqWiX+FwYvFypDUSF3iMcCyMUYuWPIo47EyCS4UQSSDw1fBDMANIYt3FmyAAMkgVxSP52ud/W3FltUr31tayPdPCC4aKMvIZmRUrGsMRo7EldKhmINSU1r8aSLHJqSVmQofIkgWMoySuqt4vWGIA1Pbm4/SfarTqKll7hmuCM8QPPH2Dy+Y6JtWhZFjkJRjSmQaDgSAaZrwqfP5Hp82/lt2UlVXUu1MjuGkrc7ha/b2Sp9vVeSgqszt6rpk/iuEr48dIs+RwtVSUgNRSya6d44/UmleGp7e0kWM3cMbIkglQyBSFcGqsKigYE4IzXzr0Z7Tue/WUt3FsN9dwTXVtJZ3C2byI01u6jxYZPDIMkLqlXjaqEDK0HULFw1KeXJw0tBWJjispp66SmfW4DSCWLFy1EU2VjpBH5JkWOaGOPmdfGeXJKN+n4hUn+H/PQ0r5cPl0httUVbrwY3VCMSEUJ44XUC9PMUIoe4UPWGc46SGkSmiqaWpippTXzVdfHWU9ZUamkh+wp6bGU8mPUxkKUklqLvcl1HpGxrBJOQTigpT7anPVHMJWIIrBwvcWYMCeI0gKNP2EnPn5dK7Y339BX0+aoIMhXLFVCir6PE4gZWuFNP9u0SMk8fgjhyZLxho2EwMZW6eRWKa7YMPCOgY1AuaDzB8uI8vtPp0abRHMjpcxLIx1+GyQprehAIoDijftwAOPViWyZKRcLnq2TeWIVKrLz4hZqTG0VJDtxJ4og1HloaLz1ORzsVMrSTyTFKlJZNGlFULGHXJ8Sn07Ht1ZOWpkUrQKCaUHD/LNMMaDblYb1DQTCEhFVBEXqD4mmpkkValmbuB7QABRQSpOvsZubumDaG6c7j9vTeWDP0/8AeDGR17Zv7CaM0uE+whrYqNjkaaqBBkmWmhoo53kSTQYzS6ubi3tZLq0t3lBop0ELQNWrEkE9tPIVJoBTiEXLnLdju3ONvsW+7vDt7K/jarqMyBzGVIjCAhSXVs6mCCPWW1AaW+nh/O37V7T+Df8AIwzGz+r9oSndNd1J1V8Vc1NhUFZQdbbTy+wDtremVAx1OtDJRyYPbs+3qSTzUcMdXl6eWJpJEippzW5DWG1WVm1XUqltJI5JoNGksxNSakU8zVqnoF7N/wAiTnDf98h0xXSNcbvb28MagO6y+L4UaDw40CKzSUAACRlVWtB0vv8AhP8A/wAyDFfzRv5d+C/0m01Hke7OkqSh+PvyL21uSuh3PUb0NHtemg292RnKXLtV1uSxPcO09claa+LTUZmly0AEkUIdjK0ZPBWATeIUUKWP4sUqeNa0yfMg9BTeEl+tk3D6IWyXDtKsSVCxktUovAqFqCo4qpUHPR3PkB1N1b8Xf5VPfHSm2Nv1ld030L8B+3OvsVtuaR58pldgdedAbjwqY6tqcdBBLV5jL4TFlaiaGJHmqZWdUUsALzgpazBWFRG1C/Dgct/l6T2cqvulpNKKIZ0JCeQ1DCg14DAHWnR/wlyyFBmv5pvYuI23t7eGwqHrb+X1n8NvDb1fSZTEbeyW7anuPpWaWXG0WQrXnaKRcsamsilpqYjLiaVIwjKfYK5Fgvo7W8uLy+jn8a4lkjdWDNo1BVVyBQU09oq1FoK46HXP11BPJGIbZo1XRp7FSNkcNIhj0UVtIJViFGeJJqeiy/8ACpntja2//wCY9vzY7UNRmst1XsfpbYcW4p87NPg8ZTSbQzW/8jsg4Cnyc+HDYyv7LfJGplhgykdRVVUJtThDIYbqss+5qY5QFiShWg1Zo1VNK0PA5pUevBnlsxWW3pJcxloriq6D8AOogOw/iArjjTIIHH6GPVuE6f7f+JXXO3NpLUZ3oHtD467Qwm2EK5Lb1Xmend7da4+gwqlaaShy+DqcjsrJxC0bQ1NK7+kq6ggToFlt1BUhGQYODQjhjgegNK81tfySah9RHMTUZGpW45GRUeY6+SHsr+WT8tezP5ju+Pgt8UMNuqXuTqPvzs7YNN2Quel25i+t6PqXc2UoazsneHZOHkgi2rjcJjaCGpkqaEvWVFRURUmNgqKyppaWYOQNov8A6QFTcgFvDJFSoNCaZwPXhWnE46G98g/di34DrZt2+KAaVIDBa4Oog5APCvAVI+kt2v1/n/5bf8hTsvq3c27MX2hu747fA3emxs9uzJVWawuJ3hu6t2HksFlK2CohlTckdJVbh3A60N5YK+oAiDywyyM6H09YbOYgDUFOPKp8h+3HQVsSt5vNoWZtHiKSxyxCAZPHJC1PH8+tOr/hHx0xQbw/mM747LrKE1dJ0r8eOxs/hs29LFLGN2bx3Psvr6gmjrI3ZEq67Z+5s0PJxJIodSoJf2T2DibcqMaMkWrTnHBaZ4Urw/Z0LN5gNnyy7xKDFNdiHxMd4UGSoPnkAk/POegK/wCFd3yV7l7X/mp5H45btkTF9SfGTr/r7HdOYqOikEeQm7Y2Bsrsvf8A2A81UJXkyeZ3FkI8HNJTPFTtS7Zp4zH5Y5XkNJSoe4mkUnwxpUVoKEAnzyftHpT16C9urGGwtYZFTxiZHagZtSMwUjtBVQBihydVcUHV33/CIqg2BT/GD5x12Okyjdp1XfHW9NvGOTFVEGEHXtF1/kX6ymxublIp8jkqjcVbuz7ulUB6OFaaR+KlLKo3V2enxACo/af29F08UkUMIahQsxUiufhFc+RABH29ab381Cgosz/NB/mC57B5rH79wuX+a3ygyVLnXSrrMRVLVdxbul+yo8mK9vuKbFOv2NI9J5qXx0yEAxsliWaZvFmDFgQ1BQ0xU0xTIzXJzXBHQoith9PZ+GFZTGGcsC3dpUMKk1BUilAKAjI63Kv+EXlI9H1r8/D5KoUtXvX47zQU9S6sEm/gHbyVEkPAf/KEiQsDcErcfU+1e2EUmFPT/L0X77E0cVmTWhZ+P2R560zfltsDeHU3yH+T+yezq2XOdt7O747a2nu3LVlS+Yl3FvvG9gbgx+48vJXrPoydRkc9HLVSVCzK83k1Elr+ylldJ9L/AD1D519fn9nQuLW7bf4sMS6ywMZOKqwwNPqKg4I6AqGkkpsrjEyNFjaupONf+H01PtmWi8lJSxqszEy5CShpZ5qjxyeXRFKF1hI3vc2Re0FMgNnNfX+X7ftz1fSFmjjuVRZWiAQCPTUCgrk6dROa0B40B4lRbbw9N5Nb09PSGiqfNHkqSkqlFTLkBF4GrxG6u9RQPqEUUglKFFl1KWt78wA1GmacPXpbZIP0VKrpST+1VTUFqUJIydNMD8/PocK7bJyNfHg81JV/wrFYmrr5lloaarx7ZSMxxR1sVNUM5oaqZKCNpkScrKXv6iF0lkMyLG08cYMzNQGtMcQCaZpU0x1Jm9bNdy30G03928e3wQCR1ZNa+JUIzqpNI2cIhYBjqPrUABPuvZleKRZpq3cFXNXS0+RrvtahIKuWlrNUdbnMOc/UVp8+HFOsbfc/btPqLLYCPUYRMr90YXBoR5ClKDH+T/D1Hm47ddRaYbpptDASBgcsCSrSJ4hOV0gdwWvHhSoMfb5L7X7v+PUHl/gn94PF5U0/wb+M/wAE0aP4L5P4h9p+94beHV67ePn3vWmqmpqV9P6Nf2V8/wCXRN9HdeB431EGr6bxtOvOnxfC0001107tPpmtM9FbnqlknrZYotCVkkrBZzHUywxPUJUIqztDGwnUoFaRQhZSRYBiCJY49CRJq+EAYxWgp+z5dRvNOsktzIsVPEYmhOrSCwYAGgyKUr5iuOji/Dihyj7x3FSUeTNPWDH1DT4CWmrgWqMdS10VNkK9v4fJTI9FJXypTxCRpzMW1R6QCxHvksRt0c5hK1DgihBK4Br54qeFPP0kj24guI90mjWUrciUaoCJAUMav+o40EdupgFqW1VqoHE0Pf8A0M2WwO3ctR4bGU+T3fg6cU9RHRGkoPDt2Cjq0p8rOBFUwVP3VRHBWGCfyp5fIbg6XINq3lJrq+tw58S2k7qkE0cmmn5EA6TT5eXUhczcmWs+0bbfWaprvA8TKVKhZINLNrJIKjU4BAbzrWmCG22utsbUdW0u3ZM9uinx8MK1We29VY6mo85VzzE1KYSXJx07zvtuYgLeiq4I6yFI2BtaxqbiRrzxTEuup0spOnBydJ/F9oxU9EMO02sPLyWIv5vp2RWngkjCzFiNSx+IAT4H+kcBwFNPICa9W9DtGCiooslRYunp8fi3+xM0SvRyxa1jp8VJ4RS1BWnQMxkmkST0F4mupYWBPG1NpZslQRwIwKtkkCuOHrno1mvpBYLFCskcKKkbMhxoIq1I8BWagJNWIPbVeHRduyo8rJjZKKoqKmkiraOtqKutrqKWqkTF+EzzU0ipkVq4P4jDI5nmEjpEsZjuJGUMrjdVcECrA0ouMjh5HgfKnQZ3aCZrdw7OsUqFxJKCSYyDUU1VGvizaiBw48WffXVeC3tv/AVuFzO3do9ZPhsDi6DGZ3d23dv1uFq1pYq3cu2tr/xOtyu4dw0mFyuVkq/u66khslT4i2kRTSpbDcriwsJo7uN5b9XZjIiMwZdXY70AVGZcUByRX5AX818jbBzZzTtV7yvf2u3ckvbWsC21/eW0ElvcGJXvLa28WV7m5ghuHaQSyRrpSQISaK7lZ3BX49a+iq9uw0WHoJ8UtMaPE1eRqJkSCqrKCokylRk2eokyeTal+8I4iRJ4hGkSqsaCOCKR4XS6q8mrVVwKVoCKaaCgrT50Na16gzc7qyW7tZ9qjSC2MARkt2kJGlmRi5lLMZJdPiHOka1CqgAVRGpnzdTsXF4HCR7mpsdn8njcl2Usu4KNf7z1FTuLJx7Kjhx80FNTrjsXTtJUq9W8j1NbUSTy2ggpGiLyIFv5ppvCMyLpgbR8HYA/dqJqxFKClAABUlqi2K6v25Wstp2n66OyupUl3lDcLpuXFxIbMCLQqeHCh1/qFy8js7EIkQQX48dXZSrraiSknx1bUZDF4+enqZRjKCWQZRq7I4ynrKKGlmy9Q+Luv3Wmno2q1jSlJjSQ+0iBKKGPEEihzwxWuBn8+Py6M7mCeWa4uTCyv4qxspAVa6yzqpUDWfD/ABUVNVAmAegqz2zMLS5WhyVLUrJ9/uSpxRUS1Ui4jIpNk8fTUuQkXIxZOSqTLUC6WSKGFVItNMoLssimnVXg4KErTBqDQ4NP4T518/PoN3u2WQmhvY31F59BoSPDYFkUONWonWo4ADhkgEkO62KTECv23uKoz+iLGSyYLHUmRiixFBuLIVuHlrZqmCpV8fU4eqixzq70rIXkjp3MjCEqVylnCTQqmoP3MwqSgqMEZ1UOK/PGeiBmigW7sr95yhiPgRxuFjSdmjJLKwKtGQpB00NdB1dtCmJcfGKYT01Ss5hpI6muWYQUSxtNVfbJFjlqapKzLeIsqzGOBTHIHsGjTyspWWr6WWgJotM+Vc0FBjIzkdFz2oERkjk1Mq6pAwCgVbSNGptUlDhqKKGvEDV01+3ukfSnyOQGQ27iUatxcD4yrqaVMHR0lVTVTeSjoEm3FUumPXFzyZGKjp6ZytT9wXpPI8R8hlZPHGY5ZTkhs6ia+vbxwBny8/lkwuLo3FnaxlkUREgRIKZKqDIe2hZwqg5r21pmvUzZmUOOyP3MkopqajhWapkDy09PPC1dRx/bZiSjpayvnxkjy2KQwyyF2QkaVujN5CJFABJZiAAc+VTpFQAaDzIHHzOVuyXZt59bELDGupzwBBZVAkKqzlKtwAJqQaEDBkNobiy1PuL+8+4PsqOGokwUkSpDUVFNU7aEUVZjJKeWspRPSU8lZVwmprXKmSOJ1KNd2BO4iUBIyagEEnBDVoeFcD0rg/s6HcF3em6e8v0RdZjZQtSph0hkKlhUAkir+YBwak9Cxu7M0VZnKiATQyuZpftaiDK09TQQzCVKT7WjpWUZENR1SJ9YkhkdpAttIPttWLaQT5Dj/wAX0Y3gtopWUKCauQyuGWtaAAaQ3afkAc0Ap0Je2MvDQYyjwLAz1dBTJNkXrlqFp4qg3qdMdJEDR1Xlp/JqjAS0Z03N0PuhDO7PXt4DTSp8q1pUZ+3oxQQxWsNo5pdKA8jSBtKkEOFCg6X7a1wuDTOOs+5KChixU1dTVamH7ypUxfbinQUtjIlWylpI4HqCHVY9WqJFuSLqQ+haoUpRgoJzXPmP5ceiy4McZkdJdVt4jBW06aitQdOdNa4FcdFl7Q3JTV+0IaGm+1rqjJ1dLRrLBk46fG0D5OmMFHkKzJVjfawUsUg9UssiI4ZXLIravbttGhlq3l3HiSaZoB5/Z0Ub9eyT2MNtHIulmVVOoKqlhpDMzGigeZJp54Br0WjP7IztNSZPcWLwOVyGzMHW47bWT3ljcLuBtox7mixeP+/oJM1kcZRxU2QqKuUyCCbxSkSAqmhkJObeZZFAJpIRr0EjUFYnSSATQGmPsI8ugXuOzXsCT31vaSSbRE62z3kccvgeMqJ4ieI6KAwZgSDQ5BpQivDC47B5LCTmeo/h2TpKmCJqmemyVRtuWjqqDc80tVnZ6OqkytBn6CopKZMctJR1NDUrMRUtAY3+5blklinU6QYSCMnur200AA1Bqa1IIpgEcE9vBa3NuELiO4XJejFCO80kySrCg0lQVNQG0mp6F+qpK/F09RiPBGY2xlXUV+aeagpYp6bb+ymqpkpquuEkUmYq6fHSuKZ5iKqpj8EL+SWNfZSxBYmlAWVQACfiYKBQfhBOacBngCQLo7e5kBgXT2QSSs7uiArBA0rd8hCmRljOla1kekaVdlUpmvz26dn0eKr8qMbm6DemDkyOMlyNDjKXP0mJevmpWkoqnHT1Vbtuvyc1MJpCHSomp1R7mGZWlcjjtryWeKNHSSGTS1CxUmnmCAGABoCKip9QQLXNxvPLtnYXN41tPa7naePFrEJmWLxSnaULvbSO8dSDodowrZjkUvk3k9DWNisDtKbIV+V3BmaOprqmopKah8mXgpof4PgI5q8qMLnttz5mpFUlHP4al69FlCSxafbO3pJ+teXcYWNAwQVqNJNGftH6iSBVoWGAtRUHp/mF7JY7TZNluHuLm4lR5pCgUmQKDFABLUwS27Sya/DekhkCuFdT0GCZDIYSEYeqjjp5sVuE1Vbia/HxSmWpgMEc1NkIZov8op6afHBZaWZgjMw9JOog8I8Ya0PYydrDBFfMGmMH8ugChexuVSeICWKYF45FDDtOVZDQMKihUkV4dHBwlRtGtWul6W3rFt/beSxuLO4Nnb2wUWPwuD3LDS1tM+cq9yZqbc9bjsPWFp6qqFLkautpaZlhkrZYYIigVdbxFQbxah7pCdEluxLMhI7Qg0gtgAVUAnIUEkdZC28vLt1LcR+23MYtdhvFiF1ZbtAscUFwAyeO9xK120ULamkfw5nkjQhHmkVFbrJ1uuKrt/7ozAO36AS1LYE02y4qf+6CLtemTGz1W16uWo+6qcDuEwTVUFVVFKiYlpZnlkDzuqAMVtBEpckLqJm+Pv7u/AAYClQBQUoAAAAF3ktbzmne7x0s4o1l+nC7Vm0pbjwq2rMxd4ZdLMskjGR6+JKzuWdrJYY4JOsVqcI01fU0bfc0U6/ZyYetgmqKp46qgrKZJZJY5lrKf7Sr8iwXk4iYP5CD1kcbzHDLo8BlqcnWe1cEHA+FtS0JNK6hSnUpXkFudnvN7ilcylVgtxgoveTqRgaMD4gCtgVNaGtTSr3zuEZ7sTMWEypjZGoTBJHFClLPGT9xBAkU1RqjjksNTlZS1w4uPclWMeiLWGqG4flj/P1jHzHdG43GVGQhkJBHpXy8/l8+NepkW39szYLHUeMr6rau+xhauvz8VXUx14zuOzGIwGdwT4t6GKnx2NgyyZURLTRS/eQQxzJMkryJD7QyTzJIzTxLLZa6R+qlSykGuWIocnBPA4r0JY9s2ltts4rG7ls+ZPp2e6VmD+KkkcM0LRlAqRrIJANAOtQrBwxZU6RG66elnx+HrMXtY4pKdKmhz+Vgjy4Sq3AKiq10NfT1LtisNXQ0VD9wKKmVPHHM1y6qpC61ZlaRJbjVwKKaV04yDxYEmlfl5HHQd3iKOW3s57PZ/CVQyXEyCSjSipKOrVSJ1RC2heAJqWAB6R1JUVsJlhoqmen/AIhF9hUJDUtTrV08ssMhpaoiSNJKV5okYrJ6NSAn9NwqkWJgGlQEIdYqK0IrkfMfLPRJbzXUXiJbTunjL4LhGK61JB0NQiqkgGhxUA+XSyqNl5NIKekjocjTZRoaeSemyTY2mhnaWnqq1ko5DVeRDFTRhmib1kAu6rpsEYu0ErFqFB5qGqOAqaj5/wCEfaaHap3ijREdZqfC5WjGhJC59BWnyqfXpHp90ywRXFNDURGFZWVaWKeBal5nM0yon3SR1A5LF2uiqP0KAsZkGo/Ey5oMn5Y8q/6vPopRZToWulWFAx7QQDnPmK/5vToTtmYGp33uSKkqctR7dyP8NydTT1NF/CcfPWVFPSUuiipKLHrRfbCPHVat4rJH4KeZE0tr0IZWEMcrINcRYdrAkDJrx45B/M/Z0Itutn3O9gikkFvdBGIdCiFqBaABQNJCMMYFFIHnSyXq3aUlFjp0ejjrcDkaQUrUcFDi6dIa6OWeasqaOuTxLSZvLxOBK0kcj1BSLXLdHlIS3K7itqBZqXQWoUk5HAErxZB9tAOHp1PvKHLV/uSNLLYM2xs5hMiImgSBSzKsmFSeRcioLOQNTUDP0UzvimoNo77p+w9lGaqxtPSQUNFQ5nZ1BUY3a2Uq8DkIkiahz6VsWSq469xPFU1McrUs6gxyTNFEyq9gkv7+wNpu0KxTMxJMcjBnRXBGV0kVWtQKVGCAKgk3uzb8q8rc5x8we299Ne7MltCi/vCwiCW1zJakTJ4MzXCSFJixjkfUVIDozMqMu1z/ADu/5suxO6vg1/L6+BuK31i9pb0xnR3xI+Qnytovs8/Xz0O76/429WdndQ9X43NZCeioMjt/JUnZRzOXq5oJzHW0WOiFRDJFWD2Zbg1xHZ29nY2LSJoCmlQFXTpFD50B4cft4dAnky02W436/wB55k5pjsJlnaaEsokaSVX8TSygjwxIwoHIC5yQKstM/wDJk+XXyZ+Pn81v44S9LbnzWRxe++0Nn9Z9ydadWYvL72xXZvUW48vjqrsXBz4KI4ekzme2xg5KqqpMrMaeiweVoI6tZlo1k102xIbO2hlitpQ8hGZaB9IJUDSC1AwGpRWpBq1CuGub9x3HmLd7yG+v7UxQq1EtSWgDlQ7N4mhAzIx0O6gKCAqVRgDvDfzy/wCeh8PuoP5fvZWz/jB8hur/AJC96/Jjaud6f6/pOg+09p75HW+J3dhael3h2b2Fntk7hqzsGDAbRzxbEU1QyZPLZipp44aZ6SDJVNEt3WSzubK4sZZAyzRsjKDxUjINM0Ix86+legnsW3X0d7BuDWZ+nglQkuBpLVqo7qBqfEfkPUiutt/wkE7UylB/M13ptHL7uydYvYXxh7aooqNqH+MRZPI4Le/V26qWOvzEtO1ViqeWnoMpVtVWijmqKeKLU33KBk+1gQS+DHCI4itdIFM08wK0oABx+Rz0r3+Q3MLO9000kblQSagIDjScVqWPAAeYx1X7/NP792N80f5indfyN6xxj7r657x7N24uy8Btqpo4d7Z/bWzMThOmcchxVLS5Kt2puvtPGbGGQpoq5DUQQZKKeSnV2Ny3eJmWO+uUuY4SsbFZXFUWgqHcVWqrxIqK8KjoR7FaRmGystDStq71TLZAqqU9QaVJoBmgpXrfG/kH/wAxzqn5BfFbY/xM3jlY+svlL8RsDTdKbp6Q3zXU9FvMdebBqDtTq3N4mqnix8O9p8ZsmkxmG3BLTxR19LuCjmkq6SmhraCSpOdmvluNuszNdJJP4ahpFGhXNACyqSxUE8BUkep4kHb9tUttdzXEERNm5Lggh9Nc0ZlJGRmtSCDgkg0UPyr3j8If5DXxe+WXyG61xGx8Z8kvkdvftztLGDedRTZHffe3yF7ByO7+wsBhsz/CIsPV0PU+wKvIymnxlEMXjKLG05hjkfM5Hz1z07W+3RzTLm4kJpXJJJJAxSirX5ftNTexjvuYLi0t5cbfAo16e1VUUDGprWR6cTU/LQoAqq/4Ue/MHaPcv8in4abvq+yP4Jvv5e5346dr0XXOz89BNH2RjqHq2q3n2fhc3jsZWQHL7H6z3fubE1FYRHLT4/c0GHSVEmMYVu9lMljASwEj0JA4HGfyB6vt9vFb7tuSCMtbxlkRmBqAXGk/IlAflSvVIX/CTXsTb/Wf80TP/wB7stXYPD76+LncO3YsnNkKTHbYx9dtzL7C329bu+qydZRU9Jt+jwGz8kqTXcx1xgAHjaSSNDtrIt2NWG0kf5TX9nRtvMVzLtL+GC0HiKw41oDpFB9rkfkeqgf5wvy5i+bP8xD5bfKLb+Nq6Db+9d7R7U2RQV9Tjq9Kfr3qzEYHqbauXqSKT+GNU7gxOzIMnPDG8sVLNXyIstToNVK4zpc3fdhdVfOuBgYyK/4fyHTUYm23bnWPMnhFM6aCpqx7sGjZz+zq3L+R5/M0xv8ALG/lf/zOe0Jcjnk3ZvXfvUnUvx4r9ubM23nKPbnyj370F8pM7tXceT/jXjxu5dobXretMPNloJvu6WnhVDFDP94sMq9WkhE9QdRACVNfJqE1+fr+fRTLHBeLaFWWiFzIKGhI8OqjTxJB4g0PkeHWvJST53fmTy2d3C1TkMjm8pW57KZCqhlM+fzGRnlqqnKzTtI5nlzFVPLI0kz+WSZpHa7XPsloBQfhrX/Px6F8XiXRklcAPoyAtAfIUAxU/PiQT1t/f8JJ944LZHzM7k2Lk8rksfW9n9EZik25hkkjODyOZ2bvLa+ZqhNFE51ZCjwwrWpZjrTx+dAUZwJFNjOU3BITXQ0ZAoDxFGFfIdtf8/l0m5isg/Lq3iAVS4UkYwrB1xipGoAHJ+wZPWu58zN8v3T8kO2+8oqFsJWdz939p9iR7Z3B4a4Y+Leu9M5uOopKnIUbUFRN/AjkPtYq0eGKSsRlsyBblUN2biW6B4g6yUqaasgZFK0zT0oSATQCK52ia0t9rGtAp/QQSUFfCGktg10g4DYGqq1IFSXjH0VRE+RxVMtJU4PyY2trFzuEjyFXQZDDVH3VPPiMjOn3FNDLM6kxRO2p9MgZWQezCNplB76A4IH+XpDNBaSzR6AWiSjfqDOpc9pp8J8gK+vHp+p62H+DVtBNUUlJRzVk+Vkoo6KGPM1ciTJHIFroahnFFWmF1YCNnpk/cR1eUr7oyVl10OoLp448/L1/w8PLo3glVbJ4VmVbeSQyaNA1kigHcGqVYgj+gMg1ehEOor8Y+2sjkMhV4enmwYTL45q2DMVGXzk809LQ1WNxU+OWswlN9pSs9ZEarQHp43Ebu7Rxeyzw54rmARRyNDICsmkxhEADMHYMQ51EBDpqakVUAFuhtebxY3e3zG8EAubeTVFM5laVjRQyoUJioMsuofDXSxqAE52dmNz7a++3tt2La2eoKQVmH/hmfx2VpsdP4YfVUx47F1mN3NE7B3k+20IjyrGNN2YNrb6TaLSRpIpcStQhmGeGogoTilanFT8+lXPEV3t9m3NFkLS827U9kqTI0akqvxiJHWdali2igXVp4knonf8Adfc/j8X8Ip9H91v776/9G2N1fw/7r7z+CeP+Kf5rzej/AFen1+T8+z7xrbVXX+PR8XnppX4eP/FUp1DH7n37Rp+iav0f11fAHw6tXDV8FMV/OvQO5fYVXjsVDm6KSnyMFDh8NmdxUMlVDDX4imzoxFRh6mpx7yUmQkxuUpNw0FpoFlhSacxeZmXV7MorvxJGhk7WJZUYcDpqGAJqKqVPH7aDoM3vLk9tZJuFuRLFHDFNdISA0azCNomZah9EizR0YVAZtIYkHo1vWVRkev8APYHN7c7a6zzW/ajbG248JsPfG29zTyy43P0kVHBicvnMFUVFcm56BKuFKfEQ1lVIBO6rFFFGoILnup743VrNy5cw7Ukr6ruCSKhZGDakjYAlGIy5UDHEnrIK25Q2vbNn2vddv97tkvOfL6ytkh5euLXcDcxQ3KGPRNeRRyQJdxhowltHNNJSRgUi0aSLODrtwZHem5KPsbAYvau8X23TmnoaTcFVi6OLGzT1s1FR7L27VZTI5epwIhjNfVVlXUJNNXSNC6MsAcGMJt5LeOa0uTJCZCDIVBYkUFGKgLXyxgD0rQB6+st42Xe7nauaNjNlvf0aabcyPGFQqWVokd2lZCoEjPIwZ3YqQ2mpWdJuSgxe0t9Zqrx1flaODALSpUoDS43EV9BVRSRVNZKAaT7UUyuwjmVWg+4R1Gpl9sz/AO5VjEtwiTmQkxmhZ10moXzrWmRWtCD0rijuH2XfdzWynn2mC2VXnVD4MTB1C63A0KADUBqEa1oKsOnHcmeii6/pM7PhqfPGp+zp6FKWry0cTVOQyiSU9DlEikqloKedqtY2nijt5LF1c6j7oGCXbQiYoTwDBf4aVU0qTiua/KmOlrwsdii3p7D6qIlVbw2lIqZK6Je4iMEGmpaVPEE1PRUuxc/Tx4hY8thZ8HgM1RSUeRx9bXU80tPPSKCI6CmAjHkmy66VMSJNGI1lJliEsyrrVHeQmN9UynUCB/xYwPXB+WB0E9/vUjsRFcWLW23Tp4bxO6mmmgOkUWlZPQBgACS66n6KU+UhyO46HLZSGSmxVNksZDkJ6DH0uVmjooqku7/aZSpbG5XINSQyFIqmYQ1BTS50aiBBFE0VqY42BmKkqGJArT1A1AV44qK9RK11Dc7tb3N6HSxSZFlaNFkYIGqSFdvDkfSDRWYK1KE0qeh/GQweO2huakOz8btrcOUwmBym1tybl2xgafE7/pKDPRxx7jw+M3Nj6bG4egyeNpijU1IlTTNUOXkfWpKlBDyXkDCcyxo7I6I7aoiRlWKkkkVqCaEj5dSaZbOw5f3OGXYBZbhc2sNzZXd3bQiK+RJ6C4hWdFWKJ0UqVjDoXqWNQaIzFbjTw4PB7tpYMJj5afIZmsSWgbDY+sxwTI1+MrMamPpkSdMnLVOlMKWJoi8dx5PIPC7Pas7SSQFnyqjNTXzr5jT51px+WQ9ZbjGq2VpuiJbxFHnkUqY0KDUyGOi0bxNR06AQaYrUaVDhN+7emy+Xrq7N0WHxtbWhFWaPJ1UksUUEdRSTTJT4bI1jBKmar1xfbmIS1LN5GZUk96WznQxoI2J01NaUBJyBnT6edetnfLK4ku5WvEiheSle4mgFVJGgtxLY0kAtxNK9I3fMuXx0bRZemgm1nAVeOqI8pUbpoKnF1dHUVlPT/wATyNfUVdPT14lmlEtK5hnczRoQVlPtTbIksmGNQGVhTTQgjhTBoTwP28KDop3s3lrHouEFCInjYP4oZHQkVZmJAcVNVqCSQDXUegvyWWkyVRVTNS0dHFUNEyUdJHMaej8KhFjoDVz1VTSwML3jEnj+np9KBTFIVjoVrWpJPrX19f8AD/PoMz3b3BcuqqhAoqg0WgA7akkVpnNPlgdQ4auWCCqgiOlK2JIKn6XkhjnjqUjuAGCfcQRuRexZAT9B7uU1MrEnHCn+XplZNEciBcsKEn7a44edP2dYHiljWJ5I5EWeMyws6MqzRCWSEyREgCSMTQulxcalI+oPuwINQDkYPVCrKFLKQGFQT5ipFR6ioI+0dHo2b1Xk9/dO0e36DHdY129qfKRUFBUV1dWNXUmz8XPW5DKYqWvgrZDjcpSbo3K9XUmjEQkVRE5nEixoDrvc4dv3M3Ms1wLMqdQoKa2wpApUgqKCv24pnJfljkbcedfbyPY9ts9mk5qW5VYJZJCsy2cWt5oS5fQrLcXHiNpCk00kyalVS711fvvpPsaOgr6fbyZzZUOV29pO1dm5vDZjA5vHV+KyLT0W49r5TD7jps1hctMIpspQ1U0RlDMiTR6UOnt7DfttIJk+nmKSdskkbqyMrr3ROjoysorpYVpSpB6h++TmP235ul2+7jtxum3PJbENBBNDLGwZGJS4gkinjlRiV8WNqVqVDCgEzZuXot55vF1OYz9Lubd+5ckj1uJm/jtG+ONLhKSmglegoqb+6uRxGPoKRI8dj6VqWHF0tIIQlOqRoUL2xtY2hjt/DtFqFNFplycnLAkmrMalia1Yk0ENpuUW83UO43+5rfb7cSDxIP1VZAkSInYFEDQoi6YooyqwpHo0RqFqst54vN7Xgiy/hymU2LFkMdt7sHO19BS0Fdj83n4qmpo6R6Klyk8NPRwrR+FpzLIoaJoRIwERdu3ZWY28jBbpkLxoprqVSNR4CvEft6U7zBPbRHcbWOabZo5Ugvp5UEZjlmDGNGUSMFwhFSSO0qKgA9c6/ecyVtJV42spKna1YYMVSZHEXnmxdS1MDJQbm8rVNJSrUy0/hoGeGKatYO0PlRPIziBauACHHcQfMV/COJ86+Q/l0zfXNysNrcVR7RwIlkiyVNPhl4ha0olQC9GK6gK9LrGZ5a3FTmTNRVM0koWlRAaqgqpY5HSopkq1hKmaKJtOm7JHpAKk3u8SMk8OkcLto0JKCFwa9wJ86Gnp0EqUmey24twddVW/azamI3VSQZPFyVP3S4x5YoHg3RtfGrJSQUqVOZxEc0ipFVUqVzU8VJ+/JUKhamlW2jiult/EdG0sBxyexjQ1ortStCAMmlKhfsdjPvt/e8v3HMP0NtPEZoGlOlCVX/GII9ShBJNAjFV1x+KyrCut5ApLgmfzm08/PGaOlSow0U235sJuDBU9RRKaCWRfHm9sZiOroZq2ly6feSU1ZHNGtepMkbAFPZyIYbmANqbS/fqRyDkfhdSDSmAQRihHr1H31+47DuzA20QubUmAwXVvG6gxk4mt51dGcONTJIrd9Qy8R0IG3MdMaXIby3m9TmcxuGSWKlGWqqquy2WnmkUVE8xrWX7qZhGxkaSV5DeNbL5PWiuZI1EcMAVYUwoUAAEelOAH+ry6W2a3N3Lcbnucsk97cMWaSZmd3LGpZmYksxOSSSeHqehQyG1cbj81jNy7gwsm6cXhqVJM1tatklpKfJ0GSop6atohURZqGPEVtOqiamnhkiMEsaSvFK3LoLj6p7W5gtLvwLl1HhzBQ2gg4bScMONR5jFR0NNjOybTzFsm88y8v/vfYbaVWvtqeV4BcwHEsQmQ6oXZf7ORQfDcK5R6FWX+B3JtXLJhJ9onb+4KDr3emOraPGZrIYw7vznXooKXLdgUmCpdx0OPr83uaPDTtj5k+zq0qYaeaSnR5EprILi3uY45o52dLiaFl1oraFlNRGzBCdMeoVHcKGgJGepF2PddjvLjbrvZY7W72rZ9xjultLya3FzPt9BLfRRm5jiNxdiA+E1IZA6q7RKSsY6BzY9dgsZujelbiGyNT15uhdxdY5Pruo3BhH7Hqdu52hTLQZOhjyeOrqHRhtw4OmrhVRlBFV0cMcjyK5WVddwySwbcrxqL+MpcpcLG3hB1qtDRlpVHKgEnDEjIqADsN7sm373zHuUKyy8oXAudnk2uW5i+u8G4iOiZC8UinwZo0lLqoAkjRGJV9LB52xSTZbeW7Nw0e1sbs3FfxGpam2xjcmuTpNs4ekqUwuGxCV321GmRaljpBT/cxRRxzyxv+3EVZAY7XI8VrbW09y004UK0pXTralWagLAAnNKmnqfIBcx25udz3K8isorWAMzCBH1CNAdCRg6VDEAU1BQGI4A8QpEtUaU04lnNGs33Bp/I/wBstQUERn8OrxiXRZS9r2sL/T2a0TWCQPEpQHzpxp0GgZzCUDN9OG1FanTqpStOFaYr8wPPo5HxTCPVVrzVEFPHhq6kq6moAp8hPTw5GlmhoZYsfNP/AJRH9zLJHKsSuYy/qj1m/sP7wKsUVCXkXA+EHTxGoDGBgnj606lH27CK0l1cyBbO3dTKw0uwDghCImYFxqNG0g08xXPVykHXuOxnWtNFjcFPK+MwVPRyxVJlpsLBSUdRF9s09NRitgSZqiumhWoMsE0znUzqUBjio7ndLviLLeKqSS1UpQvkGqgtpOFUMVAYAYANcz5YXHL11tu42drZhUtLYRLDKWCOydyy0XV+JytcaipJINCNf/u3Ht/pO3dHSpRpHBK9WYkljinWGMhZfKKlo5qmquxkCoZHNNpflVZhNdo6iBCSeIX5VNPT1P8AOvWI+9QP+87ugGaycc0Fa8c/kK4+zpb7D3J1fBsahzm5967iwfYOz2k21itt0u14d743cu0KrOHcIJx+VTC4iiMGQy1UkqS5mErFAskEfma7FF9b7l9a0FpZRvYy/qPIX8PQ4XTmmpmqACCE48TQdSpyruPt8eUI915i5svbXnLbn+jtbCO0F6l1aPJ4wIWXwIYvDkkcMHuB2gNHHrJJQ3ZHaMuf3plczsSfMbSwNTQYHGw0tBJ/d+qyQwtBRxyZTMUeFrpqT76vy0ElXpM1QYS6r5ZGTyMu23bfp7VUvAklwWZ2PxAamJCqWANFFBwFeNBwAU5250j3fmK7veVPqLDZTBb26RpSBpfAhjR55Y4XZBJPKjSldUmgsFMkhXxGe+g9rYTe+9XXdOXqcRR4egfIUNdj6g0dRjchHUtVUNRj6akVJAKauJl8dPpIYkqpLXFN4ku7azc2EYeYg9jHLcARqJ4keZ/aOmeQLDZd65ltLfmTcXtNv/5SYlJEJyVfQiliqvQkIKmpoCT0Jm7MFHn4Ia3EUBxmSjyVZNUUaTVlbR1GRqaVabI19VV6Y63IZGcxVE5kMcbwipKCRmiMntAhkVKOwNcH7K1AzXhQD5+nl0dX8EN26G0gZXViaVLVbTpZq4LVOpuAoGpU0r0Dm29gV8lLuuqyOHVodrbcpZ8wtJTT7gno2yeQqchS1NZBQ11PHFVS4jHSRqUnp4442jkZ1bVc0muQTDpfDPhq6eAA8waipz+Yp59BSy2aUx7jJLanRbwgyBQZSutmZS2kqAxRKDIHA1HDo4/QGyMxvL+PZ2VKqk2/PXlMZlmz1PDUYqaLG4+lyFNEMZH/AA4TlY2ZZ08xAI85ZySwV3rebTbFVCdVzoroUEk5NDTjTh8zmg8+pz9r/brf+dXnu4o/A2TxvDF3LIkaxsFQsoc9galSWyoqNRqQCYjFw4nFYvM9e7PqYa1NtUcWTzNTh8vlW3FHHmpqjIUL19dnWyFbV1OWplf9wVIWIroDRQrpQns4J7mWPc9yDLM7aFikVNIoM0CUUaf9kjUepJ3/AHfZuX7a95G5VntpbC1ja4mvbJ5xM5dgV1tcgyOZATU1HkissS0BCe5sFVZvbeJ3NUS4yhzednonpaTFOZItzUmalkrYJnfHzHCx1jRQx1FTFC1VE9Yjmndl1uRpZSR20hUITGoKk0qVI8s5pmgrTFK04dY281WN3f26Xs80aXlwY5UWPCzLIC2rs/S1UGpwuoa66CRU9Blvrc2a717D3h2ZnTS4pclj1rPsaeVcrHhsPt/DU23dvbXx0U89K6nFbdwsVPj4pWi/yekXTZVB9mUkwtkigyX1gA5Uca1rQ4HA9A22sm3e4ur2qJCIWcgUdgQpULpqne1Cy1pWnUrqJVoN11TYLLx1Dwq81BkBV5jBNSJPTVMSVBSkyOEyctVSCUGpp4ayONmjVVmmBF0e4M36DyRUYDIqKnh5iuPQ/bj1OOWreGS7u7S1vKxO3ZJlAozkhitWA+JQc0ADE06NLn63K7uxuyaLcYxOTrtt7MwGzcTW4TZOxdnTZDC7bbI0+LjzlHtPGYgbgzt5JRU5HJiqzkyxg1FTIFVgSXAaaR2UhY17aZwMHjT58c16kjbre1sLC1t5opJLiUeJq7SXYFkC6dRoarlaBlAJAANSM3xi31/oD2d8osjtWsrcdvntHqXHdJbYqKdZ6OuoKfP9tdc783vuGmzNEmmgrqHB9ZthBHrWZ/4/5IHElMSquJwtEJyV9TjPp5ilf9XAMSbU7+LcRQsIlkI7guTQggniGBYYHE4rUdI2uxFTS4+kggpqaemqqOnf+Ofw+po8pSTY9gKjD0lQlTSU8cgari8g8Jmb0NHIoUkFyFZppi0jqyk/pagVYNwcihNO00yBxqOhhLYPY2W0C3RHhkiFZVjKSJ3UeFmqoLDUuSC2QVagxAgxuZx9emQw2UzmEq1r6eRajbeVyWAzMctNMmRgqYs5jft66mr6ereORHeRZhIzNqLMWdueOGS1e2mjjkiZSGWUK6EcKFDggjy4dGEVibzcPFCOsWpYfDt9UbaaFj3qvGtPiyampNSWL/n8DX1ddXxZGqjyMv8AFKisepasq66euqJ5xNTyVuSnmllrJV1KjSSTytqjMZ9K6Atj001qumi0yPQUoB5Y+XQI3C2uvG+neVHTx2YaGrUsags9e70qWahBU8KdGB+VHeG5/kDm+kNutnNwVHXfRvx76O6Y2LtnJT14x+2qraHVW0Md2rXYzHyZCWnphuDtHGZGWaogWJ6ukhokkCpDCkb4JZEAJ0gD/B/n6LJoNNzIpUZdqlRilTx4cBg/Z079E9r4XqHrH5B/wmSuqe1+3tg0nSe388qCCh2h1lu7KPk+5M1BXQ11JK2Z3Zhts47afjdJqaTbm5c2jhZhTsLjt1EUqeB/w0+dP256rEiSqACSFrqXypwFa40ajXiCCAR0W6v2zBuTFQ7eleGjq0cZD7oqzQXgkjl8MIqKenaQKgZ7MiXUi4UMfbOtoZPHBqCNIH2gg8Oj5bKPdLOHZ2URXCnxdb8CAwYAVAPAV/w0BPXW7e1qlOk9q/HKlppsRt/YPbfYvbz5OiyU8NHuTO7+2N0xtKmlyWNhpGOOpMNTdVSPBUGpqNYy9QEigEeuqXKxcR1ySTWuTkAYrxI4iny6BV2gtpJ4VcBUIAYHSDpyDitFPn+eKUqJ3UmMx+Rpp5G8U0dOqvRRUk80tNNkIKd1hhyH3bUsJoaWpkY1UitK/kHpRydQQ3DSRiPw1qK0atcL5laAksfIcPn0K9ptI7yG4TxlRiAVNaAkAgBtVAFUmrHJBpQHiLLfiZvXC9VQ/IPfU2Zo4ctRfGTtDZe2MNCn32TqNwd0YnH9IZuqp8RRSvWU8+E2n2pX5emdVXzVOLkkiDmJiiOeSSKeIqlHIZasdIIaoADYDNQE0yRgmmKm0CRyW5s9QkVZIpPDShcGDVIx0Cp0klVLYDEmlc9EYy1PjJsvU19G9MkSSGCjnET0ayQ0oBhqJccpCYWGVjoSNpAXYB28f09qF8URBJASxUFvPJ454sfy4evTdvFBNKtzGixkTFVDMaAAEiorRB5AVFT5qB04R4401NNXU9Nl6+hy0v8ADqPKhcchrJoiqz071NbGKHF1EchCmM3lmEt4teoA+ExYmF3UTqoZkFcVODQZZT68MZ6XJZ28KpdWkUr2Tu0SyMI6vRRVauNEbqaAjJYN21rlPYnbWRos/S0ul/4gJ5BPEtbS1FBJHXQS1MkEldNTyCKmpqaRw5H6nBjSLVZvbzzRGFpST4X2GuD6cePTFrtd9DuVtZIoG4cR3IY6OuogsQRQKTWlc1ULXoS8jjZTjTWLVY2mjxjR1FVJLTwzvRLClQtGgT7ZqaphqaiAFSzho0TWI0Clgysg1Kmlu4UA9eFfOop/M4qeja4tqpO7Tw64mEpJoSAAwAA06X1GlMgqBq0gAkAP2JlN1ZyJsTjN0q0tVjqmbKz09RTiixq/bzU8qUsoo5YgbhBLKsmsxj0NEXDoqht4YGDpCK+uRjy/1fy6DW8b7ve6Q/SNuTG3ALMlVKqeBK4IANACQeHAiuET/fDHW1f3Ti0/3R/uj49OJ/4Aa/D/AA+/8Wt/CfJ+7p/4C/4X9t+EfU/2nidOf1it+P0a0+g+ip/KnxfBXNPhr5dABi6jY22f4ti+x9iy5zOU+UoZFzFPm8tFHNQrWGGelxOLxdXt7FriZMbCRFIZ3ljlVQieIuKc1cXs7xyWF8qW5BHhlAc8SWY6m1V+VD55pqBlhLy7tUN/acz8tG53BZ42FyJpR2BiGSOON4YzG6DBLF1IGkadXhirs/PdL7vrtuSY7Ze7sBu/bNTNuWDCYjK5DcK5ej2LhM9uOmxVFuPM5apy9DRmDFqv21JT0snlZVQynTJAju4txtkn13EbWkg8MuQF0mQqtSoAUkk8SSKcaeYx2C/5K32faG27Yru35is3e9FvG8kolSzimuAi3DzGZFVIqaI0Rq00lyQUUvZWJ7l7bqtvdibJx+4cjtneebxdJR10uPpcFmMHuHI4ufB0a1hxuSq8rQbWpsWGEdeZI8dJd3mAWSIOk2+92nZ4rjZ5p0SWAGUoCCGUGpoSAC5PFeOccKgQ85cr+5Xuludl7obVtl5ebfutzb7aty6rE0M8kRSONkSVmS3VEIWc0iIWr6dSqwibY2x2/ujEbm63x21tuY3BywrFvHN9oYvOVKVO9mpYsRldw9dxUNVNT5KjhWghraOeenWmRQsekRqI3J9yu9ks7mz3WeeVro08NbcrUoCSFlqMfERQZ+foNOUeVPcrfds37kHbtntINjAP1k28xzlFvGVYZZ7Dw2bxaLGrq7KVCADTgB0ru7b/AGZs6DauxN8duY/HUmXr8DvOrrsdh8LLBt/xbrwlLJl97pX1+LP9zMB4Z6rCwGFajLZFTD9qBFEYjO2v9v3IXG4WO2mWWEOiaiQW7CSsZoas1QrZKqPPOQtvfJnNXI9xy1ylzVz3BY7fuslteTywqki26C6jQXF7FrR1toQHlgDIsszqVEWFZXrG7d60zVf2HmK/e38bn2IKGl2nium1L5DfUuQw1fSU+fymLqm3jJmt2ZcbjioXmpTBSYv7RgXjXyJET7jecwwR7QtlZpGJ3Iu2viAsSBlJ0MDHpVdJIBBZtXA0B6kjknlb2Q3SX3Vk5z5pvbm52iyA5Zi5T0mXc7p0kjie5glS+MslwLhRIY2iS38Fl1LqKjh1p8dqLc25s3kN+9f7oODXExZbNtPmjjtrU+5K55HwWGxw25iduyZ2qpcGXnqMglQsSVNRJSPG1QDLKYblzD9PDDDZXsYui2lBQFtAoGJqzU7sAAHADcOAZ9uvZNN73Tc9w5r5Q3A7BDb+NdyPI0dstxIGa3hQwxwmUiHuaTWoDsYdPiUMglVvT9FUYJFo8Pi8B/EqDG7ZpcLu7AmTL7e2piqbclXNiMNJmMjkKWt3blNxmmqo0qoI6NadPNJ5ptPssi3WcXpbWHtQDIXibLSlk7mAA/TCVFQS2rHAV6HN77abc/LA8O0ax3qdks4bHc7cL9PYxx3LPDC8sz69wnudDhHiSFYh4hZ5HAUnO+dvbUr8xu0Upy8lVgsxlNufx6vz6ZXcebrl8tHh5a+OCrbBti6agqIxXfaCnNHBRhDAl2Qiy1uLmGG2WUpRkEmhVoo8yBqGoGoxWpNa1rnrGTmbbdkud334WX1JS3uZbNLmeYS3ElCUhMmhvBKrGVEnhhFRU0hBw6eNoYism2pT4TaMWDTc+I3Jn5cNu+oxGFyOM3E0LUOKeCczY/MQUgho1rGofuV81UrtIgtfx0nZRdvPcljAyLqiDGq1q39EnJBNMDA6WbPazSbLbbbskVuN3t7udob54o3Wf+zi0sCsqLoVZDHqGp9TMBw0rTY3xlx28tgNkctHW0+66/e+VpKjOY18fj8Di8fS0SSlEh84xCYoNVxVFpIKGV5JooEaCMa3SXnMZtLx40ZfBWEMEapYkkgGgqxJ0ngTwJoehnyn7IJzRyfBuUkMy7tPu0ls92hjjto0jiV37mZYURfFQnWI6l0RWQZIWjYHXkWCzW1a7f25F7Bxu3KrP02zf7j0eCoqTcNFVGH+6O48quQyGczG96Wmq56hqRKKSLHQLJSiqNQ80MC76/cjcJcJYRHbWkC+MJSxKlSdappCLHUBa6gWPcVCgFgX/U/ku32fdtp3Hm+9i55gs2uI9pbbxHGtwkyobO4uPFM5vQjPLoWB0jQeF43is6RILfuH6qwhag2jndxbhyJo8HUx5Nxiotvaa7DU2UrAvgNTkqiojmnSn8UiUU0E7ypPFE9MUnX2Uu5yVe6gRU1MNOdXxaRxoBQAnzBFKMa1AT5p23kjbWW12Hdrq7uvBgk8YrGIKvCJZANLSSMQzKgqImVtYkijaPS6Hlx2Uqcbg5FWcY2aqqsZTTVuWpP4bFlWqleqQCZ6eDAR+CppzIKllDWMxcIwCLlkiEkox4lNRoDUimP9N+X2dBV7S7ktbNwrfSlmiVnddAk1DUKEgRChWuqlfiJoQAMfT/YGP6vy9JUbhxc00bNnaGoaLOz0yHG5XF46Y1SU2KjrK81EXiifHTR+GnrGqCfuESJpATbttp3KOQRPntYdorVW4ZoKcdQORTh1IXt7zfZ8lbpaXW67cZYQs8TgTOlUli+IeFVwwJDRkaVckHWAC3Qh91V2E7C3c+5euqjI7xpsHtPa9Pumkmodw1lJncRUUFTuInK5vH1U9NRz0opo4aqnn+wqo8iuqN5apJfAl2eG6sLP6e8URlpHKEFe0hqCimhIOTivbigByKfdDcNk5p5jO9crXMt/DBYWqXfjLM3jq0RlLSzIzKrpRUcN4bCYaqu4fSC21paWh3JVK2N3JR7lxFcKaFo9w+GXFU1LLHhp6OasjoFaaKmgcUrQOYYZoGZGmjGkEzuvFESs0ytAwpQKMk1NSCccK18j5dRntEltHfTKLWdNxjbDeMRoUUjI1BakAHTpwGGC1KdO24d6TbU3rvFGwENUcnh6ShbFZ6b+I0dHmo4KSow+fr8VUfe4+szG3aaVo4oWaWnSdn9UsLPHLeO1FxawgzEUeoZMErWhWuDRhx/2B07LvUmxbzu3+69ZPEi0eDc9ypLQGOVo6lTJBWqg1XVWupSysMuf6X6y27s7eOdoMxltwZPH46ppaWmir4cnk4dw17U1NQSTy4WOkX7CGKaWSphEU+uCVmLtoGkmTc72W5tYzEqw1zSgXSM8GNK4FCSKeQz1J1/yDydtvL+/bpDuc1zfRxaI4wwkk8dyFUs0IX9MAszqA9VPxHThObaTuPcdRnOysvT5fHSHcEVMdwRUGOjn25mfsqTLRTjb2anoMfBgDQ08bVJYDzRklBKVl0qz+74JIbKCZW0xVCE1qoJB7hmtTT9lT6hJLXnDcYNx5u3GwlijlvvCa6VFTw52RZQPCfSqoyDV/SGrSDRqJ7dndu7J4dtnO47be4cvi62HMxbimp1mx2dikiqKqjNdh4oKRKfI0VTVq4lppIVjeHxhSuu6mztYNcuhmA/32fw4oQCeI4jI+3oj3nmLcJoNuFzDDJLH/wASFwJRVmUuq0o61HcpHCnQET1uS3Fn6+vgo4XyWbrsjXvQUNPeFqiuNTUVEVDSyNM6lfM4hVS0qm3jOrT7M2EccYDt2igqfmQBwHCtPl69A8PNc3MjxRjxHJfQtSOBJpqJJNK0zX0z0OcOQoaDatTkaXD46HKQ0uEwa5PK7uw0dcj1FfSVWSo6rDqMfK8tHUZKSWb7f7mqjcxz1kStFKyFLankEJZtJ1N2qSDQYI8qY86DyBqR0MojBFYS3MUEQkVIotUk6BhqddQKGjVXUSQuthh3WitRL1HY25UwyCkOOoMfXVE9VX1NXi4JMxlaWpk+1qUjTJytj8xRUUtQ1LG9MwqyKMSSmG3pULaRamiapcDFDgGnnxIJ45FM0FadFj7xepbLJEVSFySxde91JIOkN2sqklaqdVVqdPQX5Kmjx8lNJSZNMm2oyJlqFMlBStLCVVYKZ8lSY+s8tEqoxYxIQZABwqsyyM6zKjIAgxoNPPJJpUUav8vmaEtzH9OLeWO48SQ9yzJrAwaUBYK1UoPIcfQAkbeu8RufdLYxJpZZqCHJtuesU06S1mUzEc1bXR5nKVDPPksn5HAhJYojab+NyrSMWXEkayP4YGO0mvAAU0gcB/s/l0KNrt76/jhWZiwLG4NBVnckuZHapdz5GuMcDxIlv1rT1mFy8xrnkrckpjlpTIlLW5FaLzzpPS0sMNO0D6ZpSkbLoThGRf0hIHZWWnAHUPMV/wA/Rz+7Ymtbh2b9ZhoKfCzDJwMH1p6cMdFyodp1+RyeIxsVCgkylPU0sGMrZ69q/E06LUzyZWXytiKaaSNIaipWOFnRRHaSIM6hzZZwdYR6uDqJAABp5cCacBU8fI9As2JVoTNHpiZSgVixZK1o+SoJrVqLWgGVz0e3oLYeQp4KCupcHUy10lXQUKYutx0mJqa2c1gSCLJxY2WYimEVWJJfC4lQq2jToJ9kV3IsMc0kk2gBWZn9AAcjVX8tX59SRsNoxEQFq0hYqqxsNBc1FFbR5UOdJr/DSnVjXcO8qzbG363rmny+Crtw4yWRsvt9qmskx8WNq6Gpq8JlsNl6mIU+QxmSrJmNOGlappHZY5URz7j7l2xjvbxN8FvKtu61jmIAYtqCukiA9rqFAYgaXGVJFOpG3a/iEc22pFEL1YQNDHSqA6z2uaaqsaBWNUY6SAeqQ+4dgVW2GzWQ3FXtPkayvkqsZQU1HTw0tDLX1NFJPJU1FMwSc1FFCEprBleJdQsEF5WsrgM0aoO08TnNKnzOKVyB59QNzFtM1gZmuyfEJ1ItBQatOSRx1AdpyCMjh0XD2cdA3rsgj6gjgHnjgi4P+sQffq14dbIIwRQ8ejKfGo4uLdeSnqpZJJ4cPUTR0TBYwsumohSso7Su1RPTJMFLMECJO40vcH2VbkHZI9IHGgOflWvlwH/FdDHkx7WPcJ3ua6ViZ9IwagELpzk1I/KvHo0k+apJMJhayt2rhduVmKjrqSoqMq2NSbKT1EEKpX1U+MWoghoXV5wk1bXSSASKzRiJ1QkUVq8FxeSNcu6SEMEbIWgyBUkD8gPzOepRv9+t9z2vl6D9w21rcWkckLzxBFebUah5TGgJyTRpJHahA7UCp0Cu3egclgdwS5/e0cuC2ptasyeWmgyeTkpKKFquiLbRaknx+boM3QV+SyUdJSxpZH8lKWaVh44X9eb+GjS128q91LRVdM4B7ySQVOkVJ+0epITbD7Z3NveXe881Qva7NYK1xLFcEqNTITbIFWRJVMrqka0ocEk0UKw47M3t2Nu7bVDt7GULUeOpqOngFdjo44czvYtJVwx5Sqp6ahydDgYq/FYtkfG0rFqKWZpTMwCRxoTtVjb3E+6XElXIBXWe2PNaAk9xBNNRyaYAySKrLnzmze9p2nkfZLUx2iag7W4/XvDQxhnVA4gjMSf2MeFZmdneiBG/M4rF1dLkNxbzyO16La+c3DtfZFNgK2ipcT9s0n3+4MVic/l3NPlaGi+9opaupyNdHS0KOUaVo0Yj2ZJKI3WGMymYI0tQGPCgJWlQTkUQEsaGgPQTuraS98W63I2aWDzRWnhPoQqW1SIsrmjxqShZ5nCRgkFioPXLdm0sFX4Kl/u3u2m2/Ts0NFjKGqp8JuTaU9JRMkCUk2Ux8MlZhVkR9dPJDWU8tPSSSFAsfjRawTnXOZ4i66dWoVU1IrgHBx50Oaedel27bTby7fta7buaQlphCY5fClhVEOkapIxrjzkDUpEeogadIAO9mbbqOvF3Vt+HA4/b1VjdrB8+KWaDMbemGUqKWlocbgK+TTWZCmraad6qKqhc6KadDN65LD1hMl+Le6WdmR3AWoKvg0JYEdrKcEHzBHl0g5t2qblZ922tdtjgnita3CoyywFZNOhYZCdTo6nWrKSdDDXQmnQT9U01HHLQq5Z58uatKaKOm+5jrKylenipYFaWoTxZiCWrfwx/twOCskzBQp9mt85Z3DY0nANK0+Xy885HUfcuQIGhVXLeMDQUxrGAMn4wTQcFNKtinRtcHBS5yhgrMWY5aaSChWOpmkqI8rSSTRxQiiqCSscGaa588Cys8L2GtWX2gWgVtQoamowcfL1Hz6HDqbp4Gt5C0WhCr5DAkAUNTRZTxK1qOFajoXMfiqhjNEaaoWtpCIkV4EqWWLw03ihmqnjWOZUERWnMhFmUoLkavaIiFFrqFGXGaZqakD880+3oWINwmlEf0sgaKSjVUMVUoulXbSAcLSPURQ1UZz0uKnEYzJY+OpdIA5gqlroaetrIpqirjjpnhhpqetjEVPJTSSJ5XE7toIOotpuWK11bM8RBJ1CjMq0CmoJqprmhoKD9lehdJBs27/S3cLJ9OYfghkcO0iIGUMslAAGIBJYnPxFqdAjl9sS7UkxePxmEpNr01XisbnIqVHqJo8zNkfNbMzz12WzFZm6/ItD5qmurXaSWZkhjiigjgjjMbeaK6Ep8YyssjRsTxWhytNK6QtaADAGak1PQJuNrl2Nwtqn08LKt0qliyyO1cqxkk8X4aM71Yv2UAAo3QtQVlfQUgixsFTRVEEwx8EDT1y5COGMztRwvUxVLU8707zxLNHICXYqoVQS80AAnLSEhlPE0FKmlfQ+X2DqsW6Cdtpt4bSJZIJ0YqiapCwVdZUV1MrMpYBqgEtQADpNLtjy5OStaCCBqmWqqVxiR08fjfJySSPTzynUauaNpXkm9CujXYlmQt7fjCpGg1VwM/Z/n6D91HLdX9zKLZY/1GIiIA+NiaHHcRXuNKjj5V6Djd65TGbog3LhKottnAiH/AHE0WMXLV2SSqqVxuRoqxPDAj1MdNUKinRLGsyCUCwBD8aK8JilX9Uj4tWkAg8RX5/Phjoourl7Ldk3Oxem3xv2wmMSMyt2lH7RVgDSummrupw6UGV2/TjcOO3BAxocjOhaXHVNc5qayFfuFrYsbj6uZ4gkLkeWelQrAJo0LhZPUzpIj0EdtfioPy7v8lfLoxlAbcYtwt203WNUTOamurUEjJ4CmSoIXUq1z0GNXicfkdxU2YTM00mQyks9TmsDSN4MxSijrFqaH7+nNDDQ0cdRRyrSqglf7mJiy6xqnKlCRHGGj7B8Na+lDTOfI/b0F71Vnu5LhJ1+odiZUUAMM6gWGmgBBoM5Ffk3Rzek6SmjwlViaiN5Iwsz1MhpKWGqV5LeH7qPxxNHGlILCRQWYEt9QpCC+WRRE0RGsHFa/sx5/5uhdy49oYbk34k8EJ+EAZ8iR6UqKgVzXjToZ5czSY+m3i8dZT0FDkkWnrJaGVWhyYjqjHSKzUorKYzxM5ePUsSCDWDILlSTvbSyCw1IzyIdQ1D4cZ40NPI8Tqpjz6HsM+yreXNyYoYlfUmtKFiHUoaHu41B4AFOJ6LpUZrceOkWDGn7Kopmjqa1Egx7tkglLJQF5FqqabywT0VY2pYiFcvqRrqpU4a2t5QjSAsvAZOO4N5EcCB/g9egm25bpbG8tbbTE9A0qhUJYrGYtXcrcUY/Cc1qDgEZqlqOPJQ5tcbdsrE1TuOkp8nHDTVuSxVC1Lg5ZMdBSfbyVu3oZpBDJqH20bhvXqWzqxd1QwxUK1KkA0JyTUhqfmR0XPNGvhyG3NXGqdA9FZlBWPsCgBowTQ+QNc16z0lZWyZbKzR5iXIrkKdE+1noY8dOjiJo6itx+XNSaqnq5hOIdem9rFbEt7oEHhqhTSg+dRx8x5j/N0aPcSi+nu0vGmd1AKldD0I7jG1SyvmlQKkGvmR0+pHAYMTWQIkENVHPJRzyIzsKqKRqbyRwU5jpow8RMcnked1BIBLEH2w7uAyFtTA5FfIj8zxzgDo5srW2uZIrr6fwomjYRPpIGtSRUBaIKg6TqZzxzWnQD9kVWKptx5KozWP0126JMRiqmHGywy4pMdTUNVHAkCS/Y1NJTLLNMgaSP7hpZBwVsfZjE9YgpJoKnPGpoDw8+o63aFILuWqjxZCqfptVAoqQBqo2kVIyNVSKimemv/RJtvyaPs5NX8J/hOv8AiNVo+w+1838O8t7/AHvj/btfXr/b12496+sxXW3x6uA41pX7P5U8ulH9Tz4nh6E/3HpXUaU0a/Dr/H5U46u2vRQtw763BuvHYqg3C+OyLYPHYLCYXI/wrHUeVxuC27jZMVj8IlXjqejarx/2zxs/3QnlMsIdXVnnMp3b2UFq8rQBl1szuupiCztqZqEmhr6UABpSlOo/3bmXdd9tbG33Z4pjbQw2tvL4caSJDbxmOOLVGqF0C0rr1NVQQ1S+rNQ1W36nEUcXnTb2WwuH3L95XquTqKzds2VLU2KwVDTY2KOlp2gjqpBUVFZURRtSPICJzHDSzel8ZXNIy6My0ytFAoSx1f5Kn7OIpYmwlgAe6FvcQwTVOmQvcM/YkMfhigJDHU0jKoTV8ZCxvY70R2vsWo6/w+J3zk6bYeS21FgcVicfm85NjoM3S4+jSnxW4WqsmsE1PgpckZlcgeKJVEXlOke4z3zatxXcXurBfqIZNRYqAzLXLKAuCwHAD7adZue0XPXJdxypZbVzjuf7pv7FreGzgnmkiin0KywTvLKNUVuJS2s0VQpCa6qOjLbi3XjdqYurG7srhsDRYSoxkG5cifu5oKCty0mOFM+KhlmnNdG8uZhMsgmQR8tIblggctrJr6WOayikkV6+EhxXTWurHb8J8j8uHU78wcx2/LNhd7ZzTudjYwWLwjdLiPXKI5J/CZWtUMj+NX6hS5Ei0IJclmKrTZu7K9i74/vNncnurP7x25j8gzNl8hVVFFjq2npMg9Fja2lwE86w0CXyxdIY4gtN9xIvBLXme1h2+z8GOK0jimplVAJUkVILUz6fPHl1zD5h3rmrme43K93LmG73CzVzSad2CuqMwRliZtKDvJCgUXUwGSaiVh9uds9O7q29vqOh2pR5fB658FNUSUVTQbkkr9qxR5HESfZeOvyuUyuHr1bQ1RDPrqJJYDd/IpDfvsnMdluGxyyym3caZglQyUkGkqchQrL6EGgB86ydyZP7n+x3OXJnujs9tZQb9t831e3SXASWKctbAvE6ggyma3mBI1q4EhZCrFWCL3xuLs/dy1Vd2FvDPf3cymeqcscVJX5afb9Hl5SQkuI23WVdPj1SnhyFkanDSLSl2TyAMCabdbbZaLDFt+3qskcYjVyF1aQOBfLf7PQD5u5u555pm3K45s5pu57O7vHvpLYyym3+okJJdLcssSkBiAQKhTivmOPXvZNNtzZe2Nm9i7jyNVt/duBrjtTeNBU1ZGy52m/g0u3Zsg0L5WghwdJSrqqKSKY0/wB6IVUwwcl99ZGe6ubmxgUXETDxIyB3ihIYD4SSScHjSv4upH5U5wi27l3aOW+cN4mfZr62kFhuCM9LJ9SwtCXKtKiRxoNTRKxUShACqFeu49sbd3FiMXBtGGo3JhMdm8lg8vVYPIrE+dygixwyVRUVmZXB1VbVV8emopaxoqMPT1EiqGmQqWWlmjfVcronKCQKw4DNBQVGOBGQKeQ6ZOzbbuFtaw7DS72uK6ktJJrWT+2kXTrbVKIZD4ldcbskZKsRQup6wbw7c3B1Pgdo9fbWpcHW5iOklzlRk62ug3pU4evqcxXJgqKl+3pcdiZczi4opo6umqocpRFZIoyGdJC17PbINye4u7lpEh/s9I7KgAa6mpIU4oVKkUNMU6Vb7z/uXIe1cv8AK+yW9lPuYAvnnkZbzwZTK3gIqhEhaWNQ4ljlFzCQ6KVDqw6k43K7736Nw4fc2QpFpswm3cjuDG0229vbao9w5vH0VH9hmsk38GgovtaGauWn8s1OaKNghanbwROjRhtbRoJoENYwwiLM7MikmqgliakDOST5HJrWLfebebF3rbN2vY1t76S3udwghgtrWG5nhWkM0ipDHEqRmYrUqIwSCyHQhUuuWwdYu48JU7fyk6ZiTckWKpspikyApcXXY+qosfgjgqnB4WKqyMlDJTOkM+PSepq5KVnhiLizH9vcL4EqXEY8Hww1DQkhgS2upoK8TWgFc9RLd7dcrvFjLtN6y7kLwQpLDrAjkjdUiMDQx6nKEUUxancrVFJ6RtTUVuYz9fmK6rrM5UZzKZ2atyDiny2brpqoS1GRzFTQ1RaplqpFrTUeWURGSUOUlR0Z41cSpb2sUKIsaxogC8FUCgCg8KClOJpioPmSXlzebru99ul7dS3d3d3E0s07kSzSu5LSTOGqzOxcuWYAsakMCCV44iggzxy0NTmaTDyY7CVuWxVNU00/2uUqsalG1TjEkooTHR10+FppplnkQipnplic+SYOHHYwhGCFiWCsRSua0OTw1HhXFek9rBHuD3SPdpAEiaWJXB0sU01Sqg0YxqTqI7ioBywPTbTzyrTCCZEjx0szQz1iYmhqqqPzSUE8wp6udIZ/PGtAhRBUR6VaRQVWebXcldRAP6tK6SaYzmn58af4B0mQv4QDrS2LEFwik1OkkBjQ17RQahQVpQM1RU25icRPHmaaqeqwlXjaWoyW3c3UYmsEtNlY6PHVuMh3I+EX7bHY/PNO1TTvPM8WIkpR5Hli8vkLZJGqjJ3qSAyhvIllJUtkkAUxlq4p0KLG1s2W9huXNu6oz28rRtUyAI6LKIzpRZNWoaiViK5LCvUqDJ1FFhpczJXpt5J8NSz0+GrsvWy5PP7kSrWv/j9ZTVeDqa2ux2bhkEsgjJo6pzEklQEjZIqmNJJPBXvYN3OoFAKU08SARSmeHkOr/USxWjXUh+nieIeHDI76pH1B/FIKa2Vw1TTtc0q1BQGT6XxmfzO0txVu1qzYsVZm9wRNPmnxbVWIp8ljscstDPJQ1oTcM1ZTVm4a55HyEJjEk4EERpkgZyLeHjguIVlWU6UNF1UJBOaH4BXSKU9M5qOpr9trLd9x2LcTs8+2KLi7TxLiWNXiSSKM+EzRsDOzK1xLqMqkFm7FKBGL1T9CdxbS3fl9zvlavd2Gra+tjxOPo/to13DFmYamWlNLRVdZNHttaLIvBHPUR00tNRQyglyjNH7RrzFtN1bJbqgjuEXvJ/CVwQTSjVGQKgn8uhC/sl7l8v75d7xWTcNonnMdr4WgG5WYEq0cTSEwqjlVdwjRwhxVqGnUPuXpXtOkym15oK+LYQy+06PF5jKZPdi4fCU2Ar5aqo3FU5fP0mOpqjM7VWqjp3leURIq28VHIut0c2ffNpuEvfDpc+FKQFRNT614KFJw4BIpxyany6S+5fs/7g7LuHLUV/p2hb2xj1T3d0sdusMjEzSSXEaDxLcOEZi2mgpoiYd3RYOwo6yfMUO1Mzu/Z+9v4Dhgy702vlqeVcjLLCfHT1GYz0lBBl48PXa4m8AhmqYm8zmRx6BNbSVia6itJIpGahjlGQAeFFJ0lhkcacMdQLzBaeFuEezXO/WV/DBECL6yclXZlJPfMI/EET1ViApYd1WPBMbMxcB3D/AS+IiztXPV0eHyuXymU23RUNQcfViOoapqqSD7aauWRf4bJNHE0OQ8LzL4Qys/cSMY/GAYwAamVdLVofQcaHiK8Bg16JdttYhefQB4vrnbw4pJGeJQWUipZgumoI0FgKOQWGnox22+nNv7gq6HK5uszWA2VXy4oY3FbnrKLfW+Nw7ep85W5HLVODyVDS7WwW3sRnnjTXU0ByNTSyFwahopJUnD15u11DDPFYRRybgqtRhWKJXoNIb43YrWtCFB9BUETdyt7e8sbluW0X3Nl1uG38mTSwAxOsd9uFxbLK5nltSforeOOUx6QyPK8RwZGUMHRfyG68o9j4XZMVPuipywpsrvvFYrbDbRw2NptnbKbOR7h2zHJvKm3BX7g3VkcxlM/lXkpshRwtjoYYXSaUVnhp3+X9xnvrq/LWaJblIn8cSuzSzaSko8ExhI0RVj0srtrLMCi6NThL3X5ZflwbDZruonsIRcxWVuIIka2tTdzTRJLKjtLKzvM7jxhrQMBUKVHQdbIGKyu48TFuuoposTt2eGTx4ekw2NFSXqI566Guqtu0NZW1VPVSt4VyHjqxBGF16IwqAyvS0cL+CCGcEFn1HhXT8RAxQ4wfSvHoG7H9Lc7lYDdXX6KBxqSHw4yQSpkBaJHY6q0ElH00yAoC9Hs2XjMFicDmK4JXtHHT5aTHw4+nqdz53KqIpMnDi8fj8fSsjpWNIlNF+9FEtrPKiB3QnlkkURFUr3CtSFAqQCak8BUnz+WeMobfZWYF8gkK9j+EErNI1AXVFWNSO7tWupQM1YDURCoYMDSdVZbcOYgxuzHw6Lk6PEZLOZaumq8rTNBTDHVePweOkzNbj1yFS8InpYaqAc1U6osbsKSyut9DBAjOjdpKigAz3FiQoNBWhIJwBUnp/b7Db35Tvr7c5obO4iLTRJLI7NK66V8Lw4kaVl1tTUgYDLuFVSekNsPbG1KqDHZ6l2rkaLer1W4oN0VlJUyZfGRZ2grCaqWhyUlR58ZPMZZaatSnp1hLIrU0k9OzvGaXVwaRQxgBVRV1k/ESSQdNKABSAMk1rw8wptW12LgXT2sv14klNzGoDoGQiulwdQqQQ9FpgFGZcqJnXFHksx2jh927U3Xu7ae5erq2sr8Rl8fBS5jH4eurKBqfP4/GYathqNnTM1I0VNlllo5aWoilME4lWNgpXuVpZ322XW3X1uktnOojlRjp1CuO4d6lSKqQQwNCtDQ9KINxubLe7PedvupYb6zm1QFSpVGde4KrDwDUEK4KlSO1gQCAZXNneFVhtzVmVz1PnKbIQY3M56opcFs6NYMbV5CpgrpQ1A1C9DV/a0UwggWiVaaB5SzRpMyEogjsIpbKC3iaNoi0MWtpq1VQQCTUMp1CpLGpAGSoIGsz7gW3O5vboSw3SLdThEgCnU9ZNIWgB7X00QAdxNAxBKH2XtinzOCqaWYCogXFTxieGpn0Y7QixYumajkpZaaalw0YheNI0VWcsIH031CKFirhgKEHA4V9TjOfMcfXoG73aJNaeGx8QlO4gk+HwCxgEaSsYpQgaTXsNOiILtuoxNTQ1OSpY6N481KifeRU/8LqKbHla+omMWbqaOKrVaaJkSjneB6ryIoJYlScfUGTWiMSvh19GrwoKDjUg1ANP8EZx2RtpbeaeNFKzgd1ChAOskq5AYBRTQSC1QK14iR352Bt7sjsDObj2ZTb2h2hmDST0VL2ZWYvL7hxBoHrHbA4LcSRVAxm3oI67XFRQSQ06ltCxBVhT2WbDZ3W37ZbW9/LbtuKg+I1orLGxP4zGWLFj5k1JOSfMDf3P5o27nPmzcN82Wzv4tpuAjrDuciyvCQDqhgmz4dqpP6UeqiLRBwFYfUWO3FRZ3JZLZ43BVZGLFy4+nk2/TxrXrVypTNVsJ6xlx0VLSVIDKzkkvGhBIBDqL+9hSKMXLKqHJ1cKHgCACf9X7A/yvtO6XN/L+6YZpbpVZQIB3AjBNWooHzPnj7TL5fcOy+q9o5WpjNJuXcWRyNZiN5UmZytHuPIRbmApINzY6XF11LVYWSSro5WaqKymLyF0EPj8kDB/w7/d5IxGphtsOhAK1HFWqO454H1pmtD1LH13L3IVldAiO93tme3u0lZJijiizxeG6tENSkhu417l0adSEFpews9vLA7rrsNiKCKM19Ru3P4zKVNDucTU1mNfmqymNNjIZpMJkFgajTLJU+ZCkWuRIY0Y5g26328wQamYhdKt8P+1BHBTWp0+Zrxr0Bb3mnc+Y13W/ihRA0pup4mIlHzkcEKHZWoE8XVUBVJKqB06db5Pb0lHU5SfHbhqcnDkaeLcsOOmesocnWwNAY6jH0lBkcPszOpX19Oq09I0MPhRVDTTG07uXSFT4QCaOKeRFf4sFhSvz+Q8uk+yXFprF0yz+NqAudNGDUoNUYDRwyBmXCkLQAAs3xlVDOpWbZjj2pi8Xju5aLIT0FXm6+DblPuQYfL+SSty9dLHgsUZ6GjxVcMDU0sEMwR45afRJExLpkjq0jXLlrJiG8MBtIKkYAJOdS6s0IqDg9CJt0V7XbYuX7VLfmmFJIXu9UYmkSbXqeQrFGSgglFsyAODpdO5Cai3t/atfhdvwDLZfcDblr2rBlNt0NXU0/WmLp6nLSVeKgwmKr8dRZyPIQxSNFHW1FTNHTLLPT0sbJIkgLDL4t0+iOP6UABGI/VJp3EkEqFwO0AE4LHFOpDG0JtXLlokl5ejmOSVnurdGK7ckZYtCsMTxJOZgGYeM8jKup44kIfxCiewdztuSXZ+16pBjXpIK9cY+H2xW5aCL+LUM9FBmjQViT47MmWpo5VijgD1bRRT3KQg2dt7ZbWS6uE1MGYF1Zh5Z0+oH8vz6IuY+YrrmWy5X2S9VIY7eJxA1rbyGviKB4xRqpKSykDT3kK4NFAARPmw23t4Y7C7RL7swdNPicTmqfe+LoqbO7UydYaSgy2cwsWIwmPnw23I2ydMaqgpxUFvGPJLJ6mjVxrNPAZLnSk51OvhFirCp0qdTGr4NGNOJFOiG8udj2veobHlwS3WzL4UNwd1jiE0UxAWaZBDCjRQVdS0KmQ0UapGpgye1qbIZGjpsnW4iLGtK1THLBQZgVwWOmmhi84lnpMb93mJ6enRI1ZTBSwKzhXYxsamqDQrggDNR6/8APv8AMn0yOlSMbx/rLnb3ikkNF0SV0hNIxUKGkIAx8KLU6T2noXMZj0M0MDU1K1XU0cEiVBmrBTQRrCDCscHjhkmjC1LC0YNipZG5U+y6aZSC2orEpIAAFSa5qc04ef2Hz6F1jYXEJELRJLeTqGarPpCUHhhR2hwdflwoWU8D0o+wcntzLUW1K6g64622huTZ2yMl1vX7q2xSbiotyb/xNdvL+/NRlt7f3g3LuPFybgos1KtHTVtBSYqJscgpxCRrDs2sJGpGu55Ud/qBrNQpKaFUABaLo/Dmh7jVu7phrdrP63eJILePchM1m0RdQoiBjkkSIHUugTLVXHxlnC41KQIytXR7gyEEGLjpqaoyVZQUsOLo6Dw080tWoo6QopoMfR1lZI8KyuTd2k0s0fI1LbdPpg3jOxRVJ1sa4yTUkkgDNPQY6Tb1fRbvBbrt8ccU8kqqbaNNILPRUoBHGrsaAk8SaHT6pKoxuUk3ZFU4jASRSGmlmOR+/hWriqaGaKPHxvjabGQeapFXPPZRKqRxS+OKNfUxUa4tL+K4Mf2Y86+fClP516IxZ7kby1G32TJdquoOrjVqVgq9oUd+stgHAIAUZJfp8zjNsbOyGWralIpxUa67SkDrj0kRxLWyKaSorIpUSVV+rsiyEk6hxoqZp0UIfCAwRXJrwFDnp/6hNp2q4uZr0G9diJE7ToBBq7VUkNTHHAJzXgC0+5KGtrFxKZHD5HN0GHxuul2nlcdnaWuqKySpo/J/EsXlctQ5GmpDXm0DSx+GV43k0SDSVRRlXxGRgh/iBGfShAPQTe5SWZLX6iJ7pEUEQSJIDUnOtHdWA1UoCKEitD0gt20iT5SlmjVqVtlU9dRRZyTMTff1VXQTRxx/7l5cnNTQBY4UWslmSuijSfxhjIGEbkTsY2qP7SgKin+AgeuKEZ6LtwijS/Koc2obTOXOokUAOsSEDAGonWKGlfRGSZXcCzxfb1cedOfknkoa6p8lNkcpPLWK9H901bFRwVtRPLB4aWnhmIlJ8sQEY0jYRW1hRpYUJHpwrwqaAfs4HPSF5rjUjtIZfGqEY4L5NK6qAsWFFAPd8S4wDZdQ7wnp6OkyVVCtdjqtlgkrYKlZqeqSokkZoY6uakpb5FGVlaGN5Ch+rkadaS4BkHhaqTDIrx/Mfb69CzZUKWrX00JksZKRlq9prQ0ViAC1PIGvnwORQyNXTVks0uLpWFTUQvBTOaDIJBH5EqaxvDon+7kqaaAeJpVp1jdg2qygF04jaNH8absqCakedB6UoTnj6fkKUu0vpLVLDbAL8xSRRsqPSiam1Ahi2tU7S2kA5qABlvrevsljKuRchj6IV8VBRq+JyFYKirigr/tsvTfYNi5JKCiqFjq4W9EjSIkjLKNQ0hFFusFyiNFIxh1EB1BA7SVNQwBIqD5Z4jFD0K39v721ilvHtoDdLCpe1nkq58TSy6PD7EYal4MSATqFcdMGVxtS+KGtlefFNNNVrlZFMU9WtAq0NP8AaOi5FI3AVVIRgQihbqukmBuIw6pHmpxpGOOTXhx6BybFey2M17d6VMKsX8dxUsEGhfDNJBUUANCDQAYFOk9iMA+RqKSZa6nx8jmnrzIK5SlN5qpIZqioaQeRP4d42M8ThZE03CufT7rNc6A/6ZZRUUpxNK0HrXyPD7Ontq5fN8bWQ3sUMrBJQ+sEKrOFLsRUr4eSymjClQG4dCzt+go6Oiy0NNUTZetqMkuShzWTk+6pphRmSBJcXgxBMFpclWuZb1UYd2Cjxp6ipVcyySvCzVRNGlo1FCCaE1evFQPwmnE1OOpJ5c2a2sbfdoopxcStN4sVzL3o4QlQ0dvpbtlkNR4q1OBoU6iADh6k3l2XvHd+UxmApoNv7Tx2NzG696bs7A2/t6l2vi6zMUmMyabdwW6Mrim31u+vetNLQYvFQ1tfLK66YWjhns9uG+bftSbbb3csrXN3N9PbRQW80xZ/DZwZGijcQQgLV5JCsa0ALBmUGLIOUty3vebyaHaZIttWWNbq/uJlWO3DsxeiOVE0zqjrGiirOUQGvaVb/cPG+Tx/ZY//AI8j+H6v45R+D7P7T7r+H/8AAzxaL+n9Xl+4/t+T0+3PqV06tLfHT4Wrxp6V/wAlPlnoV/1Vi8XR4cFPoKV8eLT/AGerR8dPlSurxMV19vVaLY5mlKLNSIyPpqVWoaRaclpGLoojeWopoYkJZ4fuFCrqLWYexoJ9KksrEfhNBn+dASeFdPGlK9YumzLSBBIiv+MEmi8TX4alQOJXXgaiadPWz8rndt7wxWT2nWURzmOr5P4XWSxU0lBOxjmp2cw5qCOJqeqppGAWaNJLNwqva1btIp7OVLlWETL3AGjCvzUnIPzp+XS3Yr7cdn36xvtlnjO4QTaoZGUNGSKipWVaFStcMtaeQPS1qq/cPcPYEWU7A3BUTtlPLQU+XipplohT0Ec8eOxeEhSjaKmohKhWNfEC3rJDzE6kkSW22WggsowtKMVPHPEtmpJ8/wDN0fbruu9898wvu/Ne6STzOvhCcDt0x4SOMBaLGvBRThXiemfLzdg5cyUWUq8nPknyVNt2roI6UQVOWnxeLSipjWVVBCg3DPRUFJ4zJO80oRlYM/lY+3I1sIWJiiXQF1gjNKtWgH4cmuKZPRbe3XMN8pjvbyQzs4gdSApfRGEBdlA8WiLpqxY08zXo7HU3xrfd+3xuOj2tubf+NpDT4ePA5qhr6WvxNeHyNNHQTw46VKZ/EzTSQ6op3jilaWK4a/si3HebLbnVbq/it5ZFZxqIGAQWbJxxFeArQHPQ55b5Xk3cs0Vg95BFojEcp0kVqqrigOQaYJAJIrXoLJdnbf2DJTYzJfc7ZrttUeQqK6XMSSU611VkJZjTS1NbBFBQZR5fsmgpUdFqICnqpQ3rCoytckzKQ5egXSAcDOOJA8/nx6ZO32u0CCynDWr28cjyeMStXatCxwrlgoCgjUpxo4HpizGCwVbsiox8O5sfU5XGYE5WWl27Fk67ZFPmMxX1vnoodxZ3K5GpzOehpIaZDPTo8slZkZ6GmMiwsGvHLL9Uw8Bki1AjVpDFVCmpUABQTXBIwAx44Lbyys22kKu4xy3qwlnEIdoVd2caRK7sZHC6cqDVnaNa6cgFPtOuoaqhkijoczBLXY6KIeVxjcjNPTirraWTJY6tFBTUGPaMxVEhrKWQBy6HSjvEaJdxsr+I2ghcivD55FST+Yx6nISfaLlJIGjhWZWkUDiFcnJBZW0qi0oSWQ5JGASp7eqBvTbnWTYPe9DuQJtzHZZ9sbOh2c5rotqZvcUVbuyHDRy1lHR74myE2Xjq6aapaWekjE0cMkkTvEAbfiyl3E3NlpZ5HVZpC/F1TShNf7MAChAABNCRXjlNyY/NO38kJsfNUN1Fb2NtLLttj9ENf0dzch7sQZQXzSNMsiNIzNGquqMyEqAr2t1hgsDtjcLb8p8xkKPZKZSTem3usN87cSPN5NEzEnWGd3m+eqdzY2CV83U1GKXHQ4aPJQ4+dqorG8c4kU7nuV1NNAm2zxR3E7jwZLuOQ6UGj6gRBCjYWh1F9GqimoIqEeXOR7Db+X98uOarG7n2zakrultsd9aqkkztN+7Jr1rg3UXiGRpYFt0txcJCWn7fDlDM25chhtoboxeMi3NGYTtWPP53wyQ1dJX7irMRj9xVmJhykkk9fSUaZKP7ZWWKGo80bokSsEp1VW0c11DM4tjUSaFJwaAlQaYBJABOTg1qa16DG+NtfL+82VlDvayRNYx3VwY6MpnkgjuJIg+pmVY5CY+CvqUjQrDwwiN/YOhxEeRq8xU7rx24pI6d9sYioCy0UBof4ZUz5MVbVIrWaXEVsJg/ZEYXzTfcF444HW2Mhk0LHHGYQSsjeZBqAvAilRnOTQU4noPcw7fBYR3kt7JeRbqVVrS3YDQoUK7SV1B9RjddHbSheTxKqqFObJwuxa7aW5Mjuys3JtmahdoqbclAmGz9FmnlWilpdnYnadbRYjIQZuZoZZqjLRZsRU9IVhlpdMpaRVeybgt3bparFJEwFY3DKVIOZC4YgqKii6MkV1VpRJyzY8mXWwbvPzDcbhY38Rbwry38G4jmqq6LNLR0gkSVmDM9yLoqkZCG3OqrBvXjCvlK/wDhpydPhRJWHGfeilrcm0SRynHrXGA4+lD1EqoJmjFoVZiqylQrmSeL4aeJpMv4qVA+dOPD+fy6BN19Cbu5+j8VbHU3heJpZ6CunUQEFTitBj0NMvuIx9VWibcVHS4yjTEZeCqcVVVPS453qqiF6KgiMrFIaWkmjIdpKlHMcijXqAPtPNIsdICXbUumgFT51J86kf4OltnbyTlr9I4kSOXUdTFUqSCq+dFU8cgkGla56NNnMdtv+M7gr8ZkaDL0ypkJc3ndhRbll2xuPz0VRXPAMNVY/LSw4/amViqIabJGvyEk8gSUsiaYFDO3T3c9qFvLWWDyEc+nUuSNRdSAdYAYjSoWtKE56l7nWx5dsN8vF2LdrPcEy815tn1AtpC8au0UcM6O6payl41kMsxl0hwwUhemHE7ffI47BVGWyGd3ZjaqiiysFZuPWGgr4p89H/DEpAmYpqKCJpBPV1NbUvE1RDBAA6xNY1kdWY6AqkE5TzHDj+X556BNrDN4aSTSyzJpDr49TRhU0C9wFCakk4IAyAaO22cPvTbG8Q9Diq7OYTcFTictlp8/RJlYRV0NfJCtPQsmJeqzIfHzNTSU1LTx+PywvI8UIUhJeC2mtyJn0SIuldJyQfXhQg5BPzwT0JuVBvlhusTWu3/VWc00c0qzRiRS6MAFA0M0oZW0sijzUsVUDpNbvrNwb67Qz26tybprRW7RjyFHjaylNTPVhdvrkavD4QvHkJq2GWTxSwuKaLQFZGVQJG0VtVt7Lb0srOzUJIdTAgAEtgtwAyc1JrUGvr1fmfdd95t5y3DmHmfmO4l3CzQwwzMzu4W3VjDDq1sygKNACDSAVoACad7Y7F7VpurNz7WymVr6rrrOw1eRoodzK255abMz0Qgztdgw1RHNjZpsNLLUE1FLLTyJCyJJBJMZm1Pte1/vOC/itUG5r+mzwjwyyg1VWNO4av6QpWtDSnVtq5854tuRt55Vut0lk5OumNykN7/jIScpolkhDN+k5hY1JRgQGClGct09Y3aW36LbNKm6tz7W2/T4qWkpaF6bEId3Vz1kfkQ4ykpFrMyXyvlgSapgxgqmakSRKqGJ5yVJkkkkcqjMzCrLXt8smtB20xU0p5E06Ire2s4rKOG7uLeKOMqEkC/rGoPaoUM5MlRqZY9VVB1qpfoAsxPk85jazK7jm3bka2mrZomnrMU743E4qarxSJWLeppaagyFZUtIjRreN2AU2ZxIpjFpjdI7cx0pUgMalqNiuTpHz/yU6Cl5LPewy3O4vcvKHKgug0pHqSjD4QHJqCBx+Va9Hf6f6y3VlM3W7o3VNvTbWS2Xt6l27UtvfG5eur9z4/IVdZm8RPXLkVgosJU0cZp4JcbBW1vhMeicxyozThPdbyKOEWtuiPHMxf8ASYAA0o1KEkjia0HywesguSNku7y+n3re9wvLS7262S2Y38bytOhZ5ItYfSsTKNCGJXcAL3kOpLZPkd03JPvCDeeU3HtzG7f3JFQ1Gfn3UJ8BjRu3CYOSOhosNkY6WuSPI5TBYZYzjKuoiSpaN3E6NIk1N7lO4b93T2ugiWEsIwp1NoZq0pioDEmop5DyoU3vrtEV1zfZ8wvuETruMUb3RkXwYxcQxKg0nu0Foo0BRyakM+rvBUvGytsY+sgpYqjcs4ptyZCmpMRvHa2Hqn29hMjLlpKLE4rOHF01Dl9o7hqMlRJLTU09F4J1mikDrA7TE/uNSs8iQVkUd0bHJxUkajRh5YNRT1HUT7Ta2s5tYZ92EccrUiuokYxo2sqiP4ah4nJAIDR6TqBJCGvR/uiMLQ5/bOKx9BvXFbi7ZpdpZyu3ptaTE74r8tterx9Zlqwz5bL7hw1Njd57ij27TQ109XjZqvG+SQxglU0uE9w3CSGe5S42+SLbBOiRT6ogsgbSO1VctGmslaOFbzGCD1LfKtvZ39nFIN6jHM8UDm6hlWaRqgs3imVxSabSw1aaoSpGRgteZ67jNLuubH0c1bJJjI4ty1tZS0FbhKWCuWaraqlQmEyzNH4naBIAKalNwAxEYMEu2MkSzEIrE6BkMSKClM/trk44Z6ZutosEs7qfbA014sYFwzqhiQOWJapIq3DtCDSvdhu0BBtLYc6YiGOpqtwZWto8nRZKq3WlVlMXHnaipmiip6bB0VLUrVy4qlhggpGhkSnRoYAscIQhnMTITJUxqqGo04NKeZqaV8/51r0EIrWOC0p9TNLcqys1xqddZYkaUC0JQaQpBoKCgFMkRsZ1h2bgs3W1MR3BuKrzWTgosNha7G0cEtLksYJZBFhJoBT0WLo8ekL/AHsUvkfWkesPPxKXfv8A2dY3Z72ERKmp2DVAU+bEk4I4UpXo/fkDm57mOKLbrua4uJlhghaIBi6g1WMACmjIYGpBAr3cTPbryVXhNpxbfzuHoZclurN0lPjKzcNHFj90RblqcAtFFHUZjG00f2+Cp4kSW0i1CiWdo1Du7WKLJLW5vhuG3XpeJYiGSB9UBXWTUKSw8QmoqNJoo8gB0q3ax3ixtP3bzJbyWV6kscNqLmIrKe0EByQjCNUAzRvjAFePRYN80OWno8tiDT0MbGdZnzOFqTDltDQs1TFP563HwU9PjZFSScAySRwx83Y6WEES6Sr63AIKhDw44PDiftofTou3O5W6gurWOK3161kNxGSHIKmqkFlUBTQtgkU48akq7U2PPTZjamQnoBVnICQ5CajSWn2/HFNJJWUNHJUVUaLRy5CR57ySyqI19TEKBpNY5/ChmBkC8KeWa0qD8v8AV59RtuW3l7uyfwdZYnVp+AA5AII885/nw6j7V673Du6Soei23Dg6Gj3PLiqmOTK1E+Px+TxPnqs3BncPm/4gK+ujiqKdJEd4JJhGojsCwBfebnFbMkShpJmjDx0XyNAukg1oc8AQPME16N9p5cudz1T+FHBaLcNDNWTAZKtL4iuGFRUcaFh8JAp0JezM9JtCfFTwUMa7Y3Dm/tcFn8FkMXkaisV8jVUOLpq+lrIKR8NgJoqeRKpi89WoWKNhJOrlk37tE9JryRjKFBaNgQAaCorqYk1zwA+wY6O7LmCTZJPA2iJEtJpiI7qJ1diupgtQyJ4aEYNSzUCirMCSoO/Nj5mvwJyEe3KytzWR+0lx1fDjWrY6ynEyz1S0lVlGqchBK8CIXQGOV3AQIUvYxs5o0lVC9EUUZVPDGBQU4dFvMtlcXFo92sLSXkr9srrXXnuIaQsamgJqa18qdElwdZVxU+WEFbkVqKqjWjWmo5Iqj7uFoJaWWCsxdQQK+lTHySBWQs9KVDAAWIOZwA0Y0LoySTgDNfiHwmv7ft6jmyZ/DuCsz+KQFCr3EihBBQ0Drp/NaVpToYuss5lMJU5XYddhfvYSsVbVGmggzk9BlaBGyEFD95V5iPB7Woo540qayoFLW5GCsoTFCI/JKiorqMHTdrKQcjSSFqOFSApLHyGQKHNSB0JtivHgS72WWyVqqG1hfFZXXu0BmkEcKEjU7BHcOmldKs1DC47EbjyeEqKbAYmjzhxEQmH3b0teMKs32cRrtwvTZZspjJKTHZIP5A3leOW5jAcEls0scCp4j0Dmig4qc4HqcH+fQv2uyv8AcRMu3WXiyW8etyBqEaVVS0lG1IFDg6vmMZ6x1G4sJsfrKhwOe2Dm62EYyHJYKvjyNTnsNhqijzM9ZV0nioPuqeOWOtcQ0dZVVbPTvIqopVWlDKRXM+4ePFdKsYqJU0gFiwx3EggeZAGf5dHVzulhtPJtts+5cuTzSMuuzuBKzxRhZWLqIkUhmJwjvJVK0APxdIPbW6aPH0mT3bS5/HNgaHddZictjI644vPbhpcxtiF6rI4DMVCT1mMzWHmjZQqJDQ1mlnM0axLJ7fnhJPgPEwldPEVqEhTqoAyg51ftBxTy6K9i3GC0tpN7TcovooLs2ssCP4c00csBLyQykFkeKnDTofJLAKD1Np8JJtrKdo53Zq4/cuJyCY59uU8VTR79aeneeGGtlymfh3NV0lEDU14lqmU5J1kURs0Ehi8mpJfEjsknGiXIkNClTStANIJ4YrSvHhnpyKyFjfc2XeyRrc2RCGzQlLwCMsqlpJVmZE+MayBLpbt7WpU1eyMQcfDuqfJ7u6+xWNqcnNiMMdz56bA5aizsNRSpWzVf3kNYkWX3XDXUj/cSRY6kpYUMatIzyt7Qz3ccfghbWeRtIZ/BXUAprQk1FQKHtBZqkGnA9L/pL9by7WXdreG3iuZI0S4fw3MpAVmOoEq0ilasVjUUpXj0q9vbu2/uKtbAY2rSrgxFXTU2ercRT5KoOK3BXUD1MWDeunFJiimKESjIilevSgJUSRq4De2LqCWESXIU6+Cq9BVa0LADUSTnTXSW9aHoVbJu1nfPBtryAWqFzLJbiRjHMVDLGztojCrQeLpMgiByoYV6Xe+dqCjx4qqg1uYaf7OggMZ+0jqq+pMVIaGmf7ieqq6hlXX4vSTxpILhQTcvcwRbnHOscf08qu+pHoWCipDECgQH86fOleh57se19/yJvO2xXV7b7xtFxY281vdWLyLGZJKKyIzrrnYEA4oGr2sD2gLHx0aSUNZFQwx5CkrI5Kq9VoqK7FlUoRRVlJW1+Tloq2oWMiMtHHKA4IBX0qIICTrXxTpIoMYB+KoIVdQyPOmPLzjjd0asE6WSfVRsGko5DSpRYwkiPJK0bkA0BUNQ4FKaUZuRIVeuo6OOnhpUYNJQQV0FZUQVU40y2+yk0yKsqreR9QUzWZFKW9vwlhRpCdR/FQio8uPD/Y6LNwihljaKyVfBVVPgB1Zg5wx7Ca59a01UIFKAEO081DhOvqeesp8vVtXzESUs1LGlOlQ4no6kSzeZkNFXUsjQNNpkJjfT40ZrlXagzXDRIwFOBHH1/aP9R6DPMsa2Ox2t9NHKZJidauKCtSvHzDDBOcYoDxBCk2Xvfbu6sLNjMBvPZWH3ZimyewchvLZx29NubCQUqUuUrsBT5xq7DZWnevgCPV0k1ZIkyRSgDQ/jdTcLG5W5SC9guLm3cx3KxSBvDc9yrIFOpGCmoVgME+oqEYts3CHc0gt7S5toZUVrY3MPhsyaFZtKvqVg2pTqBY0KNSnB+zeysmZqPFZjMrRS06y4vN7n/jFTHWV8UlZkJqLGZSgraKgEWSpGqoopZHLyVDB1RmV7tZZ1qHWJTXIBGAaCpGa0OccBg+XSq72yaORbSa7KuvZJKGIY0LUVgVWjLgE5JINMHKu251nhP4LW0s8mS+xgqZaEY+iqFjTMtVQRJJlZ2pJyatQsfiK6oVUxsdAFgaM7s/jMx1Vx8s449KbfbIkja20nweBVfx1FCTTjUfZ0N9QdywdTxZ7amAm3LWY2sx9NUY+nqsbTVseLqnqaKjyH2oxL1bYaCGINNKkcMFDTFBJLFdWYoR4RuqW0jlQ6sVNGI7QCcjtBzgcWzQGhpLV2u4N7bWu5WFn486TrHIoaIOFYuiMVMfiGOgNWwsa0BYEg9DNsav2vQ11RPn4M7vGjniyeGymR6+pqzHBppEqUwG4sPBXpIcjhDk4I5ZoayOOQ46dkUJPpCod3O4T2UJtmht7jVG4W6owoCPEjbSe19JOkqxAcAmq1qo5MFva7nMbaO4vvjhmexjkACMxCyxioMiEipDhewgUrUdBjX1WZFDuBUwOQlpo/tafGRU2XmxT7cd66mNJlpMbNSslcDRrJHLSLUJMklQjqKgRspVjw9dpSZakkuSoYsNJ7QailDQ1ocAigrUXvW3mS23149tl+ihCLFGsrx+BV10yaCpDHSCpj1BgXB7wp663bPjs1tZcj/Ea2KMTClzEtJkIxGJT4nlqM5nFqKeowkcMQvCzKsgjI8jDUCPWxaG5eJlFKVXy/JRTPz/l1fmJbfdeW7bcre6kB8QRXJVg4JNO6eXUpiA/ACtSPiPSS3Bu3bmJoMltCfG7ZM1PmcZWTdgzbh3FkKykfHUWSiXa+D/g+Ql2ZncPufKyQTySw0eQyEVTioBBNFTtUeV6OKWaSC7E8oj8Nv0NCgHUVYOwZPFDooIA1KtGbUhbTpBu53Vpt9zNt6eD4MVEe58ZpAzr5I8RaJ0d1FNAc6lFG01PQt7RbPNtjH4vKbdyeNz1fQUuW/utXGipMjRVuZQtiRkcVFDIYq7J0dTFUxxNJTukUhaZEa0YLJmt5LhriG4UwIxjaUVIoh76NjCsCK0INMevUucuybpFy7BtN/tky7pKgnSxbQrrLLURCSEKSJJUIdV1IQpLOMheoBr462hhpKeBcdSUMksMzyPFTU1N9oztVGomqmUvUxJOkJkaJYUjTUL6iPajwfCkd3fUx/OvpQDyxXiTXpEm6DcbC0sraEW9sjaW1EIiaWJcuz/E6hgmoqFVRUcadDf8A3G6c/iX2n+zW0f2n9yP74/ef6Ju39H+kz+6v8b/0OeH7HX5f41/kP94L/wAE8n7v6fT7B3765o8HxP8AW7m8X676XR9VZ/7i+Lo+ur4lNHh/qeD/AGtO3Tqx0t/xXXo/rwlf3z4NNF7/AGenX4tfC9M6eNcU6qP7wpqjDZKj25W7Txu36mgVpYaihminWTHiWphpaCCQ0kE4p6dLMY9bBJGNlAIJl3bm8QvIJSQeK/bQ6v5EfPrFDmmB7R4rOSzjRk4SIwNVFQFU0BIAINAcV4efQG0s321TTVJggqhT1EMxpqpGkpqjxSLJ4KiNHjd4JtOlwGUlSQCPr7M2GpWXURUEVHEfMdBSF/Dlil8NXCsDpYEqaGtCAQSD554dWV7FwO3TsJqhMZR4xNzZKm3FV1eCx+Tw9SlDGsSYutxVHIZamjxkWiVYwjFkQOdbu0jew2wbWdbklRp7iCePAn16mKGOB7cPFbLHHcMJWWFGjCrXtZFNSEFCAKkihyTU9BZurdPXGA3lisfSZOvehxOP+6SOSc5LD/xVxNRy1ciVIq85j8omOq5DGWKLF+skn27CkxiaSh01AoK188ehz/OnRNuE+1Q7hBAs5ois1SaoTw1UPerUJ48Mk8Ojx77zew4/j1hd5fGv5KSbH7/y2Tpdibh2h132XuTY2967AZBsgmX/AI9t3aVTS5veOBymGBllaClrERZRHMVK+L2AGWTdearrZeauUEuuWYY1vbS6uoI54PFQoQVZwyxSxv8ADq0tVdSVyejiRpbjah+4t2EW9PMI9FvcGOVlJoiGCMiSSiVZm0tkjPl0UzNVO0sPs+WTL5CHZ+3ZKEY2n2pJSvUZfM0NPB9tDjlTI0r5SeeroaqP7hEhp66nllSSqqo1Z2I4BlaYpFEWfJ1KQAM1rWtAPTy9OlUsNjFtTzbhfpaWdVT6d0YvIApAAUqWdmU9w0hgSDI4BJ6QVI2IymNp5arbtdiaenwFJiMBg81isdLvVazGefJSYzbeSlp5MnLjIop4lpZHSCaQ0slSixyvKxekDKZP1dQ1FiUJpQ+ZFKV9ePGleiVGguIrcfSNEohSGOOdEM2pM6IzltA/DUKW0l6Ak9A1npsTF2DBT0cc+NR8mhydKtUuMo8Vk6WWKiyck8VVDDS1dPDR00plK+MyzvIBPIoBZ8AyWsrPpwoCmmo04gVGQakeeMY6JJTDBvNrBGro7SnxU1aFRhRWYqwCsAoJrirA9xp0o892T2NsnN5zZC7rz1OU3Zjs/TS5/Ivk6TEvUYiuhlilirIcguSp6yiylI3mJEEi0wLROr6laisLK5hjvTaqXEZT9MUZgGB44pkHHzxnoQbhzjzdsN7fcrtv10luL9L0LcyeJHG7QspbSwZZA8bx92FYINQZTUM+6+wtxxVWEo5ZcXtnErS7ebIbW29sbCYegRI6OHJ/xGooI6emptw10Vfla2spRWVHkoJa11pzSiR44rWtlBJ45Ku8oLaZpJS5yaU4nQKKoIAo2mpqeKPf+bd3L7fAz29ntxjt/GsbGzit4j4alxKyBVW4lDzyurSNriMpVDGvYgiYLAVu4s5hd4VOMTdOLgWuq8dj4MZMlRR4Gqy3mkq66jSjqzWmljrKjw47zBEpyjQGefyRujmnS3tpIHbwycNXNXHAA1oKgcfXiQOBxtu3zbpu1hugthdwqS0UYXSVhZ+5mXSS2nU1I60CkadT1Uq3tLD7coo5ItwU9TDnIqSSk2ylE2Nz2R3FSZulqa+mrcUmOx1Nj5cfNiRRF55aREhSXxR/veQe0O2XjXaq1q+qEmrsaqFZG0lWqdWoNXHyr6HoU887Da7NLNb73bGHclRVtVRo52niuYzNFNEY0WJoWhMVWKimrQBr1gFWzOAnweB1xtkYL1dDjsvK2QkXFV89dDW5SH7LHjGwSTUsFPSwo7PPIVngY6TrURCe3nE87Eovw1TA1UBpk1wfOnz4+sKX1g9jt66HkSsixznWRGSwZxpTTUqFABJJNVODUBUticc9dJNIsUsy0sRl8cNNJW+SYkCmgqIKeeKrjpqmYiMyoG0Mygjn2pnmEYCk0J860x5kEilR6HoqsrV52eQJqVBwoWq34QVUhqE4qAfspXoxuK2Pk6TKT4XN1eXpMRisBBPT5faopcPPNW1eRrEoaSthoqRy2RY5KWEQmaYwMrko5mUEnNzGyrKg7y/wv3YoK8T8uNAfIGgPQ9TYrq2nms7xpfpo7cES2wCd7M2gNpHHvIpqOkg1Ulh0sdl7bo4Uix1VSZOuq6SdMnhFOVyUaPBtqtrKvG5GaSOekhlq8NAxeoheMxoxAVCAiR+a4QFjgascAOOKD5Z+39p6btNpldtIjkeRAZEGpq6YyW1k4qVAq2KDyHS53FLlc5BX4WoNdRS57KV+GWtAFRVbkwpijarp6yKqpRUY2pyFdWSU14hHLMA0qaPIPJSngUetFXNKUAP+xx9PtHRk9w+6AWoV/HmZ4tQJZpVJFQQR2sxJXtyRnBOWTbOxc51/majdG38ZittU38NpaU4JkfKVu4gtbHPLAM3msrT12ERWiiZpqZRE86aHjmULdq7mW5QwTEsa1FDgVHmAKHB8+HyzUy5asdy2G5l3na44oAIwnhsAWl0yCoDu4eOjLllwWGkhsUWG767be9ti7sqMptbIw7lps7j5MXuqm/vBuOurKTJ0NNU5PJ46NTjopaqTHVH29qdauhMELSFL/qI4LK8tNxsEtLpBtPhsHgoq5qAoBoToqCTUqa04jqTt25g5Z5o5E5tut+5euH5+/eED2+7a5p9UTozXDUMiKZmUoooksZjVjpV6Mz/sfZSBchuGnyk+9cbjsRSU9VV5DE6o8f56M0f26tjsfioKPG1SVpj+2nptStI8nmDKfIb3E8cZjwqyvwSuTQjPEnA+fQM5D5cg5k5k2/aLm6uJNveTwpJ41AZV8N6BD4WhQSODIeJNRTpqr+tKTL5N8u259146rajhxkAw0+CxcVNi6WorqmkoGSlwCHKCm/iEkaT15q6vxBUMxA97a9cKU8JNIJNM5P8AvVRw8qDrI9fuz8kyStMd/wB6ElNIKy2ooASQKfR0PxHJqaYr0yTfHba+Salkye7OwMo2PqKioo1yuZxOUhglrK2XJ1xWmyOAqaZlyGRneeoVkKzyuzOGLNfR3edA5SCIVFDQEfIZDA4HD06fX7p/t/ceH4/MO/PoJK657ZgCSWbDWZHc2TjJ49GGw2LlxsOQgTMZeqgzPYEnYWVhrZqSoirKsx0QptuBDRKKLa2OegiamgpvDUQhdAn8RKeyeecOVbwUDCPwgQDUD+Ljlj86j5dDe0+7dyfEs0Y5j3wxyXX1UitNbEMwpRKfSYRaYAoRwBpjobs/2BXbrpko8hgtsJFEsCQWxcuQNP8AbTxzQPEudrMvEZ4SgVJGVpFH0YNYgltoEstTRMxZstU0qeH4dPHjQYr5dDW+9ieU95WJbvdNyogCp32z6RWop4ttJkcAeNPPotlF0Ptig3DX7j29m9x7VnyO4sfuGoxOAh2hBth5cPXQ5LCYmfa9dtKvwVft7E10IlSiqoJ4J3AapE7KhU2l367aFYZYo3XSVq2vV8yGDhgx9QQR5U6CUH3OvbRLl7u23/fYXdw7JFLZCM0oVUxmwKFARXSQQfOuKGCysY3HHLT5aWtOOn2/uHbVViMTksltfFVuP3REtPlXraPatXhFq6lqVTEhclEV39JaR2YnO5yxjT4ETfqCT9RS+VII+Ingehg33T+Qb0/q8yb+g8JoKQz20YKsCGros1qSCePqfM9OmDo8RjsXFi6rC0WfVKf7V63PVOYrK+opWilhamqZocpSxTQtE4UgpchFvexunuN+v3NUKJn8C/zzXPS+y+557YRRBJd432UEaayXFvWmaiq2imh/ydCFityfwqCKDGYLb9A4NGa2tpqSqjyOVFFpKLkK374zkTGJDIYTCX0AE249kF1f3Fy2q4bxB3FVbKrUUNFrp+yoPQy277rHt9ZRrHZbxvELHT4skctqJJNBqA0n0moVNK6StaCvDp6xu7HxsP2eJwO3cTTPka/KvDjaKrpUfI5WskyVfWHRX3+4qa2d5GcWYsxJ5N/ZfJeOWLSxJISoj7wT2gUA40p0eW/3W+RUjSO15j32CMStPSGa1X9RjqL1+jJDV8wa/nnqfm92ZLcGIq8TOlNQrV+MvkMaauHKxVCOrtXU9fPV1MkNfKRzMPWCdSlWAYIob5rOVbiG2iDgFQACFCn8IAIAUeQ6Nr77q/JO72Uljec18wtE5Ejt9RalzIDmQu9kzGRvxNWpOeOekJTbfwzUs9NnMbR7qlqMhkcjJXZ2niWsIrqupq46Fv4ImFpZaDHJUeGnV4mdYo01O7rr9mj85bwpURmNAFAoNZ8qV7nJqaV/2MdEEP3FPZ5z/jG879KzOWLNNZA5JNOzb0GkVoMcKZrnqFn9j7I3IMfFVbQwNDSY7Ky5ilx+Hp58bQivlxNRhpJpoIKkfdO9BWzIWkLuRKwvawCROcd4QtqMbsRpLOGJIrX+MDiB8sDozm+4b7M3gQfvff4okk8RY4ZrNVDadNf9wCSdJIqTXJFaY6DKH48bMiFHTyZbdk2Kpshk8nPikyGMxpyVblMhkK+SXI7iwmFxe9JftRkWhgCZSMJGuo3mknllU/1+3aIForO1WUgLr0yMaAYoGlZfL0p+VOmU/u8fZmbSk3N3NbW4Zn8P6mwUEsSTVk2xZDSpA7qjPmSSt8T1jtXAQx43b1JDgcCGpZJNv4zFbdjoZaiEsaioNdPhKjcNOcixDTww1sVMXUOkaP6vbT+42+lg0kFs7gU1MJPP1AlCkjyNK9Glt/d0eyMamK35m5nit2IJjSfbqY9CdsLgE5IDAVyAOg1wHxl2XgNv7g2q+5N87gwe46Sio6+j3Nk8Hl2p0oKmtnjkxFU+3IqvByTrXPFOKSSFKiNUEisyhvdpfc/fTJHILGyVlrTSko4040mzSmK8Ot2f92h7GR209q3OXOEkEgAYSXW3NShb4Sdqqta0NKAjj0o6HonZtDkYqn7rN1mJ/h8GOyG1MhNia3buZWASkVeSjmw5y38QaWQSeaCrgZJI1ZNPq1MP7o7/AEC/RWdeNdElf+rtOjaH+7K9iGZSecOb/DNAU+q27Sfmf91Va/n9lOm2X449XxVuWyWKxlbtzIZCRTi63bVWmDq9qQGmNPWU+3Kihp4pVkyTHyT1daa3IGRV01CKqqGm90+Y6oTb2hULQqUcq2cEjxfKtBSgp5dGVv8A3Xn3fS0zR8083RylgySRXe3qyYyEI2v8RFSTVq5BHQR9g/HLrXCRQbuqMVk99bsatoKCKDcWRooos3VR09ZVx1+cjw1Nho5I45KKNaqoWjrv2iFellRjpG3JfPG98yXd3Z3McEVvHH4lYFcUqQKd7v5HAqPWtesL/vnfdB9pvu4bTyFvnKm4bzue57tc3EEse8zWsinwEhdGUWtnaEdz97MJRSg0UJ6Kd3llqB6LGebYW6MDgcljsPldt7i3TvuHeW3ty/wGGRUwQj2JCcdiMdloKaohpUp615ZWMNVJJGkxqYpG2lG8aat3E8yuQ8cUZQqDwzISWYeZoPSmKHAvneZf3ZtRn2G7gtZYI3t7y5ukuYZzDUFFW2TREjhSEXWxPbISFfWoi42tzlR17tLK7DpthVElLSQ10+TyNPUMVjj2/DSy4w4nACappqjDVkS0ggknqZn0gurJ4jKgdY1vblboy8aaQf6Va6jxqDWtB8qZoObSe+blXl+65ft9taSJPFNzIKtQQInhmKKpBiddGlmZiaFgV0a0HTYzMbb3Hi9vebYMmRh3NsrJZjbWHhpcRJHT4vOLns9ksYklTtmpkpFgx9NTyUjpPLMoZo4w8ZljWM6zQtI3iaGV1WRsmpUhAe1hXNa8Pn5EJ29ld7PvcNl4li97BdW0s9rD+mNKSiWcopa3YoAqoUoWOdK1GtBj69wmP2VkNxUOKyH+4TIx5uKI5Smqpqr7WsqI0qcdLl4/EJis9U81MTIGgWd1eR5CZGpIpnji8Re4FT2UFNIH8sen2Dp3bRBte47mNvci0kWZFW4DMzK7EFdS0OruJU1qoJBYnuKp6QydTT777Gx8uEp6PDw1dFv3b6Uub27s3EPhstW4jamTyNPmq2qgyud3BnqtotUCUdQ1NDFUVDPJGsciIN48PwLVfqSJnrEaxvN3KGdNSqKIigE1JUFqKDU0J7ydfvHf7vFJtRFsji8gSOSK2j8KTw4rhhIx1yyyhQANLFRqbPZpFz5Hy5XFJgdvYLcO0M424sftnceczNTJVVktK1VE89PRSYegrESFqaopKRxDJVU9THO0MrzTSqye0HLZju1uZZrCSEwzSQJGyhQdJy4JALBiSAw7aVCgA16Y5ouLy3tbOK23GOWO5Akkd5GkYKrsqRaNZ06fDRtJIauhizEU6C/bm8NpTYLc2PzHYk+89wYgwV2Jw+2K6hzGaySTyQVe4BuSsxqT7o3TXVZqTGssdVKYXdYiDMkgc0aznW4he2gVLQqVdpAwChVpH4QPYoBycUIH59JLfmBW29rS83Vry/WYSLBbsrSSCQ6pvHkQGeV2rpFHJUmlNVR0jq7O0W7cjuav2bT4ykxGOyUOMgmlocnFryMNFTHKtR4Kojw9fPSYyeJoJZZGZXrI3bQ8XBUxQSRJFFPIzSkVLGhrnzpgVBwMGnSe+3W33Ke/u9ms4YLCNxGkYDCnaAdKkI7BCvcxJBepIINOmbErRy4rCVe5qSXEKMtPJFJk61aesxlfTy1UVTV0tSchJjpAKmZfFJDO6rM1kj8v7aNzFQ0yRMrSgCqj58K4r0p2jTcQbY27RPDZGVis0jUoRqDlCWC1DEEEHDYCljQQKLtfI5vKYrqjO7x3BvfZvWkm/cl1xjNw7gfclDsir3f95ldx0Oyv4ijU+y4amrxK1OSx9GIFq/tVmcO0JmCOLYNutbvcN9tNptrbdr4RC9uIo1SS4EC6YjOygNL4aMVjZy2gMQKA0Kaz5hgi3ObYpbk3thA8rwNLokdXdWX9OVk1RKugFogQCqA8V1BNUOUxGM3tlMdkPtM/UGKgydKmcCVMZrZaF/DlIqhKSuFBLJoanKeUO5KgleA5pESYwx7QTQflSv8AhHRPuHgwbxc2+LigV6ueJYYaorpqaila1pXpdYc1WMxm4nraKhgnqKOSqjoqSkyWOw+EklUJLS45q6qrM9K1dJGXR3mETSTs8QSIxqtYyxQUcnNKmmf2AAAfZWnHNel1zCbaeRZrVImMQYRp4qqp0j4dbPKS9CctpJYlQFoAMFXkZRtfaGDGSkz1Bt8UiTwUMKZmbHPk6mSsmx8eYrcWMtUCDJPUXpXmNPHKGKftxxFSWyiRb3cLjwTHNNWpZiNWkaQxUMVHaFoQK0oDmo6lHmXQvL3KlpaXxu7a0EfipEDMImlOpolkkiV9SuHrHXQGDFCVCnpNb33dT4PamWmqcbVSSKlRPEKOY1E/hgFRWS0LOjLDXmCmjZi7GP1H6hb+1lpB4lxGfFGgChDCgrQDV/R6JOZt3O3bLdo1i4neTUksbVIXUziIkGklFAzg1PkKjpCjdu5P4dmqOlbZ1Bs+sxeMzmS3JNPVx7kpq6qby1FBQZasqIqKXBmiTyyLLHM0ckjCnkRWsrjW0DTW8xaU3AqioKaCPJiAK6vKopUca0FEFtv2+JtO87bbNt8ezTCK6nu31C4DEd0aSsygxEdxUhtLV8Mrqaot7cze0cjtOqoDg9VDV46goaGSmz8VY8dflajINS5elmkhNLDFk1nhRdT1LRuh1EROq+ya7tNyXcLaaG/Cojs7qUwyBVGkmpNVNT5A19RXqUeXOYOTbzkretpv+UnkkuYYLSydLvuhuHmmYTqCgTTMrIDqLspjNSI309BfDtWPCZY5OWasy9PS1VdT0uOrqDGYWmwL1wpqEU9RT0poYRBTzwt4p5IhZJ3s6iSQuerMZowhopOQwyT51H5eQ/YeojuNni2u/a8DNcwxsy+FIiRLExITTIoKgAMOJABqaEAnocNn4zIYrHtuLcObTFZc1MlUtL4Y4RjqOiigp6LF7fqsdSx1M9UmSjaaWpljWonl1Kz+iO5FeyrNKbOC28WIihINRU1J1hjQrp4DhQ8Opk5U2i6s9uTmrf8Ae1sbzXqVHXQVRaIiQNEhYSeJlnIDsQatUCq63tS9e/Gio2Z3jtftvpjvjOV+doqgYTG4rcO4usMRWYCjxU9Hh94xds7a2VhN60O4shk5PI0FHU7eqGopopquq0yKpfaSXvMkdztF3t15YW5gDay6pcEuXwhhaURMirmj6wGB0rgkGXO57XsdlufNVukU00030UaSvW3MfhGNnLM8UlJXJZH0qupSSzEGhdv41ujx+DwY377+Cf368H2sP2/95Puf4j/d+393/J4P7vf5R9hb7L7nm/j59iz9OurSNP8AZcfw001+L+L8XHoBeLuWjw6t9R4H1eny8XXr8OnhV/se7T8OrNaY6Iv3pkcxnc9Q7gzWBnxVRkUrYqfIS1cdUuYoaJ6ZKeQRQVEkNBNTtKxkp9CyIZQWeTUNIjsNIRlRhpwaUpQ5/wAgHUQcxeI88U0sBUtUKxIOoCnkD20JNRTz4nyZeoHaHcn3atuenWgEVdV5DamRydBlKDH05lM8sYwzx5KUvUNCt4rtGpYgE2903HKxrVe6q0YAg1p/EKU9a/8AFP8AKrtBetdILisRWQtbO6OoBOQYyHBrShGRmmejg57LR4LouqyGJ3Dma3J9l1dOc7uzd09XnM3lafJUQgkr8jmqxkihaDCUq0lNT1L0quWXTeRmEhV4Z+pEX0ieBGMLHRQM8AB881HD/ANJZrWHYZL+Pdbk7pdEKz3DPIXV1ILsxOkkKNAD0rUU8wSF4+szs1S228PV1FcuZy9HBHSrHFL/ABWr+8MdFE0dR5A8VZUzKzwM/hmkWMyBjGhU+KQiMTPEFISp8qCnyzin2jy6jW3mv5Jxt1rO8njSqgUUOslqAUPEMTla0Y01VoOricJtbfO3eo8Fkdr7czNXvKei24ucwO/zHW7Gemy+PVxRUlfRx0ea2puSsSPRHSYxhS+eQySLHAp1R1cTW825SR3N7ElppcxPCzCYMhGqqmqSRD1alKUFScZRbHebpYbPa2+zbc02+KY/q7C9o9udSEUqmie2nYUUJGQA5q2lRTokO4MlujtuloqDdOx6DZtFgd01NXl4MTW5WDHZCoppDixBgKfIS5STHUuNo2dKqdq6sNa8dOkUlNGkkqC23hisNTR3TSkoFDuFr8yxAAJJAwFAGag9RJve73nNht47vYYrBYrlnlitnkERI7VESSGRkCLUMxkcvRQCgBPUOj2xhfucXU7BqKTFUNDNSbty20c9V7gpa/7jHwqcHWZ6hqKqWtxQx9bIzeWF56SokeNiJIxCrWmnf9XxRV6aRIKYH4tNONR+Y6SWNhBWzk22ZEgVxcyW0jSA1SnhmQMappbzBKsfUAdMc+x6LK7v29mKbc2191LkqDGbk3HjsPtbOxY/ExbpgrVr3rKieqx33lJR5IBSKvIRTuZTI1PpM0PtHHuRZbq3NpJGA7IjM6klo9P4RUigI4AjyrwPRtLyrC1/s99FvlpeiSGO4uooYJ9Ma3IkBLu3hqwDindIGOrVooXUBvulMJgexarIVVD91Q4ne9G1fQs3no6ygoZKSpqqDHU0GSoKlsc8SuAonhMcMkESPEQX9r7f6i6sTbI+gvAwDLxUmqhjVSKg8ONaEmvDoM7ids2jmv6+6s1ngt9yjaW3csY5UjKu8Q0SxyeGwwdLoQpVVZD3dCPs/eGJ21nZDgsLtCtxmGq5Mhjcc2QfKZbLYTJ09ZG0eHmycOZemzmOlRZZqJomeQyHQq6RIyae1kmiEk8knjMKE6dNGGmlaFRQ+tR/k6PNp36y2ncT+7tvs3soXMkcRfxWeJw4ohkSUiRMEoQSa4phulTJkNxGiiw23abbkWF3lhNx4bJUO0arJUEWOoq6njbMQzYypp4Ksx7a+3NPIyyRwTVbr5kZZWgdsxI2mWQtqjkR0MgqSwIoSa/iFTT08+lD39+oe325IFtry1mhmjs2dVSN1749LANSEgKaYLUJDAlSqN0b6TsJ6fcG9tu4LN72wWANIMb/AHfqKuLM0tE9dXUYKPSRxV+RlhqanxRxxKKEuEmRZEkuWbTtEOywyWlhO6wSSGTuamksFDUyaL2gnieP2Adc8e5O4+5l/t3MHOO3WlzzJZ2AtBot/wC3jhaWRDIoAV5QsrotFVVUIGFQSS6VZqcltuko4sbTZWvyX3VDjKdDr/gWAwktSl5K+r0VgFHWOiNK/ih0xhQSCR7PY1AuPGMrKoo5Y0yTQ0oMDUCfXHHqHZ5Xm20WwtkkmcmJFBxHHHqzVhqOk0FcDAAOR0tNj0G6cDSS174vBQYTH4+WWTG4z7DIVv8AEElq62DNZmpmqaiu+3TGSutRLRzPIKF0WOEk+/XLwSU72ab+M8KU4ADhnhjj59K9nTcraCSZLeBdvQCsahWbVqZlkYsS+FJDFT8NBprToYqDGV1eKpq3cGLyWWqqhKvCUm1ayE0dFip6KnhpWx2GTNVtLR11fWO7vLUSPLJZhdVjEkaSUxqVKL2gUNcnz4mg/wBX29CbbFmvVuI57xTc6w0SxGgAZVFEQyEBmYgkkk8eAFVW0OTqsPj6LAQIaU1e4I8fW0m5Nq7dyFZtSKCryZyJwO/5cbl8zg6LN086irpqauWhdkVQGdkZEgttc6Xrq1UWq6HkAaoBOuMMEYjSNJIJFcU6OZbyKJbXbLS7ZLh5XtZormKFlgQsamO5Ikkj8Sp1qrBVoQCdZo1bjwqVxo8S32JgzdZSYivly1U9LuHKRQFql/4LkDE08uay0VCEYNoVqaOVYyF0spo1TEJCaAZP+z8ugYIQLz6KMKdZ8MFviahr2N/E2n5YqOHTBQ7dlxOUpotkbKy7VOaqKejrtsUGWhw+Iqq44/L0CZjLT1lFn8Xg0xssxWMUywVFWC8JVLyeVLcXKIpluplVFr3sKkCoNBShJNPMkCvnjo62vZbua6t7Pl/bJZbqfSht4nCoz0dQzkiRI9OqgoFLcMVOoZ6rDbU2Zt3HVW8JsnX5qoyVDHujbOGxcO6KjDZWOT7fOZH7Clroarc23fsPDG8a+EwUd3CmpgMLhP67fN0urhNqtokstNYriVyviKRw+BhGRmnxEkCoUNqE/wA/LPtlyfyttTc5cwX83Nb3DDctntLWOb6KSOql6/VxveRSAIrpSFYoizK0ssRhZRUG5d0di4Kq3HtDMbZ2f1DtxHw9btOkkhpt+b0YRzR7Vqd0YY4+mlwu2qeunylXQorwieRQzQyDS8K6GztLK5aCcSTbqU8UTNUooLAMFNSNRovqaenQe5K3u/3/AJz5Vv8AbPprPldLw2wtYyqzyaYpWiaVAqlY6mQrQKpJpRqVBg/hB17s/tz5lfEfqjsLEf3g2D2d8m+hevd8YH+IZTE/xvZ+9O0tqbb3NiP4phK3G5rG/wASwuSnh+4o6mnqodeuKRJArA3hRZLiJHFVZwCPkT1ldzhuN5s/JfOG7bdN4e4Wu13dxBJRW0yRwO6NpYMraWUGhBB4EEdbe/RH8m/+XZ2d88P5u/x83L0/Pt3rL487e+HUHR1ZS9rdtQVPTlR3L8dt07v39uqmymS7Am/vTOd00cOURNzPl6GmanESxJStJCxkNvtJJtxiZdKIq6Wqe2qkk5OaHOcdYp7572+5ez8gezPMdnvIl3TcpdxN+pt7ci5FteRxwxlVh/THhkp+loY1rUtQ9V4bw/lTdc/HD+VN/Mf7A736xSt+X/xa+XW3up9g9s025+wsbiqjrbL574lDD5rA7Pj3HQ7KzOB3ltbtXJ1lLUZHEz10UWUCs8c1PGsBY1lGm230k0f+NxS6K1OMp5YqCDUEjgQepg2r3k3Xmj3m9q9r5c3cryPvGySXtzZGOBm8dU3LUry6GlV4pLdFYK4UlOBDGtrny4/lrfBD44dlYTZHVP8AJP77+VO3srsfGbqrOw+rfkR8h6Tb2GzVdn9y4io2ZWRVnZmRkbM46hwVNXSMHCmDIxDSCCTbc7e2spkig2GSdCmosrTUBqRTtRxXFePnw6inkH3d9y+a9ouNx3n7xO17HdJctAtre2NiXdFSNxKKW69jM5UY4oeqrdvfEL4B/Bb4k9C/Kf589U9r979i/LSu3FuHqH45bX3xlut8BtbrWgSiraTL7h3Hhctg90ZCsp8BuTEVzTx1zRSSZKlhWB4xNUOH47e3s7KyvtwieaWYExxA6E0ig1MwUtU1DKBTBGOPWQD8/wDuv7nc+80cje1W/WG1bRsKRxbhvE8KXDyXDVBSON1eNQXjkWhWoCM2oHSoAf8AmKfB34+dc/Hz41/O/wCGGR32/wAYvkvPlNtybP7Eniyu4usuxcOc4k+2pM9SiWOtgnqdpZulMU01RNFU4eZkqJ4pF8SDcrBIrez3C1MhsptQpIBqR1NCpIABBodOOAJz1I3sl7o83bzzhzr7U+5MNoOd9lVZxcWYKx3Nu+iknhngQJYmqAARIoKqRmH/ACe/hv1j8we1u86HsfZmd7Xqun+gN09pdfdK4rddb17ju4ewMZWUNDtzYm4OwqFqaq2xjM1WVS05aCqpKn94zrKIqacFJtNim4Xk8LoXaOCSdIgdPiOhUKhPkras0ofQjo7+8d7nb/7Z8t8oS7HukO3R7nvEW33u6yQrctZW7KxkuI7dqiVkUE0ZWXGmlXXoJ/5kfU/xr6Z+SEezfjBkop9qp1zsjJdhbbx2+qftLbXW/cuQpKyfffWu1Oy6aSYb4w21ENGrVskjyrWSzwuQYgASbrHZxXISyk1JoVnGpXCOVBZFdcSKpxq9ajNKmQ/YDmTnzmnkc7p7gQEbgb6eOxne3NpLdWKsot7qa1IHgPN39oAGkKw49Ww/yaOlv5Z/zbraH449p/DjP5ju/YXT+6ezN9dz1XePbuIwe9Di+xds7epKOi2ZtHf2Bx+Fnhxm/aKINFGkbCgdmUvLq9n/ACjZ7NvEzbbf7OGuEjeU3HjSDV+oAq+GukLRXArU/DXz6x/+9Vzf94X2et5ef+WvdeCHlC93WHbrLaV2+ykkg12sspZp57aRpAWtnOSSNYANB17oPpL+W/8AMrpT+Zl3R1R8Q850/j/jP8QcLuTrPBZ/uvtndlZgu4E2n8q915Tf0VW++zDl6avg2ptiFcbklrKCNsOzLABU1ImTbdZbDvW38z3sey+B9LaBol8aSSj6Z2L1JWtdKjSQR2/M9HHOnOf3hPaLnH7uPKHM/urDus/MfNkltuM0G32MKy2Bn2WBLUr9NWMqZ7k+JGUciYAt2JpDnZnxQ+CHww+HHx6+UPzx2H2f352T8q6er3N1Z0js3d1f17gMZsGmpcXlEzeYzGIyu3c/UGTb24cbWyVEdUyNJk6WCODSJakkabZtWzbVt2777az3Fzdlmt7VW8JPDQgapJAC9WDBl08QQKcW6GO5+6fvp7x+7/Pvtl7F77tmw8vcrsLbc96vIEu5Xuizp4ccckc0Q/VikQKVBpE7lq0TofPgt8QP5UXy7+dmT2f1HhOzOzujar4j57tPN9W9l5Pfeza/qvtal7F6dwtNjaHe2z91bczu6hRYPdtfTVMDz1mPgqdTR1VaGienX8rbNyvvXMdxbQxXE22/Rmbw7g6GSXxEBUNEylgoYjhTPFsHoJe9/vB96z2i9ibbeOa73bdr54Tm6La4N121LW4W+sWs9wkZ2triCaKDVLbxsrBUkZaAxxUYOUr5WfFr4wfAX4d7A627i2LS9j/zGe8MbBv3IeTeO+8Xj/jTsHLeOOhoq7A7Y3Xjdp7i3JHJQS00K19LVpLkGrJDrpKWmFSHN322y2LZ7azvLfXzLcETvUsBaxGmlCAQrSvQ1BB01NeCF5t9ovdP3S9//eXmDmXk3fn237uGxymwjpb2rvvN1HlmWWeB7iGEhwzGN0Ij8JRSSRylzHyf/lzfCDobsDD7Q62/k/d4fJXBZHZ+P3LVb7607+7so8DictWZrcGLn2lVxZTtaSdstQUeHgrJGU6DDXxAC4Psacy7Hsuy38VrYe3lxfwtEJDNDNd0DFmXQdCyioCg8QcjHmcOfaj7yvvtz9y/ebzzL98zYeV7+K9e1Sw3TadsaWSNY4ZBcKY7Cnhs0jIPPVG3y6J/8IeoP5UfyK+N3yg7D3P8Dt20m7/g90hgt59szZD5A9yw1HaO5MfsPsfObmlwVHheyqLFbZmyeT6prSIjF9vC1dGqKEjI9kfKdpyrvOwbve3fLAa626ySV3FzP/jDeHIzGg0iLUY60AYDVwxmcffPnX73/tp7ne03LW0feEsn2bn7fpbHZxHtG2kWEL3dlFAJWlsWknCJuEea6m8NiTVugF/l8/D74XfzBPkt8sd/7T6Z3jtjpLqDr/Y26Opfh7QdrV6bw3zn8htmbHZjG1HZ+6NxLko8TX7x2lUlpZ8xRR0s+4qNXqoKeEgEnLmx7VzZvO6zwWJhtre38eHa4pqvKygLo8eVcRs47idJUyKAQAepV+8h73e+33a/an2Z5d3jnmxuufd73O7tN552k29DbWkKTh4nWwgh0GRLa4WirBIXW1lIjd3BJVP5o3SHxz6YquqYeovip8m/ifvzcKbnqOwdhd15Opz2wqWlx89DBiF623bXVe6pd8CaaaZpq2nzksMEMcaSU6zSFlDPM9vYW11Alrsl/t9wyM01veUKDuUL9OxVZZIx3BnfiaBeBJnf7nfuB7o8+R85Sc7e8fKXOfLlqbdds3HYIxDeMzq5l+utkW3FpQBdMbW4ZmLFXKKAaG/kJjcZndjrt/L5PGYyhyuSdVXIZSmw0mYraXB5mpo8DSZGaenmheueMyukTap0p/FpkD+Nxl7SsU3XdJFrqEC8BUZcZIzwNP29Y6/3sCLNyr7K20hQRPe7lUsQpNIbU6Qag5FSacaU+XRUOv8AN9dZiqwG0qfelTPv7HBtqbr2F3NkstlNrbu3PCsG12m2/uWDcE+JqscMZTwUFPTPPjFq4Yvt2o5adh7lncIb6EXVw9n4dkf1I57IKZESms600VDatRqofjXUG65d8i7jyvdzbHtsG/xTcwxMLW62jmV5vormZj4GqK4S5WLwhEI00O8AcLoMbxEjpGYGmk2fhsvlduYvZ+5qjK7i3bVzbXzdRV4HaNQnjq4sPuLZeHp8zPNU7SStpYfsMkaqOnqY/wBl6lLKsKyX/G5kgkuJYiqIfEADOBglWLLpD0NCNNRxoTnogtR/Vuxu91sdt229Wa7utVjM7R2p+NY57WJJzK9sGUeFNrCsOwyDAV+6orhmqWbdmDqdrZOoz1Jh6fcGCx1JB/GsdlUoahK+qz/8SqavLNQLW096CWaYU0YiYoLObX3BRG308viKi5RjUKRXgKChY+dP2de5J8a6R992xrO5nuQIbi1UK0sTFCHeUSM0ixqy/puzaRQ+vQx0GNyc+HyWBFSkzVdWu5aOpeKjx8tQmGozMKCGsyEtPS7gEs0wlEMCzy+WFOCZQpRvcRLNDK2oIP0mUAtQuwFSFBKgU4mgAJrwr0dxbBevZbjZicPduTdQSkhNawoW0K7siTFi1QqB31KtMuAZW3dv47K5+THDL4TNz4zFT7wpcpvyho5cfmdsLFDBmanb7VudxWNy298DmVgpq2iVIZaOGrjeJahWYRtXVy0YhVoZVVnEQ8HUSJK4DaUbRGy5DntNCDpxVPaRWsKeLNcwXV0wNxG19GGje3YaXkiLTIr3MMq6JIyFMaurL4gY6BFakSLa9FBubCnIZX+PSR0ubGRo4BJhqfHpSQxVFBkqSjSLNYeDx/aUwnC1lMAGF1LK3rk+tke1uQIPDB8LSSdRYkkFSexs6jTtPnmnSlbNV26Gz3XaxIUkZBdBwgICgA0kVE8aNSNC6h4i4PAkADSZnYGwcZlKDC7cz1Xk5sxV7njmxGzchA8tZUyY+gpV2hTk4kZalacRPC8xiTxq80JkhCuTXTcTuzOwWEALoLAjSOOo0IWnoCcYwcdBBJNp2ZLaOwhmlvi0kwkihcHxXKLG1uNSNKO0FWYKAe5dSgMUfVbjh2R46OoxO+t3VEjZWJcrisKJxg4pdFTkajLUZgpPJkUlaQO1PT0ypCDpqJHSWMqFieZiVdAo7jq4tg0AOB6ZP7PPou+utNqjaO5guriXU0cbRKNMORqaRWWpJNahQtOPiE1UpHBdMbm3juNtxTU+TzmwoIJKuhqq7JLksXS5ynMNQ0kNFU1+PmqKaqxdI8ZaKOcrUMpmiUWjVJc7rt1iVt3dVvn4lR3FKj4iATStKV8uHn0Y7D7f828yxtvNvZzT8swtVGlceCJwCxEau6BjoU6tAYhqFwKqOslT09tTbVKcvuup3FVUjbhyAieryma2Pi8NXZjDQ4/AZ+i2Hh9m7m3VupsVlxDNWV1DW0r1RjRUgeJHlfw3C5uIwLGSPQIwPgDswVqsviNIiJrXtCsppxJ4DrY5Q2XZ5HbmOK8q07BGkmktI4ZJYtMM4tI7S5ublYpNLu8TqXoFVSoLFA7Rps2Nw5nc+0pqHLYTAUFNtKvyGYbN/Z7jzAp/OKqKPNUtNW4vzVRARWgWVY+XiEkrt7MJAv08EcyESudeNNVB8qqSG/bThQ06DG2vcxbruF9tE0Utnbxi3dptemZgDRwJlV01NSg01p8ShielRR1WXr4cFVTUbUFfWy0xqpI6mujNVVs7Y6aGoo62pkhagFCjRlXLtDDd9MUiojNEhAdI7fP/AFevTyfU3Mts8opI9KEk5Pw5qfhAFPkPTA6FWkydFi8VjcBmI9y5utkgq5sTLtiiSjWhqajFyU0c8s7ZTDLQ45aqlkjqp4FkjcSCPxBzpVNod3eRAle0NqPEA54A1NDjh9vQmku4bPb7PbLqW4kddcsPgCiqWTSOLppGtSHYVqO3TXhizklRkZq+nq4Tm8AuFjWujo6imgH25MFAk60ksUcmNIEbGUwSlY1cIHAU+/RqqgUorVPHzrU0+f8AqPTu53M11NOkyPcbcYlLrHTtVdKK2kr+ke3Ok0FdNR0VOp3/ALx3dW0dNRVEWcx+OzOTpqfETUslFI+JrLSY6PJV0MUeFkpsXFRPJRVE7itiqJZiRJHb2biztooyZV0uyg1rXI40HGprkcKAHB6jefmPed0khhimEtrFK6LGV0/pt8AdlHhlU0kox7wzN8QPR8uuJtw4zb0EYxGBq6ilyNZlcnHGKpomWlqEklanpBHLUQH7ieOOoRBGkkwu9yNIDd7HE7N4kxVpF8MFaD4q/lXGD5eXHqcuTrjdILSzEFhHJ9DO19KrGQ6tBQntGaBiAwFAzfFWlAtKuOjWlxTYKhr1eXIVCx44RYaaGotUVT5anaeWqq/t56uqmApFijZ2IYlFX6MRGUyTm7dfBVQWfuFMDSeA4AHVn0z0cbmu3rZbWvLkEv70uLiRUtXWF1f9RjMPjbJdwIgq1PdgCnQlZbaVZjcJLX5taCqRqiKpq8caiWShp56lKWjphBJ9nRsftKrS2sszlyXvpOkA7b+Z7C/3P932izJJpYJKVHcBUnIZqagDQED0pXrKXmv2I5r5U9vP67cw3m13Fm89u1xt63DVilcRIKQvFCWWBnQNJGZF1OGDkagrTtTB7f7g3Jjutu+OwM5tLqHDU+48zSz0eBx+5sbjaiDB5Hc9Vg8ftuGOiqqmo3dvLBYugY18wpqKrlFUqsA6uY7kbnYbS+3nlnZ47nfZvBiZWcoXo4jV3kJNFijkdjpBJUafSkCG3PPG4Ly9zheSrtMRMsUcbQxQiNSZbiM/osS2tVKrKCBIOwFnHQb68x939x9pi/Jp+z8n8Sm+81/wb+G/c/f/AHnk+/8At/2vu7avsf8AI/Do9Xs98OLT/aNp1a6acfFwpThXNP4u6teinw7n6jV9Lb69X02rxjq/sdPieJqrq09vif77/R0ac9Vy9812Qy276yploYqPGYqpq8Hj2inplNTFT1lVJBWTYuBi2Hqa+jMdQ1PLqmCyqdRTQqDLbOyNFc/rsoZgMgHzo1BUVNPy/bivzm/1O5XEtugG3wyNDCTRWZdTaWaMFtDMoDEVJ7hkjAVXx5x9TkY9z07wQtjVipJp4zA85yTxMZJqWcmVqeWkhpHtLTsg8qy2ZrBgabgUEqHUdRHD0zjy9a9PcqRTSQ3iBF8IUYkZr5kHJFAKVFB8/Po6m0otjZVn2PuXP7fx1Mm3kr8LtrPiHMY3cki1riiiocDDjctPA+FjpGeGnWmWGKFfKCFj1IS3dxcW7RPb2zyAyaXKUBRSOJLMopXFa8TSh6kCwtNqubeeDcLuNblbfXbwvRxM+umFCuV0AEhNPDuwBXoGe+dl0OI3B1rlcRPjdo4Kr3CKluzV2tJBWYDIYiOmmxTZU/bY6SaklyE5WE1AjKvTEOSsd/avb5xKt4jgvKVIMINag4oCCQDpFSB5GuOirmaxkspuVruBRZQq6sL4xaZEeOja3FFLL4hIUsAe3Sa06OzLiu5qnrfbY3/3Xt7dnS+ar8WK/N5na+2+sNyUePxeGlqDSbX7DocnR4iPG1LKzyV1ai1Aijd7gXDx6P3JZ71KbPa5o96MUhpE0s8I1MADJCpZg/CirjPGtKTEr73um0btNuHPW1XNhBNB9Qlwlrt243Ebo8jNaz1jSaEFayzSfqCowakEmG00p5KrM1+Trty7tw+SObTZFZVZ7LUtJjMdXVUkNDXv/Dzjc5lmydOTEiyR+OAKFpwYgsjj2dZpBB4biNlasgAFSACCuTQUPnSuM5PUVbO+3wybo19FNdQTRutjK0kirGzOpSQ+HpkkDqCtCdIrjtA6b8JgMLt9pxv7BVeeyW8sbgsdjctgcfTVW5qHddBQ1ksm445K/K4wU+PMMDJLVws8yq6aEkMugUnE8rI9vMFCNlHY6WU8RhWJYHIGMjJHHr21w7Zt8dzBvm2vM97EixTwRgzRTLVvFQtJGoVgul2qx0sNIJNOgoXKZ/du9qrOVWFyVM23KPZ2GZs7ul6etw2BpIpWhTNUFNT0dfuaszeOlMkYjOikNzPriDN7fjt7WytfBjoquzSDSuGZqVoT8IDLnhXpFLuu7cx7y253iyu9rFbWpNxcUaOGIFUV0UK07PGw06a+HQ6qrUgDt2LFn6zIbthyUVV98Z6nIUI0mtw1VFWQUMFBMzSf7k6Q080Jirlt9yNbMiyI6A4t3MKwW3hEHyJ8xSpPyI/h/n59R9u4j3Ge93dboPq7nQZKPqChSSe9StCJMaskgEFejAbE/hdPsWOmpsNRblymMioYakUskWKztLW5eteeeJK6V6ynSqxcNQAjSxKyCn8btEZEjUouQ0l4z1KK2RUVBAGD9jU4j186dSDspso+XjELSO5uYlVGZTolVpGqQCdQrHXFVqAukldSqE9t7EUlGtLV4ZsTujM0O8aifN1uUpZqWmp5w08tXT4simXG0NbU0tIjxss8sZKMxGhRoVSyazR1ZUKDQqn0+GvqK9Bi2tltws9s8c92lwTKzrQVJOoDGlWIA8yMcKcOFfvuhpUeev8A4NR1FDEY8ZtzC46MwNia6hNZg4RUioqIKWqqEPleehVqeA1ABUBliOvpZJGQhW017manH8R8uHl59OPvMUQLP4QkVaRwxLgqwqgBqaM3ElRQauABA6CDGbdz0MuKnmgOOTKVX2mKzLZaPHQR1VXTTvE5qKT7mRqOaNtUrKmqSLQqOgYFl0k0BD6WqB8S6amlafipwP7Mkg9B23sr0yW3iJpMjERy+IFWrAnilTpI4nzFACvmYKjraVqmhwWayse39ytjKalp8nBlqDbbZqesghmXIR5KSSF9tU7UxV4vvoaWSpvHoiuhRC4rhp41/TBJpQkgDORmuPSvz6FEJUPBZXFwEuiAuvWsYcsOIckeGPTUFJ8hg0Ebqbblc+59j7flrsvt+LadVmMPiMxg8DTj+8UtbEcxko8xj4qLN4+rSKm8EMU+Rpo6WqQNNaWVgCXb1cmCyvbhgDUAmpwvBcMaEZzRTX5gcBl7c7S288yctbVDNJD4bvFG8EWp5agyEPGEkVu3trImkip0sxoTKb/2k8WJhyUuLXNS1GXlpcJQ4DCQ4mqjw8r5Crmqd0rW5SeCevyh/fnq3SkljvHClLGQ/sn2HdWuZJbebxPEC63MhqASF7UwBpThjUK1Oo1HUke5nIY2O1s95szBLaXE7Q20dopWQxq8lJblGlkdZbgAufEETiqqIVoaR9v7SrRDls3u2GCj21Dg0qKTAV9Linzq5CGGseqhqI6h/wCCCnmgaNFhmkleZ9Q1IjBSo3Hdn1R2+3p4kzMoJFStK5Hbn8xgefDov5R5GiEW5bvzbILXbYraRkhfw1mLhGIqJSIQDjsc63+FQKiqX3VuHI4mpxO29kQ5DDoK6kyGRrcht+jrP7wYKSqqpErIXq6WKmhiwT0wjWuglFXRzSRtZLKG9+60vXNxuUuuTFERiAhFDQ0NSGNKr8JFQa1PVBzvdcsrb7XyXaC3tQ0niXF1BDKbiJ9SrKqyxFUeAE+HOpE0MmmSNo3RaBri9wwtkqrJ7h2mNxZKm3DPtzJw7Qp6SDNZDBzVtHk8xPisHnsTjHzOUbD0s8Rgjl+3rq2mZaaqQTRtGaTQlYEgtpVQhKqZPh1AHSCyklV1edKgcQadAq23QSXm5bpuW1fV3skhiaO2KozKzK8hCPF3P4YZSFFGcHQ/ctDiZai6Lyuwaio2NjaSGo2i2X/hVTnOtcvsPP0e6s3W4OfdNMP7w4mklTL1uNrYTOlLUVWqJfGZ5EXkIbBLvzvuM292/hXcjICiTpOnhiojIKMRQaTxCmudIr1PiQ8grz57b2vIl0lxtNu0rPLLZzWUqXUkeu4jZbiONmYNIoGlpAFCjWQB0sPhB2Fs/qP5lfEftfsLL/3f2D1j8m+hewt8Z7+H5TLfwTZ+y+0tqbk3Nl/4XhKLJZrJfw3C42eb7ejpqiqm0aIo3kKqRXC6x3ETuaKrgk/IHrIPnDbrzeOS+cNp26HxNwutru7eCOqrqkkgdEXUxVV1MwFSQBxJA62hd0fzT/gzW9t/z/t3YXvmX+G/NP42dKbF+LOVg627lpJ+xt7bO+HHZHVubx0KP1/DXbHlxfYOeo6JarPpiKeQy+eKV6dHmVdJeWpO7EydssYVMHPYRThjJ8+sctv9pefhtP3dLSXl4eJsW63Nxuyme2Ihik3KCdW/tqS6oUZqR6zjSRqIHSH7y/nMdM/LX+SF2L8eO49+TUHzhr4OpdnVm2ptqb5yD9tQ9bdy9R7kbtCbelDtiq2Rj8jm9j7dnmyEOQytNUvkqCoEUWiakSRHJuKTbRLbTv8A41UKOJLAFTqJzmmDU5Ir5gdCTlf2J3/kz7we080bFtob29Q3M4lEkK/TGe1uY/pxEZBKyrNIApRCoVlqahiAl/nM/wA2rL9x/KTYW5v5fXzU77xPTFD0HtbBbmpurd6d+dGbefs6m7E7RyGanrNpZOPr6fI5ltqZTCrJkRRSpNAsUInY05jjTbxujS3CPYXkgh8Oh0llFat5YzSnQz+7x7G22xcm7nZ+6Xt5tcm/tukkkJvYbK8f6cwW6oBKvjhU8RZKJqFDU6e6pgbL+YPwP+dvw2+OXxb/AJhXZvavx87V+JiZTb3V3yC2rs3Kdobfz/X9bQ42gTAbiwuExm4d0Q1z4XbWJoHVKQp5cZTVIqQrzwKVC4try1tLK+meJ4dQimA1poNDpZAQ1RQBaVoAPn0cXXt/7p+1/uHzdzx7SbJY7vse/aZb7aZ5ltpEnBZtcbu0cRUPJI+WrR2XTUK3QK/zFPnF8fOxvj58a/gh8MMdvtPjF8aJ8puSTeHYkEWK3F2b2LmDnHn3LJgaUxR0UEFTu3N1Rlmhp5panMTKlPBFGvlLdyv0lt7Pb7USCyh1GshGp3Y1LEAkACp054EjHUheyXtdzds3OHOvut7kzWh533pVgFvZktHbW6aKR+IeJIiiWgJAEaksxODW/wArr+YB8eejPijj+ltxfIvc/wAM+4NkfKGl+QFV2Pieldx9zbO772NT7SO3p+m+wMFsmvxuerMZk4Z5o2jqp6WCjkp6Oqp6kTK4ittW4w2trLAb57a5FyLgSqhdXVU0iFgrqSC1TQ9ueIOQEvfb2b505t9wJeaLLkm35o5au+Xzsy2Ml9FZTbfOZfEF7byTq0auhANVDFgZEZaEVaf5vny0+E/yc6t6dPw03ftrbOPo+0O1Ow+0ukavpze2yd+VO/8Af09NBP2dUbxlwdZsDI0GWpcMzS46kysc0Qq4JGjkfyQ0JZzFdbRdpZTbSgiQvK8sBQq4dytXLAshVggoFbtxjJCiX7rntt7r8gcycz/66O13E8z7faWO3bst7BPbi2twSLUQCRbhWQvh2jIOlgCBRpAy/kXfLDoD4d/LTsPsz5G7+/0dbIzvx13ZsTFZv+629d3fdbryfZPUW4KHFfw3Ym3Nz5eDz4jbFdN55KdKZfBoaQO8avTk/dLDaN2uLncJ/DhaBkDaWbuLxkCigngD8uhr98T2x5491/a7YeXeQdk+v3mHfoL2SHxreCkKWl7Ez67mWFDR5kGkMWNagUBIn/yzPld0F8ffiZ/NN6z7e37/AHR3v8jvjxT7F6Zwn91t6Z7++W6o+tfkPgHxf8S2xtzNYjb1svvrFQ+fK1FDTf5Vq8miKZo0fLm7bft+0c0215caJ7m28OFdLHU2iYUqoIGWHGgz9vRp94f2v565890fuy8x8qbH9Xs3L2/m+3ibxreL6eD6zapdeiaWN5ey2lOmJXbtpSrKCL2zPlf8EPmf8OPj18Xvnjvzs/oPsn4qU9Xtnqzu7Zu0a/sLAZPYNTS4vFphMxh8RitxZ+nMe3tvY2ikp46VUWTGUs8c+ky0wRpue1bztW3bRvt1Pb3NoWW3ulXxU8NyDpkjBD1UKFXTwABrxXol3P2s99PZz3f599zfYvYts37l7mhhc7nst5OlpKl0Gd/EjkkkhiP6ssjhixNJXQrWj9Dz8FPmB/Kl+Ivzvy+8OpM12Z1f0VR/EfOdV5jtLszF763lkO1+16rsTp3Nw5ag2Xs7bO5c7tWOuwe1K6epmkpqGhmqldY6WjUQLUL+Vt55X2XmO4uYZp4dt+iMOu4Bdnl8RCW0xqxUMFrxpjgvDoJ++Hs/96v3c9iLXZ+a7Lbd055fm6LdYdr217W3SxsVtNwjKNc3E0MU5WWeNVUM7qtCZJDqKFr+QvzE+On8wj4N4DKfJ/smj2F/MO+P1TlcVsncrde7sqsd8gdgzzR5NdvZjKdf7MyO3Nt1k61Ui0ormpIKXL0pmVoqfJVbxEO57tacwbEk263VOZ7Q6I5Ch/xmEmoRii6VeMk6S2D61kYpLntt7Oe5P3effXcLX2u5ZfcPu7cwqkt9bfV26vtN0Bo8aNLu5SaZRpGrww7PC+khngjDWk/MD5v/AAF+UHZmC39sf+cf8ofjDicRsbGbPqNgdJ7F+Vm3dq5fI0G4NzZqXd+QosRs/BU0u4MhTbghopZWhZ2psfApchVVRjzJv2zbzfRXO3+4dxYwrEIzDFDdEFgzHX2tGKkMBwrjj5DGT2W9ivvCe1nLF9y/vn3K+VOa7ua/e9XcN9uthmnjR4oIhbo0lzKwhRoS4GoDVI5pkk1I/wAu75YfHvoL41fzY+t+0+zanEbt+SHRtRsjpGKs2tvnPVfYu4l2D8jMCkdVksBtvL0G3qmsye+sSHnzE1BDqrCxfTFM0YI5P3rbdq2Hm+z3C4EV1d2QigQKxDP4c6lQVVgtC6jJAzxwes0fvHez3uT7i+6P3O+Z+UuVEm2flfmBb/fzHPaQrZQ/WbNKSqTTxvMqpaTUWBZGolKVZAxff5bXY3xN6z3z2Bmvkb218i+ht3Vm2qDH9OdzfH6ryNJV9fZf+Iioz9buKDCS12Vz1LlaWKnp/sJMXX0MtL9yJAk7U0sQW2STaoryV90vL22fw6W1xYkBo5CfjbKvp0jSQh1EMwxhhLn3oOV/eXmzl7lmw9r+TOV+Y9kS7aTfNi5lVGW8j0aYVhMoSOFo2LN4gmjkD+HSqCRWOb/Nj/mCdE/IT43fH34xdU9qb4+UG5Ord6129d4fJvsXYrbCzu4FTE7kw+PwVBi6jDbZrmhrafcqCreTHQM6YejaSSonaaUnvOHMtruW17PsUFzJfS2hdpNzuE0PJqOFjBZnCUPdr7joQ1J1HqIPuVfdo9xfbL3W9y/dvnLk/b+Udq3fb02+x5S2u7+shhrJBK8zyLLOlUMB0AStQzyhVRAq9avfyg21md39SZLbuA2zlt0ZTK57B0tBTYrC4DIfw+rUVtWmUrsxm5Vl2tQQU9JLHLW0yl9EpjkeOJ3cGXtNNHBvN/JJKqAQA1YsMagOCju48D0Df72Hb7rcuTfZy1tLSWaV7+/VUjRDkxWpBZ3IMYAU1IBxWtAK9El3zsTqnYexMR19n8bLDvjK1XlbK0lRTbkq9vrVZOSqp6uhlwM5qMy+UpKCPHrUNQ08NWJQ3gj8UQhmy0ur+7v5LpJ6Wi/CpBXVQZDBqUC1rQEkEccnrkVvuzcncu8o2mw3e1tJzTcHU0wZZfABkDK8TQOTK0iqEqyKrBidHahUW8Nt3D0O04cPTU8uCyAo6uahy+EejXI00jUqUSwRZHx1T1bxxhWhEweKKRdKJD44/aOVnNz4ldUZIDKxOck18vs9SPXoYbXY2MPLgsJoTb3yo8sNxbhAwqiqF1gMW4VAaqq1QAmkdAnhsxk9l4Sto9l4Kt3NmcfUVWczyTH78UsWTkqMdJltz1+HpWz2QqIKoi9NTzwzVKq0ovFTsAZypHPIpuZtEeFWlOIoQqgnSMeZwPPj1H+x3+47RYXa7Ht73V5GzXNwDVgqOGjMkzxjx2oxyisC/wAWQnUfrDfHY1fR5qqr0h3ZBBlMdXyySPlpd1YjEATRSY3au2saqY6DI1iY6NsfQzyQRF2DBNExmj3cLaI0SL+nVc/CVavEs9a0qckDyPpTpjYLvmTcIL6Vq3QjkVloZvGjWhASCBBpDnQPDRiKkg0oxYG92BuPbO5YoosVXIN+bcoTmnwuW23Bg8sKXcFOuPDRpU08uCRtv1gWCZ6aaVqSVx5Hd9SxB+9aWCbS4P7vl7NSuSAUJbIB1949cGlMfimTluPbt62d2geL+t9hruTDJAsblJwIhQuv09LdxkrmMsCxY1EYpwUsNRtbHtQxUNJUZSCvG7MrBuOOizuPzmJSRKGWDFwUFSuZrKvK0i+OOskoxHQuJtUqSBJQxcT7wnM1xHIHawQqIF8FzGyvp1/qVCqqKckBiWFKDymTatt9sNx9kNpnsvDj52kNyd4uGv4I7iGWBWNoEsfBee5kuZQVVmkhjjiIJMveCX3K7MlycmTpMLlHyxiWnSiyskdDQ0KExmpjhqhj48ZSxNStHb9MKgKL6vUPY8Wdo40adNLkVZeJ40NBmvWK8+zR3tzdQbZeNLFEwjhnoET4dShiAgXgRU0GM+dAJw24slicxVz52t25RjCU+Qx2TpqXHZWq+5hofucl/G23JWY2kFR9hFGQlNTrUfSU+gvFEVrKsigRlixoQeHyppBJ/wCL4dBW2u5LG51XZtyiF4pEozAgEt4vilQtB5BdXA5oQpNh1pvKiFLgpIcvjNjUGdwuBgoJ+wK3G026c8uXipcniU2pg4MrVbaxKaqytSmgM9fXZB54qqaKHxGkePOZNuuJJ7ieW0kuIzLRRaBmVdA0HxyAHatASaKigFc1D9Zc+yvNFtZWVjY2m92Oy3gs6tNv80SzXEcz/URDa4JAbaFgGZVi1zTzSus1FVDAWX5IVNMuBra/Cfc5taPGVuTrZ4snNT0qJjZVauoJz45HCR3ugRkjpnu1iSwJlyjHd/Tut7CIGaTSsZGSpGHFD5j1yaeWOgp94aXl9dxjk5V3CTdrVLMSzXilkWORWPjW8mpPwNQjSdCasFjq6CLacu6DSE5P+7a42Sip6jcu3YI6+aOprcalS1FlKKvnloJIVlSvTzQOKqN4Io1NmRZPYwKxsRIpJAqEJ9POo9ccf856x1H1yO8FwsKEhTNEtaFgKgqxIIU6srnAWuVB6Y66goymNyk1Wu3lxVPJRkYeDMV0FYuXaYwzU+VSsplpZaOoCQw1GiARRSNL5UKm7BEgJwGQ5NSMcMcPtP8Ak6MQbUpt8xl+mlhVkUxrIdYbUdQcuApU0VSAooS2oUy7U2SwmMr5Z5qKiyNXTUVNQ19HEK+r86VMvgyOSNXHkI5BVVM0R0TOtQTIv6XJZ28yOUokrKa1Bx+QpQ4+X8+n4r3b7W8Elxt8MwWMRSpV21VNHkDBx3k8Go2aYbJL/Vvi5cZkX27UZbHSJisxQ7glrKHByNkshXxp9tJHIk1SIRAYz4ptTvMxKuAiAFgpIXCyhfjqgUnAHEmvE/LgPn0ax3FuthfXO3TzoDbvDctKkJLu+VAAJKjGHqS2QdKjJUdlU+eq86mLlba+1ajeObwNBBRYylxcGRmm23TVWISvwODnoqrwVeYqpZVikDwQ1FZLL44JnEKRHM/haI31yMiKxJfgKmp1NilOHyGKjPUY7Y17c3EtmtvbQzXcsKLFbqoctEpjBij0sayEk4IDOSdLHSFsjxu3H2tgzS0WUrcvL/BKqiyVNlYMbSUsgqayRkaCqxpkyRkiwlMHlLtBN95NJqj0lPYOlnF3PCs0QRRIGRlLE4AHcCAvxnFNQKita8Mmdk2m95f2jmCWzujdRvZGIrL4aqUZmYsGUmRWESmq1R9bdy0Iq14ecyYLEzP/AJLUJk5amkeCnXMUox1LkTJF9vXTTwvHkKdYDNMj0ygC5EyKCrLp45WubmMBTEY9LDVpJalBUU+Eg0BB/wBqePQY2m8s02PZbyZ5Y71LsywyeEJgsQkDEK+tSsi6S7AoMZ8RfhYbtzS7nk2lUVFXj8BiRXUtPmKGlkz9Ic5PtutNPVYTOR4esSmanGUq9Zh0NVunjLXHokMa7bsG1W+/QXCXlxPLCPB1BG8MSKGV0aQVDMqkagQor61KjNjfvvHc6c0+03M/JkOxbRtu07juM19NHGY1laN5IJomhgdEFsvjxExlWkIHapGlWIO09JjlqqbH5GeqwVPW4jLNHlqbHxZCWsy9FiJ8tQPOlXWQVSU2Tno4opjRmsqoxUXWJ20KR74klGeJBKRInYSVohYK1KA5UEkaqA0yQKnrE/coDbpt8RU2ztBKTPQHxJFiMqtV2r36FBEZd6vQAkqOon8KrfJ4vNWaPv8Aw214fX/wG+9+wv8Ac6ftvuOfuv1+Pj9XHt/xoOOPhrwb7K8P5dJfot716dD1+ppTxLf4dGrwq6vz1/FTHHqrDs7HUuOzFM9HDmpaCpnrKqbI5uqvWZ3JzyQT5LJpTyHSi1KSRXnWBI5ZAVsfGQBrZuZEfuFaAAU4AVpniR+desUN8t1triFgjmNmLs0jZdiQWOk+uKnTQ1pTHQo9W4jK04xUzZySuwGYwFW7Db2TpKWswaVGRkjalyM9dBT5QZClnp5vIKeIoqhWV5I5B7LppI3mmURFZEbSxOKmgNQK0AINfXI+fQi2+yube3spjeLNbTQeKBC4JQM5GmQsA3iIykEBaClRUEHoz2wdyQ9eGTfm1PHU7UrMk8taKuA01KtHSQyJk9y4nP1v21fkPMMdTQyxefwWhaS4curIru3jvImtXBLeg419CDX/AAdCLZruTaHbc7UstjICrPSg0/ikjc0JIIFc0xU+fSw+S3Y3xp3N15WVmA3fj8XvTMSymLDbYrstlpK/GwUcbVEVRUYSjyO38ZkqiVolUVdVG8puJCIgT7K9pg5jj3H6W5tw+3pED4pCqNerhpLBytK8FpjGelO4jk6z5Znn/rVJLvs80jLEWaWQREEafFij8IOcEBypq1CdI6rs3Rjc5uKor8tkd4LuZMFQJjNvY/eG+qOt3TLs+mSupcNUYWofI1mBr6XH1wKfwjGV9VVQTlo0geIPN7FcDQWqrFHbeFrYu7RREJrwW1YqCVHxsAD61oOo/wBxtrvdLm/upN1F0LdAkK3t0hnaBQY4jGTI0cmg0HgxO7rwVSis3Q57Uxe68h1ZBsfP9W5fJ0uCjrZ6SKlqaCkNbPVZCszcB3IsldispgjS1desRnR5ZUiRkljQKodNK0KXxuUuhVyAK8BjTRfI8K/ngnPQrtItzn5Xj2G85dk0Wqu50AVcsxkBmyrRldYXVUkAUZRQVWO1GimlwWMwNdWyydYxwHK4XeFNlpMtteqijWBVgzkdQMa+3Mo9NNLSxUz6GidHJhUR04YliPfPIgDyfiWlDXjj+IYrX58ePSqzu/EaxsLW5d4LFdXg3IcvEwAOkPXT4LkErpOQQTowvWPvCnydPVpujILJWb53Vjq2hzabdxdPlHx+3MrFBDUTx4iSDIU0dNNipCaWmqpaKqmp2ldZUXW7o9teKT/F0b/FomABYkVZan4sHBGSKgGgNTjoR88WN3tiW27XX/Jd3CF/HitlSQxwyhV1eF3qoaI1RHMcjJqYEKdTFN39j9vR71bHYfJTyYVqgUZ3PXUufo5MrClU8MmVrcfnqeDIU9ZTuhjniVEhR4dC/paRj6xecWeuWIeIoBEalWIxnKmhrX7ePHh1FHM1rtcfMM1rt180m3GQoLt0mi8RA2HaOZQ6sABqX4QQAOGorTYe2a2ekzEeKyG5qypjlq6Khl2tNt6KnieIT09Mk2QaoyE8oycdb5FSnaPwuC5Ls0b+2LiZdas0Ch8Eh9VSTnhgUBx51FBw6W7Tt0kkF0sF1O+nUENt4YVQDQFm7iS4zRaUNSSSehK3JiN54vZsDb069o6EYejm25JueozKCGoipJqRy9Zt3b2ImzFHhqWSmhWqQxA1ANlkRfKQ1E9u8yJDKc5KjFK100JNCcYoajj59Lr6z3WDbBc7jtiqi1iWcsKNp06i0aKXVRjVVaN5HB6DnJYnJbhmqUrMQ1eHxkmAoMpT7crYvMabLwVsGUwM9Q8YqWo8fAYZvJLFjqKlm5qSpiVrxyCELokoKhqahwxUEA/P7TSgA6RS2k+4PIktpr/TMKOI2BJDVDIzAV0jjUhEVql6AdImnpf41kcZSZDJZDJYOT7DCGrpWmNRHW1RqqnG4WmqJKaopqmfzwM2sRSBfIyGRgFcvL2JrWGk4q2n5cCSPiAzw4YqBx6LAguZlinuXewOmISKTXUTqVFJBVj2nNCfImtOjN4ujxVRTZjJGkmzlfubcWBw7S7lEVZiq2WVHx9Li6TLRxZOWKtoJJH8g8DRPUStGZ7jhCXogDYVRXHH1/wefoB6dC2C3ieRzHG8tzPOq/q5U8AqhqMdVSailKk5zgb9ibf37WZungxtf/DYsBVpX09aNrzKghaBMZJQ5Lc09TmKuukleo9EUEVPPIsRZyyCykm87jt1taUvqSI66THUVandUKaAUpxJ+ynUq+23J3Oe7b+By67Wt1aTiUXhhk0RaqRaXnQSuSS9AiJqahJqB2jtm8nPQxVNDUoc1Pt0QV1TmKn7eF6utT75ZMVi6HE1NJJgqmk8UUk81UrGSnfxokweRoSPbLd9wdbq2ZYbGQf2a1NQaEEu1dYyaBaKD86VkjnvdYuUoZOXt2tpb7mS0mIa8lIQRyJ4gaOO3hMItWFELtLrlZaKFKsxQGa6q3ZuaOupslPlskcbQZLKY+Dby5OrpKikRJaaePeFNRrUJW02JirEZmleCORoopWXWNRF0NvY7eoWNUTUwUFqAkngormteAH5dY+7lvHMfMc5bc72efSrPpTWw86mQDBoDUk8aAmpz0nGp66lrcJWwUxRHmgxVakEhqsXlo5I3aT7yHIrVFfDURxkxwsgSUL6rEq6woHDDV3cfQj9nRWJ3tprOTwQIQBEfNXpnuDVBzSoGKgevSbpdr4mfcVVXvNmftly9JRLRY6rq8ZSVBpZ6TJ4rH7gxsVDHNWUmMrIVmpZ66WKkhnVpE1tIpZiViqBWUcDxFaYoSDxFR6ZPn0tsraOe8keO5lCMyIVjZkDiodEkUAAhWoQznQpBK1JBIxUO7cpnkyz7o3Ds6Woy1W9Nt/G5OXbmGyeEdZI6CHGbfkaamr822WEqRxGQ1FVKzMkbMGKBFDYwWUH09skhc0LE1Orian8IoK8KAdDbl7m5zzzs/NHMl3bpYwTORHGqKYl0FAkaj9STUzAAksx8iemvc9bidhY98jvLN4rb0AhWopYshUSLX5aFqtMc0mBxkUMuRzy09XIFn+zim+2W7zeNAWFhBPKxWKFmJNO2mMVya0H59ZMSe/ntpYoz3e6zRimpdUEoLCoHYNNWzxpWnnQdQ9vb+2RnMjjsfDunF4qLLCN6XObpFds/a8S1FHma/HfxPc+6aPEYLCSZmjwFU9DHWz08lYIx4VcumpFPHNHHMwgZ2Q0ZIqSPUFQaIhZm0lhqoDSuejbb/vB+2E9xBCd3mijkys9xBJFDQh2XVJIFVNYRtGogtTAyOn6i3/sOsz8+2sVvDD5zIUdXLR1tVg0ymV2/RvFV1GPE8+66PHSbXWiqaulZaacVhiqw0bQNIssRdlra6MSTNauisKqr0VjgHCMQ9RXOMedKHo0X7x3tOlzJaxb7LM6sVdoIJXjXJFTIF8OhIwQxDY01qKr6iyGLnx1Rl48rj2oKSonp55/M1o5qckSx/5vl10EgDlgCQCAbMNY3hIT6c6qeq/5+jOH7yvtSsRmbdLrQGp/uPL8/l0w0XZ+zqvKY7C4uo3BnctmGqP4Tjtu7F35uCryTUUNXU1cVDBh9s1slRUUtJQTTSxKDJFDEzuqqCfbE22XkcTTyoiQr8TPJGoFSAKlnAGSB9vS20+9L7SzXENpbXe4zXT10Rw2NxIzUBJ0hUJJoCfkASejLP1nuyj27ld01FJTph8L5Wy8qVST1OPSnIWpeox9OJa/TTAkvpjYqqsfopsHDMkt7bWCf7lTAtECQAwycMTTy9f8I6H6e/nt3b7Vfb1JdXn0Fs4S4ItpS0ZJA7lpWlWHCv8AI9MGx4Mf2DuHd22Nj7k2tu3LbGp8PUbjG3twY/L0FNFm4a6Wj+0y1BLPiso8P8PmSpWmmlajkXROI2IBZvoLqzit5ru1kijldkQyALUg08yCK17f4vKvSrZ/vLe027z31ptm8z3E9rGksohgd6K6lqgqCDopR/4Dhqdd1eQosVjMvmq2SrTH4GifI5iSDC56ukoKCKmkqpqySnocVUzzU8MUbhmiWQeRGjF5FKhx+X911xxmBQzGi1kjFT6Cr8ek8P3u/ZcRPP8AvLcDHGNUhWyuDpHqaKcD/Y49cDu7bEFBgct/GY6jHbiosVkcZU0WPzNcngzFLHVUcdetLjZnxNWsLXqIKoQzUdiKhYiDZM3K++OzBbIVBIy8fr5d+R/h8ul8f3zPYxI4pDvF+UYA1FnNioqAcYP+Dzp0naPvHqysy+dwdJuiSprNsZZcHuKePbm7Ri8Ll5K2rxsNBXZmXAx4pZqmtx80cBSZ0qWQ+Jn9p5OTeYlVC1iBqytZI6kfIa/n0tg++77BM8sab1uDeGQsrCyn0oSSKMSozg8K18q9PNN231lWZSow9FvbDVldTYyfNTRUwyEmjDQpEz5VrUIK0IFQnrIHBvbSCQmPJfMrKH/d1BwzJHx9PjpXozT78f3fUn8Eb9fsy1aq2c3w/wAWQDTy4cep8XZGw2p8XUnc1PHHl8RX56hE2Nz8LvjMd4hWzTCTEKKWen8qloJCk4DD0ci6ZuSeZdTAbeDQ/wC/Iv8AoPozh+/T93tY0Zt83EawSB9DPWg417afz6Dit+VHQePrqnGVW/wuSpataKShj2pvmeoapZiqxwiDbEiVF2HBRmU3Fibi7h5A5rdQy7YNPGvixUx/t+vL/eB/dthZ4333c/FBppFhOSSeFMZ6UO4O/epdq1OJo89ut6OtzkUM+Ioodu7ryVZXR1FU1HSmOlxWCrp4vvaiKRafyqn3Hifx69J9pf8AW/5rcsU25SBx/ViFMfNx0aj+8I+7fbmMTbvuwZvhH0ExLVNAABXJzStK0NOll2P2HsPqrLLhN5brx1Llpce2WhoMVTZfcdRPQJTUdbPLTpt/GZIzvSUNdHPPGl5YafVK6rGjsqC25I5nv4/Gg2z9OpWrSRLkEjzceYx69Cfc/v8AP3c9huBa3u+bkZ9IcLFYzOSCA1RTjRWBPmBk46DTA/KDoHcuaocBiuy8acjkqpKOg+/we78PR1FRJcRxnI5fbtDQUxlI0p5pI9bkKt2YAvTe2/OSIZG2jtAqaSwkj8hJ/g6as/7x/wC67NcR2ycxbprLBVJsJwG+wmlPzp0KfZm89l9R4mkzPYe7MPtylyEtbDi4ZxkavIZZ8dVUFJkBisbj6CrrsgKJ8lA0xijYRxSrI1kN/Zbbci8037tHa7XqIA1HxIqCuRX9TFaH8+hbuH94V923l+Bbndd53SNXLCNfoJdT6CA2kedNQJzwNegb3r8gtvUu3cQnXbU/ZdVvv+C09DgoV3Hgdt7hpM6K2jfbtdvt2weJwG6CqzKmNqJZ5pp4no56UtII2HXJHJu8bVeblPvUAtYlTSJNUcjBlYNUINdVoK1xQZBxUYR/fS+9j7W+9+2e1m3+1Ut3ue4QXFw09pcwzWkciXSQxrF45eMCWqFdFWBJ0MDq0ksOS2KsG5cLncVkI9vy4LHnIP17u2OtlrRXtTVrVCUuTSsqsZiI6OhkFJSvSBo5I4ViLCOOPxSZHc1gkhKF1ZqCWKlKVpkcT6mvD9tcC5eXVg3Ww3OC7S2uraHxW26/1hy4VmIDglEAUaEZfioAaBQVdKXL7l3DtDBp/CKnH5ieeV3NKlQtJTwK1VWrj6ekRY8nJelaySmOPVdlX1FdVlihguHcyAJStG4+QqfIfZ/Prcu8bxvuwWVvFYP9brZaw1CBau/hqg7zQE0bFalePEHNs4en7Qi2nh6Pb+4MXkttbi37uDL71mpnx2PzWwKycNlNoU9Rl67FU88NGs1TBWGVIoqeGeSJ1mH+cUXUzWElzcSXCNBLGkaQjJWQE0ftDEkkrT5iopnom5X2lecLXYdns9luId1s7m9vLvc6+Gs23mNDJbAzPFGFiAl8RiQNMpVg4AqNHTXXmzMdicwKDMDcMOercgNqZlclMMHseB6zK46p3FtXA5TIzYGbLVUUFPFVTV9NWpGaNSs6xzMjFG63V40kEhBTwhWWPSC0pop0u4XWAudOlgTWhBpXqVfbXlXlqO23G3F2l2l7IybfdtIUhsEZpI2u7aCWYW7SuFUSGaN0QRgiVQ9Co9y7a3dX4HaqUfZu5Nu7lx+49xbMMsm9MbsLfe4FxtU43FRbY2htWWGuz2GmfD07HI1ES00iyNNEWYGGRLaXNg13PDLYo0BjS6qYmkiVWwhaWQaFfuNEBLCg1CmenuarfmAbVYWdjzpfRcyWc9xtFxGbuOzu5SsjCeG3tLQ657cm3UtLIQr1LrntZB7awe8ajdFYJd/ZzHw11VTZPIY+kw+Pq5cVBUSxLWZDddRlaiKqq1qqnXR5GRbqIdBcBY4xGdbhfW9jaxN4SMGwgJpXFRpp6DIxWvn1EnKfLm877vl8BuNxA61e6KxhjGurSzT62U6WbtkJwFNWGB0O+bwFVjsW+VXL1GTw9bqpfs6aoampoaiRZBajeoAgixcEsJZpVkWNXLP4yzG6Db93gu55IDDpuFGvGajAyRkNQ8PMefQ35o5F3HY9rtd0i3LxdpnfwiCdFHIY1QGitCGQguDQNxWpFSl14XGbMxmP7RqaHJ0ULZqiyUgbI0+PyQORq5cTWitxtJQ1eRkoAYvAk6RfuWLXdFX2fChm122sMacMkGgrip4+fUUTPJBtltab+YZLePxRwZVca20nWqqW0t8Janz4U6nyYHa8mNipdvbb/jeOxlV9zFS02eq2o6dPuTVzDHGiWuovv6SvkbzLTyKyyJZmEqhfdVLnU7OSxHE8Tilc+o/l1a7trJRHFa2Ya3Q60jVyyqD3MqlarqR/iK+fGjCnSyhhgyNIstZKk1DRxwwwUMe3qysr6ifI1tVWUuGFaY2aoroRTmWV28HohDBVCAe6O2g001ZvOooAAM/IfZ5/b0uto1uk1yTgQwgARiNizs7syxalHc2KksRhcDtp0/y1GayOLyVBjqV8fnZ8jUQvk8iIq4xUEhEE9Sw0GiCyU620zklZ/W4Cot6BoookAbtOAB+3A6V3cW87tuF+zQ6blWHiyPRtI4EseHD188nh0yYPK4qlylDksjVU9FQQx1FDi4JItJy24IqCaGix8FPkIKqOOUQieqiljNoZo1CsdWpWp45WiKQipLAseFBXjimK0FK56M9mvNqj3KDcd5cR2kVu8cKEV8ScRaVQBwwU5aQMAQrAUIqCIuN6/nrMnPWVcFBPXz4ilTHZDNZGKDKutDNW5CaKjjSMVDrUxTh9MRZNAbULDWXZbpIlQOWKsaDSKgH5ngOiWz5emvLyXw/CMyQrJ+vIqOy1Ldo4saGtFritcZ6VONo9t1GMylOYq+tmFDSY6pSTDVDVUsVck38OoTV1MiRVazJI5kggcByPUoJYe2ZDN40Q0gDOScU8/L/D0INvXYztm81klZ6Rxqphq51E6U1ls1qSVXjQVHHoGdm9LYSm3JBU10cORpc29VUTUdVgKaKmx1ZDXGpp56N2gq58NRLxEKdZKlmDfqc6QV91eSiBuI0qBQE5r5HNCf2dA3l/lW0l3W3DhWgndmrJGKIVNQQdJKqTQUBYjyqeJwa4YrBYPHV5nTF4+OOqyWTxudevpaON6KBWqcrUZHIJNBSxpROrxh5VmdmDohUEgMW8rzX08EkbNIoHhzxhSAK4SgOomvypila46nXd4LTaOVtovrW7hg26aRvqtsuWuFkZvCqboySRGGNApAUGXxGJDKgSrdeDS52i/jOOr6mtwNTFRZOg/hDpU01OuVo4QKhcg1THSJTZGazzF9KlkshTi65NNsyRyIomLEVbBbSTjTSp0jh/PoJXPh7yZr2yu5DYCJHEcPesZZFBbxNYQLI4q9QBUUWmOotP/FHfM0GQoKaopMLh4GoMzHJRNkJga3L1s7ZCKONskk81RRU7iujZ/NLMUZSw1e63UUUcls0TlTI3wmtOAUAZ00A/CfLI4dLeWtxvLq13yK/gjl+jt6JOujWvfJMxcgGUlnC0lWtWOlgdVRyipZzkIaJ6zDLUUOBqc5XQ1JgyKUCZOnq0x6T0GWo62OtrGRgIIIIpqiOr8c2tQmpU7gBHbw5cyrGNFVLUIqQysCq4ySQCtVpmhNGu47l7K0mu4GUWrXMoP6nhaw2gOkiOHalAEUMwcq+sBaiR/Bl02+wnvp06L19vvfLr/iNvvvNo0/ueLV4L86/F6fe9b8deONe34eGnhTjivHypXPSn/FuGg6/F0U/U/wByOPi/2mqmnOiunz16OzqqrtTaG8cNkaLNbrjrkbNwRqjZOqp5aylnoqCklq6GcLICjwNMQgNy7BlLySh2I1sZ0MfhIoqvmtSG8q8Kjy/L0HWKHMO3X0Nyl1ftIGkw3i01KQoJU5yeNPUgipbPRxOl9r7Qye28TTYDD0Gdiiopq3JVCrTmqhqZg8DVVdWzSU7pWyWZRFG108RW6R6R7Kryd1YvOxV64qOHyoK9D7lrbbK4jt4LC3SZSpLZAPD4ixKipocAjhTA6WHYlPt6LAVM255M1BjGmkTJYa+Ypy4Z46HG4hIsWpr63GSKyxERFg6k3tGnDdoxLADTQfC4Iz6muKGvRjzHDBDbO8zy1Y0lgcPVaqAiUFS6gY86j5DpQ9gV22t3dG7b2tgOuJKXZVPWUUdZunGY/btKMoxx1RNHX0mNp6E7jxq0xhjSM1DqUVSWiJsCgto5Yt1u7lr7VcOKpFV+1QR6sUNSTXtrmnDpm5tY7jaIImsX/cLlP1FWNRrVGBKgDxADpUAVFCCxFW6bemKHZdb1bV9f9zZLY1HXY/beRr+s91ZvahkioMti6rRHtbOVdE0LRZiXHStJS5CRgPFG1I0wASQJd7m3WC7tbzabOWWGScJdwrIMRsp/VUPgqrAakFDnUASCCIeSbLYZ7Jdp5u3O0RRZyfRTyRELHKD2rKUoxfTweuUrGWwOoqjEYd8pnMH2BiMfg85I9Y1btLKbX3BTUmZx2GiWvf8AidNDlMDtmGCOVKiqpq6plQGSOVkYSIPb8TvJ+lJaSGVe0rKrpgnyBCs1aYIGSCKjPQh3GysbC5k3DbuZbWPbrilxr2+W2uNMscXdWSMyRWy1NXikc0qrFWBXormHrs3nKr/SBBPlN0dib5p6vC19a+GoMDgcVQYaPFUWW3B9ht2nWmrsZiqWhgj896U1cshYRmeOW58+hFFriO2joyqxJY1FQtSSa1PzA/Z1D1tLe3c0m+gPd79eq8byKkaRoIyqyS6IgFKKqjNFLHIFQ1HvfMsW31oFw3XlMjZyWklw9FjaOGow+dyVG9B4cucdiKumq85R4ZcjL4VrDc1tRCzhkClk8KmTte57UQ6mY5ANe2tDpJp5DhX5joz3WVrV42tuXQv1LjwIY1rFJIuikulWUyrHrqNZPey6jShIN7y2XuwU9buXIUdHT0r1cyw4+orqBK7EJFlJ8NSUEEgq45a2RZAZQlN5IWAadrC91tvPDH4SVIQr8QqQ34jVdOPSvGmPmAfum238jX120KBkf+zZlDRd2gKra+8g5otRWrfIrTajZ/b02Izm2Zc511Xbf3Tt+aXKUmexsg2/T1TxRUMm4smYaOiwtNWx5GcEZOF4qhnCTDxyBSmuI4JXkjmQTxyoQyspzx4Djin4eAGOHRptbX9tHBcbe01jLbzIGljlUBA1FHiyUCxq+sg+J2tWjYanQrbz3NhstDlNwZHt6ozWeqcZLG8G96Cn/uvVUlbSLHFlNuYWg2ZPTS5eLIUskkGUxcRFNUxJHL5EfxypYYinh20dlSEOKeHXUCGOGOoECnENxGag56FW4S7fPaXN/NzRrvfBpS7FIXUxqA0KLAwZxIDSSMAKQEbUGAZOYHIw0NHlX3Ftv+FUePxv90qSlzLU80zUlDQVqVxjjpHgmYZOSgSWaJ6dqeKmUtBqUNJ7dkQ1Rkl1EkMSK1zQ0/In1+3OOkFjdRwfWLfbb4cccRtUSTOFBBIAI+MqCQVoFPbWleoOO2XJU7Ii/jmMx5jwGPyrU1BjIMfX18VLWrRwY/IrkpKiahatMTS1M9RVRQRQ3VysMa87knUXOpHPcaMSSBnJwM0+wnqtpsks+wq93brW2jdkSIKzUOlUbUajVSpJcALg4HRkNlbdij2tBu/ciZKv20ccsk1HTyYza9VNjcQyxVucystfNtzHUuIqZ3SZnWa9XT3anR0KBw5uO6kStY7fQ3TEaXNXUMRUKoGolqV44U/EeNJi5R5NWTbIuaeaFlPL6QsZbeExW8rxREK00rSNAkcLyMuQ2qVSfDB7Qwmbg3/VU21MTDt4Y6hqa2anxVLNtySapyuLqGzngpsPTYuOCuyWKpZJGkp2ytZR0715ElV9jHTAQMS2WxPJfXNxurl5BVysg/Taq01MxAVyFAoilhHga2bIlDmD3Vt4uV7HZOQbT6WOsVpHdW5b6m3JmMi21sql5IYzI0gkunSKS6JZxbQQkwsGlLJm8LJv/NQYylzuPeoq5Mpj8zumLb+36tqeIOJIc7WiePENR1M0kyzzKIgkYFQYo3MqjCONJIrUB2jlUArpXUaYFNI9Rin7MjrHncri8st15lle2S6sriZ0mEs3hxM/xF1mapTQ5LBj+EUchWJ6E3rHMbZqqKryVDlMpgql9j4+kqMBtOfIw5ff+Lz7maUz5FcTJQZWrvoSWERghGEoMcbxoEm5R3LGBDbpIol8USzKCsJUYNCykUzQg1HA+vVdgk2aUzVM0cht1i+ntWbXc6j8VfDcMeAKgDPcCooOg03DmYv4rl6Op2tmsfV47G4imenr4llhSjWfJzVNfS08FS0pr5nEN42s1NoEZkVDpJxbMShkWYOpqQw4UPkCONPXz49BjeVAv1tptvkhMSANG/GoJOqlagmvwn4cLWmOslJkGWkSVcPl8pHBlqRcc9dUYQUk9Bkl+2WoiqaCujmRYJKtxCtQKioiFmkVkjK+6SRu4ZeFfMccfL0Pnw/y9LNuvbe3lilWJpFRh2SFApDArXUGBBUt21DUNCwIBBh5KipqiSppP4PFuGnqMlTQ0k2QoI6CnGQoJ9eOxrSiKomqK0vLqSoolYRubjS50lwSFVUuQrBCTQ/tP2fb0hmtBLJPDaxtMjzqsTMvFq9i0FdTmv4a5p59DDvLq+gzuyhsve2KesTcNLJk63cmIrsf/eXYgxVA2agwGHymWpctUV+2dwbixVFB9hDCZZK2qmqhrVWMEe/1inn3ddx2maojkWAQyK3hvqcI8hA00eNCzVJFFUA5KhsnZPY8WPLMfLnPFmkctzZzbm99BLCbi2MNs80FurETeJBdziKJERCWlkaRWKJIYi/bD+MOwameqwu8do1dIW2nk9wxZmt3Tl6TIfwyjkgxv8UxzYuKrwS1ryVAqY0qoGiEi28U8JOg537m65tfB/dl5ruDOsBjjRHXWTXS1dLAeRoageh6Antz93223y73C15o2Q2tlHtM27rcXdxLA72sNEaaEokkTMSaprXSxFAHU4WO0YNqwdWbH2/V7Bx2Xi2dlMwM/U4OtxVJuOXGz1lfeseoraqhxlfkcVQ1cbyuv2grJI3lRl1NA1jBdx7pf353BzPMq+HHIKxo1BULQFgGIIFSdINPmUlhY7Dccl8v2H9VoXjsJp/rp7aVUuZIi7UZ9cixM0SMpwEEjAtqyUBec1uDs3EUdBW9dU+akOax9ZjclRZ/aG3M9S1GHjQxrSZSmz1LlMFPkohWGGOSOnnqKmJb+b9oBxVCLVy63T4H8LMM/lRqY86fMdQvfw71BBbXGz2cpWWq/qwxuCoqKHXqQuK0wGJ8mFMrnrbvqtxlJt6ul2ZuTbuXhkzlfk8jQ0UseBy1TW1OQrqWm2q2QkaajVsTVwiaiZ6m8FNM0EkccixRJr+w8WG6haeOS3eioDlgKCpahydQJBFKVApipMNi39IJdsuv3TdQbhH4jzMgpG7EsUEWrKqY2AZDqqFYhgGCrY30Vv3Dd6YjdWwcV2jDtrcEmxdxbi3tHU0FZtGnzNFiFWlpsLtuk35UYOrqq7JgVEZajqmq4mi/suwnMa79GOWJtu3N9pkudNzHbwMuqRozMSGkfwUfSi0FSRpzk+XU0bfzHZ79tt9tMe6eGtxoF3bW8UkfiMpKowFyUYqCzBtLBl06jQlWII9K78wPUeexNWuyQ1fSYeOmjyW3Ew2I2ruDbMFPHSYrBbwyhim3B9hH9yGJWDKVaBAfQ1gRVve2SbxC8UcsdC+smQFnjdch4xXSXFBTKj1r0Etkul5ailCWs8V+9uYIZ7fQtvJbyDS6Tt/aFCG9HYfLzl57vrsHL1GemzWL2lt7aD4jH7bOJwcu4txZCmpJMnlHqd3ZKq8s+Pqp925bOT0kS0FFSUUOPoKUus1R93UTbt9js4nt5nuppbgP4gLaVGAAqUA1dqrU6iTqZsgUVbScwb00e/RS2NnDt0qiPwkVnaJK0MqstFKzSMVVgCKKozkkpvY/de+uu8jTtmaIUVLFLNWbTh29BQy4zcUdU00VTVZmpq6vVtfK0StDWIrYzJx10twwUFpiLbeHxyNDL5h64I9NIp3DyORTqJd1u5dpqJ42Ck6ofDIZXBrqDktWNhgjtfV6Dj1Eqtp7x2fjKGClzs9fuup3dBU7jw8kueRN/wCZqsjV1Lbo3Nm8luDMT0WVStKSTtDTRw1i05St8qeKKNvUjymQqPCp2EUOgYGlQAAVp68DkdL5rS5srSO1V2/eHi0mjo4EzEsfEldpHKyBqV0qAwFHqAAJNTXbzqzT7cm6+21SbiwuVpN0ZrPwb8rqsV+LmkqHx+CxlE1FPHTTzYdfHUp5nNZGCUSEnQrYaOrSCdjEcKungfMlq8CeGMedePTxtL5pBYttkK3yUllcT1qpFVVF0katHEaiW8gpx1M7p3jjOwzt/M4HLDZGLhSGXdW1Mfs7B11Jj6zFl48xW0W08pLCcpjcGkkMi0pq3iSoi8sSGoMdke0xXlrHcJdyrcMWbw2dip0+QZgtAa4rThQV4noz5ruOX91m2ibaFlsLVIolvY0iWSkq4kkiieTU6qKEKZBVqkAVUArOfwEu/wDetdSRbkjq6mQ4/EYvJ120KjZNTu7MN9tDj6qfCRNPiqKkkkyT09G4liqnx9PE7UkUjNCDyO58CGNpI1V6ksocPpX01YNaAE4pWoqePQFvNrj3LdLiCyvXmjoqRyNAbdppKDu8KrqE1syodQYoFYxxklAjM7nFzO3jQZeGix258NPRiuq8qMjPmM3R0dMMbhsPgYKfCSUe3qDDUkkstVFLVQxVjPG6gtEqBRDH4cuuJmeBhgAii5yTU1PoMEjIPRXdzx3Fi8NyscO4xMC5k1l5RTSix6YysYUVLamCtVSvCnRs6vtDEx9e9d4vD0u1MHVPls/uvt/eWTrcpRZnK7lniwuPqEps/Bh8huDG5Fqz7ilTG4CgqqdqMF5oJaOEz+wwlncHcb6d7iWSMoqWsCqNKjLV01VcihLSMCDgEVp1MMu7bNJytyzY2dlY21wkstzvW4XEjK8j/px6Vk8KSYMrFlEVrFIClXZGRDJ0DO4O79qvFkaTrvqvC9fY3cMc1NuSvyGQot9btdJq2atej2/lnw+0pMDhpI3SN4VikZ2TU0xsiKcQ7bdhdF3fmWVcpoVo04AHVVpNR4kZGMU8+o83HmjZ5HmbY+W0s7SYlZTPKl1MAWLhY2EdvoSlATpJJqS34QabJ7or6rqLY2FqdlUuWhoaiXP4yt7OqjUV+OiWkOOxdDjqmPHUBwOEwWSNSop0jr8tNNIrVFdJH4BATwQldzvp1vMGkRSIDSPMs3Eu7CnEhaYVQSxMgbkXHK3LsE+yMY9DXMb3x7iKlF8MqieFEkmoae+QnLORoCgDPnt/4WCOb7+vyMk+W2nTyY7EQ1E+NpNqY+jgar2NhqSspxRUmOpsg8f2lPRh9SorFi3q9mrJbOxBixRiCeOsk0Y0rU0PH7fLoDx3u62gidboltcY0KKr4S6dUKhhRUDCoVfQefRokyFDVxUudqq3BYrFsKmpFNkKnHY+hpqehpqaEF5qlWqIMdQVzIkkCimKETF5CByWNbmKJlXWWqBipLVJrjzJ/Pyx5dSfa79HuG62rzvbRW5RpGWTRHFEAo0BmIxGrAVA0/iq2a9IrPZjF9gbOyvg3j1buPcmfy9bg8RsjaWP3Hj9uR0u3MDRQRVUNHumGXcb1BrNFRJU/elIpKkvQ8RqwbtRPBdRxzW9ysKR62mnMeolmJ01TSvw+WngKNnq+6HbLzl66aw5j2m83a7vmgi2/b0uBCqxxKFcJcx+LiQijeIQNQMVaVBJ8XuiPMVVDtjdVHla2ird0QzV9bg6yOt3PCqU7Y3G0O3pszNWUR+1q5jIxkkMtYqpEKiFbuwlkthGktzbaTJ4eBJUKa5OoAVyPlj0PUJ2W6RXE9ttW9RTG1a6BlktirXC0BRBCZCUqrnUakF6BQ6Cp6NDjN94egi/0c9GePFfxTdy4/bG9KvOV+Z3jHBWJiTNgKvY1Tga0xsJWqJI6mkkShNUFX7x/GpYOixmdlvt5fWPCDPEqgRas1YPUE1wCCB21OkEnqZoeb7Hb4JOXfbSN7YyXpjtdwmmaW9COsQFvJbeCQmhtbK0R0GTSvivoWondbddZCg3HWb0qhhKzcsNbnKSgzD/AMalq6LN1dCMOwrMtE9PV1MZohJejcyKFk0pJEjG6Pc5UuLf6NncRHS5RSKaQQ1QpxSo40wcjI6EvIHLt9tW5z8xObV9xVri3juJPGBW4ljaIiSaPS7EqxqlTqBoxCM1URuqjyOV7D/jMu3qPL7nwU2RpRHkmrsttvGVRpIPus1DUUdRWGirsQkkDUKV3lQ1KF9DNpcLzEp28WsNy8cDhRqFNRAzpOODcGpTBIHQBa5u/wCt91ut1s0F1vEMkwMcut4onKlTKulz3wGjRly6h1UsG8zNJncbl9m1f98K6HZtJ97jIMxvCuytZDFkqurcw06NWrRxAukM6q8NNFIaRDHGbqguG4LA7ZfyTW7NcSMjFIFCgIBxIqcaiMEsATWnHqcdy5mTmzk+2sd6gh2mCGaNbzdZJZWe5ZifDjcgaT4atQrFGSiCMNUIOi19zbfr85tKegwmQpNx/wAOykNUtRjnx0mM3LtynCVcc8GQx1QcZ4qfFZCGedoJHMdREQEjk0qgqsZwQsjo0bldRqCCrUpkGhPd60BHqOoG5u20Os0NlfJdwJKUjdNJSWJWDFgy1QDwyCdJJVq0AbgCeysftra++a3EYjFbxr8jHS4CnpcrS1kZpqOtqXqKvKy1ppK3Fw5ChNLPAaeMxrM0lMQItdyTCSSSa3V53jBLGgHpig4Ejga5pkZ6CVpb2W27ubfbbe6cqkY8QkU11YscFAyiqhRQN2ntrWppsbUYanqpKWqGUp8jRYoUa4VZjSZSnc4p1nqo9wIdNHkKmqJmlfyeaKOMyJbSCS6bW0OhGU1pk5FCeFBk46Ge1m0h3IzXEcylFKiFTpk1CNu7xOCsWyTXUACRkDp+w9BV5inyhjx+ZORpqSnydPS/xlszJUzR01cYI6WuSYUsdAGqHhkMkPlkc+QRnQGKe5aO28BnKhT2ljgeXl6+nDo+2GK+30bultDO066ZUtwTLIxVZKAPUDRkg1BJqCFx0p6CKWeqlzdPgclL9zkKbCSpkqRBi6jIT4ykr8jhIZs5BJLUz0QylMr1EJTxN+3cBmQJTR4xbNcANGpkJU0OmpCv20wdJx5/l0II7pbbdrnc49okka4ZLYQXCgprdFaaD9cM2pSyjWpBWgWoDU6RlXLj6UwzLhTS0tBPlHyVRnq+mrTE9Y1ZHSwxV09JVFBRQSuiymJYogFUaFBYGCpIy0kmBNBQqCOFCTSvmfnw6Bk9zY28plttsZIleQzCd1cgPrRFDlDQqpoG0gVAIoc9PopU2xlqeOCrxuEXG5CmY43cOKrsrLHS1tJHBSYbAU1DVwU71r1szTGdvLTq7srK/KhtqywlGBYPjUhA4GpJJyBTHr6dKEEdhfpcW00cQt2qIZ1eT4l0rGioaM9SWLGqA4IPDpSbQopMpuKIpj8j9xTirq4stV4+0FfPRQhYpWjCDy1ONadVjJhYSTc+Eabhq9lSG2mJYMtACoPAHj+RHHI+3pbsFncXu7bfGUmikEpdZmQ97qQR5ZaMkAAA1P4B1OzeJr6ymqMdksvSUGWmp6I5pqLF0aS4SprKtoI5GSti8QrsPSLHAs/2k8QldWeMjkt2UiFFkgibwQzaKmusUrjjhjUgV4D8ulnMUM6Xb2O53sZv5IYhMY4wqwPq00bAo8UYC6tBFTlTx6ETJRYmPF4WofLz1OXq6ZoMpjIKaWkyONl8TUkenI1kNStbkKuAySVE6xGLUSANIFkH+NhrpRCFiV/03JBVgaH4FppCnAFa+fHpdttzYz3kUFxDILVrdWR0NJC9WSQCVw5dzXUzaSvEAaRgPXyVPjZ6D+K0cdJLS7frquqqa/J0pi2/i8XJLW1P3bRpPRil8RmknkCRQqupmdVAYuTSNP4zRSDSZQAFX4mYACmQa8KcT5ZOOjzadsstmFgm42Om4WxkklkeVT4SRsWYuAHUrp1ajRVplmAAJ4YHJ0WTqs1Dk8ft7blHVUW6anD5fKVUmXl31TUVDR5aHHbYo6TGU9ZR1EWQlqbSyVYjMMA0MQ6xNYeInhOHlmcPGpRCFMZNQWerUK6aVAFa+XmCTe7omRLS32eCzs52nK3bnxBcRDTIREPDV1VXL0OoggChp29D9/cjZn8e/hn+knC/bf3p8f8AGP8AShJ9j/cj/Rt/e7+7H3n+jbV/F/4r/uC/iOj+D/xD/Jf0/u+wn+8t9+l8b9zPr+mr4f0g1eN9R4fjU+qp4ej9Xw6+Lo766uzoTeJyr49f3pN4f7z8PV9Ya+B4NPBr9JTVr7PE/sqdnHqk3dP8c/vBRf6Tf75f3t89B/e/+Mf8WL+7H95qXxW+x/Z/u75NOj7b/J/vb6fXp9yzBp8N/o9H0lDopXVq0mtPxaq8a5pw6xf3f636yD+sX1X757fqfF/s/C8UaeHb4NKU09ur59WR7E/0facN/db+H/wP7Gm++/hGj7XT90ft9P8AD/8AJPsv4lq1W9OjV/av7Dl/9d9LfeH/ALkZ8OvHz1Ur+KnD59TPyn/Vf99cufU0/dnir9R4fwU0ro1aMeH4vx0/Dq6est/CP7y7i8H8T+3+xi+x+58v2/8AD/u4/wCMfwPz/wCUaPP9xq8HPjvp9VvaXa/r/wB32H1NPHz4lONe7RrpitNNfn8uj7nn+qP9bOaP3L4n7q1J9PqrppWPx/Ar36PE8TR/wulO6nQN7++w/g1T/A/4j/dfyTf3x/0ffwb+/f8AeH7U/wAD/uj5/wDcD4vvPL/FftP8v8d9HPl9mtv43i93x6u3Xq0aa91ad1eFK4/LoB71+7PoLb6bX9D4Z+q+k8P6jx9B8Lw6/paa18TT30rTNerBcv8Awj/hutf49/os+0/ud/l/8I/iH96/7ifxKm/4+i3o/wBIvk+8832v7f2t/tv3NHuGrX6j/XWm0/vPwfE7fG0eF43hZ8Kmfp9OjjnxOPbXqT7zwf6m/wCMeF+7f3TD9T9N43hfTeEKeJXt+rrXxdGPE+Du09VX4n+I/wChjPf3y/ul/D/70dh+X7PV/DP7x/3Y2H9//eX+G/5X/HPtf7v/AHPg51W+5/3L/f8AuY5fA/eUf0+v6nwIa6q6tGqXRSvlq8SnnXh26eor2zV/VPef3r4X0/1Nzq0/2WvwYK6tP+jf2HiU/o+L+tr6nj/R5o63/jn8U/j/APDcj/dv+LfxL+NeH+B477r+I/w3/Ifvv4V9v4b/AOT3v4eLe9j6vTdeBp+nqNVKU4mlK548fP16NB/VbwuWv3p4n718KTwtfieLTwkrq0durw9Ph/grXTinQJ7m8X8Zz/8AdH73+I/xXC/cf3T1/wAe/hN8l93/ABH/AJStH/Ab/NerTq8n7ftWmvSmvTo0NTXXTX+j5V/y086dAW78H6y//dni/UfUR1+m/tPDq1fE/FT4a0zSte2vTju3+4H8Vi1eK/3NN9p/Ff7wfZ/wT7+P7r+Ff3r/ANx9vP4tf8P/AHvFq0/7t92j+p8BNFdH4tNK+fGmaceOOkm5fub94y6NHxfp6/E06dQ/s/FxXh8Pd/PpH7y+5/uL+1/dbx/wyi0eX+If32/u7/G6D7Tz+H9j7L+I+L/gb6b+T7fi3tRZV8aPXXTnTThWmflw9Oi3dvE/dtxo8P4F1fFr8PxFpWmKa6U1Y46c9CDtX/ZZf4kP4f8A39/jH8G3b/C/7qf3r/vN/eP+C5T+6/8Ad7w/s+X+Kfbf8CP2/D5fNxb2nvv354aeF4OnxYtXi6dOjxF8Svz0V00zqp0JuXv9bf6mXx/rvq/p7nwPpPH8XxfCk+n8LT+PxNHxdlNWvHS7z38b+/3T9tr/AIb/ABnblv71fwH+I/f/AGK+T7bR/ua+88Hm/if3f7f2/j8vHsvTT4UX8dG+DVSmOPl9nnxpivQk3b6n94719P8A7jeNBX67wvF16TTj+pqpq8WuNOnxM06EjZf8J/3F/wClH/Sl9r/FIP4d/cX7H/R7q/i2H/u9/H/9G/8Axkr+I/xzT4P4r/kf3Or7fnx+wpv/AO+KTfur6PwvDOvxtXjcG1aPG/Qpp/g760rivWQPtV/refT2H+ub/Wf6z6xfp/3R4P7q0eLF4P1n7t/3b+J9Tw8X9Lj4Xfo6T/YX9+/4bmf7r+P+7+vdf8K/vT/pK/if8O/jL/wv+K/6T/8Ach/en+D20/df5P8Ac+bw/wCTafZzsXgfT2v1On94eEnj6PB+PSNWn6f9LRq/h8qV7q9Rl7rfvP8AffMX9X/+VO+ruv3f4/70/sPHbwdf73/xz6jwaf2349fh/p06Lzs//SR/ebcv/Fz/AIl9pB/E/wCJ+D+Ef3r+w48vh9GjwW1fw7/cjfRb9rzexLL9L4cVaadRpTjpqOPl9mrFPnTqFNu/rF9buH9p4+hfE110eNpanHOr/mn+pXhjV0azO/feB/73/wB3f7jf5d/fTz3/AIT/AHw8uF/u/wDwX+Jf7k/tv4l4PP8Affjw+b9z2V22ireHX6jQv+8ZrWnb60p5VpjqQ9++q+ks/wB4eF+5vFl8avD6ns0aPE/W/g16/PRr7ul3vv8Aun99Uf3G/ifi/iFR/d77/T999zom+68nj/3J+fzar6/3L3vxp9uWH1/0kH7x8P6jT+porpr8q44Vr0Tb1+6v3ldfuTx/C1n6XX8XnXh31rw86/l1Dzv8J+3pfN9x/EP4DD999x91/EP4rqfy38n7Pg1eXR4udejVzq96sfqK3Pi/2fidmmmnT5U/FX1r86Yp0cc1/uvRsv0ur6r6FPqfF8TxfFqdeqvZTjTRmlNXdq6StJ/df7PDePV/E/4i3j/iv2/23mtT/wAD/hP3XP3f21vufH67f5r1+T2vbxtQrTw6ClK8c1+X2U+fQMH7p+li06/qNTatWmlceHprnV/F+WnNenfbP3P3VJ/GPD91/HoPs/J/Dv4n/FPuY/4P9v8Ab/5P4reL7f7b1eT/AIEeu/tFumn6C8r8PhnVXhpodX8uNfLoQ8l+P/WjYeOr6pPC001+LqXwdPlr1adNM1456kdna/4P1Z/pP/vh/pK8lbq/0Yfwn+/P8O/hFZ/ei38C/wAs/uv49H8U/g3q+11afTr9gjY/C03n7n8L6Ltp9Tr0a8aK6/8ARf4PF/FxzTrIr3L/AHz4/Kv+uR9f/XT9bX+4/p/qfB0SfUaPpOz6Lh430nb4WrR26ulrvn/SH4N0/Yeb+4f2G4vu/wCFf3Q+1+/89P8A8CvJ/v7/ALL7v7j7f7f97/gR5PR9r7Ltl/dH1u3fUeJ+8u3wPF8b+HupT9GtKav6WmmdXQ/5+/1zP6v8/fur6P8AqBSX94/u79108TxW8LXq/wB2nh+J4vh0/U8PxdX6fhdA5un+P/3V25/DP4P/AAD7frX7f7b/AEk/3m+5/u7hv4z9x/dz/fo/wD7jy/3i/i/q/iOv+Gf7j7exlaV/eA/t/E/V1eJ9P4f9o2mv+iV0U8LTjR/a/qaesZd2/fX9VY6+B+5P8V8HT9Z49fCi8TT4P6HhcfqPqPx/7j/p16DnC/xrRgP7m/6Qf7q/wvL/AGn8a+5/uz/d77iu/vh/CfJ/lv8AAv4f9/5/uPTr1/Y/uX9rpvpNNx4/hata6qca0TRqpjVwp5+vRFZ/v7wdg/dH71/dX0s3g/U6/A8HxJvqvB8/Ap4ur8OrX4fdXqBsn+939xMT/o8/v/8A3U++y/8AcX+Df3O/vtp/itR/Hf4n/Cf8o+z1/c6/uv8AdX+b9Hj9qrvwvqLn6/wtXbr1a9HwjTTVitacPPj0U8v/AL3+i2v+qX7x+nrJ9B9N4H1f9o/ja/C76aNVa/h4Yp0PUv8Aot/0P79/in8T/vd/drJfwb+8X8H/AL2fafw9/wCJfbfd/wCU/wB7PuL/AGn2X+S2+v8AZ9lj/vT957Z4On6H/RaauPlWnb4dPirmtKY6GkP9Vf6r82/Xf8lX6WTwPq9H1FaCujX3fVatWnR29P2B/vD9z099/wD3b/if929oaf4Z5f7rf3T/ANGUf2H99v7yfv8A99/D4P45b97+83l+2/yXT7TR+D9Humj6rT40mrX/AGuvx2r4ejHhf77pjwtOrNen7b96fWcifvL6bX4MPh8fp/pvpho8fxM+Ppp41e/xtWntp1Ep9dq77/yfx7+7uY/g/n/iH91ftdX+5n+Efw3/ACT+6/8ADdHht/kv3nk8n9j2s/Cnh08DxF8SlNdaDTq1fjrSvnSlM9Mvq+puvqfE/fP00v09dX0vh6n+o8Lwu36Twvhp2a9erFOi17//ALtfZU396v7v/wBwPNWfwn+D/wB4dP8AeT+DY37TyeHn+BfwjV/DPtPV5fLr/Yt7ObbxvGXw/E8TSK8NPE0/2a44dRbvH7v+gX6j6X92+O/h+H4mvVoSmqufD0f2enu1a64p0tujP70/6PG/0j/Y6P4LQf6Kf4rq/jv2mrB/wfx/wj/Lv7qfYebR916tWjwenX7pe0+qH0Xwaz49OH4tXH8daVp5cfLpfy19T+5Jv3/o+o8GP92eLq8TT+n4dNGfB0VpqzXToxq6c8B/df7PsH+GfxjX/H83/GfsvvvL/f77THfefwz/AJe/8P8AJ9PB+94v0c39+fxNENNNKefDTU14ef8Al6bt/pvF3bV4uvxH1aK6vqKL692n7O6n59IHEf6VfvOzP7j/AMA/uz/AU/iX+lT+4v8AEPDeo/gv9yP4p/uX/jVvufL/AMu3zaPv+ft/dG+m12ni+N9T3afC8XR/S8Sn6enhT8dK6fxdFz/vnXuf0Hhfu6qavrPp9fB/C8Kv6lfi1V/S1afF/wBD6iZPx/d7Z/0pfZ/xfy4D7v8Avh/A9f8Ac3+DUv8AA/4J/dn/AHG/xv8AhOnxavX4fH5P3b+200+Fc/u/4O/4dXxajrrXy11+VeGKdHtzX63Zv630+t/xfxPH8L/cXwY/A0eDjxPApSvdTTq7tXQZZj+Lf6Rav7n/AEc/w/8Ag+L/AIR/pI+2/g391Pv6j7Tw/wAY9Wv7DzfcfwL167/a/wCUW9tWvh/RWen63xPGbX9PX49Irq0401pTxPnXHXpvqP6x7l/yQ/o/oY/p/wB8+Ho+n1NTR4udejXX6bvrp8Lv6QU/8J/vQ/8ApF/vT/A/Jl/D975fvv4t/kv8X+0+y/3B/Yfxf7jR9p/a0eTi3s7XxPAH0OjxqLq0aaUzSurvrT1/z9Ad/pf3mf6y/U/u/VJp8XVr10XxNGj9DTrr8GeFfLpTZP8Au591T/3K/uR/DP7sv/dX+8v96v4t/Ffsdyfx/wAHi/37P97vuvD4f4p6/H/CvB6dXtpfF0S/V+JXxP1NGimnspWvdp4/D/S+XS/cP3b4ln+4PpPp/pB9N9T43i69Nx43D9Dxq6aeJnT9Ppxr6EbaP99/vNu/6Tf9JH8R/u3/AL9/+8Hi/u9/d376H7T+D/c/u/xX723mv+9o8mv1afbDfRf4x9B4NPF7/D+LXQV1fl/k6OP+RP8A7pv64fvPV9CPovq/7L6bxG0eBq8vE1Vp56q56eK/+7/+k7Df3P8AuvD/AANf7xf6UfJ/dz7n+Kp4/wC7P8A/3Nebzf5nw+ny6fJ/u33T9TwpPEpr1nRorqpTFdXbx/2OkqfS/vbb/pqeF4Y8f6z+y1a86fC/V+yn5+fSkl+8/v5B/fL+B/Z/cf7gf4T9z9z/AB3xZTz/AMG/5eP3v3X23k8vH2/6vVb3Q6/puyv58KYr/q+zozttH9ZU/eHh6fFbT4Oquvu06PxfFT4vLjnpH9Z/3a+83r5Pvvvf72P/AHh+8+x+5+zu38Z0/wB3/wDKvtf8/wCPR6f16f3Le3bjxvDh4afC7eP5Vrj/ACcPLpNsf7u+q3D6nxNf1v8AjFdPD/RKeD3cK8M8fxdE0yX2P3VT/Cvuf4V95Vfw7+IfafxP7XUnh+++19Pm8Wm+n9vXq0f2vYhj1U/U/tKCtK08+Ff+L9fLqKLnwPEf6TV9JrPh+Jp10x8Wn/iuNPPofN2f6P8A7bB6ftfvvssf/eD7L77+7X2t6H7LX9j+5/Hv4Pbw/aejR+vjX7I7f6rxnrWuNPDVWj14/h1cfn8+hrun7n+jtNGn6j/R9NfC0fp6Ph/Ho4U8qeVejAbf/hv3G3v4p/pY+2/iMv8AAP74/wB/f4V5vt6r+G/bfxX/AHA+P+G+T+Ha/wB/Rq/t6faZ9NZfC8DxPPT4dfKvDPHj/PoZWvj+DYfvT96/u3X+l431Ph6tLaKeJ+nXTXw65pXT0pqX/R1/e/GeHV4P43nftPD93/xcf8m+4/jX2/p/if3Wv7r7n1ePyW9Ov21L4306aqeLTNP50/Lh0Y2n7j/rBL4Wv6bxW8HVWtainieda/HXy1eXRgKv7L+JyX8f93/t4vvv4Z/AfHfyjz6fuv8AK/DfRf7X9vx2v6fZUmvwYPA1fU50+JrrWnnTHDhXNeh/c/8AJR3X99eD+6qx+L9F9PppXGnX3UrTV4eNNPw9BBjf4L9pua32P93/ACVn92/u/uP4B/CvN/kP2n8M/a8+j9Vv8n8enw+n2avr0w01a6DXopXh518uo8236au46/p/pdb/AE/i6vCpVvg8PGv0/DTh0ldv/wB0tVb/AA3+Ffxrybi/iX8P8f333f28X8P+30fvfcfw+/j/ADo0fi3uz66Jq1aKrT7Kmv5V6TWX0Vbv6fwfqfDn1/6bSuin9LRw/L5dL7H6/wCFZLV4/wC9Vs75P49o8/3H2dN/DPvPP/kf8c+9vr+49X08/o8nuk+nw00f2dRp8P0qa8Pw6af5M06W7P8AW+NfeLo+o8KX/cz+PGn4v9F1evz19urqfh/vf9wv2n3P8K/hT/df8BvuvNoj+08v3H+S/b/xP7j7f7T/ACrXe3Hh90uqeE9aatQp6cc0pn4aVrjox5Z8X98WHg+J4Pgvqpp1V0dldXb/AGldGn9Svw509Okn8R0Yj7TyeHxQ/wAY+98H+c/iNN/CtVv7X2mi2r9+9/7VvbMXwz66ac6dP+l7qfOteGOHRluP+5G1fTa/qO3xvqKVr4v6dflo0/F38fl1nrf4t5s5/C/P939pk/4j/C/H9n/DvV/GP4tp/wAu+yvqv5PRp/znGv28fpvBtPqNOnUnh6qfF+Gnlq+z8vLohl/eX128/u/xfE0z/U+FWmip8Wv4/D40r+fn0n4v4Z/cWf8Auf8AxH7H7Haf92/D959l5v2PD9j/ABbj7Xxef+HW/wAm1aPH6NfvbeL40fjaNWqTVXjSv+Hhq/n5dWh/dn7rvP3N9X4fhWvg6NWjxKLq+L8Ndfh+VdNPPqPlf4n/AKSNq/6Vv79/6O/sq/8A0Y+D+G/b/wCkj7ek8/2H23+X/wAV/uzp/g/8c/t/e/Zfv29t2v0mm++j8D6zHjV4aM0/o/Hqrp89OrFOk/NP9Z/H5b/fH7w/cvd+7/F4+P26tFP1dXg6PD8X+n4fn0IC/a/wpfFb7H7qt1+DV9r9f9zXlt+14/ufL9x4P2vNpv8Aj3eH+0b8vi48e38/SuadLt30/u+PTT4j/Y18PVo/V0/hpqrr8Pt1/l0pKz777CXxff8A8P8AJJe/j8Xi1Uvk++8f+5L7XRq+5+4/a1W/tX9l58Px2rTxainH50p+Gv8ADTNOhRbeN+6bPTq/d/hfg0af9D110/qeHqr4uvt1fOvRRO3/APS5/Ct+eD7f7L+HYD7PV97/ABf+6/8AEKj++/33h/3H/ZfxH7P7z+If5B/AreT+17NLL92eLb04az/Dp107NNe7VStNOdXDz6CfMv8AXz93b34mrV9LFx8TxfpvEP1WvT+n4evRr8X9P6fTq8uhIwX94f4N1V/FftvvPE1v4B9x9r9z53/gX8C+/wD8q8H2+i/2/wDlH3/k0/tW9p4fA8Xc9NPD/pU4Uzr+f+SnRpu/7y/dvIP1H9to7vD1adWv9PwNWdGn07vE8Ty6Un+4nw/8p3/Hvf8ANjT/ABT+If8AJP2t/wDp9q/2r2Y92r8Px/P4af4f5dAb9bwv9Xx+J/q+dfn1/9k=">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="8048625"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>304800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4099" name="AutoShape 3" descr="data:image/jpg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wBDAAYEBQYFBAYGBQYHBwYIChAKCgkJChQODwwQFxQYGBcUFhYaHSUfGhsjHBYWICwgIyYnKSopGR8tMC0oMCUoKSj/2wBDAQcHBwoIChMKChMoGhYaKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCj/wgARCAEEAcsDASIAAhEBAxEB/8QAGwABAQEAAwEBAAAAAAAAAAAAAAECAwYHBQT/xAAaAQEBAQEBAQEAAAAAAAAAAAAAAQIEAwUG/9oADAMBAAIQAxAAAAHoo+j84AAAAAUlWpaslpJQKSLay0MtDLQyoiokpZNDM1JctRYIAAAAAAAAAAAFKWyWrCklqpbUzdKzdEy2TDkVxto424uG4uGpGWosESakslLlZKAAAAAAAAAKKuooirZLbZLdJnV1c5uqmLu2cd39DN+Ze2/b8/XzbXsP1/L28d+t6i8vXz7ofvviPr5fKzyTq5ePPJJrE1JcrJYpcrJcrJQAAAAAABSlsUspbFasaauJppmatud/b+p6Rydnn32+zufq/F+08/UFAAeNey+Q9PJ1/PLnu+fx55JNcU5Mtcc3makszUsWCXIlAAAAAAtLLZbFlstasaauLW7mabYmrWe1+leZem/P+qHh1AAAAPKfVvMOjk6tnlz3/L4s8kb4s8mZrjzyYbxN5zrKyWTUlzNRqCAAAABS2XUoZtWy6m7m6mri6auLpphpq57B6h5Z6nwfVE5uyvm/J35dodA+T7c3p3yPN8+vP3L83VP2+nn675t6T57yfQ6djlz9H5PHjlzNceOTLfHjkzN8ed5m8yyWSprKyXIlAAAAWapqVlZbLrOtTes7uNazu+d3nbF3NXF1N3P1vVvJfWuD6nU+mdr6h0cWbrXTw4bJx55ZLxfo4tT09i6H3zpXzPu9FzyY+n8XGOw9k8OrzjHsnxfP38zxyY6efGN5m8Z1M7yslksakszQAAALZatluVmrLrOrnes6uN6zu41vPMx+v7Hpt4fo+YfD9E886uD9vrvj3sHP19P6f3XpfTwXTXRw5ckTjzyZmuPHJmb9h6j2nrfy/wBD59jefp/E9C7D0zpXD9T075vQe36nSsaz1cuM7xPTGdZm5LM2TWZZLGggAAC2WrZbm2Wy6zq53rOrjk1jd896zpn2Preuicnb9r5WN9nzeX2Xxj2Pk+h1rpPeOjevJveL1fP5GDLLLWc6xN+r/G+p+D5P6LzXG/0/T+L2HpvovnXh157d9b6vl0eQY1nr5M43ibxnWZ6SWZrOsyyWNBAAADWbWrLcrLZq51ZveN3z3rG7je+PkZ770fvHRvH13rG+jj37B4767yfQ+T0H0Hzz08OTXFrp+dtxjeZFZZa9Q4nL8r9B5V37z93/ACvYPGeXhx7dix13NZxrHpmY1ibmbJuSzNksakszQAAAFlLZdS2GdXOrN6xrWd7xq4+z6/4v6Lx9fL5h2Hrvtzb1x66OTl9Z8j9W5O3i829M8w1jkvHer5+2By9q+z2Dg+t8O/bc/b+Lh+n+Ga8dzcfW+CyzNTLLcyzPSZSazLJqCakJZCUAAAADVizSWy2LNaxqzk1x6vnyb4t3PJrj9J89da7B3dx9/SOyfTefp8fyr1jyTr4N3jdfBy/U+P8AZxv1YfJ/QgPzfp+Zc+PZZ+t8Jllpi5amWZtiybkszUuZURoIAAAAAWUtl1KGbrNs1rFs5bx6uPv+x+U+rcHeHh1AfN8d9d8f7fmcjjdfFy64R7D9Xw/tvB9P0N1D8fl7d38v+b8vq40menmuZGrhmaZSbQlhJUJZCUAAAAAAC3NrVzbLYZtit3Fs+n7d4B93w9vaHVvp8fZ9Z1rpm8ft6hxXv+byMN+e2BtiG2IamY1qZzLrMk1cw0hLCSoioZoAAAAAAAAFubWkWaSpblZq5qbYtcjBnkvGs5XGORxjbEOSYGpmTWpktkQhKIqEshKAAAAAAAAAAAsGrlZq5tlSlQmmVauSaZGmRpkVC2QVECLZCkQhKAAAAAAAAAAAAAoUWKUogAIAAAACwCCwSwQAAAAAAB//xAAvEAAABQIFAwIFBQEAAAAAAAABAgMEBQBQBiAhMDQQETUUJRIVIzIzExYiJIAx/9oACAEBAAEFAv8AA5SGMKUY8UpOAcmr9u6KpikrcUmThakoNyaksPpBSUWzTohCkDrJB2kLYQhjmSiXilJQB6ShWhKSbIpbMuHaStmGeXuTYdpS2Yb5u5PB7nbMPc/cxAHuFsgvI51FU06VlWpKVnKaybhd5WIudbIXyXVR63TpSYRClJhY1KPXKlD/AN6MdHtYjD+zbIrSQqacrIGOqopsNtHNYkD6lsj9HtYh+7YT0UrEYdWEao8IlBIhSUc0TrEZCgwsSTVdWk4d0an0cLRCmfLrEAbQahiIPpdMOcNVwklSsy0JUouDuGsKf39MQcKkNF6n/wAeyiPdHEPF6RQ+19A1w1YnTtNqmrOhTuQWdFoug1P/AINlnq0n+H0heJ0bfyw7Yp3WPyF1LPcXZjh7sp3gU3bquTRzJZonUKxR9NJJkJG2KW1hsjfVCd4ezFD3j5rx1YeOT07tYiCFMJZRonISqjtOwgAjT/WByMdWc5wdmF8dLax9AIlE5zHGxxbcHTxNMqZJ/wAdkjR7sJrx+UoCYzaHMYCRbUtGjGhqatytkpLVhZmTgzVwSbaiWVkvWBkhx7x0z43LFsgbp5Hwd2dqaxblcCQIUaCCo9AzZpL+OyRhAUf5XGre0w8YCRckp4/JEG+GRyySn6TG0QyILyGWR4GQhhIdg8I7R6mMBCzEh6o9ow2PuOWVP8EdlSVOkdvOnKHz5vSs+FO3y7obSxcemdpKFVTyTz8Fj3SOklmQt5toqHzFpS00zTB/MKuQ/wAif//EAC4RAAICAQIDCAEDBQAAAAAAAAABAhEDBBAFITESEyAiMDIzQEEjUYEUQlBSYP/aAAgBAwEBPwH/ABFllll7X9WyyyxW+gsE3+BaV/li00TPjjBciy/pWWWYcCnG2LBBfgSrwav2iZZf0H4NI/0/FrPYXuvWez30Px7Sz44dWS4hjXQlxCT6IjqckpK2az4xeBes92cP9jNbOXetWWWWQfNGr+FiMennPmh6VxjbYhC9R7rRQ/JqoLHOkcO6M1/zPa9kannhYhajuscSOeWW0xC9V76jUTg6RObm7Zw7+44h8oyhCMnPB/BFN8kZYuMIpmLA4x7b2Xr0ar3IZw/3M4h8pRRQjrg/gwZO6l2jNn71iyzrs2L1mM00oRXM1MlOdoZoPeziC/UKKNPolXayHcY/9SUfJS3X0seJ5HSI6TGupDDCDuJrl50UYl51vLpuhfR0q8u+t9yK2xapVUj+ox/uZtR2+S6FFfTw5OxyZ24/uSzxiTk5u2UUUUUVtX1KKKKKK/4f/8QAJxEAAQMCBQQDAQEAAAAAAAAAAQACAwQREBIxMkATICFBIjNgUYH/2gAIAQIBAT8B/DkgIzMCNUPQRqHFQSFx88eWYtNgjM8+1fspd3Hqd/dTb+PVb8BG46BCledUKQeynQsa0+FTb+PVblTtGQHsdoqf7Bg6ZrUKgONuEal3pQPL23Kq9Qqb6+2HxIMOjneUYgyxHChha4XKa0N0VZ6VLs7W/YibKMgudZSSgnLwoNMKvQKk2dukv+qVmcWUMXTXTbe/Bna4nwoGlrfOFVtVKfjjLUnRq6jv6gflfiySBgujUPKdI5wsVS7cJD8Ti3Xi1O7Gl0xkpyNq6Lz6UUGXy7izRZ/IWRyZC5yY0MFh+o//xAA5EAABAgEHCgQEBgMAAAAAAAABAgMAEBEgIVBxcgQSIiMwMWFigbETQVHBMjNSoTRCgIKR0XOS8P/aAAgBAQAGPwL9A8yQSeEaLChiqjTW2j7xXlNeCFtq3pObaWrZWekaZQjrGtdWq6qKmUnFXEyEgDhQyj/IbNzUJKlHyEfKzRzGNa8BhEaQUu8xq2kJuGxfxWa5g2r/AE7WavB7jaucQO1m/sO1vSLNTxB2GsWlN5j4yrCI1TP+xhpKikJJrAEicHubNZ69qGk6npXGrStX2jQQhP3jSeV0qoMYxI0eWzWb5Gw0vNChGsWpV52DR5xIyeBs1nFIx12KTxkYN/tLnhaUpnmjWOLVdVGiwnrXCM0ATLsPVtLPSNIJReYS4pwKJM0wEjOMd5GDfs2TxlXj9hGscQm8xUVLwiA6ARpbrCTfKMcjZ5hI0eOyQeEN45ctuPaVXBXvYaVuzzHdNGqZP7jGa5mhO+YSAyNnm2TJ5BCccuWjl9jLlI9F/wBWHk54jtREIx+2yZwwbxJmtJnjKfEzdNNU0iXnEha1evlGUBCUpGb5WHkpw9qLZ5RAxbJm6HOneRaas/OnMKW4fKTwygOI8q5po8MJDaPOvfYVQjJ+Gb2osYB2g3jZN9e8PXSTgzGJ1qKjxNiIbV8O8wEoSEpHkIVeKLGGF3ikEpBJMT5QrN5RHy57zHy5riY8NE83GH8NjodTXN5ROrPSfSaAhsFLQrr86LP/AHnDvTvSz1jWq38KL45D2sufNzE+qo03z0TGg+eqYS0sglM+6HrqLKT6z0nMJsoPZQmdw7gfy0X8NFme77UnlH6ZrJaSr4RpGllGA0QpO8ViApPxfmT6UCpRAA84zG/kp+9k3oNJ88s1LObUUq4RM+2FcU1R8t3+B/capk/uMa1ej9I3WU299JruhK0GdJ3Gj4DR0E7z6m1Zk6Tf0GNNRaVzCPxLf8xUsrPokQUI1bfDef0i/wD/xAArEAEBAQAAAwUJAQEBAQAAAAABABEQITFBUWGh8CAwQFBxgZGxwdHhYPH/2gAIAQEAAT8h+Dyz4HLPkmWe4yyyyyyz3OfIc9rLPZyyyz2Ms+T5xzjllllllllllllnHLPkucCCCyyyyyyyyyJ9zQ26K3f/AK2IlfVRB3o/g/dkQvWd45JM/JSIiLLLLLLKxnt5D8tnpfjp8v8AbnPghB/brq9/+94FGGexmfF85mZn5CRBwIiBdBA62Z90R5dZ347bzcuun6+mXX+7x33OJyM8Un48giIgiCBzw/8Ao979wLyzMzMz8aRERERFyn2L96Yr6AmZkngz8WQREREREs+v+Hvcm+lszMyTMz8URERERETz0rPcC6P4RaOJ7vQXUPufwP8AbKq/qn54HsephmZmZmZ+IIIiCIiIi5PQ6+Kgdbtv9y1+C3RXvzHr7XTp8ea2eV7njytKVVsmWn07w9Q9szMzMzM/EERERERES0+nJ4ads3A2Y/LzBZZZZMz8KXzOHoV2TMzJMzxeD789kiIiIgiIif2c4HmeH82RZZZJM3IXYItipmUm/U5vrnYu79Auql7z/dyQZ6HgzPBn2n3ZERwI4HAiLMx3t1n5vVl/TYcQfpC9ftEsXu/Si2O4z+oIgss4MzPF7y+kH+pmXJ8cfg9MbrO+nrkfdTzdmKTMzPBmffkREcDgReQR04AV7h+mJ4D0/ZHSP339cCLLJ4t2xaf1Hmd38MzNyuxSvXnNvp/+f/ZmZmZ4PvzgRHAiIiejpcNuZ0eOHkXWdeRiep2MdIek7IiImZmZ+JfpjvhD9M8OY/WDNjmn/RzMzM8GfgSI4HAiLSnjfnwIievvI83wftERbwZmbR+GGrnSmcrZ1dwIi2B5u8wf9mVtZTOg3stGSODDZmZmZmfekRHAiIiIiWZ05/PERE/Fk8o/ZP6YiG22ZmbrDtHnH7f8pZBUHB25hzhMAL7vdNkQenmR4s9Bp+6ZmZ4s+8PaIiIiLc0foWndz+XAiJaOCERbbbbMzLfBf3R+yPmTCFd4N4wE2l4PB4M+0+9PYI4EWpfXi9h2XSzAGR3mHL91sRbfaEvXO8i22225GBgDnFMv6r+YLmn3rGedIqrKpqP3FmZmZmeCz8ORERCULr7xac7x3+pUUPEcMRFovBPNer8FttttuxoGXN3O72cE6v70zMzMzLPxJEREQxGsn8HygnMP0P7Zt2Q0qObo5q/2G49z9lttttkTn6hf57RAvR/RMzwZmZn4ojgREdzmjdH++yNw71tttsS1y1/JHtC2zmH1eR5szwZZmZ+LIiIuYhyT6dPP2jvo+VtttsomOJ4zIATqc17HOhMpwLLV05ePvmZmZmfjiOBmXsB5e0THb5nL+22222xo66KhniW1+Lk89YZnY9+XkXPR3OX6fWWZZmZn4/YhmKFOQ/B8oIZ9Dt9nJRfSfQFttttttttssszMzPyIhtGjuqcvt3QzwJyPyXJ3k/TNPHS/vKPvfqL8jbbbbbbbbbbLLwZZ+SbbwIbbbbbbeG22222yyzw35NtvHbbbbbbbbbbeO2/K9tt9xttvs7w35Ftvwu/+N//aAAwDAQACAAMAAAAQ99999986gBOf/wDvvvyzgVtvPfffffffffffBoV9s5DDTjTMN/z90vPfffffffffJJv8TIRMLqHEVQWN7+CvPfffffffBpvoC7dRgpvPPBMGpPP1AvPfffffAqP4G2GZ5vPPPPBM+P59799vfffffFF+0V1R58fS6RnF2k2WiL2ivPfffeq/7CCb66OduDus0ZXxxUV66PPfffaiPxFvIMdbtZtmm5WNtTQFP1/vfffaqFlFnVMvZPpr7pa9dwnU1P1/vfffbiP2O2TIuKOIz0mYQeu3V3OyPPffffBN+9JEktS5Oc87YJ46aqf6ovPffffEmvmH6YoAyvC/PMIAkW3P13vffffffFF70H4/PNzmii+7GH5OpovPffffffbpN/mMscDMMJLeL2DOppPPffffffffLsGv/wBhGUQ69nAx/uSLz33333333333z6HLf6888/7+uIA7z3333333333333wJyAL/AP8A/wCMLyD7z3333333/8QAJREBAQEAAQMDBAMBAAAAAAAAAQARECEwMSBhcUBBUbGBofCR/9oACAEDAQE/EOxttttttttttttv0G222+p+8Nt53v7MeSFwX4t88cP5ViCYhN+gWYxh5rx8AYHo8b78BCD23lZSyy238vV+2IMMo7TypZSyy1fNt4jvE1vCR/d42N+LyyhhhlHB2WeCyyl0PeElZPGTFr9D9yhgOk28SXdHgz1Y3ktnPpkun8XR/D+peIz63Uvbg4A1SE8THkODsM8G+9vfDLaOs/D4h1/BDgLzusf86ToGsAuPX9z5PI9I4HB2WZvK629iF4vtD+hPCQR/t7WDjZicwL8KcCO2whOPFvt5hdIe10HxynAa/i6GY/5EIumQQQggjuJJJwkB6NsXY3WPbifX8acsGsHWCEI7bykkA377z1/BxDJY6LIGxjnkIQIPoEt74IY0EV519pn6YSkCO+znLPW/lln0OWWWWWWWWWWWWWWfQM9o7X//xAAnEQADAAEEAQMDBQAAAAAAAAAAAREhEDFAcSBBUGEwUbGBkaHR8P/aAAgBAgEBPxD6MIQhCEIQhPdMg3D126Q27Azp7x5+0k2eW/Dc646Tyfg46Yda+faAuEQyNnjrh0Yoz4JWWofNN5Qsot+Cx7ZCwaxMxtfr+fB7H7lo1vcg/wB5VwXserwWxIj1e/FYsXsUlbiHs2MC2q2a4LN9fL03A38vH/Ds3fCF5rZ6fngr0VEzuem0/kze/wCtbG2L7me0PaM80XEqg+w4VTR8u9GYt5qjaJC4jNzrv96PI0byQmAp/U4rkW4NTjQy2i+RI93KUpSlKUpS+z//xAArEAEAAgAEBAYDAQEBAQAAAAABABEQITFBIFFxkUBhgaGxwTBQ0eHwYPH/2gAIAQEAAT8Q/PUqVKxKlSpUqVKlSpUqVKlSpWJUqV+grEqVKlSpUr8ACpUqVKlSpWCpX6BUqVKlYlSpUrhCpUrEqVKlSpX6JUrBUr83mepWJUr9IqD8icx070auxKNQcj5RnOBIekKD3mmA5VQPzlwg7otKvUwBBK/R1BBBBBDgYpLJoJf7Ie8H3Blf6BIqFu/u1aLia1Rt6JPaVKPQ47GLpAK0cx5t+4IIIIP0IgwAgggmUKBlHyC1lyznKPc+yUqTu2/sO0GE/u4X0lRpLbu6rm2nG6RsiW2uoN+8EESJgDx4wBBBgDAtNgyu5IhE/DvKwN33C/cEEEEEEHjRBBBBBBBBG7qSeZR8/kdSBQVZXnkfUEEGAIkEHjQIIIIIIIITDqA62/qH49o6G4PZ9QQQQYAggg8UIIIIIIIIIJX60Py+ocS86nnXD5VlMJ7l92vdPYL6pAG2kwCaXZ98DENRev8AhBBBBBBBBB4sBBgCCCCCCLWUKXz2e8N8FCgDVYU0xr80GV4rRBfVzi8Ge7Q9cj2lQsNfoSWTLNXNY88EyovK7k+4aROQUdl/YIIIIIIIIIPFAggggggggmXm87h9wjiELckTdLNdpchD/kXieEEzQrMDamhoQOeRfR/qCCC4DlAYCCCJHx4AAgggjLGtd1ahF5NDs/3DVBw9EETrhxfkk0EbYhK9cnxBBEFkba0BaKrulkJ7BXpm+8BKFulfPOx2JaBmVaFemI8Y+DAGAwasFk0UJd4D3lSivKWT8RrQLsWfhBAb0U4DzmUdf84A4DSCCCCHoCesB3Ae4/mIGbzE9H+ECzDmB0FtloHdlq+tEouLLa81TmfPjQABgMSmZpmX1gyYKbVZ1p+5mY9ULr5UJodJfuga6/4gQQYWBEjgzszO+diW0dAvr/LEGbpdGTa/5M9tUGjGHoDs/d4kADgBxAsgCi0tXXIy84BBOx/mfMpsAijmaNqu+AdOCvozS6QXeDO7/k1Yi4gW5korqZfOf9v7wNbx50SWutHxg0RojcdTxIADgBgOAPfJFtakOAXi3S3zshc4ERUUWBYooosoA3J7FfUUy158s6+55JnklqDeboSsgDyIcwwK3aozkAHK8ruKsSRtkzoNWq/RgAACqer0X+01RRRSnMis9EBZ1WQUXASiiilszajoz6gL8yO194CTTbk6PMakKSwC5sZA3WaCEHiqK02l02X5ReBC5UzBoZX5fiAPhgFFNLbrc/EqfmugoHOKKKKq2rL50hLk0q7xRQxDCiiggrQe99xRhddg31FDIjRQnqTzckF3cBYs44HxQFBiiiSBaKUrp1coEKKAB2lgAt076Mu8LMUUM0slV8DL6mt5RlnwwqsM3JdgJeJM8n1VYPQYFNBW6+l17RSXWwT8ygKQSlt1oZQQuh2Rf1FFFFFFFFF8UCiiiiExbMhhEvowrUea1fk2JeuGyVMhQsAvS5kRRRTNq9f0D6lsjWMz8E5GsX0spvZ1++DeLpwS+bBRRRRRRRYC8SooooosBc4h8yFqTypftOhXETupcBchI+oldprDSOxuhCUltnoNwZklFYx0ZI4dMc3ouKKKLFFFFF4sooMUUUIwRdBMxR/+esI4bxT5kf0M3h6qsjdQPd4rYD03+AiiixYCiii8YUUUUGuws3DY6NLhlwoA1E9BvD1M3Q2DY94RDx7AcnZxz5QyJIoBusEsLU5beXkbRRRRRRRReNuKKDLkZ9SWvg4mPoQ7ZsPE7sfjR6PM8mIXTLuRRS9KgeQ8gp3gobYKDuX3lMz28h+m/W0siwFFFFF+gLAtRPDVRSeamAmGzYGXi6Qdm2+D0BP9Hp+T/iooooov0SmZHlxSs26t/wD1S88aubeVhXWp5Or3u2soT+5e9PdNKHbEHbIyeR7/AJf/AFWLAUv9KXF+BHv8PiqX+lXLxLl/kf8A3LxLly8L8deFy5cuXL4BcuXLly5fALly5eC/0C5cvEuXLly5cuXLly5cuXLly5cuXguXL/8AFf/Z">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="8239125"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>304800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4100" name="AutoShape 4" descr="data:image/jpg;base64,/9j/4AAQSkZJRgABAgEASABIAAD/7QAsUGhvdG9zaG9wIDMuMAA4QklNA+0AAAAAABAASAAAAAEAAQBIAAAAAQAB/+IMWElDQ19QUk9GSUxFAAEBAAAMSExpbm8CEAAAbW50clJHQiBYWVogB84AAgAJAAYAMQAAYWNzcE1TRlQAAAAASUVDIHNSR0IAAAAAAAAAAAAAAAAAAPbWAAEAAAAA0y1IUCAgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAARY3BydAAAAVAAAAAzZGVzYwAAAYQAAABsd3RwdAAAAfAAAAAUYmtwdAAAAgQAAAAUclhZWgAAAhgAAAAUZ1hZWgAAAiwAAAAUYlhZWgAAAkAAAAAUZG1uZAAAAlQAAABwZG1kZAAAAsQAAACIdnVlZAAAA0wAAACGdmlldwAAA9QAAAAkbHVtaQAAA/gAAAAUbWVhcwAABAwAAAAkdGVjaAAABDAAAAAMclRSQwAABDwAAAgMZ1RSQwAABDwAAAgMYlRSQwAABDwAAAgMdGV4dAAAAABDb3B5cmlnaHQgKGMpIDE5OTggSGV3bGV0dC1QYWNrYXJkIENvbXBhbnkAAGRlc2MAAAAAAAAAEnNSR0IgSUVDNjE5NjYtMi4xAAAAAAAAAAAAAAASc1JHQiBJRUM2MTk2Ni0yLjEAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFhZWiAAAAAAAADzUQABAAAAARbMWFlaIAAAAAAAAAAAAAAAAAAAAABYWVogAAAAAAAAb6IAADj1AAADkFhZWiAAAAAAAABimQAAt4UAABjaWFlaIAAAAAAAACSgAAAPhAAAts9kZXNjAAAAAAAAABZJRUMgaHR0cDovL3d3dy5pZWMuY2gAAAAAAAAAAAAAABZJRUMgaHR0cDovL3d3dy5pZWMuY2gAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZGVzYwAAAAAAAAAuSUVDIDYxOTY2LTIuMSBEZWZhdWx0IFJHQiBjb2xvdXIgc3BhY2UgLSBzUkdCAAAAAAAAAAAAAAAuSUVDIDYxOTY2LTIuMSBEZWZhdWx0IFJHQiBjb2xvdXIgc3BhY2UgLSBzUkdCAAAAAAAAAAAAAAAAAAAAAAAAAAAAAGRlc2MAAAAAAAAALFJlZmVyZW5jZSBWaWV3aW5nIENvbmRpdGlvbiBpbiBJRUM2MTk2Ni0yLjEAAAAAAAAAAAAAACxSZWZlcmVuY2UgVmlld2luZyBDb25kaXRpb24gaW4gSUVDNjE5NjYtMi4xAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAB2aWV3AAAAAAATpP4AFF8uABDPFAAD7cwABBMLAANcngAAAAFYWVogAAAAAABMCVYAUAAAAFcf521lYXMAAAAAAAAAAQAAAAAAAAAAAAAAAAAAAAAAAAKPAAAAAnNpZyAAAAAAQ1JUIGN1cnYAAAAAAAAEAAAAAAUACgAPABQAGQAeACMAKAAtADIANwA7AEAARQBKAE8AVABZAF4AYwBoAG0AcgB3AHwAgQCGAIsAkACVAJoAnwCkAKkArgCyALcAvADBAMYAywDQANUA2wDgAOUA6wDwAPYA+wEBAQcBDQETARkBHwElASsBMgE4AT4BRQFMAVIBWQFgAWcBbgF1AXwBgwGLAZIBmgGhAakBsQG5AcEByQHRAdkB4QHpAfIB+gIDAgwCFAIdAiYCLwI4AkECSwJUAl0CZwJxAnoChAKOApgCogKsArYCwQLLAtUC4ALrAvUDAAMLAxYDIQMtAzgDQwNPA1oDZgNyA34DigOWA6IDrgO6A8cD0wPgA+wD+QQGBBMEIAQtBDsESARVBGMEcQR+BIwEmgSoBLYExATTBOEE8AT+BQ0FHAUrBToFSQVYBWcFdwWGBZYFpgW1BcUF1QXlBfYGBgYWBicGNwZIBlkGagZ7BowGnQavBsAG0QbjBvUHBwcZBysHPQdPB2EHdAeGB5kHrAe/B9IH5Qf4CAsIHwgyCEYIWghuCIIIlgiqCL4I0gjnCPsJEAklCToJTwlkCXkJjwmkCboJzwnlCfsKEQonCj0KVApqCoEKmAquCsUK3ArzCwsLIgs5C1ELaQuAC5gLsAvIC+EL+QwSDCoMQwxcDHUMjgynDMAM2QzzDQ0NJg1ADVoNdA2ODakNww3eDfgOEw4uDkkOZA5/DpsOtg7SDu4PCQ8lD0EPXg96D5YPsw/PD+wQCRAmEEMQYRB+EJsQuRDXEPURExExEU8RbRGMEaoRyRHoEgcSJhJFEmQShBKjEsMS4xMDEyMTQxNjE4MTpBPFE+UUBhQnFEkUahSLFK0UzhTwFRIVNBVWFXgVmxW9FeAWAxYmFkkWbBaPFrIW1hb6Fx0XQRdlF4kXrhfSF/cYGxhAGGUYihivGNUY+hkgGUUZaxmRGbcZ3RoEGioaURp3Gp4axRrsGxQbOxtjG4obshvaHAIcKhxSHHscoxzMHPUdHh1HHXAdmR3DHeweFh5AHmoelB6+HukfEx8+H2kflB+/H+ogFSBBIGwgmCDEIPAhHCFIIXUhoSHOIfsiJyJVIoIiryLdIwojOCNmI5QjwiPwJB8kTSR8JKsk2iUJJTglaCWXJccl9yYnJlcmhya3JugnGCdJJ3onqyfcKA0oPyhxKKIo1CkGKTgpaymdKdAqAio1KmgqmyrPKwIrNitpK50r0SwFLDksbiyiLNctDC1BLXYtqy3hLhYuTC6CLrcu7i8kL1ovkS/HL/4wNTBsMKQw2zESMUoxgjG6MfIyKjJjMpsy1DMNM0YzfzO4M/E0KzRlNJ402DUTNU01hzXCNf02NzZyNq426TckN2A3nDfXOBQ4UDiMOMg5BTlCOX85vDn5OjY6dDqyOu87LTtrO6o76DwnPGU8pDzjPSI9YT2hPeA+ID5gPqA+4D8hP2E/oj/iQCNAZECmQOdBKUFqQaxB7kIwQnJCtUL3QzpDfUPARANER0SKRM5FEkVVRZpF3kYiRmdGq0bwRzVHe0fASAVIS0iRSNdJHUljSalJ8Eo3Sn1KxEsMS1NLmkviTCpMcky6TQJNSk2TTdxOJU5uTrdPAE9JT5NP3VAnUHFQu1EGUVBRm1HmUjFSfFLHUxNTX1OqU/ZUQlSPVNtVKFV1VcJWD1ZcVqlW91dEV5JX4FgvWH1Yy1kaWWlZuFoHWlZaplr1W0VblVvlXDVchlzWXSddeF3JXhpebF69Xw9fYV+zYAVgV2CqYPxhT2GiYfViSWKcYvBjQ2OXY+tkQGSUZOllPWWSZedmPWaSZuhnPWeTZ+loP2iWaOxpQ2maafFqSGqfavdrT2una/9sV2yvbQhtYG25bhJua27Ebx5veG/RcCtwhnDgcTpxlXHwcktypnMBc11zuHQUdHB0zHUodYV14XY+dpt2+HdWd7N4EXhueMx5KnmJeed6RnqlewR7Y3vCfCF8gXzhfUF9oX4BfmJ+wn8jf4R/5YBHgKiBCoFrgc2CMIKSgvSDV4O6hB2EgITjhUeFq4YOhnKG14c7h5+IBIhpiM6JM4mZif6KZIrKizCLlov8jGOMyo0xjZiN/45mjs6PNo+ekAaQbpDWkT+RqJIRknqS45NNk7aUIJSKlPSVX5XJljSWn5cKl3WX4JhMmLiZJJmQmfyaaJrVm0Kbr5wcnImc951kndKeQJ6unx2fi5/6oGmg2KFHobaiJqKWowajdqPmpFakx6U4pammGqaLpv2nbqfgqFKoxKk3qamqHKqPqwKrdavprFys0K1ErbiuLa6hrxavi7AAsHWw6rFgsdayS7LCszizrrQltJy1E7WKtgG2ebbwt2i34LhZuNG5SrnCuju6tbsuu6e8IbybvRW9j74KvoS+/796v/XAcMDswWfB48JfwtvDWMPUxFHEzsVLxcjGRsbDx0HHv8g9yLzJOsm5yjjKt8s2y7bMNcy1zTXNtc42zrbPN8+40DnQutE80b7SP9LB00TTxtRJ1MvVTtXR1lXW2Ndc1+DYZNjo2WzZ8dp22vvbgNwF3IrdEN2W3hzeot8p36/gNuC94UThzOJT4tvjY+Pr5HPk/OWE5g3mlucf56noMui86Ubp0Opb6uXrcOv77IbtEe2c7ijutO9A78zwWPDl8XLx//KM8xnzp/Q09ML1UPXe9m32+/eK+Bn4qPk4+cf6V/rn+3f8B/yY/Sn9uv5L/tz/bf///+4AE0Fkb2JlAGQAAAAAAQUAAklE/9sAhAABAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAgICAgICAgICAgIDAwMDAwMDAwMDAQEBAQEBAQEBAQECAgECAgMCAgICAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwMEBAQEBAQEBAQEBAQEBAQEBAQEBAT/wAARCAEEAcsDAREAAhEBAxEB/8QBogAAAAYCAwEAAAAAAAAAAAAABwgGBQQJAwoCAQALAQAABgMBAQEAAAAAAAAAAAAGBQQDBwIIAQkACgsQAAIBAwQBAwMCAwMDAgYJdQECAwQRBRIGIQcTIgAIMRRBMiMVCVFCFmEkMxdScYEYYpElQ6Gx8CY0cgoZwdE1J+FTNoLxkqJEVHNFRjdHYyhVVlcassLS4vJkg3SThGWjs8PT4yk4ZvN1Kjk6SElKWFlaZ2hpanZ3eHl6hYaHiImKlJWWl5iZmqSlpqeoqaq0tba3uLm6xMXGx8jJytTV1tfY2drk5ebn6Onq9PX29/j5+hEAAgEDAgQEAwUEBAQGBgVtAQIDEQQhEgUxBgAiE0FRBzJhFHEIQoEjkRVSoWIWMwmxJMHRQ3LwF+GCNCWSUxhjRPGisiY1GVQ2RWQnCnODk0Z0wtLi8lVldVY3hIWjs8PT4/MpGpSktMTU5PSVpbXF1eX1KEdXZjh2hpamtsbW5vZnd4eXp7fH1+f3SFhoeIiYqLjI2Oj4OUlZaXmJmam5ydnp+So6SlpqeoqaqrrK2ur6/9oADAMBAAIRAxEAPwDf49+691737r3Xvfuvde9+691Xf2xn49q703bW5bHLnstkohFgVyEiVWHxGQE0kFXUVmOLlqk0eOETUMTnw+R9bK4ABMXY+FF5RAcBxb0z6evrw6KlhT6id2q0pONWQv2D7KU/M9FlFVM5WaWqfyiCVI2b1GOJj6YUAsqRamb+gP8AT2yCTk+denSKEr5Y6sT2bCa3ZWxcpkPFTTVO36IBKTXJJPFTxeCN3mYMqPMUWwVbj6fj3RD2aRWgPR7bIZEDHAoOH2dDXS1dBBDQ00ciU5nj1tGKiN5IZSimTyNqILNqt9bn+ntohmJY8etiJv1CFqqn049NVfXEVLqJvJEgsqj1KbWDH/AFrfm/txRQVp0tghGjVpoxPWE5O0LIwGuxueSLLayhV5BBuP8AY+/aKnrT2tXBX4em6pyEs8X280cFUhR441kQ6okNvQ7Cx8ar9Pz/AE9+4ZHXjbAVIHHiPXpBZbHSJBUyYyKKWI6dcOrT+0dX+aLm6AvyRzYW9uI9PiGOk8tl2kgUb0P+rHQHZKJnknDgfdJJIjrqISFlPqvf9ZC83Fxzx7UawKkGo9B0VNEaZB11pn/J69JljE8nj0aooiGU2cFi1wFQ8sl2/H+HvesGgPHpjRQ4yo9epdNRQSI8pisYdet3e4QhSEUKOWYnkAe22apArUnh0tt4VKltPCpNT+zpVwNPjtlbqrWllmpqiigwlHFKdSJVVr6rrEwHKQhrBT9Rz9Pdo1/UVQeGeqXahLdiB2nA/PHRaKXKPhtwST0syhVqGv62VHhcKKmPUnIexNiOQ3591chZjQj/AFceixVqlaGoH59CZh9y0LRU8NQtOjVE8pE0ocM9OzFItUouqxAre34P09uNIgJ7vs60EY4p9vQ9UWB2U1HDUwb7pUnlgiqngmgT/JpbXkp5SnqidLHR9SwF+L+2vEY17Bx9enxHFxEhqR59O+OyuSxkzDF7gqauBdKxTw1VQKSZRaw8VTf0KeOALn6ce6OFIqVz1ZS6kgOSP9Xr0JeJ33m9Kirjpa1SBeQoYZAL2N/FZNX+w/HtkoD8ung58+lnTb0oZCoqqeelvYFwPMik/ltIDgf7A290K+hz1fV6jpUU1dR1i6qWpgnH1tHIrMP9db6l/wBiPdaHq3Um/wBf8P8AigPvXXuuvqwt9Ob/AOvb6G39Pfuvdcvfuvde9+691737r3Xvfuvde9+691737r3Xvfuvde9+691737r3Xvfuvde9+691737r3Xvfuvde9+691737r3XvfuvdJncOcfHLHRUIWTJ1Skx6hqipIb6Wqp1uNVjwif22H9AfdlWp+XWx8+kxR0wQpFKfO9UROJZjreWuiJlUyEn1mdCwt9Bfj26cUNMdVLE1oelxSzRywxzR2EbJcBQBp4sQAAL2t7bYGoHWgcmvHrKZQR9Rb+g5v/T/ABJA960mox1vptnqgtz9OObkXIvwL/4H26q0x59b6TmZy1LjoRW5Gto6KmAbVPVzJCgXSSR6mDMQRawu1/booo7jTry1c6VUk/LqBhcrFuiNv7ugV1DA3hmyrpLFjmdlvLDT1DIr1ckYIDCMHQbXPv3ixgHNT1Vo3U9y0J8uhExlHLQ0iU01QalkaQq+gRhEdyywqLsWWIGwJ5I9pnbWxanWwKCnTh7p1vr3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de697917oFexOkds9gZSHNVdRV4zIJT/bTSUMVO8dYVZTBPVxToweeGMGMPe5UgE2UD26JmCBKAgcK9MPbJI5fUVY8dJ4/yPQU9sdN7Q2n1tkZds4hYKyirKetqa6d2rMhUU7xNRzM88n+bjDTK2lAiBhe1/bts2qRwx4r/g9OqzRKkIaMHtNSeJ9OJ6UHSxh3b1BtWOCpMNbtx8jiKkg3KVFPPLURU8hc6lWSlqY21C9h9PbIJVmA9a9GljNpQYqCAD+WP83T+KhGke5jAWRXhUAMhCuNTSMRrZDpsL2sPbwFT8+j2NRUVrTqTV5iWOWWaQQpREIkKhHFVPWmRtRI5QUpTRoCgk2JNvp71w8vLPWyunSBw8v9nriK95X1o+ngKP68kl2IJFzq4/Hv1c8MdeAHE9RDOZJAsjkaWdXCnxh7c34/VYnjnn3rq2pAQtfl1Fyr1JopUgAV39MaqAxTRGJH9A51Op4J4Pv1Rgnh0xNq09uT0B+dAdlWaOawXWZHBDakN5OCQdR+j/09u4p24/1ceiSQ1ZgwyOPTVS40SwxyPIY5SzlyLEKjENFYg6gzIf8AYe2tepiAKj/VnpyO2BjVnajHJ6k4+mNVWx0dMJEjWQEyFQSyXJeqkJtd7Gygng/4e1AGgamFT/qx1pV8VhFEKIDX/ob/ADdMfYW84DBS4vG+SPA4gtFRwu4f+LZlrpUVPAtKkJuocA3LErwR7dBCIXemo5P+QdF24SxyPHBEf00/mf8AVw64YX46b2q6PG7lz8MVLSV8omqMM7TDJ09HKvkSStEaf5H5ncDxgmRR+sKePaBW8RydXn+37Pl8+m2jZFAoPs9Pt6fd5bUx23ZMFQR0lNTxPQyRvEqswE9IyxrJG7s8g86Pz9BcX+vtWi9lCPOgr0leoYZz8v8AD03bY2/Pl8vBi6IIskxDy1EpKwUdKpBqKiZj+hIU+n5Y2A5PtmUKlSDk8AOn4gZGCgD7ejVQ4XZ+Ghio8djkylTEgWaurZJZgxZbFwhZYQzEk2UWX+vtmpp3PX5DpWyImFSp+fSix0OLVV/yClja4PoS6X5ANuQL+9inVCP9VOnySmxcqlXp4Rb6ug0WH4Uaf6+60IIoTT/V+XViME0z0lq/EKL1GJyBpZ1Nh6tBNwTYuhDBzb88e3Pt6aNQcY6b496bl2+VGVo/4nRD6za7yAAX1CpjVwBb/Vj3rw1bhg/y634hHEVHSwwHZO1M9LHSQ5AUddIpYUldanZ2As6RTk+CZlJ+ga5/p7o0TrmmPl1dZEbg2fQ9L4fQcW/wvf8Aw/2PHtvq/Xfv3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de697917oPc3QimzD1SqSa5I5VZixBkgAjkj1m9gAFYL+nk+1ERqpA4jqp+fDrDVDx0nnjus0OiaO/JvG2oEDlbX/3ge7lcHqoPdQ/Z13i8mxqZqNbutRCcpSaCW8ayPorKYj6j7acH/AAj3UDy6sRTP7emTO9iYDAu0VXWiWqAa1DjkWrqgwax1aG8UYv/qiLe6s8acWz6Dp1IZXFVGPU9J6q3Lm8vSkUE9FQV8qfc0+PoI/7zZxqa2uFpoKBZKPHzSAi/kJKHg8+9B6jFAfTier+GqnuBK+p7R/PJ6BP/KavK0mUyD1VdLTVQeoqc3JFXhNUpheOGnr3XHxyxOzWUowLj6H6e2kVncGhIB4npZRVQotKkYC/7HQq4hqoVEL0G/dy0dclZqiwrR42WiqCrLGlO9DHj4KR1nAUFIgsiqb/AFFwraNTljwHSVlkRQTbDQfxZ/w9GYTVoXWAH0rqC/pDWGoD/AH2j6T9cvfuvddMwUFmIVQLlmIAA/qSeAPfuvdJXKb127im8UtclTUkXWmorVMh4vy6kQJ/yE4t790YQbZe3FCsJVP4nwP8/wDLpNx77zNfHNVYfbAraandUkR8pFHVSFubRRpBImoL9eSAfqfe6H06XDZ4EYR3N+EkIqDpJX9telftvcdDufHDIUSyxFJpKWspKhdFTRVsFhNTTL9CV1AqwurKQR710W31lNYTmCahwGVl4Mp4EdKD37pH1737r3Xvfuvde9+691737r3Xvfuvde9+691737r3XRFxb/fcG/v3XumHcWGhzuIyOJqiPt8lQ1VBMxPCiojZYpAAP1RSkH/W93jco6uOINetkB1eOmCKdEr6F3GNg703V1ZuaQ49splDHjZZCBDDnqdJKdo/JcBFylMUMLcguigct7dnUBzIvw/4RxHTNpKY28NssD/xY/PH+o9Dnujbc+JqEFHJVw0l4pGqypm87KX8lLUsRoVZNX14A+t7396Vqrg93QqtJlnjBLAP6D06TlZVGAwyShmLWdQQ5aIBeSGI0+lBa4Fv949+JoP8HV3rU56kUs9LNKJlqEg/zURMt0ihWVrqJEA/TJe5YAn3XUcnpsOQMjqc00FJWeOqmp0Q+RWlR1qwrwqCoVI2PNRq0qR/Qk8e9/6qnqldVDWo6b6rchRHhpAialZnlkVNZuNBBRr2Iv8AU/VQPftYHW2fyHwjHQe5KnE7Gf0yygMEPLALwzkLyAuvk2Fv9j70S9KasDpgxqW1FR9pz11h9ux1brJlKjRj42mlkpqUmGsYqmtAZGDKqVEtl1abqv0B97iIAIHxfPptoWfBb9PiQOPSO3dm6HDplaKik+wp73yFYXaWWiim5/g9PI3rmr6lAA7C3jjNvqTZVGKt4jjAGPs4V/zdF97cpbRtbQf2hPcQf9X+x0I3Q3Vcmbmg7I3rikWnVIm2Pg6uNtFPTrq05ypopF0h5V0Gl1gm15bD9tvaSebxjpH9kuPt/wBXn0hgh8IeI39ocj5fP7T5enRyWUEEWvcEEf1v/UH6+2un+ikdsLgcJ2Hts1ERakpNv5DKTwNL5BU1UNRUTUFMRIWK08tVEqupsGTj2ujLPFniWpX5Yr+3pHII0mQ0xQn/ADdJDYrvFiKzINAi1GcrHqTOCQz0iMyx06qRpjpVqSz2FtVh+APaeRi7vpOBj/P0/EBHECydxyPz/wAnQ5bWw1dXCOWokEFO5spcnyMgF9WnjTD+Af8AePfu0CoHVQXY93n0JlPt2OBCvlEjEArqU29NyLMDbm/uusYx05RvIjqPU4qsjVtKrIvJDI3q/wBbQeTp/wAPewy8OHVwKjyr0kMjTywqWljdSBa7KxAPJ/HI93Brw68YzStMcOkfVZOqSJokYabNqZhq1/hUF7qQfx72BWvTTChr5dB5lcRtzLI8dWtVhqwXcZLGNqKSC51TULFUcl7EspUgD8+7gtTtz69U0I1S2KeY/wA3n0lKnsftHqKXGyS5Cn3XtOaUpTyVBlqKapp1uTCk5vX4mqVTe0g0g/hh7oyh6nTnzpxH2j/L1YeJFTUaxngfX8+I6Mx1/wB6bI35FDCtX/AM1I6QnDZiSOGSWdxdVoKu601cr/2QCshP9ge2WQjhkdXWRGoAe706Gf3Tq/Xvfuvde9+691737r3Xvfuvde9+691737r3Xvfuvde9+691737r3Xvfuvde9+691737r3XvfuvdJ/clP5Mc1Sq6pKB1qgBe5iXioXj8eIlv+QfbsRo49DjrRrTHSNrZa6SGQ42jnyJiieWQRALB9uFZyhnkAieVkHpRNTt9Le1DMqYJz1pF1GpwOglpq6rzcc7U0ddW0lKgIx9DkI9v42Jqk6p467O1BWZlaIAGCNvp9Rfj204LepPoMfz6U0WOhJCmvEip/IdBhn9tGgqDLTZjbk9fWGWamwG3mr8ilEklvHD5vE88sq8ktIApt/Uj2maFsmoB9OlsDmQhFjcj1NM/l0Ku0KLd74ePGYdsbs+JSpyddRUxmyuQqGUSNIkLSXoVK/6uRTf/AG3tSq9i1UD1P+Wnn1SaBI5B4up2PAV4D0J4dKan6owz1JyFXLPlJKcvNHU5SoaodqiUBnn8QWOgpTruTZXKnkm/vWARqqTXy6VJcQQqgSIGU/FXh9gHn9vTRSZ+j2/lJ6VqOWrnoJoJaf7fw+BpYZC8szFxqLrRtINSC7BuPdmWoIrTz6Npx9XDGVXtYFGrg5wKD/TU6HjI7p29iqT76uy9DBTGMSK5qI2MiEXBjRWLuSPwAT7TYAqTQdBiOyupZDGsJDg0NcU+2vQL5jvSCab7fa2PkrISpH39RDKdTlrI0NONCiAAEl5GF78D3oHUwVFLMeAA6N4tnhjBe9ugAOIUgfzPSDl3rmdxZJaaryFVL5VkBpqeGSWhRgurxgyfbUcdSSCosj2YfX2sSxnahk0qPQ5P5gdKEuNutkP01uTQ/HwqOGGbJGfLpY0NHEKJEoKeh8uiMtRZWP8AiZaNjrapbUUUPL+ltIAB9qbeCBuyQEj1GOk27Xl9AfEjfSpFNQ9f8h6XG3dyJN95QVGMoKB6Ep4lxKylYqcoNVXoZB54457iQITIi+qzC5Dd7Z/TeHIjFoW4k0qP9Q6I7W8kuyfEZvEByCahgR60wfl1H2pT1W3N55ikmZGxe6J5arHaJdRhqoYmqzBPG1mjk8TyqrfSRVXni3svoQKkY6Eu6GO92y0nRSLiBQslRxFdNR65p9mehi9+6C3Xvfuvde9+691737r3Xvfuvde9+691737r3Xvfuvde9+6910QCLHn/AF/fuvdFg736iG5Um3Tg6G+YEKLkZKRVFY32an7OuiVAJJ5EFo5QDq8ahgLr7UwyKVMbn7OmJo6968RxH+b59JjrDvZoGpdjdpMtPWxotHRbplIajrYtASCHOM4KCVk9P3P6X48gVtTmjwsmQP2dOQ3FKVbPrwz/AJD0P9bsLEZJHqfu6qoSXVPTSJMs0QSRQ0QiZOJYfJZgLgMvH6fdC1eI6NVvmIVSg8q0/wAPQattiV5qfHwUlbHUQPURTVMyPEkuj0oYtYWFRT2BupJKm44Hv2F4nz6XakPfUaccOoku1cpTI7VMK+BRGn3HnjaRZWkfVYIGaRxa5J4RSOfx79g+fXi6HhXqRS7LkWKoqa2YIGp4paRAqkSyuzMCTe7xCDgsPp/T3oUJB9fTpssK4FTwPUybAYmKjp/sw8lXH5DPNUsEoxMF1GCMEKEp05Ik+lr393VDTJ/Z1shhUvw8ugV3ju6mxdLXLHW09LSsxppsrGQ82QYAieDb0SjTO0N/G1SR41Y+nkX9qI48lmx/kP8An+X7ei68vgiGOE5PE/5v8/T51F01UbsqcdvTetHNSbao5Vrdr7WrQXlyjMA0eZzglu0lPLZXjjcaqj9TWjsJGZ5vErGn9mOJ9f8AV/xXRZHGdXiyfEeAP+E/5ujrAAAACwFgAOAAPoAB9APbHT/Xj9OPqSLf77/D37r3REPkIK2p33kq0FI8bgtv4PGSSOyl5Mhl5KqopIIYr6mleN2JP6VVbnkj2ZQECBR50Zv2dILkEyV/CAB+ZJ6GfZu04JYMPR1SPTrRUVNCsZRVfW9NEzIwtpYcluf6+yxajPrk/Pz6OnRSqmnwjH7Ohw/g1NFEBCzr4wSushlJAFr2UEKLfQe3NVaAjpEUB4cemabMu4NK6/aqHURzAMA4Q830k6UP5I+n597AANePVihAocHrguYqEYR+UyDkG5V9Tkgix/KN+Dcce7aV9OqHV5HrO+RgmiP3EUdTzZgEGt1A/Tc8Alj9B9R71o9D1ZJWHl0la/a9HmBUyQVEdJWzB5IKYGPwLotoQleUsv1sPe6spApjp4FWX4c+ZHQFbgweXxbyxVELF/O8ajS2l1U6fIr/AKWTj8e3NYGSOm2tnI7SGqeHSBpstJRVcsdTTx1ePmieOqx9ageGQN6Po6N4mdb2I4I+vt4qHUGtGHmOmo3ktyyOtU80b/VjplyfXGJydNU5LZdUy1MTCofb9YSfI1i7RUMpA8bXHp1nQ30DAi3toFkYCTFfMcOtvaxyqZLMmg4oePT3sDujdG0A8MkrZ7GU7+Ou25X1Mv39BpN5JsdVSxvJCoVCDGdUaseQOD7s8QfIw3y6SJM8ddQJX58R0dTZXYO2d+0C1mCrladYw9ZiqnTDlKAkhSKql1Fgmo2Ei6o2uLNfj2kZSho3StHVxVT0tvder9e9+691737r3Xvfuvde9+691737r3Xvfuvde9+691737r3Xvfuvde9+691737r3XTKGBVgGVgVZWAIYEWIIPBBHv3Xuo88DNSTU9K60rtTyw08iINNO7RskUixjSLRMQQOPp7351690XPKYjN4zH0mJyENHiqPF05YJjYInFassuiryIqSzJcy2L+RRIvkAt+fatWQ1K1+w9GVhbJdS/qNkmg+3yHSqwGz6Chwkn8PpxJUZuGSoaqWMRLGrm8ZnqriaSL0g+trMTYC3tuoqx4D18+lVxOtvcBVj0iMhdNak046vn8usu3I4ME1dJkHIWIlf4fQSrVqzxnW1RVSqTBBGFIt5GW3+wHuuteCn8z07epJcpA8a1HEMw0jPkB5/kD0HG8vkDSY/KR7ewVHi2neGKWavyM7y0kCynV4liWNRNUIqXNgyC4sT+GGlRGA4t68B/n6bg2ypY3M7K3oMH9p6TOF/vXu6riyTwChxtXUTSLuGaiURyJ6gRi8fUPA9TM8i6RI1okPLGwsfB5ZaGtF9ejQRxwxFInrpAxX/AAkZ6fjt/CTVUaUGPq83kIyyua2aXIaJ01ASVTU6U2Pp4h9TDTq6k8avfvDB+Z6WRxKiM95L2nPktQfStWJ+Z/Z0tqLaOQqqZqXMLRwosqNBQ4emSgpKdT6nEn24HmmY8EnVpt9fz7VwSNCpC0yPLotvBYSFGhBoOHid3D7fLqFmNrRYeCkrKSNogKkRSvrMrwSsQ0UqOxuuuRQCPpz7Ui5IDAVz0ihj+qmdJaGgqMU/LpzxVKgqnmVvHFU0MzKqKzyq2jXUw6wSA8UyNYDixHtpJdLV+fSncbdp7BU4yKQCT+wH8wes4xBp6WTJUchSojCVepAAWClWVin0kVgRqX8i9/a6S4WULGwqvDPQatLZoZip4EkED164bszCSU+39w0cipKKrzqP7S19E4lqaMkC4uVlUg8FT/iPZXJGY2MbcAf+K6GGywiaC9s5RkpT8jgH8sfn0NdDWQ5CipK+mZXgrKeGpiZWDApNGsi+ocEgNY/4+05xjoIyxNDLJE4o6sVP2jqV79031737r3Xvfuvde9+691737r3Xvfuvde9+6914kAEk2A5JPAAH1JPv3Xuo1NWU1YjPSzRzKrFGKG9iP+iWtcH6Ecj3706dlhlhIWVCrEVoepPv3TXQNdidLba355Ksk4nKS6BUVEECTU1cEPH3lL6D5j9PNGySAfXUOPbyTsoCnK/P/J028SuanDeo/wAvQA1WF7a6QdUwFdlcptcv5Qi0zbhwsFyPJFNj2UZLGq/+qhYC35Nvb48CUV4N6dN/qxEU7k/1eXH9nSzwnyc25Wwfbbtxc1JUqms1eCf7ykYgm5WnrGpq2lf8Ff3f8T7aaAg0Vv29ORXNDUVBH7OlJUd79ZRCEw5tIoZ2V2QUVUapYnhWR4CqRPHFOZTZmuRe4/x918BqZI/aOl63MOkF5+6noaV6DXM/I3ZsdVqijyGQSFnVZmpjBApH0VYT+7JH/iALfnj25pVQNTgfz6v9fAtUjViKcRj/AA9IZuw959ly/wAC2RtXIVvldolllQx4qKFmCipyDAJB40LDUZ5fGPppPvfipHXHy+f+fpHNeXE40oKIf9XHh0YDYHx8xWJqoNy7+qYt4bqUwzQxSo38Aw0kS/tw4+hfTHUrAf0NIiovGmMEBvaZ5HkoGwo4Af6v9Xz6ZSNUNSdT+p/yf6v2dGP916c697917ro3tx9eP975/wB49+691Xl2XWVu4+5MttiB2jiyG89rwBCS6a8PRU9OJGUc20yOQL/n2vNFtvtSn7TXpKlXvFTyDA/sHRzDUCDNwCZEjfRCHKrpbTp4L2ItIFW1zbj2jYgUz8h0dlaxsR5nHS0eshaMks6RsrfuaG+gHqtxccHg/wBfdOHSHQQf8nSOeeGQvT6S6NraJyo0hVOn6+kxnSbj8n3cOPy6UlKrQ9J2qiNK0cnrjp5TpDqQ8Vhx9TbmwPHFz7stadvD06RSoEOaj59OdROPDFUq6yQwFFeSJCU1lf1VMQ9ZfTwdQuAP9j7uACcfF6Hp6HQ1BItR5MOkNuOTKo33lCxkgnjJeWnjYmISEIsaCNrji5uPrf2/GFIoxz1aeKSMDwkqnE+fSHqex6mOjq8TmqcZCnkWClFXDohqaYXMYVfJqSVgouzEryLE+7+CoNa0xivSE3MqVYLWhzTHD5dI3P4ynqY5qjBVbVf2yeeSmdQKmmRlBaCRGJaSNALgi4F7+6gaH0twPp1Z5xdRgq/6gPA+nmOkfjcjXUVVDWwyRmaIqpCkorQ8M0Li5BRm+o+v5Hu7KjqUI/1evTEc0scglXiMH5j06eNx4FczFS722xRU43DRCaXJYwrCkGVoUjkataQyOqmvp419OkapUHHqAuwtY20McjgellzGlxGLmEUelWB/1cR0hsZWzZHI0OW2jUT4jdtMXnonoHWmizaKuswU0ZAijyka6lkgIMNWt7KH4Z9grUDfCcDotWvFMSCpx5/l/k6Nv1V3vRbrNNt7d0KYLdeoUscrq8GMzdUgbWlOZF047IErY08rDySf5skkIEUkLJVh8P8Ag6VxTK9FJ7/9X+qnRi/bPT/Xvfuvde9+691737r3Xvfuvde9+691737r3Xvfuvde9+691737r3Xvfuvde9+691HqqulooWqKyogpYEBLy1EqRRqBybs5Ue/dORQyzyLFDGzyHAVRU/y6Q2VrhuIU5wtDJWrRzSlq2uRqTDTQSxGCppnknUS1MU6OCpjRl1qDfj3tWzjo6gtDt+v624VGZcRIdUla1BoKhaEeZ4Hh1GqcTmocdQ4/FJDVxqiwu1bUyY/DY+nQFkIpoQKzJpqOkBmA4BPveBXrZvYDPLOy6JSa4GuQn7T2ofs6RldtkLNT02byyZ6epmYLg8cyY/CUJCGQ1FXFA3nmiBFtAUO5tcgXPu4iciug6R5nh0/HfxuWaOsdMeI/dI3yWuB9vAdOo2tX1dfFXy1uDDU9OlLRTJtTF/c0dKiALSwVMsbzxU6iwX9wlbn3rwxWv+HpkzWiAj6Vi1aks7Gp9T8/XHSij2zT1EkMmVq63LeNQBTVcqx0kfptpFJAqxOt+fV70w4knptr50RxAix1PxLxP5np1lpZ6V6aPHwUcdKZWNWtjG0dOIm0imSJLSTGbT+sgab/AJ9+FSOPDplZvEBMhJfyJ6mxwXYELp1W5Xkkfkm/AP19+49VaWgIrXrHX42KuoKyklWwqoGjDEX8Ui+qGUccFJAPpb3rUeNOqRXDRSxuv4TX7fl0GW3tQyRopP256eSVZFA484D09QrKRqUFtDA/ke3AehJcSVtXcCqMAQflWo/l0qMPGtRjzBKB56My08qAjgM5B9IP6QbgH8Ee76zXj0WX8Sx3AZB+m9GB6DrclPJSUVZQ+jxUOapcsgI4enqb0VarLcMquzROSOPqfb0iiVY5f9qf8nSrbZ/BuQR/okRAPzGf2gV6XXUmWaow9dhJQUkwVa0dOpLMBjqsGopkjZgNa0zl4/8AAKAfaJhQ8MdJeYrcLcQ3qfDMvdT+JcH9ooehY916DvXvfuvde9+691737r3XvfuvddA3/BHJ+v8Avf8Asffuvdd+/de64SJ5EdLka0ZLi1xqBFxe4uL+/dWVtLK3oa9M9FRCjaKSGMR6qeGnnDKf3BT6gHWwD+Uj6XFiD/re7E16WTXBnDJI1e4svyrmnpTp6JsL2P44/PP+H9fdekPXBpFFwGQtewXUoLNa+gXP6iPfurBTxoaevXldiq60s7C5RfVpB/BbgEi/Pv3XiBU0aq+v+x0Hmf6j653NM1Tl9qYyWqc3eqpUkx87m9yXehkp/IW/Ja5Pu+t6U1Y6bKIclRXpFT/GnqeaWWVMPX0wl/3VT5asWKPgD9tZHkZf9iT9ffvEf+L/AAdVMUZ/D/h6l4r469UYmsjrF2+9fJFKs0EeVrqqupo3QhlH2jusE0XHKyBwfei7NWp62I0U1C/tz/h6GijoqPHU8dJQUlNQ0kQIipqOCKmp4wSSRHDCqRpcm/A+vuvV/TqT7917r3v3Xuve/de66IuLc/7D8/4e/de6r6z9NHT/ACNVg5KPvihkbys4Beagp3KqwFwwkYiPjT+CbezF6/Sp9g/w9J4T/j4FPP8AydG7jFPV101Q5lWYQtHUJa6q8QCRzJIb3WRSP9a39fZXMVB/PPQg0NoCilK46fXqJpIadoCZFV4gYT/bUL6vHq5dmYc/T6c+9Fu0evSPQKtj8+o0qo7MvjRrhfJKDoKq5azXU8yC3093BJ+3qwB9esMxUIlOjftRAxhJYUk1Am7X1DSbH6H6397H2/PqoTVXUMdBPud9wYepU4lI6jHSOprnWdo5qWjcaWheE6hU3Bvq40jgn8+3lYGlR3+v+rz6otu8ba0FYycg+X+fpKVG5J6YpURloIY7qaQT3p5pCAdZI5CgC6j6Bj+fbgoQa/t6UpIAQVGPMdB/naiDOSCtpQsTM4RgVCLrNiRNGOL2H1/I5/PtkyuvbxX0r/l69JBFcd4Wh4H7fmOkz95PQyA0E/21SkocAIJEZyAp1MeGRhxY/j24srafl/h6JprYLKQDkenl1zlqg9PPUimhin8imaGP9On6ippEHr0FgdYudN+OD7fEyHP4umfCcEDy8ulXsaoqv41SOQZKWGSnqpQGuWfzKl1XkEsjMNLDkfX3SUhhQfEfPows1bvGmsZFT9vQMbnppNpbi3VjYJJKafE7ikq8QxPimip62X7yhdFRisXiDDTpPBHt1dJRyfPuH58eiyVKSEDyPEftHS0++xvZwlq6z7XDbsEUDz6IxTY/cs8CgSVbTK3ix+X1LfWFCyHkkG596UnQEPw+vXiQ5LYD/wAj6fYeh16q7krMZX0Wx9/vWJJUSR0mEzmQDPUGV5TFHRZao1MksEsp009Tc/QBzYhgzNCFGtPzHT0M5JEcldXkf8/+fo23tL0q697917r3v3Xuve/de697917r3v3Xuve/de697917r3v3XusU88FNFJUVM0VPBEuqWaeRIoo149UkkhVEXn6kj37raqWIVQSx4AdBllexxOJafZuNbPzoyxSZOoL0WBp2c2VhVSIsuSNxbTThlJt6/e1Vm4DHr/q49HVts5Ol76XwkOQgy5/L8P5/s6DajyQq9wx43cVRLmcvkzHJTz1Rb7OjrvuiIMbQ40fs0tMItRuwJLC7c+3ZFSMAEZ456PpJhZQhrJBFbKKEJ8TAjJZuJNf5cOlo+9MlJXybf2lR001FgZ/ss1nM5FULFHVmdoo6TFUVOYHrJI9B9RYJYf0Fz5YiW7v2dB14YpdV3csRJJlUT09STXj1nOM3Rk6xhms3PU0l0aOkoIFx1EFUlgJI42eWYX49bkn2rX6eOOq/2nSFpNElIoFVK8San/JnpVUeDpY3bw09PGFKtcIFZSFspdhZiTaw/wB59svM5Hcx+zqxeNTqC93qPPp4EIQFFBBNyBwDa1yQRezD2xqJPDHW9erJOOsRazaVuSxsx/JNuP8AAkH3rBGRkdPBe2reXDrl5vGSzJrZhYX+ikj9Oki4H+9e9AdaEWsAK1AP9VesC1Ml1DlEDEgqthwBcC/JYG/+v7tQeVft6daFKEqCSM1PU8Sq4Uk/puRcn9X6dLfg/X/b+60PSQxspboJt2v/AHe3Vgs3ErClylQoyIRbpqpykNUfqo1T0kock8gxk+9BiOHR/t/+NWV1ak/qIOz88j+ePz6VdQox+eMiFJKTKKdDghVWRrK4BHpYCRVYf4Nf24pJX59UiJutu0sCJoT+0eX8qjpNZ7HtXwVZ0NJWU8EkE8bWEjxKRLE6j6myfnng+1sZ0oP4T0jSYJcoBhdVVI+fHpLbJyJwu5qdfMy01bLFQVcb2Gta5fHSTO301QV0KqCP1CU/n2mmUAkdHF/Gbnb2GnKgunyK/EB9qn+Q6Mr7TdAzr3v3Xuve/de697917r3v3Xuve/de697917r3v3XusUig2YgkqVsALgkHjUP6KTf/AA9+6sDx6xPKUhleRkuCREQByzcRKFJJLlyAP6+99XVQzqqjHn+XHpgpqKoqJAT6Ilb1SDhuCQQp5BlLA3I+l/bjMBjoylnijQgCrkcDw/P5dOv3aLVLGzskUf7SKPUJJTwCzD+nH1/PulDSv59IvBJhLBKse6vCg+XTp7r0l6h1ddR0SpJW1VLRxM1hJV1EVOrP+EVpXRWb8/X6e/db8uslNVUtZGZaSpp6qMMUMlNNHNGHABKF4mZQwBBte/Pv3WupHv3Xuve/de697917rq/Onn6Xvbjnj6/S/v3XuumJ+n9eL/73x9eB7917oiG8kTF/ISnyGQ5ok3bt6ad5lVkigraCjghkKgafHE7ggnkWv9fZk41WSlTwUfyPSFG0X4B8zj8xQdGZKtFlqqlMhAQzJIGXTrEell4BsBpIKf1+p9kd6dRqDThX9nQtiIaJXp8+llDBUTxQtGF0h7CR15Uc3A5uYh9SR+T7ugOkEj8+kEkiCR6nPp/q8+sMkBga7FLyEByg9HoLAGxsAW+pPPtwGtQevVBpTpkyMb/brpkf9aS/tyGMsYJgTGHH6kYHlDw4vfj24DQ46djAJGPPpF5apIBj8TLqBuC66jcD6twLAfg/U/4e7FgeHHpUP59A/uWCL7eaWBFiB8olSwKyeMDXLCOdDWufpZv8PfkkOQRX/P0nkiFGIxQcPX/N0HcEg1SGMMjxW8kKn9qqiKcVka3uJI72YH8e6sp4V/M+voemVkFSwFKfEB5j+IfMefWZ0glF3b1WCq4sDpP0sf7QBNwf6ce2gzLUcBXq7xRyd1M04jplZirSQJGixqrqsliSWuCQshIN1QfT/X9ugg0oPy6L2VkqHFRwB6Ebr2kMciVE3oBqIwNZCLJZg63JtcqLN/gPe5GWMLqag4ZNPy/PpbZQuwlMaMzEVwCaAedOgt7WzeJq9y5rJLj6euqa6vX7OUO13o8cq0sMthpTxkxFixFyCB7MOyOJGZa4oB/P+XQekJknk0mg1ZP8ugxx+4MlRSpVrUxmVTrR5oYpBCU5CqjKFVVv/tvbfiOaGg49e0KPy6MPs3qnfvbEuIym5XkwO1aUI1PV+GKmqamjR1ZaXCUI1SrFJqLJUS/tL9VDEW90kuDQqANVa/L8/Xp1ICdJYnRTFeNPL7OrAoYhBDFCHkkEMUcQeVy8riNQgeRzy8jWuT+T7SDGOlZznrJ7917r3v3Xuve/de697917r3v3Xuve/de697917pJbs3Sm3aeKOngWuy9bdaChaXwxkgqhqKqUK7RUySOBwCzsbD8kVJp9vRltu3PuEjVfRbpl3OaD0A8z/wAX0hKWjkyNRFJuec7ny8jkxQSIafbWIlZWUw0WGu/nSAcPUVHkke1wV497A82z0dPCtvGz236FuBkjukcepfABPkF4dLKLGQJJTuwWR6bSYmCrFRxaBYMsK+k6B9L3sP8AW9ukkimei57hijqoorYI4sa/PoEewMHV4HcOM3XRRtJTU9fT1wk+kMLRzLLKpkQ6bMpYrf63tf3qTvVWHxL0uhnW6tmtmxKAVI8/2dChFjYKGeqyeNnE1Hna6HMRKYQ8AaWjBE5ubualbN9AQb/n27HRtTE4I6IZpS6QxstGiXQT5nP+SvS84IvbSrBLAf2gbWP14tf23Ug8emhThx8+ucelG/ABAHA5P4AY/wBr6+6sQetMMcOpLgBgRb6cNb63P+3/AB+PeuqKT8P8um1gqsdA4b1KTwbX+pJ5tfj3vHS1SWA1HIweo0pBPJ+t7/Uk3vccc3ufdseY6fjGDjqG6FVVyWNiAxFiyMOLgngJz/xPvYNelCtqJX/UepMUgJ0nnSObXII0/X6ctb6j3pqg1/w9MyL5+vTFuvFfxzBV1Gir91GpraLWoIM1MLvDf6otVBqQ2t9R7qQT0/YzfS3UEp+CulvsPn+Rz02YctmNq07KdVZi1T+yDKstCio6NpvzLSOpt/Uf197U5H7Olcri03MgikUuD6UbIP5N/h6kmopnqop1a71NKsdRa4N3UxgtzcnQxv8A0HtVHXQVJ7Qajotu4SjaQncG4/4Og8OOSprJcS7mKsmositHKtv+LhjSK2mRnt6ZRJTa1twTx79OpKB6fI9GaXBjg8QCqalYj5HB/Khp0Oe1c2m4cBjcqthJPAEqkBBMVZATDVRkD9JEyGw/oR7RnoPXtubW5lh/CDVfsOR/LpQ+9dJeve/de697917r3v3Xuve/de6wxzxSEhW5uwAYFS2k2YoGsWUNxccXHv3V2RlFSMf5+uNXMtPTT1LyJFHTxSTySStpiSOFGkdpW/EaqpJ/w9+60tCyg8Cc9J7Zu8ts9hbU2zvXZ+Yos/tXee2sJu7bOcxswmoMzt3ceOpsthstQzC3lpK/HVkU0bW5SQH375+XVmjKjUMpXB8j/wAX0+BvLJHqUagGYA3vCOVjka40lmF/rz/T3v1z1amlW0tjA+31HWChk1/dQlpNCP6Q6sjxI4+hY8XJBIt9B723EHpy4XT4L0FSMkZBIPUZaUQwQOJgZfLrUshdXQPqOoIA7WTm9wL/AF49+JPd69OtNrkkBSiUoc0oeHnjj1ynzFJMmjHZChqJllQTCGpp6h4o9XrvFHKz6z+kccE+9AVPTFvGruwcEgA0A9fL8uiv9j5oZzcEyQlpqDDg0Ect5JIXrGYvWzAtdELzAotrFlj91NCeGOm5CWY4wMf6qdCR0jWqaDO4zhft6ynro0HF1q4TDIwA4FnpB/t/fhxI6p5dCnnNy47b82IgyC1V81XpjqWSCHyxRTvbS1U+tfFESwFwGP8Ah73WnHrXSg9+691737r3Xvfuvde9+690TP5H4qSh3Hhs1DIYVyuP8EUukaY8phamOopnLfgCKcHkH9PsytmDwPGfIn9h6QXQKyRSL8Xr6UNR0OW3svQ7r27hd4pIqS11PTx5SGnKVDxZGnHgqqdFQssbGRC2liGKFeL+yyWAsxibywa9H1pcM8WhQMioFcD5H7OhSpPCaaD7dg8BjXxsOdSkfU/0P9R+Pp73p09p49I31a21CjVz011bU4VzMRHGr8M4IvY2AB+hW/0/p7bINccOlUes0pk08umGtq8esbrNMrtGY/TFZnGs2+n0AYEA/wBPdhX+XSqNZQQQMfPoPtw0cDNrkq10yFtDxSIwCmzWZCQ4MSr9bcn/AGPvZeozgdKAQRwNfToPa+lOs3nSQSRPwxUBI3YLG0gHIMqEmw5v70fLNfTr1KVA6CXI0hpKglGdTTMxjJUq8i8qliv1Eimxv7fU18xTzP2f7PRdMnhtqGGGftHp+fUJWSmkSMoAKgPLSFWV1WIWaSKQsSP1i3P59syitXFdQND/AJ/z69G4UiMiisKof8K/t6zYmiqq+sgo1gaY1c4hjgK+qWeZrhUsbszf4fQe2gzahQ0NfLp8gZDZXzr+3qpn+Zcu46fvfZeAraarqdsUHT2CzeGwlX6sVQ53I7239i9z5Ckgmj8K1tXRYHGRzyE6hFHEBpDHVjx7zvcyb9t0DMfp0tAyKT2hmkcMacKkKAT8h11I+5HabNB7UcwbjbaIt8m5gmt7mdMStDHaWT28bEGvhq8szKKU1M5zTAf/ABq7oi2zurHYTsLc2UoOs6q8GalWLJZ6t2vFTY+aagn21iwKiaOmqqmBKSSkhCUy+f7nSGjl8xXyHz1e8uXYs9yupH2FlI0NV/CIBKtGMmhbDKKDOriMu/eL+71tfuHtL7zyxtUMPP0TqySxCOFbxDIBJHdPVFaRVYukranGjwiSrLoFSr7e3Fv7cdZV0v3O0dtTVM/8E25ia6s+1xuLSV/4YuYq45kk3Fm5aRENXUzWi+5aQ0sVPCVhBTv3OHMPMt/JNcXksNlU+FbxMVRV8tWkjxHpxZvOukKMdF/LnsvyN7c7LDZWO1QXm7hF+qv7mNHllkKjxCmtT4EIauiNPw08Qu9WN0Pwg3tund3WWXotzZOszi7Y3B/DMNl6+eWsqzjKjHUlauJqK6d5aisbFzSsY3kdnWCaOP8ASi+5s9r9y3G+2W5hv53mEEumKVyS2kqDoJNSdJ4EkmhA4AdYVfeG5d2XYubrGfZ7OO2N3a+LPBEoRPEV2TxFRaKgkAFQAAWVm4k9HP8Acl9QF1737r3Xvfuvde9+691737r3Xvfuvde9+691737r3QOdsbeyNcmJzmFZGyWLkdGonLB6+lVlrjDS6f1VcbUpKp9ZFJA5tejKT3DiOhNy5dwxPcWtzXwpBUHyB+Gp+WePl59P+0s9jN00ZytIkYqJEQVDFBHPpu2kyLbUsetSpB5uPbgIIBXh0m3O2nsXW3Zj4Q+EeXzp8+ldGtpTE6KAB+ANJT/EfRrAn378+itz+mHVjX5+vSErP2cVncfV0b5CnpIZ5fsgwSQxQyBqlaV3DBWWkbyxraxK297JoAwH2jo4uAH+kvIjR2oCR8xiv54PUPAMYqU4aSYTU0Cx1mEq1OlKvFzKJYrMDa6BjZb8XK/j25GQGp+E5B6LrtFJ8dRStQ49D0uqSZXhEFyzRW0N9SUtwb8Bhbg/4+9suSekamncD8j+fWddQIPJNwP9UQPqeOfx7ZI9B0oNCMcKdSZZQYwgsfoefwDY6h+fr78MnpuNTqqa9RLlxc3NlFv8AD9TY3/Pu3Ajp/Cmgpx6wmPnj6c6iCBa9+V/pyf9f37FR59Oh/2+VeuKwB1MWgMWVl9XIKck6j+UseQfezxOo4620uk660Xjj1/z9Z6OieEnWoJ0upYcrpY6NKXNwALf4+6k16YuLlXA0E8QafMeZ6xcxy2I9UblQTyQV+jf0AIPvY+Xp06KPHUHBFf29JrF0b4PclYkEL/wvLr91eNC1PS1iD92Fwo/YEsUp8ZNw/0vcW96p6DpZcuLzb49R/xiPtHqV8j86EZ6mHF6anIUUio0STipopLjUkFUmplaw1emUFR+OB7cVjgjr31KyQWtwQdRUo4+a4x9oz0iJomxO9sd5ytRF93SVIsD+3FWU0tPrJNhrjLljb6ge3NRliYDiOnMS7fL4Y0mhGfVSDT8+nbYc74Tcu5toVJVUaofM4sCyq8UraJ1jWwBJjEbcf6lj7THy9emdyjE1paXqGtBob/CK/YajoXveuiLr3v3XumqhzuFybePHZXH1smnX4qargml0j6sYkcyAD88ce/de6dffuvde9+691Bnoo5XRxrVkAVdDaNA1FtSkDUp5/HvYNBTp5J3QMMEHjXPVSXyR+WfyU2NQfJnrnt/48YfrrrbCdVV1Tsz5CbT7B3jvLb3YFLu3JPgkpsPicT1Kc5tzcGA2nTZjIbigUZGu2xDRDILT5DGmOrlbYmhFOml41IwPTPVef8ALM/mQ/Kve+2dl/FrqT4nYbuHIbLnzLVfZ2X7KfrfZfXWwc7uXL5ba9BvhdtdS5zbuAx20MZVNisbTYuOOXJUeOSOgxi+GRV0rE4p14MzdpOPmcD+Xp1aj/Mt7oyHT3RGyszR9kZfrbMY75B/GSu37uPa2QzONFJsGfuDaqb/AKWsqsbetqMDXbdSqSpoCWNXRaomR1chrsaUqetuxIxwFAKfaP8AD00/BLtLdXzK7K7i+Zydn5Reio8znOh/jv0bt/clUmCxu3tn5Onn3L3D3DtqGWFJO1+w61oajEUVdTxzYHbM0A/easWcaB1VNccOqAk5J7RgD/V69FRz/dXcVN/Ka+YvZ0Xam+R2Ps35FfIbHbV35XZ6oyWf2/i9r/Luowm3cJS1mVNUrbdxeDgXHJQSK1GMbelKeA6PdSe01+X+Tr1ahjXNWp/vRp0F2N+WW/N91nw+imny3Tvem0PmHgeqvkt1bi8hUYmWmyUfSXbGfemqsb95US5/qffQp6DM4iZpaygqYXhVaiaenZxuvCvGvW1YgrTjWhH+1P8ALh0HvbO8Ich8u/lXsntTv75z7E21tXF/HTNdX7R+LND2tujbME29NktVbwrN7YzrnrzsOPbU00tRRTY+esSiSpeeqIeUppWuampIPy68TmmaY4An/AD0OXyZqP8ARFJ8JOrNx/LLujpLqzL9l5HY3bffQ7ih2LvzJ7a2/wBP73yOKyW/ezJ6OlxElVld1UFCtRVVdMtMaifyaEcI6WIyq1PWmNAKngaEn7D1N6c+U2+NsdN/zEN8YnuPc/y/+OXxGym19z/G7vXf0WPq8r2Bl8f19ktxdk9fVPYe28Pgcf2FiNn7oShpP4tBSmQpWNIsssL06x+BoDxI8utA4Y1BAyD+Xy6f9+dMfKfpz4YVnztj+bfyD3N8oNl9W0vyS3xtLce7KOu+MW56ODA0e8929SUnRlNjaDbGF2nFtyOfH0NZQNSZAVS/dLLC0ipD6hoGqa9eYFVJ1ZHH508ujeZfujdO8/mn/L0qdu7j3Rgeuu5/i78iuyc9sKDM1kW381VyYfozObUqdxYiNoqHK5TbMW4qhaWeSPyU5nl0FRI4O+Ok9W/FTyof8I6ev5r++98da/BjtLePXO8dzbB3fjd29F0+N3TtDMVuBz9BBl++utMPlYKTJ0EsNTFBk8RXz0tQgOiemmkicMjsp83wnrR8vtH+HotP8wjeG4dvfKTrLHd/d2fJv43fBzL9P1FFiu5PjjnczsnBYX5L5PeVViY6XvXsPaeIzWZ2ttj+6VXQNhhk0hwcuRZnlZ44a3xaateNB1omhz8PVlcvXGM3X0XsXb+G31kuz3wey9qzbS7RzebxW4Mx2EKPb9JBS7uzG5MLT0WGzdVvqg/ymorKSOKlqJanzRqE0r7U28vhOCfgPHqksfiJT8Xkfn0W3YG+cj1tkKnHuJqjb1ZUSRbhxFRTha7D5SFRTyZGGJwZI6iiK/uqOJEUE8hSF0kIkpIvxj+Y9OmLS58CQB8JXPyP+rj0dXDZ2mkWBaGspamKqjpa1JaWXzU9TDVR64pIJGGi8qqbqtiDybe0bKCCaf7HR+8azr4hzUYI+Xn8+nvIPS11LNDKwpnCySK7+uKMDgNKykFVkPFh7ZKEZ8um41khYOvcvCnA/l0D+UmKNUUcxejEVPJMKgMPFIQpI0kBiWYG4BsePeipqFr+fRgZBmvxdBVVT1lRUR6qpZxdkV9ZUAMnCaC1r2/Nz7TMJK0pX063hqnI+XXIRy6Q7T6ijpT2LeRi6pqYvpvbT9B73pemR8uvY/i6YMrTz1MD/bxs7lXlVnssehTc3C+sgf6/t2OobT5Hpi4AaMEL3DrHtnaz7ijkov245fPFKjy8mM6SXmXTytKJRZgOb2v9PboU1VjXIof9X2dI1UNHIhOQdS/b/wAX0JcS7b69x8m9c/M9NWUcdVDDQTKpnlr4AyBsfECfJTOoAEpA0X/r7cS2UyE17FySeA/2empLukXepEhxT1p6fInquP5TfH7tD5O7GzPcm18XWZDOdcLkMnjcUsVRNlN64Cf7V9y7ZwGMgRvv6+goaCGro4kjeSeel+0gBlqnPuOfc7lw8w7VFc2ERbcbSrKqjLxn40Hq2AyjJwQMt1k990r3bt/bvnW82HmW6SLlTfvDhknlYKltdRlhbXDMcJD3tFKxKqFcSuaQ9Uq41qasq1lpJIWx0sccxqEZ7sZSzROSraft2Rgy24txb3i8YyzmgxTPXWy7E0EBSZWF2rFdBp5cfnqrg/t6Gvr589mtxYXaO26Sq3LuvP5ikwmEw2IYCfL19azRUlNGZTFFTIkYZ5Z5Gjp6aNHlkdY0ZgrtLee5uIbS0jaS6kcLGinLMaAD0A/kOJ6j/mcbbt+13+97rOlps1tA1xcTz8I0QAsxpUsSaBVALOSFUEkA7UXx96ig6R6r25sQ1UOSzFPHLk91ZiBDHFltz5MrPlamnDJHL9hSsEpaPyDyiip4Q5LhmOWvK+xJy7s1rtoYNOKvM4/FI2WP2DCjz0gVz1xt9zueJPcLnPdeYxC0VgxENlAxqY7ePEanJGtsu9MeI7EUFB0NXsQdR/1737r3Xvfuvde9+691737r3Xvfuvde9+691737r3TBujGT5bB11NRyGDIxotZi6hf1QZOidaqhkU/gfcRBW/qpI/PvR/n0rsZ1t7qJ5BWGumQeqnDD9h6Cja8c0G6Yczj4vBiNyYoZCogVbQxV9Sf9yNIh40GHJQuVU/S597QVrTh0IrwLJt0ltKSZ4JCinzoPhP5qR0MsyBSkq8/W3+t9R/T8G3vfy6C8bYMZPSezMRp6ynro1H7y6HuTYzItvGw5GmaAkf7D3scadG9g4lt5bZj8OR9h8/yOekbj8faOfGxSfuYaZ6vECP0OcZO5mmoXAOlxTsxMdv7Itbj3pcHT6ZHTcy6HYsOx+NfXyPS3olt43Qlhp1qxvcqwu0diL/U+32IYA+vRSaozKfLgOnpRch19J+o/1/xf6cX+vtgih+XTuCPl1xlj1RiVfSL2Zbfoe+ki3+pDe/cMdWjajaSK/PqKurWeQFsLAWvf/X5vY/7x72QfLh081NPCrV675/s/S5sDyQfyP9j73X9vWscDx66pz/lERAIC3J55Ym45H+t70QKfPrcw/Rkzk4+zp0WUlwpA51abXHP+H9fdekJjAUtX0r02ZGJlYTpwjemW39lg11NufSw4J/Hu6mgpTpbaOCDGw7vw/wCXrFTt6lnGkQBGia5uQVJAFhfUPfjSlOnJh2tCa+ITqH+fqRUx6/t6pWH7YeCTj9SPZox/VdDj35Tk/t6ZgYr4sBX4u4fIjj+0dIneOJWbHy5yk8hyOISCpZELMtTRU8weeMoB/nYkuVYEenjn3aN6MBXBx/s9GFlMUlFtJQQyEip8mIoDX04dNm7WSjlwu+MapD4n7SvljQAvV4KtVKfI0uofRqWKZ5Lfggj3QjjU5HT9khmgubCU5NU+x1yp/PoYYpY5oo5omDxSxpLG6/peORQyMP8ABlIPuvQdIKkqRkYPXP37rXRGcJVvjc1iMhAdE1LkaOQOvB0NOkcysfyjwuysPoQfej17o83vfXuve/de6DHsncu4trQY2vxC0L0VRM9JV/dU8krxVDIZaZlZJ4h45UjdSLcED+vvR691Xd8oOi90/PnN9edN7sysexOosDTZzdO8tyYI4LK7izmYqqjF4WHCbX29uXbmfpsDmBsmXOUw3GtTTVWHkysbU0NaHqI4asCxA8ut+Rz5dM3xF/l+5b+Xz8iu2dz9Xbqfd3xY7h2BBLldv7nqYh2F1lv3YGSqMlsyBsoBBSb32hXYrc+epY6rxw5Slmlo4p0qlElaNgaSc460upS1DginTb8yum8/8oeuqbZkTbZmav7d6k3pumi3fPkYsLlNm7O7EwG5N2bfIxuNys80+R2xjZ6SngaNIJnZY5JYUYyL4ivXqVFDwqP8IPTj1L1Vvfon5b7q7t6yy+16bo3uvadNRfILqvLVmZoMk3Zu0scKDr/s/qijoMJlcE+crcVGmK3BSVNTh6Z6FVrC9VVLHGnuB+Xp16h1Eg8eNekfVfEnsHdH8tr5QfGqDdvWmO7C7Y7c7r31ga3J5jcSbXxeM7D+QFT2rt+hztXTbWqs8mTbbs6wSrR42sjFcTHE8yAyHwGMcevUoGHma/zJP+Xpr+Q/wsxW8Pk/0H8kMFT0O1d/9T7uoJd7UWRmmhj3r1ZU47MNRY+qNDRVureW1Z8oHx8zeFHgmqaWpcgUzU2iM0HHr1KsHJ/L7ehF3Z8cfnBsr5N/KPvH40J8T85198mdr9F42fEd0bp7exG58HH0/wBe1O2aRqCl2PsXK4lDW1OZq3XXWTho1hNoyJFPipqxFM9eNdRIFT9v2/LpjbpHs3tzsb4Nbp7Kh6lOa6f7Gye8e6cFQzZ/JbQydfluot67Mko+vqbPbeqKrKw027s9TT0wyy0TxwReXX5o0RvZNKjPXiD2+tf8hH+E9WR91dXbM7N6M3/09laBaPYu/drVuwspj8JDTYz7fB7ldcRkhiFSnano6mOmrXaFxEVjls2k2t7sRilOrujKSrrnz/P16rJq/hp/MM390ThPhF2p3j8eV+NFFicP1xvDuzZOH7Cj+SnYvSm3PsKSk2lNtLO01T1ztLdG5NvY9cbk8r/E8svhcyGGocy+euk001x01QkaSftPr0YH5L/HL5JTd6/F/uj4j0/x9p2+P/WHb/WUm1O8M32JhcE+I7DTrakw8eEGwdq7irJP4Pj9kSKTNNBovGoWQOzR7IOKdbzWv5f4Omj5A/H35k/K74TdndJ9vSfGja3du6Oxuucntmq643F2jUdWx7F2R2R1nvqR87ktz7Nl3XDuyePbuViWGnoJKNz9oDLHrmeL1GKkYr17OMZqP8PQ0fJ3b/zb3Nl6rb3x+ofiFuLqHdnXVdtbd+A+RNN2eM5S7nylZk6XI5WKLZ+Pz23d37Nqts1cMMmGq6ehkknjkLVZil0JsgnA63n8uhC+I/x5j+LPxn6e+PC7uyW+j1dtGHb9TuzIwmimzNbLW1uVyE1LQCoqjjMPBXZCSHH0jTTtSUMcMLSyMhdtjHWgKAD0FOnHsbo2l3nXTbhxeRTBbhkhaOoZ4Flx2V0R6Kd61YiJYKmMAK0yBmZQLqSL+1cVzoARhVemJbdXOsGjf4ft6L9htz7w6dyh25uHFiooEqXqocRkX8dO8ytJH/EdtZOMMkUNWhYEcoC12RW9qGSOVfEVqE8T/nHr1SK6uLRihBKUoM+Xy+Xy6MTg+ytqbvpYIMbWtjsnWOtG2FyEsNPlPuiAxipkYiGtpXB9Eit6xYEA8e0zRunxjHr5dHNrdwT8ZAG40OP9R6yZXD65EketKoYytRHKuiTWWIKCNwP2gq24BFx9be6eGWIz0sIyTTHSelwOGkjgf9oUsbtYwpaWWYEkLoILPYgnUvB96MQHy9eqa2BOM9dtgMfUpLTUsqXicxSOisJY5tPKabDyMighvrb37TpwOPWi54mvr1ip9pRQhZXkSbxsrfalZFLwxnUzSyi/iiYIb2HvQTGT029yK6fPjXpE7l7A2T19Vz/wdXrssI3P2cTAUNNLIoaWnqZox5KixIGgG4J+o9qgnYNeE/n0USThZXZWLP6fhHQa7Ix57fzcu5d6Zs1WKxGUpxV7diaRq6ox6MJWYImmKkw9LJIqyFSCUJCkH1e25GaRWjjGlP8AVX7TTz6YUgsHlbU9akfL/NXqxOljpoaaniokhjpI4Y0pUpwqwJAqARLCE9AjCAWtxb2kpTFOlpNck9Ut/Oz+XhkMtX7j7y+POGNXl8jNX5zsHqrFxRQ1GbrauOSTL7q2LCvjjqM3WuWnr8Rw2QlaSekJrWNPWQxzx7eNcSXG87DFWVqvPbLxJ4l4/meJTzNdOTQ5/fdy+9DbWVttXt57oX4jsYlS32zeZiSsSKQI7e7OSIkHbFPwiUKko8ECSIZ/5evwrqOmMXF3D2pihT9sZ/GPSbc25VMJz1ntevjiM8E66niO+M/GoFdNdnoKQiiiKa61qk29veSv3LEN33OGm6yLSNG4xIeNfSRhx81HbirDoBfee9/o+fbx+ReTb3VyXbTB7q7TH19whOkrwP0kJ/s1wJH/AFmrSER2i+5R6w9697917r3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de6QcNPHQ5PLY8jSkdQuYohwAtJlmYVQjAsNEGUjk4/siUe/LjUvl0dLI0sNvLXJXw2/0ycP2oR+zpUxN5YTH+p4gGS5/Ut/oSf6e9notkXS+o4DY6jVdKtdQy0zXElg8Z+hjkUh4iL8/q9JP+Pv3TsEzW1yko+HgfmOB6QsUppsrRVP6LIYpj9Rw2kqRb/Ej37z+XRjeKGBpQilR0uKcAF4gOY2MiW+jRv+Bb+n09uVxxx0TTL8Mg+w9ZxIoItfQfrf/H/H8W96K9v+frS/Cc56yq9pJYG+ksepG45ZV/p9blbf7Ee6ZpX06uchZB5HPUCxFh9LAf4kH/X/AMD7uKU4UHSqtc9ZVUjhWZnkNgbgkf7wQqn8n3X8uqE1OVGkdZo6ZYWLFtT/AItwqcDkfkm17396rQU6aeZpFoBRfP1PXN20OJFKlAwcN9dQPDhT+LN9fe/kePVVGpChqGpSn+DpmyFTVwVUyGVZKWaCyRuFKrGy/u8LZ9atypP4P597UAitOjC0ht5IUcIRMr5I9fL5U9evUcc6LKksbojRpLHI5BQso4sVJF3Q3/xt72SCcHrc7xMUZHBapUgcc/7PUyC9THNAeDIgKG5H7if0W/6f9796Pk3SeUCF4pRwBz9h6w0rxyEwzKHidTBLGSbWnUwyK4/Kk/Ufj34jGBnj1edGVS6nu+IH7Minz6Rq0zUWLr9u1lm+xllpaUSgWq8XWaggjLElm8L2b83U/wBPbp7gH8jg9L7eQS3MdyvB1qaeTL/q/wAHT113XvLg2w1SxNftqpfD1CuxZ2pYhrxlRc8mOegZAp/qp/p7YIoaefSLd4PDufHQfpTDWPt/EP2/4el9710VdEPrqWTG1dbQyH9zH1VTSswa92pJniDavyT47+9eRr17oxm5+zqnBClpcdiUrpP4VjKyqraiaRaSllyUTyU1NIkKFzNJHEWALqSPp9L+/V63ToRdr5r+8OAxmYKJFJWUweeGNiyQ1KM0VREpPq0pMhtfm1ve+tdJztKj+72VlW51UbUlcthc/wCT1UWv/rE7e9HrY6pcp/5uPw/6d7c3js/eVd2cM317uHdWw9wx4jrXOZSmXP4HIPi8gtFVwssNZRLV0bhJgQrrYjgj3HN97pcs7feXVjOlwZoZXifSsdNSMValZAaVHmB1mzyz9wD7wfNvK3LPOG0W+x/ubdtvg3O0Mu4xI/g3Mayxa0Iqr6GFV8jjy6Vu8/52nwm3Rt2pxGGyPbS1NXLS+QVnVubpo2pYp0mmUsZn5bQOLe0v+u5yrw0XX+8J/wBbOjGT+7r+8dEKtbbFStMblEf+fejTdHbjwvf+2dj7y2XLXRbb3zg6TcdJPlaCTHZPHYmeMPUx5PGzEyUWWo5LwSQOf26kFSeCfchbbuFvutja7ha6vp5V1LqpX0oaEjiKYJHoT1h/zzybvHt7zfzHyRzAYTvW13T2dwbdxLEzoaaopBQPGwoVagqCD0eSoxWHgw9LgYqSjlxMERpTSzLFNZQCDI9wWErsSxkWzlze9/ZiFHBhjoPwQ6i2tDwqMdBp1jT4nGZDdr+COQ0GV+xx+RdBLPHR/vK0KSk6lUBRqK21fn8e6gVOOPVVt3kZ1QZBIoeuPcWKWposRuOBLrA5x1RKb65KeovJTO62soSoVgDf/dnvxxg9NOhQsp+NTn5dKTYOShyWysRBNOY5aFqmgksGZmWjlKxXVbWLQOgF+D72v2V6UWviBmdY64pnoJexcGcTnTmcbG0NBkZ0qInTkUuUiKySJdbhBM6iRPpc6gPp70RT7Om5oZI9Ltknifn029+/LHq3oTp/b3ZHa9dlKHE7k3hgdnUNNgMTPnctW7hb7vNV0UWNpCrRU9Jjdv1U7ySMiKiKNReSNGIeYOYtt5as4r3ci/hvII1WMAsTQngSMADJ+wcSOpN9qvZ/nH3n5hu+W+RLeCS/t7J7+4a6lEMUcSPHHl2rVmklRVABJJrQKGIK7XfzpPhHjkD1WW7OS97IOuci8hIGqwRasm5HsGt7ucqLxW6/3hf+tnWQFv8AcE+8JdNpgsdoPz+ujA/bp6Sc/wDPV+BlLK8cuU7ddtdh9v1RnJhYKD62Wo03/wBbj20feHlIUol2f9on+WXo7j/u5/vITIHSz2MCmdW5Qj/J0ez4nfMXpH5o7G3Dv/pDK5usxO093VeytxY7c+Bq9s7gxWapsZi81C1RiK1mmbG5LE5iCelqULQzAugIlilRBpy5zNtnNNnLe7YXCI+hlkChhgEGisw0nyNeII4g9Y5e9XsT7g+wXMW18s+4VnbR3t7YruNrLZzLcQyQtJJEaSpjXHLEyuhoy0BppZSTSXH9fYh6hzrv37r3Tfl8nS4TE5PM1xlFFiMdW5OsMMTTTCloKaWrqDFCl3llEUR0qOWPA9s3E6W0E9zLXw40LtQVNFBJoPM0HSqxs5twvbOwt6fUTypDHqNBqdgq1JwBU5Pl1Tsf54nwB3HiRHVzdsVmNytCkklJXdS5SWKemqYVlCSxmqkiY6HH0Jsfofz7i8+8nKcbUMd4HH9BP8kvWclz/dz/AHj7eaa3ltdiLo5jam4xcQSDxUHy6L1ub+ZZ/L4qXbIbB3L3HtauLqXoKnq7OZLAzRmw8YgmrDV0mpjyweRbcaR9fdx738oxmjJef840/wCtnSF/7uv7xK/8RNkH/UwiP/PvTFhP5s/Q2ArBUYjce/KWUMzE0Gyc/Fi6skkMtZhcjGaR0c/nTcE3+vu597+R3qJEu/8AnEv/AFs6TN/d6/ePhNVg2WnoNwjI/wCO9DHjP5zPxsr2D7n2/mMjWUqaafK0+ztz0cxeTSJBJT0mMy84Z0H1UKnH491T3p5GZtJuLtB/SiqP5Mf8HTU33DfvIW0dRtO0St/BHuNuv51lKKB/tq/LpZ0f8z/pze0wg2rurYe23qaqJKGLcBy23K6plkFqamjXdtNgochK0h9QgjYlhpt/URbf7m8ibk3hwcwxhzilxqh/nKqKfyPUV80fdY+8Ryskk+5e2F/NbopdpNt8O/CqOJYWUk5QDj3AdDzhqLubumShJ+9XBVApmOcqEFDh46ObTUCohKrElfGYmDKIldmGmxtb2Nku4njWS3dWRhVWQ1BB8wRUU/1DrH6e0vY55La7heKZGKOkqlWUjiChoQR6EdCfuX410u3dsNkcbU1+49wUconrx4AkU1KyOJTQ0SMz+amJD+pnZlBAF/bkUmpm10FeHSe4t6RVhLFgc/Mfl0D3XfWPauRzDZTbOKqsXRLLGTksu7YyiqIppLBjTzqJK+GJU1NGEe4tccj3ppFVm8/s6pHHIyoQCp9Tj/i+j1Z7dOK6R6mr91bzqK6vxexsEKzN1GGx71ldUpHKkbmhx4dGld5ZwFUsthySAD7Jd53a12Xbr3d70P8ASwrrcIKtSoGBiuT0LOUeV9y5u3/Z+VdoaL95XkgghMzeHHqoTVmodIoPQ/t6Kif5lvxoAv5uwPoDb+5k9wGNhcfffW/uOT7y8nLSou60r/Zf9DdT7/wJXu3WmjbP+yof9AdOuD/mK/HLcGZwuDoqne8VVnc3icFTT1u05aWipqrMZGmxkE9fUvWlaWhp5qoPPLYiKJWciwPtRae7fKV5c2trF9UJJZViUtGAAWIUFjqwATk+nSHc/ute6e07duO53Ue3G3treW5kCXIZisSNIwRQncxCkKPM0Hn0e33J/WOXRUu6PmX0z0Lvan2Bv6TdaZ+p29jNzRnDbdlylB/DctkMzjaQNVrUwgVJqMFPqTSdK6Tf1WAF5j9w+X+V9xTa90Fx9S0Syjwk1LpYsBnUM9h8upp5A9hefvcnl+TmblpLI7Yt1JaH6icRv4kaRO3aVPbpmWh8zX06CsfzLPjOSB59/C5Khm2bOqah9RrNbpBH+v7I/wDXk5O/5e/+cQ/6D6GX/Ale7dCfD2z/ALKh/wBAde/4cs+NFyPLv+4H/PGzENc2AUiusxJ/p71/ry8nel3/AM4hn/jfXv8AgSvdugOjbKf89Q/6A67P8yv40B/H59/a7E6Rs2e9lIVjb72/BPvZ94+TwaH6uv8AzS/6G60Pul+7ZXX4e2afX6of9AdZD/Ml+NoVnMnYARbXc7Nm02NwCD99yPSfp72feLlAcRdj/m1/0N1T/gT/AHYqF07ZqPl9UK/8c66X+ZP8a3sVl3+Qb/8AMHTC1rXJvXcfUf7f3se8XKB8rv8A5xf9Ddbb7p3uypoU2z/sqH/QHRqene5Nld6bOXfGw6ivmw4yuRws8OUo/wCH5KjyGNaMyQ1lF5ZjAaikqIamK7Xennjew1WA52Df7DmTbl3PbS/05dkpINLAqc1FTxFCM8D1DHPXI2/e3e/Py5zEkQ3ARJODA+tGSQVBVqCtCCpxhlI8q9Cp7O+gd0kt6b92V1zhZdxb83Vgto4SJ1h/iOeyVNjoJahwTFSUv3EiPWVs1rRwQh5ZDwqk+0G47pt20W5u9zvY4LcY1SMBU+g82PyFT8ujzl/lrmDmrcE2rlvZrm+3AjV4VsjOQo4s1BRUHmzUUeZ6IPvv+Y70Hj8pQybUot773nxdTPBNU4/AwYLGVNFVwGKsh8m68hgssNDrG6sKNkuv1tz7jS+95OVbdmSziurkjgyIEU/85GVv+M9ZH8v/AHUPcy7tpP3xc7dt0cihgksxlkDA1U0t0mj9cawekHT/AM0HYNM5kk6p38sKswLHJ7Ua8Ye3oK5UqzEMPqR/jb2Wn3v2uudiuPmQ8fQol+59zLMgROdNt1kcPDuBn84+hJ2v/Mt+O+crqdM8m+NiRSpoebObXTMUpn/A+42Zkty1EcbfUM9OlwPUFJt7NbH3k5RuWWO6S6tnPnIgZf8Aqk0jH/eR0EN4+6R7qbfDK22vtu46TULb3Bien2XSW61HoGPyr0arb+/OvO1cbUbj623rtveuOjjJq59u5ajyTUFdCiutNkaanlarxtXNFcGKdI5VI5A9yJte9bTvcJn2ncobiIfF4TAlT6MOKn5EA9QjvvK3NPJ8ybXzZy/d2F7UGJbqJkDqfNGI0yLX8Skj0PS1oqsvS46siLOVKQOFBIb18XHP1W4Ps4WlCK/PoONGB40Z4Urnp3rv2pNSn0PZr/S4P1F/8Pe0NRTz6QIaUrw6xtNrpRIDdqWQBTcfoYrx/sD/AL370RRuGCOlKL3U8iMj7P8AY6ku+vTMpss6a9P1CyLYSqf6sGsf9j7quK1OerqumqEZU0r8jw6kUy63VgP82rNzYaj+lR+Dyf6+9HFc9J5jpUgnif8AZPWB5C73KqrkFbC/0F7Dn8i/v1Mcfy6dCaVoCSo65KwIdBqLRATC6kqV4RhxxqU/7f3rFOqkUKseDYx+3qFXU4qaISIoE9O5dXABaRIwQY2P1ZSjG31sQPdshun4JfAuaMf03FCPIV8/29YcVUCSMwrZhFodD/zbkuJAv50rJ+P6H35gRnp2+iKsJDxaoP2jh+ZHWZ5PDOSpA0uGWxuDYHg/14Nj79mn+GvWlXxIRqU8KGuOuOTIg01qG0MoVp+Dw6r9V+mlnQf7Fh/j70p4g9estUmq2b+0X4fs/wAtD025eKPJUdFXKTdCKWZwSCYpLPCzsvKr5APqONXtxGKkgcDkdO2qmC5mt3HHvT7RxH7Ok7iLYzc8VYbRx1cMeOq25CuJnb7S5vp0w1KAL/wc+6uK9Gl7GtxtrqoJkU+IvyAHdj5g1/LoXfbfQQ6JPuLHVVNJQZKrDX3NRPn1V1KmMV9VUSNA4I/UkbIx/wCD+9fn1v06Fak29JXdS5KumDVOTyB/j4mf1TGPFtHBSRk2uY4sZSFVA4Ctx795cevefTv0pkxNiMriWe7UNctXCCST9vXxgnSD/YWogc8fTV78OtdCNu8RybY3BDIQA+GyBUnkFhTSMn4tfWvH+t731ZVZvhHXz/PkVgvuflH8mamRVvU/ILthgrhhIPLvHJmMGwuLAA3F/wDH3hfzLHXmTfyf+U64/wCrznr6avZbc/D9ivZGNSaLyhtP8rKKv8+kph9sU8dQksrISJDEQhSyrqvrEnCuW40/QG3Nh9SmNMk+fl0Kb/d5GjKIDSlc14+lPLrcL/lrBab4xdeywSMWXa89GjAAs9O+6s+7HXwY1fxAtpF2tb3l5yEAeVNl+UR/4+3Xz4feJjE3v77ovIo1DcyaGuD4aeXnno8OezCYfHVtdJIv7aBYYl481Q3EMYB9WnVyfpcX/ofYwY0B9fLqI5nS3gaVh8IxX18vtqf2cemjZaxY3BwfcLeqyEkmQrJZdP8AnZ2DJw36gkduD/j7qlFGfPpuzs5VgRif1G7jTj3Zp0tnkoctRyUFesdTjqgxpNA7M6SiJ1lVRyoVVlQH0+9kA16buLI51JV+ORT9vn1yo6XHUMBpcZS0dFSBmkMFOgAeQkBnlK/2yF5JJJ49+UUFOqJCYVC6TWv2D9nWOtoqTK0tTQV0Kz01UugxsdIBBGidCvMcsTcow5BHvZoRnq0kYdNLCo8/8329al384Pu2Wq+SuN6FwmWlyO3eh8FT5DL+N3jpz2N2Tj8Zna6irabmCpqsHsejwjRzIbK+UnThg4GMnu9vAud7t9rjc+FaIQw/puFYkHgRTSPkVYddnP7vj2jXl72f3T3C3GMDcuZ75lttQ7ht9gzwIyniPGvGuQwxUQxtwp1TzX5CfIVEtQ/pedy7aSbAkWGokm6IPp7h1mLGvn10ItrSO0iSNchRQV/1cT0xJTnysZVZDZ1vcfUnkAj6k8X4+p9sFaEVGejFpBoGk1yD1dL/ACQO+v8ART8ra7qbIVwpNufIva7bbi8rylI+wOv6XM7t2XOqysKKCOvwM2foCTplnraqiiXX6QJc9n96/d/ME22SvS3u00itAPEXKEn7KqB6t1z9/vDvbX+uHs5Z88Wttr3Tla8+ocqFqbK9aK2uQSO9jHOLaQDKqgmY0zXcNpYgmuQRNH5m8jmV2eZ3tpDOCSsfoA9I+nvKLrhhK2oqNVaYFOA+z16me/dNdJLf4vsTeo/rtLcY/wBvh6we0G6iu17kPW3k/wCOHo75ZNOZOXz6X0H/AFdTr53dJtiKnwOK8LJf+GY4ReONUBAp0uAqgiM3H0PAX6+8EpkqzPqySSfPj19Rs+7tLuV74oP9s5NT/SP7f8Nem84eSOVrSHSXchQhZWEaAlCfTZlf6i1rc+0xjaleFeHSkXyOg7c0ArwIqeP7P59ONNQ6ZAr6nYQ8+NSXMjcqukqQByOALC1/bLRAetekk1wNNVxVsV/w8epkT/bHlvGwl0EtzqK3UMwQnUim/qH+t7aKLmvrT5/z8+k7qZeAqCtcf6uJ9OlLRZIujxGDTHJZJlIDxH1Bk9DWGhhfVf8ABtb20UINCooeNOiqez7hIJKuMr6/t9fTo1Px++Ufd3x0ytNXdQ9g5va+PSsFdXbOqJHzHXme8rL91HltlVcn8GY1fjEctXSLSZNU5iqYm9XsQ7BzVv8AyxcrLtG4yRJqq0R7on9dcZ7SaYrQMPIg56hr3O9nvb73Usprbnjli3vLgxmOO/UCK9hp8Jju1Hi9tahHLw1+KNhjraC+En8wHY/yux6bU3BQ0XXvd2Nx7VmS2Ya8z4fdlDTAip3L19XVYiq8hQJGFlq8dMprsX5NLNUQKlZNlVyJ7j7fzfGtncItvvqrVoa9slBloicmgFSp7lHmwBbrj794T7snMPstcvvW13Em5+3ssvhxX+ikts7fDBeotVRyahJVPhzUqBG5MS2JgH/YAWH+P+Nh7krrF3orvzXbR8VO8HuRp2TUniwP/A2i+l+PYI9x/wDlR+Y/+aH/AD8vUxfd+Gr3n9vB67gv/HH61hadomZbIyejQwDftB7sQwuDdLHTybk/T8e8LBTICkUxx66+yqy17gc1+dP8/n0udh2m3jtAOyK3949vMsSH6NHmKIOJL3C2Q2AuSbkezjZe7dtq1UqLiI0Hyda16CnOPZyrzPpBp9Bcip9DBJSn59bcnvPLriX1r8/zNzIPk/jgnOvpfYyj68Sf3w7L0NdSGBS5PvFX3nr/AFxiA4GwiH5+JNTrpv8AdF0/60FyT5b/AHf7PprCo/Pqvf8AyiNgCQDLrLKSNFo/92K5v65GNif949xKBIpHz4/8X1k/+mwrTAp9v2fYOs+giGcfuK0iJoRjyWW3pjKhuFsSCLX593C0VqAgny6bJq8ZNCATU/5+uUbuZz6pI5GKsCDGWbQFQXZkLg8Wte1vr72mrXQ4/Z1plTwwKArnjWnn8/8AV5dOcOPqZ6hY9TyaryI0h1FX5MOkcX1j6/U3+nt4IzNRjn59I2uIYomegHkQPMedenyk2PkZgtUfOl28TmQ31anHq06Q2lL/AEsf6+30sJGOosQOBqf8PRdNzDax1iGkkCoA/wBXHq9T+XFi2w/S28aBjdou1sgzN/XydfdcOD/j6SPeU3tPF4HKrR1rS5f+ax9c2PvQ3Yvvce1uRwO2RD9k9yOjEfIbu+g6Q2UctFT0uV3fnJJsZsvb9TM8cWQyaRCSfIZEQH7pMFhY5EkqnjsWZ4oFZJJ4z7EXN3M8XLG2/UBBJuEpKW0R4Mw4s1M6EqC1PULUFgeo89rvby59w+YPomleHY7YCbcLpQCUjJoESvaZpSCEB4UZyCqMOqLN9wby7Z3RJu7sfceS3LnKtZESauKrS4iBmZ0xOBxUY+ywuKhcG0VOiqzXeQySs8jYwbpLuG+3rX27XTTXLY1N+EfwqBhF+QA9TmpPRrlx9h5K2dNj5U2uK025CCVj+KU0zJNIe6WQj8TkkDtXSoChBydW+Oepdp4xTSRqUgMayTGsQrG0gZQFK6VUWH+tz7K220KXJPaRw+fQkTnDVFCFjPig5atBpOaZ64jq6kUxRtNYjyeUrHGkKXaz2IBNl/rf+vuo21MKa/PrZ5wnOt1T001JJ+XTl/o3xkWrTEtRqLGVXQENq0hbiwYBQOT+TwAfbv0MajCg9I/61XblasVpwI/P/V/l6Uu29uS7SysOe202RwO46KNYoc1hK6rxOXhSS9gmQx8sVUsEq38kRYwyR+l1Zbj2ss0nsJkubNniuk+GSNirCvowIOfPyPn0Vbtuke92cm27uIrnapDVoLhFkjJHqjgrUeR+IHIIPVofxL753ru+prNg79o0yWQpKCqy+L3ni6QU1PU01FNjqSWk3TS08EWNostUVVd/k89MsUFYA6CCNoi0uQPt9zfuu9tJtm72/iSxoXW6QUBAIFJVAChiT2laBqEaQQScMfez205a5bW35h5auTDbTSiGXbpmLFWYO2u2cku0QC9yuWZCVOtg4CnwXxVkE0ThGkSImMkeoI51XUD6eOUD/Ye5TB0MCOHn1jdLGUNPI/4R/n6T2PqgXejdgHlR42U/QugJBtc21D/b+3pV0nV05CdSBqVI6ccdOzwyU7CzprliUk31wDTNHyLgmPn/AFx7YYZr0rnQAxzfhPa1PnwP7enWmqFjdGJPjkUIzWPBfSUYj8Afn+nvRB8uks0JdWUDvBqB9nEdcqpNEzC36vUtvoA1xe30uG+vvwzSvVYG1RL8sH8us8EVishFlKOjHmxN7H6n6Mv0/F/ejXh01LJgpXNQQOuo0ZPIlgUDBlPBBFrXtx/UXHvRPDr0jB9DVOqmek+KKWnyEjxFY6Y+WxVyrqZl5h0af0JJyDe9vduIAp+fRp9QktqiuCZRTiMYPH9nWIHUpU3BS6te1wwPLf46j7txPT1KGvkc9O6RJlKCoo5WKMNPIGoxtfUrgfXmx+n9fdGGa+XRc7tZ3UVxGKj5+fkR0yU6zUNa+MnhdaKqieOOViDHK0YLwSL9f3lIAYH8f4D34E4oMjoykaO6t0vI5AbmMhivmAcEH5dM81LLVzPTxlVeenkmR9VtEkNnDxHkNJDMisFH4J93JGPTpasscUYkaulWCkeoOM/Ig9Pn96X8Xlumj+7v3v6T/wAXT7v7L7f/AIN5uNH6vdNJ/nTos/dR1aKd31Ph8fwadVfs05r0je38RFU7ZxeWoFjaHDyxoGp7PGMXXRJCjrIlwaeOVISDe1jf3Q9Eg8+l/tCCKbZmBp3QGGbB0sUiWADJLTBZBb6eoMffvLrXQDddtJgN+VOClmeAVByGFlZbBzJRyNPSBSVbSZFgOk/Wz/4+/VyMdXVgprpB9Aeh33fC67Vy9PHJLLJPStSQ+Q63Z611pEU20l7NP/rj3Y56uJAzltAFVIouBw60YvlacBtn5S/JtXCyVEHf/bklOhGlRbeeXRWfWj8pf1jk6QFt7w25n0JzFzBX/lNn/wCrr9fRx7JQ7luPsv7PRR9tuOV9sQkZwLSL5+fl+3orNfvWzGKjKQMIUSJ7FSgMhLlW4KBl4UG9h7DrTKDQH9vU023L50656sNRJH5UGP8AD1uLfy8tvZ0/D3oLc2Br6U/xLZc0tVR17SJHIG3DmyF88d9aHTqDEKy3PPvL3kCp5Q2F1PGI/wDH36+er7zlvNafeE91TAw1fvV1KMMYVPT0I6OHV7dz2ZrY59x1VGtHSOpSgoXcwknkh5XAte9mc6mK+kWv7GDBjQtw6g5bOa7kjku5AIxkRpX+dfX/AFU6m1dWKOISW1oobQApAJXglf8ABQLAD3R3058vKnQut4PGbwxg4H2Dy69RZyUxlVjCpGqgF5BrVpQDcuAEJA5P+29+WXj1u425QwLPk+g9P59O2OyMsoVC2q0jeSx0k2JAJH1ANvz/AF9uK37ekV1apGxYDyx1A332Ft3rHY29+yt4ZBMbtPYW1M/vLcuTckx0eD21i6rLZGWMEeqVaWicKvLM9lAJIHtNfXsW32V5fXH9jDG0jU8worQfM0oPn0s5b5Y3Tm/mLl7lPY7Uzb3uV7DYWkI4vNPIscYPy1MKngBk4HXz8N7b73F2lvvfHaO7zON0dl7w3H2DuOnaqlrRQ5bdeXqszPiKeoca3x+CSrSgpF/TFSUscagKgAwf3W+l3Pcby+nfVJJIzsQKAliSSBmlSa/n19N2wcubXydy7y9ydsQX9zbRYwbZaMFC64raNYllZRweYqZX82kdmOSem6io6nIVNLRUVM9TW1k8VNTU8CmWSeonYJDBEqgtLJLKwVQBck8e0KxtIUjjQlyaAAZPp0ourqCygnurucJaxIZJHc0CqoqzE8AABU/LrNW42vxGUrMTk6OehyeNraigrqGrRo6ijrqWd6erpKqGVdUU9NUxtG6tYqykH3ponjkkikQh1JDA+RGCPtB6pbXtpuFjbbhZXCy2U0SyxSxmqujKGR1I4qykEEevSm2du7O7A3ZtXf8AtKoho937D3Rtzem1quZ54qWn3JtHNUe4sK9ZFRtHPPQplsfD50B0zQF42BDWKqxuptvvLa9tm0zwyCRWwaEGtaH08uibmLYdu5q2Le+V96iL7JuVnPt92oAZjDcxNDIU1ggOEdip4q4VgQRXr6GHT3Z+3e6uqeue3NpymTbfZWy9ub1w4kI+4p6PcWKpsnHQ1sf1p8hj2qDBURNZop43RgGUj3m5tl/Fum32W4wH9KaNZAK1pUVIJHmpwfmOvl+525T3XkPnDmjkre49O7bTfz7fcAcC8EjRllPmjadSkYKkEYPQji/N/a7oL9JPf5tsTep/ptLch/22HrPaDdTTa9yP/LvJ/wAcPR3yyK8x8viv/E6D/q6vXzxMTkJP4JhpisaL9hSBv1vaZqeNZGUXETLoP4JDf4e8FZcE09adfUPeWq/vG/jBJ/VanAYqafOv28Oo0ld55EpWBJDqGCyLEywuTcrezm/5B59tHuoDw6cS38JGlX0NK5yPXq/XYf8AI+3PvbZGzt8Y/wCRGAp6Tee0dr7ro6eo66ynnoYtw4SgzApJWXeQWoal+88YkCxl9Goqt9Amyz9l7i+s7O9TfowksSSgGJqjUoanx+VeuZG/f3ie37Nve8bJP7UTO9ndzWrsNwQBzFI0eoD6I6dWmtKmlaVPHqXlf5BXZH28kuH+Reyamt1tItPkth53HU0xbUdElbTbhzEsI1H6iB7f0PvcvsVf6D4W/QlvRo2A/aCf8HVbP+8t5f8AERL32mvFgoAWiv43YcMhWtYwcf0h1Xb8k/5dnyq+KNDVbm3ttSl3N17SyNDN2NsWtm3DtvHRvJHFFUbghFLS5vbEcryxok9fSQUrzusSSvIQvuO+ZPbrmblmN7i7tRJYA5uIDqUeVWFAyA14sAPKtespPab71ns17z3UGz7Lu0lhzS4Gja9zVYZZD5rA4ZoZzx7EfxKAtoABPRQMTkp43EXlRTdFiikLyyomnUQWCABRbVxwB9fYHAoST+eP9XHqer20iZS/hkjNWFACfsrx6F7Z+887tLcm3917Tz1Vtzde2MnRZjbO5McgGSwufxz/AHFLX0wlWWFgqsUkgmSSnqoGeGZHikdCrtLm4sbuC+spilzEweOROIZTUEV/1HoD77sO3b1tO57LvW2pd7JeQvBd2kv9nLC4oyNQg8chlIZGAdCGUEbnPwx+S+M+VnQ22OzUjocfuymlqNq9lbeoGYQbf3/g46cZinpYZKirqIMRmqWpp8rjFllkm/hmQp/Ixk12zW5L5mj5r2C13PSFux+lcxitFlWmqlfwsCGXJoCATUHrgl79+0t37M+5G78os8kuyuFvdpuZPims5i3hFiFVWliZWhlKgL40UmkaadcfnI/j+JHfElyNGxatuLg8VlF9CvqBP+HtL7j/APKj8x/80P8An9erfd3XX72+26+u5KP+Mv1qyUFZVaJCZSo1EjVCZHSVTqFrtfUENh/ib+8LlRxr0t5/iH+XrsfcwwAoNGfkfL/i+hZ66kmk3htR1ZP+Pm240rNGFdlfMUVhfUQQSbX+vF/Ztsin977YQwzcxVx/TWvQB52CLyrzMCD/AMk+50gHH9i/W3f7zx64jdUAfzNaOeo+TePkhRm09M7IW4UtY/3u7K/AIsLNyf6H3ix7zRu3OELLw+hi/wCrk3XTT7o08cftFco70rv12fT/AIjWHRBosVO9P5NUvqWLUBGAUcMTePUdIBIFuOQefcVeCzICSTUjI8qfLrJV7yNZdAAwTSp9fWnRsvjb8SMt8i6XeAxG+KDbNXtP+7NZPFksNWV4qoNyy7np4WilpshTRwtBJthwV0vfXe62GqQOTfb+fm62vpYt0WBomUEOhaurVmoZafD1BXu17623tZf7NBcctPexXaS0ZJlj0mLwqggxOTUSjzH5+RnY/wCVhvNWDN2ttZtLFkA23mBpJJPI/jBDf059jL/WOvcV5gixw/Sb/oPqIm++ZtjAgcjXGRQ1uk/7Z+n6H+WVvOPx6uzNqv4zcH+A5hHDAWQo65T06f8AW4/HtUPZa7AA/fkWP+Ft/wBB9Fr/AHvNsfXTky4FfL6lCPnUeB0s6X+X3vimh8R7A2nIRb9xsRmgx4Au18g2o8cH8e1Y9ob0Aj98w/8AONv+guiCb7z+0yvrHKdyvyE8f/Wno6/xy6eynS20dwbcy2VocxU5jdsm41qcdBNT00Ub7Y2vt8U6pUSyzM+rbxlZjbmXSAQuoydynsMvLm2Pt8s6yN4pkDKCBlVWlCSfw/z6x99zOdbfnzfrbebaxe3RLYW/huwc1EsslahVH+iU4eVfPqur5Zb5g3T35uXB1UrGDYtBiNsYqEyP4kkqcbRbgydUsRHiWqqK7L+GT/VR0sRJ9K2hT3B3QX3Nd5bOey1VYYx5ZUOxp6lmp9ijrLL2T5dfZvbXaNxhQeLuUkl5M1BUhZHhjUnjpVI9Q9C7epqFVJt+OayCZidAeC0isKgAWtdTwU/2Fvzc+w+loJDQGnpnj8uhrPubR9xjFK0bHw/8X0PPVPxpyvaCZKsXL0uDxWMq4sXV109FNmqt8g9DQZY0NNjUyeFSCOmxeVpZWqpKlizThI4H0yOgy5d5Hk3tJJ5Z/Dt1YJUrqJOkMaDUtAAwyT50Cmleor5394IOUZLazgsjcX0ieKFDCNFXUyambQ5YsyMNIUUAqXyB0MWW+DpRYIsbv+gjeRWiV6zZtaR5EGtEM1NvWLxCUAi5SS1r2P09iib2rtmjb6fcyJP6UdR/KQdAKy+8Te6pJLzl7UgyVjnANOFe6Bq0/LoEN3fGbsjaElXKMCuaolAJye0pqjcuk+YQIs+Gkx9FueOSQMGVaSjyEUIJMkyqpb2F9x9vN629WkiiE0VKloasfzSgf7AobqRNi95eWN6WBLi6a2nP+h3QEY4VxKGMRp5l2jr5Ak06CrHbSlrpqKKmpxWPWPTUtLHi5Iq6Sukq6laXHR4qWOR6aslrqyVYU/c0GVwGZRcgMW22TT3EUCRVkY6QFySa0AHkanHGleNPId3nMNva2091NPphRTIzy9oUBdTFxxFFFeFacASQDYP0HsGl2BU12Bq1pTnKtqqpyVRSN5opsjRUv+SUME0qpNNjMPSyzJS+lBK8s1UUSSplQZC8r7FDsO3pAgBuGOuVx5t6A/wrwX82OWPWIHuJzVc82XlvuhZhYpRIY2xpQnLMASBJIQC+TTtSpVF6MsKsUFank/sOiSm3H280anUCR9PUD/sLexTTWtB1HjxmaCq/On2g9J/IM9HlqqNI/wBymkinUJ/yk0k51ROlrm8T3Bt+D/h7UAeJErH/AEp6SQOFJHkTq/z9OElU0Fcs0LXc6asA/o/UBKG5Fmdbg/1P19pyDpIpno3jhWSJomHay6f837D0oatRABLHb7WosyOD+jyLr0gfTS34/wBt+Pba5rXj0gt2Mv6ch/XTBB86Yr+Xn06IgqqWCQmzKg5I1XI45BsCLi9/deHSAt4E8qAYJ6khdEYU2OgC5/2m12JH1HvXTVdTFgOJ6bWrGY/tQ/tkcO7W9Nx6igAtqHu1KcTQ9LFtlUd8neOIHWVBHPrB9DqAQT9DcWubc2uLH8+9Gopnptg0WlhlT0x1sbwTOtiFcGSwFiWHDi/10g8j/A+3FIpx6M7eRZIga9wNP83UqimMUiOxtG4ERNhxewUsfrdWNv8AWPvRGPnx6YuohIjAfGO7/Y6k5SnWePwsGvJIhgZUZmgqVVikupLlUJGlr2HNvda4Hr0ltJ2gkEq8Bhh/Ep4jpMSMyRUORiUmSllkWaGMEH7in1JVQKgX9U8R1AAckfT37iDTyz0eoAz3Fq7DQ6gqx/hamk1+Rx1g+0h8lvAfD/FP4zo1HT9v9tq0W/1P3/7mj6aufe6j1+X+z1fxZNNfE7/C8CtPOtK/box9nU3YdH9919iKHJx+aCrxs9O8UlyXoJpahIEN+R/kjLpP4Fre2/t6Cx+XSyxmOpsRj6PGUYdaWgp4qWnEjtLIIoVCJrkYlnew5J+vvfWui89oYyq27uzH7soo2EFVNSVPkVbJHlaAgyQuQSFaspY1Kk21EN9be6nrY6GE11DuWuwiUM61VKkEOdqhGdSwRlT/AA6OdgGQT1FQxPjJ1BYWNh7t8urh9KMoGSRn5en7etAz5uZiM/L75ZU0dz9t8k+6YiYwU9Tb7zAL6yTrKqFXi1xf3hVzfJTmPmBf+X24/wCrz9fTv93uwf8A1jvZWVqd/Ke1NnOPo4v9nopqzTzOhBJs2kkWsLMNClRZSqDgHi1/YYBJp/q/L7OpqaOKNWB/L/L88+fW93/LZVB8FvjYrDWf7gSHT9Ncpz+a9TOwICKB6Rb9XvM/29qOTNg/5on/AI+3XzcfejZ/+CG92yMf7uJM+g0rwHr6/Lo41YYYUledzJ/ZWLSACx4Cn6l2J+v9PYyNANTHt6hWDxJCixpT1P8Aq4dIrJBpYvMysqvdVBQkBfpdAANOlfrx7TvU93rwHR5akK4jUgkZJ/1cekekqATQKGskjLdCDqOgubK30IU6je9+Le2Kg1Ar0etGxMch8wDn/Y+eOlTgJ3FKZGIZJG0tUMNLyITpRgouWMgNzbkH2ojYlSa49eifco18YKBRxkIPI+Yr8uqh/wCd53quyPjXtfozDVxizffe7YYMvBFUPS1UPWvXM+N3XueUNGfJLBktztgsXPESEqKKvqFbUgdDFvu5vf0GwRbbE/6t0/divYlCc+R1FSP9K3Wcf93p7cnmH3Y3j3Fv7fVt/LVkWgZl1Kb++EltbjOA0dv9TMrcVkijIoaEariRpY/qAIN/1cki/wBeLsefp9feMQFfs67KMxrilf8AV/LqwD+Wr0knd/zB6jw09GlRg9m5kdmbm1LI1MMLsZ4cxTQ1IjVkC5DcMdFSEMQjCfT/AK439v8AZ/3xzVtcRSsMT+PJ6aY6NT82oPz6xd+917hN7fexPOtzHOV3HcoRs1pwr4l2CkhFcjTbeKwIyCoPSn/mt9QwdK/OHstKGkSk232vjdu9z7YpYoI4aBF3VHVYTeNMsqRRxvXSdg7XytdNGusxRZGE3AdQFnubs6bTzVeGNAlvcD6hAK/j+Mn0/U1AAeQ4dIfuX88Pz993flEzTF912WWfYLtiav8A4sVltWpU0QWVxDEpxUwv5gk1xzTo8rmKTyIdJSRgY2awJLXt6he4vxq9xySOA4eXl1lVHEyoupSGzUcfy62vv5DPf43p0Pv74+5mteXOdJ7sk3DtiOd5HeTrrs+ryGbSCOeeRpKyfDb+ps35QvopaStoYxZSo95J+z29/WbNc7PM/wCtavqjGB+m/kAOOl6kn1YdcVv7yD2z/q97mcu+5dhbhdt5hshb3RUAAX1gscLHSoAUS2bW5BOXkSZskE9Xy2/3x+vuYeucXSR7ANth72P/AGaO5OP6/wC4at49l+7Y2rcz/wAu8n/HD0ecsCvMnLw/5foP+rqdfOSx9dVLtvCsGT04/HK+h/29P2kZEIjC6RoSwJvf8D3gtPUPIKdtSP59fVLc20J3fcV0mhlehIz8RzX5n8umxahWqCHDn1XY6iGufxqJJNx/sPx7TADVWnSpoyIhpIrT8v2dfRJ+Of8A2T30R/4hrrD/AN4jB+86+X/+SDsn/PHD/wBW16+WT3D/AOV/54/6XF7/ANpMnQy+zfoH9Ra6hocpQ1mMydHS5HG5GlqKHIY+up4auhrqGrhenq6OspKhJIKqlqoJGSSN1ZHRiCCCR7o6JKjxSoGjYFWVhUEHBBBwQR07BPNbTQ3NtM0dxGweORCVZWU1VlYUIYEVBGQcjrTJ/mhfEjG/EL5DUH9xaJqPp3uLFZLePXtGTNIm1ctgKulpN99fpUMH1YnCT5rH1uM8jhzQ5IUoVxQtNJiL7ncoQ8sbwslihXa7oGSJf4CKa0GakKc8MKygknPXen7nnvVee9/tbcjmK68XnrYZksNzkNK3MUys1neEYPiyrFLHNQH9SLxSazhQQXFVTws3knF3jSZSr6ZFvYx8KjKYwfqfrb3GWjNaZ/n1kxeQq/wxGgJBqMfPjTPV3v8AJW7aq9s/IDenU9TXh8F2xsWfL09PLMbpvXryrFdjRQ04AhSSv2rnM0ayRbSSLjqVSGWMFJr9k90a032/2h3/AErqHWBx/UiyOP8AQZ+HoPTrnh/eA8lwbp7c8t86Q29Nw2fcRbMwHG1vUIfW3EhJ4YdAOAZZCKFs3jfPJinw9+QTBtJXr7IEN9NJFVR2P+w9zV7i55K5hB4eCP8Aj69c9vu3AH319sQRUHc0x/tX61SMXVGpMrBTZdP0lKqoRSv6rmynVwP6m5PvDONa68Y+3H29dobyARaBXOeI6GLq6cnemygJWMZ3Ft5ebAhxmqPSlr2ZVUkH+hH09m2xpTddq9DPH/Jx1HXPqD+qfNZKDULC5OPTwHz1uGe86+uGvVFn8xWKOf5KUMZdo5R1DskoQF0sG3Z2MvrYi6BT7xj93VDc3xZNfoYv+rk3XRr7rDtH7TXDAVT9+XdR6Ut7HgPn0S3+F04RkvpJYKgP60Gkab6TYMQb/wBbe41EahD/AKv9RPU+m8k1q1OAqfn/ALH+Xqw34Jdo9bdSS9mz773Tj9r024MR15Bipq6KveGsqcLlOyHyVPHLTUtRGk9NFnKRvGSCyS3UHS+mY/bDmDZditdzXdb5YDIYymoMa6fErwByKj9vWKX3jOSub+db3lk8ubLLeGA3Pi+GUqodbbSSGZTQ+G2fUZ4jqwtflx8cHUuvbG3SgNi3iy1h/rk43j6e5SHP/JxFRvsVPsf/AKB6xqPsj7rKdJ5Kuq+lYv8ArZ1z/wBm0+OR+nbG3PoCPRlOQfoQf4dYg+9/1+5P/wCj7F+x/wDoHqv+sn7q/wDTFXfpxj/6D64j5b/HAtpHbO2y2kMQEynCklQSf4dYXYW9+/r/AMnkgfv2L9j/APQPW/8AWR91gK/1Ku6Vpxj/AOg+ho2ju/bW/NvY7dm0MvS53buWFUcflaPyinqfsq2px1WFWeOKZXpq6jlicMoKuhFvYksL+z3S0hv7CcS2kldDrWhoSp4gHBBHQA3vY925b3S62XfLJ7bdINPiwvSq6lV14EjuRgRQ8COqLPl3iK7EfJPseRkMUlfmMDlqNwSpqqGt2ngr1AQnRLDFPC8NzYCSJ+br7xe9wbeSDnDdywoWkWRfmGjQ1/LI+0Hro17HX1ve+0/KiKdSRQTQSD+F0uZsV4gkEN9jD16TW1d01HhSF7hlcoA6jS8hQkhyLsIgDwBz/jb2UWd29ArVr5Zp0c7zs8XiM6jBFajjSvl8/wDVx6Mt1d8iNydXS1lPiabH5THZisjrchh8ilUFqa2ChpMcKynyMEvmoK00FBBBfxTp4oUBjJUMo02LnPcdiaSO3VZLZ2DGOWvEALUMMqaADgRQcPPqIucParZub1invJJYbyFNCXEOnClmfSyEUddTs3FTUnupgmqxPzW2Rkoo6fcW09z4GodgWq8dJjs7jaV1N4meT7jF5aTW4taKilP4+vuQ7L3Q2yQot7t88TE0JQq6j7alG/Yp6hm/+75zDas0u173Z3MQ4JKJIZGHnQaZIhQfxSDoYcB3l1FvCanXB74w6VlcJB/DctJNgMm1SrrGyw0OcioKmVlkAH7SuDwRcG/sW7fzdy5uRVLfdohKeCS1jY/ICQKTQ+legFuXtzzzsUcp3Ll2c28VKTQATR6aVy8JdRj1I9OPSkqOtNlybqo+x6fDU9PuTxyCtqqWWeKir6iaiqMe+UrcVHMMVPnZMfUvStkTD99JRkU7SmFURV37n24343NbdReUILLWjVFKla6S1DTXTVp7a0x0Qxcyb0u1XHK0t652rWGSNgCy0YMEVyPEEWoa/DDaNY16dVT0B+9N2vtLsOurtDNHDuHHVTaGClqSopqXz8MDqXSZBb/YH2vJ01x59GMNmLnZbZG+JoiBX11Gh/aOjIZKKGeegdJFFPXRtjzMfWgDQmagnAFidUbj8j2pQ4Y+mf8AP0Grd28Kdad60kA/OjD8j0i931EuOiweZIMbQNLhq8AuNMkD6kDC5LF49RX/AIp7W2oDNLGTWo1DpHMAklR8NdS/Y2f8PSU7W7V666c64zPa3aO8cNszY+zqUZHN7izcsqUyQzaKeCmp6elinyOXyuUrJY4KOgo4p6ytqpEgp4pZpERk8gCFtWF6M47gRp4rt2U4jJ+wDJr+WeiWfH7+bZ8WPkj21jPj3taHsnbu4d0UFW/Xu7N5bZx+J2bvrI4nESbjrNv4qspc7ks7hs5R4ykqD48vQY+OZ6Z4o5HneCOZHrUtj+fSFZ0/eImiUlS3CnGooerKTV1VDNRSJLIsdNT2mp1YSw1dLJUllj0OT46mnjZiGBBI45HHtwqMno0NvDcpcIyAs71VjgqwWlajipNMdLWnngrKdJ4TqhlDAEqyOBcowZGAZWBBBv7p0HZYpbeVo5MSLTFaj1FOmgo0blCpXQSACb+knjmwBJAHPu4yPmejEOrqHBrX/D1yDvGbxj16bFm1MCLiw8a2+v8AUe/UB4nqpVXFHPbXAFB/Prm8dTUIPLGgCEgO4CEfkkEksf8AYWuPevhOD02jQQnsdix8hnrGKSSVQIpYmRvUpFwDe1wR/Xj8e7Vpxr079Qik+IjBuBHTgyMI1DSa3F9R/SdBCgf66qR9fqfdBSvD7OkJKliVFB5DpM5DI4TH+aTJSqkVTPE7NTU9USauMqkMpZEZlnstvTa4uT9feyKCvn0cW1puFyI1tYyXRCO8r8JyRStKfb8qdQf7w7Zt/wAD6m+rz2+zqNWjX/wCt4v029Wn9Wnn3rpT+7d3/wCUVKU0/GvH+Pj/AD4dL6lp46Smp6SEaYaWCKniX6WjhjWNBYccKo966DfWf37r3ULI46jytHPQV9NDVUtQhWSGeMSRn8q2k/R0YAqQQQRcEH377eHWxggkY6Y8TtvGbapXp8dDFR0OsVFQsPlEtRMAAZJnZ3Z2uABdiQLC4A97qPIdKRIrdscQDk48wP8ALXr5/vzQ2pkq/wCY3y1lpqaVkn+SPdVWJVKtGF/v9m28SE+nWv1/oB7wp5sgeTmXf6cBez5/5vOevpz9g96tLb2I9kkllXUvKm1Jp86/RxZPy6LWlCaMxQVELRa7DUObtb6G311gfUceyAIVovDqVzcC41yRvWnl1vM/y4zG3wb+OUUfkv8A3ElOtWK8DcGaVdRH6UUfT6e8yPb/AP5U7Yh5+E1Kf6d+vnO+86rD7wfuxI9KfveTH+1X+Z6OXXRuYtaMo0XCAJd3IW4ZidTaRf8A2J9jFgfy6hC3ZQ5VgST8+Hy6TVeryQINLtKY203JJF+PJIB+lWb+n1HHtpgSKEGvRtasEkY1ASuf8w+zoO3xDyVcLxanpwyr4ll8aPISdTsTa3rNzySQLfT2hMJLAg44U4dChb5VgkV6CT1IrQen7Ol/jwkYRAi+NAAJY0UkqttWlWNlF/6jgjj2tWgoABT16DNyWfU2o6j5E/4etN/+aR3f/pz+aXZM2NrBPtHqCKj6Q2ksM/lp3qdm1NdU9gZDxf5qKvl7DymRx8rLfzU+JpyWKhQuKXubvP725ouljb9C3/xdMU+CtfkQXLMD5hh13i+537ej259geU4rq3075vhbmG+LCjBbpUWySvEoLGOKVa/C08goDWtfC3vyxNgBxcc3JYi9xc24P49x6B8+snTT+HHWzr/Ir6SkxWwO1O98pSMtZvLMU+wNuVD6NYwW2yuVz80Z0ahFXZmupYGINmkxxvyvvIj2Z2gxWO5b1KvdM4hjP9Fe5v2sQPy64+/3ivuCl/zfyj7c2c4MG2Wx3C6UVp49z2xKR6pCmoegmPr0+/z5OjX3P0Z1V3/iY4kr+n96zbN3SSzLo2D20+NxcFZOyRsZamk7JwmApqRWNo0ydSRbW11fvFs7Xe0Wm5wxEvA5R9IHwtkFjx0qVIp6t0x/du+4i7P7i86e2d4xNtvm3jcLMUrW920SSMoqcK1hNdO5HEwx14DrVu8RIJD+rSSRa/p/Kni+kn+n+t7xq0+errsR4lCBpxXB6sI/lZd8H4+/NHqHPZHIT0m0Oxa2p6V3iDLIYP4Z2PVY+i2/VzxXNNDBjOxKDBVM9TIB9vQw1B1BS/sc+3W8fuXmexlkeltMfp5fSj4BJ8lD6WP2dYt/fM9uP9cz2B51sLO2V982lF5gsqAai1krmdQfi77GS4CqPjk8MUJp1vR+8uevnZ6SHYP/AB4W9/8Aw0dy/wDumrfZfu//ACStz/555P8Ajh6PeV/+Vl5d/wCe6D/q6nXzfsNApwWLjSWUk0NAEib1v/wEh0tITwSDckgfn+nvBu4U+JLQ8WJ/n19WW4Sn95Xrsi4kclhgfEeH+TqSKIoVZ1a5NjqTklCBqH9D/r/j2yI6gZz0wZw1QrVp6Hr6IXxz/wCye+iP/ENdYf8AvEYP3nHy/wD8kHZP+eOH/q2vXyz+4f8Ayv8Azx/0uL3/ALSZOhl9m/QP697917qiz+fbt+lyHx26JzYVFyuL+RFFiKWoMaNIMdn+rOzJcnS+QgyJBLUYWllZV4Z6dL/Qe4a96rdH2DbJ9I8Zbrw1Y8QHRiafaUHXRj+7Y3Sa190vcfbySbKbldp3Wpprh3GwEbU4agsrqD5Bm9etYukpJEEKSgoSY1iVnVC7JJJ+RcuhX1HUfqLe8adBHD0667zzqxdkzxLEA+Y6sd/lkVD4r5sdBSROrt/H9y0agBi3jyfXm9sZUWcXHphyBJuSTb2OfbRmg5z2PSeLslD6GNwesTPvhRLd/d+9xfEU9sVtJX5rfWjD/B/PrZs+fZA+GvyIJ+n+jnJXvf6fcUfHFyL+8j/cMV5L5gFf9BH/AB9euSv3aP8Ap/Ptd/0tU/463WorjqtRI48pfzOsaLE+mL6m5MZA5NiD+L+8NAoUkHz8x129u4WIU6KBRUluP7ehj6nriN/bFRrHybx2rGqhwoW+dx4F0JvpVbn/ABbj2ZbJqXdNsJXP1Mf/AB8Z6jz3BtweTebaeW2XZJp/wiTzp6/y63RfednXBPqhH+ZJkzQ/J6gjR7PJ0zseyka1AO7eyzqVLXJvHzY/T+gv7xk93j/yLYhiv0UX5983XSn7qFoLj2huGK9o367zw/4jWGK/n0S/H7glltYopMYRdaazrZiCSf1DQp+ovYD/AGPuMklbj/k/LqfbrbUStQeNTQ/6uPT3S5YlGCcPqOgBioSxNjIQLsGH5H5+g92EnAACtekEtlQgnh5/P7OnAZaJDZYXUCxDFbKdAJLNGdN19fAP+w9u+KuMYHr0lNk5FS4z5f7P5ddtmqVjpVonLgtGPWSjMqFeQuq5JseLWPFvejOp4EV8utCwnXuIIpgnqPVS01XEqx6XVtQUFtFpvqVYgBljjIP+JHvzsrpjjWlOnoElgclqg+fnj5fM9XwfBRPH8XtgJ6jbO9sW1klrHuLf7Dk/ix4H4HvKv24GnkzZwPWb/q/L1zU+8I2r3c5obFfDsuH/AEr7XoO/m/0Jk9843E9p7MxE+X3RtOjbEblxOPpZ6zL5nZrTT1cVViaGminqsnk9tV9TLJ9pAonqqKqqfGJqiKmppSD3L5Tn3aGDetthL30C+HLGoJZ4qkgqBktGSTQZZWalWVVIv+757mWfLVzfcn7/AHog2a9k8e1nkIWOK6oFIkYkBI50UDW3akiR6tCNJItVdB5YIhVUrJJT1CJUwVMcqzwVEFTaSmqqWohd4qqlljIKOjMjowKm3uAgrxEmlPOvr8x6jrNCdopmEbkh17StKEEYIIOVb1rwPHp0kyNStV+3Iw9MYkkvZvSmllBPAN+CQOQT/X24ZX1YPpXpGlpEYasvrQeX7P8AJ04U2TrfDCvm9Y8iLJ+o+RpmcSop02K8gA8BeOTb29HPLQHUfT7T69J5rSDxHPh9uDT5UpQ/6s9QKjM1cUytIzssTNGY2VdE4N1fWv6XVVYn18WPts3EgbPwjGfP5dKIrCB4yqgVYVBrw+z0qR5dLnr75Edj9TsYdn7gqJsQjhpNo56SbLbWemV5WkgixxmSTClzJqWTHSUr3C+TyqNBOdk5w3zl51G33ZNuDU28lXiI9Atez7UKn1rw6DvNHtbynzsvib9tiLfEUF9bAR3AagoS9CJaU4Shxx06Sa9HWxPbW1+86OPdmKiOLyooKKh3VtermWrrMDlGikUETGCnGQxFaY9VFWiKJamPUHSKeKeCHIvlfmmw5qsTc2w8O5SizwE1aNjwzQakana1BXNQGBVcV+bPb3dvb+X91Xp8ay8RzaXqLpSaIkeVW0SoTSSOpKEghmRkdzbbXyUtb1divKfJU4etjxcztITMsVLK8FM7tq1hxSSoLk82v7FsRAf5U6h2e1WDmCdF/s5ELj0NQCf+NA9OO6KvHy7J3DV5aup8dFjsJNuiryWSnip6Gjg29FJJlKqoq6h44KeKjgpmaeRmVVjOom1z7ejk8KRH/CMH8+iW8tvDlkTHhaqAjyB7l+wf4OtMb5V/OvsX5jdrYCn69bcc2BwW4cr1x8d+q8NBSzS7tn35i6rY8W/t1YLcOBr6DcG7uwKbOTYyGjnEDYXE1qwQeKoevrKlPcTtNKSg7a4H+f16Lal9IAJPwqB88ftNadGp2p8LsN8aPm5/LG6Wx/l3B8h89ndy9t947noMrVvs5MXi8fV5jH4DauAnnC0eF2lQ7czlPFXLT0c2VWHzTJqkEFG0y6GUDjxPS2aJLF7AkFpR+pJn0OAP8/n1tJrI/lCt5SwcxmORydJgLRSq54BAZDb8e31NehWVGmq0oRWo+eQR+3oQcBHNHjWlVldKiaSenSxUQodKtqd/1lpELf05490OWPp0FtzdHvAhBBVQrH1OTgDhg06mRxSVJMjsVBsC1rliPqFB4tx/re91ApTj0y7rF2gVPp1OAgplBOlAeNTG7sT9Ln6sSP8Abe69JqyTH1+Q/wBWOk5msvpUU0URCTwy3qpGMSIeLBGW7BiP9Y+7qtcno1sLHU3jSPlWHYMk/bXHTdTbmx1PTxoXkrJlsDBi43rfGvpUvJMoWKM3uWBJa97+9Nxx0pm2i6lldgoROOqY6a+eBxP+D06w/wB5clWSyUuNxEMMyp5EfIVYeymTSsrRQoQFYA2Vmv70ASRXh1f90WsCpLd3zNETQiJaeWRUn/J1g3FuCvxmOnqFhxlW9HCKyePITR0VNFHEGLz+VyTPyumNF5va/vxFASBj/J1qz2+3mlADSqrEorJUk18qDh8z0j/9NG2dPl1YvT/Av41qs9vvfL9n9hr8Nr+T0+X639Fr+6a0/i8q9LP6sXldOuT+18Pj5cdVK/y/Poevdugj1737r3XvfuvdRKqKWdfAmhInH7srDWwW/wCiOM2GtvwxNl/ofexjPT0LpG3iNUsPhAx+0+n+HrRR+U+Knf5X/KmIRPJTH5E9yxqHZyAZN85g3DppViVYX54uL8+8NuZq/wBZN/r/AMps9P8AnK/X0aezl9Gnst7NuXAl/qvtZNKeVpF65/1Yx0BqbepZ/wBqWCOpmUQxq7IgCKHKjxgtYSLz6vz9SPZJpBPDPUhNuk0fekhSPJIqc19fl8vy63Ev5fFGIPht0XTwq3jTbmUiUNyCsG6s/GNRNhwqD/D3l3yGunlHZAB/oR/4+3XB/wC8hP4nvl7kySkajuBY/nGh/wAvR0GUAGPQTa9ypuACQfrb1MR/sAPYv4dQapJIfVx4f6vTpPVEDzM8ZBCopDC44S5YDi6gEcH88+22FSRTozjkEYVxxrjpljpVQyCwtcMFsoCqGuTp/s3ta31I9taaV/wdLzMSUOa+Z9fz6AT5ad2wfGv41dvd1N9o+T2ftGoTaVJUxP8Ab5Lfe4qin2z1/iqjxI8hp8pvTMUMM7BXKQuzEBVJ9k/Mm6fuTYty3IGkscR8Ogr3N2oaYqAxqfkD1JXsl7eye7Xu1yPyAPEFnfXym+kUjVHZwK1xeyCtBqjtIpGUVFWAHE9aKhask1S11ZPkq+eSWpyGSq3DVuTyNTI9RkcnWMeXrcnWSvNK55eWRieT7wtldpJHdq1Jrkk/4c9fRpS3WiW0Cw2ygJFDGOyONRpjjT+hGoCqPIADrqNjqQi95GC8lVAIJIuzkIv0tybf19tjNPn1qQAK3yz6/wAhk9bj/wAWvlp8Cfj18fOpun5Pln0Hjchs/Z+Nj3DDU9h7fxdZPunImTM7lnnoq+ppK2nFTuDIVMsYljRjE6G2kj3lryxvnK20bBte3xbxERHENTKGy5JLn4f4yeuDfuv7IfeW90PcnnPnweyXM8sG438kluVsZ5FWBSI4EDqrK3hwoiYJFQfPpUd7fLX+Xp8heke2Okc38xfjxSU3Zuw9xbTo69eytoVE2KzmVx88WAz9IstZURnIbezopq+lbQxWppkIHAHt/fN/5Y3baNw2192gpLEygyatIYZRjjgrAH8ukHtx7I/ei9rvcHkr3C2/2H5pebaNygvZIjYXIEkMbgzQtRVOieHXG+RVXI60vcZR1k3i+/hNNUtGprYopFnhhqFTVPCk8ZeGVUluqupKsACCb+8Riq+KwVyVqQD6iuPs6743c0Ca/ppNcIP6bEUJX8JKnIJHEHI4dPH8KaWJaeNquJpZCsklLPLSVcSMCqSU1TAwngqRcMjoQ6NypBHDq6o2Rl4hq/sznova7XU0kixsun4ZFDKfUMrCjL5EHBGD1vv/AAe78HyY+LHT/bdVOs25crtlMFvxRE1OYuw9nVM+1N7ulK/7tPRZDcWHnrKPVfyUFTBKpZHVmzG5U3cb3sG235fVMYwkpxXWvaxNOGojVT0I6+az7wHts3tL7wc88jxoRtlveGfbySGrZXKi4tKsMF1glRXp8MiupoVIBgewP+PD3t/4aO5P/dNW+zPdRXa9yH/LvJ/xw9RvyzjmTl8/8v0H/V1OvnU7Xx9KcPihLqdxiKKVXusja/sYSi3UKSRe5twNP094SOtZZCa8T/h6+pjeLqYX96UoFM7inDGs16fji4WWPxvbVKpdXbxuy6leTR5OXHHJP6rH234YqCDnosF5IGbWvAGhGfkK04dfQC+On/ZPnRP/AIhvrD/3icH7zY2D/khbLTh9JD/1bXr5jvcP/lf+eP8ApcXv/aTJ0LlTIIkEh12DBTp/1L8E/wCw/H+PtfOQqavn0FIhqYj5Vz1igqHuqShbsbKRe/0uhf8AFpU5BHF+Pr71HKdQR+Pr/q9etvGMlfLj/l/Z1r2fzwO1MZncz0h0Dj6mKordt11b3Bu9IzeTGT1tFX7O2PS+QAxiqr8dV5+WSIkSRxincrpmQmCvebdY5JNr2SJ6tHW4mAzQntQH0NAxofIg+fXT/wDu8+TbzbbD3C9y7qIrb3cabFYk8JAjpdXbU46UdbZQ3AnxBWqNSh1sZSojhSjhnf8AzkfqjZSWj/WGJJClfx6j7gsLnPXSAXcxZSQRQDgeI8+H7erF/wCVDtCfcvzR68ro6ZjT7Rw+8t3ZBo4iYoIYdrZTBQO9gBC38W3DSqCbcvb6ke5C9rbJrjnDb5NOIUklb/eCo/40w6xQ++xvse0+wu/2bS/qX93a2MdTknxlnP2jRbt1sU/zADb4Y/Is2Y264yZsoLMT9xR2AUFST/hf3PvuD/ypu/f80h/x9euXv3Zv+n9+1n/S1j/463Wn5RxTwvru4nkDRMPtfQhPOpbsLkkDkG31/PvDvSRU1PDrubOySKFx4Y7vi4/b0MHVMcy9j9eyKrMp3vtFXklhUO19wY3X69X6QBxxwR7X7REBuu26f+UiM/8AGx1HnuA0Z5J5yUkVG1XZAU4/3Hk8vXrdl95z9cAetd3+aPVSw/KrFJGdIPSWxCGswsX3j2grnUOL6Vt/h/sfeMPvBX+tsNP+UKL/AKuTddR/udQpJ7M3rNn/AJEF5UfZa7fT+fRF6KqqoGVXdQVj0LZ2YhCDfUwP+cuoOn62P+w9xfkDHHrIy4hglBKKaE1PAZ+Xy+fRtugvjz2H37R7iqtkz7YeXaseDOSpc5m63GVQTPzZ+OglghpsHk45IRJt6cOXaNrlSqt6ioz5Z5M3PmiC5nsJYQIiqsHYg92qhFEYU7T59QT7ne7HLPtne7bZ75bXjfViR43to0df0/D1AlpozX9QUoCPU8OjDL/L47+bV5V2R6r3CbuyBFiSf7W0B/aPsTf60vMh4y2/+9t/1r6i4/el9uxTRa7lX5wR/wDbV1xf+Xn3y9rJslAFKaV3bXkfS2ssdogk/wCH0H491b2j5kb/AES2GKfG3/Wvry/en9vlFPpdxJrWpgj/AGf7k9cF/l499htRXZLG9yW3bkfVxzdV2ko5/wBf6e/D2j5lGfFtq0/jb/rX1Y/eo9vStPpdyHyEEX/bT1ap8YOutxdTdKbW2BuwUQz2FyW9qqtONqpK2gK7j33uXdNGtLVzU1FLUCGhzcUbs0Mf7qNYabEzlyhtV1snL1htd5p+piMmrQar3SO4oSAThgOAz1ht7r80bbzpz7vfMu0LINvuVtxGJlCv+lbQwNqVWcLVoyQAxwRmvQ+ubD/Emw/2P/FPYikbSuOJx1Hiip6K32f8Uutux6utzuP+62XuOtnq6ysr9vpTviM3lKt5Jpa/PbdqENDU1c9XK8tRU0b0GQq3b92pawsBt75J2fe2kn0GG6YmskVKOx4l1NVJ9SKMf4upa5Q94ebeU4oLEyrebWihEguqlo0XAWKUEOigYVW1xr5J0TXdnwk7Wws7zbfOB3pSazHGcXkosHlJIxZllmwu5ZIcdSX1EaVzVSwt9fceX/tbvMDFrKaKdK+R0NTy7X7f+N9Txsv3iOVLyNYt2tbiylwSWXxUr5/qRUc/84R0Xzc/TXZe1kqmz2x924ylok8lTVzbbyM2KpVZwA8m4sVFkttKhY21PVrfVbj2Eb3lLf7IObna5gi8ToLD7dSalp9p6lDZ/cnkvd2hFjzFaPM+ArSqjH5eHL4ctaeQU8OghysCtEzKIJLnxRzRVMcsTNGpUqJYZZIC6KArC5IIsefYbmjZC+oUzSv+T8v5dSDYThypWQ6SNVKeRPGhFaHiOmKixdZUS/cM6rpRY3TQLgFdFvU+n1WuSSOB7YEblq1/LozuLyCJBEF4kkGv5+lehc6vyOX2bvPCVsNpKbJ5TF7XzNIgRY63GbjylFivKGYiKKXFZGtgrhL9Vhp5UBAla4y5K3GfZeYrGbXS3kdbeYeRWRgo/wB5cq1fQH16jzn2yseYOWN0tphR4YXu4XPFHhRpD8yHjVk0+bMp4qOrgup5vvsfuPb06RpNUww1UcbLwk8K/bOzKQLXZYmsf0/7D3lOCcHrAfmSNrS6sbxSf02Kk+orXHyIr1Sh/OU+Su53wO2fhZ1Rlqel372Rgs9vntGD+IQ4Wrbq3GUmSj/uPQ5itq6Ciaq7Fr9vVrVFAkvnrcdipaQoRkIo5/StWirxPQd3WRQyxROKOlW+ajKj7Tn/AAdFx/kyfGra+5ezt1/MDLYDPYvZO06jJ7K6Fo92VVDlRFlJcWcbvbeb52HGYSLKzbWpGlwdNUxUlPSxSVWQjYPPAGi3bxqyPITkcP8AL0hsErOspHYCQK+vn+fRwfgCch8ofm38g/5imbhqJetafM1Hxv8AjFNWRsKbIbIwEgodybww8VXBFOtDXBIZoJ4yyLW5vMUhOqBgKU1a5D+XSuKA7gdwuCO0IVjP+lz/ADp/M9Xk5fF1MmeaKlh1pWUzVcbMGWnjmhISpDyhSqSynQVH1JJP4PuwYDB6WWF7Em2h53o0bCMjixB+Gg8wM/6qdKvHouJw9OmRnggFNAPuZpJkjp4ibsymaQonjS+m5sOPeuOadEt25u76aS3QkM3YKZI+weZ6D3Kdu4CB5Kbb9NVbkq4yVd6Mfa4yIrcEy5KqEcJjQjkoGFvzb3o18h0dWfLF5PR7xxBD6tlj8goz+3pGvu3fGftU0BxkFLFMHlGN11MTiMFmp2y9Y0cJc/T9kWAuAST7sAT5jo9j23ZLJjE4kkkK6avileB0L/l6eZK7M5bC/cCWGngLKJUx0Ouzl9TMKyvOpwkn00JcC59uClONT8umVtre0v8Aw2rrpjWc09KLgVHqc9OuImxNHQ/7lMhDSsHusUk2lJSwLktFGqzzsBctqAUf4+6lvMDpi7jvZbjTZ2zyDzYCpHlxPaB6U6mLJPNWVRxUTNQSvGZK2dRRUTqqL/mUVWrJ34/AVeeT78GJ49MlY47eL61x9UAaRr3sOPEmigdRpNiYrLVj1mbapz880peKlyDCLFU1ORq0RUMOmOSNPr6yxIHPvRH8R6p++bm3iEVrphiUULJlyeGWPn9g6Wn8E23bx/YYfT/Df4Tp/h1Db7DX9z9tbwaftvL6vF/m9XNtXumlP99r+z/Vjok+pvuOuSvieL8TfFwrx40xXj8+lP730X9e9+691737r3Ueqjlmp5Y4JfBK62SXkmM3F2ABBvb37pyJkSRWkTUg4j160cfk7XIflN8oqeSdEkpvkF3FBMxSQyy6N85nUwBABMqWJYatI/N/eHfMzA8yb+P+X2f/AKuv19D/ALQ27D2c9n5ViJV+WNsZRUUFbSL/AAHy8+geEaFQs5jkWRUm8K2RrlQEeRtOqPyBgWbgWXgfX2R4rnhx6HRcg1jqGBK1OR8wB8vIfPrb1+ADQJ8OukP36dymCzCOI5Yn0Ou7M/8AtvZjpbSwJBGpQfpf3lvyK8Y5S2UeIP7Mjj/Tbrhh94wSN74e41I2Fb6o1AjHhpn5/wCX16NnU1YjsqPGQRrkPkBdwxOlFAYEG4/PsW+Iv8Y+2o6h+GAvllNa0Apwp02CRWBZ3I8xJ0a4wf6ASXNgCfp+fetakfFx+zpXpYGgX4fkf5dRjDE4aaJl/b/bbS37YYG5BPLEKWH+uTx70NJqymo4Y6d1yLRXBzkV49UW/wA4/tv72n6x+OmMrSjuG7Z3zSWnAakgkrttbCx9RpQwy01fXtl6xoi3kjnx9I5FnU+4P9394BXbdijf/l5lH7Vj/wCf6j/Snrov9xDkn6aTm73TvLeqj/dJtsmMMQk9465qGRPAjDUoVllFag9UEZvbVDN+zHS08MqMqyGIadGlXWLyK/LuWAawNvV7glkUnh10t27d7mMa3mcoRivnnNKcBTH5dI+fakUiaIPGXb0L41NxoZpZTZkuzKoUBj9QTb20Yh0fR706NqlqAM5PrgcDwJ8v29Mz7WvJEFKxwygg+QW0MbkKWdQLMP6gW/J968IGlOHn0uTeKI5NS49PP9nU2Da6IsrIqCSNXW6OzMjLdtSg2BJA50khfqB72I1XFc+vSeTdyxjBJ0GnEUqP9Xrx6UtBQU9HSoFTUhMbFwocalYF1byAEM5bkvwRx9fbgChTQY/y9FV1cyzzPVqNkAcOINOHp8upLQPaaeERxxwSMWklDWjKfo1KAskgW5IsBb/ePe1pXjgdMrKtEjkJLOOA86/tAPV/P8invGfHbh7c+OWelMMO5aODuPZMLyySIMviUxW0t/UzSTP4oZsrh5MBVUdLEAWjoq6crcOfc2+z+8aZNw2OVsOPHhHzFFcfMkUP2KeuZn94z7dxT2PJHuptqamt3OxbgwAHY/iXNm1BltDi5R3bhqhQH4R1sOb+/wCPE3rbk/3S3HwPz/uHrPc07p/yTdx/5oSf8cPXMLlr/lY+X/8Anug/6ur1863Dx1NFicXpIjvjaWGRByyEUsKiNmIK6kZv1A3F/wDbYRyAh3oeJz19S188NxfXmKjxmYH/AGxNfXI6jtXzGWmj1vI6NpKspV/GG8iaWJFgPxz/AK/tquVqenRbpolOkBT5/PgcdfQb+OVVSv8AHvolkqaZ1PTnWQDRzxSISuy8KjaXRyraWUjg/Ue81tgkT9xbL3iv0kPmP99r18v3uHDMOf8AnkGFwf3xeYKkH/ciTiCKjoV8nlsNj6KepyuWxuNoo4nkmrK6upaOnhjQanlknqJY4o0jtckkAfn2Y3E1tHE5uJ0SOmWZgAPzJp0F7Syv7meOGzspZbgkBUjRmYk8AAoJJPVbHya/mV9MdOYLK4bqzI4ru7tZEekxGH2vW/e7FwdZL51FXvXe+PMuJSkx0kDSPj8bNV5ZzoQxU8cn3McZcxe4ez7VbvDt8y3W5DEYjNYx/p3BoQPIKSTwOmtesrvaP7pfPvPe5Wd/znaTcvcmE6557xNN3Kop22to9JNTg0EsqpCMkM7L4baxfYO6ex+093bn7I35Wzbn3lu7MT5rcuYkRYJKivWGClhgpaZGMWPxWHxlPBS0dJGfFS0dPHGpsg947bhe3e6XlxuF9MZLqVizu3r5D5AAUAGABQCg6688sbNypydse0cqct262ew2MAt7SAEkKlSxLNSrySyMzyOcvIzMePSOjxOQelMZp0eSSH7pFdm1teX/AFTfmw/rY/7G/tBpz8+j1761WYP4pCBtBIpTh6dbHH8nL4712x9hbx7y3HT6Mj2K0W29nmVZo512jha2WbMZIRSKmmHO7jhSFDYhhiRIh0SgtkR7Q7BJZ2F3vdylJbj9OKuD4amrGnozYH+lr59co/v1e6NtzNzZsvt/tMtbLaA096VIIN1MqhUqCQTDDnyIaVlIquD1/PoFvhr8h1H1PXWSA+n1NTR/1sB7GnuB/wAqbv3/ADSH/H16x8+7QQPfn2uJ4fvRP+Ot1qGTVFRQyqJZktJH+3C4/cJKWTxDSRKWb88afqT7w+OD3ZrnruGkUNzGSkZwckcOOfsp/PoXupq1Knf3XoVY/RvDaIYi6lRLnMdIgPqI8guAV+v+39me0UO57aQP+JEZp/t16j33BtjFydznVmztl58+EEg/Z8+t1P3m/wBcDOteb+aFPEnykpFK6px0dsMooCtIytvTs+4UP6R+g8/j3jN7u/8AK2Rev0UX/H5euoX3Pkc+zszV7P6xXleNP9xdv9Pt6IpRU0pEJFO+hjaAxDyIWb1Eya1L3ksAG/H4/wAIv0Ejh8usjriZO/8AVFR8VccPSmMenn1cl/K6/Zqu7fO8cck2H6nkjjMkRPjhyHa0TlSpHkVHcBjbgsAfqPc/+zhC2u9AkDuix/zkHXP773/ff8kiMEhReAmh4n6U/ljy6tu80X/HWP8A5LX/AIr7mjWn8Q/b1hn4cn++2/YeveaL/jrH/wAlr/xX37Wn8Q/b17w5P99t+w9e80X/AB1j/wCS1/4r79rT+Ift694cn++2/YeuYZWGpWUrzyCCOPryOOPe6ila46qVINCCD6Hopnyw7zTq/Zo27t6vWDfm8YKiDFyx+qXb+GjKxZPcb+kpDUqJPBQB7F6p/IFkjp5lEec+81R7Rtv0dnNTdLgEIRxRBhpPkc0X1NTkKeps9lfbk84b8d03S2Lct2LK0ynhNKamOAeZXGqWnBBpJVpEPRTeh/mXW7Gp6LaHZseR3PtalEFHiN00fkyG5cFSxokSRZeKeQT7oxlPEB/lAZsqmggpWFwYwHyp7jSbWI7De0eaxUBY51zJGOFGB/tFHrXWP6dRSa/cj2Et+YpLjfOUDDZ7w5Mk9m9Et5mJqTEQKW8jH8NPBNRmKh1WX7K7K2D2NQDI7H3bg9y04VGmTG10T11EXFxFksZIY8li6kD6xVEUUin6qPc2bZvW07zF4u2bhFMvEhD3D/TKaMp+RAPWJPMHKXM3KlybXmLZLi0lr2mVCEennHIKxyL80Yg+R6W9hwbcj6H+l/6ezToO9EA+dO3upKfYZy1fSYbHdqZHK4tNsz46OOlzmci+/pIs22ejoVSfJ4PH4Qzss9WGjpavwiJ1llVJIp90YdhTafFnSNd7Z18DTQOw1DXqpkoqVy2A1KZIrkr93K95zfmj6azlnflCOGQ3qyEmGM6GMIj1VVJnm0iiUZk11BRWIq+iaKjiVGVjJI2nTpGp4iAdZJAASNFP15t7gUMqDj39ZjuHncsG7R/I/wCc9KrDvHW7o2niKOXy5fNbo2ziMZSI2gz1WR3DiKGnjU3sghmqoyxJChbm9vZxtQE+77VBGazPcRBV9ayL/gHQd3xGh5c5iu5k02cNjcSSOfICCU5/01KDzr1cB2lnsH0ljNz975mpjxmxdpbbzO4uxGSBppqLD4mgqMjX5WlghIMsgFLzGOWcgAer3lx8BNfh654x30N5tk223slJoVMkMjHBVAToNfMLXT68ONOtMDd+/u3fkt8gKbufA5rD1XYPyn7Z2riNnbSyWRwSb2683TOJMLs+vpdo7drMvlR1X0niZ2o4MzXDGNnRFLXVVJIsjhWa6j6nh0GE8VmTQx1sygDifQU+QA6ux+UzVXTPxg+PX8rr40S1MXdvblPN1di83R09JHLtfpvGePId19rb1jpZGqKI7qinyT1MkMSyTmfIy0rpU0sYKk1UCJOLCn+r7el9xCYGW0tiSJFXPmCMMfsIHVtnRnR+yOl+n9gdQbFkhxGz+s8Hh8HgJ65YnlyJpXWvr8xmZIVpoJcvuGukqK6tnVY1lraiSSwB0+/UKjTQ8KdHBdbOGGC3hZ10GtDmhBBPzNT0YzJ7lp6WoSkpIHr6uWMyxiJ0+1RALtNPONQWFByWH492WIkAsaDoO29o82pmqIwaEniT6AeZ6LxuCort4Zd1krDlxSkrVOZnpdlbaiViS9ROLfxCr02BRB5HawB490ZlGAMf6uJ6HdhbxbZb6jDplb4V4yyE+XyH8h59Ne/tx7L6g6y3n2vvJjQ9f9a7Wy27dzbkytIqxyUOFopKqaHa20UeE5PIVhjENFDM5kqqiSONbs4HutaCpGOP+odI7vcPBV2urj9SlRDCalR/Tk9fkOiY/BX+Z71t8xd5722Vjund/bL3htLARbtwMWWy+I3hSZvac2Ugw0s9VJgKekx+0szQV9VB5sb45YRHKHhqpwsnj0rg4ofy6KLW4ud0Z7ZJ47eCmtq4FKgZOSWz5k16s3jp8tUpLLWtHhoZ5JJRTxFJqlFf1NGH1SJCdR4RWNvb1cUp+3oxD2kBSOANcSKKamwp+dMEj5nrPR4yhhbzQUihiSVmqgJJzc3aRvIT45C1zxz72PWn5danu7hx4bz4HFUwPsxxHT7AhRdagh0UFQQPGo+raQbWup5P596rSlfs6LpG1EL+GuT5nrilb5GeU6lXyMhjcFFbSdOpFHKofqL2v78pJqStDw680GlQgGaVrx6l+eL/AGn+n6l/Va2j+l7f7D/H37SfX+XTWhuGf2eXSx9tdEfXvfuvde9+691737r3Wgh8p96UkHy7+XFJXu0Rg+UPdUEc1jIDTQdgZtFJA40WP0vyPeF/M06DmPmHUaf4/cfymcdfSz7N7BNL7IeyM1stQ3J+1MV4dzWUX8+gopd201bJUTJLDUPCIY4jcxqOCsikO6SK2jhTcqoJtz7Jw4Zu1vs/4roaTbHLAsSFGVWqW8/mPKnHj5np2kyDTutQZisDtDBEsVQ7LBGgZxF6ZUEhIsWJFyRyLe3AwIr5dIkthGrRBP1QCxJUdxOK5GP9VD1JhmoHljgjq5Gkd2j8bTuHnVCX8YWOYrqGsMbG4Bv9PpsMKgasnpmSO5VHkeBQgFa6RRa+eR8qdTKox06SeOokghikRJCZpJmaZCRaObzvG2m3/JIPPPvxOMcemIA8rrrhDSMCRgAUPqKA/wCz1sI/yXmFDsbv2gFUiYmk3JsnOuzTF6X+IZHBZunr8rNNOxYzzY/C0kcjkgaKVOBa5yB9nH07dvet6RLIjGvAdrVOeHDP2dcuPv7M9zzh7eymMm6bb54FUCjaVuAVjAA4a5GIHqx9eqXPkl3zU99d/dpdtisrZsNuTcci7Tp5Fmg0bGwzjb2x1popjIaRa3AY+CukisFWtrJ5CFZifcOcy7y2+77uW5knwpJD4Y4EIvagI9dIFfn10G9qPbeH239tOTuSDBGu4WlqPrXBBrdyjx7ssRTVomdow3ExxouQB0AtVk2lmZ2MckkbelHP7qRqVL05BRryRGw1E2fn/X9kRbPz49SRDZhYwoBCkZI4V8m8sHjTy6Oh8fPgX8hvkzsqr7F6xx22jt2j3NU7fWr3HuSkw89XkqSgoMhVrTU8sEjvRUyZaGN5DpUyalW5R7C7YuSN+5js5L/bo4/AVzHV2C1IAY0qPLUP8HWPnuj95j2w9ouYo+U+a5L191e0W5ZLKDxFRHd1TUS6/qN4ZYDPaQTxHQ7y/wAm/wCaM6Oj4vrFQWbRbfVMwVDyQV+wRdbkkEjj6cezj/Wr5tPGKD/nIvUax/f29homVl/fhIGa2i5/6r8B6fz64j+TZ8ztQb+EdZw6Vsgg3/ANDnSC0ZbH+gWUXH9v82t79/rV82GtYIP+cg62fv8AHsRSld7avHVaJw9D+vn5enQOfIf+X98hvjJ1/B2V2hhdtJtSfcOM27W1e3NwwZ1qPJZVamTG1GThipIBR0VdV0wgEzHxieSOI2aSMMT77yTv3L9kt/uMKC3LhCUYNQkEioHljj/n6H/tV9572y94OaJOUuUZ74b0trJdRreQiIMkekOsZEjlnRW1aeOkM3BTQkStA6OsQ8pEayGNgJZC0nklknja+ho1F7fp4P1P09hDH8q9ZEkSqVZzpqaBuAxQAHzB6Gv4591yfHXu/q/uSjFS8Wwt10mTzNHEkhqcltGupqrE73xlHCkiCorq/Z+VroKRHvGKqSJiLoCDrl7dn2Tedu3JK0ikBcDzU4cf7ZCR8q9R77r+3w90/bvnDkSYL4u42TR27kiiXMbLLaOxIOlFuY4y5FDo1AYPW8DvGtpMj1zurI0FTBWUFdsnOVtHWU0qTU9VSVWCqp6epp5oyySwTwuHRlJDKQR7y53CRJNqvZY3Bja3dlYZBBQkEH0p189ewQTW3NOy208TJcR7hCjowoyssygqQcggihHXzzaespk2/iWmNSYJsdj6iIpHd4yKWOMTGRmKIr6r+P6k/wBSPeFMhAZq8K/5evqCkglbdL0R6fEWV0apwe4mlOJp69QJ8IkwozjqlZROrxuwVm8cBLDU1yeGUiwPq1Hj8e2iimmk58/9Xr0qj3AxmcXURGk1HlU+nTJBj54asupneQ86kqKmF4jDqZyqrIPSqp/QagP6e6AMKgHh0vluongCkKF4ZVSDXGcedfy6Gba2TvNTJkqZax4G1U8tfAtWiiZC0ixiocmI+RFJK+phwfb4NcEY6AO82lEla0mMath1iJU4OK044JGeHQ84TLNVRxq7CKOKQBA8nqAa6oosdEypcgWHpH+I9uCuAcjy6jbcbMQuxXudhkgft+w/4ehAjSCaEwpoEZLTl9aszStZFP7l2IKrZrkgj/W93IBFPLoNM0sbhzXV8NKcB+X29Hk+IXwqznyM3LSZbKU2RwfVGFr1Gfz8nkp6nNyUzI9Rtra07A+fKVB9FRUcxYqFjLJqmNPTVI55M5JueY7pbidWj2lG734FiPwJ6k+Z4KMnOkHG/wB9vvB7f7XbVcbZts8VxzvPH/i8AoywBh2z3A4BQMohzKaAAJrddnfb2BxW18Hidu4Kgo8VhsHjaHE4rGY+nSloMfjsbSxUVDQ0VMnpgpKOkgSKJbkqiAEk8nKG3t4rWCK3gQLCihVVRQAAUAA8gAKDrkZuF/ebrfXm5bhcvNfXErTTSysWd3dizu7HLMzEknzJPRV/n9HUS/DP5Ex0rslS3XWR8DpYusoqqMoVBBBOofSxv9PYU9wM8nb9/wA0h/x9epn+7Q0ae/Xtc0wBiG6pqB4U0vXrT4zcmVjEB0sZKd0NM8pLz1EE6lZIDYhihqJTdD/QcccYgEHhWnXc7blsmMor2uO4LgKVNQft0jj9vSu6bi3WvafW8bxqKQb52W9UoYFUgTdOLaZmYksZSGYn8k/4e120K/7120eXjx/8fHQb9x5NlbkLnVwx8b903uj5n6WWn5cOt5n3nF188XWu5/NEij/2bPDylSX/ANCGx1JF29P97u1AqhCbH1Nf/Ye8ZvdwD+tsB/5co/8Aj83XUf7nzt/rK3yA9v8AWG7x/wBQ23Vz9nRK4cy1Pqhf9swiIRgITpREBs8gtYBuSLcj/Ye401FdS/s/LrIGSwEpDjOqtc+ZPp/Lp9os2tUhjYxO0T3Ea3EYEikegp4yw5+lr/737sslaauA6LrjbzEQ1CARxPHB/OnSrpMmJVM0Wl1XSAADrCsVMqODdCpRebXNh7c1VBOKdE09ppIRxQn9nnSnn0oocy0SQJBHEhjCzyrNMxaRZDeGKBGdjLoIuxa319uiTTp08RnPRU9gHaRnYmvaCo4U4k4x0r0rF8YZo4kaSFQuoCWxkCgEqOQWMnI+oA9u6u1SR8uiRoWL0DsQCa0xw+f5dW6/CLKVkPTW74EEtfDhd/ZNMRjYZIECU1RsbY2fnoqB6mSCGI5HPZepnJmkVRPUuWZV+mQPIVzJFys8aDUyzOQoPloRiBU0GpifQVJ6wS9/LeKX3Ds3kcRtNZRCWVgTkTTxBm0gk6I0UYBOlRQE8aWfmX8sx13uqu3l2RjcnlN67qzGSxlPsemqBDU7Zxm2pPtK2gq/uog2Kwm066eGiqHEPmlr6rymJmmldY9tdg37nTe9yubxvAZG0yGUGkZBosCjBLKATTFaFjlszruHOfJns/ydy5te2Rm8jkTxbcW5UNOrAGS9kfuojsVFe6mpI1GmM6Ul0P3bhu8du5XMUGNlwuSwGZXEZ/EGo+/+wqpaOCvjQZBqPHJMwhn0yIIwYZEYDUul3JeZOW5+XLqCCWbxI5U8SOSmmoBIONRoMYzw+eAL+QPcCz5+2+8u7e1MFzbyeBNAzl9LFQwGrQlTQ0IpggjIoSNIWCnrYq6kmkgqYCPDVwK8NZTnUNX2tbGwlhkjBFipBP5PsNYVw6MQ44EYI9aHy6kImWW3e3njDQsO5GoUOPxJwIJ6Eug7E7DhDo3ZnZaopWEUydgb0igVioEMZp485HAiKU0/S3+w9nUO9bwoKnerwDgB48oA/IPToJXHK3K7lWHKO0EkFtRsrUmnmdRhLVPTHXztU1NZXVj1OTyWRkSpqq6snnrchW2YDVVVMzzVE7LYga2LXPI/PtHK+p5ZJGZ5WILMxJY/aTUnoytoxFFBbQKsVrECiRxqFRMfhUABR9g6RMlfMks9VLDFTLRxVEcMkvjdJDUMUjJRr654lAFh9eT9PZe0hUliAAOFfn0IEtUZI4VcuXILAVBGnJz5A9D18CuoslufulOwcm1auzNlNUrDSZRY6yPM78aBp8caOrnj89NFg46/72RI20xTih+vkOmQfabli4u94ffpi37utqqgfIeY+ak5AQGppipX8oo+81zxabbyIOUrPwzvl6VeV4qqYrRSKq6g6S0rIFBOSolxwq/fzsfktL050v1707icdtTKZDu7c9XnM1Rb2MlXtXJ7N6hyO1915LZ2XxWPraXIVke/Nx1+KpJEnMeKnxsddT1UyeaKOXJKQkUp/Prnc7swGqnClT/q49U9fyrcdsPZ2Y7q+ePeVLDgupvi5tHM4rBZiipqGObJ9jdhUC0FThMOspgirtwYXbuSpMZiaMPTIs25qWBWKjSmk4lzwGfz6U2QeHVfatKRUAY8Cx/D61IP8+rj/wCXl112Ln9872+c/wAlcLHQd1fJfDRDaey6thWN0v8AHtov49sbrvGrNSUs+JyGdCw5LMJoikmk8ElTDBXNWoVKKXUyEnOOPSlbZ5Y/rXGm4YqUp+EVpT9h/wBWerU90z7XXCV2Ky8k+Kw1fQU0kFZRJPUCeKoQNTSQyIrJI1NLxo1EaAObe6k4bUc+vRlt0N+ksFzZBZZEdlZGIGmhyKE1AI8/Xos/dFL8gaDrGDG/HnO9Sbr3Y1Riqenh7fr98bI2bBgHaaWvrchkNn7d3JuDNxwpEkUePR8YJjKXatjEQim9qkKKNQ0jh0v7muJ7yz2gJfuxq0j6kX1bSo+P0p9vRK6fK/zjtj4+hnxPUvwo+Q23sGamslwuyqjsbrfcOSllnlqVhxlTv3OYPY7VdAsqwwVGqqaSOMGRDKSzMktgAA/Porv5t1s5Ga6vImlYUYRtR6fw8NSj9nVT/wA4fn58p+zNvR9G/J/4uf6PKXYu69u7j7c2bJuzduHw29Eq6HcB68wmSgwsVJVYzaEm6Meuagmos3kkylXg4VjqEiWTXQsxweiqW+MkAgW2RI6gvpJJbjTUSeAPp5jqJ/Kt+Rm6fjBgOyM3sf4U/Ib5H9g9sZ/B46k3h1ztytj2TS7N2hTzww4CDOR7by1BQ1i7qy9dUZF42FI6tTrK0ZpReyNpqQtemYH0B6QszNgEeX2fOvW2nsjcOe3Vsvae4d1bSqtg7nz228LmNxbGyOTxWaq9lZzJ4+nrcrtarzOCkqMHlKnb9bM9LLU0bvTzvEXjYoQfalfI16OYkZUQshU0HaTU/YT59PYqg7EKNSLe0i8gkfgAksbE34HPvYPpnpaYdKjUe4+R6zNPpW73ANmNiAtyfQGsebtzb8e91px6bEdWOnj1xEgZSOSxJIsCObfrJJvcH/Yc+/fZ1soVIPAedf8AB1145vpc/q0/QfqtfX9f1W9+x6/8V1vVF/COHr/L7OhL9sdBPr3v3Xuve/de6jzeR7ImkRlh5XJ/sf2kA/Jb6f63+PveOnE0CrMc+Q+fWj18qPgf8vt1fKr5PbkwHxw7ZyWC3V8g+3NzbYy2N2fkMnjMzt3O74y2Sw+bx1TjlqqSegyWOqI5o2D6lD2dVcMgxK5k5N5mu9/3ue32S5aF7uZ1dY2IIaV2Ug0oag8fPr6FPZ77zHsTsns57RbPunuptEW5WPLG22d5BJNoeKeG0jSWJw4Uh43BU+VRUEggkKa7+Xp8w9aGP449vIPt6ctKNjZ4BZoxGrxR6aEFGjYH1cgk+ys8jc1lsbBdVxnw2/zdDG2+9V7DFTr90tnJ1HHjrwNaE5yDjr0P8v8A+Y0f26D489wjzTs7KuyNwssL6gEeQGhGp21EluSB/X3v+o3Nf/RguqH+g3+brcn3pPYRvEc+52zkBaV8dM+oGcD5dKSH+X58uYjP/wA4+9tCNppWIOxtyh+fSGUpRBjI30axvp9uDkjmgEj9wXVP+abf5uimT703sW/h/wDMTNo1gAVE6U/4rrNSfBb5k0Ll6b489xSULzNqp5dkbkKssEgMJl/yHTEwAB9PpYCx+vvY5L5qU45fuiONPDf/ADdNzfeW9gbkBZvc/ZhcBcMJ4/xDNPX8+HVl3x862+UnUvww+Ye2MZ0l2dTdldoLsHYm1sO238jjtwRYDcS57b++d342mKUuSddrbVy1TPBNSxTEV/gRVb1aZE5e23mPaeUeaLRdnuBuFy0cUaFGqVYOJGpg6QtRUcCR1iF7lc4ezfO33h/ZTfrzn/am5P2eK43G8n8QPEZ7dhPaWr/Ev+MXCRqysR+lrJIxUgJ+F3yvIFPB8d+3Epj4/Gg2LuRRGqR+OK5Sg1LZRZgljYkAj2ATybzUTnYbqn/NN/8AN1lB/wAEP7JBjLJ7n7QZs1JnjNamp/2K9eovhF8upJ55X+OHbQjmqIi039w9xO6KgOm6pjnsQVUni2k/4e6jk3mioDbDdcc/pN/m69cfeP8AYtY4o1909o1BD2/UIASePE/b+fW2/wDDPpCn6J+NvU/X1RCn8Xx+1KTI7kRoY4yN0bjaTP7kSVUZ1lamyuRkp0YkkQwoosBb3k7yntf7l5f2uwpSVYw0n+nfub9hNPsHXEj3w9wZfcj3S5z5sjc/R3F862uTX6eGkNv6U/RRSfmSePRqvYh6iPr3v3Xui/8Ayp6XpvkN8de4Om5UozW732VlaPblRXxeakxm9McqZrYubljEkJYYLeONoawAOhvBww+vsk5j2sbzse57bSryRHR5d69yflrAr8upN9mufpfa73T5G58RpPA2/cI5LpYzRpLV6xXcQNDTxrWSSPgfi4HrTjp/gp8xPJTSSfGruaIuA08P9x88op3PPjeSKkKsaIkr+0WjkK6lZlIJxa/qbzQKj9w3R/5tP/0D13Sm+8v7C6ZUX3X2U0wreOp1D1AOe/jmhAOQD06P8F/l8xCH459yyRJKJS/9xdwrK5ZGU+MNjyVk5Gpif9bn3v8AqdzR2/7orqn/ADTf/N0jX7yvsSKsPdLZQ5XTTx0IGfPPD0H7etnX4KT9tVfwgxnXPauwd47R7E6x2tuTqijw+68PWYTK7g23gsO8HXeRx9Pl2jqaqnbatXRYySplYCfI4+pa+mx95CcrNuc/J72O42Usd/DDJbhJFKsyhT4ZUGmNJCj5qeuRH3hf6jx/eDvuaOSuZLK95V3W+g3l57Rw8cM00oa9jfwxRaXCySqqjtikjHGo61b8f8CfmAmGxlLN8be5YXWhpoain/uFnT9nUR08VyVSjkSdYpUtZXdb30sQQfePbcnczmpGw3VK+cb/APQPXYe6+897EHcLyaP3U2Vl8RmVvqF71LHzPCoNa0GKVHXk/l6/K+CaJ6T47d1QSFj9zImyNx+GpN/KDLHJjrrEjfoCi6uB+PbY5K5mB1DYrsev6b5/l14/eq9k5I3Sf3P2Nkp2AzpVfKgIPE+fy6fqb4F/LRhFPU/HbtxKrS9lj693J44ltp8MhehZqhpo+PIbFST+D7cHJvNFP+SFdV/5pv8A9A9Fkv3nPY4F44vc/aDDXiblKk+ooaCh8vP7enaD4E/LSWqhjHQHbStIDrkfZO4aeGnkUKAIZJqOGGOOUWLtcFioH0v72OS+aCQP3Hc/842H+TpDL9572Pjgkc+5O0kLwAmVmYfMCpJHkKdGL60/lf8Ay73XO33vXEOyaDyRxmo3zuXC0PjV+XqWxuNqcznWMViQIqQt9FK39m9h7b803ZOuwEK14zOo/kCWx9nUWc2/fJ9kdmjH0XMU25XFCdO328pyOC65hBHQ+pY+vVofR/8AKn2RsqVc33RvCr3xloYhLDt3CQVOE2eZlsftK2UON0bhFNMBpRGxCyI5DxypcEbbT7bWNmzNu9y0lyFJRFwhI8v42IPl21B8x1h77iffM5p5kiaw5G2WPa9vY0e5lYTXVMgspIEMOoHjplZSKq4PVumy8VicHg6DDYXF0OHx2KoaGhocdjqSloKKhoIqZDSUVHRUcUFJR0tMjELFHGiAkm2osTLWymIWaQxxKgjATSoAAFAQABgAfL/DXrCjerm7vdwuL29upJrmZ2kkllZnd3LHUzMxLMzHJJJJ+ynSt9m/RT0Wb5lba3JvH4ud27Y2hg8huXcuZ2RW0eIwWJgapyOSqTUUsngpKZGSWomESMwjjvK4WyKzlVIX50tLm+5X3i0tIGkuXjAVEFSe9SaDzwP83Ut+w+8bTsHvB7f7zvu4R2m0W+4LJPcTGiIoVhVjQ0FSBU4Fc0FT1rGD4ffJqRi8vQnazkRtLGzdfboDgsA0cKscQrwsCCGso5IP9feMZ5M5p/6MN1/zif8A6B663H3/APZ5QFX3G2oCtCBcx/mfiof9Q6EHrv4vfI7D712pWZHofs+joKfc21chV11Tsbc9PBRx0mboZqyepq58bHBDBT0sZkkeVkjUKSSLe1m3cpczQ39lLLsd0I1mRmJjcAAMCSTTAHr0Eec/en2n3LlbmO1s/cXbJLuSwuoY41uIyXLwSKgVQ2WZiAAKnI62ywb8jkHkEfn3lx1xk6or/mOdL9yb++RuO3BsTrXfW6sF/oi2dilze3tq5XPYkZah3Z2DUV2PmqsRSVkkFVS0uUp5XSTQSkilNXNoA9zuXt73TmOK527a55oBaRprjRmWoeQkVAORUddE/us+4vIPKvtZc7XzLzXYWe5HfLqf6e4mWOTw3trJUcK5AKs0bAEVyDWnRIaf4y/I3yx6+lO1FjTxoRJsLd/+6zpWY+PBBZCqmwH1K/X3H39TuaDQfuK6x/wt/wDoHrIGT3n9ptLBefdq1GpqLiLzzTL4r5/Ppyh+N3yGWR3j6R7WhlLegt1/u0xFlW0UzOMMSBYEGy6gCP6e9Dk3mev/ACQbvj/vp/8AN0kf3i9qjGqtz9tTJTNLmKtDxAGv8+PSjpfjt8g4TqHTnZSlv3UX+4e9SI3kXQyrbb6iKynkHULX/r7cXk7mgAkbFc/Z4b/9A9Fcvu97WPj+vO2nyJ+oh4D/AJuZ/l0B/fe5c18dYMTT9gbR3VT723RSVkmz9inb+Vo91boTEU8r1tbR4bK0VPWQ4imSNvPXmNqenjic+t18ZNdr5C5i3G9EFxam1twAZbi4UoqCtARqALMchVHEj7SAXzZ78e3HLe0Pe2G5rul8xZbWw290lllemogshZY4kwZHbCgg0JIBL38aflf2X3X3Bt/q+s2HjGk3lBmRtRdm02Zy+cfK4jHVOVkpq+jjjrajJxPi8dOGlhghZGjDadBOkacwe2kVhtT3ez3FxPfRsoeJ1B1BiFJVVFQQSMZx1BPIX3j7rmDmmPaub9rsLHZLiOTwbmKSRfCZFMgWRpX0FWVSKgJ3UNKHG0d8Jttbk251nu2i3bt/MbfyM3YdTWpjs7iq/C1mQhfYmwaCCY0GVpaOvSnkyGOnQO8SiRomK3WzEScjWNxabM9ve2zxzLM1UdSpYlE0ihANCVJ6i7333fat45ytbzZNxhubP6BE8WB1kVaT3DMNSllqFZcA4rQ5x0CHzs/l8fHv5z7m2VQbu7Ji6s732tjqyfD1G2ava2R3LuHZlbLTmqo9ybNysyZTN4eiqcez0NXTy0z0crSjyPGzxEfWtrJEJ5QsaXMunXUFg2n4SwDKTpBIFCOPUJz3Czi0t7iSWSygLmJVYKU8TTr0FkkVdRVSaqcgdF72t/Lf3J8YdmpszrnDVe/NtUlbVZeq3HjK+mqtyZzIVc0aVeWz+36w4+upa2eJIkjo8X/E4o6eFU1+nmJeceUuZ9z3GXc3VLmMALGsHbpUE0GhjUUrWgZySTnrKj2q9yfbvl7Yrbl+GaawlLNJM17V/ElcCrePGug8NILJCFAUAefQZb+oG60wGa3F2NS5DZWEwlFUZfK5HcuEzO3kx1FBbXWNTZjGUNXLqMoRVSNzLI6ogZ2AMdty7u31EVm23TC6kcKgMbKak0FNSrx/Z8+pxHPHLC2Nzuq7/aGwt4jJNIs0cgVFWrV8N2OAMDiTgCvVLnbfz27Tq8o69cY3EbE2n9tjshiqnLUkGY3vubD5HWKSrqIcjHVbd22zU8azSUrQVUtMJVDyl20pLGy+2+zRQg7k73F3Uo+glYlZeIFKO+cVqASMDrGPm/3/AObJ7t15eihsNqCrLCZVD3MsclSrMHBihqBqK6WKgirE8F38a/ln3rnu7dqdP76Q73pd+5Wg21iayLZp2jurF7mzFIHw8UWKpkpoKmkrMm5o2SSBZ5bpNE+n0Fnf+Qtrk2iW92GJo75KFYlk8VHGsJQE17jUEUNK4Oc9K+RvermSDmmz2bnW5jn2eYlXuZIPp5YCIjLqdRpBiGkg6lrSjqaYOwfsn4TbwzNNLmewS22sTSFK84aimx9ZuTIQxANPGz0hyWAwRMasvkaXI1Q5VqSFiJVI9i9rrq5dJ98fw4ahvCQgufkSKonoaFj8l49SLzF94jarWVdv5Tj8e6krF9VMGWFCagFVbTLLmhyI1/pOO0n52ZjdqbU82zMHjqbD4bZtDSZLby44VHhmw9XD9+zkt91WVUjZGeaSZ5HmqKiaRpZpJJZHdpvsbO1262jsrWFY7aJdKqnADj8zXNSTUkmpJNesZ95ud43Uje9xunnvr6RoroykFhIp0fJVGgAAABVUBVAUADTx/m79wf6ZfnHv+Wjq6Oo2v1HtXbPWe2shVy1LY/P1uApv73bwioFjjno5srBu/e9RjZo10Bhi0WUqVUe3pGDNg46BF9G8V3LC8YQxHw9Ofw8R9tSa9HW/l0/HLJfMDa3SlDmNvZzE/DP495XI74rdtbjWmjPyb+YuWaoyG8N5ZPG4ylpsLXdP9U5DJNi8UnJEdCtDM9VI2Rho7xpqFSe3z6fs0VxHNcBBaRPVsZck1IPGoFceXy49bEG86/bHWdBWdsdu792z15s/b81LVZrIbtyFDicfj6OnnFHTw1OcrshFRxwVkjRxxNKweQyaDdmA9vagFKj4aU6M7m7tmje3tRqUg/rE6FFc8CBQgk1AxXh0Tn49fPf46/I/tup+PfU3b9NUbihhy+49o47cOw9542PL4fHashWRbOyu5MDh8JnaqhxE33iRQ1LtJQrJUQCWnikdGtYauBXp6TdtpjbxBbvLeMgWRl1IrEDJJOc09M9WU0OzMFSSR1GTmlz1ah8sU+ZljqI4ZF9LtS0KJHRw2Yf6hmU/n3s548Oiqfdb6cMkQ8KLgViBH2VPE/t647p3jidiYPce6tw5Olptu7exOS3Fla2eVY6bE4TCUM2QytVKyqQkNFjqSSRvrfT+Ofe6ClemFt1mjDFShUHUacfn18/buXfHZHzj+T++OxMbTVs+9O7e1Mbgevtr52upFymDoN252HafVeynSJg7U+1cCKKCvlpoJEh8E08nDFinPc2OJ6LgC2AMk0A4ccD/AGet7Hpfq7bfR3UfXXT20Ymj251vs3AbRx0jxxQz138Fx8FLU5WuSnVY3yOXq1kq6p/1S1E7ublj7WBRQDyHQmjiEaRoCMCmB/n9el9OssitGbLGAPRGdN72PrI40Ei5t9ffiDQ+Q+XS2IxqQ4+I+Z/yfPprMxjdQWHiUlrAkAOp/UfTd/V9PwPdagcT/q/y9KggYYHdw/L/ACdZkkVtTLJ/nAGsQXC8nSqRg8A/Vj9D72DX8+qsrCgK8ONP8vUhHnkfUpLCMKgQCzOQeCHvYEX+n+9e992emiI1WhwTmvTj457W1R38H11Sf57ya/re/wCn03+v497o3y6Sa4q10mmqtKD4aU/2ehJ9s9BXr3v3Xuuje3H+x/rb/D/H37r3UOTzKg1GO5IS3q8alm4awu8jAWsOBf8APvYp08uitADTj5V4cPl1yipUUs7/ALkrtqeVgFZubhbL+lF/p70c0x1p5WagGEHAf6vPqPWY5ao6rooSN9CeJD+8xB1lrXIstrf1597FB5dOw3JiFKHJFTXy9OmaWiSkmCgCUNErkkAFSPToJA4BY3HF/d8MvCh6XxzmaOpOmjUH+GvUqWKKCCFVpwaiZTq1rq0KSNZS4AV+ePyB9fdQKn5dMozSSOWk/SU+WP2/LrBJSa43kRUkCuYli08tcKbkBbSAfkfi3v2OBHV1m0lVbBIqW9P83XKgxNHWRSy1dMGm8ssRa7xFkWwRCiFQoiP0/oefem4/5ut3N5PA6pBLSPSG8jn7TXj01Ni6anykK+QOGkUKilpQQl7io1NpjSNTp+pP+x9++Y6VC8lks5DooQMk44/w+pPHpQNSTQV/3NNHG1JLGEniUtw39hoYh+2rKeWI+o496weI6LBMklt4UjHxgaq3+EE8fs6e10hQFtpHA02sAOLC3HHv3SI18+PXfv3Wuve/de697917rjoX66VueTwOf9496oPTrdT69e0J/qV/5JH/ABT36g9OvVPqeuwqi9gBf62AF7fS9vfqAcB16pPE9daF/wBSv9foPz/sPfqD069U+vXtCf6lf+SR/wAU9+oPTr1T6nr2hP8AUr/ySP8Ainv1B6deqfU9e0J/qF/5JH/FPfqD069U+vXL3vrXUKtooKyMrMXQKUkDxsEZHhbXHIGIOlo2FwfaS5tIbgVkJBGaqaHGR+zp+GeSFjooailCK8cH9vSVwueoUpGnKTLDVVFZIpjgklcTQSN90GSJWcRNGPOnFhET/S3sl2vcYIonVwfDLsQ4FftrTPDP2dGd7YzmULUGRVUUJAweFK444Pz6WcUsc8cc0LrJFKiyRyIQyujgMrKRwQwPsRRyJKiSRsCjCoI4HondGjZkdSHBoQfXrJ7v1XrjoT/Ur/ySP+Ke9UHp1up9T17Qn+pX/kkf8U9+oPTr2o+p65e99a66IB+oB/1wD79SvHrdSOB660J/qV/5JH/FPeqD069U+p61kfm5/O/3rQb13bsL4UY7ZVdtbriraDcnde58e264995WiyNNjavD9V7ZSpoKGr28mUmFKuYmes/i2p5KKKKmFPXVTZahGkfKvVC5Nc4Gf9Q6tx7g+Xme+M3xs6XzPbm18ZvP5f8AcO3dl7N2P8f+v1egq+zfkNnMDiTn9t7apsjXZKowGwts7gyDSZbL1lRJTYrHhNcktTPSwVFzQCpXPVtTACpq3y61zvn1ufJ9CVeT607D7Lw3YHzl+SuJpcx81O4sZjGyOI6T6nzVDRTbS+LnTeMAnm2ztTI0yxz5N4ZIcvk8XRU8lUTT5KmjpqOcBSo9TgcaUr9tBx44Hp1RVKktrPiU0lgT8NSdIzhakmnDJqM9K/8AkZ/HDL9k/IvPfKPJbeo6HYXR+IrNr7WkgXJQ0OV7j3Vtylwzw4sPWypWSbc2NlquryazvJFFU5qkeKNWCmnQXc5iVUTMrEUB8yTQD9v+A+nSm2jDuSTRV4keWM/sU/zHWy38mPkNt34r9Ldmd475X7vC9dYGKahoKJJpJ9zbyztfS4Hau34Ep45ZIajcG5MpSY8SMPBRrMZpnjhSSRC+2aYXkkTEO0dO8HBc/ESPXT5eXlx6XziIWwlBI1/h8wooFA+1vPrRh61wfdvym+WHXUkm7twZLuz5E9l4qoyHY23s5HLvfDJVZoTbs3Vj67HVv8X2dT7A2zg6yso6XVRjHYnGxRwItIsQY+qWPRMFooBNWJ4/6vQdfRCVdKqt2bSoXUxuzWFrseLsfz7e6c61zP52/wAp9x7X3f1n0rt3b+x94bH6/osJ3L3ZtXe1fjZMbuur3nWbp2L1Ftyba0+cxOY3VR4GuxOW3BLFS0+Qp6PJ0mIrKyNIYQs7bkcNIr5H0xTHpg0+w9aOryY0wSPI5BFQeNGFR5AgHyHRRf5ZH8qDbvycmqPkL3WufpfjVBncjS9U9enPVZ3D22mNq3o67Nbp3Zj6PblfSbJxeQppKNmx9PjqvO5GCaWNqXHww/xHSL5n/V/xXWiNWK9vH7erztufyuvg/wBT91bY+Su1tiz7ByPWFHNmcZt6n3jlKPqPDZXGY+viTfldtjKVU9DS5fCY+rnlWX7iKgimvWPAatRUDfhxinaKDyoKev8Ah6c1vq1F21cK1PoR6+hI+w9Dt8afmn8bvmDL2JB8f9/DfcfWeTxWL3POcDuDAwSxZ+nrpcPmMMNxYzFzZrbmUkxdZDT10CNTzSUkmhmTQ73BBrTqobgVPTP2XvDHdWYXee+8nULt+frLC7lzNYtYpSHI7SwuNq8z97RTyqKaWKChgkuGICKpB5X34moLcCPLqToWSfbTJcJ4+2SxePIUIBjkQd4fiVJpx8+PA9aRHSOzd8fN75S9b9dZKurxle8u5d07mzcT5meLGbcw26spmO2O35dtJVR1K4vIQbfosrU04APmqEgDKTZiyBU9RoHDsgldvD1VPE0qatSvn1uR9/8AdPxw/lt/Hrb9fv2rpMZhNu4b+6vTfS2zZExdRuaqwFFHJTYDa2KabzLQ41GjmyuZrpDT0gmEtVI880STqCwA4ftPRpNuscS+DttokMORqIDSH7WIoK/Ida7vzxT5B9r9J0vy1+d2fy/XE3YtfS4j4VfD/aBWkxWChrKamzOX7N7P/i0VTUY2LB7KqJmlkq4f7y5TKVlNTyHDUJTHhpySAWJrXh0TFnc1k/LPnmuKYoP2/LzEL+Qt8csr2L8it1/JLPplY9tdCYCr2xtmtLiKHK9k7+wldharHyyTRSy1sG1uvK6qeeJWiaKTK0Laiq6DpBmvVgcg+nW3HUw0qR6pgyAARr4wS/p9WhNIOkX5P0ufqfb9WPSqF52eiUJrU1/w/wCrh1RR/Ob+SW39s9LH4u7a7A29he0O4JcdV72w9XmGxlbg+hsaMzl90V2QycaTQ4xd8ZHb8GBpKR0kqs1HWVUFPBKiTNHWQgDBof8AV/l6WXk6hBCkncx7vs86+np/k6q4/kjfHc76+VeV7gy6Y2owfx52PTZ2m8eTpa8z787eoMxg9kSU8FJHPSxJjdnUWemrIqiZKyirmpAYUfV46QrU6ieHSWwiMs+qnao8/U4/wV623xKbjUp0eoBUBLFiQ2pm+hGr/YD6n2oBNK+Xp0JdAodLZ9T/AJOg67X7W2H0r19uztPtDcmP2d1/sPDVu4N0Z6rSrqoKHG0ekMVo8dT1uSylfUzypBS0dLDPV1lTKkMEUksiI2iQBUkU9OrMY4YnmkaiAVLHy+wUr+zp5gycGUpaHJUrO9JX0tPV0cs0c0JlpqxFnhlaCojhqIWMcgOh0VlPBAIt7qWOOl8KqUJBBFK0HWWjq0V20D86IjpJ+pP5sSrEAk/gX96UgEnp2eFiq6uNKt0oaCRyG9QXUdasfyTf6s3FlA/s+3F4dFlwi/w1AxQdOOkX/X/Zvexva1/J/wAFtxp+tve6fPpNXHw+dP8AY+359CR7Z6CnXvfuvdeIvwffuvdcGjV2R25MZunNrMQQTx9eP68e/dWDEAgefHrn791XrHIrtpVSFW/7hIuxX8BPwCT9b+/dWGmjVGfLqJ9p5JzPUWPib/JlUkaUHN3/ACzFr/7D3utOHTvjaYhHH5/ET/k+VOuVQsRZZZRYcRqWbSLE3BsDcsWPA/Pv2aU8utRs9CqVrxx1xXVCtPTRxSOhvHJe14ozqs7twObfQc8+/HNT1s0kMsjOAwyB6n0HWelpoqOCOnhDCOMELqOpjckkk8ckn3rqk0rzyNK/xH06ZK+G9UEBRpanzCAaiHBVBqBUDTptwD/xPuwPkTjpfbsPBJIIRKavTJ6fadZEgiWVg0ioocgADUALgW4sPp/j7qei+QqzuUFFrjrN791Tr3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de66ZQysrchgVI/wIsf9496IBBB4HrVaUYeXQUxUdNt2bINky6YuqjfD11Y1wKRP1Y6tZkuEpqqGTxliCFmUXsCfYHhhG13Fyk5/QkrAXP4a5Q4/iXA+Y6Fcsz7hHAbcDx1ImVB+KnxjPmpFfsPTptjcsJqocHNKKqSefLQ01fTx6aaWqxTxPWQPexjmkgqFlAtYHWt+B7Mtk3JTJ+7nbUat4bgUB05b+Rr/AC9OkW5bewja9QaVAQshNSA9Qp+YqCP2dCH7E/RF1737r3Xvfuvde9+691737r3VbP8ANm7/AMx8e/hH2fldqy1lNvbs18f0ps2uxtdWY3J4nK9jpWY7KZ3EVuNnp8nT5vA7Sp8lWUD07CRa6CE8KGIqxoPn1o8D1qe/y+dibNg77oe3+8q2kwvx++LG1R8neyKiephno66TblVQ4/qXadBTxVQoqrd+8OzMti1ocVUMlRkfspaTRrkClpcn5enz6qaVDYFOJPp/q/1V62Veto89sDZ3bP8ANo+aW1cpQ9w1PW2UbpboqaoleX499K5OWnbr7pzBY2shhjHfPb+aq6KPcOTqIY6wZLJrjI4qKBammkc4VY9bFfiP7B/g+3rUmyFD3h8nvknk8ZX4Oo3F8iu7e3q+KvwNbHV0EMW+9wZup/iOErqTINNNgNtbQ0tDKJ3CYjD44q9o4DZrj+fXuAPCv+r/AAdb5Hxw6J2l8U+k9hdF7MnT+C7FwtRi6fL1yQQZHd2463yZTc28sssCiCLIZzOVdRUTRKpjVptKEIqKAxc3jwXUviSopLPHEWOCdPHzoFHbSmTno6gtxJEiojsAFaSg4CvD5knNfy61/f523yo2hu/dOwvhxjs1lxjdk1R7H7hr8FVY2GGPdVZtTKL1Xsmr+/q6emqo6eTMR5zLJMVjp6SagmgE1TaOJXssFIROfgppj+YrVm+xjw+Qr59M7lKDKYgcg6m+2nav5DJ+3pk/kFdXf387z7F7ty8WSyWO6R6qwnXe0KuvpMbSUOL3V2TlMhXZ+DHinjmqshUYnbO2/FFUSTJLHTZaRZUIkh0n6DNeizz+QwOtrXI5HH4fH1+Wy1fR4vFYujqsjk8nkaqCix+Ox9FA9TW19fW1LxU1JR0lNE0kssjKkaKWYgAn271vrRi+ZuYx/wA4P5jtPltlVW6MN1p8iOyuiOsOr9zbnxsmBr8xsfNRbZ6v/wBK2zcLm1iqZthZ7I47KZLDVhjC1ioNaR1LvToyaF+qmpGPsH+freA2htTa3Wuy9tbJ2pjqLbey9ibaxO2tvYqnIgx+E23tvGwY3G0aNI1kpqDHUaLqdr6Vuxvc+3urdatn81b+ZfT/ACMzEfxE+M29sdjemavdWM2j3V3pNXT47ZG9cjkcjFQQ7Xod10MdYYOmMHKk9TnsrDFL/eBKRo6MTYuKZso2zVwOHr1Ugtw4f4f9jo8v8kXbdVtL4+/JH5B9m7121mZOw+7t2VGV7UqMjDBiMxsvpzDQbcq93Vm5MrT4f7faSZ6PN1VM9VDSJBRkzOkQkZV2mBXrYqak+v8Asf5Oil/zIvk/3p8wOhtz7x6Vqcj1f8J6TfW2+sdi57LT5Ha+9vnT2FuTL1WGraXZ2NmNA1B0LtLDUlfkpZcrJS0+c+za6TSRS01B5qkDT/xfVNWGY4jFM/nT/V69V2/y5e8OpvidvLf3yt7aliy8nVfTtdt7o/rGWposZvnffZ/ZmZahrq7acUlGY5Nn7ewWAykOb3HUMIsTR5IQLHVTlKc0Sg7uPViSNRIpTh1dz8IfhV2b8lezqb+Yx/MQpKXcHY+5KXG5foPojIU9Umyun9oxL93tnOZHaOVmrYsbkaeGQVmFw07zSY2Wd8rlDPn5x/CnAK1J/LrQBOW/Z/q/1f5KEv5kXzYrvk/8t9x9q7LzlXR9edU6didL1VHVtJSzbf2XnKrLVHYUVNKZKBqre+60bJwS+JZGxdPjI5V8lOCG2NSf5dbBwWOB1trfyy/jf/ssPw46q2blsX/DOwN4Y7/St2v5ohHkpOwd/wBPSZSvoMuygCWv2lhUoMFqFx4sUnJ+pcUUAr1sCn2+fQo/L75V7B+I/TuX7N3bHU5/PVlXBtLrHr7Bx1FZufs7s7OxVMe0th7doqOGqqZa7MVkDGaRYpDTUscs2hygR9nArTpwhowrMpAJx8/s60WPkRmu0cx8le0Mt8o8rHX9vS7gkPZb7eqMFn6Lbm4aPD0Ro9l42Kly7bebDbKijpcNPRiskWhhpZo2klqIneRlqknVx8+vNq1sZT3+f+r0HW17/J46Lq+m/hRtHLZ3FjGbp7ozWY7hzNLLR1NFV02M3ClJj9k0VQKuGCqVU2RhsfU+NlCRy1UgTUDrdREtEz59HVghihRjhn7uHkcD+XVmlepjhaoqJI4oKeJ5ZpZZI4Y6eNRrkkldxpVVRSSSbAD3dga1PDo5ikjGqhpX+fVQtLWn+ZV3lDU0kLTfA34w79qJYaoZAVOC+Xnfu258dPjKlKWnjSPL9KdOZSF51d53xm4MpJF+3WQJItI2SW+E9oPSFSNzugWB+giNa+TsOHzKr/PqzjNVhooHdxFrOlfUSbohusUYRjeRiTYm9x7Zlfw1NaV9f9jobWEH1MiqtdPH9vma+XUfC5HzskiFY2nQlif7CBgqkhwDeRrgcW496ikBOMVHTt/a+ECjCqqaD/LkenS7ikMbwWDGIRmwRC1r3uxNiS0jcgfj2qBwFHD/AFfz6DjqGEhOHJ8/9Xl0ovK1r+BrePX9f913t4/1Xvq/P1/2Hu9T6Hot0f8ADfOn5+vQm+2egj1737r3Xvfuvde9+691737r3Xvfuvde9+691iezg2UHTezMtwrr+bcMbf4e/dWU0Iz+zrHTvK4LSxvHYALqZfUP9UUUnQx/ofoPez1aRUU0Rwfs/wBWepPvXTfWIwxmXzFfXo0H+hANxcf1H/E+/dX1to0V7a16y+/dU697917r3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de697917plzkdEuPraqvqI6SjgpKg5CeVPJAceI2apWoiBu6LHcgj1KwuPyCX39rFNEzyOFUKQ5IqCnmCP5gjIPDpTYyTJMkMKFmLAoAaEP5EH/COB6BjD53C0WQxe9cqKmClyCVeFgq5g1NRCouVxWcSlndRTndGKogl9PM0dvzf2E7S4gtL4XsyuURGUkKa1phyvoyDy8wT0Lbuzu5baXaYChlDCWgyafjjqP8AfTnh5A9D1S1MFbTw1VLKs1POgkilT9Lq35F+QQeCDyDwfY4iljniSaFw0TAMrDgQeB6BkkbxSPFIpEimhB8iOs/tzqnXvfuvde9+691737r3WvD/AMKKMjlKXob44UsMhhw03eeUr6yRHdZf4xjet90rhlREOpgtFW18lwLq0a2PNi2/AdVamK+v+Q9EC/lKfBPdHZnyX3FVdozzzdP9GL19vbfm3dublOV2LvzuJTRb06o6+3VW4GubbW7ajrf7k5/LUIlrVxeQjpaOpQCrmRtICTXy62RU0/1f6h0en/hQv3hJgeteh/j9jGqVqt+7vzfaO4pqesrKWKLB9cY+LC4KgrI6SrphWCv3TvSPIU6SrLElThFlsHjjPvcnADrx8h0U/wDkN9BRbm7a7D+Tu4cacs3XiTdbdbVElZBPPSb/AN14dMh2BuiSnkH3P3mD2FlKalhqJHWOWPPVSgO41RkG7bm1pJb2NvGWu51YJp/CBSrZpWgr+zoxsbIXKXFzJIFhhIrXzJ8seuP29bCPy9+RyfHfpym3HtfbVPv/ALv7K3BjeqPjV1jqiFVv/treEktDtWhqGnqKJKLbuJVXy2dq5Z6eGlxdHLeVZDEGUbZbQT20V1JGr1FIywr2jgTX8TcSfy8um7yaa2le3RyCCNYBpVjxH2Dy/M9akv8AM3+NuT+LPb/T+19y5OLe3YG/uh6Psjuvs7I+SsXszvfdvY3Y9V2huCJqiKkegxOPdsfS46OGCnalxqQHR5We5oVC6VA6RZqSxrXJJ9fPq6H/AIT/AOPxGM60+TtPt/KVmawx7S6/qIsnXYiXBS1GQrOqdv1uW8WMmnqJYaKGqqdEDs15olDgBWW94/Prf8X2/wCQdC12r2BuT+aT27nfiv0Zlaig+C3V2doKf5b/ACH27kJFp+8Nw4+WmyX+yy9QZugkijq8FOvifc2Yo5pA1MwQPDTNSLnt11YHDqvxGn4fP/N/n6ET57/yxMf8jYulOxPjfndo9A98/HCLamK6syibeWm2MdmbCyQ3BsDZT43B0ksW1aXrzdMMVdgaimx9dTUCPU0zUM0dSrU+2WtCOPXitQAMdApvn4GfzMflth4dkfMD5n9YbT6kyVRTjd/Wfx62NlFhztDj5YjGk+eyNHsevyc2VVGkemypymFpqjRN/Dqho40j0VY8Tj5depWmo4/1f6uHVBXzt6C6x6j+U25vjp0Ft/ctbsnobrPby9nbqneq3DuPNbgjw7763z2hu0Y+LG4n7famF3vjaV6bH0tBQ0sdGYo4o9R90YAHh1414V/4vq4P+Xp8Uu2Plj8X+g9md74dOrvgr15T1O48P0xhshXpuD5obuyW6cxvFOzu4MgrUNfiel4ctlEqMXtuzLmquEV0pNFHjCbrUqART/L1ULU5/s6cPU+vTf8Az7eyH2pRfF/o7rWrg25UbQxe/e2qvAYGLH4qi21tjB4Gi6w2VPiaJYoaagmp6XcGbgxgpRHJR/as0PjdI3SshAoOnPMft/1ft6Iv/Kc+GtB8rPks2995nEbl6f8AjPXYDPbvFVktw5iDsve1ea/I9Y7Vgjy8FFDV7V25X4Z8nkkkhghqYqWmpJqWeGtkddIKmp61SvA462N/5pvfsvx3+D3dW6sVkxi94bww0PU+w5o6n7WvXc3ZM393JMhipARIcltrbdRkMxGE9QGOY8AEhxjQHrx4Y49akX8vf42YP5EfL/ozqrGpQb42XRrge2u1vvMdV4qn2ttDryoocvubZ81JXzpDnqLKZ+bE7eqKiGGWGqjyoaJYkWSRGlFSPTr2O0fn+zrem7U7O2B0317u7tDtDc2P2hsHZGDq9wbn3DkpJEp8fjaQKCI4oElq67IV1RJHT0lJAktVW1U0cEEck0iIz/Dj1cEp3+Q9eqX+uUz3f2Q3P/Nk+UG1q3A9X9Mdbb73r8LPj1uHx0qbL6+xmFnzc3eu80kM+Ok7T7Qo8RHJjAqTU9BRtSzRSVTxY+en8M9zUxwr0oizS5mkNFroUnPD/Vj/AFDVj2FtrcXyT7d2lsWpkabe3f3dlNSZypo45Hjx9b2duWJ9155YI6eRpKegOZrK52MxEcVM5ZLEv7YHcQBx6SgFyFIyzUNPnx6+hVhsPj8Bh8VgMRTR0OGwWOocRjKKItJFS47GUsVHQUodi0jLTU0Crckk2uSfa0DhXoSCkYAUZpQdVD/KjtDeHza7mzv8vj437jqcRsLb9C8fzo7zwUFJXUmytm5pKvHy9DbTr6uKpxlR2LvuCKppchZJBQwxzQsJTT5Wnp22JZtKN9p6TOz3LvYxGicJm+X8I+3z/Z69WUbA6x2R1DsLafWHW+3qXa2ytkYWjwW2tuUBdaaixlBHZfLNLJLWV9XVyFp6qqneWqq6qR555JJZHdtlVFAB9g6EFoEhRY0oIlFK8T/xfqfPqBk4vLXyRzDjxlUURh4rK37irb9Egb6N/qb+0j1LtXhSnQstG02yNH65NaH5H5inl01PW/wdpJBD5pZpQCVISMLpJKtqDMFJSwAFuOLe9xqFZqcePRXv+6tY21q4gLqxKipoAQK1J8yf+L6Xe2csu4A7yFqU0ZjSanV7qRa8bIwUFke1vwRb/Y+1S1YjNAPLoO2u4pdW7skNJ60auePmD6dLrVB/qJrW030C+m/67f6jVx/W3Pu9Pl8uvUl/iWta/n6fb59Cl7Z6B3Xvfuvde9+691737r3Xvfuvde9+691737r3Xv8AePfuvdcJFZ0Kq7RsbWdQpYWIJsHVl5At9Pfvz69+XXP37r3Xvfuvde9+691737r3Xvfuvde9+691737r3Xvfuvde9+691737r3Xvfuvde9+691737r3Xvfuvde9+691737r3WCpp4quCamnUPBUQy080Z+jxTI0ciH/BkY+6SRrLHJE4qjKVI+RFD1ZHaJ0lQ0dSCD9meg0osfjYXp8buCjoqlRQ6KN61UeBJsez46tpI3lPjQtS+KeJR9BI5W1j7A6x21o6C+iDVFO4k0aM6HUE+q0ZR8zToTTTXEyyT2UjA6u7RxIfvViBnDVUn5CvUramQ/heRbbMs0VVQyeeXb2QhkEqzwQqJZKSdkJT7mGE3uOGMb359rdhvvBuZNoYhocvbyKahlrUjGKgGv7emN0tjPbjcQpWcUW4jYUoTgMPOhP+ToSPYu6D3Xvfuvde9+691737r3RJvn78NsR84vj7kOoZ9w0my9043cWE3t1/vWrwa7hg27unBvPBItXjVrcZUzYzcG38hW4ypMNRHJFFWGVRIYxE+iKinWiK06C/+Vz8LewfhB0VvTr/ALM3PsvP7n332zmuy58d16ucl2ltaCt2rs/aNPh8blNx02OyuYlqINoLWTTPR0ixSVPgVHEXml0ooOvAEVqeqEv59me3RuP5pbc2xHjquuwGyuhtgUWOMNDPUw0mb39vXf8AWzuJ4IrQ5PNJt6Cnhjd2MqUjeNbhj7bkYA5Pl/g63knAx/nJH+Tq2z+WTTdcdA/yzesOwN+5vBbP2/Jhd9dy9mb3y7nHU+KxGS3vuTIY1aurRfuJp02/FSUwQCSaYRrDGrftJ7B+7xwXt+llBEGuKq8751ALURxqRw1Elm+Va8ehBt88trZ/USPpiAYRrihLfE7A4OnAB9aU6F34g7E3j8l+2l/mDd3bZrdq4cbYrdl/B3p3cNOP4r1T0ruBdec7k3NSSTT02K7c79oft2mjp1WXE7cihoXqaoTOIhhBCkEMUSCiKoUDyFMdB93eaaSaQZY1zxzkn/V6de/mS/y2YvnQnWe8to9jwdX9udR/xqnwGTzG3V3RtHc+DzU+NyUmC3Fj46qhyFBU4/NYeCeir4WqYoElqo56KqE0bU7jLq+3rRBNCDw6rs+M38kv5NbZrN9bf7r+V83X3T/ZdKsHaGwPjLubddFku2IIp8kkeH3HmM/tzbeFwWGamrpFmaLG5CWppKqej0wxMXNQhzU468QSKVp9nWxL1j1j1/0xsLa/V/Vm08NsfYGy8VBhttbYwNMKXH42hhLOx5L1FZXVlRI89VVTvLVVlVLJPPJJNI7tcCgoOt9Lv3vr3RLPlZ80tpfHar291ltDbeS7x+UnZUNuovjdsaoSTeO5fI9TAN1bsq0hrIOuusMW9HPJX7hyaR0cMFJUGPymCYR6JpT160WAx5+nWjx3Pmd0dqb73LuiYYfJdr9ub931V77qMDPlZqHJ9ob63xk6Cr2PtRP4hm8XNhNtSZakgopKOuqqasoZKN/JJJH7Y45/1D7etE8QRRq0z5/Z19CPrLY9D1l1v191ti5TPjOvtkbT2PjpzBFTGah2ngaDA0kppoP2KcyU9Ap0J6EvYcD2oGMdW61Xf55PTnyF7F+Y2ycvtfo/sreu0K3p/ZGw+vtw7F2dnt4UOW3FHuvfed3BhZZtvUFcuN3N9xl4QlPWvB/kURnjDI0jxtODXh1o8Rjy6vh/lofF3N/Ej4jbB6z3pi8Hi+zsxX7i7B7SjwTU08I3fvDKzVkGLrMjRtJSZbIbR2nDi8HJUwyS00n8LHgdoBGxcUUFOvD7Pn1VZ/woQ3nhZV+JHVeWy+UGNyO4u0OwNxYDBpSvlDDhcBhdr7bzlMuTmpMXNV09XuivgghkmVpxLKq829tyHgOvGmKjzr/q/b0yfyGdhbMwW1fk/wDMDe77e2tR4FcV1Gm7crUDBYHbG1Nj7Uwu/wDtHN5DI5zITjG0eVqK7E1OSqJ544E/hgfTCoZF3GKkmmTinWsKCzHAHE+nHoyOz6XMfzgu3aPsbc+FzGG/lpdIbumk602nnsfV4t/mR2dgJ6/H1e9d0YisejyCdUbMr4xHSUVTBoqp/NTVINT/ABCjx1vi8u3rVfE8zpB/b/sdGg/m97wn2N/Lt+Rj4unopJs5gdp7I8NQrGOGh372Js7ZWQanijKk10WOz0rUoNlWZUJBC6Ttq6SenyjNE8hOBQD88da5X8mfrGi3x8+tsZRYsdUUHUPWm9+z1mopqqvpP4rksFheuKOnNbVRQO1RDJ2LUy+NkAjqaeTQWEat7pEKuD09aD/GUYjCgmo9aUH+Hq+b5jfKbsjcvY1D8EPhhU0OT+TG+cJPVdl9io0tRt/4qdaVsNLDXb73TU0LFafe1VSZONsNQM6zo81PMy66mgiqnmYntT4vM9LLmZnYW8BPjNxb+H58OPRt/jB8YetPiJ07gunOrcfIaOgebMbk3Lklil3Nv3eeSSEZzem665Y1NXmMq8CKL/t01LFDTQhYIIkW4ARcdK7SFIVADER1qSfP1P59DZLC5SSQEvJ+jWeNVjcogtwFP5/It71Qk16OFdaqpwvGnSXfEzNUuoiHNpgX1FQ6glxc863vbm490MdSMdGq3iCIHVn4ccaeX5dIjc+NnpaYTzaVZqhLoBc2dX0+senQn0A+vtvQVap/Z0V8yXMdxtkSR1IWVTX8j5ep6hbUrMjSVFWMZj/4hVTxwLGHk8VPSmJ5GM07EqCGDWAuPp7cUkE0FT0F9ukuIzOLeEuWABzQDjxPSzv2H+r/AHE/8rWmyfov4/s/0/p/t/8ARf493/U9f8HS/wD3a/8AC+P+of6v29Ga9t9B7r3v3Xuve/de697917pJVOVrq01n2TxY3F0QY1GZqiqoREGNQYhINCRxKL6zf/Yeywz3Fy0i2/ZAMeK3n60+XRzFaW8Hgi4Blu3ICwJxzwBp5n06C2ftvZlLUy065rPZlKe+uupo5Y6Nn/TemkBRagD8aRp/xPtjxbdCyyXMrkcSDT9mR0L4+SuYZoY5Rt1tAW4RuRqp/SBrT889YKXubZkjugzu48eyqby5GhNRSKwP6C6CYgm/B/p7bW8ty1I7yVafxUYfyqenZeQ+YUUN+7bWVTwETgN+w06W2N37BXQiXGZbC7hS4utNULBVKG4QPFfWpJNjePg/X2pW5uVFUeOYV4A0b9n+x0Hbzl+S0fTe2Vxan1dSV/b/ALPSnh3XRhxHkKepxrn+1Komg4tf96HVbk/lR7e+vRG0XMTRN/SFR+0dE52uVhqtpUlX+iaH9h6UFNWUlYgkpKmGoQ/2oZFkA/19JJU/6/tXHLHKNUcgYfI9IJYZYW0yxsrf0hTqT7c6b697917r3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de6S25tvrncfW0JYxirRWjqEXXLQZCAH7LJ08RdVkeBrB1updQLH8eybc9tF2kihao9GPqHGA4FRXGGGCRSmejHbr/6GaKSuVNKfxIfiQniK+R8ugrpKObF7mxM2ZfHUE0lf99kcjFHKv3OWxuNlpP4RSUka6I1y1FP98vCkHyCzED2EbCD6PdYnuT4YiYlyQTkrw7cdwIIx/MU6FEzC5265S11yVQLGmMIXB1knJKMNB4+XAdDzDNFURRzwyJLDNGksUsbBkkjdQySIwJBR1Nwf6e5FR1kRZEYFGAII4EHgegOysjMjqQ6mhB4gjiOsnu3Wuve/de697917r3v3Xuvf77/ff19+60TQda1v86L4Vdvdr9vba+Q3TvXG5e44F6lXrHdO0NkxUmQzuB3LtrcuWzO3NyVu2o6yl3Fu3F1OE3nkY1XFJU1WPr6CneZDTyyAFZ3GylvHsY7hTdLgoONaEkfaBx6e+luEiWZoT4RFan0JoD+Z4dCN8Fv5c/yT3v1/1Xiv5hm5P4l0L1FBjMh0z8N5RtyTHLl8VWx1m3Nwd9V+0aSmpt6Uu2oYVOO21ka7OUw8iitMYimoZVUVnbxyyTrComc9zDz4cfn/ALHTTSyyBYnkJiWlFrwpX+XWwYBbgcAcAD8e1XXuve/de697917r3v3Xuqnu+fnXvrtTsbM/Ef8Al1UGI7Q72pHp8d2n31V08WX6G+LmMyEk1NV5rcWbCz4jevYuPSKX7DBU4q4fvYZEqEqZKSqx5rXyHVSTWi8fP5dKROkeqv5dPxn+R/yJz2czvbHe1d1hn9y9z/IXfs09d2J2/vGlxlTDt3DxI9RXUOy9qTZ+qo8biMHjfFQUFKlKkrTyQmpb1AoJ8+tgBan8z1q7/wAu3Eby7L+VHwy6wy1bns51yvc+F3nkKA4+jocBPuzorYFXu7HyQ1lPTxZCvTB7a23jI6lKgiJw2m0gKSlpSxbP2f7HVQoGkEYrXh5049b4vt/q/Xvfuvde9+691rL/AM9/bXaVD3T8X+x9n7Ezu9MY2wO0Nl4Cq29tHcu5qnbPYhyu38vjq1ztphIudlp5oavCQ1AliebF1T+CpVJIw1J5derQjBPHy+zpt+DHwC+UPf3x36z6I+T+Kznx++F+zd1Z3sfcPVlKK/aXd3yq3Xnd1LuzG0nbWuqfN7G6z2pLakgpGXGZisFPHMYEnjx2SobKDQV4f6uPVBUmmdI/nXP8utlPb+Gwm08LiNp7Sw+IwG3Ns4rH7ewG2Nu0FJjsLt7E4ukiosXi6Ghoo6eixeNx1FCkUNPEiJHEoVVsAPblP2dKxGugFhReOo4r8gPPoin80DpLe/eXwU7x2J1via3c++Xptnbxxm3sVCanMbnXrzsHau/MrgMFESZZs7ksVt2eKgSNXmmqzHHGjM4U6ckqQBj061PKzgoBRBSg+zP8+taD+Xz1Z/MP2zvPfUfxf6Y3D1puXtPbI2DubuPurrrcu1dldVbdgzUNfPn9sV+8/tFz254K6HxyUkeLz88bqLUf65YW1DjIHHqkRlq3hChOCT5f7PW058Qvhf138OusanbO16rK727E3nk23d3V3Jux3qt+dub/AK2Spq8juXcWQqamtqqfH09ZX1H8PxxqJ1o455Hklqa2orK2qeTB45Pn0/asInZNWD5nz6NHUJpJiYLqADSPe+nUPoxAAL2/s/193HGo4eXRjE1e8E0OAPX8uoMca2uQWGqy2ABvYWPP1diOf6e9npQ7tWlaGmf9Xp1mGNV45JfE5Okali1yOxJJAYgkKSeP8ffiRw6obwqyqHFPU0A/L16CHd+GytXi8hma8/YR0bxyUmHiZZnFOsywGoydQl0NU8TlljjOmMcEsSSKNUivl0mupJri3OtqRqaog8/mfU0/IfPpr66j1/xb8euiDEC7gET20f1e4sPr78lO7pzZ2AFx64P+Hj8uhX0Nb9En+p/U39b6Lav1X/P+x/w9uZ6N6r/EPX/Z6FX2x0DOve/de697917qLVsPEyaxEGVjLKxCrDAovNIzH0rZLgE2AJv+PdJMqVrSvE+g8+nYgdQYKSQcAeZ8h0UzfG5K3sfJrt3a0pg2biCEmqDripMrVRllFRNps9TQxj/MQkgTEGRhbT7KJWe7YQWwAt1FCfL7T/kH5/ZNPLu0W/Ktn+9d5TVvs4qiYLRqfIV+Fz+I/hHaM16Z6TYNCCPFDVZGeI6S/r8MjWvpigBCEr+AAx92TbYFoSpdh5nh+zowm5muWrrdIozmgpUfaePTlN17XJoJx9PTRnk21VLxggH91FQKpsfoCSPbxseGmJQOkic02xLUuWdv2A/YSf8AJ0x1HWUbzvPCTDKwu0kcqwk8ceFYj501/wCJ+gt7TvtSsSwJFfQ/4OjGPm9hGsUg1R1wCCf217T1wo5t97ePjxmfqJ6eNmtS5JYsnTj1AMhFUhmS4/1Lgj3QW95DiO5qno4DD7M9VuLbljdO+72pEmPGSGsbfb24P5jpX4/sJqeZRubb5pHDoUye16uVZh5ASDPQOUIAPq4c291KRswM1vokrhoDT+RPRFc8ph0J2fdfEWhrDeqKfYHFf5joXcJvjH1YSOg3Visi2rxCizDpj8grgahG0vpLOQQLlTz+fauOSVR+ndpIP4ZO1v2+v7egTuHL93b1a62aeIU1eJAC6U9aZoPz6Wy7ghisMjSVePvb95ozU0RubDRV04dP+SgvHt/60RnTcwvGfWlV/aOiE7c71NrOkv8ARB0t/vLU/lXp6gqaeqQS008U8Z5DxOrr/t1JsfaqOSOVdUbhl9R0ikilhYpLGVf0YU6ze79N9e9+691737r3Xvfuvde9+691737r3Xvfuvde9+691737r3Xvfuvde9+691737r3XvfuvdcWXUCLkEgi6mzC4sSp/DAfT/H3oioIr+zr3oafkegYqtp08lTHiJ8jXRVH3L5KHIRHSwztI8tXjZ2L6mEsNPLqve0o1oeB7jWWzks9xW2a6k1MGPiHNZBUrx89JqD9oHQ2XcjJbteR20ZjACmM+UbAK4xihIp8sHpc7Yr5RrxFbLqrqZNRGlVW6CMVKQ2WMmATSa4ri/icD+z7EHLe5mYS7dcSVuEqy18x5gcOBOPkR0R7vbKCl9AtLd8HP+8k8c0FD8x8+lh7FfRL1737r3Xvfuvde9+690yZOaR3FLFI8ShBJO8bFJG+pjhjcFWUtpLMV50i359hLmS+nBTb7W4eI6fElkT4gK0VQeILEEmmaD59GFlGgBuJEDGulA2R5VYjgacB8+kDtXHVQ3bWzU9bLUYfCY44pnkiVUkyNXOa2qp0bURNPT+l55v8AOF2CHgEeyvlO0c39xdxXBe0RDFqYZZiQxGriSprU8fXo93q5iO0wJJAEvJ5PFCgnCKNINPINwUcKCo6Fn3IPQQUUHz69791br3v3Xuve/de6ov7D767W/mf9wb2+KfxI3jW9c/D/AGBM+B+UXyy22Q+f7Cnlk0VPUXQmS1mjWjztPFLFUZpRNFV0TPVA/wANNHBuOh76gHHVKljQfD5n/V/q/l1bX0L8fOnvjJ1xiOqOj9jYfYeycQTOKDGRu9blsnJBT01Vntx5epebK7j3DXQ0kSzVtZNNUOkUaahHHGq2AA4DqwAAAHVVf8+fuifrv4eYPrfFyrHme8O1Np4OR1laOpots9f1I7NyuTplUEylc/tnEUTqbKY683P4NXNBTrx8vt6rO/kJdWTbu+WXZvcFbgailxXVXS0WMx8mWEtVUxbm7c3DTrhMvjqyamox4p9p7MzcQdEKSx1ZZTZjekYzXyHXvM+tP5H/AIrrbq9vdb697917r3v3Xuve/de697917rgsaIWKKqa2LvpAGp2td2sPUxt9ffutliaVJNMDrn791rrEAXL61XTfStiDqXg3b8ghvfurGgAoT8+u2QXDgDUBYlixAS92sOQT791qppp8ug+3fuGm22IqnJXWOrlljpYaWEyzzNGBIQTcRiTSQSxYBQR9fp7uGAAr0Ywz28UVSWLjy/1eXTXtbdWF3MtUUjqqWqpJI1emmEXkMU1xFUpKrOjLqQhgBq1f4H34MxrTq6XEkxIiGAKmv+x/xQ6C7sqqyOM3fUwUOSyNJEtBjZoEp62oiWNnhZHZUSQJdpIyTcfU+6HJJPHoukleRtTNn/Vw6GJKQ7p2NSVFUzvV1u2gSVFxLUfaG0snAvLJKAf8D9Pewe2nkeno7ho45IgAVbjXjkdBR1FeWtzMRjLP9nQzabFtLCaaN+B+fXb35Txzjq1o+jxO6gNK/wA+jF/w6l/5UYv815P1t/nb/wCb+v8AvPvetvXr31Mv/KQeNPLh69OnuvSPr3v3Xuve/de6L323u2WsqD17gZW+9yCRybjrYmNqDEg6zQalYMJa0A67EERkj+17L7pzI4toz3H4iPIf5vX9nmepL5I2VIYzzPuSf4tCxFpG3+iS/wAVPRPL1P2dRds7epaGlp6OGmKxDiKlS4aZ9IvUVTDkk/ULwqr9f6e1MMCRoERccaevzPSjd9zmuZ5biWarn4nPkP4V6Feix6UqoQgeskjCuyL9B9fDCv0WMD8/U/n2oHQMuLppmarUgBqAT/M+p6yVkuIwEDZLPV0NOgKtDT6x6nTlVWNLyVUrG3ABH+9+9M4UZNFHTUCX25yC02y3ZmIoz08j6ngo/n0G1ZvyTN1vjipKbF42MSO71UCyZOcIQkLarBadWc/QXaxtf2ysmpsYX18+hZb8trt1vrknea7NAAjUjFcnHFqdMmUpI545NETKVsVkKXbU4Dq4CcuT/vXvzqGqQPz6MrOZ42TU1anIB/z+nQcmierdUcLEz6rrL6FJVtJOtrAD6cA3J9oipc8AOhSJ1gUkVYD0z/LrnVbSjmhBgljmqDZpIJUMkUdySWSosJl+moXHH496e1qKq2fQ9ag3xo5D4iFYuAYGhP2jh8usUFdvHbba6LKZSlgC2Cw1X3sBAPpvBOsq+P8ABBA+vtuk8IBVjT5ZHVpbbYN2Gm4soXkrxK6G+eRTPT/R9rZSBg+Uw1NWyxoNVZhql8Dky2rUHlj0yUMx0g3BCgn2yxQtqMQEn8SEofzpUH9nRXcck2rjTZbg8cZP9ncKJU/I4cfz6EDFdzYyd4ohX+KVtIag3NCuMqBf6iDKUweiqCD6QWFmP5Hv3100Jw+pPSUU/Y61H7R0Fr/ke+gDu9nqjB/tbMmRftZDRl/ydCpQbyxNWiNUebH+RVZZalQ9C+q1vHkYDJRm9/7TKf8AD2tj3KAgGYGOvm3w/wC9Co/bToHzbPdRswiKyUNKKe7Hqho3+HpUxyRyoskTpJG4DI8bK6MD9CrKSrA/4ezBWVgGUgqeBHRWysjFXUhhgg4PXP3vqvXvfuvde9+691737r3Xvfuvde9+691737r3Xvfuvde9+691737r3XvfuvdJncmDTLY/JRK00UlbjZ6GSSmfx1KKwbxz08gKlKin1taxBIJAPsk3jb/qYZpYlrLo4UrUqdSn50NceYJHRjtt79LPBqAMYkDCvD5qfkf5HpKbWgpMHWY7HjyNBPSvRUs1TLLVVdNk8bTRxVmMqKyod5mSpgT7mMMbliwFwFHsm2Y28N9EzxqHmBAfzEgFGjr5KR3KPU9Gu6GW5tZ3Byh1kDAZHNVcAClVPaT9nnXoTwwJ0kjVYNb+qn6H/W9jT59BgEcOuXv3W+ve/de6xTzxU0MtRPIsUMEUk0sjmyRxRKXkkY/hUQEn3SSRIo3lkakagsxPkBkn8h1tUeR0jjUmRiFUDzJwAPn0GldBPuzJYo49hQmjVc/JU1UP3DUf3MBgxUBp1mTTU1K6pmViAioL3vYxzJZy8zbi8kDtAgUTF27ioI0xjTWgLgFyK4FOPQst5ItktLkXS+LrJt1RTpDaTqkbVQ4XCggZJ6X+KxlNiKGCgpQ3jh1s0kja5p5pXaWoqJpDy808zlmJ/r7HthZQbdaQ2duD4SClTxJ8yT5knPQXuruW/uZLiXifIYAAwFA8gB04+1nTXXvfuvde9+691WJ/OE7W3J1J8Cu2MrtbKZ3A5DdeU2N15W57behcxi9tbx3disdu8UdQ400c2Z2qKzGpMCkkT1qtE6ShHWrmi/PrR4HoW/5bfU21Om/g58Z9tbUo8PAuc6k2V2FuTIYWSOqpNwby7E29jt37nzq5BNRyMFVksq0dK5ZlioIYIY7QxRqu14Dry4Uf5Ojwe99b608P5x3fnX/yO7jrKYb4zGJ6/wCi6dOt+p8nS7ckyuzN/b2y+Znq/kH2FFn4MnBWnaexhtXG7Zpp6LHZJK7OUFYkMgijd/bTny8uq4qSTwHz6v2/lbdBZro/4l7FyG+sVU4ntbtygxXZO/8AG19JW0FZteGuwmOxuwuu4sXlJJ8lt2h6/wCv8fjqF8W7hKTJ/euscTTOguooM8etj/UPT/V/s9WM+7db6b6zLYrHsqV+SoKJ2tpSrrKenZr/AEIWaRCR7917rukyuLr5Gioclj62VE8jx0lZT1MiR3C62SGR2VNRAuRa/v3Xup/v3Xuve/de697917qDka+nxlFVV9XKkNNRwSVE8sjBVVI1LAXYga3PpUfUkgDn37r3QDUPdtX98rZLC08eKkkAb7OWVq+mjZuJWEtoqplU3ZAEJP0J96znrePLodEy+KqFiEOUoH+4VTDoq4NciuLqY08mok3+lve+vD5joGe7Uf7Xb0hctH97XRhQosjfbRnUXtqZm0Ee/enWyRpA091ePTd0pRpJW5+udQRT09BTKW5AeV6iUm3+q0pYe/A5I62GZVIBweP5f8X039zURg3Fj64CyV2KCFrEAy0c7hgP+Cxzr/rX96/LqvkOhs2URT7M24H/ABh6Q2/r+x5D/wAm+99eoegV6dqlXdWXhNozXY2peJRwA0Nekuhf8FjlP+wHuq/Lh17zJI8+jJ2b/H6f1/2F/p+u3/Ivduvfn59Zffutde9+690GnZe/E2djI6bHotZufMB6fCY5SGfXYiSvnj5IpaQc3PDsNP8AUhJdXHgqETM7fCo4/b/q8/z6FXKnLjb9eNJcN4e0QUa5mPADyQH+JuHyGege2bteShhfKZaoeqyuRmerramT92Wonk0u7u3JKK36V/JP+t71a2xiBaQ1kJqT0O993hLhlsrGIR2MK6I0XAUDGPt8z0OuGxXhTyMt6moUCQkXMcbNr8d/wG/tf1PH49reHEdRzf3uttAP6SnAHmeFfy8um7c+8aXbZfG42H+J7gkjBFOgPipEIur1LKCQoHIQcn6mw9tPIExxb06U7RsM+7hbq7k8HawaF/Nj5hf8p6RlDhazLucpnZfva0yBhNOCtNSI9jppYtWiy/jSAOPr72sZPfJk+Q8h9nQgub6CxQWW3J4dvSmlcs1P4jx/b+zrjkcXQsFFNoLotmqFRSXfVY6bgWUAX4/2/vzIGpTrdpd3ClvFqAT8NeA+fXGAzjUpiX0goJVZv0W0qWWxJIH4/wBt7utR9vW5RGSKOacaH9uOuMdEjyjVCJGN7h0HJv8AX6WGkj/b+9AD0r1t7hgho9BilOuNXjo3j0wjTPZ0QpwVZLHSwBGvSPwfz70yAjHHrcFy6uTIax4Jr8/T06Rsm3soZZCiOI9SkHWrX+l2IYk6QB9P6n2mML1PR8m6WgRQxGrporsJPrIqcctT6LJIbxOw+retDwyC/FzwB7aeH+JPz6XW24oFBiuylTUgZA9MHy6RuSwVLJGw8jQhgo8M8Znjt9bawvk1KT/j7Ry24P4qfI/5+hBablMrAhAxB+JTpP7OHTVS5HdGzmRMdkqmkpZGWRKditdiZwTbiCYaPWD+m6/63sukSW2I0khTxpwP5ZHT9xt2x8wBnurRWuBguvZKPtI40+w9Cltvs+qZ71NJV4udIwWnwreWhqJS1ystDIBAjlRrPpHHAv7dhZ6l4yUfz0Yr9qnt6A+78mNCKW9xHcRE/DONLgfJhUkVxx6GDb/ZjZAqjxQV4LKrCI/YZKJWcKZJKCo9Ey83HjYXH49rotwnQ0nQMvqO1v2HB/I9AXceWntDlXiby1dyH5Bxw/MdDD7Ougl10TYE/wBPfuvdM1fmqWhUmV1Wx/JA/wBcXP59+690lZuxsHC2l6qFSODqdfre319+691h/wBJmA/5Xaf/AKmL7917r3+kzAf8rtP/ANTF9+6917/SZgP+V2n/AOpi+/de69/pMwH/ACu0/wD1MX37r3Xv9JmA/wCV2n/6mL7917rr/Sbt8kj72nuLX/cXi/09+4Cvl1qvTRW9xbep6paJKmmEzRibzTy+OlVNWgL5FVi0pP44Fvz+PZTebn4Egt4Yw0xFasSFHyrQkn8qfPpdb2XjRGZz+nWmlct9tOFP9VOkbkd/4OvrgKqpCxQ5Cmq1jx8nietyVJ+9SeKYEtAkUTFZG48icGwt7Cr213f7gYphpiD62WIYZwMaScrpB4/4MdHKXUVjZmSEB5ShRdeaK2DUcDU8PTp1m7PWDHrFR5KmqchJWyyVbRtGzQQNeRoKYveMvHwDcWvcD3ItlERGgvCCQvH1qcV9T/h6B80rknwa6ifLgPkB1yi7ThgpY5K3Jp91JJOY4ZRTaRTkgRGoERCs4bkKDqsfr7UiOB3dUXs9a/4OmS06hSxOs1xTj9vTi3auNaiarpayE1CxN5aTyh0+4ViV06wXSGQ/05C2/p7Jd0gukjeWymbxUFQmKOAa0+R/wjoxspIXdBOP02NGP8NfP5jpGz9uwZbH5LGZ00opq+FoFahJjnpZQQArq8n7yh1DEcE8rYg+we9/fbhbXdjuMdI5VK1jqCp/bmh/zdCpLW1srq1vLGSssbBqSZDD9mMf5+lPhOxttYemd6jJrXZPLVBrayo8P20lROYo4o4oqQlmp4KWmiRI4yTYC55J9ibZbNLW3K+IWmkJkkkcaak+VPwgAUA/z9EW6XX1MypHFpt4gI0jU6qCpJJbgSSSSelSO0Nu3VTXUyyOuoRmVNXAF+L8lR9bfT2b0NK0x0XrQCnWT/SZgP8Aldp/+pi+9dW67HZeBY2FZAT/AISKT7917p8oN3Y6vYCGZGv9LMpv/trW9+690F/yW6G2r8p+iOxOjN211bicVvzDQ09LuDFBXym2Nw4nI0Wf2punGxu8STVm29zYqkrFhZ1SfwmJyEdveiKih4daPA049a8/TPdfz8/lMbX3V1l391rkO2uhthZSi/0dDDbX3jncFl9uZPLZJM7W9e96bVodwYHrTF4hWXJptrfWLpZ51lano6ihSP8AdpUoM8OtCvn+Q/P+WP8AVjpA97/zqu5vlRFUdNfHHq3dHW2A3Thc3DnazaH95+xO+910oosgINkbSXZe2JabrXIbveFKGTL0UWcqcfFWipp6immhJGi5JouB/P8A4vrRJpwr60qf8Hl8+hZ/lq/ypu4K/O7O7K+WtXv/AG31B0/unA7u6J+Pm66uClqNw7hxMlVuDFbv3jspc3uWDrjamAzuZnng26ZIcnksoZ5chHT0qmDJ7RfxHj1sivafhB4dbPXtzq3XvfuvdFL7YWNt8V5CrcUWMDmwJLfbX5/x0Ff9gPesZHXvTpjwUmZ2ulBvWhiQUKZGXFubjTU/tiWppJo9NxDNEDocHiVOLEe/EgZ690cqnmSpggqI7+OohjmjuLHRKiyJcfg6W97690GG9uyJNpZmkxkGNgyKPRCrrCatoJ4TJM8cMSgQyoCyRlvV+CP9jrr3U7b3Z+3868NPMtRh6qeUU8S16qKSapK6xTQV8ZNO05Q3CPoZh9Afe+vdMncuWFJgKTEJ/ncxWq0nP0paApUSEr9bPUGIf0+vv3Xug86lwAy24nyU8QejwcQmAdQyPkKgMlItj9TAgeT/AAYL7117oN8pDGmTycUaKoXJ18aAALpH3kyrYixFvevKp9et9GK7Yx2vZWOnjDN/CqvHsWOokQSwtRuzE+r9ciXJ97PXuBNePUHpFF/h24GsNTZCkVuPwlKSv+8sfe+veXULttp81JW0tGqtDs3HRZbJyaSXM2XlWnipUfkAw0cRnZfyCP6D3o9a8j+3oU8AUj2njFRGtT4GlGpraCy0KFgGv9QfqbW/Hvfp046FCAx49Fz2UtRt/d20a2pAWDPQF6d7+hqXJGpo1DH6B4541JvxYg/n3X06p0av76k832/mXzfd/YaLtf7r7H+J+H6fr+x/c/1vdutdTPfuvdIvfW9cfsbCS5WrQ1NS7CDHY6Nws9dVvxHGnDMI1JBdgDYf42Hti4nW3iMjZ8gPU9HvLuw3XMO4x2NudMfxSyngiDiT8/QeZ6Lzt/FZXL5abde6ZhNm68FyqpqhxdDKDLT42mQ2ETOkh1D9Sj6kkklJawu7/UXBrK3AfwinD5E9ShuN3ZWFjHsuzR6dvj8zxlcYaRj55GP83Q1YKg+4mDqh8VOQii1g85sSOeCkSEH/AANvZkKfl0ANyufCj0s3e2T8h/snrJuLdq4xZMVhbVWXZhFLLGnkSmZjbSq865ADwPoDzz9PdXcgUGW8h1TatkN4UvdwBSx+IKTQsPn8ukdicEmNmbJ5eRqvKT+eQQtK0jfuMLvVNchizfj/AIj6aSMqdT5fo9vNwN0gtLJNFmtAWoBwHBR9nT8HqayTQmok/piCftrpH6PH/YQA259udFxWGBSzU+bHj+3p8ptrVc5DzyRwIbekKWZR9SQpK3LX/Nhb37h59F029QxdsaFz/h6kPtCGNNT5Uxqt7l4IUjLFja7604vbi/vXTK77I7aVsaseFCSf2U6jSYF4xG6VtJPC1mQpJHEW0lRcF3Pksf8Aavr/AE92BHmOnk3RWLK9vIrjiKE/5MdIiuqYZ83S7Yo6paWrq6esq6muTxyvAtM2mNEkv4/LU1LKgN7AX59sySd6Qoe5gTX0HQhgjkj2+bd54dcKOkaxmoqWGSRxoq56TuH3JPQzti84jLXU7NFVXRo5RpJCyKrBPIjfX6A/kX9txSkdkgzwr0a321RXEYu9vatu4qlMjPl8ulZLLR1MLujRzSM6sqo4uOCDdOG/S3IsOf8AW9qKhs1zXomVJ4pACCqgUJP+fpN1+ERzeWMaC5ABjJdlIJa/AaNT/Z9syRA+X5dGttuDL8D91PXzr/P59BNu2D7MKkfiEEMEpKTMDYMQysQ3AuAPr9B+fZXeKwWgAK0OD0Ntkk+oJZtXiswyv8+hI6s68yM2zpc1URUzT7gm+7pcdXRskbY+GEwUFQsh8hiNTqaVfR6kKm/Pu+2W7pbs8iirngfQVp/MnoJ85c0Wqb8ljE7iK1Xw3ljNTrJ1OtMV04HHBqOk1uzZ2dwVVT5dkehixmQoKhljJaEU0dVE0s1NVD0tGq31Rsw9H492ubYkE/h9P8BH59Gmz75tu6QS2FRI80bqK8dRBoGXjU+RHn0cpWDKrKQVZQwI+hBFwR9eCPZr1BRBBIIz1hqWKQyMPqFJ/wBsCf8AiPfutdU5/wA1P5bb5+KXxb7b7h65pdu5HeeysbhqrBUG7aTJ1+3aifI7qwOEqUyVHhsxgMlPGlDk5WQRVcJEqqSSoKslu5mgt5JUA1CnHhkgeVOht7c8t2PN/OuwcublLKljdSMkjwFVkAEbuNJdXUGqjipx1pzVP/ChX5zZKQyy7W+PsRYk6YNpdkqg4vYeTtuVrf7E+yU7vcrWiJj5H/P1mdH91H27etd53r/nNbf9sfXOP+f183XBJ250PwfxtXsX/wC2qfbTb5dgE+HH+w/9BdGUX3RfbaTjve+flNa/9sfTlF/Pu+bD2vt7ovn+m1+w/wCl/wDn6Z9sNzBeLSkUX7G/6C6MY/uc+2T1rvu/f85rT/ti6cYv58fzUc2O3+jvr+Nsdg/4f17RP9fbB5lvgK+FDw9G/wCgujGL7l3tc9K79v8A/wA57T/th6nxfz2Pmg/1wPSI5A42zv8A/P8Ar9nH2nbmrcFpSGH9jf8AQfRjF9yP2peleYOYf+c9n/2wdT4/55/zMcEnBdKcH8ba39/9s0+0z84bmpoIIP8AeX/6D6MofuL+0kldXMXMf5T2X/bB1Li/njfMlyL4Tpf6Dgba33a9ib/8zKvf2mfnbdVqPp7fjT4X/wCtnRlH9wr2gcAnmTmX/sosvn/0j+s5/nYfL2pcNNgemXYcBjtvfWoDm4v/AKSOQbeyyfnTcZKF7G11eul6/wDVzo0t/uC+0A7RzTzOFPEfUWP/AHrupUH86b5eB4/9w/T50SiRb7d3v6W8eni3Yo40tb/W9pF553W3cMlrbVzxV/s/350Zj+759mZwNfM/M/5XNj9v/Ru6cE/nRfLsFnTE9QxsxOopt3eovzq5v2GQefdn9zt/AzaWZ+1ZP+tvSiP+7l9kWz/WrmofZc2H/es6kN/On+Xcg0vhunmH1s23N7EXUXHB7EI+vtOfdDmBD22ln/vMn/W3oxT+7d9jZNIbmrmulf8AlJ2//vWddJ/Oj+XQYMuH6gTgrZdu72AIAvz/AMZEuTc+2G91OYSChs7On+kl/wCt3S6L+7S9iWOr+tfNop5C62//AL1fXBv5zPy1eZZ2w3UJdbcHb29tJZf0sw/0h8sv/I/aJ/cnegyyfQWWoY+CT/rb0bxf3aXsWyNH/W7m4L8rrb/+9X1lT+c/8uVcMcR1Czk/5xtvb2Lc3FuOwwo+v9Pe/wDXX5iQkCzsj9qS/wDW7pVH/dgewUhFebucPyutu/71XXL/AIeh+XIa/wDB+oLgnn+7297/ANLn/jInJt703u9zMCP8Ssf94l/63dLYv7rL7vr8ecOcs+l3tv8A3qeuQ/nS/Lwf8unqE/4Hb29zb/W/4yJx7Zb3g5mB/wBwbH/eJf8Ard0Zxf3VX3em015y5zyf+Uvbf+9R1yH86z5fQsrrh+niR/qtu74I4t+P9Io9tt7xczAf7g2P+8S/9bujKH+6f+7rISG5z51/K72z/vUdW5fypv5mHefyi7H33tPtXHdf47G7XweByOIm2dityY6uqKzJZCspahMhJm927igmgSGmBQRRwsGuSxHHsce3/Pe781bne2e4W1skUcHiqYVcGupVzqkcUoT5Vr59YNfft+5x7Y/dg5b9vN45B33fry63e9ube5XeJrSVFWGKN1MYtrK0IYlzXUWFKUA62jto17V+OhmJvqRTf+t1v/vFvct9c1ulb7917rBDS0tOWNPTQQF/1mGGOIvb6aiirq+v59+691n9+691737r3XvfuvdE+7LlZ97Z52BvG1JGo/qsVDAFtf8Ar716nr3Sw3XQNTbX6/2NTaXyGUqKetqUC2cPOH1ysP6ieuf6/iM/096oAKeXW6dGHvT46hu7COloKS7u30jp6WH1Mf8ABY0v7t1rok2ezEudy+SzM5YGuqXlRWJJhpltHSwj8gRU6KLf1v718+vdL+TD/wAI25tnbtXBrzm79yYzMS07C8lBQU0kUVPGyclZ5Y30t9CNTg/p9+631j7dyJrN3GlDAxYvH01MArXAmqC9XPcAkBwsiA/63v3n1roUerqanweyWy9dJHTRV0tVlaiolOhY6OIeGFnJ+iiGDUP66v8AH34dbPRcsu0bZvJyRMXhky1VPC5R49cE9W88LmORVkTXDIDZgCL+9UqCPn17gR0ajsSqhp9l5JJRGfvkosdCJBqQTV1VTwI9h9TCGLj/ABX3brXQVbFy8uxKvdOEy9HVSZNmo2xmNgikkqMrWK01PFDQaUYSR1KyRv5BdVS5P0PvQPH1630IFNt6qi29k6LJFKnO7m+8q82YgrxtkK+FoIKOOUXKUuMj0olrDShP593HnUeXSu2QaXZqAaTk+WM48/TqdV10kGwKR6Ri1VV4WjxFLGiX15GshjoF0i4CGOoZi7G+lVJt9fdK49emE7iaip4jOf8AZ6wZTY+PzGPwOJp69qCu2vBQHHZCCGOcqaZYlZZIpGQVEUjwqxGoaW5/JHvdDxp15o3WJWK4J6h/3Kl+n95Mp5f4v9/5/t4PP/eb9X8eva1vsv8AJvtbfb/b8Wvz7tQfy6d8NaV0/wChauPz/wBQp0u9w7hxm2MTV5nLVCwUlJGXNz65X4CQxL9XkkchQB+T7ZkkSJGkkaigVPTu27bebtewWFjEXuJDQDyHqT6ADJ6KpDJl98ZwbwzkJjYiRdv4qQ6osTQBjorJ0IF6mQm6AfU8n8ey6NXuZFuZRj/Q19B6n/J+3qZHjseXduOx7dIGNQbqccZHp8C/0R59Cni8a07RUtOG9Xq1ty5c/rqJRfliw4ubfj2ZKABQdBC9uxGHmlpjFPKnko6VeSrTioVxWPcGdkVamcMP8nDAXjW1h5nJu7H9I/2FrE+XRHaW/wBc5vbpf0gexT+L5/YPIdIcZDFYwyrHUBpnZzUzxfv1U8jFiyiRbpEBzzckD8j3TUiVzU+dP9VOhGbW8uwhkiIjA7FPaoHkacT1Mo6moyRVMZh8rVo6F2rDTeOCzN47pUTWhkc6frqPAv78JQ1Aqn7emJkgta/VX8KOMaA1T65AyOl9jY8rjom8eCZneUEvJWUZmYaVXyMxI0Cw4UfT3evy6DV21lduC+5UAXgFan2fb8+sWU3TkKFP3MRXUUS38tXLSvUxJo5/b+1E0fNuCxA/w96Lgca063Z7LbXDUW+jkY/CisFJr66qH9nQS5rf+Tr8hR4jbmOXNZfIySLSx1858MUaANNUSQx2hjihFzdrWtz7TTXRUpHDHWRuFf8AUOhvYcs2dtaz326XZt7CIAu0YySeCgnJJ6aqih7kppizthZTo1mlWfHokKXPjVYWiFtdjYarm3tum5fhNfX4elsVzyHLHpVbgCtNZD1J8zWvl6069ttq/DT5fMbzwWWqcjkZKenD4ykSrkoqGlVjFFHFQu6x0lRKxkIFze1+fe4DIrSTXMbaz2inkB/IV/ydV3YW9+tjY7BuUCWUKlqTMVDuxySXpVlFB0pJcns7dgWkmyEVVPT2WOnrklxO4KUPbiCZ1Uzxqf1Lc8Dke1JaGcUY/Kpx/PosS033ZT46WxSN8l4iJIWp/EBWh+ePt6Ysvsio8d8dnalJI2OiKvpRM5OrVpNRSyRyArcclSbe2ZLZyDokz/SHRlY8wRBx9VtqFTxMTUHD+FgR/PoPa+Dd+Dp3Ez1dTTKHE7Y+trJbLp1PM8Uh85QXsdIOk8Wtz7QuLuFTqU6fMoSf9noTW0uxbjIpRUSX8IlRRnyFRiv28elX1/1tkt6z02d3MKiLayOlTSUk8zSVWe0k+ONtR81Lilt+5q0vL+lQBdvdIbWS6YPMT4FagEmpp5eoHr/L5E3M3NlpsMUu27PpbeCNDuoosPqR5NJnFMDiSTjo3CIkSJHGixxxqqRxooRERAFVEVQFVVUWAHAHs7AAAA4DqEmZmYsxJYmpJ4k9dSRRzRvFNGksTjS8ciLJG6n6q6MCrA/0I9+IBFCMdbV2Rg6MQ4yCMEfn1yACgKoCqoAVQAAABYAAcAAe99aJJJJOeotd/wABZv8Agjf70ffutda0f8+6V/8AZJu+49R0HFbc4/8AJ62sfaDcgPopvy/48OpV9kP+nqcnf813/wCrMvWj/wDCDr3Z/bnzK+I/VHYWI/vBsHs75N9C9e74wP8AEMpif43s/enaW1Nt7mxH8Uwlbjc1jf4lhclPD9xR1NPVQ69cUiSBWAchRZLiJHFVZwCPkT10j5w3G82fkvnDdtum8PcLXa7u4gkoraZI4HdG0sGVtLKDQgg8CCOtvfoj+Tf/AC7Ozvnh/N3+Pm5en59u9ZfHnb3w6g6OrKXtbtqCp6cqO5fjtund+/t1U2UyXYE396ZzumjhyiJuZ8vQ0zU4iWJKVpIWMht9pJNuMTLpRFXS1T21UknJzQ5zjrFPfPe33L2fkD2Z5js95Eu6blLuJv1NvbkXItryOOGMqsP6Y8MlP0tDGtalqHqvDeH8qbrn44fypv5j/YHe/WKVvy/+LXy6291PsHtmm3P2FjcVUdbZfPfEoYfNYHZ8e46HZWZwO8trdq5OspajI4meuiiygVnjmp41gLGso022+kmj/wAbil0VqcZTyxUEGoJHAg9TBtXvJuvNHvN7V7Xy5u5XkfeNkkvbmyMcDN46puWpXl0NKrxSW6KwVwpKcCGNbXPlx/LW+CHxw7KwmyOqf5J/ffyp29ldj4zdVZ2H1b8iPkPSbew2ars/uXEVGzKyKs7MyMjZnHUOCpq6Rg4UwZGIaQQSbbnb21lMkUGwyToU1FlaagNSKdqOK4rx8+HUU8g+7vuXzXtFxuO8/eJ2vY7pLloFtb2xsS7oqRuJRS3XsZnKjHFD1Vbt74hfAP4LfEnoX5T/AD56p7X737F+WlduLcPUPxy2vvjLdb4Da3WtAlFW0mX3DuPC5bB7oyFZT4DcmIrmnjrmikkyVLCsDxiaocPx29vZ2VlfbhE80swJjiB0JpFBqZgpapqGUCmCMcesgH5/91/c7n3mjkb2q36w2raNhSOLcN4nhS4eS4aoKRxurxqC8ci0K1ARm1A6VAD/AMxT4O/Hzrn4+fGv53/DDI77f4xfJefKbbk2f2JPFldxdZdi4c5xJ9tSZ6lEsdbBPU7SzdKYppqiaKpw8zJUTxSL4kG5WCRW9nuFqZDZTahSQDUjqaFSQACDQ6ccATnqRvZL3R5u3nnDnX2p9yYbQc77Kqzi4swVjubd9FJPDPAgSxNUAAiRQVUjMP8Ak9/DfrH5g9rd50PY+zM72vVdP9Abp7S6+6VxW663r3Hdw9gYysoaHbmxNwdhULU1VtjGZqsqlpy0FVSVP7xnWURU04KTabFNwvJ4XQu0cEk6RA6fEdCoVCfJW1ZpQ+hHR39473O3/wBs+W+UJdj3SHbo9z3iLb73dZIVuWsrdlYyXEdu1RKyKCaMrLjTSrr0E/8AMj6n+NfTPyQj2b8YMlFPtVOudkZLsLbeO31T9pba637lyFJWT77612p2XTSTDfGG2oho1atkkeVayWeFyDEACTdY7OK5CWUmpNCs41K4RyoLIrriRVONXrUZpUyH7Acyc+c08jndPcCAjcDfTx2M725tJbqxVlFvdTWpA8B5u/tAA0hWHHq2H+TR0t/LP+bdbQ/HHtP4cZ/Md37C6f3T2Zvrueq7x7dxGD3ocX2Ltnb1JR0WzNo7+wOPws8OM37RRBoo0jYUDsyl5dXs/wCUbPZt4mbbb/Zw1wkbym48aQav1AFXw10haK4Fan4a+fWP/wB6rm/7wvs9by8/8te68EPKF7usO3WW0rt9lJJBrtZZSzTz20jSAtbOckkawAaDr3QfSX8t/wCZXSn8zLujqj4h5zp/H/Gf4g4XcnWeCz/dfbO7KzBdwJtP5V7rym/oqt99mHL01fBtTbEK43JLWUEbYdmWACpqRMm26y2Hetv5nvY9l8D6W0DRL40klH0zsXqSta6VGkgjt+Z6OOdOc/vCe0XOP3ceUOZ/dWHdZ+Y+bJLbcZoNvsYVlsDPssCWpX6asZUz3J8SMo5EwBbsTSHOzPih8EPhh8OPj18ofnjsPs/vzsn5V09XubqzpHZu7q/r3AYzYNNS4vKJm8xmMRldu5+oMm3tw42tkqI6pkaTJ0sEcGkS1JI02zatm2rbt3321nuLm7LNb2qt4SeGhA1SSAF6sGDLp4ggU4t0Mdz90/fT3j93+ffbL2L33bNh5e5XYW2571eQJdyvdFnTw445I5oh+rFIgUqDSJ3LVonQ+fBb4gfyovl387Mns/qPCdmdndG1XxHz3aeb6t7Lye+9m1/Vfa1L2L07habG0O9tn7q25nd1Ciwe7a+mqYHnrMfBU6mjqq0NE9Ov5W2blfeuY7i2hiuJtt+jM3h3B0MkviICoaJlLBQxHCmeLYPQS97/AHg+9Z7RexNtvHNd7tu188JzdFtcG67alrcLfWLWe4SM7W1xBNFBqlt42VgqSMtAY4qMHKV8rPi18YPgL8O9gdbdxbFpex/5jPeGNg37kPJvHfeLx/xp2DlvHHQ0Vdgdsbrxu09xbkjkoJaaFa+lq0lyDVkh10lLTCpDm77bZbFs9tZ3lvr5luCJ3qWAtYjTShAIVpXoagg6amvBC82+0Xun7pe//vLzBzLybvz7b93DY5TYR0t7V33m6jyzLLPA9xDCQ4ZjG6ER+EopJI5S5j5P/wAub4QdDdgYfaHW38n7vD5K4LI7Px+5arffWnf3dlHgcTlqzNbgxc+0quLKdrSTtlqCjw8FZIynQYa+IAXB9jTmXY9l2W/itbD28uL+FohIZoZrugYsy6DoWUVAUHiDkY8zhz7UfeV99ufuX7zeeZfvmbDyvfxXr2qWG6bTtjSyRrHDILhTHYU8NmkZB56o2+XRP/hD1B/Kj+RXxu+UHYe5/gdu2k3f8HukMFvPtmbIfIHuWGo7R3Jj9h9j5zc0uCo8L2VRYrbM2TyfVNaREYvt4Wro1RQkZHsj5TtOVd52Dd7275YDXW3WSSu4uZ/8Ybw5GY0GkRajHWgDAauGMzj7586/e/8AbT3O9puWto+8JZPs3P2/S2OziPaNtIsIXu7KKAStLYtJOETcI811N4bEmrdAL/L5+H3wu/mCfJb5Y7/2n0zvHbHSXUHX+xt0dS/D2g7Wr03hvnP5DbM2OzGNqOz90biXJR4mv3jtKpLSz5iijpZ9xUavVQU8JAJOXNj2rmzed1ngsTDbW9v48O1xTVeVlAXR48q4jZx3E6SpkUAgA9Sr95D3u99vu1+1Pszy7vHPNjdc+73ud3abzztJt6G2tIUnDxOthBDoMiW1wtFWCQutrKRG7uCSqfzRukPjn0xVdUw9RfFT5N/E/fm4U3PUdg7C7rydTnthUtLj56GDEL1tu2uq91S74E000zTVtPnJYYIY40kp1mkLKGeZ7ewtrqBLXZL/AG+4ZGaa3vKFB3KF+nYqsskY7gzvxNAvAkzv9zv3A90efI+cpOdvePlLnPly1Nuu2bjsEYhvGZ1cy/XWyLbi0oAumNrcMzFirlFAIm/yPpHj7q7OKEgnAbSB/wBY5PLex17Miu+7p/zyf9ZE6xe/vfP+VI9kv+lpf/8AVi363putCWwNGT9TBGf9iV95H9cJuhJ9+691737r3Xvfuvde9+691737r3RUd+09O3ZVVFVzJT0ctVhXq6iS/jhpmpqV6iRwASVEangcn3U0630Jm04F3dvHKb5aNxiMcgw+3BKpUyGKLx1NYkbAGNAJHAFgQ0hH1U22M58uveXTl2fuqgxGEq8LqE+UzFLJTx0yOL01NKCklZVWuY4gLhAeZG4HAYjxPl1rouu14lfPYy+Lq80IZjULi6JUaaskp42kgRmktHHTpOqtK7elUU+/Hy690OdXS1GBOQ7I3saaTNQ04pcFhKaQy0eLaRZEpaVZyV+7rJGkYu6gKil2FzYr6ma9e6BbN7b3PBBT5zK0VVMM8j5CWqjimmaGeqdpDHXKiFqWZ0YOgPGggXupA91voWqdqzf1Xi8DjqGsx/X2DFGa6oqoJKWTOPQJGYKPxtpPg8qLdATxd3N9Cj3Wug/7Vx/8P3hkJAhWLIUtNkYjawZjF9vOV/4LNTn/AFr+9EcetjoSuwatstS9eYaBgWzmUxldIt+fDDFTkMfp6Sao/wCHF/x7t1roaGRCwk0KZUVgr6AzqD9VVragG/p7917r0caIWcIqvJYyMPqzAW5txce/V6sWYgKWJUcOmp8NRRCR4V8J80tWuppJYqeaYlqmSmhdjHTvOSSxQDkm31N9g0NerwvokB018qfb11A0VJC1ZOLyPxCb2d0/sqqH9JP1J/2Puxqxp0pcPPIII/hGT6A+Zr1G/i0l7+D/AHZr/Qbfp06L2vqt/a+t+LW970fPp36JaU8Xypx/n/sf5eiwVmVyvY+Rp8xmI/tsJTzyPt/CMG1VbB9MVfkIjcGMAXjX6XJNyOSRJrvis0q0twaop/EfU/IdS5bWFnyrayWVk/ibm6gXVyOCCmY4z6+p/wCK6ErG4wo0VPCplqZCCW4AbXe/NvTGluB+PZsqBft6C13eBg8rnTCP9X7T0s66so9q45kWRFyEyKpcL5TEfoqqACzSAsQq/W/J92JVRU9B+3gn3q6DMp+lU1A4V+35evQbRw5LcU4oKBJSzF3qCGJbSxN3rKz6BCzXNuGbgX+ntkkuABw6FryWm1xm5uWFAAF+3+gv+qny6E/BbAxeOSObJJFlK5bH1ofsYSNNlhpnusmkj9UlyfwB9Pd1jApXJ6CG5cyXl2zJas0Nv8j3H7WHD7B/PpfKqooVVCqoCqqgBVAFgABYAAe3Og4SSSSc9d+/da697917pEZzC4ClyFPnlxlJBmNElO2SgjEVT9kql54maPSJPISFuwJF7A+6CJNfiae8Dj/scPz6P9vv9ymtn203btY1DiJjVdfAGh4U49MtPC9fJJKHIgeXU8tgPWRbxRva+lLW4+g9vY4DowlkFqippBkAoF/yn7en6lpYoDppke7g65FBd3APA1Lcn68X9+oM16LZ5mkBMzCg4A0A6bs/svG7npPBkMf4py6yw5KFYYK+inQ/tzxzgB30/Qo2pWXgj2zLFHKKEd3qOlG28wXW0XHiWt1VODRNUowPEEcB9oyD0Do3BnuvM0u3dzrFk6GSJaqHIKrt56LymFayNmjMnkhI0zREsY7ggkFSUwmeB9Eo1J69D0bbtvNO3nddo1Q3AbQ8R8npXSc0zxU4r9oPQu0x2xm4CzwxBvC1Sk9HKFk8OnV5ImRmjdWuLH8/ke1lVamk4pX/AIroDTDeNvkARz8WgrIKivoaio6jYpqjEVsUWL81VBUan/hv7ZknjJF5HsUgp5Iw1/JcK30b68aKBaUx8h59PXixXsDvd6UkXHi5oD6DzYH04jy6FIfQXFv8P6f4cce99BDr3v3Xuve/de6iV3/AWb/gjf70ffuvda0H8+8H/ZKe+zY2/hW3Of8Ayedre0O5f7hTfl/x4dSr7If9PU5O/wCeh/8AqzL1pBfCDsLZ/UfzK+I/a/YWX/u/sHrH5N9C9hb4z38PymW/gmz9l9pbU3JubL/wvCUWSzWS/huFxs8329HTVFVNo0RRvIVUhuF1juInc0VXBJ+QPXSPnDbrzeOS+cNp26HxNwutru7eCOqrqkkgdEXUxVV1MwFSQBxJA62hd0fzT/gzW9t/z/t3YXvmX+G/NP42dKbF+LOVg627lpJ+xt7bO+HHZHVubx0KP1/DXbHlxfYOeo6JarPpiKeQy+eKV6dHmVdJeWpO7EydssYVMHPYRThjJ8+sctv9pefhtP3dLSXl4eJsW63Nxuyme2Ihik3KCdW/tqS6oUZqR6zjSRqIHSH7y/nMdM/LX+SF2L8eO49+TUHzhr4OpdnVm2ptqb5yD9tQ9bdy9R7kbtCbelDtiq2Rj8jm9j7dnmyEOQytNUvkqCoEUWiakSRHJuKTbRLbTv8A41UKOJLAFTqJzmmDU5Ir5gdCTlf2J3/kz7we080bFtob29Q3M4lEkK/TGe1uY/pxEZBKyrNIApRCoVlqahiAl/nM/wA2rL9x/KTYW5v5fXzU77xPTFD0HtbBbmpurd6d+dGbefs6m7E7RyGanrNpZOPr6fI5ltqZTCrJkRRSpNAsUInY05jjTbxujS3CPYXkgh8Oh0llFat5YzSnQz+7x7G22xcm7nZ+6Xt5tcm/tukkkJvYbK8f6cwW6oBKvjhU8RZKJqFDU6e6pgbL+YPwP+dvw2+OXxb/AJhXZvavx87V+JiZTb3V3yC2rs3Kdobfz/X9bQ42gTAbiwuExm4d0Q1z4XbWJoHVKQp5cZTVIqQrzwKVC4try1tLK+meJ4dQimA1poNDpZAQ1RQBaVoAPn0cXXt/7p+1/uHzdzx7SbJY7vse/aZb7aZ5ltpEnBZtcbu0cRUPJI+WrR2XTUK3QK/zFPnF8fOxvj58a/gh8MMdvtPjF8aJ8puSTeHYkEWK3F2b2LmDnHn3LJgaUxR0UEFTu3N1Rlmhp5panMTKlPBFGvlLdyv0lt7Pb7USCyh1GshGp3Y1LEAkACp054EjHUheyXtdzds3OHOvut7kzWh533pVgFvZktHbW6aKR+IeJIiiWgJAEaksxODW/wArr+YB8eejPijj+ltxfIvc/wAM+4NkfKGl+QFV2Pieldx9zbO772NT7SO3p+m+wMFsmvxuerMZk4Z5o2jqp6WCjkp6Oqp6kTK4ittW4w2trLAb57a5FyLgSqhdXVU0iFgrqSC1TQ9ueIOQEvfb2b505t9wJeaLLkm35o5au+Xzsy2Ml9FZTbfOZfEF7byTq0auhANVDFgZEZaEVaf5vny0+E/yc6t6dPw03ftrbOPo+0O1Ow+0ukavpze2yd+VO/8Af09NBP2dUbxlwdZsDI0GWpcMzS46kysc0Qq4JGjkfyQ0JZzFdbRdpZTbSgiQvK8sBQq4dytXLAshVggoFbtxjJCiX7rntt7r8gcycz/66O13E8z7faWO3bst7BPbi2twSLUQCRbhWQvh2jIOlgCBRpAy/kXfLDoD4d/LTsPsz5G7+/0dbIzvx13ZsTFZv+629d3fdbryfZPUW4KHFfw3Ym3Nz5eDz4jbFdN55KdKZfBoaQO8avTk/dLDaN2uLncJ/DhaBkDaWbuLxkCigngD8uhr98T2x5491/a7YeXeQdk+v3mHfoL2SHxreCkKWl7Ez67mWFDR5kGkMWNagUBIn/yzPld0F8ffiZ/NN6z7e37/AHR3v8jvjxT7F6Zwn91t6Z7++W6o+tfkPgHxf8S2xtzNYjb1svvrFQ+fK1FDTf5Vq8miKZo0fLm7bft+0c0215caJ7m28OFdLHU2iYUqoIGWHGgz9vRp94f2v565890fuy8x8qbH9Xs3L2/m+3ibxreL6eD6zapdeiaWN5ey2lOmJXbtpSrKCL2zPlf8EPmf8OPj18Xvnjvzs/oPsn4qU9Xtnqzu7Zu0a/sLAZPYNTS4vFphMxh8RitxZ+nMe3tvY2ikp46VUWTGUs8c+ky0wRpue1bztW3bRvt1Pb3NoWW3ulXxU8NyDpkjBD1UKFXTwABrxXol3P2s99PZz3f599zfYvYts37l7mhhc7nst5OlpKl0Gd/EjkkkhiP6ssjhixNJXQrWj9Dz8FPmB/Kl+Ivzvy+8OpM12Z1f0VR/EfOdV5jtLszF763lkO1+16rsTp3Nw5ag2Xs7bO5c7tWOuwe1K6epmkpqGhmqldY6WjUQLUL+Vt55X2XmO4uYZp4dt+iMOu4Bdnl8RCW0xqxUMFrxpjgvDoJ++Hs/96v3c9iLXZ+a7Lbd055fm6LdYdr217W3SxsVtNwjKNc3E0MU5WWeNVUM7qtCZJDqKFr+QvzE+On8wj4N4DKfJ/smj2F/MO+P1TlcVsncrde7sqsd8gdgzzR5NdvZjKdf7MyO3Nt1k61Ui0ormpIKXL0pmVoqfJVbxEO57tacwbEk263VOZ7Q6I5Ch/xmEmoRii6VeMk6S2D61kYpLntt7Oe5P3effXcLX2u5ZfcPu7cwqkt9bfV26vtN0Bo8aNLu5SaZRpGrww7PC+khngjDWk/MD5v/AAF+UHZmC39sf+cf8ofjDicRsbGbPqNgdJ7F+Vm3dq5fI0G4NzZqXd+QosRs/BU0u4MhTbghopZWhZ2psfApchVVRjzJv2zbzfRXO3+4dxYwrEIzDFDdEFgzHX2tGKkMBwrjj5DGT2W9ivvCe1nLF9y/vn3K+VOa7ua/e9XcN9uthmnjR4oIhbo0lzKwhRoS4GoDVI5pkk1I/wAu75YfHvoL41fzY+t+0+zanEbt+SHRtRsjpGKs2tvnPVfYu4l2D8jMCkdVksBtvL0G3qmsye+sSHnzE1BDqrCxfTFM0YI5P3rbdq2Hm+z3C4EV1d2QigQKxDP4c6lQVVgtC6jJAzxwes0fvHez3uT7i+6P3O+Z+UuVEm2flfmBb/fzHPaQrZQ/WbNKSqTTxvMqpaTUWBZGolKVZAxff5bXY3xN6z3z2Bmvkb218i+ht3Vm2qDH9OdzfH6ryNJV9fZf+Iioz9buKDCS12Vz1LlaWKnp/sJMXX0MtL9yJAk7U0sQW2STaoryV90vL22fw6W1xYkBo5CfjbKvp0jSQh1EMwxhhLn3oOV/eXmzl7lmw9r+TOV+Y9kS7aTfNi5lVGW8j0aYVhMoSOFo2LN4gmjkD+HSqCRWOb/Nj/mCdE/IT43fH34xdU9qb4+UG5Ord6129d4fJvsXYrbCzu4FTE7kw+PwVBi6jDbZrmhrafcqCreTHQM6YejaSSonaaUnvOHMtruW17PsUFzJfS2hdpNzuE0PJqOFjBZnCUPdr7joQ1J1HqIPuVfdo9xfbL3W9y/dvnLk/b+Udq3fb02+x5S2u7+shhrJBK8zyLLOlUMB0AStQzyhVRAq9Bd/JLWM9z9mtKJGRMBtQlI7nUDk8qCSAQSEBv7EHsuCd+3QDj9J/wBZE6i/+9+0jkj2RLf9HPcP+rFv1vMda5L+H4THw5JwsMqwwU1dwELOl40qQCTET9NZshJF7E+8kigcakGeJH+brhSO4Ejh5j0/2Ohk9tde697917r3v3Xuve/de697917ot27cAdx9rDD+QwR1lJQz1Uy/rSlp6NmqPFcECZ0i0IfoGN/x7qRnj1voRN07uwvX+Jp8NiYqd8mlOlPi8TESy06EWWprQhMojuS1jeSdzx9WYb+zr329BFTbA3VuCjzO5syaiGpekqK6miqk/wByOUqkTXGppiF+ypBGpEakBraQqgc+/fOnXupXTb0i7kr56iaOJo8HNJTmV1jUp9xA9U2pyAPFCgJ/otyeB79jj17pXpWL2VvenjiRqjaG1GapZ2U/b5LJkFYXe66ZEaQXRGveFGaw8lvfuPWuhx97691737r3QU9p7Oq9x0FJkMVCKjJ4vyq1MCqyVtBMFaWKIsQrTwSIHRTbUCwBuQD7r3SW2RhNyZTPYPKZ/GVONoNo4cY6iFZFJDNWVCiaOKRYpDrZ1WYl2A0AooHPvX5de6H76j6fX8H/AIkf19769137917riwJFgFN+Dq+lv9b8+/dbBoa9RpoFqNMMsV0VbiZSEKPcWWNeSLgcn/Ye9gkcD04khjq6t3V+H5fPrH/DKT/jmfr9NTW0/wCo+v6b8/6/vetvXpz6ub1H7B0CmHwzB4YI4vJUkAalHARgFKJcftwoLCw/1/bSJpHD8+h9fX40vKzaYhmn86n1J6XVW9FtihZh4zXvGQ0wAdg3BKx39QCn+n1bj6+3MAEnh0HIBPu9yAai2Bwvl+fQfY7F5TeGTlLSvHSxuDVVTAsKNGUftU4a6tWzKxvc8A3PAALBq5/1Y6E11d2ex2aBUBlI7EH4jXi3og/1ZqQOONxWPxFOtLj6WKnjVUViijyzFBYSTy28k0n+1MSfboAUUA6j66vLm9lMtzMzvXFeAr5AcAPkOnD3vpN1737r3XvfuvdeJABJNgOSTwAB9ST7917oB90bwoabKCXKSV7RMGfH4qgoKrIVDUcTaUq6qKABaWKokXUCxuRb8e2JLiOIqHqWOQBxp/LqQ9n2S5ltCtnHHrrSSaV1RQx/Cpb4iB11R9u7GpqcxSPkIp40YSCuw09FSxnn0KraqcBf635+v9B7bW/hJo2pftA/yE9WueSOZJZPEWOIxk1Hhyq7H5+vTtj+wqfMsyYGaKqKAM0CNacIR6WFPGmqOJgPTwefb6TRS4iIJ6RXPLD2ADblEyA4DHhX7SaEjp+GeysId6qmdI10soM/icqbkC1S/Or6829u1HE9FzbbZvpEMoLEEGgrw/0o8ukb2JVQ7h25SsUp46mjzWO11MrwLJSUVVOIcgTOmtUjaFgWsdJIF/oPaa5VWVfTVQn0B6PeVoZNq3aWjMYZIHogrRmUVTGKmvD86dIwSUmKxdTVYquo8hBSqkMNKKpC8hUFI6ani1GUjUdUpAAsD7oXjjQmJgwHAV4/5ft6EGie8vIory3kilclmfSaCuSzHh/pehL6dys+Rw2UgrQJq3G5SSB65ogktRBVotdDEzEeR0ozMYluT6UA/Hv1pIzq4c1cHj9vQT56so7TcLSSDtt5oQwjBqAV7CacAWoCfmehf9q+gP1737r3XvfuvdRqsaqeQfW6kf7wffuvdUXfzg/jl2L8gvib3J1z1bhIs7vnc+MwkOAxk+QocVBVz0W79v5SrSTI5OeloaYR4+hmcGR1DFdIuSAUd9E89tJHGtXNKDh5g+f2dD72v37beWOfeXN93iYx7bbSu0rqpYgGJ1FFUEnLDgOtI6f+UB89cbJ4avqTHRyKSGC762dKAQLH1R5h1+v+PsPtt18dVLc/tX/oLrOuP7yPtOla7zcf9k0//QHWZP5TXzjiVjJ1ZjlFxyd6bUt/S3GUPPtPJtt8FNben+2T/oLo0g+837RLx3q5/wCyWf8A6A6dof5UXzeAF+rqAcA/8fjtc3BFuLZMn8e2X2jcjSlqf96T/oLoyi+9N7NrWu+XP/ZLP/0B05w/yrPmunqbrHHgA8/7/DbP+H/Vx/oPaZtk3XT/ALiHh/En/QXRnF97D2WWld9uuP8AyiT/APQHU6D+V38zF1X62x9lILH+9u3SB/QXFdYk+0b7HuxpSzP+9R/9B9G0X3tvZNQNW+3f/ZJcf9AdOsP8r35lhST1tQC54vuvb4P+2Ndf2nflve2NRY/8bj/6D6MoPvh+xaE6uYLv/sjuP+gOnKL+WB8yEALdcUA4H/MVYA/g/wBK0j2jflbfm4WB41+OP/oPo1i++d7CqADzDef9kdx/0B04J/LL+YMZu/XdAATYf7+nAm5seOKz6+0T8ocxGlNv/wCNx/8AQfRnD99X2ABFeYrz/siuf+gOp0X8tH5eKVJ69oLcH/j58J/qQP8Ala9pX5L5mY1G2/8AVSL/AKD6NIvvv/d8QCvMV7/2RXH/AEB1PT+Wx8uALHr+gv8AX/j5sL/h/Sp9o35F5pIxtn/VSL/rZ0ZJ9+r7uyAauY77/shuf+gOu2/lt/LWLl9g0ABJX/j5cMeSDxxUf4e07ch81mhG1f8AVWH/AK2dGUP38fu5VX/kSX/r/uDc/wDQHXFf5cHyxFv9+HQcE/8AMSYj8i3/AB3v7YPt/wA2nI2r/qrD/wBbOjKL7/H3b0qDzJuH/ZBc/wDQHWX/AIbh+WHH+/Ex/PN/7x4m3+x/e9tv7fc3kY2j/qrD/wBbOl8X94B92pK6uZNw/wCyC5/6A64j+XL8rBIqf3Hx2o3YW3HiiCEF2/3b+B7TH285wLADaMnh+rD/ANbOjSP+8I+7NGutuZNx0jj/ALr7n/oDrk38uP5W3v8A3HxvPIH948Xc/ngeXk+6N7cc6E42b/qtB/1t6Ww/3i33X1pXmXc/+5dc/wDQHXf/AA3D8rgyqdkYwF/0A7jxnq/rpHkubfn2ll9uec1oTsuP+a0H/W3o1i/vHfutoATzLuZAOabdc/8AQPXKX+W18sFUO2yMWqA2LnceN0r+PUdRt9PdB7bc6yfBslf+b1v/ANbejCH+8s+6nESW5m3T8tuuf+gerd/5S/wx7y6M7Q39meytu4rGQbiwG36bbpps5j8oauux+QrKmogeKklZoz9vUAjVwTcfUW9yX7Xcn8w8v7tuF1vO3mC3e38NT4kbEtrU0pG7EYHE9c/P7wv70/s594jlb2y27203a7ubra7+6mvFubWa3CpNFEiFTIoDdyEEDh1tfbLxdU2LTI5akkTwYytj+xqBJpYR05AlelkbQiJKALKLsSDa/udCwRAkRGWGeuV8kixlkVqggkkf6s/5Ohd27k67IUzpkqD7CspVpRIquHhlFRSxzo8RvqWwaxU8gj2R2d3PcS3sVxAEkik0gg1VlIqrA/Yellxbxwx2skUupJE1UIoVINCD+fSh9r+kvXvfuvde9+691737r3QE71xEtR2Xt5YcjW4g5vFy0yZLHyGGqhqKNasmOKRWQnyoyBhflTb+nvRr69b6D6pXP9a7r+5qkpsnO6mdampi80eWpWca5Ip5lkqKOujcWZg2pW+pdG5917o1GLyNPl8bQ5SlJ+3r6WGqiDW1Ks0YfQ9rjWhNjbi497610zT7J2lU1H3Mu38YZblm0U6wxyMxLM0sEOiCZnLHUWUlr8+9U63Xp9oqChxsP22OoqSgpwzOKeipoaWHW1tT+KBI01NYXNrm3vfWupfv3Xuve/de697917r3v3Xuve/de697917rgzEMv00m4+jFtR/SBYEAWBuT791YAEH165G/H1+vNv8Aif8AD37qvXfv3XukoIaTb1HJMWDVMiqC5F2PFgi3/Sosf9f3vj9nRuZJ91uFSlIQeH+U/PoNpY67dWUjpKRmRGYu81rxUtMps1S4/N72jU/qc3/xDbEuaAY6FqNb7NZNNOAWpQL5s38I/wAp8h0MmLxlJiKKCgoo9EMK2LHmSaQ/5yeZ/rJNK3LH/bWFh7sBQUHQEvLua+uJLm4asjHy4AeQA8gPLpw976Tde9+691737r3XvfuvddMoZSrC6sCpH9QRYj/Yj37rYJBBByOg5ym2pklkangmqFkkaRJoyJJlQ2Pgm1OkhUEC1rgj+nveAPn5noUWe6oyIssgUgUKnAr6jBFekZkNkZrKlUgoKCkHku9VWQ+SR4l/Si08QOkhjzqPI9sSxeJSir9p9P59HtrzFYWdTJcyvjCRmgB9Sx/ydRpOnqajV8s0mWmq4EeRqXb1SuFnnuDrhpmjlDhX+pBkBINgL2HtkWcanXU6h/CAP8NenV56uJytkEgW3Y0D3S+KF9C1RTH2dI6bb81dLHPR4FIFHqV6nI1uUyC2a1pKqtmdUqFP10oSDx+PbYgJaqx0+dSf9jo/Tco4EeO43MufMIiRp+SoB2/aelHJt/M1VN9rUZVqOGaHxyQOscpkisLh6SGIyyLcf0DX9vmGRloZCFIzXoqTc9vhl8aKyDyK1QwJFD5dxNAestJ1yjiKRaDLZXSVdw4p8LTSkX4Rp2+7AIHNrfX3VbdAFrU/y6rPzUyl1NzBDXApqlYfbTt6FfY2AbBY2s82PTGVGQyVRVtRpUCrMFOoWCkiepDMJXEEQYm5sWI9vRoE1ELQk9AvmLchuN3AUuTLHFEqCQrpqeLEL5Cpp+XS19u9EHXvfuvde9+6910w1KR/X37r3SKz20qTNIyzwq4P4Kg/7AD6e/de6B/JdIbYLrNVwUcIlcqrzeNFaQqz6dT2UMVQn/G3vwXVWgr1UsFyxoOg+rOpdn1E8ka47XTRSpBBMsC+Kolcp5JF5DGBLgFrWAufp7IL6WRrh1VlEUfEedfM+mPLpdB4fhoVqXf0Hl5dPcXQ+CjCxikpjGAWik8SchvpG/1YqBe359vWt8QyxSCoIqp41889emgUqZVNDwYdN1b0fgpDHDFQU3llIX7dFDMHb6aiFt+nnn/W9vtcNLKEVc1pQeR/y9bt7QBDNIaRDIPr050Xx5wGgRmhp3ZW/cbwAesjkepeQv4PswjiCCrGrdNSmprwXyHToPj/ALZB0ijpmZWswCIdJtfn8fm3u3VAhoGKmlOuf+y+7dXkUNOLfkRpwf62tz79xweqgZAI65t8edtyKvkx9M1gSbIB9RzpItyfeqDrWoqx0HHUc/HTbJsUpUQc3GhGP9Pq19JN/e+r+KQCCoJ6xn457fBvHTwgjkK0S/4WuwBvc+/dXEqkUaP9nTdlfj3hxSuY8ZBJP+3JF40GgtG1mVmCkqCG/PvTCo7ePSmz8AzLrakeQa8aEfz6ZovjmlQiaMLS0+tTqNW8SeJla1mSNZWYn6i1xb3U6/ID8+l7y7ZEx1TF6cAgrWv20p06QfGHEPGorzCGJ9cdBAscYFzwJpVeQ3/qAp/p79pYjuan2dI5NxgVybe1HyMhqf2Cg6cW+NO0YEeanw9NJVRQymEyiR9cgQ6Va7G4YgD6X9+K0BKjvAxXpKLuWVljkkIiZhqpQYr/AJOgU2l1vhNy/cCuoIEljd0dBFFBFFLET5IBEovGEsfqSeOTfj2j225a6gDyA6/Py4eg4U6H298tR7WYxDmMgEHiSD51869S9y9Nbdp5cVJSUiq8q1gjkSMPDHNAYmCkkHRqb/YW9rpURwMdFtht51XCzAaBQkH0Nc/Ppcba6Z2nuaklp3o6VKyOJVyVIAvkppGFoqiIMo80Dup0sPpcqefaCPxrW5BqDEfU9Em67ZJYlTQ+Cx/TemD6g+hHmOsmM6uXYuViSqxkSxyRVQwOTR42gjrFVgizhj5NcEd2UEavp9fZq1zaoiSPMqxn+L/VnpAV8dKJWtR4ij06FjE5ieLC1FCBWPCska12arSscGPpG8Zlph5HNWZ9ILsG/UtgObD2T7jvVrHFN4ZIAWmsigFcV9TQcBxPWlsJp54UijBkc0CLk4+zAr5+Q6lbO37io8tl4ci81EmVrvNj6iW5o44UQQwwS24pmaJVIcjQSSCRbkC8tb/ZW13uKXcnhpPKHjJOBilCPL7eHrToX75sF09nYtbAO0EemQD4ieJI9c+XHoclYMoZSCGAIINwQfoQRwQR9D7kwEEAg46AvyPHz6797691737r3XvfuvdBn2ZA9NQ4Xc8KkybVzdHkJrfnHzSJT1oP5KhWUkf0B96+fn17/B009xwUtXtXH5FWRngydK1JMOdcNdDKsiqfysqBW/5BHvxPDr3Ss64JOx9uX/5USB/rConC/wDJo9+HWz0tve+tde9+691737r3Xvfuvde9+691737r3Xvfuvde9+6911zccf65/p7917rxFwR/X/G3+8j6e/de6xaXv9eL6L8X0Wvqtb66+P8AW59+6tUemf8AV/KnQX7s+81t5dfisb6bf5vjzaf+blvrbnT9Pfm4CnDoYbL9PpHh/H/l8vy/y9P+xPsv4XL4f+Lh5z/E9Vtfk5+38f5+z8P+a/2P5v7qvD59FvMX1H1a66/S6f0vSn4q/wBKvH8vKnS3926D/Xvfuvde9+691737r3Xvfuvde9+691737r3Xvfuvde9+690h67+B/wAVbR955PX95/DdH2/n8h8nmt6/ur31+P1/159+HHHQgt/3j9INWjTjR4tdVKYp/R9K49MdKHF/wax/hn2uvnyaLfc/UavN5P8AKL3+ur8+/efz6Lbv66o+r108q/D+Xl07+/dIeve/de697917r3v3Xuve/de697917r3v3XukTunw/wAQwv8AELfwzXPr1avF9xeO33NuPDo/r/j7V2/wTU+Ogp/sdJLj44tXw/PhX59Z4/tvI/8AwF/4DPo8Xg/4A35/zHp8P9b8+0rfu76g6/D+o8POr+GueOOPV1+u8Lt1+Drxp9aYpTPDh1wqb+aH7e2jw/5d4reC39nxaf8Ad3j/AFaeP9j7D154f7w/xGlKd3pX5fP1p0axa/pR4/8AaeXr+fULG+P7iuvo/iOs/r1+PRxb7XT/AM2bf4fW/PtbtvxSa/7ep4+ny6W3OnwrWlfpNIpTjX5/n0/D7n/dt/p/un/Mf4atH5/1/Zpnz49Jv0KfpU/23H+fUqHTqj0fr1DV9babeu/4+n+xv790y+qjV4eXU5vobWtfnV/qf7X0/NveumBxFfioesvHP1/xt/qf7P8Asbf7x79031x/236fx/vF/wDG9vfut/4euha/P+82/p6fr/vHv3VTwx0kc7995o/+BP1X7D7LyafLxbXo/wB3eS19Xp0/4X96bT59H22/S+G1NHn4vieny/o09M16VlL9z9rD954/uvEvn8N9Hk0jVpv/AI/7C/09+HAV49EU/g+M/g18LVjVxp8+pI+g+v8Asfr/ALH/AB976YPE166/tD9X0/w0/wCx/N/futjgPXy9eijbQ+w/i25PtvJb+9GZ+3/V4P4f9/Lf7nV/uz7jVpt6tNvx7K9s06Xp8Os6afw1xX59Tlvf1X0O1eNT/cOLX669A+H5aaV/z9KLcdvLTaf0eWp8Hit47+CPyeO3H+cte/8Aj7NTXV8s06IbKmiSvx6Rqrx446ZMB/E/4/g/4F9x/FPvk8+jX9r/AAfyD77+IX58X9fxe1vVb2mudPhHVSte37elm4fTfu67+u0/TaccNWv8Oj5/5Pl0NHY38F/g8X8Z+7v98v8ADf4Z5P4h934z/wABtHr/AM3fyX9Gj6829hreddLfTp8TxD4dfhpQaq1/yfLqOrHVql0/Bp76/binz6BKX7P+I4L7j73+DeWi833Xl8f2Xjb7z9XH3Xlvr1/u/XT7BF99T+9P92/i/uvxF01po/Omafb+fl0LbDR+7G/dvg/vTS2vT/aflXzp6Y6GH/ft+NfN/BPNen1fc6ft/F4l+18Gr93/AIC/1/H+PsUw/uqh1eDr8VNGnw6UqPz4f7PQVf8AedFr4+nS2rVr40/z8f5dCfSf5iL9Gnxp49F9Pj0jRa/H0+lvxb2PW01Oj4fl/k6Io9VO7j/P8+pHuvTvXvfuvde9+6902Zv+HfwfKfxbR/DPsKr7/XbT9p4X8/1/teO9vze1uffuvdFn3V/Hv7h7G+81fwu1V4fL5PvP92fwP+IX/b1/wm+m39q9+be658v9Xp1v7eh+2H4P7m7b+3v4v4TS2v8AXXo/dvb8+XV7t1rpW+/de697917r3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de697917r/2Q==">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="8439150"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4101" name="AutoShape 5" descr="data:image/jpg;base64,/9j/4AAQSkZJRgABAgEASABIAAD/7QAsUGhvdG9zaG9wIDMuMAA4QklNA+0AAAAAABAASAAAAAEAAQBIAAAAAQAB/+IMWElDQ19QUk9GSUxFAAEBAAAMSExpbm8CEAAAbW50clJHQiBYWVogB84AAgAJAAYAMQAAYWNzcE1TRlQAAAAASUVDIHNSR0IAAAAAAAAAAAAAAAAAAPbWAAEAAAAA0y1IUCAgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAARY3BydAAAAVAAAAAzZGVzYwAAAYQAAABsd3RwdAAAAfAAAAAUYmtwdAAAAgQAAAAUclhZWgAAAhgAAAAUZ1hZWgAAAiwAAAAUYlhZWgAAAkAAAAAUZG1uZAAAAlQAAABwZG1kZAAAAsQAAACIdnVlZAAAA0wAAACGdmlldwAAA9QAAAAkbHVtaQAAA/gAAAAUbWVhcwAABAwAAAAkdGVjaAAABDAAAAAMclRSQwAABDwAAAgMZ1RSQwAABDwAAAgMYlRSQwAABDwAAAgMdGV4dAAAAABDb3B5cmlnaHQgKGMpIDE5OTggSGV3bGV0dC1QYWNrYXJkIENvbXBhbnkAAGRlc2MAAAAAAAAAEnNSR0IgSUVDNjE5NjYtMi4xAAAAAAAAAAAAAAASc1JHQiBJRUM2MTk2Ni0yLjEAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFhZWiAAAAAAAADzUQABAAAAARbMWFlaIAAAAAAAAAAAAAAAAAAAAABYWVogAAAAAAAAb6IAADj1AAADkFhZWiAAAAAAAABimQAAt4UAABjaWFlaIAAAAAAAACSgAAAPhAAAts9kZXNjAAAAAAAAABZJRUMgaHR0cDovL3d3dy5pZWMuY2gAAAAAAAAAAAAAABZJRUMgaHR0cDovL3d3dy5pZWMuY2gAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZGVzYwAAAAAAAAAuSUVDIDYxOTY2LTIuMSBEZWZhdWx0IFJHQiBjb2xvdXIgc3BhY2UgLSBzUkdCAAAAAAAAAAAAAAAuSUVDIDYxOTY2LTIuMSBEZWZhdWx0IFJHQiBjb2xvdXIgc3BhY2UgLSBzUkdCAAAAAAAAAAAAAAAAAAAAAAAAAAAAAGRlc2MAAAAAAAAALFJlZmVyZW5jZSBWaWV3aW5nIENvbmRpdGlvbiBpbiBJRUM2MTk2Ni0yLjEAAAAAAAAAAAAAACxSZWZlcmVuY2UgVmlld2luZyBDb25kaXRpb24gaW4gSUVDNjE5NjYtMi4xAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAB2aWV3AAAAAAATpP4AFF8uABDPFAAD7cwABBMLAANcngAAAAFYWVogAAAAAABMCVYAUAAAAFcf521lYXMAAAAAAAAAAQAAAAAAAAAAAAAAAAAAAAAAAAKPAAAAAnNpZyAAAAAAQ1JUIGN1cnYAAAAAAAAEAAAAAAUACgAPABQAGQAeACMAKAAtADIANwA7AEAARQBKAE8AVABZAF4AYwBoAG0AcgB3AHwAgQCGAIsAkACVAJoAnwCkAKkArgCyALcAvADBAMYAywDQANUA2wDgAOUA6wDwAPYA+wEBAQcBDQETARkBHwElASsBMgE4AT4BRQFMAVIBWQFgAWcBbgF1AXwBgwGLAZIBmgGhAakBsQG5AcEByQHRAdkB4QHpAfIB+gIDAgwCFAIdAiYCLwI4AkECSwJUAl0CZwJxAnoChAKOApgCogKsArYCwQLLAtUC4ALrAvUDAAMLAxYDIQMtAzgDQwNPA1oDZgNyA34DigOWA6IDrgO6A8cD0wPgA+wD+QQGBBMEIAQtBDsESARVBGMEcQR+BIwEmgSoBLYExATTBOEE8AT+BQ0FHAUrBToFSQVYBWcFdwWGBZYFpgW1BcUF1QXlBfYGBgYWBicGNwZIBlkGagZ7BowGnQavBsAG0QbjBvUHBwcZBysHPQdPB2EHdAeGB5kHrAe/B9IH5Qf4CAsIHwgyCEYIWghuCIIIlgiqCL4I0gjnCPsJEAklCToJTwlkCXkJjwmkCboJzwnlCfsKEQonCj0KVApqCoEKmAquCsUK3ArzCwsLIgs5C1ELaQuAC5gLsAvIC+EL+QwSDCoMQwxcDHUMjgynDMAM2QzzDQ0NJg1ADVoNdA2ODakNww3eDfgOEw4uDkkOZA5/DpsOtg7SDu4PCQ8lD0EPXg96D5YPsw/PD+wQCRAmEEMQYRB+EJsQuRDXEPURExExEU8RbRGMEaoRyRHoEgcSJhJFEmQShBKjEsMS4xMDEyMTQxNjE4MTpBPFE+UUBhQnFEkUahSLFK0UzhTwFRIVNBVWFXgVmxW9FeAWAxYmFkkWbBaPFrIW1hb6Fx0XQRdlF4kXrhfSF/cYGxhAGGUYihivGNUY+hkgGUUZaxmRGbcZ3RoEGioaURp3Gp4axRrsGxQbOxtjG4obshvaHAIcKhxSHHscoxzMHPUdHh1HHXAdmR3DHeweFh5AHmoelB6+HukfEx8+H2kflB+/H+ogFSBBIGwgmCDEIPAhHCFIIXUhoSHOIfsiJyJVIoIiryLdIwojOCNmI5QjwiPwJB8kTSR8JKsk2iUJJTglaCWXJccl9yYnJlcmhya3JugnGCdJJ3onqyfcKA0oPyhxKKIo1CkGKTgpaymdKdAqAio1KmgqmyrPKwIrNitpK50r0SwFLDksbiyiLNctDC1BLXYtqy3hLhYuTC6CLrcu7i8kL1ovkS/HL/4wNTBsMKQw2zESMUoxgjG6MfIyKjJjMpsy1DMNM0YzfzO4M/E0KzRlNJ402DUTNU01hzXCNf02NzZyNq426TckN2A3nDfXOBQ4UDiMOMg5BTlCOX85vDn5OjY6dDqyOu87LTtrO6o76DwnPGU8pDzjPSI9YT2hPeA+ID5gPqA+4D8hP2E/oj/iQCNAZECmQOdBKUFqQaxB7kIwQnJCtUL3QzpDfUPARANER0SKRM5FEkVVRZpF3kYiRmdGq0bwRzVHe0fASAVIS0iRSNdJHUljSalJ8Eo3Sn1KxEsMS1NLmkviTCpMcky6TQJNSk2TTdxOJU5uTrdPAE9JT5NP3VAnUHFQu1EGUVBRm1HmUjFSfFLHUxNTX1OqU/ZUQlSPVNtVKFV1VcJWD1ZcVqlW91dEV5JX4FgvWH1Yy1kaWWlZuFoHWlZaplr1W0VblVvlXDVchlzWXSddeF3JXhpebF69Xw9fYV+zYAVgV2CqYPxhT2GiYfViSWKcYvBjQ2OXY+tkQGSUZOllPWWSZedmPWaSZuhnPWeTZ+loP2iWaOxpQ2maafFqSGqfavdrT2una/9sV2yvbQhtYG25bhJua27Ebx5veG/RcCtwhnDgcTpxlXHwcktypnMBc11zuHQUdHB0zHUodYV14XY+dpt2+HdWd7N4EXhueMx5KnmJeed6RnqlewR7Y3vCfCF8gXzhfUF9oX4BfmJ+wn8jf4R/5YBHgKiBCoFrgc2CMIKSgvSDV4O6hB2EgITjhUeFq4YOhnKG14c7h5+IBIhpiM6JM4mZif6KZIrKizCLlov8jGOMyo0xjZiN/45mjs6PNo+ekAaQbpDWkT+RqJIRknqS45NNk7aUIJSKlPSVX5XJljSWn5cKl3WX4JhMmLiZJJmQmfyaaJrVm0Kbr5wcnImc951kndKeQJ6unx2fi5/6oGmg2KFHobaiJqKWowajdqPmpFakx6U4pammGqaLpv2nbqfgqFKoxKk3qamqHKqPqwKrdavprFys0K1ErbiuLa6hrxavi7AAsHWw6rFgsdayS7LCszizrrQltJy1E7WKtgG2ebbwt2i34LhZuNG5SrnCuju6tbsuu6e8IbybvRW9j74KvoS+/796v/XAcMDswWfB48JfwtvDWMPUxFHEzsVLxcjGRsbDx0HHv8g9yLzJOsm5yjjKt8s2y7bMNcy1zTXNtc42zrbPN8+40DnQutE80b7SP9LB00TTxtRJ1MvVTtXR1lXW2Ndc1+DYZNjo2WzZ8dp22vvbgNwF3IrdEN2W3hzeot8p36/gNuC94UThzOJT4tvjY+Pr5HPk/OWE5g3mlucf56noMui86Ubp0Opb6uXrcOv77IbtEe2c7ijutO9A78zwWPDl8XLx//KM8xnzp/Q09ML1UPXe9m32+/eK+Bn4qPk4+cf6V/rn+3f8B/yY/Sn9uv5L/tz/bf///+4AE0Fkb2JlAGQAAAAAAQUAAklE/9sAhAABAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAgICAgICAgICAgIDAwMDAwMDAwMDAQEBAQEBAQEBAQECAgECAgMCAgICAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwMEBAQEBAQEBAQEBAQEBAQEBAQEBAT/wAARCAEEAcsDAREAAhEBAxEB/8QBogAAAAYCAwEAAAAAAAAAAAAABwgGBQQJAwoCAQALAQAABgMBAQEAAAAAAAAAAAAGBQQDBwIIAQkACgsQAAIBAwQBAwMCAwMDAgYJdQECAwQRBRIGIQcTIgAIMRRBMiMVCVFCFmEkMxdScYEYYpElQ6Gx8CY0cgoZwdE1J+FTNoLxkqJEVHNFRjdHYyhVVlcassLS4vJkg3SThGWjs8PT4yk4ZvN1Kjk6SElKWFlaZ2hpanZ3eHl6hYaHiImKlJWWl5iZmqSlpqeoqaq0tba3uLm6xMXGx8jJytTV1tfY2drk5ebn6Onq9PX29/j5+hEAAgEDAgQEAwUEBAQGBgVtAQIDEQQhEgUxBgAiE0FRBzJhFHEIQoEjkRVSoWIWMwmxJMHRQ3LwF+GCNCWSUxhjRPGisiY1GVQ2RWQnCnODk0Z0wtLi8lVldVY3hIWjs8PT4/MpGpSktMTU5PSVpbXF1eX1KEdXZjh2hpamtsbW5vZnd4eXp7fH1+f3SFhoeIiYqLjI2Oj4OUlZaXmJmam5ydnp+So6SlpqeoqaqrrK2ur6/9oADAMBAAIRAxEAPwDf49+691737r3Xvfuvde9+691737r3Xvfuvde9+691737r3XvfuvdYJqqmp7Cepggva3mmjivqNhbWy3ueB7usbv8AAhP2CvVWdFwzgH5nrKjpIoeN1dT9GRgyn/WKkg+6kFTQih+fWwQwqD+zriYoi4kMcZkFrOUUuLfSzWuLe96mA0hjp9OtaQTUjPrjrJ7r1unz69791vr3v3Xuve/de697917oo/yz6Pre0drUm49rUpqt6bPjqXpqGOwlz+EnKy12IivbXXwyRiakF/U+uMcyCw95F5lj2W9ks72TTt1wRVjwRxgMfRTwb8jwHQF535dfeLOO7s0ruEANFHF04lR6sDlR9o4kdVBapYJJYJo5IZ6eV4KinmjeKenniYpLDPDIqyQzRSAhlYAqRY+58FHAZCCpFQRwIPCh8/8AL1BRDKWVgQwNCD5fLqZFUf4j/WP++4t7qy14jrYNM+fU9KkL+SBwOeeTwB9OST9Le2ihH2dX1cB1aN8Sel8ltKgqewt2UctFnc7RrR4HF1UZjqsVg5GSaarrInAeCuy0iIQhAaKBAG5kZVhbn7mOK+lTaLGQNbxNqmdeDOMBQfMLmvqfszMvIvLstlG+63sZW4kXTEh4qhyWPoW8vQfbg6nuNupGGMde9+691737r3Xvfuvde9+690FW4OluutyVb11dgvtqqZzJPLi6uqxoqHblmlhppUpy7H6sEDH8n2ILPmferKMRR3eqMCgEgDU+wnP8+iC75Z2a8kMslrpcmpMZK1+0A06VG1NibS2TBLBtnCUmMNRp+6qE8k1bV6f0/c1tQ8tVMqnkKX0KfoB7Qbhuu4boytfXLPp+FcBR9iigH+HpfY7VYbajJZWypq+I8SftY1J6Vvsu6MOve/de697917r3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de697917rhJJHDG8srpFFEjSSSSMqRxxopZ3d2IVERQSSTYD3tVLEKoJYmgA8+qsyoCzGijJJ4AedT1Xp2n8p8hm8nWYHrqtOMwFJLJSy7ihAGTzTxuVknx0ji+OxjEftuo88q+q6Ahfcv7ByLBbQx3W8RiS8I1CE/Cg9GH4m9fIcM8eoj37nie4mktdok8O0BIMo+N/mv8K+nmflw6A6l3BUVkwqK2qnrKhzqeasnlqZXLcsWknd3uf9f2LHtFRdEaBU8gBQfsHQUS9kZg8shZjxLEk/tPQo7Y3xmcJNHPiMrWUMi6bxxTEwOqsDplpXLU80ZtyCp9kO4bRbXakTW6sD6jP7eI6EVhu1xbMrQTsvyBx+Y4Ho6nWnZ1NvWE4+vWGk3BTQ+V4ozanyMC2D1VGrEsjxkjyREkrfUCVvpjHetjk2xvFjq1oTSvmp9D/kP+XqSdm3qPclMUlFugKkDgw9R/l6Fr2H+j7r3v3Xuve/de697917r3v3Xuve/de6ALtH419W9rVEuVzOKnw+45U0vuTbk6Y3JTkKRG2QjaKegyZTj1TwvJpFgwHsU7LzhvWxosEEwktBwhmGpR/pTUMv2A0+XQY3nlLZt6dpp4THdHjLEdLH/TChVvtIr8+i5N8AcKKrXF2fmloweIJNt42Spt+B92mQhivb/mx/sPYvHunPoo2yp4nqJDT9mg/wCHoJn2xg11G7v4foYxX9usD+XQ99afFrqzrarpsvDQ1m59wUrLJTZfc0sFZ9lOtyJ8fjoIKfHUkwPKyeN5UIurj2F94533vd43gMiwWrYKQ1FR6MxJY/YKA+Y6E20cl7LtMiziNprkGoeYg0PqqgBR8iakeR6Mf7B/Qt697917r3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de697917rizKis7sqIoLMzEKqqOSWY2AAHvYBYgKKk8AOtEhQSxoBxJ6Z/wC8WE/52NP+vRfU1v8Ag19P+avxr/Tf8+1f0F5/vhuFf9Xz+XHpJ9fZ/wC/140/1fL58OgO7a79pNg1r4HBY6HN56BVauepmeLGY1pFWSOnlMF5qqraNwzIpQRgi7XNgKOXuUJN2hF5dzGK0PwBR3NTBOcAftr0F+YObo9qmNnaRCS6Hxlj2rXyNMk+vCnQQ7S+YMoy9PQ7+wNBR4qpmSB85g2qgccZH0rU1uPqpKhpqOMkeVopA6KCwRrW9n+4+3ifTvLtN07TqKiOWnd8gwAofSop5Y6I9v5/k8ZU3S3QQE0MkVQVr5lSTUetM+leHR5o5I5o45YnSWKVFkjkjdXjkjdQyPG6kq6OpBBHBHuLWVlYqwIYGhB4g9ScrB1DKQVIqCM1HkR0EG/u6ts7HmkxqRVGfzkX+dxuOeNIqNiAVXI10mqKmcg/oVZJB+VHsSbRyxfbqqzMwhtDwd+Lf6VeJ+3A+fQe3bmWy2tmhCmW6HFE4D/TNwH2ZPy6AZ/lVuNKgsdmYj7QN/m/4rW/c6Prby/amLVb86Lf4exWOQbIpT95SeJ66RSv2Vr0Fjz5eB/+SbH4fpqNf20p/LocOu+9Npb/AKmPE6KnAbgkUmLF5No2jrSoLMuNr47Q1bqov42EctudFgT7C+88qbhtKNcAiazHGRK1X/TKcj7cj59CbaOaLDdZFgzFdHhG/n/pWGD9mD8uhr9hfoTdFb+Xm9qnaPUtTQUEzwV28cnTbaE0bMkkePmhqK3LaHUhlM9FSNAbf2Zj+bexxyBtqX++rNKtY7dDMAf4qgL+wmv2joFc+bi9jsbRRNSS4cRV/o0LN+0Ch+R6qagqWjI0kra1gABYf4f4D3O5APHqDATgjpW4/NFbBnt/Q/T/AG/tPJECOHTySUPS8x2ZuF9d/pax+lrG459l8sHHHS6GehFDnoU9p7xqMBlsZmaaUrLjauGpOlra4lbTUQuBa6T07MjD8g+yPcNsjvbea3kXDqV/PyP5Ho/27dHtLiGdGoyMD+XmPzHVo9PPHVU8FVCdUNTDFPEx4vHMiyIfz9VYe4GdGjd42+JSQftGOpzRg6K6/CQCPz6ze69W697917r3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/dar1737rfXvfuvde9+691737r3Xvfuvde9+691737r3Xvfuvde9+691737r3Xvfuvde9+691737r3XvfuvdIDs/svavUey8vvreFY1NicVGoSCAJJX5TIT3ShxGKp3eMVWSr5hpjTUqgXdyqKzBZY2NxuN1HaWy1kbzPADzJ9AOkl9ewbfbSXVw1I18hxJ8gB5k9Updo/MjuTs/I1SY3O1nX+1mkkWh27tWqejrftSxCfxnPwiPI5Cqkjt5FjaGmDcLHbkydYctbZYopeITT+byZFfkvAfzPUb3vMW43zHRKYYK4SM0NPm3En9g6DTbO/99UNWtbR753lT1iOGFTHunOeXV/qizV7BrDjn6D2suLS1YaWtYyp8tC/5ukUN3dKwZbmQH11H/P1Yf0V8tc/T1dFt/tOsGYw9S0dPBuswRRZTFSOQqSZhKdY4shj9RGuUIs8YOo+QAgA3dOX4irTWC6ZBkx1wf8AS14H5cPs6GG2b7KGWG+bUhwJPMfb6jqyWORJUSWJ0kjkRZI5I2DpIjgMjo6kqyMpuCOCPYMIIJBGeheDUA9c/eut9e9+691737r3Xvfuvde9+691737r3Xvfuvde9+690E3YealjqqXDRuUhaBauqCkjzM0jrDE5H1jTxFiPoSR/T2J9itEMcl2y1fVpX5Yyf59Bffbx1lisw1E062+ecA/LHSB+5Nvr/uvT/h+v/ev+J9nfh/4a9Evin18uiddqR1lNvbdsGQ1/epuDKPMZCbyCaoaaCQEi7JJTurKfoVItx7H+yNE+17e8NPC8FKfsAp+Rr0Ad7EqbpuCz/wBr4zV+dSTXoAMvIFSZmvp0n68cWFxf/EH2JIh3dEUvwdWuYjL5vZXQmzzXGSPcn91cFi4fOSZqWqqaFBEZA51CbH0S3IP0eOx/p7gqW1td05t3AR0NmJ3kanAgHNPkzfyPU3xXNztnKlgXqLwwJGteIJGPzVf5joqVVjWkeSSUySyyO0kszsZJJZHYu8kjtdneRySSbkn3Ikc1AFFNIwAP83UePHUktXUTUk8Sfn8+mKoxF/7AP+I4J/3j6D/Ye1KTfOh6YaGvl0zPjZYJY5qeSannp5EmgmiYxzQTwuJIpopVs0csTqGDDkEe3hIrAqwBQihByCD5EfPpkxlWDo1HXIIwQRwI+Y6sc6p3bPvPZWLylaQcpT+TF5ZgAokyFBpjkqAASB93EySkcAFyALD3C/MG3Jtm6TwRD/F2/Uj+St5fkaj8upk2DcG3LbIZ5f7dapJ82Xz/ADFD+fRYfndjambrzaOYiVmpsTu8QVhB9Ma5TF1kNPK63uR9xAqA/gv/AI+xj7YTou6bhbse94NS/wC1YVH7G/l0EfcqF22uwnWulJirf7ZTT/B1V/FUf4/7YAH8X+n+HuaStft6hoNQmnDpxin+hBt/vh/tvbZFMHpwGvT/AEOTeJhc3X+n+2tyb/X200Yb7erqxFPTpb47LPOFij1NLLaGNF/U0kpEaKLclncgW/x9opIQMngMnpVFKxoo+I4HVzmDqqKlpsXt2WvojnKDA42aqxYqoDkY6ZIlo/vHohIalKR6mF0WQroLqQDcH3jRdusl3cyJ8LSMw+wkkdZK2qNFa20bfEsaqftAAPSV7K7d2D1HHsuXf2b/AIJF2Bv7bnWe15TR1lVHXbx3ZLNBgsbK9JDMtHHWTQMvml0RK1gzC49pq06f6LV3N8xs5sftiu6S6Z+PPY3yU7E2vtzA7w7GxeyM9sjaVDsPbe5quenwk1Zl9/ZrB4/L5rJw0c80NBSu0rRR3LLfjROaAdbpitP8H+Ujo7sTmSON2jeJnRHaJ9OuMsoJjfQzJrQmxsSL/Q+7da65+/de697917r3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de64SSRwxySyyJFFEjSSyyMqRxxopZ5JHYhURFBJJNgPe1VnZVUEsTQAcSfTrTMFUsxAUCpJ4dE17B+Ym2MLXT4fYWOj3ZVU8jQzZupqGpdvrKhKsKIxK1XlUVhbyJ4oW/suw59yNtHt5eXMS3G6zmBCKiJRV/zrhfsyfWnUebv7gWlrK1vtkIncGhlY0j/ACplvtwPQnoLKf5a9kTTiVqPaqxE3+1XHVvjA1X0iQ5Mz208fqv7ELcgbIEK659X8WoV/Zpp0H15+3otq8ODT/Dpb/Dqr0O2wvk/hc5PBj94Y5NvVE5CR5WkmeowxkYgKKlZQKrHqb/qJlQf2mUc+wruvItzbI022zGZBkxsKP8AkRhv5dCfaueba6dIdxhELnhIpqn51yv8x0aeORJUSWJ0kjkRZI5I2DpIjgMjo6kqyMpuCOCPYCIKkqwIYGhB6HikMAwODkEdc/eut9e9+691737r3Xvfuvde9+691737r3Xvfuvde9+691737r3Xvfuvde9+691737r3VMP8xzsCty3Z21OtoqiRcPtLbke4qylViI6jPbjmqoYZ5VBtI1FiKELFflPuJLfq9ybyVZrHY3F8R+pI+gH+itP8JP8AIdRvzldtJfW9mGPhxprI9Wav+AD+Z6r/AKX6qT+R/Qf4f8T7FrcaDh0FE8+lphWs5H++N/p/tyPaSYcD0qTBHy6GLBOPR/S9jf8AIP1FvZZKDw6NYz1b/wDGDdNTuPq6ipK2VpqrbNdU4ASyMzyPQwJDU40O7EkmGkqViH+0xj3He+QLDfMyigcB/wA+B/mOh7ss7S2SqxqUOj8uI/kejE+yfo3697917r3v3Xuve/de697917r3v3Xuve/de697917oFe0cZURVdFnY0Z6QwLQ1ZUE+CVJHenkk49McolKg/QMAPyPYu5cuI2ims2NJa60+Y8wPmKdBDmO1kEkV6o/Tpob5GuCfka9Bj9yLfq/3X/vGr/X9iHw/l59BzxD6eVOhU7N6T2t2Y8ddWS1WGzkMQgXMY1YWeogX/Nw5ClnRoaxIbnQ10kUGwbTYAK7HzRf7IrQxqstqTXw3rg+ZUjhXz4j5V6Fu98sWO9MJnYx3YFPEQDI8gw86eXA/PoOdmfEzY+3M1TZzO5PIbvloJ46qhx9fTU1FiEqYmDxT1dFC0717QygMqPJ4bgakb2b7lz9uV5bvbWkC24caXdSWan9E0AX7aV9COivbuRNutLhLi6na4KmqoQFSvkWFSWp9tPUEdCd3DSSVGCxsigmODKDygfQGWmmWNmH+DCw/xPsp5XkCXc6/iMePyI6NOZo2a0t2qdIkz+YNOi1y0A54tf6/1/obcWI9jtZh59AYxV6a5scObpb/AH31/p9Pb6zeh6TtAPSnTTNi78ab/wBFK8/8juPb6zHj0y0R+3oy3SEtDt3alXPlq+ixdPmN1Lj8Z/EKuCkSsyM9PTwQ0VGaiSP7irq5kKxxpd3KkKDY+495xnSW/tgrAlYhUj5k06kHlGCSKwuCykBpSQCPQAHqf3Rl+sc82A6E3tuGDE7p7uod002wMe9NUy1WQr9l42DcOSrqCdYGo4qnAwmKp0SyxNMqlU1eqxJtG6S7NuVpuEGXjauk/iXgyn7VJHy49HW7bbDu23XVhPhJFoG/hIyrD7CK/wAuterfXZOY2l2B2R1ftvqzsPsXefVG5jtTd6YVNpbY25Flftaevgai3HvvdW3Ia2kq8fVxzJJDDKfG4NjddU2Q87jcTIuy7JcXOmlTVUAqMA1r1DsvJAsFR933mK3B8qE8PQkr1F372D2Dhtz9S7S2ZtXbAr+yo95/xTJb3zWQGO2lVbUwWJ3AuPaDbEFQc5X1dLUVaDxVMURelJVmU6g9vG87zDc7LYWVtDHcXaEt41TocAErUGh8xXqmz7Jss1vvF9eTSyW1rIVHhkAOnk3CvDPEdJzHd670x+w/kXkN2bV2z/fzoGPOa6Pa2WyFftXdIGxYt6bXrInr4YczhVq1qBBX0sxkmptBcMQ4VUMXMt+m28w/WQx/vGxFNUWUYkUU5rwPH5dKpuWbA7hsTWbyfu+7NSkmGFBqI8jQjHyPT3S9L/IfaHx3y3yi253LvfN9qdT7UxnbFdHunMxV3UfYmQw0dBuTdWyKTYEGNxuCodpLhxVLSVFJFBPTTRwHyFtWkKbwk9jtdvfpvdxJvM0YklXV2aXHctPIZoPXjQdCfbpI7vcbjbpNngTa4XKRNp7iy/CRjjip9OFT1YRHvXz/ADl+MPbuJlFFt/5A/FHfm3dWsiomzOGyuzeytuU6zKVVjBhspkQRb1WvwB7CbIj3lo5QaJYuB6EmqRLW5QOdUcnHz8v9npf/AMy7I5vJfEDeW4KCVFzXVO7erO4MTlAg89B/o37H2xuPLzcWVg+ApKpC3BUOSbi/trctujjheeEFSMkeX+x05YblJJKIpWqDwbzxnPrw6x/Mba3xxo89tP5Hf7OLVfCPvDduwJItn9m43eG1MfgexttbeigzFHit8bD3xSZHa/YeFwlRuGI+EJBW3qUjSblUJIy6WzhujuoYVDUHrj/L0a74S9qdm90/GTq/sft/E0eL35n8dlBk6jG42qw2L3LRY7OZPGYLe2Mw1c71uIoN6YOjp8nHTS2aEVOkDTp96U1APVz0av3brXXvfuvde9+691737r3Xvfuvde9+691737r3Xvfuvde9+691737r3VfXzb7hrMLTYzqjA1TU02cohmN21EDss38FaaSnx+GDIwKx5SeCSSoHBaGNV/TIwMre3GwRztNvt0lRG3hwA8NVAWf7QCAPnXzA6i/3C3x4Ej2a2ehkUSTkfw1OlPzoSR6U8ieq56OuKFeeP6/S3H+9e5eZAR1EgJXzx0sqDJfT1ccfn/eVv7SyR9PI/n5dLOhyNwt2BB/qeD/X/AH2iki+XSxJfTh0ff4v9jz5GKr2DlKgzNj6Vsjt6SViZFoY5EjrcZdmJZKR5UkiH9lGZfooHuKOedmSIx7vAlNTaJgOFadrfnSh+dPn1KfI+8NMH2md66F1wk8QK9yflWo+Vejg+456kbr3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de6o3/AJiO2q7Ed+Y7cUqOcfu7Y+Iaim0HxCqwFVXY/IUof9LSxxz08hH1VZQfz7lXkydJNpeAHvjlao+TAEH/AA9RfzhC8e7RzH4JIhQ/Nagj/B0Sal+o/wAbD/Yj/jY9iZxw6Daen+ry6V+IY+YcfX8f7zb/AG59pZuHSpDmvz6GDBPbQf8AEfU/09lkvn9vRnGcL1bX8RsNUUHWlXlZ0eNdwbhraulDggSUlDBTYxJ0uTdJJ6WQD/gvuPuYZFe+WNfwIAftOf8AL0O9gjZLIuR8Tkj7BQdGn9kXR51737r3Xvfuvde9+691737r3Xvfuvde9+691737r3WOWKKeN4Z40mhlUpJFKivHIjCzK6MCrKR9QfdlZkZXRiGBqCOI6q6K6lHUFTgg8D0lP7h7Uvf+EQ/5/wA9vJPa+jR4reX/AID39Xj/AE6ubezP997nT/co/DTgP28OPz6LP3Ltta/Srxr5/s48Pl0r/ZV0a9e9+690WD5eb9g2Z8e+2sjitz4jB7ux+0JqnbtRVV+Binx2Yqq2ix2Gyj0+dzODx/2lPlK2HW1RVUsGk2aVAdXtyKeW3fxYXKyAcR88dNyQR3KGKVaoeIPy6rO6y/mVfFTfm0etajI9g/w/snsBaLEQdXUG29y7h3t/e2WrbFyYb+DbZxWZSmkq66IyQtJMITTuJPJoDMBnbb/aNDF4jnxyKFACTXh6Uz0C7jY7kTyiJR4IqQxIGOP246FL5fdnbo6Q2b1n2Bh8jSYbbFP3v1Vg+1azI0dLUU9H1bunMy4HdNdUSzh3x6Yl6+nqXlivIqwlRe/tVud5JbxWs0cmhfFUSf6U149J9utYpZbmGRNTeGxT7RSn7ekd8KN0Z35W7g7q7vxO6ZMx1/uDftf1r1TtWkyssmH2z1513US4mbeuYx6iF8ZuPsXOS1OS0TxLUpjhSRqW+vtJbblCfr9yuZz4LVijjrmgHkPVv5dKptvm/wAS2+3h7xSR3pivzPoP83QMZnbe4d0/ygPk513K1ZLvr44dodxUGDrPv6qbN4h+oe7ajde2M1SZKVmrqXLU+y1jmhlVg8TMArWF/YIdmcMScjoaKgVdP29Nu/8AuLvnqjtP4EbE78jqewYsR8k9i5Tp/wCW2IoVptt9odKdibDzm2M/tbsGkE7nbna+MqM5SO7KzU2Wo4VnVVdXL0JIoTw9er1NaU/1U6cvkPsPozH/AMw/5BUfyO+TO4vjZ1pvLqzpfuLa/wDAewNudbUm7Nz4X+K7K3RPX5zP4nKM8tPDgKWNoaUwyVMMzI5cC3tXaX17YySNZ3ssLNTV4bFdQHAGhFc9Jbi0tLpV+rt430/DrVTTjUioNMU6Z/lD0V1b3Btjojfvxy7D3xv/AGBL8jtlR5rO7F/iDZfG7WzTbj2Vumswmf2/BisrDjcdJlIZKmpAjjWnjJEumzAcbjv13zDYbTNc2wVobgKXgZlYrSjepUn1B6B9jtFrsN9ucFtc6kmi8QLKFIDEmnCgIHpTo1uxvg70Rsfae4NnQY/IV+G3VTZ2HcMEtfUpLmanclDJjcvlMzkqupyOczmWqqSXR9xWVUzhURf0IqqeCdIduudssbJIraYESsavI9RSpdvP0xjy6D5WSbcbfc7q5eSeL+zUdiLT0UV4+ec9ARF8Wvl7X9GN8Qc73r10ej/4U2wqntui23mm72znTkkj08mzanETypsbG7mn245xL5eNplFNaUwPPrLBP93bkY/o2mT6bgXA7ivpn5Y6E37w28ObkI/1HHTwGr1r0aLt34sbT7Sx/RlFh98b/wCp5vj5kTU7AyfXGSxtHlqfHNtKTZb4Wprszi8y70D4R1RrAOxUFiT7Vz7Wky26rIU8LClePAD/ACdJYN0MTTs8YbWchuHn/n6UW0PjX13tvaHZOyNw5nsjtnb/AG5jf4Pv2h7i7F3V2FSZXFPjq7F1eNoMdmq98VtyhyNHkZRUx42ClWc6C+oxx6dxbZFHHLEzO6v8Wo14V/Z16Xc5JHjkCqpXhpHr0Z3ZW1evKun25svL7J2llMHtehp6PZFBlsBi8pTbZjx9JT0sNFhUyNNUfw+D7KiiVRHY/sqPZZvO3KtulxElDGApH9HgP2f4OjXZtxY3D28r1Dksp/pcT+3oyqIkSJHGixxxqqRxooRERAFVEVQFVVUWAHAHsL9Cjrl7917r3v3Xuve/de64syorO7KiKCWZiFVQPqWY2AA97AJIAFT6DrRZVBLEADiT0mKnem2aV2jfKwyyI2llpkmqrH/g8Ebxn/b+zGPadwkAYWxA/pUH+Ejouk3fb4zpNwCf6IJ/wDrJS7v27VsEjyUSOxsFqElp7/8AIUyIg/2/usm130QJaAkf0SD/AID1aLdLGUgLOAf6QI/w9KISxsAyyIysLqQ6kEH6EEGxB9oCCCQRnpeCCAQcdd61/wBUv+3H/Ffeut9cvfuvde9+691R98ua+pm+Q+/VqSR9qm3KSlUkG1Im28VLGVtaytLO5t9bn3kfyNGq8q7VoHHWx+0yPXrHznVpG5l3LVWgKAfZ4adABTzMxsoYkWNgCf8AY8ezbdt62bYbcXe97va2dqTpEt3KkKV9NUjKK/KvRJYbbuO6SGHbbCa4mGSkEbSGnrRQTTp9pqt4yoOpfobFSLj+v09lVtzlyduERnsOa9tnhDaS8NzA4BABoSrkVoQaccj16WTcucw2zhJtivI3pXS8Mikj1oVHmKdKugyqqQDILj+ze304sf8AEeznVFMiyROrRsAyspqCDkEEcQRwPRdpkjZkeNhIDRlIIIIwQfQjoy/xwy7DtzZwhm0meXKQSgN+qCTEZAyo4+pUaA3+uAfYS5xiQ8vblrAwFI+0OtPz6FfJ8jjmDbqAipYH7NDV6tfDofo6/wDJQ/4r7gPqeOva0/1S/wDJQ/4r7917ru4P0IP+x9+69137917r3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de6Lv8lugsX8gNgPt9qiHF7qws0mW2ZnZldocfljEIpaSvEaPM2Hy8CiGpCAulklUFo1UnOx7vJs94JqFrdhplQeY9R8xxH7PPon3rak3a0MJIWZe6Nz5H0PyPn+3qhPenX28+sNwT7Z35t+t27l6ZyqrVJqoq+MOVWsxGSjvR5OiltdJInb+jBWBUS1bXltfxLPaTB4iPLiD6MOIPUVz2l1YytBdxFJB68D8weBHWHGyKkqMWVR9CWIA50j6nj6j36UEqaDrykY9ejkdCdHbv7ZyNNLTUtTitnwzr/Fd01NO8dL4EYGalwvkVRk8jInpXReKInVIw4BDO7bpb7eh1MGufwxg5/P0HQk2rbbi/ZaKVtx8Uh/yep/l69XPYTDY7buIxuCxFMlJjMTRU9BQ06fSKnpo1jjBb6u5C3ZjyzEk8n3G0srzSPLIauxqT1IscaRRpFGKIooB9nTp7b6v1737r3Xvfuvde9+691737r3Xvfuvde9+691737r3Xvfuvde9+691737r3XRAIIIBBBBBFwQeCCDwQR7917qkH58fFLpToHYvYPcfQ3WMuH7Z7qq6LYGT2ns59zvR7yqMjPktyzQ7d2ltvJ02QodzZytoftR/CInR2qjLNRVCLKGbYUGOJx1Yedft6Ip/LG+J3anw0+XWHX5afHtqWk7W2DVYLq/t1IaTduB2V2DVyUeQm25kMxhpqvGbRy+68I1VR66pYJGqolp6eR1mdTaF3gkWRGKuOBHl028SyK0boGQjPV5Pzv+M1b3/8TO7OqOucTin3/uzbFPHs+PLZCajxb53GZrF5mjhq6mZpoqaCp/h7RlypCh/a6fcby4hMMsupDTFB5fMDpJFt1nBIZYYtMlDmp8/z6RWN+Fec6s7g6p7s+Lua2l0gDgtt7M+RXS8mFmr+se0tn4ynhjTIY+mwk2NfAdp7cBkjos4iyrVAIKuKZA6yIiDUH9o6WgUFB0Luz/iVgtvUny7wWW3bmM5tL5Z7w3JufK4GOkosadj027+vcRsTcON2/WxLM1Q9a+Pkr1nmQslRMfTYW9604YevXvOvQjwfHbq6o6R2V0BuzBL2BsDY22tk7bxcW83GVys/+j+lxlPtzOVWTRaeoTcVLNiYZ/vITFKJgWUi5HvdBSnl14YoR0uc51j1xufcNHu3cmw9n7g3PjseMTQbgze3MTlMvRYwVMlYKClr66knqIKUVUzyBFYKHYn6k+/UB4jrdSOB6LFlayEZfLClggpaYZKsWCmpY0gp4oo53ijjiijCRoiIlgFA9ytY2yw2drGq8Ixw+Yqf29RRe3ZmvLqRiTVz+yvAdQhXfgmwH+PH+x559qfCHHTnpN4w65ivA+rf7Y8fX3oxfb1YSg58uoNdujDYlfJlcvjcYhBIfIVtNSLpF7nXUSxjSLH8+wpzPzpyRyXbm75y5x2vabUIZDJud3BappFatqnkjXSKHPDB6Odq2Lft+fwti2O8vZK6dNpDJKamlBSNWNc9IHKd8da4nUJN0Q1kqrdYsZBWZDWbnhaimgkpAxt/akHvF3nD7/n3RuTBIl37wWd9dAVWLZ4bm/1fIS20MluDj8Uij59Szsv3dPeXfChi5Lmt4ScvevFBp+1JHWU/kp6x7b+THWz5zGN/GKnHtDX0ciTZGjqKemIWdPIHqAskMCiO92lZFsfr7C3LH94x90nnS/Owj3Bl224nUpFLu9pcW1uzEGga4KNDCBxLTNGn9KuOjvcfuy+8mwRR7mOXUuo42DOllNHLIACCSI6q714UQM3y6sax+bxuUhiqKGqgqYJ40lgmglSWKaKVQ8csUiEo8ciEFSCQR7yTt7i3u4ILq1nSW1lQSRyRsGV1YVVlYEhlYGoINCMjoJSRyQySQzRskqMVZWBBBBoQQcgg8R07XvyOR7e6p1737r3RV/kJ8kKTqUw7bwFPS5XelZTLVyJV+R8dgqGXUIaiuSF45KisqtJMMAZLJ+45ClFk56/fU+/Dafdw+k5G5I2yDc/dW7gFyy3Wo2thbvqCS3ARkaaeUqfDgV1oo8WRgpjSac/aT2dn59Em87tO9vy3G/hgx08SdxSqoSCFRa9z0Oe1RWpWvfPfIXtPccjvlN6ZN4nYsKOlWloKFOSVUUlHTwQtoBsCwZrfUk++OO4ffx+95uO4T7j/AK89/bSOSRHZw2kEaAmoVEit1FBwqasR8TE56ylj9j/bNbeO2k5St5UXzmaVyT6ktIan+XpTpHt2dvMggbqzyg3/AM3laxCL/wCpZZlKkf4W9hO5+9596u8imil+8HzaFcEMY9yuYzn+FkdWQ+hUgjy6MI/Z72yiZGTkPa6j1to2H5hlIP516iy9ibulXTNurckq3B0yZzJSLcXsdLVZFxf2GLv7xn3jr+IQ33v9ztNDUNol33c3WorQ0a6IqKnPRnD7acgwNrg5I2hHpSqWVspp6VEY6wPv/dBVUO5M+US+hXzGRKrqtq0qaiw1W5t9fYdvfdr3f3NkfcvdTmS4dahTNud7IQDxoWnNK9GsHJ/LVqCtty9YxqeIjt4V/wACdL3ZXyF7G2VV070+4q/L4xJE+4w2Zq5q6klgBAeOmkqTNNj30j0tEQoaxZWF1M++x332Pf8A9lt6sJhzje77yksi/VbLvU8lzHJEKBkt5pTLNZvproaI6A1C8Uq1Qg7m/wBnOTObbSZDtUVnuZU+Hd2qLGyt5F1XSsorxDZpwZTkWcdVdz4fsHF0dbSy6HqIwz08rL5oZFus0MoViNcMoKki6m1wbEH39KPtb7k8t+73t/yt7j8pTM2xbrai4iWTT4kTAlJoJQpZRNbzK8UgDMA6HSSKE8/eZuXtx5U33cuX91QC+tpNDFa6WBAZHWoBKuhDLUA0IqAcdD0jB1DL9CLj2P8Aoi6qp+c3WjU3Y+2uwInRcZuvE/wrLqJFWZMrt3xrC4VjqMdbi6uJAVB0mna9tS+4a+9J98W3+6h93/c96262huvca8uv3dy1Z3AJiM0qtJJczqpDNBZorSMoI8R2hi1KJC6q+RvZKT3W9yLSO4d4+Wo4fqNzljNGpGQixKTWjz1UA0wqyNxABKfTyUdOgigRIkH4S3PN7sb3Y8/Uk+/lL9zfdT3M95eZ7vnL3S5zv975kmJJuL6QsEBNfDgiAWG3hB+GKFEjXgqgddPOW+UNg5Q2yHZuWdmt7HbIxiK3ULU/xMfidz5sxLHiSepIqYT/AGvcd+G/8PR8YmHkf9X59eM0LCxII/oQCOORwf8AH29bT3dlcRXdnPJDdRtqjliYq6kcCrKQQfmD01JbiZGimhDxtgqwBB+0HB6z0tc1FMlTR1MtHURhhHPTSPBMgZSrBJYSrqGU2NjyPYutfcf3HsUmSy593qFJKCQRX1ygbTldQWUaqE4rw6LX5d2aVkaXZLVmWuktDGSK8aduK9KKHfO7oEVIN37khRCSqQ57KRopJLHSqVQCksb/AOufZvbe9XvPZRRwWfu1zPFCmVSLdL5VFTU0CzgCpNceeek0nKnLUjM8vLlizniWt4iT5Zqnp08RdsdlQvrTsXepIuLSbpzcyc8cpLWuhP8AsOPYntfvPfeTtJlni9/Ocy4rQS7xuEi5FMpJcOh/MY4jPRZJ7e8iyqUbkvawP6NrCp/aqA9KLHd/du41lal39l5CtgBX/ZZMGwYcrk6WrDE6zyeSbH6gWkDZPv0/e15f0fQ+9W5yBRQfXRWl5wBGfq7aevxHJzwPEChNd+z/ALcXwYTcpW6g/wC+jJF6f77dPT/D6noUcB8wOysY6LmKbBZ+AW8jPTy42tewt6aiklNGhP1P+TN7yT5H/vX/AH32OaCPnblXYd929R+oUjlsbpiABUTRPJbrXJP+LHJxQY6AW7/dw5Ou1Ztq3C8s5jwGpZox9qsA5/5yDoxezfl/sbONDTbip6za1W+kM9XprsWZGNtK5GlRZEUW5aaCFf8AH3n57Rf3nP3ffcKS02znL6zlLfZAoP7zAmsS5rVUvoR2qtMvcQ265FDXAhjmX7v/ADrsqyT7UYtytB/vjsmp6mJzn7EZz8ujQ4fc2FztLBW4vIUlbSVKCSCppKiKop5oz9HimiZo5EJFrgn30L2jeNp3/bLHeth3S2vdmuYxNbXdpIk0MsbZV4pY2ZJEbyZSQfI9Qjc2tzZXEtpeW8kN1GdLxSqVdT6MrAEH5EdPwIIuDcf4ezHpjrv37r3Xvfuvde9+691737r3Xvfuvde9+690y57be3d00Rxu5cFh9wY9iWNFmsbR5OlDEadawVsM0ayAfRgAw/B9uwzzW764JWR/VSQf5dNSQwzKUmiV09GFR/PoOMf8fOjcVVpX4/qbYNNVozMky7ZxblWY3JCyU7pe5/px7WvvG6yKUfcJivpqP+fpGm07ZGwdLCIN66R0LsMMNPFHBTxRQQQoscUMMaxRRRoLLHHGgVERQLAAAAey4kkkk1PqejAAAAAUHDrJ711vr3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de697917phy219u57Ibdyuaw2PymQ2lkp8ztqqrqaOpkwmXqMdV4iXJ44yqwpq84zITwCVbOsUzqCAx96oD5dbqR0+squCrqrKfqrAMDY3Fwbg2I9761137917r3v3XuuDyJGrNI6IqgszOwVVVRcsxJAAA+p91ZlRWd2AQCpJwABxJPkB1sAsQqgliaADpspc9hK6SSGiy+NrJYSRLFS1tNUSRFdGoSJDI7IV8q3va2of1Hstsd72XdJZoNs3e1uJoyRIkEscjKRprqCMStNQrX1HqOlVxYX1oiSXVlLEjfC0iMoNa0oSBXgf2HpzWRH5Vlb/WPs06SdVxd176xHVmVziZQSVNfLlK7+F4qF1jnrVkcVMc7OwYU1Gsc6a5SrW1WVWbj3Hn3kPvY+3n3YeQNs5i5pVr7mW+jMe07HbOqT3bxgB2Z2DCC2iJHiTMraagKkjkIae2vsxzP7rc07ltW0Ut9qtpNV5uEqkxxK5JUAAgySuKlUBFaEllUV6JlmPkdvqtdxj2xmFhLN4hTUaVU6of0iWbIGrikkX+qxoCfx74o87/3rP3n+Zbi6HKabHy5Ylm8AWdmLqdFPw65b5riKRx/EII1J/AOHWdvL/3OvarbIov3uL/c7ig1mecwoT56VtxEyqfQux/pdBrlOz97ZbUK7dWakVgQ0MVdPSU7g/UNTUbQU7D+l094p83/AHq/vL8+ErzL73cxywEUaC2vJLSFq/xQWhghb80NM04nqZdk9mPa/l4htq5E2xJBwkkgSWQfZJMJHH7ekPNk2di7ys7ubszOS7E/kn6kn3A1wbq9nmu7yd5bqRizyysWdmPEszGpJ9TnqSYbKKGNIYYwsSiiqoAAHoAKAdQnyK883H+8j/b/ANPeltuGOlC2/ov+r8uoj5K9uSf8Qf8AiPbq23y/1fz6dEHDHRxPiz35mts5b+5uRr5Z8NIv3GJSaTV9jIJUWppIixLCnnWQOq/pRka36vfY/wDuzPfLf767372M5jv3uNrt7Ft02NpTVoFjkSO5tVYksY2EqSRJSkeiWhoygYYfeo9vLG0tdu5/222Ed1JcC0vwgoH1KzRSkYAYFCjHi2pK8M3ObWzkWcxsFVGwYSRq/BBNyoPvsH1hT0p/fuvdUC917nrcv292VW17SipG9dxUXjnLCWnpsXk6jGUNI41cGjoqOOL8fo9/J/8Aec3TdOafvEe9W8byz/WnmW/tgsg7kitbh7WCI/OKCFI/9r11S9ttottv5A5NtrQL4P7tt5arwZpY1kdhj8buW/PoN6KesydbSY2gilqq7IVVPQ0VLHcyVFXVzJBTwR34LyzSBRc/U+4b2vYL3etz27ZtqtGn3S7njtraFPikllcJGi1oKs7AD5noYXIgs7ee7unCW0SNJI54KqgszHHAAV6HOH42fIGoRJI+tM2quSAJqrEUz8MV9cdTkIpIxcf2gLjn6e8nbf7i/wB6i6jSWP2cvwrcBJNZxnjTKyXKsv5gYzw6jST3i9qomZH5ytSR/CsjD1wVjIP5dPsPxI+Rs0mh9hRUykEmWfdmy2S4/BFNn55bt/wW3+PsU2n93Z97O4mEc3tjHAlCfEl3TaSv2fpX0j1P+lp606K5Pfz2iRdS80s5/hW1vK/8agUfz6THYHx87Z6w2vNu7eWJx2MxENdSY9jFm8bX1LT1pZYNENDPOPGWU3JYEW+nsK+6X3LvfD2a5Kuufef9ksbXYormK1YRXcM8peY0QhImcaa8SSCPTo65V92OROdN6TYeXdwmnv2iaahhkjXSlNWZFXOfTov5yv8AtX+9j/em94ufR/0epSFr/R6Mn8cd71eK3KlEk7CCapR9Go6QzBFbgt9CE/Hvv3/dZbhe3HsHzVtlxKWtbPmi4S3B/AklnYysg9F8Rmf7XbrAf701jDa8+7RPGlJJtrjaSnmVmnUE/PSAPsA6up25VmtxdPOTcsiG5+puo5/Pvph1jR1XB8/8wYdxdcY7W4WDDZ6tCkjxaqytx8BZASbSEUA1G30A98Rf7225a55n9lNrLPogsNxuAK9tZpbRCQK/F+gK/LT1ml91SyDbTzjd6RV7iCOvn2JI2fl34/PqvsZX/av9ueP94X3yA+jPWWP0o9OjfdbfE/e3ZuxNv77xG5tuY+lz65B4sflo8rFUQRUGVrsWHaWlo6lJBUtQmRbADQ4599BPZv8Au5vcD3p9rOU/dDY+eNpsrbdRcMtlfxXKyRrBdT2wYtGkgYSeDrXAGhlNT1APOHvvy1yZzPuvLG4bNeSzWpjDSweEVYvEktKM6kaddD8welTN8Ge3Edvt9y9dzRAXVpcnuWGVjpuQYhteaNTq4HrN/rx7GF3/AHTvv3HLKLHnflCW3FNDSXG4xu2BWqDbJFXNQO81FCaVoCSP7znILKvi7Nu6t50jtyB+f1IP8umOb4Yd4Qxl412lUtcDxU+ekSQg/Vr1OPgisP8Ag1/YXuf7rj7y8MReOTlyZq00R30gb7f1LVFx9vRnH94z20kbSz36D+JoKj/jLsf5dNc3xD77hZRHt/E1IIuXp9zYdApuRpP3NTTtf/WBH+PsP3f92d96e3ZUh5Z2udSKlotxtgB8j4jRmv2Aj59L4vvAe1kgJfd50NeDW83/AD6rDppn+LPyFpxMx2BJLHFrOuDdG0JTIqE+qGFM/wDcvrAuF0av8L8ewrd/3d33uLT6hv8AWlEsUZPfDuW0NqAPxIn14kIPEDSG9VBx0vi98/aeYxqOa9LNTDW92KfIkwaR9tafPpH5bpTunBxvLkOtd3mOIM0klBiqjMRxoih3keTEiuVIlU3LE6RY88G0dcw/c++8ryvFJPuvsnv5hWpZ7O2N4FAAJYm0M9FAOWOOOcGghsPcr263JlS05z2/W1AFllWIkk0AAl0Ekny4/tHQV1NTV0NRLSVsNTR1MLaJqaqhkp6iF/rplgmVJI25+hAPuAdw2LcNqvLjbt0sJrbcIm0ywXCNHIhoDR0cBlNCDQgYPQ4hSG5jSe3lWSFhVXQhlI9QRUHrEMp/tZ/5NH+9n2hNmR+E9OfSnyH8ultsztTdewq1a3beZno1Lh6igeQy42ttpBFVRFhC7lVCiRdMqj9LD3Onsl94b3e+79vC7l7cc0zQ7e0niXW03Jabb7n4QfGtSwTWVUL4sZSdVwkigmoL5u9uOWedrU2++7YrzhdMdzGAs0f+kkArQHOlqoTxU9WQ9LfKbB75MGHzRjw24ggDUc0wNPXaB65cbO9vMLAs0TWkQX/Uql/f0Cfdc++r7efeOtYtjmVdl9zo4y0+y3EgKzhRV5bCUhfqECgs0ZAmjAbUrRr4rYN+5fs5zB7fSPfJW85bZqJdotDHU0CzqK6DXAb4GNKEMdIOLR11PWxLLDIrhhcaTcG4vx7zQ6h/qZ7917r3v3Xuve/de697917r3v3XuvEgfU2/1/fuvdM9ZuLAY6TxV+bxNFKSR46vI0lPJdQpYaJZUa4DC/8Ar+w/uXNvKuzSiDeOZtvtJzUBLm4hibFCcO6nAI/aPXpfb7Xud2niWu3Tyx/xRxuw/aAfTqJHvDacriKLc2Blka+mOPLUMjtYFjZUnJNlBJ/wHtHb8+8jXcyW9rzntMtw1dKR3duzGgJNFEhJoAT9nTr7HvUSGSTZ7pYxxZopAP2lentKumkCsk8TqwDKyuGVlIuCCOCCPp7FSsrqrowKEVBGQQeBB8weiwgqSrChGCD1nDK30YH/AFiD7t1rrv37r3Xvfuvde9+691737r3Xvfuvde9+691737r3Xvfuvde9+691737r3Xvfuvde9+690AHc3yP696VWOizk9Tl9zVVP9zSbYw/hlrxA1xFVZKaWSOnxlHK4srOTK4BMcbhTbFr7w33u/aj7uawbfzNcT3/OM8XjW+y7cFafQcLLO7ssdtExwC5LtQmON9LUlT289oObPcYvc7bGlvsyNoe9uKhKjisagFpHA4gUUcGZajoke4/5hO76kyrtbYu3cOpGmGTNV+Qz0yj6GQrSjARaz9VBDKp+usDnnBzZ/eue4N6J05I9qto28HCSbncT3zAebaYRYLqPEDIU8dY45IbR91DYIvDbe+aLy4biy20ccAPy7/HNPXgT5U6AncXzD73z4lQ71OGpnN/tsBjMZjdH0Fo6wUkuUUD/AKiD7xr5q+/z96nmppVHuKNssn4QbTaW0AX/AEsxie6H/OY9SbtP3ffa/atLf1c+plH47uWWSv2pqWL/AIx0Bm4Oxd47nLHcm7dyZ8OwZhmM3kskl1/SAlbUzooQH0gABRwLD3jfzR7je5PPOsc58/b1uyswYruN7c3C1HCiyyOo0+QAAHlTqTNq5S5d2QKNm2GztKClbaGOM/PKKDnzznpLU2dq8dUxVlBW1NDWU7iSnrKOompqiCQfR4Z4HSSJwD9VIPsN7Vebpsm4Wu67LuM9nukLa4bm1keKWNvVJI2DqfmCD0c3G22t7BJbXlqk1s40vHKoZWHoysCCPtHViPxs+W2YrZjtTsDJisqaKmaox+fq3RJquhg/z8GSeypJVUaWYTfrljuXuyl37pfcN+95vnuha7x7Z+7G6JNzXtdk1/ZbvMVRrqziIE63JoqGe1DK3ifFLEWaQa4nklwT+8B7LWnKkllzTylZsu0Xc4t57NASIpnzGYhk+HKQRp4I9AuHVVJd3x29P212buTd4LJjJqhcdgIHDKYsHjU+1oGZWsyT1iIaiUG+mSVhewHvld96D3jvPfr3j5m51M8jcuxv9BskT1pFYwMwhIUgFGnYtO6nIklZa0A6y39qfb+DkDkza9kESjc2UXF+60q9w4GupHERgCNT/Cg6DTAYbdG767+F7U2/ndzZJYjO2P2/ia/M1qwqyRmdqbG09TOsKvIoLkBQSBfn3EXLHJHNnOl+21cn8r7hu25hPENvtttNcyhagFikKSMFBIFSKVIz0ON03LZththe75uttZ2ddPi3UqRJWhNNUjKK0HDj0Pm3fh/8j9z6Xj6+qsNTMqE1O5cpicJ49diqtRVdd/FiwBubU502sbGwOTnKv3EPvOc0lHX24fb7UgEy7pcW9tStKAxNKbitMmkRpShoaAxfu3v37SbNVZOa47iXPZZxyzVp/TRPD/a+fLHQ8bc/lxdjV3ifdnYG0sAjWMkeGo8tuWpiU/VWWpTbdMZQP9TKy/4n3khyt/dZe4t6sT84e5Oz7cGyyWENxeuo9D4n0SFvsYj5nqMd3+9vyjba12Pla/unHA3DRW6n51UztT7VB+XTz2v8Qul+g+r9xdgb13dvDdOSoqZcft7FwzYrb+PzG58gssWLo3p4qOuyLQiVfNNoq1aOlhlazEAAW+6v3HfYT7vvtbzL7h87c2b3vG5W8P0+3WYeC0huL2UFYIyiRSTFdXe+mYFYkkajUFC/kj379wvc/nTaeV+XtgsLKzkYy3czCWd4rdKGRwxZEBp2rVCC7IMCvVVD5Am41Ej+vJt/yL3ydW1Pp1mutufJelx1nU1Em6qOWAkmC1ypuQZXVVFhz6lVj/sPfR7+7Q5Q3O+96OYubIoj+59r2SSGeU8PGu5Y1hj+1kilb7I/n1ix97jdbOw9v9r2V5B9fe7gjxp56IEZpH+xWdF+1utgjoWeql2xQmfVcwR31X49PI/2/vukOA65ydGC97691rkd91Roe7u26fyawOxt4zaiNJH3OerqrTbUf0ebTf8ANr8fT38sX3l9p+j+8P73xBtermrc560p/bXkstOJ+HXSvnSuOHXW72sQ3HttyHLpp/uotFx/RgRa/nSvSO2FnHg33sqeKQeWDdu3JY7i6iSPM0TpcfRgGUewV7XpJZ+5ft5eQqBNFvthIlRiq3UTD+Y6EfM1iJuW+YIZFOhrGdT9hicHrZo9/Wl1xu697917onfzuCL8c9yVDqWakzu1JomBYeN3zdNSlyFYBgY6lls1x6r/AFt7wf8A7w+0juvuu82l0JaK/wBukQ5wfq4krjHwuRnGfWnWQH3ZWb/XZ2qJWoJLW5VhjIETNT9qg/l1RCcp+fIf96H+8H387gs/l10x+k9R/g6HToTI+Xd1PZiSlRT8/X9RNufz+n32z/usZo19vfdKxowkj3q3mYn4SJLbSoBrWoMRrgChGTmmBv3vbR4eYuT56jw3spUA86pKCf5OP5/nfvsGTXgKPkH9mM8f8FHvqh1iB1Vp/MXyktP2bsak1ARR7HNQg4U66jO5OOQkn9QK0q2H45/r74c/3qLS3Hul7a2hp4EfL7yLjOqS7mVs+lI1/n1nz90m1R+T+ZpwO87kEP2LBGR/x49V7jL/ANWH+3F/94NvfLX6T5dZX/S/L/V+zrYE+KMZj+PPV13D+XBVNVqAsLVmZydUF+puYxNpv+bX9/Tl9zGzNh9172cty+qu2NLXh/a3E8tPy10+dK9csPfN9fuxzodNKXKJ/vMMa/zp0Yb3k91E3Xvfuvde9+691737r3XvfuvdJjc+ytob1o2oN27awu4qUqVVMtjqaseG9/VTTyxmeklUsSHiZHUngj2DOdPbrkL3F29tq585O23d7AigS/t45tPHMbOpaNhU0ZCrDiCOjvZOZN/5buBdbDvNzaT1qTBIyA/6ZQdLD5MCD6dEY7Y+COGyMdVlupcw+Arwskq7Wzk89bhqlhqcQUGWfzZLGs3CqJ/ukJtdoxc++Z3vj/dfco7zHeb57Gb0207oAzjZtxd5rOQ5ISG5bXcW5PAeJ468MoM9ZMci/ed3C0aCw58sBc2tQpvrVVSVRw1SRYjk9To0H5Meqx934HdGwc9WbY3hiK3AZygI89BXKFYxuW8dTTTRtJT1lHPpJjmhd4pByrEe+OfPXttzl7acyXvKPPnLtxtnMVvQyW1wBUqa6XjdS0csTUOmSNmRqHSxp1mbsO77JzPtdvvOwbhHdbbL8EsfCvmrAgMjr5qwDDzA6T8GcmppoqinqZIKiCRJYZ4ZpIpopY2DJJFJG6ukiMAQQQQfYd2y53PY9xst32XcJ7TdraRZre6tpHjlikU1V45Iyro6nIYEEHgejC62y3vbea0u7ZJbWRSkkcihlZSKFWUihBHEHqy34yfJyTNGHam66xf4zTRqIKqRljXKUyWXyhbhVrIv92qosw9Y41Kn0Lfcj+90Pfjl9+S+fLiKP3Y2yENI6gIu5WyhV+rRAAqzqTS4jUaQaSxhUcxw88vfL2bl9v79d82SJ25SuXooyTbSmp8JicmNv9DY54o2QGeyjG5CHI06TQurhlBupuOf+J95+dY+dOPv3Xuve/de6Yty7n2/s/DVe4Nz5eiwmGoVDVNfXzCKFCx0xxIOZJ6iZvTHFGGkkY2VSePYY5x505U9vuXtw5s523+22zl21UNPd3bhEWpoqjzd3Y0RFBd2IVVJIHRps+y7rzBuFvtWy2ElzuEpokUQqT6k+SqOJYkADJIHVfHZPzraSWfG9WYVIoFZ4zubckOuaYDUnlxuEjlVIF1AMklTJIzKbNAh98fvfL+9QvzPc7J7A8potqrFDvu+IWZwNS6rWxRwIwSAySTuxKkq9sjdZY8m/dhVUjvOeNyLSkA/RWZoB8pJiKt6EIBQ8JCOijbi7o7H3jLJLuLemdyCSklqRa6WhxoubnRjKH7XGx8gfpiH098yPcH7xXv57nzzzc7e7G93cUnxWqXDW1rxriztfBtV/KMcB6DrIDZ/brk3l6NE2jlq0iZeEhQPJj1lfXIfzbpGpkwbXsf6ni3+349wS1qw6EzW+f8AJ1KWuib6m3+8X/2/tkwuPLpowMOHHp/xW58zhnWTC53LYiQHUr43JVlAwN731Us0Rvf2L+V/cP3D5GcScmc87ztDg6q7Ze3NrnjX9CROincdg2jdVZN12e2uUOD9REkn/Hlboa9sfJrtfbzxiXOw7hpE4+1zlNHOxUk6rV1L9pkC5vwXlcA/i3BzH9uf7yf70HIk8Ee88yWnMm0qQDbb3boX017tN1bfT3Osg4aR5VBA7CKgxXvvsP7fbwrm22+SwuTwe0cgV8qxvrjp9iqT6+fRp9j/ADB2xlWhpN20FTtuqfRGaoMcjiWckLc1EUSVNN5GN/XDoQfqk/Pvpb7M/wB6P7Kc+PZ7T7l7bc8o79Iwj8aYm725mYhV/wAaijSWHUcsZoFijHxTEAt1AfNX3eea9nEtzsFxHuVmudCjwpwP+abEq9P6Llj5J5dGzw26MNnqWCtxlfSVtLUoJIKilqIqiCZD/biliZ45EP8AUE399J9o3jaeYNssd62HdLe92a6jE1td2kiTQyxtlXiljZkkRhwZSQfI9QNc2tzZTy2t5bvFdRnS8cqlWU+jKwBB+RHSgBBFwbj/AA9mPTHXfv3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de6bsvkocNicpl6hWenxWOrcjOiW1tDQ00lTIqX41skRA/x9lu8bnDsu0brvNypa3tLaW5kC8SsSM7AfMhcdK7C0k3C+srCJgJZ5UhUngC7BQT8qnrWv3lvzMb43Nnd25+paqy+fyNRkaxyW0RtM58dNTqzMYqSjhCxQx3skSKo4Hv5Lefeb+YPcnnTmTnvmq6M+/7pdvd3D50gse2NASxWKJAsca8FRVUYHXYLl7lvb+Wtl2zYdrgCWFrEsMYxU0GWY+bOasx82JPn0k/vpJZEijVpJJGWOONAWkeRzpSNEF2d3Y2AAuSePYZgspZpI4IImeZ2CoigksxNAABkknAA49HZhCqXdqIBUk8AB5k46EnbvTXc28Arbd6z3tkYZLaK0bfyNJjmuOB/Eq6Glx/I/5u+5l5V+7l75c6aW5a9p99uIGpSZrSWKE14frzLHD/AMb6B+7e4Pt/sGpd25x26GVeMZnjaT/nGhaT+XQ8bc+B/wAh88YmyeN2ztCOQ3ZtwbkpaiWOOxOowbZj3C2tgPShKm5AbTyRklyr/dvfeQ3/AMB9327aNliY937xvUkZVznTZLeZI4CoyQG05pGO7/eb9qNsDizvLy/kGKWtuygn7bgwCnzz8q4qFvyL+PW4vjtJs6PPZ/G5/wDvfS5iZJsXSVlPS0dVhZcelVSCWsIeqvHk4XDaIzyRp4uY3+8l91XmD7tknJMW+cyW25neIrl1e0ikjSJ7ZoQ6apCTJVZ0IOlfMU8yMvaj3X2j3XTf32vbJrUWLxKVmZWZllDlWomFzGwpU8OPRZky80DM0MzRO0U0JZDp1RVEMlPOht/YlglZT/gT7x52bcd22C5nvNmvZLe5ltbiykeM5aC6gktriI14rLBK6H5NUUIBEr3e0We4wxw3tossKSxzqr+UkMiyxt9qSIrD7PTpvfIH63t/W/H+9/09oVtfl0Yi3PmB1et8AeozsbqU76y9H4dydmyQZaJpVHmptpUquu3oFBTVEuRMstcdLWkinh1C6C3fP+729lx7de0Lc8btZaOZ+aHW7q47ksIwRZoMVUS6nnND3LJHUVQU5rfei57/AKy88DlqxudW0bODC2ng101DOeOfDoseR2sr0w3R8fefnWMnXvfuvdUBfP75BjsntKTYeBrDLs7rKoq8UHhkvT5XdhIhz+QuraJY8dJH9lCeQPFK6nTL74O/f197W9zvc08i7Jd6uTuWpHtqoe2e/Pbcy4NGEJHgofLTIwNH66g/dh9r/wCp/JScyblb6d/3hVnIYZjtuMEfqC4PiN/plByvRADkGdlRBrd2CoqguzMxAVVA1EsxNv8AX94M2e1XN9dW1jZ27y3s0ixQxRqWd3chVRVGWZmIAAySaDrJmYQWsE11cSLHbRIZJJHICqqglmY8AFAqSeA6O/8AHPraqyuUx4khZ38qS1BAJBkYi/J40xgBR9AQL/X39In3ZPZa29jPafYuU3RP6yT/AOP7zMprrvJVXWgbzjgVVhSlAQmugZ2rx895/cWX3L573PfI2b9zRf4rt0bY028ZOliPJpWJkatSC2mtFHV73XuAXBYOkpwukrCi2At/ZA5/rc+8hOoo6X/v3Xutar5ZTNj/AJG9uUzqsJ/vZUVOhSmnRW0lJWpL+2SuqdKgO39q7G/N/fzWfe92w2/3lfd5GhClt18WgpkSQxSBsYqwap86nOa9dd/YtVuvaPkOVWLD6EJU14o7oRn0K09MYx0A+IzkNJlsXVTTeOGmyNFUSyAOxSKGpikkcCMM5KopNgCf6e4E2NYbHe9nvZmKQw3UUrsATRVkViaAEmgHlnqT73b3msruKNKu8TqorxJUgDOOPW2b7+s7rhz1737r3RTPnMkr/FftbxadUUG0ak6jYeKl39tWpmP/AAYQxNYfk8e8UPvw2ct/91r3Vt4QC4jsJTX+GLdLKRvz0oafPqcfu3Mi+9XJOv4S10n5tZXKj+ZHWuOcqD/aJ/1wwH+9+/nUFl8h11lFpTyH7OjC/HPIebdsg18RzY5rD6gu9QpPPNjpHvrp/dc3Esdt717c8o8BZNpmjjxhnG4rI1aaiCI0HmBTFCTXBL76lmkUvtxdLGfEZb6NmzSimzKj0HxN8z+XWxD1o+vblGfr+xFz/rqv/E++s329YLdU6fzKstEvfe3qaKYl6Tq3b8VQmlgI5pNzbyqQvqChi1PPG11uObXuCBwr/vMfCu/fvlpY2q8PKlrG4ocMb7cnpnB7XU4xmnEHrpL90Gyf/Wx3eV0oJN7nZD6gW1ov5dykZ/wdV8jKj/Vf7yB/vBb3ztNn6g9ZT/SN6HrZc+LkccXx46d8SFFl2Hg6kgljeSsp/upXu5Y2klmLC3Avxxb39Nf3W7aO0+7t7NQxJpX+r9o9M8XjDsc/xMxPpnGOuQXvS7v7r8/F2qw3KVK44KdIGPQCnQ9e576jDr3v3Xuve/de697917r3v3Xuve/de697917oFu7+jdn957UmwO4YEpMvSxyybb3RT08b5XAVzgENE50PU42odVFTSs4jmUA3WRY5Egj3++75yL94PlCbl3mqzSLeYVZtr3aNFNxZytTKNgvC5A8WEkLIAPhdUdZE9t/cvf8A213uPc9qlMlg5Au7J2IjnT5jIWRR8DgVU+qllOvf2dsvc/Um9c1sTd9MKbL4ecKJoS70WSoZrvRZbHSuqNNQV8FnQkBl5Rwrqyj5wfdP2m5p9oOeN75C5vtBHutm/bIhJinibMU8LEDVFKuRgEGqsAysB1R5O5j2bnnl7b+ZthkL2FwtdLU1xuMPHIATR0bB8jxBIIJSWM3PWYivo8njap6WtoaiOppZo3ZWjlibUONXqRvoynhlJBuCfZDyZzJzB7f82bBzrypfta8w7bcpdWsyE4ZTlWAI1xSKSkiHteNmRgVYjow33lrbeYto3HY94tfF226iMUqEeR8wfJlNGVhlWAIyB1d58XO8affW3ceZp1WpMYgqINd2p6uH0VEJuAbBxdSfqhB/Pv6gPZb3U2f3n9tOWPcPZgES9hpc29am3uYzouIGqAf05QdJIGtCrgaWHXI33A5Mv+QObd35X3CrNbyVhlIoJYW7opB5dykVArRgy8QejzxyLIiuDwwH+8/8j9yn0DOkT2P2JtfqvaGW3ru6t+zxGKiHoj0PWZCsmOijxeNgZ0+5r62X0olwALu5VFZlAHuf7l8p+0XJO9c+86X/AIGyWSVIWhlmkbEcECEjxJpWwq1A4sxVFZgJeUeU95523+x5c2G38S/nbiahI0GXkkYA6UQZJ48AAWIBob7j+Qm8O69xNl9w1Jo8TSySrgNs0k8pxWFpXYgaVYoKvJTR2E9Wyh5SLAJGqRr81f3hvvDe4X3i+aW3vm26MGwwOw2vZrd2+mtIyTQgGni3DLQSzsoZyKAJGEjXp37fe1nL/txtAsNph8S/kAN1eyAeLMw+YrpjB+FAaL5ksWYhVHlRfh7f7H/ez/xv3jq1p8uh21r8uhm666i7V7RCTbK2dlcpj2kMbZqZYsZg0dL+Vf4xk5aWhlkhC+qOOR5L2Gm5AMze1/3Zvev3nCT+3vt/eXm1l9B3CXRb2YIJDUurho4XKUOpUZnHDSSQCAObef8Akjkqqcx8wQQ3VNX061kmoeB8KMO4B8iQB86Do1GE+CPa1VCk2Z3PsvDs4YmmiqMvlKmKx9KzGPGU9LqYj+xK4Atze4GY2wf3UnvLfwRzcxc88u7e7VPhRNdXLr6BqQQx1J/hdhSma1AhLcfvQcjQSPHYbLuNwo/GVijU/MVkLftUdPc/wP7DjiLUe+doVEwvaOphzVJGfSxF5o6OucXew/zZsCT+LEz3H+6V9zY7Z22r3S2Ca8zpjuIruFDg0rIkc7CrUB7DQEnJFCXxfej5Sd6XHLW4JH5lDC5/YXQcPn0G24viV3rtxJJodv4/csERbVNtnMU1S5VTYPHR5EYzJzB7XASBm/qB7gXnX+7d+9DylFLPZ8rWO92yE6n2W7jc0HmIbkWs7g+QWMt6qOhltHv37YbuyJJu0tnK3BbyJlH2F4/EjFPm1PQ9ABmKHP7ZrTjdx4fL4DILcmizOPq8bVWBtrENbFDKUv8AQgWPvDTmrkLm3kncW2jnLlbcNp3QCv02428ttJThUJKiMV+YwfI9Svt97te82wvNo3GC6tDwlt3SRfs1ISK/n1Fjyh/1Q5+vNv8AY8+wm1p8ulLWvlp/Z0IWyO1N0bDrVrNv5KSCIyK9Tj5i0uNrLaQfPTawPIVUDyIUkA4DAe599hvvKe7/AN3Pevr/AG/5gb9ySSiS92W81S2F1gAmSDUpjlKgATRNHKAAuspVSBOc/bflnni0MO82P+NBdMN1FRZo/sencv8ARYMvnSuerIem/kpgd9Rx46vdcZnURfNj53B8oH6p6KYhBUwC3NgHT+0oBUn6G/uw/fD9tvvL7WbXa3/dfuHbwiW/2C6cGQLwaa0logu7YNgsqq8dV8aOPXGXwZ9xfarmD29ufEuV+p2J20w3sYIWvkkq58KT0BJDZ0saEA11LVw1cayQuGVgCLG9wfz7y36i/qV7917r3v3Xuve/de697917r3v3Xuve/de6C3cvdHW+1KiSiye5KaavhbTNQYqKfLVMLC4KTCgjnjgkUjlXZWH9PZ9Zctb1fossNkwiPB5CEB+zVQn8uiO95k2awZo57xTKMFIwXI+3SCAft6TD92dU7wxuUwD7hlxyZfH1mMZ8pj67GxslfTyUrlameFaeJtMpsXdBf8+0vMHt/u+4bNum13Vrqtbq2lt5fBYMwWVGRqAGpNG8ur7Rzvs8G42N3DdaZ4ZklTxVKgsjBgKkUpUefWuHk3qMbX1uOqiv3NBV1NDUqja0WelmeCYI3GpPJGbG3Pv5Ct22C92Ldt02TcYtF/Z3ElpOmcSRO0bjIBwykZA+zruhYSQbjZWl/aHVazxJNG3qjqGU4xkEdGD+Hu8htn5I9XVEkyJBlM3PtmVXAIlbc+MrcFSR/UMr/wARroSpFvUovcXByY+5ZzB/VL7y/tbePKFt7q8k2yQHg31sEttGvyPjSIRTzABxUGLvfvYTvHtHzpCq1khtheLTiPppEmY/7wjV+R9etjL39JPXJnr3v3Xuq3f5m23jWdNbS3VEuqXbG+6elnbQCYsbuHE5CCeTXYst8jQUi2+jarnkD3zm/vLOVTu/s7ypzJEgM2176iOSOEN1BKjEHy/VjhFOBrXiBXLj7ne7fT8/b9srmiXm2mRc8ZIJUIFP9JI5+VPn1RW+T/x/25/2/FxyP9b3xFW1J66SC3+R6HT4y9VVfe/cm1tjBJf4GJznN31UOofZ7WxLxzZMmVReGbIs8dFC/OmoqUJ4B9z19272an96fdrlnk9on/cYf63dpFxos4CrS5GVaUlYUPk8ingD1G3u/wA7we2vIW9cxkr+8dH09ijfjuZARHjzCZkYfwo3Wz3S0tNQ01NRUcEVLSUcENLS00EaxQU9NTxrFBBDEgCRxQxIFVQAABYe/pStra3s7a3s7SFY7WJFjijQAKqKAqqoGAqgAADgOuOM881zNNc3ErPcSMXd2NSzMasxJySSak9Z/b/TXRQfmt8gk6A6byVfi6sQ773iZ9s7IRG0z0tZPCP4nuFPS4CbdoZfKhIKmqeBG4f3jB97P3r/ANZb2p3G92u50c5bpq2/ZwPiSRl/VuRg/wC4sZ1iooZDGpw3U7fd69rm9zufrS3vYNXLW36bzcSfhZQf04Dw/t3FCOOgORkdayMuRkdmdmLOxLM7szMzE3LM35Yn6k8n389ZhZ2Z3JLkkkniSeJJ8yeuwKWyqAqgADAA6E7qnbdRuTNx1TR+SmpJlihGkFJKx7EG1jcU8ZDc2OplI+h99DvuA+xq83c7XXurv1kG5e2FxHYCQVWXcGUMGHr9JGwc1H9pJCQaqaYe/e79zByxyvb8g7Tc6d73ZS92VPdHZqaEH0Ny4KD1RJAeI6vn+MXVkeJx1NXz09ndFfUyWNzyeTb6e+0YB4HrmV0fOKNYo1RRYKAP99b3br3WT37r3Wsr88nTF/LLt2kiLsprdqVbGRkuJMjsPa2QmUaVUaFlqmC8XCgXJPJ+ev76u2pb/ed90UjLFWksZTq41k22ykbgBgMxp8qVqc9dffuzBrz2P5FmkVQ2i6jx6R3tyg8zkhRX5+nRQTk2/q3+wb/ig94ti0+XU7/SL8utxjEVxyeKxmSaMRNkMfRVxiViwjNXTRTmMMQpYIZLXsL29/VXtt2b/brC+ZNLTQJKVBrTWoalfOleuC1/bCyvr2zDahFM8Wo4rpYrWnzp04e1vSTorPzZgWf4r9zqzMgi2xT1YK2uXoc5iaxFN+NLvAAfzYm1j7x1+9parefdz914XJA/dwkx6xzwuPyJXPy6mj7vEhi96eQCqgk3bJn0eGVD+wN1q4/xFv8AVf7wf+K+/nY+kHoeuyf0oHAf6v29GS+MleX3nUKTewx73/oFmnBH5Pq1e+oH92c4t9/927TQayWdhJX/AEkl0tOHn4n8usFfvw2hXZvb24rhbm7SnrqSA1/LR/PrZP6nm8m2qL+v28X+8KvP499ceud3VF/8y/MM3ybqqXRpFBsXalMrBv8AOCT+JV2siwCkGsK254W/598Kv7wom7+8HIpSng7JZxA141M0lfl/aU/Lrql90KxUez8U2qpl3K5fPlTw0p/xiv59V/DKH/faT/vJ94NfSH/VXrKE2g9Otsf4/QS03Q3SVNOFE1P1F1tBMFOpRLFs3CxyBWHBXWpsff01eyNrLY+y/tDZTU8aHlfaonpkaksYFND5io64je6EiS+5nuJLH/Ztvt+y19DdSkfy6F33KHQF6DbuXLzYDqDtbPU1bU42ownW2+cvBkaKWeCsx82N2xlKyKtpJ6UiphqaV4RJG8ZEiuoK829gL3V3KXZva/3I3eC8kt57TYNwuUuIWZZImitJnEiMneroV1KV7gQCM9C72/sY9z585J22a3SaG43ezgeKQKyuJLiNSjK3aVYGhBwQaHHWszSfKf5BUhcxd39qN5NIYVe+9z1wGm5Gj73I1KxHnnTa/wCfx7+eG09//fyy8Qw+83M5LUr425XcvD0Esr6ePlSvnw66+z+zXtfPpD+3Wyin8Flbp+3TGtfz6UdH8y/klQiEQ9zb0fwNqT7yvjyJJ1F7TGvp6k1C3P0k1C3Frcez61+9L946yEQh93d4bQajxXWXzr3eKj6h8mqKY4dFU/sH7S3JkMnt/t41Ch8OPR5UxoK6fyp68eh56/8A5mffe1qinTdzbc7IxaaEqIcvjKTA5doVa9qTLbcp6CniqStl8lRSVdxyVLer3NnIn94L78ctT26c1/Qcw7aKCRLqBLacqP4J7RY0VqY1PDLUZIJz1GfNH3QvbHeopTsS3W03pqVaCVpo6n+KKdnJWuaI6egIGOrfvjx8qer/AJH4qaTaVbLit046nSfO7JzLwJm8fH+1HJW0hidocthvuJQi1MViCVEqRMyoeqfsX947299+tsll5auHteYrdA15tF2VFxEMAyJpJWaDUaCRfOgdUYhesEvdT2W5x9p71F3uBZ9llfTbbjbgmJzkhHqKxS6RXQ3HOlnAJ6Mr7n7qIuve/de6IF/ME6Qh7C6nqexcNSFt5dXUtRlS8EWqfKbP1LLuDHzGNDJIMVEDkISxKxCKcADzMfeCH39PYy29yva6bnvarSvOPLUb3Ksi1aaxqGuoWoCT4QHjpXC6ZAKeIT1lB91v3Hk5V53i5Tv56bBvLrCAxoI7rhC4qaDxT+k1MsShPwAda/wy5/1R/wBix/4jn3wgNmPMHrqB9J8ul5szube3X8vh2rnpcLT5GriNbLTxxNVo2jxrJSzzxv8Aas4UB2Ua/StiOb9Yv7q33CtNv575v9od9PiWG6W/732xHI0LdWwVLlQvFmntirZqALbhnrBH78nI9zJynsfuBtZKXFjL9BesnxGCYkwsW/CI56rihJm+XRpqHem5t0QR1+V3NuDJzyKGM1bmslUyE/Ucy1L2sfpawFuPx7+giwjtY4VWC3jSP0RQB/IdchtwM7TM08rO5PFyWP7TU9Ap2P2Rmc1VjbUufy9dgsHUs0dBV5Wuq6EZYI0VTVpTVFQ8KTQK7QqwXUBrsbOffzUf3mn3gG93Peef265fu1PIfKUj2Y8HC3G5YW8ncqdL/TsPpoqjs0TFTSZq9lPub+zh5E9tbbmvdrdl5o35FumD8YbQ5t4gCO0yLSV/Usgb+zHQdx5Qi3r/ANfkj/eT+ffM5rPiadZdNa8cY6t0+I/wyoq7EYrs/uXGtVnIxQ5Da+xK1HSmSikCy0mX3RAwSSolqks8NC37SxEGcOX8UfXP7nn3D9nuds2v3T979oFw1wi3G1cvXCkRrGaFLi/Q0MjOKFLc9gQgzB2bw48FffX7wlza317yb7f3YjMRMV7ucZBbWMNFbHIULwaT4tVQlKamtRpqano6eGkpIIaWlpokhp6amiSCnghjUJHFDDEqxxRRqAFVQAB9PfXK2tbayt4LSzt0itIlCRxRKFRFAoFVVACqBgACg6wmmmmuJZJ7iVnndizu5LMxOSSTUkk8Ses3t/pvr3v3Xuve/de6YdxbW23u7Hvid0YLFZ/HSXJpMtQ09bCrcWkiE6OYZlIBDoVdSLgg+wtzfyPydz/tEuwc78r2G7bM+TbbhBHOgOCGUSK2hwQCGWjAgEEEdGu0b5vPL92t/sm6T2t4P9EgdkJHoaEah6g1B8x0Qjt74N0c8dVmuncg1BWAPMdnZuseWgn5v4cPmp9dVRyaeEjrGmRmPM0a/Tlb94D+6+2PcYb7mL2A3M2e45kPL+5Sl7d/PRa3b6pYWp8KzmRS1KyxLwyl5B+8zcRPBt3uDaiWDCjcLZKOPnNCO1h6mMKQOCMeq2M1SZva2XrcDuPGV2FzONmNPXY7IQPTVVPKLEakcamjkQhkdbpIhDKSpBPGvmrkrmLknfty5X5t2O527mCzkMVzaXSGORD5YPxKwyrCqupDKSpBOYe23e3b3YW+6bTeR3G3TLrimiIZWHyI8wcEcQaggEddUOfqaGpgrKOplpaqmkWaCogkaKaGVDdXjkUl1YH8i3tDy/u++8o77tfM3LG6z2PMFjMtxaXdsxSSKRThlYUPyI4EEqQQSOqbjs9lulnc7fuNqk1jMhSWKQVVlPEEH/UDnj1ZX8c/kkNwCLb246hIs1Toih2YJHkIQApqYl40SCw8iAWUkEcGy/R19zP7322feL5dfl/mXwbP3Z22BWvrZKKl7EO3621StaaqCeMA+E7KQdDqBzz94vaK79u79dw24PLyrcuRDIakwvx8GVvsrob8QBrlTWwWgroa+BJoXVg6g8EHgj/Dj3nH1CPU337r3Xvfuvde9+691737r3RRPkJ2jk6eqfYO2KyWiYQI+5cjSuY6nTUorw4elnjIen1wMHqGWzlXVAQC95F5P2GB4xu19EGz+gjcMcXI888P2+nUec3b7MjttNjIVNP13XjkYQHyxx+2nr0UanxJ4sgUXvb+p+pvb6m/+xPuRGm+fUfrCaeg6fKfEAi2i9xa5FhyLf0/4j2naX59PrCPTqqnuijO2+z96YkhUVMxLXRqvCrDl4YcxEqryFVI64AACwtYe/lG++RyYnJ33oPenaI4QkMu9SbkiqMBdxRL8afID/GeAwOAoBTrvf8Adx3f+s3sf7a7mWLuu2pZuxyS1mzWjV86kwceJ4npDbX3hUbW3Ttrc9K8gqdubgw2epzDYSCfEZGnyERjJIUPrpxa/F/r7gvlLc5eV+aOWuZbfV9Rt24W9/Hp46reZJVp5VqmOpe3nZY952bdtnnUeDd20ts4PDTKjIa/Kjdbb1HV02QpKWvo5VnpK2mgq6WdQwWamqYlmglUOFcLJE4IBAPPPv6pLW6gvrW2vbWQPazRrLG4rRlcBlOaHIIOeuGlxbzWlxPa3CabiN2jdT5MpIYYxgjqT7UdM9Fa+a22Duv4u9w0SRrJNi9s/wB64WK6miGz8hRbnqpEIIKk0GKlQn/UMb3Fx7xy+9tyyvNf3dfdOw8PVJb7f+8kPmpsZEu2I/2kLD7Cepn+7zvI2T3l5EuGekc939Ew8j9Uj26g/wC3kU/aB1q5vXMfyB/hyf8Ae/fzsi2HmOuya24p1sK/y2ujm686gfsrOUhj3V2v9vk6XzR6Z8fsqkMn936ddQvH/GHlkr2Km0sMtPcXj99xvuF+zQ9v/bB+ed2tNHMvMmm4XUO6OxSv0yZFR4xLTGmGVoq5Xrlt97b3GHNPPS8o7bPXZdk1RPpOHu2p4zGnHwgBEK5DCSmG6sc9529YndY5ZYoIpZ55Y4YIY3lmmldY4ooo1LySyyOQkccaAlmJAAFz7pJJHDHJNNIqRIpZmYgAACpJJwABxPV443ldIokLSMQqqoqSTgAAZJJ4DrVn+afyMf5A905jM4uqkl2LtXy7W2JFykUuJo6hzV57x3AM248hrqAzKJBS+CN+YgPfz7feo95JPer3T3Lc7Gctyjt2rb9nXgGiRjruKDzuZKvU93h+Gp+CnXZj7v3tUvtf7f2G3XcKjmO9pebk3EiVlGmGvpAlEoMa9bD4uim0a1WSraagpE8lTVzJBCvNtcjAanKj0og5YnhVBJ49wfynylvHOnMmycqcv2vjbzuFylrbpwGpzSrEA6UQVZmp2qCTw6lrmHets5V2LdeY96n8LarKBrid8fCgrRRirMe1R5sQBk9Ww/FrqL7mfFwiAvBS+MtIym80pOuadueDJIxNr8cAe/o59rPbvaParkPlvkTZFBtLG3CSS0o00zEvPO39KWUs1PIEKMKB1w99wuddy9w+cd85u3QkT3cxaOOtRFEvbFEvyjjAFfM1Y5J6vA2hgocJiqanjjVNESg2ABJ0jk29yH0DOlb7917r3v3XutZj+Zb5KH5abyZ3j01239lVcIUsWWNduUVERICFCv5aNiALjSRze4HCv79ti6feJ5gmYArNYWMi08gLdY6Go41Q+uKddd/uiFbj2R2JUBrHd3aNX18d3xxxRh6Zr0Qb7/8A2v8A33+394di3Poesm/AP8P+Hrco6xrDkOtuva8ziqNdsfadYalXWRag1OBoJvOsiEo4m16gRwb3Hv6b+Rpzdck8nXLS6zJtVpIXBrq1QRnVUYNa1r1wR5yg+l5v5qthHoEe5XMegimnTO4pQ8KUp0uPYp6DfRdPl3TGq+MHfCLT/dGLrDdlYY/EJdC4/GTV7VOkg2+zWmM2r+xo1cWv7hX7xtqbv2H924RD4hGw3cmmlaeHEzlqf0AuqvlSvl1K/sXMIPeL22Yy6Ad3t461pXW4QL/ti2mnnWnn1qQmv/2pv9v/AMUYX9/Ot9NTzHXcD6cfLox/xeyV+wpYfIwLY5ZhHdvWIa+kQvzxdPP/AK/q99Ev7uWdYfcjn2wM1Hl2NZhGK58K6hUt6dvjAf7b7esI/vy2BHIPJ98Iaqm8eEZMY8S2mYL693hE/wC1+zrZz6Ym8u2KG3/KvHf+v6R/vNx77A9cxOtfX+ZPldfy539Tfc+X7HD7IpvGHD/a69oYet8DAE+It935dJsbSavoR74TffnY3P3jOalE2rwrOxj0g10VtIn00/DXXqp/Sr59dfvukWZX2N5al8HT4lxePWlNVLqVNXz+HTX5U8uiIff/AO13/wB9/gfeH/039HrJT6c+nW471FTJRdT9YUcbM8dJ15sqmjd7a3SDbeMiVnsANTKlzbi/v6Z/bm3Wz9vuRLRGJSLZrKME8SFtogCf2dcGOe5muOeOcp3ADvut25A4VNxITT9vQh+xl0FOgD+VOQOM+NXfNUsYkLdS78o9JYoAMltzIY1pLgHmFasuB+StvcPfeDujaexfu/Kqai3Lm4Q0OMS20kRP5B6/OlOpN9lrUXnu57awlqU3uzkqM/2c6SU/PTTrUlFf/vrk/wDEW9/OF4HoP8PXcD6f5dCTh+u9356hpq7E09JVx1cKzwxJVCOYq/0VlljSMOByfVa3595Xcs/cq96OcuUNi505dt9ruNr3G0W8t4zdaJdL1orLJGqK9BU95X+lXHWOPMH3nfanlbmbd+Vd8nv4Nxsrhrad/py8epQCWUxuzFc0HbX5Uz0ndw4Hc21Jo6fceHr8S81zC1TEPBPptrFPVRu9NOUuNQRmK3F/cH8/+0PuH7W3sNhz9yldbbNLXwnlCvDJTiI54jJBIV8wrkioqBUdSxybz5yT7g2kt7ybzFb38UdPEWMssiV4eJDIEljB8iygGhpwPTn152dujq/eWA35szJyYvcW3K+KuoJwS0Mun0z0VbAroKvHV9OzQ1ELHTLE7Kfrf2Uckc28xe3fNWzc48qXxt98sZhLC4yreTRyLjXFItVdThlJHRpzRyjs/OOwbny1v9mJtqu4jHKh4ivB0NDpdGoysMqwBHW2Z0t2jh+6erdldnYRBBR7sw0VdNReZZ2xmUgkloc1iXmUASvisvSz05aylvHqsL29/Rz7X8/bb7o8gcrc+bUmi23G1ErRVDGKVSUnhJHExTI6VxXTWg4dcRvcHk2+9vuc+YeT9wbVPZXBjWSlPEjYB4pAPLxImVqZpWlT0KHsfdA3qNWUdLkKOqoK6CKqoq6mno6ylmUPDU0tTE0NRBKh4eKaJyrA/UH2xdWtve21xZ3cKyWs0bRSxuKqyMCrKR5hgSD09b3E1pcQXVtKyXETrJG6mhVlIKsD5EEVHWoP27tV+su0+wuvpGdhs/eG4MBTyyFw9TQ4/JVEGOrPVZrVlAscov8AUP7+Zb3M5IbkP3C515NNSm27ncWkbH8UccrCJ8ivfHpb8+u6vI+9pzfybyvzOigfX2EF0yina8kas64/geq/l0HMlfdG9dtPrB139SEOvFz+R7F/3dua5/b3309qeboJFRLXe7ZJ2bh9PPILe6FcUJtpZAD5E1INKdB33j5Si5w9q+f+XZIizz7XO0IH+/okM0B+dJo0NPOlMcejZbJ3b9hsfI5hmDS43F1E8IkI0PUrARSo314kqCi/ng/n39Pnu57hn2x9nPcrn+Ohutq2a6urZTwa4ETC2QnNA85RSaGgNaHgeCvt5yQOf/c/kbk5h/i+4bnBDPTiINYacj5rCrkDFSKVHHot65aR2Z3dnd2LPIza2ZmN2Ys3qJJ5J/J9/IjdrcXlxPd3czy3UrtJLLISzu7EszMxJLMzEkkkkk1PX0Qpt8MEUcEESpCihERAAFUCgUAUAAGAAMDo6PwX6ppu7O98PQ5mnWr2rsyjk3ruSmmUNDXw4yppYMViZlc6JIa/M1cHmjs3kpo5VtYkjKD7m/s1Z+7HvVs8O9Wqy8sbPGd3v43AKyiF0WCFhUArJO6F1odUaupFDUQH94/neb289tdwudvlKb1fyDbrRxxRpFYySA+RSJW0nFHKnrZU9/Qn1yL697917r3v3Xuve/de697917r3v3Xuve/de6L9358etp954Boa1IsRvDH08g27uyCFTVUr+p0oMmqgNkcLLKfXEx1RFi8RRi2rGP7y33XeRvvG8sta7rCllzvaxMNq3qJAZYmyRFOBQz2rN8UZNVqWjKsSTKvtd7r777aboJLdmn2CVx9XYse1hwLx+UcwHBhhqAOCAKUN7wwW5Ovd0ZfZ+7cfJi89hKk0tbSOyupOkSQ1FNMhMdTSVULrJFKhKSRsCPfzd8/+3PM/tpzbvPJPOO1tacwWEpiniJBU4BWSNxUSRSKQyMMMpB66dbBu+081bNY7/sd0J9suU1xSAUPoVYHKupBDA5BFD1DxG56vD5CiydBO1PWUM6VFPIpK2dD+lrFSySC6sv0ZSQeD7b9vucOYfbDnblrn7lW6MO/bVdpdQNkK1MPFIFILRTRlo5Fr3Ruynj0xzHyvt3M+yblsG6wB7C6iaJxior8Lrxo6NRlPkwB8ursfjn2mN24WjWWUs7QxNZmuw1Kpsf8AEf7D39Z2w7xa8w7Hs2/WVfo760hvIg3HRNGsi1+elh1yD3Gxl2zcL/bbinj28zwPT+KNip/mOjfg3AP9QD7NukfXfv3Xuve/de697917qtbPwTZLcu4cjU8zVmcys8pIu3qrZlVefpoRQth9Le5ysykNlZwp8KxIB/vI6hK81TXt3M/xtK5P7T1xgxg/1F7W5Yce7tN6nptY/QV6eIcdyCRf/WH4t/Xj6e07Sn1x0+sRIz1VN838I2D7UxeTjQRQbh2rQzu4Wxeux1bXUM9zaz6aNabm9+bECwvwG/vP+Uv3d787BzNHGv0+7bBCXIGTNbTTQvXFDSHwaGtfIgUBPYf7hO8jcvaLdtkkYmbbd3lVQeAinjilWnpWQy4p865IBLnrCfqxP+x/3i3HvnALf5dZxiEAcOtrv4pbu/vz8cOmdxtIJZ5th4XFVkoNzLkNtwnbWRlY8/uSV+IkLD8MT7+kT7u3Mbc1+xvtZvUj6p22a3t5W9ZLZfppD9pkhYn59cUPezYv6ue7PP8AtSrSMblLOg9EuD9Qg+wJKKfLowXuZ+ou6Y9z4Km3RtvcO2axtFHuLB5bBVT6BLppsvQVGPnbxsVWTTFUE6SQD9PZTv20wb/se87FctS2vbSa0kNK0WaNo2NMVw3Dz6Mtm3OXZd42reLcVntLmK5QVpVonVxnNMrx61T/AI4dH5juvv3bnVE0UsVFSZiqqt91EIe+L2ztuqH94pC7BTDLVMi0VOxWwqqmK4sT7+er2Q9nNx9zveHZfb2eJltYbppN2dRiK2tX/wAYOaULkCJDT45EqKV67T+7HuLY+3vtpu3OqOrTvbqm3IxH6lxOv6Ap5ha+Iw/gRqdbYlHSUuPpKWgoaeGkoqKngpKOlp41ip6alpolhp6eCJAEihhiQKqgAKoAHv6Jba2t7O3gtLWFY7WJFjjjQAKqKAqqoGAFAAA8h1xLnnmup5rm5laS4kcySO5qzMxqzEnJJJqT1I9vdNdVlfzNfkkvUvU6dXbbyIg332zT1NFUmnlZazC7DibwZ3IXikV4JM9If4dBqFpIWqipDw3GEP33/eb+oPt6ORNku9PNXMKPE5QkPDYjtnkqCCpnP6KVwymWmUxl990L2mPO3Ozc57ta6uXNkdZEDAFZbwisKZFCIR+q1MhhFXDda3DVp/1X+2t/vXBv74qrAPJc9dYxDXy6M98dNhVG4MomcmgL+WY0eKDKWNtRSsq0BBszG8SEEHiQHgj31L+4J7KiGHcveffrEeK+uw2MSLkKKrdXS1/iP6CMKGgnHBgeudX31vdUGWx9ptlusLovN4KHzNGtrZqegpM4IpmEg1BHWxD8dOtodvYWkqJIAkrRIblRfkBr3IB599PKevXPPo3iqFUKPoBb3vr3Xfv3Xuga7h7x2f0zi6epzrTZHNZJZP4NtrHPF/EsgIuJKmVpCI6DGxOQrzycajpRXb0+xFy9y1f8xTsltRLZP7SZ66R8h/E1PL9pHQe3/mOw2CBXuCXuHFY4VpqPzNfhUev7AetZ/wCeHZk3Zvez7wnwkGBkyW0MFF9lBWz1waOiqsrSQzyVE8dODM0MKowjjSO6fS5Yni9/eOcpw8vfeEtYIWd/H5es52kYU1N4t1FUCpFAIwMeYPnXrrp9wPfJOZvYia8lRF8LfLuBUUg6QI7eSjHFWJkJyBgjyp0S41/+wH9bkf72D7wK+hP8P+DrNvwB/D/g63Aegd8rVdDdJ1MGPYJUdR9bTxmWpAbRLs7CyLrRISA2luQGIB/J9/QZ7W81K/th7cPFZHSdh28jU2c2kPEAH/D1wu9zeWzF7le4Ucl3ld8v1OlfMXUowSf8nQptvCuJOilpVH4DeZyP9ciRL/7Yexs3M0/4bVB9pJ/zdA0bBbfimevyp/mPQOfITP5LLdB94YvRQwjJdQdl4/y+KoJi+82XmqfyW+450eS/0/HuPPdjd73dPa73K2zREq3OwbhBqoxp4lpMlfi8q9Dz2u2q0svcz27vNUjGHfbCXTUZ03UTU+Hzp1qCff8A+1/77/b++BI2/wCXXcz6ceh6Md8Wsgf9KUSg6teEq1P14tkMU9xa/N195wfcEja096d6ULiXl25jJ9P8asX/AMKdYaffmtA3s9tEhJHh7/buPnW2vVp/xqvW010TL5NrUJJuftk/6F99ih9nXJfrW1/mK5lKv5md2SRBo1ir9n0JVyNXkxvXe0MdK403GiSWlZl/Oki/PvhF975V3D7xfuTcohA8W0izTjFt9pET9hKVHy67WfdWsDb+wXt8jsCzR3UmPSS+upAOHEBgD8+iU/f/AON/+Qv+KD3jV9A38PWQf049Otyra+azGP2zt2g/bo/scFiKP7QUkEQpftsfTw/biIRAReDRp02Gm1vf0R7JvG42ey7RZiNIxFaxR+Hppp0xqumnlSlKdcFt526wut43a6zJ4lzLJr1sdWp2Oqtc1rWvn0ol3VlgAC1OxH1LQ8n/AF9LKP8AbAezYcxbgPKP9h/z9FR2SxNe1h+fRaPmfvLIp8We7g5o6ZJtlVVI8qCSNylZV0dI8KtJOyaqlJjGBa512HJ9wx94zmG9m9jvcyBhGiybY8ZZag97KpGWPxA0p516l32A2C1PvL7esviOy34cKaEdqO1cKD20r+XWqoK8fgk/7En/AI174Smzbrs4bf0r1cn8NdoUG4sNtYVUKOsuIx8nqGrmWCN2/UOCS3+wv7+hb7vUEdv7He1EMYIX9w2bGuctCrNx/pEnrhZ76O8nvJ7mGQ1Yb1dJ+Syso/kB1Y52l8S9n9j7Byu3KqjhjbIY6ZaOtSJGnxmRELfZZOlsoIqKGchxYjUAVa6swIr9yPb/AGD3P5L33kvmO1SSxvIWVHKgtDNQ+FPGT8MkT0YHzypqpIIZ5B523n285s2fmzY52W7tZQzoCQs0VR4kMlOKSrg+mGFGAI1aMtHWYPK5PC5EGLIYfIVuLroQ9xFWY+plpKmMHi4SeJh/sPfzj7psl3tG57jtN4ii8tZ5LeULkB43KMAcVGpT13p2+e33Tb7Hc7NtVpcwpPESKEpIodSfnQjrYM/lI7/jyPRW9dqZGrCna/Y9XPjjO7hI8duDB4ip+2RnvGipkqOplIuOZibfk9c/7vzmUP7VcycvX06qLHeXeAsafp3EMTaRXGJFdv8AbfmeYf33+WXt/cbl7e7WCovNpVJdIFS8E0o1HzJMboP9r1bDFWUkxtDVU0p/pFPFIefpwrE/n3n0k8Ev9lMjf6Ug/wCDrCd7e4jFZIHUfNSP8I6k+3emetWX+Y3SQYL5hdrxUqpHDkV2ZmPFHrOifIbG249c7l2Yl6mvSWY29I8lgABb3wb++fssNh94zn1oEAiuRZ3OkVwz2Vv4mTXLSBm/21B12Y+6ncS7l7E8lPMS0kX1VvqNMql5OEAoOCppX1x0R8ZBv6/7c/74+8WvpfkesiPpv6P+r9nQ1UmXaHrDMR6iBPNjYLrY+n7+mnsSeQpENv8AG9vp7+g777/MVzN9zPmC4SRhJui7QkhUg1D3VtcMNWO1vDoacQaHBI64lfdP5dgH3p9rtSgK7cdzZAwpQpBPADT1HiVoeHHiB0GCV/09QP8Ar8f7b6f717+eJrc+nXadrc5xjq8X+UJiYJMP3fudlVqmfJbJwMMha7RQUdLuLIVKIugFFqJK+IsdR1eJeBY6urP92vskMO2e6+/FK3ElxY2at6LGlxIwApjUZVrk10jApnnV9+m+lW99utoBpCsV3csPUs0CKSa50hGp/pjxri5r30/6wC697917qjz+abvfs7Hb82dtI1GWxnVtXtNMhQpSSVNNidw7kbJV0OaTJSwyLBX1eKpI6QJTyhvt45vIoHmJPIT+8b5j9w4+beVuWfHurf24k27xohCWWG5ujJIs4mKkLI0SCPSjfAG1Ad9eujP3MOXuT7nlnft8WOCbnJL0xSlwrSwQCNDFoBBKJIxerL8RXST2UFXm2t/7q2lWRZHa25c/tqvjdZI67AZivxNWrqQVZaigqKaYG6j8/j3zf2Pf+Z+Vbtb/AJX5iv8Abr1TqWaxnlgcEUyGidDXA8/LrMfduWtm3y3e03naba7tWFGjuYklUj0IdWHn6dHu6g/mUd1bElpKDfT0XaW3I2jjljzQTG7pggDMzmj3JRQf5TMdZJNfBWM1godBz7zL9rPv8+8vJEtrY86mLmbl9SAwu6RXirXPh3Ua95yf7ZJScAMo6xt57+6T7ecypPc8upJsu7GpU21Xty1Ma7dzRRjhE0Y86Hq6Hoz5H9WfIPCyZPYGb1ZKihilze1cqsVFubB+XSoatx6zTJPSGRtC1VPJNTM3pEmq6jrV7Oe/Xtx747Q+48k7sTfworXm23IEd3b6v9+RhmDJXAkQvGTgNXHXPz3I9pedPa3cEtOZtv8A8TkYrb3sFXt5qZor0BV6ZKOFcDNKZ6Hf3M3UadFD+Ufy22h8ecOcZTvR7h7KytK7YXayVClMZHJG3gzm5hE4mo8WstvHFdZqwgrHpUSSx4n/AHm/vU8rewGytYWgi3H3HuoibLa1YUiBU6bm80nVHAG+FcPMahKAO6Tv7Mexu+e6l+L2cSWnKELgXF4VoZCCNUNvUUaSnxNlY8FqkqrUG7w7J3P2HuTJbu3hmqnN5/LSrLV11UVHpjURQU9PDGEhpaOlhQJFFGixxoAAPfz8c+c381+5PNG584867xLfcw3bBpZ5aDCjSiIoAWONFAVUUBVAwOunuw8p7PyrtFpsWwWCW21wLRIk4ZNSzE5ZmJqzEkkmpPTTSV0tRLHBDdpJmCoBf6n8mwLaABcm3AF/aHkzkLffcHm3l/krlmzM++bndJaW6AMQC57pHKqxWKJKySNQhI1ZzhT0n5k3TbeV9i3TmHeJlj22zhaaVjQVCjCrUgF3aiqOLMQoyR1bZ8PaWuj8FxJ4VWNV/Vb08CxN7W459/Vby/s9vy9sWy8v2bE2ljaQ2cRbjohjWNa1JNdK+p+3rjDud9Lum5bhuc4AmuZ5J3A/ikYufTzPVqcFxDGD9dC3/wBe3P8AvPs46Q9Zffuvde9+691737r3RMd/bVfB7syieLTSZGeXK0MljpaGrkMssak3u0FSzKw+v0P5HuU9mvxd7bbtq/URRG4+a4/mM9RdvG3m13Gcaf03bxE9KNkj7QcdJyKhUWuCef8AbAcfS/HPteZR0iEdMdOEdJ/tPPHP+w/3n2y0hPTqx+YB6rk/mN7aaPavXG7lXSMdn8tt6aQL6m/juOiyMAZ7fojO3ZNNzwXNvqffKv8AvR+Vxfcm+1vOKRVkstzudtdwM0vIFmUMQOANkaV4FjTieui/93nvhi5p9w+Vmf8A3K2+C/RSfO1laJiBXiRdrWgzQV4DqpR6wflif9ibf634F/fGMW59OurAgPWx5/Ks3n/eT4zT7fknd5tib/3JhIqdySIMdlosduqB4vUyiCavztXwLHyK9xyCe233AuYf3r7FvsrzEy7Tu9zaqh/DHMI7pSv9FpJ5PTIbHmeUP30Ng/dPu7FuaRgR7ltcFwzj8UkRkt2rwyEiT8iM+Qsr95vdYj9e9+690UL42/GSg6W33392JVRU75ztjsvcOVwxQxyth9iS5Spy2MxiOry+GStymQnmmUNdoY6YOA8ZAx39l/Y6x9sua/drnGWNDuvMG93Fxb0ofBsTK0scQNTQvLI7tnKiIMAV6nX3a937n3A5b9suVYJGG3bLtEENxWo8W8EaxySEUFQkaKqmmGaQgkMOje+8iOoK6Yt0bmwezNuZzdu5sjT4jb228TkM3mslUsRDRYzF0stbW1DgAu/ip4WIVQWYiwBJA9lm9bxtvL20bnvu8XawbVZwPc3Ez8EjjUu7HzNFBwMngM9GWz7RuW/7rt2ybRaNPul3OlvbwpxeSRgiL6CrEZOBxOOtO/5I985r5Cdw7v7OzDSwU+WrPs9uYuRwy4PauO1U+CxMYB8ayRUg8k5UASVUssn1c+/n394/cDc/dz3D3/nbcQVjnk8OzhbPg2sdVhiHlUL3N6uzNxPXdz2n9t9u9r+RNj5PsArSQR67qYDM1w/dNKfOhbC14IFXgOgewFKM7nMXhzVw0gyFZDTNU1EqxRRI7XchpCqNMUBEa39bkL9T7J/b3kpOdudeWOU5dyhs4b+8jt5LmdlRI0Jq7am7S+kEIv430qMno7585ifkvkzmXmuPbZryWxtJLhLaBWdpHUdo0rVgmogu34EDOcKer4fih1LTSvjPFTIlJQxQQU8YGrTFCqqoJPJchbkm5LEk+/oY5d2Ha+V9k2nlzZLRYdnsbeO2tolHwpGoVa8Kk0qx4lqk5PXAzft83PmXet15g3m5M263tw9zcSHzeRizUHkoJoAMAUAwOrk8FjIsZQQU8SKgWNVsBb6D2d9FPT17917r3v3XuqI+7N312+O3d9ZyulkkSHP5HB4yKQkpSYfA1c2MoaeJbKqIy07StYDVJKzHkn3k7y3YRbbsW220SgExLI5Hm7gMxP5mn2AdY18xX0u4b5uNxIxIErIg9FQlVH7B+0nqrv5bk02/dvzaxpn2hTRBCOQafM5li17m+r7gfji3viP/AHn21a/evkjctdfE5Xig0U4eFfX71r56vG4UxT547cf3YMwl9k+dbLwjWLmmaXV6+JYWC0p5U8L86/LJUzXf74H/AIoffNr6D+h10oFuPQ9bbfxRrZsh8Z+hqicqXHVGyKVSq6R4aHAUVDTgj8sKenUE/k8++z3s5LJL7U+3Zk+JdntY8ekcKov/ABlR1xJ96reO193PciKIHT++rt8+rzM7f8aY9GB9yV1GPSB7Wp46zq7smkmVniqtg7xp5UUsGeOfb2RidVKWcMysQLc/09hznCFLjlHmmCQVjfbrlGA8wYXB/wAPQm5LleDnHlOeNqOm52rgnyInQg9abJrv9f8A2BP/ABB98Q/of6HXeL6Y/wAI/YejC/F3JIvb2HiZ2BqKDIxKPwzJHHU2b6cBYCf9ce8svuXgWnvdYrUhpdtu4lA4E6FkoflRCftp1iL99yxeT2Kvpgi6YdztJGr5As0dR86uB9hPW198fKlW2rROzBVWmQsSbABUuSf6AAH32FUVoq58h1xoJABJOOtUv5b72qt5/JPuHc9WyrJlt4VU8SKOIqKKmpabHQf4+CggiS/JOm598SPvWbaYfvC+6VuQP09wWKvCuiCFK/adOfn13K+6koufu7+1V0qmk23GfJ4eJNK9AfQFqD5dAFjXORyFBj0lEb11ZS0ayNcqjVU6QK7KvqKqXuQOfeP9vtYubi3txhpHVAc41ECv8+p8ugLW2uLloyVjjaQgHjpBNP5dbqXvu/1wC697917onXz+r4sb8Q+5aqYSFDjtrUg8YUsJcjvza2PgY6mQBEmqlLG9woJAJ4MHfeSkSP2T57LglWigjx6vd26D8qtn5dTt92a3e698eQ4kpXxbh8+iWdw5/Oimnz61bxkP9qY/7E++QP0A/h67FG2FOtg/4I0rLhNoCUetduYFXsbjWMZShgCOCNQ+vv6BPaO1ex9qvbKxlp40PL23RPThVbSFTQ+eR18/Hu1cRXfur7mXUFfBl5h3GRK4OlryYio9aHq6eNoYccJJ5I4oIqZpJZZWVIoo40LvJI7EKkaKCSSbAD3ILukaNJIwWNQSzE0AAySScAAdABEeR1jjUtIxAVQKkk4AAGSSetIjsvd1HufsfsDcuOa2P3DvfdedoQDcfZ5bO19fTeopGW/ZqF5sL/0Hv51+c5Lfe+b+at6tx/i93uVzdR+fbLO8i5oK4br6IOUNkn2blHlbZ7o/41abdbW0nl3RQojeZ819T1eN/KdwlZT9K793NUKyU+4OxXoqBWJ/dgwOAxSy1SDQB4nq8nJFfUSWhYWFgW6E/cs2aaw5B5m3KQUiut1KRj1EMMYLcOBZyOPFTgefPD76u4wy8/cs7RG1ZbXa/EkPoZppKKc8QsYPDgwyfK1D3mT1hp1IiqqqD/MVM8N/r4ppI7/6+hhf2/HdXMVPCuHWnoxH+Xpp4YZcSRK3+mAP+HrWT/mMbiTJfLvsxRMaiTHUeyMdPOZVn8k8Wxtu1Eq61ZiGpzU+JlPKvGQfp75Dfevl/e3vlzbMW1vHHaQs9QalbSAnh/Dq0nzqD111+6vtb2nsfyj+lpWV7uVV00opvJwMY+KmoHgQQeiQiv8A99cD/iL+8cDt/wDR6yF+lP8ACejDUlLJP1TuCSJDI1FHjKvgH9ENfSLO49X6UpmZje9gD77v/ek5Vn3P7k24bdbfqz7dte0XQNCCVt5LQSvQE6aQl28xQEcc9cPPu4cwxWn3xbS5uP0odx3PdrYgmtGnjumjStM1lCKKUqSPs6BVK8/1uf63/wCK298BXsSPLrtobceQ6u1/k5dh0aZ/ubrSpnC1uWxW2d64aFpHBkhwdVkMLnyqMxiZwc7jz6Qr6VN9QA0dJ/7uvmOG03T3I5LuJAJ7iG23K2UkgkQtJDPQHB/touGaA1qKU57/AH8uV7h9r5B5thjJtoJ7jb52pwMypLDU8afoy8aipFKE5vh99TeubPXvfuvdIrf/AFxsbtPbdVtHsLbGK3Xt6sIeTH5SEv4Z1Vljq6GrheGuxlfErsEqKaWKdAx0uLn2FuceSOUvcHY7jlvnTYLfcdlly0FwtaMODowIeKQVw6MrDyI6EPLHNnMnJe7Q75ytvE1luiYEsJ4jzV1IKSIaZVwynFR1T73b/KlydM1Vmug94x18JaSUbJ31MtNWRKSGWDEbppIPtao+oqkdZTwaVUaqlyT75n+6393XcRm43T2f5kEiVLfurdiFYDFFhulXS3nQSotAMyEnrO728++rZzCHb/czYTFJQL+8NuBZCfWW3Y6l+ZjZ6k4jA6ql7C627K6jzBwPZOzM/s7J6nESZeieOlrljOl5sXk4zJjctTKePLSzTR3/ALXvnZzt7Z88e3W4naud+Vrvbb2p0C5QhHpxMUo1RSr80Zh8+s1eVubuU+d7Abnylv1tf2eNRgcFkrwEiYkjb+i6qfl1C2N2Puvrjc+K3lsnO1u3dyYadZ6DJULqsiH6SQVEUqSU1bRVCeiaCZJIZkJV1ZSR7LOUeaeZeQuYdu5q5Q3eax361fXDPCRUeqspqjxuMMjgowwwI6Ucx8q7JzZs97sPMO2x3e03C6JYpBg+hUijI6nKspDKcqQc9XB5v+arQydH42TA7eKd8ZGCoxGVhmpGXaW3qiCGJf74UjTPOMpDX+bVSY8sWinSQVBMSR/c9ON5/vDbc+0li+z7Kf8AXjnRrW4R0Is7Z1UD61SxYTLJWscNaq4YS9ir4uCW3fctmX3FuxuW6V9tYmWeAq3+MzqSf8VagHhlKUeX8SldFGZvDqDz+9c/u7O5Tc25svWZzP5uslr8rlsjO81ZW1Up9UksjEgBQAqKoCRooVQFAA5V8xbrvXNW87lzFzHuU15vl5KZrm6uGLPI7cSSfIDAAoFUBVAAAGde2bBtmx7dZ7Rs9jHbbZbxiKGCJQFRRwAA/aTxJqTUknrjjpqzI1UNHRxST1EzaURACfxdnb06EX6ljYD8+1fJvt9zP7h8ybbylyhtEl5vl04SOKMYAr3SSN8McSA1d2oqjJPRTzRvmxcn7Jfcw8xbhHbbVbrqkkc8T5Kg+J5GOFVQSxwB0c7prpnJZmtpdULzzytH55gjmNbsLwwlhcRj8ki7nk24A7u/dk+6tyt93/Zv3jciK/8Acq7h0bhuYBKRqaMbazDAMkAIGpyBJOwDOFUJGnKP3r98d591tya0tg9pybBJqtLIkanIwJrgqSGlIrRQSsYJC1Op2u26Q6vi2fiqbVEqyGNNXp5vweePeWQHrx6gfoygFgAPoBb/AG3vfXuu/fuvde9+691737r3Se3HtrG7nohSV6MrxM0lJVxWFRSTFdJeMkEMjjh0PpYf4gELbG/n2+XxYTg4ZTwYfP8AyHy6RX1hBfxeFMMjKsOIP+riOgSres8/QysKeGLJQX9E1LIkchH4108zo6MB9bFh/j7F8O/2MqjUxjfzDA/4QCOgjNsF9E1EUSJXBU/5Dw/n1zodhbgndVOONMt/VLVSxRqv41aVZ5DY/wBFv71LvNjGK+PqPotT/kHXotmvnIHgaR6sQOiy/wAwXqWln+JHYOSQGuzm1qnbW6YZgmmOKKhz1BR5RYE5KImGyNU5cgs2gA6QTbDL77u3S84/d95wWOMatvkttyiXz/SnRJGJ8iIJJD/LzqMufud3EXK/vjyssklRuEdxt8rcBSSFnjUDzrNHGP8AVTrWRas/xP8Ar/T/AG3PvgytoT5fy67XCD5dXX/ya97Ebg7v6/mkZhX4fae8cfDrGiH+D1uUwuXkVLglqj+OUIZgOPEAfqPfTH+7s3trfcvcrlSQnTLBa7hECeBieSGU0/peNH/vPXPr7+3L9dq9vOZkQAxXFzYSHzPipHLGCf6PgyU/0x6vk99R+ubHTXVZrGUlxLVxFxqHjiPmk1L9VKxatBv/AKqw9objcrG2qJbhdQ/CMn9grTpbDt15PQpAdPq2B/Olfy6T1TvBBdaOkZuBaSocKAfzeKPUSP8AkMeyWfmaMVFtbk/NzT+Qr/k6NodgbBuJwPkg/wAp/wA3TBU7jy1TcfcfboTfRTKIrf60nqmH/JXsnm33cZsCUIPRBT+Zqf59GcO02MVD4WpvV8/y4fy6YK2KPJw1NNko0yFPWwy01ZBWotXDV088bRTwVMU4kSeGaJirowKspIIt7JrkC9jlivB4sTqUdZe4MrCjKwaoIIwQcHo0t3e0khltGMUsbB42jOkqymqlSKEEHIIyD1Q583P5f9bscZbtrorF1Ffs0NNX7q2FRLNU5LaxlleSbJ7apo4nes2xEGvLTAmagUal10+rwc5vfv7sjbAbznP28si+x1Ml5tqVZ7epJMkCgVaAeafFGMiqV0dI/u9/eatuYzZcle412se/4jstychY7igAEc5JotwfJvhkODR6a6hGq/8AG3+8f8aJ94braU/D1nCIfRQP9X5dWn/Bn53U3W+Zxuw+2qsDA1M0dLht61LFnxckjxR09BuKQg68cTfTXMS0Bt5rx3kj6Kfdv+9VNYCw5D91NwZ7LEVjvMxJaPgqQ3bcWj/hmJqvCQle9edn3lfugfXjcOf/AGm24Le0M1/skC0WTizzWa8BJ5mACjZMXdRG2Vdr7qx24qCnq6KpinimiSRHjdXVldQyurKWDKwNwb++kisrqrowKEVBGQQeBB8weuYzKyMyOpDg0IOCCOII8iOlb7t1Xr3v3XuqTfkl1tkuuu2txvNTyDBbuyOQ3Pt2u0n7eojyc7VmSoRJyoqsZkKh1dCdXjZHtpYe8j+Tt4h3bYrTSw+pgRYZU8wVFFb7GUVHzqPLrHjm7aZdq3u71Kfp5maaJvIhjUj7VJofyPn1UZ81f8n3DsWq0BRUYXKwCYaQZDS11PIYz/aIiFWCL8evj8++Sv8AeZ7br559sbzwB37VcRa/M+HcBtP+18Sv+2Pz67L/AN1VOJ/b73WsvGqYt4tpfDNaDxLYrqHl3eFT17c+XRJfvx/qj/tx/wAU98y/oQOCnrquLc+R623fgrWRV/xH6LqIZTKg2b9sXIdbS0WXydFPHZwrftT07Jf6HTcEix99X/Yxlb2m5I0NULaFPzWSRSM+hFOuJf3jYHtve73FikSjfXa6Y4PFGwOPUMD/AIc9Gy9yx1CnTTn6SfIYLNUFMFNTW4nI0lOGYIpnqaOaGIM54VTI4ufx7RbjBJc7ff20Q/VkhdFr6spA/mel22Tx2u5bfdTE+FHPHI1M4VwTj7B1o+GuX8H/AGPpP/FPfF0WJ9OvoXFqf4T0PHxkybL3dsqJSAtTJmYJNQHKjAZScBTfhjLCtv6/T3kR91bXZ++XJ1CAkiXkbV9PorhhThnUo/wdYvffM22OX7unPkzI2uB7GVKep3C1jNfUaHb/AA+XW3R8bZBPtejRgHVoFVgbEEFbEEf0IuPfX9WNQRg8R1wyIBBB4daivycip8F8i+8sBT1H3MW3+19+YBZrSLrOD3JkcU/DqjemSjI+ljbi4sffFT3+mj3n3s909zjysu+XZNa4ZZWVhn+FgR6Yxjr6Avu4bLNtXsH7PWMy6WTl2xIpTKtAjq2P4lYN6iuaGvQfddzQ1vYGxqKe7QVm8ds0syB3XVFUZqiikUMpDKWRyLjke402Pbkk3vZ45F/Ta6iVh8jIoOfs6k3mdHt+WuYZ4yRIljO6mnmsTkfzHW7J77PdfPz1737r3RBv5mtfNQ/DnshImVY6/LbBo6nUoJMK762/XKFJ/Q33FFGb/wBAR+fcCfeXeQe0HMECfDLNao2K4FzE/wDx5B1kr90a2juPfblVnHdFBeSJ9v0kyZ9e1z1q3DIE/wBsf7cE/wC8ce+X5sT6U/LrsR9OfQdbB/xC7v6R2Th8KNzdvdbYNcfhsdHMMrvbbVLVAwUUSOn2smRWoedSliioW1CwF/fa3lX3O9rNo5Q5as5vcfY1a2262iZTfWpcGOFFIKCXVqFMila1x1wP5t9nfeXeOc+Z72D2n5iK3W53MyOu23gjIkndgQ5h06DXBJpTNeoPzq/mmbEzGwM70x8b8nW7grt0Y2bCbs7OjpqvF4jGYOtiNPlMPtWOvp6bJ5LKZKmeSCWt8cNPTwsWp3mdxJDjJ94H70uy7hsG5ck+2lzJcTXkZgu91AaONImFJI7cOFd3cEqXoqqK6CxIK5b/AHbfubcy2HMO1c++69nHawWUq3Fls7MskskyHVHLclGaOOONgGWOrM7CkgQAq9Ee1sRn957iwm09r4ypzO4tx5KkxGGxdFHrqa7IV0ywU0Ea3sup39TMQiKCzEKCRzz27YL3eNws9r2y1aa/uJFhhiQVZnY0AH5/s4nrpJvF/t2w7XuG9bxcpBtdrC0880hoqIgqzE/YOHEnAqetvv47dQ0nRXTGw+sKeSCpqtu4dTnK+nUiLJblyU0uU3DXxs6rM9PNlqyUQeS7pTrGh4UAdfPbbk2DkDknYOVYirS20P68ijDzOS8zDgSDIx01zpCjy64b+6XPE3uNz7zJzfIrJBdT/wCLROcxwRgRwoaYDCNRqpguWPn0NXsc9R/1737r3WnZ8iuyYuyu9e2d8Ucxmx24N97hqcRLrD+TB09fLQ4Nr8A3xFLDx9B9PfGr3I3Ec08+c3cwRmsFzfzPEf8AhQcrF/1TC9d1va7lRuU/brkrl6eOl1a7bAk4pwlKBpf+qjN0D0FW080UKEl5pI4kHH6pGCL+T+T7DeyctT79vWz7HbV+qvbqK0joK900ixriorluFR0Jt/3C15d2He+YLtf8UsbSa8l8uyGNpGzmnapzTHVkPT+2IdxbZy+Fqwftsxi6zGzta7IlbTPTtIn0tJGH1KRYhgD+Pf0s71yftvN/JXMXI1/H/uq3HbJtscHJCSwtDqHmGQNVSKEEAgg56+YTZ+cNx5R505e53smrum37lDuSeQZ4Zll0niNLkEEGoKkggg9ELzVJkNuZnK4HKxGnyWHr6rHV0TXstRSTNDJoP0eJympGHDqQwNiPfzLc2cm7pyfzJv3Ku+Wpi3fbruWzuUIIo8TlCRXirUqpGGUgjBB6+mPlffdo5z5Z2HmzYZxNs25WkV7bSKQaxyoHWo8mFaMvFWBU5B6EvpDuvcvRnZ+0uz9rTP8AxHbdf5Kii+4kp48xiKuJ6PMYapkjuywZPHTyR6rMYnKyKNSL7W+3nNm7+2vOWx85bG7C8s5asgJUSxMCksTEfhkjYjzoaNxA6JvcPkDaPcXlDe+UN5UfSXcVFcqCYpVIaKVQcao5ADTzFVOCets7pf5Cbe7o2Jht/bFzNPmcNkYRFU0tQqfxHCZSONGrcLmYozHPTZOgeQBgxKyIVkQvG6O3arkL3UseeuXrHmPYb1LixlFHRwBJFIANcUgFCsiE5rxFGFVIJ4oc/wDtdufIHMd/y1zFYNBfRNVJEromjJOiWImqtG4GKcDVWowIA2028KduKulliNh64WWZSf7RKt4mRf8Ako+5Fg5lt2oLiBkPqvcP8h/w9R3NsEozBOrD0bH+Ctf5dKKlymPrLCnq4XYmwjLeOUn68RSBJD/trezq3vrS6p4FwrH0rQ/sND0UzWV3b1MsDBfXiP2io6n+1fSXpObr2ftTfeEqtt7023hN14CssanD7gxlHlsfI6BhHN9tWxTRpUQ6iY5FAkjblSDz7JeYOXOX+a9rn2XmbZbXcNol+O2vIkljJoQDpcEBhXDDI4gg9G2yb9vfLW4w7ty9u1xZbnH8E9rI0bgYqNSEEqaZU4PAgjqoX5JfyrcdXR5DdfxuyRxWR/eqZes9yV5kxFWxOv7fa+5KtjU4qSwslPkXmhd25qYEAHvnP71/cB2y+W73/wBl7v6a9JLtst7JWFs1021w1WiPokpZSf8AREGOs6Pab7591btbbL7s2njWuEXd7RKSL5ariBe2QerRBWA/0Nya9Uj7kw24tl5/J7W3bhMlt3cWFqno8rh8vSTUNfQ1KWJjmgnVZArowZGF1kRgykqQTy637lneeWt1vti5g2uez3e2cxz21whR0YeRU+R4gjBFCCQQeuhm07htW/7babzsl/FdbVcIJIZ4GDo6nzDKSPkRxBqCKjprTIC36iOf68f7zf6eyNrY+meljW/Vg/xw6vxO6o8dUYl/vlrfG1VXMtppJVa0lO0epvthBJdfGCbWuST6j3n+6V7Z+1vJvtjs/MXt5dLuN9u1ur7hvEi6Z5ZFJ1wFKt9OlvJVPBB4rqdpG7zxx+8lzv7hcxe4G67DzrbNY2u3TstntiNqiRGA0TB6L47TJRvEI4Giqg7ReL090zi9rY6llamj8oRW1FV/I/rY+8q6dY79GXhgjgQJGoUAW4HvfXus3v3Xuve/de697917r3v3Xuve/de697917r3v3Xugu7u2cewunu0NjrGJZd2bC3ZgKZSuq1ZlMHXUdFIqggmSKrmR15BDKOfYQ9wNgHNfIvOXLJj1Nf7XdWij+lLC6IR8wxBHzHQt5C37+q/PHJ/MhfSljudtdueHbFMjuD8ioIPyPWkm1afw3+2/41Yj388K2Y9OvoWFvwrjqwH+WF2FJs/5bbVo0qBDHvfbO79nTF2fwyeTF/3lpIJVV01iXJbZgCA3Xy6DbgWyj+6FvknLPvVs4ik0rf2lzYNqrQ6o/GVTQ5rJAtAcaqdYy/e95Xj372S3qVo9T7fd21+tBkUk8BmBIxSOdq/0a9bN9VVV9ZcVFTK6G14wRHEbfS8UZVCR/Ui/vrXcXV/c1E05Kn8IwP2CleuRkNtaW9DFEA3rxP7TnqB9t/h/vv8Akr2i8Bv4R0p8QfxHr323+H++/wCSvfvAb+Ede8QfxHr323+H++/5K9+8Bv4R17xB/Eevfbf4f77/AJK9+8Bv4R17xB/Eevfbf4f77/kr37wG/hHXvEH8R6pR+dv8t9suMz3H8dcKseY/dyO8OrcXFFBBlAPLPXZ3ZdOHWOHKEeqbFxgLU2LUwE1oZsJvfP7tC3Rvecfb2wC3RrLebXCAA/EtLbrwDeZiAo2Sgr2noD93L71YsfoORPdHcSbLEVjvMxJMfAJDdNSpj8lmJquBIdPetBM87QySQzK8U0LvHLFIrJLFIjFXjdGGpZEYEEEAgjn3g0LNlYqyEMDQg4/b10njiWRVdHDIRUFcgg8CCPLqyj4RfzCc/wBB5HGbD7Frq7M9WSSw0lBXHXU5LYqtK15IURJKrJbfUyfuUw1S06C9OCAYXzF+73946/5Caz5O51me45LqI7efLS2VT5UBaS3zlMsgzHgaDhF95r7otn7jx33PPt3bR23PwBlurXCRbhQD1ISK6xh8LIcSUJ8QbRvXfZO3d/7fxeewGVosti8rRU9dQZChqI6mlrKSqiWWCop54mZJYpY3BBBII99OrG+s9zs7XcNvuo57GeNZYZomDI6MKqysMEEcD1yC3Hbr/Z7+82rdbOW33K3laGeCZSkkciEqyOrAFWUihB6EsEEXHIPtX0i6Sm8tj7V7Aws23934akzWLlYSLFUKyzUtQoKpV0NVE0dTRVcYY6ZInVrEi9iQV+3bnfbTcrdWFw0cwwacCPRgcEfI9Idw22y3W3Nrf26yQ8aHiD6qRlT8x9nWtB/OQ6W2x0nk+gana2Qy89Lu2DtJJaLLz01UaH+AS9evF9tUx09PNIk38cYESamGgeo3PvBf7+m5XfMt57XXt4iCVIb+H9MEAgNZtXJOTq/l10+/uwdkt9osfenb7MsYfH2uer0JBddwWmAMDw/59UnHJf7UP9gR/wARx759CwH8P+Drqx9N8v8AV+zrb2/lp1hzPwi6LrjEIrUG9aHSH16hiey954oS3sljOKLWRb0lrXNr++mXsHEze0nKPaBRbhf95u7gf5OuIH3sbcWP3gvcS38Qn9S0k9P7SwtZKflqp0en7b/D/ff8le5g8Bv4R1jr4g/iPXvtv8P99/yV794Dfwjr3iD+I9aFWdaLF5vMYuGWV4sblchQRySsPK8dHVzU6NJpATWyxgmwAv749SbcI5ZU4hWI/YevpC2/VeWFjduoDywpIQOALKCQM1pnoV/jfk1j7w68J1MGy9RCB6f1T4rIQIfqOA0gJ/w9y97Aoln7w8izspp9UyY9XhlQcfQtn5dQD97Xb3m+7p7oKpAZbOGSprwS7t3I88kKQPn1uN/F6o1bbox9f2lH1/wAt/vHvrkOvn8606/k9uA5T5K/IbKMngbI95dtV7QLIzrCazf24KgxKxC61jMlgbC9vfFv3DjN/wA/c8XxTS028XkpUVoNdzI1K/KvX0ke0G2Cx9pfa6zDFli5d22IMRSuizhWtK4rTqH8dJKjKfIPonGUg8lVku5OsKCmjLrGJKir3tg6eFC7sqIGkkAuSAPz7Q8nbXLcc38qwQrWZ9ytkQE07jMgGTgZ6Ve6PhWftn7i3c5pDFsV/I540VbSViaCpOB1vB/bf4f77/kr31n8Bv4R189niD+I9e+2/wAP99/yV794Dfwjr3iD+I9Vr/zW8Zlq/wCJeRoMJi8rmMlV7/2YkNBh8bXZSqkSCXIVk7vT0ENS6QQwUzMzuAgIAvqKg4/feVsp7j228CGB3d9wgGmNSxwJGyFBwKcTj86dZX/cxurO296ra5v72GC1TbLotJO6RqKhFAq5AJJYAAZ/IHrVkrKDceNgNVkcLl6CmDKhqK7G1tLAHc2RTLNBHGGc/QXuffPF9pmjGp4GC+pUjrsVBd7bdSCG13C3llpXTG6MaDjgEnpp/iR/LD/ff7E+05sP6P8Ah6WfTfL/AFft6Mv1H8Ufkl3dkKWj2D1Ju6qoqiREk3LmsXVbb2nSIzWeao3Hm0ocW4hUFjFC8s7AeiNiQCM+W/aznXm6ZI9i5duZIyaGd1McK/6aV9KD7K19Aeon5295van2+tZZ+ZOc7FLhQSLSCRZ7lj6LBEXkFeFWAX1YDPWxX8J/5e+1/jDCu9d4V2P3x3HXUX28mZp6ZhgNnQVCMtZjtopVpHVy1FSjmOfIzJFPNF6I44I2lWTOb2h9hNt9uyN63WSO85rZNIlA/TtwRRlh1CpZhhpCASO1QoLauXH3gPvObv7vOeX9it5Nu5Fjk1CBj+tdFT2vclSVCrxWJSyqe5mdgpWxf7b/AA/33/JXufvAb+EdYs+IP4j177b/AA/33/JXv3gN/COveIP4j0Rv+YV37SfHv437rr6WtFPvXf8ABUbB2PDHIq1aZDN0k0eVzcSkuyR7ewhmqBJpKCq8CNYyL7hv305vHJnIW5mGQLvF+rWVoARqBdSJJAONIoyTXyYoPPrIf7sXtrN7m+6uy280BfYNsZdy3BiDpKRMDHEeAJml0rStSmsj4T1qN/xP/G3+x/4offL/AOg/o/y/2eu2303Qy9EbWHYfY+IwswmbH0sVTlck0BEc0dPSIsdO0b2aztkqiBfoeCTY2t7nr7s3J7777ycqXBgDWu2SHdpiwqB9PQwkioH+5BiHyrXy6xb++PzXFyb7B84xfUMl9vCrstuFNC31VROK5/4iJMf5efWwb0p8Xdt4faFfu3O9hLtTbeGx1Rlsvlc7QUIoMTjKKBqiqra3IPXUMEMFNChZ3YAAD32lPuNabDYXW5brBFFYwRmWaeSXQiIoJZmLKQAB8+uAEft5uHMu42W07M0s+5XMqw29vFEZJJHc6VRFVqszE0AA6pD+VfYHWu9u489k+rJa3I7apI4MR/emupExb7yqsbrp33FDiCGlx1DNEqQ0wmdp5aeGOSRYnYwpxN+9J7h8pe73uruXNvKOwfS2phS2muamt7JFVBcsmlSlYwqLXuKIpah7R3z+6V7Qc7+zns9tXJ/PO/fVX/jyXUNrpxYRzUc2gkDMJKSFpGp2q7uqlgNRLwlef9V/seeP9jf3jU9j8s9ZLNbnPb0YHoD5N9nfHLdabm6+zJSjqpIF3FtbItLU7Z3RSQM2mny2PWWIieJXYQ1ULR1VOWbQ4VnVhv7f8/c2e2W7/vXlq90wuR9TaS1aCdRXtkSoyKnSykOtTRgCQYz9y/aTlD3U2Zto5n2+syA/S3kQC3Fux/FE9Dg0GpGBRqDUpIBGxD8bP5gvRnf8VDhcjk6frLsWYQxSbQ3XkYIaPJVjq2pNr7jmFHQZoM62SF1pqxri0BHPvor7a/eE5H5+S3sb2dNq5jYAG0u3AR29IZyFR/kraHNaBTx65d+633Y/cT21e4v7S2fd+V1qwvbJGLxqPO4gGp4scWGuMebjh0ff7b/D/ff8le8gPAb0HWNniD+I9OdLX5Gj0iKpcxrYeKU+WPSp/SA7Eop/2kqfZjb32429AkxKfwvkfzyPyp0jms7OepeIav4lwf5cfz6UVLuMGy1dOUP5lgOpb3/MTnUqhf6Mx/w9nlvvgai3MOk/xLkfs4j+fRRPs5FTbzVH8LYP7Rg/sHT/AAVVPVLqgmST8kA2dRe3qRrOvP8AUD2cw3EM41QyBh8uP5jiOiiWCaA0ljK/4P28D0Sr5o/Dna/ye2TU1mNpqLDdu7dop5dm7oASmGRaNTINr7lmWNmq8JXMumJ3BkoZmEkZ0GaOXHD7xv3d9g97eW5p7e3it+fLSMtt99QLrpn6ec074npQE5jbuU0LK2QX3f8A353j2f5hht7yaSfkW6kAv7PLeHXH1EAJ7ZU/EBiRe1hUIy6qGXpcttzMZTb+eoqnFZvCZGtxGXxdfE1PW47J46pkpK6iqoXs8VTTVULI6kXDKR74abnsF9tN9e7XuVo8G428rwTwyAq6SISroyngysCCOu0NjcWW62Nnue3XKT7fcRLPBNGao8bqGR1IwVZSCD6dG2+GfdcvXXZ+OwtfN/uB3XVQ0ZDsNFJmzZcfUpq5X71gKZwouzNGT+j3mZ9yL3Yu+RfcFfb3cpz/AFX5glCRqxGmK+C0hcehuAohYDLMYq4XrEL74ntJBzZyJJz3ttsP6xbFGZJGUZlstVZkNOPgVMyk/Colpluto3rnc9NuDC0s8Lq2qJPpza6g/UfX32U65KdCT7917r3v3Xuve/de697917r3v3Xuve/de697917r3v3XuuEiho3U8gqR/vHv3XutIP5H7Y/0ed+9zbKVNEG3Oy9546gURmINi1z1bLiJFjJJiWXGSRPpuwGqwJHJ4K+53LI5c9x+etjVf0rbdrqOPFP0/GcxmnlVCDTP2nj19DHtLvK80+2Ht/zCTWW62i1llzX9TwUEor50kDD8uA4dRfjvvs7B766c3izlafAdlbOrch6wpfEnO0UOYhD6W0GfFyzJqsbar2PvXtxf/wBXOfeTd8p+nbbnbyyD1QSr4gr5VQkdKvdDl0cy+2/Pewqv6t1tN1HHUVpJ4LmI0xXTIFNPl1umfbj+h/2x/wCK++3H059OuBGs9e+3H9D/ALY/8V9++nPp17Wektvfde3uu9nbo35uutGO23tDBZPcWbrGAJhx2JpJayp8KM6eepkSLRFEDqllZUW7MB7K983Gw5d2fc993WUR7daQPcTNj4UUsQKkVY0oo8yQBk9HPL2ybpzTvuz8ubLb+Lut9cx2tvHnLyMFWpzRQTVjwVQScDrV563/AJl/aeyvkjvTuLLGuzuwOx9wiXdXWkte8tLQ7bpdNDgRtqSdzT47cO2cLFHFHKBHFW6GWcetZI+ZnLf3gObNl9xt65yuC8+y7lcarvbixKiIdsQiJwksMYCq2A1KNg1HYHmv7pnJvMHtRsHItksdtzJtVrpst2CAM07d83jhRqeG4lJYrkx1BTgQ2zR1P2n1/wB37Gw/YvWe4aXcu1s0jeGrp9cdTRVkQX7vFZahl01WLy9A7hZqeZVdbhhdGVm6S8q8x7FzpslpzBy7erPt0uAQKMjD4o5FOUkWuVPyIqCCeSHOvJnM/t7zFfcrc27W9pvFue5Gyrqa6ZI3HbJE9O1lJByMEEAR/tx/Q/7Y/wDFfYi+nPp0FNZ699uP6H/bH/ivv3059Ovaz1Ud/MA/luY7vGny/b3SdHR4PuOKKev3Bt5dFJh+zRDBqYgsyUuJ3m4jAjqjogrWOmpKuwqFxZ97vu8WvN/1fNnKECQ80UMlzbigS7oMkZolwaccLIfiox1HNz7s/wB6y79vZLHkb3Ane45EYiK1uiC0thU/m0lqK5TLRjMdQNB1hc/Q5rbOZye3tx43IYLPYSuqcZl8PlqSegyWMyNHK0FXQ11FVJFUU1VTzIVdHUMpHPvAO42q6srmezvLaSK7icxyxSKUZWU0ZWU0IIIoQc9dddturHd7Gz3Ta7yO4264jWaCeFg8ciMAVdGWoZWBqCD0dj4ZfPPenxcz8GHyktfuXqjIVnlym3VmMtdgZpS3kyu12qJUhgkeRg89IzCGosSDHKTIcgvZL3v3r2uul2rcfEu+TJXrLbVq8JPGS3JIAzloydL5+Fjq6xZ+8n91LYfeuwk3/YvC2/3Igj0xXZGmK6VeEN3pBJoMJKAXTAOpAFG2z0p3nsjuXZ+G3fsvcGO3Bg8zSpUUVfQziRG/sTQTIbS0tbSyqY5oJQksEqskiqykDp5sW+7RzLtVpvWxX8dztk66o5YzUH1BHFWU4ZSAykEEAinXEjmjlbmHkrftx5Z5q2max320k8Oe3nXSyniCPJkcUZHUlXUhlJUg9DsrBgGU3B+h9m/RB1r2fz+oZYtl/GvKqkZiptz9j495CR5kkyOK2pUxIgsWMbrinLfi6rf8e8Mvvg2hn2/kOWg0pNdqSf6S25H/AB3rp5/doyI3MPuxZknW9lYygeRCS3Kkn5jxBT7T1rMHJ/0Nj+b2P/EA394OCyb+HHXXEWYP4etw3+UTWPkvgr1kHqPuBQbh7Jooowwf7RG37n640+lTeMtJXNLpPP7t/oR76G/d4R39sdsjZ6iO4uEAwdIMpenyyxP5164Zffdt1tPvE82aItJktbGRjQjUfo4U1fPCAflTy6sx+3H9D/tj/wAV9zh9OfTrErWevfbj+h/2x/4r799OfTr2s9fP97kdsX272pjfF9l/DuyN8UP2YhWEUn2m58pT/bCFQoiEHj06QBptb3yZ3XbzFum5RGPSVuJFK8KUcilPKnX0v8ix/Wck8nXYkMgl2q0k18dWqCNtVfOta18+nToLNNT91dXt9wsPl3pg6QM1gG++rEovENS21T/caB+btxz7GntNH9L7mcizK2n/AHaW6V/08gQj8w1Pz6jb7zO1fV/d+93ovpzIV2K6moAf9BTxdWPJNGo+VBnHW6f8Vajybfplvf8AbXn+nAv+PfWQDr5vutJft/Ptke2u0a/70V333Yu9qw1iyioFX9zubJzfdCdNazCo16w4JDXvfn3xu32D6je94uC5YyXUr6q1rqkY1r51r19RPIu2fS8k8nWog8Pw9qtI/DpTTpt4xpocjTSlPLoX/hKqZj5f/GWimnlRP9OXWdaDFpDNJi92YvKQxtrVv25ZqNVf86SbEGx9nnt3Yh+f+SQeA3a0b9k6Ef4OgV94DXY+x3u3cIgLf1dv4+7hSS2kjJx5gNUfPreo+3H9D/tj/wAV99Q/pz6dfOtrPXvtx/Q/7Y/8V9++nPp17Wevfbj+h/2x/wCK+/fTn069rPXvtx/Q/wC2P/Fffvpz6de1nqMcVRNVpkGo6dq+OBqaOtNPGatKZn8jU6VJXzLAz8lA2knm3to2EJmFwYE+oC6RJpGoLxpq40r5dPC8uRA1qJ3FsW1mOp0luGorWlaefHqT9uP6H/bH/ivt36c+nTOs9e+3H9D/ALY/8V9++nPp17Wevfbj+h/2x/4r799OfTr2s9I7sDfGzerNm7g7A7Az9BtfaG18fLks3m8nIYqakpoyFVFVdU1TV1UzrFBBErzVE7rHGrOyqSzedx23l/bLzeN4u0g26BNckj8APIADLMxwqgEsSAASej3lnl3f+cd92zlnlnbJLzfLyURW9vCKszHJPoqqAWZiQqqCzEAE9aaHzf8AmPmPlt3HWbtCVGK6/wBspU4DrPbc7fu4/b/3Akny+SRCYv7wblnjWoqyurxIsNOHdadXbmj7pc733uPzLLukiNHtcIMNjbmnZFWupqY8SQ9zHPktSFHXeL7vnsVt/snyJBsmpJuZbsrc7tdrwebTQRx1z4MAJVK8SXkoC5AJt/FV/wBX/vfuNfoh/D/IdTp9If8AVXq2L4Pde0m3dsVnZO76iiwdFmUTJTZTMTR0NHitp44M8NbV1VUYoqWGtkeScktpeHwtzwB0G+7JyZackckbtz9zA8dq+4AOssxCCOzirpYs1AolclvmojIrUdcZ/vy+4V57le7Gy+0vJ0U19HsrG3aC1VpGn3KfT4kaIgJdoEVY/VZDMtBmqF+YvzqyvdcKdTdb1Vbg+kcDUoZFQS0Vf2NlKKQGHN52M6JocFTTIHx+PcAghaioXzeOOmx49+vey/8Acm7k5f2GSSDkmF8LlXu3U4llHERg5jjPD43GqgTLz7rP3UbL2e22Hm7nCCK49zLmLPB47CNxmCFsq0zA0llBpxjjOjU0pA6etlmkihhEk000iRQxRq0kkkkjBI440UF3d2ICgAkk2HvGNtvLGgWpJpTj/s9ZiywrGryOwCKCxZuAAySTwAHWx78BP5ZGIw+2l7T+T21KXNbj3RiJ4Nu9XZ6lMtHtbDZakeCTJ7opHILbsq6Sc+CnNjigQ7WrLClzf9lPu22NvYnmT3E2tZru5iZbfbZh2xRyKQZJhUHxmU9q8YuJ/Upo5XfeV+9xf327Hk/2h3h4Nss5w11vFsaNcSxsCI7dh/xGVh3N/o3Afpf2lXvzg+IO7fiR2NLDFBkcv1Luiqqanr/eLxPMiwl3kbaufqUjEVPuXERkA3CrWwWniA/djhxo94vZvcvbLf5IljeXlq4YvY3VK9tf7KQjAljHHgGFGHEgZgfd798dk96+Vo5Hkjg50s0VNzsAaGtKfUQqTVoJT9pjaqN+FmJPHkh/qhf/AF7H/bn3C72Jzjqf2tfkPs6O30N/MH+R/QoocZhd4tu/Z1HpRdlb9FRuHDQ0wPNPi616mDPYONAxKR0lXFThzqaJ+QZc5H97PcnkDwLbb94N1tCY+hv6yxBc4QkiSIZ4I6ivEHh1j97kfdj9qvck3F3uOw/Q77Jk7htumGUt6yKFMMx4VLozUwGHHq6/4+fzW+gO1pKDAdlpP0ru2qMNOkueq/4lsWuqnBB8G7oqelXDoxUsTk4KSnjBCiokb65lcg/eh5I5naCw5nhbZt1aihpT4lszHGJgB4dTn9RVUDi5PXP73O+5h7lcmJc7nyky7/siVYrbr4d4i/O2LN4p8v0Wdjk+Go6tJpXpa6lpq6hqIKyirKeGqo6yllSopaqlqI1mp6mmqIXeKennicMjqSrKQQSD7yehWK4iingkR4HUOjoQVZSKhlIJBBBqCMEdYeTJPbTS29xC0dxGxR0cFWVlNGVlNCGBFCDkHqQsJRgyllZSGVl1Agg3BBBuCD7dWJ0YMhow4EYPTJbUCGUEHiD070+TqogFlHnQcXYFZLAWHrF7/wCxBJ/r7NIL+5joJRrX54P7f9X29IJrGKSpTsb5cP2f5utZb+bR1/jdkfJml3hhYEpqHtXZuO3NkIkiWAR7nxdXV7ezTCJCUY1dHj6KqeQWMk9RISLgs3J375/J1ltPuym/bdEqwbxYx3cqgBaTozQy4GDrVEcnzZmrnJ65fcn5mvOYPaKXY9wYvc7LfyWcTEk1t5FWeLJ4aWeRAPJUWmMCsqizE1FU09ZSzNDUUk8NTTzKbPHPBIssUin8GORAR/iPeJNn9Ttl9Z7nYuY7y3mSeGQcVeNg6sPmGAPWWe4bTa7nZXe3XsGuzuInhmQ5DI6lWU/IqSOtqf4a9kndG1cDWGQ6MlicdkI0LX0rW0sVSqg34AEv+8e/oZ5Y3qPmTlvl7mKFQIr+xgvVA4BZ4llHrXDevXzuc0bJLyzzNzFy3cMTPt99cWLk+bQSvET+1OrGkbUqt/UA/wC3Hs96IuuXv3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de61Gf5tW0jsz5nbwyCp4oN/wC1dl71p00eNLfwn+6NXJEbASCfJbSnkdh9ZHYfUH3yV+9ly7+7fejebxY6R7haW16oAoP7MW7EetXt2J+deu3X3IN7/f3sFsloTqk2u+u9vc1qf7X6pQfSkd0oA9AOqynrx+XH+w+v+sPrx7xxW04VH7esvRB8+t6vo7d0fZXTHU3YQZpX3r1xsrdE7O3lkWrze3cdkKyKaQWDVEFXO6SH/VqffbXkjcBzBybyrvjMWku9ut7hyTU63iRnBPqGJB+fXzoe4mytynz9ztyxo0rt+63dmoAoNMU7ohA9CoBHyI6FL7Zf9T/yaf8AivsUfTj0P7egb4zdBH39sBOyOju39heBppt3da70wNGqL+6mSyG3shBjJ4bh189NkWikjurDWouCOCE+fOX15g5J5s2XwS73O3XESD+mYm8Mj5h6EfMdDj2z5mflX3E5G5k16Ust2tbiQnh4aToZAeGGSoPDB4jrQ5et/q3+Nif+KfU++Ni2eOHX0eCDo3fw5+au/viH2Cmdwhm3BsHPT0sHYHX9RUmKhz1BG2hcjjnfVHjNz4yJmNJVBSDzFKHidl9yt7V+4++e2G9i/sCZtnmIW+sSSElUeYOdEqA9j0xwIKkgwh76+wXLXvfywdt3ALbcy2ys22bmqgvC5/A4GZLeQga0r/SWjgHrcU6Y7e657+67wPaHV+dg3BtXPw3jkVRFX4rIRKn3+CztB5HlxecxcjhJ4H5Fw6F43R26jcqcx7FzrsdnzBy/deNt8w+QeNxTVHItTokSuR9hBKkE8LOfeSOa/bPmjcuT+cNsa23m2bIOUkQ10TQvQCSKQCqsPmCAwZQKf2y/6n/k0/8AFfYj+nHof29A3xm699sv+p/5NP8AxX376ceh/b17xm6rL+ff8uLZvywwVXvXZKY3ZffeIoH/AIXuEU6UmI31HTRRimwG+jTwtNK6xQiGjyYD1FGCFcTQKsaQL7w+xe2e4NtJvG0Rx23OEadsuAlyAMRz0FdQAoknECitVQNOW/3avvVb97MbjBy/zCZr/wBtp5P1rWpaWzLE6prTUQAKnVJCaK+SulyWOob2NsrfHU+8s9192JtvJ7S3htqulx+YwmVh8NRTzRMVEsTreGtoapAJKepheSnqImWSJ3Rgx55bnsG5bJuN3tW7WTwbhA5jlikFCpH7QQeIIqCKEEgg9dv+Vt/5f5z2HbeZuV90hvdju4xLBcQGoYHyIwUdThkYBlYFWAII6H34l/NLsj4n7zjyuAqZ83sfJ1UTbs2LVVksdBkI9USS5TElmaPFbjip4wqVCqySqoSZXVU0Sb7V+5/MPtjufi2bNPsMzD6uwdiEfgC8fERzACgamRQMCAKQx94P7tHKHv3y/wCFeqllznbRkbdu8aAuhyRDPQAzWrMalK1QktGVJYNuJfGL5U9bfI7YeK3psTOw5KhrUEVVSTGODLYbIoB9xic3jxJJJQZKmY2ZSWV1KyRtJEyO3S/lLm/Yudtmt985fvBLaOKMpoJI2845UqdDj0yCMqSpBPBf3J9tOcfafmq/5O522prbdoDVWFWimjPwzQSUAliccCMg1VgrhlFWn/CgaOD/AEAdF5n1+Wm7frMdG6kmNYslsvOVUysP0l3bFRlTe4Cn+vvHz71Nos/LvKspB1peyKD5UaKp/wCOj+fWeH92RJI/ud7iWS08N9hWUjzql3CoI+QEhr+XWqGckP8AVf7fj/iT7wk+i+X8uu0osj6Hrch/kg5Cny/wcoEiSXXiu1ewsbUNIqaHmdsPlFaApI5aIU+TjBLBW1hhawBOdn3cIkb2/uECmqbjMp8smOFsfk3XCX+8JtpbH7w1wXIKzbLZSrTiB+rHQ1HHVGeFcU+wW+/bL/qf+TT/AMV9z79OPQ/t6wd8ZuvfbL/qf+TT/wAV9++nHof29e8Zuvnq/LLXg/lN8lsLNJHLLiPkB3Ji5JEDKkj0HYu46R5Iw6ghHaK4B5t75f8ANu2G15s5ntGozRbjcxlhwJWZxX86dfTx7LCPcfZ32n3BFKrPyztcwB4gPYwMAaeYr0gunsx4e3OrZgFYxdjbIlC3IDGPc2MYLcXte39PankiIWvOnKFyEqY90tZKf6WeM+ny6a98dtW49lPeC210EnK27JWlaarC4Ffyr1vHfEyo14OHkcIP9hZDb/X/AON++qAFOPHr5dutD/ObijyubzOUiV44sllchXxRzEeWOOsq5qhEk0OyeRVkANiRf8++Rc1skkssgTDMT+016+s/btpay26ws5CDJDAkTEVoSqhSRXyqOjpfy0j/ABf53fGWi+1Ws/4yNT1nh8Qm0DGYjK5I1Whg1jQik82r6oY9QIIv7GvtlYCT3B5PAi1Uv4mpSvwtqr+VK/KnUB/exAsfu5+7dwJ9B/dTJUGlfEkjTT/t9WmnnWnn1vj/AGy/6n/k0/8AFffSb6ceh/b184XjN177Zf8AU/8AJp/4r799OPQ/t694zde+2X/U/wDJp/4r799OPQ/t694zde+2X/U/8mn/AIr799OPQ/t694zde+2X/U/8mn/ivv3049D+3r3jN177Zf8AU/8AJp/4r799OPQ/t694zde+2X/U/wDJp/4r799OPQ/t694zdEh+U38wD4wfErH1sPYO+aPN78ihY0HVmy5aXP76q6j1CJMhQw1K0m16R2Rr1GUmpI2VGEXlkAjaNuc/c7k7kqOaO+vxPuq1C2VsQ8urhR6HTEPXWQaV0hjjrIT2c+7P7v8AvXc28nLPLklvy2zDxN5vw0Noq4qUcrquGAPwwq5qRq0r3DU4+aP8w/t35l7hWPPyps3q7D1zVW1Or8JWzS4qklVXihzG461lgfc25PDIyiokjjhp1dlp4Yg8hfB/3C9weYfcK8Dbg/g7RG2q3sYiTGnkGYmniSUxqIFKkKFBI67Tewf3X+SfYfbC22R/X83zx6L3eLhAJGGCY4FBIt4KgHQCWYgF3YhaEWGT/ow/3gj/AHnj3Gpsj/D1kQbNvMDoxXxw6iyndO96ejeGZdp4Wanq9zVqFlWWJnLU+GppIwCK3KGNhcMDFCrvfUFVpS9pPay49wuZooLiNl5ftist/KK/DXtiU/78loQPRQzfhocWfvXe/m2+wnt9PNZzo/P+5o9vs1saEq1KPdyKf9BtgwOah5CicCxUdvmd27X025z0Vt6U4raOx4MSudoqG1PBmM/JQUmQp6apWEqr43bdNPFDBAQqLVLI5DFYSg5+8Zzpc7jvY9vtoIh5Y2tY43hh7UklCKQCBQaIFoiLSgYMc9tIP+4d7IWO3cmD3y5nj+r565gknltri5q8kFt4skbupap8e8dWeSSpJjKKCNUgYj8eS/o55/J5P+t+be8XWsvl10Ea04Yz1tVfy1f5X0HVNNtvv75DYyOv7Tngiy+yuva2KKpx/XKTrHNQZrOoS8dbvtYzrji5hxJYH1VahqfN32S9gYtj+h5x5xtw28kCWzsnA029aFZZR5z+arwjwT+p8HGz72P3v5ecpt19tPa+6aPk9WMG4bpGSr31Kh4oeBS0rgtxm+URpJeJ9sv+p/5NP/FfeVv049D+3rnl4zdIvsLrLZHa2z83sHsPbWN3VtLcNKaTK4bKU5lgmUMJIaiGRWSejr6OdVlp6iFo56eZFkjdXUEFG+8s7PzLtd3su+belztk66ZIpMj5EHirKcqwIKnIIPR/yvzfzFyXvu38y8r7pLZb3avrhnhNCPIqRSjIwqGVgVZSVYEEjrW5+WH8nTtXr+syO7vjVNUdqbJkmmqTsatqKWk7F25TkGTw0ck7UuN3nRQWYK0Jp8hYogppyHlOB3uR91fmHZJJ9y5HLbltFS30rFRdRD0Aws6jhVaOa/AaFuurXst9+rkzmeC12T3YjXZuYAoT94RqzWM7cKsBqe1Y+YbVFxJkQUXqmrP4ncmzsvVbf3bgM7tXO0DBK3CbixNfg8tRs3KrVY3JwUtbAx/o6C/vFi+2W72+4ltL+zkgu0NHimRkdT6MrAEfmOs79svdq3yxh3PZNyt7zbpMx3FrIksTf6WSMlG/I9QI8kePXf8A1/8AjfPPssew/o9KmtjnHWyD/JH3h2zuPanbm3M5LlMl1Bteo26NoVeUNTNS4bdeQbJz5zA7bqJ3K/ZS0AgqqymjJjpZnikCo1U5lzu+5/dc0XFjzRtl20knKlv4RtjITSOdixeOIk/CyUZ1FQp0nBc6uVP94NsfJW17xyRuu3Rwxc83iz/XJDpDS26eGIppwPxh9SRuaF1DLVhGNN7v2y/6n/k0/wDFfean049D+3rnH4zde+2X/U/8mn/ivv3049D+3r3jN1rlfzs87RR9q9JbeQwCux/X2fzNSFXTU/aZzcYoaIzNe5gM23qjxj8MH/r75zffWEUvNnJliFXxYtuklb1pJMVWp9KxGn5+vXVP+772+d+SvcHdGDfTybpDAh/Dqig1vQetJlr8qdUppX/Sz/7c/wDFbn3hI9jxOnPWfzW5/wCL62N/5eeSqP7mbGST0329irBWuDEKaPwt9f1NHpJ/oT77b+xYlHs97bLMoDjZ7cAD+EIAp+0rQn59fPz94JIk97/dRYXJT9+XdSf4vFbWPsDVA+Q6u/o21UsDf1jX/evcsdQ91J9+691737r3Xvfuvde9+691737r3TZlcvQYWm+6r5vEhYRxoBqlmkIuI4kuCzWFz9ABySPai2tZruTwoEq3EnyA+fSa5u4LSPxJ2oK0A8yfQDpMU+/cbNJpennijJsJNSSMB9AWjW1h/rE+zF9luFWokBb0z/h6Lo96t3ahjYL64/wdLWCeKpijngkWWGVQ8ciG6sp/I/x/qPqD7KHRo2ZHUhwaEHo3R1kVXQ1U8D1ri/z3tmfZbi6A7JgRyMnid6bJycgWyRHEVeGzuFQvc6mqRm8gbECwivc34wG++dsAbceRuYFFTJDcWcny8No5I/t1eK/7Pnjqr/dwb949h7n8pyEVimtNxhFePirLDMaf0fCi+3V5Uzr5NW/0N/8AW/4pzx7wmW0p5fy66fLB6Drcj/lM73Xffwd6tSWVZa7ZWQ3jsavZZGe38K3Pkcjio2U8xNDt7MUaabkELqFgwUdTvuz7kN09otigP9rZTT2bkmvCVpV8sUjlUfl+Q4RffX5e/q594fnB1SlvuENruMYpT+0t0jkPzrNFIa/OnEVNkfhX/fX/AOK+588L5DrFDxPl17wr/vr/APFffvC+Q694ny60Avk1tJ+rfkP3h14ac0sGz+1d94THxkKqth6TcmRXCVMYUsFirMQYJYwQCEcXANx746c4cv8A7h5u5n2VV7LXcLi3T5qkrKpHyKgEdfTF7Sb2Ocfa/wBveaNeuS/2azuZT/w14EMqn5rJqU/MdAM2Qb+vH9Df/eSD7IVtT6dSOtt8ujk/Cn5zdi/DPsdNwYJ5txdebgnpYOxeuqirMOP3FjomKLksbIwePFbqxcTsaOrCm/MUoeF2X3KPth7h757Z72Nw28mXa5SFvbJiQkqDzHHRKlTocDGQQVLKYH9//u7cre/XKrbXuara80Wys21boq1eBznQ4wZLeQgeJHX+kpDgHrdU6Q7p60+RHW23u1uqdwwbi2luGC8cigQ5HE5GFU/iGAz+P8jy4rPYqVwlRTuTa6uheJ45H6bcq8y7Jznslpv+wXSy2MooQcPG4pqjkXOiRK5HDgykqVY8BPcPkDmz2t5s3TkvnTamtd7tWyDlJUNdE0L0AkhkAqrD5ggMGUCz4V/31/8AivsReF8h0CfE+XXvCv8Avr/8V9+8L5Dr3ifLqov+ZN1h8FPkBsiSDtbv/prqTuLbdE8ext/VO8dtzbmokV3qW2/m9r0uXTNbn2tVyuxaARmajlkM1OyM0iTY7+8mx+1nOG3PJunNm22fMtulLe5WVHkpUnwpYY2MkkRJPlqQnUvFlfN/7qHN/wB432y5hR+TPbPft65Fu5A247attOLdsBfGhuHi8KC4UUo1dMgGlwQFZNNfOomGzOVxCZXF5pMXka2gjzGDnmqsPlY6SokgTJYuoqKekqZsfXIglhaSKKUxsNaI11GBL2IjkkjDq4ViA61o1DSo1AGh8qgH5dd4NuL39jZXrWk1u00SyGC4ULLGWUExyBSyh0Jo1CwqDQkZ6M/8J/k/uf43d67U3Bi8pVQ7U3JlsZtzfmH87CgyODyFWtKmRmp2cRnI7elqvuqaThxpeLUI5pVaT/abm+95F5u268inYbVcSJb30X4XiZqaqcNcROtTxqCK6WYHHr71nsftHvF7Q8yWstkh5p2y1m3LZ7rT+ok8SGRoQwFfCulTw3XhUq9C0aEXl/zrN5Lvf4JbAycNREP4R8hdkZGpDM2qSOXr/tHFBI9IYeQT5NG5sNKnm9gctPvHwG45G2xRxG6xN/1QuR/l65q/3ZEyJ94LmC3dSWn5Uu4lp5EXu3SVPypGR9pHWpscuv8Aq/8Aif8Aem94Tfu9vTrvQLHq4H4L/wA4TM/CTo6u6aouj8T2OavsLP73i3JXb+q9sCCkzmG23jv4IcNT7SzJmnpazByz/dmrUOlQsXgUxeSSZ/b73SvOQNhn2S12OO4Ml290ZZJCtA0cSaAiqeHh1rqzWlBSpwa+8V9xew+8H7h2/Ptz7hzbVo2uHbzaRWaz1aKWd/F8VrmKgZZgujRgqW1nVpU09d/wo77ReeZsb8a+uqWmYL4Ia3fG5chPGwjUMZqinxmNjmDSgsAIo7KQvJGoi6T7w3M7Oxg2CwWPyD+Kx/Mh1Bz8h/l6hu3/ALqvk1Y4xd+6+6vL+Jo7SBAc+SmSQjHzOc/LoP8AIf8ACiv5RSUxXFdNfH2jq9alZq/H9j5KnCC+tTS0/YOJkLMPofMAP6H2k/4IHng/DtO1f845/wDtp6E1r/daeziyg3nPnM7wUPbG9jG1fLuNlIP+M/mOqSO1+3cv292f2J2vuChxOL3B2ZvfdO/89j9vRZGnwVJm935utz+XixEGUyWZyNPj/wCI18hijmqp3RCF1m3uD92efed13PeLqNVubu4kuZFjBChpXLsFBLEKCxpUk04k9dBuS+SLHkflDlbkva7mebbNo2+32y2luihmaK2iSGIyNHHEjPoQVKooJzQdNvXm4UpuwdjVBlkj+33jtiYyxeRpY/Dm6Fy8axAztImm4CAtf6c+97TbC23TbbkEqY7iNwRWo0uDUUzUU8s9IPczaDd+2/uDaiFH8XY7+PS9ArarWUUYsdNDXNcU4463s/jXlKzH7Gztdjhqr8fgcpWUS+Mzaqulx089OphF/NeaNfT/AGvp76ZX8stvt99PD/bpC7pivcqkjHnkdfKBtEEF1u22Wt0aW0lxHHIa07WdQ2fLB4+XWgqM0P8AVj+lvIP+IPvmCdu/o9fXydv/AKB/Z0JPUveW/ejew9s9rdW7gG2N/bOqqqs25nv4XhM3/Dqmtx1ZiamX+F7jx+YwtZ5MfkJo7T00qrr1ABgpC7aZb7YtxtN22ufwtwgbXFJpVtJoRXS4ZTg+YI6CnOvt5y17icr7vyZzhtX1nLV+ix3dt4ksWtVdZFHiQPFKtHRT2uDihwSOrGMd/PE/mG0lPDBUdv7dy0sRYyVdf1V1klTUBpWcLMmK2rjaRVRWCDxxRnSBclrsZF/14Pc4f87HX/qGtP8ArR1ixdf3eP3Xp5ZJIuRrqBDwSLcdwKrimPEuJGzxyTn5Y6EGh/n4/OylnE1RV9Q5KPSy/a1vXTRQEtwHLY7PUFVqT8WkA/qD7WRe9fuRG4ZtwgcfwvBFT/jKqf59Bm5/u1/u4zRmOO33yJ611x31T9nfC65+zpZY7/hQt80KKKSOq2R8ccuzvrWbIbI7CjliXSB4kGJ7WxUJS4v6kZrn62sPZnb+/fPsCsstrtspJqDJDICPkNEyCn2gn59EF3/dg+wNw6tDv/NcCgUKxXdkQfmfE26Q1+wgfLpf43/hRd8jIzR/xfo/o2tCJEK/+HPv3FGpkEYEzUhqd2Zj7FJJblVcVBReCWPq9qF+8JzqGGvaNrK+YEc4P5H6g9Bq6/usvat/H+i9wuYo6k+H4v0cmkVxq020WsgcSNNeNBw6VI/4UbdtH/uXHrP/ANC7dVv9uaYe3v8Agh+bPLYNv/ZN/wBbeij/AJNXcjD/AMGpu/8A2TW/+fpF7r/4UQ/JrJQyw7P6i6N2sZdKrVZWl3vumtp18dneApu3A0JmM3KmSnkRV9JRj6gjuvvBc8yo6W+2bbFUYYRysw+Y1Taf2qej7Zv7rv2gtJEk3znfmK9AyUha0t0bOA3+LTPSnGjA1zUcOiG9w/zUvnB3fT1WM3T31uTBYCqZg+3+uocf1xQGBtWqjqKzaNJi87lKJg5DR1tZUq4sGuAPccb77ie4HMMZh3HmWcW5qDHb6YFIPkwhWPWP9NXrJDkT7m33evb2WG72X21tLjck4XW6l756/wASrctJFG2MGNEp5dENfNNNI8sszSSyu0kskkjSSO7sWd3drs7uxuSTck+49+hb06yQXb/DVURQqAUAGAAOAA8qddjKr/q/9s1vejYt/D142Z8z0YHoXozfHfGeSkwVNNQbao6mKPO7rqYpGx9CpMbSUlGPQuSzDQyApTow06laRo0IYjnkX2x3znvcltrGExbajD6m8cdka+YH8chHwoDU8SQtWGNX3i/vIchfd35da53u4S75xuImO2bJCy+NM2QsktKmC1DCjSsM0Kxh3GnrZu+JnxTxW18Tg9v4LEvS4egEbPNOiPW5OsYRipyuUqEjhFTkKxlBdtKqBZEVI1RV6Ccqcq7Nyds1rsex2/h2keWY0LyOQNUkjADU7UzwAFFUBQAPnf8Ac/3O5u93uct255513Dx93un7USoht4gSY7e3Qs3hwRA0VaknLOzOzM1AH8xDYmc6l+Zve21s1TSUorN3NuzDu0figrcBvCipNxYqopH1yR1EUcNead2Q8TwSIQroyrz292tmuNv9xebormOjSXj3K+hSY+Kh/wB5fOeIIwRTr6EPuf71tnNP3bvam722QMLbbV26cA1KTWjNBIrCgKklNYB/CykVBBJNo8ofqSOPp/vh/T3GjWgP4esjXs1pw62hv5R380XFZ6g2t8UPkPuAUe5KNabAdOdjZqsApdw0a6YMT13uWtqGX7bO0SBafEVUjaK6IJSOVqUhNVl17G+7kaQ2XI/NVxRlpFt15IcEcFt5CeBHCNjgiiGhC6uP/wB9z7nl5t1zvPvT7XbZ4m1yFrnfdqt17oW4yX0CL8UTmrToBWNqyisZfw9kHwr/AL6//FfeXHhfIdcpvE+XXvCv++v/AMV9+8L5Dr3ifLr3hX/fX/4r794XyHXvE+XSC371L1h2njlxPZnXuyewcbHq8NFvPa2F3LT07Nz5KWPMUdYKWZW5V49LqwBBBAPsl3nlfl/mKIQb9sdnexAEKLqJJNNf4S6kqfmKEdCXlvnbm/k26N7ylzPuG2XR+KSwuJYC3ybwmXUPUGoIwRTor8n8tj4OS5IZZvjpshaoSLKIoptxQY3UosAcNDnI8OYz+U8Gg/kH3HjewPtG83jnkm211rQSThf94EuinypTqYE+9j94dLT6Me6W4GGlNTLAZP8AnKYTLX56q9G72nsraWw8Bj9q7J21gdobZxMRhxm39tYmiwmGoI2dpHWkxuNhpqSDySMXcqgLuSxuST7k3bNl2zZLKHbdn26C12+MUSG3RY0WuTRVAFSck8ScnPUH71zBvXMm53W88w7rc327zHVNdXcryyuQKDU7lmNBgZwMDHSi8K/76/8AxX2YeF8h0VeJ8uveFf8AfX/4r794XyHXvE+XWlH/ADGPkBQ98fLfs3cuDro6/aW1qmm642dVwsHgqsLs4S0VZX00wdlqKLL7llyFbTuLBoKhOL8nkf77cyx88+5nMG62sofbYWFlaMOBig7dSnzWSTXIPkw6+gL7rPtnce23slyjtO42xi3u8Rt0v0bBWW6o6owxR4oBFGwz3IeiUQ5B3ZEQl3dgqqBqZmbhVVR6mYk2AHJPuGTt7OyqiEuTQACpJ9MZr1P8sSRI8srBY1BZmagAAySSaAADz62kPg3tiTCYvbWJNz/CMLiMczhQNb0VFT00jkqCuuSSMk/1J/r77bcm7L/VvlLlfl7TRrHbre0PDJiiRGOPMlST6k9fNPz7zCebueecuafLct0ur4DOFnneRQK5ooYAegFOroKNdNLAv9I19iboJdSffuvde9+691737r3Xvfuvde9+690WnujI1dNuPEwM7LSjE+anFz42mermSob+nlCpGD/QW/r7HvKkEb2Nw4FZPFo32UFPy4/z6APNc8kd/bIT+n4VV+0sa/ngdBtTZ+VLXb83Nj/T/X5+vsQPZqa46D8d2RTPRj+qcjPkcHWtJqMEORaOnYg2uYIpJlUkfRXYcfgn2BOZIEhu4QvxmOrftNP5dDzlueSezmLfAJKKfyFeqy/53GyH3H8Nl3ZDCzS9a9m7O3HPOoN4cfmhktjSpIfoIZsjuqkv/taKL/1xJ+9Rsp3P20iv0jq9juEM7N6I4eA/kXlT86ddBf7vrmAbV7+LszyAJu+z3doqnzeLw7wEfMJbP+RPWoG9ex/tf8QSP9Y3FvfOdbQ+nXcxbb5dbOv8gXsNMn1r8g+sXnHk23vnau+6eAm2tN6YCp29WzRL/aETbCgEhH01pf6j3nT90XciNp5x2Fn7YriG8jWvHxUaNyPs8FK/aOuRP95dyu1pzX7Y83rH23e3XG2u/obWZZkB9K/WMR9h9Otgv3mH1zG697917rSp/nM7KbYfzw7Cr44GpaLsbbGw+wKFNRMcgqNvwbUydRGTd7VOf2lWOwJNpGa1lsBzY+8FsZ2/3U36VYdEF2kN0nHOqJUdhWvGVH/Prv8AfcM5g/rJ93Dle2aQPcbXd3m2SHzGmdriNSP6MNwgHyArmpNXuFx+Y3LkP4VgqKbJ5N6WvrIsfTASVdTDjKKoyVaKWHVrqp4qKlkkESBpHCEIrNYGKNt2O+3W4Fnt1q810UeQRplisaNI+keZVFJoMkDAJ6yu5j3/AGPlDbP31zLuUdns4nhtnuZsRRvcTJBD4jUIjR5pETW1EUsCxVakJ568f6on/ffXi1h7YW0Hp0JFtSejU/FD5yd5/DPdtfufqLMYypx+apZaXcWxN4Q5PLbD3Gxj0UldlMNjMvhKyPK4xwr09XS1VNUqAY2doHkicfci878ye3u5PuOwXC6XXRNbThmhlHlrRWQ6lOVYEMMiuksDDnvR93b279+djttn53sJUubdw9ruNiY4ryDNWSOWSKVTHIKh0dHQ/EAHCsDCdg/zmvnxvrVDS9s4vYFC5l10OwNkbWxesvcLpy2Yx2d3FCIVYhfHWpe921MFIF25e9/uhuiuh5jMEJ/DaxRRkfY4Qyj/AHv+fUYcsfcL+7Vy5SSbkuXcrgUpJud3cScOP6cbxQGvnWM+goCQSLdhfJXvvtYzDsvurtPfcM6NHJSbs37ufN4/xOFDQQ46vyU1BBA2kXRI1Qn8e4+3Pet/3sht53u8uyMA3M0klB6DWzUHWRnLHtP7a8meH/VLkDZ9tdSCHsrO3heo8y6Rhy3zJJ6BJ68c+of7f/ejzz7LBb/Lofrbn+HqM9eP9USP9t/xon26tsTwXPTy2x9Olr1bhsjvXsnY+1sTFJLXZnc+Ip18a+RqemSsjqK+ukVSLw4+ghlnkP8AZjjY/j2IeWtgut737Z9qtIyZ57iOMUBNAWGpjTOlFqzHyAJ6jz3h5l2vkL2q9web96mVLCx2m5kOo01yNGyQxKf45pmSNPVnA62hPlH0NvD5K/BPs7ZW0KGoy29dtpiexdnYiCIz1OZyuzZ2razDUENjJLlMztyWupaNEIMlXLGl7MR7z+91eXJuZuTb61tUL3cDrdRIBUsY6hgAKkkxs2kAVJoPPr5//uWe6u0e0H3huSuYuY7gQ8s3fibRuE7HSsMV2uhJnPARwziJ5CeEaseIHWmXLuMwSyQzCWGaGR4pYZA0csUsbFJI5EdQySIwIINiCLe8K12g0BAwfP8A1Hr6kI9oWVEkjAaNgGVgQQQcggjiCOFOsDboUf22J/wLW/5Nvb24NoPp0+Nk/oj/AFfl1hbdAPPqY/QfqNv+SkHH+x92G0fZ1cbKP4R1iO5j+A3/ACcP+JPu42gedP5dXGzDz006xNuV/wAKx/xtf/eypv7cG1L5kdODZ09R0cT4RdR7n7x7s2tNT4+qGzdj5rF7m3ZmDHItKP4XVR1+MwMU2mWKWvzdZTLGYrq60olkBBQXGvIPJUnMHMlggjJsbeRJ7lqHSEVqhSRSjSEaVHHieCmmGH36Pezlv2P9kOaLCS/ibnnmGyn2nZ7IEGQ/URmGe7K6gyxWsTltdCpl8OMg6jTe5+J+BqqPERSSRsokQX1Bh9R/iL8+82hmmevmB60vP5qPwd7C+E3yD3XV0O3qyfoHsPcuWzvU27KOJpMRjqTJzyZKXr/MSwwLHis9tZp3ggjkI++oYkqIix88cOFXO/IcnK27zxGJv3XK7Nay8QVJJCE/xoMEYJpqAoR19Qv3K/vJcp/eH9stmsbvdo091NptI7bfLCQgSyGMCMX0IYkywXAAZ2X+ylZo3AHhs9XY3DUf0/1/of8AbE+wUdti9eszjtUR8+sg3HOPqpP+ufp/rWK+6HaovXqn7oj9R+zrKNyyD6q3+wAB/wBuXPup2pD5jqp2dD5jrKNzN+Q3/Jx/4oPdDtK+VP5dNHZl8qdZV3QR/qxf8i6j/YgBj7odn9KdUOyD+Fesy7pH5Zh/T9Z/29wAPdTtB9OqHY/6I/b1lG6E/Ln/AGLf8UHts7Of4emzsh8k/Z/s9ZV3RF9PJ/ib6f8AeGc+6HZ3H4eqHZG/gPQkde7P7F7WyK4rrvZu4d3VZmWCVsTjpJqCikZDIpyeWIjxWKjZBfXUzRJ9OeRdZYcq7pu1wLXbLCWe4x2xKWpU0BbFFFfM0A8z1GvuL7g+2ftLtrbt7kc7bds9poMiLeTIssoBofAtwWnuGr+GJHbjjB6tn+O38sLceZqsfm+6K5nUmKZdi7ZmdgWvG4g3BuOMAFANSSwUH1NilXa4M38pewLSPFec4XGiIEH6KBgWOeEkowB6iOtQcSKR1ya9/f7zmCSO/wCXPu+7G6sdUZ5i3WMAgZGuzsjXPArJc8MhrbgRsNdA/EahwtBicfQ4KiwuExsccVFjaGjipKKliDFmWKCFVQFySzH6sxJYkkn3krt22WG0Wdvt+22kcFlGulI4loo8+A8zxJOSckk565Gcw8x79zbvO4cxcz7xc3++3UhluLu7kaSWRj5s7Ek0GAOAAAAAAHVpuxuvcbtWiihggjVkVQSEANwP9YfT2v6Jeqr/AObp/L2X5ZdcQdjdb46CPvrrTGVP93dLU9MN97ZDvWVexsjUzNDEtSlQ71GKmmcRwVTyRMVjqZHSF/eD20TnTbV3TbIR/WO1SiDA8aOtTESfxAklDwqSp+Kq5wfcq+9K/sLzg/LnNlyze1e8TL9cKMxsp6BUvY1UElaUWdVBLxhWALRqp0kKyprsRkK7E5WkqsblMXW1ONyWOrYpKWuoMhQzyUtXRVlLMqTU1VS1MTJJG6hkdSCAR7wem2wo7I8ZV1JBBFCCMEUPAjr6IbZLTcbO13GwuI57GeJZoJoiGjeN1DI6MKqyspBBBIIIPWeHNaWVlkZGUhlYGzAjkFSLFSCL/wCHtE+3keWeqybeCGBWoODXrYD+An88beHTVDgup/lLT5vtDrahFJi8F2RQSrW9kbMxykwxw5uKskT+/wBhKNSmlpJ4spTwq2l6u0VOs/8At173bvyxFBs3NEcl9sqdscykGeFfIVagmQeQYhlGAxAVOuZv3lv7vDYufbjcedPZ2W32fmyQtNcbVKCtjdOckxFQfo5nzWimF2IqIqs52nekvkN0p8jtqRb16R7J2x2JgGEQqpMHXA5LDzzJ5I6LcOBqlps5t3IFOft66np5rc6bWPvLfl7mnl/mq1+s2DdYriIU1qpo6VrQPG1HQmmNQFeIqOuN/uF7Xe4HtVvT7B7hcqXm17kCdAuE/TlANC8Ey6oZ0r+KNmX59DN7EHQC697917r3v3Xuve/de697917qkP8AmrfzKdtdH7Q3H8eumty0+U7x3TRT4XduXwtWssfU2Br4TFkBUV9LOppd/ZKklMdJTI3moI3NVL42+2WbF/3794rbYtsvuTeWLwPzFOphupoji2jIo66gcTsMADKAkmjaeuhX3M/unbr7g75tXuhz7tTQ+3tnILixguFodxmQ1QhGHdZxsKu57ZSBGuoeIV1Mo8l/Rzbg/W9/9j+PfPl7LrtW1p8v8vRhvjTtGq7E7Y23QiIy43C1Ee48u1tUYpcVNFLTU8lwVf77JGGIpcExs550n3KfsjyK/N3uPsNtLDq22zkF/dkiq6IWDKp9RJLoQ/JifLrFv733uLb+1/sfzXdpOE33dYzs23KDRvEuVZZZF8x4NuJHDAYcIMagetu/4lbPajx8FZJFYuqG5X6j635/PHvqkPsx1893ViK6UVUuAQALXH9Px7tQ+nWqj165+9db697917r3v3Xuve/de697917pF722PjN746OkrJJKSspXMuPyUCq09LIwAdWRrLPTTADXGSL2BBBAPs12ndp9pnMkahomw8Z4H0+wjyPRTu+0QbtAscpKyqao44j1x5g+Y6BOi6Ezi1SrW7kx60Ov1yUlJUtWMnH6Y5isCOR+SzAH8H6exZLzjaeHWGyk8XyDEU/aKn+XQTi5Nu/EAlvkENclQSafYaAft6MXhMLQbfxlLicbEYqSlTSuo65ZXYlpZ55LAyTzOSzH+p4sLD2B7u7mvbiS5uGrIx8uA9AB5AdDiztYbK3jtoFpEvCvE+pJ8yT0Vz56bCPZfw4+Ru044mnq5uqd1ZrGQInkefMbToG3bhoEQI7F58tg4UGkFgWuObe4291dpG9+3POW3/iNjJMtBWrQjxlH5tGB1Of3c+ZRyj77e1O+O4WBN7toJmJoFiuXFtKxNRgRTMetAN68fl/9t9f9j75braeo6+mRbZj/AKv83R8fgD89Kz4Lb97C3rHsI9lUu9thDaybdbczbThhzdNuHEZTF5uqyYw24PJSY+hiro2gWm8kr1C2liAYmUvazn6X2z3jct2i2sXYuLQ23hGQxAMZEdZCQkmrToI00FdXxDrHH7y33bYfvF8tcscvvzL+6ptv3L6w3XgfUkxGCWOSJY/FhozuYyGL0UKaqxpQ4fYf8/v5V7h89PsDYfUHXNE7Ew1L4rP7y3BAPTZfv8tm6TBS8g3JxYvfi1uZG3T7yXP96rx7fa2FmhNVeONpJAPQmV3Q/wDOMdQZyv8A3aHsztfhy8y8yb5us4+JBJDawn/aRRNMP+c3RFuw/wCZ987Oy/uUz/yV7BxlPUa1al2LPi+tYUhb0/bqev8AHbbqHiEfpOt3Zx+tmJJMe7n7pe5G8sWvecL1QRQi3f6dSPQrAIlOPUZ8+siuV/uhfdy5S8Jts9p9smlShD7isl+Sf4v8decA1zgADyAx0Svc++N0byyk2c3huXPbqzU6hJ8xuTM5HOZSZQ8kgWWvylTU1coEkrNYufUxP1J9gaY3F3K09zM8k7ZZ5GLMftJqT+3qfto5e2fYrOPbtj2i2s9vU1WC1iSKMYAwkaqowAOHkOhc+Ks1bV/Ifqynx5VqiTcMnkBDkfYLi8g+UJCFW1fwxZiLnSDy3F/che01vdf643KBtB+r9YpPH4AG8Tga/wBnq/y46x/++Km3xfdl93n3MUtv3aoWlP7U3EAt/ix/blPn6Zp1aL8v/wCXRnN0bPr+9uisFJV5yhp5slvnYGKpbSZ+mjDTVW49sUUK+rPwqC9VRRrevW8kQ+5DJUz97x+ysd2Lnm3lCyC3Iq95ZRDD+bSwqPx+boPi+Id1Q3P77ln31H2GXa/aL3k3lm5fYrb7Nvd05JtSe1LW7kYk/S8FilY/oYRz4Gkw0RS5DQSrekgkMrXBBB5DKbWsR9PeJi2benXaRLUMAwyDkEdQnyY59f8AtuCf+KD2+tl0oW0+XUYV8k8scMCSTzTSJDFFEryyzSyMEjiijQMzu7kAAAkk8e1KWVSAFz1d4YreKWe4kWOBFLu7kKqqoqzMTgAAVJOAOhX230T3vvF0XbvU++6uOS3jrKjb1ficc/8AULk8vFQ44sPz+7cexXtvIXNW6BG2/lu8kjY0DiF9H+9kBR+3qG+aPvFewHJSueYvd/l+KZfighvIricfbBbNNNT07M9GL2l/Lp+Te6DTtksXtraEMsieUZvPLXVUMBYa3SDbdPm4ZJQnKo0yAtwWXkiQNt9h+e7wj6q0t7RPWeVW8q8IfFP5Gnzp1jjzX/eR/dq5eFymyXG875OqnwzYWZijZvIF717VlWvFgjUFSA2Abc/h/wDy9KTqWtXKytU7p3lkIlpa3clVQikhoqR3V5aDBY/XUNRU0zBfNI8sk02n6ov7YyL9vPanaeRdd/JN9VvrpoM5GlYwfiWJakivAsTqYDGkEqeWH3nvvic7feOlt9l+gXZ/b62l8aDaoZDI00gws15NpQSuoJ0IqKkdThm7zsTdK9aJtbBQwywhXeJdQK83t/S49yuOHWH3VP38wr+TL8ce7a/eHdW3aLM9Ub7ejyu49yZDYQoY8FuerpKOesqa/NbVraWXHDJ1XhLS1FC1DLUSkyTmWRixjPf/AGm2LmC8NzYytZX0rDUYgGiZicsYiVox/osoJqSCxJ6zx9if7xL319i9htuVp2tOY+TrWPRa2m7+J41ui5EdvdxssojAwqSiVUWixhFAHWtfD/L1otaGbde4pomUEiCgx8TgsAR+4y1C2W/Pp5/w96H3bYI3Pi81SMnCi24U/tMzf4Opvuf75f3FlipY+zOxxzVFGlu7qRaeY0qsRr6HV+R6VNB/Ll25N/n9wb2fVbT4XwkNuOQwkw9Rcn/Ye1EX3dNoXV4+/wB2x8tCIv7a6q9Ed1/fG+9jlPovbPlSMZ1eKL+SvpTTeR0/n+XSopf5aOzJQBJm+wyx5umQ28ink/QNtWQiw/x9q4/u98rBAJdz3Jn8yrQqPlgwN/h6KZv74b7xbSE2/IvJCRHgr2u6MfnUjd0HH5D8+j0dH/yc+kd7bXx25clhd65eaGtrcfXUlRuqqp6Crmop1UPIMTT46siMsDoWEcyDUxsALAFlx7I8qbfeqGur+WIANokkjofkSkKN+wjoN3P96b96rebK5FpuOw2Mrs2mW025WaOpNAguZbhCFBFNaucZJzW4bob4O7e66osdgdsbUxO1tv0L64cXiqCOjp/KwXy1M5VfNVVk5S8k8rPNI3Lsx9jrato23ZLRbLabJILYZ0pxJoBqZjUu1AO5iSacesJOeOfudPcrmG75r5+5nvN25hmoHur2RpH0iulEB7Y41r2xoFRRhVA6tg2Dsul2rjIKWGMJoRQbCw4ABH+8ezToIdNva3VW0+09s5Pa+8NvYXc+By1O9NkcJuDF0OZxFfA/1grcbkYKmjqoif7MiMD/AE9pruztL+3ktb22jmtm+KOVQ6mmRVWBBoejPZ963nl3c7TeuX92ubHeLdxJBd2crwzRsODRyxsrow9VIPVMfYH8mn4oZCurajH9GbTo0qzIrR4uTN4mBFkVl/yanxmVpIKNgOQYVQqeQQfYJk9sOR5HZ22OjHNFmnUfkFlAH5DrJrb/AL8X3sdsjt4rb3v3dliIKm4FvOTQ172ngkaQeocsDwNR0X2u/kffGFl0QdU1lKyvq8lPv7sl5GADDxkVW7amPQSQTYargc/UFqb2s5JkUBNraPNapNMT9nc7D+X59DW3/vHfviwOXl92I5lpTTJtWzADhn9Pb0Nfzpnhw6CfsP8Aks/HDau2M/ucbL3JSxYfFz1Kwwb03O8LVCjRT6zV19VKRJUSorWcC30t7rY+yfKe57ha2sZu01sFISQHAqSe5GNadL5/7zz72217dczTc57bM6ioeXbLIGpoFFI4o1oD8q/PogVX/LF6ymiljjXeFE8i+melzkTyQEm94lrMbWQmw49aSC3159jZ/uxcmNXTf7ov2Sw/5bY9Jdv/AL3v71NpcW8068r3cSfFFPt8gSTFO8wXcLj17WXPyx0mpf5WuxuPFuLsZQL38mR21KW+ltOnakWm3P1v/sPaG4+7DyudP0287klK6vEML/ZSkKU/n+XQytv75r7w66/q+QOSJK00+Fb7mlONa6t2krXy4U+dcNr/AMrPbTSN4t274jj+qpKMHJIBYDmRcTErXa/IUeyqX7r23628Lme5CeQaFGP5kMtf2Do9g/vofeMRItx7U8rvP+Jo3vlU/YpuHI/3o9P+O/lb7BiqI5KrL9hZBFYk002SwkEEilSLSGl23FUmxII0SpyObi49mMH3ZeVl1fU7xuT5xoMKftrC9f5dBfd/75H7x17bPb7bydydZSsP7ZbW/lkXINUEm5GIVAIOpHwcUND0YLZf8vHp/BS+WHrvG5GV9CvJuOSv3GjBCxBFHm6quoISdRuUiXVxe9hYa7V7E8g7YY5BsH1Eymuu6d5K/bGWER/NOsaeef7xf73PPMX024e9F9YWgrpj2SO320jVSv61nFDctwxqlbTnTSprdd8X/jDQZrYeNCUNLSw4SrqMO1PSU8MECLTGKWArDFHHGl6SoQcAXIPu+9bJa7DeCzsbSOC0KB0iiVURa1BCqoAGR1jzY8xblzOk26bvuc95ubSETXFzI0srnBq7uWZjQ8SerAsX03s/rfb2X3PmaZUxu2sNks7k5Y4hJJHQYeinr610jOgvItNTsVF+SLX9kF3cw2NpdXs9fBhjaV6DOlFLHHmaDo92vbrreNz27aLJQby6njtoQTQF5XCKCfIamHU74pfJX49fK7rWj7K+Pu88ZuzAEU8GXx2j7Dc+0snNGz/wbdu3pyMhg8kpikC6wYKgIzwSSx2clPL3M2z8z2ZvNpudWmglibEkZPAOtTStDQiqmh0kgdSL7vey3uR7Gc1Tcoe5PLktjuQq0Evx29zGCB4ttOvZLHkVp3LUB1VsdGj9n/UV9R6mnSpiaJ1BDAgg/kH8e/de615f5qX8ojGfIh8v3f0PDjtq95pCs2bxchSh232fFSQSKkWVdFWPF7vKLHHDkj+3NGixVQtonghT3H9qbbmNpt62ONY97OZY6hUnpXNeCynFCSFb8VD3ddGPubffp3b2Oay9vPcrx9x9pWciB0BkudsLsCWhBNZbStWeDipJeI11JJpt70xO9er915nYvYm2c5szd+36t6HM7fz9DUY7I0VRGSLtDMumWnmUB4Zoy8M0TB42dGVji1ebBPazzW1xA0dwh0vG4Ksp9CDQg9fQXyvuvK3PvL+3c18mb5abny5eRiW2vLOQSRuD5VGVdThkajowKuFYEBrp9yxtp/cX/W/x/pxzwOf979lUu0uPwY6MpdlYV7D0JfXncm/Or9xUW7+td8bp2FumgYGj3Bs/cGT27l4BqBMS12KqaWpMEmmzxljHIOCpHtqCG+264S8sLmWC7Q1SWFmR1+aspDA/YegjzRyDy5zftdxsfNfL9luWzy4ktb6GOaNvmUkVhUeRpUcQR1cl0Z/P8+Z3WlPR4rsMbC72w1OFjep3pg329vDwIx0RQ7l2bNiaKWUKdJmrcdXSsBdmLXJlHZvejn/Z0WG5uIL6AUA+rSrgD0eJo2JPq+s9YH+4v92f7C82Sz3vLA3Lly/Y1CbfKJrap4kwXQlYDz0xyxqPIU6tB67/AOFIHQeVhpV7S+P/AGrs+qcIlU+xs5tLsGjjkK2aVP45Vdc1Zg8nNvGzhCbByAGknb/vFbexA3jle4iFONtIkpJp/C4gpU/0jT1PWH3NP91P7lWTzHk/3M2a+hFSg3GG5smIrwPhLfLqp8wK+g4GYoP5938v+sp0mnzHbOMlYuGo67rad6iMKxUM7Y3L5CkKyAahplY2PNjx7PV+8FyQVq1luSn+ExRV/lOR/PqJLn+7Z+8xBIyR2OySoKd8d8Ap+wPEjY+Y6DvfH/ChP4f4SmnTY2wO7N+5RXlWmE+E2ttLBTiMyKjy5TIbpr8vTrOVVlAxkjBGJYKw0Eq3H7x/LEELnbdh3Ce4BwsvhRIRnOsSSsPL8Hn+XQp5e/uwvfLcJozzFzNy/ttoQC2mW4uZhWmBGlukRpkH9YZGKjPVUPyY/nofJ7u2gyW1+q6DE/HfZ+SjNPPNtTI1Of7GnpZFKywN2BVUmLGKEnBEuKx2Oq0tpE5UkGFOcfffnfmKOez2vTte3Pgi2JM5XGDcGhGfONYz5GorXNH2k/u6/aH29ubTeOcbibmnfoTqUXqLDYqw4H6JWk8SnpNLKh46AQOqcpc5UVlRPV1dVNV1VVNLU1NVUzPPUVNRO7SzzzzTM8s000rFnZiWZiSST7gF7YsSWFTXJPWdibfFBEkMMKpCihFVAAqqBQBQKAADAA4eXU6iqqmtqaajo4J6usrJ4aWlpaaKSepqqmokWKCnpoIVeWaeeVwqIoLMxAA59tLt7zyJFDCzzOwVFUEkkmgAA4kngPXpDfCzsLS6v7+5jgsII2mmmmYIkcaAs7u7EKiIoJZiQAASTQdbCfwQ+Mtbs7CUP8XpFO69wy02T3JIpSUUCop+xwiVEepHjxccjeQqzIaiSQqzJoPvof7Ke2o9vuXGa+iX+sd8VluyKExgD9OAEcdAJLUwXZqEgKevne+9994Ee+vuO7bHO/8Arf7PrtNoVtSiapHjXhRqFTcMo0ggMIkjDBX1Dq77EZ6vw2Jiw22pnxdBAixy19MPHXVzqAGaGW2ulpdQspWzuPUSAbe8pdl5ft4Y0uL6MPcEVCNlV+0eZ9a46wO3vf7mV2t7CQpAMF1wzfYfIenn/g6YKpqyWQzyVdZLKxLGZ6ud5dV738jSFzzz9fYwQRqAqxqF9ABT/N0DpGlY6jIxb1JNf28elltHtDc+0qqFKirqc1hdSrUY2umeeWOK51Nj6qYtLBMgNwpJjY8ED6gr3LYNv3KNmSNYrr8MiADP9IDBH8+jXbOYL/bpFDyNLbecbmtB/RJyD/Lo6GIy1DnMZRZfGzeehr4EqKeS2k6W4KOp5SWNwVdTyrAj3Flzby2lxNbTrSVG0kf5vkfLqVLa5iu4IrmBqxOKqf8AP8wePTj7Y6f697917r3v3Xuve/de697917r3v3XuoOToabJ46vxtbDHU0dfR1FHV08o1RVFNUxPDUQSC4vHLE5Uj+h9tzRR3EUsEyBoXUo6ngQRQg/aOnreea1nhubeQpcRuJEccVZSCpHzBFevnK/JXprdPxs7u7F6Y3dTVkNfsrcmQoMfWVMLxJn9uNO8229zUbmKBZqDPYV4amNlUAFypCsrKvLjmXle95X37c9hvoyJ7aUoGoQHXijrUAlXUhgfQ9fVD7Q+4Oze7nt1yp7gbFMjW24WqSTRoQTBcAAXFu9CxV4ZQyEEngCCQQSAj5Af1/wBuR/xHI9lAtG9OpNFqT1DkyQ/1Q/2HN/8AAE/j2+tmen1tPl1DfKL/AKs/7f8A3r2+tl6jp9bP5dO238JuveNaMdtLbWe3NXEqv2mBxFfl6hdZsNUdDBO0an8s1gBzf2Z2GyXu4zrbbfYyz3J4RwozsfyUE9EHM3NPJ/JNidz5y5p27atvAJ8bcbiG3Q040MrpU/IVJ8ursvgP8Md3bNzq7+3/AI9IN35Cm+wwuDjkjq221jaoxtW1FdUReSmObrgoj0ws609PqUuzSukeXPs57U3PK8rczcwRKm7tGUtrfBMKt8TuRUCRlwAD2qWDdzUXiH9+b74Oye8UVp7Xe19xLJyHa3Audw3FlaMX88dREkKNR/pIalquFMkulggWNGfaj6V6/TH7Wp6ashUl4ACrJybqPwR9bf737yHp1zY6rv8Amd/LG+LW/wCDePbm4+uKXFZygxuU3HnM9tPI5LatblTRU0tZVTZGmw9TBicpka1orNUVNNLUM3+7OSDH28+0fJXNV/49ztAi3GaQaprZmjLEnJZQfDYkmpYqWPr1kt7c/fH+8H7QbKmy8sc/yvy5bx0isdxihvI4lUYWEzo8sKL5JG6p/R4U178Z8O9pU9XJPDteErLMzx09dU1+VSniZi0dPprp5opPApClit2tc/09jLbPYL2z2kJp5bW4nWlZLqSSQmnqhfws/JR0Xc2ff9+9RzerRXHuxc2NpnTHtMNtZaa8aTW8KXBxw1SGnEUNeh72r8asfjUjWjxtDjkRkdVoaOGjCMtijp9vHHpdLcEWIP09yJtvK+ybOunadmtLVfS3hjj/AG6FHl1jRzL7i8585XD3fN/OG6brdMamTcbue5YmtctNI54548ern/h31RSdibVyeM3AGq85tCoo6aWtns9RkMTkI5pMfU1DEBnqoHppYZG5LhEZjqY3Jd729bKdHjH6UgOPIEcR0ztF8byKRHNXQ8fUHh+fVg2G+OO2aHQTRQ8W5MYP0+v1+nPskp0cdCzg+tcDhdBgpIFZLWKotxb6EG3497690IUMEcCBI1CqOBYfj37r3TLufb9Jujb2c29WWWnzmHyeImk06ikWSopqOSTTddRRJibXF/6+3IpDFLFKBlWDfsNem5Y/FikiJoGUr+0U61f8xsyq2XuTO7N3FRGlzm2MrV4PJQyIFIqKGUxCZQeHgq4Qs0TDh4pFYEgj3MaeDdQxXER/SdQyn7f8o6iV5Li1mkt5cOhKn8j/AKvy6UGNoKEBR4k/r+kf69re2XhUHI6eS4dhx8+lpSUdEqhzEgCAs11B4Av+L2/r/U+2DEpqP2dOiZ/M9Xb/ABo6xTZvT+1qTMUPgy2VWq3HXU0sYWWkfNTtV0tNKDdlnhoDCHUgFHup5HuOd4nS43CZozWNaID604n9tepA2iF4LCESCjt3kfbw/l0YeHH0dP8A5qBE/wBZQP8AegD7K+jPqba3A4Hv3Xuve/de6xNBC/LxI3+uo9+691HbH0bcmnj/ANsPfuvdAD8ncNA/RXYTU0KiWHG0NQ+lFYtBT5rGz1I+lwPAjEn8AexTyWU/rNtgcYJcfmY3p/PoNc3hzy9flOI0H/qonVNaQU5teJbfT6D8fgGx/r7n8xIeCjqEvHkHBupK0dG3IiXj86V/3oDj22YozxXrYuJs0bqRHQUXF4lv/wAFH+P5tz9fdTBEa9vXvqZv4unCGjokI1Qof6HSCBcW+n4/2HuptYvJaHqv1UtaFunuCCmQDRGn9RwPx/Q2/F/fvBRaUUV60ZZD+I9WSfDimcbF3LVMv7E265I4LjjXBisd59P4+si3t7iH3EKfvKxQU1iCp+wsaf4D1Kvt8H/d185+EzUH2hRX/COg4/mqdvHpH+Xx8pN509cmPylf1lktgYOf0GYZjs6opevqRqNXZQaumXcjzoeSniL2Omxgb3H3D93cmb3IpHiSxi2UHz8ZhG4HzEbMflSvl1m79zLkce4X3nvZzYJLYy2ce7x7ncrmnhberXraqfhbwAp9dVKiteqbf+Ez/R02L2h8kPkPkaWpRd0ZraHU20KmajjxuvE7Xx0m6NwTPQxIYzPkRn8NIZFllVjGW1uzOxjX2R23U++by8ZooS1jauKn9SUfl+n9mes8v7273EjvN89qPa61mQmzt7ne75FYyUluHFvCA5NaR+DcChC0rSgAA62mPeQPXG/r3v3XuotXSRVcTRyqrBgRyLjn+vv3Xuqy/m5/La6F+X235oN/7SiXctJSywYDfmAWnxm99vF/KyDH5r7ao+5oVmkMhoquOpoXf1NCWAYBTmXkzY+aYgNwt9N2oolzFRZFArQVpRlye1gQKkihz1P3sR95j3c+7rvf709u+YmXbJJA97s93qlsLqlK+NBqXS5UafFjaOZRhZAKjrUM+V/8mv5Q/HusyuX2Ji5O7thUpqKiKs2tRPBveho0Z2VMlstpZqvJzollviZK5pDdjFEOBjzzB7X8y7KXltYPrbEcJLcHWMgDVDUuD/pdYAyWHXcz2H/vL/Y73Pjsdn9wZv6oc4PpjYbg+rbpHNATHfhVSFSak/UrCqig8Rznqpmvo8thK+rxeVpMhicnQTyUtdjsjTVFFXUVTEdMtPV0dUkc9NURsLMrqrA8Ee42aNalWTINCD6jBH5HrohY3u27xY2u5bZdwXW2zoJIbi3dZI5EOQyOhKup8iCQeuMeTrI7WlJt/X/jVhwPp7Ya0gfinTjWdu34KfZ04xbgqUtqF7f0N/8Ain0/1+faZ9tibgekr7XC3A/t6doNz24bUvA/JH+w/px/yL2ik2itadIJdlBrQA9PVPuWJrfuD6f8T/VT/X/Yf19oJNqcfh6LpdmYV7T08wbgRrWl/wBs1/r/AIfXn/efaGTbWFapnouk2pxjT0vNlYjdW/8AO0m2tmYTJbkzlYV8GOxlM9RKIzJHC9TUOP2KKhgeZRJUTPHBEGBdgOffrLl2/wB2u4rDbbGSe8c0WONdTH544AeZNABkkDoDc880co+3HL95zVz1zBabXy/AO+5u3CLXSzBEHxSyuFOiNA0jkUVScdXx/C74JVmz6yh3ZvKngze/6mMfbQQoajE7RinBWWLHzOumtzEsbaJqoKFjGqOH0l5Jct/az2ateUpI9/39Y5eYqfpxjuS2rxoeDS0wWGFyEJ+I8GPveffX3H3sNzyF7erPt/tekn68j1S43MqQVMyg/pWqsNSQ1JY0eXuCpHsPdY9MJtHZ9XXSwFKqWCKFW02ZfupIoXP9QfG5/wARf3kbtMaybhbhhVQa5+QJ/wAPXOvdpGj2+4KGjEaa/aadKWfEiBAkahQgsLCwstuOPp7kqKUYFeo1lhNTXjw6YpqYj0kWtf8A5H/hz7WJJ59InTND00TUoNyB/ha1v98fahW4Guekzp+3oynQVdO+GzuKkYtDjsjBUUwN/QuQgdpkW/ITzU5a3+qY/wBfYD5yiQXVpcgd7oVb/akU/keh7yZM5tby3Y9qOGUf6YZ/mOh99g3oade9+691737r3Xvfuvde9+691737r3XvfuvdVwfOz+Xv0r8yMLT1W9sLVYzfGGpGpdvdhbYkp8fuzG0geWoTGT1E1NVUeYwn3Mzv9pVxSpGZHaExSO0nsA87e3HLfPUSNukLR7jGumK7hoJFGSFaoIdKmukjGdJUknrIX2I+837pfd73CeXkvco5thuH8S72e/DSWkzUA8QKrI8M2kAeJGysQAH1qNPWvXuX+R7uDA5uRV7oydfhRPJppk67ggyJgsyxxnJ/3xqKVpVaxLikCsARoH1EOj7tsIep5vPh14fS5p9v1FK/l+XWeTf3r26fu3wo/Y62G8aAPHbdXMOquT4A28PpI4Dxqg51HgX8/wAqrpnrXbeQ3Zv1t97nosbEhmhyWajx8VZUyusNLRY+m2/RYSq81ZM4VVeoe1yxYKCQNNl+7xyeJ4I7ie8upj8Qd1jjPqaIgcCn9M/b1BvOP95v94fdIpW2WPYtkgX4Ws7Qzy/LU17Lcxs32RqPl59BfiukcBhKyKbaPVHXG2qSlZRQx5DbFJvTMRxjhDU5/dy5atmqSnDyJ4ibn+p9zXs/sp7dbUgWHla2kf8AinBl/Z4pcj9tesS+cPvgfeN51e6O++8e+eBKavBaXDWkLZrQw2ngQ6a/hCBRigwKWRfFqTGbs3Nh+td+4fE4bJZV/s9s5rDUwoMTXV6q7w4atxhaSOgq6qOMrTvE3ilkAj0KzLcSX3K0O2WnibZGEtoxmFQAFGMqAAKD7OoUi5on3W+J3S5eW9lNTNKxZmY/xMxJJPr69XN7D+PWD2y8U32sZdCGuUAsR9LW9hvo66M1Q0MNDAkMSqqooUAD6AD3vr3SI7b2hPvzrLfu0KQotduLambxdAz6Qv31TQTJRq7MVVY3qdKsSeASfauwnW2vbW4cdiSKx+wHP8ukt9C1xZ3UC/E8bKPtIx1rxRbdaiqJqWsonpa2knmpKylniMc1LVUztDU000bgMssEsbKwIuCPcq6lYBlIKkVBHp5H8+oxGtSVaoYYNeNfP9nSlpMcq2CRj6kHgWBP+wPuhKinV9LHjw6tB+Cez6/G4Lem8KmF4aHPVmNxGKZl0rVphVq5MhVRgm7wpV1ohDDgvG4/B9gvma4V5ba3BGpQWanlq4D9g6F/LkDJHcTkdjEKvzpx/wANOj9+wt0Juve/de697917r3v3Xuii/I/4i7O75ki3LR1p2f2JR0q0ke5aakWrpM1SQqftcfuXHiSBq2KmPENRG6VEKErd0CoD/aN/uNrBhZfEtCa6CaEHzKnyr5jgeiLdtig3I+MraLsCmulQR6MP8vHohL/Anv7HV/2tO2yMnRh9IylPuKopoSg/TI1LWYuOsXVflQpt/U+xQOaNqdKt4ob+EqD/ADB6DX9Wt0R6Dwyv8QY/4COjddI/CfHbMydBufsvLUG6stj5UqqDbuNgl/u1SVkRV4KqvnrUjqs1LTyepI2ihgDqCyyfgg3LmN7hGhs4zHGcFz8VPQU4ftJ6Pdv5fWB1mvJA7jIUfDX514/4Oj7ewv0Jeve/de697917r3v3Xuve/de697917pk3JgaLdG3s3tvIgmhzuKrsTVWALLDX00lM8iX48kQk1KfwwHtVZXUljd215D/aRSLIP9qa0+w9Jb22jvbS5tJf7ORChPpUUr9o49UJbo25l9lbkzW087CYMrgK+fHVSEELMIW/YrICf10tfTFJonHDRuD7ycs7uDcLS3vbZqwSIHU/b5faDgj16x4ureazuZ7S4TTNGxVh8x/kPEHzGemqOY/1t/vf/G/bxHr+3pjqckwP1+vP+sT/AE/1yT7oQRx699vUuOUi35H59668R5eXThTSSvLDFTxyTTTSRww08Ss8k800ixxQwot2eaWRwqgclj70xAUsxooySfKnn1VVYsFSpr5dXQdK7Gl686429t2rVRlRBJks0VNx/FspI1XVxahw32nkWAEcERAjj3jtzLui7vvN3dxmsFdEf+lXAP8AtjU/n1PvLm2ttW021tIKTEeJIP6TZI/2ooPy6oT/AOFInd2F2r8cerujqiuKZftHdWZ3hDQRRiY1NL19TY3GxR1yMGjjozWb3+5jZ7WqKBWQ+RFBxr979xZbPYtnjbMkzXMlOIEY0LX5N4jfaV+XXXf+6i9vdw3r3W5w9xIretjs9lFYtKxppa9aSQlDxLabTQQPwyEEaWPVmn8qrpdOi/gV8d9rSU5gyu4Nk0XYmaaRdFTPVb9Vdw4z76MSSLFX0W2augpZkBsr05Fh9PY49stq/dXJm0h0AnuVN3JQ8fFOpD8v0tA/LrEb75vP7e433lPdLeUlDWVruD7XbgZULZnwJNBoCUadZHU+Ybqwz2PusXuoOTyVBhsbkMxlauDH4vE0NXkslX1TiKmoqChgkqqyrqJW9McFNTxM7seAqk+2p5oraGa4nkCwRqXdjwCqKkn5ADpRZ2lzf3drYWUDS3k8iwxRoKs7uwVVUeZZiAPn0xbF31s7s3Z22+wevtyYjd+yt34ijzu2dzYKsjrsTmcTXRiWmrKOpiJDKwOllbS8bqyOqurKGbG+tNytLe/sLhZbSVdSOvAj/CCDgg0IIIIBBHRlzHy5vvKG+7tyxzPtM9jzBYztbXdpcqUkikQ0ZWU/yPAihBIIPSpZFcaWAI/ofavol6Re4Nj4fOxOlRSwuXBB1ICefze319+691X58hP5dnRPecMh391jtHdlQInhgyORxMAzdHGwdfHQ5+lWmzdAhD3tDUJ6rH6gew/vHKvL2/gndtqilkoB4lNMlBwAlQrIB8g1OpS9ufe33b9o52n9tvcPddoVmDvBaTsLeRgQQZbZtVvKcfjjbFRwJ6pd7g/kC9SVk1RVdfbg7A2HJ+54qGOtpd1YSMC+lhT5qnObZlP11ZGxA/B59xxuPsts0+pts3S4t3JrSQLKg+QH6b/mXPWeHI39677/APL8cdtzny/sXMEAI1TPE9lcn1Gu2YWwr/zz8fljqvfen8i/vbB+YbW7P2bnihbw/wB4Nv5/ayyAMukynGvvEw3S5Ng9iAOb3ARuvZbflkIst0tJIa/FL4kbU/0qpKK/LV+fWVHLv9757c3TRf1t9n97sVNNZ266tb4jGdImG36s+pXGccOgOqP5PHy3pndHqermCsyh03JuXS4Uka1D7LRwrfUagD/h7LG9oubwSAtsaGlRLx/ao/z9SSn96/8AdnZVY7HzapIqVNlZ1HyNNxIqPkSPn08bf/k5fJSvqUXPbp62wtGQdUmPq905yvVxJGBajfbOIpShjLEH7oNqAGnklVEXs3zVIoaS5so80KtJITT17YmB/b0Qb9/e2+w9nbt/V7kPmq+va4W4isbWIih/0QXtxICDQU8KlCTXFCcrqj+SrgqOqpKrsLee797tFMJHxeHoYdn4WpQ6h9vWaanN5qWIagdUFZSOWH4Fx7Fm3eyO2o2vd93knXBEcCCMV8wWYyFgfkFNPPrFL3H/AL2j3R36C5svbb272nYY3XSt3eyPuVyhx3x1S1tlbHCSGZQD5mh6uU6F+BO1evsfBidnbLxG1MYxgNRHjqEJU1zwosUc+TyMxlyOUqljUL5aiWWQgct7lnZeXdk5eha32bbIoIz8RUVdqcNbtV3pXGpjTrmz7ie63uP7tbx+/vcjnK/3fchq8NruQmOIMdTLBCumG3jJNdESIvy6s/606Hw21YoJGpY/Kiob+MA3A+vI/B9nX29R90P2SwsU+FqsfAiqzQgxADjyQsssYAA+rMlv9j7V2c309zFKfhBz9hx0lvYfqLaWIcSKj7RkdAJW462oFCpBsQwNwRwQR/VSPY6inxx6AssHHtz0k63G/X0/1449mMU3r0WywkVDDHSWqaJlvxe30PPH+v7XJJwoekMkRAJpjoyXTWClxe36rJTqyPnKpKiFG/5U6WMw08tuCBOzOw/qpB/PsB803iXF7HAhBEK0JH8RyR+WOh5ytZPb2Uk7ihmbUB/RGAfzz/LoX/YY6FHXvfuvde9+691737r3Xvfuvde9+691737r3XB0WRSrgEH8H37r3Serdq4iuJaamiYk8kop/wBubc8+/de6I/8AOLZcUPWm15aClH8Og3nT/wAV0KAgMuKycePaUD6p9yxAv9HZfzb2JOWTH9ZMG+Mx9v7RXoP8x+J9HEUPb4gr+w06qulwVOt9EKW5FrD6/QD2OxSmBjoEsW869Tdo4Gvm3ps2LCxy/wAXfd22hixThvN96MzRNTNGUs91cAm3Nr+/XEii2uDJTw/DbV9lD1WGJjcW/h11610/bUdbJHuIOpY697917r3v3XuixdtfFTrztPKTbkSSs2lumqKmvy2Fjp5KbLMoCibK4udRBUVdlAM0bRSsB62bix1Y75d2UYhw8I4K1aj7CPL5Z6J77ZbW9cy1KTHiy+f2j16DXavwZ2ji66Kp3Pu/Lbjo4pA5xdFj4cDBVBWuIqupSryFYYWtZhE8LEfRh7WTczTspWC3VGP4idX8qAdJIeXIVYGe4Z1/hApX7TUn/B0dfFYrG4PG0WIw9DTY3F46njpKGho4lgpqWniXSkUUSAKqgf7Enk3J9hySR5XaSRizk1JPE9CFESNFjjUBAKADpw906t1737r3Xvfuvde9+691737r3Xvfuvde9+691737r3Xvfuvde9+690z5/cGD2tiazO7jy1BhMPj4jNWZHJ1MVJSQIPoGllZQZJG9KILu7EKoJIHtRa2lzfTx2tnA0lwxoqIKn/ih5ngOJ6T3N1b2cElxdTrHAvFmNB/sk+Q4ngOiO71/mA9eYWpmpNmbXz+9PEzIMlPLFtrEzFWID0zVkFZlJYmUXBeliJ/p7kbb/bDc50D7hexwV/Ao8Rh9tCq/sJ6AN97jbfCxSws3nI/E58MH5jDN+0DpDYn+YxSGoCZ/qqsp6QudVRh9z09bURoSLWpa3E0EcrKt7/vLf2Yz+1TBCbbeQXpweOgJ+0OafsPSGH3Kq4FxtNI/MrJU/sKZ/aOjkdUfILrDuWJk2hndOZgh81ZtnLxfw3cFLHYF5RRyO8ddTx/RpaaSeJSRqYEgewDvfK+8bCdV7b1tyaCaPuQ/KtAVPyYCvl0Nto5j2rexptJqT0qYpMP+QqQ1PMqTTzp0hvkX8cqDuCjjz2BlpsPv/FU3hpK2cFKDPUSEumJzLRxvJG0TEmmqVDNEWKsrIRoNOU+bZNikNpdgvtbmpAy0ZP4l9QfxD8xmtS3mbliPeUF1alU3BRQE/C48g3oR5H8jihFTu69obr2HlJMNvLA5Hb2QjZgq18OmmqVVtHmoK6MtRZCnZh6ZIXdT/h7nGyv7LcYFuLC5SWE+anh8iOIPyNOoeurK6sJmt7uBo5hxVhx+YPAj5io6Ykl+nII+gP8AX6/U+1BHp0nB/b0+Yagymdr4MVg8fXZnJ1LrHBj8ZSzV1ZI7EKAkECSOBc8k2Ufkj2nmkit4nnnkWOFRVmcgAD1qcdOxRyzyLFDGzSsaBVBJP2AZPVlHx2+MNRtKtot+dixwNuKmtPgttI8VTT4KVl9GRycy64KjMxgkxJGWjpidWppLeOI+bOc0vYpdr2lj9M2JZuGsear5hT5nz4cOMocscovaSRbjuaj6he6OLB0nyZjw1DyHlgnOAd/3GvUidaQf86HtDafyT/mdbf6cy2Uqh1x0dgNvddbsrsVTV9bW0OQyKHdm8K/G4+hoqrKZGqx1TuWnopoaGOaonkx7L4yI0b3iR7qbsm5843SLNS3tljsw4BIqpLSmnmVd2U4/DivX0M/cE5P3v2m+6FunPljZp/WvmK6m3SyjnZER0Q/TWqSO7rHGrrA0itIVVRKDqGojovn8w7+br2l8pN3bQ2x0Hk9ydF9CdO1mPyPW+0dr5bJYXdeTyu2lnxmP3Nu3cG3K6JlqcZjKcSY2io5zR0FJMxaaWpXye0XNXO97zDJaW9pG1nslrpFpAjUZdKgJIzCn6g4LT4BhakszSf8Adc+49yd7ObJvm8e5Vnacx+5W+o8W7X15HHLbRxz0ke3toZ0PbJI1JpJF8SR1FEWM6etwf4U9m712p/L86Y7k+XnaFBNmY+paTsbfPZW8EodutS7QzIn3Bter3bUR1UtFLnKXaFdQxVUy2kqaoWIlnZpJciuUNyurTkfbN25n3AV8EzPPIc+EzExamyXcoVoaamJAoWyeFn3gOUOX96+85z9yH7HcnyrYHe22rbtpsS8+q5ipDcLbAqHELXKSFFOEThpQBV1t/nh/MK7+/mc75xnxj+HGI3wOity7lye0zt/a8Fbi92d5/wANlpy+c3XnZMdLS7U2BFIRKcfUXp6aiQ12Vaxip6aCub+e94543JNh2K2mG2s4WKBPjnYGoeQCnaANQUnStNTGoBXrB92/7r/tn90Lly893ffi+27/AFx7S0jvRc3jJJbbR4gakNtCHDXN4R2+Kvc8h8G2GGeQl+9Ov/lZ0H311Z8H/i13P3BnO4OvM9WQ5SPYW+qzb+x8R8he1dv0+7t37K2LuCurMPBQ4nb21MJSU2Smqn8WQraavml+3SdlULS2e97XvVpy/t1/K+6QyBFW2kZQlxIFWRYypUAiixuxIqUJrpA6n3YOZvZf3L9tucvvD+8fIOxW/I26WytCdys0mu5dk26Zra2u7uFFlZ5J7mZ3iVBWKN4EXxGQEnyw/wDOF/mQfB7N0ex/mF1xPvmClhSOPCd17GrOrOwstRUCOJW2T2nsSizGwd7iKBk89fW0cklRJo0DVIT7Gdn7lc+cszrY77bGYKAPDvIykmkYqrgIxr/Gwkr1jbffcU+6l94fb5+YfYvmpdukdiTccv3a7jZRs9KfV7deNFeWlWB0xRyAKK1wo62HfgR/Mc6K/mDbRzuZ6tp9x7Z3dsuHDvvzYG7KWBcnt98199HRVFDlaCWoxedxVRUY2dEmjaKdQqmaCHyRhpv5P552znCOdLaGSG/hVWlgkoaBsakcYdailaKfVRUdcuvvK/dU9xvuw75tthzjLaXeybg0o23c7Jm8OYRaC6vG4WSGRRIpKmqmpCO+lqWAFQ3BAI/xF/Y26xk6b6jFUNSCJaeNr/1UH/ex7917pNVuwsDW38lJCb/1jX/XP4Pv3XuktVdPbZqCSaKn5J58aj/eLWt7917qLF0ttiNgRQ0/1v8A5tP9v9D7917pS0HW23qHSY6OAEfX9tf63+oH+Hv3XuljSYigo1CwwIthbhQOPx9P6e/de6cgABYCw/w9+69137917oPt70m3sVispunN5rD7YxOJo58hmsznq+kxOCoKKnQvUV+SydbJBSY6CFATJNI6xgcsRyfa6Peodtt3lv5kSyQVaR2ChB6lmIAH2npNFy5fb/f21hs1jNcbtcOI4ba3RpJJXbCqkaBnZ2PAKCT1St2T/Oc/l5bD3NNtcdv1+9pqWZoazNdf7N3JubbNPIvkB8WeShpKDLRAxi0tA1XE2oEMRcgH3XvtyLZT+DHNdXKg0MkEXaCP+arRk/aoI9CesxOWv7sn73fNW0LvA5AttuRxqjt91vbe3uGGOMOp3jOeEojYUNRWlTofF75O/EL5Z1ER6i762JvzJxxCrk2DT1dbt3fBhWGWqkes2fuqjwO6mo6eKnczPDSPEAhvIB9RNt/upy1v/wDi3L25o16R8MoMcnAk6I3Cl9IGSuoD+fUDe5P3Tfe/2Vk+o91/brcNv2zXpF0qrPaMdQUA3ls0tuCxIopcMa0p1YwiJGixxqqRoqoiIoVERQFVVVQFVVUWAHAHuhJYlmNScknqPAoUBVFFGAB1y96631737r3VG8vyO7oxVUauk7K3K0itr8dbUU+RpPrezUlbTz0xQ/00jj3KK7NtjjS1ilPlUH9o6jR943GM6lvHr5Amo/YQejXdCfOSDcuboNkdtw4/EZLIzRUWH3nQIaPDVtdM6x09FnaOR5ExM9VIwVKiNvti5AdYv1Eh3blZoInu9vJZBlojkgeZU+dPTj9vR3tXMyzSpbbgAshwsgwpJ8mHkT68Ps6sa9gzoYde9+691737r3Xvfuvde9+690nN3bTwe+Nu5Xa25KNa7D5imanqob6JENw8NTTSgFoKulnRZInHKOoP+Ht63nltZo54WpIpqD/q8j0zPBHcxPDKtY2FD/q9R1XDuj4N73p8hKu1Nx7ezGIeRvtnzL1eKycEJ5VKtKajrKSd1BsXjZA1r6F+nsXwcy2xQePE6yeenI/LIPQUm5duQ58GVGj8i2D+eCOh16F+JWO6yzUG9N35Gj3HuyiWUYaloYZFwmCkmjMUldE1UiVGQynhZkSV0jSEMSilrOCzdN+e9jNvboUgPxE/E3yxgDoy2zZFs5BcTsGnHwgcF+fzPRzPYd6P+ve/de697917r3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de697917qLXVtJjaKryNfPHS0NBS1FbW1UzaYaakpYnnqJ5W/sxwwxlmP4A9uRRSTyxwxIWldgqqOJJNAB9p6blljhjkmlYLEilmY8AAKkn7B1Rr8ge7s73ZuqoqDPVUmyMTVSx7UwGto4BToWiXNZKAHxz5fIJ6yX1fbxsI0PDFskeWOXLXl2xSMKrbg4Bnl8yeOlT5KvAevEjrHvmTmG5328Z9RWyQkQxeg4aiB+Ijj6cOHRe2ph/S3PNx/vR59ijX8ug3U8P5dYGpv8L/APFf99/re9hhnPXgRWpqOpOLrcpgcnQZrB19ZicxjKmOsx2Tx88lNWUdTE10lgmiYMpvwR9GBIIIJHuk0MNzDJBPGrwuCrKwqCDxBBwenYLiW3lSaGUrKpqrKaEEcDXBr1eL8Y+8R3ZsVqrKiCDee2poMXuqmp1EcNTLJEXoc5SwrxDS5eKJyUFhHPHIgGkLfHLnHlv+r24hYKnb5gXhJzSnxIT5laih8wR516n3lTmD9+WBM1BfRELKB51+F6DA1UNfmDQUp0P2WwmGz9I+PzuJxuZoX5ejylDTV9Mxta5gqopY9QH5tcewxb3VzaSeLa3Dxy/xRsVP7QR0I7i1truPwrqBJY+OmRQw/YQegqk+O3R8tR903WO1BLe9o6DwwE/40sUiUp/2KezxebuZFTQN3lp86E/tIr0TnlbYGfWdsTV8iwH7A1P5dCNt7aO1tp05pdsbcwm34GUK8eHxlHj/AChf0+ZqaGNpiPwWJPsou9xv79g17eSykZHiMWp9gJoPy6NLWwsbEEWdpHFXjoUAn7SBU/n0ovaPpUBTh1737rfWnbu7+Rb80O0Pmzv3O723ntHD9S9mbw3pvbd/e2Gy8Wbr6vb27s2mdz2zsdtLIZDH7qj3JuGfNVlPLDPTJjIqTyRHIVNOxgkxck9pubr3mCdL94/pZpWmlv1YMpLklmEdRKZO6lCACa91BqPdnY/7xn2C5P8Au+ctbdy/sF9PzttFja7fY8t3ERiRZ7aIww3T3KI9sYIFijcMrmZn0t4EcgDqT3+aZ1N8afin3RgPiz0pg6+Lb+x+op6Xsjc8uROe7Q3p2tu2bFbpkqNwZWfwQVT4zryfHtSU8ccFFTCokgSKLzN5Qjz9tO0bDvqbJswYi0ijE8shqXlerliQAoARkFFAAocVqTOv3N+dfdv3o5A3L3k9wNxibdNx3wPtNmI/B2+1262EluFhjFSokvVl1sS0j6VdmfQNAk/6SvmL/O435jeius9p5DYHxe64rsBSY3baVM9H1jsDau3aahxmCzPZ27gJaveW/WoNckdFRwCp0r4KIUsU1XV+zUzc1+4t9Y7LtyaNqtkVY4AT4MCKuhZJG/G4XFTVj3aEAqOgn/VL2J/u9uWrr3H5u3qLc/eHdY5nluyoa/vbidnkmi2+2wtrZ66AySNoqdc3iOkUXWyR178fvj1/KW+J3a3a2NgO5M5191nk8zu/sHOU1LSZ/dr4aGWp2/sfAUkc7Uu0trZLdFTFBQ4eklERq6oSzyVFU71DzfYcvbL7Yct7pu0X6+4pCTJcSijSMSAkaip8ONpCooCckFiSARyf5o9zfdD77PvVyXyXdy/Sbdum7x29jtduzNDbCUhZ7uZiNVzcJbqzSTuurQmhFjiCxjXK/lUfMD4q9T/Kff3dPyv3vnMZvLclRncjtHs2s2dlqjY+Q7D7VyNTU9j72z1di56/J7daHGSwYbFz1NHPSSUddWzS1MZbiDfbnfNi2rmabeuZbiX6oq3gvpLhZJCfEkkKnXqKkigVh3sTpoOuqn3zvYv3n519m+WeQfZbl63m2G0SGK+2hLqJbtLHbkVbG0hSRUjnrIGuJlR1cSRwosbAdbgGRxfxv+YnVBpq6Dqn5EdPbpiUo6Sbd3/tKtk8Ec0c1JWU0lfTUeWpIqlHSSJ4qumZlYFGsfeUMkXLvN23UYW19txNKgq4VqeRBrHIAfIhlr5dcMbW891vYnnQS20m9crc92ZyCJ7K5QVIIZWCM0bFSCGBRwCCCOtcL+bR0Z1V/Lb+IGC6m+HSbx6tzPyM+S1J2Dla7D7wy0u5oMf1nsnJ10eExW55cjR7kpdsYHJ1NBPTxy1dS1LLJLJqLSm8Ge4+y7XyTs1nt+zNKhvb36mRnapCwIVVAwAYqrTBl1ajXOqvXVn7k3uLzn97D303HnX33aw3mw5V5SbbIY57WIW7Pf3caGWS3EbQNcTRrIrFUQOAq0AUdF56T6d/nqT9G9ed49Ydu92di7O7A2hid8bexdD8ltv5XOwbZzePfK4lhtHurA5J3qRR1KXgiral6lipViCHUisNr91pNtt912y8v5LB01x0uSTpzkRtMGycgBDUcB1KPuFz3/dzR+4vNHt3zhyPy9tW/bZfSbddTS7DNHCbiJxHJ/jO1TRgLqU9zRoEFQRUEEyHwi+df84Wh+W/VHxy+U3WG5MxtPfO6hh81uXtPo89fVmJ2vS09dkMtnsZu7ZWMwO15q+LG4qZ6XynIU9RUkU4J8scsQg5a5x9w4uYto2feFkaOeZY5IryDw2CE97owSNiVUEgnUD1FP3hfu5fcVufZHnX3W9m+b7SDe9usvHt7TZt2+tSS4ZkSOGS2u5JrgIXkUPTwmRKyEDSytbLtT+br8Vd6fKAfEjBUXZdR2nJ23urpqmmbEbL/u3U7m2XVZuk3FkjUw7+mztDtykkwUvinq8fTz1epRBDK4kVJGg90dguN+HL0VneG7N0bUSFIxGWDlNQPi6tFRUdtafh8usJ96+497z7B7Pn3u3KfaE5NGyW+/Ovi3Xjrb3SxNBHpNmIXnYTLVUlZUoS7qNJY+ncndnVHx82Hkuz+6d9YLrvYeJqsZQ125NwTyRUcddmK6HHY2jhip4qisrKqqqpwBHDFI4QNIQI0dlGu77ztmxWbbhu12sNoGC6iCSSxwFVQWY+dADQAk4BIxs5D9vudPc/mS05Q5A5cud15knSSSO0tQCxSJC8jEsVVVVRxYgVoo7iAQ66o+ZHxd7y2Rv3sjqbu3Y299k9XUNTk+xc9ichMsGzMbS4yvzM2Q3DTVtNS12Oov4XiqqdJXiCSR08hQtoaxft3N3Lm7We4X+37mslraoZLhtLqY1AZtTKyq1KK1DTNDTh0KudPYf3h9u+YeWuVOdfb3cdu5h3mRYdqtp0Gq6kaRIgkLKzI7+JIikBqgstaVHQA70/m1fy4thGpXOfLXq6tlpSySQbRqM1v2UyIoYxRjY+H3Csj3Ong2DXBIINie49y+SLYsr74rEf76jlkB+wpGy/z6kzYPuS/er5k8E7f7JbzGj5DXyxWYp6n6uWCg/yZHl0XBv5/n8tT7yemi7O31PDC7/7kF6p3pBRywo4U1ECVuPpa+RCDqEfg87D6Rk8eyV/eLlFX0BLsrWmoRCn2/GGp9o6lYf3Zv3tPAjlflDblkYD9L942pYEj4SVdkB8q6tP9KnVie8/mH8WeuqPaVZvzv3q3aLb7g2tVbRxe4N3YvGbjztLvSGkqNs1VHtWqnj3L9rlKetikEj0iJFG2qUooJAvuecuVrOG3mut9t0WVEkRS3fokAZGMY/UVSpBqVAA406xa2D2K95Oap97g5b9tN5vhtrXCX01rbSSQQtalluFa4UGDVGyMKBySRRamnSp+RnZu4uluhu3+3dqbMHYe4Os+vN075x2yTlpMH/eNtsYmpy9RjlykOMzEtM70lJIyhaaVpGUIAC2oLeYdyn2fZNz3W2thNLbwtL4ZOkELliSATRVq1POlKiteiX2r5R2vn/3J5G5H3rf/wB17Zu+6W+3S7h4Yl8D6iRYlfwzJEGAZgDVwADU1pQ6EHzs/mOfIz5z7zym2d+VVPjdibQqpxgOrdh53K7c69qo8amSodx5LJJVVb1u/wDLpmDC+PyVXJTrHR0L6KGBqiWJMP8AmjnHeeapY59zugtuv9nBECI0PENpJJLUxqJJzig6+lX7uH3VPav7unL9nu/LcLS8yXyD6nedyhjnvVMhjeCOPSoSyjMWoSxIGJkkFZnEasbcfhz/ACD+hPkJ0D1929vH5Ob+y2N3xjItx4fD9O7e27sig2xXIRQV2D3BV70we58/mt1bYydJVUVbJUwUckFVHIiIqgl5F5Q9qLDftmtN5ut+LLOldECfAQaMjM/EqwIICgV4FhQnCH33/vK/cr2w9zOZ+R9i9odsgu9umNpPPvs8929wh70mhW1mt4Yre4jZJIwjSBkKsxJPaEHzZ/kb9lfDzalT8jfiJ2juDc+F651Zzd9H/Da2h7Z2bteimp6ms3vgavE1lZRbok2nHT/xCoehgw1bRRwNPAkpS8JdzZ7V7ny3aSbxtt+buzh/UcBTHLEFyHBUkMq8WYaSvxadIYgc/d9/vEuUvfXeovar3x5OtbO/3X/F7GTxEfbbq4YFUtJlkVXtxclvCUSNPHIWCOVr33y/ymPm1kvmJ8fZqffuWpcr3J1LUYnb2+sjE1Ckm68Rl6GSq2nvs0+PCUgOZWirKGeaFUp6utxk9TCqQzxIsre1vN8/NGyy2+4yat3s2EcrHi6NXQ5wO40Kt811H4qdc2/vsfd8tPYn3Ojl5asnh5D3tZbrbom10tpYnC3Nnqerfpa45FViXSOZI3JdGJtQ9yf1hr1737r3Ws/l8hdiityTY25/qf8AW/1vc2xR8MY6hiR9RznpF1UoYMrcqQQefrf6i5+lr8e1YGR0mY+vV9fw27Or+0OjcBXZqoarz22Kyt2bl6uV9U9a+FEBx9bPcl2nqcRVU5kY8vKGb8+4m5lsUsN1lWIUikAlUDy1cQPkCD1KXLl819tkTSGsqExMT56eB+2lOjU+yDo+697917r3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de6LT8t87U4To7c0NG7Rz7gqsVtwyIxVlpsjWI9eoI/47Y+mljP9Q59jPkK1S55ktWcVWJGmofUCg/YWB/LoH883T23LtyqGjSusVR6E6j+0KR+fVM70lv7JH+uPpb/AFufp7yErx6gOo4cOorUp+tv+J4+l/x7317/AAdRmpv9p/230/4i/vdT17iP8PWBqf8Aw/P5Fv8Ae/8AD/H3vVw61Tzr+3o2/wAJM9VYPu6DExuwot2bdzGMrIvUVebGxLmqGYrcqHhNHIob6hZGH5PsDe4lqlzy3LOw/VglSRT9p0EfZRuhtyDdPb8wRQA9k0bIR9g1g/aCn+Hq5H3j91O/Xvfuvde9+691737r3Xvfuvde9+691r3/ADF/kKbU+VPykr+/IvkJvDa22ew90U+5e29k5DC0mcyDT01FTY2UdeZqOox9Fh1rcTjqWiiWvo6w0KQ+TyVIKwJCnMPtF+99/l3W23kpbXErSXCyLqdampETCgIPABh28atw66fexH95RvXsz7OW3to/tfY3m77XZtabJuEUrQpRnaQfWxFXeXRI7yExyR+IW06Y8ubseiehepfjV1pgOoulNmYrY2xduo5pcVjIj5q6vqAn3+bzVfKXrc1nsm8Yaoq6h5JpCFFwioqyrsuybby/t8W27VbiO2XJ82ZjSruxyzGgyfIACgAA59+4/uVzt7tc27nzx7gb/NuPMd0RrmmOERa6IokFEihjBoiIAoyaVJJox/4UMd5V9H1D078TdpVpk3J3zvrG5TcWHpEq6iurdv4PKUeM2diJaSlWY1UOd39kYq6KnMM33g29NEAp5MP+9m9tHa7Vy7bvWWZjczItdWhO2MGmCruWp56kB8s9Ff7r327tp+eOe/eve7em08tbbJDazuVCJNNG0l1IGamkw2aNGX1L4f1SMa9Nm6f+E5nQG8+n+taHGdn9i9Yd6YXZGJxu+96wVEW+Nubq3FNhIabPNX7YydfRzUlItWXhhTG5Okpft9WqKR5Gc+/1lLKXarDw9ykt948JTcalWSIuRVgFBUjSxoCGIoBgnPSzZ/71P3N2Hnrmy4vOT9q3j25uNxkl23b2U2k9tAJi0Oi4jRgzaaMxmhd9dKMoUDqw/wDle/y9YP5eXTm8dhZDd2G39vLfW9zubP7sweEyG36ObFY7D0OH27h/sMjlcvPJLRNHW1ck2tQZcg8aqIoowBt7f8lvydZX6XVwkt/cShnePVpCIKIndTgSxrQfFTNKnFz74X3oJPvRc+bDzLa7HcbZsO27d9HbWVxKkziR5Xlnl1xxxgBwY0C0PbEGJLM3VIf/AAos7Hp5vkN0JsOTJRSf6Nuid4dhQ4eRBkKYZLs/fNBseWprMaJYqcvHg9oTMGqZqVUBV0lUBmER++F5JLv21WGqsMdqHpjDSSOGHmQSsaH9ny66F/3WPKkqe13uTzItow/e3MlrtbTg6G8Pb7R7sKslC1DNcqKIr1yCpwDZL0F/O7/lpY/aewero979hdU4zaO2cJsTbsXYnVu4IaVaLZ+Lpdv0NIa7Yab2xETCDHogImESsQuoEgex3sHuryVb2Fjtpe6t7e3gSFXniB7UQKtRC0pBIHp1id7l/wB3p97W53rmbnF+Xtr3q7vruXcro7XuEJbVdSNM7aLz6SQ5cn4dRGaHq72grqPKUNFk8fUR1dBkaSmrqGqhOqKpo6uFKimqImsLxzQyKyn+h9y7DLHcRRTwuGhdQ6MOBBFQR9o656XNtPZ3NxZ3URS5ido5EbirKSrKfmCKdfPR+PXZnW3SH8zmm+THcO5MvhNlbV+QXcO+NxVFNjKzPV5lqNl743hTY2CWCO+QzGe3Nl6TGUqSeEyvMZHZUEjxYTcvbtb2nM1huu4M4t4pzcvoGpyVYsFAJFSzACpIFTUkDPX1B+6HKPNnuH90OX2j5F2mC45gvOWNr261V5FhSi3dpatIQT2RQwRPM5GrSF0gE6Qw+713V8uP59fyjyuK2bT1u0+otj1T0Wx8BXw01T1/0/s/K1Uqybs37Ola01Vv3P0GPDTVNNDPPVTqaWkaKCCOJxFf3fMvuhzJHFbQ1RSfCjqwitoifidgOJoC7U1OQAq0CIsacv7N7I/3a/s7ZXu/SR3vPG4p4m43MZZb3c7qNQRbWYKUWzhd6Kjsqop8SUM7sw2hcL8Iuqvh7/Lt7/6I6qhSSsyfx17YpN47/wAlQUlNnd87pn6s3BipNxZqKgVYaWkiaRjTUUJMdOjOzNNUzVNTPOTcpbdypyFzNYWXfcybfcNcXDCjSv4Lip46UXgiAkKPMsWZuPe4feE5z99fvSe2fuPznIRBDzTtr2G2ROzQ2luNxhkEERfLMad8jZYgABI0jjTWq/krfy7uifma/e1Z27uPtylqurqfqKXCL1pu+TZOClTfeM3zX1NPkqiTFZDL1tbTri6ephaKakRGnlBjtcGFPbfk3aucpd5XdJLiMW3hGMwGMV1mUNrLRvnsGmlOBrXHXWf+8B+9J7j+wi+3EHI+1bG8G8Pua3H73thdzA2cloitGokSJEbxGRqq5IVTq6vCyP8Awnq/l9ZUmSv/ANPFVU+A08dXU9sSVdTBHd2QRPWYCoUCKSQsqsrJqJuDc3lYeyvKoFFvr8fY8P8A1o6542v96B952yAS2/q2kWrUUTbQqk4rULMvEChPGnn1Rz/Pt+PkXTnyo6zm2VDlKbFdq9QbMgoaunqftqnP5DqXCRdd1uGystFEFq8rS4DbuBkpHWmSAT5GYsFvcRH7o7DFsPMUSw1NlJZQaCwBIMai3zSgJ0xBmoBWvXRH+7W9z3579mubk5gkhe82XfLppEddSwpuUpvkljDntjaae5DguW0xJQnoyX8o7+c1Rbaw2B+JHzXzf3mxMjCm1OoO6M48tZRYrEzzfwWLrzsquyMjVMm06eFxDj8tUlpcfBpp6y9L4pqcScge40VjbjlrmZzJtJXwopnz4SsKeHL6w0OD/ofw5jp4cT/fe+4Rcbtf7l73fd92/wAPmOJje77sFuAjySKPFN7YIg0i5YjVLClBK1Xi/U1JJWNurqHrbrX5mw/ELfFLTbUpNud0by6bm3zjaGjY1+yezc1g8Z1HvSEzKTXVO2INz4TdsK+SURT0lQxj8dQWaLLraBY7/NstzMPAS5MBmNfhLaBNQGpXT3AVyCOsvNm545s5s9hJPfLl6Z72a72C135dumdhou9vimk3O1Ok9i3Bt7ixbA1K8Y1ao6C3f+Ut8ud0/FP5MdhfAP5K/b7Rr6rftXtbG07ZOerwOF7FhqpsXg62iqasJDT0PYdBT0UKvHLVTZWaposgViRq6cyT7Z8w3PKPMNzypvTGO0mmMJDHEdyvbUUJGmQjSWGCdBrpBPWDv32fY/Z/ef2k5X+8x7S6762TbVvJW8NVmlsSoklR1XLPZO0jUKosKpNACxEKdbWtfQUWUoa3GZKlgrsdkaSpoK+iqo1mpqyirIXp6qlqIXBSWCogkZHUghlJB95OTRRTxSwTIGhdSjq2QVIoQR6EdcX7a5uLO4t7u0maO6idZI5ENGV1IZWUjIKkAg+R601/+E/+5arZ/wA9u/OqdrUL1uyMrsbfVUa7HslZQUmDxO8NvVuzqnIVyv5CMdFM9PSLpMQky1VqKuy68WPZy6li5v8AChUtBPaSJJx7QpVg58uKhc/xdd5v7zTaYd9+7X7ac6bzciPmGHcbNPDlqjtNJazpdKiUp3kBnPGkEVAVBpuZ+8q+uCXXvfuvdautVUFiWJuSf9iAePz/AIe52VaCnUJM3E9MM8vP1tf+n5/x49vqP29Jmapp1dF/LfxNXR9Jbhy04kWmz/YWYqMeH1ASU+OxmHxUs8QKhfG9ZSSrcE3ZG+lvcZ87SK26Qxg9yQgH8yT/AID1JHJkbLtksh+F5mK/kAP8I6sG9g7oXde9+691737r3Xvfuvde9+691737r3Xvfuvde9+691737r3Xvfuvde9+691737r3Xvfuvde9+691737r3XRNgT/T37r3TNXZqmoVYyuq6frcj/Yjn8j37r3SXm7EwsLFXqYVI4OqRRz/AK/HvVR17rD/AKSsF/yuU/8A1NT/AIr79UfPr3Xv9JWC/wCVyn/6mp/xX36o+fXuvf6SsF/yuU//AFNT/ivv1R8+vde/0lYL/lcp/wDqan/Fffqj59e6L98m9wYrdnU+UpaWpgkmxmTxGaEayKS0VJVeGoIANz46eqdv+QfYu5Iv0sd+hZzRZI3jr9oqP5r0FecrB9w2SWNPiSRJP2Gh/keqxpFoz/uxOf8Aawef9v7mr98QfxDqHP3HPShB6gSR0hJIki/1rgcf7f3cbxCcE4/b1o7DNxAPUB0pwT6k4/2q/wDxN/z7uN3g/jHXv3FcjhXqG6wcgvGf8Q3/ABX+vu374t/4ut/uK4oe09GL+J4pabuTGZuaWNKXb+GzdZO5fQoespP4VTRkkkEu9YTb+in2Eued4t25euLdWBeV0QfkwY/yXoUcnbJNFvlvcsCFiVmP5qVH826tZ/0lYL/lcp/+pqf8V9wZUfPqZevf6SsF/wArlP8A9TU/4r79UfPr3Xv9JWC/5XKf/qan/Fffqj59e69/pKwX/K5T/wDU1P8Aivv1R8+vde/0lYL/AJXKf/qan/Fffqj59e67HZOCJsKuAn+gkQn/AG1/fq9e6e6DdmPryPDKjA/SzA3/AKfS3v1R17pTxSrKoZSCCL8e99e61Df5x3w+/mH5/wCV+Q+VmwNjZnsvr7ZdXsTJ9U7m6dnnq999aYbYlIuYp8bkdn4qqp98mqxm6J8rkTX4xmjeSrWQzQkJFFjF7kcsc4PzLe8wLbSzWI0/TzW1SYlQal7VJkjKEFi9NNasCK0Hcn7h/vp91zbfZW19l+ZuY4No5n3CO8h3q030Ktnfy3jeE0kd1IrWmmS3EMXhzAEBCuh6szFV6D/n4fO/prO1e1O1odpd+YnCvXQz7d35h67B9iqtNDUV9RBj96bIwVP+9QimZWfM4ytljjkAkI8bPGT7L7r82bWkS3F0t5agUIuVGoCuT4ilXLfNi4+XCkz+5f8Adqfdv5926DeuS5L7lq9uAjLdbbKk1j3FUUva3cxw+oECCaMEiqjuCttY/wAv75/dY/zCepsv2X15tnduy6/aWei2rvbau66eCY4jPy46nykaYfcOPZsZuLFz0dQrJKq09Sn+7qaHVHryE5N5ys+cLO4ngtZIbmEqs0b9wBYEgo4ADg0PEKQRlaEE8YPvN/dm5w+7BzrY8pc07vY39tfWxvdvvbJiPFhDmMmWF/1IJAykFTqQ/gkehprpfMnrPFfM/wDnz4fozM1OTfZtNBtHY+7KXD5BsXksnsnanWeK37vOioshj/DX0sX3GVyMfnLyLFNSyePTLG6rBHNFkvNHuvNtOWtnuYIWKEVCRxKZqcQCoV/LHmPLrqf7Dc23vsH/AHbV97i2EUI392udxsXnTxI47u5v5LO1dkeqMdMcR00GpXXVVWBNjtX/AMJxfg2N0Y/cGA318itt0NJUrLU7do967Mr8fWUzER1eP+9yvXlZmaemraMvC5FS0oWQlXBC2kOX2T5cdgF3S+ER+JSYiePkREKfmD1inB/er/eJOz3W17ny5ytd3DppS6ktLpHRuKvojvViZkajDsC4AIOa3zZnJ0e2Nu5XMVGiPH7ewtdk5vJIyRx0eJoZaqTXMVmdESCnN2sxA5sfct3M0dhZXFwwpDDEzmp8kUnjnyHz65t2FpPvG6WVhHU3N1cJCtBUlpHCigwCatwx18tyh2dvPsSpyu8U2vmc7gtv0OW3ZuiKhpskJsLt6qzk+UaryWUq6Oio61amqz4eMw1CvUo6xq8U0sV8Ch2q6oTqAy3EDgKmnAVoM+Z6+xe437YOVobLYW3iC23K6kisrNpGjpLOsIj0xxqzumlYaHUtEILEMit1umf8J9e+upd+/E3J9MbWwO09rdodLZ7wb+GBjpKet7Hw24A9TtDtKvHmkydXWVmPhOLrBOS1HUUCxlYVeOFcmfZndNvn2W62qO3ji3OGQySkfFKrk6XPmxQ9h4gAIcaqdcA/7zr22525a967Tn3eNyvbzk/f7bVtn1JZlsZYaLc7emBGqo58aPTiRZSwLkMxul7pxn8b6c7Zwwp56w5frPfmMFJSrI9TVff7WytJ9vTpCDM88/l0oEBYsRbn3JvMcRm5e32EKWL2U6hRxNYmFBTNT1gFyBefu/nzkm/8VU8Dd7ObW9Aq6LiNtTE4AFKmuKdfPZ+J/wDMt+RPw1qt503QFPtKkou0sfsKlys259mf323FmJuscHk9u4SpNJFunGR0clX/ABOp87KGLBUC6vGxbDvl3mre+VRfHZ7pI2nKeNqVWHZr0ga1anxnh69fT/70/dJ9rPfmHYZvcyW+e42eW8eFbO6+kgiG4TRzzLqNvIXC+GmkGnE1pqFNkf8Ak3fP35z/ADE7g39jfkfgqlusMX1vmMzhM/i+oJNm7Ypd3R7p2dSYfHLu5aZIK2qrMPWZfTRmaWQrS+Q/pJ9zR7Zc4808xb7dwbtdNPti2rMGWKNVWXWmkF0ReK6qAnP5Y5Qffx+7P93P2J5F5au/ajckHOE27RW9xbTbmLq4a2NvdNK/02olFWVYKyaQKvp8wOll/wAKFuvqup+KOxe8cFRUc24uoOycfhZchXUvnpcNtbs+ShxGRyk0wBNM0O5sLhoEc2W1S6m4Yo7/AL3bSLrZtp3UKxe3naJtI/BKtak/J41A+bdEP919zPBF708xe3e5XEi7Vvm0vcCKNqNLcbeHkSMD8VbeWdiOPYCOFRr/AHTPwug+Z/8AL03X2r0xt+Kq78+Ke9Nz47dOwITUVMvbXRO4J6ndm16vFTRSpk5N+7LyAzVLjqmWGKor8ZjTQEyLFBT+4f2zlo77yzue57bU7vt0gNxEqirwSLqVxStZEZZCw/ElKHUoU9NOfvf6T2C+9DsvJfP25lPbXnSwt5bPc20qNt3iELbXCyAgxizu0+neVAxWKaXxwFLPJ1WdQ13Ym9Nxbaqtz1+VyO5sJR7W2/tXM7rGTq5KiLAZ3auCweKpsm1fHUVsW1MDXUH28sUhNLiqaOm0mmWBowbLJ4neZS1QF45oqUVangABQDyFKUpTrLi5t+VeX9q3eDaLaGLaLiS4ur23svDUKZobmaaRo9BVDczJJqUijzu0lfELhtmr+aR8Zsd8nPi10N/M42JS1MW86bqPaOP+RsmAoy+SGGSgpKd+waZII6as/jXTm/6SWCtmhR5pMUoZQsdGLzHzzsx5g5X2Hn/bxrunt4k3CgpqZQIzJSg+GQGNvUaDhVJPIv7nXu5d+0XvH7k/dE5jlRtgfe7mXlVblv0/FLs30TEll8LdLJg0asQomNDVpT0x7u/nnbtrfgJsjrHCY+vrvmdvHbOZ603vvzJj+H7L2zt7GYmOjm71j3N5Bjspkd1bcqvuKcQyJHS5aGtllVEp4YKjdz7tTy8mQ7Qus8wOjW087eUdNIkBrVpnU0PCjBn4aQTHZP7unY7f7y3MPN+4XUcfsHYXkW77ftsPfdTzySlhtBt6eJGlvOultQJeFoVUkyM6HC/4T9/CzcPR/TO7vkd2BS1MG4u9ocZQdcwZGmlo8rT9RYcrLQ5ytpJqiepohvetgp5qammsYsbjqSRVQ1EgIs9m+WZbO0u+ZryLRLdIIrYHj4QbUzfZI4FKitF1AlWHUF/3m/v/ALX7h8+7H7VcsTI218uNJLurRMGjbc5cPCjABX+kQsruvxSyyqS2hSNhv3OHXLrr3v3XutV6ea5J/wBj/t/+J4/23ue1Ffs6gt2r0u+peod695bwpdn7Monf92J8/n5YXbDbXxjOFnyOUqBpj8qR38NMG81RJZVBF2CbcNytdptmuLp/9In4mPGg/wAp8ulFht11ulwttbKf6T+Sj1P+QefWxp17sbB9abJ21sPbcLRYbbGKp8ZSGSxmqGjBeqrqlhw1XkKuSSeUjgySMRYe4WvLqW+up7uc1lkbUf8AIB8gMDqY7O1isrWC1hH6aLpFePzJ+ZOT0svabpT1737r3Xvfuvde9+691737r3Xvfuvde9+691737r3Xvfuvde9+691737r3Xvfuvde9+691737r3XvfuvdYKlikMjD6hSf9sCf+I9+691Tr/NU+Wu+vij8We2+4+t6XbmR3psnHYOqwdBu2kylft2omye7sBgqlclR4bMYDJzImPyczIIqyAiVUJJUFGS3k729vJMgBYEAV4ZIH+Xob+3HLVhzfztsPLe5yzR2N1I6SPAVWQBYncaS6uoNVHFTivWnTUf8AChr5z5GQyybT+PUJYk6afaPZSIDa/p19uyN/vPslbdrkV7Ex8j/n6zNj+6j7dvWu871/zmtv+2PrJH/woB+cDgk7b6F4P42r2N/9tc+2W3q5AJ8KL9h/6C6Movui+20nHe98/Ka1/wC2Ppyi/n6/Nt7X270Tz/Ta3Yn9L/8AP1D7YbfrtaUhi/Y3/QXRjH9zn2yetd937/nNaf8AbF04xfz6fms5sdvdGfX8bX7C/wAP69pH+vtg8x3oFfAh4ejf9BdGMX3Lva56V37f/wDnPaf9sPU+L+e/80n+uA6PHIHG2OwPz/r9oH2nbmi/WlIIP95b/oPoxi+5H7UvSvMHMP8Azns/+2DqTJ/PO+ZFbTz01Vt3pCWCoieCaJtsb/KSRSoUkRh/pO5DKxHtn+uW6QSJJHDAHU1B0tgjh+PowT7intFcK6Scw8xaSKEePZcCP+eDpCR/zc/k89gdvdQj6Hjb29P6E/2uwD9PZg/utzKtaQWnH+GT/rb1WP8Au8fZN1BPMfM2fS4sf+9d1NT+bN8mXJBwHUv+wwG8b/k/nfx/p7TP7wc0in+LWf8AvEv/AFu6MY/7ub2OkoDzJzR+VzY/963qQn81r5JuQDgeqBci5GA3ffkA/nfZ/r7Sv7zc1qcW1l/vEv8A1u6MIv7tn2JehPM3NVflc2H/AHrOpQ/mnfI9hc4Pqu9/xgt3D+n/AGfXtM3vdzcBUWlj/vEv/W/oyj/u0PYZuPNHNf8A2U7f/wB6vpW7X/m+/KTaQrBicB1CHrmjaomn29vR5mWBW8UQaPsGECJGZja31Y/4WKtw94eaL8xi4tbLSoNAElpnif7Y9HVj/dpexFsT4fNPNlW4n6nb/L/qV9K0fzsPmAbf7h+neSf+Yd3z+AD/AM/G9lJ90t/BI+isv94k/wCtvR1H/dq+xbgk8182/wDZVt//AHq+uf8Aw9d8v/8AnT9Pf+g7vj/7Y3uje6nMAFRY2X+8Sf8AW7pdH/dl+w71rzbzd/2Vbd/3q+ux/Ot+X5IH8H6e+v8Azzu+P/tje2G92OYgSPobH/eJf+t3RhF/dgewb0rzdzh/2Vbd/wB6rrx/nW/L8Ej+D9PfX/nnd8f/AGxvbbe7fMYNBYWP+8S/9bujCL+62+789K84c4/9le2/96nrr/h675f/APOn6e/9B3fH/wBsb203u9zIDQWFh/vEv/W7oxi/uqvu9Pprzlznk/8AKXtv/eo68P52XzAiZWGG6cJH+q25vkji39Oxx7bb3h5mHCwsP94l/wCt3RjD/dP/AHdZCQ3OfOv5Xe2f96jq3D+VN/Mx70+UvZG/Np9q4zr3GYza2BweTxMuzMTuXG1tRWZHJVVLUJXyZzd246eaFYIAUEccLBvqxHHsccgc+7xzVut3Y7jbWyQx25lBhVwdQdFodUjilGPl+fWDf37fuce2P3YOWfb3eeQd9368u92vbm2uF3ia0lRUhijdTGLaytCGJc11FhTgB1tF7TrzX4+Ka9wyKb/1uL/X/Ye5bHDrmr0rPe+vdEw+Uf8AL5+I/wAxcfNF3l09t3NbiaJo6PsLAxnavY2NbTCkbwbwwf2mUrooBTpppq41dHYWaEgkEJ7/AMkct8xh3v8Ab1W8P/EiHslrQCpYCj0AwHDAeQ6nz2d+8773+xN1G/t1z3dW+1hqybXcn6ixk41BtZtUaE6jV49Eno46fPhZ8P8Arz4O9I03RPWWTzOb21Sbs3Vutc1uWPG/3lyNVuavWp/3O1eJpMdQZKsxtDDBRR1CU0BalpYVKXUsz3KfLFtyntkm2Ws7SxtM0xdwAxLBQNVMEhVAqAK04Dov9/8A305o+8R7hTe4/N1nb2+7vZW9kbe0MngItumn9FZGd41kctIVLtR3Yg0NBp0/MLcfz9+N/wDMO7q+UmyOn+7OssvSb87Ig23vk9YLu/ZWW2dk9xZugo8vhs9nNqbv2YMZnNr0eOimMflneASR+WAMFXF/e25l2Dmzdt9FtNaXhvJ5Ypnj7aMzKCpdSjqVJFQSpHr13b9itq+7N7rfdc5A9neYeeuXt3sX22xa72794fS3cd1HBE7RSwxXNtdeJDcNKVrRQ2ltL0JLnsr/AIUDfzC9p5Oam3fn+p98TYiepeuxW6+s9t0kVVTUDmWelfMbJ3Z16hyMkTyRhKaIuZIYwiO7uvtfa+7HO9u0cj7jFcJ/DNDGAft8JEan+2H29JOYP7sf7r29WaTbHtm97dHOqiOayv52Ks4orCK7tr06AQDVzSjMWYAA9X3dNfzGt5fK3+VJ8svlLvrrTG9Z5vZOxe8dm0EOByldkMBufJYrrallx2cwkdd/uWx1K+d3MlE0Mssumane05Fykq2nOd5zF7dc17puNrHFNHHNaBotQVmeJQpCsWZaNKPMj58QOa3Pv3Vdh9l/vo+yns3y5zbLu+37huO0X8rXMaJNbxyX7B4ZSn6bsIYDIGUCqsKpwrWF/Iw6fwHcM3yc6v7D2fmoNn73+Nuy9u1GVyGMqaSlytVU5v8AglfntmVuQpnx2Qnwk+z8TU09bGjtTV9LGGAaIXjH2o2e032+5j26/Qm2udvdPKqgzRkMtajUrgMMYZesvf7xbnnc+RU9oucOV99t233b+bLu6WGKRWaNVi8VIbpEYOglF1OjRkgPG7UNGPVc/RG/N9/ycf5iG58XvzI5pKLrvM1ezd97extHlFxXbHV25s/hPFlMNR1SQr4anZtXTblxM883pyGIWmkLeQAke23m6+3/ADcWlSs1rKYLlFqBLEaVpXThxSSOopXQxGOsqvcjlvlv7+H3W9nvOW7S3NxukC3+23UzR+Jtu4W8MtY5WUnK3SvaTqq5inMigacb921907Q7T2Nhd37PzlFubZG+9uUuXwGfxMxejy+BztCs1JW0kjKsiCelqAdLqskbXV1VgQMvra5st42+O6tJxJY3EVUdfNWHzyD6gioOCKjr5ot42ffOTeYr/Y9926Sz5h227aC5tpxR4poXoyMOBoy+RIIyCQQetSf/AIT7z7A6f74+WmK3/k9o7GqsPs/Zgjqt1bmxFFTRQU+arI4FSszWRiEGUp5I6mWoChNKzqUZ4WiPvGX2fvtvs983CfdbuCKMWh0tcMiAMJErQsQK09Pn121/vOY+Zuevbf2SveWbS+3GGe+uqpZW8rsWMSlqrEhrGQUVK1qVIIDhh1sh7s/mFfBXZDvDuT5efHajqI0SR6Ol7a2XmK4JJUSUoP2OFy+QrCVnhZXAS6aSWsOfc+3HPPJ9qC0nMdow/wCFOJf+rev/AGOPXKPZfuv/AHjOYUWTafY7mmSEkgSPtt1ElQob45YkXgRTOa4qeoffGF6v+enwy7l2d1TvTY/aW1+z9gbiw+1tw7ZzWL3TtiXeeJiizW2IqurxtVPAkuN3XQUL1EJeOohA/sNYhPvyWHOvKG8W20XkdwksRETRMD+rHSRFP8J1qtQaEA9P+2+4c4fds9++Qt9505f3HZt42fc4J7y1vIpLe4FrITFcFVkUEiS3eQK1Crf0hUdaoP8AIw+SuP6I+ZG2OrNwVDYfH/IbBZjqrc2OyRDVGJ7M29k56jr2nllC0bR1dVW4jIU00TrI38R3L5NK/calx39qd7/c/N1vBK3+KXi/Sk5pqYgxGleJcBB8mPpjtN/eLe0t17j+w+8c57ZGJ7nle5i3mzli4S2E8aresB3VVVliZWBA8K001Ph0Jr/5uX8pjcm1ezofkl8TuuN97h2f2HuuoyfafWPUkGTr8ns3fuVoKqhg37t/Z2Jgrqyp29ka+ulq6mOjppvsqmWoiMf2dWi0og9y/bu6sb1935d29pdtnP6kEKljFJWp0qoLeE5qRTCHA0jQOoW+5D99jad65Qf2n96+a9ttd92uyWHZt33wxpHdWcbq7Wc11KUVZkRFRDI6+IgjbV4sRMtqn8mzZPyK258N8/0h8sel8vsKk2rvje239m4nev2Mq7p623mZM/kMTLtqVDV02DxuUztbSoatfHV082hVAice5D9q7Ldo+V7zZd/2mWOzWRkiW5XTrjkWsiGNgG0hiTU4bWQPhPWGX38+YPazdffjbPcP2V5/g3Ke9260ur+fb9Y+nv7WkKSCcHS00kcMbnQaoy1J7geg8+OH8iL49dM71r9x9j7+3J3ztWjzc1fsvrPcm3MTtzZ2GxEW4K/c+C27uqKhrspWb0xO3s/kHr4aIPjsRPkGaepoZj41jQ7L7MbPYX4u913KS9gQ/pwFPDTz/tKO5k8jQaFJHcCCR0Kfdb+8f90OfuX7bauVOWbTlventxFuG72k8k91LKYUt5p7cuka2ss8KCJpKSzrEBHHMg1Fry4oo4Y44YY0hhhRIoookWOOKONQiRxogCoiKAAAAAB7mVVVFVVUBQKADgB6DrnW7vI7SSMWkYksxNSSckknJJPXP3vqvXvfuvdEnx38v/460Nb93UYvdmXi16v4flN2V7UJF76CtCtDUNGfyDKbj2KH5w3pl0iSNT6qgr/Oo6DScp7OrFikjD0ZjT+VOjY7R2XtPYWGg29szbuJ2zhaY6o8fh6KGjgMhAVp5vGoepqXCjVLIXka3JPsPXN1cXcpmupmklP4mNf+K6Pre2gtI1htolSIeSin/FnpT+2On+ve/de6YdyblxG1MXLlszU+CmjIRFUa56mZgSlPTRXBklcKfyAACSQAT7VWdlcX8629slXPH0A9T8ukt3eQWMDXFw9EH7SfQD16K9mflXDjKo+HaiT0SMdQlzPirGQEcgJQywK5seLkf4+x5bcgNNH+puGmWnklQP8AjQPQGuufEglolhqjr5vQ/wDHSB0OvWfau0+1MTPkdt1LrU0EiQZfEVYSPI4qokUtGs8asyy084RjFMhMcgU8hgygJ73sN/sU6w3iAo+Y5F+FgPT0I8x5fZnoU7Nvtjvlu01oxEikCSNviUn19QfIjj9uOhK9kvR11737r3Xvfuvde9+691737r3Xvfuvde9+691737r3Xvfuvde9+691737r3Tdl6mno8bW1dXPFTUtLTTVNTUzyLFBT08EbSzTzSuVSKKKNSzMSAoFz7siPI6RxqWkYhVUZJJwAB5knqrukaPJIwWNQWYnAAGSSfQdaqX88buTCb2+HnfeI27T1VTjWx23VTLzkU8VSIN9bZl8tLSMpnaCRovSz6Cym+ke1vMHL1zt20Tz3coEw0nw1zSrrgt6ivl+3qQfYTeIr33b5NS3jPhGeQBziv6Euaen8/kOtNb4Qde7P7c+ZXxH6o7CxH94Ng9nfJvoXr3fGB/iGUxP8b2fvTtLam29zYj+KYStxuaxv8SwuSnh+4o6mnqodeuKRJArCPoUWS4iRxVWcAj5E9dOecNxvNn5L5w3bbpvD3C12u7uIJKK2mSOB3RtLBlbSyg0IIPAgjrb36I/k3/y7Ozvnh/N3+Pm5en59u9ZfHnb3w6g6OrKXtbtqCp6cqO5fjtund+/t1U2UyXYE396ZzumjhyiJuZ8vQ0zU4iWJKVpIWMht9pJNuMTLpRFXS1T21UknJzQ5zjrFPfPe33L2fkD2Z5js95Eu6blLuJv1NvbkXItryOOGMqsP6Y8MlP0tDGtalqHqvDeH8qbrn44fypv5j/YHe/WKVvy/+LXy6291PsHtmm3P2FjcVUdbZfPfEoYfNYHZ8e46HZWZwO8trdq5OspajI4meuiiygVnjmp41gLGso022+kmj/xuKXRWpxlPLFQQagkcCD1MG1e8m680e83tXtfLm7leR942SS9ubIxwM3jqm5aleXQ0qvFJborBXCkpwIY1tc+XH8tb4IfHDsrCbI6p/kn99/Knb2V2PjN1VnYfVvyI+Q9Jt7DZquz+5cRUbMrIqzszIyNmcdQ4KmrpGDhTBkYhpBBJtudvbWUyRQbDJOhTUWVpqA1Ip2o4rivHz4dRTyD7u+5fNe0XG47z94na9jukuWgW1vbGxLuipG4lFLdexmcqMcUPVVu3viF8A/gt8SehflP8+eqe1+9+xflpXbi3D1D8ctr74y3W+A2t1rQJRVtJl9w7jwuWwe6MhWU+A3JiK5p465opJMlSwrA8YmqHD8dvb2dlZX24RPNLMCY4gdCaRQamYKWqahlApgjHHrIB+f8A3X9zufeaORvarfrDato2FI4tw3ieFLh5LhqgpHG6vGoLxyLQrUBGbUDpUAP/ADFPg78fOufj58a/nf8ADDI77f4xfJefKbbk2f2JPFldxdZdi4c5xJ9tSZ6lEsdbBPU7SzdKYppqiaKpw8zJUTxSL4kG5WCRW9nuFqZDZTahSQDUjqaFSQACDQ6ccATnqRvZL3R5u3nnDnX2p9yYbQc77Kqzi4swVjubd9FJPDPAgSxNUAAiRQVUjMP+T38N+sfmD2t3nQ9j7Mzva9V0/wBAbp7S6+6VxW663r3Hdw9gYysoaHbmxNwdhULU1VtjGZqsqlpy0FVSVP7xnWURU04KTabFNwvJ4XQu0cEk6RA6fEdCoVCfJW1ZpQ+hHR39473O3/2z5b5Ql2PdIduj3PeItvvd1khW5ayt2VjJcR27VErIoJoysuNNKuvQT/zI+p/jX0z8kI9m/GDJRT7VTrnZGS7C23jt9U/aW2ut+5chSVk+++tdqdl00kw3xhtqIaNWrZJHlWslnhcgxAAk3WOziuQllJqTQrONSuEcqCyK64kVTjV61GaVMh+wHMnPnNPI53T3AgI3A308djO9ubSW6sVZRb3U1qQPAebv7QANIVhx6th/k0dLfyz/AJt1tD8ce0/hxn8x3fsLp/dPZm+u56rvHt3EYPehxfYu2dvUlHRbM2jv7A4/Czw4zftFEGijSNhQOzKXl1ez/lGz2beJm22/2cNcJG8puPGkGr9QBV8NdIWiuBWp+Gvn1j/96rm/7wvs9by8/wDLXuvBDyhe7rDt1ltK7fZSSQa7WWUs089tI0gLWznJJGsAGg690H0l/Lf+ZXSn8zLujqj4h5zp/H/Gf4g4XcnWeCz/AHX2zuyswXcCbT+Ve68pv6KrffZhy9NXwbU2xCuNyS1lBG2HZlgAqakTJtusth3rb+Z72PZfA+ltA0S+NJJR9M7F6krWulRpII7fmejjnTnP7wntFzj93HlDmf3Vh3WfmPmyS23GaDb7GFZbAz7LAlqV+mrGVM9yfEjKORMAW7E0hzsz4ofBD4YfDj49fKH547D7P787J+VdPV7m6s6R2bu6v69wGM2DTUuLyiZvMZjEZXbufqDJt7cONrZKiOqZGkydLBHBpEtSSNNs2rZtq27d99tZ7i5uyzW9qreEnhoQNUkgBerBgy6eIIFOLdDHc/dP3094/d/n32y9i992zYeXuV2Ftue9XkCXcr3RZ08OOOSOaIfqxSIFKg0idy1aJ0PnwW+IH8qL5d/OzJ7P6jwnZnZ3RtV8R892nm+rey8nvvZtf1X2tS9i9O4WmxtDvbZ+6tuZ3dQosHu2vpqmB56zHwVOpo6qtDRPTr+Vtm5X3rmO4toYribbfozN4dwdDJL4iAqGiZSwUMRwpni2D0Eve/3g+9Z7RexNtvHNd7tu188JzdFtcG67alrcLfWLWe4SM7W1xBNFBqlt42VgqSMtAY4qMHKV8rPi18YPgL8O9gdbdxbFpex/5jPeGNg37kPJvHfeLx/xp2DlvHHQ0Vdgdsbrxu09xbkjkoJaaFa+lq0lyDVkh10lLTCpDm77bZbFs9tZ3lvr5luCJ3qWAtYjTShAIVpXoagg6amvBC82+0Xun7pe/wD7y8wcy8m78+2/dw2OU2EdLe1d95uo8syyzwPcQwkOGYxuhEfhKKSSOUuY+T/8ub4QdDdgYfaHW38n7vD5K4LI7Px+5arffWnf3dlHgcTlqzNbgxc+0quLKdrSTtlqCjw8FZIynQYa+IAXB9jTmXY9l2W/itbD28uL+FohIZoZrugYsy6DoWUVAUHiDkY8zhz7UfeV99ufuX7zeeZfvmbDyvfxXr2qWG6bTtjSyRrHDILhTHYU8NmkZB56o2+XRP8A4Q9Qfyo/kV8bvlB2Huf4HbtpN3/B7pDBbz7ZmyHyB7lhqO0dyY/YfY+c3NLgqPC9lUWK2zNk8n1TWkRGL7eFq6NUUJGR7I+U7TlXedg3e9u+WA11t1kkruLmf/GG8ORmNBpEWox1oAwGrhjM4++fOv3v/bT3O9puWto+8JZPs3P2/S2OziPaNtIsIXu7KKAStLYtJOETcI811N4bEmrdAL/L5+H3wu/mCfJb5Y7/ANp9M7x2x0l1B1/sbdHUvw9oO1q9N4b5z+Q2zNjsxjajs/dG4lyUeJr947SqS0s+Yoo6WfcVGr1UFPCQCTlzY9q5s3ndZ4LEw21vb+PDtcU1XlZQF0ePKuI2cdxOkqZFAIAPUq/eQ97vfb7tftT7M8u7xzzY3XPu97nd2m887SbehtrSFJw8TrYQQ6DIltcLRVgkLraykRu7gkqn80bpD459MVXVMPUXxU+TfxP35uFNz1HYOwu68nU57YVLS4+ehgxC9bbtrqvdUu+BNNNM01bT5yWGCGONJKdZpCyhnme3sLa6gS12S/2+4ZGaa3vKFB3KF+nYqsskY7gzvxNAvAkzv9zv3A90efI+cpOdvePlLnPly1Nuu2bjsEYhvGZ1cy/XWyLbi0oAumNrcMzFirlFAIo/yOXZO7+ztJIvtzaoP+t/Fcl/vPsb+zX/ACsG5/8APET/ANVI+sX/AO98/wCVG9kv+lpf/wDViDraB+TfyX3h15Rbd6w68yT4HLZTBwZ3c25aUKcrRUNVNNTY7FYiSRWjoairNLLLPUAGVIxGIyhZj7zH5U2S2vY5b+9TXGraY0PAkZJPqBwA+3r59OZ95uLNo7O0fQ7DU7jiB5BfQnzP7Oi29T96dwbYz8WYpN/bmyjGdJKzG7izGQzmJyaliZIa6kyNRUACVSR5IjHKl7qwI9ifcdr26eIxNZxrjBQBSPsIHQbsNy3GGUSLdu3mQ5LA/aCfPq9LY+6abe20dvbrpYmp4s7jKeuNM51NTTuClVSl7Lr+2qkdA1hqC3sL+4quoDbXE0DGpVqV9fQ/mOpOtphcQRTqKBlBp6eo/I9Kr2x0/wBe9+690CvZXxu+PnclPWU3a/SHVHYiV6yCqm3jsDa+frXaSN4WmjyORxk9fT1XjkYCWOVJVBNmHskv+WuXt0MjbhslrLK/xSPEmv7Q9NYPzBr1IHKfuv7n8hy283JfuHvW1tFTQtje3EKAAg0KJIEZaj4SCD5jpM7W+IXxr2V0vuT467a6i2zjuj93VWRrNwdZO2Ur9rV82WehlyIWhyWRrGoqeqqMdDM0NO0UInUyhRI7sya35R5dtdoutig20DaZ38SWFnkYFu3NWcsKaFIoRQioz0b7z75e7PMHP+0+6e7c8XkvuJYokdru48NLhBEHCd8aLrZVdlDMGbTRSdIADt098XPjv8fa3KZHpLpzYXV9bm8dS4rM1OzcFTYWTK0VHUy1cCZD7YKKyf7qZpHmkDTStYu7WFndo5W5f2GaS42ja44J2jETMlalQagGpPn58TQVOOkXPfvF7pe51vZ2vuFz5uW8W9vK00C38zSiN2UKSmr4RpAAUUUDgBnoqnzY/lY/GT507hoN8dnjeW1uwsVtVdpUm8NhZHB0VRW4yjyUuZwce48Xn9vbhxWfjweUnlaESRJIYJ5YDJ4n0gP81+3Ox82XabhdSzw36x+GHgKgNSukurK2qlaYKkigrhaTN93375Pu793Pa7nl3k82F5yvNe/XPY7kkzqsjRiKUwSQzwSQmaMANQkalV6alr0JvwV+GNL8Guqch09g+4uwu1doNnp83tqj35DgoY9lLXB5Mni9tx4ahpjSYvI10hqHpy5p4pbtFHG0kzSruTOU35QsrmwG7yXNu7h0R1CrHju0irHvOTmlcgAliQj94338m+8Vzpa89bjyJtey76LYW93JtpmJu9FBHJOZXbVIiDSGpqK4ZmCoF1k+5f8AhPt83d2d19p7w6/3T8f6HbOW7A3bl9n5fK723rtrOVO3s3X19ZjC+LwOy83Hi5aSiyCwSxyVMrmaFgHanKJ7gqb2d5q+qvEh+nNqJW8NmcAMtag6dLFccQeB9fiPXbkL+86+71svt9ybsXM+zczSbvBtltBfQQ2lrPCs8KIslJJrqIyBnQsCEUaWGA4J6x0P/Cab5YNUvTVfenx3x2EeCsi00tT2NlciwqBFJElbJD19tVsmlPWQRzRiWXxxSRqRGw1Kz6+y3NlavfbdX1Ek38gYMdWuP72r2VESzQe3PNMu4BlarrYxoNNQSgN7c+GWVip0rUgnuBoRsY/yvvhtvz4J/Gd+ht/br2jvXI03YO6t3UG4NnpmYKKbHbjixeikrKTNUVJPDW0s9A5JRnRkdRwVJaY/b3ljceVNnu9u3KWB5HuWnVoGZhRkjSh1IhqNFfz+WeVv3wffnlv7x3u2PcnlrZb7b7V9st7GS1vjEXDwGTuVonYFWDjiAQQfXCoxf8s74RYvubI99jonAZLses3rN2LQVOaym4svtrbG9avI0mbyO5dp7GrsvLszAZjJ7ho0yE1TDQCY1YDKyqqIrsPt3yhDuk27jagbt5vHAZ30K2CdMeoJQtmhBAOFAGOie8+9x94W85CtfbX/AFx7mLlWPbxtUqW8cEVxcWio0SQXN2kQupoo4HMSo0mnRggkkk9/sb9Y39e9+691737r3Xvfuvde9+691737r3Xvfuvde9+691737r3XvfuvdEm+Vu46nG5bbeOMjJSNh6ytiU3EbVUlX9vO176WeOGJB/UB/wDH3J/IFnHNbXs9B4viBCfkBUfzJ/Z1GXPl9JDPZQCvhmMt+ZND+yg6r2z245ap3RJPTyCwJJ/xA/PuWILdYwPXqKppjIxqehs+HWayMHeFDQUbyGjy23dwQZeNSShpqOnjrqWSVQdN4shFGqsfp5CB+r2FfcG3iflqaWQDxI5UaP7S2kgfapP7OhXyDPMnMUMcZPhvG6uPkF1Any+IDq3b3AXU79e9+691737r3Xvfuvde9+691737r3Xvfuvde9+691737r3Xvfuvde9+690W35b1eSo+ht5PjfIPNJgqTIPHcMmLqs7j4K3Uy8iKRHCP+CjkHg+xbyQkL8xWni0qFdkB/iCGn7BU/l0GebnlXY7jw60LoGI9NQ/wmg/PrU6/mrG/w07n/wC1PgB/6+G3f9f2Z+4f/JKvftT/AKuL1IX3bP8Ap7HI/wDzXk/6sTdat/wg7C2f1H8yviP2v2Fl/wC7+wesfk30L2FvjPfw/KZb+CbP2X2ltTcm5sv/AAvCUWSzWS/huFxs8329HTVFVNo0RRvIVUwbC6x3ETuaKrgk/IHrq5zht15vHJfOG07dD4m4XW13dvBHVV1SSQOiLqYqq6mYCpIA4kgdbQu6P5p/wZre2/5/27sL3zL/AA35p/GzpTYvxZysHW3ctJP2NvbZ3w47I6tzeOhR+v4a7Y8uL7Bz1HRLVZ9MRTyGXzxSvTo8yrpLy1J3YmTtljCpg57CKcMZPn1jlt/tLz8Np+7paS8vDxNi3W5uN2Uz2xEMUm5QTq39tSXVCjNSPWcaSNRA6Q/eX85jpn5a/wAkLsX48dx78moPnDXwdS7OrNtTbU3zkH7ah627l6j3I3aE29KHbFVsjH5HN7H27PNkIchlaapfJUFQIotE1IkiOTcUm2iW2nf/ABqoUcSWAKnUTnNMGpyRXzA6EnK/sTv/ACZ94PaeaNi20N7eobmcSiSFfpjPa3Mf04iMglZVmkAUohUKy1NQxAS/zmf5tWX7j+Umwtzfy+vmp33iemKHoPa2C3NTdW70786M28/Z1N2J2jkM1PWbSycfX0+RzLbUymFWTIiilSaBYoROxpzHGm3jdGluEewvJBD4dDpLKK1byxmlOhn93j2Ntti5N3Oz90vbza5N/bdJJITew2V4/wBOYLdUAlXxwqeIslE1ChqdPdUwNl/MH4H/ADt+G3xy+Lf8wrs3tX4+dq/ExMpt7q75BbV2blO0Nv5/r+tocbQJgNxYXCYzcO6Ia58LtrE0DqlIU8uMpqkVIV54FKhcW15a2llfTPE8OoRTAa00Gh0sgIaooAtK0AHz6OLr2/8AdP2v9w+buePaTZLHd9j37TLfbTPMttIk4LNrjd2jiKh5JHy1aOy6ahW6BX+Yp84vj52N8fPjX8EPhhjt9p8YvjRPlNySbw7EgixW4uzexcwc48+5ZMDSmKOiggqd25uqMs0NPNLU5iZUp4Io18pbuV+ktvZ7faiQWUOo1kI1O7GpYgEgAVOnPAkY6kL2S9rubtm5w5191vcma0PO+9KsAt7Mlo7a3TRSPxDxJEUS0BIAjUlmJwa3+V1/MA+PPRnxRx/S24vkXuf4Z9wbI+UNL8gKrsfE9K7j7m2d33san2kdvT9N9gYLZNfjc9WYzJwzzRtHVT0sFHJT0dVT1ImVxFbatxhtbWWA3z21yLkXAlVC6uqppELBXUkFqmh7c8QcgJe+3s3zpzb7gS80WXJNvzRy1d8vnZlsZL6Kym2+cy+IL23knVo1dCAaqGLAyIy0Iq0/zfPlp8J/k51b06fhpu/bW2cfR9odqdh9pdI1fTm9tk78qd/7+npoJ+zqjeMuDrNgZGgy1LhmaXHUmVjmiFXBI0cj+SGhLOYrraLtLKbaUESF5XlgKFXDuVq5YFkKsEFArduMZIUS/dc9tvdfkDmTmf8A10druJ5n2+0sdu3Zb2Ce3FtbgkWogEi3CshfDtGQdLAECjSBl/Iu+WHQHw7+WnYfZnyN39/o62RnfjruzYmKzf8Adbeu7vut15PsnqLcFDiv4bsTbm58vB58Rtium88lOlMvg0NIHeNXpyfulhtG7XFzuE/hwtAyBtLN3F4yBRQTwB+XQ1++J7Y88e6/tdsPLvIOyfX7zDv0F7JD41vBSFLS9iZ9dzLCho8yDSGLGtQKAkT/AOWZ8rugvj78TP5pvWfb2/f7o73+R3x4p9i9M4T+629M9/fLdUfWvyHwD4v+JbY25msRt62X31iofPlaihpv8q1eTRFM0aPlzdtv2/aOaba8uNE9zbeHCuljqbRMKVUEDLDjQZ+3o0+8P7X89c+e6P3ZeY+VNj+r2bl7fzfbxN41vF9PB9ZtUuvRNLG8vZbSnTErt20pVlBF7Znyv+CHzP8Ahx8evi988d+dn9B9k/FSnq9s9Wd3bN2jX9hYDJ7BqaXF4tMJmMPiMVuLP05j29t7G0UlPHSqiyYylnjn0mWmCNNz2redq27aN9up7e5tCy290q+KnhuQdMkYIeqhQq6eAANeK9Eu5+1nvp7Oe7/Pvub7F7Ftm/cvc0MLnc9lvJ0tJUugzv4kckkkMR/VlkcMWJpK6Fa0foefgp8wP5UvxF+d+X3h1JmuzOr+iqP4j5zqvMdpdmYvfW8sh2v2vVdidO5uHLUGy9nbZ3Lndqx12D2pXT1M0lNQ0M1UrrHS0aiBahfytvPK+y8x3FzDNPDtv0Rh13ALs8viIS2mNWKhgteNMcF4dBP3w9n/AL1fu57EWuz812W27pzy/N0W6w7Xtr2tuljYrabhGUa5uJoYpyss8aqoZ3VaEySHUULX8hfmJ8dP5hHwbwGU+T/ZNHsL+Yd8fqnK4rZO5W693ZVY75A7Bnmjya7ezGU6/wBmZHbm26ydaqRaUVzUkFLl6UzK0VPkqt4iHc92tOYNiSbdbqnM9odEchQ/4zCTUIxRdKvGSdJbB9ayMUlz229nPcn7vPvruFr7XcsvuH3duYVSW+tvq7dX2m6A0eNGl3cpNMo0jV4YdnhfSQzwRhrSfmB83/gL8oOzMFv7Y/8AOP8AlD8YcTiNjYzZ9RsDpPYvys27tXL5Gg3BubNS7vyFFiNn4Kml3BkKbcENFLK0LO1Nj4FLkKqqMeZN+2beb6K52/3DuLGFYhGYYobogsGY6+1oxUhgOFccfIYyey3sV94T2s5YvuX98+5XypzXdzX73q7hvt1sM08aPFBELdGkuZWEKNCXA1AapHNMkmpH+Xd8sPj30F8av5sfW/afZtTiN2/JDo2o2R0jFWbW3znqvsXcS7B+RmBSOqyWA23l6Db1TWZPfWJDz5iagh1VhYvpimaMEcn71tu1bDzfZ7hcCK6u7IRQIFYhn8OdSoKqwWhdRkgZ44PWaP3jvZ73J9xfdH7nfM/KXKiTbPyvzAt/v5jntIVsofrNmlJVJp43mVUtJqLAsjUSlKsgYvv8trsb4m9Z757AzXyN7a+RfQ27qzbVBj+nO5vj9V5Gkq+vsv8AxEVGfrdxQYSWuyuepcrSxU9P9hJi6+hlpfuRIEnamliC2ySbVFeSvul5e2z+HS2uLEgNHIT8bZV9OkaSEOohmGMMJc+9Byv7y82cvcs2HtfyZyvzHsiXbSb5sXMqoy3kejTCsJlCRwtGxZvEE0cgfw6VQSKxzf5sf8wTon5CfG74+/GLqntTfHyg3J1bvWu3rvD5N9i7FbYWd3AqYncmHx+CoMXUYbbNc0NbT7lQVbyY6BnTD0bSSVE7TSk95w5ltdy2vZ9iguZL6W0LtJudwmh5NRwsYLM4Sh7tfcdCGpOo9RB9yr7tHuL7Ze63uX7t85cn7fyjtW77em32PKW13f1kMNZIJXmeRZZ0qhgOgCVqGeUKqIFXoPP5HY/4zd2b/ht3ap/9auS9nfs3/wArBuf/ADxH/q5H1Gf975/yo3sl/wBLS/8A+rEHWy58r+ht3Z8bd7c2hh63cFHT7dpMFu3HYynkrMljlx8tRUUGbjooFepqqF4KtoagxqzQ+NGI0FiuZ3KG7W0UMu3XMgRy5eNmNAa8VrwBxUevXz3c1bXPLJHf28ZdQumQLkinA0409fTou3Umxd2btzFNh9vbdy2RyE8yp40oqiKGmBbSZshVTRpT0NPEAS7ysoAB/PHsS7jdwW8ZkmmUIPmM/YPOvQc2+1nnkEcULFj8v8J8ur6evdq/3H2TtrahnFVJhMXBST1CghJqolpquSMMAwiaqlfRex029xPeXH1VzNcUpqaoHy8v5dSjaQfTW0MFalVoT8/PpZe03Snr3v3Xuve/de697917rokKCzGwUEkn6AAXJP8ArD3sAkgDj1o4BJOOg8rN1ySyMaeXwwg2jUD1styA7Na92tew4A/2/s+h2xVUeItW8+iCXdGZj4Zonl1Jw+6DNWQ0VS4lWpYRRSWAZJT+hWItqVzx9L39tXe2hInliFCoqR6j/JTp203ItKkMpwxoD8/9npd+yXo7697917r3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de697917oDO9+moO4NswUdLXR4jcuGkmqMDkplkekLVCItTj8ksIaY0NYIkJZAzxOisAw1Kwo5W5jfl68d3jMllJQSoOOODLXGoV8+I9OIDHM/Lqb/AGiKjhLyMkxOeGeKtSpoacfL9oNaGQ+LvfcWT/habGeqLOUTIU2ZwzYl1JAEprZa2IxRkG/rRXA+q349zHFzpywYfHO6ADzUq+r7NOkmv2Y6iGXkzmVZvB/drHPxBk0/bXV/hp9nR8/jR8cn6cp8huHctZR5Le+cpI6OYUGuTHYHF+RKh8ZR1EscUlXU1FRGjVE2hFJjVEGldTxdzjzcOYGitLONk26NtQ1fE7ZGojyABNB86n0Enco8qHYFlurpw+4SDSdPwotalQfMkgVPDAA8yTX+wL0N+ve/de697917r3v3Xugz7X7JousNqzZ2en+/yE8oosNjPJ4hWV7ozgzSWZo6OmjQvKygmwCjlh7PNg2WXfL9bVX0QgapHpWi/L5k4H7fLok37eotksWumTXMTojStKt8/kOJ/Z59Vc7r+Uveb5Z62j3n/CkWQvFjsdh8OMbEoYlYTFWUNZPOluCZJHY/1v7mq05J5ajhET7cHNMu7PqP5hhT8gOobuOdOY5LhpBuGheIVFXSPlQg1/OvRx/i58najuGSv2bvCmo6LfGIoTk4KygT7eg3Fio5oqeoqI6V3b7PJUMs8fmiRmR0cOgUBlWOudOTk2ER39gzNtztoKtkoxqRnzU0wTwOCTUdSJyhzY+967K9UC/VdQYCgdQaHHkwr+eSAKHo5fuPuh31737r3Xvfuvde9+690xbmwmM3LgMtgMzSR1+KzFBU4+vpJQSk9NUxNHItwQyOAbqykMjAEEEA+37W5ms7iG6t3KzxsGUj1H+Eeo8xjpi5t4rqCW3mTVE40sP9XAjyPkc9a3P80T4Ddq7++OPbuwOm46TeeX3FQ4mHbOJyVfR4LJSfa7pweRmp6rI5CWmwxNPQUkh8ryw+TRYKGIUnnMe/pvmz3MH0zLftpwCNJo6k0JIpgE0P7ehH7Oy2XI/uNy1v27XdNltpZGkkCszgNDIgqigknUwGPtoOtRmo/k+fPrGyeGs6gx8cikghd+bJlFwLH1RZxx9fcYNt96dVLc/70v8A0F10Oj+8h7TJWu9z/wDZNP8A9AdSIv5SnzqUEHqah5P/AD220P8A68e2G2vcCCBan/ek/wCgujOH7zftCnxb5cf9ks//AEB06xfynfnGttXVNCLf9nptM/i34y3tO+0bmaUtD/vSf9BdGkX3pfZta6t+uf8AsluP+gOnWH+VN83UN26toRzf/j8dqn8j/q6f4e0zbJupFBZnh/FH/wBB9GcX3rvZZAK7/c/9klx/0B05w/yrvmun6usKEcg2/vhtg/T/AMiVvaZtg3hqUsT/AL3H/wBB9GcX3uPZBKauYLr/ALJLj/oDpxi/la/NFQQes6Dk/wDPXbb/APrh7SSct72xqLA/73H/ANB9GkH3w/YpPi5hu/8AsjuP+gOp8X8rv5mpbV1rQ/gf8fZtz+hH/K/7SPytv7Vpt54/xxf9B9GkX3zfYVVAbmK8x/y5XP8A0B05xfyw/mOpuet6Ef8Ak1be/wAf+m72iflDmI0pt3/VSL/oPozi++t939KV5kvP+yK5/wCtfU6P+WT8w1IJ66oeCD/x9OA/oB/yu/4e0j8l8zMcbZ/1Ui/62dGcX34Pu8pQHmS9/wCyG5/619Tl/lofL4Cx67ofr/z1GC/+rPaNuRuaiKDav+qsP/Wzozj+/V93RePMt9/2Q3P/AFr6yD+Wj8vf+fe0A+o/4+fB/kf9Rfth+Q+bCajaf+qsP/Wzowj+/n929SteZb7H/Lhc/wDQHXJf5aPy8Fr9fUHBP/MT4T8gf9NXtOeQObqn/dR/1Vg/629GMX3/AD7taAg8z3//AGQXX/QHWI/y3/lgG0HZGHD3toO7cAGv/TT95e/vze3XOrLUbE9PXxIf+tnSyP8AvCvuwoSG5svq+n0Fz/0B1LX+Wl8urg/3Ax1uDf8AvNhuf9a1R7Rv7d85VNNlP/OWD/rb0axf3h33YUpXmjcf+5fdf9Addn+Wl8uiSf7g476/89Nh/wDr/wC2m9uedCajZD/zmt/+tvRjF/eMfdcSleaNy/7l91/0B17/AIbQ+XP/ADwWN/8AQmxH/X72y3tvzsTUbGf+c1v/ANbejOL+8i+6ummvNG54P/Ruuv8AoDrw/lmfLuVlRdh4y5Nhfc2JA5/x8tgP9f2y/ttzvT/khH/nNb/9bujOD+8s+6ihJbmnc/8AuW3X/QHVxv8AKH+DPfvRHae/tydrbVocNic/t/A0WGqKPOY3KvNW0OTq5qmKWGinklp1EM4IZhpP0+vuRPbLlLmLYN4v7veNu8C3e2Mat4kT1YujUpG7ngp4065/f3hf3qPZz7w/KvtptftjvN3c3u1391Pdrc2s1uAksUaIVMigN3IagZHW3JsijaixUETAgrGo5Fvovub+uV/S2CqtyFALG5IAFz/U2+p9+61Qdd+/db697917r3v3Xuve/de697917rHNH5YpYrlfJG8eocldalbgf1F/dkbSytTga9VcalKeoI6LPlGq8RWS0FejQzQkgarhJk50TxMbCSN15BH0+h5uPchW3hXMSzwkFD/I+YPoeo9uDLaTPBMtHH8x6j5Hp42dT1eZzVI0CsaShmSprKix8UaxEPHCH+jTTOAAByFufoPaTdZYrW0lDn9V10qvma+dPQdKtqjlvLyMqp8JDqZvLHl9pPRhPYG6HXXvfuvde9+691737r3Xvfuvde9+691737r3Xvfuvde9+691737r3Xvfuvde9+691737r3Xvfuvde9+691737r3Xvfuvde9+691737r3Xvfuvde9+690UD5eY6sm27tbKRxu9DQZHI0tW4BKQTZCmgNI8lrhRKaV0BP9qw+p9yN7dzRrd7hASPFZFZfmFJr+yo6jv3Chla0sJ1BMSOysfQsBT9tOqq9zcTv/AK5/3sDg/wBOfc1wGq9QzKaH9vQ3/CfBZXJ9/wCLytEkpx+29v7hrs1MoYQpT5HHS4ihp5HHo8lRX1iOiE3YQswHpPsJ+4lzDDyzcwyH9WWREjHnVXDk/wC8qf8AUehlyDbzTcwW8yA+HErs58qFGQf8aYf6h1dJ7x66njr3v3Xuve/de697917rphqUj+vv3XukXntp0mZjdJoVcG/BUH68cD6fn37r3QUVnReCq5TI9FASTflFPJ/1/eqevXuon+gDb3/KhTf9S09+oPTr3Xv9AG3v+VCm/wCpae/UHp17r3+gDb3/ACoU3/UtPfqD06917/QBt7/lQpv+pae/UHp17r3+gDb3/KhTf9S09+oPTr3Xv9AO3v8AlRpv+pae/UHp17r3+gDb3/KhTf8AUtPfqD06917/AEAbe/5UKb/qWnv1B6de69/oA29/yoU3/UtPfqD06917/QBt7/lQpv8AqWnv1B6de6LFvnZuJrslVY3E08MGJo5np/JCFR8hLCxSWVnU6vtvILIosGA1H62EgbTy/HDBHPcIDcsNVCPhBzT7fXoAbtzA8s8sFu1LdTpqD8VOJ+yvDoPv9E2I/wCVKn/x9Kc/1/1/Z3+719Oib95SfxdK7a2z8bg66FK6kjqcPJIiVUDBZDTRsbNU0pb9DRX1FAdLgEcGx9lm48vQ3kTmNAtyBVWpx+R+R/l0Y7fzDLaSoJCWtiaMvp8x6Efz6NbH0JtuWNJYqOkeOVFkjdUQq6OoZGUjgqym49xwyaWKstGBoQepGVlZQymqkVB65/6ANvf8qFN/1LT3qg9Ot9cl6C2+rBhQ0wIN+EQH/b+/UHp17pc4DrPGYV1aCmjQpaxVR+P6Ecg8+99e6FKlp1p4wiiwAta1v9j7917qV7917r3v3Xuve/de697917r3v3Xuve/de697917qLU0NFWhVrKSlq1QkotTTxThSfqVEqOFJ/wAPbkc00JJilZSf4SR/g6akhhlFJYlb01AH/D1kgp4KWMQ00ENPEv6YoI0ijW/9EjVVH+291d3kYtI5ZvUmp/n1ZI0jULGgVRwCgAdZvder9e9+691737r3Xvfuvde9+691737r3Xvfuvde9+691737r3XvfuvdQcZ/E/4fR/xn7D+K+BPv/wCGfcfw/wC5t+59n91/lPgv+nX6v6+7Po1t4ddFcauNPnTqia6DX8fnTh+XU73Xq/Xvfuvde9+691737r3Xvfuvde9+691737r3Xvfuvde9+691737r3SZ3l/db+6+a/vr9j/db7J/4z/Er/afa6ltq0fu+Xy6fF4/3fJp0eu3tdtv1/wBdbfuzX9fq/T0ca/4KU41xStcdIdy+h+iuP3lp+h0/qa+FP8Na8KZrSmeqat/f6Df7yTfwf/Sp/d7zj6f3Y+58Woeb7H+I/wCV+G3+b+4/ctbVzf3kRt39Y/o1+r+j+rp+HxKcMaqfzpj06gC9/q79afpPq/pNX4tGqnnprmnpXPr1ZR8Yv9Cn9xJf9DHl+1+8j/vN/F7/AN7v4r4j4f7za/3NXg1fb+L/ACPTr8P9v3DPOf8AWL95L/WCmrSfB8P+y0+fh/nSte7hXFOpf5R/cP7ub9xVpUeN4n9rq8tdMetNPbxpmvRk/YP6F3Xvfuvde9+691737r3Xvfuvde9+691737r3Xvfuvde9+691737r3XvfuvdFU+UX+ln+A47+4n3f92tNR/eb+B/cfx7zXX7Xy/bf5X/BvHq1/b+ryf5z06fZ/sX7v8V/q6eP+DVTT/PFft/Loi3v67wl+lr4X49NdXy4Z0/Z+fRFOs/9mD/vrjf9HX94f4h97D99/EP4n/dn7XzJ9z/eT73/ACP7Dx31/wDKR/xy/c0+xVe/uf6V/rdGimNNNVf6NM1/l69Bq0/e31KfR69dc6q6aV/F5U/n1clF5fFH5/H5vGnm8WrxeXSPJ49fr8eu9r82+vuNzSppw6kEVpnj1k96631737r3UPI+X+H13gv5vs6nw2+vl8L+O3+Ou3t630+PDr+DWK/ZUV6ZuNXgTaPj0Gn20NOiFjxaV1fW351Xv+b2/wAfcxd+acOob7fl+fXY8H+H+x1f8T73+pn/AGevdny68fDY/S35t/xvj6e/DxK549e7aeVOjs7M83909u+e/k/hFD+q99HgTw/Xn/M6fcTbtp/eV9o+HxW/bXP8+pa2rX+7bHX8XhL/AIMfy6U3sv6MOve/de697917r3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de6//2Q==">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="8772525"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4102" name="AutoShape 6" descr="data:image/jpg;base64,/9j/4AAQSkZJRgABAgEASABIAAD/7QAsUGhvdG9zaG9wIDMuMAA4QklNA+0AAAAAABAASAAAAAEAAQBIAAAAAQAB/+IMWElDQ19QUk9GSUxFAAEBAAAMSExpbm8CEAAAbW50clJHQiBYWVogB84AAgAJAAYAMQAAYWNzcE1TRlQAAAAASUVDIHNSR0IAAAAAAAAAAAAAAAAAAPbWAAEAAAAA0y1IUCAgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAARY3BydAAAAVAAAAAzZGVzYwAAAYQAAABsd3RwdAAAAfAAAAAUYmtwdAAAAgQAAAAUclhZWgAAAhgAAAAUZ1hZWgAAAiwAAAAUYlhZWgAAAkAAAAAUZG1uZAAAAlQAAABwZG1kZAAAAsQAAACIdnVlZAAAA0wAAACGdmlldwAAA9QAAAAkbHVtaQAAA/gAAAAUbWVhcwAABAwAAAAkdGVjaAAABDAAAAAMclRSQwAABDwAAAgMZ1RSQwAABDwAAAgMYlRSQwAABDwAAAgMdGV4dAAAAABDb3B5cmlnaHQgKGMpIDE5OTggSGV3bGV0dC1QYWNrYXJkIENvbXBhbnkAAGRlc2MAAAAAAAAAEnNSR0IgSUVDNjE5NjYtMi4xAAAAAAAAAAAAAAASc1JHQiBJRUM2MTk2Ni0yLjEAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFhZWiAAAAAAAADzUQABAAAAARbMWFlaIAAAAAAAAAAAAAAAAAAAAABYWVogAAAAAAAAb6IAADj1AAADkFhZWiAAAAAAAABimQAAt4UAABjaWFlaIAAAAAAAACSgAAAPhAAAts9kZXNjAAAAAAAAABZJRUMgaHR0cDovL3d3dy5pZWMuY2gAAAAAAAAAAAAAABZJRUMgaHR0cDovL3d3dy5pZWMuY2gAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZGVzYwAAAAAAAAAuSUVDIDYxOTY2LTIuMSBEZWZhdWx0IFJHQiBjb2xvdXIgc3BhY2UgLSBzUkdCAAAAAAAAAAAAAAAuSUVDIDYxOTY2LTIuMSBEZWZhdWx0IFJHQiBjb2xvdXIgc3BhY2UgLSBzUkdCAAAAAAAAAAAAAAAAAAAAAAAAAAAAAGRlc2MAAAAAAAAALFJlZmVyZW5jZSBWaWV3aW5nIENvbmRpdGlvbiBpbiBJRUM2MTk2Ni0yLjEAAAAAAAAAAAAAACxSZWZlcmVuY2UgVmlld2luZyBDb25kaXRpb24gaW4gSUVDNjE5NjYtMi4xAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAB2aWV3AAAAAAATpP4AFF8uABDPFAAD7cwABBMLAANcngAAAAFYWVogAAAAAABMCVYAUAAAAFcf521lYXMAAAAAAAAAAQAAAAAAAAAAAAAAAAAAAAAAAAKPAAAAAnNpZyAAAAAAQ1JUIGN1cnYAAAAAAAAEAAAAAAUACgAPABQAGQAeACMAKAAtADIANwA7AEAARQBKAE8AVABZAF4AYwBoAG0AcgB3AHwAgQCGAIsAkACVAJoAnwCkAKkArgCyALcAvADBAMYAywDQANUA2wDgAOUA6wDwAPYA+wEBAQcBDQETARkBHwElASsBMgE4AT4BRQFMAVIBWQFgAWcBbgF1AXwBgwGLAZIBmgGhAakBsQG5AcEByQHRAdkB4QHpAfIB+gIDAgwCFAIdAiYCLwI4AkECSwJUAl0CZwJxAnoChAKOApgCogKsArYCwQLLAtUC4ALrAvUDAAMLAxYDIQMtAzgDQwNPA1oDZgNyA34DigOWA6IDrgO6A8cD0wPgA+wD+QQGBBMEIAQtBDsESARVBGMEcQR+BIwEmgSoBLYExATTBOEE8AT+BQ0FHAUrBToFSQVYBWcFdwWGBZYFpgW1BcUF1QXlBfYGBgYWBicGNwZIBlkGagZ7BowGnQavBsAG0QbjBvUHBwcZBysHPQdPB2EHdAeGB5kHrAe/B9IH5Qf4CAsIHwgyCEYIWghuCIIIlgiqCL4I0gjnCPsJEAklCToJTwlkCXkJjwmkCboJzwnlCfsKEQonCj0KVApqCoEKmAquCsUK3ArzCwsLIgs5C1ELaQuAC5gLsAvIC+EL+QwSDCoMQwxcDHUMjgynDMAM2QzzDQ0NJg1ADVoNdA2ODakNww3eDfgOEw4uDkkOZA5/DpsOtg7SDu4PCQ8lD0EPXg96D5YPsw/PD+wQCRAmEEMQYRB+EJsQuRDXEPURExExEU8RbRGMEaoRyRHoEgcSJhJFEmQShBKjEsMS4xMDEyMTQxNjE4MTpBPFE+UUBhQnFEkUahSLFK0UzhTwFRIVNBVWFXgVmxW9FeAWAxYmFkkWbBaPFrIW1hb6Fx0XQRdlF4kXrhfSF/cYGxhAGGUYihivGNUY+hkgGUUZaxmRGbcZ3RoEGioaURp3Gp4axRrsGxQbOxtjG4obshvaHAIcKhxSHHscoxzMHPUdHh1HHXAdmR3DHeweFh5AHmoelB6+HukfEx8+H2kflB+/H+ogFSBBIGwgmCDEIPAhHCFIIXUhoSHOIfsiJyJVIoIiryLdIwojOCNmI5QjwiPwJB8kTSR8JKsk2iUJJTglaCWXJccl9yYnJlcmhya3JugnGCdJJ3onqyfcKA0oPyhxKKIo1CkGKTgpaymdKdAqAio1KmgqmyrPKwIrNitpK50r0SwFLDksbiyiLNctDC1BLXYtqy3hLhYuTC6CLrcu7i8kL1ovkS/HL/4wNTBsMKQw2zESMUoxgjG6MfIyKjJjMpsy1DMNM0YzfzO4M/E0KzRlNJ402DUTNU01hzXCNf02NzZyNq426TckN2A3nDfXOBQ4UDiMOMg5BTlCOX85vDn5OjY6dDqyOu87LTtrO6o76DwnPGU8pDzjPSI9YT2hPeA+ID5gPqA+4D8hP2E/oj/iQCNAZECmQOdBKUFqQaxB7kIwQnJCtUL3QzpDfUPARANER0SKRM5FEkVVRZpF3kYiRmdGq0bwRzVHe0fASAVIS0iRSNdJHUljSalJ8Eo3Sn1KxEsMS1NLmkviTCpMcky6TQJNSk2TTdxOJU5uTrdPAE9JT5NP3VAnUHFQu1EGUVBRm1HmUjFSfFLHUxNTX1OqU/ZUQlSPVNtVKFV1VcJWD1ZcVqlW91dEV5JX4FgvWH1Yy1kaWWlZuFoHWlZaplr1W0VblVvlXDVchlzWXSddeF3JXhpebF69Xw9fYV+zYAVgV2CqYPxhT2GiYfViSWKcYvBjQ2OXY+tkQGSUZOllPWWSZedmPWaSZuhnPWeTZ+loP2iWaOxpQ2maafFqSGqfavdrT2una/9sV2yvbQhtYG25bhJua27Ebx5veG/RcCtwhnDgcTpxlXHwcktypnMBc11zuHQUdHB0zHUodYV14XY+dpt2+HdWd7N4EXhueMx5KnmJeed6RnqlewR7Y3vCfCF8gXzhfUF9oX4BfmJ+wn8jf4R/5YBHgKiBCoFrgc2CMIKSgvSDV4O6hB2EgITjhUeFq4YOhnKG14c7h5+IBIhpiM6JM4mZif6KZIrKizCLlov8jGOMyo0xjZiN/45mjs6PNo+ekAaQbpDWkT+RqJIRknqS45NNk7aUIJSKlPSVX5XJljSWn5cKl3WX4JhMmLiZJJmQmfyaaJrVm0Kbr5wcnImc951kndKeQJ6unx2fi5/6oGmg2KFHobaiJqKWowajdqPmpFakx6U4pammGqaLpv2nbqfgqFKoxKk3qamqHKqPqwKrdavprFys0K1ErbiuLa6hrxavi7AAsHWw6rFgsdayS7LCszizrrQltJy1E7WKtgG2ebbwt2i34LhZuNG5SrnCuju6tbsuu6e8IbybvRW9j74KvoS+/796v/XAcMDswWfB48JfwtvDWMPUxFHEzsVLxcjGRsbDx0HHv8g9yLzJOsm5yjjKt8s2y7bMNcy1zTXNtc42zrbPN8+40DnQutE80b7SP9LB00TTxtRJ1MvVTtXR1lXW2Ndc1+DYZNjo2WzZ8dp22vvbgNwF3IrdEN2W3hzeot8p36/gNuC94UThzOJT4tvjY+Pr5HPk/OWE5g3mlucf56noMui86Ubp0Opb6uXrcOv77IbtEe2c7ijutO9A78zwWPDl8XLx//KM8xnzp/Q09ML1UPXe9m32+/eK+Bn4qPk4+cf6V/rn+3f8B/yY/Sn9uv5L/tz/bf///+4AE0Fkb2JlAGQAAAAAAQUAAklE/9sAhAABAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAgICAgICAgICAgIDAwMDAwMDAwMDAQEBAQEBAQEBAQECAgECAgMCAgICAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwMEBAQEBAQEBAQEBAQEBAQEBAQEBAT/wAARCAEEAcsDAREAAhEBAxEB/8QBogAAAAYCAwEAAAAAAAAAAAAABwgGBQQJAwoCAQALAQAABgMBAQEAAAAAAAAAAAAGBQQDBwIIAQkACgsQAAIBAwQBAwMCAwMDAgYJdQECAwQRBRIGIQcTIgAIMRRBMiMVCVFCFmEkMxdScYEYYpElQ6Gx8CY0cgoZwdE1J+FTNoLxkqJEVHNFRjdHYyhVVlcassLS4vJkg3SThGWjs8PT4yk4ZvN1Kjk6SElKWFlaZ2hpanZ3eHl6hYaHiImKlJWWl5iZmqSlpqeoqaq0tba3uLm6xMXGx8jJytTV1tfY2drk5ebn6Onq9PX29/j5+hEAAgEDAgQEAwUEBAQGBgVtAQIDEQQhEgUxBgAiE0FRBzJhFHEIQoEjkRVSoWIWMwmxJMHRQ3LwF+GCNCWSUxhjRPGisiY1GVQ2RWQnCnODk0Z0wtLi8lVldVY3hIWjs8PT4/MpGpSktMTU5PSVpbXF1eX1KEdXZjh2hpamtsbW5vZnd4eXp7fH1+f3SFhoeIiYqLjI2Oj4OUlZaXmJmam5ydnp+So6SlpqeoqaqrrK2ur6/9oADAMBAAIRAxEAPwCkf31S/H+fXF/rkn6h/sf96Pu5+Dqr/CepKfX/AGH/ABI97T4R0z1l92691737pp+PWSP8/wCw/wCJ9+6p1JT6f7H/AIge/dNPx65+7n4B9vVOs4+g/wBYf71783Bem5PLrLH+f9h/xPt3pvrMn6h/sf8Aej791V/hPWb37pnr3v3Xuskf5/2H/E+7J8Q6bk8upEf5/wBh/wAT7tJ5dN9ZPbfTT8esyfpH+x/3s+3k+EdU65e7de6zj6D/AFh/vXv3TB4n7esh+qf6y/73791U8D1nT9Q/2P8AvR9+6Y6ze/de6zj6D/WH+9e/dMHift679vJ8I611mT9I/wBj/vZ9+HxN0y/xHrOn0/2P/ED3bqvXP37pp+PWSP8AP+w/4n37qnWdPr/sP+JHv3VH4fn1l9+6a65J+of7H/ej791V/hPUhP1D/Y/70ffumes3u6cetHgeux9R/rj/AHv270x1n9+691I9+6T9ZU+n+x/4ge/de65+/dMv8R6yp9P9j/xA9+6r1IT6f7H/AIge/dNPx6l0sXmqIo/wWBb/AIKvqb/eB7dpXR0mnk8OGR/MDHS4936DvXvfumDxP29dj6j/AFx/vfv3WupA+o/1x791o8D0lpZfNUSS/wCrdiP+C8hf9soHv3R2ieHCqegHXvfuq9SYqyph/RK1v9Sx1r/sA1wP9h790y9vDJ8UYr6jB/l07w5hwAJolbgeqM6T9P8AUm4J/wBiPdlOk16Qy7eozHIR8j/n6eKauppiAr6WYgKjgqSeeB9VJ/2Pu6kEsei2a1mjqxWq+o6cPdhxP29JesqfT/Y/8QPe+mn49c/fuqdMtfFom8g+kqi//Bk4P+8Ee/dGtnJqi0Hip/keoPv3Svrkn6h/sf8Aej791V/hPWcfUf64/wB79+6Z6z+/de6rf9gn8f59Zkdck/UP9j/vR93PwdVf4T1JT6/7D/iR72nwjpnrL7t17r3v3TT8eskf5/2H/E+/dU6kp9P9j/xA9+6afj1z93PwD7eqdZx9B/rD/evfm4L03J5dZY/z/sP+J9u9N9Zk/UP9j/vR9+6q/wAJ6ze/dM9e9+691kj/AD/sP+J92T4h03J5dSI/z/sP+J92k8um+sntvpp+PWZP0j/Y/wC9n28nwjqnXL3br3WcfQf6w/3r37pg8T9vWQ/VP9Zf979+6qeB6zp+of7H/ej790x1m9+691nH0H+sP969+6YPE/b137eT4R1rrMn6R/sf97Pvw+JumX+I9Z0+n+x/4ge7dV65+/dNPx6yR/n/AGH/ABPv3VOs6fX/AGH/ABI9+6o/D8+svv3TXXJP1D/Y/wC9H37qr/CepCfqH+x/3o+/dM9Zvd049aPA9dj6j/XH+9+3emOs/v3XupHv3SfrKn0/2P8AxA9+691z9+6Zf4j1lT6f7H/iB791XqQn0/2P/ED37pp+PT7h4rtLMR+kCNT/AIn1N/sQAP8Ab+3xwH2dFW4yUVIx55PSm976Keve/dMHift67H1H+uP979+611jrpfFTOQbM9o1/134P+xC3Pv3T9smuZR5DJ/L/AGek4n6h/sf96Pv3Ru/wnrN790z1737r3WcfQf6w/wB69+6o/D8+nrDxa5w5HESs3/ITEqv+8XP+w9uJ59Fl/Jph0ebGn5DPSn93HE/b0S9ZU+n+x/4ge99NPx65+/dU6i1kXkp3I+sREg/1gCGH+2N/9h790otZNE6g8Gx/m6Yffujjrkn6h/sf96Pv3VX+E9Zx9R/rj/e/fumes/v3Xuq3/YJ/H+fWZHXJP1D/AGP+9H3c/B1V/hPUlPr/ALD/AIke9p8I6Z6y+7de697900/HrJH+f9h/xPv3VOpKfT/Y/wDED37pp+PXP3c/APt6p1nH0H+sP969+bgvTcnl1lj/AD/sP+J9u9N9Zk/UP9j/AL0ffuqv8J6ze/dM9e9+691kj/P+w/4n3ZPiHTcnl1Ij/P8AsP8AifdpPLpvq8P+XD/L1b5QfCj58drT4h6vdFJs+i2R0bURw+Wrl3vsGbFdy7qx9Csg8aVG4VxGBwyzAErDkqlbqfcF+5HuGOVudvb/AGkSgWrTGe+B4CKUNbRsaeSFpHp6ovHrJv2c9pDzx7ae6u9GAtuDQLabWVpq8a3KXkiDUNIEzLDHq46WcArx6pGT9I/2P+9n3OyfCOsXOuXu3Xus4+g/1h/vXv3TB4n7esh+qf6y/wC9+/dVPA9Z0/UP9j/vR9+6Y6ze/de6zj6D/WH+9e/dMHift679vJ8I611mT9I/2P8AvZ9+HxN0y/xHrOn0/wBj/wAQPduq9c/fumn49ZI/z/sP+J9+6p1nT6/7D/iR791R+H59ZffumuuSfqH+x/3o+/dVf4T1IT9Q/wBj/vR9+6Z6ze7px60eB67H1H+uP979u9MdZ/fuvdSPfuk/WVPp/sf+IHv3Xuufv3TL/EesqfT/AGP/ABA9+6r1IT6f7H/iB7900/HpXY+LxUsQP1ceRv8AXfkf7ELYe3U8+g7dyeJO58hgfl/s9Ovu/Sbr3v3TB4n7eux9R/rj/e/futdNGWlvJDCP7P7jf67Gyg/4gA/7f37oyskorSHzNB03p+of7H/ej790sf4T1m9+6Z697917rOPoP9Yf71791R+H59KrDR6KYuRzK1/+QVLKv+83/wBv7cTz6INwfVME8lH8z07+7jift6Q9ZU+n+x/4ge99NPx65+/dU65oAQwIuCLEf1BuCPfuqOSCpByOkxLGYpHjP1RiP9cfg/7Ec+/dCCNxJGjjzFeuKfqH+x/3o+/dbf4T1nH1H+uP979+6Z6z+/de6rf9gn8f59Zkdck/UP8AY/70fdz8HVX+E9SU+v8AsP8AiR72nwjpnrL7t17r3v3TT8eskf5/2H/E+/dU6kp9P9j/AMQPfumn49c/dz8A+3qnWcfQf6w/3r35uC9NyeXWWP8AP+w/4n27031mT9Q/2P8AvR9+6q/wnrN790z1737r3WSP8/7D/ifdk+IdNyeXUiP8/wCw/wCJ92k8um+t9n4EfHneHUnSnwb6n2F8h9tdcbg6w2xl+5Pll0LSYrbOd352HB3fi/7z4Cg3LFXZOoy+y4Nm5usjxgqv4eTWwITT1UD0yLPgHz/zFZ7tvfPe7X/LklzbXUq2W0bgWkSKI2raHKEKFkMijXTV2n4lIY06p+13Ke5cvcs+2ewbfzRFZ3NjbNf77tWiKSeY3qtIiyHWTCsMxKhgp1haK4092pH/ADMvjv8A7LF82u9utaKgXH7VrN2VG/dhRRACkTZPYF90YahobKpNNt98hLi+RcSULC7W1HMH2v5jHNHI2wbm8mq7EIguCePixdjE/N6B/sbrn5738oHkr3O5o2qOHRYSzm9tOFPBuP1AFA4LGxaMVoez8yQ72P8AqJ+s4+g/1h/vXv3TB4n7esh+qf6y/wC9+/dVPA9Z0/UP9j/vR9+6Y6ze/de6zj6D/WH+9e/dMHift679vJ8I611mT9I/2P8AvZ9+HxN0y/xHrOn0/wBj/wAQPduq9c/fumn49ZI/z/sP+J9+6p1nT6/7D/iR791R+H59ZffumuuSfqH+x/3o+/dVf4T1IT9Q/wBj/vR9+6Z6ze7px60eB67H1H+uP979u9MdZ/fuvdSPfuk/WVPp/sf+IHv3Xuufv3TL/EesqfT/AGP/ABA9+6r1OpIvNLHF/q5AD/gosWP+wUH3sdJrl/DR39F/n5fz6Wvu8fn0GOpHtzr3XvfumDxP29dj6j/XHv3WuktUS+apkl/DSen/AIKPSv8AyaB790eRJ4caJ6D/AIvrkn6h/sf96Pv3Vn+E9Zvfumeve/de6kIC2lRyW0gD+pNgP959+6bkIC1PDpcU6CKNYx9ERF/5JFr/AOx9uqKFh9nQXlbXI7epr1I92HE/b031lT6f7H/iB7300/Hrn791TrJH+f8AYf8AE+/dNyeXTPlItMiSgcSDS3/BltY/65X/AHr37oz2+SsbRk5U1H2H/Z6bU/UP9j/vR9+6Xv8ACes4+o/1x/vfv3TPWf37r3Vb/sE/j/PrMjrkn6h/sf8Aej7ufg6q/wAJ6kp9f9h/xI97T4R0z1l92691737pp+PWSP8AP+w/4n37qnUlPp/sf+IHv3TT8eufu5+Afb1TrOPoP9Yf71783Bem5PLrLH+f9h/xPt3pvrMn6h/sf96Pv3VX+E9ZvfumehE6o31jet9+7e3fm9gbN7SwmLrFfM7B37R1VXtrc2Mey1eOq5cdVUGWxszx8w1VJPFPBKAfWmuNy/dbGTcrC5s4b+a1ndaJcQEB0byYVBU/MEEEfOhB1y9u8Ox7xZ7lc7TbX9rG36tpdrqjlQ4Kmncp81ZSCCBxFVO5d8FOpf5NPz12PJnOs/jD1xt/sDBUNNPv/qLcFdnv737QllaOF62ApnoY9y7Vkq5BHBlaVBExZEnSnnYwLhnz3u/vPyBfCDcuabmTb5GIt7yMJ4cnnQ9p0SU4oc8SCwz10P8AbTaPu/e6O1tebLyTYR7lEB9VYzJ+rCT58aSRk/DIuDwOlgVDT8y/5e/wrxPdHwi+OPTfx22RtXe/eHex3bvfLYj+KzVVL0D0jh5N49qUE7ZHM1NNjTugVNDQ080iHykyxRrJIQvtRyV7ic7S7JzzzNvXMc81jYWHg26OVFbu5bw4GFFBbw6MxA4YJIGekfuL7We3a8w+2vJ2w8n2MG4bnun1F06ws3+IWKeNdITqCp4xMcYLVB1MArHhat8aZOt+1t69xfJCi+Ou/OlO3K7d2X6Q3Rnu08BVbb3jv7aXWkuP/uxuTGYufI1Ah2dmKKpgamkanpZpZKdlbzRRQTyRNzOu5bRY7Ly0/MdvfbQsK30UdqweOKSbVrRmAFZFINckAHyJIE48pvte9bhv/NCcp3O3b0bhttlmvY/DluIrY/pyoNRPgNq7CwUmhwVCsX/vP4SfFP5Lbpxm9e9ektodk7rw2Ap9rY3O54ZRa+l29S5HJZamxKSY7JUKvSQZLM1UyBgxV53IPPtjYeeebeWLSWx2DfZrW0eQytHHpoXIVS2VOSqgfkOnuY/brkbm+9i3Lmble0vb+OIQJNOmphGGZglcdoZ2IHkWPr0WDsf+XL/Ks6g2TuHsfs74+9N7H2NtTHyZLP7m3DkNwUONx9LGQiKZJM+ZKmsq53WGmpoVkqKqokSGFHldEIq2z3K92d5vrfbdq5ivZ7+VtMcUYQsT/vGABkk0AFSSAK9A7dvaf2R2Hbrvd955P2m22yBNcs8yhUUfMk8ScADJJAAJIHWnr87/AJCfFPtPdn91Ph78aNm9LdV7fr5THvZ6HJP2L2HLCZIkrapMllclS7T203D09FCv30nD1Mw1faxZm8gcuc2bTZ/V85c0T327SLmCo8GGuaCiqZH9WPaOCj8R51+7XO3IfMF621+3fI9ntuxwyH/HBHpubgrUVyT4MJ4hfjOC5XKAy/8AJL+J/QHy6+QnaWx/kNsH/SDtfbfTNRuvC4v+9O9dp/ZZ+Pe+0cQlf97sfce2sjU2x2Unj8Us0kPr1aNSqwDHvnzdzDydy5tN/wAubh9Ndy3whd/DikqnhSNSkqOB3KDUCvz6Fn3ZeQOUfcLmrmDbecNp+ssoNv8AHiTxZotL+NGmqsEkbHtYihJHyr0UP5Q/HmKg+e3cHxo+POx6+aKHvHM9cdXbDxtdlM1WBGygocRikyu4cjkMlPFAGvLVV1W4iiVpZpQiswGfKfMZk9v9l5o5k3BQTYLc3dw4VR8NWbSigD5BVycAVx1HPuDyUIfdvmLkbknZ3YDcDa2FnGzO2QKLrlcmgqSWd6KKszBQSLiPmv8ACv4A/wAuX4Z7Pw/Y/XtF3X80t/YKfE7fzFZ2L2lgaf8AvFVJJPuPfsm09q75weBg2N149WtLjo5aQy5OpWmSfya6uSKGORuefcP3L53vZts3JrHke3cPIiwwOdAwkXiSRM5lmpViDRBqK0ooORfud7Ye0Hsv7a7fFvGyjdfca6jMMEklzdRBpTmScxQzoggttQCjTVz4auxLO4rB/lTdEdU/JP5s9Y9Rd1bV/vp15uHCdiVeY29/HNx7d+8qMFsDcObxUn8W2nmMFnKf7XJ0MUtoqlFfRpcMhKmVvdzmDd+WORN13nY7vwNyjeEJJpR6B5kVu2RXU1UkZH2Z6gL7v/KXL3O/uhtPLvNG3/VbPLDcPJD4ksdSkLup1wvG4owBw2fOo6ev5tfx+6i+MnzN3X1P0ftL+5OwMbszYOWosB/Htz7k8OQzWBjrcnUfxXd2az+ak+5qWLaHqWRPogUce6+zfMe881cj2e779eePuLTzI0mhEqFeijTGqLgfL7elf3i+TOW+RPcibYOVNt+l2kWUEoi8SWXvcNqOqZ5HzThqoPIdWGbO/lI7I+SH8rDpvvzoXbVRjvlQMPu3dediO4dwV1B3FjsTvXduFm2suJzGXrMHtvcdPiMVA2Klx8FHDUVETU9UrGpWppo4vPeS+5X93N85d5iug3KOuOGM6EBtmaKNhJqVQ7oWY6wxYgHUvw6Wl6z+7ntXO3sJy3zZydt+j3BML3MmqWQreKssqNDpd2iik0KDGVVFLDS5AfWmu3VUVbjKusx2RpKrH5DH1dRRV9BW08tLW0VbSytBVUlXSzpHPTVVNPGySRuqujqQQCPeTEckcsaSxOGiYBlZTUEHIIIwQRwPWFE8E1tNNbXMLR3EbFJI3BVlZTRlZTQqykUIOQcHrYd/mc/BX4rfHn+X18au7+n+rf7ododgby6cxW7tz/337Gz/APFqDdXSe/t3Z+D+C7o3fm9vUH3+4cJS1GqmpIXi8XjjKRM6NjV7Ue4PN/MvuRzTsG97v4+020Fy8MXhQppMd1DGh1Rxq5ojEZY1rU1ND1mf94T2i9vOSPaXk/mflfl76XfLq9tIZ5/HuZNSS2dzK40SzSRrqkjU1VQRSgIBIJff5KPxO6A+W3dXb+0vkHsH/SBt7a/V1JuPBY/+9O9dqfY5mTdmJxj1n3eydx7branVQ1UieOaWSIar6dQBAl99+ceZOTNi2W95a3H6a5muzFI3hxSVXw2alJUcDI4gA9Ar7rHtxyX7j8wc1WPOezfW2ttZxywr408Ol2k0k1gliJqMUJI+XVmfZHXH/CdLqDf27esOw8N/d7fWxs3W7c3Tg/4j858t/C8xj5PFWUf8Twddk8PW+GTjyU1RNE39liPcV7Vun3nN626z3bbJ/F2+4jEsMmnal1KeB0uFYV9CAepv5h2H7k/K+8bhy/v1p4G72khiuIdW/PocCpGuNnRsHirEfPqvb58f8My/6Ap/9ka/5np/fHbfh/7Kq/49K1f/AHh/5m//AL8/6+D6/wCU/wDHL+17kv25/wBfP+sa/wCuB/yr3gPX/kn/ANpjR/uN+p6/L16hX3f/AOBY/qXc/wCtR/yuHjxeH/yV/wCz1fq/7mfofD659M9CZ/JI+EXxg+XW3PkPkPkN1j/pBq9i5vraj2rL/fTsLaf8Lp8/Qbzmy8fj2PuzbUVd93Jiac3qVmaPx+gqGa5V798/c28lXXLMfLO7fTJcRztMPChk1FDEF/tY3pTUeFK1z0e/dT9pfb73L2vnK4525f8ArZrS4t0tz49zDpV0lLCkE0QapUfFWlMdGsj6Y/4Tydm7oHVe1N1JsDe4zpxf3r7x+S20VORpa5sVNhTuHuZKzYH+UV8oX9XlcpeKQIGJB5337zG02n74vLP6mw8PXp8Kxk7SNQfRa0mwB9nqK06kWHlH7k++bu/K9hdJa70sxiOu43WDvV/DMYlvG+nLFzQAEs3FcAnqs3+aH/LAqPgZW7P3rsbeOX390r2Dl8jt/GVu46Ojpt2bL3NR0z5Kj23uWtxkVJh8+M1h4J6mjrqWmovI1HVRyUsIiikqJc9oPdpPcVL6w3CxS23+2jWR1iJMcsZOkyRhqsmhiAyszU1KQxqQuPH3hfu+Sezkm3bvs+5y3vKN7K0EbzhBNbyqgZYpWXSsviqHZHREFEZWUEK0hWvg18KOx/nL3LT9Y7Jqott7exFIme7E7DyGPnyOJ2RtoVC04qDRwzUf8X3BlZ7w43HCop2q5Vdmlhp4aieEZe4XP21e3mxNu+4IZbl28O1tVYK0r0rSpB0ooy70OkUwWKqY19oPaTfveDmj+r+0Si2soo/Gvb+SNnjt460FQCoeVziOPWpejGoVHZb5t1fFj+RD8RMmepvkTvmv3v2dj0hbPTZvdXeWez+Kq/tKWWSjy+N+PNJj9v7WeoWpSeKkr4hWCKQHU6jV7xzsucfvGc7xfvrlfblt9ob+zEcdoiMKkVVr0s8lKULKdNfIdZm7v7c/c39r5l5c553Nrnf0FZjLPuEsynSrUlj2wLHCSGBVXRWINRUZ6DP5Hfycuge1OkMh8if5c/ZFTvaho6HKZiDr59xwbzwO6qXGSzT5PCbR3DJHDuDB7txUAaJMdlWq5aiWNIZHp5SXc35V99eZdm5hj5X90tqFvIzLGbnQYnjLABXlTKPGxzrTSADUBhgB/n/7qXI/M3KUvO3sTvX1AVGljshOLiC4CE644ZiTJHOuVCyMwLKEbQSW61rUBAIIIIYgg8EEWuCP6+8sOuevWxN87vgr8V+mf5anSnyA626t/u325u7H9CT7h3b/AH37GzH8Ql3rsSTM7mb+A57d+U2zSfxLJKJLQUUQh/TFoX0+8XPbn3G5y373Z37lndt48XZIXvBFB4UC6RFLpj70iWQ6VxljXzqes8/en2V9suU/YHYud+X+Wvp+aJotuaW6+ou31GeNWl/TkneIayfJBT8NOteFPp/sf+IHvKPrATo2Pwi682l2p8qOiOv9+4n+O7M3j2ftPbW5MP8Af5LGfxLEZXJw09dSDIYasx2VozNTkr5KeeKVb3VgefYR5/3S/wBk5K5m3fbJ/C3C3tJJYZNKtpZRUHS4ZTT0II6H/tHy9svN3uvyDyrzFZ/UbJfXyxXUGuSPWmljp1xMki5AyrA449WL/wA4f4s9D/Fjs/qDbvQ+xf7iYfdOwsxms7R/3n3luf77J0u4XoYKn7jeW4dw1VL46UadELxxn6lSefcbewPOvM3Omz8wXXM25fUzwXKRxN4cUelSlSKRIgOfUE9S998b2n5A9qt55HtOQtg+gt7y1uJLlfHuZ9bRyRKhrcTTFaBj8JANc16dv5Zf8tPbHyr29uvvPvXcmR2v0ftDI5DB0dDiMhSYTJbnzGIx1PlM9ksjn8hDPT4HaG3KKsi8syIXqpmkUSwCmkMjfvJ7w3nJN1Zcs8s2izcyTosrPIpdY0ZiqKqAgvLIQaDgophiwoq+6992Ta/dLbtw595+u5IeSreR4Le3ifwnuJI1BlkklP8AZ28QNO3ud9XcgjIc+G3uiv5Dvc+dfq3rzdGOwG9Z6042iysHYXeu25a2up2qIzT4LOdrVVR19nJK2SnYRfbLUioJTwX8iaoxvOZvvN8vWq71u1m8m3BdbIYLKQKpoaulsBOlK51aaZrwNJ32f29+4dztus/KvLl3brvokMKlb3dIi7gsKW8l5L9NcVKmhj8QMKFahlrrZdo4jaGF7D39geu8rlMzsfE7t3HiNn5zNijGWy+3cflKuiw+XyCY9I6JKrI0UKTMsQ0KXsL295fbJPuF1s+13W7QpHuclvHJcRx10pIygsq6qtRSaZzjrmhzhY7FtHN/MW28t3M1xy/a300FpNOUMksUchRZGKKqHWF1YAFCOgqfGVUZBCiUAjmM3P1/1JAYn/WB9mfRel3C3FqH5/6qdYQrK+llKsL3DAgjj8g8+/dPEhkJU1Hy6y+/dNde9+6907YyLyVMR/Ea+Q/8ggBf+TiPdlFWHSO+fRAfUmn+r8uldH+f9h/xPtwfE3Qdf4j1k97HE/b1XrKn0/2P/ED3vpp+PXP37qnWSP8AP+w/4n37puTy6wV0Xlp3A/Ug8i/8g8kD/Erf37p20k8OdPQ9p/PpOJ+of7H/AHo+/dHr/Ces4+o/1x/vfv3TPWf37r3Vb/sE/j/PrMjrkn6h/sf96Pu5+Dqr/CepKfX/AGH/ABI97T4R0z1l92691737pp+PWSP8/wCw/wCJ9+6p1JT6f7H/AIge/dNPx65+7n4B9vVOs4+g/wBYf71783Bem5PLrLH+f9h/xPt3pvrMn6h/sf8Aej791V/hPWb37pnr3v3XuhD6r7T7E6V33t/s3qneGc2JvvatdHkMFuTb9Y9HX0kwBWWCUDVBXY6ugZoaqkqElpaund4Zo5InZCi3Ha9u3qyuNs3azjuLCZSskUgqCP8ACCDkEUKmhBBAPRjtG+bxy3udnvOw7lLabpA4eKaFtLAgg0PkyNwZGBR1qrKVJB24P5c/bnyF/mD53vX5oZvIdfdbd17I+PmG+GnQO5Mhj2rth03ambmzXYW8Owodu16VaU24FkqcLLJRRJXeaCd4SPtB9u2I/uTtHLvt3b7ByTBFcXOxz7i29bhEppKYFCwxwlxQlMOKkrQgH4u7rPz2g3/mj3ZuOZvci4a3seYLfaU5c2yUlngW5Yvcz3HgN2qxLQHT3EgFSdIp1sQdbY7e+H692Pi+y9w0G7exsftLb1Jv3c+KoIMVic/vKDFUqbmy2IxlPSUMWPxFdmRNJSweJGip2RWuwJOOW5y2M2438u12zQ7a0zm3iclmSMsdCsxJqwWlTXJr1lXtMW4wbXt0O73ST7skCLdTRroSSUKBI6J+FGepVfIUFTx6mb53HU7P2TvHd1Fgshums2ttbcO46TbOJeGPK7iqcJiavJwYLGSVBFOmQy8tKKeEuQgkkBbi/ulhbJe31lZvcLEksqRGV/hQMwUu1M0WtT8h07f3L2Vhe3kds80kULyrDHTU5VSwRakDUxFBUgVOevnefOj+Yh3588t5x5XsfKDbvXeCrZqjYvUO3aupXZ+1wwnhiyNYr+J9zbsekneObKVSeXS7pAlPA3hHR7kP245e5AsjDtcXibjIoFxeSgeJJwwP4I6ioQY4EljnrkR7o+8HNfurfpLvEgg2aFy9rt0JPhRnIDsTQyzaSQZGAwSEVFYr0RIfQf6w/wB69j/qIjxP29bFP/Cbr/sq/u//AMV3q/8A35OwfeN/3mf+VQ2L/pZD/qzN1mJ9zH/leOa/+lT/ANrEXV3/AMWPgFH1h8s/l384ew9upn+yN+dn9ljorbUM1D97gNjT1NbSVmdhmyVRSYuh3V2QUalpZJZo0pMQ3rmVa6ojigrmz3D/AHpyfybyHtt0Y9sgtIP3hKQaPKACE7QWMcPxEAZfgDoUnKHkn2mi2X3E9wPdDd7RZd6vLyVdrjBqYrfSFZ+7SizXDAqDU6Yqdw8SRRprfNn5GdtfKP5I9j9n9y4+r25utM1W7Upth1Uc0P8Ao0we2K+tx+P6/SnqIKWeOo27KJUrHkiilqMg888iLJKyjNjkblrZ+U+Wdt2nZJRLZ6BMbgU/XaQAmbBIo+KUJAXSASB1zS90edOYefedd43zma1NtuKubUWZr/iqRMwFvkKxMbFtRIUs5ZtK1oDmfyNP+3kXS/8A4bfbf/vrN2ewT79f9Ox3z/mrb/8AaRH1I33U/wDp9Ww/8813/wBo8nSi/nyf9vEt8/8AiO+rf/eXh9t/d6/6dpYf89U//H+l/wB7r/p8Fz/0rrb/AAP1sIfArvja3xl/k79Gd473oslXbQ2NgauXckeIRZslT4fP/ILNbWrsnSUzf8DZcPBnDV/bgq1QIDErKzhhjf7h8vXfNXvXzBsFg6re3EgERfClks1kCk+Woppr5Vr5dZhe03NW3ck/dz5T5o3dXO2WltWcxirKj3rRs4HFtAfVQZIFBk9EJ/nFfy6sH25tiX+YF8T4cZumhzm3aPePbuF2aYa/G7x2xLj46yn7p2otBriq6qPFaJM6kItU06fxAjzJWyTSN7Je5txst0vtvzjrhkjlMFlJPUNG9aG1k1cBq/syeBOjgUCw395X2TtuaLJ/eL2+dLgSW63O4Q2xDpcQ6Qy3sBWoZhHTxAKh0AkWjh/EXn86H/t1H8Of/EhfHr/4G/tP2W+xX/T3+dv+eW8/7Tbfo4+9f/04f2//AOllY/8AduvOio/8Jw/+yje/v/EJ0P8A73WB9jH7z3/Kscuf895/6tP1HX3IP+Vr54/6V0X/AFe6PD8kv5B/+zC9+ds94f7Nd/dD/SjvbM7w/ux/oL/j/wDA/wCL1Hn/AId/Gv8ATHhf4n9v9PN9pT6/roX2AuVvvF/1a5d2bYP6neP9JbrB4v1ejXpFNWn6ZtNfTUft6k/3A+6D/XrnLmHm3/XD+l+vuTcfT/QeL4dQBp8T62PVw46R9nWtV81fjP8A7J98lexPjx/fX/SJ/cGPZ8n98P7t/wB0v4t/ezYu2t6W/u//AB7c/wBh9h/eL7b/AIGzeXw+T0a9C5U8ic1f115V2rmf6D6b6nxf0NfiafDmki+PRHWvh1+EUrTNKnAf3R5G/wBbXn3mHkf96fW/QGAfVeH4OvxraC4/s/El06fG0/Ga6a4rQbBn/Cbf/j0Plp/4cnT3/us7E941/ek/3N5M/wCaVz/x6HrNr7jP/JF9w/8AnqtP+rc3Veo/knfzAOwe39wfxXrHbvXm0s/vLN5D+++5+yuucnjKPE5HcEki1hw+zN1bn3RPOKCqM6wiiUsIyjMjlQZN/wBfr232zZbbwd2lub2OBV+nhgnViypw1SxxxgVFK6vOuR1Cc/3UPePmLnHd3udlgsNouL2aYXlxc27qI3mJBEcEsspbQ2oKVUYoWU06sc/nzdnbJ6++MXx8+I9JuOLcXYNLuDaG6q9J5YpcxSbL682Tn9nUuezdNG0r4+r3Zmswppmdv3hSVYXUFJEZfdy2jcNy5t5l51e1MW2NFLCpFdJlmlSUohxqEaLn01Lwr1N33zeZNo2nkHlL26i3BJd9NzDdPG1GkW2ghmhErgZQyysApPxaZAK6WoIP8kvGY3qP+XT3z3ph6SCs3dkNzdo7orJKiIIJqbq7YlG+2sHK6NrnoqetFbOCdJDV8gH0uSz3/ml3v3R5d5encrZJDbwqAeBuJjrcehI0j/ajo++6PY2/LfsdzDzVAge/uLm7unJABpaxBI468SoKMw9C7fnqUbhz+a3Xn83unceSqszuHcmXyWezuXrX8tZlMxl6ybIZPI1clhrqa2tqHkc2F2Y+81rW2gsra3s7WIJaxIsUaLwVVAVVHyAAA65hbhf3e6X99ue4TmW/uZnuJ5WpV5JGLu5pQVZmJPzPWyJ/wnS7D3FHvr5FdUPWzS7SrNpbZ7Dgx0jlqeg3Fjcx/durraSMnTDNlsblYY6ggXlWigB/zY94r/ek2u1O38rb0IwL1ZpLUuOJRl8QA+oVlJHpqPr1nn9xHe7763n/AJcaZjtvhW96kZ4LLqaJ2A8jImgN66F9OqZ/nlszC9f/ADP+T209uwCkweN7o31NjKJFVIsfS5bM1GZTG0yLwtHjv4gYIQbsIo1uSbn3PPtvf3G58hco3t01bh7CEO3mxVQmo/NtNT8z1if75bPa7F7v+4m22VRaruk0qKadvjHxigoB2oZCq+ekCtTnrYl/me/9ucPjh/2qvi3/AO+xl94ue0X/AE/bmj/mpuH/AFf6zw+8Z/4ityx/zR2j/qynWpWn0/2P/ED3mz1yx6Pn/Lpi8XzQ+K/Hqk7s2LI3/IeYp9P/ACZb2APdT/p3POf/AEr5f+O9Sb93mTxPf/209BuSgfkj/wCXq1f/AIUE/wDM6ugP/EXbg/8Aesk9w991j/kgc1f89kf/AFb6yV/vCf8AlYvbT/niu/8Aq7D0If8AJ2+V/R9T0rvn4Vd053FbQq915PdTbWq85kEwuI3rgOwMMmJ3FtaLNztHRY/ctLLFIaeOWSN6xKtUpw8kTL7Kvf8A5G5jTmLb/cTl+2e4ihSLx1jXW0LwNqjkKDLRkUqQDpKnVQEHoSfcz93eTLnkm/8AZfmy9itNwaWc2fjt4aXcN0D4sSyEhROjFu0kF1ZdGoq9Cv8Ay+/kv989JPuDevR7N3f1ZQpNkRjscni7V2/j4wJJ48htVIhDumKkDhUmw8lRVzqjyPRQItyNeQvvD8s8xC127mUfu3emITW+bZ28iJK1iJ8xIAowA5r1EXvH9yfnjk+Tct99vW/fXKyKZRbL/wAlCJRUsvhBQtyFFNJiJkbh4IpU0wvFJDM8M0bxTRSNFLFKjRyRyRsVeORGAZHRgQQQCCPeQ6srKGUgqRUEcCOsIZI5IZJIZo2SVGKsrAggg0IIOQQeI6yj6j/XH+9+99NngesjxxyCzorj/alBt/rXHHv3TSu6fCxH2dQ3xtO59OqIn/UnUtz/AFDXP+2I9+6ULeyqO6jD5/7HUKXE1CXMbJKP6A6G/wBs3p/3n37pQm4QthwVP7R/Lp1xNM8KSPKhR2KoAwIOlRckfgqxP+8e7pxPSS+mWRo1RqqBXHz6e4/z/sP+J93HxN0VP8R6ye9jift6r1lT6f7H/iB7300/Hrn791TrJH+f9h/xPv3Tcnl1k9+6b6S80XhqHj/AY6f+CkXX/eD790IY5PFgV/MjP2+fXY+o/wBcf73791rrP7917qt/2Cfx/n1mR1yT9Q/2P+9H3c/B1V/hPUlPr/sP+JHvafCOmesvu3Xuve/dNPx6yR/n/Yf8T791TqSn0/2P/ED37pp+PXP3c/APt6p1nH0H+sP969+bgvTcnl1lj/P+w/4n27031mT9Q/2P+9H37qr/AAnrN790z1737r3WSP8AP+w/4n3ZPiHTcnl1u/fB3oj4+bP6P+Efwo7v6r7DznZ0+3sJ/MQg3HHjs3QdX4HsOk3BX5LEU289w4zOY7GZHcW28HVQYmow1fR12OemSMzWkmgZsIOet+5ivN855532LdrZNr8RuXDFVTO8JRQxjRlLKjuC4dWVq1pgN10w9tuU+V9v5a9tvbnmPYryTeooY+bBNokS2juRIWVZZUdUeWIPoMTB10gFxUoSJnfv89r4ZdHd14TqSgm3J2zioMlNjey+yutxj8rtHYE1zBDHjZZZ4j2FPR1NmyH8LcwU1PfwS1dUj0ilXL/sLznvuyTbvL4VnKU12trc1WSUce6g/RqPh15J4hVo3RhzZ953235W5lt+XfFnvkWTw727swrw25OOJI8cqTV/D1aRUAtIDH1bN1V211r3hsXB9l9R71wG/wDYu46f7jEbk25WpWUU2mwnpKlLJVY3KUMh8dTR1McNXSzAxzRpIpURHu+z7psN/Pte8WMlvfxmjxSih+RHkykZDAkEZBI6nbY9+2bmba7Xetg3OG72qYExzwMGU0JDDHBlYFWU0ZWBVgCCOvnXfzCehj8avmd8hOoqeiOPwWF7ByWc2bTgh4o9i72jg3psuCKdSUqDQ7bz9NTSsDxPDIrBXVlXpF7dcwDmfknlzeS+qeS2WOc+fixVilPyq6Ej5EcePXIb3f5VPJnuTzdsKxhbRLtp7YKKKIJ6TQquTXRHIEJH4lOBwBOx9B/rD/evY06i88T9vWxT/wAJuv8Asq/u/wD8V3q//fk7B943/eZ/5VDYv+lkP+rM3WYn3Mf+V45r/wClT/2sRdGM+Qn85vs3pj+aRkNr5pKvHfF/qDNZLpLfmw8eVyFRn6aaup23H2w0bJGZd24XKwwy46BCoXGUj0ilHraqVw3y37JbVvntRHdQaW5rvUF9b3DdoQ0Oi3r/AL7Zahj/ABsGNQigDLnP7yW8cq++0m13YKch7e37uvLdRrZ9WlpLsUGrxI206VFf01ZQA0hPSS/npfBbEZWixP8AMF6EpaTNbQ3pQbek7jj2vTw1GJmhzNJTf3Q7mo56NjFNjdy0tTS0eSmRNLTtS1RLNUVEgW+wfP00Tze3PMLmO9gZxZeKSGqpPiWxB4NGQWUempfwqOiv71ftTDdwwe7vKkfi2k6RjcxBpKFGX9G9UjirAqjkVHwPT426IF/I0/7eRdL/APht9t/++s3Z7kT36/6djvn/ADVt/wDtIj6hv7qf/T6th/55rv8A7R5OlF/Pk/7eJb5/8R31b/7y8Ptv7vX/AE7Sw/56p/8Aj/S/73X/AE+C5/6V1t/gfq1ZP+4bsf8AiNz/APBRH3EX/sT/AP1Ff9qHU+P/AOIWH/pW/wDeQ6KB/JQ/mW/6H9xYz4h98bhjXpzemSmpuq9zZ6pLUPW+8MzUPI+1a6ecPHSbH3tkqltJYrT47KzGVwsNVUzQjb329rP31azc68vW5/fkCA3cUYzPEo/tBTjLEo+1kFBlVBjH7rXvkeX7219s+a7kf1euZCu23MhxbzOa+A1ceDOxOk/gkOQVkJSxn/hQ9Q0WM+DPUeNxtHS4/HY/5ObBoaCgoaeKkoqGipOoO7IKWjo6WBI4KalpoI1SONFVERQAAB7jL7tMjy+4G8yyuWkbaZmZmNSSbm1JJJySTxPUw/fTjSL2o5diiQLGu/26qqigAFnfAAAYAA4Dqvf/AITh/wDZRvf3/iE6H/3usD7kn7z3/Kscuf8APef+rT9RD9yD/la+eP8ApXRf9XuqvP5kv/ZfHyz/APE17z/9z/cue1n/AE7rk3/ngi/wdY+feB/6fH7hf9LFv+Or0Sb2Puob62tP+E2//HofLT/w5Onv/dZ2J7w9+9J/ubyZ/wA0rn/j0PXRj7jP/JF9w/8AnqtP+rc3VVfbX83D+YjXbk3zs7/Zk81jcFR7tzePpE2/sbqrbGVpaPE52pWhgp9x7c2JitxwqiUyI5WrBmS6yF1ZgZh2X2X9so7Xb77+qsb3DQozeLLcSKSyCpKPMyHj6Y8qdY6c2feV97k3rf8AaouepI7KK9mijWK2s0ZVjlYKBIlusmAAD3VPnWp6rN3Punc+9twZXdm89x57d26c7VvX5zcu58vkM/uDM10gVZK3K5nK1FXkcjVuqAGSaR3IA59y5YWdpt9vDZ2FrHBZxrpjihVURR6KqgKo+QHWO257luO8Xlzue77hPdblMdUtxcu0sjmlKvI5ZmNABUk462tv5C3YW0u1fif398Vc9WrFmcVuPceSqaGKQRVtV132xtah27UVdCkgPnkxmcxVcs8i3WH7umDhdal8OvvHbZe7Pzny3zjbR1geJEDHIE9tIXAPpqRlp66WpwNOkP3MeYLDmH225s5AvJh9Xa3MjmMAg/S3kYUEE4YiVJa0+EFKgVBOtL8gPjv2n8a+1dydR9nbXy+H3Bg8zW43G1U2Oqosdu3Hw1Ijx24dr1TK8OXxGZppIpoXheQqJRG+mQMgyw5Z5o2fmzZrTe9ovEe2kjDuoYFomI7kkHFWU1BrThUYoeuf/PXIPMnt7zLfcs8wbdLHcxzNHBIUIS4QGiSwnIdHBBFCSCdLUYEDZg/ke/F7dvxv637s+WHfmNr+rcNunatPTbfpt50k2Aq8f1ltOKs3bursDN0desdZjcDkWhgajeeOF5KWhkqVD089PI+KH3hOb7LmvdeXuS+WpVvbiGYmU25DhriUiOOBCuGdanVQmjMFwysBnv8AdA9vt09vuW+c/cXni3fa7W5iCxLfL4JS0tg8s11KHIaOJye3WqdsZkFY3RjrV/JXtde9PkJ3V3DDFJBRdjdm7x3XiaaVPHNSYPKZqrmwNHOv/Hekw3gic/UuhP595YcpbL/V3ljYNiJBktbSKFyOBdUAcj5F6nrAD3H5oHOnPvN/NSV8C+3CaeEEUIiLkQgj1WIKD8x1s1/zPf8Atzh8cP8AtVfFv/32MvvEf2i/6ftzR/zU3D/q/wBdEfvGf+Ircsf80do/6sp1qYUsZmkjiH9uQKf8BxqP+wHvNkZx1ytlfw43c+Q6P3/L4AHzZ+LQAsB3XsUAD8AZinsPYC91v+ndc5/9K+X/AI71JH3biT78+2JPH95L/wAcfq0r/hQT/wAzq6A/8RduD/3rJPcOfdY/5IHNX/PZH/1b6ye/vCf+Vi9tP+eK7/6uw9Up7P6P7f7B2dursDYvW+7937O2RXYvHbszu28LWZimwVXmEqJMeldFQRz1aRSJTMXlEbRQ6k8jJ5I9WRm4czcv7TuFltW57xb2+4XKs8EczhC4Wmqhag88CtTmlaHrCDYvbvnnmjY915k5c5WvL7ZbKVIbqa1jMmh3FVGhayNjLFVIQEFiKit4f8kn5MfJPN9vt0Rlslurf/RcW0M5WyTZqLIZmj6tyGKjFZiHxm4ZlmbEY3M1Upo/4dJN9u8k6PCiMra8bfvG8ncn2uxLzLbwwWvMpuEXTGVQ3CthtUYpqZANWsCtAQxNRTOj7kPuf7obxzRd8lbrc3e48iR2UjrPcK8gs5UZSiLcEEhZA5XwmY/hMYUBtRGP5umzNl7J+eHbNDsimoaClzNLtDdWexmO0LS0G7Nxbbx+Qz5ESEiCfK1MgyEycfvVjEAAgCS/YXcdx3H2z2STcXZnjeWCJ34tEkhCZ8wo7B8lHUCffK2XZNl99+YV2VET6q2t7y7jjpRbiRP1MD4WkCrIw82ct59Vsj6j/XH+9+5j6xWPA9Z/fumOux9R/rj/AHv37rR4HrP790x1nH0H+sP9693Tj17rLH+f9h/xPu4+JumX+I9ZPexxP29V6yp9P9j/AMQPe+mn49c/fuqdZI/z/sP+J9+6bk8usnv3TfTTk4rNDOB9Q0bf64uV/wBuCf8Abe/dGdjJ2SRE/Mf5em4fUf64/wB79+6W9Z/fuvdVv+wT+P8APrMjrkn6h/sf96Pu5+Dqr/CepKfX/Yf8SPe0+EdM9Zfduvde9+6afj1kj/P+w/4n37qnUlPp/sf+IHv3TT8eufu5+Afb1TrOPoP9Yf71783Bem5PLrLH+f8AYf8AE+3em+syfqH+x/3o+/dVf4T1m9+6Z697917oUukqbriq7c65j7gys2F6pj3lt+r7Gr6Whr8lXDZVBkIa7ctHjKHGwzVdTl8piaeWlo1AVPupo/I8ceqRS3eG3Jdq3E7NEH3bwHFsrEKPFKkIWLEAKrEE+dAaAmg6OeXF2R+YtjHMlx4XL4uo2vW0ux8FWBkVVjVnLOoKrQUBILFVqwtb/mEfzl+6fmAmZ6s6rhr+jvjY6/w4bRxdTFBvTfmLijamRewM7jHEcGHqYb/7gce645Vbx1MleY45Viv299l9l5MMG67qy33M9dfjsD4cTcf0Vb8QP+iMNXmoSpBm73b+8XzD7gx3OxbDG+2cnOpjeAEePcIcETutQqFcGJDpoSHaQUpTF7mbrGt+PRvviD83vkJ8Jt8x706T3fJSY+smiO7Ovs6arJ9e74pI3jvTbk26lVSqatY49EOQpJKXJ0qllhqEV5FcK83cjcu88bb9DvlmC4H6VxHRZojnKPQ4zlSCp81NBQfe3vudzd7aboNx5b3AiBq+PZTFmtpgaf2kQZRrGkUdSsiioDBSwJjv5nfy96f+dG6OlfkJsrb+S2H2rN15Vde929e10ZqqPG5TaeVOU2vubBblhpYKXc2J3BR7pq6SOSQQV8CYpI56eNBBLOHva3k3eOQ7Pe+Xb25S42kXIuLG4XBZZF0ujpUlGQxgmlVOuoYmoUZe+PuJy37oX3K3NW1Ws1tvxsmtNztJBVIzE4eJ0lAAlWTxpFBwwEY1InaWrCH0H+sP969yn1Ap4n7erFv5bvz5/wCG+O2N7dn/AOij/S5/fPrqXYX8D/v1/cH+G+bcuA3D/Ff4l/c3en3mn+B+HwfbxX8uvyenS0b+5vt9/ri7PY7V+9/o/AuRceJ4Xi6qI6adPiRU+OtanhSnUw+zPu1/rQ73u29fuD94fU2n0vheP4Gn9RJNWrwZq/BSlBxrXy6LL8le5/8AZifkB233n/dv+5/+lPfOc3n/AHX/AIx/eD+Bfxmoao/hv8b/AIXhP4p9te3m+0p9f10L9PYq5X2T+rfL2z7D9V430lusHi6dGvSKatOptNfTUft6AXPfNP8AXbnDmDmv6H6b664M/wBPr8TRUAadeiPVw46R9nVovw6/nKZv44/GbLfFXt7oLHfJbrWog3BgsLT5vsiXZb43YW66Wohz2wcpFLsPfCZ3AvPW1D0vNLJSxVDwgvEsKwxXzp7KQcy80wc3bLzC217oCkjmOESapYyCkykSxaHoBXjUgHjWs5+3P3lbrk3keXkLmPlFN82ekkMYnufCpbyghrd1a3nEkfc2nI0qdAGkLQlPw8+WWC+Hvyxw/wAkdr9WV26Ntbcl3/Dt/rLJ9gJQ5Glwu8cDnNvYvHV+/wCPZNbHkazAUWXQyVIwsIrXhJ8UGv0DrnXlCfnTlCbli63ZYbmUQmS6WHUC0bo7MIvFFA5U0Gs6a8WpmKPbf3Etfbb3CXnWx5faexjNysNg1xpZY5ldEVrjwX1tGrAFvDGsitFrQR/nl8t/9nb+ROc78/0f/wCjL+Nbd2tgP7p/3r/vn9t/drFpjfu/47/dvafm+90a/H9mnj+mpvr7Ue3fJ39ROWbfl794/VaJZJPG8Pwq62rTRrkpT11Z6r7u+5H+upzhJzZ+5voNVtFb/T+N4/8AZg92vwoeNeGnHqejXJ/NP/7FuD+Xz/oJ/wCYbO3v9Ln+k/8A7+keyfu/7hf6PP8Aqi8f8a/5vav91ewgPaP/AJiifcf+sH+i+L9F4H/Lv4FPG8b/AG1fD+Xz6Hb/AHgv+YLH2e/qj/xG+n/eP1X/AC8ePq+n+m/2tPF+dfLqpRPp/sf+IHuZ+sberI++P5kfZHyO+FPU3xJ7R22M7n+peyMLvDH91VG56ifNbi23tvaO9Np4PbO5Nt1GGlNbm6Kl3jZs0Mmr1EFFEs1K9Q01VJF/L3tftfLHPe8857TdeHbXtq0DWAjAVHeSKR5EcNhSYv7PRgsaMFAUTXzn7473zx7Xcue3W/2JmvtuvY7ld1aYtJLHFDPDHHLGUq0gWbMviVYKNSlizmP/AC3/AJ9f8N/dj9gdgf6J/wDS1/fnZNPs7+E/37/uH/C/DnaDNfxH7/8AubvP73V9j4vD4YbatWvjSb+5/tz/AK5G17dtv74+i+nuDPr8LxtVUK6aeLFTjWtT9nTfsh7y/wCs1u2+bp/Vz95fW26QaPqPp9Gl9erV4E+qvClB9vVwy/8AClXUbf7Jdb/y4z/9BHuFP+BY/wDD7/7Mv+3vrI9vv06RX/Wt/wC6l/24dEt+fH85L/Z4egp+jf8AZcv9GHm3jtvdn96P9L399dP93hXj7D+Cf6L9pX+7++/zv3Y8en9DX4Hntz7Hf1A5jXmD+tH1dIHh8H6bwvjpnV48nCnDTn16i33f+9J/rrcl3PKH9RvoPEnin+o+t8enhNq0+H9JDXV66seh6B7+Wz/M5/4b3xHbWJ/0I/6Xf9KWS2fkPuP9JP8AcH+Bf3TpdxU/h8X9wd6/xP8AiH8fvq1U/i8VrPqup37pe0/+uVPs037/APovpElWngeNr8Qoa/20Wmmj51r5U6C3sb94D/WWseYrT+qX7z+vlil1fVfT+H4SutKfTz6tWvjUUp516rK3Lmv7ybn3DuL7b7L+PZ3L5r7PzfcfafxSvqK77b7jxQefwefTr0JqtfSL29yzaQfS2ttba9XhxrHqpSukAVpmladY+bvf/vXdtz3TwvD+puJJ9FdWnxHZ9OqgrStK0FfQdNPtWnHouPA9C/0T3v2l8buzNv8AbfTu6avae9NvSSpBWQpFU0ORx1WBHkcHnMXUrJRZjCZOEBZqeZGUkLIumWOORCjmLlzZ+a9pudl3yzWawl4qcFWHwujDKup4EfMGoJBEnJfOvMft/wAw2XM/K24Nb7pDUVpVJEb44pUOHjcDIPAgMpDKrDYE2d/wo83tQ4OCn7A+Ke1tz7kUr91ltndsZbYuDmAp4FcQbezexOxK+mLVSyuC2TltG6pYlDI+Nd991jb5Lhm2znKaG0/Ck9sszjJ4uk0AOKfgGanzoM0tt+/fucVpEm8e2sE9+ANcltevBGTQVKxvbXDKCakAyNQECppU15fMz+bV8mvmNt2q66yZ2/1Z1JXSU8mV2HsJK4TbpNJKlTSpvLdGTqKjK5mlpatfItHTigx8jLG81PLLDHKso8h+yvKPIt0m6RCW83tQdFzc0pHWoPhRqAqEjGo6mGaMASOoI91/vO+4XulZz7G3g7XyrJiSys6lph2kC4nfvkCsCQqCJCDR0cqrCr5Pp/sf+IHuX+scetkLqr/hQT/oy6v6362/2Uj+N/6Pdg7P2P8Axr/T1/Df4v8A3T29jsD/ABT+Hf6F6/7D7/7Dy+Dzz+LXp8j21HFXefuy/vfeN13X+u3h/VXMtx4f0erT4js+nV9UuqlaVoK8aDrPbYPvyfuHYtk2P/Wv8X6OzhtfF/eWnX4Uax6tP0DadWmtKmnCp49CbQ/8KMTW+Q/7Jz41Swv/ALMJruT+Lf6D1+gHsvX7qer/AJ3z/sy/7e+llz/eBi30/wDMJak/9JSn/eOPVQU/y3+6+b4+Zf8Ao/0ae5KTtr/Rx/evVf7Wugrf4B/fD+7a/wCc8On7v+F8Xv4T9Pc9LyH4ftyfb3961/xE2X1nheoPf4XifP4df59YeT+9Ov35X3t/q1Sm4Lf/ALs+o/hjEej6jwPOldXhfKnn0vf5gvzr/wBns3r1/vD/AEWf6LP7i7WyG2v4d/ff++/8U+/yzZT737v+6G0PsfFq0ePxTav1ah9PaH2q9tf9bXb92sf319b9TMsurwfB06V00p4sta8a1H2dGX3hPfz/AF+Nx5Zv/wCqf7q/d0E0Oj6r6nxPFZGrX6e30adFKUateI6En4NfzRuwPhPtKu65xvVWxN/bDym46jdWRhlqchtPeVRlqyCjoqqQ7spI8zRzRmgoIYYhUYyoMKxLpNtSsV+5XsrtfuLfx7vLvl1a7mkQhU0WWIKCSAIiUI7iSaOK1PQl9jPvV737K7DJyvFybYbhsbTtcsVd7a5aV6BmeYLMj9iqq1iqqqBUgU6OP2d/woB7Uz+358d1R0FtPrbO1NNV053Huje1b2WaGSc0601di8RBtTYdDHV0UQmKirNbA8rxs0RSN45o/wBn+6zstrdJLvnNM93agg+DBCLfVStQzmWY0Jp8Ok0rQ1IIlzmP+8I5lvNvmt+V/bm0sNyYFVubu7e8VcjuES29qCQuqlWIqQSCAVahjd+8N0dgbqzm9d657J7n3ZufKVOYz+fzFS9ZkspkqyTyT1NTPISSSTZVFkjQBVCqoAye2/b7LarK123bbVIbGFBHFFGKKqjgAP8AUScnPWAe+77vHM+8bjzBzBuMt3vN3KZri4mNXdz5nyAAoFUAKqgKoCgDpjH1H+uP979rOig8D1n9+6Y67H1H+uP979+60eB6z+/dMdZx9B/rD/evd049e6yx/n/Yf8T7uPibpl/iPWT3scT9vVesqfT/AGP/ABA976afj1z9+6p1kj/P+w/4n37puTy6ye/dN9cKiLzUzoP1WLL/AMGU3A/2Nrf7H37p6B/DlRvLgfz6TY+o/wBcf73790ddZ/fuvdVv+wT+P8+syOuSfqH+x/3o+7n4Oqv8J6kp9f8AYf8AEj3tPhHTPWX3br3Xvfumn49ZI/z/ALD/AIn37qnSv2XsreXYe4cdtDYG0tzb43ZmahaXEbY2hgspuXcOUqZGVEp8dhsNS1uRrZndgAscbEk+013eWe328l3f3cUFqgq8szKiKPUsxCgfaelFntu47tdx2O1bfPdXz/BDbxvLI3+lRAzH8h1b10l/IW/mGdv01Bk85sbZ3R+EyCeeKt7h3fFjcp9srFX8u09oUO8t242sYowSCvoqJ2Ni2hGD+4n3v339vdo1ww3817OpoVs4ywr8pJDHGw+asf246nTl77snulviLNd2NttsBIob6UaiPURwiZwfk4Q19BnqwDan/CYrftXADvf5e7Q29UeEkxbV6fzO8YfuBMyiPz5ff+xX8JpwG1+PUHJXRYayArz7zW3qQLHlGaRQeMtwseKeixS5r/xfUmW/3Ob2RQbzn+KN6cIrNpBX7WuYvL5dKDJ/8JhMvBRSPg/mnjsjkNUYipcr8fanDUToXAlZ6+k7nz08bIhJUCmYMeCV+oah+89CzgT8lssfmUuwx/YbdB/PpyT7msoQmH3FVn9GsCo/aLxv8HRM+3f+E8nzt69o5cpsGs6l7vpY/KwxWzd31O290rHDGHaSXG9h4rauCbyXIjSnylTM5UjQCV1DTZ/vD8h7i4iv1u7Fv454w6fk0LSN+ZQD59R9zD91D3J2yKWbZ7iw3KMfDHDIYpT6nTOqRD8pST/Lqm3tHp/tXpHdNTsnuDrrefWm7KUF5MDvbbuU27kJYNWlK2jiyVNTjIY6ceqKpgMlPMhDI7KQTM217xtW92q3uz7jBdWh4SQOrivoSpNGHmDQjgRXrHXfOXd+5avX27mHZ7myvQSPDuY2jJAJGpdQAdCRhlqrDIJBB6Dj2Y9E3WSP8/7D/ifdk+IdNyeXR+fhd/Ln+Q/zuoewsj0Y2w1p+tKvbVFuT++e5qnb8hm3VDm58X/D1p8NlRVJowE/kJKaDp+t+AJzx7j8uchybbHvv1Gq5DtF4KB8IVDVqy0+MU6lH239nebPdKHdp+WpbNI7Jo0l+qkdKmUOV06Y5K00GtaeXHyPB/0D0/zAf+OnRn/oyMl/9iHsB/8ABEe3vpf/APOEf9bOpKb7onumTUXm0f8AOeX/ALZ+si/8J7P5gAAGvo3/ANGRkf8A7Efbq/eJ9vAAP8e/5wj/AK2dV/4EP3U/5TNn/wCyiX/tn6qI7t6g3b0D2xvzpnfjYpt49c7gqts7iODrZMjif4nRrG04oK6Wmo5KqnHkADmJLn8e5j2PebPmHaNv3vb9f0VzGJY/EFG0nhUVND+fWPXNXLW48n8w7ryzuzRHcbOTwpTCSyE0DdrFVJFD5gdBoPoP9Yf717NegweJ+3q8z/oHw+ft1Pl6M4Av/wAZHyf4/wDJQ9wP/wAEX7eel/8A84V/62dZTH7n/uqQR9bs/wD2UTf9s3WRf+E+fz8BB8vRv/ox8n/9iHv3/BF+3npf/wDOFf8ArZ03/wAB57rf8puzf9lE3/bN0ld/fyI/ntsDZO698VGH6x3NS7RwGU3HWYLaO96vLbnydDh6SWurafA4mo27QLlcp9rA7RUqSiaoZRHErysiMs273+9vtxv7OwWe6ieaRYlkmiCxqWNAXYOdK1OTSg4mgqei7d/um+620bXuG6E7dcLbwtMYLWaV5nCAsVjQwKHcgYWtWOBUkDqnEAgAEEEcEHggj6gj+vubOsXiakkcOu/byfCOtdZk/SP9j/vZ9+HxN0y/xHpQbZwdbufP4PbWNMC5HcOaxmDoDUyNFTCty1bBQUpqJVSRo4BPULrYKxC3Nj9PbV1cR2dtc3ctfCijaRqcaKCTT50HSvbbCfdNxsNstioubmZIIy5ouqRgi1IBIFTnB6un/wCgf357f8d+jh/5UXKf8Rs/3Bf/AAR3t3/DuH/OFf8ArZ1lA33NPdomovdm/wCyib/tm65r/wAJ/vnqt7z9Hc2/5qJlP/sP9+/4I727/h3D/nCv/Wzqv/AZ+7f/ACm7L/2UTf8AbN0Wn5W/ys/k/wDDPrKj7b7hl62falduzFbMhXaW7K3N5QZjMUGXyVGXo6jAYyNaP7fBza3EhKtpGk3JAr5O93eU+ed2k2bZBdfWLC058aMIulWVTkO2auPLqP8A3K+7xz57X8upzLzHcbc+3G5S2payyO4d1dlJV4Yxp7DXNeGPSuX3KHUCdWW/Fn+VN8pPl71XT9x9STdZrtCoz2Z25Gu6d3V+GywyODaBK3VRQbeyMYgJqV0N5TqF+B7ivm73h5R5K3htj3oXf1ojWU+DGGXS9aZLrnHp1P3t/wDdt9wfczlmDmnl2521dtklkiUXM0iPqjbS1VWFxSvDPRkV/kD/ADxBB8/SH/ow8p/9iHsMf8Ed7d/w7h/zhX/rZ0Mv+At93v8AlN2X/som/wC2brJ/wwT88P8Ajv0j/wCjDyn/ANiHuy/eQ9ugaldw/wCcK/8AWzrR+5Z7vEEfW7L/ANlE3/bN1yH8gn53gg/cdIfX/n4eV/8AsP8Ad/8Agkvbn+HcP+cK/wDW3qn/AAFPu/8A8p2yf9lE3/bL1k/4YM+d3/Kx0iP/ACoWV/4jZ/v3/BJe3P8ADuH/ADhX/rb1r/gKfd//AJTtk/7KZv8Atl6zf8MH/Oz/AJWekf8A0YWV/wDsP9+/4JL25/h3D/nCv/W3pv8A4Cb3g/5T9j/7KZ/+2Xrmv8hH51gWNR0l9f8An4WV/wDsQ9+/4JL25/h3D/nCv/W3rX/ATe8H/Kdsn/ZTN/2y9Mm6P5Gnza2htncW7MvUdM/wna+Cy+4sn9rv3KTVP8OwuPqMlW/bwnacYmn+2pm0LqXU1hce1Fp94j2+vbu1soFv/GmkWJKwqBqchRU+JgVPSG/+5f7uWNneX817svgQxNM+m4mJ0opY0H0wqaDGeqn8VF4qNCR6pSZT/rMBp/5MA9z2nA9YVXsmudqcF7f8/wDPp3T6f7H/AIge6P8AEei9+PXP3aPz6p1I9ude69790weJ+3rsfUf64/3v37rXUuGOSaWKKKN5ZZZEjiijVnkkkdgqRxooLO7sQAALk+9MwUFmICgVJPl1ZI5JnWKKNmlYhVVQSSTgAAZJJ4DpU7o2Zu7ZFXQ4/eW2c9tTIZPE0mdocfuLFVuGyFThsg0y4/JpQ5CGnqhQ14p2aCQoFmjs6EoysUdjuW37nHLLt17FPEkhiZ4WDqHUAsupSRUVFR5HBz0Yb3y5v/LU9ra8w7Nc2N3PALmKG7jaKQxMzqr6HAcKxRtJIFQNQqpBKbH1H+uP979reiQ8D1n9+6Y6zj6D/WH+9e7px691lj/P+w/4n3cfE3TL/EesnvY4n7eq9ZU+n+x/4ge99NPx65+/dU6yR/n/AGH/ABPv3Tcnl1k9+6b6zJ+kf7H/AHs+/de6TVTF4al0H6dQZf8Agrcgf7C9v9h790dW8niRI1c8D9o669+6e6rf9gn8f59Zkdck/UP9j/vR93PwdVf4T1JT6/7D/iR72nwjpnrL7t17r3v3TT8eryv5Zf8AJW7U+aMOJ7d7hrM3078a55Vmx+WhpYYew+0YI2QuvX1DlqSpocXt6RGYfx+tgqKVpAFpaastM0EJ+5PvNtXJhl2naUS85kGGQk+DD/zVKkEt/wALUg0yzLiuRHtL93zeufkg3zmCSTb+UnUlHWguJ+FDCrqyrGQSfFcEGgCo4JZd0j43/En47fEnaEOy+gerdt7CoDBHFlcvSUprt3bmlRg5q917wyLVW49w1DS+pRU1DxQCyQpHGqIuG3MfNnMPNl2bzftzknetUQmkafJIxREH2Cp4kk56z+5W5M5Y5KsF23lnZ4bW3/GyCsjn1kkaskh+bE0GBQADox3sOdCfr3v3Xuve/de697917oF+9vjv0n8mdjVvXPenXG2+xtqVaymGkzlHfIYarmj8TZTbOdpXps7tfMrH6VrMfUU1SFuuvSSCd7DzHvfLF8m5bDuUttdjiUOGAzpdDVXX+iwI+XQf5l5U5d5x2uXZ+ZtphvNvevZKMqSCNcbijxOATR0KsPI9aTn80X+UBvr4Q1FV231XVZfsj4zZHIR07ZiriFTvDqutrpxFQ4nf60NJT0dZgq2aVIaHNwxxQyVBFPUxU8z0zVebXtb7wWHPKrtO6IltzOq10DEc4Ay0VSSGAy0ZqQO5SwDaecnvZ7Bbl7bySb/sTSXfJbsBrbMtqzGgSegAaNjQJKKCp0OFbSZKVo/z/sP+J9zanxDrG6Ty623f+EyP/HqfMP8A8OHpL/3W9oe8SPvQ/wC5nJv/ADSuf+PQdZ5fcx/5JvP/APzXtP8Ajk/W0v7xU6za697917r5yn80T/t4R8tv/Ex7i/6FpffSj2q/6d1yf/zxJ/l65Ce/X/T3+fP+e3/rGnRER9B/rD/evcgdQ2eJ+3r6rPvkv13f697917r3v3XutMv+eD/Ln/0E77qPld1Bg1g6e7Qzvj7DwOKpStJ1z2TlpJZ2yUdPAgjodo77qNTxGwhpMqZILotTRxe83PYf3L/rBt68o7zPXerSOttI5zNAuNNTkyRDj5lKNnS565rfeq9mRyxur+4vLtsf3BfzUv4Y17be5ep8TtFFhuD5mgWU6a/qIo18/eSSfCOsOOsyfpH+x/3s+/D4m6Zf4j0J/TH/ADN3qv8A8STsf/3psV7LN9/5Im8/88kv/VtuhHyZ/wArhyn/ANLO1/6vp19Ov3yk67p9e9+691Rp/wAKC/8Ashfbv/iwewf/AHkexveQP3bP+ng3X/Ssm/6uQdYn/fL/AOnQRf8AS3tv+OT9aVXvO/rlP1u+/wAhP/sgHFf+Jb7J/wCt+I94CfeK/wCnjz/88UH+Buutf3Q/+nLbV/z3Xf8A1d6uj9wV1k71737r3Xvfuvde9+691737r3XvfuvdBZ3pH5uku4or28vVnYUd/wCmvaWXW/8AvPs45eNOYNjPpeQ/9XF6JeZF1cu7+vrZTj/qk3Xzl0AUaQLBTYD+gAAA/wBt76zL5/b185RJJJPHqQn0/wBj/wAQPbb/ABHpl+PXP3aPz6p0M3VXQHd3eOQGM6h6q352HOsnjqJ9r7byeSxePI03fLZqOnGHw8ILqPJVTwx6mUXuwBJN85q5b5aiMu/b5a2i0qFmkVWb/SpXW5+Sgnob8o+2vP8Az7MkPJ/KF/uAZiviwQsYVIFT4k5Ahj/27rkgcSB1Zx1Z/JL+Su6a7BUnbW9+qeiqjcZdcNtzP7kpt2b9yzU9FNkshHiNtbankxeRlxmOppJqhFyivEiMxUKrMsNb3947lCyjuX2LbL7cki/tJo0MUK1IVS0kg1AMxAHZn7cdZQcqfcV9x91e0/rhzHtexmcfpW7P9VclgpdlEUbJExRQSdMzUoTwFej+dCfyeviLk6DZm5ajKd5fITC7sXc5G5J6eHpPr3EHajyUZbP4HKx4rtNKbcuaQ0uPlxpyKyxo8/FOonaLOZvf7n2KW+tEi23ariDw/wBJf8bnfxc9jqXt6xplg+ihovxdoyI5G+5j7MCHbr+7O97/AG1yJR407fQW8ZhJUlogILwLK40oVMoIGsdlHNgO5NsfC3+XJ1Rku38j1P1T1zPjqekiwsG3MPHnt/5zc741Gj2htzeu5hLuzc1TUZCOVoqhxRRQ0t554olSV/cW2d57h+7e+QbBFvl9eByTIZnKQpHqzK8Uf6cYC0qO4k9qk1A6n7crH2Z+7rynfc3ycsbVtMMSKoNpChuZpAvbBHM48ad2aukkigqzBQGbrTf+QPdu7fkZ3Jv7uferKud31nZsmaCGeaoo8Hi4o46LBbdx8tQfK2O2/hqWCkhLWZkhDN6iffQjlTlux5R5e2vl3bs21tEE1kAF2OXkYDGp3JY/bTriZ7l8/wC7+5/PHMHO+9DTd302tYQxZYYlASGFSQKrFGqrWg1EFiASegdH1H+uP979iHoCHges/v3THWcfQf6w/wB693Tj17rLH+f9h/xPu4+JumX+I9ZPexxP29V6yp9P9j/xA976afj1z9+6p1kj/P8AsP8Aiffum5PLrJ79031mT9I/2P8AvZ9+6902ZOK/imH1DCNv9Yklf9sb/wC39+6WbfJ3SRE/0h/l6bPfujTqt/2Cfx/n1mR1yT9Q/wBj/vR93PwdVf4T1JT6/wCw/wCJHvafCOmesvu3Xur2P5KP8sWl+ZvZFd3Z3Ph5Z/jb1JmIKWbEVCSJT9s9hwR0uRptkmRWjP8AdfBUdTDWZt1JaZJqajVSKmaWng/3n9y25O21Nm2eYDmO7QkMOMEWQZP9OxBVPSjN+EBsjfu/e0Kc9bvJzJzDa6uU7Fwojbhc3AowiI84owQ0nk1VTIL6d76goKHF0NHjMZR0mOxuOpKegx+PoKeGkoaChpIUp6Sjo6SnSOClpKWCNUjjRVREUAAAAe8GpJHld5ZXLSMSzMxqSTkkk5JJ4nroyiJGiRxoFjUBVVRQADAAAwAB1K906t1737r3QW9g95dJ9SmNe1e4erOsjLCaiIdg9g7S2YZKdUlkaeMbjy+NLwrHA7FhdQqMb2B9mu37Hve7AnatnurkA0P08Ukmf9op9eijdOYNh2NA+9b3aWaca3U0cQ4E8ZGXyBP5dJ/YPye+NXauSTDdXfIbo3sjLySGKPFbB7a2DvDJPKqq7RpQ7ez+RqmkCOpIC3sQfz7UX/K/Mu1RGbdOXb62hGS9xBLGv7XQDpLtXN3Ke+yGLZOZ9uvJRgra3MMp/ZG7HocvZF0Ieve/de6ZNy7awG8tu53aW68Pj9wbZ3NiMhgdwYLK00dZjMxhstSy0OSxtfSyho6ikraSd45EIsVY+37W6uLK5gvLSZo7qJxJHIhoyspqGBHAgjpPd2lrf2tzY3tuktnNG0UsUgDK6MCrKwOCrA0IPEdfPe/mo/Aet+B3yMq9u7ejyFZ0l2TBWbt6bzddI1RUQ4uOaFM/sjJVTFnqMxsfIVkcBkYs9TQT0lQ5Ek0iJ0O9p+fk595dS6uNK73bEQ3qKKDUQdEijyWVQTTyYMowATyj99fa4+2HNwtbIMeWr1Wn252bUwVdIlhYnuLQswFTWqMhJLFgLpf+EyP/AB6nzD/8OHpL/wB1vaHuFfvQ/wC5nJv/ADSuf+PQdZFfcx/5JvP/APzXtP8Ajk/W0v7xU6za697917r5yn80T/t4R8tv/Ex7i/6FpffSj2q/6d1yf/zxJ/l65Ce/X/T3+fP+e3/rGnRER9B/rD/evcgdQ2eJ+3r6rPvkv13f697917r3v3XukX2N15sztrYm7OtOxMBQ7o2RvfB1+3dy4HIoWpshi8hCYpkDoyT0tVCxEtPUQsk9NOiSxOkiKwXbZuV9s+4We6bbcNFfwSCWKReIZTUfIg8CDgioIIPRdu+07dv217hsu72iz7ZdRNBPE/BkcUIxkH0IoQaEEEA9fPS/mAfCneXwZ+QGd6uzX32X2PlfNuLqbfNRAFh3fsmonIpvuJooYaVdzbekb7LLQIseiqj8qJ9tPTvJ0l9uOebHn7lu23aDSl+n6d5bg5ilHGgJJ0P8SHNQaE6lYDjr7w+125e1PN91sU/iS7PLWbbrxwP1oSeBKgL40R7ZAAM0YKEdKkmT9I/2P+9n2Ox8TdRI/wAR6E/pj/mbvVf/AIknY/8A702K9lm+/wDJE3n/AJ5Jf+rbdCPkz/lcOU/+lna/9X06+nX75Sdd0+ve/de6o0/4UF/9kL7d/wDFg9g/+8j2N7yB+7Z/08G6/wClZN/1cg6xP++X/wBOgi/6W9t/xyfrSq9539cp+t33+Qn/ANkA4r/xLfZP/W/Ee8BPvFf9PHn/AOeKD/A3XWv7of8A05bav+e67/6u9XR+4K6yd697917r3v3Xuve/de697917r3v3Xugx7s/5kz25/wCIx37/AO8rlvZvy/8A8l7ZP+eyH/q4vRPzD/yQN8/545v+rbdfOTX+1/wY++s6/i+3r5x+j/8AxF/lwfJT5fmHNbM27DtDrX7vwVfaG+PucXtuTxm1Qm3aZIJcruyqh0spFFE9NHKNE08JN/cWc+e7fKPIZe3v7o3G8aarZ21GkHp4hrpiB/pHVTIU9ZBe0n3Zvcn3e8Lcdvs12/lYtQ7nfBlRh5/Txga7gj1WkdaqZAQR1eD0V/Lw+EXVG1uzM1sfAQ/zCO+unKzC4fdGwptx7cosBTbsy9dDRrg6fbtRUnZGOhp4oamapGaqcy1OKSoQlZF8S448ye63uNvd7tFtuN2eVuWb9WkhuRHIXMSgnWZAPGatQB4YjB1KaUz1nVyH93H2P5O23mK72bak58522phBdWk01uyrO2kGAQOy2kRFCx8cyOlGBf8AD1bvtHaHaL5LrHJx1m2uoOs6DrV6He3x729tnC181JvrKQM7x4TsjA12NhxWF2xPUMkP8Po0+8aPynxa9KQVfX2zCHeITHNfbw13qt90lkdQYVP44HDFnkAzqbt4Zp1lpt+38wtcbBceLb7dsSWBS72aGJXYXDhSPDukdAkcPcKLH3mjVTh0nZ9p/HD4x7B2Tn+0t24WGh6lTdcu1e2fkFvKn3TvnG5DeVUcluyox2+t71E2ZbObmmVUeCgZJJ0CU8UWjTH7WLfc2847nuNts1jIZb7wxPY7VEY4WWIaYw0MICaIxmrYGWJrU9FL7byD7dbHtF/zHukSW21+KLfdd/ufHuI2uXrLS8u3aXXMxC6VbI0xqtAq9Vb/ACL/AJ8/RGyv4jt/47bVyvcO4Yi0FPu7cUVdszrqCWxH3VPDWU8e79wRwSCzRGmxcco9UdSVsTM3KX3Z+Zdy8K55rv49vtDkwR0lnI9DQ+ElfXU5HmvWMXuR9+Pkbl1biz5B2e43zclwtw9be0ByCauPqJNNOAjVWHCTz61x/kF8m+6PlJvV999y70rdz5BdcOHxcdqLbG2KB5NQxu2cBTMKDFUgsNbKrVFQy655JZLucveU+TOXeStuG28vbesMRzJIe6SRv4pHOWPy4DgoAx1zI9zPdfnr3Y3lt5513h53WogtUqlvAp/DDCCVX5sau1BrZqdAZ7FPUY9dj6j/AFx/vfv3WjwPWf37pjrOPoP9Yf717unHr3WWP8/7D/ifdx8TdMv8R6ye9jift6r1lT6f7H/iB7300/Hrn791TrJH+f8AYf8AE+/dNyeXWT37pvrMn6R/sf8Aez7917rhPH5Ynj/LD0/8GBuv/Jw9+6rFJ4U6v5A5+zz6Tnv3QhqPXqt/2Cfx/n1mT1yT9Q/2P+9H3c/B1V/hPUlPr/sP+JHvafCOmelp19sbcfZ+/dk9a7OoTk929g7t25sna+ODaDXbh3VmKPB4ak1kEIKjI10aFjwoN/ae+vbfbbG83G7fTaW8Tzyt6IilmP5KD0u2zbrrd9z27aLFQb27uI7aFWNAZJXWNAT5VZgOvp5/Fv49bN+KvQHV3QWxYYhg+udr0WInyKUyUs+49wS6q7dG66+KMsFyO6NxVVTXTC5CPOUWyqoHNDmjmC85p3/dN+vSfGuJS4WtQicEQfJEAUfZ1145S5asOT+W9n5a21f8VtIVi1UALtxeRqADXI5Lt8yeh+9kHQi6bM3msRtvDZfcW4MnQYTA4DGV+azeZylVDQ4zEYjFUstdksnka2oeOno6CgooHlmlkZUjjQsxABPt2CGa5mht7eJnnkYIiKKszMaKoAySSaAdNTzw20M1zcSqlvGpeR3ICqqirMxOAABUk8B1pe/zIP583a/bO4dwdUfDLcOY6l6fxtXPjKntvEtPi+0eyhTS2fJ7fyMkFPlOs9rzzoGpBSGHOVESLJPUUyzS0EeZvt17E7Ts9tb7tzjbpebwwDC0ejQQ1/Cy1KzuBx1VjBNArUDnn77tfeW3nfLi62L2/upLHY1Zka/jJW4uBQisZID20dTVSpExopLJVo+tdzK5jLZ/I1eZz2UyObzGRlNTkMrl62pyWSr6hgA09ZXVks1VVTMALu7sxt9feQqQxQQxQwRKkKiiogAAHoAMDrFG9urm9nkury4klunOp5JWLMx9WZiST9p6j000tPLHPBLJBPBJHNDNC7RywyxtrjlikQq8ckbqCrAggi49qCAwKsKg4IPSZWZGV0YhwagjBBHAg+RHV+P8tb+dv3B8c9y7c6s+Tm6Nw9ufHmunp8Udw56at3J2R1PA2mnpcnhszUSz5jdG0MamlajEVLVE1PSoDjmjMX2lTAvuV7I7PzJbXO6csWsdnzGo1+HHRIZ/VWUAKkjeTigJ/tK11Lk77RfeP3/lO8s9l51vZb/lNm0NPKWlubbUcOrkl5oVqdUZ1MFp4RGgRPu77e3Bg92YDB7q2zlqDPbb3Lh8ZuDb+cxVTFW4vM4PM0UGRxOWxtZAzw1dBkaCpjmhlQlZI3DAkH3hBc289ncT2l1C0d1E7RyRuKMrKSrKwOQQQQR69dGrW6tr62tr2znSWzmjWWKWMhldHAZWVhgqykEEYIz0Sn5Z/wAyX4ifDCCopO4ezaWp3wlOail6p2LFDu7sqsvCZ6dJ8DS1UFJtuOtjH7FRmqrGUkx4WU8+xvyj7ac386sr7PthWwrQ3dxWOEZoaMQS9PMRh2Hp1HXPnu7yH7dRuvMO8qdy0aksLakty+CV/TBAjD6SFaVo0JxqHWnv/Mu/m0br/mDUOH6+pepNpdc9TbM3Wu69qNWyz7k7RqMrHjsjhWq8rutTj8VjcZkcfXs8mKo6IxrLo8tVVmCCRMx/bD2ls/b2WbcDu01zu88PgzUASALVWosfcxZWFNbNUjgq1YHn570e+9/7rQ2+zx7DBZ8v29z9Rb6i0lyXUSRhnkBWNVeN6mIIQrcZHopFr/8AwmR/49T5h/8Ahw9Jf+63tD3E33of9zOTf+aVz/x6DqdfuY/8k3n/AP5r2n/HJ+tpf3ip1m11737r3XzlP5on/bwj5bf+Jj3F/wBC0vvpR7Vf9O65P/54k/y9chPfr/p7/Pn/AD2/9Y06IiPoP9Yf717kDqGzxP29fVZ98l+u7/Xvfuvde9+691737r3RFP5hPwj2f86Ogcz1vlfs8T2BgBWbj6i3pPH69s7zjpSkVLWzRxy1B2xuVI0pMpEqveEpOiNPTwlZB9tufL32/wCY4N0hq+2yUivYB+OKvEeXiJ8SH1qCaMeos93/AGw2z3V5QuthuyI90jrPt915xTgGlcGsUnwyDzU1FHVSPnwb+2DvHqzeu6OuOwcBX7W3rsrN5Dbu5sBkkVKvGZbG1DwVMDNG0kFRCzLrimid4J4mWSJ3jdWPSDbdxsd3srbc9tuVmsJ41kilTgysKg5oR8waEHBAI643b3s26cvbtf7Jvdi9tu1rIYZ4JKakdeIqCVYeYZSVYEMpKkEv/TH/ADN3qv8A8STsf/3psV7Z33/kibz/AM8kv/VtujHkz/lcOU/+lna/9X06+nX75Sdd0+ve/de6o0/4UF/9kL7d/wDFg9g/+8j2N7yB+7Z/08G6/wClZN/1cg6xP++X/wBOgi/6W9t/xyfrSq9539cp+t33+Qn/ANkA4r/xLfZP/W/Ee8BPvFf9PHn/AOeKD/A3XWv7of8A05bav+e67/6u9XR+4K6yd697917r5me7d3bsG7dzAbn3CANxZkADNZIAAZOpsAPueAPfWSxsbL6Kz/xOL+yT8C/wj5dcDt73veRvO7gbvdU+ql/0V/42/pdMv9792f8APUbi/wDP3kv/AKp9qvobL/lDi/3hf83RX++t5/6O11/zlf8A6C6z/wB7t1/89PuH/wA/WS/+qffvobL/AJQ4v94X/N0n/fe8nju91/zlk/6C6ypu7dhHO59w/X/ndZL/AA/6affvobL/AJQ4v94X/N17997z/wBHa6/5yv8A9BdLHEbs3dHQsn96dx6KnU0sf8byeh0cGPS6fdaXVoxyD9Qfe123b2OprCEsOBKLj7MdE15zTzGkkkUPMF8kR7WVZ5QD61Aeh9Oro/5Yn8vPZXaW2878t/lU0GD+OGwBksphsbmqpsXi98S7WaWo3DndwVPolGwNuvRvBKkbA5KrSSC/jhlSWAveL3V3HZbyDkXkkNJzZdEJI8Y1ND4lAiRj/f71qD+BaHiQRl192D7u+y8ybZde7fuqscXINmGmtYLhtEU/gEtNcXBNALSLSRpJpKwYN+mtJNkXaJr++H+Ovbvx57qj2Z8XsRiK7MybA211rFg6jsQ0ytgsBhJ6vcdHR1G3dk42karjloafHQOtRTxPFIW8UlLiRfCLlr+texc08vm45xeQRfVS3BcQZ1u4EZIklYhaMXIoSCOIbpBtck3Og5D5r5I5tFt7eLA1wbOC0CG8DIEgUtMqtDbopYlFjViwQhgBToeMtV9T9F7Q3lvbJpsrq7ZdJU5be++c9HQ4nbOJlymTqPuMvuLNy0VPTLkc7ma+YeSZxLV1tTIqjySuoIagTe+ZL6w26E3F7uDBbe2iq0jaVFEjQEmiKowBRVA8gOhfdTcucobVum7XRtNu2eMyXt5OQkMYZiXlmkICgu7GrMaszHNSetc35j/z6MqJq/ZHw621Bj4WWaCXuXf+KSqyLKV0pV7L2FWhqGiZJV1R1OcWrEkZKvjo2s3vK7kX7tESLFuPP10WfDDb7V6Lx4TTLk1HERFaHIkPDrn17r/fiaZbraPZ2yAjyjb1fRVOVPda2z0AZWIIe4VgaFTAQQ3Wvr2P2v3T8it6DcPZW8979r70yEksdG+XrchnqyJZmEj0GBxMQemxVACgK0lDBDAgX0oAPeTmzbLy/wAq2JttpsLey29BVtAVBj8Tscsf6TEn59YMcw81c7e429Jd8w7vfbrvMjERK5aQiuSkMSjTGuK6I1VccOhp67+AvzR7UFHJsv40dt1VHkOaHLZzalbszA1aaihlg3DvQbfwckAcFTIKjQGBF7g+yTdfc72+2XWNw5vsQ6/EkUglcfakOt6/KnQs2H2E95eZgP3T7cbpob4ZLmI2qH5iS6MKEfMGnR5evv5Ffzo3KIJ9wt1N1ajxrLUQbs39Llq6IeVEenWHr7Cb0x89WI2LgGpWEhbeUGwMd7l95P24siy2hvrwg0BghCqccf13hYCv9Gvy6l7Z/uOe8u7RQSbo2z7eGoXjurlpJEBIqP8AFoZ4y4FSAJNJ4ahx6PDsX/hPpWKkc/ZXyehZtTrLitldYs11tEUlTcOb3fENROtShxf0Ctr5KiPtx+9VxTaOTvskubj7ceGkX2Z1/l1LGz/3eNgJVl5h9y5Whoaw2NoENcUImlnkxxqPC9DXy6NPtf8AkQ/ETDqkm4t5d37uqQ6NIlRufamGxrLHLr0R0uJ2VDkIxKnocmsc25TQefYLvvvN8/XBItLDbbdPLTHI7fmXlK48u0fOvUn7R9wv2V28ltxvt7v2NO2e5ijQUOaCC3ifuGDVj8qHoW6D+TH8C6SOJKjr7eGUaN9bzV/Ze8Y5J116vFKMZksdEEC+n0KjW/N+fZFL94f3RkJK7tboD5Lbw4/3pWPQti+5X93eNVV+TriQg8Xvr2p+3TOo/YOn3Jfye/5f1d4PtemcrhfD5Nf8M7S7Ul+51+PR5/4xvLLafDoOnx+O+s6tXpsnh+8D7rRatXMaSV/jtrXH2aYV4/OvSmX7mX3cpNOjkF46cdF/uJr9uq7bh8qdA7vL+Rr8P89Syja2d7e2HX6f8nlx+6sTnscJPIzXrKDce3chWVEYjfSFiq6c+lSWPq1CHbfvM+4VpJW9t7C6iPEPEyN+TRyKAftU/ZwoDd/+4b7HbrFTa23fbJwahra5EgPHDLcxzkjP4SpwM8a1n/If+SB351xRV+4uk91YbvDB0aS1D7fNGdn9hLAkaSFaHE1VbkcDnXiAcERZCGplIXxUzM+hZo5R+8xyvu8kdpzNYSbbdMQPGB8WCvDuYBZE8uKsBmrClTiv7lfcF575eiuNy9vN8h3yxQM30cyi2uwBSgSrNBMeNe+I4GlGJoKXMjisng8jX4bNY6vw+YxdZUUGTxWUo6jH5LHV9JIYaqir6GrjhqqOrppkKSRyKrowIIBHvJOC4guoIrm1mSS2kUOkkZDKynIKsCQQRwIx1gRuNje7Ze3O37lZy29/C5jmgnRo5I3U0ZXRgGVgcEEAjz6h+3ekXWSP8/7D/iffum5PLrJ79031mT9I/wBj/vZ9+691zH1H+uP979+6YPE/b1H+0Gq2kafvPNe39jw6tP8AwXy8f09+6V/UnTxOrwtH56v83VX3sE/j/PrOTrkn6h/sf96Pu5+Dqr/CepKfX/Yf8SPe0+EdM9XXfyB+nKftX+YpsrPV9KtXjOk9h767bqYZdIgNdTUtDsPb0jElS09BuHflLWQqp1eSlDEFFf3DvvvvDbV7e30CNSW9nitARxoSZX/akRU/I+tOsgPu0bGm7+6VldyE6NvtZr2mKE0ECg1Hk04YUoaqPKo639/eBfXSjr3v3Xutar/hRn8vMt1v1B178Udl5WfH5nvBqzdvZc1G8kNSvWO2K6GlxOAklUoRSby3YrtL4yS0GGlhk/anKvkj93flKLcd23Dmu8iDQ2VIbYNkeM4qz/bHHw+bgjIxiZ96znqfZuXNs5M2+dkudzLS3TIaEW0RHYSCCBNIRXyKo6nDUOmJ7zKPwD7eufXWcfQf6w/3r35uC9NyeXWWP8/7D/ifbvTfWZP1D/Y/70ffuqv8J6sE2z/M7+Z+x/jVtz4q7D7cyWxutttS5yOkyu1kfG9hzYXN1smRbbH9+vuJs1isBjKyomaljxrUMyxztC8skAjjQAXXthyXfcy3PNd/tCz7nKFqkvdDqUU1+FTSzsAKltQxUAGpMp2fvb7i7ZybZcj7XvjW21Qa1WaGouSjkt4XjliyIhJ0eHoYDt1aQB0QmsrKvIVdTX19VUV1dWzy1VZWVk8tTV1dVUSNLPU1NRMzzTzzSsWd2JZmJJJPseoiRoscahUUAKoFAAMAADgB1FMssk0sk00jPM7F3diSzMxqWJOSSTUk5J6xx/n/AGH/ABPtxPiHTEnl1tu/8Jkf+PU+Yf8A4cPSX/ut7Q94kfeh/wBzOTf+aVz/AMeg6zy+5j/yTef/APmvaf8AHJ+tpf3ip1m11737r3XzlP5on/bwj5bf+Jj3F/0LS++lHtV/07rk/wD54k/y9chPfr/p7/Pn/Pb/ANY06IiPoP8AWH+9e5A6hs8T9vX1WffJfru/1737r3Xvfuvde9+691737r3WvP8AzxP5dH+mrZNV8uOn8FLU9t9b4OOHs7AYqn1VG/8ArbDxSv8Ax+Knis1XurYNLdiQpmrMOrRamajpIWyU9gvc0bFfrybvdwBs11JW0lc4hnb8BPlHMfyV841MesO/vUeyv9bdpf3B5asmfmixiC3kMfG5tUqSwX8U1uCSKdzx1TuKxr1qWdMf8zd6r/8AEk7H/wDemxXvMfff+SJvP/PJL/1bbrnhyZ/yuHKf/Sztf+r6dfTr98pOu6fXvfuvdUaf8KC/+yF9u/8Aiwewf/eR7G95A/ds/wCng3X/AErJv+rkHWJ/3y/+nQRf9Le2/wCOT9aVXvO/rlP1u+/yE/8AsgHFf+Jb7J/634j3gJ94r/p48/8AzxQf4G661/dD/wCnLbV/z3Xf/V3q6P3BXWTvXvfuvdahmc/4TzfKLJ5zMZOHufoNIchlchXxJLWdhiVIqusmqI0kCbEdBIqSAGxIv+febdv95zlCG3ghbYdy1KiqaCHyAH+/uuaG4/ci57vNwvruPm/aAkszyKCLioDMWANIjnPTf/0DtfKb/n9PQH/nZ2L/APYH7e/4KDk//owbn+yD/rd0i/4Bnn//AKbDZ/8As5/609J7ef8AIE+Tmytn7r3lXdwdEVdFtLbWd3NWUtJW9gfdVNLgcXVZWop6bzbFjh+4mhpCqa2VdRFyBz7V2H3leUb++s7FNj3JXmlSIMRDQF2Cgn9bgK9Fu5/ci5/27br/AHD+tmzuIIHm0VuRq0KWpXwDStKVoadUVwIZGSMfV5Ao/wANRAv/ALC/vIzrCqRwiO54AV6ETF0FRX1dHjKCLy1VbUUtBRwa44/LUVEq09PF5JWjij1yOBdmVRe5IHvzSxwRTTytSJFLscmgAJJoM8OiCC1udxvbSytY9d5PKsUa1A1O7BVFWIAqxGSQB5nrfQzuJ7F+P+2fiX8demeicN2l1LWtierO48tkZY4sNsPYGKoNv4vJ7mrqOoknfMVecjrK+reOenqI6yaF1neNpg55mW0+1c0XnPHNXMHMklnvg13tgiCrzzszssYIoECUUVBGkEaQaU670XVtvfI23+2fIvJfJMe4cr1j2zcZZJQkdnZxRohlYPreZ3GohdLa2B1utdXR18bjcdhsdQYjEUFFisTiqKlxuLxeNpYKHHY3HUMEdLRUFBRUscVNR0VHTRLHFFGqpGihVAAA9x9LLLPLJPPIzzOxd3ckszE1JJOSScknJPUrQww28MVvbxLHBGoREQBVVVFAqgUAAAoAMAdJPsbrLr7t3aldsbs/Zu3t97QyUlNPWbe3NjKbK42WooplqKOqEFSjiGrpJlDRSoVkjP6WHtdtO8brsV7FuWzbhLbX6AhZYWKsARQio8iOI4Hoq37l7YuadruNk5k2e2v9olKmS2u41ljYqwZSUcEVVgCDxBFR0XnA/wAv74SbbqIqvHfFjpCaphDeKbN7AwO53QmRZRIp3LS5YeaN1Hjf9cf0UgexTde5/uJeKUm503LSeOid0/44Vx/h6A1l7H+zu3lWtfbDYgVNRrsoHoa1r3o2QeB4jy6MptXYextiUpodkbM2ps2iZIo2o9q7dxG3qVo4ECQxmnxFHRwlIUUBRaygWHsI3u5bjuL+JuF/NPJWuqZ2c545Yk56kOw2rbNqiEG17dBbQAABLeNI1oMAUQAUA4dKv2i6X9e9+691737r3Xvfuvde9+691737r3Xvfuvde9+691rDfz4eo9h7Y310r21gaPHYnefZNDvPB7yhpIlgl3FHs0bXkw24aqKIrHLkKSHcD0c9Qy+WWJadCxESgZr/AHWt/wB1vdt5k2C6d5Nts2hlty2RGZfEDxg8QrFAwFaA6iBk9cp/7w/kzl3bt15D51sY4YeYdwFxaXiLhrhLcQtFMQDQtF4hRmpqYNGpNEUCgD3lj1zX6yR/n/Yf8T7903J5dZPfum+syfpH+x/3s+/de65j6j/XH+9+/dMHift6z+/da6qv9gn8f59Z4dck/UP9j/vR93PwdVf4T1JT6/7D/iR72nwjpnrZ9/4TF4Snn7z+UG428f3eK6n2dhILwRtL9vuDeFRX1WipJ8sMfl2zDqjHpkOknlF941/eWmZdi5Ztx8DXcjnPmsdBj/bn/UeswfuiW6NvPOl0QPES1gjBpmjvITniBWMVHnj063KPeHvWc/XvfuvdaDv/AAoC3ZktxfzId9YeunqJaXYXWvVG08NHNMZY6bG1m1498ywUqEAU9O2X3pVyFBe8sjv/AGveePsHaR2/tzYTRqA09zPK9BxIkMVT6nTGB9gA65o/ejvpLv3WuoHrptbG3gSvoVabHoNUp/PqlH3NR+Afb1jr1nH0H+sP969+bgvTcnl1lj/P+w/4n27031mT9Q/2P+9H37qr/Ces3v3TPXvfuvdZI/z/ALD/AIn3ZPiHTcnl1tu/8Jkf+PU+Yf8A4cPSX/ut7Q94kfeh/wBzOTf+aVz/AMeg6zy+5j/yTef/APmvaf8AHJ+tpf3ip1m11737r3XzlP5on/bwj5bf+Jj3F/0LS++lHtV/07rk/wD54k/y9chPfr/p7/Pn/Pb/ANY06IiPoP8AWH+9e5A6hs8T9vX1WffJfru/1737r3Vcn80/5A9hfF34m5DvHrDILRbr2P2d1PWJTVGp8ZnsRU70x1HntsZuBSDUYbcOInmpZwpWWNZPJE0cyRyJJntLy7tvNfOEew7tFqs57S4Wo+JGETFJFPkyMAw8sUIIJBiH3y5t3bkX28vuatkl039pd2bhTQrIhuolkieoPZLGWQkdwBqpDAEGW+LPyV67+W/SGy+8us6p2wW6qMpkcPVSRvltp7mogkWf2nnEisqZPC1pKFgAlRC0c8d4pY2IX5t5X3Lk7fr7YN0UePC3a6/DIhyki/0WH5g1U5B6GHI3Omze4HK+181bFITZXKVMb01xSLiSKQCoDxtUGlQcMpKkEmF9hvoXde9+691ppfzM/wCXSfip8r+rO8OqME1P8fu3e49nyHH4+m04/rDsGt3LQ19ftMRwosFDtvPCOaswyjSkKpPSBVWniMmcPtX7m/1w5N3nYN4ua8yWVjL3MczwiMgSfN0wsnmahs6jTmz71eyg5B9zeVObuW7HTyduO72xeOP4bW5adGaOn4YZctEB2qQ0Y0gIDuW+8Huuk3XvfuvdUaf8KC/+yF9u/wDiwewf/eR7G95A/ds/6eDdf9Kyb/q5B1if98v/AKdBF/0t7b/jk/WlV7zv65T9bvv8hP8A7IBxX/iW+yf+t+I94CfeK/6ePP8A88UH+Buutf3Q/wDpy21f8913/wBXero/cFdZO9e9+691737r3XvfuvdBN33/AMyL7p/8RN2N/wC8fmfZzy5/ysOxf89sH/V1eiTmX/lXOYP+eGf/AKtN182/ERa59Z+kXP8AyE3pX/eL/wC299YQK1+zr57L+TTCEHFj/IdLSiqZ6OpgrKWV6eqpZ4ammniYrJDPBIJYZY2HKvHIoIP4I968NJY5YpFBjYaWB4EHBH5joniuJ7S4tru2lKXMTiSN14qykFWHzBFet+LIVXZ/yQ2V8Se8+ju4qHrfaEuS2h2l2dhaihlr8RvvrzNYClyOb2hUopgrKfI0FWGplEtRTx07SSyS6pIUjbmNFHs/Ke488ct8ybA13fhJbKzkVgrQzo5VJQcgqRnANcAUBr13zln37n3aPbPnHkjmxLDZ5JbfdL6OSLxEu7KWHW0BBKPG9WFG1LoNSytTSTL9e9o9cds4eq3D1lvna2/cJRZXI4Osym1M3QZujpMviqqSkr8fUy0E8ywVMMsRIVreSNlkTVG6MwR3TZt22SdLXd9umtrhkWRUnRkJVgCrAMBUEH/Icg9DzZeYNj5jtZL7YN3tr2zSV4WltZEkUSRsVdCUJAZWBBHS89lvRv1iknhieCOWaKN6mUwUySSIj1EywzVLQwKxBllWnp5JCq3IRGb6AkWCswYqpIAqaeQqBU+mSB+fWiygqCwBJoK+ZoTQfkCeguwXePUu7N07/wBi7O39treW+OrYPLv3Z+08pS5/cO2pi9ZCuOyWOx0s8kGXNXQSwNSMRPHOvjdVYgezi55d3uys9s3G/wBsmt9uvDS2nnUokgwdSs1KrQg6uBGQSOg/Y82ctbpuO9bPtW+W11u+3U+utbaRZJYCdQCyIhJRyVI0mhqKU6KJS/zFNgdhfELuL5Z/H7ZG5uz8f1Hla/CVWxs9JHsjNZatxEu2KnL1CT0lNvGajx9Ltvcy5KJmpnlnjhaMpExLKOn9qtz2rnrYeSOadxhspb5FkW5jHjIoYSBRQmIFjJHoPdQE1qfOKovffYuYPazmz3P5A2qfdYNqeSJrKUm2kkaLwmkodEzKBDKJF7CWA00BOEj2v3v82uyfiv8AHPun4i9T0H+kjsTKben7N6v3bT4ukye3cJV4vJT5p6DJ78yW0cdQUdDn8L9mtTUxtJNTZCKZIgAXVdsnLXt3tPOnNXL3PW+N+6LVHFnewFiruGUJVYVlZiUfVQGgKlSfIl3NfOnvFvHtnyJzf7V8mxyczX0kEm47VfFY3hiaJ3lVZLl7ZVKSoI9TKSVcOE9B17R6r+Uue+WHSHZ/XXcmK278d9o4Ctx/a/UeQra+Co3hlqiXcMC5OhoaTamQo8hIcfmac3q8jAIJsdEYo1Znl9hzZt65MtuSOYtn3bYHl5rnlD2N+gBESgIdLEyqR3IfhQ1DmpIAHQy5g5c9yLz3O5O5i2Lm+OD2/treSPddpk4zyHxQkiUgYk0kUtqlABiTSoLM3WbbXS2W6s+TnbvyK3j8lM1kthdlbVo8Jt3pvedXUUO2Ou5cVDtibJZTA5jK7zmxDU71GHqpjDT4ih8CZBg8shVpJfXnMVvvfJuwcp7fyhGm6WczSTbhbgGS4DmTSrosIaoDKKmRq6cAVoKbTyXufLvuVzpz9uvuJcT8v7pbQxWuy3RZYLEwpEJHhd7ho6SMjMQsMdNZqWIqQR6h6n6Z6Z2H351li/mtFk8r3wm5Z8RuHKdo7bXdvWS5vCZfDQ1ew5v71vkYZtvfxD7mkmEiPFUU6OWuCfYi37fd/wCYN05X3mb270QbX4YeFLaTwrnQ6uROPD0nxNNGFMgkdBnlvk7lrlfYufeWIPdy6lud+e5liuZr6M3NiJ42jH0LeJqjW3rqiOSrCtT0JzdefKDrT459XbQ+PPcW2+7uw9u7spshujsz5B5TN5xuwth12Uz1bX0ArcZVZmrkr6SLJUUFPKMhCfs8e1pjNJck43bkzeObd63DmzYJtu2maArBZ7SqJ4E4RArUYKApKsSNJy/Cg6OBy57lcr+33LGx8g83Qbzv9rdIbrcuZXlla6tGkkaQF4as0qq6rGxYVVO5izE9G22TvjanYGFbObO3PgN34umyFdhKrN7Yrocng5M1h5vs81SUOQppailqv4fkEeCXxyyCKZHiZvIjgAXcttvtquBbbhZS28zIsqxzKVfQ41ISpAI1LQioFQQRgjqU9p3jbN8tDe7TuUF3aiR4WmtnEkfiRMY5UDqSpMcisjAE6WBU9wIGbeu9dp9c7Tz++d85/G7X2jtfG1GXz+fy9QKagxtBTAF5ZXILvI7lUiiRXlmldY41Z2VTXbtuvt3vrXbNstXnv53EcUUYqzMeAA/wngBk0A63vG8bXy/td/ve938VrtFrE01xcTMFSNFFWZmPAD9pOBnrSZ/mDfMOr+ZHe9dvDGw1WO622hSy7U6wxFaiRVq7fiqnnqs/lI0H7WX3RWn7mSIlvtoRDT6nMJkfpT7R+3ie3fK0dhOyvvVwwnvZFyNdKCNT5rEMA+Z1N50HCD7zvvfJ73e4LbjYBk5R29GtNpjcUZkLVkuHFKh7hlB0n4UVFI1BiSK+5S6xw6yR/n/Yf8T7903J5dZPfum+syfpH+x/3s+/de65j6j/AFx/vfv3TB4n7es/v3Wuqr/YJ/H+fWeHXJP1D/Y/70fdz8HVX+E9SU+v+w/4ke9p8I6Z62Xv+Eym6VpPk58h9k+V1bcHRFFukQCKIxyLs/sHbeJaVpipmjeE75AVVYK4kJYEqtscvvKWpflnl+9oKR35irX/AH5E7cP+bX+qvWWv3SNwSPmnmvaiT4k23pcAUxSGZUNT5Gs4oPPPp1uj+8Nus8+ve/de60Xf+FFXVtbsz534zsHwP/Ce4untmZ2KuCaYXzm0JsnsXLY4PYeSposVgsbO/wBbJWR8/gZxfd63NLzkSSw1fq2d5JGV89MmmVT9hZ2H5HrnL96/Z5bH3Gs91EJFtfbdGwkxRpImeN19aqgjJxwYUPGlCPueT8A+3rGHrOPoP9Yf71783Bem5PLrLH+f9h/xPt3pvrMn6h/sf96Pv3VX+E9Zvfumeve/de6yR/n/AGH/ABPuyfEOm5PLrbd/4TI/8ep8w/8Aw4ekv/db2h7xI+9D/uZyb/zSuf8Aj0HWeX3Mf+Sbz/8A817T/jk/W0v7xU6za697917r5yn80T/t4R8tv/Ex7i/6FpffSj2q/wCndcn/APPEn+XrkJ79f9Pf58/57f8ArGnRER9B/rD/AHr3IHUNnift6+qz75L9d3+ve/de6p1/nu/9u5eyv/D46p/97jF+5p9gP+nl7X/zz3H/AFabrHn703/TleZv+a1p/wBpUPWtX/KW/mEV3wk7ujwW9a+qn+PnbVbjMN2PQtJNNDs7KGVKXD9n4ykVjpnwQl8WUSJWkq8Uz2SWenpVXKH3g9uY+e9hM9jGo5js1aS1agrItKtAx9HpVK4V6ZAZusHfu8e8cntfzSbDdpXbk7cpEju1riCSulLpVJoNANJaZaPNGaNF6306CvocrQ0WTxlbSZLG5Kkp6/HZGgqIayhr6GshSopK2iq6d5KeqpKqnkV45EZkdGDKSCD758SRyQyPFKhWVSVZWBBBBoQQcgg8R11ljkjmjSWJw0TAMrKQQQRUEEYII4HqX7p1fpFdhdd7L7W2jlNi9g7foNzbWzDUMtbisghaP7vFZCly+IyFNKjJPR5PD5eggq6SoiZJqephSRGVlB9r9s3O/wBnvYtw225aK7SoDr6MpVlPkVZSVYHBBIPRdu20bbvljLtu7Wcc9i7I5jkFRqjdZI3Ho8ciq6MMqyhgQQD0tfaDox697917qjT/AIUF/wDZC+3f/Fg9g/8AvI9je8gfu2f9PBuv+lZN/wBXIOsT/vl/9Ogi/wClvbf8cn60qved/XKfrd9/kJ/9kA4r/wAS32T/ANb8R7wE+8V/08ef/nig/wADdda/uh/9OW2r/nuu/wDq71dH7grrJ3r3v3Xuka3YvXyMytvrZqspKsrbnwgZWBsVYGuBBBHI9rxte5nI26en/NN/83SI7ltwrW/h/wB7X/P11/pG69P035sz/wBCjCf/AFd79+6t0/6Ntx/zjf8Azda/ee2nhuEH/ORf8/QV97dgbDqOkO5IIN7bRnnn6q7Dhhhh3JhpJZpZNo5dI4oo0rWeSSR2AVQCSTYezjl7bNyXf9jZtvnCi8hJJjagHiL8uiXmXcdvPLm/gX8Nfop/xr/vpvn1867FReOnViPVK+s/8FvpUf61hf8A2Pvqqo7WPXz2X0mucqDhRT/P0+R/n/Yf8T79H59F0nl1fT/Kw/mf7Q6L2o/xk+SryHqCprMmdk71moajOUmzk3DUNLmtp7pxEUVXNU7KyVZVz1KTQwyvST1EyyxvTyhqbGX3p9mtw5kvm5x5QUfvwAfU2wIQy6B2yxsSAJVAAIJGoAEHUKNnz91j7z+zcm7TF7Z+5M5TlwOw2/cHBdIRK1Wt51AYiAsxZXoQmohqJQreJUdDdK9qfFLffTPwY7b2R03gd/5sbyG9um62n3VFi8tks5jM/kvBHgd1YytwRy8WIhxxWKpgbH0KeCKFVjWIY4rzNzDs3O227/7kbHc7hdWsf05ttwBjLKqMi11xsH06i+QdbZJzXrOGfkflbmP2t3nlL2W5otNjsNwc3MW47HolWN5JVlkaMQypp8QL4fa6lE7U06QA0/Iv4hfITs/qb4rbG63+ReT2pu3oifZku/8AfGUze9qTIdsPtfbmDxVdU5upwWSOTyFRuDKYqSsqPvZ5i7zsWZnJYucrc88sbRvfOm5bryqk1juQlFtbIkRW28SR2AQOulfDVgq6QMD06pzl7Y86b3yv7abJsXuDc225bHLave30rz+Jfi3hWNxOY5FZzO6631s1Sampz0ie+9ifGzG/OHp35tby+Y3UvU+V6h6/rdh1fXWZzeyYqnetLVwb+inllymQ3vR1kcr4vf00YghxFVUf5PG6SAhBGZcs7nzbN7db/wC3lhyJfX0N9dC5F1GspEJBhNNKwkfFCDUuoyQR6kHPHL/INl7y8oe8e++6W2bVPtlg+3/QXMlun1GoXND4klwhFEuX7REzGikMKdFck+d/8qb41fIDuX5JbA7A7L7K7X7jo46Le+H6/wABnMntorT/AMDmb+BJuqg2PtY1NfV4dKhp/wCKVVpZZwHjRxGBivtt70c3cs7BynuW12dpstgS1u906LJnWO/w2mkoA1KaFwFwaV6jiX3x+7J7fc7c58+bNzBe7hzXuiol7HYRzSRNoWPSITKsFqSdAJbxW7i41CpUFGl/nh9bdP4vLbX+Inwt2P1xhMlk6nNVWQz2Tx+GXM5epCxyZXPbT2JhaFq7JvDGiNPLnJ5TGqxhgiL7Ha/dz3ffpYLznr3BuLu5RBGEiVn0IOCpLM50rUnAjArniT1Ek330+WOVIr7b/az2ftbKxlc3DSTPHB4kzYaSW3tYiHYqqjWZyxApgKKk+7C/nUfPvfclSmM7G2t1nQVcjF8d15sHbkCRRM+tYKbK7vp947jpkiIADpWiUgWZ2BNx7tX3e/bHbQhm2qe8kH47qaQ/mViMSGvzWny6h7f/AL5fvpvRpZ71Z7ZGSapt9rHn5arr6lxT5MD6k9FQzny9+VvYklTNvT5Hd2Z6nc2GPquyt2xYdHZhI7QYSkytPiKdrqv+bgXgAfQD2P7DkHkjbABY8o7dGR+IW8Rb83Klj+Z6g/mX3r9295kDbh7lb2zMdRRLyeOP8o43SMfko4dAzWV1bkqt63I1lVX1kxj81XW1E1VUy+NEij8s87ySyeOKNVW5NlUAcD2KooYoI1igiVIhwVAABU1NAMceomvb283CeW8v7uWe7emuWZmd2oAoqzEsaKABU4AA6FrpXoftn5D71otgdP7Ky+8txVbwmdKCIR43D0ksoiOU3BmKgxYzB4qJj6p6mWNOLC7EKSTmTmjYeUtuk3XmDcY7e0WtNWWcj8MaDudj6AH546FPIHtvzn7n75Fy/wAlbHLeXxK+KyikUKsaeJPKaJEgock1NCFDHHW3T8Lfjj2H8MujNvdYbJih7t3nvHtWI9w5aXe1TtLrvqqm+0oV3SNtpU09bmclPi8VTmmhbH0Pmr8u4epamjjEceBHuLzftXuHzNd73uJO27fb2RFhGIRLPcmp8LxKFUUM5qdbUSPC6yans97I+2G++yPt9tPKO0yDe93udz17rM9w0FrZq+nx/AVhJIRFGulAiVlnOpzEpOiZvj5PfCf+WT1dD09t3Lmtr9v1O4cjgendp5c7t3mmQ3HmMpnpos9XVtZLHtrHLX1rRrJk50mSlVRFHUMultbXyX7ke9O9tv8AdW9I5RGku4Tr4UOmNFjGgADxG0itEBqa1K9N8x+6Xsb91vlSHlG3vVRrcyy2ux2bm4utU8ss51B3JhjMjNRpWVQKKtaAda0XzJ+fvdvzLzipu2rTaXWmMrFrNs9VbfqpZMBjZ40eKLJ5queKmq907g8UjD7qoRIotTCmgp1d1bM/269qOWvbq2LWKG43p10zX8oAdgaHSi1IiT5CpP4magpyq98fvJc9+9954G5OLDlCNg9vs9s5aMMtaSTSaUa4lzgsFRcaEU6ixH0+n+x/4ge5Q6x0fj1z9+6p1kj/AD/sP+J9+6bk8usnv3TfWZP0j/Y/72ffuvdcx9R/rj/e/fumDxP29Z/futdViQYqSoRZIqiBlb/g9wf6MNFwR7BgSrVr59ZwS7gsLlJIWB/LqSuBqBY+aH/W9f5H/BfdyjafKnTLbrDpP6bfy/z9Z1wsw5M0V/6AOf8AebD35F8gemTusXlE1Py6s5/k99wQfHr+YN0FurNZGno9r7xzWQ6l3PLPVfYUsdD2XjZ9tYerrKyX/JqehxW76rGVs7SjxCKma7JxIkb+72wSb97fcwW8KarmGMXcQAqSYWDsAOJLRhgKZqfPh1MvsBzpBy/7qcsvOfDtLx22+VmOP110x1PkPH8MmuKenEfRS987+uq/XvfuvdVG/wA5H4GZD5v/ABkjfYVGKru/pKuym9+sqRURp90UNdRQU29evYJZZoo6afdNDjqWppWIPkyWMpYWKRyyOst+znPcfJXMxXcJNOx3wWC6Y8IyCTHMQOOgsQfRXY5IA6g7379s5Pcbk4/uyENzNtxe5sR2gyVUCW31N8ImCqRkDxEj1ELXrQGqtrZGgq6rH16SUNfQ1E9JW0VZTT01XR1dNK0FTS1VNMqTU9TTzIUdHUMjAggEe+gCFJYkeOQNGwDKy5BByCCMEEdcqJ75raaa2ubSSO4jYpJG40srKaMrKaEMCKEHIOD1xGDlAA88f0/1Le3PDLgAHh0w25xtT9Jv5dc0wkoNvPHyR/Zb3cKW4dM/vWP/AH037R1Mp9vVc88UEDeeeaRIoYYopJJZZZCEjijjQM7ySOQFUAkk2HvzLpUszAKBUk8AOtruPjMkMVs7SswVVXJJJoAAMkk8B1s3de/8Jy8zvv4r7E3bm+18x1d8pM7jKvcWf2VujEU2V66xVNkpzPtvaGUTHU1Luvb24qHEGNsrViTIpDWSPTpRkQ+WXFzcvvHW9hzXfWUG0pdcqxuIo7iFiszECjyLqJjdC1dAotVoxbNBnDs/3RZty5K22+vt+msed5o/GmtpVSS2j1VKQnQqyrIFp4ja5AHqFUgAmlj5Q/y7flZ8QMiYe6etclj9uSy+LHdh7dV9zdd5ViAUSDdOMSSlx1XJzppMgtFWkKW8On1e5v5U9wOU+dIq7HuyNdAVa2l7Jl+2NssPmupfn1jRz/7W8/8AttKx5j5clO2/hv7U+NbNw4yKKxmpoBIqMaGgIFeifR4OXn9+P8f2W/x9jdUINSeopfdI6V8I/tHW2n/wmfxz0Oz/AJeSvIjifcvTKAKCCpgxfZDEm/11ecW/1veIf3oG/wAe5OX0iuT+1of83XQL7lMguNk59uQKA3VslD/RjlNf+NdbQvvFbrN7r3v3XuvnW/zQcNLJ/ME+WUgmjAk7fz0gBVrgSRUbgH/EBvfSn2oBf255PI/5Q1H7CR1x2+8HfJbe8vP0LRkkXimo+cMZ/wAvRFBg5bD9+P6D+y39PY/OMdQudyQknwj+3r6nvvkv13x697917qn/APnpUrVf8ursuJXCEb16qe5BI43ziRbj/X9zT93/AP6eZtQ9YLj/AKtN1jp96yUQeyHNMpFQJrPH23cI60WFwsnA86Xt/qW/A/1/fQPw/n1yJO5IST4R/b1tf/yKv5gE2VxNH8J+49wxSZbB0c0/x+z+Rmk82TwlJFLVZPq6eomJDVWBpo3q8MGPqoVnpQVFPSxviB94P20+mkbnzZLc+DIwG5RoMKxoFnoPJz2yf0qN+JiOiX3RvfBN3t09rOY7kLf28erZpZGq0sSgl7XP4oFGqMVzHqUACIV2aPeKXWd/Xvfuvde9+691737r3VIH8/8Ao2rfgzg1V1Qw9+7BmOoEhh/dfsCHSLfQ3mv/ALD3kB92009w518226Yf8bhP+TrE/wC+b2+zTTHhHutqxHrUSr/z91pbrhZWNvNGP+QW9556D1yW/eKeUZ63b/5D9I1H8BsPGzq5btfsiQFQQADU4tbc/m6e8AfvFf8ATybgelnB/gbrrz9z9/E9kNllAoGvbs0+yZh/k6uY9wV1lB1737r3XzEt3f8AH3bn/wDDjzX/ALs6n31usf8AcKz/AOaSf8dHXz975/yWt4/56pf+rjdMntV0V9SkQyOka/qdlUf67EAf73790lZgisx4AV6WsahAiLwqhVH+stgP94HtxfgboNMxZmY8Sa9TY/z/ALD/AIn36Pz6ak8uuS/2v+DH3Zfxfb0304UFbWY6ojrMfV1NDWQMxhqqOeWmqYSyGNjFPC6SxlkcqbEXBI9sTxRTB4po1eM8VYAg+eQcdXt7y7sLmK7sbqSG7SuiWJmR1qCDRlIIqCQaHgadTMvms5noft8znc5k4PT+1XZfIVUXobWpMVRUSREq/IuDY+2raxsoCWgtIkb1RVU/yA6MbnmXmC9Tw7/erq4i46biWSQfsdj0lXwhBvDNf6+mRbf8nLf/AHr2r0YIB6TDcaikkf5j/N1CloaqL9ULMP8AVJ6xb+p03I/2PvyqQc9PJcwOaCQV9Dj/AA9cPd+njwP2ddj6j/XH+9+/dMdLShi8NLEpFmYa2/4M/Nv9gLD/AGHv3QfupPEnc+QwPy6OZ8csD8LaRqbdXym3/wBq5OGGWSSLqnqDZsRrq1YPN4k3BvrceVw1FRxVTxr/AJPj4pHZJBesgYHTH3N937jSF7HkjaLJCQAb+/mwK0r4cKK5NPV/T4G6nD2w2n2Bt4Id792+bdynkFW/cm020gJpWgmu30L30HbERSuZRmltWO/nLfHToHZjbB+InxCqNtYOFj9k+6s3iNqpJMA+nLbipNvpvLM7oyTCys1TmPOynmoIUKYKl+7zzfzTuP705959Wa5PxeAjyn/SoZPBSNf9KlP6OestIfvwe13IOxRbB7Rez88Fih7Irl4LRBUGsjiD6t5pCaV1OGNSTJUUNfnfH81L5k99RVmMq+xV602rWCRJNrdTU0+0KeSCQaGhq9w/eV+862KSL0yRyZI073P7Qvb3LXKnsb7ecsPHOu0/W3y0InvyJTUeYjosQzw7Kj16xt9wfvge9vPqzWib+mz7S9QbbZ1MBKk41XBZ7kkDB0yKpz2+XVdxkkmklmmkeWWV2kllkZnkkkdmZ5JHYlnd2JJJJJJ9zCiqlVVQFAAAHACnAdYtTyyTTSzTSM8zsWZmJJJOSSTkknJJ49d+7Dift6a6yp9P9j/xA976afj1z9+6p1kj/P8AsP8Aiffum5PLrJ79031mT9I/2P8AvZ9+691zH1H+uP8Ae/fumDxP29Z/futdVb01VNSSCSJvyNSHlHAP0Yf8T9R7BQJD49es6poI510yD7D5jpZUVfDWINB0yKPXExGpbWFx/ql/x9qNQZPn0HLu1ktqhhVPJhw/4vqd78nHpB1KpZ56WWKppppaepp5o56eogkeKeCeJlkimhljKyRSxSKGVlIKkXHtxlV1ZWUFSKEHgR6Hq8ckkMkc0MjJKjBlZSQQQaggjIIPA9fRD/lc/NLF/Nb4sbS3fX5KCXtjYdPR7E7kxQZxVQ7sxlIqUm5fFNNNO+O3vi4kyEU1zH9y1TACWp5Lc6PdPkqXkjmu8so4yNpnJuLJ/IxscpgAVibtI9NJ8x1199mPca39yuR9u3gyL++YALbcYxjTOgFWAJJ0SrR1NTxK1qppY37jfqWOve/de6pb/mEfyY+mvmJlcr2r1tlKPpPvnIK9Rl85SYkVWx+wq3U8pqd74GhamqKXP1cjWkzNGWqXB1VEFWwTTNvt17171yZFDtO5RNfcvrhIy1JYR6ROagoP4Gx/CV6xy93vu48r+5ks297dMNs5tYDXdRpqinp/v+IFdT0x4ikPw1awoXrWt7W/kvfzDurcpNSQ9IP2ViBO8NHubq3cu39z46u0OVEiYievxm8KGNk0sGq8ZTqQ1gSVYLk9s3vd7cbpFrfffpZqAmK7R0I/2wDRn8mP+DrCjfvuv+8Oy3TQ23L0e4W34biymiKnJxolaKUGmcpTOCc0RvXP8pD+Yb2TlaTH4/407z2tBOdU+X7Fnw2wMXQQLM0Lz1R3PksfkJdDJfxU9PPUMlmWNlIPtbf+8XtxtcMksnM8MrDglsGlYn0GhSB9pIHz6KNn+7Z7y7xcQwjk+S1iY9015JFEiDOWBcyHhwVGPnSmetk7+Xd/JN68+K+ewncne+cxPb/dmGlhyG2cZjqOZetuvMmiHRksXBlIIshuzclHIddNkKuGlipHs8NKs6JUDGX3J99Nz5tt59l2CB7LYnqsrMf1pl9GKmkaHzUEk8C1MdZr+zf3Zdi9urm35i5iuk3LmtKNCQtLe2NMmJW7pJAeEjAUxpRTUm9r3APWUnULJYzG5nH1uJzGPocrislTTUWRxmSpIK7H19HUIYqikraKqjlpqqmnjYq8bqyMpsQR7cillgkSaGRklU6lZSQQRwIIyCOqSRxzRvFLGrRMCrKwBBB4gg4IPWoF/PS+M/wm+OtR1xP01stuve+OxslXZ7MbQ2dkzRdfxbApTkYKzc2Q2hUUtbT4XI5LcTRUmNjxcuOo2jpastC7RA+8zvYDmnnvmUbmu9331PL1sgjSadazeMaEIsgILKqVZi4Y5XIr1zm+9vyR7W8oW+zXHL+0LZ8430xdoLRtEH0611yvDpZFYyFVTR4eruJ1aCOjN/8ACbH/AI8n5Z/+HT1F/wC6nf8A7Cn3oP8Ako8of80Lj/j0XQ5+4/8A8qzz3/z3wf8AVputm/3ix1nH1737r3Xzzv5nn/Zf/wArP/Es5n/3GoffSv2k/wCnbcn/APPGP+PN1xk+8d/0+33A/wCetP8AqxD0RcfQf6w/3r2PjxP29Ql19Rn3yW6+gjr3v3Xuqi/54n/bvHsz/wAPLqz/AN7rEe5p+7//ANPO2j/mhcf9WX6xt+9r/wBOK5s/5rWf/aZB1o2p+of7H/ej76D9ceen7bu4c5tLP4TdW2MrXYLce28tj87gc3jKiSkyWIzGJq4q7G5KgqoislPWUVZAkkbqbq6g+2Lq1t762uLO7hWS1lRo5I3FVZWBDKR5gg06VWG5X+z39ju213TwbjbTJPBNGaMkiHUrA+oIr1vofy0/nVhPm70VRZnKVFDQ90bDioNv9ubcgEVN5cr9sBR70xFDHpEe3d3LC8saqNNJVpPTcrEjyc5vdX28uOQOYpLeJWbYrgmWylOe2uYmP8cfA+oo3njtB7D+79j7vcl2+5O8aczWoWDdLZcaZdOJUXiIZssvGh1JUlSerGPcX9Td1737r3XvfuvdUofz7v8AshzFf+J12D/7z2+fc/fdt/6eM3/Svm/49F1id99D/pyV5/0s7T/jz9aZKfX/AGH/ABI959dcgOt1v+Rf/wBkF4T/AMSl2P8A+5mO98/PvF/9PKuv+eOD/jp67G/c6/6cVsH/AD2Xn/aQ/VxXuCuso+ve/de60k9wfyNPn7kdwZvI020uuWpq7MZKtp2bsvBI7QVNbNPEWQrdWMbi4P0PvP22+8N7bRW1vE95d6lRVNIG4gAevXKLc/uee8V3uO4XUUW2eFLPJItbnNGYkV/T40PTZ/wxV/MD/wCeR64H/lTcD/xC+3/+CJ9tP+Uy7/5wP0i/4DT3m/31tf8A2Vf9c+nOg/kYfPuOoWSfavW8aorEE9lYVrsRpAskbngG/wDsPej94r20H/Eu7P8AzYb/AD9JZ/uWe9U0TRou0qT5m6P+SI9KEfyPfnkCD/dzrX6/8/Ixf/1N7sPvG+2gUj6m8/5wH/oLou/4B33s/i2b/sqf/rR03Z7+S984dr4DO7ly+3+uosVt7D5LOZKSHsLGzypj8TRT19a8UKU2uWRaanYqo5Y8D29Z/eF9ubq5gtIbi8M0rrGgMBHcxoM6sZPSW9+5L70WlrcXkz7P4MMbSvS6cnSoLGg8DJoOi7/DP4H9w/OHIdgY7qbPde4B+uaTb9bnqnsLKboxVHMu5p8vBjYMdNtrZ+7TJUk4OdnWZYPQt0L2bSL+fvczYPbeLbZd8tbuUXbyLELVY2I8MIWLCSWLHeOFfnTqKfZv2H5w975eYYuU9w263O2rC053CSeMHxzKECGG3nqR4LV1afKlc0Pov8gf5iAWPZPxp+v/AD2PaP8A9pv3GLfee5BJJ/dG8f8AOK2/7aupwb7gvvCTUcyctf8AZRe/967rl/wwT8xP+fk/Gn/0Me0f/tN+7L95/kFa12jeP+cVt/219V/4AT3i/wCml5Z/7KL7/vXdZf8Ahgz5h/8APyfjV/6GHaP/ANpz3b/goeQP+jRvH/OK2/7a+vf8AJ7xf9NLyz/2UX3/AHruvf8ADBnzD/5+T8av/Qw7R/8AtOe/f8FDyB/0aN4/5xW3/bX02fuA+8ZJP9ZeWf8Asovv+9d1jf8AkDfL2Q/udifGd/8AE7v7Q1W/wb/Q5ce/f8FDyB/0aN4/5xW3/bX1dPuDe9Efwc0ctAen1N9/g/d3UU/8J+vlzrVl7K+NyAMCV/vj2gykAgleenNQv/rn37/goeQP+jRvH/OK2/7a+nx9w33oCkHmTlgmmD9RfD/vHdPH/DCfzA/5+P8AGz/0MO0P/tO+/f8ABQ8gf9GjeP8AnFbf9tfRf/yb995f+mm5Z/7KL7/vXddj+Qn8wAQf9JHxs+v/AD2HaH/2nffv+Ch5A/6NG8f84rb/ALa+tH+7995SCP6zcsf9lF9/3rusn/DC3y//AOfj/G3/ANC/s/8A+0979/wUPIH/AEaN4/5xW3/bX03/AMm+veb/AKablj/sovv+9d1kH8hn5fAAf6R/jd9P+ev7P/8AtPe7L96LkAGp2feP+cVt/wBtfXv+TfXvN/003LH/AGUX3/eu6yL/ACG/l6t79jfG7m3/ADF/Z3/2n/dh96P2/qT+594/5xW3/bX02393v7zkk/1m5Y/7Kb7/AL13VS3bvWWe6X7P331PuirxFfuLr3c+V2pmq3AVFbVYWqyOHqXpambF1ORoMVXTUTyITG0tNA5X6op49z1y7vlpzLsm27/YxyJZ3cKzxrKAHCsKgMFZlB+xiPn1h7z1yduft9zdv/Je8zwS7pt1wbaeS1Z2iZgASUZ0jcrnzRT8ulTt/wCN3yJ3Pipc3troTuncOGhp1rJsvg+rd85bGRUbxySpVS19Bgqiljpnihdg5cKVQm9gfaS55z5PsphbXnNm2RXBOkRy3UCtXhTSzg1qeHRhbe0nuruMAvNv9suYZ7TSH8WHbrx00mpDalhK0IFa1p0GOd29uDa2Smw+5sHmNu5ensajFZ3GVuIyUF2ZR5qHIQU9TFdkI9SjkH+ns8tLyzv4VubG7imtzwkiZXU/YykjoHbtsu8bBeNt++7Tc2V+BqMF3E8MgBJAJSRVahIPl5Hprj/P+w/4n2p6KJPLrJ79031mT9I/2P8AvZ9+691zH1H+uP8Ae/fumDxP29Z/futdVX+wT+P8+s8OskLvHIroxR1NwymxHB93OEBHTcqq8bK61U+R6VtBk1qLRTWSb8N9Ek/pb/Uv/h+fx/T27GwNCePQcu7BoqyRVMfmPMf5x0+J9P8AY/8AED290XdHb+BvzZ7G+C3d+M7S2WXy+2skKfCdmbEnqJYsbvbaDVCyVFKwWRIqfPYrU8+Mq2DfbVPDB4ZJo5ARz9yPtvPmxS7Ve9l0lZLWcDMclMH5o3Bh5j5gESd7T+6O7e1XNMW8WYMu1zBYr+1riWIGtVyAJY6kxk8CSDhj19BD45fJXpz5W9X4XtvpPdlNujauWUQ1cDJ9nnts5mONGrtt7qw0rGpw2dxrvpkjbVFKumaCSankimfnpzJyzvPKe6T7RvlmYrtDg8VdfJ0bgynyPEcCAQQOs3KfN3L/ADvslrzBy1uC3G2yjBGGRh8SSIe5HU8QftFQQSPHsh6EnXvfuvde9+691737r3Xvfuvde9+690Vr5ffLrqb4X9O5rtvtPJpeJJ6HZuzqSpij3F2Bus07y0G2sBCyysGmZQ1VVsjQUFNqml4UKws5M5N3jnjeoNm2iLjRp5iOyGOuXc/LyHFjgdAf3C9weXfbTlu75k5iudMKdkECkeJPKQSsMS+bNTJ4KtWYhQT18+P5H/IXsP5Tdz747v7OrxV7m3lkvOlFA8v8L27haVBS4PbGCglZjTYbBY6NIIl/XIQ0shaaSR26Ocr8t7bylsdhsO1R0tYFoWPxO5y8jnzZzk+nAYAHXG73A533n3E5o3XmvfJP8auH7IgSUhiXEcMdeCIvyGpiznuYnrZS/wCE2P8Ax5Pyz/8ADp6i/wDdTv8A94vfeg/5KPKH/NC4/wCPRdZzfcf/AOVZ57/574P+rTdbN/vFjrOPr3v3XuvnnfzPP+y//lZ/4lnM/wDuNQ++lftJ/wBO25P/AOeMf8ebrjJ947/p9vuB/wA9af8AViHoi4+g/wBYf717Hx4n7eoS6+oz75LdfQR1737r3VRf88T/ALd49mf+Hl1Z/wC91iPc0/d//wCnnbR/zQuP+rL9Y2/e1/6cVzZ/zWs/+0yDrRtT9Q/2P+9H30H6489ZvfuqPw/Po03w4+Vm+/hz3rtXuPZMklXS0UoxW9drNMYqHemyq6aL+N7frL3SOd44xNRzkE0tbDFLZgrKwO565N27nnl282O/AWRhrt5vOKUfC4+Xkw81JHoepL9pPc/ePafnPb+ZttZnsqiK/tQe2e3YjWmcB1+KNvwuBXtLA/QN6a7f2F331js3t7rLMx57ZO+cPDmMNXBVjqIgzPBW4zJ0weQ0OZw1fDLSVlOzFoKqF4ySVv75rb5sm48ubtfbJu1uY9wt5DHIvl8mU+asKFT5gg9ds+WeZNm5v2Ha+ZeX7xZ9ovIRNBIMYPFWByroaqynKsCpyOhN9lPR71737r3VKH8+7/shzFf+J12D/wC89vn3P33bf+njN/0r5v8Aj0XWJ330P+nJXn/SztP+PP1pkp9f9h/xI959dcgOt1v+Rf8A9kF4T/xKXY//ALmY73z8+8X/ANPKuv8Anjg/46euxv3Ov+nFbB/z2Xn/AGkP1cV7grrKPr3v3Xuve/de697917r3v3Xuve/de6DHuz/mTPbn/iMd+/8AvK5b2b8v/wDJe2T/AJ7If+ri9E/MP/JA3z/njm/6tt1ruf8ACfQlcN82GUlWXHdHlWBIIIpe8iCCOQQfeVv3pBWf29B4eJe/4bPrnN9wAkWfvSQaERbZ/wAd3PrYF2NUOM/CjPIwlpqlLFyQCI/Lcgnn/N/7f3i1uKL9NUACjA/5P8vWfmxSt9eqsxIKEcfz/wAnQ2eyDoa9e9+691737r3XvfuvdcBJGZGiEiGVEjkeIMpkSOVpFikZL6lSRoXCkixKm30PvdDQNQ6SaA/Zx/w9aqKla540/wBX2dc/eut9e9+691737r3Xvfuvde9+690V3Z/w1+Ouze1d9d203XOGzvaPYG5a3dOV3duqko89XYqurpI5pIdrQVVKKDbkKSR38tNElZKSxmnkJJ9jW/8AcLm3cNj2zlp93lj2O0hEMdvASisBXMhBrIc8GOkeQHUa7R7Q+3ezc277z3b8s28nN24zmee/uFWSRWIVaQlgRCtFFdABY5YsST0279+UnxB2PvWq697B756825vahmjpcjh83vt4anCVNRGsyU+XqJq6TG4KfxSK5jqnhKIyllCkXd2vkXn/AHTbY922nlW8m21xqSWKCocDFVoupxUUqoPn0g5g90/Z3l/ep+X+ZPcXabPfYyBLb3V8iPEWAYCQPJSMlSDRqYINKEdY+7/jv1D8idgrQb5wWD7X2VX441WIy71FLV5/Cw1EDeDP7F3rjg9Xj3RJTIj00hp5BxLFPEWU+5a5t5g5P3Xx9qu5bDcUekkYBCPQ5jmhbDDHmK+hUgHr3Pftzyj7i8vNt/Mu12+8bDImuMy0aWOqkCa1uF742AY0ZCMHIYEjrUD+Z/xK3H8Re15No1NZUbg2JuWmmz/Wm8ZqdYHzu31n8M9Bk44h9tT7m25UOtNkIozoLlJkAinjHvoX7a+4Fn7g7D9ekYh3WBhFe24NdElKhlrkxyDKE54qcqeuJH3gfZPcfZTnBNqNw91yxeq1xtN64AaSIEB4pQKKLiAsFk09rVVwFDhVKH7kPqB+syfpH+x/3s+/de65j6j/AFx/vfv3TB4n7es/v3Wuqr/YJ/H+fWeHXJP1D/Y/70fdz8HVX+E9SU+v+w/4ke9p8I6Z6UFBlTHaKpJaPgLL9WT/AIP+WX/H6j/H26r0weHRVd7eHrJAKN5r6/Z0qYmDIGUhlbkEG4IIBBBH1B9u9EEgIahFD6HozPxe+XPfXw73+nYnRO9qvbWRnSOmz+Bq0OT2dvHHR+TTjN2bankWhy9PEJnMEvoq6R3MlNNDJ6/YY5q5P5f5z287dv1iJYxmORe2SM+sbjKn1HA8GBHQ25C9x+bfbbdTuvK24mMsKT28lXgmA4CWOoDU8mBDrnSwqa7avxJ/n8fGLuGixe3fkPS1Px27DdIaapylWlduDqrL1niAkqaDcdFTT5TbEdRKjN4crTrT0ysqmumN294i83fd95p2Z5bnl1huW3DIVaJOorwKE6Xp6oan+EddA+QPvV8g8zxwWnNDHZt4OG8clrZjQklZwOwY/wBFCAVADMerxNm762R2NgqfdHXu8dq772zVuyUu4tm7hxG6MFUuqRyMlPl8JWV2PmdY5kYhZCQrA/Qj3Bd7YX22zta7jZywXQ4xzIyMPtVgCOHp1kxY39judtHebbew3Fm4qksDrIjDjhlJU49D0qvaTpX1737r3TbmMzh9vYytzefyuNweGxkDVWRy+YrqXGYzH0yW11NbX1ssFJSwJfl5HVR/X27DDNcSpBbxNJOxoqICzE+gAqSem5ZoreJ5p5VSFRVncgKB6kmgA6ph+YX88b4s/H6jy+2um8hT/IztSFKykpabaFbp6zweRjEsMVRuDfyJJRZmmhqAH8GEFcZ1Uo09MWWQTdyX7Dc28yPDdb1Gds2g0YtOP1mXBokPFSR5vpp6Nw6xr9yfvR+3vJEdxZbJdLvPMIBVYbNgYEbI/VuBVKAjKx629Qta9agXyc+Vfdvy87Hqezu792zbhzPikosJiKRHodrbQw7TGdcHtPBeaaHE41ZDqc6pKiof9yeWWQlzmfyryhsPJm2LtWw2YjhrqkdsySNSmqR6DUf2AcAAOubPuB7j81+5m9fvvmq/8SVQUggjBWGBCalYoyW0gniSSzUGpjQULxH+f9h/xPsTdAN/hPW2L/wmx/48n5Z/+HT1F/7qd/8AvD770H/JR5Q/5oXH/Houui/3H/8AlWee/wDnvg/6tN1s3+8WOs4+ve/de6+ed/M8/wCy/wD5Wf8AiWcz/wC41D76V+0n/TtuT/8AnjH/AB5uuMn3jv8Ap9vuB/z1p/1Yh6IuPoP9Yf717Hx4n7eoS6+oz75LdfQR1737r3VRf88T/t3j2Z/4eXVn/vdYj3NP3f8A/p520f8ANC4/6sv1jb97X/pxXNn/ADWs/wDtMg60bU/UP9j/AL0ffQfrjz1m9+6o/D8+ve/dNnj1dr/Jw/mDt8Y+zR0d2lnJIuiO2M3TR01dX1KrjutN/wBYI6Kj3IHnZY6Lb+4dMNLljqEcOiGqNhFN5IB98/bMc2bSeYtntweYrKMllUd08IyUxxdMlPM5XzFMxPuoe+J5F35eROZb1hyjuUoFvJIRotLlsBs/DFOaK+aKwV6AF2O6X7wN66t9e9+691Sh/Pu/7IcxX/iddg/+89vn3P33bf8Ap4zf9K+b/j0XWJ330P8ApyV5/wBLO0/48/WmSn1/2H/Ej3n11yA63W/5F/8A2QXhP/Epdj/+5mO98/PvF/8ATyrr/njg/wCOnrsb9zr/AKcVsH/PZef9pD9XFe4K6yj697917r3v3Xuve/de697917r3v3Xugx7s/wCZM9uf+Ix37/7yuW9m/L//ACXtk/57If8Aq4vRPzD/AMkDfP8Anjm/6tt1rXf8J+8m53j8qtrpLUA5rYGx8mKdGAppXw+U3Vj1llTXqaoh/vJpiIRrLI/IuA2XX3o4gLDku8IH6d1OtTx7libHyOjP2Drmz9wCXVd+7VgCay2lk1Bw7Wu1/b+pjHr1sSbPlWLceNZm0qz1EX+u0tJPHGp/reRh7xSvxW0lx6H+Y66A7OwXcrYk0BqP2qafz6Hv2G+h71737r3Xvfuvde9+691Rp1F83Jc9/N37j6rq8vK3W26tpw9J7KEtS6Y1t79MnI5qplpmKmknefceS3XRqUIaSSeFdRKhDklvvtwtr7D8v75HAP3xBcHcbmgGoQ3elAD5gCNYGz5VNPPrCvlP3sk3D723OXJc1x/yGriwXadvYs2h7vbTJLNoxoLeJNdRtTNY0BNRTq8v3jb1mp1737r3Xvfuvde9+691737r3TLuTcOH2jt7O7q3BWwY3BbbxGRzuZyFTIkUFFi8TSTV1dVSySskaRwU0DMSSBx9famztLi/u7aytYy9zNIsUajJLMQqgU9Sekl9fWu2WV5uN9OsVlBE000jkBVRFLMxJoAAASevnc7j3Dld3bj3DuzO1L1mb3PnctuHMVcjzSyVWVzVdPkshUvLUSzzyPPV1LsWd3ck3Zibn311sbODbrKz2+1XTbQRJDGuMKihVGABgDyA6+aHf93vOYN73fftxYNuF9cy3k7CtDJNI0jkaixoWY8ST6k9Wu/yl/mdu3pDvTafSm5NwVdX0x25nINsfwTI1ckuP2jvfOzLTbd3HgknnWDEnKZl4aPIhNMU8M4lkVpIIyIH9/Pbiw5l5Yv+ZrK0VeY9vjMxkQUaWFBWSN6CraEqyVyKUGCesx/uX++u88k8+bR7cbxubPyRvE300MMzEra3cp/ReGpoizykJIowzOHpqBrbr/Nx6Vxu9fi9vjMR0kJzPUuSw/Z21ag3E8ONrclRba3lioDGllo6nE5I1ToRZmxUFzdb+8ffYDmWXauetrt2kP024I9jOPIsFMkLGvmHWlf6bdZo/fK5Ct+ZfZ3miZIFN/s7R71ZMSQVVWEd0ooODQO50nBMaVyKjUd99BOuJHWZP0j/AGP+9n37r3XMfUf64/3v37pg8T9vWf37rXVV/sE/j/PrPDrkn6h/sf8Aej7ufg6q/wAJ6kp9f9h/xI97T4R0z1l926905UOSlozpN5ICfVGT9P6shN9J/wAPofdlbT9nRde2cdxnhJTDf5+lhBURVMYlhcMp/wBgVP5Vh9QR7eBB4dByWJ4XKSLQ9SE/UP8AY/70ffumX+E9LnZHYW/ut8sM713vjeGws2oQrmdl7lzW1sqviYtFbIYOtoaseNnJX18Em3tFfbbt+5xeBuVhDcQfwTosi5+TAjow2nf992CZ7jYt6u7K4agZ7SaSFjStKtGyk0qafb0cfbn80D+YJtaNI8Z8s+4KpY4zEp3HuCPeEhUrGt3l3bSZuWSS0Q9bEuCSb3ZiQfN7Ve3V2WMvKFmM1/TUx+v++yvUmWf3gPeSxRY4efbxlAoPGEUp8uJljck44k1/aenrJfzXv5iWXpxSVfys7HiiMgfVjE21hKm+iSK33uGwFBWaNMp9Pk06gGtqVSGbf2i9t4mLrylbE/0tbD9jOR1eX7xvvVMuh+fLgD+hFbKf2rAD0VPsfvbuzuSsNZ21292Z2ZUGQyK2+987l3UkB1M6JSw5vJVsFHDEW/bjiVI4xwoAAHsZ7Xy9sOyKE2fZbW1UCn+LxJGT9pVQST5k5Pn1G2/8684czrIOYuaNwvUZtZS6uJZEBrXCMxRQDwAAA8gOgv8AZx0E+ve/de6yR/n/AGH/ABPv3VX+E9P2Kz2cwyzJiMzlsUk7I0643I1lCszIGCNKtLNEJGQMQCb2v7Ymtba4Km4t43I4a1DU+yoPSqy3bddtV027c7iBGNWEMjoCRwJCkVI6dv7770/56/dH/n/y3/1X7Z/du3f8oEH+8L/m6W/1o5m/6aK//wCyiX/oPrMu+N66R/v790fn/mIMt/X/AKi/fv3bt3/KBB/vC/5umm5p5n1H/kR3/wD2US/9B9MNVV1VdUS1dbU1FZVztrnqqqaSoqJnsBqlmmZ5JGsALkk2HsxijSKNI40CoBhVFAPsA6Jbi5uLuaS5u53luHNWkkYsxPDLEknHr10PoP8AWH+9e6Hift6Z6uNxf8oj+Z9l8bjstQbWM1DlKGkyNFMe8tnxGWkraeOpppTHLu1JYy8MqnSwDC9iAfcHTe8/tLDNLDJNSRGKsPpH4g0P+h9Zaxfds+8fNHHKm5djKGH+7JuBFR+Lpw/4Z4/mlf8APKf+x22b/wDZf70Pe32gAzNn/njf/rX1f/gaPvI/9HH/ALqTf9BdYaz+TX/M6yVK1Fktj0mQpJCpkpa7u3ZFXTSGNxJGXgn3XJE5R1DC44Iv7di98/aSBxJDdMkg4MtpID+0JXpJefdb+8RfwvbXtzHNatTVHLuGtTQ1FVYkGhFR8+iS97/CD5XfGSEZDu3pHeGzcH51pv70Rx47cuzxUS8QQSbu2lX53bcFRUX/AG4pKpJH5AW4IEh8ue4PJvNj+FsHMEE9xSvgnVHJTz/TkCOQPMgU6hDnP2Z9zvb+A3nNfKFzb7eDQ3KFJoRmg1SwPIiVrjUVJ4ceiz4+hqcpX0OMo0ElXkaymoaWNnWNXqauZKeBGkchEDSyAEkgD8+xbNKkEUs0hpGilmPyAqf5dRvbWk1/d2lhbAG4nlSGME0BZyFWp8snq13/AIZF/mI/8+o2t/6NXrr/AOyH3DP/AAQPtl/0dp/+yeb/AKB6yaP3Ofe3/o22H/ZXH/m6JF8lPiz3P8Rt9YrrfvLb1Btvdub2nQ73x1DjtwYXckEu3clmM7gaSrauwVbXUkUsmT21VoYmcSKIwxGllJkLlPnDYudtum3Xl+4eWyjnNuzOjIdaqjkUYA00yLnh1C3uN7a80+1m92vL/N0EMe5TWq3iCGQSr4TySxgllwDqhbHpQ+fQTR713kFCjdu5gFsqgZ7KgAAAAACrsAB7Ojtm2nJ2+Cv/ADTX/N0Gm5r5pWgXmTcAKcBcTf8AQfS+6zou3+3OwdndYbF3FuLI7w35uHGbX21QVG7azG09ZmcvUpSUFPNX1uQgo6OOWeQAySuqLe5IHtDurbBse17hvG5WUK2FtEZZWESsQqipIULU/YOj3la45+5w5h2nljZOYr1t2vZhBAsl1KiljWlWL0Axx6shrv5OP8zHKwfa5XZNDk6XWsopsh3TsqtgEqXCSeGp3RJH5FDGxtcXPuLIffb2jt38S3unSSlNSWkimn2hAep/vvupfeL3KD6a/uIp7fUG8Obcda1HA6WJFRXquHu7pLsP46dp7o6b7WxVLhN/bOGF/j2Losrjs3TUv94dvYjdWL8eTxNRVY+p82FzlNI3jkbQzlGsykCXOXOYdr5q2az37Zpmk22fX4bspQnQ7RtVWAIo6Efz6xk535M3z295o3PlDmSONN6s/D8ZYnEiDxYo50o4waxyLX0NR5dBTW7q3FjaWnxeOz+aoaPyPUfaUeUrqWlVje7iCCdIgzuSSbXJHtfPaWkkniyWsbS0oWZVJp9pFek+1btvNvbNbW+7XMdkp7YUldUBJqSFDBa/l59Gq+LvxF+YPzGpN5V/QVDkd20mwanB0m55K/snDbY+yqNxRZSbFJEm5Nw4x6zzx4ecsYg4TSNRBYXAvNvOvJPI72MfMkqwvchzCFgeSoTSGroRqU1Dj1L/ALee2/ur7pQ7rccnPLcQ2bRpOZLtYqNIGKgCSRScIa0xw6MFv7+VX/Mi6y2LvTsjeOzpMbtHr7aW4977pyMPc+yq+ag25tTD1mezlbFQ0O8KitrZKXGUErrFDG8shXSiliAQ9tfvD7WbruVhtVlfB725mS3hU2soBkkYIgqYgBViBUmg8+hpvf3ePfvl/Zd337c4Cm22NrLeXDLfxsVihjaSQhVlJYhVJoMngOqyBu/dlx/v6NxfUf8AL7yX9f8AqJ9y79DZf8ocX+8L/m6x1/fm9f8AR3uv+csn/QXR1vjD8Pfmz8ppYcz05svsPL7UinmibfuYztRtTYwqad5IaiGj3RuHI47H5iroZkIngx7VdTC2kPGuoXA3NnPPt9ybWHmC+tUuyK/SxoJJiDSlY0VioIOC+kHNDjqT+RfbD3p9ykW45OtL/wCg1U/eM8zwWwoWB0TOw8UqyFWEQdkJGoCoPVk1N/JP/mGz4uXIS9pdWUdXGyqmDqe2uw2ylQCISXimo9j1WFVVMrA+SsQ3jawIKFovf7wXtSswiGxXjIf9EFrBpHHyMwfy/h8/tpMo+6F95B4TJ/rg2CuP9DO5bhqPDzFqV/415fZ0Xntj+Wb/ADI+o6Koy9bs7eG+8LRpVS1GR6v31LvaZIaQa3lXb1DkYd3SpJECy6McxsCCA3HsV7F7u+0O+OLdbu3trhiAq3sAiFT/AMMKmIUPGrDoA82fd3+89ypA93rvtytEVnd9qvpZ2AXOIWaOdyw4BI2JpSlaA11125uwMfVV2JzG4N40VbSSzUWQxuSy2bpqqmnjZoqmkraOqqElhlRgVeN1BBuCPctW1hs8yJPBZWzxsAyOiIQRxBBAoR8x1jXuHMnO1nPPYbhv26xXMZMcsM09wrKRgq6MwIPqCOrdf5EW9P7ufNDL7ZkkHg7C6e3ng4oSqnVkcNlds7up5lbh1eLH4CrW19JEhuCQpEGfeW28XXt9BeBe+13GJ6/0XSSMj82Zf2dZVfcQ3iSy93d42oy0t73ZZhooMyRTQSIa8aqnifI1yMCm0YP9w+c59X8MynNr+taOq/2Bs6x/7Y+8Mcz23zdP8I66Z/7h3/yil/krf5adGK9hbqReve/de697917oF/kZ21SdE9Eds9v1gR/9H+xNwbhoaeTTorc1TUMke38adbKt8nnJaenFz9ZfYh5T2OTmXmbYthjNDdXUcLH0UsNbY/hSp/LoJc+802/I/JXNXN9yuqLbrCa70ClXaNCyIKkCrvRR8z1qTd59tfL34lbc+M/SXaWA2Bg6vYW/sV8u9kbh29W1FVvTdWWz+f3Fk6v/AEhVhystRqqM3X19PUwPQ0QdY/EfPHCmjOnljYeQefLvnHmLZLm7kjubRthuIZ1AiiVEjVfAGkDtRVIOpiOPaSa8nvcbnf3l9mdv9seS+brLbEnsd0Tm61urGaTx7l3mnkmjvCW1DxZZpA48NEI7FDqlF3Euv97YTsrYmzOw9tTip29vna2A3dhJwyvrxe4sXS5ai1lPT5Fp6tQ4+oYEHke8BN02652jc9w2q8Qrd20zwSA4oyMVP8x1162TeLHmHZtp37a5lk229toru3kU1DRyosiEH5qw6V/tB0ade9+691737r3USvr6TF0Fbk8hOlLQY6kqa+tqpL+OmpKSF6ipnk0hm0QwxsxsCbD3eKN5pI4YlrK7BVA8yTQD8z03LLHBFJNKwWJFLMx8gBUn8h1o4fIT+Yp8rPkZg8tsbe/aOQbrnIZKtnO1sRg9s7WjyOOfIS1WNoNw1O2sVj6zMwUFP4oxDNNJAxiV2V5LyHpnyh7Qci8oXNvue37Kp3lEUePI8kmltIDNGJGIQsamoFRWgIGOuDHuf96L3b9zLTc+X9w5meLlGaWSlpBFDA0kJkZo0neJQ76UIUrq0NTuDGpJHk+n+x/4ge5S6xtfj0K3RlFksl3Z09jsMjyZiv7T6+osVHGpd5MlVbtxEFCiKstOzO1VIoAEiEn+0PqCHmqSKHljmOW4NIFsLhnP9EROT5Hy+R6G/tdFPN7me3cNqP8AGn32wWOn8RuogvmPOnmPt63M/wCYjLR0nxe74qatlRJelt9UZZ0MimeoxdXTY1Sqo5DPkaxArHhWINxa/vnH7SCR+euVETiNyt2/IOC3/GR13L+8a0UftL7lSSGgPLm4IftNvIE/42wp8+tIH3066+fLrMn6R/sf97Pv3XuuY+o/1x/vfv3TB4n7es/v3Wuqr/YJ/H+fWeHXJP1D/Y/70fdz8HVX+E9SU+v+w/4ke9p8I6Z6y+7de697900/HqXR1MtNIZImseNSnlXHPDD8j/eR72CQek00Ec6aJF+w+Y6WVBXRVYGn0SAeuMnkcclT/aW/5/H59uhgft6Dl3ayW1Qcp5N/q4Hp2T6/7D/iR7t0g6y+3I/Pr3XY+o/1x/vfv0fn0n6kp+of7H/ej7c6q/wnrN790z1737r3WSP8/wCw/wCJ9+6q/wAJ6kR/n/Yf8T790z1k9+691mT9I/2P+9n37pl/iPXL2+OA6r1nH0H+sP8AevbJ4n7evdfTm64/5l5sP/wzNr/+6Oh98pNz/wCSluH/ADXk/wCPnrv7Yf7g2X/NFP8Ajo673N2L19suopqTeO+9m7Tq6yFqmjpdzbnwmBqKqnRzE09NDlK6lknhWQFSygqG4vf3q123cb5Wey2+eZFNCYkZwD6EqDQ9autx2+yZVvb+GFmFVErqhI9RqIr1E2/2p1huzJJh9rdj7C3Ll5YpZo8Vt/eG3szkpIYF1zypQ47I1NU8UKcuwWyjk+73G07rZxGa72y4ihBoXkjdVqeGWAGeqW+67XdyCG13K3lmIrojkRjQccAk46VeZwuH3Hisjgdw4nGZ3B5ejnx+Ww2ZoKXKYrKUFVGYqmhyOOrYp6Oto6iJirxSoyOpsQR7SQTz200dxbTPHcIwZHQlWUjgQwoQR6jpVPBBdQy21zCklvIpR45AGVlOCGU1BBHEHHWkj/M5+E2C+HHy+2FJ15SNQdP9w5XH7v2Jii1TLHtbI47ceOpN27Mp6mqeWWqosLU1tLU0rM7PHR18MTFmjLvnz7T8/XPPPI26ruj6t7sY2guHx+orRsY5SBwZgCDjJUnzoOUXv37Sbf7X+73KF1sEIi5Z3e8iuLaAVpDJHPGJ4VrX9MF0ZM4D6aAKK7wHvAHrrF1pyf8AChT/ALLQ6y/8Vg2X/wC/W7q95zfdl/5UPdv+lvL/ANo9r1yr+/J/09nl7/xXYP8AtMv+qJ0+n+x/4ge8iusLn49HK/l6f9ly/FH/AMTr15/70FJ7Avuf/wBO550/6V8v/HT1MX3ev+n1+2//AEs0/wADdfQp98yeu4fWip/OP/7eR/I7/W6h/wDfD9Xe+jXsP/06jlX/AKif+0y464t/ez/8SB5//wCoH/u22fVTNdN5q2RgbqpMa2/ogI/3lrn3LDGpPUIW8fh2yDzOT+fW1P8A8Juv+PT+Wv8A4cXTn/ut7H94efek/wBzOTP+aV1/x6Dro99xX/kje4v/AD1Wn/HJ+ryPnD/2RX8vv/FXe/8A/wB9Pu33j/7ff8r7yR/0uLP/ALSI+ssvd3/p0/uf/wCK7uX/AGhzdafX8oL4M7e+Znf2Zr+yqSeu6a6XxmI3NvbEwTSU39687m6yrg2ZsyrqYWSopsTl3w9dVVrxMsslLQPAjRtOJY84fe/3CuuROWoI9pcLvt+7Q27kV8NEAMsoBwWXUoWuAWDGtKHmJ9132h2/3S5zvbrmCPxOWNojjnuoK08aWVmEELUz4beG7PQ1ITR+Ko3lsRiMTt/F47B4HF47CYTEUVNjcTh8RRU2NxeLx1HEsFHQY7H0cUNJRUVLAipHFEioiABQAPfPSeea5mluLmZpLh2Lu7kszMcksxqSSeJPXXi3t7e0ghtbWBIraNQkccahVVQKBVUABVAwAMDoGV+UvxjbOz7XX5GdENuWll8FTt1e3uvjnaefVEnhnxI3D9/DLrmQaWjBu6j8j2fnk7m4Wy3p5V3L6NsrN9NNoPHg2jSeB8+gqvuFyC+5zbInPGzneY/7S0F5bGZeHxReJrHxDiPMeo6HGnqIKuCCqpZ4amlqYY6imqaeRJoKiCZFkhngmjZo5YZY2DKykqykEG3sOsrIzI6kODQg4II4gjyI6FysrqrowKEVBGQQeBB61uP58uQ+L+MxuzMKdnYis+Vm4JaPKxbowMkWLyuC66pJpIJajfv2kZ/vHFm6inakxEFUplh8VRNHNGkZiqct/uyw85TXG4XAv5F5JiBRoZO5XnIqBDX4CgIZyuD2qQSarzv+/bd+2VttO0WVxtEEnuncFHt7mEhJYbRHOp7gqKyxyENHEj/iLuhGhgaR/gb2jF0z8xPj12FVVTUWNxfZmGxGarFZU+129vIT7K3FUSFiAYYcHuGoaQXGpAR+feRXuZsrcwcgc27XGoaV7R5I1Pm8NJkH2l4xT59YSfd95mi5R96PbrfJyRAu4rbSEUGlLtWtHY1xRVnJPyB63l99UX2udkmA9FdBDUiy2VXUGnlW/wBGYtDrP/B/fNzbZNdsF81JH+X/AC9dtt9h8K+ZxwkUN+fA/wCCv59CftitFfgsfNe7xwLSy3bU3kpf2Czm5OqRUD/6zeyi7j8O4lXyrUfYc9CjbJhPY2z1yF0n7Vxn7aV6Bz5I/Gnrb5Rde1ewew4MpRsgnqNt7v21XyYfd+zstNEIxk8DloQSFcon3FJOs1FViNBNE+hCp/ylzdu3Jm6x7ptTI3ASwTKHilUfhdT/ACYUZanSRU9Bjn7kHY/cXl+65f3tp4gynwbuzkaG4t3IxJDKuQQQKqQyPSjqwx1pz/NP4ffJz4Wbsal3buXdW6utctWPDs3tXCZTOx4DNIxkkgxuYp2rZ5Ns7ojp47zUM0joxDNTzVEYMnvP327575J9xLHXY7fbwbyi1uLGRIy6+rIdI8SMngwAP8QU4648e+HtV7x+ym5s9/zNud7ylK9LTdoZ5xG1a0jmXxCYJgPwklW/AzZAOJDNsDqf4FfFDqL5Ab53JtvAfM7ueq7l7r3JR/xrcG5sT0fsWSjXb2Px0MdBm6mNczV0+FraQikqkjllnkWGUqxUAFN13v3P5433lPa4Zbrl7bxt+3Qtojja8mqJGbuQHSDKD3LUBQWGAZr+q5e5V+777R8oe6XMt3DYc67qd43q6rcXMy7dbhZoVjIWVk1stngIwBeVlUkFhUl3nUbYPa28cTsPfm6+yuudsZ3JbZ653fvKqqanL5XZeKyNWuIqljqYaQ0VDWGWSohhWnpgqzajDG7MonrldLwbFt8+57Vb2W7zxrNd29sAEWVlGoYJqwAAJqeFKkAdYWe5tztkvOe+Wmw8zX+78t2krWm2324yGWV7eMnTQkKBGXLMgCqKNXSCT0i6Xd266KCKlotz7hpKWnQRwU1LmslTwQxj6RxQxVKRxoPwAAPZnJtu3Su0kthA0hNSzIpJ+0kVPQbt+a+aLOCK1tOZL+K2RdKRx3EyqoHAKquAAPQdWZ/BD4HfI75j5Wn3PkN373686NoKwRZjsOuymYFVuBoHZanEbAoKqoWPOV6Ohjmqz/kFE1w7PKogeGfc73M5O9voWsYdstbvmZlqlqqJSOvBp2A7B5hfibyoO7rK37v/ALH+7fvNPHvW582bxtnICPR75ricSXFPiSzVmo9ODSkGNTUd7AoNu7pjpbr7oPYeL6762xM2NwWNUS1FVkK+qy+dzuTaGGGrzm4czXSS1mUy9cIFLyMQiKFjiSOFEjXA3mDmHdOZ9zm3Xd5w9y+AqKERFqSERFACqK4H5kkkk9eOVOVNl5L2S02DYbd0solA1Su8ssjUAMksshZ5JGplmPyFAAAK3sk6EnRPfn92enUXw3+Qe8BVx0dfL13l9p4SZnRZVz2/BHsrES0iNfzVVHWZ5ahVswtCWYFFb3IHtXsh5g9w+U9uMZeH6xJ5QP8AfcP6z19AVQj88Z6h/wB/uaxyV7M+43MC3Qhuk2uaC2kxUT3C/TwFQQQWEsqkAgjGRSvWiD76jjift6+efrKn0/2P/ED3vpp+PVyP8mr4sZXtz5B03eWboJU656LqTkqesliP22b7KqKQjbeHpmeJo5W2/DVfxaoZHDwSRUgItOD7x1+8ZzzBsHKb8r20oO8boNLKOKW4P6jnOPEI8MYoQX/h6zn+4t7RXnNvuIPcm/hI5a2At4TnhLfPHSOMAqQRBHIZWIKlX8HiGNLOP51Pc9Hsr4/t1vSVoiz/AG3mMLtpaRJESpbbe1shRb13LkImDrOtPFWxYmimABWRK9kY6SymE/u28tybpzgN5kirZ7fG85Y8PEkVoYlOKVoZGHoUqM06ys+/Zz3b8u+1tzy3FdFd13uaKxjRGCv4MMiXVy4yGMYCxxPSoPjBTgnrVB957dcYesyfpH+x/wB7Pv3XuuY+o/1x/vfv3TB4n7es/v3Wuqr/AGCfx/n1nh1yT9Q/2P8AvR93PwdVf4T1JT6/7D/iR72nwjpnrL7t17r3v3TT8eskf5/2H/E+/dU6lwsyEOjFWVrqymxBsOQR79wyOmZVVu1hVSMg9KrG5VZSIqkhJbWWT6JJ9Pr+Fc/7Y/7x7eBqAT0QXdg0VZIRWPzHmP8AOOn/ANvR+fRZ12PqP9cf7379H59J+pKfqH+x/wB6Ptzqr/Ces3v3TPXvfuvdZI/z/sP+J9+6q/wnqRH+f9h/xPv3TPWT37r3WZP0j/Y/72ffumX+I9cvb44DqvWcfQf6w/3r2yeJ+3r3X05uuP8AmXmw/wDwzNr/APujoffKTc/+SluH/NeT/j567+2H+4Nl/wA0U/46OtVL/hRn/wAzz+O3/iJ9xf8AvYS+8wvuv/8AJA5o/wCeyP8A6t9c7Pv0/wDJd9vP+eS6/wCrkPWvjtaPcsu4MGmzUzkm7GylF/dtNsrXvuI5oVKNjv4IuKByRygqgpg8H7vktp5t7yXvDaLa3BvzGLLQfF8bTo007tert0041x1gxta7s+62S7Etwd58VTbC01+N4gyvheH3668NOfTr6RPx1HZa9B9Lr3Nf/SyvV2xR2NrZ2qP75DbWOG4Pv2YkNlP4j5PuypMZqfJo9Gn3y05m/dR5j307F/yRvq5fpfTwtbaKf0dNKfKlc9d4uT/36OU+WhzRp/rJ9BB9fp4fUeEvi/8AG618q8MdUm/z+vs/4F8Ndfg/iH+mnO/a6tP3H2f2e2PvvFf1+Dz/AG/ktxq0X/Huevu46/qOe6V8P93CvpWr0/Olafn1i198DwvovaStPG/rJFp9dOnup8q6a/l1sL+8aesyOtOT/hQp/wBlodZf+KwbL/8Afrd1e85vuy/8qHu3/S3l/wC0e165V/fk/wCns8vf+K7B/wBpl/1ROn0/2P8AxA95FdYXPx6OV/L0/wCy5fij/wCJ168/96Ck9gX3P/6dzzp/0r5f+OnqYvu9f9Pr9t/+lmn+BuvoU++ZPXcPrRM/nNTeD+Y38k5b2Kx9Raf+Dt0P1cq/8nH30Z9iDT2n5VP/AD0/9plx1xg+9anifeG58TyJsa/Z+7bOvVSi/qH+x/3o+5X6hRvhPW1p/wAJuv8Aj0/lr/4cXTn/ALrex/eH33pP9zOTP+aV1/x6Dror9xX/AJI3uL/z1Wn/AByfq8j5w/8AZFfy+/8AFXe//wD30+7feP8A7ff8r7yR/wBLiz/7SI+ssvd3/p0/uf8A+K7uX/aHN1R1/wAJwtw4JtqfKbaiyUkW5oNw9Y7hkhZokr63BVWN3djYJIkIWeppMZkKOQSFSyQPVpq0mZdeQf3prW5F7yfekMbQxTxA5oHDRsfkCykU9dJ40xiX9xO/sm2P3A2tdI3FLu2uH4ajG8ciJ8yFaNvs1DhqzsbdibKx3ZXX++uusxWZPHYnf2ztz7KymQwlUKHM0OO3VhK7BVtZiK0xyijydLTV7PTylG8cqq1ja3vFza9wl2nc9u3WCNHmtp47hFkGpC0bhwGHmpIoR5jrOTe9qg33Zt22S6lljtry1ltZHgYpIqyo0bNG4yjgNVWGQaEdatvbX/CfvvHBz19X0x3F172Bi43WSjxm9KTM7C3JJA6jVTo9DT7swFTVQSNbXJU0ccqAvZGtGcydj+8/y9cLHHzBsF1bTU7ntisyV9aMY3APyDEHGePXM7m77hHNVu8s3JPOlldwa6rDuKSW8gSnDxIhOjsDTisYIqcUoQR2FhP5qf8ALByo3DHsHfs3VePqoKvcu20n/wBJ/TGSx5JkqZ8iNqZLM02zJqiJChyCNjatG0K7EaUYR7lceyvvFbm1bdLZd7ZSIZiPp7pW4ADxFXxqH8HeKVpTJ6CXL9j96n7tN0t2uxXt5yfG48e1Rje2LRgFmIELO9piv6mmPuprDCimsLuLt/fPfXZ28u2+x8tJmd371y82VydQbrT0sbAQ0GJxsFytHiMPQRR0tLCvEUESrzYkzRy3sO28sbNY7HtMHh2NvGEQeZPFmY+bO1Sx8yesUOfOdN99wead35u5iuTJul5KZG/hReCRRj8McaAKo9BU1JJIIVdZNHWl6eaSF6dwEeJ2RlkQ6ywKkEMrn/ePZswBLAjHRXZRBIY3p+pXWD5g+RB4gjrfw+J3dMPyi+G3SHcwrP4huObaFDi97u0vlqk3rti+1d9NUxeSWenNbn8Q9fCJj5DRTRyElXDHmZzrsB5O595h2Hw9FoJy9uPLwpP1IaGgBojBTTGoEeVB3N9uubF9yPafk7nDxRJuD2ireFQR/jEX6N0ApJZR40bMtSeyhqQakyvXuTEdRVYmRrCpH3VMCQB54l0zootdnkhAb/ARH2E90hqqTgZHafs8v5/4eh3y9dBXltGOG71+0cR9pH+DoWPZL0LOknvnYmzezdp5zYnYG2sRu/Z+5KGXHZvb+do4q7HV9LLY2kikBMc8EirJDNGUmgmVZI2V1Vgu23cr/Z7623La7uSC/hYPHLESrKR6EeXkRwIwQR0W7xs21cw7Ze7Lvm3Q3e03MZint51Do6niGU1B+XmDkZHWtL8v+4t5df8AbvfnY+y/jZs7s74vdK9dUHwN2vuDehxNft/rPcWEoMPW5UYPBZKpys+QyOK3jmaSmaeooakzQ4+KE1MLeRVy95B5d27dti5X2jcOcJ7LnPcbtuZZobcMHuI2LBNbqFChokZgAwoXLaTivO33f585g5V5r5/5p2j2utN29rtk2yPkqG6u5IvBtJh4bzeFC/iNIBPNDE/6ZB8BU8RSGA15h9R/rj/e/eWvXMI8D0f3+Wj1L013f8vOvOue8aeoyO1cvSbhrcVglyJxmP3HunBYqbN4vBZyojVaqXE1tNQVJaCGWnkqZ0ii1lXaOSLveTfuYeW+Qd13blpgl6jRrJLp1NHE7aGdBwDAsMkEKCTSoBGQn3V+TuSOevePY+XufIjNtrwzTW1qW0xz3MKiRIpsVaMxrIxQFdbKqklSyNvH4XC4jbmJxuA2/i8fhMHhqKmxuJxGKpIKDG43H0cSwUtFQ0VKkVPS0tPCgVERQqqLAe+a1xcT3c8tzdTNJcyMXeRyWZmOSSTkknruta2ttZW8FnZ26RWkSCOOKNQqoqigVVAAVQMADA6c/bPT/Xvfuvda+P8APn7ujxmyOovj3jaoiv3Vmars7dMKABo8Ft2OrwO2IJiwJaDK5rIVsoC/R8YL/i+WP3WuWTPuu/8ANkyfpW8QsoCf9+SUeQj5qiqP9v1zr/vCOfRt/KfKPt1aTEXO43J3G7Ap/YWw0Rq1c0knk1CnnCanyOsb7zWHE/b1yb6sh+En8tnuf5c5THbhq6Cv686ThroDmOxczRNBLmaNWV6mi2DjatY5NxV0sIZBVqpx1NJ/nZGceF4d9yveblzkCCazhlS85lKnw7SNqhDwBnYV8MA/h+NhwAHd1lL7D/dT5395Lu13fcYZdq5BDqZdwmTTJOmGK2cbgeIWU0EpBiUn8ZUp1twbW2v0h8MuhVxWNOO696h6q2/UZDJ5TISmSQoh8uRzeZq0i+5zG4c7kJdTlUaWpqZVihTmOMYCX19zL7ic0m4n13fMF/MERFHmcKiDgiIooPJVFSeJ67LbRtPI/s1yEljZLDtnJez2rO7ucKi1aSWRjl5JGJZmNWdz5kgdaYXzT+UuZ+W3ee4ux54qzGbSo2kwXXm3aubXJh9qU1XUzwVFbEkklMmdz1TO9bX+IlEml8KMYYYrdHfbPkW39v8Ale02dWWTcXpLeTKKa5SACFPHRGBpSuSBqOWPXCj7wnvFee9PuDfcxaJIuX4NVttds5JKQByfEda6RNOx1yU4dsYLLGp6KX7kHqC+syfpH+x/3s+/de65j6j/AFx/vfv3TB4n7es/v3Wuqr/YJ/H+fWeHXJP1D/Y/70fdz8HVX+E9SU+v+w/4ke9p8I6Z6y+7de697900/HrJH+f9h/xPv3VOpKfT/Y/8QPfumn49c/dz8A+3qnShx+VaIJFUkvFYBZPq8fH0P5ZP95Ht1HC6a8D0VXlirEyQijniPI/5j0pkZX0srBlaxDKQQR/UEcH25H59B1lZSVYEMOIPUtP1D/Y/70fbnVH+E9Zvfumeve/de6yR/n/Yf8T791V/hPUiP8/7D/iffumesnv3XusyfpH+x/3s+/dMv8R65e3xwHVes4+g/wBYf717ZPE/b17r6c3XH/MvNh/+GZtf/wB0dD75Sbn/AMlLcP8AmvJ/x89d/bD/AHBsv+aKf8dHXe5uuuvt6VFNV7x2Js3dlXRwtTUdVubbGEz1RS07uZWgppspQ1UkELSEsVUhS3Nr+9Wu5bjYqyWW4TwoxqRE7ICfUhSKnrV1t233rK17YQzMooplRXIHoNQNOsO3usetto1hyO0+vdj7YyDKUNft7aeBwtYUKSRlDVY2gppypSVhbVazEfk+7XO67peJ4V3uVxLH/DJI7D9jEjqtttm22bmS02+CKT+KONFP7VAPShz+fwe1cLlNybmzGM2/t/CUU+SzGbzNdTY3FYvH0qGSora+vq5IaalpoYwSzuwUD2mtra4vJ4bW0geS5kYKkaAszE8AAMknp+5ubeyt5ru7nSK1jUvJJIQqqoFSzMaAADiT1pJ/zNfm3hfmT8vtiJ19UvWdP9PZih2fsLJsk8K7orq/cmPqN2b1gp5yHp6HPVVBTQ0YZI5HoaKCSRUd2RM+fajkC45G5G3RtzTTvd9E09wmP01WNhHESOLIGJbJAZiBwqeUXv17uWHuh7u8o22wyiTlnaL2K2tZxWk0kk8ZnmX/AIWxjRUxkLq4MKbwfvADrrJ1pyf8KFP+y0Osv/FYNl/+/W7q95zfdl/5UPdv+lvL/wBo9r1yr+/J/wBPZ5e/8V2D/tMv+qJ0+n+x/wCIHvIrrC5+PRyv5en/AGXL8Uf/ABOvXn/vQUnsC+5//TuedP8ApXy/8dPUxfd6/wCn1+2//SzT/A3X0KffMnruH1oefzrfLD/Mc+QaPHJGtUvUdTEzoyrNBH0Z1nT+SJmAEkX3ETpqW41xsPqCPfRX2JdT7U8rKrAkG5DU8j9XOaH8iD+zrjh96W3kT7wXPs8kbBGWxMZIIDD932ikr6gMpFR5gjiD1VIn6h/sf96PuW+oEf4T1taf8Juv+PT+Wv8A4cXTn/ut7H94ffek/wBzOTP+aV1/x6Dror9xX/kje4v/AD1Wn/HJ+ryPnD/2RX8vv/FXe/8A/wB9Pu33j/7ff8r7yR/0uLP/ALSI+ssvd3/p0/uf/wCK7uX/AGhzdaJHwn+VnYnw671wXb+wStfBT0tRht6bSqqmamxO9tn18kDZDAZF4QzQSiogiqqOoCuaWtp4pdDqrxv0X575K2zn3l+52Lcu1ifEt5wKtFKtdLr64JDDzUkYNCON3tf7q717P82WXNW0jxYD+heWbGi3EDEF0JodLKQGRvwuorVSytul/G7+aJ8PfkhisaMb2hhOt97VMEIr+ve0chQ7QzVNXtCjz0mJyeTng2/uiNZNYjagqpZXjTU8URuowK5s9nue+U5pvH2aS629SdN1ZqZUK1oCwUF4/sYD5E9dYfbz7xntP7j29qNs5ogtN4kADbduDLBOH06iqByEmoK5iZxg8M9WEU9RBVwQVVLPDU0tTDHUU1TTyJNBUQTIskM8E0bNHLDLGwZWUlWUgg29xgysjMjqQ4NCDggjiCPIjqcVZXVXRgUIqCMgg8CD1m916t1rp/zkf5eHXFN1buL5adMbVoNn7r2ZPTV3a23Nu0cVDg92bbyNZBj5t1x4mnaKkx+4cFXVMUlVJTRotZSSTSzAyRB2ys9gvdbdV3m25I5gvGnsLgFbKWUkvFIqlhHqNS0bgEAE9rUAwadYB/e++71y/uHLV/7o8pbalrzBZFZNyit1Cx3MDMFeZkFFWaCusuBV0DBgxCEanIYtqZjdmYsT/Unkn/b+8zOuaQAAAHDrY+/kC/KWmwW7uwPiNu+vVcX2GKvsLrKKqkQQHdmJxSU2+NuwhyZZZ8/tWggrooxaNFxFQf1zc4rfeX5Oe5sNs53sYz41rS1vCta+EzVhfHAJIxUnj+ovp1n79yH3Kitdy332q3aceBehtw20ORQzImm5hFTVjJCqyKoFAIpSTU9bGddTVW2M5aJmD0k6VFJI2oCenLFoi5Xx61kS6SAWBOpfeK0TpeW3d5ijD0P8/tH5dZ2TxS7XfUQ5RtSH1HlXhxGD+Y6HXH10OSoqaupzeKoiVwLglG+kkTW41xSAqf8AEew5JG0Ujxt8QNP9X29Dq3nS5hjnjPawr9nqPtB6Dnu/tHEdJdP9l9t5wxHG9ebK3DuqSCZmRa6pxWOnqMdikZPV58vkVipYgOTJMo/Ps35c2WfmLftn2K2B8a7uI4AR5BmAZvsVak/IdEXOHMllydyrzFzXuLUstuspryT5iJGfSKZJYjSB5kgdajo+M3b/AMitsdUde/GX5D7h78bu4V/bnyM6+jrMjhun+iux3kx2Vqcju2vnyEuPpMjX5HcFfFEv8MjrqxsczU/3mqNY86l5x2DlK93vdecuU4tr/dumx2i6Khru8t6MgEagAsqrGpJ1lV10bRmvKG99r+dvcrZ+WNh9r/cubfoeYNe78z2Pi02zbL3Uk7mVwW8EyTXD6Y/C8WTwy48TSNJ/94/yC8DF0rQQ7F7gyNV3/jKeevyNfuCjipOtN01k0VOw29T0NLT1Od2zSUckTLT5AyVryF2M1OAyCCMdv+9FeHmOR9z2BBys7BVSIk3EQBP6mokJISCKpRRjtbjqmrfPuAbEeR4Lbl/m2f8A1wYkZ3ubkAWdw5C0iMahpII1IIR1LsNRLq/aFo4gwPc3wg+R+yMp2Bs3O7J371Xvfbu7osZkYFSHM0WGy1PVyticijSYzOYPNUkMlP8AcU0stPKkjLquGAyVe65e9yuT9zg2ncIrnbL62kg1qcozqQNa/Ejo1DQgEUB9OsDrfbed/u/e6nLt9zPstzZbvtV/FdaaDTPCjgyeDJ/Zyxyxlk1KSO4qSGBA35sBnMbubBYXcmGqFq8PuDE47OYqrS2iqxuWo4a+hqFsSNM1LUIw5PB98u7q3ls7m4tLhdM8TtG49GUlSPyI6+gC0uoL21tr22cNbTRrLGw4FXAZT+YPTt7Y6Ude9+691rp/IH+V78rvml8m+xe4+y917D6g2RkstBgtlY+rr598bpx2wcArY3b3jwO3zDgo6uro4TX1cL5mMLXVkqqzL6hlzyj728j+2/Jm08v7Nt11uG5KhluXAEEbTv3Sd76nIBOhT4fwqCQDjrnD7ofdN91PfT3U5i505p5k27Z+XmZbXbYhrvJ0tYarHWNBDErSd0rDxjpeRlBIAPR1vjv/ACfvib0fUUed3Ticj3lu+leOdMj2QlFNtekqYngkWTHbFookwzxCSC4XJNk2GpgHsQBHHN33gefeZkktbO4TbNvaoKWVRIQQR3TMS/A/g0DhjqbvbT7mvs37eyxbhebbJvu9KQyz7vokjQjSR4dsqrAKMtQXWRxUgPTAN78hPld8f/iXtOLK9qbwxe3/ABUkUW3tjYRKev3hmoYV8FNS7d2pSSxT/ZxCMR+eT7eggAAkmjFvYA5S5F5r58vzb7DtzzEtWW5kqsSVyTJKcV86CrHyB6mX3G92fb32i2YbnzpvsNpFpC29rH33EtKALBbp3sB5mgRRlmUZ61LfnN/MQ7T+ZmcOHdajYvTOHyDVO2uuKGukm++mhZlpc/vSri8UWczwjJMSBBS0IcpCrOZJpc+PbD2h2P26thckrdcySJSa8ZaaQeMcINSiep+J+JoKKONf3hfvQc1++F221W6PtvIMMuq325Xq0xU9kt2woskg4qg7IycF2Gs17R/n/Yf8T7l3rFqTy6ye/dN9Zk/SP9j/AL2ffuvdcx9R/rj/AHv37pg8T9vWf37rXVV/sE/j/PrPDrkn6h/sf96Pu5+Dqr/CepKfX/Yf8SPe0+EdM9Zfduvde9+6afj1kj/P+w/4n37qnUlPp/sf+IHv3TT8eufu5+Afb1TrOPoP9Yf71783Bem5PLpzoK6Wla3LxXBaMn6fW5Q/2W/3g+3gxHSC5tI7kVOJBwb/AD9LGlqIqlVkia4/IPDKbfpYfg+3gQeHQduIZICySCh/w/Z1N976Sde9+691kj/P+w/4n37qr/CepEf5/wBh/wAT790z1k9+691mT9I/2P8AvZ9+6Zf4j1y9vjgOq9Zx9B/rD/evbJ4n7evdfTm64/5l5sP/AMMza/8A7o6H3yk3P/kpbh/zXk/4+eu/th/uDZf80U/46OqIP5yvz9+T3w97T6d2x0NvTE7Yw28Ov8xns7TZLZ21tyvU5Oj3HJj4J4qjP4qvnplWlAUpGyoSL2vz7yG9jfbblPnjaN8u+YrKSWeC5WOMpK6UUpUghSAc9Yh/eh96OevardeUbXlC6t44by3nknE8Ky1aN4wtC3DDGvVNz/zuv5i0sMiL2/tuB5I3RZ4uqOszLCzAqssYm2vNCZIybgOjLccgjj3Oa/d/9sQwJ2eYgHgbiah+WHB6xSl++D72MsiLutipIIDLaRVFRxFaio8qgj1B6J33n80vlR8l4lou7u797b4w4nNT/dqSqo8BtA1IlSojqW2dtajwe1mqIJolaJzRloregqPY75d5C5P5UbxNg5ft7eelPFoXkpQiniyF5KEHPdnz6iTnL3g9y/cCAWnNvOF1dWNam3GiGFjUMC0MCRROVZQVLKSp+GnQH7G/4/bZ/wD4dO3/AP3bUnsQbn/yTdw/5oSf8cPQS5X/AOVn5a/6WFv/ANXU6+mv75O9d/OtWD+eD8WPkf3h8r+vt2dP9I9ldlbax/x52nt6uzuzdqZXO4ykztJ2T2zkqnEz1dDTywx18GPy1LM0ZOoRzo1rMPeYP3fucuVeXeTdzst83+1tLttzklWOdwrFDBbKGAPkWUivqD1zp+917W+4XO/uTsm68p8pXl/t0exw27zW6gqJFurxyhJI7gsin7COqcU/l6/OQDn4od7/AF/59zuL/wCovc5/66Ht3/02W3/85l/z9YqP93v3rJx7b7n/ALwP+gupexth92fCX5CfHDtXvHqrfnVtBh+19rbvx/8AfXbFfhjn8Nsbc+2q/eMGMjyNOhrDSYrJRxzGP1xfdRkFWKn3u/3Ll/3B5W5s2bl7eLe8keykhb6dw2h5Y5BEWocVZSRXBofKvV9i5e5z9lvcL265k522G52u2XdIp1e5Qd8MMsX1Wkd1dMUtD5jUCM0I+g1R1lJkKSlr6Cqp66hrqeCsoq2jniqaSspKmJZqaqpamFnhqKeohdXR0Yq6kEEg++Zjo8TvHIhWRSVZWFCCMEEHIIPXbxHSRFkjYNGwBVgagg5BBGCCOtbL+dT/ACy+3u8N/Y35SfHnbVTv7NSbZxW1uz+vcQ0bbqqGwLTU+B3jtqgldGz4OLmjoK2igJq4lpYJYopleoaHKb2I91tk2DbZeUeZrsW0Alaa0uX/ALMa6F4nI+DuBZWPaasCRRa4Ofeo9heZuc92s+feSbI3d6LdbW/skIErCMkxzRA08Q6W0OoOqioVVu6muptb4T/MDeG5o9o4D4w98VGfNU9HUUdb1bvLCw42aOb7aU5vJZvEY7GYGCCp/bklrZoIo39LMDx7ycu+fOSbG1N7c82bcLamoMtxExYUqNCqzM5IyAoJPWD9j7Re6e6XibbZ+3m8/Vs2mktpNEqnz1ySokcYB4l2UVxXrdH/AJU/wezfwh+OtTt7fs9DUdt9lbhO9Ow4MXVJX43bzRUUWM29s+iyMJFPk/4JjommqaiMGNq+sqEieWCOKV8FPeHn+35/5nS521WGy2sXgWxcUZ6nU8hU5XUxoBx0qpIDEgdS/u7+0117S8inbN3lR+Yr24N5eiM6kjOlUjhRqDUERQWOf1GfSSuk9LT+af2pjupPgP8AJHLVtXDBVbv2BkOq8NTSGLzZLI9o6dkzUlJHKGE01PhsxV1bhRqSCmkcW0XCL2e2eXevcjlWCNCUguVvJD5Ktv8AqgmnqyqPtIHn0Z/eF5ht+W/Zn3Au7hqG42+Tb41xVnux9MAAeNBIWPmFUny61KP5XvwkyXzN73ocPl6Wsh6h2NLQ7n7azUPkhV8LFUOMZs+irEK+LMb0raeSnQqyyQ0cVTULdoArZs+7fuDFyByzLcQOp326rDYxnNGp3SkfwxA1+bFV8+uX33ffZyb3g5+t7e/hb+pu2aLrdJBgOCax2wPHVOVoaZWMOQQ2mtnXzR/kYb7wueze/vh7NQ7r2jXzz17dOZzLw4vdW2zM8s8tFtPcGbqIcRuPC0yi0MVdVU2QjXTGGq3u/uJ/b77x23T21vtnPatDeqAov41LRvwFZUUakY+ZUFTxovU8e8v3JtzS9vN/9opI5bGQmRtmncI8ZNSRbTORG6eiSMpXydsAVd7c63/mMfHbOJjtm7H+XXVuUpHZ4qbaG3+1cRj6pZZmZ2hGBpf4NmaGon1B9PnglfUDc3HuZLrdvafmu2M1/uOxXkLYLTvbswoPPWdaEDhwIHWNG38u/eX9u7yOx2PZeb7B4GqsVlFetASTqNBCHt5VJJrTUpNa5r1tofyztw/M/cnQ1bX/ADSxdfj92LuWWDY0u6MLRbc7Br9oR0FJeo3nhMfBQpRTRZMyxUpqqamyUscbPUK4aKWTCL3dteQLTmaOP2/mVrDwQbgQuXhWXUcROxNQVoTQlATRSMgdTvu733vBuHIbT+8tqY9++pYWpmjjiuHt9KlWuI4gqo4csoBVH0gF1r3MJP8AMTzeGwHwW+V1dnYopqGfo7fuEgSaRo0GZ3LhZ9ubclDIkhMsG4crSui2s7qFJAJIKPa63nufcXkuO2YiQbjDIafwxuHcfYUUg/LoS++NzbWns77my3VPCOyXcQrjvkheOP8APxGWnz6+eyn0/wBj/wAQPfTvrhX0uuuN/wC6+qt9bS7J2LlZ8HvDY+4cZubbuUgJ1UuUxNVFV05ljuFqKSZo/HPC9454XaNwUYgoN02yy3nbr7adxgEljcRNDKh81YUP2EcQeINCMjo02Hf905V37aOY9kuTDutlOlzBICcMjVo1CNSN8LLwZSVOCet+741fIPZXzY+PGzO6tjSUkGanokx+8Nsw1Qnqdn76oaWlbdWza0tpmKU9TKs+PmmSNquhmp6jSiz2HNPm7lfcPb3mm/2DcVY24bXBMRQSwknw5R5ZAowBOlgy5K9dueQOeNm94uQto5w2R4xeMgS7tkfUbe5VVM9s5IU1UkFCyrrQpIAFcdDJs3cAxVU+OrnEVFVScPINIpKvhNTk20RShQrk8KQDwAx9kF/a+MgmiFZAPLzH+cf6vLoUbNuH0krW05pCx4n8LcM+gPn6fLPSX+U/x4o/lL1YOm87u3M7T2Tnd1bayXYH93khGa3JtTbtY2aba1BXVHkgxLZPPUdBJJUtDUaIYHURlmBVfyXzXLyXvX9YLWyjn3GKGRLXxa6I5JBo8QqMtpQtQVGSM46R+5fINp7m8rTcnbpuM9vslzPC98LY6ZJYYnEpgV86BI6IHahOjUooSCBE6l6d6y6J2Ti+u+pdm4bZG0MSp+3xWHpyrVFQ4UTZHKV07zZDM5aq0gzVdXLNUSkDU5sPZVvm/wC8cy7jPu2+7hJc38nxSSHgPJVAoqqPJVAA8h0fcrcp8uck7LZ8u8qbPBY7NAKRwQLQVPFmOWd2OWdiWY5Yk9CX7J+hD0AfyF+MnS3yj2XLsfuXZlDuSgjE74XMRgUO6Nq106BDk9sbghT77FVQKqXQF6aoCBJ4pY7oRRypzlzFyVuK7ny9uLQzYEicY5FH4ZEPaw/mOKkHPQF9wPbbkv3Q2OTl/nXZIryxy0TntlhelPEhlWjxOPUGhGGDKSC7fHrqqt6N6Z2D1BWbnm3lF1zhjtXDbjqqNcfW1u18XWVUW06evo45p4Y67Ebb+1opWjfxzPTGVVjVxEjHNe9x8y8w7pv6WYt2u5PHkiU6gJGAMpU0B0tJqYVyAaEkipWch8rtyRydy9yh+8Wu4dttlsoJ5FCu0EVUgDgEjWkIRWIoGKlgqg6QM3sPdC7otXcPzE+MXQOXk29293RszZm4oqGlycu3KqqqsnuKKgrS4o6mTA4OkymXSOqEZaO8ILINQGkg+xjy/wC3/OnNUAutg5cubm0LFBMqhY9Q4jW5Vaiuc9Rzzh7ve2PIF0bDnHnjbrDcPDE3000o8bQxIVhCuqUqxBodOaHqvnsv+eN8SNqRzw9f4bsrtfIK7LTy47b8e0MBKqgkPNkd21FDm4FdrBdOLkP1uBYXljZfuz8/7gwO6TWdhF5iSTxX/JYgyH/ex1jhzR9/H2S2RKbENz3icmg+mtzAgxxZrswuAfkjH5dVU97fzsflH2bT1WI6xx22uicHUpJE9Rt8f3r3mYpG9Sf3pz1FFRUjeMaRLR42kqFJLLIptadeV/u18k7M6z73PNulypqFl/Sh4f77Rix+xnI9R1iFz/8Af090+ZoXs+TtttOX7VhRpYz9Xc8c6ZpY0iUEYxDqHEMDSlSW4t0bl3pm8jubd+4M1unceWqHqspndwZOszGXyFQ9tU1ZkchNUVdRIf6s5sOPp7n+xsLLbLWKy260igs4xRIoVCIo+SqAB1hRvu97zzFudxvG/wC63F7usx1S3F1I0sjH5u5LGnkK0AwMdMvtX0UdZI/z/sP+J9+6bk8usnv3TfWZP0j/AGP+9n37r3XMfUf64/3v37pg8T9vWf37rXVV/sE/j/PrPDrkn6h/sf8Aej7ufg6q/wAJ6kp9f9h/xI97T4R0z1l92691737pp+PWSP8AP+w/4n37qnUlPp/sf+IHv3TT8eufu5+Afb1TrOPoP9Yf71783Bem5PLrLH+f9h/xPt3pvqZTTy08qyRMVI+o/ssP9Sw/IPv3DI6YuIY5oyki1H+D7OlhRZCKrGn9EwF2jJ+o/LIeLj/eR7eVq/b0GbqzktzXjH5H/P04e7dJOskf5/2H/E+/dVf4T1Ij/P8AsP8Aiffumesnv3XusyfpH+x/3s+/dMv8R65e3xwHVes4+g/1h/vXtk8T9vXuvpzdcf8AMvNh/wDhmbX/APdHQ++Um5/8lLcP+a8n/Hz139sP9wbL/min/HR1qpf8KM/+Z5/Hb/xE+4v/AHsJfeYX3X/+SBzR/wA9kf8A1b652ffp/wCS77ef88l1/wBXIetdVP0j/Y/72feUHWA7/EesifqH+x/3o+/dV6V+xv8Aj9tn/wDh07f/APdtSe0O5/8AJN3D/mhJ/wAcPR5yv/ys/LX/AEsLf/q6nX01/fJ3rv51737r3Xvfuvdaw/8Awo9/7k2/8uG/+Yb7y8+6r/zvn/UF/wBrfXOv7/X/AIKf/qaf947rF/Kr/m87M2psnbnxr+WG54ts0u06SjwPV3cGZeofDfwCJxTYvZ2/a4LMMKmBgaOnx+Uk0US0MaRVTQmETTa95vZC/utwu+bOTLPxTMxkvLGOmoOctLCMatZyyDu1ElQa0Cv7tX3o9oh2fbvb/wBy9zFtcWyCDbt0mr4bxDCQ3D0pG0S0VZGojIAHYMNT7M2B3Bgd1YfH7h2vm8RuTAZaAVWLzmByVFmMPkqYsyCox+Tx81RRVkBdCNcbstwRfj3iXc21xZzyW13bvFcoaPHIpVlPoVYAg/b10Ctrq2vbeK7s7iOa1kGpJYmDIw9VZSQR8wenf2x0/wBBR3D3p0/8f9qT737n7F2r1ztmES+Ov3Lk4qSbIzQqjSUWExaeXLbgyQWRSKWhgqKlgeEPs52Pl7fOZLxbDYtrmurs8ViWoUHzdsKi/NiB8+g/zLzXy3ydtsm780b3b2O3L/olw4XUeOlF+KRz5KoLHyB60r/5p38yWu+c2+sPtHYFNl9v/H3rqvqKraeKyoFNlt7bomhloajfm4cfDJLDRNHRTSUuKpGeSWkpZppHZZaqWGLPX2d9rI/b6wnvNxdJeZrpAs7plYo6giFD55ALtgMwAGFBPKT7x3vy/u3usG07Ijw8j7fIZLYSCj3E2kqbmRfwAKxWJPiVSzMQ0hRDh/yjv5lnS/xZ2jN8f+5tp0mzdvZzclRn4O59vY6qr558rkUjgaHsjH0qVWUqKKhhgjho62iSQU8I0SU4Guf2EPe/2i5g5wvV5m2C9a4uY4REdvlYCirmsBNFBYkllalTkHy6Gv3WfvJ8l8g7U3IXOO3JYWst008e8QqWEjyGlLwKC40KFRJBVQgAcKF1Hav2D2T192pt+l3X1pvfau/dtViI9Pm9o57G5/HMZEDiKSpxlTUxwVKDh4pNMsbAqygggYYbltO57NdPZbtt81tdqaGOdGRv2MBUfPh10y2ffNm5hsYd02Hdba926QBkntZEljYH0ZCR0tfZf0adMu4dybe2jh6/cW689hdsbfxcDVOTzu4cpQ4XD46mQXeor8nkp6aipIEH1eR1Uf19qLW1ur2eO1sraSa5c0SOJS7MfQKoJJ+zpNeXlnt9tNe393FBZxqWklmZURVGSWZiFUD1J61IP5wP80LbHyMov9ln+P2QkynU2KzdHlOwt/rFLT03YWcwlQZ8Xgdu09VBFUnaGCyUaVT1jhDka6KJoVFPAstXm17Hez93yrJ/W3meLRvbxlLW2rUwI4ozuQaeK6mmn8Ckg9xIXmF96b7x22c92ze3fIlz43LCTK+4X4HbdPE1UihqKmCNwHMn+iMFKfpjVJQKn0/2P/ED3kt1g71IT6f7H/iB7900/Hqw7+XV89d3fBvt3+LutduDp3e0tBje1tk05Es9RQU8rCj3XtqKappqaHd23UnkMPkdYaunklp5SuuOaCM/dT21sPcTY1g7Yt+t1ZrK5PAMQKxyUBJiegrTKmjCtCrTx7Be+O6+zPM/jSa7jk+8ZU3OzXJoMLPBUqBPFXzOmRao1DodN2Xa+Z2H3xszbPbPUW6cPubaW88fFlMZmqKaU4/IU76o5C6CE1eOy1DUxNT1lJNFHPBURvHMkcyOp573lvuXLV/d7JvllJDfW7FHjYCqnj60ZSDVWBIIIIJBHXX2wuNl512nbuaeVdzhuNrvIxLHMhOhxwrw1I6kFXRgGVgQwVgR0K+3qTNUFN9nlZqOpjhULSzQSzvMqDjwyiWniDIg/S17gcc8WJLl7eR9cCsCeIIFPyoT0KNvivYIvBu3RgPhZSSaehqB0ofabow697917r3v3Xuve/de6I/85/m/1/8AC3rGbP5aSiz/AGbuOmq6brPrv7grVZ7JxgRtl8ssDCooNpYWSRXrKi6GQgQQt5pFtJPtp7bbt7i70tpbhotmhIa8u6YjX+Fa4aV+Cr5fEe0HqD/fb3y5a9j+VJN33N1n5iuFZNr20NR7iQD4mplLeIkGSTgBRVq7Kp0jex+xt5dub63R2X2Dm6rcW8955aozefy9WRrqauo0qkUESAQ0dBQ00aU9LTxBYaamijijVY0VR0n2PZ9u2DbLLZtpthFt1vGI4o18gPMniWY1LE5JJJyeuEHNnNW+c78ybxzZzJetcb3fTGeeU+poFVR+FEUBEUYVFVRgdI2P8/7D/ifZsPiboMP8R6ye9jift6r1lT6f7H/iB7300/Hrn791TrJH+f8AYf8AE+/dNyeXWT37pvrMn6R/sf8Aez7917rmPqP9cf73790weJ+3rP791rqq/wBgn8f59Z4dck/UP9j/AL0fdz8HVX+E9SU+v+w/4ke9p8I6Z6y+7de697900/HrJH+f9h/xPv3VOpKfT/Y/8QPfumn49c/dz8A+3qnWcfQf6w/3r35uC9NyeXWWP8/7D/ifbvTfWZP1D/Y/70ffuqv8J6zqzKwZSVZSCCDYgj6EH37pggMCrCoPl0pKHKrLpiqSEk4CyfRH/Fm/1Ln/AGx/w9uq1cHoku9vMdZIASnmvmP846f4/wA/7D/ifd+il/hPUiP8/wCw/wCJ9+6Z6ye/de6zJ+kf7H/ez790y/xHrl7fHAdV6zj6D/WH+9e2TxP29e6FCPuTt6OOOOPtXshI0RURE3xudURFUKqqq5QKqqosAOAPZU2w7GWJOzWla/75j/6B6EY5855AAHOe7ADAAu7j/rZ0mdwbt3Xu2anqN1bn3DuaejjeGkn3BmslmZqWGRg8kVPJkqmpeCN3AJVSATyfZhZ2NlZIy2VnFCrGrCJFStOFdIFeijc983re2hfed4urt4wRGbqWSUqDSoUyM1AaCtOPTIn6R/sf97PtZ0Sv8R6yJ+of7H/ej791XqTHJJDIksTvFLE6yRyRsySRyIwZHR1IZHRgCCDcH3ogMCrCqnBB61reJklicrIrBlZTQgjIIIyCD0I/+mfuH/n6/ZX/AKHW6P8A66eyn+r+w/8ARks/+cMf/QPQnPP3Pf8A02u7f9llx/1s6zR90dxW/wCZsdl/X/nu90/0H/V19+/q/sP/AEZLP/nDH/0D1r+v3Pf/AE2u7/8AZZcf9bOs6dz9wkc9r9lfX/nut0f4f9XX37+r+w/9GSz/AOcMf/QPTb8/8+A4523f/ssuP+tnSd3FvPeG7/s/72bs3Luf+H/cfYf3izuUzX2P3fg+6+z/AIlVVP233P20fk0adfjW99IsYWO32Fj4v0NjDDrpq8JFStK0rpArSpp9p6Jd15g37ffA/fe93l54WrwvqppJdGqmrT4jNp1aRWlK0FeA6Q2Ul0xJEPrIxY/8FS3B/wBdmH+29q3PAdJbJKu0nkv+E/7HSr6+7i7c6mqpK7qvtPsfrOtmLmWs6+3xubZlVKZIjBIZKjbmUxsrmSAlGuTdDY8eyfctk2XeUEe8bRa3cY4LcxRygZrwdWHHPQy2TmvmjloyHlzmS/28uat9FcTQVNKVPhOtTTGfLHQ4VPz3+b1fSJj6n5c/I80yqqHw9y7/AKWeREiaLTPWUuehrKhXRjrEkjCQ8tc8+yFPbvkGOQyryXtWs+trCRxrgFKD8hjoTz+8fuzLbR27+5W++GlKFb24VjQae51kDvg51E1OTU56LhuHdO5945aXObu3Hnt1ZqoGmfMbjy+QzmUnUFmAmyGTqKqrkAZyRqc8k+xVa2lpYwrb2VrHDbjISJQij7FUAdADct13Pebpr7d9xnur0gKZrmR5XIFaAu5ZqCp8/PqPi4fNWR3F1ivK3/IFtP8AyeR7VpxPRJfy+HbPTi3aPz4/y6WHt3oN9Kjam894bJr2yezN17l2jkmRUbIbYzuUwFcyI11VqvFVVJUFVLEgarC/tHe7dt+5RiHcbGGeIcFmRXH7GBHRvs/MO/8AL00lxsG+XljO4AZ7OaSFiBWlTGyk0qadGUo/np81qGkNFB8re/nhPk9dZ2nvDI1f7t9Vq/IZWprha/p/c9H9m3sJSe2Xt5LJ4rclbYGxhbeNRj+iqhf5Z6kWD7wHvXZWwtIfc/eTFnMtw8r54/qSF5Ps7seVOgK39272t2bIK3svszsLsaqgbzxTb63nuTd86TRxyIjxy5/JZCRZAkjKCCCFYj6E+xRtexbJs0brtGz2topFCLaKOLGMdirjHQB3rnDm/mswxcz817luKBwyi/uppwpyNQ8Z3AIBIr6Ejz6BEkkkte5JJv8AW5PN/wDG/sx6aNBgcOsifT/Y/wDED37rXUhPp/sf+IHv3TT8eufu7cF6p0t9tb+3/t6GLEba3xvDb2NkqXnNBg9y5rFUXnlCiao+0oK2ngMzpGNTadRCi549oJtq2y9kMt5t0EstANUkaMaDyqwJp0b2vNPMmyWUlvtPMN9a21S/h288saajQE6UYCpoATSvDoUR3J2+AAO1eyQALADfO5+APoP+Lp7a/q5y/wD9GKz/AOcEf/QPRYfcb3Cqf+R5vP8A2W3P/W3rkO5e37j/AIyt2T9R/wAxzuf/AOunv39XOXv+jFZf84Iv+getf64/uH/03m9f9ltz/wBbes69ydvXH/GVeyPqP+Y53P8A/XT3r+rfLv8A0YLL/nBF/wBA9ePuR7iUP/I93r/suuf+tvWf/TJ29/z9Xsj/ANDnc/8A9dPfv6t8u/8ARgsv+cEX/QPTP+uV7i/9N9vf/Zddf9beu17k7euP+Mq9kfUf8xzuf/66e/f1b5d/6MNl/wA4Iv8AoHrTe5PuLQ/8j7ev+y66/wCtvSXzu49w7orVyW5s9mdxZFIEpUr87lK7L1q00TySR0y1WQnqJ1gjeV2VA2kFiQOT7MbWzs7GMw2VrHDCTqKRKqCp4migCuOPQW3Xet5365W93zdrq9vAgjEt3K8zhASQoaRmYKCxIFaVJ9em0fQf6w/3r2sTj0WdZY/z/sP+J93HxN0y/wAR6ye9jift6r1lT6f7H/iB7300/Hrn791TrJH+f9h/xPv3Tcnl1k9+6b6zJ+kf7H/ez7917rmPqP8AXH+9+/dMHift6z+/da6qv9gn8f59Z4dck/UP9j/vR93PwdVf4T1JT6/7D/iR72nwjpnrL7t17r3v3TT8eskf5/2H/E+/dU6kp9P9j/xA9+6afj1z93PwD7eqdZx9B/rD/evfm4L03J5dZY/z/sP+J9u9N9Zk/UP9j/vR9+6q/wAJ6ze/dM9e9+690+43KtDaKoJeHhQ/1eMc2/xdB/T6gfT+ntxWOB0VXtgsgLw4kPEeR/zHpWwusi60YMrAFWU3BHP0PtzoOsrIxVgQw4g9ZvfutdZk/SP9j/vZ9+6Zf4j1y9vjgOq9Zx9B/rD/AHr2yeJ+3r3TlSUNVWECBAQLXY8D6fT8k/7D2kur23tRqleny6M9r2Dct3YraQVXhqPDp+i2rXyAksq/S1lZr3/2K2t7KH5psIyF1V/PoYQe12/zKWJAHyBP+UdSl2jXAD9wf63j4/6GLe6/1ssPUft6s3tPv2TqH+8n/oLrIu0chcHWv/Utj9f8Lj3b+tm3U45+3qn+tRv/APF/xk/5+s390Mh/x0H/AFJcf72/uv8AWyw/1Hrze0u/0+Mf7yf8/Xf90a78yrf/AJZkf9F+9/1t2/0/mOqH2k5gJ+Mf7yf8/WdNoVtv88vPPMbf0H9G96HNu3mv+cdb/wBaLf8AFJR/vJ/z9Z02jWgf51Tc/wDHM/63+q92/rZt/wDqP+x00/tFv+r+0H+8n/P1kXaFYb3l/pa0RP8A0X73/W6wXh/hH+bqg9o9+zWWn+0P+foN81TVMeTqadYKiVaVjTh1hkKs0Z/cI0hhxJcf7D2ZR71ZzRpL4yCorQkV/wAnRBNyxuu2zT2ZspnZHILrG1CRjFK46bRBVf8AKrU/9SZP+jB7uN2svO4T9o/z9MnZt0/6N0//ADjf/N1lWlqtQ/yWp/8AOeX+n+Ke9/vax/5SE/3odVOzbuQR+67j/nG/+brMtPVAgmkqv/OeX+n/AAX3797WP/KQn+9Dpv8Acm7/APRsuP8AnE/+boRdqbXrq2klrijQLLIYolkibWyRcO+klSqmQ2H9Sv8ArXRz8zbdbSeF4is1Kk1x+3o1tvbfmLfLVblYHiiDEKHQ1NOJoStBXA9c/Kqq/uhW/wDHT/rCf+vntOeb9vBA1D9v+x06PZzmDzc/7wf+gusibPrAeZvx+IT/AIf6p7e9nm7bx5j9vVh7Ob9+J2p8kP8An6znZ1WP92/9Yj/xDH37+t+3+o/b/sdUf2c3w0pI3+8f9Ddchs6ruP3SbG9hH/0n72OcLD4RT9v+x0yfZzfgQfEOnz7D/wBBdQq3ac6pqkjjmP51RlSBY8hwS44/p7MLXmCyuSAp4/Ov+boj3P275g2hC6yEkcRpIH+E16SMuGQFlRnhdSQUf1gHi35DWI/Nz7PU0yLqVqjoEvdz20jQ3EXeuCOB/wA3UNsbVRAkJ5Vv9YjqP0/1JAe/+w9+IpivVvrYHIq2k+jf5+HUQgqSGBUj6gggj/XB592bgvT4IIqDjp5wsOqaSY/SJNI/4NJ/xRQf9v73H59F+4yUjSMcSa/kOlN7c6ITxP29dj6j/XH+9+/da6kD6j/XH+9+/daPA9Z/fumOux9R/rj/AHv37rR4HrP790x1nH0H+sP9693Tj17rLH+f9h/xPu4+JumX+I9ZPexxP29V6yp9P9j/AMQPe+mn49c/fuqdZI/z/sP+J9+6bk8usnv3TfWZP0j/AGP+9n37r3XMfUf64/3v37pg8T9vWf37rXVV/sE/j/PrPDrkn6h/sf8Aej7ufg6q/wAJ6kp9f9h/xI97T4R0z1l92691737pp+PWSP8AP+w/4n37qnUlPp/sf+IHv3TT8eufu5+Afb1TrOPoP9Yf71783Bem5PLrLH+f9h/xPt3pvrMn6h/sf96Pv3VX+E9Zvfumeve/de6yR/n/AGH/ABPuyfEOm5PLp1oK6akY6TqiJBaJj6T/AFK/6lv8f9v7ux0kdIbm1juVzhxwYf5fUdK+nqYqqPyRNf8A1SnhkP8ARh+D/vB92BBFR0HpoZIH0SLQ+Xofs6nJ+kf7H/ez730kf4j1y9vjgOq9SEGrQv8AXSP9vYe2HOnW3pU9XjTXJGnqwH7T0pN952s686x3JvDD01BU5LCUFLPSQ5OKeaikklr6OlYTx0tVR1DL452PpkU3tz9R7xv93ectw5e2PctysAjXcZTQsoJXukVDUKynCsaZGf2ddIfui+znLvuP7hcncn8wPcR7PetIk0loyLKAkEso0NJHKgqyLWqNgkYNCCXw/NTtNgP9wHX4v/qcVuIfi/H+/qv7xKm96Ob3LExWg+xJP+t3XZq1/u9/Y+NNA3jmGnznsv8AvX9OUXzL7QcG+D2Hwfxi9wf8Tug+0re9HN4BPh2n+8Sf9bujeL+7w9jZOO88xflcWX/ev6dIvmB2W9r4PY3+wxmf/pf/AJ6Y+2W97OcVpSKz/wB4l/63dGUf93N7EvUHe+ZKf89Fj/3runKL5bdjufVhNkfW3GMzn+H/AGcf+PtOffHnMCvg2XD+CX/rd0YRf3bPsI9K75zN/wBlFj/3renGH5W9hv8AXDbLHIHGOzg+v/kxH2w3vtzotKQWX+8S/wDW7oxi/uzvu/vSu/cz/wDZTYf963pwi+U3YLA3xGzhawFsfmv+J3AfaV/fzndTQQWP+8Tf9b+jKH+7C+73J8W/80/lc7f/AN6zqfD8oN/twcTtD+vGPzP5F/8Anf8A+HtM/wB4LnleFvYcf4Jv+t/RjH/da/d1cAtzDzXX/np27/vV9OUfyY34xscVtL/YY/Lf0P8AXOH+ntG33iufFpS22/8A5xzf9tHRhD/dU/dxY55j5tz/AMvW3f8Aeq6bl7v3VNIWfGbbLO2pm+yyNyzepif9y31JPvT/AHmvcRKKLXbaf805/wDtp6vH/dGfdjkOtuY+cNR4/wCNbb/3qepady7mIv8Aw3bo5txR5D/66e0zfei9x1GLXbP+cc//AG09L0/ugPuvP8XMvOP/AGV7Z/3qOs47o3P/AM63bv0P/KHkPwL/APO19sN96X3IU4s9r/5xT/8AbT0vj/udfusuVB5l5zz/AMve2f8Aen65L3Rue4P8N279T/yh5D+n/a1/x9tH71XuUCR9Jtf/ADiuP+2rpfH/AHNX3VXBJ5n50/7K9r/70/T/AE3yG3pSQx08OL2sI41KregylzcliSRmQCSxv7Sy/ej9x2Jc2e1lif8Afdx/209HVv8A3N/3WVQRrzVzqFHCl5tf/em6zj5Hb5JH+43a31H/ACg5X+v/AGu/aZvvTe44JH0W1/8AOK4/7aujOL+5o+6u9K8287/9lm1f96brl/sx++QT/uL2r9SOaDKn/wCTfttvvU+5ANBY7V/ziuP+2rowj/uXfupyAaubueP+yzav+9L13/syW+/+dZtX/wA4Mr/9e/bTfes9ygaCx2r/AJxXH/bV0YR/3KP3TpNOrm/nrJ/5Tdp/70nXR+Su+0IIxe0/9jQZf/D/AKvnuh+9f7lrkWG0/wDOK4/7aujCP+5E+6TNVW5x58A+V7tH/ej6GvpvszOdlPuSDO0WGpRiIsW1KcXT1sDSGtNeJvP93kK4MEFKunSEtze/Fshfu8e//OXuDzTuO0cwWtjHaQ2njo1qkyuW8REoTJPKCtGOAAa0z5Hlp/el/wB3F7IfdM5A9t+Y/bDe+Y73cd6v7q0u13y4spo0SCGORDELXb7JlYs5qWZxSlAOPT3uOlFNXCwt5Fe4/wCCMLcf8hn30q5cuTc2eon0/wAHXy/e5W2R7bvoCChYGo+w/wCz0yp9P9j/AMQPZ2/xHqNn49eeKOUaZEVx/RlB/wBtf6e7J5jy68kjxmqOQfl1kgp4aZWWFNCsxci5PJAH1JJsAPdwAOHW5JXlIMjVIFOs/vfSQ8T9vXY+o/1x/vfv3WupA+o/1x/vfv3WjwPWf37pjrsfUf64/wB79+60eB6z+/dMdZx9B/rD/evd049e6yx/n/Yf8T7uPibpl/iPWT3scT9vVesqfT/Y/wDED3vpp+PXP37qnWSP8/7D/iffum5PLrJ79031mT9I/wBj/vZ9+691zH1H+uP979+6YPE/b1n9+611Vf7BP4/z6zw65J+of7H/AHo+7n4Oqv8ACepKfX/Yf8SPe0+EdM9Zfduvde9+6afj1kj/AD/sP+J9+6p1JT6f7H/iB7900/Hrn7ufgH29U6zj6D/WH+9e/NwXpuTy6yx/n/Yf8T7d6b6zJ+of7H/ej791V/hPWb37pnr3v3Xuskf5/wBh/wAT7snxDpuTy6kR/n/Yf8T7tJ5dN9SYZ5adxJE5Vh/T6MP9Sw+jKfdASDUdJ540lGl1qOlhQZGKrQKf25gOUJ4b+pjP5H+H1Ht4Gor0HLu0kgYsMxnz/wA/Tn7UDgOkXUyn/wA7B/y0i/6GX2kuP7Kf/St/gPSqx/3NtP8Amqn/AB4dSu/Lf6Bt9cf8uug/922NPvDb35Y/1d3YeWqP/q9H12L+4ao/14PbxqZ8aX/tEn6JF8IOvdn9ufMr4j9UdhYj+8Gwezvk30L17vjA/wAQymJ/jez96dpbU23ubEfxTCVuNzWN/iWFyU8P3FHU09VDr1xSJIFYYZQoslxEjiqs4BHyJ67184bjebPyXzhu23TeHuFrtd3cQSUVtMkcDujaWDK2llBoQQeBBHW3v0R/Jv8A5dnZ3zw/m7/HzcvT8+3esvjzt74dQdHVlL2t21BU9OVHcvx23Tu/f26qbKZLsCb+9M53TRw5RE3M+XoaZqcRLElK0kLGQ2+0km3GJl0oirpap7aqSTk5oc5x1invnvb7l7PyB7M8x2e8iXdNyl3E36m3tyLkW15HHDGVWH9MeGSn6WhjWtS1D1XhvD+VN1z8cP5U38x/sDvfrFK35f8Axa+XW3up9g9s025+wsbiqjrbL574lDD5rA7Pj3HQ7KzOB3ltbtXJ1lLUZHEz10UWUCs8c1PGsBY1lGm230k0f+NxS6K1OMp5YqCDUEjgQepg2r3k3Xmj3m9q9r5c3cryPvGySXtzZGOBm8dU3LUry6GlV4pLdFYK4UlOBDGtrny4/lrfBD44dlYTZHVP8k/vv5U7eyux8Zuqs7D6t+RHyHpNvYbNV2f3LiKjZlZFWdmZGRszjqHBU1dIwcKYMjENIIJNtzt7aymSKDYZJ0KaiytNQGpFO1HFcV4+fDqKeQfd33L5r2i43HefvE7Xsd0ly0C2t7Y2Jd0VI3Eopbr2MzlRjih6qt298QvgH8FviT0L8p/nz1T2v3v2L8tK7cW4eofjltffGW63wG1utaBKKtpMvuHceFy2D3RkKynwG5MRXNPHXNFJJkqWFYHjE1Q4fjt7ezsrK+3CJ5pZgTHEDoTSKDUzBS1TUMoFMEY49ZAPz/7r+53PvNHI3tVv1htW0bCkcW4bxPClw8lw1QUjjdXjUF45FoVqAjNqB0qAH/mKfB34+dc/Hz41/O/4YZHfb/GL5Lz5Tbcmz+xJ4sruLrLsXDnOJPtqTPUoljrYJ6naWbpTFNNUTRVOHmZKieKRfEg3KwSK3s9wtTIbKbUKSAakdTQqSAAQaHTjgCc9SN7Je6PN2884c6+1PuTDaDnfZVWcXFmCsdzbvopJ4Z4ECWJqgAESKCqkZh/ye/hv1j8we1u86HsfZmd7Xqun+gN09pdfdK4rddb17ju4ewMZWUNDtzYm4OwqFqaq2xjM1WVS05aCqpKn94zrKIqacFJtNim4Xk8LoXaOCSdIgdPiOhUKhPkras0ofQjo7+8d7nb/AO2fLfKEux7pDt0e57xFt97uskK3LWVuysZLiO3aolZFBNGVlxppV16Cf+ZH1P8AGvpn5IR7N+MGSin2qnXOyMl2FtvHb6p+0ttdb9y5CkrJ999a7U7LppJhvjDbUQ0atWySPKtZLPC5BiABJusdnFchLKTUmhWcalcI5UFkV1xIqnGr1qM0qZD9gOZOfOaeRzunuBARuBvp47Gd7c2kt1Yqyi3uprUgeA83f2gAaQrDj1bD/Jo6W/ln/Nutofjj2n8OM/mO79hdP7p7M313PVd49u4jB70OL7F2zt6ko6LZm0d/YHH4WeHGb9oog0UaRsKB2ZS8ur2f8o2ezbxM223+zhrhI3lNx40g1fqAKvhrpC0VwK1Pw18+sf8A71XN/wB4X2et5ef+WvdeCHlC93WHbrLaV2+ykkg12sspZp57aRpAWtnOSSNYANB17oPpL+W/8yulP5mXdHVHxDznT+P+M/xBwu5Os8Fn+6+2d2VmC7gTafyr3XlN/RVb77MOXpq+Dam2IVxuSWsoI2w7MsAFTUiZNt1lsO9bfzPex7L4H0toGiXxpJKPpnYvUla10qNJBHb8z0cc6c5/eE9oucfu48ocz+6sO6z8x82SW24zQbfYwrLYGfZYEtSv01YypnuT4kZRyJgC3YmkOdmfFD4IfDD4cfHr5Q/PHYfZ/fnZPyrp6vc3VnSOzd3V/XuAxmwaalxeUTN5jMYjK7dz9QZNvbhxtbJUR1TI0mTpYI4NIlqSRptm1bNtW3bvvtrPcXN2Wa3tVbwk8NCBqkkAL1YMGXTxBApxboY7n7p++nvH7v8APvtl7F77tmw8vcrsLbc96vIEu5Xuizp4ccckc0Q/VikQKVBpE7lq0TofPgt8QP5UXy7+dmT2f1HhOzOzujar4j57tPN9W9l5Pfeza/qvtal7F6dwtNjaHe2z91bczu6hRYPdtfTVMDz1mPgqdTR1VaGienX8rbNyvvXMdxbQxXE22/Rmbw7g6GSXxEBUNEylgoYjhTPFsHoJe9/vB96z2i9ibbeOa73bdr54Tm6La4N121LW4W+sWs9wkZ2triCaKDVLbxsrBUkZaAxxUYOUr5WfFr4wfAX4d7A627i2LS9j/wAxnvDGwb9yHk3jvvF4/wCNOwct446GirsDtjdeN2nuLckclBLTQrX0tWkuQaskOukpaYVIc3fbbLYtntrO8t9fMtwRO9SwFrEaaUIBCtK9DUEHTU14IXm32i90/dL3/wDeXmDmXk3fn237uGxymwjpb2rvvN1HlmWWeB7iGEhwzGN0Ij8JRSSRylzHyf8A5c3wg6G7Aw+0Otv5P3eHyVwWR2fj9y1W++tO/u7KPA4nLVma3Bi59pVcWU7WknbLUFHh4KyRlOgw18QAuD7GnMux7Lst/Fa2Ht5cX8LRCQzQzXdAxZl0HQsoqAoPEHIx5nDn2o+8r77c/cv3m88y/fM2Hle/ivXtUsN02nbGlkjWOGQXCmOwp4bNIyDz1Rt8uif/AAh6g/lR/Ir43fKDsPc/wO3bSbv+D3SGC3n2zNkPkD3LDUdo7kx+w+x85uaXBUeF7KosVtmbJ5PqmtIiMX28LV0aooSMj2R8p2nKu87Bu97d8sBrrbrJJXcXM/8AjDeHIzGg0iLUY60AYDVwxmcffPnX73/tp7ne03LW0feEsn2bn7fpbHZxHtG2kWEL3dlFAJWlsWknCJuEea6m8NiTVugF/l8/D74XfzBPkt8sd/7T6Z3jtjpLqDr/AGNujqX4e0Ha1em8N85/IbZmx2YxtR2fujcS5KPE1+8dpVJaWfMUUdLPuKjV6qCnhIBJy5se1c2bzus8FiYba3t/Hh2uKarysoC6PHlXEbOO4nSVMigEAHqVfvIe93vt92v2p9meXd455sbrn3e9zu7TeedpNvQ21pCk4eJ1sIIdBkS2uFoqwSF1tZSI3dwSVT+aN0h8c+mKrqmHqL4qfJv4n783Cm56jsHYXdeTqc9sKlpcfPQwYhett211XuqXfAmmmmaatp85LDBDHGklOs0hZQzzPb2FtdQJa7Jf7fcMjNNb3lCg7lC/TsVWWSMdwZ34mgXgSZ3+537ge6PPkfOUnO3vHylzny5am3XbNx2CMQ3jM6uZfrrZFtxaUAXTG1uGZixVyigEoHxaNq3ev/LDA/8AQ2Y95B/dKJHPe80/6N//AFmj6wG/v2gD7TextR/y1tx/7Rrfoct3f8CojYXJl+n+tH/vXvspyaSbHJ/COviS95gBv0dPV/8ACOkqn0/2P/ED2LH+I9Qs/Hrn7tH59U6ke3Ovde9+6YPE/b12PqP9cf73791rqQPqP9cf73791o8D1n9+6Y67H1H+uP8Ae/futHges/v3THWcfQf6w/3r3dOPXussf5/2H/E+7j4m6Zf4j1k97HE/b1XrKn0/2P8AxA976afj1z9+6p1kj/P+w/4n37puTy6ye/dN9Zk/SP8AY/72ffuvdcx9R/rj/e/fumDxP29Z/futdVX+wT+P8+s8OuSfqH+x/wB6Pu5+Dqr/AAnqSn1/2H/Ej3tPhHTPWX3br3Xvfumn49ZI/wA/7D/iffuqdSU+n+x/4ge/dNPx65+7n4B9vVOs4+g/1h/vXvzcF6bk8ussf5/2H/E+3em+syfqH+x/3o+/dVf4T1m9+6Z697917rJH+f8AYf8AE+7J8Q6bk8upEf5/2H/E+7SeXTfWT2300/HrPGSoUqSCDcEGxBB4II5B9vL8I6bIBBBFR6HpS0GVD6YaohX4CynhW/wf8K3+P0P+Ht5X8j0S3e3lKyQCq+a+n2evSop/87B/y0i/6GX2nuP7Kf8A0rf4D0ksf9zbP/mqn/Hh1K78/wCZDb6/7VdD/wC7bG+8Nffn/lXd2/00X/V6PrsZ9w3/AKe/7ef81pf+0SfokXwg7C2f1H8yviP2v2Fl/wC7+wesfk30L2FvjPfw/KZb+CbP2X2ltTcm5sv/AAvCUWSzWS/huFxs8329HTVFVNo0RRvIVU4ZwusdxE7miq4JPyB671c4bdebxyXzhtO3Q+JuF1td3bwR1VdUkkDoi6mKqupmAqSAOJIHW0Luj+af8Ga3tv8An/buwvfMv8N+afxs6U2L8WcrB1t3LST9jb22d8OOyOrc3joUfr+Gu2PLi+wc9R0S1WfTEU8hl88Ur06PMq6S8tSd2Jk7ZYwqYOewinDGT59Y5bf7S8/Dafu6WkvLw8TYt1ubjdlM9sRDFJuUE6t/bUl1QozUj1nGkjUQOkP3l/OY6Z+Wv8kLsX48dx78moPnDXwdS7OrNtTbU3zkH7ah627l6j3I3aE29KHbFVsjH5HN7H27PNkIchlaapfJUFQIotE1IkiOTcUm2iW2nf8AxqoUcSWAKnUTnNMGpyRXzA6EnK/sTv8AyZ94PaeaNi20N7eobmcSiSFfpjPa3Mf04iMglZVmkAUohUKy1NQxAS/zmf5tWX7j+Umwtzfy+vmp33iemKHoPa2C3NTdW70786M28/Z1N2J2jkM1PWbSycfX0+RzLbUymFWTIiilSaBYoROxpzHGm3jdGluEewvJBD4dDpLKK1byxmlOhn93j2Ntti5N3Oz90vbza5N/bdJJITew2V4/05gt1QCVfHCp4iyUTUKGp091TA2X8wfgf87fht8cvi3/ADCuze1fj52r8TEym3urvkFtXZuU7Q2/n+v62hxtAmA3FhcJjNw7ohrnwu2sTQOqUhTy4ymqRUhXngUqFxbXlraWV9M8Tw6hFMBrTQaHSyAhqigC0rQAfPo4uvb/AN0/a/3D5u549pNksd32PftMt9tM8y20iTgs2uN3aOIqHkkfLVo7LpqFboFf5inzi+PnY3x8+NfwQ+GGO32nxi+NE+U3JJvDsSCLFbi7N7FzBzjz7lkwNKYo6KCCp3bm6oyzQ080tTmJlSngijXylu5X6S29nt9qJBZQ6jWQjU7saliASABU6c8CRjqQvZL2u5u2bnDnX3W9yZrQ8770qwC3syWjtrdNFI/EPEkRRLQEgCNSWYnBrf5XX8wD489GfFHH9Lbi+Re5/hn3Bsj5Q0vyAqux8T0ruPubZ3fexqfaR29P032Bgtk1+Nz1ZjMnDPNG0dVPSwUclPR1VPUiZXEVtq3GG1tZYDfPbXIuRcCVULq6qmkQsFdSQWqaHtzxByAl77ezfOnNvuBLzRZck2/NHLV3y+dmWxkvorKbb5zL4gvbeSdWjV0IBqoYsDIjLQirT/N8+Wnwn+TnVvTp+Gm79tbZx9H2h2p2H2l0jV9Ob22Tvyp3/v6emgn7OqN4y4Os2BkaDLUuGZpcdSZWOaIVcEjRyP5IaEs5iutou0sptpQRIXleWAoVcO5WrlgWQqwQUCt24xkhRL91z2291+QOZOZ/9dHa7ieZ9vtLHbt2W9gntxbW4JFqIBItwrIXw7RkHSwBAo0gZfyLvlh0B8O/lp2H2Z8jd/f6OtkZ3467s2Jis3/dbeu7vut15PsnqLcFDiv4bsTbm58vB58Rtium88lOlMvg0NIHeNXpyfulhtG7XFzuE/hwtAyBtLN3F4yBRQTwB+XQ1++J7Y88e6/tdsPLvIOyfX7zDv0F7JD41vBSFLS9iZ9dzLCho8yDSGLGtQKAkT/5Znyu6C+PvxM/mm9Z9vb9/ujvf5HfHin2L0zhP7rb0z398t1R9a/IfAPi/wCJbY25msRt62X31iofPlaihpv8q1eTRFM0aPlzdtv2/aOaba8uNE9zbeHCuljqbRMKVUEDLDjQZ+3o0+8P7X89c+e6P3ZeY+VNj+r2bl7fzfbxN41vF9PB9ZtUuvRNLG8vZbSnTErt20pVlBF7Znyv+CHzP+HHx6+L3zx352f0H2T8VKer2z1Z3ds3aNf2FgMnsGppcXi0wmYw+IxW4s/TmPb23sbRSU8dKqLJjKWeOfSZaYI03Pat52rbto326nt7m0LLb3Sr4qeG5B0yRgh6qFCrp4AA14r0S7n7We+ns57v8++5vsXsW2b9y9zQwudz2W8nS0lS6DO/iRySSQxH9WWRwxYmkroVrR+h5+CnzA/lS/EX535feHUma7M6v6Ko/iPnOq8x2l2Zi99byyHa/a9V2J07m4ctQbL2dtncud2rHXYPaldPUzSU1DQzVSusdLRqIFqF/K288r7LzHcXMM08O2/RGHXcAuzy+IhLaY1YqGC140xwXh0E/fD2f+9X7uexFrs/Ndltu6c8vzdFusO17a9rbpY2K2m4RlGubiaGKcrLPGqqGd1WhMkh1FC1/IX5ifHT+YR8G8BlPk/2TR7C/mHfH6pyuK2TuVuvd2VWO+QOwZ5o8mu3sxlOv9mZHbm26ydaqRaUVzUkFLl6UzK0VPkqt4iHc92tOYNiSbdbqnM9odEchQ/4zCTUIxRdKvGSdJbB9ayMUlz229nPcn7vPvruFr7XcsvuH3duYVSW+tvq7dX2m6A0eNGl3cpNMo0jV4YdnhfSQzwRhrSfmB83/gL8oOzMFv7Y/wDOP+UPxhxOI2NjNn1GwOk9i/Kzbu1cvkaDcG5s1Lu/IUWI2fgqaXcGQptwQ0UsrQs7U2PgUuQqqox5k37Zt5vornb/AHDuLGFYhGYYobogsGY6+1oxUhgOFccfIYyey3sV94T2s5YvuX98+5XypzXdzX73q7hvt1sM08aPFBELdGkuZWEKNCXA1AapHNMkmpH+Xd8sPj30F8av5sfW/afZtTiN2/JDo2o2R0jFWbW3znqvsXcS7B+RmBSOqyWA23l6Db1TWZPfWJDz5iagh1VhYvpimaMEcn71tu1bDzfZ7hcCK6u7IRQIFYhn8OdSoKqwWhdRkgZ44PWaP3jvZ73J9xfdH7nfM/KXKiTbPyvzAt/v5jntIVsofrNmlJVJp43mVUtJqLAsjUSlKsgYvv8ALa7G+JvWe+ewM18je2vkX0Nu6s21QY/pzub4/VeRpKvr7L/xEVGfrdxQYSWuyuepcrSxU9P9hJi6+hlpfuRIEnamliC2ySbVFeSvul5e2z+HS2uLEgNHIT8bZV9OkaSEOohmGMMJc+9Byv7y82cvcs2HtfyZyvzHsiXbSb5sXMqoy3kejTCsJlCRwtGxZvEE0cgfw6VQSKxzf5sf8wTon5CfG74+/GLqntTfHyg3J1bvWu3rvD5N9i7FbYWd3AqYncmHx+CoMXUYbbNc0NbT7lQVbyY6BnTD0bSSVE7TSk95w5ltdy2vZ9iguZL6W0LtJudwmh5NRwsYLM4Sh7tfcdCGpOo9RB9yr7tHuL7Ze63uX7t85cn7fyjtW77em32PKW13f1kMNZIJXmeRZZ0qhgOgCVqGeUKqIFXqq/4tf8Dd6/8ALDAf9DZj3M33S/8Alet5/wClf/1mj6xb/v2f+nTexv8A0ttx/wC0a36HLd3/AAKi/wBeX/eo/fZTkz/cH/ajr4kveb/kvR/a/wDhHSVT6f7H/iB7Fr/EeoVfj1z92j8+qdSPbnXuve/dMHift67H1H+uP979+611IH1H+uP979+60eB6z+/dMddj6j/XH+9+/daPA9Z/fumOs4+g/wBYf717unHr3WWP8/7D/ifdx8TdMv8AEesnvY4n7eq9ZU+n+x/4ge99NPx65+/dU6yR/n/Yf8T7903J5dZPfum+syfpH+x/3s+/de65j6j/AFx/vfv3TB4n7es/v3Wuqr/YJ/H+fWeHXJP1D/Y/70fdz8HVX+E9SU+v+w/4ke9p8I6Z6y+7de697900/HrJH+f9h/xPv3VOpKfT/Y/8QPfumn49c/dz8A+3qnWcfQf6w/3r35uC9NyeXWWP8/7D/ifbvTfWZP1D/Y/70ffuqv8ACes3v3TPXvfuvdZI/wA/7D/ifdk+IdNyeXUiP8/7D/ifdpPLpvrJ7b6afj1mT9I/2P8AvZ9vJ8I6p1y92690oMZlXpWiWbVJCpQgjmSMKQfTf9Sj+n4/H9PdJBqRx6gjouktl8dJ48SK4bHnQ1/b0JHY2Hr+wOotz7d20sFdlMxj6WLHxvURU0UssOSoqh1eedkjiZYoGuGIsRb6+8W/ejlvc922HdLPb7YyXrGMolQtaSoxyxC/CD5566Xfcz9yuWeTPcnknmXmPcPB2O1kla4lVWcqGt5ox2IGcnWwBAGPPgeiCxfFDupLBsBjhb/q/wCJP4/2mpPvDmX295xQsG2Vq/8ANSH/AK2ddu7f74vsGw1LzZMQf+XS5/61dOcXxZ7jUENgscLkf8vzGH/epz7St7e84kUGyt/zkh/62dG0P3zPYBPi5rn/AOyO5/619O8Pxh7eW18Jjx/5Gcfb6W/Evth/brnM0psjf85If+tnRnF99b7vS1rzZcf9kdz/ANa+naH40dsqecRjvr+MxQn+n9H/AMPaVvbfnUin7jbh/vyH/rZ0Zxffg+7olNXNtz/2RXX/AFr6dIPjd2ov6sXjhyD/AMXej/H/ACF7TP7Z88GlNhb/AJyQ/wDWzoyi+/X925ANXN9z/wBkV1/1r6cofjr2eoIbG44XP/O1pT+P8CfaST2u57Y1GwN/zlg/62dGkH39fu1JWvN13+Vjdf8AWvqcvx97IgRpJaHGqiLqZv4nCQAAb/RTf2lb2n9wH+Hl85P+/YP+tvRkn94F92KNaPzheCnH/Ebr/rX1kh6W3wDcwY7/AM70/of+bftM3s57jtw5cP8Azmt/+tvS2L+8S+6wlNXOd4P+oC6/619OEfTe9FIJhx3Fj/wOH9AP+OXtLJ7L+5RyOWz/AM5rf/rb0ZRf3j33UkoG50vf+yC6/wCtfU9eot4Acpjvr/yuH/rz7RN7J+5pFBy0f+c9v/1t6M4/7yj7pi8edb7/ALl93/1r6zDp/eN7BMaSbj/gY35Fv+OHth/Y/wB0Ca/1YNP+a9t/1u6MIv7zH7pCla863/8A3L7v/rX06L0R2Bwftcd+T/wPF+QP+bX19pD7I+5xJP8AVk/857b/AK3dG8X95l90lAQectw/7l13/wBa+sv+gnf/APyrY3/zv/7A+229kPdAig5YP/Oe2/63dGEX95190Va15z3H/uXXf/WvrkOiN/XH7GM+o/5Tj/149p29jPdImo5XP/ZRa/8AW/oxi/vRPugJQtznuX/ctu/+gOuX+gbsAknwYwc/mvP/ABEB9tN7Fe6hNRysf+yi1/639GMX96d9zpaA86bl+W23f/QHXf8AoD7B/wCOGLH/AFXP/wARTH2w/sR7rE1HKp/7KLX/AK39GMX9619zVNNedNzwf+jbdf8AQHXZ+P3YTkAQ4n/Y17//AFMfbbewvuwcDlM1/wCei0/639GUP97L9y+IktzputP+lZdf9A9D10f1xuPr+Xc1RuBaBVycOKWk+0qTUkmjORM/kUxRlOKhbfW/P9PeSX3Z/aXnvlPm7dNy5m2M2tnJZ+FG3iwyan8VGpSKRyMKcmg65O/3tH34vYD7yftz7X7L7Scx3d3ue07jd3F6l1aTWwWOaCNEKtKoVzqQ1ANRg06VW6ZxLXIFNwFckXvySluPxwP9j76pcrQGCyoR6dfKD7rXy3m+xlHBADEgfMjpPJ9P9j/xA9iJ/iPUUPx65+7R+fVOpHtzr3XvfumDxP29dj6j/XH+9+/da6kD6j/XH+9+/daPA9Z/fumOux9R/rj/AHv37rR4HrP790x1nH0H+sP9693Tj17rLH+f9h/xPu4+JumX+I9ZPexxP29V6yp9P9j/AMQPe+mn49c/fuqdZI/z/sP+J9+6bk8usnv3TfWZP0j/AGP+9n37r3XMfUf64/3v37pg8T9vWf37rXVV/sE/j/PrPDrkn6h/sf8Aej7ufg6q/wAJ6kp9f9h/xI97T4R0z1l92691737pp+PWSP8AP+w/4n37qnUlPp/sf+IHv3TT8eufu5+Afb1TrOPoP9Yf71783Bem5PLrLH+f9h/xPt3pvrMn6h/sf96Pv3VX+E9Zvfumeve/de6yR/n/AGH/ABPuyfEOm5PLqRH+f9h/xPu0nl031k9t9NPx6zJ+kf7H/ez7eT4R1Trl7t17rOPoP9Yf71790weJ+3p/wW4cjgKgSUkjGF2BmpXP7UwNgSLg+OSw4Yc8c3HHsq3DarfcI9E0YJpg+Y/1f6vXo32bftx2K4FxYzkLWrp+Fvy8j6EZ+0VBGbH9gU9VCHAdXsNcZALIebqdJNwPwfz7CMvIlvIxKqp6keL3qu7WMJOsivThxH5HpxG94/oFJ/105/3v22Pb+HzRevN76yCprL+w9ZF3tGSB42+o50f7zb6+9/630H8K9N/6+01RmWlfTrP/AH1iH9lj/hoI/wB7J9+/1voP4V6u3vu9MNJ+w9d/32i/45v/AMkD/ivvX+t/D/AvTf8Ar8SfxSfsPUhN7Q6RYP8A4+g/Ww96/wBb+L/fa/tHVz78viksnD0PTBuXfEpxv29HdZqmZVaRlsFhjs72BNyzMFH0tYn2qtOQrJJdc8YKgcBTj0W7l73bpfWz2+2yMJiRqdwaAenEVJ/wV6QC7ly/4li/H9j/AKNb2af1L2j/AJR/9X7Og0fdLm/yvl/NT/0F1kG48wf92xf8kH/r4D79/UzaeH0/+D/N1Q+6fNw43q/sb/oLrmNyZcf247/10n/r578eTNqP+gD+XVT7p82n/iev7D/n6e8LuHIS5Ok+6kiNNHKJpwkZLFIvXp4kY+twF/2PtuTknbWjdYof1CKCpH+bpy393eY7a4gmvrv/ABVWBcANU0zTj59C4N709/0sf8PGR7K/9b2D/fS/tHQnPv8AmmGlr9h6zLvamt+l/wDgoR+P94t79/rexf77T+XWv9f40BMsgP2Hrl/fWnuPRJ/sUf8A4p70fb6HzjSv5de/1/h5zyfsPWVd7Uq3LalABudB4/PPpFhb3X/W9i/32P5deX7wAJoJpQfsP+QdZU3zRMNSM7g/mNGI/wBuFIPvw9vIv4F/aOvP7/lTRppQf6St/m6zDetLcD9z6/mNj/0b/vXuw9vYhnw1/l/n6YP3ggSKzS0+w9RqzdwliKwh2JuLBSLfUjUCALX/AKezrbuT4rV66AKefQP5i95JNxhKxO7E1FMjy860/wAvSKlnepleaQnUxta99IH0HP8Ar+xzbQpBEI0GB1BG4Xs24XUl1O1Xb+Q9OuSfT/Y/8QPdn+I9Fr8eufu0fn1TqR7c691737pg8T9vXY+o/wBcf73791rqQPqP9cf73791o8D1n9+6Y67H1H+uP979+60eB6z+/dMdZx9B/rD/AHr3dOPXussf5/2H/E+7j4m6Zf4j1k97HE/b1XrKn0/2P/ED3vpp+PXP37qnWSP8/wCw/wCJ9+6bk8usnv3TfWZP0j/Y/wC9n37r3XMfUf64/wB79+6YPE/b1n9+611Vf7BP4/z6zw65J+of7H/ej7ufg6q/wnqSn1/2H/Ej3tPhHTPWX3br3Xvfumn49ZI/z/sP+J9+6p1JT6f7H/iB7900/Hrn7ufgH29U6zj6D/WH+9e/NwXpuTy6yx/n/Yf8T7d6b6zJ+of7H/ej791V/hPWb37pnr3v3Xuskf5/2H/E+7J8Q6bk8upEf5/2H/E+7SeXTfWT2300/HrMn6R/sf8Aez7eT4R1Trl7t17rOPoP9Yf71790weJ+3rIfqn+sv+9+/dVPA9T6P7jzp9tq8n+0/S3+1/2dH9b8e9itccekU/heG3jfB/q4fPpdRavGmvTrt6tN9Or86b82v7fHAV49BiSmttNdNcV6zJ+of7H/AHo+/dU6ze/dUfh+fXvfumzx6yp9P9j/AMQPfutdMOY1+aK/6PGdP9NWo6/9ja3v3RlY6dD/AMVc/Z5f5emyP8/7D/ifful3WdPr/sP+JHv3VH4fn1l9+6a6f8Bo809/85oXT/wS51/4/q0+7pxPRVumrw4/4a/z6VPt3ok65p9f9h/xI9+6o/D8+svv3TXUes1/aVPj/V4m/wCSbjX/AMmX9+6fttPjxauFf+K/n0nYfPr/AMn8uv8A5tar2/x0/j/X49+6NZPD0/q6dP8AS6UVH/EfT5/FbUP85/nLcWt4/T/t+fdxqoacOii4+jz4WrV8uH8+nyP8/wCw/wCJ97j8+i6Ty65L/a/4Mfdl/F9vTfWdPp/sf+IHtt/iPTT8eufu0fn1TqR7c691737pg8T9vXY+o/1x/vfv3WupA+o/1x/vfv3WjwPWf37pjrsfUf64/wB79+60eB6z+/dMdZx9B/rD/evd049e6yx/n/Yf8T7uPibpl/iPWT3scT9vVesqfT/Y/wDED3vpp+PXP37qnWSP8/7D/iffum5PLrJ79031mT9I/wBj/vZ9+691zH1H+uP979+6YPE/b1n9+611/9k=">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="8963025"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>304800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4103" name="AutoShape 7" descr="data:image/jpg;base64,/9j/4AAQSkZJRgABAgEASABIAAD/7QAsUGhvdG9zaG9wIDMuMAA4QklNA+0AAAAAABAASAAAAAEAAQBIAAAAAQAB/+IMWElDQ19QUk9GSUxFAAEBAAAMSExpbm8CEAAAbW50clJHQiBYWVogB84AAgAJAAYAMQAAYWNzcE1TRlQAAAAASUVDIHNSR0IAAAAAAAAAAAAAAAAAAPbWAAEAAAAA0y1IUCAgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAARY3BydAAAAVAAAAAzZGVzYwAAAYQAAABsd3RwdAAAAfAAAAAUYmtwdAAAAgQAAAAUclhZWgAAAhgAAAAUZ1hZWgAAAiwAAAAUYlhZWgAAAkAAAAAUZG1uZAAAAlQAAABwZG1kZAAAAsQAAACIdnVlZAAAA0wAAACGdmlldwAAA9QAAAAkbHVtaQAAA/gAAAAUbWVhcwAABAwAAAAkdGVjaAAABDAAAAAMclRSQwAABDwAAAgMZ1RSQwAABDwAAAgMYlRSQwAABDwAAAgMdGV4dAAAAABDb3B5cmlnaHQgKGMpIDE5OTggSGV3bGV0dC1QYWNrYXJkIENvbXBhbnkAAGRlc2MAAAAAAAAAEnNSR0IgSUVDNjE5NjYtMi4xAAAAAAAAAAAAAAASc1JHQiBJRUM2MTk2Ni0yLjEAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFhZWiAAAAAAAADzUQABAAAAARbMWFlaIAAAAAAAAAAAAAAAAAAAAABYWVogAAAAAAAAb6IAADj1AAADkFhZWiAAAAAAAABimQAAt4UAABjaWFlaIAAAAAAAACSgAAAPhAAAts9kZXNjAAAAAAAAABZJRUMgaHR0cDovL3d3dy5pZWMuY2gAAAAAAAAAAAAAABZJRUMgaHR0cDovL3d3dy5pZWMuY2gAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZGVzYwAAAAAAAAAuSUVDIDYxOTY2LTIuMSBEZWZhdWx0IFJHQiBjb2xvdXIgc3BhY2UgLSBzUkdCAAAAAAAAAAAAAAAuSUVDIDYxOTY2LTIuMSBEZWZhdWx0IFJHQiBjb2xvdXIgc3BhY2UgLSBzUkdCAAAAAAAAAAAAAAAAAAAAAAAAAAAAAGRlc2MAAAAAAAAALFJlZmVyZW5jZSBWaWV3aW5nIENvbmRpdGlvbiBpbiBJRUM2MTk2Ni0yLjEAAAAAAAAAAAAAACxSZWZlcmVuY2UgVmlld2luZyBDb25kaXRpb24gaW4gSUVDNjE5NjYtMi4xAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAB2aWV3AAAAAAATpP4AFF8uABDPFAAD7cwABBMLAANcngAAAAFYWVogAAAAAABMCVYAUAAAAFcf521lYXMAAAAAAAAAAQAAAAAAAAAAAAAAAAAAAAAAAAKPAAAAAnNpZyAAAAAAQ1JUIGN1cnYAAAAAAAAEAAAAAAUACgAPABQAGQAeACMAKAAtADIANwA7AEAARQBKAE8AVABZAF4AYwBoAG0AcgB3AHwAgQCGAIsAkACVAJoAnwCkAKkArgCyALcAvADBAMYAywDQANUA2wDgAOUA6wDwAPYA+wEBAQcBDQETARkBHwElASsBMgE4AT4BRQFMAVIBWQFgAWcBbgF1AXwBgwGLAZIBmgGhAakBsQG5AcEByQHRAdkB4QHpAfIB+gIDAgwCFAIdAiYCLwI4AkECSwJUAl0CZwJxAnoChAKOApgCogKsArYCwQLLAtUC4ALrAvUDAAMLAxYDIQMtAzgDQwNPA1oDZgNyA34DigOWA6IDrgO6A8cD0wPgA+wD+QQGBBMEIAQtBDsESARVBGMEcQR+BIwEmgSoBLYExATTBOEE8AT+BQ0FHAUrBToFSQVYBWcFdwWGBZYFpgW1BcUF1QXlBfYGBgYWBicGNwZIBlkGagZ7BowGnQavBsAG0QbjBvUHBwcZBysHPQdPB2EHdAeGB5kHrAe/B9IH5Qf4CAsIHwgyCEYIWghuCIIIlgiqCL4I0gjnCPsJEAklCToJTwlkCXkJjwmkCboJzwnlCfsKEQonCj0KVApqCoEKmAquCsUK3ArzCwsLIgs5C1ELaQuAC5gLsAvIC+EL+QwSDCoMQwxcDHUMjgynDMAM2QzzDQ0NJg1ADVoNdA2ODakNww3eDfgOEw4uDkkOZA5/DpsOtg7SDu4PCQ8lD0EPXg96D5YPsw/PD+wQCRAmEEMQYRB+EJsQuRDXEPURExExEU8RbRGMEaoRyRHoEgcSJhJFEmQShBKjEsMS4xMDEyMTQxNjE4MTpBPFE+UUBhQnFEkUahSLFK0UzhTwFRIVNBVWFXgVmxW9FeAWAxYmFkkWbBaPFrIW1hb6Fx0XQRdlF4kXrhfSF/cYGxhAGGUYihivGNUY+hkgGUUZaxmRGbcZ3RoEGioaURp3Gp4axRrsGxQbOxtjG4obshvaHAIcKhxSHHscoxzMHPUdHh1HHXAdmR3DHeweFh5AHmoelB6+HukfEx8+H2kflB+/H+ogFSBBIGwgmCDEIPAhHCFIIXUhoSHOIfsiJyJVIoIiryLdIwojOCNmI5QjwiPwJB8kTSR8JKsk2iUJJTglaCWXJccl9yYnJlcmhya3JugnGCdJJ3onqyfcKA0oPyhxKKIo1CkGKTgpaymdKdAqAio1KmgqmyrPKwIrNitpK50r0SwFLDksbiyiLNctDC1BLXYtqy3hLhYuTC6CLrcu7i8kL1ovkS/HL/4wNTBsMKQw2zESMUoxgjG6MfIyKjJjMpsy1DMNM0YzfzO4M/E0KzRlNJ402DUTNU01hzXCNf02NzZyNq426TckN2A3nDfXOBQ4UDiMOMg5BTlCOX85vDn5OjY6dDqyOu87LTtrO6o76DwnPGU8pDzjPSI9YT2hPeA+ID5gPqA+4D8hP2E/oj/iQCNAZECmQOdBKUFqQaxB7kIwQnJCtUL3QzpDfUPARANER0SKRM5FEkVVRZpF3kYiRmdGq0bwRzVHe0fASAVIS0iRSNdJHUljSalJ8Eo3Sn1KxEsMS1NLmkviTCpMcky6TQJNSk2TTdxOJU5uTrdPAE9JT5NP3VAnUHFQu1EGUVBRm1HmUjFSfFLHUxNTX1OqU/ZUQlSPVNtVKFV1VcJWD1ZcVqlW91dEV5JX4FgvWH1Yy1kaWWlZuFoHWlZaplr1W0VblVvlXDVchlzWXSddeF3JXhpebF69Xw9fYV+zYAVgV2CqYPxhT2GiYfViSWKcYvBjQ2OXY+tkQGSUZOllPWWSZedmPWaSZuhnPWeTZ+loP2iWaOxpQ2maafFqSGqfavdrT2una/9sV2yvbQhtYG25bhJua27Ebx5veG/RcCtwhnDgcTpxlXHwcktypnMBc11zuHQUdHB0zHUodYV14XY+dpt2+HdWd7N4EXhueMx5KnmJeed6RnqlewR7Y3vCfCF8gXzhfUF9oX4BfmJ+wn8jf4R/5YBHgKiBCoFrgc2CMIKSgvSDV4O6hB2EgITjhUeFq4YOhnKG14c7h5+IBIhpiM6JM4mZif6KZIrKizCLlov8jGOMyo0xjZiN/45mjs6PNo+ekAaQbpDWkT+RqJIRknqS45NNk7aUIJSKlPSVX5XJljSWn5cKl3WX4JhMmLiZJJmQmfyaaJrVm0Kbr5wcnImc951kndKeQJ6unx2fi5/6oGmg2KFHobaiJqKWowajdqPmpFakx6U4pammGqaLpv2nbqfgqFKoxKk3qamqHKqPqwKrdavprFys0K1ErbiuLa6hrxavi7AAsHWw6rFgsdayS7LCszizrrQltJy1E7WKtgG2ebbwt2i34LhZuNG5SrnCuju6tbsuu6e8IbybvRW9j74KvoS+/796v/XAcMDswWfB48JfwtvDWMPUxFHEzsVLxcjGRsbDx0HHv8g9yLzJOsm5yjjKt8s2y7bMNcy1zTXNtc42zrbPN8+40DnQutE80b7SP9LB00TTxtRJ1MvVTtXR1lXW2Ndc1+DYZNjo2WzZ8dp22vvbgNwF3IrdEN2W3hzeot8p36/gNuC94UThzOJT4tvjY+Pr5HPk/OWE5g3mlucf56noMui86Ubp0Opb6uXrcOv77IbtEe2c7ijutO9A78zwWPDl8XLx//KM8xnzp/Q09ML1UPXe9m32+/eK+Bn4qPk4+cf6V/rn+3f8B/yY/Sn9uv5L/tz/bf///+4AE0Fkb2JlAGQAAAAAAQUAAklE/9sAhAABAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAgICAgICAgICAgIDAwMDAwMDAwMDAQEBAQEBAQEBAQECAgECAgMCAgICAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwMEBAQEBAQEBAQEBAQEBAQEBAQEBAT/wAARCAEEAcsDAREAAhEBAxEB/8QBogAAAAYCAwEAAAAAAAAAAAAABwgGBQQJAwoCAQALAQAABgMBAQEAAAAAAAAAAAAGBQQDBwIIAQkACgsQAAIBAwQBAwMCAwMDAgYJdQECAwQRBRIGIQcTIgAIMRRBMiMVCVFCFmEkMxdScYEYYpElQ6Gx8CY0cgoZwdE1J+FTNoLxkqJEVHNFRjdHYyhVVlcassLS4vJkg3SThGWjs8PT4yk4ZvN1Kjk6SElKWFlaZ2hpanZ3eHl6hYaHiImKlJWWl5iZmqSlpqeoqaq0tba3uLm6xMXGx8jJytTV1tfY2drk5ebn6Onq9PX29/j5+hEAAgEDAgQEAwUEBAQGBgVtAQIDEQQhEgUxBgAiE0FRBzJhFHEIQoEjkRVSoWIWMwmxJMHRQ3LwF+GCNCWSUxhjRPGisiY1GVQ2RWQnCnODk0Z0wtLi8lVldVY3hIWjs8PT4/MpGpSktMTU5PSVpbXF1eX1KEdXZjh2hpamtsbW5vZnd4eXp7fH1+f3SFhoeIiYqLjI2Oj4OUlZaXmJmam5ydnp+So6SlpqeoqaqrrK2ur6/9oADAMBAAIRAxEAPwDf49+691737r3Xvfuvde9+691Xf2xn49q703bW5bHLnstkohFgVyEiVWHxGQE0kFXUVmOLlqk0eOETUMTnw+R9bK4ABMXY+FF5RAcBxb0z6evrw6KlhT6id2q0pONWQv2D7KU/M9FlFVM5WaWqfyiCVI2b1GOJj6YUAsqRamb+gP8AT2yCTk+denSKEr5Y6sT2bCa3ZWxcpkPFTTVO36IBKTXJJPFTxeCN3mYMqPMUWwVbj6fj3RD2aRWgPR7bIZEDHAoOH2dDXS1dBBDQ00ciU5nj1tGKiN5IZSimTyNqILNqt9bn+ntohmJY8etiJv1CFqqn049NVfXEVLqJvJEgsqj1KbWDH/AFrfm/txRQVp0tghGjVpoxPWE5O0LIwGuxueSLLayhV5BBuP8AY+/aKnrT2tXBX4em6pyEs8X280cFUhR441kQ6okNvQ7Cx8ar9Pz/AE9+4ZHXjbAVIHHiPXpBZbHSJBUyYyKKWI6dcOrT+0dX+aLm6AvyRzYW9uI9PiGOk8tl2kgUb0P+rHQHZKJnknDgfdJJIjrqISFlPqvf9ZC83Fxzx7UawKkGo9B0VNEaZB11pn/J69JljE8nj0aooiGU2cFi1wFQ8sl2/H+HvesGgPHpjRQ4yo9epdNRQSI8pisYdet3e4QhSEUKOWYnkAe22apArUnh0tt4VKltPCpNT+zpVwNPjtlbqrWllmpqiigwlHFKdSJVVr6rrEwHKQhrBT9Rz9Pdo1/UVQeGeqXahLdiB2nA/PHRaKXKPhtwST0syhVqGv62VHhcKKmPUnIexNiOQ3591chZjQj/AFceixVqlaGoH59CZh9y0LRU8NQtOjVE8pE0ocM9OzFItUouqxAre34P09uNIgJ7vs60EY4p9vQ9UWB2U1HDUwb7pUnlgiqngmgT/JpbXkp5SnqidLHR9SwF+L+2vEY17Bx9enxHFxEhqR59O+OyuSxkzDF7gqauBdKxTw1VQKSZRaw8VTf0KeOALn6ce6OFIqVz1ZS6kgOSP9Xr0JeJ33m9Kirjpa1SBeQoYZAL2N/FZNX+w/HtkoD8ung58+lnTb0oZCoqqeelvYFwPMik/ltIDgf7A290K+hz1fV6jpUU1dR1i6qWpgnH1tHIrMP9db6l/wBiPdaHq3Um/wBf8P8AigPvXXuuvqwt9Ob/AOvb6G39Pfuvdcvfuvde9+691737r3Xvfuvde9+691737r3Xvfuvde9+691737r3Xvfuvde9+691737r3Xvfuvde9+691737r3XvfuvdJncOcfHLHRUIWTJ1Skx6hqipIb6Wqp1uNVjwif22H9AfdlWp+XWx8+kxR0wQpFKfO9UROJZjreWuiJlUyEn1mdCwt9Bfj26cUNMdVLE1oelxSzRywxzR2EbJcBQBp4sQAAL2t7bYGoHWgcmvHrKZQR9Rb+g5v/T/ABJA960mox1vptnqgtz9OObkXIvwL/4H26q0x59b6TmZy1LjoRW5Gto6KmAbVPVzJCgXSSR6mDMQRawu1/booo7jTry1c6VUk/LqBhcrFuiNv7ugV1DA3hmyrpLFjmdlvLDT1DIr1ckYIDCMHQbXPv3ixgHNT1Vo3U9y0J8uhExlHLQ0iU01QalkaQq+gRhEdyywqLsWWIGwJ5I9pnbWxanWwKCnTh7p1vr3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de697917oFexOkds9gZSHNVdRV4zIJT/bTSUMVO8dYVZTBPVxToweeGMGMPe5UgE2UD26JmCBKAgcK9MPbJI5fUVY8dJ4/yPQU9sdN7Q2n1tkZds4hYKyirKetqa6d2rMhUU7xNRzM88n+bjDTK2lAiBhe1/bts2qRwx4r/g9OqzRKkIaMHtNSeJ9OJ6UHSxh3b1BtWOCpMNbtx8jiKkg3KVFPPLURU8hc6lWSlqY21C9h9PbIJVmA9a9GljNpQYqCAD+WP83T+KhGke5jAWRXhUAMhCuNTSMRrZDpsL2sPbwFT8+j2NRUVrTqTV5iWOWWaQQpREIkKhHFVPWmRtRI5QUpTRoCgk2JNvp71w8vLPWyunSBw8v9nriK95X1o+ngKP68kl2IJFzq4/Hv1c8MdeAHE9RDOZJAsjkaWdXCnxh7c34/VYnjnn3rq2pAQtfl1Fyr1JopUgAV39MaqAxTRGJH9A51Op4J4Pv1Rgnh0xNq09uT0B+dAdlWaOawXWZHBDakN5OCQdR+j/09u4p24/1ceiSQ1ZgwyOPTVS40SwxyPIY5SzlyLEKjENFYg6gzIf8AYe2tepiAKj/VnpyO2BjVnajHJ6k4+mNVWx0dMJEjWQEyFQSyXJeqkJtd7Gygng/4e1AGgamFT/qx1pV8VhFEKIDX/ob/ADdMfYW84DBS4vG+SPA4gtFRwu4f+LZlrpUVPAtKkJuocA3LErwR7dBCIXemo5P+QdF24SxyPHBEf00/mf8AVw64YX46b2q6PG7lz8MVLSV8omqMM7TDJ09HKvkSStEaf5H5ncDxgmRR+sKePaBW8RydXn+37Pl8+m2jZFAoPs9Pt6fd5bUx23ZMFQR0lNTxPQyRvEqswE9IyxrJG7s8g86Pz9BcX+vtWi9lCPOgr0leoYZz8v8AD03bY2/Pl8vBi6IIskxDy1EpKwUdKpBqKiZj+hIU+n5Y2A5PtmUKlSDk8AOn4gZGCgD7ejVQ4XZ+Ghio8djkylTEgWaurZJZgxZbFwhZYQzEk2UWX+vtmpp3PX5DpWyImFSp+fSix0OLVV/yClja4PoS6X5ANuQL+9inVCP9VOnySmxcqlXp4Rb6ug0WH4Uaf6+60IIoTT/V+XViME0z0lq/EKL1GJyBpZ1Nh6tBNwTYuhDBzb88e3Pt6aNQcY6b496bl2+VGVo/4nRD6za7yAAX1CpjVwBb/Vj3rw1bhg/y634hHEVHSwwHZO1M9LHSQ5AUddIpYUldanZ2As6RTk+CZlJ+ga5/p7o0TrmmPl1dZEbg2fQ9L4fQcW/wvf8Aw/2PHtvq/Xfv3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de697917oPc3QimzD1SqSa5I5VZixBkgAjkj1m9gAFYL+nk+1ERqpA4jqp+fDrDVDx0nnjus0OiaO/JvG2oEDlbX/3ge7lcHqoPdQ/Z13i8mxqZqNbutRCcpSaCW8ayPorKYj6j7acH/AAj3UDy6sRTP7emTO9iYDAu0VXWiWqAa1DjkWrqgwax1aG8UYv/qiLe6s8acWz6Dp1IZXFVGPU9J6q3Lm8vSkUE9FQV8qfc0+PoI/7zZxqa2uFpoKBZKPHzSAi/kJKHg8+9B6jFAfTier+GqnuBK+p7R/PJ6BP/KavK0mUyD1VdLTVQeoqc3JFXhNUpheOGnr3XHxyxOzWUowLj6H6e2kVncGhIB4npZRVQotKkYC/7HQq4hqoVEL0G/dy0dclZqiwrR42WiqCrLGlO9DHj4KR1nAUFIgsiqb/AFFwraNTljwHSVlkRQTbDQfxZ/w9GYTVoXWAH0rqC/pDWGoD/AH2j6T9cvfuvddMwUFmIVQLlmIAA/qSeAPfuvdJXKb127im8UtclTUkXWmorVMh4vy6kQJ/yE4t790YQbZe3FCsJVP4nwP8/wDLpNx77zNfHNVYfbAraandUkR8pFHVSFubRRpBImoL9eSAfqfe6H06XDZ4EYR3N+EkIqDpJX9telftvcdDufHDIUSyxFJpKWspKhdFTRVsFhNTTL9CV1AqwurKQR710W31lNYTmCahwGVl4Mp4EdKD37pH1737r3Xvfuvde9+691737r3Xvfuvde9+691737r3XRFxb/fcG/v3XumHcWGhzuIyOJqiPt8lQ1VBMxPCiojZYpAAP1RSkH/W93jco6uOINetkB1eOmCKdEr6F3GNg703V1ZuaQ49splDHjZZCBDDnqdJKdo/JcBFylMUMLcguigct7dnUBzIvw/4RxHTNpKY28NssD/xY/PH+o9Dnujbc+JqEFHJVw0l4pGqypm87KX8lLUsRoVZNX14A+t7396Vqrg93QqtJlnjBLAP6D06TlZVGAwyShmLWdQQ5aIBeSGI0+lBa4Fv949+JoP8HV3rU56kUs9LNKJlqEg/zURMt0ihWVrqJEA/TJe5YAn3XUcnpsOQMjqc00FJWeOqmp0Q+RWlR1qwrwqCoVI2PNRq0qR/Qk8e9/6qnqldVDWo6b6rchRHhpAialZnlkVNZuNBBRr2Iv8AU/VQPftYHW2fyHwjHQe5KnE7Gf0yygMEPLALwzkLyAuvk2Fv9j70S9KasDpgxqW1FR9pz11h9ux1brJlKjRj42mlkpqUmGsYqmtAZGDKqVEtl1abqv0B97iIAIHxfPptoWfBb9PiQOPSO3dm6HDplaKik+wp73yFYXaWWiim5/g9PI3rmr6lAA7C3jjNvqTZVGKt4jjAGPs4V/zdF97cpbRtbQf2hPcQf9X+x0I3Q3Vcmbmg7I3rikWnVIm2Pg6uNtFPTrq05ypopF0h5V0Gl1gm15bD9tvaSebxjpH9kuPt/wBXn0hgh8IeI39ocj5fP7T5enRyWUEEWvcEEf1v/UH6+2un+ikdsLgcJ2Hts1ERakpNv5DKTwNL5BU1UNRUTUFMRIWK08tVEqupsGTj2ujLPFniWpX5Yr+3pHII0mQ0xQn/ADdJDYrvFiKzINAi1GcrHqTOCQz0iMyx06qRpjpVqSz2FtVh+APaeRi7vpOBj/P0/EBHECydxyPz/wAnQ5bWw1dXCOWokEFO5spcnyMgF9WnjTD+Af8AePfu0CoHVQXY93n0JlPt2OBCvlEjEArqU29NyLMDbm/uusYx05RvIjqPU4qsjVtKrIvJDI3q/wBbQeTp/wAPewy8OHVwKjyr0kMjTywqWljdSBa7KxAPJ/HI93Brw68YzStMcOkfVZOqSJokYabNqZhq1/hUF7qQfx72BWvTTChr5dB5lcRtzLI8dWtVhqwXcZLGNqKSC51TULFUcl7EspUgD8+7gtTtz69U0I1S2KeY/wA3n0lKnsftHqKXGyS5Cn3XtOaUpTyVBlqKapp1uTCk5vX4mqVTe0g0g/hh7oyh6nTnzpxH2j/L1YeJFTUaxngfX8+I6Mx1/wB6bI35FDCtX/AM1I6QnDZiSOGSWdxdVoKu601cr/2QCshP9ge2WQjhkdXWRGoAe706Gf3Tq/Xvfuvde9+691737r3Xvfuvde9+691737r3Xvfuvde9+691737r3Xvfuvde9+691737r3XvfuvdJ/clP5Mc1Sq6pKB1qgBe5iXioXj8eIlv+QfbsRo49DjrRrTHSNrZa6SGQ42jnyJiieWQRALB9uFZyhnkAieVkHpRNTt9Le1DMqYJz1pF1GpwOglpq6rzcc7U0ddW0lKgIx9DkI9v42Jqk6p467O1BWZlaIAGCNvp9Rfj204LepPoMfz6U0WOhJCmvEip/IdBhn9tGgqDLTZjbk9fWGWamwG3mr8ilEklvHD5vE88sq8ktIApt/Uj2maFsmoB9OlsDmQhFjcj1NM/l0Ku0KLd74ePGYdsbs+JSpyddRUxmyuQqGUSNIkLSXoVK/6uRTf/AG3tSq9i1UD1P+Wnn1SaBI5B4up2PAV4D0J4dKan6owz1JyFXLPlJKcvNHU5SoaodqiUBnn8QWOgpTruTZXKnkm/vWARqqTXy6VJcQQqgSIGU/FXh9gHn9vTRSZ+j2/lJ6VqOWrnoJoJaf7fw+BpYZC8szFxqLrRtINSC7BuPdmWoIrTz6Npx9XDGVXtYFGrg5wKD/TU6HjI7p29iqT76uy9DBTGMSK5qI2MiEXBjRWLuSPwAT7TYAqTQdBiOyupZDGsJDg0NcU+2vQL5jvSCab7fa2PkrISpH39RDKdTlrI0NONCiAAEl5GF78D3oHUwVFLMeAA6N4tnhjBe9ugAOIUgfzPSDl3rmdxZJaaryFVL5VkBpqeGSWhRgurxgyfbUcdSSCosj2YfX2sSxnahk0qPQ5P5gdKEuNutkP01uTQ/HwqOGGbJGfLpY0NHEKJEoKeh8uiMtRZWP8AiZaNjrapbUUUPL+ltIAB9qbeCBuyQEj1GOk27Xl9AfEjfSpFNQ9f8h6XG3dyJN95QVGMoKB6Ep4lxKylYqcoNVXoZB54457iQITIi+qzC5Dd7Z/TeHIjFoW4k0qP9Q6I7W8kuyfEZvEByCahgR60wfl1H2pT1W3N55ikmZGxe6J5arHaJdRhqoYmqzBPG1mjk8TyqrfSRVXni3svoQKkY6Eu6GO92y0nRSLiBQslRxFdNR65p9mehi9+6C3Xvfuvde9+691737r3Xvfuvde9+691737r3Xvfuvde9+6910QCLHn/AF/fuvdFg736iG5Um3Tg6G+YEKLkZKRVFY32an7OuiVAJJ5EFo5QDq8ahgLr7UwyKVMbn7OmJo6968RxH+b59JjrDvZoGpdjdpMtPWxotHRbplIajrYtASCHOM4KCVk9P3P6X48gVtTmjwsmQP2dOQ3FKVbPrwz/AJD0P9bsLEZJHqfu6qoSXVPTSJMs0QSRQ0QiZOJYfJZgLgMvH6fdC1eI6NVvmIVSg8q0/wAPQattiV5qfHwUlbHUQPURTVMyPEkuj0oYtYWFRT2BupJKm44Hv2F4nz6XakPfUaccOoku1cpTI7VMK+BRGn3HnjaRZWkfVYIGaRxa5J4RSOfx79g+fXi6HhXqRS7LkWKoqa2YIGp4paRAqkSyuzMCTe7xCDgsPp/T3oUJB9fTpssK4FTwPUybAYmKjp/sw8lXH5DPNUsEoxMF1GCMEKEp05Ik+lr393VDTJ/Z1shhUvw8ugV3ju6mxdLXLHW09LSsxppsrGQ82QYAieDb0SjTO0N/G1SR41Y+nkX9qI48lmx/kP8An+X7ei68vgiGOE5PE/5v8/T51F01UbsqcdvTetHNSbao5Vrdr7WrQXlyjMA0eZzglu0lPLZXjjcaqj9TWjsJGZ5vErGn9mOJ9f8AV/xXRZHGdXiyfEeAP+E/5ujrAAAACwFgAOAAPoAB9APbHT/Xj9OPqSLf77/D37r3REPkIK2p33kq0FI8bgtv4PGSSOyl5Mhl5KqopIIYr6mleN2JP6VVbnkj2ZQECBR50Zv2dILkEyV/CAB+ZJ6GfZu04JYMPR1SPTrRUVNCsZRVfW9NEzIwtpYcluf6+yxajPrk/Pz6OnRSqmnwjH7Ohw/g1NFEBCzr4wSushlJAFr2UEKLfQe3NVaAjpEUB4cemabMu4NK6/aqHURzAMA4Q830k6UP5I+n597AANePVihAocHrguYqEYR+UyDkG5V9Tkgix/KN+Dcce7aV9OqHV5HrO+RgmiP3EUdTzZgEGt1A/Tc8Alj9B9R71o9D1ZJWHl0la/a9HmBUyQVEdJWzB5IKYGPwLotoQleUsv1sPe6spApjp4FWX4c+ZHQFbgweXxbyxVELF/O8ajS2l1U6fIr/AKWTj8e3NYGSOm2tnI7SGqeHSBpstJRVcsdTTx1ePmieOqx9ageGQN6Po6N4mdb2I4I+vt4qHUGtGHmOmo3ktyyOtU80b/VjplyfXGJydNU5LZdUy1MTCofb9YSfI1i7RUMpA8bXHp1nQ30DAi3toFkYCTFfMcOtvaxyqZLMmg4oePT3sDujdG0A8MkrZ7GU7+Ou25X1Mv39BpN5JsdVSxvJCoVCDGdUaseQOD7s8QfIw3y6SJM8ddQJX58R0dTZXYO2d+0C1mCrladYw9ZiqnTDlKAkhSKql1Fgmo2Ei6o2uLNfj2kZSho3StHVxVT0tvder9e9+691737r3Xvfuvde9+691737r3Xvfuvde9+691737r3Xvfuvde9+691737r3XTKGBVgGVgVZWAIYEWIIPBBHv3Xuo88DNSTU9K60rtTyw08iINNO7RskUixjSLRMQQOPp7351690XPKYjN4zH0mJyENHiqPF05YJjYInFassuiryIqSzJcy2L+RRIvkAt+fatWQ1K1+w9GVhbJdS/qNkmg+3yHSqwGz6Chwkn8PpxJUZuGSoaqWMRLGrm8ZnqriaSL0g+trMTYC3tuoqx4D18+lVxOtvcBVj0iMhdNak046vn8usu3I4ME1dJkHIWIlf4fQSrVqzxnW1RVSqTBBGFIt5GW3+wHuuteCn8z07epJcpA8a1HEMw0jPkB5/kD0HG8vkDSY/KR7ewVHi2neGKWavyM7y0kCynV4liWNRNUIqXNgyC4sT+GGlRGA4t68B/n6bg2ypY3M7K3oMH9p6TOF/vXu6riyTwChxtXUTSLuGaiURyJ6gRi8fUPA9TM8i6RI1okPLGwsfB5ZaGtF9ejQRxwxFInrpAxX/AAkZ6fjt/CTVUaUGPq83kIyyua2aXIaJ01ASVTU6U2Pp4h9TDTq6k8avfvDB+Z6WRxKiM95L2nPktQfStWJ+Z/Z0tqLaOQqqZqXMLRwosqNBQ4emSgpKdT6nEn24HmmY8EnVpt9fz7VwSNCpC0yPLotvBYSFGhBoOHid3D7fLqFmNrRYeCkrKSNogKkRSvrMrwSsQ0UqOxuuuRQCPpz7Ui5IDAVz0ihj+qmdJaGgqMU/LpzxVKgqnmVvHFU0MzKqKzyq2jXUw6wSA8UyNYDixHtpJdLV+fSncbdp7BU4yKQCT+wH8wes4xBp6WTJUchSojCVepAAWClWVin0kVgRqX8i9/a6S4WULGwqvDPQatLZoZip4EkED164bszCSU+39w0cipKKrzqP7S19E4lqaMkC4uVlUg8FT/iPZXJGY2MbcAf+K6GGywiaC9s5RkpT8jgH8sfn0NdDWQ5CipK+mZXgrKeGpiZWDApNGsi+ocEgNY/4+05xjoIyxNDLJE4o6sVP2jqV79031737r3Xvfuvde9+691737r3Xvfuvde9+6914kAEk2A5JPAAH1JPv3Xuo1NWU1YjPSzRzKrFGKG9iP+iWtcH6Ecj3706dlhlhIWVCrEVoepPv3TXQNdidLba355Ksk4nKS6BUVEECTU1cEPH3lL6D5j9PNGySAfXUOPbyTsoCnK/P/J028SuanDeo/wAvQA1WF7a6QdUwFdlcptcv5Qi0zbhwsFyPJFNj2UZLGq/+qhYC35Nvb48CUV4N6dN/qxEU7k/1eXH9nSzwnyc25Wwfbbtxc1JUqms1eCf7ykYgm5WnrGpq2lf8Ff3f8T7aaAg0Vv29ORXNDUVBH7OlJUd79ZRCEw5tIoZ2V2QUVUapYnhWR4CqRPHFOZTZmuRe4/x918BqZI/aOl63MOkF5+6noaV6DXM/I3ZsdVqijyGQSFnVZmpjBApH0VYT+7JH/iALfnj25pVQNTgfz6v9fAtUjViKcRj/AA9IZuw959ly/wAC2RtXIVvldolllQx4qKFmCipyDAJB40LDUZ5fGPppPvfipHXHy+f+fpHNeXE40oKIf9XHh0YDYHx8xWJqoNy7+qYt4bqUwzQxSo38Aw0kS/tw4+hfTHUrAf0NIiovGmMEBvaZ5HkoGwo4Af6v9Xz6ZSNUNSdT+p/yf6v2dGP916c697917ro3tx9eP975/wB49+691Xl2XWVu4+5MttiB2jiyG89rwBCS6a8PRU9OJGUc20yOQL/n2vNFtvtSn7TXpKlXvFTyDA/sHRzDUCDNwCZEjfRCHKrpbTp4L2ItIFW1zbj2jYgUz8h0dlaxsR5nHS0eshaMks6RsrfuaG+gHqtxccHg/wBfdOHSHQQf8nSOeeGQvT6S6NraJyo0hVOn6+kxnSbj8n3cOPy6UlKrQ9J2qiNK0cnrjp5TpDqQ8Vhx9TbmwPHFz7stadvD06RSoEOaj59OdROPDFUq6yQwFFeSJCU1lf1VMQ9ZfTwdQuAP9j7uACcfF6Hp6HQ1BItR5MOkNuOTKo33lCxkgnjJeWnjYmISEIsaCNrji5uPrf2/GFIoxz1aeKSMDwkqnE+fSHqex6mOjq8TmqcZCnkWClFXDohqaYXMYVfJqSVgouzEryLE+7+CoNa0xivSE3MqVYLWhzTHD5dI3P4ynqY5qjBVbVf2yeeSmdQKmmRlBaCRGJaSNALgi4F7+6gaH0twPp1Z5xdRgq/6gPA+nmOkfjcjXUVVDWwyRmaIqpCkorQ8M0Li5BRm+o+v5Hu7KjqUI/1evTEc0scglXiMH5j06eNx4FczFS722xRU43DRCaXJYwrCkGVoUjkataQyOqmvp419OkapUHHqAuwtY20McjgellzGlxGLmEUelWB/1cR0hsZWzZHI0OW2jUT4jdtMXnonoHWmizaKuswU0ZAijyka6lkgIMNWt7KH4Z9grUDfCcDotWvFMSCpx5/l/k6Nv1V3vRbrNNt7d0KYLdeoUscrq8GMzdUgbWlOZF047IErY08rDySf5skkIEUkLJVh8P8Ag6VxTK9FJ7/9X+qnRi/bPT/Xvfuvde9+691737r3Xvfuvde9+691737r3Xvfuvde9+691737r3Xvfuvde9+691HqqulooWqKyogpYEBLy1EqRRqBybs5Ue/dORQyzyLFDGzyHAVRU/y6Q2VrhuIU5wtDJWrRzSlq2uRqTDTQSxGCppnknUS1MU6OCpjRl1qDfj3tWzjo6gtDt+v624VGZcRIdUla1BoKhaEeZ4Hh1GqcTmocdQ4/FJDVxqiwu1bUyY/DY+nQFkIpoQKzJpqOkBmA4BPveBXrZvYDPLOy6JSa4GuQn7T2ofs6RldtkLNT02byyZ6epmYLg8cyY/CUJCGQ1FXFA3nmiBFtAUO5tcgXPu4iciug6R5nh0/HfxuWaOsdMeI/dI3yWuB9vAdOo2tX1dfFXy1uDDU9OlLRTJtTF/c0dKiALSwVMsbzxU6iwX9wlbn3rwxWv+HpkzWiAj6Vi1aks7Gp9T8/XHSij2zT1EkMmVq63LeNQBTVcqx0kfptpFJAqxOt+fV70w4knptr50RxAix1PxLxP5np1lpZ6V6aPHwUcdKZWNWtjG0dOIm0imSJLSTGbT+sgab/AJ9+FSOPDplZvEBMhJfyJ6mxwXYELp1W5Xkkfkm/AP19+49VaWgIrXrHX42KuoKyklWwqoGjDEX8Ui+qGUccFJAPpb3rUeNOqRXDRSxuv4TX7fl0GW3tQyRopP256eSVZFA484D09QrKRqUFtDA/ke3AehJcSVtXcCqMAQflWo/l0qMPGtRjzBKB56My08qAjgM5B9IP6QbgH8Ee76zXj0WX8Sx3AZB+m9GB6DrclPJSUVZQ+jxUOapcsgI4enqb0VarLcMquzROSOPqfb0iiVY5f9qf8nSrbZ/BuQR/okRAPzGf2gV6XXUmWaow9dhJQUkwVa0dOpLMBjqsGopkjZgNa0zl4/8AAKAfaJhQ8MdJeYrcLcQ3qfDMvdT+JcH9ooehY916DvXvfuvde9+691737r3XvfuvddA3/BHJ+v8Avf8Asffuvdd+/de64SJ5EdLka0ZLi1xqBFxe4uL+/dWVtLK3oa9M9FRCjaKSGMR6qeGnnDKf3BT6gHWwD+Uj6XFiD/re7E16WTXBnDJI1e4svyrmnpTp6JsL2P44/PP+H9fdekPXBpFFwGQtewXUoLNa+gXP6iPfurBTxoaevXldiq60s7C5RfVpB/BbgEi/Pv3XiBU0aq+v+x0Hmf6j653NM1Tl9qYyWqc3eqpUkx87m9yXehkp/IW/Ja5Pu+t6U1Y6bKIclRXpFT/GnqeaWWVMPX0wl/3VT5asWKPgD9tZHkZf9iT9ffvEf+L/AAdVMUZ/D/h6l4r469UYmsjrF2+9fJFKs0EeVrqqupo3QhlH2jusE0XHKyBwfei7NWp62I0U1C/tz/h6GijoqPHU8dJQUlNQ0kQIipqOCKmp4wSSRHDCqRpcm/A+vuvV/TqT7917r3v3Xuve/de66IuLc/7D8/4e/de6r6z9NHT/ACNVg5KPvihkbys4Beagp3KqwFwwkYiPjT+CbezF6/Sp9g/w9J4T/j4FPP8AydG7jFPV101Q5lWYQtHUJa6q8QCRzJIb3WRSP9a39fZXMVB/PPQg0NoCilK46fXqJpIadoCZFV4gYT/bUL6vHq5dmYc/T6c+9Fu0evSPQKtj8+o0qo7MvjRrhfJKDoKq5azXU8yC3093BJ+3qwB9esMxUIlOjftRAxhJYUk1Am7X1DSbH6H6397H2/PqoTVXUMdBPud9wYepU4lI6jHSOprnWdo5qWjcaWheE6hU3Bvq40jgn8+3lYGlR3+v+rz6otu8ba0FYycg+X+fpKVG5J6YpURloIY7qaQT3p5pCAdZI5CgC6j6Bj+fbgoQa/t6UpIAQVGPMdB/naiDOSCtpQsTM4RgVCLrNiRNGOL2H1/I5/PtkyuvbxX0r/l69JBFcd4Wh4H7fmOkz95PQyA0E/21SkocAIJEZyAp1MeGRhxY/j24srafl/h6JprYLKQDkenl1zlqg9PPUimhin8imaGP9On6ippEHr0FgdYudN+OD7fEyHP4umfCcEDy8ulXsaoqv41SOQZKWGSnqpQGuWfzKl1XkEsjMNLDkfX3SUhhQfEfPows1bvGmsZFT9vQMbnppNpbi3VjYJJKafE7ikq8QxPimip62X7yhdFRisXiDDTpPBHt1dJRyfPuH58eiyVKSEDyPEftHS0++xvZwlq6z7XDbsEUDz6IxTY/cs8CgSVbTK3ix+X1LfWFCyHkkG596UnQEPw+vXiQ5LYD/wAj6fYeh16q7krMZX0Wx9/vWJJUSR0mEzmQDPUGV5TFHRZao1MksEsp009Tc/QBzYhgzNCFGtPzHT0M5JEcldXkf8/+fo23tL0q697917r3v3Xuve/de697917r3v3Xuve/de697917r3v3XusU88FNFJUVM0VPBEuqWaeRIoo149UkkhVEXn6kj37raqWIVQSx4AdBllexxOJafZuNbPzoyxSZOoL0WBp2c2VhVSIsuSNxbTThlJt6/e1Vm4DHr/q49HVts5Ol76XwkOQgy5/L8P5/s6DajyQq9wx43cVRLmcvkzHJTz1Rb7OjrvuiIMbQ40fs0tMItRuwJLC7c+3ZFSMAEZ456PpJhZQhrJBFbKKEJ8TAjJZuJNf5cOlo+9MlJXybf2lR001FgZ/ss1nM5FULFHVmdoo6TFUVOYHrJI9B9RYJYf0Fz5YiW7v2dB14YpdV3csRJJlUT09STXj1nOM3Rk6xhms3PU0l0aOkoIFx1EFUlgJI42eWYX49bkn2rX6eOOq/2nSFpNElIoFVK8San/JnpVUeDpY3bw09PGFKtcIFZSFspdhZiTaw/wB59svM5Hcx+zqxeNTqC93qPPp4EIQFFBBNyBwDa1yQRezD2xqJPDHW9erJOOsRazaVuSxsx/JNuP8AAkH3rBGRkdPBe2reXDrl5vGSzJrZhYX+ikj9Oki4H+9e9AdaEWsAK1AP9VesC1Ml1DlEDEgqthwBcC/JYG/+v7tQeVft6daFKEqCSM1PU8Sq4Uk/puRcn9X6dLfg/X/b+60PSQxspboJt2v/AHe3Vgs3ErClylQoyIRbpqpykNUfqo1T0kock8gxk+9BiOHR/t/+NWV1ak/qIOz88j+ePz6VdQox+eMiFJKTKKdDghVWRrK4BHpYCRVYf4Nf24pJX59UiJutu0sCJoT+0eX8qjpNZ7HtXwVZ0NJWU8EkE8bWEjxKRLE6j6myfnng+1sZ0oP4T0jSYJcoBhdVVI+fHpLbJyJwu5qdfMy01bLFQVcb2Gta5fHSTO301QV0KqCP1CU/n2mmUAkdHF/Gbnb2GnKgunyK/EB9qn+Q6Mr7TdAzr3v3Xuve/de697917r3v3Xuve/de697917r3v3XusUig2YgkqVsALgkHjUP6KTf/AA9+6sDx6xPKUhleRkuCREQByzcRKFJJLlyAP6+99XVQzqqjHn+XHpgpqKoqJAT6Ilb1SDhuCQQp5BlLA3I+l/bjMBjoylnijQgCrkcDw/P5dOv3aLVLGzskUf7SKPUJJTwCzD+nH1/PulDSv59IvBJhLBKse6vCg+XTp7r0l6h1ddR0SpJW1VLRxM1hJV1EVOrP+EVpXRWb8/X6e/db8uslNVUtZGZaSpp6qMMUMlNNHNGHABKF4mZQwBBte/Pv3WupHv3Xuve/de697917rq/Onn6Xvbjnj6/S/v3XuumJ+n9eL/73x9eB7917oiG8kTF/ISnyGQ5ok3bt6ad5lVkigraCjghkKgafHE7ggnkWv9fZk41WSlTwUfyPSFG0X4B8zj8xQdGZKtFlqqlMhAQzJIGXTrEell4BsBpIKf1+p9kd6dRqDThX9nQtiIaJXp8+llDBUTxQtGF0h7CR15Uc3A5uYh9SR+T7ugOkEj8+kEkiCR6nPp/q8+sMkBga7FLyEByg9HoLAGxsAW+pPPtwGtQevVBpTpkyMb/brpkf9aS/tyGMsYJgTGHH6kYHlDw4vfj24DQ46djAJGPPpF5apIBj8TLqBuC66jcD6twLAfg/U/4e7FgeHHpUP59A/uWCL7eaWBFiB8olSwKyeMDXLCOdDWufpZv8PfkkOQRX/P0nkiFGIxQcPX/N0HcEg1SGMMjxW8kKn9qqiKcVka3uJI72YH8e6sp4V/M+voemVkFSwFKfEB5j+IfMefWZ0glF3b1WCq4sDpP0sf7QBNwf6ce2gzLUcBXq7xRyd1M04jplZirSQJGixqrqsliSWuCQshIN1QfT/X9ugg0oPy6L2VkqHFRwB6EnrqglMyzFHJ8yHSFPrVGDgtbkhAQxP0A93aoAHSm2ARZWrx8/l0FXa+axVVuXNZJcdBW1NbXqKOUO13pMcq0sMhA0p4yYixYi5Bt7XdkcSMy1xSn+r06IpGMk0hU0Bbj0GWP3BkqKVKtaiMyqdaPNDFIISnIVUZQqqt/8ePbfiMaGg49e0KPy6MNs3qnfvbEuIym5XkwO1aUI1PV+GKmqamjR1ZaXCUI1SrFJqLJUS/tL9VDEW90kuDQqANVa/L8/Xp1ICdJYnRTFeNPL7OrAoYhBDFCHkkEMUcQeVy8riNQgeRzy8jWuT+T7SDGOlZznrJ7917r3v3Xuve/de697917r3v3Xuve/de697917pJbs3Sm3aeKOngWuy9bdaChaXwxkgqhqKqUK7RUySOBwCzsbD8kVJp9vRltu3PuEjVfRbpl3OaD0A8z/AMX0hKWjkyNRFJuec7ny8jkxQSIafbWIlZWUw0WGu/nSAcPUVHkke1wV497A82z0dPCtvGz236FuBkjukcepfABPkF4dLKLGQJJTuwWR6bSYmCrFRxaBYMsK+k6B9L3sP9b26SSKZ6LnuGKOqiitgjixr8+gR7AwdXgdw4zddFG0lNT19PXCT6QwtHMssqmRDpsylit/re1/epO9VYfEvS6Gdbq2a2bEoBUjz/Z0KEWNgoZ6rJ42cTUedrocxEphDwBpaMETm5u5qVs30BBv+fbsdG1MTgjohmlLpDGy0aJdBPmc/wCSvS84IvbSrBLAf2gbWP14tf23Ug8emhThx8+ucelG/ABAHA5P4AY/2vr7qxB60wxw6kuAGBFvpw1vrc/7f8fj3rqik/D/AC6bWCqx0DhvUpPBtf6knm1+Pe8dLVJYDUcjB6jSkE8n63v9STe9xxze592x5jp+MYOOoboVVXJY2IDEWLIw4uCeAnP/ABPvYNelCtqJX/UepMUgJ0nnSObXII0/X6ctb6j3pqg1/wAPTMi+fr0xbrxX8cwVdRoq/dRqa2i1qCDNTC7w3+qLVQakNrfUe6kE9P2M30t1BKfgrpb7D5/kc9NmHLZjatOynVWYtU/sgyrLQoqOjab8y0jqbf1H9fe1OR+zpXK4tNzIIpFLg+lGyD+Tf4epJqKZ6qKdWu9TSrHUWuDd1MYLc3J0Mb/0HtVHXQVJ7Qajotu4SjaQncG4/wCDoPDjkqayXEu5irJqLIrRyrb/AIuGNIraZGe3plElNrW3BPHv06koHp8j0ZpcGODxAKpqViPkcH8qGnQ57VzabhwGNyq2Ek8ASqQEExVkBMNVGQP0kTIbD+hHtGeg9e25tbmWH8INV+w5H8ulD710l697917r3v3Xuve/de697917rDHPFISFbm7ABgVLaTZigaxZQ3Fxxce/dXZGUVIx/n67mLLE7qfUilxe9jpBNmCgsQbfjn37rSAFlB4E064RzpN+3yshiV3S41Jq4ZfST6kJ5t/X3unVnjKd3Fa0B8j/AMX1iDeWSPUo1AMwBveEcrHI1xpLML/Xn+nv3rnq1NKtpbGB9vqOsFDJr+6hLSaEf0h1ZHiRx9Cx4uSCRb6D3tuIPTlwunwXoKkZIyCQeoy0ohggcTAy+XWpZC6ugfUdQQB2snN7gX+vHvxJ7vXp1ptckgKUSlDmlDw88ceuU+Yo5k047IUFRKsqCYQ1NPUPFHq9d4o5WfWf0jjgn3oCvTFvGruwcEgA0A9fL8uiv9j5oZzcEyQlpqDDg0Ect5JIXrGYvWzAtdELzAotrFlj91NCeGOm5CWY4wMf6qdCR0jWqaDO4v0r9vWU9dGg4utXCYZGAHA9dIP9v78OJ6p5dCnnNy47b82IgyC1V81XpjqWSCHyxRTvbS1U+tfFESwFwGP+HvdacetdKD37r3Xvfuvde9+691737r3RM/kfipKHceGzUMhhXK4/wRS6RpjymFqY6imct+AIpweQf0+zK2YPA8Z8if2HpBdArJFIvxevpQ1HQ5bey9DuvbuF3ikipLXU9PHlIacpUPFkaceCqp0VCyxsZELaWIYoV4v7LJYCzGJvLBr0fWlwzxaFAyKgVwPkfs6FKk8JpoPt2DwGNfGw51KR9T/Q/wBR+Pp73p09p49I31a21CjVz011bU4VzMRHGr8M4IvY2AB+hW/0/p7bINccOlUes0pk08umGtq8esbrNMrtGY/TFZnGs2+n0AYEA/092Ff5dKo1lBBAx8+g+3DRwM2uSrXTIW0PFIjAKbNZkJDgxKv1tyf9j72XqM4HSgEEcDX06D2vpTrN50kEkT8MVASN2CxtIByDKhJsOb+9HyzX069SlQOglyNIaSoJRnU0zMYyVKvIvKpYr9RIpsb+31NfMU8z9n+z0XTJ4bahhhn7R6fn1CVkppEjKACoDy0hVldViFmkikLEj9Ytz+fbMorVxXUDQ/5/z69G4UiMiisKof8ACv7es2JoqqvrIKNYGmNXOIY4Cvqlnma4VLG7M3+H0HtoM2oUNDXy6fIGQ2V86/t6E7dmdg2Ds2SJA9HnM356cabrNjMXBanrZobgtG9XL+3F/VmJH09mkKBqu+Avr69F19MI1EUZy3QIdb9Tbi7cy9TkQ74ba9PUJBWZdh5G/bCt/DMXG5H3FUkRBZv83FcFuSAWZ5iWoB3U/Z9v+bpBDDqWpPZ/hPy6B/uv5udSfGzt3cPSuzOgcb2FJsp8LRbz3NuXdpw8h3BksRQZ447GU9TtDdQr4qHDZamaWoZ6aP7mR4li0xmRoe5o9005f3mbabfajceEAJZGk0DUQCVUBGrQEVJpmopipzV9qvugXXuDyDtfPO684DbU3ASSWNtFai5JhjkeHxJXNzBoLyxvRAG7AGLVbSD+fGf5YdXfJjD1x2aK3b+5tvQUz57Y2cWliy2Oo5j4abJ42Sjmmocxt+WZTGlRAwaJtK1EUDuiEVcqc57TzZDL9HqivYgDLbyU1AHGpSMMlcVGR+ICorC3u17Kc3+0V7bLvgjudmuWK2u4W2oxOy5MbhgGimAyUYUIqY2dQSE92x82uour9y12zaf+Kb33PiJvtc9S7Z+xOMwFYrFZMdlczW1UFN/E4GGmanp1qJKdxomET+n2Ucxe5mw7DdybeiyXV7GdMqw00of4Wcmmr1Cg0OGocdG3JX3e+eOcNpt9+lMO3bROuu2e71+JMvk8cSKW8M/hZioYZTUM9DV073NtDuzbM24tqmtpnx9b/DM3hcrFHBlMPkPBFVJFOIJaimqKaqpplkgnhkeORSRdZEkjQSctczbdzRYteWGpWRtEsUlAyNSorQkEEZBBofkQQI/585B3z293ePat6EbrLH41vcQkmOVKlSRUKysrAhlYAg5ypViLXsRdAjr3v3Xuve/de697917r3v3Xuve/de6Bztjb2RrkxOcwrI2Sxcjo1E5YPX0qstcYaXT+qrjalJVPrIpIHNr0ZSe4cR0JuXLuGJ7i1ua+FIKg+QPw1Pyzx8vPp/2lnsZumjOVpEjFRIiCoYoI59N20mRbalj1qVIPNx7cBBAK8Ok25209i627MfCHwjy+dPn0ro1tKYnRQAPwBpKf4j6NYE+/fn0Vuf0w6sa/P16QlZ+zis7j6ujfIU9JDPL9kGCSGKGQNUrSu4YKy0jeWNbWJW3vZNAGA+0dHFwA/wBJeRGjtQEj5jFfzweoeAYxUpw0kwmpoFjrMJVqdKVeLmUSxWYG10DGy34uV/HtyMgNT8JyD0XXaKT46ilahx6HpdUkyvCILlmitob6kpbg34DC3B/x97Zck9I1NO4H5H8+s66gQeSbgf6ogfU8c/j2yR6DpQaEY4U6kyygxhBY/Q8/gGx1D8/X34ZPTcanVU16iXLi5ubKLf4AH6mxv+fduBHT+FNBTj1hMfPH051EEC178r/Tk/6/v2Kjz6dD/t8q9cVgDqYtAYsrL6uQU5J1H8pY8g+9nidRx1tpdJ11ovHHr/n6z0dE8JOtQTpdSw5XSx0aUubgAW/x91Jr0xcXKuBoJ4g0+Y8z1i5jlsR6o3Kgnkgr9G/oAQfex8vTp0UeOoOCK/t6TWLo3we5KxIIX/heXX7q8aFqelrEH7sLhR+wJYpT4ybh/pe4t71T0HSy5cXm3x6j/jEfaPUr5H50Iz1MOL01OQopFRoknFTRSXGpIKpNTK1hq9MoKj8cD24rHBHXvqVkgtbgg6ipRx81xj7RnpETRNid7Y7zlaiL7ukqRYH9uKsppafWSbDXGXLG31A9uajLEwHEdOYl2+XwxpNCM+qkGn59O2w53wm5dzbQqSqo1Q+ZxYFlV4pW0TrGtgCTGI24/wBSx9pj5evTO5Ria0tL1DWg0N/hFfsNR0L3vXRF1737r3TVQ53C5NvHjsrj62TTr8VNVwTS6R9WMSOZAB+eOPfuvdOvv3Xuve/de6gz0Ucro41qUAVdDaNA1FiysBqVufx72DQU6eSd0DDBB41z1KViWIsdI4U/6qxsTe/4966apgZ6Jr8Z/k9Sd59j/JvYQO2fvek+1IMRgqTA10lVk5essthlxm3M5uOnqIqaahzWe3xtLcskUOnxNiVoahHeOoR20prWp4Hpz4tQkfOKf7Pp0aKs3dtrD5RMNkspDR5CeOOoKT+Qwr53KxJPV+P7eGRgp0q7KNAv9CL7J4dVZiTg4GB0XWf5v/F6j+PW6PlRWdmwY7pDamd3HtjN7xyG3N2UVQNxbW3bVbFymFx22arBxbpzWTfdNI1HSw0lFO9Y+kwB0Ib3qooM46pqFKse0V/kf8/T52f3/wBUYAdS9d7izecwO8vkxit0f6INv5Pae8aHL5yr2ntCLfWcoM3G2EVtl5HG4KRWmpsyaCUS6oNPlV4x4kefWyQTXAJ4Dotm0u3tk1vZW7dgbX3NSN2V1fS7YzG6dvfa1tLXYjG7woait27kVNZSU9Jl8Xk6aCZDLSSVEUcqNFKUlGn3qtTj1z14Ghw2fT/P0pcP3l01nujO/d04rdL1FP8AHHeu4qfu2tfbe54JNq5nZ+Bod05+ijiqMNFV7kXGbSy8U4kxiVsUrSMkTPIGX37FK9arxFeH/F9AP8dv5kHxN3V2RtLae2t87zymR7RrsPtHaXj6Q7zp8ZlM3ncjTwYTVnazrimwdDj5ZZG11tRURUcEep5JURWYeDqTSuevAgior+w/5uha+T/8xH4f9Ob5zPUPZPZ2UwHYPW2V2Rnt20NP1h2tuHFbZxufpqHMY+ty26NtbJzG3KOmrMLk45AzVWlWYIxDgqPFl4Vz16oA4fn0dKHvHp6o6j/09wdl7Mk6XG1pd6t2cueoP7mpteCKSWozEmbMwpI6en8TJIrESJMpiZRICnu1evVxXy6LH07/ADK/hz3nv7bPWWxuy81Sbv33RVeS66o9+9Ydp9X0HZNBRKZJ6jr7Odi7N2xhd3M0H7scVFUSzzR3ZEYK2nQYE0/PqupcZ48K4/Z69GSbvbq9O94vjS24Zh3NN1U/dUe1f4JnTA3W8e6v7lNnv7xDGnbSyjcn+T/ZmrFbb9zxeP1+/VzTz63UVp59c+9O8+sfjb1duTubuPcEu1uutoyYOPP52DC53cMlE+49w4rauHC4jbWNy+ZqhVZzN00JMNPIIxJrfSisw8TTJ68SAKnou3zY+Q/x76c2xtLB9tbwr8XvXfFbXT9WbU2rs7enYm+dy1mGpVnzMmO2b17t/cu6JcHTUFSErKs0y00DSR6n16UZ+CYQvU/CePTcyB1oePl5/wCDoDvjf8ids57aOE3911majdHVG+UqqhzV4TK4TIUlZQVlThavJx4fcOPxuaoKvG19BJHNHLBGZVi1c+hvaxo0nUTR5P8AhA8umrac28oVzSOtceXz/wA/VimGztNIsC0NZS1MVVHS1qS0svmp6mGqj1xSQSMNF5VU3VbEHk29pWUEE0/2Oj141nXxDmowR8vP59PeQelrqWaGVhTOFkkV39cUYHAaVlIKrIeLD2yUIz5dNxrJCwde5eFOB/LoH8pMUaoo5i9GIqeSYVAYeKQhSRpIDEswNwDY8e9FTULX8+jAyDNfi6CqqnrKioj1VSzi7Ir6yoAZOE0FrXt+bn2mYSVpSvp1vDVOR8uuQjl0h2n1FHSnsW8jF1TUxfTe2n6D3vS9Mj5dex/F0wZWnnqYH+3jZ3KvKrPZY9Cm5uF9ZA/1/bsdQ2nyPTFwA0YIXuHWPbO1n3FHJRftxy+eKVHl5MZ0kvMunlaUSizAc3tf6e3QpqrGuRQ/6vs6RqoaORCcg6l+3/i+hLiXbfXuPk3rn5npqyjjqoYaCZVM8tfAGQNj4gT5KZ1AAlIGi/8AX24lspkJr2Lkk8B/s9NSXdIu9SJDinrT0+RPQZbI2LuPvbO1O6NzSVNHs375JKh5C0VVlpIA3jocamjxxQU6aY3kACIrHTqe9rSz1Hhx/D/g/wBnouSJnYyy+ZrT1/2Oj447G0GIoqfHYyjpqChpY1ip6WliSGCJFFgFRABfjknknk8+03Snj1q5fzIeravZHy+7EzFcKhaTtWk2x2Ftmo0SxUlVTxbfxe0M1RfeuDTS1mNzG1pGlgU64oKqnZwBMhbFj3L2t7Pmu9lkX9O40zxn1BAVvzDqcfZ69djvupc4wcw+x3K1hbaPH2Z7ja7tcFlYzSXMTaPiCyRXACscFkkAJ0tQuHUfbO9unt1U+89iZSowO6KSky+MpclHFTzM2NzdAaLI0tVR1AkpZac+mZfIrCKoghmUCSNCAftm432y3gvtsmaK7VWUN8nUqRQ4Ioa/IgEZA6lbnfkrl7nvZ5dh5js0udnd4pniJYd8L60ZXWjBuKmh7lZ0PaxHQlbLzVBDUQSmadyGZg0rGqE80xeSqlkmkLyTTSyOWd3LNJIxJOon2zBHGH8Sp48DmpPnXif8p6Cm/wBhcPE6eGoFKY7aAUCgAUAAGABQAAeXV5n8vDC1j7L3xvd6eelxu4czjsFjBICsVcdrR1/8Sr6e4tJDFkMu9Hq5KzUsqHlSBkB7S2DxWO6bkVIimkWNPRvD1VYD7X019QR5dc7PvSbhAu/8vcvLKr3drA9zNTin1BTw0b0JSIPT+F1Pn1Yn7l3rFnr3v3Xuve/de697917r3v3Xuve/de6YN0YyfLYOupqOQwZGNFrMXUL+qDJ0TrVUMin8D7iIK39VJH596P8APpXYzrb3UTyCsNdMg9VOGH7D0FG145oN0w5nHxeDEbkxQyFRAq2hir6k/wC5GkQ8aDDkoXKqfpc+9oK1pw6EV4Fk26S2lJM8EhRT50Hwn81I6GWZApSVefrb/W+o/p+Db3v5dBeNsGMnpPZmI09ZT10aj95dD3JsZkW3jYcjTNASP9h72ONOjewcS28tsx+HI+w+f5HPSNx+PtHPjYpP3MNM9XiBH6HOMnczTULgHS4p2YmO39kWtx70uDp9MjpuZdDsWHY/Gvr5Hpb0S28boSw061Y3uVYXaOxF/qfb7EMAfXopNUZlPlwHT0ouQ6+k/Uf6/wCL/Ti/19sEUPy6dwR8uuMseqMSr6RezLb9D30kW/1Ib37hjq0bUbSRX59RV1azyAthYC17/wCvzex/3j3sg+XDp5qaeFWr13z/AGfpc2B5IP5H+x97r+3rWOB49dU5/wAoiIBAW5PPLE3HI/1veiBT59bmH6MmcnH2dOiykuFIHOrTa45/w/r7r0hMYClq+lemzIxMrCdOEb0y2/ssGuptz6WHBP493U0FKdLbRwQY2Hd+H/L1ip29SzjSIAjRNc3IKkgCwvqHvxpSnTkw7WhNfEJ1D/P1IqY9f29UrD9sPBJx+pHs0Y/quhx78pyf29MwMV8WAr8XcPkRx/aOkTvHErNj5c5SeQ5HEJBUsiFmWpoqeYPPGUA/zsSXKsCPTxz7tG9GArg4/wBnowspikotpKCGQkVPkxFAa+nDps3ayUcuF3xjVIfE/aV8saAF6vBVqpT5Gl1D6NSxTPJb8EEe6EcanI6fskM0FzYSnJqn2OuVP59DDFLHNFHNEweKWNJY3X9LxyKGRh/gykH3XoOkFSVIyMHrn791rojOEq3xuaxGQgOialyNHIHXg6GnSOZWP5R4XZWH0IPvR690eb3vr3XvfuvdBj2RuXcW1YMbX4haF6KeZ6Ss+6p5JXiqChlpmVkniHjlSN1PFwQP6+9Hr3VT3yY67xNJv/G/L2DtXuTr3JddTtn959V7U7a3RjuqO6c9UY0bL64xybOzu/8AbmzdpbxbfmZw8gYSx4bNtCafIU+qoesj0cGvWwKkGpr6eXWtD0rk9/8AyB+YtHsTr75Cbr6LftzcWU2iOyNqZrf2AFPtHZ2FzmaxNIu3aLsKozEtPl/7sP8AwvBzZ2oxlDmK9YYZlgUWaAzg9VqS1a0JxUV/1U62zOp+sMP1FsrHbMxGc3xuoUxNTkt09lbzzm/t8bkyksUMVVl9xblz9VU1NVW1SwLeKBaeigAEdNBBEqxh4D163wAHVCfx07F3FtPMfHffnyX2YK34EdJfMjvag2rVU+T+2oaf5E7237vWt2Z3V2ViKs/YZXY/XW6amfD0NXK9NT4ivqJJnaQ2inbFcV4dVNOJ4Bj+0k56un+W++MNnvmt/Kpzjk0cNB2Z8oRlKKYrNU0mnoeYhCsOozrVJ/mtKnyMdIuQQLEjUvVjhkx5n/Aeq7+9Oru1k/mBfKbuzo1srT9xfHTr346bkwHVs1VBFhu4eu984/d9Xv3qfc0scM0seTy+2NswtiGGpKfNx08jKskcc0NadzUPDrR4kjiAMfmcfy6GX4u9l7R7w+DH847t/aNBmsfs3srdvyR3rhsRnYKajzuMpK74t7RmkxWRhpKispYKzG11PJD6JHFkBve492Hwv+fWg2os3kT/AJB0N/8AK9pvkdiNl/G/I9h726byvTWQ+PmxaLY+3drbA3dhexcWuR2ltuXZ67n3bkt+ZXbuaai22jU9a1NiKM1FYySJpVW8nlrQV6svDORQUoM/LNf8nQZbg3d8jMF/MP8A5lGN+OXQ+yO8p917V+HVJuur392lSdcYPYlVSddVqbWqKrG1G3c/Xb5xGdlqKr7ykpWpJI4qYDyjyL71nU4p6deKskjKV7qCoP5/I9Jr5K/G7I/Ef+Wj8OPj323uTA7g2LRfNTpGo+U+Rw8VVjevP7h787e3X2BunBrHVLSyp19hN15bG0iy1EMAqEpkneCAyeKPZBA4+eeq07QD6j/D0bn+ctTYen+LnV/8Ap6CDt6h+UXxth+OYo4qeHN0/Yv+knCJHS7UMYSeGQ7Shr/IkBUeBP6qnvbcOttSg4VqKftH+TpQyhj/ADtqD6kj+WNVM1h9Afk6ouf6C5A/1/e/M/Z17zHUr+dX/wBu1fkP/wBRnTP/AL/nrH3p/hPXjw/PpYfLT4ud3bn7b6q+X3xR3hsnEfITqDYG5euptg9r42urus+3et9zV1Jm67aNfl8RUQZzY+fp8pTNNRZOlDrJMyRVGiAM3veQQw49eIOCDkf5fXqB8e924j5zdTP3RjduV3TPZ2C3ZvTqvtbr7LVFLnaPb3ZnXeUkwW5cHLmsfFSwZaClqVR4cjBGpnp5EDxLKrKFcN1pUK61X/B0nkgWTvGH8/yxnpWYbc+8OncodubhxYqKBKl6qHEZF/HTvMrSR/xHbWTjDJFDVoWBHKAtdkVvalkjlXxFahPE/wCcevVYrq4tGKEEpSgz5fL5fLoxOD7K2pu+lggxta2OydY60bYXISw0+U+6IDGKmRiIa2lcH0SK3rFgQDx7TNG6fGMevl0c2t3BPxkAbjQ4/wBR6yZXD65EketKoYytRHKuiTWWIKCNwP2gq24BFx9be6eGWIz0sIyTTHSelwOGkjgf9oUsbtYwpaWWYEkLoILPYgnUvB96MQHy9eqa2BOM9dtgMfUpLTUsqXicxSOisJY5tPKabDyMighvrb37TpwOPWi54mvr1ip9pRQhZXkSbxsrfalZFLwxnUzSyi/iiYIb2HvQTGT029yK6fPjXpE7l7A2T19Vz/wdXrssI3P2cTAUNNLIoaWnqZox5KixIGgG4J+o9qgnYNeE/n0USThZXZWLP6fhHQa7Ix57fzcu5d6Zs1WKxGUpxV7diaRq6ox6MJWYImmKkw9LJIqyFSCUJCkH1e25GaRWjjGlP9VftNPPphSCweVtT1qR8v8ANXqxOljpoaaniokhjpI4Y0pUpwqwJAqARLCE9AjCAWtxb2kpTFOlpNck9SPfutdE++afxbovlF1U2Gx0lBjOy9m1FRuLrLP5BStFFmWpxFXbbzU8UM1VFtndlLGsFU0auaeeOnqxHM1KsThHnLlePmfazClF3GKr27nhq80J46XpQ+hAOaUM6ewPvFcez/OQv7pJZuUr9Vtd3toviMWqqTxKSFM9sxLJUjUpki1IJCw1YqzBZvZ+5s5h94YKu29uvA1tbiM7t7KRiKvoa7Et4qyiqY43mhFQNQMckTPFUxFZYneN0c4rT2ctncT291EyXEbaXRhQgjBBHXY633Hb992nbr7YtyjutluY1ntrqE1R0kyrKSAdOMggMjVVgGBAMZ8Zel96fIXs7EddbOilxOFZo8xvLc8KtLT7J2mk+mtyc3nXxtm8hIv22LpTc1NU2oqKeGpmiO+WtgveZN0i2+1UpAe6ab/fcY4n5k8FHmT6VIi33c5+2D2w5Rvead9kWe/AMFjZnDXdyR2RimfCQd0z/gTFS7xo21bs3aG39g7VwGy9qY+LFbd21jKXE4mhiJbxUtLGEDzSteWqrKl9Us80haWeZ2kcs7MTljYWNtttnbWFnGEtokCIo9B5n1J4k8SSSc9cZd+3zc+Zd53Pf95ujNul3M080h82Y1oBwVVGFUYVQFAAAHSl9q+inr3v3Xuve/de697917r3v3Xuve/de697917pBw08dDk8tjyNKR1C5iiHAC0mWZhVCMCw0QZSOTj+yJR78uNS+XR0sjSw28tclfDb/TJw/ahH7OlTE3lhMf6niAZLn9S3+hJ/p72ei2RdL6jgNjqNV0q11DLTNcSWDxn6GORSHiIvz+r0k/4+/dOwTNbXKSj4eB+Y4HpCxSmmytFU/oshimP1HDaSpFv8SPfvP5dGN4oYGlCKVHS4pwAXiA5jYyJb6NG/4Fv6fT25XHHHRNMvwyD7D1nEigi19B+t/wDH/H8W96K9v+frS/Cc56yq9pJYG+ksepG45ZV/p9blbf7Ee6ZpX06uchZB5HPUCxFh9LAf4kH/AF/8D7uKU4UHSqtc9ZVUjhWZnkNgbgkf7wQqn8n3X8uqE1OVGkdZo6ZYWLFtT/i3CpwOR+SbXvf3qtBTpp5mkWgFF8/U9c3bQ4kUqUDBw311A8OFP4s3197+R49VUakKGoalKf4OmbIVNXBVTIZVkpZoLJG4UqsbL+7wtn1q3Kk/g/n3tQCK06MLSG3khRwhEyvkj18vlT169RxzosqSxuiNGkscjkFCyjixUkXdDf8Axt72SCcHrc7xMUZHBapUgcc/7PUyC9THNAeDIgKG5H7if0W/6f8Ae/ej5N0nlAheKUcAc/YesNK8chMMyh4nUwSxkm1p1MMiuPypP1H49+IxgZ49XnRlUup7viB+zIp8+katM1Fi6/btZZvsZZaWlEoFqvF1moIIyxJZvC9m/N1P9Pbp7gH8jg9L7eQS3MdyvB1qaeTL/q/wdPXXde8uDbDVLE1+2ql8PUK7FnaliGvGVFzyY56BkCn+qn+ntgihp59It3g8O58dB+lMNY+38Q/b/h6X3vXRV0Q+upZMbV1tDIf3MfVVNKzBr3akmeINq/JPjv715GvXujGbn7OqcEKWlx2JSuk/hWMrKqtqJpFpKWXJRPJTU0iQoXM0kcRYAupI+n0v79XrdOhF2vmv7w4DGZgokUlZTB54Y2LJDUozRVESk+rSkyG1+bW97610nO0qP7vZOVbktRtSVyAC5Jp6qLX/ANYnb3o9e6JjXdJ7X73zO0tq71ye4YNqYXPru3M7dweQix1DvyHFY6vpI9nbxdqWoqa7ZdfJkxPW0cD08lU9NEjy+Eyxy+IBwetg06dvll8N/j/2bsHq8PsbEbH3N0bn9kT9Hb069xuL2tuHqyPaGRpclh8Dtr7Oh/hbbKEeMWCbB1NPPinhN1gSZIZotMB+fDrVBg04Z6UO2dv1G581S4infwrLqlq6nTf7WhhsaicD6GWxCoDwXYXNr+95x1vj044n4YfHvbnxv3b8URtqr3H0pvut7DrNz7f3ZnqzPZGWq7K3LlN256opc1USLk8ZUUWfyz1GNnp5I6jHzRxSROskYf3YIKUPDpTDAH1iRGoQSOPnx/w9Bn1h8RumqDcPSWayNVvzPZf4fZPPY/prcea3plsjkJKPcW0p9j16b0mLxpvGSDb6okUtUplR116iWfVUJU06qts7syoKlSQASa+n5npe76+P2xdsdob/APkjt6DMje/b2M6+2rv2oq81W1mIqMZ13Q5mh2hLi8JMTR4WVEzM6VDw2+4ZkZgGBLeK0Jrx6bdDGzKR3jj/AKq/PqF1n8Zej06p762djcHV4HB/J7L70r+5cXiMnXUVPlc1u3Z1FsLdeYwkVK8f93MjuXB0qVFTJTFDNkpZas/vSOTtR8Xn09bIxEmmOqEUPlx9D/m6KhT/AMuXp7o7cuwc519vj5KUuB2LksDkNpbfr/kf21kto0FXtqWOooMHX7Vfco29W7dYwr/kElP9pNHqiZGS6mpTT546pJbtCqE1ofm37OPR39gdN9b4jf3a/wAitv0uWpuxfkZJ1Dg+yairz1ZW4eol6opZdvbeXE4KaQ0eCeHH1MomEIX7lisjc3vug4+vVGWMFTGe4jPHHy6HTtLq7rvu7r3dfVXau1cRvnr3fGKlw259sZmN5aDKULyRVEZElPJDV0dbRVcEVRS1VPJFVUdVFHPBJHLGjrv5HpsjiCOie9N/y0fjF032DtDs6jpu0Oxd09Z0k+O6jfujt7f3a+J6jx9RTpStB1xgN35iuw22XipI0ihlSB56eONfFIhF/eqAZ68VQaSta086/wAq9Knv34DdHfIrtjE93bxzPce1eyMLsGLrOk3F1P3FvnqypfZ0Odyu4/4VVPs3KYyWpSXKZiZ5NT2lAQMD40torXNevUH5/aR/gPXdd8COj838a96/FPdOc7l3v1dv/c1BuvcFTvruTfW8t9nIYzP7X3LQUmN3xuPKZHPYvC02V2jSOtHDItOLzHTqnlZt6RSnWqYoa0+0/wCGtelD8h/hf1T8lNw7O3fu7c3dOyt27Gweb2vhNydOdz9gdVZN9s7jqcdWZ3A5IbTzNFRZCgylViaZ5TJCZmMCDyaVUDxFevEA0rX9pH+DoYOkuj+rvjr1tgOpendqUmzti7bWragxdPPWV1TU12Rq5q/K5jMZfJ1FZls5nMvkKh56qsq5pqiaRiWawAHgKCnW6AcB0JlfQUWUo6jH5Gkp66iqomhqaWqiSaCaJxZkkjcFWH+9fj3YEggg560QCCDw6Lbuj4z4GaRq/YeTn2rXlwXx9SZMngpo7cxCCVmq6QseSweRbcaR7eSdlOemmhQ8MdA1X47t/q+t+6FBXxIpLtXbceWvwFXquCtbipVlpQjH66kUre/19v8AiRSAhh/n6apNEaqxp6DI/Z11H8mkFpN07FxWZyFIxhgrqSofFVQc6VmMsM8NRpuBa6EAkfS3tsqq8HYfLj0ojvJaFSP2H/V/h6TWZ+Tmcq5JEw+28Hh1eQyw+M1FbUhUB8aTlnSCSxOptMYBNh73qQY7j+fTbTSNk0A8q1PXeMxfdncFVTQVUORpcSzwJPla6BsZjaancidpAhSH7zTGQwWNGc+kX91M4UdlK/L/AD9a8OaYgMTp4Zx/Lz6Ercvxrpdu7YbI42pr9x7go5RPXjwBIpqVkcSmhokZn81MSH9TOzKCAL+9xSambXQV4dUuLekVYSxYHPzH5dA9131j2rkcw2U2ziqrF0Syxk5LLu2MoqiKaSwY086iSvhiVNTRhHuLXHI96aRVZvP7OqRxyMqEAqfU4/4vqyDa+JqcFt7E4isqkraqgo44KiqRDGk8oLM7oh5VCW4vzb2nY1JPqa9K0XQirXgKdP3vXV+ve/de6Ir8wvg3sf5P4yXcOJqKXYvcmOoUpsPvmKhWeizlLTLJ9rt7fVDCI6jLYdDIft6mJ0r8e5DRO8XlppwRzbyTY8yxtcRkQ7sq0WamGA4LIBxHkDxX5gUORfsZ94jmH2gu02u9ifceQ5ZNc+3M9HhZqaprRzVY5TTuRgY5RhgG0yILnxh+NWzfjD1zBszbcr5nP5OaLL773rWwJBk937k+3SB6t4VeVcbhcfEvgx1AjulJTD1PNUSVFRMa8s8t2XLO3LZ23dO1GnmIoXb1+Sjgq+Q9SSSCfd73Z373e5qk37dVEG2wqYNt2+Mkx20GokKDQeJK57pZCAXfgFjVI0Md7EXUVde9+691737r3Xvfuvde9+691737r3Xvfuvde9+690ltzaqM4vNpGZFxtYIK5Re5xeTC0lW1h6mEEhilt+AhPvXp0YWFJPHtC1PEWqH+muV/bkfn1nhBpqsQ3LrqFn/rE92W31uSv+8j24citM+fVpKTW+ulD5j5jj06GOU1KyK0a05SxUITK7HgMWuFjUH+gJ/r7rinz6Qaho0kd3SZzuMMjTVMYJJheZgB+mop1VhYfU+eMEf11D3rpfbzholib41YafmD/mPWKiqy9LjqyIs5UpA4W5Devi45+qk39urShFfn1towPGjPClc9O9d+1JqU+h7Nf6XB+ov/AIe9oainn0gQ0pXh1jabXSiQG7UsgCm4/QxXj/YH/e/eiKNwwR0pRe6nkRkfZ/sdSXfXpmU2WdNen6hZFsJVP9WDWP8AsfdVxWpz1dV01QjKmlfkeHUimXW6sB/m1ZubDUf0qPweT/X3o4rnpPMdKkE8T/snrA8hd7lVVyCthf6C9hz+Rf36mOP5dOhNK0BJUdclYEOg1FogJhdSVK8Iw441Kf8Ab+9Yp1UihVjwbGP29Qq6nFTRCRFAnp3Lq4ALSJGCDGx+rKUY2+tiB7tkN0/BL4FzRj+m4oR5Cvn+3rDiqgSRmFbMItDof+bclxIF/OlZPx/Q+/MCM9O30RVhIeLVB+0cPzI6zPJ4ZyVIGlwy2NwbA8H+vBsffs0/w160q+JCNSnhQ1x1xyZEGmtQ2hlCtPweHVfqv00s6D/YsP8AH3pTxB69ZapNVs39ovw/Z/loem3LxR5Kjoq5SboRSzOCQTFJZ4Wdl5VfIB9Rxq9uIxUkDgcjp21UwXM1u4496faOI/Z0ncRbGbnirDaOOrhjx1W3IVxM7faXN9OmGpQBf+Dn3VxXo0vY1uNtdVBMinxF+QA7sfMGv5dC77b6CHRJ9xY6qppKDJVYa+5qJ8+qupUxivqqiRoHBH6kjZGP/B/evz636dCtSbekrupclXTBqnJ5A/x8TP6pjHi2jgpIybXMcWMpCqgcBW49+8uPXvPp36UyYmxGVxLPdqGuWrhBJJ+3r4wTpB/sLUQOePpq9+HWuhG3eI5NsbghkIAfDZAqTyCwppGT8WvrXj/W976sqs3wjrXN+WP80jsX4XfJResNt9I7S3/FRdfbO3nHl83v7MbbmqId802YBonoaHaGcRPszjf1eXk2PN7LD/N3uTe8tb3c7Wm3RvCipoc6iSWRWNQCoFNVBSvXST7tP3F+VPfb2j2/3K3j3L3Da7ufcLuyNrbWUNwgFt4VG1vdQtVhIDSnH7KkDdx/z8O4N4YuLGV3xa66oYvvaeqSal7f3NPLqiEiKuiXrdF9YlP59h3/AF5b4iv7qi4/0h/z+epvk/uwPb9Q3h+9G7lh67Xbj/tfPVj/APLO+ae6flTl+44dydcYTr+TaGH2bLhZcFuqv3O2Zos9WbhhyyZAV23MB/CTQ1OIp/GYmqDUrK1xH4xrkTkTnKbmx9wW4s1ieEIw01zqLA1qT6D06w++8592Hlz7vv8AUp9j5yu93fcmuluBd20duITAIDH4fhzzeL4glbVqC6Cq01ajS0PPZhMPjq2ukkX9tAsMS8eaobiGMA+rTq5P0uL/AND7kRjQH18usVZnS3gaVh8IxX18vtqf2cemjZaxY3BwfcLeqyEkmQrJZdP+dnYMnDfqCR24P+PuqUUZ8+m7OzlWBGJ/UbuNOPdmnS2eShy1HJQV6x1OOqDGk0DszpKInWVVHKhVWVAfT72QDXpu4sjnUlX45FP2+fXKjpcdQwGlxlLR0VIGaQwU6AB5CQGeUr/bIXkkknj35RQU6okJhULpNa/YP2dY62ipMrS1NBXQrPTVS6DGx0gEEaJ0K8xyxNyjDkEe9mhGerSRh00sKjz/AM329IzB7MzmEy1NT/xWnl23T5WDN+Jwy1UtbSxSR00bx28asQ4LlW0voU2vYBnRSgHDoqFsxY0NU8vXqvj53fzPan4p9w4DqDZPXuA7Cyq7Jpt4bxqctujIbeOAkzlbU0+28TBFj8HlhNVz4/Gz1U4doykU9OQG1kiLec/cV+WN0j2y0so5pBGHlLkihbIXHmFoT6hh6Zzb+7j90GH3m5F3LnrmHme52uzO4NY2CQW6TeMIUVp5CXmjood1RaA1ZZKkUFSF5L/hQFvqg/ao/jjsas0AqWbs3cKKCjBWBc7Lkdz+Qbc+wU3vVuINP3PBXz7m/wA46yStP7szl25Oqf3U3GOuQPoIDx4f8ShTpC1X/CiDuHyyLQ/FfrhkCk+WbuHcqMEUnlYh1xMgLkfkn+ntse919gHaIq0rjUf8LjoSQ/3XPImhTce8u7B600rtcBH7frlOOrhf5aHz3i+dnX3YeZzWycZ1x2L11u2jxm6Np4rcNbuehqNv7jxz1+zt1UOUrsZiKj7bKtQZGheJoFKVWLmYDxunuUOQ+c/642N5LNAsV5BJpZErTQ1dDZJoTRgRU8K1zQYJfe0+7afu5c1cs7bt3MM268sbpYGe0vZ4Ft3E0L+Hc27xpJKuqPVHICGNUmQHuB6st9jvrE/r3v3Xuve/de614vlH/Ou7Q+PvyO7k6OxHx02TurF9Ybug23Q7jyPZG4MRW5mnn25gc6KyfHU+y8hT00gbMMhVJnUeO1z9TBXMfu1uOx7zuW2JtUDxwysisS1SAaVORk0rwx/PrqJ7Pf3f3J3ub7Vch+4d97qbhZ3m8WJu5LSKxhlSJhPNDoEjXaMw/SBqVHHh0Bf/AEEGdquTHJ8W+vND3Wzdr7iYODwQVOwtLDnnm3sib3y3NTjZIP2v/n6kQ/3Y3JYUsPeLdKj/AKRsH/bZ0mMl/PEzudcS5X4b9QVUisS0r9h5pmkKn6Fk2Ajyj82NwPr7bPvtuoAB2SD/AHp/8/TLf3ZXJY4+7m5k/PbYK/8AaZ06Yr+dxlMa0clF8OeoaGZBoV4N8ZIyqrOWukj7C8nLG55v7bb343WlTsVuT6F36St/dpcoxkhPdncaev7vgH+C66Grbf8APkyz1UUW6fi9QpQcK9XtjuCapqwyn1/7jcv1xQU0cbJbSv3jcixIHPtVD7+SrpFxy0pHmUmK/sBjb/D+fQa3b+7csVhZ9m94ZTc0wl3tgVaeXfFfOx+Z8P8ALy6PF1V/OC+IvYNZT4vdlVvfpnI1LIkU/Yu34JduSlkU+Z91bNyO6cTi6MOSvlyZx6+kk2FiRrtPvPyhuDrFemeylNMzrVM/0oyxA+bBR1jvzn9xf3v5ZglvNki2/frVBVl2uZhOM8Pp7pLeSR6Z0w+Kfz6s721ubbm8sJjtzbR3Bhd07cy9MlXic9t3KUOZw2TpZBdKmgyWNmqKKrgYfRo3Ye5StLy0v7eO7sbmOa1cVWSJgyn7GUkHrEXdto3bYdwuto3zbLiz3WBik1tdRvFLGw4q8bhXU/IgdPvtT0Xde9+690W75V95ZX48dS1PZGG2/i9zVlPuLb2GOMy+TqsTSGDMVhp5qj7qjochMZ4VHoTx2ZjyRbkHc88zT8pbE2729qk0gmSPQ5IFGrU1AJrjqV/Zj27svdHnaLlS/wB0mtIGtZ7jxoI1kasS6gulnQUPma46rZ/4df3uf8305s9uFIvvPMi6kEsf+PeP6RY+4dPvpuZrp2G2NPPxH/6B6yw/4Czl4Gjc+X3n/wARYv8Arf06Yr+alu+pyGNiyPUO16XHzZGgiyE1Nu3L1FXHjXqov4jPRU74GJZ6yLH+R4Y2ZVeUKpIBJCq197dxnubWGTY4FR5FUkSPWhIqRVeNOHz6Qbl9zjYbOw3C6g55vHmit5JI1a2iCl1QlFYiYkKWoGIBIFSK9XR+8iesB+iLfMn5cbi+MOR62ocDsbDbxG+aHelZVvlc7W4d8d/dWo2jBClOlJja4VC1Y3K7OWK6PCoAOokRl7h8+XnJb7Slptsdx9QsrN4jFdPhmMYoDx1/y6yN9hvZDavd+05suNy5insDt0lrGghhSUSfULckltUiadPgClK11HhTJNv+HWN+ElR0vtEkKrW/vpmLkN/TTt5gxHNwD7jz/Xx3Qmg2C3/5yP8Ay7ep3/4DDlsCp5/vuNP9xIv+t/XM/wA1ffRdEj6a2kzOwUq28cyj6vyqr/AG1Ef6/vR98d11aRsFvX/mo/8A0D14fcx5cCsz8+3oAFai1iP/AFmx10381bfojDr0xtJyzuiou8syW1rYhCo2+SGK3P4Fh73/AK+O6Ur+4LetSP7R/wDoHrQ+5ly2WKnn69AABqbWL9v9tw6kL/NP38Rc9N7PjvyDJvTLqCt1H1G32OoE8i3Fv68e7j3u3Yip2C3H/Nx/+gemz9zXlsYHPl8T8rSLj/zn6wt/NX3uCW/0O7RMIZh5hvHNWIBtdUO3gxsOT/xPup98NzAJOw29PXxH/wCgerj7mPLxx/Xu+18dP0sX/W/pU7I/mdbq3NvXZG3Ml1Ttmhxm5t37W27ka+g3VlqysoKPcWexuDeupKWTBwx1U9I2RWTxsyhtOksL3BltXvHf3+57dZS7PAsU08cTMrsSA7hSRihIrXoh5m+6Psuxct8xb1b86XklzZ2M91HHJbRqrtDE8oRmExKq2ilQCRWtD1b7V00VZS1FJMNUNTDJBIP9olQo1r/kA8f4+596wejdo3SRT3KQR+XSXx0ksuPp2qWVa3DTyUNc7OBGFpH0PPI5IUK0SrLc8BXv72WADMxotKkn5fPoyloLiRYwTDOutAONT5Aetcfl0SXtv+Yh03sGaqwuyIK/tvcFIZh5dtVVNR7LhqEPFPPvKoFRDXB7n14ymyMalSrsjce4q5g92uXtqeS321GvrpcExELCD6eKa6vtRWHzr1kRyP8Ada595mjhv+YpYtk216HTdqz3RU/iW1WhT7JniJqCARnolW5f5mfdWYVJNvbQ6/2nSTJI3jq6HP7oq9LAooFc2VwUEixc6iKRGPBAH09xxd+83Ms5H0djawRnOVeRv2l1H/GR1kDtP3Rfb6wLDc983O9nBAqjw261H9ARzEV8u8jpDUX8w35F4yFI6b/R3IC0ciw/3PyulmdiCzK2543UMbCwbm/tCPeDnFRXVan5GI/9BjoQS/dX9p53cuN0UGoJ+qj+3/lHP+DoWdvfzQN+xJBDvXqDbW4abQYKuv2vmcptyspzqJeWlx2Ug3LBOwltpjNTD9P129n+3+927RSJ+8NhhlT8RgZ4/wA6N4gP2Y+3oD7x9zjle4Wc7Bzxd2spzHHeRRzqfQF42gK/bpb7OjndN/NfpHtKeLCNl8hsPcNd46ePB9gUsGFFXUzuYqWLH52nrMjteuqKySyxQJW/dOSAYgx0iT9j9zuVd+dIvqHtLwmgiuwErXFFcExmp4AkMf4ese+dfu8e4/I8T3rWUW6bXGCxutrZpdIXLF4WSO4QKPiYx6BT4yM9HAx1QzwyU7CzpqliUkk64BpmTnkEx8/429j9hmvUKzoAY5fw/C1PnwP7enWmqFjdGJPjkUIzWPBfSUYj8Afn+nvRB8uks0JdWUDvBqB9nEdcqpNEzC36vUtvoA1xe30uG+vvwzSvVYG1RL8sH8us8EVishFlKOjHmxN7H6n6Mv0/F/ejXh01LJgpXNQQOuo0ZPIlgUDBlPBBFrXtx/UXHvRPDr0jB9DVOqmek+KKWnyEjxFY6Y+WxVyrqZl5h0af0JJyDe9vduIAp+fRp9QktqiuCZRTiMYPH9nWIHUpU3BS6te1wwPLf46j7txPT1KGvkc9O6RJlKCoo5WKMNPIGoxtfUrgfXmx+n9fdGGa+XRc7tZ3UVxGKj5+fkR0yU6zUNa+MnhdaKqieOOViDHK0YLwSL9f3lIAYH8f4D34E4oMjoykaO6t0vI5AbmMhivmAcEH5dM81LLVzPTxlVeenkmR9VtEkNnDxHkNJDMisFH4J93JGPTpasscUYkaulWCkeoOM/Ig9Pn96X8Xlumj+7v3v6T/AMXT7v7L7f8A4N5uNH6vdNJ/nTos/dR1aKd31Ph8fwadVfs05r0je38RFU7ZxeWoFjaHDyxoGp7PGMXXRJCjrIlwaeOVISDe1jf3Q9Eg8+l/tCCKbZmBp3QGGbB0sUiWADJLTBZBb6eoMffvLrXQDddtJgN+VOClmeAVByGFlZbBzJRyNPSBSVbSZFgOk/Wz/wCPv1cjHV1YKa6QfQHod93wuu1cvTxySyyT0rUkPkOt2etdaRFNtJezT/6492OeriQM5bQBVSKLgcOtOf8AnHYOFPn9uflo6ej6O6UpIVKKreOij3fCCU1F01mxFwLj8+8W/dJAebLwedEP/VKL/N13q+4TdtD917YLdACf3/uhJB9fpfyxTqvOiwFIhV51PpVGKlTEsdQRqVJSCwYlGvdePx7jsIMFuHWUlxucxBEZwSRjNV9R6Zxnq+L+TNjsl/efu+XbklHHUUm29hffxVhlhhq4pslunxodGrxsGiJ4tpv9efc5ezdfqd50nPhx4/NuuXn94TJeNB7YzIykeNfAK2RTTa1yP+L6vYq9u57M1sc+46qjWjpHUpQULuYSTyQ8rgWvezOdTFfSLX9zwwY0LcOuZ62c13JHJdyARjIjSv8AOvr/AKqdTaurFHEJLa0UNoAUgErwSv8AgoFgB7o76c+XlToXW8HjN4YwcD7B5deos5KYyqxhUjVQC8g1q0oBuXACEgcn/be/LLx63cbcoYFnyfQen8+nbHZGWUKhbVaRvJY6SbEgEj6gG35/r7cVv29Irq1SNiwHljpR00zySsFYnVy0guVAHACEiwN15J92FfPotlRVQEjhwH+fqTkcrjsHjMhlcxWQY7E4ehrctlq+rnWKloaDH00tZW1lVPLZIoKWmhZ5HY2VVJ9t3E0VtDNcTuFhjUu7NwCgEkn5ADpi1srncLy2srG3aW9nkSCGJBVneRgqKoHEsxoB5160Cu9+/wDM/IPu7tjvWoeSEdpb0yu4cDFICtTQ7IjWDC7AxdUt7CpxuxMVjoJgOPOkh/PvCXmTdZd33vc9xmBDyykhWoSorQLUYOgDSD6Dr6YPbj2ysPbH2+5L9uI1DHZrCO1uWHwvd1Mt7Ivqr3kkrL/RKjoD5WecnW9yRbUbnTySF+o9JJ/rx7D7Vbj+3qRFURjtHUOKmAL+RQ5IP6dTC44J+n+v7a05FRXp55Ph0mlD546ta/k89+f6DfmjszCZKs+x2h3xRSdPbjEpjSi/jeRdsp1hkZfT5GyKb1p0w9OAQoTPzMfoPcl+1e8ttPNNtbu9LW6Bt2B/ibKED11hRXyBPWFX37vbX/XB9hN53W1g8Te+WpRvdrSpbwRSK/jHloNsfHY8f8WUDj1uvi/N/eWXXADrv37r3XvfuvdaQX8xTHUMvzk+Us7t+6OyKN5VZzfT/cbaIDKC1lRQv+xPvDPn+NDzdv8AXj9Q3+qv29fQt91q7uU+7v7OxqOz90sAQP8Al7ucH7eiFVGDjUmwJKCSQrwPQQLF3DNpcH1Achvp7BRjrXOB1klFuDGg8iQPXP8Am64x41ER9BcnRFEBqDnldRDc+hvyRbj6ce2igzQV6s90WI1DFSSeH7PXpxkiEKwShI414TUzm7FFDSPYFrDm2ngn8e2WUAVp59I1cymVaknjQDh6D/Z6y0ta8TEQkm0gDI3AdNQsR6rhy34/p7aIyaceqTW6uoMgzTBHEHpXY+umJW5DMbJGA58baQWVdIYKqwn8X5X6+6BSKivdwz0S3NtGAxHw+fqP89f8PRpPjp8k+5PjduhNz9PbuqtuNWVMVRnNr15myHXu721RCeHdu0zUw0dbLJFTLEmQpmpstTQkrT1cQZgRDy5zPvnK12LnZrtkqR4kbVaKT5OnA4xUUYZ0kHPUO+6ftPyH7r7Q20c97Il0EUrb3kdEvbbjQ21zpLIAWJMTh4HbLxNQdbYPw3+aPXny92ZUVuGSHa/ZW2YKQdg9bVGQWvrcDLVmSOlzGGrzBR/3g2jlZIX+1rkijZWBhnjhnUx+8vOSueNt5ysmeGkW5xAfUWxNSteDKcakPrxBwaYrxZ9+PYLmj2O3+K3v2a85Tu2b92bsqaFmC0LRSpVvBuYwRrjLEEUdGdCG6OX7G/UDdV7fzOHKfFrIMPr/AH/2CFJv6ScxYNx9bX/1vcUe83/Klv8A89UP+E9ZP/dDXV7x2oPD92Xn/VrrXsp5dZ1FIwz2iDry2tFJRl/Pk1/W3A/p+PeJgq1cDjQ9dP5Yyo0hjQd1D/P8unzEGN66mWR3eW1nYodELx+o/gFvIfpwB7M9rOq/slZqt4i1BHChHRFv+obPuhUUTwXp8wVI/l1uAe89+uH3VLv82Y6dxfHlwQCmH7eIF+WJrerAABYhube8dvfWv1PKxHHRc/4YOs+vuU52v3QBGDPtn/HNx6qSeFwCyyF2DL4yo0mJ35lbSv6gF+pH9Pp7gNojkhqniPl1m6HBoGSg86+foK9SoY/WjkK6pqYMtxIYyBcFGFv0i+v/AFvbqgYOPkfM9MuwowBIPDPCv2/5OsLq4BNlZC7ShACHdXICm6MGXjkm9/dSrVqRUcaDpwMD6hqUr5Cn2jpzhoRUQ6olUlCCpsWI1mwZbk2KOLj8f19vqmoArwGTw/1Y6RyXHhSBWbB/1f4OlPjtpS5TwSWikH+alZr6VckiQ2JBU3H9LX+ntRHaeMEYAHGSeim63tLMupJB4qB5jy/1cehZ622JHjN9bGqGvej7F60ljPOkhd/7ba1+fUCBe/F/z7EnLllHFvW1NSjLdQ0p/wA1U9eo9565ie75R5nir2vtd6p4f8okw62ePeZ/XI7qoD5edzZHsHdG4Ortm5Orodg4yqON3q9DMIE3xnaQ/a5CheohKTvt/DSR/byQBljr6mOQyh4o4i2PvuFzXPu13PsO3TldqhJScqaeK4PcCRnw0IpTgzVJqAvWcvsZ7f2nK+0bdzlv1mknMs6eNYCQV+khbuRwDgTyg6g1C0aFdJVmahJafr3GqsitBH+GjGljGEW4Edg4LXtYW/r7i9bFM1H2Y6yGl5nuiVIlPz9a+vDHTcOt8XTpNEHnbzVLTMzECOlDqCUjseQv0IJJJ4Hto7fGoIANSSelJ5qvJDG5VRpQCg4t8z9vUhNh4gThmpXCRqgsdbsxNtIYFrH1fk8Ae9/RR1qY+HVG5kvjGQJu4k+gHU5dn0PIpqbS0d0f0FrayzNcWIZrX0j6AD6+3fpBkJ5GnSU75cmhllwcj8uHTjHt1FR6dKamb9pUN0jeKaGTjSfICkiC3J/qfdxbsAVCj/P0mfdWLiRpXA1V4kEEfZkH/J0c74g727Pwu7aPZMVfWbm2GIp6yeiyzvL/AHDoKKlqYoavB18hkrv4Zkct9tj48Y7SRBZDJTLDHTVIeXfbLdOYPrP3V4pn2ZVJYSEkwgA6TG3HSz0UIcUqVppauPnvtsPJ15s8m+vapaczuwjWS3AH1bMVLCZBRNcceqQzABq0WQuZIytp9WogAljt9rUWZHB/R5F16QPppb8f7b8e50XNa8esOLdjL+nIf10wQfOmK/l59OiIKqlgkJsyoOSNVyOOQbAi4vf3Xh0gLeBPKgGCepIXRGFNjoAuf9ptdiR9R7101XUxYDiegG7a+S/QnRQxv+mPuDrPq4Zl1jxMW/N7YDbdZkg0ixNPR4/J1tNV1FLFe8sqIYoV9TsoufdqBeLUPSrwY4x+rMA44gdC/islidw46iy+HyFFk8XlKCkymJy2Nq4K/GZTG5CnjqaHIUFdSSS01bQVlPKrxTRsySRsrKSCD71kUz8+qtqi0sMqeoFbG8EzrYhXBksBYlhw4v8AXSDyP8D7cUinHozt5FkiBr3A0/zdSqKYxSI7G0bgRE2HF7BSx+t1Y2/1j70Rj58emLqISIwHxju/2OpOUp1nj8LBrySIYGVGZoKlVYpLqS5VCRpa9hzb3WuB69JbSdoJBKvAYYfxKeI6TEjMkVDkYlJkpZZFmhjBB+4p9SVUCoF/VPEdQAHJH09+4g08s9HqAM9xauw0OoKsf4WppNfkcdYPtIfJbwHw/wAU/jOjUdP2/wBtq0W/1P3/AO5o+mrn3uo9fl/s9X8WTTXxO/wvArTzrSv26MfZ1N2HR/fdfYihycfmgq8bPTvFJcl6CaWoSBDfkf5Iy6T+Ba3tv7egsfl0ssZjqbEY+jxlGHWloKeKlpxI7SyCKFQia5GJZ3sOSfr731rovPaGMqtu7sx+7KKNhBVTUlT5FWyR5WgIMkLkEhWrKWNSpNtRDfW3up62OhhNdQ7lrsIlDOtVSpBDnaoRnUsEZU/w6OdgGQT1FQxPjJ1BYWNh7t8urh9KMoGSRn5en7etTb+cdWYfHfOXc1VUqsrnqjqxAot6NC7pRCx+oEliisbqLH3jB7olV5svCR/ocf8Axxeu4v3Ebe/uvu67PDCdK/vrcTX1qbc/y4/s6qNye+buGiXQDVDUsYa1o1a0IDepkjFuSASLH3Gj3CClPWn7PLrNyz5cAUhzUhPP5+fyJ+XV9f8AITyH8S3H8kmmYzsuD67YHkF3kyO8CvkdrgLGFNhb6n3OHso+u530j/fcefzbrmh/eT2xtbf2mEa6QXvh9gC2taD59bFlYYYUledzJ/ZWLSACx4Cn6l2J+v8AT3P5oBqY9vXL2DxJCixpT1P+rh0iskGli8zKyq91UFCQF+l0AA06V+vHtO9T3evAdHlqQriNSCRkn/Vx6R6SoBNAoaySMt0IOo6C5srfQhTqN734t7YqDUCvR60bExyHzAOf9j546VOAncUpkYhkkbS1Qw0vIhOlGCi5YyA3NuQfaiNiVJrj16J9yjXxgoFHGQg8j5ivy6WtPMgVQhZo1sgUKRpJ9VmYX4Fj/Xge3wR5HohdGapPxmpr1Vv/ADk++E6i+F+5tl4+pSPdXyGr4em8VTo7ak2nmoJ8l2fkXRLEUw2DQVdB5LgJVZGnHOoAx17n73+6eWZYIpCLq6PhLQgHSKM5+YOEPyfrMb7hvtu3O/v7tHMF1ETsvK0R3+ZyBm5iIj29M/i+seOSnmkUh8qjTriAT6IEF7RlhZEU/wBQDYBBwLCx94lUGCRx8uu6rktxb5n59LPaG0Nx793HidpbRxNTmtxZuZqbFYqkVDU11QsbzmKNSyqSIInYkngL7U29pPezx29rEXnbCoPM+nQe5h5i2flTZ7/f+YL9LbaLYBp53rpQFgoJoCcswH59J6FW1jQ2kagEkW4FiPRyDpvb/efaULg+nRzKy6DqFTTI/wAPz6eKDJV+KqqLJ4avlw+exFbQZTCZiNBLXYbM4mqir8XlqONxoFTi8nTxVELfqWWMf6/t6GR7eWOaNiHRgykGh/b0W3dla7hbXNhuFsJ9ruInguYK0WWGVSkkbEZpJGzK3kVJ6+gd8VO8sd8k/jr0/wB349IYJN/7KxWTzmOglSZcHu+lRsVvbbjSp6Xk27u7H1tCxFgzU9xwR7zX5f3VN72Xbt0RgfFjBagoNY7XABzQODT5dfMh7w+3t37U+5/PHt7eMX/de4SwQSkEeNbk67WcA5AntnjkHybowXs56jbr3v3XutHX+YnUyt86/lXFdbRdkUBDCNZSsY2Ns8uhLEBHOq9iCNJB4PvDXn2p5u3/AOdw3H/V8uvod+63Ei/dz9mXoattL4rTP1lzn5jojVVlSuiRnbS4ERDHQoazW02F2jUEfUXH+29goseB+3PWRMVmDVQMjOM/6j1at/La+AGxPm3tztPJbp3/ALo2VkOvcvtGlhj21j8LkqPJ0+5KbcE7SVf8XieRZomwgChCo0tzckWk32/5EsucYNzkub6WFoHQDwwpB1huNfTT1hR97L7znNX3f985R27YeXLC+tdytZ5Wa9MyujRPGtE8J0FCHzWueFOrMJ/5DHUM5BbvnstQrFkC7c2jZSRbjUjXFv6+5BPsdtBNTvdx/vCdYkx/3kPuNGMe32yE+ZL3f/W7oGuxf5BWSgop6rqb5CQV+Ri1ywYjsLaBx0FU/rIgOf27ksg1KGNrN/Dnsf6XuCfcfYpwjNtW+hpKGiTpQE/6ZSafs6HvKv8AeWMbiOHnf2wUWhIDTbXcnUoxUiGdKP8AZ4q/b1Sn3r8d+6PjHvUdf9z7Rqtr5p6ObIYesDLX4DP4qNo0mzG2c/QvJjc3TQySosyo/npXlWOoSKQ6PcLb9y1vHLV4bLd7QxyEVVuKsP4kYYI9fMHBoeugntr7r+3/ALw7AeZOQt6W6tFdY7mFhongkYErHPC3fGWAOlso+ljGzgE9IvEZPhHaollWML/YCK7BdTL62F1BFyPZKtPOvyx0Jr60HcoiVWJPnwHrw6Mf0F3vvPoDs/afbuwqqV8/tGqaWoxDTfaY3d+1si8X94tkZiZdUbYnPUSBVaRJBR10dPWIvnp4iDvl7e73lzdrXd9vb9aJqla0V0PxI3HtYY+RyMgERT7l+3Gw+5nJ+9ckcyRKNtvkos4GqS2uEB8C7iHHxYXNSAR4kZkiJ0SMOt2TrDsba/b3Xeyu0NlVjV21d+bbxO6MHPKnhqVostSR1S0tfTEs9Hk6B3aCqgf109RG8bgMpHvOLa9xtt326y3OzattPGJE4VFRwNK9ynBHkQR18/HN/K28ckc0b/yhv8Aj3nbbuWzuFBquuJipZG4NG9NSMMMpDDBHRIf5pjmP4nZNlF2/0hdeAC1xds4qi/8AQAn6/j3HHvKK8mMKY+rh/wAJ6yG+5wob3ptATj913v8A1Z61zqGaVIXvNOAxACKVDaozdhbi2scMf6c+8T1iIU0ZgK/I9dULlELgCNccT9v+bpfYFpZKunKzsAjo7cpqdXB02ZQSVa9rf09mO2IfrrSjH+1T/COgdzHoTadzrGKmCQDjghT5dbhnvPXrhv1TR/Ndo5KvcHx/Ea6imG7c+hUN6q3q4C2r63I948++cZkueWNNaiO54fbB1np9y6dIdr9zdZoDcbb/AMc3DqqOlw8p1GTyrLE0pvdACpW4W5+mkNZv63v7gpIia1JLD19Os05r2NdOmnhmnQy9AdQY3tntjZnXmUyuQwdPuutzGKORpaaDJS0Rodn7n3RGy09RLBERNJgBGbt6VckAm3sTcocuW/MG+2O13E0kUUmoF0oSKRu/A4yV6jn3T59v+RuSt45m2+zhuLi2EUgilLKrB7iGE1K5wJaj5jqy0fyq9pLYf6X9yEC977UxBJubm5/il/8AjXuZR7H7SOG+XP8AvKdYjn75XNBJP9Tdv/5yzf5+nKl/lfbYpBaLtrO2F9IbaWKIS976QMuBzf8AN/byeyu1R/DvU/8AvCdJZvvf8yzfHyhZfP8AVm6e6D+W5hMcwem7Vygfj1Ns/HG9iWHAzircE/09vJ7ObbH8O8zf7wn+fovufvW7/dDTLynaafQTS/5ulZivgZRYrK4nKjsqrqziczg8ylI21KSlWolwWax+cp6f7lM5O1Ok9TjkRn8chVGayk29rrT2ss7O6t7pN2lZ45EkClFAJRgwFa1AJWh+XRDuX3jNz3Lbr7bpOWLdEnglgZxLISBLG8TNQihIVyRwyB0cPt7ds2w+rOw95U1vvNtbN3Dl6K9yor6PGVMlCXtz4xVhNX+039j3mG/ba9i3fcU/tIbd3T/TBTp/nTqGORtkj5k5y5W2Gb+wu7+CCT/SNIoenz01p1RFtmoxmTWmhBVJFRneSViJZJiB+5PJdmmllckl/wA3/wAfeKlnJFLQHjSpr69dId2iu7MyyEEoSAAvAD0A4AD06Eqh2zBkGihhCCqlmSCQFgUBe0cTRcAE3II0+ziKxExUV/VqAQMD7egnc7u9sJHkJ8EAsKccZIPRtes/ifhN17Qwe8s7uDL0tJuCjhy+PxeEpsLTtDjqsvJi6nI5DMY3cElZWVuP8dRJHFBSR07T+K8rRmV5Q2D28sLuxtr2+mkrKgkVE0igbK1JVyWpQ4oBWmaVMB82+9m77dve47JtVlDqtnMLzTGRizrhwqo8YVA1QCSzMF1HSCFAddj9FYHbe4q3HUG6M8lNS5XHpGcpjtrZKIUM8FO7yOmPwe36yZkLP9Khb2tx9fZpde22zSJ+lcTxuDx7GHyqNAP7COvbV7w8wrZQXFzt9tIzocKZ0NakChMrqOHmp6zb1+Lm99qRfd4qOi3hiKhmEdbtVZaPJJEtMawz1W0sjUVVVLDUQfoTH5DI1cjkLHTMSB7Cu5e2252qPJZutxGKtSPtan+kYmv5MT6KehNy9727FuzJDuSSWd0oBIuDrQ5piZFUKQf441UcS4p0CUe3SAHZFqGWpOPano0UT1Vb90KCLEU0cxhNLl48mwppKecRSU89xOIwj6Qja7PdXF3BaJCWmZwmhRnVwAzSjVOQaafxUAPUjXXMdpbWk17JcBbVYzN4jmoVdOouSK6kKiqlah8BNRIrZD1L1lQ7G2tTeBaGpztbOmSzNfTgtFVTPTeGKlp6ho4Znw2Jp38NICqFlMtQyiaqmHvIrl3YIeX7BbVQDO3dK4/E/wAv6IGF+WTlj1iHzdzfd82bu94zOtmg8O3iY5VK1qRUjxHPc/zoo7UXowNM332AkidjEYRJCXc20GmdZITr59BFhf8Ap/j7OGw3QDmH026K4FQxDUHnqFD02GrqqGaikSWRY6antNTqwlhq6WSpLLHocnx1NPGzEMCCRxyOPe9Nanz9Olht4blLhGQFneqscFWC0rUcVJpjqpP+aJ/Mvq/jnDjfjt8foGz3yL7I2vkcvX5uioTmH6T2JPT10Mu8TgTojze/ZaOirKrE46odKWmipDX196bwU9ayzaeHHoOywywTGJ8SDjmo9ajrVo2Z0v3N3vie9+9MLj8tubYfVe1c1v8A7R7b7hy1bUZLcVBTGmMu3E7HzFJlpd1dp5mkp7wY6CrEsQNleJ54VmboSCfTrwBOpgCaCpJr/h9fl1tvfyZarOP/AC6ehnyYqQIqrtSlwRrZamoZdr0vb++oNvQQCcmQUFPjo1iplU6I4ERUsgUe1CCqip6UwqHhUSV0gmgFOH2/Z1aQ8dTUIPLGgCEgO4CEfkkEksf9ha497+E4PVkaCE9jsWPkM9YxSSSqBFLEyN6lIuAb2uCP68fj3atONenfqEUnxEYNwI6cGRhGoaTW4vqP6ToIUD/XVSPr9T7oKV4fZ0hJUsSooPIdJnIZHCY/zSZKVUiqZ4nZqanqiTVxlUhlLIjMs9lt6bXFyfr72RQV8+ji2tNwuRGtrGS6IR3lfhOSKVpT7flTqD/eHbNv+B9TfV57fZ1GrRr/AOAVvF+m3q0/q08+9dKf3bu//KKlKafjXj/Hx/nw6X1LTx0lNT0kI0w0sEVPEv0tHDGsaCw44VR710G+s/v3XuoWRx1HlaOegr6aGqpahCskM8YkjP5VtJ+jowBUgggi4IPv328OtjBBIx0x4nbeM21SvT46GKjodYqKhYfKJaiYAAyTOzuztcAC7EgWFwB73UeQ6UiRW7Y4gHJx5gf5a9abf87rLpB8+t2UlvX/AKG+oJiFVL6P9/j4YmmSwKFgTbkC4594re7DaOarsnzVKflFH/n674f3e1i0n3aNjnr2fv7c0yT/AMutTT7OqcmqpZmZU1G9mVS1yDflrixDkcXP1HuKtTE+f+r/AC9Z2CFIwNVPmeHl/g62M/5AIf8AjfyTRjIGbBdb6dJKldOR3j+sqLKBqPII59z97H18ffuPwR0/a3XKT+8y06PaZgBQSX/z8rXh1smV0bmLWjKNFwgCXdyFuGYnU2kX/wBifeQjA/l1yot2UOVYEk/Ph8uk1Xq8kCDS7SmNtNySRfjySAfpVm/p9Rx7aYEihBr0bWrBJGNQErn/ADD7Og7fEPJVwvFqenDKviWXxo8hJ1OxNres3PJJAt9PaEwksCDjhTh0KFvlWCRXoJPUitB6fs6X9AEjCIEURoABLGqklVsG0qxsvq/qOD9Pa1aCgAFPXoM3JZ9TajqPkT/h6f8AyKrJoRVsLaGZiLWNvKq6lLAD8/S/t0n9np0XaWINSftH+TrUR/nK96v278v5uvqCp8+0/jztWg2RSqrl4X3/ALtipN3dh1tORYFUx0mBxki8mOpxUy8HUPeLvuzvY3LmAWMb1gtF8KlaqWwXNPJg1VI/oDruH9w324Tkf2Mi5nuItO980Xj7i5OD9FbFrayRvmZBczD1SZD6dVUxRoNJI4BUgG4F+Rf1fRbj8+4tAFRUfPrMt3ehCn16uu/kh9Gp2F8osj2pkaHVhOldo1uRjnaJzTPu3dsVTt3BIk7DxRTQ4eXJT6f1XiU/ke5Y9pNoN3zHJubJWG0jLVIxrcFVAPCtCx/Lrnr/AHh/uK/LftJt3JFpcH6/f79VdQRX6W1KzS1HGjT+CAeHEdEX+e3TbfHf5l9+9bLBFTYAb1m31sSH9mOl/wBH/ZMCbwwdLQQxJEI8dtuuyFbhIvRx/CDcsQWIS512dNl5k3K0RAtv4hZAAQoVu5VBPEhGFfnXrJT7tnPS+6PsL7Z81+IX3I7eNt3Fs6vrbAm1mZySavOiR3DZ/wBHGBw6J/LOrySeJ9cZtodwUcgAkOT9Tf6D+t/YQahOAKeVep0jjIRdQo/mBkfZ1s0/yAO/Uq9u90fGLMVdqrA5WLujYFPLLAA239xmh252BisdTx6ZEpcHumkx+RmYr+5VbjkNyQ1sg/ZrezNb7jsUz98ZFxFWpJU0V88KL20A+fXIn+8x9tWtt65D93LGD9C7gOxbm4Df29vqms5HJxqmtmkiUDgloMcOtjv3OPXK7r3v3XutFP8AmP1M6/PT5ZRq6BR2TQmJdTIUK9f7L1zsI/UxuQB/W3vDXn0E82b6af8AEh/+PEdfRl91SKM/dt9k20mv7pfUeNf8du6AVwOq/amrZmjaQeST9OoD9R4+v1H0+pt+PYIbNCVx1kzFCED6MLxp6dbPv/CexlfZ/wAn2VSt9w9U3ubkt/Dd+XP+B/w95EexlPpeYqD8cP8Agl648f3nQK81+1AJr/iF7T/nNB1sY+5565d9e9+690Wr5YfF7rz5cdO57qnftLHBUSpJldj7whpo5s319vampKmDDbswcrGOQSU5qHhrKbWsWRx009HPqhnkUh/mXl6y5m2m42y7UamBMUlKmN6drD8+I8xj59St7M+7vM/spz3tfOvLU5KoRDf2TMRFe2jMpltphkFW0hkahaKVUlSjopGijn8BuXZe7d19e7tpI8RvHZG6c9sXdWPgeV4KPce0MpWYPNQUU08NNJVY419C70tQY0+5pmjlHpce8Ir+yl2+9urG4UieGRo3FeBU0INKjBHX0bbbuO07/sey8z7JOZ9i3Gzh3KzlampoLqNZYmcKWCyaHAdanQ4ZTkHp2xtXqhjj+5sxLI0kUjhfGAVfUpXSJSef9b6c+0YjFCKD/Y6Q3UPezGH0NGA4+Xnw62ff5JnbFRuHpjsvpqvqknfqzeNLuTb0QYj7TbHZqZLIVFAqMxLMm98FmK12X0/7klX6j3k/7J7o1xsV9tMjV+mlDx1P4JamgHoHVj9rdcfP7wHkyPavcTlfni2gKpvNgbe5JHxXFiUjDVA/5RZLdKHP6ZPRiP5r0hi+IeWcEDT2L1sefoR/eKK6n/gw49m3vFQ8mvXh9VF/z91G33LUD++FmpH/ACyr7/qyetbnGVH3CSvoBJdmvrKqvpChdQufVbgfQD3ikiVViU/1cOurl3H4TIofy9OhF2vMf4hjQskhjYKAGIBDgnSBYgEBSR/r/j2ZbYlL+xIxV1/kwx0CuaErs28VQBxDJ+zSf8vW5T7zv64TdVDfzQBE+4+h45C66sJ2uytGAW1JXdZHTyOAb8n/AA9wF71qGuuWQR/odxT7awdZx/c+LrtXuQ6UxcbcDX0KX/VakGNgVVdyvMRN2OsOxb1yW4OgXC3+l/x7hdIlycdZaSXUhJUA11Uxj7B9vQ8fGTNbb2L3p1pu3cdcmMwO3dw5qty+Samqao0NLkOvN84SnmeGjinneH+KZimidlRjGkms+hWIFvIt9Y7VzLYX19N4drGzl3oTSsUigkKCaVIH8+ot95dt3jmX295h2baLUz7hcRRJFEGVdRS7t5GALFQDoRiASKkU4kdXLL8w/jU7BF7XwrMfoBjtwm/JHB/g9jcg+8hB7h8mk0G+JX/SSf8AQHWCp9ifdoDUeS7gD/Twf9beuf8As4Hxt5/4ythLi1x9huC4vcC4/hFx9Pe/9cHk7/o+R/7zJ/0B1X/WL92Mf8gy4p/p4P8Arb15vmB8bEBLdr4MAKXJ+xz1go5J4xH49+/1wuTeH78j/wB4k/6A68PYv3YagHJdxWtPjh/629Pu1/k10TvTcOH2ptjsXE5bcOfnlpsRjIaPMwy1s8FBVZOSJJKrGQU8bChopZBrddWmwuxAKux505Y3K7t7Cx3ZJLuUkRoFcVIBY5KgDAPE9Fu8e0fuNy/td9vO8crTQbZbKHnmZ4iEDOsYJCyEnvdRgHj6V6ePkBhqvcPR/bOHoIWqK2t6/wB0pS0yDVJU1EWIqp4qaNfzJUPEEUf1Ye3+bLeS65Z36CIVka1k0j1IUmn50p0h9sr+HbPcPkm+uXC28e525dzwUGVVLH5LWv5da8WIqJqCseppnDQMsEj+A3R2k9TeMknSCoFtP45PvESNmSRnRqqfTrqNexJcwCKQUkFQNXlTGfXz49D3hN01DwxuXOpEikYPdSq/qTxPGSY5LjlwRa1x/X2ILa8OlSRkcc/s6je/2iJZGGntJKgj/LXj8h0ZHrn5Q7x2HjoNuR0uM3Ft2lDtHiq6KajqaCGV2kaDEZWlY+OmWVy4WeCdVB0p41AX2N9j5+3baIorTw0ms04I4IKj0RhwHHBDU4Cgx1EvNXs3sHMl1LuxmmtN0k+KaIhlcj8UsTDLEeaspPE6iSenvcPfu2N45f8AiGR2/mMLLUUUdNV6DR5vHiaKNgWhkhamyc5sBa9EoI55sPY3tPc7a5iq3u3zwswqSmmRR/NX/wCM9BN/ZzebGxW3sdztrjQ7FQ+qJ9JyKghoxQ1/0Tozuxe5dgbk2BhMPDu/DNuDHy09KmMyFW+LzE1HFPLTUs0VJlFo6yodKZlVtCsV03Nh7GG182cu7jIqWu6xeIRhJCY2Py0uFJ6inePbrm3ZN4u7m62C4G3sCTNEoljBIDEF4y6jPqRXpVZ3rjaO56io3cMNEu+VxS1sGWiaVGyLUFM+LlSrpklWhyVfT0ZamjqZY3qoaaZ4opFillRzlbCx/eMG6fTr9Wo0FxxKkEZ8jQMQCcgEgEAkdBO43jebbbp+XheudlMlVhOQpJEg01GpFLAEqCFLBWYFlUids2ulnxsMUr6pqYNTyxWNwihjG8mrSdWg2+l7r7N7ihJIHRXZIRWpxwPS121M882dwckn7ksCVNO0lzH43UwtpUEE6dSXsfaB+IPSjc1EX0V7SoRyrDz9Rn9vRavkv8hdp/GPp/dfbG8Kinb+EpFiNrbfr8pT4yTdu+8nI2L2rs6nrqkiClfNZlkSapf9jH0azVk5Smp5ZF9r0ip4fPowuZUt7dpqjh2kYqWytPtr1pKYt+3PkXvHM7bqd3Z3dnyH757N2jTph6ukmya9t7qz1blMRDmKjd8DSwbI2p1rj6g6IYtGLbb6+hYoaNQEmSc8T0DWZmJZmrIxz51P+x/g6u+/mQ7B258Nfgf8dv5dvTBlzu++/wDsbCNuOZneKv37k8NncBlNx7gyAed1xMO7+3Mtt+loqd2MMVAjU0ZdadmDr0VQoOfPpyYCONYQamvn/q9ethv449RUXx76B6a6XirKTIN1j1vtDZVZl6Wl+xhzWWweEo6LMZqKj1O0AzOUjmqtBLMplILM1ybAUAHTYDPRRUgYp9nQi5rL6VFNFEQk8Mt6qRjEiHiwRluwYj/WPtxVrk9G1hY6m8aR8qw7Bkn7a46bqbc2Op6eNC8lZMtgYMXG9b419Kl5JlCxRm9ywJLXvf3puOOlM20XUsrsFCJx1THTXzwOJ/wenWH+8uSrJZKXG4iGGZU8iPkKsPZTJpWVooUICsAbKzX96AJIrw6v+6LWBUlu75miJoREtPLIqT/k6wbi3BX4zHT1Cw4yrejhFZPHkJo6KmijiDF5/K5Jn5XTGi83tf34igJAx/k61Z7fbzSgBpVViUVkqSa+VBw+Z6R/+mjbOny6sXp/gX8a1We33vl+z+w1+G1/J6fL9b+i1/dNafxeVeln9WLyunXJ/a+Hx8uOqlf5fn0PXu3QR697917r3v3XuolVFLOvgTQkTj92VhrYLf8ARHGbDW34Ymy/0PvYxnp6F0jbxGqWHwgY/afT/D1pW/zvNv1U38wPdBo6aeWKTpnp6mhZCXKyp/fNnaV2DaUAkAueLm39PeK3uwhfmu5Va6+w/l4UQH+A9d/v7vfc4Y/uxbMJ5VDjf90dgcYP0oAWn2dVLR4mfFhlq6aVGQsHZhZgoAuQPoAPcYiJoh516zUe+jvCpglGkitB1sV/yDIg2d+R4hIk14Prdm5BQn+I7wYE3tYW+nue/ZIUm3ynEpH/AIW65Wf3lT0i9qDIKUe//wCO2vWykygAx6CbXuVNwASD9bepiP8AYAe8guHXKRSSQ+rjw/1enSeqIHmZ4yCFRSGFxwlywHF1AI4P559tsKkinRnHIIwrjjXHTLHSqhkFha4YLZQFUNcnT/Zva1vqR7a00r/g6XmYkoc18z6/n0609P6S506Qn9hNBCNcCzcDUT9fqSP6e3AMf5vTpHLJVqCta+ZrnpD9z9nbe6J6f7K7h3Yyw7d602Vnt5ZCKHSauvTCY2esgxdIjelq/L1MSU0CfWSeVFHJ9ot13CPadtvdxlA0wxlgCaampRVBOAWag+09CTkHlDdPcbnrlLkTZBq3XdtwhsIi2FQyyKhkY/wRKS7HyVSetAfLZzcW68znd4btrRXbu3nns3vLd9eLiOt3TurK1ef3LVxqSTHFUZfIzPGgNkQhRwLe8I765mvLy5uppC8kjlmY4JqeJp5nifn19MFlt+1bLYbdseyQeHsdhbRWFjEaVS2to1hgU04lYkUE+ZzxPUWMtcEFnYk6RHZjc3ChdQ+l/qP9f2lyMj16dYLkECnz63H/AOTR0rT9ZfEnDbtykQpc73Nmavfk7qp8z4Omd8BtWmu0YYQy0VDJXIBcA1zWPJvlV7WbR+7eV4rl0Hj3bmUn+iO1P5An8+uDH37PcCTnH3v3XarOTXtuxQrtSV4CQVluTx+ISuYyfMRjojP/AAoH6LmOR6E+S2EpFMNTHmOjd+VMEUJkPj+/351pWVMyqXFLQzw7kpmJLL5a6FQBf2D/AHl2gsNu3mNcU8Bz6EEsgA9WBapPkgHWSf8Adke4yfSe5ftLuE/6iGLmPbUcmmdFnfqo4anBtH8jpic+XWuH4nN2DXNjcHkab8q3F/r+R+D7gQqeOrPXVXWooCMV6Nn8Du9m+Nfyx6S7crK2Wj2vjd3rtbfz6444H6931C+1N01FcWIaTHbahykOeMSkM8+IhsGZVUijkrd/3FzFt1+70tw+iWtfgaqsaDiQpNPn1B/3lvboe63sl7g8mQW4k3h7L67bRQk/WWZ+ogVAP9En0NbAmoAnbgCT1v8AIIIBBuDyCOQQfoQfeZXXzS9e9+691offzJowf5gHyvcSvH/xkii1M/4K7A2SoSICwKaebH6k8+8N+fQf6274a48d/wDjx6+j/wC6ixH3ZvZUFAw/dLUA/wCe274/PoirUhd2P7mgASIStgADb1AD0lr/AE9gwISct1kWJqKASNVaEDrZy/4T7FafZvygazaf7ydUqRH+A+N34rfj8W/2/uffZYCOz5iOf7SH/BL1x+/vNayc2e1IJ/5Z97x+U0HWxZBUPdUlC3Y2Ui9/pdC/4tKnII4vx9fc7RynUEfj6/6vXrl48YyV8uP+X9nU32o6Z697917rSa/mjbQg29/MF+Rz4yNVpsxl+u91TQQRKmnIZ3qrYyV9kFvK9RXUktTI31d5zf3h97l2yw867yqABNSPQerxo5r9rMT19A/3Pd8k3L7sftULtiZYIL2zVmJNUh3G7KfYFVggHkFHRKKSid3COWDhW8g1IqqBKSsjxLyjSC1x/h/Q+wGY6rpP8usgZ51VSVppqKcfTIB86dXwfyQaqSDuztrHhlK1/VK1dRpBGp8Ru/b0NGXtZPSmbm08cajb6n3NvsmSu77uoaoNsCfydaf4euav94dEsnJvIE+k1j3SVF/5uQEt+3wlr+XVlP8ANtYJ8O8yTpt/pH6z/V9L/wB5IbH/AGB/2/sfe8A1cnsK/wDEqLj/ALbrFn7kor762IH/AEar/h/zQPWsdjqkKGBkZjNJZUiYeE2BPpUgE6gLgX4PvFNVpUHz9OHXXW7iJKnRhRkkZ6ETZ9c38WxmpWYPW08aKrHSHZlAX9X6VjJY/kn2t2vUL6zJTPir/hHQL5thB2LeiCBS1lJrx+Bv8vW7B7zx64DdU5fzUq8UG5fj9Jr0k4XtshDp0uBXdWgmxHLIH4/1/wA+4D96jS65aP8Awu4z+cHWd33NbY3O0+5q6cfUbbn/AGm4f4adVjUG4HYopZGCSG7FCVKAEsVVrHSbA82+lx7hFZGqMjj1l5c7ao1NQ5GM+fl0oYcuTMWbRyodvGQCwa+kR3tp0I30PJPHt3xKHVip6LXsqIAtcGgr/l/PpyXKQoNTqWcHggEssSHUhdhbS4BPA5Hu4kAGRnpKbNySFbt8/tPp1mXLQaANcaMvIDmzlWU2upA8hPJufqP6e7CdBilD02bKSpopKn04f7HXFK+kntpMasV1RqjFtbabyRnULAaTf6nk+/LIpNPw9ea2mjB1VOaGvl6HoVPjpEP9P/UM6ag3+kLbmoq50u3ncMui5tGuof65/wBt7EnJYA5u2JgO4XAH8j0A/eB2/wBa3nWM0p9A35DWma+vHrY6IDKVYAhgQykAggixBB4II95d0qKEfl1yyBINQcjgeqGfkd0XV9K9iV+KoMdLFsTdM1bl9g5KIEwFJfLW5TafkA/by+140fRC13nxIinjaQx1a0+LPOXKk3Lm6ypDEx2uYl7ZhwAyTGT/ABR+Q4lKMK0bT0h9qfcq35/5Ztrm7ulPMtmqw7jExyaUVLkDzjnNKkYSYsjBQ0XiBDQVFTTNCoHjiLEg/QeMAahpNxdCvP4sfYUjd49IHDoe3McMolYmreY+f+z1kTJ1d5lik8alZLPcFWN2ZSxILmOxvb66vd/GkqwVqDqrWcPYXWpqMf6sV6eI8pWusao+ljDEqMQXdBHDplNlIBEg/Ux+n4HtQk8mkd2CMf5ekL2cCsxZagMa0wMnH7PIdNcubnEyvMdcYVonp3jXROr6o2doRdZNCmxLfS/09sfUyajq+EClD59LE2+IxlUNH4hgeFMjPEV+XS02F37v/q2eiba+fqqvHY6p+4g2tnpJ8lt7wNrjq6WOkM6TYWKeJtK/YyQLcK0iyBQvs92PnLfeXmAsrsta+dvMS0dPQAmqfahX514dBrmj2u5W51jk/fO2LHeOtDe2oEc+rGli1CJqefiBvMKVJr1Y/wBId17X7bWbNYKJsPkXSCDce055xVVe38jVeZ4WjqlhpkyWIrJoJTSVyxRLURqVeOKdJoY8l+U+bdu5v2n6i37L6KgntyashPAg0GpGodLUFaGoBBAwo5/9t999tN/Xb79hPtU9TZ3qLpSZVpUFSW8OZNQ1xknSSCGZGV2MUJExmfwmTLFTNMcfNZxZ4aqyWdbjUYpJARxxp49n7/C3yz0DplNzZ3VvTGnUMcCuf59asv8AO6+UcvaHyS2r8c+qa+uyNB0fkJ5dy/wJZalsv3dvXDDDNt+gghgqI6+q2ftHJtSSeK8hrs7VUrKJKdvaV2riuOgzJcvLDbQmv6dc+teH7Af59DF/IN+K+Kmy3ZXzG35T01KNi12Z6Z6xpsmkNPBicz/D8dWdnbykesF6aupqCup8FTSo6eOOTKROCHFtoPPpOod2pGpLcAB/q/1U6eehMvtf+YZ/M17P+Z2S2XktydG/G+m23sXo/HZWsL43O752hkarIbP3g804XHUmOxktTXbpSiU66aoy2JlkDSJIfessxIFadG20bQ26ySs04jto6BnIrnNAAOJp+zHnTq/N9274z9qmgOMgpYpg8oxuupicRgs1O2XrGjhLn6fsiwFwCSfbwBPmOhXHtuyWTGJxJJIV01fFK8DoX/L08yV2Zy2F+4EsNPAWUSpjoddnL6mYVledThJPpoS4Fz7cFKcan5dMrbW9pf8AhtXXTGs5p6UXAqPU56dcRNiaOh/3KZCGlYPdYpJtKSlgXJaKNVnnYC5bUAo/x91LeYHTF3Hey3GmztnkHmwFSPLie0D0p1MWSeasqjiomagleMyVs6iionVUX/MoqtWTvx+Aq88n34MTx6ZKxx28X1rj6oA0jXvYceJNFA6jSbExWWrHrM21Tn55pS8VLkGEWKpqcjVoioYdMckafX1liQOfeiP4j1T983NvEIrXTDEooWTLk8MsfP7B0tP4Jtu3j+ww+n+G/wAJ0/w6ht9hr+5+2t4NP23l9Xi/zerm2r3TSn++1/Z/qx0SfU33HXJXxPF+Jvi4V48aYrx+fSn976L+ve/de697917qPVRyzU8scEvgldbJLyTGbi7AAg3t7905EyJIrSJqQcR69agX832jqYfnfudGkapDdUdVPI2kRuyr/ek3DMzm63Fz9ODx/TF/3RP/ACLrzFB4cf8A1bXruX9xueFvu37OwXTTetxAHGlfp/s/Z9nVZo27TzsUq41eGWZ5VRg7zSGS91kZlGpP9SR6v68e47IU4I49ZaHdZY1Bhch1UCuABTzGcf4Or4f5HeFpsPuT5AmniEMdTt7r1/EEtp8eW3eqi7DU66W+pF+Pc3ezChbnfBT/AENP+PN1zW/vDtwmvrb2wEramSW+Fa+qWp/ycOtgupmeOyoOCPJISSXYMxCooBFjcfn3PmeHXNGGMOAWOeA9MDj02AOy6nWX98khfSD/AEAkvwAT9Pzx71mnA58uldQDQEdv+rHUNoI21SpYFB42sSEDAm45GpgrG305P091oB3fl0+JGHaeBNR6/wCqnUincxaA9wbDSrEk3/AWMDguf03/ANj72DSnHpuRQwbTw9R/n/w9UX/z0++X231F1r8c8VVxQ5Ttzco3vvWnWRXnXrzrWtocjjqOcq6zU38d7EqcZLCxUpNDiauO/wDWHPeHe/pdstNmiaktw3iSDj2L8IIPkzVIPqg66Lf3dHtuu7c782+6l5AWs9jtP3dt7fh+tv0dJGFRRvBsVmDCtVaaJutYZiVuSGvwGuBfUfpqI/w943H59delANACKeVP8nQh9R7Ere0OztidcY+rpKCr3punC7eXJV1VS0FDjIcrXw0tTla2trJIqWmpcZTSPPI7sFCRn/W9rtttDf39pZqwUySKmpiABUgVJOABx6CHuBzRByTyVzPzfcQPLHt9lLciFFZ2kZEJSNVUFiZHoo+Z/Pr6Bmw1622dtLbmzsJmMBSYfaGCw+2cTGc5Qaf4VhsbT0GP0OKlVcfaQodS8MTqB595oWtztlpb29rBfQ+DHGsad6/CoAHn6Dr5lt+j5r3jdtw3m/srqS9vJ5LqZvCfMkjs717cHUTxz5dFx+fHU+0fkr8RO7OqMbntuNuer2fLuXYUn8cxqtT772BNFvTZymVq2MRUlZm8JFTVV2VHpJ5Vf0M3sg5xhsN65d3O0F1E0wQyxgOtSyd1ASaAsAVr5A16lr7tXOm9+0vvh7f86XW2XY2dL4Wm5jwZDqs70G1usaDVlilLpiodVIyB1oeYsjIrBPG0iR1sMc6LMjxyLE6iZQ8UirJHIFIuhAKn6j3iH4bLIyMcg0NKevkfPr6P7xfpGljcAvGxUlSCKjGCMEfMfl06S4qKekmpZoxU09UzU1RBIhaKamkBjlEqNw0UkbkEA/Qn+vuygx6XViCCKU4+o+w46RrevHPFPG+iVO9WBpRhwoR5g9bzP8sTvuT5A/DXqrOZbJSZPeuwaGTqPsCepmimyM25NgQ0uOostlWhCRjI7s2hLi83IAq2OStb3l1yHu43nlnb5Wes8I+nl/0yAU+0lCpJ9SevnT+9t7bL7Ye+/Om1WVoIdg3CX987YqAhBb3haQxx6slLa48W3BqcwnPVgHsY9Y2daK38xugSo+fPyrkmLFG7NoUjGkWV/wC4WyvzqBPLXv8Aj3h7z0lebN7FcfUPX82PX0Y/dWuDH92r2YWMd42hyf8Assu+ignEQlzGkivo1RojMSXXSGYqGF15+pPPsJ+EpJAPU4fXOF1MlAck+n7Otkj+QRRmPavyfgl1K0ub6qZgQFK3pOw1W1uCFVRY/Q+579l4gbTmJT5vCP5Sdcl/7yqYNzP7UyJSgsr0D/nJb9bAsl4ovULvE5WNVU3ZAwaSI6ebqPWh/p7l1yVShB1qaCny4j/KOuaaUdq+RGfkfI/5D06U8omj1ghhqZQ4+jgHhh/W4/2F/ZjC/iJq+dK+vSaRNDaes3t3pvrSF+Y++KHuz5Y/Ijs7FVkcmAz2/Ditt1kUwlpsjg9i4vGdf4jK0kqvLG1BnKDa65CHSQGjqg1gWI94Zc4bim8czbzuETBonmKxkcCqURT+aqD19CnsTy7ce33sr7W8oXsJG5W22+NdxsKMk15JJeyxsKA64XuDE1eBQjgOi4TYyCntJ4YZHUpG7cnyLKLRm4Ya2Fj/AKx/x9hrT24Wp6lWO8kl7fEYKcj5U49XrfyPdrVcu/O8N5CL/IMTs/b21/O3J+8z+cmyngBt+kQbYDfU/X3N3staSfXb1eUPhCFY6/Nmr/z51zc/vD94gG0e3GxiT/GpLm5u2Ufwxxxxq35mUj8uj7/zdzp+GmcNwD/pG6zC3vYsdywgL6QT6jx7Gnu6K8osDw+pj/wN1jt9x8V9+du9P3Vf/wDVg9autBrgJkR6cvKmhEAl0xFSLi/J1D6W494saaauFfs67CXIWXSpVgoNScVPS/2oWXcGGYaJr5KiDuFkUktUR8BeEGgG4/qPanbo6X1nQ1Hir/hH7OgbzWFPLu+jK0s5iBj/AH235563h/ed3Xz4dUk/zd6s0u4/jla12w/cTgk2OqKv6nK24Itqb3AHvb/uRy0f6Fx/hg66D/cdhE21e6lQaePtg/am49VRUNdVqI2cEq7iQOxQa3ChvCnHJ4P1/r7hAGnHjxPWaNzbwEsEPcBQgVwOFT0LnXu2N19lbmoNo7SxM2d3DlZ6hcdjKWfH09RUNRYzIZep0z5KroaZDBjsbPIQ8ik+MgAkgEy2rbL7ebuPb9vty909dKggfCCxyxA4KegHzZvuycnbPcb7vl4INsiCiSVldgNbrGvbGrMau6jAPHoyX+yj/I8kIeqdyKgJ5+92m35BBIO5/wBQ9iz/AFuubqU/dL/tT/oPqIf9fv2oFSObYdX/ADSuf+tHXJviB8hW1aurdxM8igF3qdqFEsD+of3n1tz9LHi/591b255sKmu0PX1Jj/b8fXh7/wDtYCKc1xaQeAjua/8AVjqI3xB+Q4AUdZ7kIVVYqtVtXXquQGFtzWAb8f1t/h7ZHt/zUeG2ORTPdH/0H0+Pf32sOTzNDUk58O5p9n9h0MPRHxk702l3B1puLcHX2exeEwu9MJkcpkays2+9NS0UFUrSySpRZ2tqWN7WCRuS1hwLkCflTkjmXbOYdnvbzbXW2jmDO5KYGR5MT5+Q6j73O95fbnmHkPmrZ9p5iil3G4tGjhjWOcFm1KeLxKowPMj9uOrzfeSPXPvpPbq2ntvfGCrts7tw1DnsHkVjFVj6+LWnkglSelq6aVClRQ5Ggqo0mpqmB46imnRJYnSRFYJryztb+3ktL2BZbdxRkcVHyPyIOQRkHINejHat23LY7+33TaL2S3v4jVJYzQiooQfJlYEhlNVZSVYEEjogfYXwVqDNUV3Wm6KaeneR3h29vMzw1NGjtJIYaLd2NpK16qCC6rFHXY6epfkzVrE6vcUbx7WRyM0mzXukcRFPU0+QkAJ4/wASsfVuskOWPvGTRRxW/NW0l2AANzZUGo+rQMVUE+fhuijyj6JtmejO0Nu1dZQ5fYG60mpllmmfF4dt0UccKLd5vvtoSbgjjRUuf3kha3JA9x7e8i8yWOoy7ZI0YFS0Q1j/AIxqb9oHU87f7o8mblBb3FvzDbqr0AE7+CxPoRMIxX7GPQWS0bmpekWWlkqqdxFLSU0xNfT6bq8c+OkK5GncAchowQb8W9hqayuYWVJYircKGoP+8mjD9nQ3t9wtZohLFJqiYag5oUNeBDiqH8j0xZiBwJQ0VSk2o3jLMpDaDrHiNmF+P9Ye0cikFqqa1zXo4sJFOijoY6cR6eWek/S0VbUVH3CrGqaNLghj6SvjYFQLsxNvp+fbAVydVBTozmuIIo/DJOonHD7R0KvWW68r1ZvHFb0gRYaTEyKm5aVWaOPIbTlngk3FFJpDFpcdQw/f06i2uqpI0uFd7irlLdrnl3frLcEJEQPhzjyaJyA9f9KO8f0lHUf8/wCxWXOfK+47FJ33Dr4tm9KslygPglf+ajExN/QkY8QKWofIntPHdJ/H/tzvPIjHVkfVWysxvHD4qvr0xdHubL4ukNZt7bByTxzikm3NlBBQwOscshqKhAkcjaY2yzZiASeFOueN5d/SxkpHqqhLZpSoK/8AHj1oY7q3VPvuvO8Hqs/le8uxeyd37w3nWRxUuIxLbi3nn4a3CRbVqqfISZAVuV3FlqqSqaeOFaT9hInf9xgk6B4qBj4v8vWwx8vd2VHxN+KPRH8vPpTLY3ePyG7b29iOpqan2tHDtzCUUW5qkYbsHsSaMzTGDcPYe6srPTR19TIhikqqyv8APqxzr7echV0A5/1fz6E8/ibZYQ7fDCBuFwACQO8g4NeJFTgfmere/iJ8U9pfGbonYfT+0aSGsotsY41u7N8ZynFHT7s3rkyK3dO56Db50SSQVmSkYUgrHc01BHT06nxwoo2ooAKY/wBXl0rg07dbJaPNqn8oYeNTxLv5E+g4dGkTM7bxzxyUcOR3HkFMsNKYYjVDUltbRQQKtHRUIFiAEjAt+fxfAp/gHV2s9zmBillitoMF6mlPkfxFvzPUqOny1Sksta0eGhnkklFPEUmqUV/U0YfVIkJ1HhFY293rilP29eD2kBSOANcSKKamwp+dMEj5nrPR4yhhbzQUihiSVmqgJJzc3aRvIT45C1zxz72PWn5danu7hx4bz4HFUwPsxxHT7AhRdagh0UFQQPGo+raQbWup5P596rSlfs6LpG1EL+GuT5nrilb5GeU6lXyMhjcFFbSdOpFHKofqL2v78pJqStDw680GlQgGaVrx6l+eL/af6fqX9VraP6Xt/sP8fftJ9f5dNaG4Z/Z5dLH210R9e9+691737r3Xvfuvdaln82+aJvnNupEjWWYdXdV8gxAMni3K0alm1ft+X6m3HPvGH3PP/IuvPUJHT/nGvXbD7kkbj7uuzMz6U/fG4+vrBX86dVsLE7v5DBFIQzKZFJ0jV+lYyrHS0bsAG4sn+PuPTSuR1lczhV0iRgKVof8AL8j6evV4P8l2Pxbk77s0k6jbewgkklzqYZXdVvFyC8aNcL/hz7m72b/3I3o8f04/8Ldc6vv9NrtvbSoCnxr2oHl2W3H0J6vuRmdfHJ6CbuxYA2P0sSSRqBP1559zz6Hz65xsADrTPkB10YAWsSbIQU1G4A+oGiwPqv8A7G3vX2Hr3imlQMnjT/P8uunhPpHHF/VoA1MP0lhz9Pxb3vj9nW1lGTnPlXrunptLl3UPK5sr2JVAOLqtyRqHHvVKVPn1WWWqhVwg4j1606f5gnYdP8h/ln2dvIhcjtjas0HVWyqinaNvNtrr6tylFLURTJJLFUU2Y3nk8tXwSJZXo6qG41A+8R+e94/fvMu4XCtqto2MEPmNKYqD6Mat/tuu7P3ZOV5fa72U5R2H+y3e8Vt63BHri4vUjcKQQCGitY4ImByHR806r+yWzoROyUYk0IFUoSRy2okeRj62VxYngKtvYKMS8M9ZM2m/SGINOy6zU1/2PLH7T0yVW2Z4ZFZA8dmclgzlo4wyrGFI06i0gup4uDxf234Xn5/5OjGHdo5FoSD6Vpknj/LpJv1ziZ6mRJNv4mVw33Lytj6V3dnYu8pYRFjMzOWY8m5559vCa5FAlxIKCmGNKenR2nNd/FEpXdJ1WmgASMBThSleHp04UvXmIpSKmPC45JodE0Ej46jVo5EcFJFPiNpkb1LaxuP8PdhJOQQZnyOBJofXpLNzTuE1YW3KXw27WHiPkHiOPA8D0IlBh6amg/eVJJWKs8kpuxVm/dZn/JfUbBefz7oEVR/S416C1zfzSyfp1CcAF/lj5fPqZJRwJLIIqbXokC3UW9Efr0HUbJpvbUTcj6+7KM9MR3DvGheWlR/hxX5/Z1dj/I874G0e9eweisxPLR4fuXBtuHbVLNJBHQR9k9e09TU19Dj4gweXKbn2DU1VROwuDBtuPgWv7l72i3j6fdLvZ5DSKdNSf6dKn7AChavzAHXPb+8P9t/3z7f8q+5FjGJL7Y5/ort1DFzY3hHhu54CO3vFCrw7rs8etpn3kN1x460X/wCY4kyfPL5UzRxFwOzKFvULoW/uHsxNBU/qRh9bXPH+HvEHnqv9bN7IP+jsKfn19Ff3VDGfu3ezMbvSu0v9v+5l0a/b0Sqqycuqf/NqjxpIF1aXuliVVj6tJUc/6r6c+weWJx1kBDaIFjrUsDT9v+X/AAdbKf8Awn8qDU7U+TchJNs31QvJuVtQ9gtpv/gG/wBt7n72V/3F5gqc64f8EnXI/wDvMIxFzR7VoB/xBvT/ANVbfrYRybQwUslXKGvTaZUZASwkU6UOkEBv12P+0k+5muwiRPMfjUVB+fl1zMttTSrEDhsEfLpqps5TxtFHZTSTKZYp1kRRToX8ckUkbWYrTynlvwjA/Qe0UG4Rp4aP/ZN8LVGK+R+QPn6dKpbN31la+KuCtDn5jjkjy9eqbf5if8yPa+39sbn6C+PWe/vNvvcNNWbZ332Ptqq8mC66xNdTvBl8Xt3O0r+PL9gVtLK0CPRO0OH1SSyTJVxJD7jD3A9wrWG0udk2K4El3IDHNOhqqKcMqNwZyMEjC1wdXw56/da+6lvG57vtHuX7n7b9Jy5aut3tu1Xa0mvpEIaKSeFhWKyRgGIkAaeiqqGJi/WuDIDHppqejkptYiiSBUAQRRkKqoCoGkBPqLH8e8edIrx66rpRqzSzh6VYsTmp9f29Sp6GpnNOtPSSiaWSSnRSPRrVwFDFuFdgDp5tc/X3Wh8hk8OmIriKMTNLMpjADE+dPl69bZ/8rnoyfpv4wYTK5igjot0dr13+kHJqYWiq4cLW0dPS7Qo6pWsVY4KBa3TpBRq9lPIPvKv2y2Vto5ahlmSlzdN47eoUgCMGv9HP+264k/e79xIuf/eHdYrC4Mmz7Qg2u3IIKl42Y3DqRUEGdmUGuVRT00fzbQT8O8wFF2/0kdZEcX5G5If7Njq/1vaP3c/5VFsf8SY/8DdG/wByWn+vrY14fuq//wCrB61hBUPA8vnpI9CI7rKAAFHABZhYiQ6jYEG9v8PeLlM94+fXXxohIi6J2qSAR/hA+XDoRNrTQSZXBhI3H+W0l7FHHqkSRZLcelh+bWPPtbt4H1toR/vxeP2joE81RyLsW/6nH+4svy/AwI63a/ecvXAHqlL+bdHDJub46CYKwXB9zOFYgKdNZ1SPUf1AXI+n/FPcB+9QBueWyf4Lj/DD10B+5I0ibR7pFDQ/UbWMf6XceqlaLxvGhuTGwQiRwxhRFJtFEOWCu4tqP0HPuEaA06zZuC6ucdwqKDifmfs6Ol8IUA+UXSISMLo3NuwSsA4vbqPsnSFf6TqCxNz9PY89tABzftOO4tIT/wA4ZOsdvvHN/wAwi5y1NWsVvQY/5TrX9h62RfeV3XK7qLVTCNLXA4LNf8IOOP8AEsQPaG9mKKI14kVJ9AP85x0/Cmpq0+Q+3qEsRE0dmbyMVlnsbqj/AI/xJCNa309po1IkVQx1jub0B/z+XTxbsY07eC/MdO/s2AoAOkXXve+vdEB+T3yiz+w944TZvWlZR/xLbFZBmt71FVTU1djq4vSu1JsapV1aojino6kVddNTtDUwXphFLqMyCJeeOeLvatytdt2SRfGhYSXLEAqcYhNc0IOpiKEdtDXUOsmvZ/2d2zmTYdx37m2CT6W8ja325UZkdKN3Xa07SQy6I1YMjfqFlpoPQ49L/JzrvuKGlxsNZFtjfLU0ctXsvL1UYq5XKMZJdu5Bkp6bctADGxDQqtTHGA08EBYL7FHLXO+z8xpHEsgg3MjutpCKk/8AC2wJB9lGpllHUdc/+0PNPIkk908BvOXQ5VNwgU6QPIToCzQPkYYlCahHcCvQu5PHSLnsfXQFVDs3nj1ePyhI2UkH6O66gbH6j2NBWn2dAS1ulO23Vu4qR8J40qR/LpOZXbG1s7mnx25tv4LcVBXxpMKHPYqgy1ItYA1pUp8hT1ESSMykagt/V9faa4tLW7QpdW0csf8ADIoYfsYHpbbbjudntyXO3Xs1vcRNQSQOyNp/0ykH/iuiCfMH4+dabD2VBvfZgfbOU/j+KxrbUhrZqvG5tMtUNBK2GpchNPJhq7FRN920dPJHRPRU86+AymOWOHPcblPZNv2obtYxCCYSpH4SntfUSO0HgyjuNKAqGqK0IyY9hvcvm/f+Yn5d3yQ3m3m2km+rkXvhMa1HiOoHiJIaRjVVg7IQ4XUrENp1hpYWkkdVLt43Jva5IWMqt73F7XFhfke4aACrqZhXrJyZnnkCqKjiP8vUncOhdvZtmaIRjAZfXG+hzLCMTVguymxlI54/p7UOAyNRhlTj1Gk9JLUsbu3VQS/jJQ8KHWuPl0yfzsu56aDpToT4mYDIUeJ3R2hPt3tLdn8RzEGHw/8Ao76/wNbVY6nzeWyEsFHFLnN/CD7JHZxJLh3UWk8QbL6JmFrbo4PiaFrX7B/l65kb1pN5cpHMGrPLg40gOf2VwR1UP8LG6m3jvrqPIdp7awm0elvidjt4fIfv/smjo2pstvjI4rMxydR7Z3NNUSSpWZZN21VDj8TRUBWpz0IelFJJNGri6gE54Dj0X22kvG3hgLF+o7NwND21HrXAAyeFOreP5ZHSO9PlN3jvj+Zl2xsuRKncudz+3fjXtHJVUS7R2Ps7GxTbUbccK+LVk5sHQx1ODoRGkaT1jZfJywvJXU06bGSTp+z06MrdoriSXdd0vmWVj2ImXYUp/tQOA4edOtgmq2jPUUq1O5cjLl5IX8rUlGz43GU6aGDLHBHJ5qhLmx1vyPx+Pbor5npVBu6RzGLbbcQqw0h373J+ZOAfy/PqbSmlgip4aGlpqSmiVRHFRwrFE1zrYsoAVgxFyfz7cAzWuPXpuVZHaVp5XaVjkuakY8vTrg8yylrMrXLHVpCxKSxJ0ALpUL+bc/197HyOOrLH4YXFMcPM/tz1AFUHYhRqRb2kXkEj8AEljYm/A597B9M9KzDpUaj3HyPWZp9K3e4BsxsQFuT6A1jzdubfj3utOPTYjqx08euIkDKRyWJJFgRzb9ZJN7g/7Dn377OtlCpB4Dzr/g668c30uf1afoP1Wvr+v6re/Y9f+K63qi/hHD1/l9nQl+2Ogn1737r3XvfuvdR5vI9kTSIyw8rk/wBj+0gH5LfT/W/x97x04mgVZjnyHz609/5weXo4P5gm9MdI6U8tL0x1HURsAIgVnG7QkZItdUeO+nn6+8XPdAj+t18SchEH7Ioz/l67o/cYsJ5fuxcv3SqWSTf9zRhxpp+mqfzB49V0R5sBKSjEhhMshkM+pCheSMSXYrdZOB6VIA1W59x6WNFHr1lK+2ktPPp1ACgXNaA0+0fMjoauqPkx3H0ZNlK7prsHMbJrdwJSUudlosfg8jFUUmOlqXpkqqHPYvMYupkheqlaOQQ64fI2krqa5xtPMO8bG0r7VfNCXpr00NaVpUEEYqeo9509oOQ/cQWac+crwbhFahmthJJNGQ0gXVpaGSJwDoAIJoaCoNOhzh/mOfOCoUSD5DZpFk1H/j0OqdWpHvqMY2IWtpNgbkG5Ps8HuFzkaf7vH/3mP/oDqPpPurfd6iOg+19sSMf7k7j5j1+s6mxfzGPnCUaZvkJnEb6+AbN6rLOw/T4S+xQL6RY3t+ffv9cHnE/8tuTPlpj/AOgOkz/dY+7zVYx7X2xHDV9VuH86XnWem/mMfOCpq9c3fefSlpZkqqiAbN6tLzRIPIlPK42L+xT1DoAzfq0t6Tfn25H7gc4vIoO9yFaivbH6/wCk6Yuvus/d5t7WTwvba1NwyMqN9TuFAf4gPrO5l9OFRnrY0+Z/e8nQ/wAWOxO0Keoipd0Vu3qPbGxKbyqqrvbfDQ4LA1SlnikqUwdRXtkJUUhjTUUhH0t7yE5x3s7NyzfX4fTcPGI4aYOuQUBB9VFW/wBr1yv9gPbpPcr3h5T5RliLbQly17uT0/4iWgM0y8CFMoQRAnGuRR1p40FfFS4+GkighRYqVaejpmYmaeCNbBRN+kyMFLO/B4Atx7xG1VqT13VubZ5rqSd5GJL6pHHAE/L0zQD8+ml54JA8RBZZonMCy+VYyxb0xadNyVcG/Nyf8PdcVNOPSxYpUo9aFW79NCft/P8AZ0qqHrvfOQo6avodibsyeLyVEr01fSbey9XTVMfkIhnpJ4qKWOWAPGfUrEAg/wBOFK2V26K6WkjRkdpAY1H206D91zpynZ3E1pd827dBfwykPFJcwoymncrqXBDUPA56wy9WdkS+GaHrrf0JDLcx7VzazJEG9TFTQ+t20/RRzfkW592O33vAWUv+8n/N1dOfuSF8WN+ddoavrdwEE/8AOTAHz65R9VdjqXEfXu+Wh+rpPtHOqkwkcFlkAoS3mCj9Y9IHHv37vvTn6SX/AHlv83Wn9wOSW0l+c9pD+RW8tyRQeX6nD5ceuOa2HuPb1BDPnNsbgwtBUziCnqsxh8njIVqNBnlp6eetpokZxCpsAS1ube25bS4gUNLA6ITSrAgfZnpzbebNj3m7ki2rfrK6u0TW8dtPFK2mukMyozGlTxOK46T6U8UaSnUvjnVppmgIURqWZUikFhZvQVJsB/j7YpjB/Po4aV3ZKg1U6VDeeOI6XvUe/wDM9LdjbD7X2vqkzfXG5sLuzG0lPOscmRgxNalRXbfklJW1PuXHmox1Qb3NNVuCSCfZhtV/Lte4WW4W5/VikV1H2GtD8jwPyPQX575XsfcLlPmXkrdyBY7raSWcjsDSNnWkc1BxMEgSVR/Eg63wdm7u2/v/AGhtbfW08hDltr7z27hd1bcylOyvBkcHuDHU2VxVbEyMylKmhq0cWJ+vvMy1uYry2t7uBqwyosiH5MKj86Hr5xd82bcuXN63fl/ebVoN3sbmWzuoXwUlhdo5EPzV1I60pf5iyRv86PlCZVikA7Cpo25RWgRtj7ReKZiWChVk5NwWIHvEvnkf8ivez/w9uvoD+6yzr93T2eCEiu1sR86XdyCPXI6ILW4aonSaSFkqIo0UhoLMD4iylwSdRJ1HUPwOb+weYyc1BHl1krBfxxNGkgKOTwbHHNOhi6V+VfyV+NdNnYuiuz831lS7rONnz8WNxG1M1DlP4UKqnoJZKbdmA3BSxy0/3kwR440kAcjVp9m20cxb3sAmG03rwrL8aihrTgcg5FT0Aef/AGW9ovde62+49xuT7fd7qzV47ZpZbmIxhyGZa200BIJANCSPTo0WG/mmfO+f9rK/I3P11I7r5Hm2T1TCyILAgpDsGPyMj2a4tz/gPZ2ef+bpFZJd4cr6FUz/AMZ6iLcPucfdvQF7L2qto5gDQLd7ic/abw0qMdSNy/KLvHtTHLjuxu4t/wC6sZWJLR12Cm3A2M25koJHOpanbu2UwuByEjatX+UwSDTwDx7KLvfd5v0KXm4zSQnihY6fX4RRf5dJ9o9nfbrky7N1yryHtlldxkSR3Kw+JPGR5rPOZZkGKdrDOek3S09NXxND44I4QU8SJThFhRSFWNEXToC6fwCLcAD2XAavs6N5pZbaQPqYyZ1EtWpNcknj07yYqmrZUdBBHErvKpkQFUkjHqbkKxSQXK3J0n8e9FKnHDpCt7LboVbUZKAEA8Qf8o/n69Hy+DXwtrO99+0W5d14iWPqHa2TirNwNLGYqbduVhMdXBs/Hzn/AD0VVqWTKSRXFLQkoSk9TT3kDkPkyXfr+O8u4j+6Ymq9f9EYZEY/5+PkuOJHWM33jvvAQ+3nLtxsOxXwPPF7CY4dBq1rEwKm4cD4XAxCDQs/flUYHaApqeKkp4KWCOOKGnijhiiiRYoo441CJHFEgWOKJFACooCqoAAAAHvKFVCKqqKKBQAdciZHaR3kcksxqSckk+p8z8/Pqs/+bhPLT/DvKSwxJMw7M6vVkkJVdEm5oUdtS8gorav9hb3GXu5X+qJp/wApMf8Az91lv9yONJffWzSRyo/dG4Go9RASP29atWaycYnhqWgaR4WmpqzxhlgDxx2Soij1hVmkduSQfQbC3194utUkUXPDrsXt9oxSSESUDAOleNCeBPoAP29OOx91TjcuAoxSygVeVxcJlYMrAtVwRFlTm0SI9gPoAL+1Ngx+ttBQ/wBov/Hh0Uc5bNH/AFZ5hn8deyznIUf803NPtqP29b3fvOjr50eqQv5viOd0/GuRJShTE9xLpA/zgfJdQ3BP0ACqfcB+9QP1HLZH8Fx/hh66FfccYDZ/dhSlQZ9sP2Uj3LqsTFT0kMCUzQhyyzSOTpANm9MZLEK4+hsOfcMLpU0IFCP+K6y+u0mkdpVkoAQAP8vy6EbZW+8vsvcOK3LtPI1OD3Hg5ZavEZalMazUNY+OrcVJNSx1CPSzJPjclUQyI6yRyxzMkisrEe1u3bld7ZdRXlhOYrpKlXWlQaFfOoNQSM9BPmPlfbuZNsudq360W52uaglhetGAdXAJUhhR0UihBBAII6MtT/M75ISr/wAzYzcutiCy4DZWuMkABvGm2AFQG5F/zx7FP9f+bsf7vJKnj2Rf9a+opl9hPahDjkq3FBWhmuqH8/qOnqm+X/f1U7NVdp5MxojiZHwmznS0bjTYjbqGTVJYaeefdDzxzVKay7y5pggpHn/jHr0Xy+xntnEoEPJsOokUIlugcj/muaY8+nrH/LrvmqVyOycxDPclkkwe1FYsxCxBl/u8XWwH59uxc880AjTu7g8T2x/l+DyHSC59j/baEj/kJQNHwqJbj8/9H6UGM+Z/ZO3dx7Trd9dzUeG21/efayZaTdkmysDha3FVO4sXS5uCtr5cNST01LDh6maSR4m8iImoEWv7Ptj5v5uvt0sYv3hPNCJovFURoRpMihtWmOoXSTUjhToEc4+13tfsvLe9XL7JZ2t4bS4+mkeeZWEqwO0ZjEk+l3MgUAGoJNCM9G97E/mUfFGk27l8f1N8gOoOwuyqqrbbm1tvYPeWJyyS5+oRtFZK1JUtBW47HwhpwIpNNY6LTxuHkBE1c07xcbLst3eWVs0t4FpGFUsFJ/G9BhEGTWlSNNQT1iR7c8s7dzbzbtm0btuUdttZfVOzOiO4X/QYdRGqWU0VaV0gl6ELQ1g1dVW18tTW5Kqqq7J11ZV1dbkKuV3qq/I1tQ9ZW11ZI3+eqqqomeR2+juxPvFGSSSZnlncvMzFmZjUliakk+ZJNT10pght7ZIoLSJI7OONUjiQAKiIAqIg8lVQAB5AdYjSLIwjbSrLolXUy60mjOuJ006SsiNazjlTyDf3Uiv28fs/1evVxPpXWMjKmnDScEfYR5efQybT+QfeOzEp6HHdhZyuoKOoM1PRbnei3TAojUhqeGrzlPX5enpwrFUjjqY1AFlAFvYo27nLmna6RW+7yNEOCTUlH2VcMwHyBHQC3v2v9ueYGluLrle2juXXS8lmHtzk/EVhZI2bzJKE+vWDdH8zSTac8Kb47X6Ww+RgrvHFAlG8+bhqGdyaeahodz1syRQlb3kp9K/n2O9v5q9x9yiLW+3Iy0rqFuwqPUMXCnqH945J9iuXGkt7zmCSMv8AptC97E2aeaJAZFPqaj7R0gqnvKH5DQDd0/aVL2VFS1LQQy42ux74zBPLKzNTLiMPFRUmJrZIlAkaWBKqSNEDswVfYG5kn5huLlP6yzTeOv8AZrINCqDx0KoCZ8yBU0AJx1LHIsfJdpt7LyBDZjbzQSvbOZHZgOEruzy1BqQjEAEkqor0nPv6Soq49JeVKVZzPDqEZLqClKUbTp0Owvf6/T2FC6FhgmnEf4P29SMLWaKFuCs+nSeP+mr9nUbpvbm5O2u5dq7IrYzmdq1Nc+V3XLRLWRybc21i6iCfJQzQwU0xyU1fjdGOiJsoqq6LUOT7MuTNqvuYOZrCwZfEs1bxp3GPDRCDQ47tWF+1uk/ubvGz8k+3e971BJ9PvTR/TWYfSfHmlBUMpJHhhDWX/SxkDy6qA/mW9yYjtr5id0qJ9wZ3A9b7ixfUmwJqvIQ0NPtPbmw4cnT772tR4lMZIKxantLJZSeKtkqGOiIqgeF4fFl7Ie81GRjrlZfTC4uppahiaDWvA0UAkY/ERWvSV+APxC3v81O8aPqXG1W4sP09RzYPdPyD3NjKiqosXjdk4itnqsRh5pgwx1RvfdVck1LgI5BPPRs9VkY4nio5z7qBU9JQGaqqCRitK/l/sdb423cRt/rvb+F2btHF4vD7T23icXt/a23MRFDQ4vAYDC0cGOx2IxtLAgipqPH4+mWONB9Ao/x9qQuBTowjthcIlEKFRQmnH0651cs+SGqdnSMLJ+0hdIniZi8Ynj1lJJUH5Fv9497Cj1z6dGEEcdrTwwC9Rk0JBHGhpgdQ9QCFQGAA/tEX1fUiycWUH+vu9K8enypJBJFfl/s9QZ1lkVozZYwB6Izpvex9ZHGgkXNvr70QaHyHy6VRGNSHHxHzP+T59NZmMbqCw8SktYEgB1P6j6bv6vp+B7rUDif9X+XpUEDDA7uH5f5OsySK2plk/wA4A1iC4Xk6VSMHgH6sfofewa/n1VlYUBXhxp/l6kI88j6lJYRhUCAWZyDwQ97Ai/0/3r3vuz00RGq0OCc16cfHPa2qO/g+uqT/AD3k1/W9/wBPpv8AX8e90b5dJNcVa6TTVWlB8NKf7PQk+2egr1737r3XRvbj/Y/1t/h/j7917qHJ5lQajHckJb1eNSzcNYXeRgLWHAv+fexTp5dFaAGnHyrw4fLrSm/nbQTf8OI71CSM0h6Z6ZZ3IKt6hvU2CobBV94pe64J5tvCP6H/AFZi6+gP+75kT/gWuXyyUX+sG6gD/sk6q+ooMnFR0eQikqVZpZqb91vIWAsBEsZuGc6r/wBbe44RX0K4Y14dZf3Elo9xNauiHtDYx+dfTHTzQ53c0LBrh0RHkkjeD9sAa4vNLxdGA4AW30F/bgeXHA4z0X3O27TICNJBJABBz5Gg6dqet3HNHTEFxGXlidY4bGSyXuSguilG+oNyR7vWUUJPnQ9I5LfakeaoGqgIJPD9vHPT2MtuSlpqZAyzUazLpjqKZ/LLJ4mcvO6qZJGMa2vwq/0v7cBkUDOPTovNjtM0sraSs5XirCgFRwHAZ/b0rsBmBUTVU7rJC9VGUlp5JGCqjICiskinXqlBItYKth7ftz+opGDX9nQd3qwMVqIgQyoCVcAVNAa5BxQftPV2P85nthMhvjqT46Y+aSWg2Lsyl7Z3jGyyywNuPc8WU2psegYl7DJ4TCY7MzSxctHHk6dzbUvuYfdjdjNNtOyo/ZFGJpRX8bCigjiCq5Hyf7euf33BuSmtOWecvdO6jC3O43x2SwIoG8C38O5u34f2csrwKD5mGRfI9UmzRwRxSeNXjiSk8C8zNNGVKtqRm5QFnuP7TfpB9w3WlSPs66DRvKzrqYFy+vyofLNPs+wcelb1tsXM9kbv2fsnbkVTX7i3duDAYDGwKkhH8UzuTpsbSMyhS/giaW72sVVSbj2qsrOW+vLazt1JnkkWNR82IA6IeceZ7DlDl/mDmTdWSPbLC1mupDUVKQxs5UHhqagA9SQOt9DrzZOJ652Fsvr/AAaePD7K2vgtrY0KdGqjwWMpsbBKwSy+SZKYO39WYn3mdYWUW32NnYwikUMaxrT0UAV/OnXzccxb7fczb/vfMW5Satwv7uW8mY5q8zs7fzbpY6R/Vv8Akt/+jvaug+fRNU9e0j+rf8lv/wBHe/UHz69U9Ei/mK9Gyd+fEPtvauLo3rN37aw3+knYawxLPXPuvYRbPQ4vHiS4So3ViKaswxYciLIvaxsQEOetoG8cs7jCqVniX6iLiTqjyQPmyalHzPWQf3WvcNPbb3x5I3q9nCbHdXH7q3EsaILe8/RMj0/DbyMk/wBsQrjrSZp66rYxVEcimCZItMtQA6mEjypPKqtaczq/pKjm9/eJZ1AgefX0Ey20ADxOv6ik4THdwKj0pTpym8yxsjReCUmIQ+PWrELJfi49SNe5JtpPvxOP59I4/DLBg+pMltVDTH8iP5jra2/kyd5T9ifGfJdT56ujqd1dEbnqcNAhnWWon673jPX7k2PWMlwYKTH1hyuFpowAqU2GjtwQBkt7V7x9fsDbfI1Z7R9I/wBI9WX9h1D5ADri59/H27TlT3dg5x263K7NzJaLdE0oBe24WC7Wvm7gRXDn+K4Pp1r/AH8xGh8nzk+VTSRiell7Kx8sqycKjJsfZqBiV9TxBU5sVKke4T54WvNe+A/D47V66cfdcuNH3d/ZkK+mYbS6inmDd3X5A/tr0Rpdv5mE1DUEqR0/1eCoDuteTIGXwsAUWJ1PqPBB5/HsH+E4PY3+r06yJO6bfJ4QuUJl8mWlUx5+ZI8h06RYmavEcVRSmKsWJmRKZS9PBAHuzSVCL4mplYWFvWy8+7aC2nUufTpG98lrqkinrAWyXwxNOAByG/l5dOtPtySJEiSj8s8VPGpEmrwSxRElpvIg1FZAxIIBJ0/6/u/h0P8Aq/1U6RS7srMzNPSIsTj4gT5UOKin8+lbiKavhhDqqmlW0iGWGQGZS2ggQqty39oKOVHJ9+0tkgfl0SX81vJIQT+scGhGPz/lXz8uh/682n2DvrI0+L2ZtvcO78tUkRDGbcxVbmpY5IkMjGT+H085ggWnUuWlEaJa7MBz7X2lheXjCO1t3kf0UE/M8Oos5u5l5Q5WtpLrmLerSwtlGrXcyLGWBNO1WOpzqx2gk+Q6uW+NH8sDeGflxG5+/MjDg8CuiqTZG28tTV+cysRUSQpmtw0IqsNtun1+mVKGTIVzjgNSMBKJX5Z9sJ7nwbze5Qtse4QxMCzempxVVHyGpv8AS8esCfdv74W02iXuz+2Vm8t8aodyvIykcfEEwwNSSYkZDSiNB5pIDTq9LaGz9vbGwGL2ztfE4/C4TD0cdDjcZjKVKOgoqWNmk8FLTIW8aNNI0jszPLLK7SSu8jM5nWzs7ext4ra2iVIUXSqqKAD0A/1EnJJOeueG77vuO+7jd7ru15LcbhPIZJppmLu7HizMck+XoBQAAADpTe1XRZ1Wz/Nd0f7KHmfIFZf9IPXVw6GRT/ufT6qP97+g+p9xn7s55TI/5eY/+fussfuXav8AXwstJIP7rvuBp/oPWsBUY2Ouk8tRGwEQWR4jGvgIglCrJMoHkYqTc2H0seQfeL5XNfLrr5HdtbrojbLYBBNcjIHl0APbPbNXszP47BbTqlxuTp/tMll89T0sVRXYajaXyU0OKp6opT/xWbxtMjyErHEIyPVICkze2/I1pulu/MO8RF7cOUtYqlQ7L8TuRRtCt2gAipB8hnAL72X3jd+5V3GP2t5Gv1g3JoBNvV6FWSSGOYUS2hVwYxK8Xe7ENpUoooWJF9H8qn56fMPfXyJX4vfIqg3L2ZtvcnWtV2tszsXPbYxuK3ts7aM2Px2Y2hnN35HbSLgsxsbfeLyEcVHVVHkr48rPFCaidXKQ5AxE6VDDNBjJ8vU5I+ZqT59c0GNZHo1VqSCQFJFcEhaKCR5AADNMdGA/m/1ENLnPjxUz2WKDB9ySPK00UMcapW9UMzSGRlGlVBYm9lC88e4N95UaS65aSNSXKzhQMkktAAABxJPXQH7kksUGy+7E886RW6S7a8kkh0qqrHuTMzMcKqgEknAHVGey+/uv9+5ur25hcg/8SoZamKkWtgNFT5mliJ1ZLByFyuTp6V1IYghyh8mnx+v2AN75H5i2Lbrbcr+zH07gayjajETwSUD4W/aK4rXHU98ie+3tp7h8ybtyxy3vUn71hdjALhDGt4sfxyWbMf1UxWh0vp79OnI98gN/5nYOyKaTa0rjde5cvjds7fFjK9NXZx2iGQhp5VCEwQpIYQ3o8pUvdVYF3kLl+13zfB+8T/ustoXupxwBVBhSfIEnPyBAyeiX7wvuBu3IXILNy4g/rPul7FtNg6gFkeUnVIoyGdEFBXAZlY4FOkf8at49n4XsPenU/Ymdfc8+2sPic5S5WorJclWRfxExRrTpkTDDNkaWaGqikUTx+SF0db6So9ibnyw5eudl2Xmrl+1+njuZngaMLoB0g50CoVgQRg0YEHj1E/sPvPuPtvPHO3tF7h7v+8LnbLOK+juHk8Z0LlAUE5Cs8bo4NGGpHBGAej5QZETRSRBJRMxgVpBDIodww1rp0EQyENqNuQOf8PcV1DBlANf8vn9nWT8lrodZCQUGo0qMYx55Hl0EPevyMouitpzVcVM2Y3vuLz0e0MRUOvjq6ilTXVZbKFSsybexxljMrApJO7JFGVLl4xtyXypPzPuBDsybZEQ08x9CcIo83by8gKk8KGCvev3M232z2K3kjjjuOY7oOthZZpUDM0tOEUWKitWYhBxJFP279xZ/c24cjvfsLLz9jVdsfPNlmknfCUjZdJJGxWMop4ov4S9FCksFLHRQGOGrhF/IB6sjNvtbSxtYNv2y3FpGNVIxTWQn4mYV1VwWLGpU+Xlzr37ct03ncrvfuZb47pcHQWnaphUy1Phoh0+HoyqLGNIdc6hxvW6t/kVZ3NfFvfXandXYu4tndm5XrfI9g9YdPYRKWmwuxc5SYGtzuBo+3svlcfVV2dzs8IgpK6DG0+LbEP5tFRVOAUOQpUaq91OI/n+R9Og4yLIChB0E4B8vQ146h64NeFOhP+FGz+4e3fhz1R3tlsLX7noMlBuXBHO45Js1lZaHZudqdtQZzcGFpaUZgNVfYyRvU0sdeplo5pqp6dSjSQRzhyJewX93uW02mvbXbWEj7ilVBbsA1BQxIGkNSmQoAJzP9qfeTar/AJf2rYeZN18Pf4k8JpbghFmCsyxnxSdBkKKpbWUrUaS7FgomtjY5IZKlZYpaOOOVjUUk8dRGjRsyOTNEZEjSMglg7Bgfr7jM2zgsCnAZA/1Y6yCTcEAQhqMaHuwCOPnSuPMY6pM+U/ysyHZuV3FsHqrcbbb6821TVi5PNU1VXwZntLIUcopq2gwdVjkeelwEKs5RQ0X3yRySySCPQjTlydyRbbNFa7lutp4u5ykaEahW3ByGYNgv+3SSABWp6w191/eHcubLjc+XuWd1+m5ctwwlmQssl6ymjJGyAssIzQVXWASTpoOi6dNdC7l7t3ueudqY2DbVVg6Rc1u7dmWi8yYTGT+FnbJQUD6Mvmq6pmC4uBZonaIN5SFSSRRdvfMFtsdidzu5DKjkpDChpqIr8JPwqAO40OeGSB1F/J/I1/znvQ5d2q3W1liXxbu6lFRGjUy4U98jMf0xUGldRoC3R1aDqyr+IXyn6Kxmx87nN1YHuqgrNs7wo820bVOTq6IwRVmRqKbHwwII6GqrYaqjJEklNpliMjq5uBJt0TnXk/f5r+zjjnsiJrfw64BrRc1yQCDTjg0BHU0WvLUvtF7qcjWeybpPPZbwhtb7xitWKkBnIWgopYOlale5dRB6t52h1dvbsvKVG3tl4qeurvIEycnkho6LFwAh/wDc9mHAoMJTuW1ATOKiYDTBDNJaMxJtfLu6b5Obfb7cnPcxNFUf02OF/wAJ8gTjrKXmDnrlrk61j3Dfb1VTTWKNau7n/hUdQ0hxxACD8bqM9Wb7P682R8H+gu2e4M6RlcxtXYO5ewN75tIhT1GSg2jga/MU23MHDVlJaXGRvA0dLFKRNWVk5mmCM0UFPkVyfyjZ8rWTrH330tGnmIyxHBQDkItTQcSSWOTQYK+6vunu3uVusMlxWLZbUMtnaA1CBqapHIw00lBqYYVQEXtFW0GqivyeRZazdclbLkMlNX56rlMAjqp67ccsuarch5KiNJKuDJZKr8iyO73jJK/UexX1Ew4dXpfAL5P9rYX47Yf4x/C7Z20dib3xVbu3t/5hfMHvCCipuoeosBmMlkYcRloIzk4IMjmKXZ+Ix9HSNk5AkrYmo8dDNRpVV1A4pIWij8+n4XlB0RU/iJPAfM9Sv5Z3yd+Wvafz9wXX4+RXaHyB6QwWL7VO68pu6k+1wWX68xlHX021OwZMDW0rZDa1bnt7viWxqzzNkI6esNNITGJlXaFtYpU9KLSad7hUWYlM1rwp6n/J1tayO6fqawUXIDAer6KtzcBR+fz7U8KVPRsqqagDz8x/qr01iU3GpTo9QCoCWLEhtTN9CNX+wH1PvQJpXy9OlugUOls+p/ydQqitjilggeSnikmabwUwkTXUmJdcgVSwMpjU3a3AHPA96Plw+zp1FHrk+Z/ydNU87M6sQR+FMhuramN2+g+h+n4v7qWOP8PS2OMBWFR60HWKjq0V20D86IjpJ+pP5sSrEAk/gX96UgEnpyeFiq6uNKt0oaCRyG9QXUdasfyTf6s3FlA/s+3F4dFlwi/w1AxQdOOkX/X/AGb3sb2tfyf8Ftxp+tve6fPpNXHw+dP9j7fn0JHtnoKde9+6914i/B9+691waNXZHbkxm6c2sxBBPH14/rx791YMQCB58eixdp/C34r92byqOwu0+jdibz3tWY3H4et3PlMfOmXrsbiRMuLpa6qoaqkatTHx1DpCZdbRo2lSF49h7cOVOXt1umvdw2qKW6IALmoJoKCtCASAAK8aADyHUr8pe+3vFyJsUPLPKHuNuu38vxyvPHZ28xESPLQyMiGoUuVBalKkVOekE38uH4RmOKBPjj16lPG2oR+HM6V4teJP4voRjaxNr29ov6ico0AGxw44Zb/oLoQD7z3v/qeRvdjeTIRSvjf4e3PWNf5cPwnLztL8dtgiJzpWJFzao8QsT5lGX9ZLD6fSw97/AKi8o0oNjh/41/0F1Y/ef9/AqBPdXd9YyWMorX5duOsh/l3/AAnp1j0fHjYsESXSNUbNxIvkJLEKmZHqdj/sfexyLykBpGxxU/23/QXTf/BL+/kmrV7p7uznJrICcfavl10f5ePwuD04Px12TM5JV5XGaLxIysut5P4x+QLWHNvezyLykan9yQ/tf/oLqw+8t78ESn/XW3VRxCiUUOeFNPWSH+XJ8JYEVF+O+xWK/wBuQZp3Y/W7k5ezg/kEWI4It71/UXlKtf3HFX5Fv+guqSfec9/ZSxb3U3ah8hKKfl29P/Y/wz+M3Ze8q7ee+un9nbn3ruFaf+K7krIq2lzGbnxuPpcbS1eZkxlXQxZGqpcdSRU8c0qs8cESRqQiqoWXfKfLu4XD3V9tccl01NUjVq1BSpoRmg6Qcse+XuzytsdpsPL3Pu5Wew2lRDaxSfpRCSRpGWJW1aA0jFyBgsSxFST0yQfy7vhgsCJN8fdjO+lDJ/xfApdbEXAzNiVb6H/Y+0f9RuU/+jJF+1v+gulsn3l/fcyMye6O7Bamn6o4f7z0rdm/CT4r9eblw28NkdMbU21ufb9ZHX4bM48ZRqrH1UZOmenSryNTTCYKzAOYyy6iVIaxD9ryfy3ZXEV3abVHHcowZHBaoI+0kdEu+++/u/zPtV7sfMPP+4Xm0XK6J7eZwUdag0agBIqAaVzQV6NT7EvUS9e9+691737r3XTKrqysoZWBVlYAqykWKsDcEEHke9EAggjHWwSpDKaEZBHRKx/Lo+ESaVh+OHXdNFEbU1NSUuUpKOjiDFo6WgoqbKQ0lBRUwOmGCFI4YIwEjVUUKAs3JHKjsztssRYkkmr8T/tup0b7zfv+5d5PdneXkY1d3m1MxPFnZgWZmOWYksxqSSST1mP8vH4Wkkn497HJIKk3ztyCbkX/AIz9Cfdf6jcp/wDRki/a/wD0F03/AMEr78/+FS3X/nIP+gehQ6k+LfQfQ+by24eoOtcDsHLZ7GRYfN1ODbIg5XHU9T95S01ZHWV1XE4paos8bBVdS7C9mIJjtnLmzbPM9xtlisMjLoYqWyKg0ySOI6CXOXuz7je4VlZbdztzdebnZ20rTW6XTBhG7KFZkwKFlAB9aD0HSU3p8IPif2HuzcG+d49GbHzW6911gyO5M1JS11JVZzIilp6E5DJLjq+jp6qvko6SKN5mQyyLGoZjpHtPd8o8t39xLd3e0xvcOasx1Cp8zQEDJ/nno62T3895uW9n2zYNk9x90t9mso/BtLdJapCmpn0RhgdKBnYhRgEmgz0mR/Lv+FgUIPj1scIAwCg53SAw0sAv8ZsNQ4PtN/UblP8A6MkX7X/6C6M/+CW9+alv9dPdtXr4g/6B65p/L0+GEenR8fdkJpQRrpbOrZF+iC2ZHpF/p79/UblP/oyRftf/AKC6qfvJ++7V1e6O6mpqayDj6/Dx6zL/AC/PhsgAToPZigWsFkzwA03C2tmRbTfj3v8AqPyp/wBGWL9r/wDQXVD9473zY1b3N3Qn5yD/AKB6fcN8H/iXgHWXGdA9aJKh1I9dtylzZVr31KM//FUVr83AB/x9uxcm8rwmseyQV+a6v+PV6Ldw9+febc0KX3uXvLxnBVbmWMU+yNk6XOD2htfr+CtoKbD47CbcnhbDViY2gpcbj6NFIfGVzUmPiho0gqYXEesxnRMguQCfZRbWkOzzXEMiBbZ6wE0oFrlDjHcuBXzHQa3Dddw35ormS6kmvwfHBkZnZj+ManJaqtnjkHpW7X3JAaqDBSyrVSTz5aGmrqePTTS1WKeJ6yB72McskFQkoUCwOtb8D2bbJuSmT93O2o1bw3AoDpy38jX+Xp0T7lt7CNr1BpUBCyE1ID1APzFQR+zoRPYn6Iuve/de6QvY3WWwu29sT7N7I2vi93baqKujr2xeVikeKOvx8vnoa+mmglgqqOtpJeUlhkjkUEgNYkFDuG2WG7W/0m42qzW+oNpf1HAilCCPl0IOWea+Y+Td0Te+Vt5nsd1EbRePbtpYo4o6HyZWHEEEH06Ldm/hX8Ott4XNbiyvTG2IMZhcVX5jLVBrNxtox2KopayrkcNnbOsVLTsbHiwt7If6jcpZ/wB0kX7W/wCgupD/AOCB96O0D3E3DHDuTH2dnWi3hdvVfyJ7Uz0WCqdkbRqt9T7n7Jx1Fk87Bh8di8NRUdbnP7h4STKS0eOrd14/bMC0+Px8tTD95JSLCk4dwWO7S0t7KG2tbVAlvFGIkUYFK1J/Mkn7T1Fu7b1ue/7lum97zdvcbpe3DXdxNKSzs7ALknJIUBf9r1tk/wAjr424Tqv4n0feNVFk6nfvyOnfO1OSzCyRTUfWG083uLDdVYfE0Mk0wxuHr8NLNnAgtI0mY0OSkMIRcgoOi0evr/qHRT/+FAXyJ6zpcF1z8ccRR4/Kd1VDneW5c7/DxJV7D6lzCVlDNt6PNkxmjyXZu4MLSs9JEZWOOxUj1CRLPSNKhutusLq7sb64tke8tmLwOwqVJHH9oBHzAP2n+3c1cybPsvMHLm1bzcW+ybskce428TlUnSNiUDqMNhnXP4XcDj1TJ/LH6IpvkR83elNiZWjNTtfb+QynZW9EQyRW2vsKgauNG7QvFJHBn8/UY/FTFHSRYK92UhlHt2eCK8guLS4QNBKuiQHzWoJB+0Cn51Geizbr672nc9t3bbp2iv7SUT28iGhSRQQjA+qlgR5GlDgnq9X+b18Y+rem9gfG3vjZHWlNQbL6w+TPX8vdMuN/i+QFH1zuKrjx02ayDVeSnkipaPKU8GPhAaOP7jLKCQzAgrteWdj26O+Sy29IkuYGt5tNTVWKmuT5aeHnU9C7e/c/nrmKfYZ995juLqXbL9NwtDIV7JFVlNAFA7tQJNCQVHz6A74Cda/HrvL+Yn88twYajwe9uqduYnA0XVWSwGTytPsipxe6Mi3200clLV0tRVzY+DaTwUXraA6KiQA/ssCvddp2iLaNv2ie3iNpG8nhK9QNbamU1BxoBK+mQTkDp3aueucYuad85vtN6uF368jiW5uUILlFVFcGoIbxGRWJpUEEDBPV5NJ8TvjRjcRXZ7NbCxNDhsVRVddW5Cs3Hummo6ejoYnqcjlKqobcSxxUtNBC5Z2IVVUsbD2X7PyZy/PEbifa0MRwlS3d6thvM8Pl0JNw96PcxJPDTm+518WxHj0X4PTrSZ+UnZnU3d3fMHY22M/kcd17uvLOgwdFtbJUr9Q9bU266zEbcwFDHmsrV1W8d21GzaGLcOWljkWjfK5M0kEjiJmAusNssNptjZ7bbJFblmchRxY4qcmtFAAz5fM9Rvv/ADNvvNm4pu/Me5y3d6sSQo0hrojXOlaAABnZnNBxNOAHVt/8oz4YbF+SfbeY+U+6euaDBdNdKVmF2f1NhIY8z/Be0e2dtJ5Mz2dlcbuTK5mqp4cHIlNXTY6Jv4cudrTTxkR46aCRWkFYWikkZwWqzHBK0AEZyarUVOe7gRpJXotFzS7W6itkj0IURBkB9RJmXC6ZKEqMHRhgfEAk6ta/msfLlupOo5PjL0+H3j8t/lTj5OsOpuusFIk+fxuJ3rLNtjMb9y2iopxt7Gw0s1VS4uqqJIklyYMy6qWgyMtMqbh9vSUtxUfF6fbw/LHRzvh70HR/F/4x9LdDUlRU1b9d7JoMdlampqYatptyZKaoz+65IJ6enpYTQHc2Wq/tVVBoptCksQWPgKADq2BgcOqy/wCd93R1/wBOdBUOz6HBbcpu5vkDVZLbWH3cmHpDubA7F2pDQ5rfGSgylNStkvLmFkodvwa5EjjbNNMWCwOCW3W1bXczRXVzt8L3SMrpIyKWBVgwzSpFRkVyOjuz5m5j22yuNt2/fbqHb5keKWBJXEZWRGRuwMF1UbBpg0Pl1qgdZYrF5qhGzNv7Wquwe3OwNx4rrvrnYMFLU0Yhym5YUx+3Nz4XcVNkaWnhzsOdlWh/h1VGaWWlqGqJXWOA3dlheaWKT6hkCsC4UA6xWpVq8AfXiPLj0W21xDa211ALGOWR0KRM7FfBbTRZE05LJU9pOlhx4Z3Jvjp/LB6a+MnSONwu4N+5mlzmPw0u5e2t9UVTtDAYHI5unppK3NZqas3FtbK1uP27gaSMxU71VYEgo4NbCPU49kW78o2W+3IudxuZ2cdqIhUKi1NFUFGPnkk1Y5xwA95V9y905K247dsW3WaxFvEmmmWRpJX0gM8jLKi0x2qFARe3OSSFfE/q7YXzr/mC7o732hhs/uD4ffFLEVmwuut6Z2ojkxvb3a9VBQrlHnx9fi6Ra3b8lFlKnIyxUkNMqQU+KM6ha2SD2/t/K+0bfYXW2xQ+JazSK8okOvUEA0oQwA+LJoKeVMkkv3n3F5m37fdv5imu/Bv7OCSC1a3HhmNpSdciFSTXQQqksWHxVBAC7HeF25gtu0NLjMHicdicfRJoo6HG0VLj6GlFiCaWhooaejpmcH1GONS35v7PYLa3to0ighVI1+FVAAH2AAAfkOgpeX95fzy3N7dSS3DmrySMzM3+mZiWb8yetZn+dv8AL/dO9srmfit1VQUuY6y6XynWW7/lFuJ3ebC1u9txZyPIdT9OZaWOppYBjBUY5ctk4A7S1U6QRrJTmhqxJdj5DpEcmn7f8nWuHl80MzujPZzIYTCwR19flql9t7ZSTEbbxK1L1RpsdtuGllrTi9vYCZ0+1gWV0EEKxl2ViS31boaR8i5R8Vsp8XpdoYTFbY/vnjezf7y4nL53FZfdO/ocxaszfZdEstRgt647HbSipcXhsfULSUWJ+0WrVamtEUkOwSBTrVMEHhx/4vq2T+U5/MD6O6KzewPjVUdBy7Iqu58zt7Cbk+QcW65Ny5zf3bGerThtnz7q2/Ubcx0+A2BVy5KLFYiKhraqkw8kvmkjb7yurUdjYDtOOltpPGrpG0eGbL18/L8utqawkVyVJHP6robgXI+npAJ+n19qMZrw6Psqyiv7M8ek9nKykxONrszmK6jxeIw9BVZLKZLIVUFDQYvHUcL1ddXV9XUFIKalpaaFpJJHYIiKWJABPurDNTwp0rjkjXUQaDjXjw6o0+H4z/z8+Z+8vnzuNc/Q9EfH+TcHVHw4xU08MWLzlXl6LP7a7G35VYieSPI0GTrMRWpLUvJS05lbK01E0szYQqrQqxLVx5dFtkTf35v3H6EfbF5fI441p/qx1cnmqw0UDu4i1nSvqJN0Q3WKMIxvIxJsTe49tSv4amtK+v8AsdDuwg+pkVVrp4/t8zXy6j4XI+dkkQrG06EsT/YQMFUkOAbyNcDi3HvUUgJxio6dv7XwgUYVVTQf5cj06XcUhjeCwYxCM2CIWte92JsSWkbkD8e1QOAo4f6v59Bx1DCQnDk+f+ry6UXla1/A1vHr+v8Auu9vH+q99X5+v+w93qfQ9Fuj/hvnT8/XoTfbPQR697917r3v3Xuve/de697917r3v3Xuve/de6xPZwbKDpvZmW4V1/NuGNv8PfurKaEZ/Z1jp3lcFpY3jsAF1MvqH+qKKToY/wBD9B72erSKimiOD9n+rPUn3rpvrEYYzL5ivr0aD/QgG4uP6j/iffur620aK9ta9Zffuqde9+691737r3Xvfuvde9+691737r3Xvfuvde9+691737r3Xvfuvde9+691737r3Xvfuvde9+690y5yOiXH1tVX1EdJRwUlQchPKnkgOPEbNUrURA3dFjuQR6lYXH5BL7+1imiZ5HCqFIckVBTzBH8wRkHh0psZJkmSGFCzFgUANCH8iD/hHA9Axh87haLIYveuVFTBS5BKvCwVcwamohUXK4rOJSzuopzujFUQS+nmaO35v7CdpcQWl8L2ZXKIjKSFNa0w5X0ZB5eYJ6Ft3Z3cttLtMBQyhhLQZNPxx1H++nPDyB6HqlqYK2nhqqWVZqedBJFKn6XVvyL8gg8EHkHg+xxFLHPEk0LhomAZWHAg8D0DJI3ikeKRSJFNCD5EdZ/bnVOve/de6LF82K3I434c/KyvxMkkOTo/jn3RUUUsK6pYqiLrrcTJJEOT5EIuP6Ee9HgevdfPJymNpo9r4+locdj5a19rjPz19PuCnypamipqxjTVNEhipcRWUvgUtSPrq0KqefIB7T+fVfw8PLrfC318oenPgZ8B+rey9yPFNg9t9M9abY6w2XSV0FHld/biTYGOG2Nq4iomjlEK1FLRGora0xSpQ4+GeqdHERRn60UHqzUBPWo/8vNi/I7a+Q6o+YXyHzVHQ9t/NA9n9lDZcmJMGW2Hs/bg2jtrbNNkqXNtkqXHYvMbL3TSw4THyLJVYrGUkK1Tit8qRNsDx6qDTP4iOrVP5CHRE2L+Q/yb7RraTdWEh642LtHq/C4bdmIlwGcqP9J+QTfdXU53D1cSVlDWY/C7LxbQkBYp4ckZF1LoPvcfEnreRXHyHWxr2dl9p53Zu8Nuby2zjN07Dze1NwUu5MZnaeir8JndsnGVf94UyNBXpLR1GFONSZZBMNDji1iPYUueZTLeDbrK2YmUUimqKH+J1HmqgH0yPTo8j2ZUt3u7icAx5kjIOPRSfVsdauf8nT4+fJHtTbXdne3xk+RWO+MdC2/aTZVZsLcfT+N7v2ruSix+3Id27YxNfl9y7lwuVpn2Hjt8JQx1FMwrJI3LyyESGMiY28UukyRqxX4SwB48fsr0SpLIgPhOVDcQPsqK/ZXobv5mXQ3y16k+KO9ez/kz/ML3/wBqVOf3PtLZG2uleuNh4PpvqjP126MyFyOH3JSbdybZDcuDodqUlfWrTVKEM9IPKZQbq6V0qBXHAAdUIY1LOSf9X2n+fWuTS0Gaxz42fFU9XBnstUpR4HGti4K6ryEOfoBSY+fF4aohqKvJplXrDBSyR07xyyEeFvKBpp/g63mtPPrap6I3v/M5xXx06w+MPxZ+AuB+LlNszaOI2vJ3p8gex9v1OMpaiSiM+5t7wdYUWGi3F/e7c+6ayqys7VNJl4Y6moczUs5ZgrgLUAA61ngFp9v+xXo8Pwr/AJcuH+Oe9dz/ACI7t7FyvyT+X3YSSHdfdG7KRYqfbdPV04pavAdcYmd6mXBY/wCwWOhepLrI9BAlNTQ0FETRC4FKnzPXgtMnJ9erMve+rdaK/wDNR+TOM+YHzJ3Nmev6yXOdYdRbfp+rtl5nHSffYvL0G3MvX5DfvYNJJEzUFNgcjuXKSwxV5kMFVjcZSVBdUkUKyxqeq1rU+Q/1HrF/LNy/buy/kKO1+sPiZuz5f1HTm39z4nbeC2tk8LtKh2FuzsGrp6Kk3llt71mLyWFNbU7coMxSUkFS8pMdZLLA0aRFvfk41A698wK/LH+WnV6e7/jH/Mb/AJilWcP8t904P4YfFaqq4Zsp8d+n9xY7e3a++cbBPHNHjN+b+pYqvbTRyrdw2ufHpKsZkwrzRJUK5Qnjw69RjxNB8url+qep+uujuvNrdUdUbTxWyOv9mY1cXt7beHidKWkgM0tVVVM880k1ZksrlK+olqq2tqZJquurJpaiokkmkd2t1sAKKAY6Kv8AzDfmJTfDH49ZbfGGxybp7f3pkabrzorYMdPU5Gu3d2XuFXhxZXDUCvkspi9uw66+rghCPVCFKNJI56qAnRNOvMaAnz8uqFvnL0Evwv8AgB8fNs9kZSl373d3x8sMP8hflXHuCVxP3Fu6i2luzeO7do5TdGNP8Uo9t4PIVVJilmpCjTVVTJWRiCSpce22FFFcmvVaUA9a1Pz8+qUsVg9ydvduR9d9Rdd0m1twds9h1mM2D15R5msj/g1JvSud8B12+7NzVME0+1cHjJ44hXZACSSCH7idiSfdAKkU6tStBTPp1tgfDD+Tt0B8ddu4XfPfWEwXd/d1HRQ5vM5LctM2T6r2FWxxGqmptjbSyVPHjsnFhCgCZrMU02RnkiNTClAsn20ahY1FCTnpdHDCih5mVm9PQ+n2/Pqrv4qVcf8AMi/m2ZXu/LVGSy3U3UL1PZ+yaXJ4alwj0my+vcxR4jonbVXQY8tHRVf96sv/AB1kmaWaf7GZZLXKJRRrkr5V6rCDc3WunYO70wOA/b1tikF+DpCBj6V9Sm3IUkckrbn/AHn2pA8yM9HQ7eGWPrx6ow/mVd1dgfIztvaf8sD41yZFt09jJhcv8nd/YW8tP1d1FV1WOyFfishNFUU6UwrsDUR1+WjmkgFZQ1VBiovPJmjHG1IdRCLx9ekVzJLKwsIOLEeI3oPT/P8AkPPq1zq7qDYXRvW+0eqOsdv0229nbLxNPi8PiaSKCAzLEGlrMrk5aeOFslms3XSSVmQrJAZ6ytnknlZpJGJsUAoACehFZqlvGscYCxAUqB/P7eu8nF5a+SOYceMqiiMPFZW/cVbfokDfRv8AU39pHqXavClOhbaNptkaP1ya0PyPzFPLpqet/g7SSCHzSzSgEqQkYXSSVbUGYKSlgALccW97jUKzU48eivf91axtrVxAXViVFTQAgVqT5k/8X0u9s5ZdwB3kLUpozGk1Or3Ui142RgoLI9rfgi3+x9qlqxGaAeXQdtdxS6t3ZIaT1o1c8fMH06XWqD/UTWtpvoF9N/12/wBRq4/rbn3eny+XXqS/xLWtfz9Pt8+hS9s9A7r3v3Xuve/de697917r3v3Xuve/de697917r3+8e/de64SKzoVV2jY2s6hSwsQTYOrLyBb6e/fn178uufv3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de697917r3v3XusFTTxVcE1NOoeCohlp5oz9HimRo5EP+DIx90kjWWOSJxVGUqR8iKHqyO0TpKho6kEH7M9BpRY/GwvT43cFHRVKih0Ub1qo8CTY9nx1bSRvKfGhal8U8Sj6CRytrH2B1jtrR0F9EGqKdxJo0Z0OoJ9Voyj5mnQmmmuJlknspGB1d2jiQ/erEDOGqpPyFepW1Mh/C8i22ZZoqqhk88u3shDIJVnghUSyUk7ISn3MMJvccMY3vz7W7DfeDcybQxDQ5e3kU1DLWpGMVANf29MbpbGe3G4hSs4otxGwpQnAYedCf8AJ0JHsXdB7r3v3XukzvTamK33s7dmx87H5sJvLbOd2rmIbX8uL3Di6rEZCO1xfXSVjj6/n345x14Yz1oO9q/y3fmJ0bVbm2vvf47dt7nGJrIcTt3eXVG08h2ZsHdFDFVS075xshtCDL5nGUeUxUaz0sNXSUlZDLJ4qmKNxp9slSDSnVcgZGOH+rz6u2+Ef8u75H/JreHUvyJ/mQ1OZl2H0jtjb23/AI9/G7dNDRYuZqHAU2PTEZXsHZlFTU1DtnA0/wDCqOafF1iSZzcdZTRfxoxUNJHQ1lgpNNXl16hLaj0Vr+f7uZKn5abC25lWrpk278dMDXbQoBT0s+E+/wB3dhb8pd21+V+4kSpjqDjtvUIpDThv36dTL6BY6fj1bz6PV/Ihp6iH4qdz78zOaq8pm9/d75mmy+Vra+ry2bTB7I6/2JioFyFZVy1FdJV3rJYqWNixSF4yvpKgBzmG/NtaizjZlknqGdeKxgd5H9I10r8yD5dGm0WpmnEzKGCMNCnzc4WtfwilT8h0Zv8AmvdvY/pH4K9v11HWUdFvDtHF4vqnAzGoeCaGbsNv4NV4vCOVVoZcLsEZfJFLAsKKQsQTcFG1WlsZ7GCGJDMAtzcMM+GACIYUPlSufsNePRjf3MyQ3DtIwj7oIgad5JrJI3qTmh8sU4dCD/KC6fg6e/l/dDU/iaPKdk4Sq7mzTPTy0srz9m1LbhwscsMwEokx+0JcbSEn9X29xZSAB6ooB0GFGB/q+fVfv/CircklN1P8Ytns8i0mb7U3nuiRUj8iSVe0tlfwilWQeWMran3vPYi5v/T6isnADqx8vt/yHqnr4RdUdZ9k/On4rbX2/vHMV9Oe68XvvAYzONj62soOtOp8Bke2MRjt4ZfGSNjo9+ZPP7Wjx7YehT7agpUdnd/KpFF+IU60aGgPW9x7f631737r3VRP8x/5L7xy+5tkfy7PjPV5Vfkx8nKehpdzbvxME5oeieislW1dLvbsLMZOCz0uXrcDi6+KligZKqnpllqFkgqnxi1dWNe0ceqk5CjietQ+o2L1xtDfHcPXc29c1R1ew915bZm29zyUWPxm18rgdnbxzG3t9T5zCLXPmcpV5TbWLhqcFiKNw9XWlqedgoR2Zpx+3rdAMemP9VOtq7+Q91lgNn/E/f8AvzAZWTM4/tjvrf2RwdXWU60uYh2dsYY/r3bVNnqWMCKky9U236rIywoWSIZAJe4Pt1OFevDhUcCf9j/J1dx7v1vpObw3dtvYG09y753jl6Tb+0tnYHLbn3NnK9mWjxGCwdDPksrkakoryGGjoqZ5GCqzkLZQSQPfuvdUj/ELb24/5kXyqb+Y72XQZ7A/HjpbIZrYvwc6wzsMsD5aemNRjd3937goZYxQx1ldkRpgWnM7DI0yQPOf4HBJVVGTU/l1QdxDeXl/n6AP/hRjLEm2fiPG5Bf+9nbkviDKHkp4sHslJioZWsoMyqW0kKWHusn4erny+3/Ieqvv5XGAxXYv8yvoqjweDpMVtnbm5N+9lrRnOV26J6PHbV6x3FR4PHLuTMQUNfmKeiz1dSSJI1PFIzMbroRbUTiOtH4hT7f8n+XrZa/m1fIXK9DfEPc2E2dWQ4/sDvnLRdG7Ryk9RJSxbdXeeKy9XvPdM9XDeagG3tgYnK1ENV9KarEMhvp0l1zRSenCpKamPmFH+r5AdE0/kMdC0myfi/u3u6ojp/4x3nvjI0eKkQ6mh2D1TW5PZOIogWsyvJu+LPVDEWDxyxXvpHu0QFD69GFhREL0NScEeg4dHk/mB/NHavwu6Hze6TXYmv7f3VQVu3ejuvpw9blt2b1q1p6KHJnB0cgyNbtTaM2Qiq8pIvjV18VGkoq6ylSS7vpGD3dPXNwIU1VrITgfPoHv5ZHw53F8eOtM93D3VJks/wDK/wCSEsG+e5M3uGpatzODStrMhmMLsqQskdPR5CgGWepzPiQI+VleBWelo6IR+QaQWI7j1awg8MGaZjrb4iT5f5T1ZLLC5SSQEvJ+jWeNVjcogtwFP5/It73Qk16PldaqpwvGnSXfEzNUuoiHNpgX1FQ6glxc863vbm490MdSMdGq3iCIHVn4ccaeX5dIjc+NnpaYTzaVZqhLoBc2dX0+senQn0A+vtvQVap/Z0V8yXMdxtkSR1IWVTX8j5ep6hbUrMjSVFWMZj/4hVTxwLGHk8VPSmJ5GM07EqCGDWAuPp7cUkE0FT0F9ukuIzOLeEuWABzQDjxPSzv2H+r/AHE/8rWmyfov4/s/0/p/t/8ARf493/U9f8HS/wD3a/8AC+P+of6v29Ga9t9B7r3v3Xuve/de697917pJVOVrq01n2TxY3F0QY1GZqiqoREGNQYhINCRxKL6zf/Yeywz3Fy0i2/ZAMeK3n60+XRzFaW8Hgi4Blu3ICwJxzwBp5n06C2ftvZlLUy065rPZlKe+uupo5Y6Nn/TemkBRagD8aRp/xPtjxbdCyyXMrkcSDT9mR0L4+SuYZoY5Rt1tAW4RuRqp/SBrT889YKXubZkjugzu48eyqby5GhNRSKwP6C6CYgm/B/p7bW8ty1I7yVafxUYfyqenZeQ+YUUN+7bWVTwETgN+w06W2N37BXQiXGZbC7hS4utNULBVKG4QPFfWpJNjePg/X2pW5uVFUeOYV4A0b9n+x0Hbzl+S0fTe2Vxan1dSV/b/ALPSnh3XRhxHkKepxrn+1Komg4tf96HVbk/lR7e+vRG0XMTRN/SFR+0dE52uVhqtpUlX+iaH9h6UFNWUlYgkpKmGoQ/2oZFkA/19JJU/6/tXHLHKNUcgYfI9IJYZYW0yxsrf0hTqT7c6b697917r3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de6S25tvrncfW0JYxirRWjqEXXLQZCAH7LJ08RdVkeBrB1updQLH8eybc9tF2kihao9GPqHGA4FRXGGGCRSmejHbr/6GaKSuVNKfxIfiQniK+R8ugrpKObF7mxM2ZfHUE0lf99kcjFHKv3OWxuNlpP4RSUka6I1y1FP98vCkHyCzED2EbCD6PdYnuT4YiYlyQTkrw7cdwIIx/MU6FEzC5265S11yVQLGmMIXB1knJKMNB4+XAdDzDNFURRzwyJLDNGksUsbBkkjdQySIwJBR1Nwf6e5FR1kRZEYFGAII4EHgegOysjMjqQ6mhB4gjiOsnu3Wuve/de697917r3v3XutWX/hRL1HlKfeHxx78pKKeXB5LA7p6Z3DkkU/b47NUNcN77Jop2A4kzlDWbgMf/UCR+Rdtx59aPEf6v9XDrJ/IL+Ruw9vYrt740bnzGOwm9czu9+4uulzFQlJQ7hpf7sYfbO9qCiqp9FKMvtaLbVJXzUxcTz0MrTxo0dHUPET7pDLMLUQwhpRJ2kiukkYY/wBFeJ+YHSyzkVDKGkKxle6nmBxUfM8PsPSZ+Ue96P8Ams/zCekPil0tm/75/HDpnJ1u4ux97YtJW29uanx+UopO3N6QZCkkNNlsDHioKTaO3smEENVk8vUyU0slHUR1Dubbtke3qyLIXdjVpCAGbzJanE18/sHl1W7u2vHVigVAMLWoA9BXgKY+0nra3p6eCkghpaWGKmpqaGOnp6eCNIYIIIUWOGGGKMLHFFFGoVVUAKBYezjpN1Ql/wAKDOqMxuv4w9X9r4mikrKXpvteIbqkiQscVtXsXDz7X/jExCkili3hDhqaT+gqwx4U+6OMdaPD8/8AY/y9U+/yQc5jMJ/MJ2DBkaCKaXdnXPbO08HUTxKRjc7Ft+h3YaqklkDaK6bBbVr6ey6X8NRIASpYe6J8XXvMfZ/m63dPb3W+qmPnV/M3wvRmYpPjt8X8PR/Ib5obyyMe3tt9Y7cp6zc2L2PXTLLJPkN/nB1FOFyVBRwSTjDCspamKBPu66SioR9w9S3kMnqpYDA+LpY/y5/gnl/i9jN/dy93bhj7D+XHyGr23P3NvQyJW0mBOQr6jOvsHatWY0AxVLlq1pq6aBYYK2pihSONKSjoo4/AUyePWwKfb59ahHzy6pzHS/zR+Suws5Ry0obtrdW8cFI0DxxVu0OycnPvrauRoSdMdTCMXnRTSMhKCrpp4+GRgGmFCet+Z+3/AA9bff8AJ5zNBmP5dfx3SixsGJlwdDvvbGVo4VWNjmtvdl7xxmTr6uMKjJX5iogNZOHGvy1Bvc8l1fhHXhwHR9uzO0euumtlZvsXtXem3dg7H27TGpy+5dz5KnxeNpgbiGmjknYPWZGtltFTUkCyVVVOyxQxvIyqbcMnr3WvruPc3cf87/s09c7Nxe4uof5aPWW86HMbr7Mqsfk8Lvb5A5/bs1XTJgMC9XLFSeCaZ5WgohBNHt4LHkcoXyf8OxcDeXx5dUy+Pwf6v9X+zw2KNrbX29sjbO3tm7Rw9Bt7au08Ji9ubbwOLgWlxuFwWEooMdicXQU6emCjoKGmSKNR9EUe3Or9Vu/zKf5ch+feM6kqsT2u/Ve7uoK/d0mKqq3a3979vZvFb1h27/FaOuxsOc27X0OTpK7alDLSVcVTJGkfnjlp5fJG8NWXV59aI4EdAB/Lw/lEYv4kdlt31212JSdr92YmHP4nZdLtGirsJsXZFLuKinxOVzVStbN/FNw7oymFqZafXUCCjo4KmVI6eWXRVL5Y6ZPTyxGmtzRPInH7BxJ6qw/nm/Iyu3Z8paHoKkw9FuTCdLddCCkoJa7KwMO5O4sZQZOPdMYxeQpEq8ptbbH8JgxcFWssKSV9W0iOsyhayNUhfLr08rOaAUVR2j/V5/5+tijbUPT/APLs+GWxcf2Duug25sbo7rLD4rM5SskhWr3DuSDHNVZZcLQvLHJl9zby3RNUNR0EWqapq6kRoCTw6p0inl0/FOEiKsD4a+fr6D7T1WX8HOk+3Pnn39QfzPPlZt2l27s/BQSYv4e9LPTLLBhtt0dbkHxXYOUesp4pK+DGVFXLVYyvnQVGZzMz5Wnio8fSYaN6r3PqIoPIdNQOZJ/Emb5qPT0H5D9pz9l9FQmktEwXULNI9wdBYfRiAAXt/Z/B9vDjUcPLo1iaveCaHAHr+XUGONbXILDVZbAA3sLHn6uxHP8AT3s9KHdq0rQ0z/q9OswxqvHJL4nJ0jUsWuR2JJIDEEhSTx/j78SOHVDeFWVQ4p6mgH5evQQ7vw2Vq8XkMzXn7COjeOSkw8TLM4p1mWA1GTqEuhqnicsscZ0xjgliSRRqkV8uk11JNcW51tSNTVEHn8z6mn5D59NfXUev+Lfj10QYgXcAie2j+r3Fh9ffkp3dObOwAuPXB/w8fl0K+hrfok/1P6m/rfRbV+q/5/2P+HtzPRvVf4h6/wCz0KvtjoGde9+691737r3UWrYeJk1iIMrGWViFWGBReaRmPpWyXAJsATf8e6SZUrWleJ9B59OxA6gwUkg4A8z5Dopm+NyVvY+TXbu1pTBs3EEJNUHXFSZWqjLKKibTZ6mhjH+YhJAmIMjC2n2USs92wgtgBbqKE+X2n/IPz+yaeXdot+VbP967ymrfZxVEwWjU+Qr8Ln8R/CO0Zr0z0mwaEEeKGqyM8R0l/X4ZGtfTFACEJX8ABj7sm2wLQlS7DzPD9nRhNzNctXW6RRnNBSo+08enKbr2uTQTj6emjPJtqqXjBAP7qKgVTY/QEke3jY8NMSgdJE5ptiWpcs7fsB+wk/5OmOo6yjed54SYZWF2kjlWEnjjwrEfOmv/ABP0Fvad9qViWBIr6H/B0Yx83sI1ikGqOuAQT+2vaeuFHNvvbx8eMz9RPTxs1qXJLFk6ceoBkIqkMyXH+pcEe6C3vIcR3NU9HAYfZnqtxbcsbp33e1Ikx4yQ1jb7e3B/MdK/H9hNTzKNzbfNI4dCmT2vVyrMPICQZ6ByhAB9XDm3upSNmBmt9ElcNAafyJ6IrnlMOhOz7r4i0NYb1RT7A4r/ADHQu4TfGPqwkdBurFZFtXiFFmHTH5BXA1CNpfSWcggXKnn8+1cckqj9O7SQfwydrft9f29AncOX7u3q11s08Qpq8SAF0p60zQfn0tl3BDFYZGkq8fe37zRmpojc2Girpw6f8lBePb/1ojOm5heM+tKr+0dEJ253qbWdJf6IOlv95an8q9PUFTT1SCWmninjPIeJ1df9upNj7VRyRyrqjcMvqOkUkUsLFJYyr+jCnWb3fpvr3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de697917riy6gRcgkEXU2YXFiVP4YD6f4+9EVBFf2de9DT8j0DFVtOnkqY8RPka6Ko+5fJQ5CI6WGdpHlq8bOxfUwlhp5dV72lGtDwPcay2clnuK2zXUmpgx8Q5rIKlePnpNQftA6Gy7kZLdryO2jMYAUxnyjYBXGMUJFPlg9LnbFfKNeIrZdVdTJqI0qq3QRipSGyxkwCaTXFcX8Tgf2fYg5b3MzCXbriStwlWWvmPMDhwJx8iOiPd7ZQUvoFpbvg5/3knjmgofmPn0sPYr6Jeve/de697917r3v3Xui8fJvoXrr5SdR7w6I7Tx1RXbN3hjo1rKrHTRUeeweXop0rtv7h2zkZYalMduHAZSmjq6eRopoWMXinimgklicM73us9tcW9tbPp0jxZiRXt4KlP6WSaZAGOPSy3gjeJ5JRWp0JmlOFW/LgPn1ro1n8iTvneXYe8aar+RXT+4tn1WNotr1vYe5+qszWb0MNK9CaOtpNp02Xp8DBvXD4nHQUslfTZiANFqUqvkkBU7TuMO5rKbaNhEhoXPwlvMKeJp5/wCz1a9sprWK3muJF1zKSqUOrSDQMwwBXy9aVp1er8HvgP0x8FNjZPbvXX8S3NvTdpx0/YfaG5kpBubd1Ri451xtBFT0MUVBt7auFarm+wxlMCkAld5ZKioeSdzwAAdF6jzPE9Hg976t0md57N2r2JtLcuw98YHG7o2dvDCZLbe59u5enWqxmaweYpJaHJY6tga2uCqpZmU2IYXupBAI917rWm70/kP9pdb7ui7U+CveMtBktu56HcWytjb8yWR2zu7ZdTTyPPCNo9w4Y138TahkYQ00WWxsUr0t0qq+oJcytlDWoPWqfP8Ab/n6WWM+E387jull2Z3n82Mf1j13nsdUS7ky2zdwU+T3LTeM09PFgUxvXe0+rq6rOThkczCHcFPR6EcSGXWI39pY8T1qj+bD8v8Aih/h6tR+D/8ALj+PvwWwtbN1/QVu7u0Nw0EdDvHuLeMdHUbvzFN5lrKjD4aKlhjoNobWmyCidqGiUPVSRxPWz1k0Mcq3Ap1sCn29H897631XN89v5avTXzuxmGzGeyeS627k2jjZsRs/tvbdBSZKtTCSzz1o2rvPb9XLSU289oQ5Gqkq4KY1FHWUVTJI9JV04qKpKirLX7etEVz59U69f/y2P5wfxWym5uvfi98iNiY/rDP5P+OSZul3auGwlfkViigOVqNhbw2Rvir2luWvgp4o6s4yapiqUijE1TKI0000sK0693V4j/V8qHox/Xv8nbuv5A7i2t2b/M0+UO8e6KvFf5bH0ltXOZOLa2KnNSNWNl3lDJhqShx9fQwqtcm28HgquRnZRkHCCR7aScsetaSa6j1frtXam2Ni7bwmztl7fw21Np7axtLh9vbb29jqTEYTC4qiiWGkx+MxlDFBSUVJTxKAqRoqj3fq3T/7917r3v3XuuCxohYoqprYu+kAana13aw9TG319+62WJpUk0wOtHr+Z51P3L0v8+u6eysz1ruLcG2N1dkbK7a6435k9obg3BsbLw09NtbI0GGbKY6JsVNPh8vgZcJWYqpmWoNHCrJEI5oJWZcEGp6pXJxwoeH2f5urYerfiz8sf5o+/euPkB/MV29RdSfHvrs/xHrX4uYSgzu3avf+Tl8LVW598YTOZXI5/b+Fy/iEEoyTx5asoVenp6agpKiSprr01UJ693NxHb6f6v8AV/l2GqTH0WOpaSix1JS0FDQUsFDRUVJClNRUVDSxpDT0lJSQKkFPT08MapGiKqqoAFgB7v1eppp8ukPu/cNNtsRVOSusdXLLHSw0sJlnmaMCQgm4jEmkgliwCgj6/T3cMABXoxhnt4oqksXHl/q8umva26sLuZaopHVUtVSSRq9NMIvIYpriKpSVWdGXUhDADVq/wPvwZjWnV0uJJiREMAVNf9j/AIodBd2VVZHGbvqYKHJZGkiWgxs0CU9bURLGzwsjsqJIEu0kZJuPqfdDkknj0XSSvI2pmz/q4dDElId07GpKiqZ3q63bQJKi4lqPtDaWTgXlklAP+B+nvYPbTyPT0dw0cckQAKtxrxyOgo6ivLW5mIxln+zoZtNi2lhNNG/A/Prt78p45x1a0fR4ndQGlf59GL/h1L/yoxf5ryfrb/O3/wA39f8Aefe9bevXvqZf+Ug8aeXD16dPdekfXvfuvde9+690XvtvdstZUHr3Ayt97kEjk3HWxMbUGJB1mg1KwYS1oB12IIjJH9r2X3TmRxbRnuPxEeQ/zev7PM9SXyRsqQxnmfck/wAWhYi0jb/RJf4qeieXqfs6i7Z29S0NLT0cNMViHEVKlw0z6ReoqmHJJ+oXhVX6/wBPamGBI0CIuONPX5npRu+5zXM8txLNVz8TnyH8K9CvRY9KVUIQPWSRhXZF+g+vhhX6LGB+fqfz7UDoGXF00zNVqQA1AJ/mfU9ZKyXEYCBslnq6GnQFWhp9Y9TpyqrGl5KqVjbgAj/e/emcKMmijpqBL7c5BabZbszEUZ6eR9TwUfz6Das35Jm63xxUlNi8bGJHd6qBZMnOEISFtVgtOrOfoLtY2v7ZWTU2ML6+fQst+W12631yTvNdmgARqRiuTji1OmTKUkc8cmiJlK2KyFLtqcB1cBOXJ/3r351DVIH59GVnM8bJqatTkA/5/ToOTRPVuqOFiZ9V1l9Ckq2knW1gB9OAbk+0RUueAHQpE6wKSKsB6Z/l1zqtpRzQgwSxzVBs0kEqGSKO5JLJUWEy/TULjj8e9Pa1FVbPoetQb40ch8RCsXAMDQn7Rw+XWKCu3jtttdFlMpSwBbBYar72AgH03gnWVfH+CCB9fbdJ4QCrGnyyOrS22wbsNNxZQvJXiV0N88imen+j7WykDB8phqatljQaqzDVL4HJltWoPLHpkoZjpBuCFBPtlihbUYgJP4kJQ/nSoP7Oiu45JtXGmy3B44yf7O4USp+Rw4/n0IGK7mxk7xRCv8UraQ1BuaFcZUC/1EGUpg9FUEH0gsLMfyPfvrpoTh9Sekop+x1qP2joLX/I99AHd7PVGD/a2ZMi/ayGjL/k6FSg3liatEao82P8iqyy1Kh6F9VrePIwGSjN7/2mU/4e1se5QEAzAx182+H/AHoVH7adA+bZ7qNmERWShpRT3Y9UNG/w9KmOSOVFkidJI3AZHjZXRgfoVZSVYH/D2YKysAykFTwI6K2VkYq6kMMEHB65+99V697917r3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de697917pM7kwaZbH5KJWmikrcbPQySUz+OpRWDeOenkBUpUU+trWIJBIB9km8bf9TDNLEtZdHClalTqU/OhrjzBI6MdtvfpZ4NQBjEgYV4fNT8j/I9JTa0FJg6zHY8eRoJ6V6KlmqZZaqrpsnjaaOKsxlRWVDvMyVMCfcxhjcsWAuAo9k2zG3hvomeNQ8wID+YkAo0dfJSO5R6no13Qy3NrO4OUOsgYDI5qrgAUqp7Sfs869CeGBOkkarBrf1U/Q/63safPoMAjh1y9+631737r3WKeeKmhlqJ5Fihgikmlkc2SOKJS8kjH8KiAk+6SSJFG8sjUjUFmJ8gMk/kOtqjyOkcakyMQqgeZOAB8+g0roJ92ZLFHHsKE0arn5Kmqh+4aj+5gMGKgNOsyaampXVMysQEVBe97GOZLOXmbcXkgdoECiYu3cVBGmMaa0BcAuRXApx6FlvJFslpci6XxdZNuqKdIbSdUjaqHC4UEDJPS/xWMpsRQwUFKG8cOtmkkbXNPNK7S1FRNIeXmnmcsxP9fY9sLKDbrSGztwfCQUqeJPmSfMk56C91dy39zJcS8T5DAAGAoHkAOnH2s6a697917r3v3Xuve/de697917r3v3Xuve/de697917r3v3Xum+sy2Kx7KlfkqCidraUq6ynp2a/0IWaRCR7917rukyuLr5Gioclj62VE8jx0lZT1MiR3C62SGR2VNRAuRa/v3Xup/v3Xuve/de697917qDka6mxtFVV9XLHDS0cElRPJIyqqLGuoAFiBrdgAo+pYi3Pv3XugGoe7av75WyWFp48VJIA32csrV9NGzcSsJbRVTKpuyAISfoT71nPW8eXQ6Jl8VULEIcpQP8AcKph0VcGuRXF1MaeTUSb/S3vfXh8x0DPdqP9rt6QuWj+9rowoUWRvtozqL21MzaCPfvTrZI0gae6vHpu6Uo0krc/XOoIp6egplLcgPK9RKTb/VaUsPfgckdbDMqkA4PH8v8Ai+m/uaiMG4sfXAWSuxQQtYgGWjncMB/wWOdf9a/vX5dV8h0NmyiKfZm3A/4w9Ibf1/Y8h/5N9769Q9Ar07VKu6svCbRmuxtS8SjgBoa9JdC/4LHKf9gPdV+XDr3mSR59GTs3+P0/r/sL/T9dv+Re7de/Pz6y+/da697917oNOy9+Js7GR02PRazc+YD0+ExykM+uxElfPHyRS0g5ueHYaf6kJLq48FQiZnb4VHH7f9Xn+fQq5U5cbfrxpLhvD2iCjXMx4AeSA/xNw+Qz0D2zdryUML5TLVD1WVyMz1dbUyfuy1E8ml3d25JRW/Sv5J/1verW2MQLSGshNSeh3vu8JcMtlYxCOxhXRGi4CgYx9vmeh1w2K8KeRlvU1CgSEi5jjZtfjv8AgN/a/qePx7W8OI6jm/vdbaAf0lOAPM8K/l5dN25940u2y+NxsP8AE9wSRginQHxUiEXV6llBIUDkIOT9TYe2nkCY4t6dKdo2Gfdwt1dyeDtYNC/mx8wv+U9IyhwtZl3OUzsv3taZAwmnBWmpEex00sWrRZfxpAHH197WMnvkyfIeQ+zoQXN9BYoLLbk8O3pTSuWan8R4/t/Z1xyOLoWCim0F0WzVCopLvqsdNwLKAL8f7f35kDUp1u0u7hS3i1AJ+GvAfPrjAZxqUxL6QUEqs36LaVLLYkkD8f7b3daj7etyiMkUc040P7cdcY6JHlGqESMb3DoOTf6/Sw0kf7f3oAeletvcMENHoMUp1xq8dG8emEaZ7OiFOCrJY6WAI16R+D+femQEY49bguXVyZDWPBNfn6enSNk29lDLIURxHqUg61a/0uxDEnSAPp/U+0xhep6Pk3S0CKGI1dNFdhJ9ZFTjlqfRZJDeJ2H1b1oeGQX4ueAPbTw/xJ+fS623FAoMV2UqakDIHpg+XSNyWCpZI2HkaEMFHhnjM8dvrbWF8mpSf8faOW3B/FT5H/P0ILTcplYEIGIPxKdJ/Zw6aqXI7o2cyJjslU0lLIyyJTsVrsTOCbcQTDR6wf03X/W9l0iS2xGkkKeNOB/LI6fuNu2PmAM91aK1wMF17JR9pHGn2HoUtt9n1TPeppKvFzpGC0+Fby0NRKWuVloZAIEcqNZ9I44F/bsLPUvGSj+ejFftU9vQH3fkxoRS3uI7iIn4ZxpcD5MKkiuOPQwbf7MbIFUeKCvBZVYRH7DJRKzhTJJQVHomXm48bC4/HtdFuE6Gk6Bl9R2t+w4P5HoC7jy09ocq8TeWruQ/IOOH5joYfZ10EuuibAn+nv3XumavzVLQqTK6rY/kgf64ufz7917pKzdjYOFtL1UKkcHU6/W9vr7917rD/pMwH/K7T/8AUxffuvde/wBJmA/5Xaf/AKmL7917r3+kzAf8rtP/ANTF9+6917/SZgP+V2n/AOpi+/de69/pMwH/ACu0/wD1MX37r3XX+k3b5JH3tPcWv+4vF/p79wFfLrVemit7i29T1S0SVNMJmjE3mnl8dKqatAXyKrFpSfxwLfn8eym83PwJBbwxhpiK1YkKPlWhJP5U+fS63svGiMzn9OtNK5b7acKf6qdI3I7/AMHX1wFVUhYochTVax4+TxPW5Kk/epPFMCWgSKJisjceRODYW9hV7a7v9wMUw0xB9bLEMM4GNJOV0g8f8GOjlLqKxszJCA8pQouvNFbBqOBqeHp06zdnrBj1io8lTVOQkrZZKto2jZoIGvI0FMXvGXj4BuLXuB7kWyiIjQXhBIXj61OK+p/w9A+aVyT4NdRPlwHyA65RdpwwUsclbk0+6kknMcMoptIpyQIjUCIhWcNyFB1WP19qRHA7uqL2etf8HTJadQpYnWa4px+3pxbtXGtRNV0tZCahYm8tJ5Q6fcKxK6dYLpDIf6chbf09ku6QXSRvLZTN4qCoTFHANafI/wCEdGNlJC7oJx+mxox/hr5/MdI2ft2DLY/JYzOmlFNXwtArUJMc9LKCAFdXk/eUOoYjgnlbEH2D3v77cLa7sdxjpHKpWsdQVP7c0P8Am6FSWtrZXVreWMlZY2DUkyGH7MY/z9KfCdjbaw9M71GTWuyeWqDW1lR4ftpKicxRxRxRUhLNTwUtNEiRxkmwFzyT7E2y2aWtuV8QtNITJJI401J8qfhAAoB/n6It0uvqZlSOLTbxARpGp1UFSSS3Akkkk9KkdobduqmuplkddQjMqauAL8X5Kj62+ns3oaVpjovWgFOsn+kzAf8AK7T/APUxfeurddjsvAsbCsgJ/wAJFJ9+690+UG7sdXsBDMjX+lmU3/21re/de6VEUqyqGUggi/Hv3Xusvv3Xuve/de697917r3v3Xuve/de6KX2wsbb4ryFW4osYHNgSW+2vz/joK/7Ae9YyOvenTHgpMztdKDetDEgoUyMuLc3Gmp/bEtTSTR6biGaIHQ4PEqcWI9+JAz17o5VPMlTBBUR38dRDHNHcWOiVFkS4/B0t7317oMN7dkSbSzNJjIMbBkUeiFXWE1bQTwmSZ44YlAhlQFkjLer8Ef7HXXup23uz9v514aeZajD1U8op4lr1UUk1SV1imgr4yadpyhuEfQzD6A+99e6ZO5csKTAUmIT/ADuYrVaTn6UtAUqJCV+tnqDEP6fX37r3QedS4AZbcT5KeIPR4OITAOoZHyFQGSkWx+pgQPJ/gwX3rr3Qb5SGNMnk4o0VQuTr40AAXSPvJlWxFiLe9eVT69b6MV2xjteysdPGGb+FVePYsdRIglhajdmJ9X65EuT72evcCa8eoPSKL/DtwNYamyFIrcfhKUlf95Y+99e8uoXbbT5qStpaNVaHZuOiy2Tk0kuZsvKtPFSo/IBho4jOy/kEf0HvR615H9vQp4ApHtPGKiNanwNKNTW0FloULANf6g/U2t+Pe/Tpx0KEBjx6Lnspajb+7to1tSAsGegL0739DUuSNTRqGP0DxzxqTfixB/Puvp1To1f31J5vt/Mvm+7+w0Xa/wB19j/E/D9P1/Y/uf63u3Wupnv3XukXvreuP2NhJcrVoampdhBjsdG4Weuq34jjThmEakguwBsP8bD2xcTrbxGRs+QHqej3l3YbrmHcY7G3OmP4pZTwRBxJ+foPM9F52/isrl8tNuvdMwmzdeC5VU1Q4uhlBlp8bTIbCJnSQ6h+pR9SSSSktYXd/qLg1lbgP4RTh8iepQ3G7srCxj2XZo9O3x+Z4yuMNIx88jH+boasFQfcTB1Q+KnIRRawec2JHPBSJCD/AIG3syFPy6AG5XPhR6WbvbJ+Q/2T1k3Fu1cYsmKwtqrLswilljTyJTMxtpVedcgB4H0B55+nuruQKDLeQ6ptWyG8KXu4ApY/EFJoWHz+XSOxOCTGzNk8vI1XlJ/PIIWlaRv3GF3qmuQxZvx/xH00kZU6ny/R7ebgbpBaWSaLNaAtQDgOCj7On4PU1kmhNRJ/TEE/bXSP0eP+wgBtz7c6LisMClmp82PH9vT5TbWq5yHnkjgQ29IUsyj6khSVuWv+bC3v3Dz6Lpt6hi7Y0Ln/AA9SH2hDGmp8qY1W9y8EKRlixtd9acXtxf3rpld9kdtK2NWPChJP7KdRpMC8YjdK2knhazIUkjiLaSouC7nyWP8AtX1/p7sCPMdPJuisWV7eRXHEUJ/yY6RFdUwz5ul2xR1S0tXV09ZV1NcnjleBaZtMaJJfx+WpqWVAb2Avz7Zkk70hQ9zAmvoOhDBHJHt827zw64UdI1jNRUsMkjjRVz0ncPuSehnbF5xGWup2aKqujRyjSSFkVWCeRG+v0B/Iv7bilI7JBnhXo1vtqiuIxd7e1bdxVKZGfL5dKyWWjqYXdGjmkZ1ZVRxccEG6cN+luRYc/wCt7UVDZrmvRMqTxSAEFVAoSf8AP0m6/CI5vLGNBcgAxkuykEtfgNGp/s+2ZIgfL8ujW23Bl+B+6nr51/n8+gm3bB9mFSPxCCGCUlJmBsGIZWIbgXAH1+g/PsrvFYLQAFaHB6G2ySfUEs2rxWYZX+fQkdWdeZGbZ0uaqIqZp9wTfd0uOro2SNsfDCYKCoWQ+QxGp1NKvo9SFTfn3fbLd0t2eRRVzwPoK0/mT0E+cuaLVN+SxidxFar4byxmp1k6nWmK6cDjg1HSa3Zs7O4Kqp8uyPQxYzIUFQyxktCKaOqiaWamqh6WjVb6o2Yej8e7XNsSCfw+n+Aj8+jTZ9823dIJbCokeaN1FeOog0DLxqfIjz6OUrBlVlIKsoYEfQgi4I+vBHs16goggkEZ6w1LFIZGH1Ck/wC2BP8AxHv3Wuqc/wCan8tt8/FL4t9t9w9c0u3cjvPZWNw1VgqDdtJk6/btRPkd1YHCVKZKjw2YwGSnjShycrIIquEiVVJJUFWS3czQW8kqAahTjwyQPKnQ29ueW7Hm/nXYOXNyllSxupGSR4CqyACN3GkurqDVRxU4605qn/hQr85slIZZdrfH2IsSdMG0uyVQcXsPJ23K1v8AYn2Snd7la0RMfI/5+szo/uo+3b1rvO9f85rb/tj65x/z+vm64JO3Oh+D+Nq9i/8A21T7abfLsAnw4/2H/oLoyi+6L7bScd73z8prX/tj6cov593zYe19vdF8/wBNr9h/0v8A8/TPthuYLxaUii/Y3/QXRjH9zn2yetd937/nNaf9sXTjF/Pj+ajmx2/0d9fxtjsH/D+vaJ/r7YPMt8BXwoeHo3/QXRjF9y72ueld+3//AJz2n/bD1Pi/nsfNB/rgekRyBxtnf/5/1+zj7TtzVuC0pDD+xv8AoPoxi+5H7UvSvMHMP/Oez/7YOp8f88/5mOCTgulOD+Ntb+/+2afaZ+cNzU0EEH+8v/0H0ZQ/cX9pJK6uYuY/ynsv+2DqXF/PG+ZLkXwnS/0HA21vu17E3/5mVe/tM/O26rUfT2/Gnwv/ANbOjKP7hXtA4BPMnMv/AGUWXz/6R/Wc/wA7D5e1LhpsD0y7DgMdt761Ac3F/wDSRyDb2WT86bjJQvY2ur10vX/q50aW/wBwX2gHaOaeZwp4j6ix/wC9d1Kg/nTfLwPH/uH6fOiUSLfbu9/S3j08W7FHGlrf63tIvPO627hktbaueKv9n+/OjMf3fPszOBr5n5n/ACubH7f+jd04J/Oi+XYLOmJ6hjZidRTbu9RfnVzfsMg8+7P7nb+Bm0sz9qyf9belEf8Ady+yLZ/rVzUPsubD/vWdSG/nT/LuQaXw3TzD62bbm9iLqLjg9iEfX2nPuhzAh7bSz/3mT/rb0Yp/du+xsmkNzVzXSv8Ayk7f/wB6zrpP50fy6DBlw/UCcFbLt3ewBAF+f+MiXJufbDe6nMJBQ2dnT/SS/wDW7pdF/dpexLHV/Wvm0U8hdbf/AN6vrg385n5avMs7YbqEutuDt7e2ksv6WYf6Q+WX/kftE/uTvQZZPoLLUMfBJ/1t6N4v7tL2LZGj/rdzcF+V1t//AHq+sqfzn/lyrhjiOoWcn/ONt7exbm4tx2GFH1/p73/rr8xISBZ2R+1Jf+t3SqP+7A9gpCK83c4fldbd/wB6rrl/w9D8uQ1/4P1BcE8/3e3vf+lz/wAZE5Nvem93uZgR/iVj/vEv/W7pbF/dZfd9fjzhzln0u9t/71PXIfzpfl4P+XT1Cf8AA7e3ubf63/GROPbLe8HMwP8AuDY/7xL/ANbujOL+6q+702mvOXOeT/yl7b/3qOuQ/nWfL6FldcP08SP9Vt3fBHFvx/pFHttveLmYD/cGx/3iX/rd0ZQ/3T/3dZCQ3OfOv5Xe2f8Aeo6ty/lTfzMO8/lF2PvvafauO6/x2N2vg8DkcRNs7Fbkx1dUVmSyFZS1CZCTN7t3FBNAkNMCgijhYNcliOPY49v+e935q3O9s9wtrZIo4PFUwq4NdSrnVI4pQnyrXz6wa+/b9zj2x+7By37ebxyDvu/Xl1u97c29yu8TWkqKsMUbqYxbWVoQxLmuosKUoB1tHbRr2r8dDMTfUim/9brf/eLe5b65rdK337r3Xvfuvde9+691737r3XvfuvdE+7LlZ97Z52BvG1JGo/qsVDAFtf8Ar716nr3Sw3XQNTbX6/2NTaXyGUqKetqUC2cPOH1ysP6ieuf6/iM/096oAKeXW6dGHvT46hu7COloKS7u30jp6WH1Mf8ABY0v7t1rok2ezEudy+SzM5YGuqXlRWJJhpltHSwj8gRU6KLf1v718+vdL+TD/wAI25tnbtXBrzm79yYzMS07C8lBQU0kUVPGyclZ5Y30t9CNTg/p9+631j7dyJrN3GlDAxYvH01MArXAmqC9XPcAkBwsiA/63v3n1roUerqanweyWy9dJHTRV0tVlaiolOhY6OIeGFnJ+iiGDUP66v8AH34dbPRcsu0bZvJyRMXhky1VPC5R49cE9W88LmORVkTXDIDZgCL+9UqCPn17gR0ajsSqhp9l5JJRGfvkosdCJBqQTV1VTwI9h9TCGLj/ABX3brXQVbFy8uxKvdOEy9HVSZNmo2xmNgikkqMrWK01PFDQaUYSR1KyRv5BdVS5P0PvQPH1630IFNt6qi29k6LJFKnO7m+8q82YgrxtkK+FoIKOOUXKUuMj0olrDShP593HnUeXSu2QaXZqAaTk+WM48/TqdV10kGwKR6Ri1VV4WjxFLGiX15GshjoF0i4CGOoZi7G+lVJt9fdK49emE7iaip4jOf8AZ6wZTY+PzGPwOJp69qCu2vBQHHZCCGOcqaZYlZZIpGQVEUjwqxGoaW5/JHvdDxp15o3WJWK4J6h/3Kl+n95Mp5f4v9/5/t4PP/eb9X8eva1vsv8AJvtbfb/b8Wvz7tQfy6d8NaV0/wChauPz/wBQp0u9w7hxm2MTV5nLVCwUlJGXNz65X4CQxL9XkkchQB+T7ZkkSJGkkaigVPTu27bebtewWFjEXuJDQDyHqT6ADJ6KpDJl98ZwbwzkJjYiRdv4qQ6osTQBjorJ0IF6mQm6AfU8n8ey6NXuZFuZRj/Q19B6n/J+3qZHjseXduOx7dIGNQbqccZHp8C/0R59Cni8a07RUtOG9Xq1ty5c/rqJRfliw4ubfj2ZKABQdBC9uxGHmlpjFPKnko6VeSrTioVxWPcGdkVamcMP8nDAXjW1h5nJu7H9I/2FrE+XRHaW/wBc5vbpf0gexT+L5/YPIdIcZDFYwyrHUBpnZzUzxfv1U8jFiyiRbpEBzzckD8j3TUiVzU+dP9VOhGbW8uwhkiIjA7FPaoHkacT1Mo6moyRVMZh8rVo6F2rDTeOCzN47pUTWhkc6frqPAv78JQ1Aqn7emJkgta/VX8KOMaA1T65AyOl9jY8rjom8eCZneUEvJWUZmYaVXyMxI0Cw4UfT3evy6DV21lduC+5UAXgFan2fb8+sWU3TkKFP3MRXUUS38tXLSvUxJo5/b+1E0fNuCxA/w96Lgca063Z7LbXDUW+jkY/CisFJr66qH9nQS5rf+Tr8hR4jbmOXNZfIySLSx1858MUaANNUSQx2hjihFzdrWtz7TTXRUpHDHWRuFf8AUOhvYcs2dtaz326XZt7CIAu0YySeCgnJJ6aqih7kppizthZTo1mlWfHokKXPjVYWiFtdjYarm3tum5fhNfX4elsVzyHLHpVbgCtNZD1J8zWvl6069ttq/DT5fMbzwWWqcjkZKenD4ykSrkoqGlVjFFHFQu6x0lRKxkIFze1+fe4DIrSTXMbaz2inkB/IV/ydV3YW9+tjY7BuUCWUKlqTMVDuxySXpVlFB0pJcns7dgWkmyEVVPT2WOnrklxO4KUPbiCZ1Uzxqf1Lc8Dke1JaGcUY/Kpx/PosS033ZT46WxSN8l4iJIWp/EBWh+ePt6Ysvsio8d8dnalJI2OiKvpRM5OrVpNRSyRyArcclSbe2ZLZyDokz/SHRlY8wRBx9VtqFTxMTUHD+FgR/PoPa+Dd+Dp3Ez1dTTKHE7Y+trJbLp1PM8Uh85QXsdIOk8Wtz7QuLuFTqU6fMoSf9noTW0uxbjIpRUSX8IlRRnyFRiv28elX1/1tkt6z02d3MKiLayOlTSUk8zSVWe0k+ONtR81Lilt+5q0vL+lQBdvdIbWS6YPMT4FagEmpp5eoHr/L5E3M3NlpsMUu27PpbeCNDuoosPqR5NJnFMDiSTjo3CIkSJHGixxxqqRxooRERAFVEVQFVVUWAHAHs7AAAA4DqEmZmYsxJYmpJ4k9dSRRzRvFNGksTjS8ciLJG6n6q6MCrA/0I9+IBFCMdbV2Rg6MQ4yCMEfn1yACgKoCqoAVQAAABYAAcAAe99aJJJJOeotd/wABZv8Agjf70ffutda0f8+6V/8AZJu+49R0HFbc4/8AJ62sfaDcgPopvy/48OpV9kP+nqcnf813/wCrMvWj/wDCDr3Z/bnzK+I/VHYWI/vBsHs75N9C9e74wP8AEMpif43s/enaW1Nt7mxH8Uwlbjc1jf4lhclPD9xR1NPVQ69cUiSBWAchRZLiJHFVZwCPkT10j5w3G82fkvnDdtum8PcLXa7u4gkoraZI4HdG0sGVtLKDQgg8CCOtvfoj+Tf/AC7Ozvnh/N3+Pm5en59u9ZfHnb3w6g6OrKXtbtqCp6cqO5fjtund+/t1U2UyXYE396ZzumjhyiJuZ8vQ0zU4iWJKVpIWMht9pJNuMTLpRFXS1T21UknJzQ5zjrFPfPe33L2fkD2Z5js95Eu6blLuJv1NvbkXItryOOGMqsP6Y8MlP0tDGtalqHqvDeH8qbrn44fypv5j/YHe/WKVvy/+LXy6291PsHtmm3P2FjcVUdbZfPfEoYfNYHZ8e46HZWZwO8trdq5OspajI4meuiiygVnjmp41gLGso022+kmj/wAbil0VqcZTyxUEGoJHAg9TBtXvJuvNHvN7V7Xy5u5XkfeNkkvbmyMcDN46puWpXl0NKrxSW6KwVwpKcCGNbXPlx/LW+CHxw7KwmyOqf5J/ffyp29ldj4zdVZ2H1b8iPkPSbew2ars/uXEVGzKyKs7MyMjZnHUOCpq6Rg4UwZGIaQQSbbnb21lMkUGwyToU1FlaagNSKdqOK4rx8+HUU8g+7vuXzXtFxuO8/eJ2vY7pLloFtb2xsS7oqRuJRS3XsZnKjHFD1Vbt74hfAP4LfEnoX5T/AD56p7X737F+WlduLcPUPxy2vvjLdb4Da3WtAlFW0mX3DuPC5bB7oyFZT4DcmIrmnjrmikkyVLCsDxiaocPx29vZ2VlfbhE80swJjiB0JpFBqZgpapqGUCmCMcesgH5/91/c7n3mjkb2q36w2raNhSOLcN4nhS4eS4aoKRxurxqC8ci0K1ARm1A6VAD/AMxT4O/Hzrn4+fGv53/DDI77f4xfJefKbbk2f2JPFldxdZdi4c5xJ9tSZ6lEsdbBPU7SzdKYppqiaKpw8zJUTxSL4kG5WCRW9nuFqZDZTahSQDUjqaFSQACDQ6ccATnqRvZL3R5u3nnDnX2p9yYbQc77Kqzi4swVjubd9FJPDPAgSxNUAAiRQVUjMP8Ak9/DfrH5g9rd50PY+zM72vVdP9Abp7S6+6VxW663r3Hdw9gYysoaHbmxNwdhULU1VtjGZqsqlpy0FVSVP7xnWURU04KTabFNwvJ4XQu0cEk6RA6fEdCoVCfJW1ZpQ+hHR39473O3/wBs+W+UJdj3SHbo9z3iLb73dZIVuWsrdlYyXEdu1RKyKCaMrLjTSrr0E/8AMj6n+NfTPyQj2b8YMlFPtVOudkZLsLbeO31T9pba637lyFJWT77612p2XTSTDfGG2oho1atkkeVayWeFyDEACTdY7OK5CWUmpNCs41K4RyoLIrriRVONXrUZpUyH7Acyc+c08jndPcCAjcDfTx2M725tJbqxVlFvdTWpA8B5u/tAA0hWHHq2H+TR0t/LP+bdbQ/HHtP4cZ/Md37C6f3T2Zvrueq7x7dxGD3ocX2Ltnb1JR0WzNo7+wOPws8OM37RRBoo0jYUDsyl5dXs/wCUbPZt4mbbb/Zw1wkbym48aQav1AFXw10haK4Fan4a+fWP/wB6rm/7wvs9by8/8te68EPKF7usO3WW0rt9lJJBrtZZSzTz20jSAtbOckkawAaDr3QfSX8t/wCZXSn8zLujqj4h5zp/H/Gf4g4XcnWeCz/dfbO7KzBdwJtP5V7rym/oqt99mHL01fBtTbEK43JLWUEbYdmWACpqRMm26y2Hetv5nvY9l8D6W0DRL40klH0zsXqSta6VGkgjt+Z6OOdOc/vCe0XOP3ceUOZ/dWHdZ+Y+bJLbcZoNvsYVlsDPssCWpX6asZUz3J8SMo5EwBbsTSHOzPih8EPhh8OPj18ofnjsPs/vzsn5V09XubqzpHZu7q/r3AYzYNNS4vKJm8xmMRldu5+oMm3tw42tkqI6pkaTJ0sEcGkS1JI02zatm2rbt3321nuLm7LNb2qt4SeGhA1SSAF6sGDLp4ggU4t0Mdz90/fT3j93+ffbL2L33bNh5e5XYW2571eQJdyvdFnTw445I5oh+rFIgUqDSJ3LVonQ+fBb4gfyovl387Mns/qPCdmdndG1XxHz3aeb6t7Lye+9m1/Vfa1L2L07habG0O9tn7q25nd1Ciwe7a+mqYHnrMfBU6mjqq0NE9Ov5W2blfeuY7i2hiuJtt+jM3h3B0MkviICoaJlLBQxHCmeLYPQS97/AHg+9Z7RexNtvHNd7tu188JzdFtcG67alrcLfWLWe4SM7W1xBNFBqlt42VgqSMtAY4qMHKV8rPi18YPgL8O9gdbdxbFpex/5jPeGNg37kPJvHfeLx/xp2DlvHHQ0Vdgdsbrxu09xbkjkoJaaFa+lq0lyDVkh10lLTCpDm77bZbFs9tZ3lvr5luCJ3qWAtYjTShAIVpXoagg6amvBC82+0Xun7pe//vLzBzLybvz7b93DY5TYR0t7V33m6jyzLLPA9xDCQ4ZjG6ER+EopJI5S5j5P/wAub4QdDdgYfaHW38n7vD5K4LI7Px+5arffWnf3dlHgcTlqzNbgxc+0quLKdrSTtlqCjw8FZIynQYa+IAXB9jTmXY9l2W/itbD28uL+FohIZoZrugYsy6DoWUVAUHiDkY8zhz7UfeV99ufuX7zeeZfvmbDyvfxXr2qWG6bTtjSyRrHDILhTHYU8NmkZB56o2+XRP/hD1B/Kj+RXxu+UHYe5/gdu2k3f8HukMFvPtmbIfIHuWGo7R3Jj9h9j5zc0uCo8L2VRYrbM2TyfVNaREYvt4Wro1RQkZHsj5TtOVd52Dd7275YDXW3WSSu4uZ/8Ybw5GY0GkRajHWgDAauGMzj7586/e/8AbT3O9puWto+8JZPs3P2/S2OziPaNtIsIXu7KKAStLYtJOETcI811N4bEmrdAL/L5+H3wu/mCfJb5Y7/2n0zvHbHSXUHX+xt0dS/D2g7Wr03hvnP5DbM2OzGNqOz90biXJR4mv3jtKpLSz5iijpZ9xUavVQU8JAJOXNj2rmzed1ngsTDbW9v48O1xTVeVlAXR48q4jZx3E6SpkUAgA9Sr95D3u99vu1+1Pszy7vHPNjdc+73ud3abzztJt6G2tIUnDxOthBDoMiW1wtFWCQutrKRG7uCSqfzRukPjn0xVdUw9RfFT5N/E/fm4U3PUdg7C7rydTnthUtLj56GDEL1tu2uq91S74E000zTVtPnJYYIY40kp1mkLKGeZ7ewtrqBLXZL/AG+4ZGaa3vKFB3KF+nYqsskY7gzvxNAvAkzv9zv3A90efI+cpOdvePlLnPly1Nuu2bjsEYhvGZ1cy/XWyLbi0oAumNrcMzFirlFAIm/yPpHj7q7OKEgnAbSB/wBY5PLex17Miu+7p/zyf9ZE6xe/vfP+VI9kv+lpf/8AVi363putCWwNGT9TBGf9iV95H9cJuhJ9+691737r3Xvfuvde9+691737r3RUd+09O3ZVVFVzJT0ctVhXq6iS/jhpmpqV6iRwASVEangcn3U0630Jm04F3dvHKb5aNxiMcgw+3BKpUyGKLx1NYkbAGNAJHAFgQ0hH1U22M58uveXTl2fuqgxGEq8LqE+UzFLJTx0yOL01NKCklZVWuY4gLhAeZG4HAYjxPl1rouu14lfPYy+Lq80IZjULi6JUaaskp42kgRmktHHTpOqtK7elUU+/Hy690OdXS1GBOQ7I3saaTNQ04pcFhKaQy0eLaRZEpaVZyV+7rJGkYu6gKil2FzYr6ma9e6BbN7b3PBBT5zK0VVMM8j5CWqjimmaGeqdpDHXKiFqWZ0YOgPGggXupA91voWqdqzf1Xi8DjqGsx/X2DFGa6oqoJKWTOPQJGYKPxtpPg8qLdATxd3N9Cj3Wug/7Vx/8P3hkJAhWLIUtNkYjawZjF9vOV/4LNTn/AFr+9EcetjoSuwatstS9eYaBgWzmUxldIt+fDDFTkMfp6Sao/wCHF/x7t1roaGRCwk0KZUVgr6AzqD9VVragG/p7917r0caIWcIqvJYyMPqzAW5txce/V6sWYgKWJUcOmp8NRRCR4V8J80tWuppJYqeaYlqmSmhdjHTvOSSxQDkm31N9g0NerwvokB018qfb11A0VJC1ZOLyPxCb2d0/sqqH9JP1J/2Puxqxp0pcPPIII/hGT6A+Zr1G/i0l7+D/AHZr/Qbfp06L2vqt/a+t+LW970fPp36JaU8Xypx/n/sf5eiwVmVyvY+Rp8xmI/tsJTzyPt/CMG1VbB9MVfkIjcGMAXjX6XJNyOSRJrvis0q0twaop/EfU/IdS5bWFnyrayWVk/ibm6gXVyOCCmY4z6+p/wCK6ErG4wo0VPCplqZCCW4AbXe/NvTGluB+PZsqBft6C13eBg8rnTCP9X7T0s66so9q45kWRFyEyKpcL5TEfoqqACzSAsQq/W/J92JVRU9B+3gn3q6DMp+lU1A4V+35evQbRw5LcU4oKBJSzF3qCGJbSxN3rKz6BCzXNuGbgX+ntkkuABw6FryWm1xm5uWFAAF+3+gv+qny6E/BbAxeOSObJJFlK5bH1ofsYSNNlhpnusmkj9UlyfwB9Pd1jApXJ6CG5cyXl2zJas0Nv8j3H7WHD7B/PpfKqooVVCqoCqqgBVAFgABYAAe3Og4SSSSc9d+/da697917pEZzC4ClyFPnlxlJBmNElO2SgjEVT9kql54maPSJPISFuwJF7A+6CJNfiae8Dj/scPz6P9vv9ymtn203btY1DiJjVdfAGh4U49MtPC9fJJKHIgeXU8tgPWRbxRva+lLW4+g9vY4DowlkFqippBkAoF/yn7en6lpYoDppke7g65FBd3APA1Lcn68X9+oM16LZ5mkBMzCg4A0A6bs/svG7npPBkMf4py6yw5KFYYK+inQ/tzxzgB30/Qo2pWXgj2zLFHKKEd3qOlG28wXW0XHiWt1VODRNUowPEEcB9oyD0Do3BnuvM0u3dzrFk6GSJaqHIKrt56LymFayNmjMnkhI0zREsY7ggkFSUwmeB9Eo1J69D0bbtvNO3nddo1Q3AbQ8R8npXSc0zxU4r9oPQu0x2xm4CzwxBvC1Sk9HKFk8OnV5ImRmjdWuLH8/ke1lVamk4pX/AIroDTDeNvkARz8WgrIKivoaio6jYpqjEVsUWL81VBUan/hv7ZknjJF5HsUgp5Iw1/JcK30b68aKBaUx8h59PXixXsDvd6UkXHi5oD6DzYH04jy6FIfQXFv8P6f4cce99BDr3v3Xuve/de6iV3/AWb/gjf70ffuvda0H8+8H/ZKe+zY2/hW3Of8Ayedre0O5f7hTfl/x4dSr7If9PU5O/wCeh/8AqzL1pBfCDsLZ/UfzK+I/a/YWX/u/sHrH5N9C9hb4z38PymW/gmz9l9pbU3JubL/wvCUWSzWS/huFxs8329HTVFVNo0RRvIVUhuF1juInc0VXBJ+QPXSPnDbrzeOS+cNp26HxNwutru7eCOqrqkkgdEXUxVV1MwFSQBxJA62hd0fzT/gzW9t/z/t3YXvmX+G/NP42dKbF+LOVg627lpJ+xt7bO+HHZHVubx0KP1/DXbHlxfYOeo6JarPpiKeQy+eKV6dHmVdJeWpO7EydssYVMHPYRThjJ8+sctv9pefhtP3dLSXl4eJsW63Nxuyme2Ihik3KCdW/tqS6oUZqR6zjSRqIHSH7y/nMdM/LX+SF2L8eO49+TUHzhr4OpdnVm2ptqb5yD9tQ9bdy9R7kbtCbelDtiq2Rj8jm9j7dnmyEOQytNUvkqCoEUWiakSRHJuKTbRLbTv8A41UKOJLAFTqJzmmDU5Ir5gdCTlf2J3/kz7we080bFtob29Q3M4lEkK/TGe1uY/pxEZBKyrNIApRCoVlqahiAl/nM/wA2rL9x/KTYW5v5fXzU77xPTFD0HtbBbmpurd6d+dGbefs6m7E7RyGanrNpZOPr6fI5ltqZTCrJkRRSpNAsUInY05jjTbxujS3CPYXkgh8Oh0llFat5YzSnQz+7x7G22xcm7nZ+6Xt5tcm/tukkkJvYbK8f6cwW6oBKvjhU8RZKJqFDU6e6pgbL+YPwP+dvw2+OXxb/AJhXZvavx87V+JiZTb3V3yC2rs3Kdobfz/X9bQ42gTAbiwuExm4d0Q1z4XbWJoHVKQp5cZTVIqQrzwKVC4try1tLK+meJ4dQimA1poNDpZAQ1RQBaVoAPn0cXXt/7p+1/uHzdzx7SbJY7vse/aZb7aZ5ltpEnBZtcbu0cRUPJI+WrR2XTUK3QK/zFPnF8fOxvj58a/gh8MMdvtPjF8aJ8puSTeHYkEWK3F2b2LmDnHn3LJgaUxR0UEFTu3N1Rlmhp5panMTKlPBFGvlLdyv0lt7Pb7USCyh1GshGp3Y1LEAkACp054EjHUheyXtdzds3OHOvut7kzWh533pVgFvZktHbW6aKR+IeJIiiWgJAEaksxODW/wArr+YB8eejPijj+ltxfIvc/wAM+4NkfKGl+QFV2Pieldx9zbO772NT7SO3p+m+wMFsmvxuerMZk4Z5o2jqp6WCjkp6Oqp6kTK4ittW4w2trLAb57a5FyLgSqhdXVU0iFgrqSC1TQ9ueIOQEvfb2b505t9wJeaLLkm35o5au+Xzsy2Ml9FZTbfOZfEF7byTq0auhANVDFgZEZaEVaf5vny0+E/yc6t6dPw03ftrbOPo+0O1Ow+0ukavpze2yd+VO/8Af09NBP2dUbxlwdZsDI0GWpcMzS46kysc0Qq4JGjkfyQ0JZzFdbRdpZTbSgiQvK8sBQq4dytXLAshVggoFbtxjJCiX7rntt7r8gcycz/66O13E8z7faWO3bst7BPbi2twSLUQCRbhWQvh2jIOlgCBRpAy/kXfLDoD4d/LTsPsz5G7+/0dbIzvx13ZsTFZv+629d3fdbryfZPUW4KHFfw3Ym3Nz5eDz4jbFdN55KdKZfBoaQO8avTk/dLDaN2uLncJ/DhaBkDaWbuLxkCigngD8uhr98T2x5491/a7YeXeQdk+v3mHfoL2SHxreCkKWl7Ez67mWFDR5kGkMWNagUBIn/yzPld0F8ffiZ/NN6z7e37/AHR3v8jvjxT7F6Zwn91t6Z7++W6o+tfkPgHxf8S2xtzNYjb1svvrFQ+fK1FDTf5Vq8miKZo0fLm7bft+0c0215caJ7m28OFdLHU2iYUqoIGWHGgz9vRp94f2v565890fuy8x8qbH9Xs3L2/m+3ibxreL6eD6zapdeiaWN5ey2lOmJXbtpSrKCL2zPlf8EPmf8OPj18Xvnjvzs/oPsn4qU9Xtnqzu7Zu0a/sLAZPYNTS4vFphMxh8RitxZ+nMe3tvY2ikp46VUWTGUs8c+ky0wRpue1bztW3bRvt1Pb3NoWW3ulXxU8NyDpkjBD1UKFXTwABrxXol3P2s99PZz3f599zfYvYts37l7mhhc7nst5OlpKl0Gd/EjkkkhiP6ssjhixNJXQrWj9Dz8FPmB/Kl+Ivzvy+8OpM12Z1f0VR/EfOdV5jtLszF763lkO1+16rsTp3Nw5ag2Xs7bO5c7tWOuwe1K6epmkpqGhmqldY6WjUQLUL+Vt55X2XmO4uYZp4dt+iMOu4Bdnl8RCW0xqxUMFrxpjgvDoJ++Hs/96v3c9iLXZ+a7Lbd055fm6LdYdr217W3SxsVtNwjKNc3E0MU5WWeNVUM7qtCZJDqKFr+QvzE+On8wj4N4DKfJ/smj2F/MO+P1TlcVsncrde7sqsd8gdgzzR5NdvZjKdf7MyO3Nt1k61Ui0ormpIKXL0pmVoqfJVbxEO57tacwbEk263VOZ7Q6I5Ch/xmEmoRii6VeMk6S2D61kYpLntt7Oe5P3effXcLX2u5ZfcPu7cwqkt9bfV26vtN0Bo8aNLu5SaZRpGrww7PC+khngjDWk/MD5v/AAF+UHZmC39sf+cf8ofjDicRsbGbPqNgdJ7F+Vm3dq5fI0G4NzZqXd+QosRs/BU0u4MhTbghopZWhZ2psfApchVVRjzJv2zbzfRXO3+4dxYwrEIzDFDdEFgzHX2tGKkMBwrjj5DGT2W9ivvCe1nLF9y/vn3K+VOa7ua/e9XcN9uthmnjR4oIhbo0lzKwhRoS4GoDVI5pkk1I/wAu75YfHvoL41fzY+t+0+zanEbt+SHRtRsjpGKs2tvnPVfYu4l2D8jMCkdVksBtvL0G3qmsye+sSHnzE1BDqrCxfTFM0YI5P3rbdq2Hm+z3C4EV1d2QigQKxDP4c6lQVVgtC6jJAzxwes0fvHez3uT7i+6P3O+Z+UuVEm2flfmBb/fzHPaQrZQ/WbNKSqTTxvMqpaTUWBZGolKVZAxff5bXY3xN6z3z2Bmvkb218i+ht3Vm2qDH9OdzfH6ryNJV9fZf+Iioz9buKDCS12Vz1LlaWKnp/sJMXX0MtL9yJAk7U0sQW2STaoryV90vL22fw6W1xYkBo5CfjbKvp0jSQh1EMwxhhLn3oOV/eXmzl7lmw9r+TOV+Y9kS7aTfNi5lVGW8j0aYVhMoSOFo2LN4gmjkD+HSqCRWOb/Nj/mCdE/IT43fH34xdU9qb4+UG5Ord6129d4fJvsXYrbCzu4FTE7kw+PwVBi6jDbZrmhrafcqCreTHQM6YejaSSonaaUnvOHMtruW17PsUFzJfS2hdpNzuE0PJqOFjBZnCUPdr7joQ1J1HqIPuVfdo9xfbL3W9y/dvnLk/b+Udq3fb02+x5S2u7+shhrJBK8zyLLOlUMB0AStQzyhVRAq9Bd/JLWM9z9mtKJGRMBtQlI7nUDk8qCSAQSEBv7EHsuCd+3QDj9J/wBZE6i/+9+0jkj2RLf9HPcP+rFv1vMda5L+H4THw5JwsMqwwU1dwELOl40qQCTET9NZshJF7E+8kigcakGeJH+brhSO4Ejh5j0/2Ohk9tde697917r3v3Xuve/de697917ot27cAdx9rDD+QwR1lJQz1Uy/rSlp6NmqPFcECZ0i0IfoGN/x7qRnj1voRN07uwvX+Jp8NiYqd8mlOlPi8TESy06EWWprQhMojuS1jeSdzx9WYb+zr329BFTbA3VuCjzO5syaiGpekqK6miqk/wByOUqkTXGppiF+ypBGpEakBraQqgc+/fOnXupXTb0i7kr56iaOJo8HNJTmV1jUp9xA9U2pyAPFCgJ/otyeB79jj17pXpWL2VvenjiRqjaG1GapZ2U/b5LJkFYXe66ZEaQXRGveFGaw8lvfuPWuhx97691737r3QU9p7Oq9x0FJkMVCKjJ4vyq1MCqyVtBMFaWKIsQrTwSIHRTbUCwBuQD7r3SW2RhNyZTPYPKZ/GVONoNo4cY6iFZFJDNWVCiaOKRYpDrZ1WYl2A0AooHPvX5de6H76j6fX8H/AIkf19769137917riwJFgFN+Dq+lv9b8+/dbBoa9RpoFqNMMsV0VbiZSEKPcWWNeSLgcn/Ye9gkcD04khjq6t3V+H5fPrH/DKT/jmfr9NTW0/wCo+v6b8/6/vetvXpz6ub1H7B0CmHwzB4YI4vJUkAalHARgFKJcftwoLCw/1/bSJpHD8+h9fX40vKzaYhmn86n1J6XVW9FtihZh4zXvGQ0wAdg3BKx39QCn+n1bj6+3MAEnh0HIBPu9yAai2Bwvl+fQfY7F5TeGTlLSvHSxuDVVTAsKNGUftU4a6tWzKxvc8A3PAALBq5/1Y6E11d2ex2aBUBlI7EH4jXi3og/1ZqQOONxWPxFOtLj6WKnjVUViijyzFBYSTy28k0n+1MSfboAUUA6j66vLm9lMtzMzvXFeAr5AcAPkOnD3vpN1737r3XvfuvdeJABJNgOSTwAB9ST7917oB90bwoabKCXKSV7RMGfH4qgoKrIVDUcTaUq6qKABaWKokXUCxuRb8e2JLiOIqHqWOQBxp/LqQ9n2S5ltCtnHHrrSSaV1RQx/Cpb4iB11R9u7GpqcxSPkIp40YSCuw09FSxnn0KraqcBf635+v9B7bW/hJo2pftA/yE9WueSOZJZPEWOIxk1Hhyq7H5+vTtj+wqfMsyYGaKqKAM0CNacIR6WFPGmqOJgPTwefb6TRS4iIJ6RXPLD2ADblEyA4DHhX7SaEjp+GeysId6qmdI10soM/icqbkC1S/Or6829u1HE9FzbbZvpEMoLEEGgrw/0o8ukb2JVQ7h25SsUp46mjzWO11MrwLJSUVVOIcgTOmtUjaFgWsdJIF/oPaa5VWVfTVQn0B6PeVoZNq3aWjMYZIHogrRmUVTGKmvD86dIwSUmKxdTVYquo8hBSqkMNKKpC8hUFI6ani1GUjUdUpAAsD7oXjjQmJgwHAV4/5ft6EGie8vIory3kilclmfSaCuSzHh/pehL6dys+Rw2UgrQJq3G5SSB65ogktRBVotdDEzEeR0ozMYluT6UA/Hv1pIzq4c1cHj9vQT56so7TcLSSDtt5oQwjBqAV7CacAWoCfmehf9q+gP1737r3XvfuvdRqsaqeQfW6kf7wffuvdUXfzg/jl2L8gvib3J1z1bhIs7vnc+MwkOAxk+QocVBVz0W79v5SrSTI5OeloaYR4+hmcGR1DFdIuSAUd9E89tJHGtXNKDh5g+f2dD72v37beWOfeXN93iYx7bbSu0rqpYgGJ1FFUEnLDgOtI6f+UB89cbJ4avqTHRyKSGC762dKAQLH1R5h1+v+PsPtt18dVLc/tX/oLrOuP7yPtOla7zcf9k0//QHWZP5TXzjiVjJ1ZjlFxyd6bUt/S3GUPPtPJtt8FNben+2T/oLo0g+837RLx3q5/wCyWf8A6A6dof5UXzeAF+rqAcA/8fjtc3BFuLZMn8e2X2jcjSlqf96T/oLoyi+9N7NrWu+XP/ZLP/0B05w/yrPmunqbrHHgA8/7/DbP+H/Vx/oPaZtk3XT/ALiHh/En/QXRnF97D2WWld9uuP8AyiT/APQHU6D+V38zF1X62x9lILH+9u3SB/QXFdYk+0b7HuxpSzP+9R/9B9G0X3tvZNQNW+3f/ZJcf9AdOsP8r35lhST1tQC54vuvb4P+2Ndf2nflve2NRY/8bj/6D6MoPvh+xaE6uYLv/sjuP+gOnKL+WB8yEALdcUA4H/MVYA/g/wBK0j2jflbfm4WB41+OP/oPo1i++d7CqADzDef9kdx/0B04J/LL+YMZu/XdAATYf7+nAm5seOKz6+0T8ocxGlNv/wCNx/8AQfRnD99X2ABFeYrz/siuf+gOp0X8tH5eKVJ69oLcH/j58J/qQP8Ala9pX5L5mY1G2/8AVSL/AKD6NIvvv/d8QCvMV7/2RXH/AEB1PT+Wx8uALHr+gv8AX/j5sL/h/Sp9o35F5pIxtn/VSL/rZ0ZJ9+r7uyAauY77/shuf+gOu2/lt/LWLl9g0ABJX/j5cMeSDxxUf4e07ch81mhG1f8AVWH/AK2dGUP38fu5VX/kSX/r/uDc/wDQHXFf5cHyxFv9+HQcE/8AMSYj8i3/AB3v7YPt/wA2nI2r/qrD/wBbOjKL7/H3b0qDzJuH/ZBc/wDQHWX/AIbh+WHH+/Ex/PN/7x4m3+x/e9tv7fc3kY2j/qrD/wBbOl8X94B92pK6uZNw/wCyC5/6A64j+XL8rBIqf3Hx2o3YW3HiiCEF2/3b+B7TH285wLADaMnh+rD/ANbOjSP+8I+7NGutuZNx0jj/ALr7n/oDrk38uP5W3v8A3HxvPIH948Xc/ngeXk+6N7cc6E42b/qtB/1t6Ww/3i33X1pXmXc/+5dc/wDQHXf/AA3D8rgyqdkYwF/0A7jxnq/rpHkubfn2ll9uec1oTsuP+a0H/W3o1i/vHfutoATzLuZAOabdc/8AQPXKX+W18sFUO2yMWqA2LnceN0r+PUdRt9PdB7bc6yfBslf+b1v/ANbejCH+8s+6nESW5m3T8tuuf+gerd/5S/wx7y6M7Q39meytu4rGQbiwG36bbpps5j8oauux+QrKmogeKklZoz9vUAjVwTcfUW9yX7Xcn8w8v7tuF1vO3mC3e38NT4kbEtrU0pG7EYHE9c/P7wv70/s594jlb2y27203a7ubra7+6mvFubWa3CpNFEiFTIoDdyEEDh1tfbLxdU2LTI5akkTwYytj+xqBJpYR05AlelkbQiJKALKLsSDa/udCwRAkRGWGeuV8kixlkVqggkkf6s/5Ohd27k67IUzpkqD7CspVpRIquHhlFRSxzo8RvqWwaxU8gj2R2d3PcS3sVxAEkik0gg1VlIqrA/Yellxbxwx2skUupJE1UIoVINCD+fSh9r+kvXvfuvde9+691737r3QE71xEtR2Xt5YcjW4g5vFy0yZLHyGGqhqKNasmOKRWQnyoyBhflTb+nvRr69b6D6pXP9a7r+5qkpsnO6mdampi80eWpWca5Ip5lkqKOujcWZg2pW+pdG5917o1GLyNPl8bQ5SlJ+3r6WGqiDW1Ks0YfQ9rjWhNjbi497610zT7J2lU1H3Mu38YZblm0U6wxyMxLM0sEOiCZnLHUWUlr8+9U63Xp9oqChxsP22OoqSgpwzOKeipoaWHW1tT+KBI01NYXNrm3vfWupfv3Xuve/de697917r3v3Xuve/de697917rgzEMv00m4+jFtR/SBYEAWBuT791YAEH165G/H1+vNv8Aif8AD37qvXfv3XukoIaTb1HJMWDVMiqC5F2PFgi3/Sosf9f3vj9nRuZJ91uFSlIQeH+U/PoNpY67dWUjpKRmRGYu81rxUtMps1S4/N72jU/qc3/xDbEuaAY6FqNb7NZNNOAWpQL5s38I/wAp8h0MmLxlJiKKCgoo9EMK2LHmSaQ/5yeZ/rJNK3LH/bWFh7sBQUHQEvLua+uJLm4asjHy4AeQA8gPLpw976Tde9+691737r3XvfuvddMoZSrC6sCpH9QRYj/Yj37rYJBBByOg5ym2pklkangmqFkkaRJoyJJlQ2Pgm1OkhUEC1rgj+nveAPn5noUWe6oyIssgUgUKnAr6jBFekZkNkZrKlUgoKCkHku9VWQ+SR4l/Si08QOkhjzqPI9sSxeJSir9p9P59HtrzFYWdTJcyvjCRmgB9Sx/ydRpOnqajV8s0mWmq4EeRqXb1SuFnnuDrhpmjlDhX+pBkBINgL2HtkWcanXU6h/CAP8NenV56uJytkEgW3Y0D3S+KF9C1RTH2dI6bb81dLHPR4FIFHqV6nI1uUyC2a1pKqtmdUqFP10oSDx+PbYgJaqx0+dSf9jo/Tco4EeO43MufMIiRp+SoB2/aelHJt/M1VN9rUZVqOGaHxyQOscpkisLh6SGIyyLcf0DX9vmGRloZCFIzXoqTc9vhl8aKyDyK1QwJFD5dxNAestJ1yjiKRaDLZXSVdw4p8LTSkX4Rp2+7AIHNrfX3VbdAFrU/y6rPzUyl1NzBDXApqlYfbTt6FfY2AbBY2s82PTGVGQyVRVtRpUCrMFOoWCkiepDMJXEEQYm5sWI9vRoE1ELQk9AvmLchuN3AUuTLHFEqCQrpqeLEL5Cpp+XS19u9EHXvfuvde9+6910w1KR/X37r3SKz20qTNIyzwq4P4Kg/7AD6e/de6B/JdIbYLrNVwUcIlcqrzeNFaQqz6dT2UMVQn/G3vwXVWgr1UsFyxoOg+rOpdn1E8ka47XTRSpBBMsC+Kolcp5JF5DGBLgFrWAufp7IL6WRrh1VlEUfEedfM+mPLpdB4fhoVqXf0Hl5dPcXQ+CjCxikpjGAWik8SchvpG/1YqBe359vWt8QyxSCoIqp41889emgUqZVNDwYdN1b0fgpDHDFQU3llIX7dFDMHb6aiFt+nnn/W9vtcNLKEVc1pQeR/y9bt7QBDNIaRDIPr050Xx5wGgRmhp3ZW/cbwAesjkepeQv4PswjiCCrGrdNSmprwXyHToPj/ALZB0ijpmZWswCIdJtfn8fm3u3VAhoGKmlOuf+y+7dXkUNOLfkRpwf62tz79xweqgZAI65t8edtyKvkx9M1gSbIB9RzpItyfeqDrWoqx0HHUc/HTbJsUpUQc3GhGP9Pq19JN/e+r+KQCCoJ6xn457fBvHTwgjkK0S/4WuwBvc+/dXEqkUaP9nTdlfj3hxSuY8ZBJP+3JF40GgtG1mVmCkqCG/PvTCo7ePSmz8AzLrakeQa8aEfz6ZovjmlQiaMLS0+tTqNW8SeJla1mSNZWYn6i1xb3U6/ID8+l7y7ZEx1TF6cAgrWv20p06QfGHEPGorzCGJ9cdBAscYFzwJpVeQ3/qAp/p79pYjuan2dI5NxgVybe1HyMhqf2Cg6cW+NO0YEeanw9NJVRQymEyiR9cgQ6Va7G4YgD6X9+K0BKjvAxXpKLuWVljkkIiZhqpQYr/AJOgU2l1vhNy/cCuoIEljd0dBFFBFFLET5IBEovGEsfqSeOTfj2j225a6gDyA6/Py4eg4U6H298tR7WYxDmMgEHiSD51869S9y9Nbdp5cVJSUiq8q1gjkSMPDHNAYmCkkHRqb/YW9rpURwMdFtht51XCzAaBQkH0Nc/Ppcba6Z2nuaklp3o6VKyOJVyVIAvkppGFoqiIMo80Dup0sPpcqefaCPxrW5BqDEfU9Em67ZJYlTQ+Cx/TemD6g+hHmOsmM6uXYuViSqxkSxyRVQwOTR42gjrFVgizhj5NcEd2UEavp9fZq1zaoiSPMqxn+L/VnpAV8dKJWtR4ij06FjE5ieLC1FCBWPCska12arSscGPpG8Zlph5HNWZ9ILsG/UtgObD2T7jvVrHFN4ZIAWmsigFcV9TQcBxPWlsJp54UijBkc0CLk4+zAr5+Q6lbO37io8tl4ci81EmVrvNj6iW5o44UQQwwS24pmaJVIcjQSSCRbkC8tb/ZW13uKXcnhpPKHjJOBilCPL7eHrToX75sF09nYtbAO0EemQD4ieJI9c+XHoclYMoZSCGAIINwQfoQRwQR9D7kwEEAg46AvyPHz6797691737r3XvfuvdBn2ZA9NQ4Xc8KkybVzdHkJrfnHzSJT1oP5KhWUkf0B96+fn17/B009xwUtXtXH5FWRngydK1JMOdcNdDKsiqfysqBW/5BHvxPDr3Ss64JOx9uX/5USB/rConC/wDJo9+HWz0tve+tde9+691737r3Xvfuvde9+691737r3Xvfuvde9+6911zccf65/p7917rxFwR/X/G3+8j6e/de6xaXv9eL6L8X0Wvqtb66+P8AW59+6tUemf8AV/KnQX7s+81t5dfisb6bf5vjzaf+blvrbnT9Pfm4CnDoYbL9PpHh/H/l8vy/y9P+xPsv4XL4f+Lh5z/E9Vtfk5+38f5+z8P+a/2P5v7qvD59FvMX1H1a66/S6f0vSn4q/wBKvH8vKnS3926D/Xvfuvde9+691737r3Xvfuvde9+691737r3Xvfuvde9+690h67+B/wAVbR955PX95/DdH2/n8h8nmt6/ur31+P1/159+HHHQgt/3j9INWjTjR4tdVKYp/R9K49MdKHF/wax/hn2uvnyaLfc/UavN5P8AKL3+ur8+/efz6Lbv66o+r108q/D+Xl07+/dIeve/de697917r3v3Xuve/de697917r3v3XukTunw/wAQwv8AELfwzXPr1avF9xeO33NuPDo/r/j7V2/wTU+Ogp/sdJLj44tXw/PhX59Z4/tvI/8AwF/4DPo8Xg/4A35/zHp8P9b8+0rfu76g6/D+o8POr+GueOOPV1+u8Lt1+Drxp9aYpTPDh1wqb+aH7e2jw/5d4reC39nxaf8Ad3j/AFaeP9j7D154f7w/xGlKd3pX5fP1p0axa/pR4/8AaeXr+fULG+P7iuvo/iOs/r1+PRxb7XT/AM2bf4fW/PtbtvxSa/7ep4+ny6W3OnwrWlfpNIpTjX5/n0/D7n/dt/p/un/Mf4atH5/1/Zpnz49Jv0KfpU/23H+fUqHTqj0fr1DV9babeu/4+n+xv790y+qjV4eXU5vobWtfnV/qf7X0/NveumBxFfioesvHP1/xt/qf7P8Asbf7x79031x/236fx/vF/wDG9vfut/4euha/P+82/p6fr/vHv3VTwx0kc7995o/+BP1X7D7LyafLxbXo/wB3eS19Xp0/4X96bT59H22/S+G1NHn4vieny/o09M16VlL9z9rD954/uvEvn8N9Hk0jVpv/AI/7C/09+HAV49EU/g+M/g18LVjVxp8+pI+g+v8Asfr/ALH/AB976YPE166/tD9X0/w0/wCx/N/futjgPXy9eijbQ+w/i25PtvJb+9GZ+3/V4P4f9/Lf7nV/uz7jVpt6tNvx7K9s06Xp8Os6afw1xX59Tlvf1X0O1eNT/cOLX669A+H5aaV/z9KLcdvLTaf0eWp8Hit47+CPyeO3H+cte/8Aj7NTXV8s06IbKmiSvx6Rqrx446ZMB/E/4/g/4F9x/FPvk8+jX9r/AAfyD77+IX58X9fxe1vVb2mudPhHVSte37elm4fTfu67+u0/TaccNWv8Oj5/5Pl0NHY38F/g8X8Z+7v98v8ADf4Z5P4h934z/wABtHr/AM3fyX9Gj6829hreddLfTp8TxD4dfhpQaq1/yfLqOrHVql0/Bp76/binz6BKX7P+I4L7j73+DeWi833Xl8f2Xjb7z9XH3Xlvr1/u/XT7BF99T+9P92/i/uvxF01po/Omafb+fl0LbDR+7G/dvg/vTS2vT/aflXzp6Y6GH/ft+NfN/BPNen1fc6ft/F4l+18Gr93/AIC/1/H+PsUw/uqh1eDr8VNGnw6UqPz4f7PQVf8AedFr4+nS2rVr40/z8f5dCfSf5iL9Gnxp49F9Pj0jRa/H0+lvxb2PW01Oj4fl/k6Io9VO7j/P8+pHuvTvXvfuvde9+6902Zv+HfwfKfxbR/DPsKr7/XbT9p4X8/1/teO9vze1uffuvdFn3V/Hv7h7G+81fwu1V4fL5PvP92fwP+IX/b1/wm+m39q9+be658v9Xp1v7eh+2H4P7m7b+3v4v4TS2v8AXXo/dvb8+XV7t1rpW+/de697917r3v3Xuve/de697917r3v3Xuve/de697917r3v3Xuve/de697917r/2Q==">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="9163050"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1246,8 +1628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1641,8 +2023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2084,8 +2466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2461,10 +2843,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L45"/>
+  <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24:B25"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2624,13 +3006,13 @@
       <c r="H19" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="I19" s="28" t="s">
+      <c r="I19" s="26" t="s">
         <v>101</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="K19" s="28" t="s">
+      <c r="K19" s="26" t="s">
         <v>103</v>
       </c>
       <c r="L19" s="1" t="s">
@@ -2647,7 +3029,7 @@
       <c r="E22" s="12"/>
       <c r="F22" s="12"/>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" ht="15.75" thickBot="1">
       <c r="A23" s="12" t="s">
         <v>42</v>
       </c>
@@ -2667,258 +3049,335 @@
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="41.25" customHeight="1">
-      <c r="A24" s="47"/>
-      <c r="B24" s="49"/>
-      <c r="C24" s="49"/>
-      <c r="D24" s="49"/>
-      <c r="E24" s="49"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="45"/>
-    </row>
-    <row r="25" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A25" s="48"/>
-      <c r="B25" s="50"/>
-      <c r="C25" s="50"/>
-      <c r="D25" s="50"/>
-      <c r="E25" s="50"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="46"/>
-      <c r="K25" s="3"/>
-    </row>
-    <row r="26" spans="1:12" ht="26.45" customHeight="1">
-      <c r="A26" s="52"/>
-      <c r="B26" s="55"/>
-      <c r="C26" s="55"/>
-      <c r="D26" s="55"/>
-      <c r="E26" s="55"/>
-      <c r="F26" s="22"/>
-      <c r="G26" s="58"/>
-    </row>
-    <row r="27" spans="1:12">
-      <c r="A27" s="53"/>
-      <c r="B27" s="56"/>
-      <c r="C27" s="56"/>
-      <c r="D27" s="56"/>
-      <c r="E27" s="56"/>
-      <c r="F27" s="22"/>
-      <c r="G27" s="59"/>
-    </row>
-    <row r="28" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A28" s="54"/>
-      <c r="B28" s="57"/>
-      <c r="C28" s="57"/>
-      <c r="D28" s="57"/>
-      <c r="E28" s="57"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="60"/>
-    </row>
-    <row r="29" spans="1:12" ht="26.45" customHeight="1" thickBot="1">
-      <c r="A29" s="61"/>
-      <c r="B29" s="62"/>
-      <c r="C29" s="62"/>
-      <c r="D29" s="62"/>
-      <c r="E29" s="62"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="51"/>
-    </row>
-    <row r="30" spans="1:12">
-      <c r="A30" s="47"/>
-      <c r="B30" s="49"/>
-      <c r="C30" s="49"/>
-      <c r="D30" s="49"/>
-      <c r="E30" s="49"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="45"/>
-      <c r="H30" s="14"/>
+    <row r="24" spans="1:12" ht="30.75" customHeight="1">
+      <c r="A24" s="68">
+        <v>1</v>
+      </c>
+      <c r="B24" s="70">
+        <v>126</v>
+      </c>
+      <c r="C24" s="70">
+        <v>4</v>
+      </c>
+      <c r="D24" s="70" t="s">
+        <v>179</v>
+      </c>
+      <c r="E24" s="70" t="s">
+        <v>90</v>
+      </c>
+      <c r="F24" s="66" t="s">
+        <v>105</v>
+      </c>
+      <c r="G24" s="72"/>
+    </row>
+    <row r="25" spans="1:12" ht="26.45" customHeight="1" thickBot="1">
+      <c r="A25" s="69"/>
+      <c r="B25" s="71"/>
+      <c r="C25" s="71"/>
+      <c r="D25" s="71"/>
+      <c r="E25" s="71"/>
+      <c r="F25" s="67" t="s">
+        <v>44</v>
+      </c>
+      <c r="G25" s="73"/>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" s="80">
+        <v>2</v>
+      </c>
+      <c r="B26" s="83">
+        <v>132</v>
+      </c>
+      <c r="C26" s="83">
+        <v>4</v>
+      </c>
+      <c r="D26" s="83" t="s">
+        <v>179</v>
+      </c>
+      <c r="E26" s="83" t="s">
+        <v>90</v>
+      </c>
+      <c r="F26" s="74" t="s">
+        <v>105</v>
+      </c>
+      <c r="G26" s="86"/>
+      <c r="H26" s="14"/>
+    </row>
+    <row r="27" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A27" s="79"/>
+      <c r="B27" s="82"/>
+      <c r="C27" s="82"/>
+      <c r="D27" s="82"/>
+      <c r="E27" s="82"/>
+      <c r="F27" s="74" t="s">
+        <v>44</v>
+      </c>
+      <c r="G27" s="85"/>
+      <c r="H27" s="15"/>
+    </row>
+    <row r="28" spans="1:12" ht="41.25" customHeight="1" thickBot="1">
+      <c r="A28" s="81"/>
+      <c r="B28" s="84"/>
+      <c r="C28" s="84"/>
+      <c r="D28" s="84"/>
+      <c r="E28" s="84"/>
+      <c r="F28" s="75" t="s">
+        <v>106</v>
+      </c>
+      <c r="G28" s="87"/>
+    </row>
+    <row r="29" spans="1:12" ht="15" customHeight="1">
+      <c r="A29" s="68">
+        <v>3</v>
+      </c>
+      <c r="B29" s="70">
+        <v>143</v>
+      </c>
+      <c r="C29" s="70">
+        <v>4</v>
+      </c>
+      <c r="D29" s="70" t="s">
+        <v>180</v>
+      </c>
+      <c r="E29" s="70" t="s">
+        <v>90</v>
+      </c>
+      <c r="F29" s="66" t="s">
+        <v>105</v>
+      </c>
+      <c r="G29" s="72"/>
+    </row>
+    <row r="30" spans="1:12" ht="26.45" customHeight="1">
+      <c r="A30" s="76"/>
+      <c r="B30" s="77"/>
+      <c r="C30" s="77"/>
+      <c r="D30" s="77"/>
+      <c r="E30" s="77"/>
+      <c r="F30" s="66" t="s">
+        <v>44</v>
+      </c>
+      <c r="G30" s="78"/>
     </row>
     <row r="31" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A31" s="48"/>
-      <c r="B31" s="50"/>
-      <c r="C31" s="50"/>
-      <c r="D31" s="50"/>
-      <c r="E31" s="50"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="46"/>
-      <c r="H31" s="15"/>
-    </row>
-    <row r="32" spans="1:12" ht="41.25" customHeight="1">
-      <c r="A32" s="52"/>
-      <c r="B32" s="55"/>
-      <c r="C32" s="55"/>
-      <c r="D32" s="55"/>
-      <c r="E32" s="55"/>
-      <c r="F32" s="22"/>
-      <c r="G32" s="58"/>
-    </row>
-    <row r="33" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A33" s="54"/>
-      <c r="B33" s="57"/>
-      <c r="C33" s="57"/>
-      <c r="D33" s="57"/>
-      <c r="E33" s="57"/>
-      <c r="F33" s="24"/>
-      <c r="G33" s="60"/>
-    </row>
-    <row r="34" spans="1:7" ht="26.45" customHeight="1">
-      <c r="A34" s="61"/>
-      <c r="B34" s="62"/>
-      <c r="C34" s="62"/>
-      <c r="D34" s="62"/>
-      <c r="E34" s="62"/>
-      <c r="F34" s="19"/>
-      <c r="G34" s="51"/>
+      <c r="A31" s="69"/>
+      <c r="B31" s="71"/>
+      <c r="C31" s="71"/>
+      <c r="D31" s="71"/>
+      <c r="E31" s="71"/>
+      <c r="F31" s="67" t="s">
+        <v>106</v>
+      </c>
+      <c r="G31" s="73"/>
+    </row>
+    <row r="32" spans="1:12" ht="30.75" customHeight="1">
+      <c r="A32" s="80">
+        <v>4</v>
+      </c>
+      <c r="B32" s="83">
+        <v>147</v>
+      </c>
+      <c r="C32" s="83">
+        <v>4</v>
+      </c>
+      <c r="D32" s="83" t="s">
+        <v>180</v>
+      </c>
+      <c r="E32" s="83" t="s">
+        <v>90</v>
+      </c>
+      <c r="F32" s="74" t="s">
+        <v>105</v>
+      </c>
+      <c r="G32" s="86"/>
+    </row>
+    <row r="33" spans="1:7" ht="26.45" customHeight="1" thickBot="1">
+      <c r="A33" s="81"/>
+      <c r="B33" s="84"/>
+      <c r="C33" s="84"/>
+      <c r="D33" s="84"/>
+      <c r="E33" s="84"/>
+      <c r="F33" s="75" t="s">
+        <v>44</v>
+      </c>
+      <c r="G33" s="87"/>
+    </row>
+    <row r="34" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A34" s="68">
+        <v>5</v>
+      </c>
+      <c r="B34" s="70">
+        <v>120</v>
+      </c>
+      <c r="C34" s="70">
+        <v>4</v>
+      </c>
+      <c r="D34" s="70" t="s">
+        <v>181</v>
+      </c>
+      <c r="E34" s="70" t="s">
+        <v>90</v>
+      </c>
+      <c r="F34" s="66" t="s">
+        <v>105</v>
+      </c>
+      <c r="G34" s="72"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="47"/>
-      <c r="B35" s="49"/>
-      <c r="C35" s="49"/>
-      <c r="D35" s="49"/>
-      <c r="E35" s="49"/>
-      <c r="F35" s="19"/>
-      <c r="G35" s="45"/>
-    </row>
-    <row r="36" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A36" s="48"/>
-      <c r="B36" s="50"/>
-      <c r="C36" s="50"/>
-      <c r="D36" s="50"/>
-      <c r="E36" s="50"/>
-      <c r="F36" s="20"/>
-      <c r="G36" s="46"/>
-    </row>
-    <row r="37" spans="1:7" ht="26.45" customHeight="1">
-      <c r="A37" s="52"/>
-      <c r="B37" s="55"/>
-      <c r="C37" s="55"/>
-      <c r="D37" s="55"/>
-      <c r="E37" s="55"/>
-      <c r="F37" s="22"/>
-      <c r="G37" s="58"/>
+      <c r="A35" s="76"/>
+      <c r="B35" s="77"/>
+      <c r="C35" s="77"/>
+      <c r="D35" s="77"/>
+      <c r="E35" s="77"/>
+      <c r="F35" s="66" t="s">
+        <v>44</v>
+      </c>
+      <c r="G35" s="78"/>
+    </row>
+    <row r="36" spans="1:7" ht="26.45" customHeight="1" thickBot="1">
+      <c r="A36" s="69"/>
+      <c r="B36" s="71"/>
+      <c r="C36" s="71"/>
+      <c r="D36" s="71"/>
+      <c r="E36" s="71"/>
+      <c r="F36" s="67" t="s">
+        <v>106</v>
+      </c>
+      <c r="G36" s="73"/>
+    </row>
+    <row r="37" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A37" s="80">
+        <v>6</v>
+      </c>
+      <c r="B37" s="83">
+        <v>120</v>
+      </c>
+      <c r="C37" s="83">
+        <v>4</v>
+      </c>
+      <c r="D37" s="83" t="s">
+        <v>182</v>
+      </c>
+      <c r="E37" s="83" t="s">
+        <v>90</v>
+      </c>
+      <c r="F37" s="74" t="s">
+        <v>105</v>
+      </c>
+      <c r="G37" s="86"/>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="53"/>
-      <c r="B38" s="56"/>
-      <c r="C38" s="56"/>
-      <c r="D38" s="56"/>
-      <c r="E38" s="56"/>
-      <c r="F38" s="22"/>
-      <c r="G38" s="59"/>
-    </row>
-    <row r="39" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A39" s="54"/>
-      <c r="B39" s="57"/>
-      <c r="C39" s="57"/>
-      <c r="D39" s="57"/>
-      <c r="E39" s="57"/>
-      <c r="F39" s="24"/>
-      <c r="G39" s="60"/>
-    </row>
-    <row r="40" spans="1:7" ht="26.45" customHeight="1">
-      <c r="A40" s="61"/>
-      <c r="B40" s="62"/>
-      <c r="C40" s="62"/>
-      <c r="D40" s="62"/>
-      <c r="E40" s="62"/>
-      <c r="F40" s="19"/>
-      <c r="G40" s="51"/>
+      <c r="A38" s="79"/>
+      <c r="B38" s="82"/>
+      <c r="C38" s="82"/>
+      <c r="D38" s="82"/>
+      <c r="E38" s="82"/>
+      <c r="F38" s="74" t="s">
+        <v>44</v>
+      </c>
+      <c r="G38" s="85"/>
+    </row>
+    <row r="39" spans="1:7" ht="26.45" customHeight="1" thickBot="1">
+      <c r="A39" s="81"/>
+      <c r="B39" s="84"/>
+      <c r="C39" s="84"/>
+      <c r="D39" s="84"/>
+      <c r="E39" s="84"/>
+      <c r="F39" s="75" t="s">
+        <v>106</v>
+      </c>
+      <c r="G39" s="87"/>
+    </row>
+    <row r="40" spans="1:7" ht="26.25" customHeight="1">
+      <c r="A40" s="68">
+        <v>7</v>
+      </c>
+      <c r="B40" s="70">
+        <v>148</v>
+      </c>
+      <c r="C40" s="70">
+        <v>4</v>
+      </c>
+      <c r="D40" s="70" t="s">
+        <v>107</v>
+      </c>
+      <c r="E40" s="70" t="s">
+        <v>90</v>
+      </c>
+      <c r="F40" s="66" t="s">
+        <v>105</v>
+      </c>
+      <c r="G40" s="72"/>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" s="47"/>
-      <c r="B41" s="49"/>
-      <c r="C41" s="49"/>
-      <c r="D41" s="49"/>
-      <c r="E41" s="49"/>
-      <c r="F41" s="19"/>
-      <c r="G41" s="45"/>
+      <c r="A41" s="76"/>
+      <c r="B41" s="77"/>
+      <c r="C41" s="77"/>
+      <c r="D41" s="77"/>
+      <c r="E41" s="77"/>
+      <c r="F41" s="66" t="s">
+        <v>44</v>
+      </c>
+      <c r="G41" s="78"/>
     </row>
     <row r="42" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A42" s="48"/>
-      <c r="B42" s="50"/>
-      <c r="C42" s="50"/>
-      <c r="D42" s="50"/>
-      <c r="E42" s="50"/>
-      <c r="F42" s="20"/>
-      <c r="G42" s="46"/>
-    </row>
-    <row r="43" spans="1:7" ht="26.45" customHeight="1">
-      <c r="A43" s="52"/>
-      <c r="B43" s="55"/>
-      <c r="C43" s="55"/>
-      <c r="D43" s="55"/>
-      <c r="E43" s="55"/>
-      <c r="F43" s="22"/>
-      <c r="G43" s="26"/>
-    </row>
-    <row r="44" spans="1:7">
-      <c r="A44" s="53"/>
-      <c r="B44" s="56"/>
-      <c r="C44" s="56"/>
-      <c r="D44" s="56"/>
-      <c r="E44" s="56"/>
-      <c r="F44" s="22"/>
-      <c r="G44" s="26"/>
-    </row>
-    <row r="45" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A45" s="54"/>
-      <c r="B45" s="57"/>
-      <c r="C45" s="57"/>
-      <c r="D45" s="57"/>
-      <c r="E45" s="57"/>
-      <c r="F45" s="24"/>
-      <c r="G45" s="27"/>
+      <c r="A42" s="69"/>
+      <c r="B42" s="71"/>
+      <c r="C42" s="71"/>
+      <c r="D42" s="71"/>
+      <c r="E42" s="71"/>
+      <c r="F42" s="67" t="s">
+        <v>106</v>
+      </c>
+      <c r="G42" s="73"/>
     </row>
   </sheetData>
-  <mergeCells count="47">
-    <mergeCell ref="A43:A45"/>
-    <mergeCell ref="B43:B45"/>
-    <mergeCell ref="C43:C45"/>
-    <mergeCell ref="D43:D45"/>
-    <mergeCell ref="E43:E45"/>
+  <mergeCells count="42">
     <mergeCell ref="G40:G42"/>
+    <mergeCell ref="E34:E36"/>
+    <mergeCell ref="G34:G36"/>
     <mergeCell ref="A37:A39"/>
     <mergeCell ref="B37:B39"/>
     <mergeCell ref="C37:C39"/>
     <mergeCell ref="D37:D39"/>
     <mergeCell ref="E37:E39"/>
     <mergeCell ref="G37:G39"/>
-    <mergeCell ref="A40:A42"/>
-    <mergeCell ref="B40:B42"/>
-    <mergeCell ref="C40:C42"/>
-    <mergeCell ref="D40:D42"/>
-    <mergeCell ref="E40:E42"/>
-    <mergeCell ref="G34:G36"/>
+    <mergeCell ref="E29:E31"/>
+    <mergeCell ref="G29:G31"/>
     <mergeCell ref="A32:A33"/>
     <mergeCell ref="B32:B33"/>
     <mergeCell ref="C32:C33"/>
     <mergeCell ref="D32:D33"/>
     <mergeCell ref="E32:E33"/>
     <mergeCell ref="G32:G33"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="B34:B36"/>
-    <mergeCell ref="C34:C36"/>
-    <mergeCell ref="D34:D36"/>
-    <mergeCell ref="E34:E36"/>
-    <mergeCell ref="G29:G31"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="G24:G25"/>
     <mergeCell ref="A26:A28"/>
     <mergeCell ref="B26:B28"/>
     <mergeCell ref="C26:C28"/>
     <mergeCell ref="D26:D28"/>
     <mergeCell ref="E26:E28"/>
     <mergeCell ref="G26:G28"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
     <mergeCell ref="A29:A31"/>
     <mergeCell ref="B29:B31"/>
     <mergeCell ref="C29:C31"/>
     <mergeCell ref="D29:D31"/>
-    <mergeCell ref="E29:E31"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="B34:B36"/>
+    <mergeCell ref="C34:C36"/>
+    <mergeCell ref="D34:D36"/>
+    <mergeCell ref="A40:A42"/>
+    <mergeCell ref="B40:B42"/>
+    <mergeCell ref="C40:C42"/>
+    <mergeCell ref="D40:D42"/>
+    <mergeCell ref="E40:E42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2926,8 +3385,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -3028,85 +3487,85 @@
       </c>
     </row>
     <row r="17" spans="1:12" ht="23.25">
-      <c r="A17" s="31" t="s">
+      <c r="A17" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="32"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="32"/>
-      <c r="J17" s="32"/>
-      <c r="K17" s="32"/>
-      <c r="L17" s="32"/>
+      <c r="B17" s="30"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="30"/>
+      <c r="K17" s="30"/>
+      <c r="L17" s="30"/>
     </row>
     <row r="18" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A18" s="32" t="s">
+      <c r="A18" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="32" t="s">
+      <c r="B18" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="32" t="s">
+      <c r="C18" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="32" t="s">
+      <c r="D18" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="E18" s="32" t="s">
+      <c r="E18" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="F18" s="32" t="s">
+      <c r="F18" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="G18" s="32" t="s">
+      <c r="G18" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="H18" s="32" t="s">
+      <c r="H18" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="I18" s="32" t="s">
+      <c r="I18" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="J18" s="32" t="s">
+      <c r="J18" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="K18" s="32" t="s">
+      <c r="K18" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="L18" s="32" t="s">
+      <c r="L18" s="30" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:12">
-      <c r="A19" s="33" t="s">
+      <c r="A19" s="31" t="s">
         <v>113</v>
       </c>
-      <c r="B19" s="33" t="s">
+      <c r="B19" s="31" t="s">
         <v>114</v>
       </c>
-      <c r="C19" s="33" t="s">
+      <c r="C19" s="31" t="s">
         <v>178</v>
       </c>
-      <c r="D19" s="33" t="s">
+      <c r="D19" s="31" t="s">
         <v>115</v>
       </c>
-      <c r="E19" s="32" t="s">
+      <c r="E19" s="30" t="s">
         <v>117</v>
       </c>
-      <c r="F19" s="33" t="s">
+      <c r="F19" s="31" t="s">
         <v>116</v>
       </c>
-      <c r="G19" s="33" t="s">
+      <c r="G19" s="31" t="s">
         <v>119</v>
       </c>
-      <c r="H19" s="32" t="s">
+      <c r="H19" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="I19" s="34" t="s">
+      <c r="I19" s="32" t="s">
         <v>123</v>
       </c>
       <c r="J19" s="8" t="s">
@@ -3120,7 +3579,7 @@
       </c>
     </row>
     <row r="20" spans="1:12" ht="14.25" customHeight="1">
-      <c r="I20" s="32"/>
+      <c r="I20" s="30"/>
     </row>
     <row r="21" spans="1:12" ht="23.25">
       <c r="A21" s="11" t="s">
@@ -3148,365 +3607,329 @@
       </c>
     </row>
     <row r="23" spans="1:12" ht="16.5" customHeight="1">
-      <c r="A23" s="70">
+      <c r="A23" s="63">
         <v>1</v>
       </c>
-      <c r="B23" s="71">
+      <c r="B23" s="64">
         <v>136</v>
       </c>
-      <c r="C23" s="71">
-        <v>2</v>
-      </c>
-      <c r="D23" s="71" t="s">
+      <c r="C23" s="64">
+        <v>2</v>
+      </c>
+      <c r="D23" s="64" t="s">
         <v>124</v>
       </c>
-      <c r="E23" s="71" t="s">
+      <c r="E23" s="64" t="s">
         <v>54</v>
       </c>
       <c r="F23" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="G23" s="64"/>
+      <c r="G23" s="65"/>
       <c r="K23" s="6"/>
     </row>
     <row r="24" spans="1:12" ht="26.45" customHeight="1" thickBot="1">
-      <c r="A24" s="67"/>
-      <c r="B24" s="69"/>
-      <c r="C24" s="69"/>
-      <c r="D24" s="69"/>
-      <c r="E24" s="69"/>
-      <c r="F24" s="35" t="s">
+      <c r="A24" s="62"/>
+      <c r="B24" s="58"/>
+      <c r="C24" s="58"/>
+      <c r="D24" s="58"/>
+      <c r="E24" s="58"/>
+      <c r="F24" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="G24" s="65"/>
+      <c r="G24" s="60"/>
     </row>
     <row r="25" spans="1:12" ht="27" customHeight="1">
-      <c r="A25" s="66">
-        <v>2</v>
-      </c>
-      <c r="B25" s="68">
+      <c r="A25" s="61">
+        <v>2</v>
+      </c>
+      <c r="B25" s="57">
         <v>120</v>
       </c>
-      <c r="C25" s="68">
-        <v>2</v>
-      </c>
-      <c r="D25" s="68" t="s">
+      <c r="C25" s="57">
+        <v>2</v>
+      </c>
+      <c r="D25" s="57" t="s">
         <v>126</v>
       </c>
-      <c r="E25" s="68" t="s">
+      <c r="E25" s="57" t="s">
         <v>54</v>
       </c>
       <c r="F25" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="G25" s="63"/>
+      <c r="G25" s="59"/>
     </row>
     <row r="26" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A26" s="67"/>
-      <c r="B26" s="69"/>
-      <c r="C26" s="69"/>
-      <c r="D26" s="69"/>
-      <c r="E26" s="69"/>
-      <c r="F26" s="35" t="s">
+      <c r="A26" s="62"/>
+      <c r="B26" s="58"/>
+      <c r="C26" s="58"/>
+      <c r="D26" s="58"/>
+      <c r="E26" s="58"/>
+      <c r="F26" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="G26" s="65"/>
+      <c r="G26" s="60"/>
     </row>
     <row r="27" spans="1:12" ht="27" customHeight="1">
-      <c r="A27" s="66">
+      <c r="A27" s="61">
         <v>3</v>
       </c>
-      <c r="B27" s="68">
+      <c r="B27" s="57">
         <v>120</v>
       </c>
-      <c r="C27" s="68">
-        <v>2</v>
-      </c>
-      <c r="D27" s="68" t="s">
+      <c r="C27" s="57">
+        <v>2</v>
+      </c>
+      <c r="D27" s="57" t="s">
         <v>127</v>
       </c>
-      <c r="E27" s="68" t="s">
+      <c r="E27" s="57" t="s">
         <v>54</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="G27" s="63"/>
+      <c r="G27" s="59"/>
     </row>
     <row r="28" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A28" s="67"/>
-      <c r="B28" s="69"/>
-      <c r="C28" s="69"/>
-      <c r="D28" s="69"/>
-      <c r="E28" s="69"/>
-      <c r="F28" s="35" t="s">
+      <c r="A28" s="62"/>
+      <c r="B28" s="58"/>
+      <c r="C28" s="58"/>
+      <c r="D28" s="58"/>
+      <c r="E28" s="58"/>
+      <c r="F28" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="G28" s="65"/>
+      <c r="G28" s="60"/>
     </row>
     <row r="29" spans="1:12">
-      <c r="A29" s="66">
+      <c r="A29" s="61">
         <v>4</v>
       </c>
-      <c r="B29" s="68">
+      <c r="B29" s="57">
         <v>136</v>
       </c>
-      <c r="C29" s="68">
-        <v>2</v>
-      </c>
-      <c r="D29" s="68" t="s">
+      <c r="C29" s="57">
+        <v>2</v>
+      </c>
+      <c r="D29" s="57" t="s">
         <v>127</v>
       </c>
-      <c r="E29" s="68" t="s">
+      <c r="E29" s="57" t="s">
         <v>54</v>
       </c>
       <c r="F29" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="G29" s="63"/>
+      <c r="G29" s="59"/>
     </row>
     <row r="30" spans="1:12" ht="41.25" customHeight="1">
-      <c r="A30" s="70"/>
-      <c r="B30" s="71"/>
-      <c r="C30" s="71"/>
-      <c r="D30" s="71"/>
-      <c r="E30" s="71"/>
+      <c r="A30" s="63"/>
+      <c r="B30" s="64"/>
+      <c r="C30" s="64"/>
+      <c r="D30" s="64"/>
+      <c r="E30" s="64"/>
       <c r="F30" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="G30" s="64"/>
+      <c r="G30" s="65"/>
     </row>
     <row r="31" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A31" s="67"/>
-      <c r="B31" s="69"/>
-      <c r="C31" s="69"/>
-      <c r="D31" s="69"/>
-      <c r="E31" s="69"/>
-      <c r="F31" s="35" t="s">
+      <c r="A31" s="62"/>
+      <c r="B31" s="58"/>
+      <c r="C31" s="58"/>
+      <c r="D31" s="58"/>
+      <c r="E31" s="58"/>
+      <c r="F31" s="33" t="s">
         <v>106</v>
       </c>
-      <c r="G31" s="65"/>
+      <c r="G31" s="60"/>
     </row>
     <row r="32" spans="1:12" ht="27" customHeight="1">
-      <c r="A32" s="66">
+      <c r="A32" s="61">
         <v>5</v>
       </c>
-      <c r="B32" s="68">
+      <c r="B32" s="57">
         <v>116</v>
       </c>
-      <c r="C32" s="68">
-        <v>2</v>
-      </c>
-      <c r="D32" s="68" t="s">
+      <c r="C32" s="57">
+        <v>2</v>
+      </c>
+      <c r="D32" s="57" t="s">
         <v>126</v>
       </c>
-      <c r="E32" s="68" t="s">
+      <c r="E32" s="57" t="s">
         <v>54</v>
       </c>
       <c r="F32" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="G32" s="63"/>
+      <c r="G32" s="59"/>
     </row>
     <row r="33" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A33" s="67"/>
-      <c r="B33" s="69"/>
-      <c r="C33" s="69"/>
-      <c r="D33" s="69"/>
-      <c r="E33" s="69"/>
-      <c r="F33" s="35" t="s">
+      <c r="A33" s="62"/>
+      <c r="B33" s="58"/>
+      <c r="C33" s="58"/>
+      <c r="D33" s="58"/>
+      <c r="E33" s="58"/>
+      <c r="F33" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="G33" s="65"/>
+      <c r="G33" s="60"/>
     </row>
     <row r="34" spans="1:7" ht="16.5" customHeight="1">
-      <c r="A34" s="66">
+      <c r="A34" s="61">
         <v>6</v>
       </c>
-      <c r="B34" s="68">
+      <c r="B34" s="57">
         <v>116</v>
       </c>
-      <c r="C34" s="68">
-        <v>2</v>
-      </c>
-      <c r="D34" s="68" t="s">
+      <c r="C34" s="57">
+        <v>2</v>
+      </c>
+      <c r="D34" s="57" t="s">
         <v>128</v>
       </c>
-      <c r="E34" s="68" t="s">
+      <c r="E34" s="57" t="s">
         <v>54</v>
       </c>
       <c r="F34" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="G34" s="63"/>
+      <c r="G34" s="59"/>
     </row>
     <row r="35" spans="1:7" ht="26.45" customHeight="1" thickBot="1">
-      <c r="A35" s="67"/>
-      <c r="B35" s="69"/>
-      <c r="C35" s="69"/>
-      <c r="D35" s="69"/>
-      <c r="E35" s="69"/>
-      <c r="F35" s="35" t="s">
+      <c r="A35" s="62"/>
+      <c r="B35" s="58"/>
+      <c r="C35" s="58"/>
+      <c r="D35" s="58"/>
+      <c r="E35" s="58"/>
+      <c r="F35" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="G35" s="65"/>
+      <c r="G35" s="60"/>
     </row>
     <row r="36" spans="1:7" ht="27" customHeight="1">
-      <c r="A36" s="66">
+      <c r="A36" s="61">
         <v>7</v>
       </c>
-      <c r="B36" s="68">
+      <c r="B36" s="57">
         <v>268</v>
       </c>
-      <c r="C36" s="68">
+      <c r="C36" s="57">
         <v>3</v>
       </c>
-      <c r="D36" s="68" t="s">
+      <c r="D36" s="57" t="s">
         <v>129</v>
       </c>
-      <c r="E36" s="68" t="s">
+      <c r="E36" s="57" t="s">
         <v>54</v>
       </c>
       <c r="F36" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="G36" s="36"/>
+      <c r="G36" s="34"/>
     </row>
     <row r="37" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A37" s="67"/>
-      <c r="B37" s="69"/>
-      <c r="C37" s="69"/>
-      <c r="D37" s="69"/>
-      <c r="E37" s="69"/>
-      <c r="F37" s="35" t="s">
+      <c r="A37" s="62"/>
+      <c r="B37" s="58"/>
+      <c r="C37" s="58"/>
+      <c r="D37" s="58"/>
+      <c r="E37" s="58"/>
+      <c r="F37" s="33" t="s">
         <v>106</v>
       </c>
-      <c r="G37" s="37"/>
+      <c r="G37" s="35"/>
     </row>
     <row r="38" spans="1:7" ht="26.45" customHeight="1">
-      <c r="A38" s="66">
+      <c r="A38" s="61">
         <v>7</v>
       </c>
-      <c r="B38" s="68">
+      <c r="B38" s="57">
         <v>148</v>
       </c>
-      <c r="C38" s="68">
+      <c r="C38" s="57">
         <v>4</v>
       </c>
-      <c r="D38" s="68" t="s">
+      <c r="D38" s="57" t="s">
         <v>107</v>
       </c>
-      <c r="E38" s="68" t="s">
+      <c r="E38" s="57" t="s">
         <v>90</v>
       </c>
       <c r="F38" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="G38" s="63"/>
+      <c r="G38" s="59"/>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39" s="70"/>
-      <c r="B39" s="71"/>
-      <c r="C39" s="71"/>
-      <c r="D39" s="71"/>
-      <c r="E39" s="71"/>
+      <c r="A39" s="63"/>
+      <c r="B39" s="64"/>
+      <c r="C39" s="64"/>
+      <c r="D39" s="64"/>
+      <c r="E39" s="64"/>
       <c r="F39" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="G39" s="64"/>
+      <c r="G39" s="65"/>
     </row>
     <row r="40" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A40" s="67"/>
-      <c r="B40" s="69"/>
-      <c r="C40" s="69"/>
-      <c r="D40" s="69"/>
-      <c r="E40" s="69"/>
-      <c r="F40" s="35" t="s">
+      <c r="A40" s="62"/>
+      <c r="B40" s="58"/>
+      <c r="C40" s="58"/>
+      <c r="D40" s="58"/>
+      <c r="E40" s="58"/>
+      <c r="F40" s="33" t="s">
         <v>106</v>
       </c>
-      <c r="G40" s="65"/>
+      <c r="G40" s="60"/>
     </row>
     <row r="41" spans="1:7" ht="26.45" customHeight="1">
-      <c r="A41" s="66">
+      <c r="A41" s="61">
         <v>8</v>
       </c>
-      <c r="B41" s="68">
+      <c r="B41" s="57">
         <v>147</v>
       </c>
-      <c r="C41" s="68">
+      <c r="C41" s="57">
         <v>4</v>
       </c>
-      <c r="D41" s="68" t="s">
+      <c r="D41" s="57" t="s">
         <v>108</v>
       </c>
-      <c r="E41" s="68" t="s">
+      <c r="E41" s="57" t="s">
         <v>90</v>
       </c>
       <c r="F41" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="G41" s="36"/>
+      <c r="G41" s="34"/>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="70"/>
-      <c r="B42" s="71"/>
-      <c r="C42" s="71"/>
-      <c r="D42" s="71"/>
-      <c r="E42" s="71"/>
+      <c r="A42" s="63"/>
+      <c r="B42" s="64"/>
+      <c r="C42" s="64"/>
+      <c r="D42" s="64"/>
+      <c r="E42" s="64"/>
       <c r="F42" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="G42" s="36"/>
+      <c r="G42" s="34"/>
     </row>
     <row r="43" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A43" s="67"/>
-      <c r="B43" s="69"/>
-      <c r="C43" s="69"/>
-      <c r="D43" s="69"/>
-      <c r="E43" s="69"/>
-      <c r="F43" s="35" t="s">
+      <c r="A43" s="62"/>
+      <c r="B43" s="58"/>
+      <c r="C43" s="58"/>
+      <c r="D43" s="58"/>
+      <c r="E43" s="58"/>
+      <c r="F43" s="33" t="s">
         <v>106</v>
       </c>
-      <c r="G43" s="37"/>
+      <c r="G43" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="52">
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="G32:G33"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="G34:G35"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="G25:G26"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="C41:C43"/>
-    <mergeCell ref="D41:D43"/>
-    <mergeCell ref="E41:E43"/>
-    <mergeCell ref="G38:G40"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="A38:A40"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="C38:C40"/>
-    <mergeCell ref="D38:D40"/>
-    <mergeCell ref="E38:E40"/>
-    <mergeCell ref="E36:E37"/>
     <mergeCell ref="G29:G31"/>
     <mergeCell ref="G23:G24"/>
     <mergeCell ref="A25:A26"/>
@@ -3523,6 +3946,42 @@
     <mergeCell ref="D23:D24"/>
     <mergeCell ref="E23:E24"/>
     <mergeCell ref="D25:D26"/>
+    <mergeCell ref="G38:G40"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="D38:D40"/>
+    <mergeCell ref="E38:E40"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="C41:C43"/>
+    <mergeCell ref="D41:D43"/>
+    <mergeCell ref="E41:E43"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="G25:G26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="G34:G35"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="D32:D33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3533,7 +3992,7 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -3621,61 +4080,61 @@
       <c r="A12" s="8"/>
     </row>
     <row r="17" spans="1:12" ht="23.25">
-      <c r="A17" s="31" t="s">
+      <c r="A17" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="32"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="32"/>
-      <c r="J17" s="32"/>
-      <c r="K17" s="32"/>
-      <c r="L17" s="32"/>
+      <c r="B17" s="30"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="30"/>
+      <c r="K17" s="30"/>
+      <c r="L17" s="30"/>
     </row>
     <row r="18" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A18" s="32" t="s">
+      <c r="A18" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="32" t="s">
+      <c r="B18" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="32" t="s">
+      <c r="C18" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="32" t="s">
+      <c r="D18" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="E18" s="32" t="s">
+      <c r="E18" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="F18" s="32" t="s">
+      <c r="F18" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="G18" s="32" t="s">
+      <c r="G18" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="H18" s="32" t="s">
+      <c r="H18" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="I18" s="32" t="s">
+      <c r="I18" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="J18" s="32" t="s">
+      <c r="J18" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="K18" s="32" t="s">
+      <c r="K18" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="L18" s="32" t="s">
+      <c r="L18" s="30" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="15.75">
-      <c r="A19" s="33" t="s">
+      <c r="A19" s="31" t="s">
         <v>131</v>
       </c>
       <c r="B19" s="8" t="s">
@@ -3687,7 +4146,7 @@
       <c r="D19" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="E19" s="32" t="s">
+      <c r="E19" s="30" t="s">
         <v>135</v>
       </c>
       <c r="F19" s="8" t="s">
@@ -3696,24 +4155,24 @@
       <c r="G19" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="H19" s="32" t="s">
+      <c r="H19" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="I19" s="41" t="s">
+      <c r="I19" s="39" t="s">
         <v>138</v>
       </c>
-      <c r="J19" s="41" t="s">
+      <c r="J19" s="39" t="s">
         <v>139</v>
       </c>
-      <c r="K19" s="41" t="s">
+      <c r="K19" s="39" t="s">
         <v>140</v>
       </c>
-      <c r="L19" s="42" t="s">
+      <c r="L19" s="40" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="14.25" customHeight="1">
-      <c r="I20" s="32"/>
+      <c r="I20" s="30"/>
     </row>
     <row r="21" spans="1:12" ht="23.25">
       <c r="A21" s="11" t="s">
@@ -3741,165 +4200,171 @@
       </c>
     </row>
     <row r="23" spans="1:12" ht="16.5" customHeight="1">
-      <c r="A23" s="66">
+      <c r="A23" s="61">
         <v>1</v>
       </c>
-      <c r="B23" s="68">
+      <c r="B23" s="57">
         <v>291</v>
       </c>
-      <c r="C23" s="68">
+      <c r="C23" s="57">
         <v>0</v>
       </c>
-      <c r="D23" s="68" t="s">
+      <c r="D23" s="57" t="s">
         <v>142</v>
       </c>
-      <c r="E23" s="68" t="s">
+      <c r="E23" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="F23" s="40" t="s">
+      <c r="F23" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="G23" s="63"/>
+      <c r="G23" s="59"/>
       <c r="K23" s="6"/>
     </row>
     <row r="24" spans="1:12" ht="26.45" customHeight="1" thickBot="1">
-      <c r="A24" s="67"/>
-      <c r="B24" s="69"/>
-      <c r="C24" s="69"/>
-      <c r="D24" s="69"/>
-      <c r="E24" s="69"/>
-      <c r="F24" s="35" t="s">
+      <c r="A24" s="62"/>
+      <c r="B24" s="58"/>
+      <c r="C24" s="58"/>
+      <c r="D24" s="58"/>
+      <c r="E24" s="58"/>
+      <c r="F24" s="33" t="s">
         <v>106</v>
       </c>
-      <c r="G24" s="65"/>
+      <c r="G24" s="60"/>
     </row>
     <row r="25" spans="1:12" ht="27" customHeight="1">
-      <c r="A25" s="66">
-        <v>2</v>
-      </c>
-      <c r="B25" s="68">
+      <c r="A25" s="61">
+        <v>2</v>
+      </c>
+      <c r="B25" s="57">
         <v>121</v>
       </c>
-      <c r="C25" s="68">
+      <c r="C25" s="57">
         <v>0</v>
       </c>
-      <c r="D25" s="68" t="s">
+      <c r="D25" s="57" t="s">
         <v>143</v>
       </c>
-      <c r="E25" s="68"/>
+      <c r="E25" s="57"/>
       <c r="F25" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="G25" s="63"/>
+      <c r="G25" s="59"/>
     </row>
     <row r="26" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A26" s="67"/>
-      <c r="B26" s="69"/>
-      <c r="C26" s="69"/>
-      <c r="D26" s="69"/>
-      <c r="E26" s="69"/>
-      <c r="F26" s="35" t="s">
+      <c r="A26" s="62"/>
+      <c r="B26" s="58"/>
+      <c r="C26" s="58"/>
+      <c r="D26" s="58"/>
+      <c r="E26" s="58"/>
+      <c r="F26" s="33" t="s">
         <v>106</v>
       </c>
-      <c r="G26" s="65"/>
+      <c r="G26" s="60"/>
     </row>
     <row r="27" spans="1:12" ht="27" customHeight="1">
-      <c r="A27" s="66">
+      <c r="A27" s="61">
         <v>3</v>
       </c>
-      <c r="B27" s="68">
+      <c r="B27" s="57">
         <v>89</v>
       </c>
-      <c r="C27" s="68">
-        <v>2</v>
-      </c>
-      <c r="D27" s="68" t="s">
+      <c r="C27" s="57">
+        <v>2</v>
+      </c>
+      <c r="D27" s="57" t="s">
         <v>144</v>
       </c>
-      <c r="E27" s="68" t="s">
+      <c r="E27" s="57" t="s">
         <v>54</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="G27" s="63"/>
+      <c r="G27" s="59"/>
     </row>
     <row r="28" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A28" s="67"/>
-      <c r="B28" s="69"/>
-      <c r="C28" s="69"/>
-      <c r="D28" s="69"/>
-      <c r="E28" s="69"/>
-      <c r="F28" s="35" t="s">
+      <c r="A28" s="62"/>
+      <c r="B28" s="58"/>
+      <c r="C28" s="58"/>
+      <c r="D28" s="58"/>
+      <c r="E28" s="58"/>
+      <c r="F28" s="33" t="s">
         <v>106</v>
       </c>
-      <c r="G28" s="65"/>
+      <c r="G28" s="60"/>
     </row>
     <row r="29" spans="1:12" ht="43.5" thickBot="1">
-      <c r="A29" s="38">
+      <c r="A29" s="36">
         <v>4</v>
       </c>
-      <c r="B29" s="35">
+      <c r="B29" s="33">
         <v>89</v>
       </c>
-      <c r="C29" s="35">
-        <v>2</v>
-      </c>
-      <c r="D29" s="35" t="s">
+      <c r="C29" s="33">
+        <v>2</v>
+      </c>
+      <c r="D29" s="33" t="s">
         <v>144</v>
       </c>
-      <c r="E29" s="35" t="s">
+      <c r="E29" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="F29" s="35" t="s">
+      <c r="F29" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="G29" s="39"/>
+      <c r="G29" s="37"/>
     </row>
     <row r="30" spans="1:12" ht="41.25" customHeight="1" thickBot="1">
-      <c r="A30" s="38">
+      <c r="A30" s="36">
         <v>5</v>
       </c>
-      <c r="B30" s="35">
+      <c r="B30" s="33">
         <v>89</v>
       </c>
-      <c r="C30" s="35">
-        <v>2</v>
-      </c>
-      <c r="D30" s="35" t="s">
+      <c r="C30" s="33">
+        <v>2</v>
+      </c>
+      <c r="D30" s="33" t="s">
         <v>144</v>
       </c>
-      <c r="E30" s="35" t="s">
+      <c r="E30" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="F30" s="35" t="s">
+      <c r="F30" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="G30" s="39"/>
+      <c r="G30" s="37"/>
     </row>
     <row r="31" spans="1:12" ht="43.5" thickBot="1">
-      <c r="A31" s="38">
+      <c r="A31" s="36">
         <v>6</v>
       </c>
-      <c r="B31" s="35">
+      <c r="B31" s="33">
         <v>89</v>
       </c>
-      <c r="C31" s="35">
-        <v>2</v>
-      </c>
-      <c r="D31" s="35" t="s">
+      <c r="C31" s="33">
+        <v>2</v>
+      </c>
+      <c r="D31" s="33" t="s">
         <v>144</v>
       </c>
-      <c r="E31" s="35" t="s">
+      <c r="E31" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="F31" s="35" t="s">
+      <c r="F31" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="G31" s="37"/>
+      <c r="G31" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
     <mergeCell ref="G27:G28"/>
     <mergeCell ref="A25:A26"/>
     <mergeCell ref="B25:B26"/>
@@ -3912,12 +4377,6 @@
     <mergeCell ref="C27:C28"/>
     <mergeCell ref="D27:D28"/>
     <mergeCell ref="E27:E28"/>
-    <mergeCell ref="G23:G24"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3928,7 +4387,7 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4021,56 +4480,56 @@
       </c>
     </row>
     <row r="17" spans="1:12" ht="23.25">
-      <c r="A17" s="31" t="s">
+      <c r="A17" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="32"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="32"/>
-      <c r="J17" s="32"/>
-      <c r="K17" s="32"/>
-      <c r="L17" s="32"/>
+      <c r="B17" s="30"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="30"/>
+      <c r="K17" s="30"/>
+      <c r="L17" s="30"/>
     </row>
     <row r="18" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A18" s="32" t="s">
+      <c r="A18" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="32" t="s">
+      <c r="B18" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="32" t="s">
+      <c r="C18" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="32" t="s">
+      <c r="D18" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="E18" s="32" t="s">
+      <c r="E18" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="F18" s="32" t="s">
+      <c r="F18" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="G18" s="32" t="s">
+      <c r="G18" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="H18" s="32" t="s">
+      <c r="H18" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="I18" s="32" t="s">
+      <c r="I18" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="J18" s="32" t="s">
+      <c r="J18" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="K18" s="32" t="s">
+      <c r="K18" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="L18" s="32" t="s">
+      <c r="L18" s="30" t="s">
         <v>29</v>
       </c>
     </row>
@@ -4087,7 +4546,7 @@
       <c r="D19" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="E19" s="32" t="s">
+      <c r="E19" s="30" t="s">
         <v>152</v>
       </c>
       <c r="F19" s="1" t="s">
@@ -4096,7 +4555,7 @@
       <c r="G19" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="H19" s="32" t="s">
+      <c r="H19" s="30" t="s">
         <v>33</v>
       </c>
       <c r="I19" s="1" t="s">
@@ -4113,7 +4572,7 @@
       </c>
     </row>
     <row r="20" spans="1:12" ht="14.25" customHeight="1">
-      <c r="I20" s="32"/>
+      <c r="I20" s="30"/>
     </row>
     <row r="21" spans="1:12" ht="23.25">
       <c r="A21" s="11" t="s">
@@ -4141,28 +4600,28 @@
       </c>
     </row>
     <row r="23" spans="1:12" ht="16.5" customHeight="1">
-      <c r="A23" s="43"/>
-      <c r="B23" s="44"/>
-      <c r="C23" s="44"/>
-      <c r="D23" s="44"/>
-      <c r="E23" s="44"/>
-      <c r="F23" s="44"/>
+      <c r="A23" s="41"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="42"/>
+      <c r="D23" s="42"/>
+      <c r="E23" s="42"/>
+      <c r="F23" s="42"/>
       <c r="J23" s="6"/>
     </row>
     <row r="24" spans="1:12" ht="30.2" customHeight="1">
-      <c r="A24" s="47">
+      <c r="A24" s="52">
         <v>1</v>
       </c>
-      <c r="B24" s="49">
+      <c r="B24" s="55">
         <v>105</v>
       </c>
-      <c r="C24" s="49">
-        <v>2</v>
-      </c>
-      <c r="D24" s="49" t="s">
+      <c r="C24" s="55">
+        <v>2</v>
+      </c>
+      <c r="D24" s="55" t="s">
         <v>157</v>
       </c>
-      <c r="E24" s="49" t="s">
+      <c r="E24" s="55" t="s">
         <v>55</v>
       </c>
       <c r="F24" s="19" t="s">
@@ -4170,17 +4629,17 @@
       </c>
     </row>
     <row r="25" spans="1:12" ht="27" customHeight="1" thickBot="1">
-      <c r="A25" s="48"/>
-      <c r="B25" s="50"/>
-      <c r="C25" s="50"/>
-      <c r="D25" s="50"/>
-      <c r="E25" s="50"/>
+      <c r="A25" s="53"/>
+      <c r="B25" s="56"/>
+      <c r="C25" s="56"/>
+      <c r="D25" s="56"/>
+      <c r="E25" s="56"/>
       <c r="F25" s="20" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="57.75" thickBot="1">
-      <c r="A26" s="30">
+      <c r="A26" s="28">
         <v>2</v>
       </c>
       <c r="B26" s="24">
@@ -4200,19 +4659,19 @@
       </c>
     </row>
     <row r="27" spans="1:12" ht="41.25" customHeight="1">
-      <c r="A27" s="61">
+      <c r="A27" s="51">
         <v>3</v>
       </c>
-      <c r="B27" s="62">
+      <c r="B27" s="54">
         <v>262</v>
       </c>
-      <c r="C27" s="62">
-        <v>2</v>
-      </c>
-      <c r="D27" s="62" t="s">
+      <c r="C27" s="54">
+        <v>2</v>
+      </c>
+      <c r="D27" s="54" t="s">
         <v>158</v>
       </c>
-      <c r="E27" s="62" t="s">
+      <c r="E27" s="54" t="s">
         <v>55</v>
       </c>
       <c r="F27" s="19" t="s">
@@ -4220,29 +4679,29 @@
       </c>
     </row>
     <row r="28" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A28" s="48"/>
-      <c r="B28" s="50"/>
-      <c r="C28" s="50"/>
-      <c r="D28" s="50"/>
-      <c r="E28" s="50"/>
+      <c r="A28" s="53"/>
+      <c r="B28" s="56"/>
+      <c r="C28" s="56"/>
+      <c r="D28" s="56"/>
+      <c r="E28" s="56"/>
       <c r="F28" s="20" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A29" s="52">
+      <c r="A29" s="43">
         <v>4</v>
       </c>
-      <c r="B29" s="55">
+      <c r="B29" s="45">
         <v>262</v>
       </c>
-      <c r="C29" s="55">
-        <v>2</v>
-      </c>
-      <c r="D29" s="55" t="s">
+      <c r="C29" s="45">
+        <v>2</v>
+      </c>
+      <c r="D29" s="45" t="s">
         <v>158</v>
       </c>
-      <c r="E29" s="55" t="s">
+      <c r="E29" s="45" t="s">
         <v>55</v>
       </c>
       <c r="F29" s="22" t="s">
@@ -4250,17 +4709,17 @@
       </c>
     </row>
     <row r="30" spans="1:12" ht="41.25" customHeight="1" thickBot="1">
-      <c r="A30" s="54"/>
-      <c r="B30" s="57"/>
-      <c r="C30" s="57"/>
-      <c r="D30" s="57"/>
-      <c r="E30" s="57"/>
+      <c r="A30" s="44"/>
+      <c r="B30" s="46"/>
+      <c r="C30" s="46"/>
+      <c r="D30" s="46"/>
+      <c r="E30" s="46"/>
       <c r="F30" s="24" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="57.75" thickBot="1">
-      <c r="A31" s="29">
+      <c r="A31" s="27">
         <v>5</v>
       </c>
       <c r="B31" s="20">
@@ -4281,21 +4740,21 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
     <mergeCell ref="A29:A30"/>
     <mergeCell ref="B29:B30"/>
     <mergeCell ref="C29:C30"/>
     <mergeCell ref="D29:D30"/>
     <mergeCell ref="E29:E30"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4305,8 +4764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4394,56 +4853,56 @@
       <c r="A12" s="1"/>
     </row>
     <row r="17" spans="1:12" ht="23.25">
-      <c r="A17" s="31" t="s">
+      <c r="A17" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="32"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="32"/>
-      <c r="J17" s="32"/>
-      <c r="K17" s="32"/>
-      <c r="L17" s="32"/>
+      <c r="B17" s="30"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="30"/>
+      <c r="K17" s="30"/>
+      <c r="L17" s="30"/>
     </row>
     <row r="18" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A18" s="32" t="s">
+      <c r="A18" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="32" t="s">
+      <c r="B18" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="32" t="s">
+      <c r="C18" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="32" t="s">
+      <c r="D18" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="E18" s="32" t="s">
+      <c r="E18" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="F18" s="32" t="s">
+      <c r="F18" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="G18" s="32" t="s">
+      <c r="G18" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="H18" s="32" t="s">
+      <c r="H18" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="I18" s="32" t="s">
+      <c r="I18" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="J18" s="32" t="s">
+      <c r="J18" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="K18" s="32" t="s">
+      <c r="K18" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="L18" s="32" t="s">
+      <c r="L18" s="30" t="s">
         <v>29</v>
       </c>
     </row>
@@ -4460,7 +4919,7 @@
       <c r="D19" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="E19" s="32" t="s">
+      <c r="E19" s="30" t="s">
         <v>152</v>
       </c>
       <c r="F19" s="1" t="s">
@@ -4469,7 +4928,7 @@
       <c r="G19" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="H19" s="32" t="s">
+      <c r="H19" s="30" t="s">
         <v>33</v>
       </c>
       <c r="I19" s="18" t="s">
@@ -4481,12 +4940,12 @@
       <c r="K19" s="18" t="s">
         <v>170</v>
       </c>
-      <c r="L19" s="28" t="s">
+      <c r="L19" s="26" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="14.25" customHeight="1">
-      <c r="I20" s="32"/>
+      <c r="I20" s="30"/>
     </row>
     <row r="21" spans="1:12" ht="23.25">
       <c r="A21" s="11" t="s">
@@ -4514,71 +4973,71 @@
       </c>
     </row>
     <row r="23" spans="1:12" ht="30.2" customHeight="1">
-      <c r="A23" s="61">
+      <c r="A23" s="51">
         <v>1</v>
       </c>
-      <c r="B23" s="62">
+      <c r="B23" s="54">
         <v>301</v>
       </c>
-      <c r="C23" s="62">
-        <v>2</v>
-      </c>
-      <c r="D23" s="62" t="s">
+      <c r="C23" s="54">
+        <v>2</v>
+      </c>
+      <c r="D23" s="54" t="s">
         <v>172</v>
       </c>
-      <c r="E23" s="62" t="s">
+      <c r="E23" s="54" t="s">
         <v>55</v>
       </c>
       <c r="F23" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="G23" s="51"/>
+      <c r="G23" s="47"/>
     </row>
     <row r="24" spans="1:12" ht="27" customHeight="1" thickBot="1">
-      <c r="A24" s="48"/>
-      <c r="B24" s="50"/>
-      <c r="C24" s="50"/>
-      <c r="D24" s="50"/>
-      <c r="E24" s="50"/>
+      <c r="A24" s="53"/>
+      <c r="B24" s="56"/>
+      <c r="C24" s="56"/>
+      <c r="D24" s="56"/>
+      <c r="E24" s="56"/>
       <c r="F24" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="G24" s="46"/>
+      <c r="G24" s="48"/>
     </row>
     <row r="25" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A25" s="52">
-        <v>2</v>
-      </c>
-      <c r="B25" s="55">
+      <c r="A25" s="43">
+        <v>2</v>
+      </c>
+      <c r="B25" s="45">
         <v>193</v>
       </c>
-      <c r="C25" s="55">
-        <v>2</v>
-      </c>
-      <c r="D25" s="55" t="s">
+      <c r="C25" s="45">
+        <v>2</v>
+      </c>
+      <c r="D25" s="45" t="s">
         <v>173</v>
       </c>
-      <c r="E25" s="55" t="s">
+      <c r="E25" s="45" t="s">
         <v>55</v>
       </c>
       <c r="F25" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="G25" s="58"/>
+      <c r="G25" s="49"/>
     </row>
     <row r="26" spans="1:12" ht="41.25" customHeight="1" thickBot="1">
-      <c r="A26" s="54"/>
-      <c r="B26" s="57"/>
-      <c r="C26" s="57"/>
-      <c r="D26" s="57"/>
-      <c r="E26" s="57"/>
+      <c r="A26" s="44"/>
+      <c r="B26" s="46"/>
+      <c r="C26" s="46"/>
+      <c r="D26" s="46"/>
+      <c r="E26" s="46"/>
       <c r="F26" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="G26" s="60"/>
+      <c r="G26" s="50"/>
     </row>
     <row r="27" spans="1:12" ht="57.75" thickBot="1">
-      <c r="A27" s="29">
+      <c r="A27" s="27">
         <v>3</v>
       </c>
       <c r="B27" s="20">
@@ -4599,71 +5058,71 @@
       <c r="G27" s="21"/>
     </row>
     <row r="28" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A28" s="52">
+      <c r="A28" s="43">
         <v>4</v>
       </c>
-      <c r="B28" s="55">
+      <c r="B28" s="45">
         <v>114</v>
       </c>
-      <c r="C28" s="55">
-        <v>2</v>
-      </c>
-      <c r="D28" s="55" t="s">
+      <c r="C28" s="45">
+        <v>2</v>
+      </c>
+      <c r="D28" s="45" t="s">
         <v>175</v>
       </c>
-      <c r="E28" s="55" t="s">
+      <c r="E28" s="45" t="s">
         <v>55</v>
       </c>
       <c r="F28" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="G28" s="58"/>
+      <c r="G28" s="49"/>
     </row>
     <row r="29" spans="1:12" ht="41.25" customHeight="1" thickBot="1">
-      <c r="A29" s="54"/>
-      <c r="B29" s="57"/>
-      <c r="C29" s="57"/>
-      <c r="D29" s="57"/>
-      <c r="E29" s="57"/>
+      <c r="A29" s="44"/>
+      <c r="B29" s="46"/>
+      <c r="C29" s="46"/>
+      <c r="D29" s="46"/>
+      <c r="E29" s="46"/>
       <c r="F29" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="G29" s="60"/>
+      <c r="G29" s="50"/>
     </row>
     <row r="30" spans="1:12" ht="41.25" customHeight="1">
-      <c r="A30" s="61">
+      <c r="A30" s="51">
         <v>5</v>
       </c>
-      <c r="B30" s="62">
+      <c r="B30" s="54">
         <v>114</v>
       </c>
-      <c r="C30" s="62">
-        <v>2</v>
-      </c>
-      <c r="D30" s="62" t="s">
+      <c r="C30" s="54">
+        <v>2</v>
+      </c>
+      <c r="D30" s="54" t="s">
         <v>175</v>
       </c>
-      <c r="E30" s="62" t="s">
+      <c r="E30" s="54" t="s">
         <v>55</v>
       </c>
       <c r="F30" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="G30" s="51"/>
+      <c r="G30" s="47"/>
     </row>
     <row r="31" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A31" s="48"/>
-      <c r="B31" s="50"/>
-      <c r="C31" s="50"/>
-      <c r="D31" s="50"/>
-      <c r="E31" s="50"/>
+      <c r="A31" s="53"/>
+      <c r="B31" s="56"/>
+      <c r="C31" s="56"/>
+      <c r="D31" s="56"/>
+      <c r="E31" s="56"/>
       <c r="F31" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="G31" s="46"/>
+      <c r="G31" s="48"/>
     </row>
     <row r="32" spans="1:12" ht="57.75" thickBot="1">
-      <c r="A32" s="30">
+      <c r="A32" s="28">
         <v>6</v>
       </c>
       <c r="B32" s="24">
@@ -4684,7 +5143,7 @@
       <c r="G32" s="25"/>
     </row>
     <row r="33" spans="1:7" ht="57.75" thickBot="1">
-      <c r="A33" s="29">
+      <c r="A33" s="27">
         <v>7</v>
       </c>
       <c r="B33" s="20">
@@ -4706,6 +5165,18 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="G25:G26"/>
     <mergeCell ref="G28:G29"/>
     <mergeCell ref="A30:A31"/>
     <mergeCell ref="B30:B31"/>
@@ -4718,18 +5189,6 @@
     <mergeCell ref="C28:C29"/>
     <mergeCell ref="D28:D29"/>
     <mergeCell ref="E28:E29"/>
-    <mergeCell ref="G23:G24"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="G25:G26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>